<commit_message>
Update CDC Press and COVID-19 Statistic on 20200830
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -563,7 +563,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5338" uniqueCount="1760">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5350" uniqueCount="1764">
   <si>
     <t>案例</t>
   </si>
@@ -6549,6 +6549,19 @@
   </si>
   <si>
     <t xml:space="preserve">國內新增1例境外移入COVID-19個案，女赴墨西哥工作返國確診 </t>
+  </si>
+  <si>
+    <t>#488</t>
+  </si>
+  <si>
+    <t>2月-8/27 菲律賓</t>
+  </si>
+  <si>
+    <t>8/27 採檢
+8/29 確診</t>
+  </si>
+  <si>
+    <t>新增1例境外移入COVID-19病例，男赴菲工作返國確診</t>
   </si>
 </sst>
 </file>
@@ -6876,13 +6889,13 @@
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="17" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0" vertical="center"/>
@@ -35888,7 +35901,7 @@
       <c r="G487" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H487" s="63" t="s">
+      <c r="H487" s="8" t="s">
         <v>1750</v>
       </c>
       <c r="I487" s="9">
@@ -35925,7 +35938,7 @@
       </c>
     </row>
     <row r="488">
-      <c r="A488" s="64" t="s">
+      <c r="A488" s="16" t="s">
         <v>1754</v>
       </c>
       <c r="B488" s="6">
@@ -35934,7 +35947,7 @@
       <c r="C488" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D488" s="65" t="s">
+      <c r="D488" s="7" t="s">
         <v>76</v>
       </c>
       <c r="E488" s="7" t="s">
@@ -35944,29 +35957,29 @@
       <c r="G488" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H488" s="63" t="s">
+      <c r="H488" s="8" t="s">
         <v>1755</v>
       </c>
-      <c r="I488" s="66">
+      <c r="I488" s="9">
         <v>44062.0</v>
       </c>
       <c r="J488" s="10">
         <v>44027.0</v>
       </c>
-      <c r="K488" s="67" t="s">
+      <c r="K488" s="13" t="s">
         <v>1756</v>
       </c>
-      <c r="L488" s="68" t="s">
+      <c r="L488" s="12" t="s">
         <v>363</v>
       </c>
-      <c r="M488" s="67" t="s">
+      <c r="M488" s="13" t="s">
         <v>1757</v>
       </c>
       <c r="N488" s="25"/>
-      <c r="O488" s="63" t="s">
+      <c r="O488" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P488" s="63" t="s">
+      <c r="P488" s="8" t="s">
         <v>1758</v>
       </c>
       <c r="Q488" s="19"/>
@@ -35981,29 +35994,59 @@
       </c>
     </row>
     <row r="489">
-      <c r="A489" s="69"/>
-      <c r="B489" s="70"/>
-      <c r="C489" s="34"/>
-      <c r="D489" s="34"/>
-      <c r="E489" s="34"/>
+      <c r="A489" s="63" t="s">
+        <v>1760</v>
+      </c>
+      <c r="B489" s="6">
+        <v>44072.0</v>
+      </c>
+      <c r="C489" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D489" s="64" t="s">
+        <v>59</v>
+      </c>
+      <c r="E489" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F489" s="34"/>
-      <c r="G489" s="34"/>
-      <c r="H489" s="21"/>
-      <c r="I489" s="19"/>
-      <c r="J489" s="10"/>
-      <c r="K489" s="22"/>
-      <c r="L489" s="23"/>
-      <c r="M489" s="22"/>
+      <c r="G489" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H489" s="65" t="s">
+        <v>1761</v>
+      </c>
+      <c r="I489" s="66">
+        <v>44070.0</v>
+      </c>
+      <c r="J489" s="10">
+        <v>44063.0</v>
+      </c>
+      <c r="K489" s="67" t="s">
+        <v>1762</v>
+      </c>
+      <c r="L489" s="68" t="s">
+        <v>363</v>
+      </c>
+      <c r="M489" s="67" t="s">
+        <v>518</v>
+      </c>
       <c r="N489" s="25"/>
-      <c r="O489" s="21"/>
-      <c r="P489" s="21"/>
+      <c r="O489" s="65" t="s">
+        <v>85</v>
+      </c>
+      <c r="P489" s="65" t="s">
+        <v>334</v>
+      </c>
       <c r="Q489" s="19"/>
       <c r="R489" s="19"/>
-      <c r="S489" s="20"/>
+      <c r="S489" s="61" t="s">
+        <v>1763</v>
+      </c>
       <c r="T489" s="20"/>
       <c r="U489" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#488</v>
       </c>
     </row>
     <row r="490">
@@ -36689,15 +36732,16 @@
     <hyperlink r:id="rId48" ref="S486"/>
     <hyperlink r:id="rId49" ref="S487"/>
     <hyperlink r:id="rId50" ref="S488"/>
+    <hyperlink r:id="rId51" ref="S489"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId51"/>
-  <legacyDrawing r:id="rId52"/>
+  <drawing r:id="rId52"/>
+  <legacyDrawing r:id="rId53"/>
   <tableParts count="2">
-    <tablePart r:id="rId55"/>
     <tablePart r:id="rId56"/>
+    <tablePart r:id="rId57"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20200903
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -563,7 +563,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5350" uniqueCount="1764">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5363" uniqueCount="1769">
   <si>
     <t>案例</t>
   </si>
@@ -6562,6 +6562,23 @@
   </si>
   <si>
     <t>新增1例境外移入COVID-19病例，男赴菲工作返國確診</t>
+  </si>
+  <si>
+    <t>#489</t>
+  </si>
+  <si>
+    <t>-8/16</t>
+  </si>
+  <si>
+    <t>8/31 採檢
+9/2 確診</t>
+  </si>
+  <si>
+    <t>持有登機前3日內檢驗陰性報告，入境迄今無疑似症狀，入境後直接前往防疫旅館進行14日居家檢疫
+原預訂於9月2日出海，8月31日由公司安排專車送至醫院自費採檢</t>
+  </si>
+  <si>
+    <t>國內新增1例境外移入COVID-19個案，為印尼籍船員</t>
   </si>
 </sst>
 </file>
@@ -36050,29 +36067,59 @@
       </c>
     </row>
     <row r="490">
-      <c r="A490" s="69"/>
-      <c r="B490" s="70"/>
-      <c r="C490" s="34"/>
-      <c r="D490" s="34"/>
-      <c r="E490" s="34"/>
+      <c r="A490" s="63" t="s">
+        <v>1764</v>
+      </c>
+      <c r="B490" s="6">
+        <v>44076.0</v>
+      </c>
+      <c r="C490" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D490" s="64" t="s">
+        <v>59</v>
+      </c>
+      <c r="E490" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F490" s="34"/>
-      <c r="G490" s="34"/>
-      <c r="H490" s="21"/>
-      <c r="I490" s="19"/>
-      <c r="J490" s="10"/>
-      <c r="K490" s="22"/>
-      <c r="L490" s="23"/>
-      <c r="M490" s="22"/>
+      <c r="G490" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H490" s="65" t="s">
+        <v>1765</v>
+      </c>
+      <c r="I490" s="66">
+        <v>44059.0</v>
+      </c>
+      <c r="J490" s="68" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K490" s="13" t="s">
+        <v>1766</v>
+      </c>
+      <c r="L490" s="68" t="s">
+        <v>1674</v>
+      </c>
+      <c r="M490" s="67" t="s">
+        <v>1442</v>
+      </c>
       <c r="N490" s="25"/>
-      <c r="O490" s="21"/>
-      <c r="P490" s="21"/>
+      <c r="O490" s="65" t="s">
+        <v>85</v>
+      </c>
+      <c r="P490" s="65" t="s">
+        <v>1767</v>
+      </c>
       <c r="Q490" s="19"/>
       <c r="R490" s="19"/>
-      <c r="S490" s="20"/>
+      <c r="S490" s="61" t="s">
+        <v>1768</v>
+      </c>
       <c r="T490" s="20"/>
       <c r="U490" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#489</v>
       </c>
     </row>
     <row r="491">
@@ -36733,15 +36780,16 @@
     <hyperlink r:id="rId49" ref="S487"/>
     <hyperlink r:id="rId50" ref="S488"/>
     <hyperlink r:id="rId51" ref="S489"/>
+    <hyperlink r:id="rId52" ref="S490"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId52"/>
-  <legacyDrawing r:id="rId53"/>
+  <drawing r:id="rId53"/>
+  <legacyDrawing r:id="rId54"/>
   <tableParts count="2">
-    <tablePart r:id="rId56"/>
     <tablePart r:id="rId57"/>
+    <tablePart r:id="rId58"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20200905
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -563,7 +563,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5363" uniqueCount="1769">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5375" uniqueCount="1774">
   <si>
     <t>案例</t>
   </si>
@@ -6579,6 +6579,23 @@
   </si>
   <si>
     <t>國內新增1例境外移入COVID-19個案，為印尼籍船員</t>
+  </si>
+  <si>
+    <t>#490</t>
+  </si>
+  <si>
+    <t>2019/9月-2020/9/1 日本</t>
+  </si>
+  <si>
+    <t>9/1 採檢
+9/4 確診</t>
+  </si>
+  <si>
+    <t>8月25日出現流鼻水症狀，並至當地診所就醫
+，經服藥後症狀改善；個案9月1日返國入境時無症狀，因主動聲明曾有不適症狀，由機場安排採檢後送至集中檢疫所</t>
+  </si>
+  <si>
+    <t>女赴日工作感染COVID-19，返國入境檢驗確診</t>
   </si>
 </sst>
 </file>
@@ -36123,29 +36140,59 @@
       </c>
     </row>
     <row r="491">
-      <c r="A491" s="69"/>
-      <c r="B491" s="70"/>
-      <c r="C491" s="34"/>
-      <c r="D491" s="34"/>
-      <c r="E491" s="34"/>
+      <c r="A491" s="63" t="s">
+        <v>1769</v>
+      </c>
+      <c r="B491" s="6">
+        <v>44078.0</v>
+      </c>
+      <c r="C491" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D491" s="64" t="s">
+        <v>59</v>
+      </c>
+      <c r="E491" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F491" s="34"/>
-      <c r="G491" s="34"/>
-      <c r="H491" s="21"/>
-      <c r="I491" s="19"/>
-      <c r="J491" s="10"/>
-      <c r="K491" s="22"/>
-      <c r="L491" s="23"/>
-      <c r="M491" s="22"/>
+      <c r="G491" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H491" s="65" t="s">
+        <v>1770</v>
+      </c>
+      <c r="I491" s="66">
+        <v>44075.0</v>
+      </c>
+      <c r="J491" s="10">
+        <v>44068.0</v>
+      </c>
+      <c r="K491" s="67" t="s">
+        <v>1771</v>
+      </c>
+      <c r="L491" s="68" t="s">
+        <v>426</v>
+      </c>
+      <c r="M491" s="67" t="s">
+        <v>482</v>
+      </c>
       <c r="N491" s="25"/>
-      <c r="O491" s="21"/>
-      <c r="P491" s="21"/>
+      <c r="O491" s="65" t="s">
+        <v>85</v>
+      </c>
+      <c r="P491" s="65" t="s">
+        <v>1772</v>
+      </c>
       <c r="Q491" s="19"/>
       <c r="R491" s="19"/>
-      <c r="S491" s="20"/>
+      <c r="S491" s="61" t="s">
+        <v>1773</v>
+      </c>
       <c r="T491" s="20"/>
       <c r="U491" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#490</v>
       </c>
     </row>
     <row r="492">
@@ -36781,15 +36828,16 @@
     <hyperlink r:id="rId50" ref="S488"/>
     <hyperlink r:id="rId51" ref="S489"/>
     <hyperlink r:id="rId52" ref="S490"/>
+    <hyperlink r:id="rId53" ref="S491"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId53"/>
-  <legacyDrawing r:id="rId54"/>
+  <drawing r:id="rId54"/>
+  <legacyDrawing r:id="rId55"/>
   <tableParts count="2">
-    <tablePart r:id="rId57"/>
     <tablePart r:id="rId58"/>
+    <tablePart r:id="rId59"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20200907
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -563,7 +563,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5375" uniqueCount="1774">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5410" uniqueCount="1788">
   <si>
     <t>案例</t>
   </si>
@@ -6596,6 +6596,53 @@
   </si>
   <si>
     <t>女赴日工作感染COVID-19，返國入境檢驗確診</t>
+  </si>
+  <si>
+    <t>#491</t>
+  </si>
+  <si>
+    <t>-9/3</t>
+  </si>
+  <si>
+    <t>9/3 採檢
+9/5 確診</t>
+  </si>
+  <si>
+    <t>移工</t>
+  </si>
+  <si>
+    <t>國內新增2例COVID-19個案，均為境外移入</t>
+  </si>
+  <si>
+    <t>#492</t>
+  </si>
+  <si>
+    <t>6月-9/4 印尼</t>
+  </si>
+  <si>
+    <t>9/4 採檢
+9/5 確診</t>
+  </si>
+  <si>
+    <t>打噴嚏 流鼻水 發燒 嗅覺異常 味覺異常</t>
+  </si>
+  <si>
+    <t>#493</t>
+  </si>
+  <si>
+    <t>-9/3 菲律賓</t>
+  </si>
+  <si>
+    <t>9/3 採檢
+9/6 確診</t>
+  </si>
+  <si>
+    <t>發燒 喉嚨痛 咳嗽 呼吸急促 胸悶 肌肉痠痛</t>
+  </si>
+  <si>
+    <t>長期居住於菲律賓經商
+自述曾接觸同住有上呼吸道症狀之菲律賓籍友人，該名友人於9月3日就醫並確診COVID-19
+採檢後前往集中檢疫所隔離檢疫，初次採檢結果為陰性，因個案胸悶、呼吸急促等症狀持續，經醫師評估再次採檢</t>
   </si>
 </sst>
 </file>
@@ -36196,81 +36243,167 @@
       </c>
     </row>
     <row r="492">
-      <c r="A492" s="69"/>
-      <c r="B492" s="70"/>
-      <c r="C492" s="34"/>
-      <c r="D492" s="34"/>
-      <c r="E492" s="34"/>
+      <c r="A492" s="63" t="s">
+        <v>1774</v>
+      </c>
+      <c r="B492" s="6">
+        <v>44079.0</v>
+      </c>
+      <c r="C492" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D492" s="64" t="s">
+        <v>116</v>
+      </c>
+      <c r="E492" s="7" t="s">
+        <v>205</v>
+      </c>
       <c r="F492" s="34"/>
-      <c r="G492" s="34"/>
-      <c r="H492" s="21"/>
-      <c r="I492" s="19"/>
-      <c r="J492" s="10"/>
-      <c r="K492" s="22"/>
-      <c r="L492" s="23"/>
-      <c r="M492" s="22"/>
+      <c r="G492" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H492" s="65" t="s">
+        <v>1775</v>
+      </c>
+      <c r="I492" s="66">
+        <v>44077.0</v>
+      </c>
+      <c r="J492" s="68" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K492" s="67" t="s">
+        <v>1776</v>
+      </c>
+      <c r="L492" s="68" t="s">
+        <v>426</v>
+      </c>
+      <c r="M492" s="67" t="s">
+        <v>108</v>
+      </c>
       <c r="N492" s="25"/>
-      <c r="O492" s="21"/>
-      <c r="P492" s="21"/>
+      <c r="O492" s="65" t="s">
+        <v>85</v>
+      </c>
+      <c r="P492" s="65" t="s">
+        <v>1777</v>
+      </c>
       <c r="Q492" s="19"/>
       <c r="R492" s="19"/>
-      <c r="S492" s="20"/>
+      <c r="S492" s="61" t="s">
+        <v>1778</v>
+      </c>
       <c r="T492" s="20"/>
       <c r="U492" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#491</v>
       </c>
     </row>
     <row r="493">
-      <c r="A493" s="69"/>
-      <c r="B493" s="70"/>
-      <c r="C493" s="34"/>
-      <c r="D493" s="34"/>
-      <c r="E493" s="34"/>
+      <c r="A493" s="63" t="s">
+        <v>1779</v>
+      </c>
+      <c r="B493" s="6">
+        <v>44079.0</v>
+      </c>
+      <c r="C493" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D493" s="64" t="s">
+        <v>116</v>
+      </c>
+      <c r="E493" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F493" s="34"/>
-      <c r="G493" s="34"/>
-      <c r="H493" s="21"/>
-      <c r="I493" s="19"/>
-      <c r="J493" s="10"/>
-      <c r="K493" s="22"/>
-      <c r="L493" s="23"/>
-      <c r="M493" s="22"/>
+      <c r="G493" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H493" s="65" t="s">
+        <v>1780</v>
+      </c>
+      <c r="I493" s="66">
+        <v>44078.0</v>
+      </c>
+      <c r="J493" s="10">
+        <v>44058.0</v>
+      </c>
+      <c r="K493" s="67" t="s">
+        <v>1781</v>
+      </c>
+      <c r="L493" s="68" t="s">
+        <v>363</v>
+      </c>
+      <c r="M493" s="67" t="s">
+        <v>1782</v>
+      </c>
       <c r="N493" s="25"/>
-      <c r="O493" s="21"/>
+      <c r="O493" s="65" t="s">
+        <v>85</v>
+      </c>
       <c r="P493" s="21"/>
       <c r="Q493" s="19"/>
       <c r="R493" s="19"/>
-      <c r="S493" s="20"/>
+      <c r="S493" s="61" t="s">
+        <v>1778</v>
+      </c>
       <c r="T493" s="20"/>
       <c r="U493" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#492</v>
       </c>
     </row>
     <row r="494">
-      <c r="A494" s="69"/>
-      <c r="B494" s="70"/>
-      <c r="C494" s="34"/>
-      <c r="D494" s="34"/>
-      <c r="E494" s="34"/>
+      <c r="A494" s="63" t="s">
+        <v>1783</v>
+      </c>
+      <c r="B494" s="6">
+        <v>44080.0</v>
+      </c>
+      <c r="C494" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D494" s="64" t="s">
+        <v>59</v>
+      </c>
+      <c r="E494" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F494" s="34"/>
-      <c r="G494" s="34"/>
-      <c r="H494" s="21"/>
-      <c r="I494" s="19"/>
-      <c r="J494" s="10"/>
-      <c r="K494" s="22"/>
-      <c r="L494" s="23"/>
-      <c r="M494" s="22"/>
+      <c r="G494" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H494" s="65" t="s">
+        <v>1784</v>
+      </c>
+      <c r="I494" s="66">
+        <v>44077.0</v>
+      </c>
+      <c r="J494" s="10">
+        <v>44075.0</v>
+      </c>
+      <c r="K494" s="67" t="s">
+        <v>1785</v>
+      </c>
+      <c r="L494" s="68" t="s">
+        <v>363</v>
+      </c>
+      <c r="M494" s="67" t="s">
+        <v>1786</v>
+      </c>
       <c r="N494" s="25"/>
-      <c r="O494" s="21"/>
-      <c r="P494" s="21"/>
+      <c r="O494" s="65" t="s">
+        <v>85</v>
+      </c>
+      <c r="P494" s="65" t="s">
+        <v>1787</v>
+      </c>
       <c r="Q494" s="19"/>
       <c r="R494" s="19"/>
       <c r="S494" s="20"/>
       <c r="T494" s="20"/>
       <c r="U494" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#493</v>
       </c>
     </row>
     <row r="495">
@@ -36829,15 +36962,17 @@
     <hyperlink r:id="rId51" ref="S489"/>
     <hyperlink r:id="rId52" ref="S490"/>
     <hyperlink r:id="rId53" ref="S491"/>
+    <hyperlink r:id="rId54" ref="S492"/>
+    <hyperlink r:id="rId55" ref="S493"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId54"/>
-  <legacyDrawing r:id="rId55"/>
+  <drawing r:id="rId56"/>
+  <legacyDrawing r:id="rId57"/>
   <tableParts count="2">
-    <tablePart r:id="rId58"/>
-    <tablePart r:id="rId59"/>
+    <tablePart r:id="rId60"/>
+    <tablePart r:id="rId61"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20200908
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -563,7 +563,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5410" uniqueCount="1788">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5425" uniqueCount="1796">
   <si>
     <t>案例</t>
   </si>
@@ -6567,7 +6567,7 @@
     <t>#489</t>
   </si>
   <si>
-    <t>-8/16</t>
+    <t>-8/16 台灣</t>
   </si>
   <si>
     <t>8/31 採檢
@@ -6601,7 +6601,7 @@
     <t>#491</t>
   </si>
   <si>
-    <t>-9/3</t>
+    <t>-9/3 台灣</t>
   </si>
   <si>
     <t>9/3 採檢
@@ -6643,6 +6643,32 @@
     <t>長期居住於菲律賓經商
 自述曾接觸同住有上呼吸道症狀之菲律賓籍友人，該名友人於9月3日就醫並確診COVID-19
 採檢後前往集中檢疫所隔離檢疫，初次採檢結果為陰性，因個案胸悶、呼吸急促等症狀持續，經醫師評估再次採檢</t>
+  </si>
+  <si>
+    <t>新增1例境外移入COVID-19個案，男自菲律賓返台確診</t>
+  </si>
+  <si>
+    <t>#494</t>
+  </si>
+  <si>
+    <t>2月-9/3 尼泊爾</t>
+  </si>
+  <si>
+    <t>9/5 採檢
+9/7 確診</t>
+  </si>
+  <si>
+    <t>發燒 流鼻水 頭痛 肌肉痠痛 腹瀉</t>
+  </si>
+  <si>
+    <t>參加宗教活動
+個案登機前3天之檢驗結果為陰性，9月3日與友人返國入境時無症狀，入境後返回居住地居家檢疫</t>
+  </si>
+  <si>
+    <t>國內新增1例境外移入COVID-19病例，男自尼泊爾返國後發病確診</t>
+  </si>
+  <si>
+    <t>#495</t>
   </si>
 </sst>
 </file>
@@ -6653,7 +6679,7 @@
     <numFmt numFmtId="164" formatCode="mm&quot;月&quot;dd&quot;日 &quot;dddd"/>
     <numFmt numFmtId="165" formatCode="m/d"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="17">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -6730,10 +6756,6 @@
       <u/>
       <color rgb="FF1155CC"/>
     </font>
-    <font/>
-    <font>
-      <color rgb="FF000000"/>
-    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -6779,7 +6801,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="65">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -6969,24 +6991,6 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -6997,7 +7001,7 @@
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
-  <dxfs count="62">
+  <dxfs count="63">
     <dxf>
       <font>
         <color rgb="FF0000FF"/>
@@ -7651,6 +7655,18 @@
       <border/>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE06666"/>
+          <bgColor rgb="FFE06666"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
       <font/>
       <fill>
         <patternFill patternType="none"/>
@@ -7690,14 +7706,14 @@
   </dxfs>
   <tableStyles count="2">
     <tableStyle count="3" pivot="0" name="臺灣武漢肺炎病例-style">
-      <tableStyleElement dxfId="59" type="headerRow"/>
-      <tableStyleElement dxfId="60" type="firstRowStripe"/>
-      <tableStyleElement dxfId="61" type="secondRowStripe"/>
+      <tableStyleElement dxfId="60" type="headerRow"/>
+      <tableStyleElement dxfId="61" type="firstRowStripe"/>
+      <tableStyleElement dxfId="62" type="secondRowStripe"/>
     </tableStyle>
     <tableStyle count="3" pivot="0" name="臺灣武漢肺炎病例-style 2">
-      <tableStyleElement dxfId="59" type="headerRow"/>
-      <tableStyleElement dxfId="60" type="firstRowStripe"/>
-      <tableStyleElement dxfId="61" type="secondRowStripe"/>
+      <tableStyleElement dxfId="60" type="headerRow"/>
+      <tableStyleElement dxfId="61" type="firstRowStripe"/>
+      <tableStyleElement dxfId="62" type="secondRowStripe"/>
     </tableStyle>
   </tableStyles>
 </styleSheet>
@@ -36075,7 +36091,7 @@
       </c>
     </row>
     <row r="489">
-      <c r="A489" s="63" t="s">
+      <c r="A489" s="16" t="s">
         <v>1760</v>
       </c>
       <c r="B489" s="6">
@@ -36084,7 +36100,7 @@
       <c r="C489" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D489" s="64" t="s">
+      <c r="D489" s="7" t="s">
         <v>59</v>
       </c>
       <c r="E489" s="7" t="s">
@@ -36094,29 +36110,29 @@
       <c r="G489" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H489" s="65" t="s">
+      <c r="H489" s="8" t="s">
         <v>1761</v>
       </c>
-      <c r="I489" s="66">
+      <c r="I489" s="9">
         <v>44070.0</v>
       </c>
       <c r="J489" s="10">
         <v>44063.0</v>
       </c>
-      <c r="K489" s="67" t="s">
+      <c r="K489" s="13" t="s">
         <v>1762</v>
       </c>
-      <c r="L489" s="68" t="s">
+      <c r="L489" s="12" t="s">
         <v>363</v>
       </c>
-      <c r="M489" s="67" t="s">
+      <c r="M489" s="13" t="s">
         <v>518</v>
       </c>
       <c r="N489" s="25"/>
-      <c r="O489" s="65" t="s">
+      <c r="O489" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P489" s="65" t="s">
+      <c r="P489" s="8" t="s">
         <v>334</v>
       </c>
       <c r="Q489" s="19"/>
@@ -36131,7 +36147,7 @@
       </c>
     </row>
     <row r="490">
-      <c r="A490" s="63" t="s">
+      <c r="A490" s="16" t="s">
         <v>1764</v>
       </c>
       <c r="B490" s="6">
@@ -36140,7 +36156,7 @@
       <c r="C490" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D490" s="64" t="s">
+      <c r="D490" s="7" t="s">
         <v>59</v>
       </c>
       <c r="E490" s="7" t="s">
@@ -36150,29 +36166,29 @@
       <c r="G490" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H490" s="65" t="s">
+      <c r="H490" s="8" t="s">
         <v>1765</v>
       </c>
-      <c r="I490" s="66">
+      <c r="I490" s="9">
         <v>44059.0</v>
       </c>
-      <c r="J490" s="68" t="s">
+      <c r="J490" s="12" t="s">
         <v>1442</v>
       </c>
       <c r="K490" s="13" t="s">
         <v>1766</v>
       </c>
-      <c r="L490" s="68" t="s">
+      <c r="L490" s="12" t="s">
         <v>1674</v>
       </c>
-      <c r="M490" s="67" t="s">
+      <c r="M490" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N490" s="25"/>
-      <c r="O490" s="65" t="s">
+      <c r="O490" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P490" s="65" t="s">
+      <c r="P490" s="8" t="s">
         <v>1767</v>
       </c>
       <c r="Q490" s="19"/>
@@ -36187,7 +36203,7 @@
       </c>
     </row>
     <row r="491">
-      <c r="A491" s="63" t="s">
+      <c r="A491" s="16" t="s">
         <v>1769</v>
       </c>
       <c r="B491" s="6">
@@ -36196,7 +36212,7 @@
       <c r="C491" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D491" s="64" t="s">
+      <c r="D491" s="7" t="s">
         <v>59</v>
       </c>
       <c r="E491" s="7" t="s">
@@ -36206,29 +36222,29 @@
       <c r="G491" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H491" s="65" t="s">
+      <c r="H491" s="8" t="s">
         <v>1770</v>
       </c>
-      <c r="I491" s="66">
+      <c r="I491" s="9">
         <v>44075.0</v>
       </c>
       <c r="J491" s="10">
         <v>44068.0</v>
       </c>
-      <c r="K491" s="67" t="s">
+      <c r="K491" s="13" t="s">
         <v>1771</v>
       </c>
-      <c r="L491" s="68" t="s">
+      <c r="L491" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M491" s="67" t="s">
+      <c r="M491" s="13" t="s">
         <v>482</v>
       </c>
       <c r="N491" s="25"/>
-      <c r="O491" s="65" t="s">
+      <c r="O491" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P491" s="65" t="s">
+      <c r="P491" s="8" t="s">
         <v>1772</v>
       </c>
       <c r="Q491" s="19"/>
@@ -36243,7 +36259,7 @@
       </c>
     </row>
     <row r="492">
-      <c r="A492" s="63" t="s">
+      <c r="A492" s="16" t="s">
         <v>1774</v>
       </c>
       <c r="B492" s="6">
@@ -36252,7 +36268,7 @@
       <c r="C492" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D492" s="64" t="s">
+      <c r="D492" s="7" t="s">
         <v>116</v>
       </c>
       <c r="E492" s="7" t="s">
@@ -36262,29 +36278,29 @@
       <c r="G492" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H492" s="65" t="s">
+      <c r="H492" s="8" t="s">
         <v>1775</v>
       </c>
-      <c r="I492" s="66">
+      <c r="I492" s="9">
         <v>44077.0</v>
       </c>
-      <c r="J492" s="68" t="s">
+      <c r="J492" s="12" t="s">
         <v>1442</v>
       </c>
-      <c r="K492" s="67" t="s">
+      <c r="K492" s="13" t="s">
         <v>1776</v>
       </c>
-      <c r="L492" s="68" t="s">
+      <c r="L492" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M492" s="67" t="s">
+      <c r="M492" s="13" t="s">
         <v>108</v>
       </c>
       <c r="N492" s="25"/>
-      <c r="O492" s="65" t="s">
+      <c r="O492" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P492" s="65" t="s">
+      <c r="P492" s="8" t="s">
         <v>1777</v>
       </c>
       <c r="Q492" s="19"/>
@@ -36299,7 +36315,7 @@
       </c>
     </row>
     <row r="493">
-      <c r="A493" s="63" t="s">
+      <c r="A493" s="16" t="s">
         <v>1779</v>
       </c>
       <c r="B493" s="6">
@@ -36308,7 +36324,7 @@
       <c r="C493" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D493" s="64" t="s">
+      <c r="D493" s="7" t="s">
         <v>116</v>
       </c>
       <c r="E493" s="7" t="s">
@@ -36318,26 +36334,26 @@
       <c r="G493" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H493" s="65" t="s">
+      <c r="H493" s="8" t="s">
         <v>1780</v>
       </c>
-      <c r="I493" s="66">
+      <c r="I493" s="9">
         <v>44078.0</v>
       </c>
       <c r="J493" s="10">
         <v>44058.0</v>
       </c>
-      <c r="K493" s="67" t="s">
+      <c r="K493" s="13" t="s">
         <v>1781</v>
       </c>
-      <c r="L493" s="68" t="s">
+      <c r="L493" s="12" t="s">
         <v>363</v>
       </c>
-      <c r="M493" s="67" t="s">
+      <c r="M493" s="13" t="s">
         <v>1782</v>
       </c>
       <c r="N493" s="25"/>
-      <c r="O493" s="65" t="s">
+      <c r="O493" s="8" t="s">
         <v>85</v>
       </c>
       <c r="P493" s="21"/>
@@ -36353,7 +36369,7 @@
       </c>
     </row>
     <row r="494">
-      <c r="A494" s="63" t="s">
+      <c r="A494" s="16" t="s">
         <v>1783</v>
       </c>
       <c r="B494" s="6">
@@ -36362,7 +36378,7 @@
       <c r="C494" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D494" s="64" t="s">
+      <c r="D494" s="7" t="s">
         <v>59</v>
       </c>
       <c r="E494" s="7" t="s">
@@ -36372,34 +36388,36 @@
       <c r="G494" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H494" s="65" t="s">
+      <c r="H494" s="8" t="s">
         <v>1784</v>
       </c>
-      <c r="I494" s="66">
+      <c r="I494" s="9">
         <v>44077.0</v>
       </c>
       <c r="J494" s="10">
         <v>44075.0</v>
       </c>
-      <c r="K494" s="67" t="s">
+      <c r="K494" s="13" t="s">
         <v>1785</v>
       </c>
-      <c r="L494" s="68" t="s">
+      <c r="L494" s="12" t="s">
         <v>363</v>
       </c>
-      <c r="M494" s="67" t="s">
+      <c r="M494" s="13" t="s">
         <v>1786</v>
       </c>
       <c r="N494" s="25"/>
-      <c r="O494" s="65" t="s">
+      <c r="O494" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P494" s="65" t="s">
+      <c r="P494" s="8" t="s">
         <v>1787</v>
       </c>
       <c r="Q494" s="19"/>
       <c r="R494" s="19"/>
-      <c r="S494" s="20"/>
+      <c r="S494" s="61" t="s">
+        <v>1788</v>
+      </c>
       <c r="T494" s="20"/>
       <c r="U494" s="18" t="str">
         <f t="shared" si="1"/>
@@ -36407,39 +36425,75 @@
       </c>
     </row>
     <row r="495">
-      <c r="A495" s="69"/>
-      <c r="B495" s="70"/>
-      <c r="C495" s="34"/>
-      <c r="D495" s="34"/>
-      <c r="E495" s="34"/>
+      <c r="A495" s="16" t="s">
+        <v>1789</v>
+      </c>
+      <c r="B495" s="6">
+        <v>44081.0</v>
+      </c>
+      <c r="C495" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D495" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E495" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F495" s="34"/>
-      <c r="G495" s="34"/>
-      <c r="H495" s="21"/>
-      <c r="I495" s="19"/>
-      <c r="J495" s="10"/>
-      <c r="K495" s="22"/>
-      <c r="L495" s="23"/>
-      <c r="M495" s="22"/>
+      <c r="G495" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H495" s="8" t="s">
+        <v>1790</v>
+      </c>
+      <c r="I495" s="9">
+        <v>44077.0</v>
+      </c>
+      <c r="J495" s="10">
+        <v>44079.0</v>
+      </c>
+      <c r="K495" s="13" t="s">
+        <v>1791</v>
+      </c>
+      <c r="L495" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M495" s="13" t="s">
+        <v>1792</v>
+      </c>
       <c r="N495" s="25"/>
-      <c r="O495" s="21"/>
-      <c r="P495" s="21"/>
+      <c r="O495" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P495" s="8" t="s">
+        <v>1793</v>
+      </c>
       <c r="Q495" s="19"/>
       <c r="R495" s="19"/>
-      <c r="S495" s="20"/>
+      <c r="S495" s="61" t="s">
+        <v>1794</v>
+      </c>
       <c r="T495" s="20"/>
       <c r="U495" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#494</v>
       </c>
     </row>
     <row r="496">
-      <c r="A496" s="69"/>
-      <c r="B496" s="70"/>
+      <c r="A496" s="16" t="s">
+        <v>1795</v>
+      </c>
+      <c r="B496" s="6">
+        <v>44082.0</v>
+      </c>
       <c r="C496" s="34"/>
       <c r="D496" s="34"/>
       <c r="E496" s="34"/>
       <c r="F496" s="34"/>
-      <c r="G496" s="34"/>
+      <c r="G496" s="7" t="s">
+        <v>25</v>
+      </c>
       <c r="H496" s="21"/>
       <c r="I496" s="19"/>
       <c r="J496" s="10"/>
@@ -36455,12 +36509,12 @@
       <c r="T496" s="20"/>
       <c r="U496" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#495</v>
       </c>
     </row>
     <row r="497">
-      <c r="A497" s="69"/>
-      <c r="B497" s="70"/>
+      <c r="A497" s="63"/>
+      <c r="B497" s="64"/>
       <c r="C497" s="34"/>
       <c r="D497" s="34"/>
       <c r="E497" s="34"/>
@@ -36485,8 +36539,8 @@
       </c>
     </row>
     <row r="498">
-      <c r="A498" s="69"/>
-      <c r="B498" s="70"/>
+      <c r="A498" s="63"/>
+      <c r="B498" s="64"/>
       <c r="C498" s="34"/>
       <c r="D498" s="34"/>
       <c r="E498" s="34"/>
@@ -36511,8 +36565,8 @@
       </c>
     </row>
     <row r="499">
-      <c r="A499" s="69"/>
-      <c r="B499" s="70"/>
+      <c r="A499" s="63"/>
+      <c r="B499" s="64"/>
       <c r="C499" s="34"/>
       <c r="D499" s="34"/>
       <c r="E499" s="34"/>
@@ -36537,8 +36591,8 @@
       </c>
     </row>
     <row r="500">
-      <c r="A500" s="69"/>
-      <c r="B500" s="70"/>
+      <c r="A500" s="63"/>
+      <c r="B500" s="64"/>
       <c r="C500" s="34"/>
       <c r="D500" s="34"/>
       <c r="E500" s="34"/>
@@ -36563,8 +36617,8 @@
       </c>
     </row>
     <row r="501">
-      <c r="A501" s="69"/>
-      <c r="B501" s="70"/>
+      <c r="A501" s="63"/>
+      <c r="B501" s="64"/>
       <c r="C501" s="34"/>
       <c r="D501" s="34"/>
       <c r="E501" s="34"/>
@@ -36909,6 +36963,11 @@
       <formula>B357&lt;44108.0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="L1:L501">
+    <cfRule type="containsText" dxfId="58" priority="65" operator="containsText" text="自費">
+      <formula>NOT(ISERROR(SEARCH(("自費"),(L1))))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink r:id="rId2" ref="S440"/>
     <hyperlink r:id="rId3" ref="S441"/>
@@ -36964,15 +37023,17 @@
     <hyperlink r:id="rId53" ref="S491"/>
     <hyperlink r:id="rId54" ref="S492"/>
     <hyperlink r:id="rId55" ref="S493"/>
+    <hyperlink r:id="rId56" ref="S494"/>
+    <hyperlink r:id="rId57" ref="S495"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId56"/>
-  <legacyDrawing r:id="rId57"/>
+  <drawing r:id="rId58"/>
+  <legacyDrawing r:id="rId59"/>
   <tableParts count="2">
-    <tablePart r:id="rId60"/>
-    <tablePart r:id="rId61"/>
+    <tablePart r:id="rId62"/>
+    <tablePart r:id="rId63"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20200909
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -563,7 +563,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5425" uniqueCount="1796">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5435" uniqueCount="1801">
   <si>
     <t>案例</t>
   </si>
@@ -6670,6 +6670,24 @@
   <si>
     <t>#495</t>
   </si>
+  <si>
+    <t>2019/12-2020/9/6 法國</t>
+  </si>
+  <si>
+    <t>9/6 採檢
+9/8 確診</t>
+  </si>
+  <si>
+    <t>頭痛 肌肉痠痛 流鼻水</t>
+  </si>
+  <si>
+    <t>長期在法國工作
+8月30日出現頭痛、肌肉痠痛等症狀，曾於法國當地就醫並診斷為流感，經服藥後症狀改善。
+個案9月6日返國入境時，因流鼻水症狀，主動向機場檢疫人員通報，經安排採檢後前往集中檢疫所</t>
+  </si>
+  <si>
+    <t>女在法國工作染COVID-19，返國入境採檢確診</t>
+  </si>
 </sst>
 </file>
 
@@ -6679,7 +6697,7 @@
     <numFmt numFmtId="164" formatCode="mm&quot;月&quot;dd&quot;日 &quot;dddd"/>
     <numFmt numFmtId="165" formatCode="m/d"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="19">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -6756,6 +6774,10 @@
       <u/>
       <color rgb="FF1155CC"/>
     </font>
+    <font/>
+    <font>
+      <color rgb="FF000000"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -6801,7 +6823,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="70">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -6990,6 +7012,21 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
@@ -36487,25 +36524,49 @@
       <c r="B496" s="6">
         <v>44082.0</v>
       </c>
-      <c r="C496" s="34"/>
-      <c r="D496" s="34"/>
-      <c r="E496" s="34"/>
+      <c r="C496" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D496" s="63" t="s">
+        <v>76</v>
+      </c>
+      <c r="E496" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F496" s="34"/>
       <c r="G496" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H496" s="21"/>
-      <c r="I496" s="19"/>
-      <c r="J496" s="10"/>
-      <c r="K496" s="22"/>
-      <c r="L496" s="23"/>
-      <c r="M496" s="22"/>
+      <c r="H496" s="64" t="s">
+        <v>1796</v>
+      </c>
+      <c r="I496" s="65">
+        <v>44080.0</v>
+      </c>
+      <c r="J496" s="10">
+        <v>44073.0</v>
+      </c>
+      <c r="K496" s="66" t="s">
+        <v>1797</v>
+      </c>
+      <c r="L496" s="67" t="s">
+        <v>363</v>
+      </c>
+      <c r="M496" s="66" t="s">
+        <v>1798</v>
+      </c>
       <c r="N496" s="25"/>
-      <c r="O496" s="21"/>
-      <c r="P496" s="21"/>
+      <c r="O496" s="64" t="s">
+        <v>85</v>
+      </c>
+      <c r="P496" s="64" t="s">
+        <v>1799</v>
+      </c>
       <c r="Q496" s="19"/>
       <c r="R496" s="19"/>
-      <c r="S496" s="20"/>
+      <c r="S496" s="61" t="s">
+        <v>1800</v>
+      </c>
       <c r="T496" s="20"/>
       <c r="U496" s="18" t="str">
         <f t="shared" si="1"/>
@@ -36513,8 +36574,8 @@
       </c>
     </row>
     <row r="497">
-      <c r="A497" s="63"/>
-      <c r="B497" s="64"/>
+      <c r="A497" s="68"/>
+      <c r="B497" s="69"/>
       <c r="C497" s="34"/>
       <c r="D497" s="34"/>
       <c r="E497" s="34"/>
@@ -36539,8 +36600,8 @@
       </c>
     </row>
     <row r="498">
-      <c r="A498" s="63"/>
-      <c r="B498" s="64"/>
+      <c r="A498" s="68"/>
+      <c r="B498" s="69"/>
       <c r="C498" s="34"/>
       <c r="D498" s="34"/>
       <c r="E498" s="34"/>
@@ -36565,8 +36626,8 @@
       </c>
     </row>
     <row r="499">
-      <c r="A499" s="63"/>
-      <c r="B499" s="64"/>
+      <c r="A499" s="68"/>
+      <c r="B499" s="69"/>
       <c r="C499" s="34"/>
       <c r="D499" s="34"/>
       <c r="E499" s="34"/>
@@ -36591,8 +36652,8 @@
       </c>
     </row>
     <row r="500">
-      <c r="A500" s="63"/>
-      <c r="B500" s="64"/>
+      <c r="A500" s="68"/>
+      <c r="B500" s="69"/>
       <c r="C500" s="34"/>
       <c r="D500" s="34"/>
       <c r="E500" s="34"/>
@@ -36617,8 +36678,8 @@
       </c>
     </row>
     <row r="501">
-      <c r="A501" s="63"/>
-      <c r="B501" s="64"/>
+      <c r="A501" s="68"/>
+      <c r="B501" s="69"/>
       <c r="C501" s="34"/>
       <c r="D501" s="34"/>
       <c r="E501" s="34"/>
@@ -37025,15 +37086,16 @@
     <hyperlink r:id="rId55" ref="S493"/>
     <hyperlink r:id="rId56" ref="S494"/>
     <hyperlink r:id="rId57" ref="S495"/>
+    <hyperlink r:id="rId58" ref="S496"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId58"/>
-  <legacyDrawing r:id="rId59"/>
+  <drawing r:id="rId59"/>
+  <legacyDrawing r:id="rId60"/>
   <tableParts count="2">
-    <tablePart r:id="rId62"/>
     <tablePart r:id="rId63"/>
+    <tablePart r:id="rId64"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20200911
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -563,7 +563,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5435" uniqueCount="1801">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5447" uniqueCount="1806">
   <si>
     <t>案例</t>
   </si>
@@ -6687,6 +6687,22 @@
   </si>
   <si>
     <t>女在法國工作染COVID-19，返國入境採檢確診</t>
+  </si>
+  <si>
+    <t>#496</t>
+  </si>
+  <si>
+    <t>2月-9/4 印尼</t>
+  </si>
+  <si>
+    <t>9/8 採檢
+9/10 確診</t>
+  </si>
+  <si>
+    <t>9月4日入境時無不適症狀，入境後前往防疫旅館居家檢疫，9月7日晚間出現發燒及流鼻水情形，8日通報衛生單位協助安排就醫</t>
+  </si>
+  <si>
+    <t>男子自印尼返台，居家檢疫期間發病確診COVID-19</t>
   </si>
 </sst>
 </file>
@@ -6823,7 +6839,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="72">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -7026,6 +7042,12 @@
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="18" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -36574,34 +36596,64 @@
       </c>
     </row>
     <row r="497">
-      <c r="A497" s="68"/>
-      <c r="B497" s="69"/>
-      <c r="C497" s="34"/>
-      <c r="D497" s="34"/>
-      <c r="E497" s="34"/>
+      <c r="A497" s="68" t="s">
+        <v>1801</v>
+      </c>
+      <c r="B497" s="6">
+        <v>44084.0</v>
+      </c>
+      <c r="C497" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D497" s="63" t="s">
+        <v>100</v>
+      </c>
+      <c r="E497" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F497" s="34"/>
-      <c r="G497" s="34"/>
-      <c r="H497" s="21"/>
-      <c r="I497" s="19"/>
-      <c r="J497" s="10"/>
-      <c r="K497" s="22"/>
-      <c r="L497" s="23"/>
-      <c r="M497" s="22"/>
+      <c r="G497" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H497" s="64" t="s">
+        <v>1802</v>
+      </c>
+      <c r="I497" s="65">
+        <v>44078.0</v>
+      </c>
+      <c r="J497" s="69">
+        <v>44081.0</v>
+      </c>
+      <c r="K497" s="66" t="s">
+        <v>1803</v>
+      </c>
+      <c r="L497" s="67" t="s">
+        <v>426</v>
+      </c>
+      <c r="M497" s="66" t="s">
+        <v>651</v>
+      </c>
       <c r="N497" s="25"/>
-      <c r="O497" s="21"/>
-      <c r="P497" s="21"/>
+      <c r="O497" s="64" t="s">
+        <v>85</v>
+      </c>
+      <c r="P497" s="64" t="s">
+        <v>1804</v>
+      </c>
       <c r="Q497" s="19"/>
       <c r="R497" s="19"/>
-      <c r="S497" s="20"/>
+      <c r="S497" s="61" t="s">
+        <v>1805</v>
+      </c>
       <c r="T497" s="20"/>
       <c r="U497" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#496</v>
       </c>
     </row>
     <row r="498">
-      <c r="A498" s="68"/>
-      <c r="B498" s="69"/>
+      <c r="A498" s="70"/>
+      <c r="B498" s="71"/>
       <c r="C498" s="34"/>
       <c r="D498" s="34"/>
       <c r="E498" s="34"/>
@@ -36626,8 +36678,8 @@
       </c>
     </row>
     <row r="499">
-      <c r="A499" s="68"/>
-      <c r="B499" s="69"/>
+      <c r="A499" s="70"/>
+      <c r="B499" s="71"/>
       <c r="C499" s="34"/>
       <c r="D499" s="34"/>
       <c r="E499" s="34"/>
@@ -36652,8 +36704,8 @@
       </c>
     </row>
     <row r="500">
-      <c r="A500" s="68"/>
-      <c r="B500" s="69"/>
+      <c r="A500" s="70"/>
+      <c r="B500" s="71"/>
       <c r="C500" s="34"/>
       <c r="D500" s="34"/>
       <c r="E500" s="34"/>
@@ -36678,8 +36730,8 @@
       </c>
     </row>
     <row r="501">
-      <c r="A501" s="68"/>
-      <c r="B501" s="69"/>
+      <c r="A501" s="70"/>
+      <c r="B501" s="71"/>
       <c r="C501" s="34"/>
       <c r="D501" s="34"/>
       <c r="E501" s="34"/>
@@ -37087,15 +37139,16 @@
     <hyperlink r:id="rId56" ref="S494"/>
     <hyperlink r:id="rId57" ref="S495"/>
     <hyperlink r:id="rId58" ref="S496"/>
+    <hyperlink r:id="rId59" ref="S497"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId59"/>
-  <legacyDrawing r:id="rId60"/>
+  <drawing r:id="rId60"/>
+  <legacyDrawing r:id="rId61"/>
   <tableParts count="2">
-    <tablePart r:id="rId63"/>
     <tablePart r:id="rId64"/>
+    <tablePart r:id="rId65"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20200912
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -563,7 +563,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5447" uniqueCount="1806">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5472" uniqueCount="1816">
   <si>
     <t>案例</t>
   </si>
@@ -6703,6 +6703,41 @@
   </si>
   <si>
     <t>男子自印尼返台，居家檢疫期間發病確診COVID-19</t>
+  </si>
+  <si>
+    <t>#497</t>
+  </si>
+  <si>
+    <t>-8/30 台灣</t>
+  </si>
+  <si>
+    <t>9/10 採檢
+9/11 確診</t>
+  </si>
+  <si>
+    <t>與家人於8月29日自菲律賓經香港轉機來台探親，登機前3日內檢驗結果為陰性
+8月30日入境台灣時無症狀，由檢疫人員安排採檢，結果為陰性
+9月10日因需緊急生產，由衛生單位協助安排送醫，待產前再次採檢，於今日確診</t>
+  </si>
+  <si>
+    <t>國內新增2例境外移入COVID-19病例，均自菲律賓入境</t>
+  </si>
+  <si>
+    <t>#498</t>
+  </si>
+  <si>
+    <t>1月-9/9 菲律賓</t>
+  </si>
+  <si>
+    <t>9/9 採檢
+9/11 確診</t>
+  </si>
+  <si>
+    <t>發燒 乾咳 背痛</t>
+  </si>
+  <si>
+    <t>7月14日出現發燒、乾咳及背痛症狀，於菲律賓當地就醫及採檢，結果為陽性
+經治療後分別於7月31日及8月7日兩次採檢結果皆為陰性，8月8日出院，迄今無不適症狀</t>
   </si>
 </sst>
 </file>
@@ -36652,55 +36687,115 @@
       </c>
     </row>
     <row r="498">
-      <c r="A498" s="70"/>
-      <c r="B498" s="71"/>
-      <c r="C498" s="34"/>
-      <c r="D498" s="34"/>
-      <c r="E498" s="34"/>
+      <c r="A498" s="68" t="s">
+        <v>1806</v>
+      </c>
+      <c r="B498" s="6">
+        <v>44085.0</v>
+      </c>
+      <c r="C498" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D498" s="63" t="s">
+        <v>116</v>
+      </c>
+      <c r="E498" s="7" t="s">
+        <v>205</v>
+      </c>
       <c r="F498" s="34"/>
-      <c r="G498" s="34"/>
-      <c r="H498" s="21"/>
-      <c r="I498" s="19"/>
-      <c r="J498" s="10"/>
-      <c r="K498" s="22"/>
-      <c r="L498" s="23"/>
-      <c r="M498" s="22"/>
+      <c r="G498" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H498" s="64" t="s">
+        <v>1807</v>
+      </c>
+      <c r="I498" s="65">
+        <v>44073.0</v>
+      </c>
+      <c r="J498" s="67" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K498" s="13" t="s">
+        <v>1808</v>
+      </c>
+      <c r="L498" s="67" t="s">
+        <v>426</v>
+      </c>
+      <c r="M498" s="66" t="s">
+        <v>1442</v>
+      </c>
       <c r="N498" s="25"/>
-      <c r="O498" s="21"/>
-      <c r="P498" s="21"/>
+      <c r="O498" s="64" t="s">
+        <v>85</v>
+      </c>
+      <c r="P498" s="64" t="s">
+        <v>1809</v>
+      </c>
       <c r="Q498" s="19"/>
       <c r="R498" s="19"/>
-      <c r="S498" s="20"/>
+      <c r="S498" s="61" t="s">
+        <v>1810</v>
+      </c>
       <c r="T498" s="20"/>
       <c r="U498" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#497</v>
       </c>
     </row>
     <row r="499">
-      <c r="A499" s="70"/>
-      <c r="B499" s="71"/>
-      <c r="C499" s="34"/>
-      <c r="D499" s="34"/>
-      <c r="E499" s="34"/>
+      <c r="A499" s="68" t="s">
+        <v>1811</v>
+      </c>
+      <c r="B499" s="6">
+        <v>44085.0</v>
+      </c>
+      <c r="C499" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D499" s="63" t="s">
+        <v>100</v>
+      </c>
+      <c r="E499" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F499" s="34"/>
-      <c r="G499" s="34"/>
-      <c r="H499" s="21"/>
-      <c r="I499" s="19"/>
-      <c r="J499" s="10"/>
-      <c r="K499" s="22"/>
-      <c r="L499" s="23"/>
-      <c r="M499" s="22"/>
+      <c r="G499" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H499" s="64" t="s">
+        <v>1812</v>
+      </c>
+      <c r="I499" s="65">
+        <v>44083.0</v>
+      </c>
+      <c r="J499" s="10">
+        <v>44026.0</v>
+      </c>
+      <c r="K499" s="66" t="s">
+        <v>1813</v>
+      </c>
+      <c r="L499" s="67" t="s">
+        <v>363</v>
+      </c>
+      <c r="M499" s="66" t="s">
+        <v>1814</v>
+      </c>
       <c r="N499" s="25"/>
-      <c r="O499" s="21"/>
-      <c r="P499" s="21"/>
+      <c r="O499" s="64" t="s">
+        <v>85</v>
+      </c>
+      <c r="P499" s="64" t="s">
+        <v>1815</v>
+      </c>
       <c r="Q499" s="19"/>
       <c r="R499" s="19"/>
-      <c r="S499" s="20"/>
+      <c r="S499" s="61" t="s">
+        <v>1810</v>
+      </c>
       <c r="T499" s="20"/>
       <c r="U499" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#498</v>
       </c>
     </row>
     <row r="500">
@@ -37140,15 +37235,17 @@
     <hyperlink r:id="rId57" ref="S495"/>
     <hyperlink r:id="rId58" ref="S496"/>
     <hyperlink r:id="rId59" ref="S497"/>
+    <hyperlink r:id="rId60" ref="S498"/>
+    <hyperlink r:id="rId61" ref="S499"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId60"/>
-  <legacyDrawing r:id="rId61"/>
+  <drawing r:id="rId62"/>
+  <legacyDrawing r:id="rId63"/>
   <tableParts count="2">
-    <tablePart r:id="rId64"/>
-    <tablePart r:id="rId65"/>
+    <tablePart r:id="rId66"/>
+    <tablePart r:id="rId67"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20200915
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -563,7 +563,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5472" uniqueCount="1816">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5485" uniqueCount="1821">
   <si>
     <t>案例</t>
   </si>
@@ -6738,6 +6738,22 @@
   <si>
     <t>7月14日出現發燒、乾咳及背痛症狀，於菲律賓當地就醫及採檢，結果為陽性
 經治療後分別於7月31日及8月7日兩次採檢結果皆為陰性，8月8日出院，迄今無不適症狀</t>
+  </si>
+  <si>
+    <t>#499</t>
+  </si>
+  <si>
+    <t>-9/10 台灣</t>
+  </si>
+  <si>
+    <t>9/10 採檢
+9/14 確診</t>
+  </si>
+  <si>
+    <t>來台目的為工作</t>
+  </si>
+  <si>
+    <t>菲籍女子來台工作，入境採檢確診COVID-19</t>
   </si>
 </sst>
 </file>
@@ -6825,10 +6841,10 @@
       <u/>
       <color rgb="FF1155CC"/>
     </font>
-    <font/>
     <font>
       <color rgb="FF000000"/>
     </font>
+    <font/>
   </fonts>
   <fills count="7">
     <fill>
@@ -6874,7 +6890,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="71">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -7065,25 +7081,22 @@
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="18" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="18" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
@@ -7818,7 +7831,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="B1:U501" displayName="Table_1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="B1:U551" displayName="Table_1" id="1">
   <tableColumns count="20">
     <tableColumn name="新聞稿發布日期" id="1"/>
     <tableColumn name="性別" id="2"/>
@@ -7846,7 +7859,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:A501" displayName="Table_2" id="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:A551" displayName="Table_2" id="2">
   <tableColumns count="1">
     <tableColumn name="案例" id="1"/>
   </tableColumns>
@@ -36584,7 +36597,7 @@
       <c r="C496" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D496" s="63" t="s">
+      <c r="D496" s="7" t="s">
         <v>76</v>
       </c>
       <c r="E496" s="7" t="s">
@@ -36594,29 +36607,29 @@
       <c r="G496" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H496" s="64" t="s">
+      <c r="H496" s="8" t="s">
         <v>1796</v>
       </c>
-      <c r="I496" s="65">
+      <c r="I496" s="9">
         <v>44080.0</v>
       </c>
       <c r="J496" s="10">
         <v>44073.0</v>
       </c>
-      <c r="K496" s="66" t="s">
+      <c r="K496" s="13" t="s">
         <v>1797</v>
       </c>
-      <c r="L496" s="67" t="s">
+      <c r="L496" s="12" t="s">
         <v>363</v>
       </c>
-      <c r="M496" s="66" t="s">
+      <c r="M496" s="13" t="s">
         <v>1798</v>
       </c>
       <c r="N496" s="25"/>
-      <c r="O496" s="64" t="s">
+      <c r="O496" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P496" s="64" t="s">
+      <c r="P496" s="8" t="s">
         <v>1799</v>
       </c>
       <c r="Q496" s="19"/>
@@ -36631,7 +36644,7 @@
       </c>
     </row>
     <row r="497">
-      <c r="A497" s="68" t="s">
+      <c r="A497" s="16" t="s">
         <v>1801</v>
       </c>
       <c r="B497" s="6">
@@ -36640,7 +36653,7 @@
       <c r="C497" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D497" s="63" t="s">
+      <c r="D497" s="7" t="s">
         <v>100</v>
       </c>
       <c r="E497" s="7" t="s">
@@ -36650,29 +36663,29 @@
       <c r="G497" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H497" s="64" t="s">
+      <c r="H497" s="8" t="s">
         <v>1802</v>
       </c>
-      <c r="I497" s="65">
+      <c r="I497" s="9">
         <v>44078.0</v>
       </c>
-      <c r="J497" s="69">
+      <c r="J497" s="10">
         <v>44081.0</v>
       </c>
-      <c r="K497" s="66" t="s">
+      <c r="K497" s="13" t="s">
         <v>1803</v>
       </c>
-      <c r="L497" s="67" t="s">
+      <c r="L497" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M497" s="66" t="s">
+      <c r="M497" s="13" t="s">
         <v>651</v>
       </c>
       <c r="N497" s="25"/>
-      <c r="O497" s="64" t="s">
+      <c r="O497" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P497" s="64" t="s">
+      <c r="P497" s="8" t="s">
         <v>1804</v>
       </c>
       <c r="Q497" s="19"/>
@@ -36687,7 +36700,7 @@
       </c>
     </row>
     <row r="498">
-      <c r="A498" s="68" t="s">
+      <c r="A498" s="16" t="s">
         <v>1806</v>
       </c>
       <c r="B498" s="6">
@@ -36696,7 +36709,7 @@
       <c r="C498" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D498" s="63" t="s">
+      <c r="D498" s="7" t="s">
         <v>116</v>
       </c>
       <c r="E498" s="7" t="s">
@@ -36706,29 +36719,29 @@
       <c r="G498" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H498" s="64" t="s">
+      <c r="H498" s="8" t="s">
         <v>1807</v>
       </c>
-      <c r="I498" s="65">
+      <c r="I498" s="9">
         <v>44073.0</v>
       </c>
-      <c r="J498" s="67" t="s">
+      <c r="J498" s="63" t="s">
         <v>1442</v>
       </c>
       <c r="K498" s="13" t="s">
         <v>1808</v>
       </c>
-      <c r="L498" s="67" t="s">
+      <c r="L498" s="63" t="s">
         <v>426</v>
       </c>
-      <c r="M498" s="66" t="s">
+      <c r="M498" s="64" t="s">
         <v>1442</v>
       </c>
       <c r="N498" s="25"/>
-      <c r="O498" s="64" t="s">
+      <c r="O498" s="65" t="s">
         <v>85</v>
       </c>
-      <c r="P498" s="64" t="s">
+      <c r="P498" s="65" t="s">
         <v>1809</v>
       </c>
       <c r="Q498" s="19"/>
@@ -36743,7 +36756,7 @@
       </c>
     </row>
     <row r="499">
-      <c r="A499" s="68" t="s">
+      <c r="A499" s="16" t="s">
         <v>1811</v>
       </c>
       <c r="B499" s="6">
@@ -36752,7 +36765,7 @@
       <c r="C499" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D499" s="63" t="s">
+      <c r="D499" s="7" t="s">
         <v>100</v>
       </c>
       <c r="E499" s="7" t="s">
@@ -36762,29 +36775,29 @@
       <c r="G499" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H499" s="64" t="s">
+      <c r="H499" s="65" t="s">
         <v>1812</v>
       </c>
-      <c r="I499" s="65">
+      <c r="I499" s="66">
         <v>44083.0</v>
       </c>
       <c r="J499" s="10">
         <v>44026.0</v>
       </c>
-      <c r="K499" s="66" t="s">
+      <c r="K499" s="64" t="s">
         <v>1813</v>
       </c>
-      <c r="L499" s="67" t="s">
+      <c r="L499" s="63" t="s">
         <v>363</v>
       </c>
-      <c r="M499" s="66" t="s">
+      <c r="M499" s="64" t="s">
         <v>1814</v>
       </c>
       <c r="N499" s="25"/>
-      <c r="O499" s="64" t="s">
+      <c r="O499" s="65" t="s">
         <v>85</v>
       </c>
-      <c r="P499" s="64" t="s">
+      <c r="P499" s="65" t="s">
         <v>1815</v>
       </c>
       <c r="Q499" s="19"/>
@@ -36799,34 +36812,64 @@
       </c>
     </row>
     <row r="500">
-      <c r="A500" s="70"/>
-      <c r="B500" s="71"/>
-      <c r="C500" s="34"/>
-      <c r="D500" s="34"/>
-      <c r="E500" s="34"/>
+      <c r="A500" s="67" t="s">
+        <v>1816</v>
+      </c>
+      <c r="B500" s="6">
+        <v>44088.0</v>
+      </c>
+      <c r="C500" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D500" s="68" t="s">
+        <v>76</v>
+      </c>
+      <c r="E500" s="7" t="s">
+        <v>205</v>
+      </c>
       <c r="F500" s="34"/>
-      <c r="G500" s="34"/>
-      <c r="H500" s="21"/>
-      <c r="I500" s="19"/>
-      <c r="J500" s="10"/>
-      <c r="K500" s="22"/>
-      <c r="L500" s="23"/>
-      <c r="M500" s="22"/>
+      <c r="G500" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H500" s="65" t="s">
+        <v>1817</v>
+      </c>
+      <c r="I500" s="66">
+        <v>44084.0</v>
+      </c>
+      <c r="J500" s="63" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K500" s="64" t="s">
+        <v>1818</v>
+      </c>
+      <c r="L500" s="63" t="s">
+        <v>363</v>
+      </c>
+      <c r="M500" s="64" t="s">
+        <v>1442</v>
+      </c>
       <c r="N500" s="25"/>
-      <c r="O500" s="21"/>
-      <c r="P500" s="21"/>
+      <c r="O500" s="65" t="s">
+        <v>85</v>
+      </c>
+      <c r="P500" s="65" t="s">
+        <v>1819</v>
+      </c>
       <c r="Q500" s="19"/>
       <c r="R500" s="19"/>
-      <c r="S500" s="20"/>
+      <c r="S500" s="61" t="s">
+        <v>1820</v>
+      </c>
       <c r="T500" s="20"/>
       <c r="U500" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#499</v>
       </c>
     </row>
     <row r="501">
-      <c r="A501" s="70"/>
-      <c r="B501" s="71"/>
+      <c r="A501" s="69"/>
+      <c r="B501" s="70"/>
       <c r="C501" s="34"/>
       <c r="D501" s="34"/>
       <c r="E501" s="34"/>
@@ -36850,328 +36893,1478 @@
         <v/>
       </c>
     </row>
+    <row r="502">
+      <c r="A502" s="69"/>
+      <c r="B502" s="70"/>
+      <c r="C502" s="34"/>
+      <c r="D502" s="34"/>
+      <c r="E502" s="34"/>
+      <c r="F502" s="34"/>
+      <c r="G502" s="34"/>
+      <c r="H502" s="21"/>
+      <c r="I502" s="19"/>
+      <c r="J502" s="10"/>
+      <c r="K502" s="22"/>
+      <c r="L502" s="23"/>
+      <c r="M502" s="22"/>
+      <c r="N502" s="25"/>
+      <c r="O502" s="21"/>
+      <c r="P502" s="21"/>
+      <c r="Q502" s="19"/>
+      <c r="R502" s="19"/>
+      <c r="S502" s="20"/>
+      <c r="T502" s="20"/>
+      <c r="U502" s="18"/>
+    </row>
+    <row r="503">
+      <c r="A503" s="69"/>
+      <c r="B503" s="70"/>
+      <c r="C503" s="34"/>
+      <c r="D503" s="34"/>
+      <c r="E503" s="34"/>
+      <c r="F503" s="34"/>
+      <c r="G503" s="34"/>
+      <c r="H503" s="21"/>
+      <c r="I503" s="19"/>
+      <c r="J503" s="10"/>
+      <c r="K503" s="22"/>
+      <c r="L503" s="23"/>
+      <c r="M503" s="22"/>
+      <c r="N503" s="25"/>
+      <c r="O503" s="21"/>
+      <c r="P503" s="21"/>
+      <c r="Q503" s="19"/>
+      <c r="R503" s="19"/>
+      <c r="S503" s="20"/>
+      <c r="T503" s="20"/>
+      <c r="U503" s="18"/>
+    </row>
+    <row r="504">
+      <c r="A504" s="69"/>
+      <c r="B504" s="70"/>
+      <c r="C504" s="34"/>
+      <c r="D504" s="34"/>
+      <c r="E504" s="34"/>
+      <c r="F504" s="34"/>
+      <c r="G504" s="34"/>
+      <c r="H504" s="21"/>
+      <c r="I504" s="19"/>
+      <c r="J504" s="10"/>
+      <c r="K504" s="22"/>
+      <c r="L504" s="23"/>
+      <c r="M504" s="22"/>
+      <c r="N504" s="25"/>
+      <c r="O504" s="21"/>
+      <c r="P504" s="21"/>
+      <c r="Q504" s="19"/>
+      <c r="R504" s="19"/>
+      <c r="S504" s="20"/>
+      <c r="T504" s="20"/>
+      <c r="U504" s="18"/>
+    </row>
+    <row r="505">
+      <c r="A505" s="69"/>
+      <c r="B505" s="70"/>
+      <c r="C505" s="34"/>
+      <c r="D505" s="34"/>
+      <c r="E505" s="34"/>
+      <c r="F505" s="34"/>
+      <c r="G505" s="34"/>
+      <c r="H505" s="21"/>
+      <c r="I505" s="19"/>
+      <c r="J505" s="10"/>
+      <c r="K505" s="22"/>
+      <c r="L505" s="23"/>
+      <c r="M505" s="22"/>
+      <c r="N505" s="25"/>
+      <c r="O505" s="21"/>
+      <c r="P505" s="21"/>
+      <c r="Q505" s="19"/>
+      <c r="R505" s="19"/>
+      <c r="S505" s="20"/>
+      <c r="T505" s="20"/>
+      <c r="U505" s="18"/>
+    </row>
+    <row r="506">
+      <c r="A506" s="69"/>
+      <c r="B506" s="70"/>
+      <c r="C506" s="34"/>
+      <c r="D506" s="34"/>
+      <c r="E506" s="34"/>
+      <c r="F506" s="34"/>
+      <c r="G506" s="34"/>
+      <c r="H506" s="21"/>
+      <c r="I506" s="19"/>
+      <c r="J506" s="10"/>
+      <c r="K506" s="22"/>
+      <c r="L506" s="23"/>
+      <c r="M506" s="22"/>
+      <c r="N506" s="25"/>
+      <c r="O506" s="21"/>
+      <c r="P506" s="21"/>
+      <c r="Q506" s="19"/>
+      <c r="R506" s="19"/>
+      <c r="S506" s="20"/>
+      <c r="T506" s="20"/>
+      <c r="U506" s="18"/>
+    </row>
+    <row r="507">
+      <c r="A507" s="69"/>
+      <c r="B507" s="70"/>
+      <c r="C507" s="34"/>
+      <c r="D507" s="34"/>
+      <c r="E507" s="34"/>
+      <c r="F507" s="34"/>
+      <c r="G507" s="34"/>
+      <c r="H507" s="21"/>
+      <c r="I507" s="19"/>
+      <c r="J507" s="10"/>
+      <c r="K507" s="22"/>
+      <c r="L507" s="23"/>
+      <c r="M507" s="22"/>
+      <c r="N507" s="25"/>
+      <c r="O507" s="21"/>
+      <c r="P507" s="21"/>
+      <c r="Q507" s="19"/>
+      <c r="R507" s="19"/>
+      <c r="S507" s="20"/>
+      <c r="T507" s="20"/>
+      <c r="U507" s="18"/>
+    </row>
+    <row r="508">
+      <c r="A508" s="69"/>
+      <c r="B508" s="70"/>
+      <c r="C508" s="34"/>
+      <c r="D508" s="34"/>
+      <c r="E508" s="34"/>
+      <c r="F508" s="34"/>
+      <c r="G508" s="34"/>
+      <c r="H508" s="21"/>
+      <c r="I508" s="19"/>
+      <c r="J508" s="10"/>
+      <c r="K508" s="22"/>
+      <c r="L508" s="23"/>
+      <c r="M508" s="22"/>
+      <c r="N508" s="25"/>
+      <c r="O508" s="21"/>
+      <c r="P508" s="21"/>
+      <c r="Q508" s="19"/>
+      <c r="R508" s="19"/>
+      <c r="S508" s="20"/>
+      <c r="T508" s="20"/>
+      <c r="U508" s="18"/>
+    </row>
+    <row r="509">
+      <c r="A509" s="69"/>
+      <c r="B509" s="70"/>
+      <c r="C509" s="34"/>
+      <c r="D509" s="34"/>
+      <c r="E509" s="34"/>
+      <c r="F509" s="34"/>
+      <c r="G509" s="34"/>
+      <c r="H509" s="21"/>
+      <c r="I509" s="19"/>
+      <c r="J509" s="10"/>
+      <c r="K509" s="22"/>
+      <c r="L509" s="23"/>
+      <c r="M509" s="22"/>
+      <c r="N509" s="25"/>
+      <c r="O509" s="21"/>
+      <c r="P509" s="21"/>
+      <c r="Q509" s="19"/>
+      <c r="R509" s="19"/>
+      <c r="S509" s="20"/>
+      <c r="T509" s="20"/>
+      <c r="U509" s="18"/>
+    </row>
+    <row r="510">
+      <c r="A510" s="69"/>
+      <c r="B510" s="70"/>
+      <c r="C510" s="34"/>
+      <c r="D510" s="34"/>
+      <c r="E510" s="34"/>
+      <c r="F510" s="34"/>
+      <c r="G510" s="34"/>
+      <c r="H510" s="21"/>
+      <c r="I510" s="19"/>
+      <c r="J510" s="10"/>
+      <c r="K510" s="22"/>
+      <c r="L510" s="23"/>
+      <c r="M510" s="22"/>
+      <c r="N510" s="25"/>
+      <c r="O510" s="21"/>
+      <c r="P510" s="21"/>
+      <c r="Q510" s="19"/>
+      <c r="R510" s="19"/>
+      <c r="S510" s="20"/>
+      <c r="T510" s="20"/>
+      <c r="U510" s="18"/>
+    </row>
+    <row r="511">
+      <c r="A511" s="69"/>
+      <c r="B511" s="70"/>
+      <c r="C511" s="34"/>
+      <c r="D511" s="34"/>
+      <c r="E511" s="34"/>
+      <c r="F511" s="34"/>
+      <c r="G511" s="34"/>
+      <c r="H511" s="21"/>
+      <c r="I511" s="19"/>
+      <c r="J511" s="10"/>
+      <c r="K511" s="22"/>
+      <c r="L511" s="23"/>
+      <c r="M511" s="22"/>
+      <c r="N511" s="25"/>
+      <c r="O511" s="21"/>
+      <c r="P511" s="21"/>
+      <c r="Q511" s="19"/>
+      <c r="R511" s="19"/>
+      <c r="S511" s="20"/>
+      <c r="T511" s="20"/>
+      <c r="U511" s="18"/>
+    </row>
+    <row r="512">
+      <c r="A512" s="69"/>
+      <c r="B512" s="70"/>
+      <c r="C512" s="34"/>
+      <c r="D512" s="34"/>
+      <c r="E512" s="34"/>
+      <c r="F512" s="34"/>
+      <c r="G512" s="34"/>
+      <c r="H512" s="21"/>
+      <c r="I512" s="19"/>
+      <c r="J512" s="10"/>
+      <c r="K512" s="22"/>
+      <c r="L512" s="23"/>
+      <c r="M512" s="22"/>
+      <c r="N512" s="25"/>
+      <c r="O512" s="21"/>
+      <c r="P512" s="21"/>
+      <c r="Q512" s="19"/>
+      <c r="R512" s="19"/>
+      <c r="S512" s="20"/>
+      <c r="T512" s="20"/>
+      <c r="U512" s="18"/>
+    </row>
+    <row r="513">
+      <c r="A513" s="69"/>
+      <c r="B513" s="70"/>
+      <c r="C513" s="34"/>
+      <c r="D513" s="34"/>
+      <c r="E513" s="34"/>
+      <c r="F513" s="34"/>
+      <c r="G513" s="34"/>
+      <c r="H513" s="21"/>
+      <c r="I513" s="19"/>
+      <c r="J513" s="10"/>
+      <c r="K513" s="22"/>
+      <c r="L513" s="23"/>
+      <c r="M513" s="22"/>
+      <c r="N513" s="25"/>
+      <c r="O513" s="21"/>
+      <c r="P513" s="21"/>
+      <c r="Q513" s="19"/>
+      <c r="R513" s="19"/>
+      <c r="S513" s="20"/>
+      <c r="T513" s="20"/>
+      <c r="U513" s="18"/>
+    </row>
+    <row r="514">
+      <c r="A514" s="69"/>
+      <c r="B514" s="70"/>
+      <c r="C514" s="34"/>
+      <c r="D514" s="34"/>
+      <c r="E514" s="34"/>
+      <c r="F514" s="34"/>
+      <c r="G514" s="34"/>
+      <c r="H514" s="21"/>
+      <c r="I514" s="19"/>
+      <c r="J514" s="10"/>
+      <c r="K514" s="22"/>
+      <c r="L514" s="23"/>
+      <c r="M514" s="22"/>
+      <c r="N514" s="25"/>
+      <c r="O514" s="21"/>
+      <c r="P514" s="21"/>
+      <c r="Q514" s="19"/>
+      <c r="R514" s="19"/>
+      <c r="S514" s="20"/>
+      <c r="T514" s="20"/>
+      <c r="U514" s="18"/>
+    </row>
+    <row r="515">
+      <c r="A515" s="69"/>
+      <c r="B515" s="70"/>
+      <c r="C515" s="34"/>
+      <c r="D515" s="34"/>
+      <c r="E515" s="34"/>
+      <c r="F515" s="34"/>
+      <c r="G515" s="34"/>
+      <c r="H515" s="21"/>
+      <c r="I515" s="19"/>
+      <c r="J515" s="10"/>
+      <c r="K515" s="22"/>
+      <c r="L515" s="23"/>
+      <c r="M515" s="22"/>
+      <c r="N515" s="25"/>
+      <c r="O515" s="21"/>
+      <c r="P515" s="21"/>
+      <c r="Q515" s="19"/>
+      <c r="R515" s="19"/>
+      <c r="S515" s="20"/>
+      <c r="T515" s="20"/>
+      <c r="U515" s="18"/>
+    </row>
+    <row r="516">
+      <c r="A516" s="69"/>
+      <c r="B516" s="70"/>
+      <c r="C516" s="34"/>
+      <c r="D516" s="34"/>
+      <c r="E516" s="34"/>
+      <c r="F516" s="34"/>
+      <c r="G516" s="34"/>
+      <c r="H516" s="21"/>
+      <c r="I516" s="19"/>
+      <c r="J516" s="10"/>
+      <c r="K516" s="22"/>
+      <c r="L516" s="23"/>
+      <c r="M516" s="22"/>
+      <c r="N516" s="25"/>
+      <c r="O516" s="21"/>
+      <c r="P516" s="21"/>
+      <c r="Q516" s="19"/>
+      <c r="R516" s="19"/>
+      <c r="S516" s="20"/>
+      <c r="T516" s="20"/>
+      <c r="U516" s="18"/>
+    </row>
+    <row r="517">
+      <c r="A517" s="69"/>
+      <c r="B517" s="70"/>
+      <c r="C517" s="34"/>
+      <c r="D517" s="34"/>
+      <c r="E517" s="34"/>
+      <c r="F517" s="34"/>
+      <c r="G517" s="34"/>
+      <c r="H517" s="21"/>
+      <c r="I517" s="19"/>
+      <c r="J517" s="10"/>
+      <c r="K517" s="22"/>
+      <c r="L517" s="23"/>
+      <c r="M517" s="22"/>
+      <c r="N517" s="25"/>
+      <c r="O517" s="21"/>
+      <c r="P517" s="21"/>
+      <c r="Q517" s="19"/>
+      <c r="R517" s="19"/>
+      <c r="S517" s="20"/>
+      <c r="T517" s="20"/>
+      <c r="U517" s="18"/>
+    </row>
+    <row r="518">
+      <c r="A518" s="69"/>
+      <c r="B518" s="70"/>
+      <c r="C518" s="34"/>
+      <c r="D518" s="34"/>
+      <c r="E518" s="34"/>
+      <c r="F518" s="34"/>
+      <c r="G518" s="34"/>
+      <c r="H518" s="21"/>
+      <c r="I518" s="19"/>
+      <c r="J518" s="10"/>
+      <c r="K518" s="22"/>
+      <c r="L518" s="23"/>
+      <c r="M518" s="22"/>
+      <c r="N518" s="25"/>
+      <c r="O518" s="21"/>
+      <c r="P518" s="21"/>
+      <c r="Q518" s="19"/>
+      <c r="R518" s="19"/>
+      <c r="S518" s="20"/>
+      <c r="T518" s="20"/>
+      <c r="U518" s="18"/>
+    </row>
+    <row r="519">
+      <c r="A519" s="69"/>
+      <c r="B519" s="70"/>
+      <c r="C519" s="34"/>
+      <c r="D519" s="34"/>
+      <c r="E519" s="34"/>
+      <c r="F519" s="34"/>
+      <c r="G519" s="34"/>
+      <c r="H519" s="21"/>
+      <c r="I519" s="19"/>
+      <c r="J519" s="10"/>
+      <c r="K519" s="22"/>
+      <c r="L519" s="23"/>
+      <c r="M519" s="22"/>
+      <c r="N519" s="25"/>
+      <c r="O519" s="21"/>
+      <c r="P519" s="21"/>
+      <c r="Q519" s="19"/>
+      <c r="R519" s="19"/>
+      <c r="S519" s="20"/>
+      <c r="T519" s="20"/>
+      <c r="U519" s="18"/>
+    </row>
+    <row r="520">
+      <c r="A520" s="69"/>
+      <c r="B520" s="70"/>
+      <c r="C520" s="34"/>
+      <c r="D520" s="34"/>
+      <c r="E520" s="34"/>
+      <c r="F520" s="34"/>
+      <c r="G520" s="34"/>
+      <c r="H520" s="21"/>
+      <c r="I520" s="19"/>
+      <c r="J520" s="10"/>
+      <c r="K520" s="22"/>
+      <c r="L520" s="23"/>
+      <c r="M520" s="22"/>
+      <c r="N520" s="25"/>
+      <c r="O520" s="21"/>
+      <c r="P520" s="21"/>
+      <c r="Q520" s="19"/>
+      <c r="R520" s="19"/>
+      <c r="S520" s="20"/>
+      <c r="T520" s="20"/>
+      <c r="U520" s="18"/>
+    </row>
+    <row r="521">
+      <c r="A521" s="69"/>
+      <c r="B521" s="70"/>
+      <c r="C521" s="34"/>
+      <c r="D521" s="34"/>
+      <c r="E521" s="34"/>
+      <c r="F521" s="34"/>
+      <c r="G521" s="34"/>
+      <c r="H521" s="21"/>
+      <c r="I521" s="19"/>
+      <c r="J521" s="10"/>
+      <c r="K521" s="22"/>
+      <c r="L521" s="23"/>
+      <c r="M521" s="22"/>
+      <c r="N521" s="25"/>
+      <c r="O521" s="21"/>
+      <c r="P521" s="21"/>
+      <c r="Q521" s="19"/>
+      <c r="R521" s="19"/>
+      <c r="S521" s="20"/>
+      <c r="T521" s="20"/>
+      <c r="U521" s="18"/>
+    </row>
+    <row r="522">
+      <c r="A522" s="69"/>
+      <c r="B522" s="70"/>
+      <c r="C522" s="34"/>
+      <c r="D522" s="34"/>
+      <c r="E522" s="34"/>
+      <c r="F522" s="34"/>
+      <c r="G522" s="34"/>
+      <c r="H522" s="21"/>
+      <c r="I522" s="19"/>
+      <c r="J522" s="10"/>
+      <c r="K522" s="22"/>
+      <c r="L522" s="23"/>
+      <c r="M522" s="22"/>
+      <c r="N522" s="25"/>
+      <c r="O522" s="21"/>
+      <c r="P522" s="21"/>
+      <c r="Q522" s="19"/>
+      <c r="R522" s="19"/>
+      <c r="S522" s="20"/>
+      <c r="T522" s="20"/>
+      <c r="U522" s="18"/>
+    </row>
+    <row r="523">
+      <c r="A523" s="69"/>
+      <c r="B523" s="70"/>
+      <c r="C523" s="34"/>
+      <c r="D523" s="34"/>
+      <c r="E523" s="34"/>
+      <c r="F523" s="34"/>
+      <c r="G523" s="34"/>
+      <c r="H523" s="21"/>
+      <c r="I523" s="19"/>
+      <c r="J523" s="10"/>
+      <c r="K523" s="22"/>
+      <c r="L523" s="23"/>
+      <c r="M523" s="22"/>
+      <c r="N523" s="25"/>
+      <c r="O523" s="21"/>
+      <c r="P523" s="21"/>
+      <c r="Q523" s="19"/>
+      <c r="R523" s="19"/>
+      <c r="S523" s="20"/>
+      <c r="T523" s="20"/>
+      <c r="U523" s="18"/>
+    </row>
+    <row r="524">
+      <c r="A524" s="69"/>
+      <c r="B524" s="70"/>
+      <c r="C524" s="34"/>
+      <c r="D524" s="34"/>
+      <c r="E524" s="34"/>
+      <c r="F524" s="34"/>
+      <c r="G524" s="34"/>
+      <c r="H524" s="21"/>
+      <c r="I524" s="19"/>
+      <c r="J524" s="10"/>
+      <c r="K524" s="22"/>
+      <c r="L524" s="23"/>
+      <c r="M524" s="22"/>
+      <c r="N524" s="25"/>
+      <c r="O524" s="21"/>
+      <c r="P524" s="21"/>
+      <c r="Q524" s="19"/>
+      <c r="R524" s="19"/>
+      <c r="S524" s="20"/>
+      <c r="T524" s="20"/>
+      <c r="U524" s="18"/>
+    </row>
+    <row r="525">
+      <c r="A525" s="69"/>
+      <c r="B525" s="70"/>
+      <c r="C525" s="34"/>
+      <c r="D525" s="34"/>
+      <c r="E525" s="34"/>
+      <c r="F525" s="34"/>
+      <c r="G525" s="34"/>
+      <c r="H525" s="21"/>
+      <c r="I525" s="19"/>
+      <c r="J525" s="10"/>
+      <c r="K525" s="22"/>
+      <c r="L525" s="23"/>
+      <c r="M525" s="22"/>
+      <c r="N525" s="25"/>
+      <c r="O525" s="21"/>
+      <c r="P525" s="21"/>
+      <c r="Q525" s="19"/>
+      <c r="R525" s="19"/>
+      <c r="S525" s="20"/>
+      <c r="T525" s="20"/>
+      <c r="U525" s="18"/>
+    </row>
+    <row r="526">
+      <c r="A526" s="69"/>
+      <c r="B526" s="70"/>
+      <c r="C526" s="34"/>
+      <c r="D526" s="34"/>
+      <c r="E526" s="34"/>
+      <c r="F526" s="34"/>
+      <c r="G526" s="34"/>
+      <c r="H526" s="21"/>
+      <c r="I526" s="19"/>
+      <c r="J526" s="10"/>
+      <c r="K526" s="22"/>
+      <c r="L526" s="23"/>
+      <c r="M526" s="22"/>
+      <c r="N526" s="25"/>
+      <c r="O526" s="21"/>
+      <c r="P526" s="21"/>
+      <c r="Q526" s="19"/>
+      <c r="R526" s="19"/>
+      <c r="S526" s="20"/>
+      <c r="T526" s="20"/>
+      <c r="U526" s="18"/>
+    </row>
+    <row r="527">
+      <c r="A527" s="69"/>
+      <c r="B527" s="70"/>
+      <c r="C527" s="34"/>
+      <c r="D527" s="34"/>
+      <c r="E527" s="34"/>
+      <c r="F527" s="34"/>
+      <c r="G527" s="34"/>
+      <c r="H527" s="21"/>
+      <c r="I527" s="19"/>
+      <c r="J527" s="10"/>
+      <c r="K527" s="22"/>
+      <c r="L527" s="23"/>
+      <c r="M527" s="22"/>
+      <c r="N527" s="25"/>
+      <c r="O527" s="21"/>
+      <c r="P527" s="21"/>
+      <c r="Q527" s="19"/>
+      <c r="R527" s="19"/>
+      <c r="S527" s="20"/>
+      <c r="T527" s="20"/>
+      <c r="U527" s="18"/>
+    </row>
+    <row r="528">
+      <c r="A528" s="69"/>
+      <c r="B528" s="70"/>
+      <c r="C528" s="34"/>
+      <c r="D528" s="34"/>
+      <c r="E528" s="34"/>
+      <c r="F528" s="34"/>
+      <c r="G528" s="34"/>
+      <c r="H528" s="21"/>
+      <c r="I528" s="19"/>
+      <c r="J528" s="10"/>
+      <c r="K528" s="22"/>
+      <c r="L528" s="23"/>
+      <c r="M528" s="22"/>
+      <c r="N528" s="25"/>
+      <c r="O528" s="21"/>
+      <c r="P528" s="21"/>
+      <c r="Q528" s="19"/>
+      <c r="R528" s="19"/>
+      <c r="S528" s="20"/>
+      <c r="T528" s="20"/>
+      <c r="U528" s="18"/>
+    </row>
+    <row r="529">
+      <c r="A529" s="69"/>
+      <c r="B529" s="70"/>
+      <c r="C529" s="34"/>
+      <c r="D529" s="34"/>
+      <c r="E529" s="34"/>
+      <c r="F529" s="34"/>
+      <c r="G529" s="34"/>
+      <c r="H529" s="21"/>
+      <c r="I529" s="19"/>
+      <c r="J529" s="10"/>
+      <c r="K529" s="22"/>
+      <c r="L529" s="23"/>
+      <c r="M529" s="22"/>
+      <c r="N529" s="25"/>
+      <c r="O529" s="21"/>
+      <c r="P529" s="21"/>
+      <c r="Q529" s="19"/>
+      <c r="R529" s="19"/>
+      <c r="S529" s="20"/>
+      <c r="T529" s="20"/>
+      <c r="U529" s="18"/>
+    </row>
+    <row r="530">
+      <c r="A530" s="69"/>
+      <c r="B530" s="70"/>
+      <c r="C530" s="34"/>
+      <c r="D530" s="34"/>
+      <c r="E530" s="34"/>
+      <c r="F530" s="34"/>
+      <c r="G530" s="34"/>
+      <c r="H530" s="21"/>
+      <c r="I530" s="19"/>
+      <c r="J530" s="10"/>
+      <c r="K530" s="22"/>
+      <c r="L530" s="23"/>
+      <c r="M530" s="22"/>
+      <c r="N530" s="25"/>
+      <c r="O530" s="21"/>
+      <c r="P530" s="21"/>
+      <c r="Q530" s="19"/>
+      <c r="R530" s="19"/>
+      <c r="S530" s="20"/>
+      <c r="T530" s="20"/>
+      <c r="U530" s="18"/>
+    </row>
+    <row r="531">
+      <c r="A531" s="69"/>
+      <c r="B531" s="70"/>
+      <c r="C531" s="34"/>
+      <c r="D531" s="34"/>
+      <c r="E531" s="34"/>
+      <c r="F531" s="34"/>
+      <c r="G531" s="34"/>
+      <c r="H531" s="21"/>
+      <c r="I531" s="19"/>
+      <c r="J531" s="10"/>
+      <c r="K531" s="22"/>
+      <c r="L531" s="23"/>
+      <c r="M531" s="22"/>
+      <c r="N531" s="25"/>
+      <c r="O531" s="21"/>
+      <c r="P531" s="21"/>
+      <c r="Q531" s="19"/>
+      <c r="R531" s="19"/>
+      <c r="S531" s="20"/>
+      <c r="T531" s="20"/>
+      <c r="U531" s="18"/>
+    </row>
+    <row r="532">
+      <c r="A532" s="69"/>
+      <c r="B532" s="70"/>
+      <c r="C532" s="34"/>
+      <c r="D532" s="34"/>
+      <c r="E532" s="34"/>
+      <c r="F532" s="34"/>
+      <c r="G532" s="34"/>
+      <c r="H532" s="21"/>
+      <c r="I532" s="19"/>
+      <c r="J532" s="10"/>
+      <c r="K532" s="22"/>
+      <c r="L532" s="23"/>
+      <c r="M532" s="22"/>
+      <c r="N532" s="25"/>
+      <c r="O532" s="21"/>
+      <c r="P532" s="21"/>
+      <c r="Q532" s="19"/>
+      <c r="R532" s="19"/>
+      <c r="S532" s="20"/>
+      <c r="T532" s="20"/>
+      <c r="U532" s="18"/>
+    </row>
+    <row r="533">
+      <c r="A533" s="69"/>
+      <c r="B533" s="70"/>
+      <c r="C533" s="34"/>
+      <c r="D533" s="34"/>
+      <c r="E533" s="34"/>
+      <c r="F533" s="34"/>
+      <c r="G533" s="34"/>
+      <c r="H533" s="21"/>
+      <c r="I533" s="19"/>
+      <c r="J533" s="10"/>
+      <c r="K533" s="22"/>
+      <c r="L533" s="23"/>
+      <c r="M533" s="22"/>
+      <c r="N533" s="25"/>
+      <c r="O533" s="21"/>
+      <c r="P533" s="21"/>
+      <c r="Q533" s="19"/>
+      <c r="R533" s="19"/>
+      <c r="S533" s="20"/>
+      <c r="T533" s="20"/>
+      <c r="U533" s="18"/>
+    </row>
+    <row r="534">
+      <c r="A534" s="69"/>
+      <c r="B534" s="70"/>
+      <c r="C534" s="34"/>
+      <c r="D534" s="34"/>
+      <c r="E534" s="34"/>
+      <c r="F534" s="34"/>
+      <c r="G534" s="34"/>
+      <c r="H534" s="21"/>
+      <c r="I534" s="19"/>
+      <c r="J534" s="10"/>
+      <c r="K534" s="22"/>
+      <c r="L534" s="23"/>
+      <c r="M534" s="22"/>
+      <c r="N534" s="25"/>
+      <c r="O534" s="21"/>
+      <c r="P534" s="21"/>
+      <c r="Q534" s="19"/>
+      <c r="R534" s="19"/>
+      <c r="S534" s="20"/>
+      <c r="T534" s="20"/>
+      <c r="U534" s="18"/>
+    </row>
+    <row r="535">
+      <c r="A535" s="69"/>
+      <c r="B535" s="70"/>
+      <c r="C535" s="34"/>
+      <c r="D535" s="34"/>
+      <c r="E535" s="34"/>
+      <c r="F535" s="34"/>
+      <c r="G535" s="34"/>
+      <c r="H535" s="21"/>
+      <c r="I535" s="19"/>
+      <c r="J535" s="10"/>
+      <c r="K535" s="22"/>
+      <c r="L535" s="23"/>
+      <c r="M535" s="22"/>
+      <c r="N535" s="25"/>
+      <c r="O535" s="21"/>
+      <c r="P535" s="21"/>
+      <c r="Q535" s="19"/>
+      <c r="R535" s="19"/>
+      <c r="S535" s="20"/>
+      <c r="T535" s="20"/>
+      <c r="U535" s="18"/>
+    </row>
+    <row r="536">
+      <c r="A536" s="69"/>
+      <c r="B536" s="70"/>
+      <c r="C536" s="34"/>
+      <c r="D536" s="34"/>
+      <c r="E536" s="34"/>
+      <c r="F536" s="34"/>
+      <c r="G536" s="34"/>
+      <c r="H536" s="21"/>
+      <c r="I536" s="19"/>
+      <c r="J536" s="10"/>
+      <c r="K536" s="22"/>
+      <c r="L536" s="23"/>
+      <c r="M536" s="22"/>
+      <c r="N536" s="25"/>
+      <c r="O536" s="21"/>
+      <c r="P536" s="21"/>
+      <c r="Q536" s="19"/>
+      <c r="R536" s="19"/>
+      <c r="S536" s="20"/>
+      <c r="T536" s="20"/>
+      <c r="U536" s="18"/>
+    </row>
+    <row r="537">
+      <c r="A537" s="69"/>
+      <c r="B537" s="70"/>
+      <c r="C537" s="34"/>
+      <c r="D537" s="34"/>
+      <c r="E537" s="34"/>
+      <c r="F537" s="34"/>
+      <c r="G537" s="34"/>
+      <c r="H537" s="21"/>
+      <c r="I537" s="19"/>
+      <c r="J537" s="10"/>
+      <c r="K537" s="22"/>
+      <c r="L537" s="23"/>
+      <c r="M537" s="22"/>
+      <c r="N537" s="25"/>
+      <c r="O537" s="21"/>
+      <c r="P537" s="21"/>
+      <c r="Q537" s="19"/>
+      <c r="R537" s="19"/>
+      <c r="S537" s="20"/>
+      <c r="T537" s="20"/>
+      <c r="U537" s="18"/>
+    </row>
+    <row r="538">
+      <c r="A538" s="69"/>
+      <c r="B538" s="70"/>
+      <c r="C538" s="34"/>
+      <c r="D538" s="34"/>
+      <c r="E538" s="34"/>
+      <c r="F538" s="34"/>
+      <c r="G538" s="34"/>
+      <c r="H538" s="21"/>
+      <c r="I538" s="19"/>
+      <c r="J538" s="10"/>
+      <c r="K538" s="22"/>
+      <c r="L538" s="23"/>
+      <c r="M538" s="22"/>
+      <c r="N538" s="25"/>
+      <c r="O538" s="21"/>
+      <c r="P538" s="21"/>
+      <c r="Q538" s="19"/>
+      <c r="R538" s="19"/>
+      <c r="S538" s="20"/>
+      <c r="T538" s="20"/>
+      <c r="U538" s="18"/>
+    </row>
+    <row r="539">
+      <c r="A539" s="69"/>
+      <c r="B539" s="70"/>
+      <c r="C539" s="34"/>
+      <c r="D539" s="34"/>
+      <c r="E539" s="34"/>
+      <c r="F539" s="34"/>
+      <c r="G539" s="34"/>
+      <c r="H539" s="21"/>
+      <c r="I539" s="19"/>
+      <c r="J539" s="10"/>
+      <c r="K539" s="22"/>
+      <c r="L539" s="23"/>
+      <c r="M539" s="22"/>
+      <c r="N539" s="25"/>
+      <c r="O539" s="21"/>
+      <c r="P539" s="21"/>
+      <c r="Q539" s="19"/>
+      <c r="R539" s="19"/>
+      <c r="S539" s="20"/>
+      <c r="T539" s="20"/>
+      <c r="U539" s="18"/>
+    </row>
+    <row r="540">
+      <c r="A540" s="69"/>
+      <c r="B540" s="70"/>
+      <c r="C540" s="34"/>
+      <c r="D540" s="34"/>
+      <c r="E540" s="34"/>
+      <c r="F540" s="34"/>
+      <c r="G540" s="34"/>
+      <c r="H540" s="21"/>
+      <c r="I540" s="19"/>
+      <c r="J540" s="10"/>
+      <c r="K540" s="22"/>
+      <c r="L540" s="23"/>
+      <c r="M540" s="22"/>
+      <c r="N540" s="25"/>
+      <c r="O540" s="21"/>
+      <c r="P540" s="21"/>
+      <c r="Q540" s="19"/>
+      <c r="R540" s="19"/>
+      <c r="S540" s="20"/>
+      <c r="T540" s="20"/>
+      <c r="U540" s="18"/>
+    </row>
+    <row r="541">
+      <c r="A541" s="69"/>
+      <c r="B541" s="70"/>
+      <c r="C541" s="34"/>
+      <c r="D541" s="34"/>
+      <c r="E541" s="34"/>
+      <c r="F541" s="34"/>
+      <c r="G541" s="34"/>
+      <c r="H541" s="21"/>
+      <c r="I541" s="19"/>
+      <c r="J541" s="10"/>
+      <c r="K541" s="22"/>
+      <c r="L541" s="23"/>
+      <c r="M541" s="22"/>
+      <c r="N541" s="25"/>
+      <c r="O541" s="21"/>
+      <c r="P541" s="21"/>
+      <c r="Q541" s="19"/>
+      <c r="R541" s="19"/>
+      <c r="S541" s="20"/>
+      <c r="T541" s="20"/>
+      <c r="U541" s="18"/>
+    </row>
+    <row r="542">
+      <c r="A542" s="69"/>
+      <c r="B542" s="70"/>
+      <c r="C542" s="34"/>
+      <c r="D542" s="34"/>
+      <c r="E542" s="34"/>
+      <c r="F542" s="34"/>
+      <c r="G542" s="34"/>
+      <c r="H542" s="21"/>
+      <c r="I542" s="19"/>
+      <c r="J542" s="10"/>
+      <c r="K542" s="22"/>
+      <c r="L542" s="23"/>
+      <c r="M542" s="22"/>
+      <c r="N542" s="25"/>
+      <c r="O542" s="21"/>
+      <c r="P542" s="21"/>
+      <c r="Q542" s="19"/>
+      <c r="R542" s="19"/>
+      <c r="S542" s="20"/>
+      <c r="T542" s="20"/>
+      <c r="U542" s="18"/>
+    </row>
+    <row r="543">
+      <c r="A543" s="69"/>
+      <c r="B543" s="70"/>
+      <c r="C543" s="34"/>
+      <c r="D543" s="34"/>
+      <c r="E543" s="34"/>
+      <c r="F543" s="34"/>
+      <c r="G543" s="34"/>
+      <c r="H543" s="21"/>
+      <c r="I543" s="19"/>
+      <c r="J543" s="10"/>
+      <c r="K543" s="22"/>
+      <c r="L543" s="23"/>
+      <c r="M543" s="22"/>
+      <c r="N543" s="25"/>
+      <c r="O543" s="21"/>
+      <c r="P543" s="21"/>
+      <c r="Q543" s="19"/>
+      <c r="R543" s="19"/>
+      <c r="S543" s="20"/>
+      <c r="T543" s="20"/>
+      <c r="U543" s="18"/>
+    </row>
+    <row r="544">
+      <c r="A544" s="69"/>
+      <c r="B544" s="70"/>
+      <c r="C544" s="34"/>
+      <c r="D544" s="34"/>
+      <c r="E544" s="34"/>
+      <c r="F544" s="34"/>
+      <c r="G544" s="34"/>
+      <c r="H544" s="21"/>
+      <c r="I544" s="19"/>
+      <c r="J544" s="10"/>
+      <c r="K544" s="22"/>
+      <c r="L544" s="23"/>
+      <c r="M544" s="22"/>
+      <c r="N544" s="25"/>
+      <c r="O544" s="21"/>
+      <c r="P544" s="21"/>
+      <c r="Q544" s="19"/>
+      <c r="R544" s="19"/>
+      <c r="S544" s="20"/>
+      <c r="T544" s="20"/>
+      <c r="U544" s="18"/>
+    </row>
+    <row r="545">
+      <c r="A545" s="69"/>
+      <c r="B545" s="70"/>
+      <c r="C545" s="34"/>
+      <c r="D545" s="34"/>
+      <c r="E545" s="34"/>
+      <c r="F545" s="34"/>
+      <c r="G545" s="34"/>
+      <c r="H545" s="21"/>
+      <c r="I545" s="19"/>
+      <c r="J545" s="10"/>
+      <c r="K545" s="22"/>
+      <c r="L545" s="23"/>
+      <c r="M545" s="22"/>
+      <c r="N545" s="25"/>
+      <c r="O545" s="21"/>
+      <c r="P545" s="21"/>
+      <c r="Q545" s="19"/>
+      <c r="R545" s="19"/>
+      <c r="S545" s="20"/>
+      <c r="T545" s="20"/>
+      <c r="U545" s="18"/>
+    </row>
+    <row r="546">
+      <c r="A546" s="69"/>
+      <c r="B546" s="70"/>
+      <c r="C546" s="34"/>
+      <c r="D546" s="34"/>
+      <c r="E546" s="34"/>
+      <c r="F546" s="34"/>
+      <c r="G546" s="34"/>
+      <c r="H546" s="21"/>
+      <c r="I546" s="19"/>
+      <c r="J546" s="10"/>
+      <c r="K546" s="22"/>
+      <c r="L546" s="23"/>
+      <c r="M546" s="22"/>
+      <c r="N546" s="25"/>
+      <c r="O546" s="21"/>
+      <c r="P546" s="21"/>
+      <c r="Q546" s="19"/>
+      <c r="R546" s="19"/>
+      <c r="S546" s="20"/>
+      <c r="T546" s="20"/>
+      <c r="U546" s="18"/>
+    </row>
+    <row r="547">
+      <c r="A547" s="69"/>
+      <c r="B547" s="70"/>
+      <c r="C547" s="34"/>
+      <c r="D547" s="34"/>
+      <c r="E547" s="34"/>
+      <c r="F547" s="34"/>
+      <c r="G547" s="34"/>
+      <c r="H547" s="21"/>
+      <c r="I547" s="19"/>
+      <c r="J547" s="10"/>
+      <c r="K547" s="22"/>
+      <c r="L547" s="23"/>
+      <c r="M547" s="22"/>
+      <c r="N547" s="25"/>
+      <c r="O547" s="21"/>
+      <c r="P547" s="21"/>
+      <c r="Q547" s="19"/>
+      <c r="R547" s="19"/>
+      <c r="S547" s="20"/>
+      <c r="T547" s="20"/>
+      <c r="U547" s="18"/>
+    </row>
+    <row r="548">
+      <c r="A548" s="69"/>
+      <c r="B548" s="70"/>
+      <c r="C548" s="34"/>
+      <c r="D548" s="34"/>
+      <c r="E548" s="34"/>
+      <c r="F548" s="34"/>
+      <c r="G548" s="34"/>
+      <c r="H548" s="21"/>
+      <c r="I548" s="19"/>
+      <c r="J548" s="10"/>
+      <c r="K548" s="22"/>
+      <c r="L548" s="23"/>
+      <c r="M548" s="22"/>
+      <c r="N548" s="25"/>
+      <c r="O548" s="21"/>
+      <c r="P548" s="21"/>
+      <c r="Q548" s="19"/>
+      <c r="R548" s="19"/>
+      <c r="S548" s="20"/>
+      <c r="T548" s="20"/>
+      <c r="U548" s="18"/>
+    </row>
+    <row r="549">
+      <c r="A549" s="69"/>
+      <c r="B549" s="70"/>
+      <c r="C549" s="34"/>
+      <c r="D549" s="34"/>
+      <c r="E549" s="34"/>
+      <c r="F549" s="34"/>
+      <c r="G549" s="34"/>
+      <c r="H549" s="21"/>
+      <c r="I549" s="19"/>
+      <c r="J549" s="10"/>
+      <c r="K549" s="22"/>
+      <c r="L549" s="23"/>
+      <c r="M549" s="22"/>
+      <c r="N549" s="25"/>
+      <c r="O549" s="21"/>
+      <c r="P549" s="21"/>
+      <c r="Q549" s="19"/>
+      <c r="R549" s="19"/>
+      <c r="S549" s="20"/>
+      <c r="T549" s="20"/>
+      <c r="U549" s="18"/>
+    </row>
+    <row r="550">
+      <c r="A550" s="69"/>
+      <c r="B550" s="70"/>
+      <c r="C550" s="34"/>
+      <c r="D550" s="34"/>
+      <c r="E550" s="34"/>
+      <c r="F550" s="34"/>
+      <c r="G550" s="34"/>
+      <c r="H550" s="21"/>
+      <c r="I550" s="19"/>
+      <c r="J550" s="10"/>
+      <c r="K550" s="22"/>
+      <c r="L550" s="23"/>
+      <c r="M550" s="22"/>
+      <c r="N550" s="25"/>
+      <c r="O550" s="21"/>
+      <c r="P550" s="21"/>
+      <c r="Q550" s="19"/>
+      <c r="R550" s="19"/>
+      <c r="S550" s="20"/>
+      <c r="T550" s="20"/>
+      <c r="U550" s="18"/>
+    </row>
+    <row r="551">
+      <c r="A551" s="69"/>
+      <c r="B551" s="70"/>
+      <c r="C551" s="34"/>
+      <c r="D551" s="34"/>
+      <c r="E551" s="34"/>
+      <c r="F551" s="34"/>
+      <c r="G551" s="34"/>
+      <c r="H551" s="21"/>
+      <c r="I551" s="19"/>
+      <c r="J551" s="10"/>
+      <c r="K551" s="22"/>
+      <c r="L551" s="23"/>
+      <c r="M551" s="22"/>
+      <c r="N551" s="25"/>
+      <c r="O551" s="21"/>
+      <c r="P551" s="21"/>
+      <c r="Q551" s="19"/>
+      <c r="R551" s="19"/>
+      <c r="S551" s="20"/>
+      <c r="T551" s="20"/>
+      <c r="U551" s="18"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="J468">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>(J468&lt;I467)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C501">
+  <conditionalFormatting sqref="C1:C551">
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="男">
       <formula>NOT(ISERROR(SEARCH(("男"),(C1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C501">
+  <conditionalFormatting sqref="C1:C551">
     <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="女">
       <formula>NOT(ISERROR(SEARCH(("女"),(C1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G501">
+  <conditionalFormatting sqref="G2:G551">
     <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="境外">
       <formula>NOT(ISERROR(SEARCH(("境外"),(G2))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G501">
+  <conditionalFormatting sqref="G2:G551">
     <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="本土">
       <formula>NOT(ISERROR(SEARCH(("本土"),(G2))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E501">
+  <conditionalFormatting sqref="E2:E551">
     <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="臺灣">
       <formula>NOT(ISERROR(SEARCH(("臺灣"),(E2))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E501">
+  <conditionalFormatting sqref="E2:E551">
     <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="台灣">
       <formula>NOT(ISERROR(SEARCH(("台灣"),(E2))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E501">
+  <conditionalFormatting sqref="E2:E551">
     <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="中國">
       <formula>NOT(ISERROR(SEARCH(("中國"),(E2))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E501">
+  <conditionalFormatting sqref="E2:E551">
     <cfRule type="notContainsBlanks" dxfId="7" priority="9">
       <formula>LEN(TRIM(E2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B501">
+  <conditionalFormatting sqref="B1:B551">
     <cfRule type="expression" dxfId="8" priority="10">
       <formula>B1&lt;43856.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B501">
+  <conditionalFormatting sqref="B1:B551">
     <cfRule type="expression" dxfId="9" priority="11">
       <formula>B1&lt;43863.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B501">
+  <conditionalFormatting sqref="B1:B551">
     <cfRule type="expression" dxfId="10" priority="12">
       <formula>B1&lt;43870.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B501">
+  <conditionalFormatting sqref="B1:B551">
     <cfRule type="expression" dxfId="11" priority="13">
       <formula>B1&lt;43877.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B501">
+  <conditionalFormatting sqref="B1:B551">
     <cfRule type="expression" dxfId="12" priority="14">
       <formula>B1&lt;43884.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B501">
+  <conditionalFormatting sqref="B1:B551">
     <cfRule type="expression" dxfId="13" priority="15">
       <formula>B1&lt;43891.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B501">
+  <conditionalFormatting sqref="B1:B551">
     <cfRule type="expression" dxfId="14" priority="16">
       <formula>B1&lt;43898.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B501">
+  <conditionalFormatting sqref="B1:B551">
     <cfRule type="expression" dxfId="15" priority="17">
       <formula>B1&lt;43905.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B501">
+  <conditionalFormatting sqref="B1:B551">
     <cfRule type="expression" dxfId="16" priority="18">
       <formula>B1&lt;43912.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B501">
+  <conditionalFormatting sqref="B1:B551">
     <cfRule type="expression" dxfId="17" priority="19">
       <formula>B1&lt;43919.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B501">
+  <conditionalFormatting sqref="B1:B551">
     <cfRule type="expression" dxfId="18" priority="20">
       <formula>B1&lt;43926.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F345 F347:F501">
+  <conditionalFormatting sqref="F1:F345 F347:F551">
     <cfRule type="containsText" dxfId="2" priority="21" operator="containsText" text="南">
       <formula>NOT(ISERROR(SEARCH(("南"),(F1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F345 F347:F501">
+  <conditionalFormatting sqref="F1:F345 F347:F551">
     <cfRule type="containsText" dxfId="19" priority="22" operator="containsText" text="中">
       <formula>NOT(ISERROR(SEARCH(("中"),(F1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F345 F347:F501">
+  <conditionalFormatting sqref="F1:F345 F347:F551">
     <cfRule type="containsText" dxfId="20" priority="23" operator="containsText" text="北">
       <formula>NOT(ISERROR(SEARCH(("北"),(F1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F345 F347:F501">
+  <conditionalFormatting sqref="F1:F345 F347:F551">
     <cfRule type="containsText" dxfId="21" priority="24" operator="containsText" text="東">
       <formula>NOT(ISERROR(SEARCH(("東"),(F1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P1:P389 P394:P501">
+  <conditionalFormatting sqref="P1:P389 P394:P551">
     <cfRule type="containsText" dxfId="22" priority="25" operator="containsText" text="R.I.P">
       <formula>NOT(ISERROR(SEARCH(("R.I.P"),(P1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M1:M501 P1:P389 P394:P501">
+  <conditionalFormatting sqref="M1:M551 P1:P389 P394:P551">
     <cfRule type="containsText" dxfId="23" priority="26" operator="containsText" text="首起">
       <formula>NOT(ISERROR(SEARCH(("首起"),(M1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M1:M501 P1:P389 P394:P501">
+  <conditionalFormatting sqref="M1:M551 P1:P389 P394:P551">
     <cfRule type="containsText" dxfId="23" priority="27" operator="containsText" text="首次">
       <formula>NOT(ISERROR(SEARCH(("首次"),(M1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M1:M501 P1:P389 P394:P501">
+  <conditionalFormatting sqref="M1:M551 P1:P389 P394:P551">
     <cfRule type="containsText" dxfId="23" priority="28" operator="containsText" text="首例">
       <formula>NOT(ISERROR(SEARCH(("首例"),(M1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L1:L501">
+  <conditionalFormatting sqref="L1:L551">
     <cfRule type="containsText" dxfId="24" priority="29" operator="containsText" text="自行">
       <formula>NOT(ISERROR(SEARCH(("自行"),(L1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O1:O501">
+  <conditionalFormatting sqref="O1:O551">
     <cfRule type="containsText" dxfId="25" priority="30" operator="containsText" text="未知">
       <formula>NOT(ISERROR(SEARCH(("未知"),(O1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L1:L501">
+  <conditionalFormatting sqref="L1:L551">
     <cfRule type="containsText" dxfId="26" priority="31" operator="containsText" text="自主">
       <formula>NOT(ISERROR(SEARCH(("自主"),(L1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P1:P389 P394:P501">
+  <conditionalFormatting sqref="P1:P389 P394:P551">
     <cfRule type="containsText" dxfId="27" priority="32" operator="containsText" text="重症">
       <formula>NOT(ISERROR(SEARCH(("重症"),(P1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J394 J397:J466 J469:J501">
+  <conditionalFormatting sqref="J2:J394 J397:J466 J469:J551">
     <cfRule type="expression" dxfId="0" priority="33">
       <formula>(J2&lt;I2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K344 K346:K501">
+  <conditionalFormatting sqref="K2:K344 K346:K551">
     <cfRule type="expression" dxfId="28" priority="34">
       <formula>AND( I2&lt;&gt;"", (LEFT(K2,4) - I2 ) &gt;= 7 )</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B501">
+  <conditionalFormatting sqref="B357:B551">
     <cfRule type="expression" dxfId="29" priority="35">
       <formula>B357&lt;43933.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L1:L501">
+  <conditionalFormatting sqref="L1:L551">
     <cfRule type="containsText" dxfId="30" priority="36" operator="containsText" text="回溯">
       <formula>NOT(ISERROR(SEARCH(("回溯"),(L1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B501">
+  <conditionalFormatting sqref="B357:B551">
     <cfRule type="expression" dxfId="31" priority="37">
       <formula>B357&lt;43940.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B501">
+  <conditionalFormatting sqref="B357:B551">
     <cfRule type="expression" dxfId="32" priority="38">
       <formula>B357&lt;43947.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B501">
+  <conditionalFormatting sqref="B357:B551">
     <cfRule type="expression" dxfId="33" priority="39">
       <formula>B357&lt;43954.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B501">
+  <conditionalFormatting sqref="B357:B551">
     <cfRule type="expression" dxfId="34" priority="40">
       <formula>B357&lt;43961.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B501">
+  <conditionalFormatting sqref="B357:B551">
     <cfRule type="expression" dxfId="35" priority="41">
       <formula>B357&lt;43968.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B501">
+  <conditionalFormatting sqref="B357:B551">
     <cfRule type="expression" dxfId="36" priority="42">
       <formula>B357&lt;43975.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B501">
+  <conditionalFormatting sqref="B357:B551">
     <cfRule type="expression" dxfId="37" priority="43">
       <formula>B357&lt;43982.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G501">
+  <conditionalFormatting sqref="G2:G551">
     <cfRule type="containsText" dxfId="38" priority="44" operator="containsText" text="敦睦">
       <formula>NOT(ISERROR(SEARCH(("敦睦"),(G2))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L1:L501">
+  <conditionalFormatting sqref="L1:L551">
     <cfRule type="containsText" dxfId="14" priority="45" operator="containsText" text="集中">
       <formula>NOT(ISERROR(SEARCH(("集中"),(L1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O1:O501">
+  <conditionalFormatting sqref="O1:O551">
     <cfRule type="containsText" dxfId="39" priority="46" operator="containsText" text="軍艦">
       <formula>NOT(ISERROR(SEARCH(("軍艦"),(O1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B501">
+  <conditionalFormatting sqref="B357:B551">
     <cfRule type="expression" dxfId="40" priority="47">
       <formula>B357&lt;43989.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B501">
+  <conditionalFormatting sqref="B357:B551">
     <cfRule type="expression" dxfId="41" priority="48">
       <formula>B357&lt;43996.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B501">
+  <conditionalFormatting sqref="B357:B551">
     <cfRule type="expression" dxfId="42" priority="49">
       <formula>B357&lt;44003.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B501">
+  <conditionalFormatting sqref="B357:B551">
     <cfRule type="expression" dxfId="43" priority="50">
       <formula>B357&lt;44010.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B501">
+  <conditionalFormatting sqref="B357:B551">
     <cfRule type="expression" dxfId="44" priority="51">
       <formula>B357&lt;44017.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B501">
+  <conditionalFormatting sqref="B357:B551">
     <cfRule type="expression" dxfId="45" priority="52">
       <formula>B357&lt;44024.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B501">
+  <conditionalFormatting sqref="B357:B551">
     <cfRule type="expression" dxfId="46" priority="53">
       <formula>B357&lt;44031.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B501">
+  <conditionalFormatting sqref="B357:B551">
     <cfRule type="expression" dxfId="47" priority="54">
       <formula>B357&lt;44038.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B501">
+  <conditionalFormatting sqref="B357:B551">
     <cfRule type="expression" dxfId="48" priority="55">
       <formula>B357&lt;44045.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B501">
+  <conditionalFormatting sqref="B357:B551">
     <cfRule type="expression" dxfId="49" priority="56">
       <formula>B357&lt;44052.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B501">
+  <conditionalFormatting sqref="B357:B551">
     <cfRule type="expression" dxfId="50" priority="57">
       <formula>B357&lt;44059.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B501">
+  <conditionalFormatting sqref="B357:B551">
     <cfRule type="expression" dxfId="51" priority="58">
       <formula>B357&lt;44066.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B501">
+  <conditionalFormatting sqref="B357:B551">
     <cfRule type="expression" dxfId="52" priority="59">
       <formula>B357&lt;44073.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B501">
+  <conditionalFormatting sqref="B357:B551">
     <cfRule type="expression" dxfId="53" priority="60">
       <formula>B357&lt;44080.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B501">
+  <conditionalFormatting sqref="B357:B551">
     <cfRule type="expression" dxfId="54" priority="61">
       <formula>B357&lt;44087.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B501">
+  <conditionalFormatting sqref="B357:B551">
     <cfRule type="expression" dxfId="55" priority="62">
       <formula>B357&lt;44094.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B501">
+  <conditionalFormatting sqref="B357:B551">
     <cfRule type="expression" dxfId="56" priority="63">
       <formula>B357&lt;44101.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B501">
+  <conditionalFormatting sqref="B357:B551">
     <cfRule type="expression" dxfId="57" priority="64">
       <formula>B357&lt;44108.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L1:L501">
+  <conditionalFormatting sqref="L1:L551">
     <cfRule type="containsText" dxfId="58" priority="65" operator="containsText" text="自費">
       <formula>NOT(ISERROR(SEARCH(("自費"),(L1))))</formula>
     </cfRule>
@@ -37237,15 +38430,16 @@
     <hyperlink r:id="rId59" ref="S497"/>
     <hyperlink r:id="rId60" ref="S498"/>
     <hyperlink r:id="rId61" ref="S499"/>
+    <hyperlink r:id="rId62" ref="S500"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId62"/>
-  <legacyDrawing r:id="rId63"/>
+  <drawing r:id="rId63"/>
+  <legacyDrawing r:id="rId64"/>
   <tableParts count="2">
-    <tablePart r:id="rId66"/>
     <tablePart r:id="rId67"/>
+    <tablePart r:id="rId68"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20200916
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -6764,7 +6764,7 @@
     <numFmt numFmtId="164" formatCode="mm&quot;月&quot;dd&quot;日 &quot;dddd"/>
     <numFmt numFmtId="165" formatCode="m/d"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="17">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -6841,10 +6841,6 @@
       <u/>
       <color rgb="FF1155CC"/>
     </font>
-    <font>
-      <color rgb="FF000000"/>
-    </font>
-    <font/>
   </fonts>
   <fills count="7">
     <fill>
@@ -6890,7 +6886,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="65">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -7078,24 +7074,6 @@
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="18" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -30746,149 +30724,145 @@
 遠訓</v>
       </c>
       <c r="H398" s="8" t="str">
-        <f t="shared" ref="H398:H400" si="47">$H$397</f>
+        <f>$H$3</f>
+        <v>中國武漢</v>
+      </c>
+      <c r="I398" s="9">
+        <f t="shared" ref="I398:I400" si="47">$I$397</f>
+        <v>43936</v>
+      </c>
+      <c r="J398" s="54">
+        <v>43922.0</v>
+      </c>
+      <c r="K398" s="13" t="s">
+        <v>1413</v>
+      </c>
+      <c r="L398" s="12" t="s">
+        <v>438</v>
+      </c>
+      <c r="M398" s="13" t="s">
+        <v>1414</v>
+      </c>
+      <c r="N398" s="25"/>
+      <c r="O398" s="8" t="str">
+        <f t="shared" ref="O398:O400" si="48">$O$397</f>
+        <v>軍艦</v>
+      </c>
+      <c r="P398" s="8" t="s">
+        <v>1415</v>
+      </c>
+      <c r="Q398" s="19"/>
+      <c r="R398" s="19"/>
+      <c r="S398" s="17" t="str">
+        <f t="shared" si="45"/>
+        <v>新增3境外移入確診，為軍艦實習生及軍人</v>
+      </c>
+      <c r="T398" s="20"/>
+      <c r="U398" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v>#397</v>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" s="5" t="s">
+        <v>1416</v>
+      </c>
+      <c r="B399" s="6">
+        <v>43939.0</v>
+      </c>
+      <c r="C399" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D399" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E399" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F399" s="7" t="s">
+        <v>564</v>
+      </c>
+      <c r="G399" s="7" t="str">
+        <f t="shared" si="46"/>
+        <v>敦睦
+遠訓</v>
+      </c>
+      <c r="H399" s="8" t="str">
+        <f t="shared" ref="H399:H400" si="49">$H$397</f>
         <v>海軍敦睦支隊磐石艦
 2/21 整隊登艦
 3/5 台灣啟航
 3/12-3/15 帛琉
 4/9-4/13 左營靠泊檢疫</v>
       </c>
-      <c r="I398" s="9">
-        <f t="shared" ref="I398:I400" si="48">$I$397</f>
+      <c r="I399" s="9">
+        <f t="shared" si="47"/>
         <v>43936</v>
       </c>
-      <c r="J398" s="54">
-        <v>43922.0</v>
-      </c>
-      <c r="K398" s="13" t="s">
-        <v>1413</v>
-      </c>
-      <c r="L398" s="12" t="s">
+      <c r="J399" s="10">
+        <v>43934.0</v>
+      </c>
+      <c r="K399" s="13" t="s">
+        <v>1417</v>
+      </c>
+      <c r="L399" s="12" t="s">
         <v>438</v>
       </c>
-      <c r="M398" s="13" t="s">
-        <v>1414</v>
-      </c>
-      <c r="N398" s="25"/>
-      <c r="O398" s="8" t="str">
-        <f t="shared" ref="O398:O400" si="49">$O$397</f>
+      <c r="M399" s="13" t="s">
+        <v>1418</v>
+      </c>
+      <c r="N399" s="25"/>
+      <c r="O399" s="8" t="str">
+        <f t="shared" si="48"/>
         <v>軍艦</v>
       </c>
-      <c r="P398" s="8" t="s">
-        <v>1415</v>
-      </c>
-      <c r="Q398" s="19"/>
-      <c r="R398" s="19"/>
-      <c r="S398" s="17" t="str">
+      <c r="P399" s="8" t="s">
+        <v>1419</v>
+      </c>
+      <c r="Q399" s="19"/>
+      <c r="R399" s="19"/>
+      <c r="S399" s="17" t="str">
         <f t="shared" si="45"/>
         <v>新增3境外移入確診，為軍艦實習生及軍人</v>
       </c>
-      <c r="T398" s="20"/>
-      <c r="U398" s="18" t="str">
-        <f t="shared" si="1"/>
-        <v>#397</v>
-      </c>
-    </row>
-    <row r="399">
-      <c r="A399" s="5" t="s">
-        <v>1416</v>
-      </c>
-      <c r="B399" s="6">
-        <v>43939.0</v>
-      </c>
-      <c r="C399" s="7" t="s">
+      <c r="T399" s="20"/>
+      <c r="U399" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v>#398</v>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" s="5" t="s">
+        <v>1420</v>
+      </c>
+      <c r="B400" s="6">
+        <v>43940.0</v>
+      </c>
+      <c r="C400" s="55" t="s">
         <v>37</v>
       </c>
-      <c r="D399" s="7" t="s">
+      <c r="D400" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="E399" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F399" s="7" t="s">
-        <v>564</v>
-      </c>
-      <c r="G399" s="7" t="str">
+      <c r="E400" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F400" s="34"/>
+      <c r="G400" s="7" t="str">
         <f t="shared" si="46"/>
         <v>敦睦
 遠訓</v>
       </c>
-      <c r="H399" s="8" t="str">
-        <f t="shared" si="47"/>
+      <c r="H400" s="8" t="str">
+        <f t="shared" si="49"/>
         <v>海軍敦睦支隊磐石艦
 2/21 整隊登艦
 3/5 台灣啟航
 3/12-3/15 帛琉
 4/9-4/13 左營靠泊檢疫</v>
       </c>
-      <c r="I399" s="9">
-        <f t="shared" si="48"/>
-        <v>43936</v>
-      </c>
-      <c r="J399" s="10">
-        <v>43934.0</v>
-      </c>
-      <c r="K399" s="13" t="s">
-        <v>1417</v>
-      </c>
-      <c r="L399" s="12" t="s">
-        <v>438</v>
-      </c>
-      <c r="M399" s="13" t="s">
-        <v>1418</v>
-      </c>
-      <c r="N399" s="25"/>
-      <c r="O399" s="8" t="str">
-        <f t="shared" si="49"/>
-        <v>軍艦</v>
-      </c>
-      <c r="P399" s="8" t="s">
-        <v>1419</v>
-      </c>
-      <c r="Q399" s="19"/>
-      <c r="R399" s="19"/>
-      <c r="S399" s="17" t="str">
-        <f t="shared" si="45"/>
-        <v>新增3境外移入確診，為軍艦實習生及軍人</v>
-      </c>
-      <c r="T399" s="20"/>
-      <c r="U399" s="18" t="str">
-        <f t="shared" si="1"/>
-        <v>#398</v>
-      </c>
-    </row>
-    <row r="400">
-      <c r="A400" s="5" t="s">
-        <v>1420</v>
-      </c>
-      <c r="B400" s="6">
-        <v>43940.0</v>
-      </c>
-      <c r="C400" s="55" t="s">
-        <v>37</v>
-      </c>
-      <c r="D400" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="E400" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F400" s="34"/>
-      <c r="G400" s="7" t="str">
-        <f t="shared" si="46"/>
-        <v>敦睦
-遠訓</v>
-      </c>
-      <c r="H400" s="8" t="str">
+      <c r="I400" s="9">
         <f t="shared" si="47"/>
-        <v>海軍敦睦支隊磐石艦
-2/21 整隊登艦
-3/5 台灣啟航
-3/12-3/15 帛琉
-4/9-4/13 左營靠泊檢疫</v>
-      </c>
-      <c r="I400" s="9">
-        <f t="shared" si="48"/>
         <v>43936</v>
       </c>
       <c r="J400" s="10">
@@ -30905,7 +30879,7 @@
       </c>
       <c r="N400" s="25"/>
       <c r="O400" s="8" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="48"/>
         <v>軍艦</v>
       </c>
       <c r="P400" s="8" t="s">
@@ -36725,23 +36699,23 @@
       <c r="I498" s="9">
         <v>44073.0</v>
       </c>
-      <c r="J498" s="63" t="s">
+      <c r="J498" s="12" t="s">
         <v>1442</v>
       </c>
       <c r="K498" s="13" t="s">
         <v>1808</v>
       </c>
-      <c r="L498" s="63" t="s">
+      <c r="L498" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M498" s="64" t="s">
+      <c r="M498" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N498" s="25"/>
-      <c r="O498" s="65" t="s">
+      <c r="O498" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P498" s="65" t="s">
+      <c r="P498" s="8" t="s">
         <v>1809</v>
       </c>
       <c r="Q498" s="19"/>
@@ -36775,29 +36749,29 @@
       <c r="G499" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H499" s="65" t="s">
+      <c r="H499" s="8" t="s">
         <v>1812</v>
       </c>
-      <c r="I499" s="66">
+      <c r="I499" s="9">
         <v>44083.0</v>
       </c>
       <c r="J499" s="10">
         <v>44026.0</v>
       </c>
-      <c r="K499" s="64" t="s">
+      <c r="K499" s="13" t="s">
         <v>1813</v>
       </c>
-      <c r="L499" s="63" t="s">
+      <c r="L499" s="12" t="s">
         <v>363</v>
       </c>
-      <c r="M499" s="64" t="s">
+      <c r="M499" s="13" t="s">
         <v>1814</v>
       </c>
       <c r="N499" s="25"/>
-      <c r="O499" s="65" t="s">
+      <c r="O499" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P499" s="65" t="s">
+      <c r="P499" s="8" t="s">
         <v>1815</v>
       </c>
       <c r="Q499" s="19"/>
@@ -36812,7 +36786,7 @@
       </c>
     </row>
     <row r="500">
-      <c r="A500" s="67" t="s">
+      <c r="A500" s="16" t="s">
         <v>1816</v>
       </c>
       <c r="B500" s="6">
@@ -36821,7 +36795,7 @@
       <c r="C500" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D500" s="68" t="s">
+      <c r="D500" s="7" t="s">
         <v>76</v>
       </c>
       <c r="E500" s="7" t="s">
@@ -36831,29 +36805,29 @@
       <c r="G500" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H500" s="65" t="s">
+      <c r="H500" s="8" t="s">
         <v>1817</v>
       </c>
-      <c r="I500" s="66">
+      <c r="I500" s="9">
         <v>44084.0</v>
       </c>
-      <c r="J500" s="63" t="s">
+      <c r="J500" s="12" t="s">
         <v>1442</v>
       </c>
-      <c r="K500" s="64" t="s">
+      <c r="K500" s="13" t="s">
         <v>1818</v>
       </c>
-      <c r="L500" s="63" t="s">
+      <c r="L500" s="12" t="s">
         <v>363</v>
       </c>
-      <c r="M500" s="64" t="s">
+      <c r="M500" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N500" s="25"/>
-      <c r="O500" s="65" t="s">
+      <c r="O500" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P500" s="65" t="s">
+      <c r="P500" s="8" t="s">
         <v>1819</v>
       </c>
       <c r="Q500" s="19"/>
@@ -36868,8 +36842,8 @@
       </c>
     </row>
     <row r="501">
-      <c r="A501" s="69"/>
-      <c r="B501" s="70"/>
+      <c r="A501" s="63"/>
+      <c r="B501" s="64"/>
       <c r="C501" s="34"/>
       <c r="D501" s="34"/>
       <c r="E501" s="34"/>
@@ -36894,8 +36868,8 @@
       </c>
     </row>
     <row r="502">
-      <c r="A502" s="69"/>
-      <c r="B502" s="70"/>
+      <c r="A502" s="63"/>
+      <c r="B502" s="64"/>
       <c r="C502" s="34"/>
       <c r="D502" s="34"/>
       <c r="E502" s="34"/>
@@ -36917,8 +36891,8 @@
       <c r="U502" s="18"/>
     </row>
     <row r="503">
-      <c r="A503" s="69"/>
-      <c r="B503" s="70"/>
+      <c r="A503" s="63"/>
+      <c r="B503" s="64"/>
       <c r="C503" s="34"/>
       <c r="D503" s="34"/>
       <c r="E503" s="34"/>
@@ -36940,8 +36914,8 @@
       <c r="U503" s="18"/>
     </row>
     <row r="504">
-      <c r="A504" s="69"/>
-      <c r="B504" s="70"/>
+      <c r="A504" s="63"/>
+      <c r="B504" s="64"/>
       <c r="C504" s="34"/>
       <c r="D504" s="34"/>
       <c r="E504" s="34"/>
@@ -36963,8 +36937,8 @@
       <c r="U504" s="18"/>
     </row>
     <row r="505">
-      <c r="A505" s="69"/>
-      <c r="B505" s="70"/>
+      <c r="A505" s="63"/>
+      <c r="B505" s="64"/>
       <c r="C505" s="34"/>
       <c r="D505" s="34"/>
       <c r="E505" s="34"/>
@@ -36986,8 +36960,8 @@
       <c r="U505" s="18"/>
     </row>
     <row r="506">
-      <c r="A506" s="69"/>
-      <c r="B506" s="70"/>
+      <c r="A506" s="63"/>
+      <c r="B506" s="64"/>
       <c r="C506" s="34"/>
       <c r="D506" s="34"/>
       <c r="E506" s="34"/>
@@ -37009,8 +36983,8 @@
       <c r="U506" s="18"/>
     </row>
     <row r="507">
-      <c r="A507" s="69"/>
-      <c r="B507" s="70"/>
+      <c r="A507" s="63"/>
+      <c r="B507" s="64"/>
       <c r="C507" s="34"/>
       <c r="D507" s="34"/>
       <c r="E507" s="34"/>
@@ -37032,8 +37006,8 @@
       <c r="U507" s="18"/>
     </row>
     <row r="508">
-      <c r="A508" s="69"/>
-      <c r="B508" s="70"/>
+      <c r="A508" s="63"/>
+      <c r="B508" s="64"/>
       <c r="C508" s="34"/>
       <c r="D508" s="34"/>
       <c r="E508" s="34"/>
@@ -37055,8 +37029,8 @@
       <c r="U508" s="18"/>
     </row>
     <row r="509">
-      <c r="A509" s="69"/>
-      <c r="B509" s="70"/>
+      <c r="A509" s="63"/>
+      <c r="B509" s="64"/>
       <c r="C509" s="34"/>
       <c r="D509" s="34"/>
       <c r="E509" s="34"/>
@@ -37078,8 +37052,8 @@
       <c r="U509" s="18"/>
     </row>
     <row r="510">
-      <c r="A510" s="69"/>
-      <c r="B510" s="70"/>
+      <c r="A510" s="63"/>
+      <c r="B510" s="64"/>
       <c r="C510" s="34"/>
       <c r="D510" s="34"/>
       <c r="E510" s="34"/>
@@ -37101,8 +37075,8 @@
       <c r="U510" s="18"/>
     </row>
     <row r="511">
-      <c r="A511" s="69"/>
-      <c r="B511" s="70"/>
+      <c r="A511" s="63"/>
+      <c r="B511" s="64"/>
       <c r="C511" s="34"/>
       <c r="D511" s="34"/>
       <c r="E511" s="34"/>
@@ -37124,8 +37098,8 @@
       <c r="U511" s="18"/>
     </row>
     <row r="512">
-      <c r="A512" s="69"/>
-      <c r="B512" s="70"/>
+      <c r="A512" s="63"/>
+      <c r="B512" s="64"/>
       <c r="C512" s="34"/>
       <c r="D512" s="34"/>
       <c r="E512" s="34"/>
@@ -37147,8 +37121,8 @@
       <c r="U512" s="18"/>
     </row>
     <row r="513">
-      <c r="A513" s="69"/>
-      <c r="B513" s="70"/>
+      <c r="A513" s="63"/>
+      <c r="B513" s="64"/>
       <c r="C513" s="34"/>
       <c r="D513" s="34"/>
       <c r="E513" s="34"/>
@@ -37170,8 +37144,8 @@
       <c r="U513" s="18"/>
     </row>
     <row r="514">
-      <c r="A514" s="69"/>
-      <c r="B514" s="70"/>
+      <c r="A514" s="63"/>
+      <c r="B514" s="64"/>
       <c r="C514" s="34"/>
       <c r="D514" s="34"/>
       <c r="E514" s="34"/>
@@ -37193,8 +37167,8 @@
       <c r="U514" s="18"/>
     </row>
     <row r="515">
-      <c r="A515" s="69"/>
-      <c r="B515" s="70"/>
+      <c r="A515" s="63"/>
+      <c r="B515" s="64"/>
       <c r="C515" s="34"/>
       <c r="D515" s="34"/>
       <c r="E515" s="34"/>
@@ -37216,8 +37190,8 @@
       <c r="U515" s="18"/>
     </row>
     <row r="516">
-      <c r="A516" s="69"/>
-      <c r="B516" s="70"/>
+      <c r="A516" s="63"/>
+      <c r="B516" s="64"/>
       <c r="C516" s="34"/>
       <c r="D516" s="34"/>
       <c r="E516" s="34"/>
@@ -37239,8 +37213,8 @@
       <c r="U516" s="18"/>
     </row>
     <row r="517">
-      <c r="A517" s="69"/>
-      <c r="B517" s="70"/>
+      <c r="A517" s="63"/>
+      <c r="B517" s="64"/>
       <c r="C517" s="34"/>
       <c r="D517" s="34"/>
       <c r="E517" s="34"/>
@@ -37262,8 +37236,8 @@
       <c r="U517" s="18"/>
     </row>
     <row r="518">
-      <c r="A518" s="69"/>
-      <c r="B518" s="70"/>
+      <c r="A518" s="63"/>
+      <c r="B518" s="64"/>
       <c r="C518" s="34"/>
       <c r="D518" s="34"/>
       <c r="E518" s="34"/>
@@ -37285,8 +37259,8 @@
       <c r="U518" s="18"/>
     </row>
     <row r="519">
-      <c r="A519" s="69"/>
-      <c r="B519" s="70"/>
+      <c r="A519" s="63"/>
+      <c r="B519" s="64"/>
       <c r="C519" s="34"/>
       <c r="D519" s="34"/>
       <c r="E519" s="34"/>
@@ -37308,8 +37282,8 @@
       <c r="U519" s="18"/>
     </row>
     <row r="520">
-      <c r="A520" s="69"/>
-      <c r="B520" s="70"/>
+      <c r="A520" s="63"/>
+      <c r="B520" s="64"/>
       <c r="C520" s="34"/>
       <c r="D520" s="34"/>
       <c r="E520" s="34"/>
@@ -37331,8 +37305,8 @@
       <c r="U520" s="18"/>
     </row>
     <row r="521">
-      <c r="A521" s="69"/>
-      <c r="B521" s="70"/>
+      <c r="A521" s="63"/>
+      <c r="B521" s="64"/>
       <c r="C521" s="34"/>
       <c r="D521" s="34"/>
       <c r="E521" s="34"/>
@@ -37354,8 +37328,8 @@
       <c r="U521" s="18"/>
     </row>
     <row r="522">
-      <c r="A522" s="69"/>
-      <c r="B522" s="70"/>
+      <c r="A522" s="63"/>
+      <c r="B522" s="64"/>
       <c r="C522" s="34"/>
       <c r="D522" s="34"/>
       <c r="E522" s="34"/>
@@ -37377,8 +37351,8 @@
       <c r="U522" s="18"/>
     </row>
     <row r="523">
-      <c r="A523" s="69"/>
-      <c r="B523" s="70"/>
+      <c r="A523" s="63"/>
+      <c r="B523" s="64"/>
       <c r="C523" s="34"/>
       <c r="D523" s="34"/>
       <c r="E523" s="34"/>
@@ -37400,8 +37374,8 @@
       <c r="U523" s="18"/>
     </row>
     <row r="524">
-      <c r="A524" s="69"/>
-      <c r="B524" s="70"/>
+      <c r="A524" s="63"/>
+      <c r="B524" s="64"/>
       <c r="C524" s="34"/>
       <c r="D524" s="34"/>
       <c r="E524" s="34"/>
@@ -37423,8 +37397,8 @@
       <c r="U524" s="18"/>
     </row>
     <row r="525">
-      <c r="A525" s="69"/>
-      <c r="B525" s="70"/>
+      <c r="A525" s="63"/>
+      <c r="B525" s="64"/>
       <c r="C525" s="34"/>
       <c r="D525" s="34"/>
       <c r="E525" s="34"/>
@@ -37446,8 +37420,8 @@
       <c r="U525" s="18"/>
     </row>
     <row r="526">
-      <c r="A526" s="69"/>
-      <c r="B526" s="70"/>
+      <c r="A526" s="63"/>
+      <c r="B526" s="64"/>
       <c r="C526" s="34"/>
       <c r="D526" s="34"/>
       <c r="E526" s="34"/>
@@ -37469,8 +37443,8 @@
       <c r="U526" s="18"/>
     </row>
     <row r="527">
-      <c r="A527" s="69"/>
-      <c r="B527" s="70"/>
+      <c r="A527" s="63"/>
+      <c r="B527" s="64"/>
       <c r="C527" s="34"/>
       <c r="D527" s="34"/>
       <c r="E527" s="34"/>
@@ -37492,8 +37466,8 @@
       <c r="U527" s="18"/>
     </row>
     <row r="528">
-      <c r="A528" s="69"/>
-      <c r="B528" s="70"/>
+      <c r="A528" s="63"/>
+      <c r="B528" s="64"/>
       <c r="C528" s="34"/>
       <c r="D528" s="34"/>
       <c r="E528" s="34"/>
@@ -37515,8 +37489,8 @@
       <c r="U528" s="18"/>
     </row>
     <row r="529">
-      <c r="A529" s="69"/>
-      <c r="B529" s="70"/>
+      <c r="A529" s="63"/>
+      <c r="B529" s="64"/>
       <c r="C529" s="34"/>
       <c r="D529" s="34"/>
       <c r="E529" s="34"/>
@@ -37538,8 +37512,8 @@
       <c r="U529" s="18"/>
     </row>
     <row r="530">
-      <c r="A530" s="69"/>
-      <c r="B530" s="70"/>
+      <c r="A530" s="63"/>
+      <c r="B530" s="64"/>
       <c r="C530" s="34"/>
       <c r="D530" s="34"/>
       <c r="E530" s="34"/>
@@ -37561,8 +37535,8 @@
       <c r="U530" s="18"/>
     </row>
     <row r="531">
-      <c r="A531" s="69"/>
-      <c r="B531" s="70"/>
+      <c r="A531" s="63"/>
+      <c r="B531" s="64"/>
       <c r="C531" s="34"/>
       <c r="D531" s="34"/>
       <c r="E531" s="34"/>
@@ -37584,8 +37558,8 @@
       <c r="U531" s="18"/>
     </row>
     <row r="532">
-      <c r="A532" s="69"/>
-      <c r="B532" s="70"/>
+      <c r="A532" s="63"/>
+      <c r="B532" s="64"/>
       <c r="C532" s="34"/>
       <c r="D532" s="34"/>
       <c r="E532" s="34"/>
@@ -37607,8 +37581,8 @@
       <c r="U532" s="18"/>
     </row>
     <row r="533">
-      <c r="A533" s="69"/>
-      <c r="B533" s="70"/>
+      <c r="A533" s="63"/>
+      <c r="B533" s="64"/>
       <c r="C533" s="34"/>
       <c r="D533" s="34"/>
       <c r="E533" s="34"/>
@@ -37630,8 +37604,8 @@
       <c r="U533" s="18"/>
     </row>
     <row r="534">
-      <c r="A534" s="69"/>
-      <c r="B534" s="70"/>
+      <c r="A534" s="63"/>
+      <c r="B534" s="64"/>
       <c r="C534" s="34"/>
       <c r="D534" s="34"/>
       <c r="E534" s="34"/>
@@ -37653,8 +37627,8 @@
       <c r="U534" s="18"/>
     </row>
     <row r="535">
-      <c r="A535" s="69"/>
-      <c r="B535" s="70"/>
+      <c r="A535" s="63"/>
+      <c r="B535" s="64"/>
       <c r="C535" s="34"/>
       <c r="D535" s="34"/>
       <c r="E535" s="34"/>
@@ -37676,8 +37650,8 @@
       <c r="U535" s="18"/>
     </row>
     <row r="536">
-      <c r="A536" s="69"/>
-      <c r="B536" s="70"/>
+      <c r="A536" s="63"/>
+      <c r="B536" s="64"/>
       <c r="C536" s="34"/>
       <c r="D536" s="34"/>
       <c r="E536" s="34"/>
@@ -37699,8 +37673,8 @@
       <c r="U536" s="18"/>
     </row>
     <row r="537">
-      <c r="A537" s="69"/>
-      <c r="B537" s="70"/>
+      <c r="A537" s="63"/>
+      <c r="B537" s="64"/>
       <c r="C537" s="34"/>
       <c r="D537" s="34"/>
       <c r="E537" s="34"/>
@@ -37722,8 +37696,8 @@
       <c r="U537" s="18"/>
     </row>
     <row r="538">
-      <c r="A538" s="69"/>
-      <c r="B538" s="70"/>
+      <c r="A538" s="63"/>
+      <c r="B538" s="64"/>
       <c r="C538" s="34"/>
       <c r="D538" s="34"/>
       <c r="E538" s="34"/>
@@ -37745,8 +37719,8 @@
       <c r="U538" s="18"/>
     </row>
     <row r="539">
-      <c r="A539" s="69"/>
-      <c r="B539" s="70"/>
+      <c r="A539" s="63"/>
+      <c r="B539" s="64"/>
       <c r="C539" s="34"/>
       <c r="D539" s="34"/>
       <c r="E539" s="34"/>
@@ -37768,8 +37742,8 @@
       <c r="U539" s="18"/>
     </row>
     <row r="540">
-      <c r="A540" s="69"/>
-      <c r="B540" s="70"/>
+      <c r="A540" s="63"/>
+      <c r="B540" s="64"/>
       <c r="C540" s="34"/>
       <c r="D540" s="34"/>
       <c r="E540" s="34"/>
@@ -37791,8 +37765,8 @@
       <c r="U540" s="18"/>
     </row>
     <row r="541">
-      <c r="A541" s="69"/>
-      <c r="B541" s="70"/>
+      <c r="A541" s="63"/>
+      <c r="B541" s="64"/>
       <c r="C541" s="34"/>
       <c r="D541" s="34"/>
       <c r="E541" s="34"/>
@@ -37814,8 +37788,8 @@
       <c r="U541" s="18"/>
     </row>
     <row r="542">
-      <c r="A542" s="69"/>
-      <c r="B542" s="70"/>
+      <c r="A542" s="63"/>
+      <c r="B542" s="64"/>
       <c r="C542" s="34"/>
       <c r="D542" s="34"/>
       <c r="E542" s="34"/>
@@ -37837,8 +37811,8 @@
       <c r="U542" s="18"/>
     </row>
     <row r="543">
-      <c r="A543" s="69"/>
-      <c r="B543" s="70"/>
+      <c r="A543" s="63"/>
+      <c r="B543" s="64"/>
       <c r="C543" s="34"/>
       <c r="D543" s="34"/>
       <c r="E543" s="34"/>
@@ -37860,8 +37834,8 @@
       <c r="U543" s="18"/>
     </row>
     <row r="544">
-      <c r="A544" s="69"/>
-      <c r="B544" s="70"/>
+      <c r="A544" s="63"/>
+      <c r="B544" s="64"/>
       <c r="C544" s="34"/>
       <c r="D544" s="34"/>
       <c r="E544" s="34"/>
@@ -37883,8 +37857,8 @@
       <c r="U544" s="18"/>
     </row>
     <row r="545">
-      <c r="A545" s="69"/>
-      <c r="B545" s="70"/>
+      <c r="A545" s="63"/>
+      <c r="B545" s="64"/>
       <c r="C545" s="34"/>
       <c r="D545" s="34"/>
       <c r="E545" s="34"/>
@@ -37906,8 +37880,8 @@
       <c r="U545" s="18"/>
     </row>
     <row r="546">
-      <c r="A546" s="69"/>
-      <c r="B546" s="70"/>
+      <c r="A546" s="63"/>
+      <c r="B546" s="64"/>
       <c r="C546" s="34"/>
       <c r="D546" s="34"/>
       <c r="E546" s="34"/>
@@ -37929,8 +37903,8 @@
       <c r="U546" s="18"/>
     </row>
     <row r="547">
-      <c r="A547" s="69"/>
-      <c r="B547" s="70"/>
+      <c r="A547" s="63"/>
+      <c r="B547" s="64"/>
       <c r="C547" s="34"/>
       <c r="D547" s="34"/>
       <c r="E547" s="34"/>
@@ -37952,8 +37926,8 @@
       <c r="U547" s="18"/>
     </row>
     <row r="548">
-      <c r="A548" s="69"/>
-      <c r="B548" s="70"/>
+      <c r="A548" s="63"/>
+      <c r="B548" s="64"/>
       <c r="C548" s="34"/>
       <c r="D548" s="34"/>
       <c r="E548" s="34"/>
@@ -37975,8 +37949,8 @@
       <c r="U548" s="18"/>
     </row>
     <row r="549">
-      <c r="A549" s="69"/>
-      <c r="B549" s="70"/>
+      <c r="A549" s="63"/>
+      <c r="B549" s="64"/>
       <c r="C549" s="34"/>
       <c r="D549" s="34"/>
       <c r="E549" s="34"/>
@@ -37998,8 +37972,8 @@
       <c r="U549" s="18"/>
     </row>
     <row r="550">
-      <c r="A550" s="69"/>
-      <c r="B550" s="70"/>
+      <c r="A550" s="63"/>
+      <c r="B550" s="64"/>
       <c r="C550" s="34"/>
       <c r="D550" s="34"/>
       <c r="E550" s="34"/>
@@ -38021,8 +37995,8 @@
       <c r="U550" s="18"/>
     </row>
     <row r="551">
-      <c r="A551" s="69"/>
-      <c r="B551" s="70"/>
+      <c r="A551" s="63"/>
+      <c r="B551" s="64"/>
       <c r="C551" s="34"/>
       <c r="D551" s="34"/>
       <c r="E551" s="34"/>

</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20200917
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -563,7 +563,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5485" uniqueCount="1821">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5497" uniqueCount="1825">
   <si>
     <t>案例</t>
   </si>
@@ -6755,6 +6755,19 @@
   <si>
     <t>菲籍女子來台工作，入境採檢確診COVID-19</t>
   </si>
+  <si>
+    <t>#500</t>
+  </si>
+  <si>
+    <t>-9/13 台灣</t>
+  </si>
+  <si>
+    <t>9/13 採檢
+9/16 確診</t>
+  </si>
+  <si>
+    <t>新增1例境外移入COVID-19病例，菲籍女子入境採檢確診</t>
+  </si>
 </sst>
 </file>
 
@@ -6764,7 +6777,7 @@
     <numFmt numFmtId="164" formatCode="mm&quot;月&quot;dd&quot;日 &quot;dddd"/>
     <numFmt numFmtId="165" formatCode="m/d"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="19">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -6841,6 +6854,10 @@
       <u/>
       <color rgb="FF1155CC"/>
     </font>
+    <font/>
+    <font>
+      <color rgb="FF000000"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -6886,7 +6903,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="71">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -7075,6 +7092,24 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
@@ -36842,34 +36877,62 @@
       </c>
     </row>
     <row r="501">
-      <c r="A501" s="63"/>
-      <c r="B501" s="64"/>
-      <c r="C501" s="34"/>
-      <c r="D501" s="34"/>
-      <c r="E501" s="34"/>
+      <c r="A501" s="63" t="s">
+        <v>1821</v>
+      </c>
+      <c r="B501" s="6">
+        <v>44090.0</v>
+      </c>
+      <c r="C501" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D501" s="64" t="s">
+        <v>116</v>
+      </c>
+      <c r="E501" s="7" t="s">
+        <v>205</v>
+      </c>
       <c r="F501" s="34"/>
-      <c r="G501" s="34"/>
-      <c r="H501" s="21"/>
-      <c r="I501" s="19"/>
-      <c r="J501" s="10"/>
-      <c r="K501" s="22"/>
-      <c r="L501" s="23"/>
-      <c r="M501" s="22"/>
+      <c r="G501" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H501" s="65" t="s">
+        <v>1822</v>
+      </c>
+      <c r="I501" s="66">
+        <v>44087.0</v>
+      </c>
+      <c r="J501" s="67" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K501" s="68" t="s">
+        <v>1823</v>
+      </c>
+      <c r="L501" s="67" t="s">
+        <v>363</v>
+      </c>
+      <c r="M501" s="68" t="s">
+        <v>1442</v>
+      </c>
       <c r="N501" s="25"/>
-      <c r="O501" s="21"/>
+      <c r="O501" s="65" t="s">
+        <v>85</v>
+      </c>
       <c r="P501" s="21"/>
       <c r="Q501" s="19"/>
       <c r="R501" s="19"/>
-      <c r="S501" s="20"/>
+      <c r="S501" s="61" t="s">
+        <v>1824</v>
+      </c>
       <c r="T501" s="20"/>
       <c r="U501" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#500</v>
       </c>
     </row>
     <row r="502">
-      <c r="A502" s="63"/>
-      <c r="B502" s="64"/>
+      <c r="A502" s="69"/>
+      <c r="B502" s="70"/>
       <c r="C502" s="34"/>
       <c r="D502" s="34"/>
       <c r="E502" s="34"/>
@@ -36891,8 +36954,8 @@
       <c r="U502" s="18"/>
     </row>
     <row r="503">
-      <c r="A503" s="63"/>
-      <c r="B503" s="64"/>
+      <c r="A503" s="69"/>
+      <c r="B503" s="70"/>
       <c r="C503" s="34"/>
       <c r="D503" s="34"/>
       <c r="E503" s="34"/>
@@ -36914,8 +36977,8 @@
       <c r="U503" s="18"/>
     </row>
     <row r="504">
-      <c r="A504" s="63"/>
-      <c r="B504" s="64"/>
+      <c r="A504" s="69"/>
+      <c r="B504" s="70"/>
       <c r="C504" s="34"/>
       <c r="D504" s="34"/>
       <c r="E504" s="34"/>
@@ -36937,8 +37000,8 @@
       <c r="U504" s="18"/>
     </row>
     <row r="505">
-      <c r="A505" s="63"/>
-      <c r="B505" s="64"/>
+      <c r="A505" s="69"/>
+      <c r="B505" s="70"/>
       <c r="C505" s="34"/>
       <c r="D505" s="34"/>
       <c r="E505" s="34"/>
@@ -36960,8 +37023,8 @@
       <c r="U505" s="18"/>
     </row>
     <row r="506">
-      <c r="A506" s="63"/>
-      <c r="B506" s="64"/>
+      <c r="A506" s="69"/>
+      <c r="B506" s="70"/>
       <c r="C506" s="34"/>
       <c r="D506" s="34"/>
       <c r="E506" s="34"/>
@@ -36983,8 +37046,8 @@
       <c r="U506" s="18"/>
     </row>
     <row r="507">
-      <c r="A507" s="63"/>
-      <c r="B507" s="64"/>
+      <c r="A507" s="69"/>
+      <c r="B507" s="70"/>
       <c r="C507" s="34"/>
       <c r="D507" s="34"/>
       <c r="E507" s="34"/>
@@ -37006,8 +37069,8 @@
       <c r="U507" s="18"/>
     </row>
     <row r="508">
-      <c r="A508" s="63"/>
-      <c r="B508" s="64"/>
+      <c r="A508" s="69"/>
+      <c r="B508" s="70"/>
       <c r="C508" s="34"/>
       <c r="D508" s="34"/>
       <c r="E508" s="34"/>
@@ -37029,8 +37092,8 @@
       <c r="U508" s="18"/>
     </row>
     <row r="509">
-      <c r="A509" s="63"/>
-      <c r="B509" s="64"/>
+      <c r="A509" s="69"/>
+      <c r="B509" s="70"/>
       <c r="C509" s="34"/>
       <c r="D509" s="34"/>
       <c r="E509" s="34"/>
@@ -37052,8 +37115,8 @@
       <c r="U509" s="18"/>
     </row>
     <row r="510">
-      <c r="A510" s="63"/>
-      <c r="B510" s="64"/>
+      <c r="A510" s="69"/>
+      <c r="B510" s="70"/>
       <c r="C510" s="34"/>
       <c r="D510" s="34"/>
       <c r="E510" s="34"/>
@@ -37075,8 +37138,8 @@
       <c r="U510" s="18"/>
     </row>
     <row r="511">
-      <c r="A511" s="63"/>
-      <c r="B511" s="64"/>
+      <c r="A511" s="69"/>
+      <c r="B511" s="70"/>
       <c r="C511" s="34"/>
       <c r="D511" s="34"/>
       <c r="E511" s="34"/>
@@ -37098,8 +37161,8 @@
       <c r="U511" s="18"/>
     </row>
     <row r="512">
-      <c r="A512" s="63"/>
-      <c r="B512" s="64"/>
+      <c r="A512" s="69"/>
+      <c r="B512" s="70"/>
       <c r="C512" s="34"/>
       <c r="D512" s="34"/>
       <c r="E512" s="34"/>
@@ -37121,8 +37184,8 @@
       <c r="U512" s="18"/>
     </row>
     <row r="513">
-      <c r="A513" s="63"/>
-      <c r="B513" s="64"/>
+      <c r="A513" s="69"/>
+      <c r="B513" s="70"/>
       <c r="C513" s="34"/>
       <c r="D513" s="34"/>
       <c r="E513" s="34"/>
@@ -37144,8 +37207,8 @@
       <c r="U513" s="18"/>
     </row>
     <row r="514">
-      <c r="A514" s="63"/>
-      <c r="B514" s="64"/>
+      <c r="A514" s="69"/>
+      <c r="B514" s="70"/>
       <c r="C514" s="34"/>
       <c r="D514" s="34"/>
       <c r="E514" s="34"/>
@@ -37167,8 +37230,8 @@
       <c r="U514" s="18"/>
     </row>
     <row r="515">
-      <c r="A515" s="63"/>
-      <c r="B515" s="64"/>
+      <c r="A515" s="69"/>
+      <c r="B515" s="70"/>
       <c r="C515" s="34"/>
       <c r="D515" s="34"/>
       <c r="E515" s="34"/>
@@ -37190,8 +37253,8 @@
       <c r="U515" s="18"/>
     </row>
     <row r="516">
-      <c r="A516" s="63"/>
-      <c r="B516" s="64"/>
+      <c r="A516" s="69"/>
+      <c r="B516" s="70"/>
       <c r="C516" s="34"/>
       <c r="D516" s="34"/>
       <c r="E516" s="34"/>
@@ -37213,8 +37276,8 @@
       <c r="U516" s="18"/>
     </row>
     <row r="517">
-      <c r="A517" s="63"/>
-      <c r="B517" s="64"/>
+      <c r="A517" s="69"/>
+      <c r="B517" s="70"/>
       <c r="C517" s="34"/>
       <c r="D517" s="34"/>
       <c r="E517" s="34"/>
@@ -37236,8 +37299,8 @@
       <c r="U517" s="18"/>
     </row>
     <row r="518">
-      <c r="A518" s="63"/>
-      <c r="B518" s="64"/>
+      <c r="A518" s="69"/>
+      <c r="B518" s="70"/>
       <c r="C518" s="34"/>
       <c r="D518" s="34"/>
       <c r="E518" s="34"/>
@@ -37259,8 +37322,8 @@
       <c r="U518" s="18"/>
     </row>
     <row r="519">
-      <c r="A519" s="63"/>
-      <c r="B519" s="64"/>
+      <c r="A519" s="69"/>
+      <c r="B519" s="70"/>
       <c r="C519" s="34"/>
       <c r="D519" s="34"/>
       <c r="E519" s="34"/>
@@ -37282,8 +37345,8 @@
       <c r="U519" s="18"/>
     </row>
     <row r="520">
-      <c r="A520" s="63"/>
-      <c r="B520" s="64"/>
+      <c r="A520" s="69"/>
+      <c r="B520" s="70"/>
       <c r="C520" s="34"/>
       <c r="D520" s="34"/>
       <c r="E520" s="34"/>
@@ -37305,8 +37368,8 @@
       <c r="U520" s="18"/>
     </row>
     <row r="521">
-      <c r="A521" s="63"/>
-      <c r="B521" s="64"/>
+      <c r="A521" s="69"/>
+      <c r="B521" s="70"/>
       <c r="C521" s="34"/>
       <c r="D521" s="34"/>
       <c r="E521" s="34"/>
@@ -37328,8 +37391,8 @@
       <c r="U521" s="18"/>
     </row>
     <row r="522">
-      <c r="A522" s="63"/>
-      <c r="B522" s="64"/>
+      <c r="A522" s="69"/>
+      <c r="B522" s="70"/>
       <c r="C522" s="34"/>
       <c r="D522" s="34"/>
       <c r="E522" s="34"/>
@@ -37351,8 +37414,8 @@
       <c r="U522" s="18"/>
     </row>
     <row r="523">
-      <c r="A523" s="63"/>
-      <c r="B523" s="64"/>
+      <c r="A523" s="69"/>
+      <c r="B523" s="70"/>
       <c r="C523" s="34"/>
       <c r="D523" s="34"/>
       <c r="E523" s="34"/>
@@ -37374,8 +37437,8 @@
       <c r="U523" s="18"/>
     </row>
     <row r="524">
-      <c r="A524" s="63"/>
-      <c r="B524" s="64"/>
+      <c r="A524" s="69"/>
+      <c r="B524" s="70"/>
       <c r="C524" s="34"/>
       <c r="D524" s="34"/>
       <c r="E524" s="34"/>
@@ -37397,8 +37460,8 @@
       <c r="U524" s="18"/>
     </row>
     <row r="525">
-      <c r="A525" s="63"/>
-      <c r="B525" s="64"/>
+      <c r="A525" s="69"/>
+      <c r="B525" s="70"/>
       <c r="C525" s="34"/>
       <c r="D525" s="34"/>
       <c r="E525" s="34"/>
@@ -37420,8 +37483,8 @@
       <c r="U525" s="18"/>
     </row>
     <row r="526">
-      <c r="A526" s="63"/>
-      <c r="B526" s="64"/>
+      <c r="A526" s="69"/>
+      <c r="B526" s="70"/>
       <c r="C526" s="34"/>
       <c r="D526" s="34"/>
       <c r="E526" s="34"/>
@@ -37443,8 +37506,8 @@
       <c r="U526" s="18"/>
     </row>
     <row r="527">
-      <c r="A527" s="63"/>
-      <c r="B527" s="64"/>
+      <c r="A527" s="69"/>
+      <c r="B527" s="70"/>
       <c r="C527" s="34"/>
       <c r="D527" s="34"/>
       <c r="E527" s="34"/>
@@ -37466,8 +37529,8 @@
       <c r="U527" s="18"/>
     </row>
     <row r="528">
-      <c r="A528" s="63"/>
-      <c r="B528" s="64"/>
+      <c r="A528" s="69"/>
+      <c r="B528" s="70"/>
       <c r="C528" s="34"/>
       <c r="D528" s="34"/>
       <c r="E528" s="34"/>
@@ -37489,8 +37552,8 @@
       <c r="U528" s="18"/>
     </row>
     <row r="529">
-      <c r="A529" s="63"/>
-      <c r="B529" s="64"/>
+      <c r="A529" s="69"/>
+      <c r="B529" s="70"/>
       <c r="C529" s="34"/>
       <c r="D529" s="34"/>
       <c r="E529" s="34"/>
@@ -37512,8 +37575,8 @@
       <c r="U529" s="18"/>
     </row>
     <row r="530">
-      <c r="A530" s="63"/>
-      <c r="B530" s="64"/>
+      <c r="A530" s="69"/>
+      <c r="B530" s="70"/>
       <c r="C530" s="34"/>
       <c r="D530" s="34"/>
       <c r="E530" s="34"/>
@@ -37535,8 +37598,8 @@
       <c r="U530" s="18"/>
     </row>
     <row r="531">
-      <c r="A531" s="63"/>
-      <c r="B531" s="64"/>
+      <c r="A531" s="69"/>
+      <c r="B531" s="70"/>
       <c r="C531" s="34"/>
       <c r="D531" s="34"/>
       <c r="E531" s="34"/>
@@ -37558,8 +37621,8 @@
       <c r="U531" s="18"/>
     </row>
     <row r="532">
-      <c r="A532" s="63"/>
-      <c r="B532" s="64"/>
+      <c r="A532" s="69"/>
+      <c r="B532" s="70"/>
       <c r="C532" s="34"/>
       <c r="D532" s="34"/>
       <c r="E532" s="34"/>
@@ -37581,8 +37644,8 @@
       <c r="U532" s="18"/>
     </row>
     <row r="533">
-      <c r="A533" s="63"/>
-      <c r="B533" s="64"/>
+      <c r="A533" s="69"/>
+      <c r="B533" s="70"/>
       <c r="C533" s="34"/>
       <c r="D533" s="34"/>
       <c r="E533" s="34"/>
@@ -37604,8 +37667,8 @@
       <c r="U533" s="18"/>
     </row>
     <row r="534">
-      <c r="A534" s="63"/>
-      <c r="B534" s="64"/>
+      <c r="A534" s="69"/>
+      <c r="B534" s="70"/>
       <c r="C534" s="34"/>
       <c r="D534" s="34"/>
       <c r="E534" s="34"/>
@@ -37627,8 +37690,8 @@
       <c r="U534" s="18"/>
     </row>
     <row r="535">
-      <c r="A535" s="63"/>
-      <c r="B535" s="64"/>
+      <c r="A535" s="69"/>
+      <c r="B535" s="70"/>
       <c r="C535" s="34"/>
       <c r="D535" s="34"/>
       <c r="E535" s="34"/>
@@ -37650,8 +37713,8 @@
       <c r="U535" s="18"/>
     </row>
     <row r="536">
-      <c r="A536" s="63"/>
-      <c r="B536" s="64"/>
+      <c r="A536" s="69"/>
+      <c r="B536" s="70"/>
       <c r="C536" s="34"/>
       <c r="D536" s="34"/>
       <c r="E536" s="34"/>
@@ -37673,8 +37736,8 @@
       <c r="U536" s="18"/>
     </row>
     <row r="537">
-      <c r="A537" s="63"/>
-      <c r="B537" s="64"/>
+      <c r="A537" s="69"/>
+      <c r="B537" s="70"/>
       <c r="C537" s="34"/>
       <c r="D537" s="34"/>
       <c r="E537" s="34"/>
@@ -37696,8 +37759,8 @@
       <c r="U537" s="18"/>
     </row>
     <row r="538">
-      <c r="A538" s="63"/>
-      <c r="B538" s="64"/>
+      <c r="A538" s="69"/>
+      <c r="B538" s="70"/>
       <c r="C538" s="34"/>
       <c r="D538" s="34"/>
       <c r="E538" s="34"/>
@@ -37719,8 +37782,8 @@
       <c r="U538" s="18"/>
     </row>
     <row r="539">
-      <c r="A539" s="63"/>
-      <c r="B539" s="64"/>
+      <c r="A539" s="69"/>
+      <c r="B539" s="70"/>
       <c r="C539" s="34"/>
       <c r="D539" s="34"/>
       <c r="E539" s="34"/>
@@ -37742,8 +37805,8 @@
       <c r="U539" s="18"/>
     </row>
     <row r="540">
-      <c r="A540" s="63"/>
-      <c r="B540" s="64"/>
+      <c r="A540" s="69"/>
+      <c r="B540" s="70"/>
       <c r="C540" s="34"/>
       <c r="D540" s="34"/>
       <c r="E540" s="34"/>
@@ -37765,8 +37828,8 @@
       <c r="U540" s="18"/>
     </row>
     <row r="541">
-      <c r="A541" s="63"/>
-      <c r="B541" s="64"/>
+      <c r="A541" s="69"/>
+      <c r="B541" s="70"/>
       <c r="C541" s="34"/>
       <c r="D541" s="34"/>
       <c r="E541" s="34"/>
@@ -37788,8 +37851,8 @@
       <c r="U541" s="18"/>
     </row>
     <row r="542">
-      <c r="A542" s="63"/>
-      <c r="B542" s="64"/>
+      <c r="A542" s="69"/>
+      <c r="B542" s="70"/>
       <c r="C542" s="34"/>
       <c r="D542" s="34"/>
       <c r="E542" s="34"/>
@@ -37811,8 +37874,8 @@
       <c r="U542" s="18"/>
     </row>
     <row r="543">
-      <c r="A543" s="63"/>
-      <c r="B543" s="64"/>
+      <c r="A543" s="69"/>
+      <c r="B543" s="70"/>
       <c r="C543" s="34"/>
       <c r="D543" s="34"/>
       <c r="E543" s="34"/>
@@ -37834,8 +37897,8 @@
       <c r="U543" s="18"/>
     </row>
     <row r="544">
-      <c r="A544" s="63"/>
-      <c r="B544" s="64"/>
+      <c r="A544" s="69"/>
+      <c r="B544" s="70"/>
       <c r="C544" s="34"/>
       <c r="D544" s="34"/>
       <c r="E544" s="34"/>
@@ -37857,8 +37920,8 @@
       <c r="U544" s="18"/>
     </row>
     <row r="545">
-      <c r="A545" s="63"/>
-      <c r="B545" s="64"/>
+      <c r="A545" s="69"/>
+      <c r="B545" s="70"/>
       <c r="C545" s="34"/>
       <c r="D545" s="34"/>
       <c r="E545" s="34"/>
@@ -37880,8 +37943,8 @@
       <c r="U545" s="18"/>
     </row>
     <row r="546">
-      <c r="A546" s="63"/>
-      <c r="B546" s="64"/>
+      <c r="A546" s="69"/>
+      <c r="B546" s="70"/>
       <c r="C546" s="34"/>
       <c r="D546" s="34"/>
       <c r="E546" s="34"/>
@@ -37903,8 +37966,8 @@
       <c r="U546" s="18"/>
     </row>
     <row r="547">
-      <c r="A547" s="63"/>
-      <c r="B547" s="64"/>
+      <c r="A547" s="69"/>
+      <c r="B547" s="70"/>
       <c r="C547" s="34"/>
       <c r="D547" s="34"/>
       <c r="E547" s="34"/>
@@ -37926,8 +37989,8 @@
       <c r="U547" s="18"/>
     </row>
     <row r="548">
-      <c r="A548" s="63"/>
-      <c r="B548" s="64"/>
+      <c r="A548" s="69"/>
+      <c r="B548" s="70"/>
       <c r="C548" s="34"/>
       <c r="D548" s="34"/>
       <c r="E548" s="34"/>
@@ -37949,8 +38012,8 @@
       <c r="U548" s="18"/>
     </row>
     <row r="549">
-      <c r="A549" s="63"/>
-      <c r="B549" s="64"/>
+      <c r="A549" s="69"/>
+      <c r="B549" s="70"/>
       <c r="C549" s="34"/>
       <c r="D549" s="34"/>
       <c r="E549" s="34"/>
@@ -37972,8 +38035,8 @@
       <c r="U549" s="18"/>
     </row>
     <row r="550">
-      <c r="A550" s="63"/>
-      <c r="B550" s="64"/>
+      <c r="A550" s="69"/>
+      <c r="B550" s="70"/>
       <c r="C550" s="34"/>
       <c r="D550" s="34"/>
       <c r="E550" s="34"/>
@@ -37995,8 +38058,8 @@
       <c r="U550" s="18"/>
     </row>
     <row r="551">
-      <c r="A551" s="63"/>
-      <c r="B551" s="64"/>
+      <c r="A551" s="69"/>
+      <c r="B551" s="70"/>
       <c r="C551" s="34"/>
       <c r="D551" s="34"/>
       <c r="E551" s="34"/>
@@ -38405,15 +38468,16 @@
     <hyperlink r:id="rId60" ref="S498"/>
     <hyperlink r:id="rId61" ref="S499"/>
     <hyperlink r:id="rId62" ref="S500"/>
+    <hyperlink r:id="rId63" ref="S501"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId63"/>
-  <legacyDrawing r:id="rId64"/>
+  <drawing r:id="rId64"/>
+  <legacyDrawing r:id="rId65"/>
   <tableParts count="2">
-    <tablePart r:id="rId67"/>
     <tablePart r:id="rId68"/>
+    <tablePart r:id="rId69"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20200918
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -563,7 +563,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5497" uniqueCount="1825">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5534" uniqueCount="1840">
   <si>
     <t>案例</t>
   </si>
@@ -6767,6 +6767,57 @@
   </si>
   <si>
     <t>新增1例境外移入COVID-19病例，菲籍女子入境採檢確診</t>
+  </si>
+  <si>
+    <t>#501</t>
+  </si>
+  <si>
+    <t>2月-9/13 緬甸</t>
+  </si>
+  <si>
+    <t>9/13 採檢
+9/17 確診</t>
+  </si>
+  <si>
+    <t>自述在當地曾與確診個案同桌用餐超過2小時</t>
+  </si>
+  <si>
+    <t>國內新增3例COVID-19個案，均為境外移入</t>
+  </si>
+  <si>
+    <t>#502</t>
+  </si>
+  <si>
+    <t>2月-9/6 英國</t>
+  </si>
+  <si>
+    <t>9/15 採檢
+9/17 確診</t>
+  </si>
+  <si>
+    <t>腹瀉 腹痛 喉嚨痛 流鼻水 鼻塞</t>
+  </si>
+  <si>
+    <t>9月6日入境時無不適症狀，入境後前往防疫旅館居家檢疫
+9月10日曾有輕微喉嚨痛
+15日出現腹瀉、腹痛、喉嚨痛、流鼻水及鼻塞等症狀</t>
+  </si>
+  <si>
+    <t>#503</t>
+  </si>
+  <si>
+    <t>3月-9/13 菲律賓</t>
+  </si>
+  <si>
+    <t>9/13 採檢
+9/16 二採
+9/17 確診</t>
+  </si>
+  <si>
+    <t>鼻塞 流鼻水 喉嚨乾癢 咳嗽 嗅覺變差 胸悶</t>
+  </si>
+  <si>
+    <t>9月13日與案500搭乘同班機(非案500座位前後二排旅客)返國，入境時主動告知有症狀，初次採檢結果為陰性</t>
   </si>
 </sst>
 </file>
@@ -6903,7 +6954,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -7110,6 +7161,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="18" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
@@ -8238,7 +8292,7 @@
         <v>國內首例確診患者已痊癒將出院 向防疫及醫護人員表達感謝</v>
       </c>
       <c r="U2" s="18" t="str">
-        <f t="shared" ref="U2:U501" si="1">A2</f>
+        <f t="shared" ref="U2:U551" si="1">A2</f>
         <v>#001</v>
       </c>
     </row>
@@ -36931,77 +36985,176 @@
       </c>
     </row>
     <row r="502">
-      <c r="A502" s="69"/>
-      <c r="B502" s="70"/>
-      <c r="C502" s="34"/>
-      <c r="D502" s="34"/>
-      <c r="E502" s="34"/>
+      <c r="A502" s="63" t="s">
+        <v>1825</v>
+      </c>
+      <c r="B502" s="6">
+        <v>44091.0</v>
+      </c>
+      <c r="C502" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D502" s="64" t="s">
+        <v>59</v>
+      </c>
+      <c r="E502" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F502" s="34"/>
-      <c r="G502" s="34"/>
-      <c r="H502" s="21"/>
-      <c r="I502" s="19"/>
-      <c r="J502" s="10"/>
-      <c r="K502" s="22"/>
-      <c r="L502" s="23"/>
-      <c r="M502" s="22"/>
+      <c r="G502" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H502" s="65" t="s">
+        <v>1826</v>
+      </c>
+      <c r="I502" s="66">
+        <v>44087.0</v>
+      </c>
+      <c r="J502" s="67" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K502" s="68" t="s">
+        <v>1827</v>
+      </c>
+      <c r="L502" s="67" t="s">
+        <v>363</v>
+      </c>
+      <c r="M502" s="68" t="s">
+        <v>1442</v>
+      </c>
       <c r="N502" s="25"/>
-      <c r="O502" s="21"/>
-      <c r="P502" s="21"/>
+      <c r="O502" s="65" t="s">
+        <v>85</v>
+      </c>
+      <c r="P502" s="65" t="s">
+        <v>1828</v>
+      </c>
       <c r="Q502" s="19"/>
       <c r="R502" s="19"/>
-      <c r="S502" s="20"/>
+      <c r="S502" s="61" t="s">
+        <v>1829</v>
+      </c>
       <c r="T502" s="20"/>
-      <c r="U502" s="18"/>
+      <c r="U502" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v>#501</v>
+      </c>
     </row>
     <row r="503">
-      <c r="A503" s="69"/>
-      <c r="B503" s="70"/>
-      <c r="C503" s="34"/>
-      <c r="D503" s="34"/>
-      <c r="E503" s="34"/>
+      <c r="A503" s="63" t="s">
+        <v>1830</v>
+      </c>
+      <c r="B503" s="6">
+        <v>44091.0</v>
+      </c>
+      <c r="C503" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D503" s="64" t="s">
+        <v>76</v>
+      </c>
+      <c r="E503" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F503" s="34"/>
-      <c r="G503" s="34"/>
-      <c r="H503" s="21"/>
-      <c r="I503" s="19"/>
-      <c r="J503" s="10"/>
-      <c r="K503" s="22"/>
-      <c r="L503" s="23"/>
-      <c r="M503" s="22"/>
+      <c r="G503" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H503" s="65" t="s">
+        <v>1831</v>
+      </c>
+      <c r="I503" s="66">
+        <v>44080.0</v>
+      </c>
+      <c r="J503" s="69">
+        <v>44084.0</v>
+      </c>
+      <c r="K503" s="13" t="s">
+        <v>1832</v>
+      </c>
+      <c r="L503" s="67" t="s">
+        <v>426</v>
+      </c>
+      <c r="M503" s="68" t="s">
+        <v>1833</v>
+      </c>
       <c r="N503" s="25"/>
-      <c r="O503" s="21"/>
-      <c r="P503" s="21"/>
+      <c r="O503" s="65" t="s">
+        <v>85</v>
+      </c>
+      <c r="P503" s="65" t="s">
+        <v>1834</v>
+      </c>
       <c r="Q503" s="19"/>
       <c r="R503" s="19"/>
-      <c r="S503" s="20"/>
+      <c r="S503" s="61" t="s">
+        <v>1829</v>
+      </c>
       <c r="T503" s="20"/>
-      <c r="U503" s="18"/>
+      <c r="U503" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v>#502</v>
+      </c>
     </row>
     <row r="504">
-      <c r="A504" s="69"/>
-      <c r="B504" s="70"/>
-      <c r="C504" s="34"/>
-      <c r="D504" s="34"/>
-      <c r="E504" s="34"/>
+      <c r="A504" s="63" t="s">
+        <v>1835</v>
+      </c>
+      <c r="B504" s="6">
+        <v>44091.0</v>
+      </c>
+      <c r="C504" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D504" s="64" t="s">
+        <v>116</v>
+      </c>
+      <c r="E504" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F504" s="34"/>
-      <c r="G504" s="34"/>
-      <c r="H504" s="21"/>
-      <c r="I504" s="19"/>
-      <c r="J504" s="10"/>
-      <c r="K504" s="22"/>
-      <c r="L504" s="23"/>
-      <c r="M504" s="22"/>
+      <c r="G504" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H504" s="65" t="s">
+        <v>1836</v>
+      </c>
+      <c r="I504" s="66">
+        <v>44087.0</v>
+      </c>
+      <c r="J504" s="10">
+        <v>44084.0</v>
+      </c>
+      <c r="K504" s="68" t="s">
+        <v>1837</v>
+      </c>
+      <c r="L504" s="67" t="s">
+        <v>363</v>
+      </c>
+      <c r="M504" s="68" t="s">
+        <v>1838</v>
+      </c>
       <c r="N504" s="25"/>
-      <c r="O504" s="21"/>
-      <c r="P504" s="21"/>
+      <c r="O504" s="65" t="s">
+        <v>85</v>
+      </c>
+      <c r="P504" s="65" t="s">
+        <v>1839</v>
+      </c>
       <c r="Q504" s="19"/>
       <c r="R504" s="19"/>
-      <c r="S504" s="20"/>
+      <c r="S504" s="61" t="s">
+        <v>1829</v>
+      </c>
       <c r="T504" s="20"/>
-      <c r="U504" s="18"/>
+      <c r="U504" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v>#503</v>
+      </c>
     </row>
     <row r="505">
-      <c r="A505" s="69"/>
-      <c r="B505" s="70"/>
+      <c r="A505" s="70"/>
+      <c r="B505" s="71"/>
       <c r="C505" s="34"/>
       <c r="D505" s="34"/>
       <c r="E505" s="34"/>
@@ -37020,11 +37173,14 @@
       <c r="R505" s="19"/>
       <c r="S505" s="20"/>
       <c r="T505" s="20"/>
-      <c r="U505" s="18"/>
+      <c r="U505" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="506">
-      <c r="A506" s="69"/>
-      <c r="B506" s="70"/>
+      <c r="A506" s="70"/>
+      <c r="B506" s="71"/>
       <c r="C506" s="34"/>
       <c r="D506" s="34"/>
       <c r="E506" s="34"/>
@@ -37043,11 +37199,14 @@
       <c r="R506" s="19"/>
       <c r="S506" s="20"/>
       <c r="T506" s="20"/>
-      <c r="U506" s="18"/>
+      <c r="U506" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="507">
-      <c r="A507" s="69"/>
-      <c r="B507" s="70"/>
+      <c r="A507" s="70"/>
+      <c r="B507" s="71"/>
       <c r="C507" s="34"/>
       <c r="D507" s="34"/>
       <c r="E507" s="34"/>
@@ -37066,11 +37225,14 @@
       <c r="R507" s="19"/>
       <c r="S507" s="20"/>
       <c r="T507" s="20"/>
-      <c r="U507" s="18"/>
+      <c r="U507" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="508">
-      <c r="A508" s="69"/>
-      <c r="B508" s="70"/>
+      <c r="A508" s="70"/>
+      <c r="B508" s="71"/>
       <c r="C508" s="34"/>
       <c r="D508" s="34"/>
       <c r="E508" s="34"/>
@@ -37089,11 +37251,14 @@
       <c r="R508" s="19"/>
       <c r="S508" s="20"/>
       <c r="T508" s="20"/>
-      <c r="U508" s="18"/>
+      <c r="U508" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="509">
-      <c r="A509" s="69"/>
-      <c r="B509" s="70"/>
+      <c r="A509" s="70"/>
+      <c r="B509" s="71"/>
       <c r="C509" s="34"/>
       <c r="D509" s="34"/>
       <c r="E509" s="34"/>
@@ -37112,11 +37277,14 @@
       <c r="R509" s="19"/>
       <c r="S509" s="20"/>
       <c r="T509" s="20"/>
-      <c r="U509" s="18"/>
+      <c r="U509" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="510">
-      <c r="A510" s="69"/>
-      <c r="B510" s="70"/>
+      <c r="A510" s="70"/>
+      <c r="B510" s="71"/>
       <c r="C510" s="34"/>
       <c r="D510" s="34"/>
       <c r="E510" s="34"/>
@@ -37135,11 +37303,14 @@
       <c r="R510" s="19"/>
       <c r="S510" s="20"/>
       <c r="T510" s="20"/>
-      <c r="U510" s="18"/>
+      <c r="U510" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="511">
-      <c r="A511" s="69"/>
-      <c r="B511" s="70"/>
+      <c r="A511" s="70"/>
+      <c r="B511" s="71"/>
       <c r="C511" s="34"/>
       <c r="D511" s="34"/>
       <c r="E511" s="34"/>
@@ -37158,11 +37329,14 @@
       <c r="R511" s="19"/>
       <c r="S511" s="20"/>
       <c r="T511" s="20"/>
-      <c r="U511" s="18"/>
+      <c r="U511" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="512">
-      <c r="A512" s="69"/>
-      <c r="B512" s="70"/>
+      <c r="A512" s="70"/>
+      <c r="B512" s="71"/>
       <c r="C512" s="34"/>
       <c r="D512" s="34"/>
       <c r="E512" s="34"/>
@@ -37181,11 +37355,14 @@
       <c r="R512" s="19"/>
       <c r="S512" s="20"/>
       <c r="T512" s="20"/>
-      <c r="U512" s="18"/>
+      <c r="U512" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="513">
-      <c r="A513" s="69"/>
-      <c r="B513" s="70"/>
+      <c r="A513" s="70"/>
+      <c r="B513" s="71"/>
       <c r="C513" s="34"/>
       <c r="D513" s="34"/>
       <c r="E513" s="34"/>
@@ -37204,11 +37381,14 @@
       <c r="R513" s="19"/>
       <c r="S513" s="20"/>
       <c r="T513" s="20"/>
-      <c r="U513" s="18"/>
+      <c r="U513" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="514">
-      <c r="A514" s="69"/>
-      <c r="B514" s="70"/>
+      <c r="A514" s="70"/>
+      <c r="B514" s="71"/>
       <c r="C514" s="34"/>
       <c r="D514" s="34"/>
       <c r="E514" s="34"/>
@@ -37227,11 +37407,14 @@
       <c r="R514" s="19"/>
       <c r="S514" s="20"/>
       <c r="T514" s="20"/>
-      <c r="U514" s="18"/>
+      <c r="U514" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="515">
-      <c r="A515" s="69"/>
-      <c r="B515" s="70"/>
+      <c r="A515" s="70"/>
+      <c r="B515" s="71"/>
       <c r="C515" s="34"/>
       <c r="D515" s="34"/>
       <c r="E515" s="34"/>
@@ -37250,11 +37433,14 @@
       <c r="R515" s="19"/>
       <c r="S515" s="20"/>
       <c r="T515" s="20"/>
-      <c r="U515" s="18"/>
+      <c r="U515" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="516">
-      <c r="A516" s="69"/>
-      <c r="B516" s="70"/>
+      <c r="A516" s="70"/>
+      <c r="B516" s="71"/>
       <c r="C516" s="34"/>
       <c r="D516" s="34"/>
       <c r="E516" s="34"/>
@@ -37273,11 +37459,14 @@
       <c r="R516" s="19"/>
       <c r="S516" s="20"/>
       <c r="T516" s="20"/>
-      <c r="U516" s="18"/>
+      <c r="U516" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="517">
-      <c r="A517" s="69"/>
-      <c r="B517" s="70"/>
+      <c r="A517" s="70"/>
+      <c r="B517" s="71"/>
       <c r="C517" s="34"/>
       <c r="D517" s="34"/>
       <c r="E517" s="34"/>
@@ -37296,11 +37485,14 @@
       <c r="R517" s="19"/>
       <c r="S517" s="20"/>
       <c r="T517" s="20"/>
-      <c r="U517" s="18"/>
+      <c r="U517" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="518">
-      <c r="A518" s="69"/>
-      <c r="B518" s="70"/>
+      <c r="A518" s="70"/>
+      <c r="B518" s="71"/>
       <c r="C518" s="34"/>
       <c r="D518" s="34"/>
       <c r="E518" s="34"/>
@@ -37319,11 +37511,14 @@
       <c r="R518" s="19"/>
       <c r="S518" s="20"/>
       <c r="T518" s="20"/>
-      <c r="U518" s="18"/>
+      <c r="U518" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="519">
-      <c r="A519" s="69"/>
-      <c r="B519" s="70"/>
+      <c r="A519" s="70"/>
+      <c r="B519" s="71"/>
       <c r="C519" s="34"/>
       <c r="D519" s="34"/>
       <c r="E519" s="34"/>
@@ -37342,11 +37537,14 @@
       <c r="R519" s="19"/>
       <c r="S519" s="20"/>
       <c r="T519" s="20"/>
-      <c r="U519" s="18"/>
+      <c r="U519" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="520">
-      <c r="A520" s="69"/>
-      <c r="B520" s="70"/>
+      <c r="A520" s="70"/>
+      <c r="B520" s="71"/>
       <c r="C520" s="34"/>
       <c r="D520" s="34"/>
       <c r="E520" s="34"/>
@@ -37365,11 +37563,14 @@
       <c r="R520" s="19"/>
       <c r="S520" s="20"/>
       <c r="T520" s="20"/>
-      <c r="U520" s="18"/>
+      <c r="U520" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="521">
-      <c r="A521" s="69"/>
-      <c r="B521" s="70"/>
+      <c r="A521" s="70"/>
+      <c r="B521" s="71"/>
       <c r="C521" s="34"/>
       <c r="D521" s="34"/>
       <c r="E521" s="34"/>
@@ -37388,11 +37589,14 @@
       <c r="R521" s="19"/>
       <c r="S521" s="20"/>
       <c r="T521" s="20"/>
-      <c r="U521" s="18"/>
+      <c r="U521" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="522">
-      <c r="A522" s="69"/>
-      <c r="B522" s="70"/>
+      <c r="A522" s="70"/>
+      <c r="B522" s="71"/>
       <c r="C522" s="34"/>
       <c r="D522" s="34"/>
       <c r="E522" s="34"/>
@@ -37411,11 +37615,14 @@
       <c r="R522" s="19"/>
       <c r="S522" s="20"/>
       <c r="T522" s="20"/>
-      <c r="U522" s="18"/>
+      <c r="U522" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="523">
-      <c r="A523" s="69"/>
-      <c r="B523" s="70"/>
+      <c r="A523" s="70"/>
+      <c r="B523" s="71"/>
       <c r="C523" s="34"/>
       <c r="D523" s="34"/>
       <c r="E523" s="34"/>
@@ -37434,11 +37641,14 @@
       <c r="R523" s="19"/>
       <c r="S523" s="20"/>
       <c r="T523" s="20"/>
-      <c r="U523" s="18"/>
+      <c r="U523" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="524">
-      <c r="A524" s="69"/>
-      <c r="B524" s="70"/>
+      <c r="A524" s="70"/>
+      <c r="B524" s="71"/>
       <c r="C524" s="34"/>
       <c r="D524" s="34"/>
       <c r="E524" s="34"/>
@@ -37457,11 +37667,14 @@
       <c r="R524" s="19"/>
       <c r="S524" s="20"/>
       <c r="T524" s="20"/>
-      <c r="U524" s="18"/>
+      <c r="U524" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="525">
-      <c r="A525" s="69"/>
-      <c r="B525" s="70"/>
+      <c r="A525" s="70"/>
+      <c r="B525" s="71"/>
       <c r="C525" s="34"/>
       <c r="D525" s="34"/>
       <c r="E525" s="34"/>
@@ -37480,11 +37693,14 @@
       <c r="R525" s="19"/>
       <c r="S525" s="20"/>
       <c r="T525" s="20"/>
-      <c r="U525" s="18"/>
+      <c r="U525" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="526">
-      <c r="A526" s="69"/>
-      <c r="B526" s="70"/>
+      <c r="A526" s="70"/>
+      <c r="B526" s="71"/>
       <c r="C526" s="34"/>
       <c r="D526" s="34"/>
       <c r="E526" s="34"/>
@@ -37503,11 +37719,14 @@
       <c r="R526" s="19"/>
       <c r="S526" s="20"/>
       <c r="T526" s="20"/>
-      <c r="U526" s="18"/>
+      <c r="U526" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="527">
-      <c r="A527" s="69"/>
-      <c r="B527" s="70"/>
+      <c r="A527" s="70"/>
+      <c r="B527" s="71"/>
       <c r="C527" s="34"/>
       <c r="D527" s="34"/>
       <c r="E527" s="34"/>
@@ -37526,11 +37745,14 @@
       <c r="R527" s="19"/>
       <c r="S527" s="20"/>
       <c r="T527" s="20"/>
-      <c r="U527" s="18"/>
+      <c r="U527" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="528">
-      <c r="A528" s="69"/>
-      <c r="B528" s="70"/>
+      <c r="A528" s="70"/>
+      <c r="B528" s="71"/>
       <c r="C528" s="34"/>
       <c r="D528" s="34"/>
       <c r="E528" s="34"/>
@@ -37549,11 +37771,14 @@
       <c r="R528" s="19"/>
       <c r="S528" s="20"/>
       <c r="T528" s="20"/>
-      <c r="U528" s="18"/>
+      <c r="U528" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="529">
-      <c r="A529" s="69"/>
-      <c r="B529" s="70"/>
+      <c r="A529" s="70"/>
+      <c r="B529" s="71"/>
       <c r="C529" s="34"/>
       <c r="D529" s="34"/>
       <c r="E529" s="34"/>
@@ -37572,11 +37797,14 @@
       <c r="R529" s="19"/>
       <c r="S529" s="20"/>
       <c r="T529" s="20"/>
-      <c r="U529" s="18"/>
+      <c r="U529" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="530">
-      <c r="A530" s="69"/>
-      <c r="B530" s="70"/>
+      <c r="A530" s="70"/>
+      <c r="B530" s="71"/>
       <c r="C530" s="34"/>
       <c r="D530" s="34"/>
       <c r="E530" s="34"/>
@@ -37595,11 +37823,14 @@
       <c r="R530" s="19"/>
       <c r="S530" s="20"/>
       <c r="T530" s="20"/>
-      <c r="U530" s="18"/>
+      <c r="U530" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="531">
-      <c r="A531" s="69"/>
-      <c r="B531" s="70"/>
+      <c r="A531" s="70"/>
+      <c r="B531" s="71"/>
       <c r="C531" s="34"/>
       <c r="D531" s="34"/>
       <c r="E531" s="34"/>
@@ -37618,11 +37849,14 @@
       <c r="R531" s="19"/>
       <c r="S531" s="20"/>
       <c r="T531" s="20"/>
-      <c r="U531" s="18"/>
+      <c r="U531" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="532">
-      <c r="A532" s="69"/>
-      <c r="B532" s="70"/>
+      <c r="A532" s="70"/>
+      <c r="B532" s="71"/>
       <c r="C532" s="34"/>
       <c r="D532" s="34"/>
       <c r="E532" s="34"/>
@@ -37641,11 +37875,14 @@
       <c r="R532" s="19"/>
       <c r="S532" s="20"/>
       <c r="T532" s="20"/>
-      <c r="U532" s="18"/>
+      <c r="U532" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="533">
-      <c r="A533" s="69"/>
-      <c r="B533" s="70"/>
+      <c r="A533" s="70"/>
+      <c r="B533" s="71"/>
       <c r="C533" s="34"/>
       <c r="D533" s="34"/>
       <c r="E533" s="34"/>
@@ -37664,11 +37901,14 @@
       <c r="R533" s="19"/>
       <c r="S533" s="20"/>
       <c r="T533" s="20"/>
-      <c r="U533" s="18"/>
+      <c r="U533" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="534">
-      <c r="A534" s="69"/>
-      <c r="B534" s="70"/>
+      <c r="A534" s="70"/>
+      <c r="B534" s="71"/>
       <c r="C534" s="34"/>
       <c r="D534" s="34"/>
       <c r="E534" s="34"/>
@@ -37687,11 +37927,14 @@
       <c r="R534" s="19"/>
       <c r="S534" s="20"/>
       <c r="T534" s="20"/>
-      <c r="U534" s="18"/>
+      <c r="U534" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="535">
-      <c r="A535" s="69"/>
-      <c r="B535" s="70"/>
+      <c r="A535" s="70"/>
+      <c r="B535" s="71"/>
       <c r="C535" s="34"/>
       <c r="D535" s="34"/>
       <c r="E535" s="34"/>
@@ -37710,11 +37953,14 @@
       <c r="R535" s="19"/>
       <c r="S535" s="20"/>
       <c r="T535" s="20"/>
-      <c r="U535" s="18"/>
+      <c r="U535" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="536">
-      <c r="A536" s="69"/>
-      <c r="B536" s="70"/>
+      <c r="A536" s="70"/>
+      <c r="B536" s="71"/>
       <c r="C536" s="34"/>
       <c r="D536" s="34"/>
       <c r="E536" s="34"/>
@@ -37733,11 +37979,14 @@
       <c r="R536" s="19"/>
       <c r="S536" s="20"/>
       <c r="T536" s="20"/>
-      <c r="U536" s="18"/>
+      <c r="U536" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="537">
-      <c r="A537" s="69"/>
-      <c r="B537" s="70"/>
+      <c r="A537" s="70"/>
+      <c r="B537" s="71"/>
       <c r="C537" s="34"/>
       <c r="D537" s="34"/>
       <c r="E537" s="34"/>
@@ -37756,11 +38005,14 @@
       <c r="R537" s="19"/>
       <c r="S537" s="20"/>
       <c r="T537" s="20"/>
-      <c r="U537" s="18"/>
+      <c r="U537" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="538">
-      <c r="A538" s="69"/>
-      <c r="B538" s="70"/>
+      <c r="A538" s="70"/>
+      <c r="B538" s="71"/>
       <c r="C538" s="34"/>
       <c r="D538" s="34"/>
       <c r="E538" s="34"/>
@@ -37779,11 +38031,14 @@
       <c r="R538" s="19"/>
       <c r="S538" s="20"/>
       <c r="T538" s="20"/>
-      <c r="U538" s="18"/>
+      <c r="U538" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="539">
-      <c r="A539" s="69"/>
-      <c r="B539" s="70"/>
+      <c r="A539" s="70"/>
+      <c r="B539" s="71"/>
       <c r="C539" s="34"/>
       <c r="D539" s="34"/>
       <c r="E539" s="34"/>
@@ -37802,11 +38057,14 @@
       <c r="R539" s="19"/>
       <c r="S539" s="20"/>
       <c r="T539" s="20"/>
-      <c r="U539" s="18"/>
+      <c r="U539" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="540">
-      <c r="A540" s="69"/>
-      <c r="B540" s="70"/>
+      <c r="A540" s="70"/>
+      <c r="B540" s="71"/>
       <c r="C540" s="34"/>
       <c r="D540" s="34"/>
       <c r="E540" s="34"/>
@@ -37825,11 +38083,14 @@
       <c r="R540" s="19"/>
       <c r="S540" s="20"/>
       <c r="T540" s="20"/>
-      <c r="U540" s="18"/>
+      <c r="U540" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="541">
-      <c r="A541" s="69"/>
-      <c r="B541" s="70"/>
+      <c r="A541" s="70"/>
+      <c r="B541" s="71"/>
       <c r="C541" s="34"/>
       <c r="D541" s="34"/>
       <c r="E541" s="34"/>
@@ -37848,11 +38109,14 @@
       <c r="R541" s="19"/>
       <c r="S541" s="20"/>
       <c r="T541" s="20"/>
-      <c r="U541" s="18"/>
+      <c r="U541" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="542">
-      <c r="A542" s="69"/>
-      <c r="B542" s="70"/>
+      <c r="A542" s="70"/>
+      <c r="B542" s="71"/>
       <c r="C542" s="34"/>
       <c r="D542" s="34"/>
       <c r="E542" s="34"/>
@@ -37871,11 +38135,14 @@
       <c r="R542" s="19"/>
       <c r="S542" s="20"/>
       <c r="T542" s="20"/>
-      <c r="U542" s="18"/>
+      <c r="U542" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="543">
-      <c r="A543" s="69"/>
-      <c r="B543" s="70"/>
+      <c r="A543" s="70"/>
+      <c r="B543" s="71"/>
       <c r="C543" s="34"/>
       <c r="D543" s="34"/>
       <c r="E543" s="34"/>
@@ -37894,11 +38161,14 @@
       <c r="R543" s="19"/>
       <c r="S543" s="20"/>
       <c r="T543" s="20"/>
-      <c r="U543" s="18"/>
+      <c r="U543" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="544">
-      <c r="A544" s="69"/>
-      <c r="B544" s="70"/>
+      <c r="A544" s="70"/>
+      <c r="B544" s="71"/>
       <c r="C544" s="34"/>
       <c r="D544" s="34"/>
       <c r="E544" s="34"/>
@@ -37917,11 +38187,14 @@
       <c r="R544" s="19"/>
       <c r="S544" s="20"/>
       <c r="T544" s="20"/>
-      <c r="U544" s="18"/>
+      <c r="U544" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="545">
-      <c r="A545" s="69"/>
-      <c r="B545" s="70"/>
+      <c r="A545" s="70"/>
+      <c r="B545" s="71"/>
       <c r="C545" s="34"/>
       <c r="D545" s="34"/>
       <c r="E545" s="34"/>
@@ -37940,11 +38213,14 @@
       <c r="R545" s="19"/>
       <c r="S545" s="20"/>
       <c r="T545" s="20"/>
-      <c r="U545" s="18"/>
+      <c r="U545" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="546">
-      <c r="A546" s="69"/>
-      <c r="B546" s="70"/>
+      <c r="A546" s="70"/>
+      <c r="B546" s="71"/>
       <c r="C546" s="34"/>
       <c r="D546" s="34"/>
       <c r="E546" s="34"/>
@@ -37963,11 +38239,14 @@
       <c r="R546" s="19"/>
       <c r="S546" s="20"/>
       <c r="T546" s="20"/>
-      <c r="U546" s="18"/>
+      <c r="U546" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="547">
-      <c r="A547" s="69"/>
-      <c r="B547" s="70"/>
+      <c r="A547" s="70"/>
+      <c r="B547" s="71"/>
       <c r="C547" s="34"/>
       <c r="D547" s="34"/>
       <c r="E547" s="34"/>
@@ -37986,11 +38265,14 @@
       <c r="R547" s="19"/>
       <c r="S547" s="20"/>
       <c r="T547" s="20"/>
-      <c r="U547" s="18"/>
+      <c r="U547" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="548">
-      <c r="A548" s="69"/>
-      <c r="B548" s="70"/>
+      <c r="A548" s="70"/>
+      <c r="B548" s="71"/>
       <c r="C548" s="34"/>
       <c r="D548" s="34"/>
       <c r="E548" s="34"/>
@@ -38009,11 +38291,14 @@
       <c r="R548" s="19"/>
       <c r="S548" s="20"/>
       <c r="T548" s="20"/>
-      <c r="U548" s="18"/>
+      <c r="U548" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="549">
-      <c r="A549" s="69"/>
-      <c r="B549" s="70"/>
+      <c r="A549" s="70"/>
+      <c r="B549" s="71"/>
       <c r="C549" s="34"/>
       <c r="D549" s="34"/>
       <c r="E549" s="34"/>
@@ -38032,11 +38317,14 @@
       <c r="R549" s="19"/>
       <c r="S549" s="20"/>
       <c r="T549" s="20"/>
-      <c r="U549" s="18"/>
+      <c r="U549" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="550">
-      <c r="A550" s="69"/>
-      <c r="B550" s="70"/>
+      <c r="A550" s="70"/>
+      <c r="B550" s="71"/>
       <c r="C550" s="34"/>
       <c r="D550" s="34"/>
       <c r="E550" s="34"/>
@@ -38055,11 +38343,14 @@
       <c r="R550" s="19"/>
       <c r="S550" s="20"/>
       <c r="T550" s="20"/>
-      <c r="U550" s="18"/>
+      <c r="U550" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="551">
-      <c r="A551" s="69"/>
-      <c r="B551" s="70"/>
+      <c r="A551" s="70"/>
+      <c r="B551" s="71"/>
       <c r="C551" s="34"/>
       <c r="D551" s="34"/>
       <c r="E551" s="34"/>
@@ -38078,7 +38369,10 @@
       <c r="R551" s="19"/>
       <c r="S551" s="20"/>
       <c r="T551" s="20"/>
-      <c r="U551" s="18"/>
+      <c r="U551" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="J468">
@@ -38469,15 +38763,18 @@
     <hyperlink r:id="rId61" ref="S499"/>
     <hyperlink r:id="rId62" ref="S500"/>
     <hyperlink r:id="rId63" ref="S501"/>
+    <hyperlink r:id="rId64" ref="S502"/>
+    <hyperlink r:id="rId65" ref="S503"/>
+    <hyperlink r:id="rId66" ref="S504"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId64"/>
-  <legacyDrawing r:id="rId65"/>
+  <drawing r:id="rId67"/>
+  <legacyDrawing r:id="rId68"/>
   <tableParts count="2">
-    <tablePart r:id="rId68"/>
-    <tablePart r:id="rId69"/>
+    <tablePart r:id="rId71"/>
+    <tablePart r:id="rId72"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20200919
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -563,7 +563,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5534" uniqueCount="1840">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5563" uniqueCount="1850">
   <si>
     <t>案例</t>
   </si>
@@ -6818,6 +6818,37 @@
   </si>
   <si>
     <t>9月13日與案500搭乘同班機(非案500座位前後二排旅客)返國，入境時主動告知有症狀，初次採檢結果為陰性</t>
+  </si>
+  <si>
+    <t>#504</t>
+  </si>
+  <si>
+    <t>-9/17 台灣</t>
+  </si>
+  <si>
+    <t>9/17 採檢
+9/19 確診</t>
+  </si>
+  <si>
+    <t>喉嚨有痰</t>
+  </si>
+  <si>
+    <t>國內新確診3例COVID-19個案，均為境外移入</t>
+  </si>
+  <si>
+    <t>#505</t>
+  </si>
+  <si>
+    <t>2月-9/17 緬甸</t>
+  </si>
+  <si>
+    <t>喉嚨癢 咳嗽 喉嚨痛 鼻塞</t>
+  </si>
+  <si>
+    <t>入境時無不適症狀，並主動告知在緬甸當地曾與確診個案一起用餐</t>
+  </si>
+  <si>
+    <t>#506</t>
   </si>
 </sst>
 </file>
@@ -37153,65 +37184,135 @@
       </c>
     </row>
     <row r="505">
-      <c r="A505" s="70"/>
-      <c r="B505" s="71"/>
-      <c r="C505" s="34"/>
-      <c r="D505" s="34"/>
-      <c r="E505" s="34"/>
+      <c r="A505" s="63" t="s">
+        <v>1840</v>
+      </c>
+      <c r="B505" s="6">
+        <v>44093.0</v>
+      </c>
+      <c r="C505" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D505" s="64" t="s">
+        <v>76</v>
+      </c>
+      <c r="E505" s="7" t="s">
+        <v>205</v>
+      </c>
       <c r="F505" s="34"/>
-      <c r="G505" s="34"/>
-      <c r="H505" s="21"/>
-      <c r="I505" s="19"/>
-      <c r="J505" s="10"/>
-      <c r="K505" s="22"/>
-      <c r="L505" s="23"/>
-      <c r="M505" s="22"/>
+      <c r="G505" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H505" s="65" t="s">
+        <v>1841</v>
+      </c>
+      <c r="I505" s="66">
+        <v>44091.0</v>
+      </c>
+      <c r="J505" s="69">
+        <v>44092.0</v>
+      </c>
+      <c r="K505" s="68" t="s">
+        <v>1842</v>
+      </c>
+      <c r="L505" s="67" t="s">
+        <v>363</v>
+      </c>
+      <c r="M505" s="68" t="s">
+        <v>1843</v>
+      </c>
       <c r="N505" s="25"/>
-      <c r="O505" s="21"/>
+      <c r="O505" s="65" t="s">
+        <v>85</v>
+      </c>
       <c r="P505" s="21"/>
       <c r="Q505" s="19"/>
       <c r="R505" s="19"/>
-      <c r="S505" s="20"/>
+      <c r="S505" s="61" t="s">
+        <v>1844</v>
+      </c>
       <c r="T505" s="20"/>
       <c r="U505" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#504</v>
       </c>
     </row>
     <row r="506">
-      <c r="A506" s="70"/>
-      <c r="B506" s="71"/>
-      <c r="C506" s="34"/>
-      <c r="D506" s="34"/>
-      <c r="E506" s="34"/>
+      <c r="A506" s="63" t="s">
+        <v>1845</v>
+      </c>
+      <c r="B506" s="6">
+        <v>44093.0</v>
+      </c>
+      <c r="C506" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D506" s="64" t="s">
+        <v>116</v>
+      </c>
+      <c r="E506" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F506" s="34"/>
-      <c r="G506" s="34"/>
-      <c r="H506" s="21"/>
-      <c r="I506" s="19"/>
-      <c r="J506" s="10"/>
-      <c r="K506" s="22"/>
-      <c r="L506" s="23"/>
-      <c r="M506" s="22"/>
+      <c r="G506" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H506" s="65" t="s">
+        <v>1846</v>
+      </c>
+      <c r="I506" s="66">
+        <v>44091.0</v>
+      </c>
+      <c r="J506" s="69">
+        <v>44091.0</v>
+      </c>
+      <c r="K506" s="68" t="s">
+        <v>1842</v>
+      </c>
+      <c r="L506" s="67" t="s">
+        <v>363</v>
+      </c>
+      <c r="M506" s="68" t="s">
+        <v>1847</v>
+      </c>
       <c r="N506" s="25"/>
-      <c r="O506" s="21"/>
-      <c r="P506" s="21"/>
+      <c r="O506" s="65" t="s">
+        <v>85</v>
+      </c>
+      <c r="P506" s="65" t="s">
+        <v>1848</v>
+      </c>
       <c r="Q506" s="19"/>
       <c r="R506" s="19"/>
-      <c r="S506" s="20"/>
+      <c r="S506" s="61" t="s">
+        <v>1844</v>
+      </c>
       <c r="T506" s="20"/>
       <c r="U506" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#505</v>
       </c>
     </row>
     <row r="507">
-      <c r="A507" s="70"/>
-      <c r="B507" s="71"/>
-      <c r="C507" s="34"/>
-      <c r="D507" s="34"/>
-      <c r="E507" s="34"/>
+      <c r="A507" s="63" t="s">
+        <v>1849</v>
+      </c>
+      <c r="B507" s="6">
+        <v>44093.0</v>
+      </c>
+      <c r="C507" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D507" s="64" t="s">
+        <v>22</v>
+      </c>
+      <c r="E507" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F507" s="34"/>
-      <c r="G507" s="34"/>
+      <c r="G507" s="7" t="s">
+        <v>25</v>
+      </c>
       <c r="H507" s="21"/>
       <c r="I507" s="19"/>
       <c r="J507" s="10"/>
@@ -37223,11 +37324,13 @@
       <c r="P507" s="21"/>
       <c r="Q507" s="19"/>
       <c r="R507" s="19"/>
-      <c r="S507" s="20"/>
+      <c r="S507" s="61" t="s">
+        <v>1844</v>
+      </c>
       <c r="T507" s="20"/>
       <c r="U507" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#506</v>
       </c>
     </row>
     <row r="508">
@@ -38766,15 +38869,18 @@
     <hyperlink r:id="rId64" ref="S502"/>
     <hyperlink r:id="rId65" ref="S503"/>
     <hyperlink r:id="rId66" ref="S504"/>
+    <hyperlink r:id="rId67" ref="S505"/>
+    <hyperlink r:id="rId68" ref="S506"/>
+    <hyperlink r:id="rId69" ref="S507"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId67"/>
-  <legacyDrawing r:id="rId68"/>
+  <drawing r:id="rId70"/>
+  <legacyDrawing r:id="rId71"/>
   <tableParts count="2">
-    <tablePart r:id="rId71"/>
-    <tablePart r:id="rId72"/>
+    <tablePart r:id="rId74"/>
+    <tablePart r:id="rId75"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20200920
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -563,7 +563,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5563" uniqueCount="1850">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5583" uniqueCount="1857">
   <si>
     <t>案例</t>
   </si>
@@ -6833,6 +6833,9 @@
     <t>喉嚨有痰</t>
   </si>
   <si>
+    <t>因工作來台</t>
+  </si>
+  <si>
     <t>國內新確診3例COVID-19個案，均為境外移入</t>
   </si>
   <si>
@@ -6845,10 +6848,33 @@
     <t>喉嚨癢 咳嗽 喉嚨痛 鼻塞</t>
   </si>
   <si>
-    <t>入境時無不適症狀，並主動告知在緬甸當地曾與確診個案一起用餐</t>
+    <t>入境時無不適症狀，並主動告知在緬甸當地曾與案501以及當地確診個案一起用餐</t>
   </si>
   <si>
     <t>#506</t>
+  </si>
+  <si>
+    <t>-9/11 日本</t>
+  </si>
+  <si>
+    <t>9/11 採檢
+9/18 二採
+9/19 確診</t>
+  </si>
+  <si>
+    <t>長期旅居日本，今年8月28日至30日出現喉嚨痛症狀
+9月11日返台奔喪，入境時因有咳嗽症狀，於機場進行採檢，檢驗結果為陰性
+9月18日個案已無症狀，因申請外出奔喪，由衛生單位安排自費採檢</t>
+  </si>
+  <si>
+    <t>#507</t>
+  </si>
+  <si>
+    <t>-9/18 台灣</t>
+  </si>
+  <si>
+    <t>9/18 採檢
+9/20 確診</t>
   </si>
 </sst>
 </file>
@@ -6985,7 +7011,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="71">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -7176,24 +7202,21 @@
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="17" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="18" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -36962,7 +36985,7 @@
       </c>
     </row>
     <row r="501">
-      <c r="A501" s="63" t="s">
+      <c r="A501" s="16" t="s">
         <v>1821</v>
       </c>
       <c r="B501" s="6">
@@ -36971,7 +36994,7 @@
       <c r="C501" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D501" s="64" t="s">
+      <c r="D501" s="7" t="s">
         <v>116</v>
       </c>
       <c r="E501" s="7" t="s">
@@ -36981,26 +37004,26 @@
       <c r="G501" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H501" s="65" t="s">
+      <c r="H501" s="8" t="s">
         <v>1822</v>
       </c>
-      <c r="I501" s="66">
+      <c r="I501" s="9">
         <v>44087.0</v>
       </c>
-      <c r="J501" s="67" t="s">
+      <c r="J501" s="12" t="s">
         <v>1442</v>
       </c>
-      <c r="K501" s="68" t="s">
+      <c r="K501" s="13" t="s">
         <v>1823</v>
       </c>
-      <c r="L501" s="67" t="s">
+      <c r="L501" s="12" t="s">
         <v>363</v>
       </c>
-      <c r="M501" s="68" t="s">
+      <c r="M501" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N501" s="25"/>
-      <c r="O501" s="65" t="s">
+      <c r="O501" s="8" t="s">
         <v>85</v>
       </c>
       <c r="P501" s="21"/>
@@ -37016,7 +37039,7 @@
       </c>
     </row>
     <row r="502">
-      <c r="A502" s="63" t="s">
+      <c r="A502" s="16" t="s">
         <v>1825</v>
       </c>
       <c r="B502" s="6">
@@ -37025,7 +37048,7 @@
       <c r="C502" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D502" s="64" t="s">
+      <c r="D502" s="7" t="s">
         <v>59</v>
       </c>
       <c r="E502" s="7" t="s">
@@ -37035,29 +37058,29 @@
       <c r="G502" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H502" s="65" t="s">
+      <c r="H502" s="8" t="s">
         <v>1826</v>
       </c>
-      <c r="I502" s="66">
+      <c r="I502" s="9">
         <v>44087.0</v>
       </c>
-      <c r="J502" s="67" t="s">
+      <c r="J502" s="12" t="s">
         <v>1442</v>
       </c>
-      <c r="K502" s="68" t="s">
+      <c r="K502" s="13" t="s">
         <v>1827</v>
       </c>
-      <c r="L502" s="67" t="s">
+      <c r="L502" s="12" t="s">
         <v>363</v>
       </c>
-      <c r="M502" s="68" t="s">
+      <c r="M502" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N502" s="25"/>
-      <c r="O502" s="65" t="s">
+      <c r="O502" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P502" s="65" t="s">
+      <c r="P502" s="8" t="s">
         <v>1828</v>
       </c>
       <c r="Q502" s="19"/>
@@ -37072,7 +37095,7 @@
       </c>
     </row>
     <row r="503">
-      <c r="A503" s="63" t="s">
+      <c r="A503" s="16" t="s">
         <v>1830</v>
       </c>
       <c r="B503" s="6">
@@ -37081,7 +37104,7 @@
       <c r="C503" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D503" s="64" t="s">
+      <c r="D503" s="7" t="s">
         <v>76</v>
       </c>
       <c r="E503" s="7" t="s">
@@ -37091,29 +37114,29 @@
       <c r="G503" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H503" s="65" t="s">
+      <c r="H503" s="8" t="s">
         <v>1831</v>
       </c>
-      <c r="I503" s="66">
+      <c r="I503" s="9">
         <v>44080.0</v>
       </c>
-      <c r="J503" s="69">
+      <c r="J503" s="10">
         <v>44084.0</v>
       </c>
       <c r="K503" s="13" t="s">
         <v>1832</v>
       </c>
-      <c r="L503" s="67" t="s">
+      <c r="L503" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M503" s="68" t="s">
+      <c r="M503" s="13" t="s">
         <v>1833</v>
       </c>
       <c r="N503" s="25"/>
-      <c r="O503" s="65" t="s">
+      <c r="O503" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P503" s="65" t="s">
+      <c r="P503" s="8" t="s">
         <v>1834</v>
       </c>
       <c r="Q503" s="19"/>
@@ -37128,7 +37151,7 @@
       </c>
     </row>
     <row r="504">
-      <c r="A504" s="63" t="s">
+      <c r="A504" s="16" t="s">
         <v>1835</v>
       </c>
       <c r="B504" s="6">
@@ -37137,7 +37160,7 @@
       <c r="C504" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D504" s="64" t="s">
+      <c r="D504" s="7" t="s">
         <v>116</v>
       </c>
       <c r="E504" s="7" t="s">
@@ -37147,29 +37170,29 @@
       <c r="G504" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H504" s="65" t="s">
+      <c r="H504" s="8" t="s">
         <v>1836</v>
       </c>
-      <c r="I504" s="66">
+      <c r="I504" s="9">
         <v>44087.0</v>
       </c>
       <c r="J504" s="10">
         <v>44084.0</v>
       </c>
-      <c r="K504" s="68" t="s">
+      <c r="K504" s="13" t="s">
         <v>1837</v>
       </c>
-      <c r="L504" s="67" t="s">
+      <c r="L504" s="12" t="s">
         <v>363</v>
       </c>
-      <c r="M504" s="68" t="s">
+      <c r="M504" s="13" t="s">
         <v>1838</v>
       </c>
       <c r="N504" s="25"/>
-      <c r="O504" s="65" t="s">
+      <c r="O504" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P504" s="65" t="s">
+      <c r="P504" s="8" t="s">
         <v>1839</v>
       </c>
       <c r="Q504" s="19"/>
@@ -37184,7 +37207,7 @@
       </c>
     </row>
     <row r="505">
-      <c r="A505" s="63" t="s">
+      <c r="A505" s="16" t="s">
         <v>1840</v>
       </c>
       <c r="B505" s="6">
@@ -37193,7 +37216,7 @@
       <c r="C505" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D505" s="64" t="s">
+      <c r="D505" s="7" t="s">
         <v>76</v>
       </c>
       <c r="E505" s="7" t="s">
@@ -37203,33 +37226,35 @@
       <c r="G505" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H505" s="65" t="s">
+      <c r="H505" s="8" t="s">
         <v>1841</v>
       </c>
-      <c r="I505" s="66">
+      <c r="I505" s="9">
         <v>44091.0</v>
       </c>
-      <c r="J505" s="69">
+      <c r="J505" s="10">
         <v>44092.0</v>
       </c>
-      <c r="K505" s="68" t="s">
+      <c r="K505" s="13" t="s">
         <v>1842</v>
       </c>
-      <c r="L505" s="67" t="s">
+      <c r="L505" s="12" t="s">
         <v>363</v>
       </c>
-      <c r="M505" s="68" t="s">
+      <c r="M505" s="13" t="s">
         <v>1843</v>
       </c>
       <c r="N505" s="25"/>
-      <c r="O505" s="65" t="s">
+      <c r="O505" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P505" s="21"/>
+      <c r="P505" s="63" t="s">
+        <v>1844</v>
+      </c>
       <c r="Q505" s="19"/>
       <c r="R505" s="19"/>
       <c r="S505" s="61" t="s">
-        <v>1844</v>
+        <v>1845</v>
       </c>
       <c r="T505" s="20"/>
       <c r="U505" s="18" t="str">
@@ -37238,8 +37263,8 @@
       </c>
     </row>
     <row r="506">
-      <c r="A506" s="63" t="s">
-        <v>1845</v>
+      <c r="A506" s="16" t="s">
+        <v>1846</v>
       </c>
       <c r="B506" s="6">
         <v>44093.0</v>
@@ -37247,7 +37272,7 @@
       <c r="C506" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D506" s="64" t="s">
+      <c r="D506" s="7" t="s">
         <v>116</v>
       </c>
       <c r="E506" s="7" t="s">
@@ -37257,35 +37282,35 @@
       <c r="G506" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H506" s="65" t="s">
-        <v>1846</v>
-      </c>
-      <c r="I506" s="66">
+      <c r="H506" s="8" t="s">
+        <v>1847</v>
+      </c>
+      <c r="I506" s="9">
         <v>44091.0</v>
       </c>
-      <c r="J506" s="69">
+      <c r="J506" s="10">
         <v>44091.0</v>
       </c>
-      <c r="K506" s="68" t="s">
+      <c r="K506" s="13" t="s">
         <v>1842</v>
       </c>
-      <c r="L506" s="67" t="s">
+      <c r="L506" s="12" t="s">
         <v>363</v>
       </c>
-      <c r="M506" s="68" t="s">
-        <v>1847</v>
+      <c r="M506" s="13" t="s">
+        <v>1848</v>
       </c>
       <c r="N506" s="25"/>
-      <c r="O506" s="65" t="s">
+      <c r="O506" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P506" s="65" t="s">
-        <v>1848</v>
+      <c r="P506" s="63" t="s">
+        <v>1849</v>
       </c>
       <c r="Q506" s="19"/>
       <c r="R506" s="19"/>
       <c r="S506" s="61" t="s">
-        <v>1844</v>
+        <v>1845</v>
       </c>
       <c r="T506" s="20"/>
       <c r="U506" s="18" t="str">
@@ -37294,8 +37319,8 @@
       </c>
     </row>
     <row r="507">
-      <c r="A507" s="63" t="s">
-        <v>1849</v>
+      <c r="A507" s="16" t="s">
+        <v>1850</v>
       </c>
       <c r="B507" s="6">
         <v>44093.0</v>
@@ -37303,7 +37328,7 @@
       <c r="C507" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D507" s="64" t="s">
+      <c r="D507" s="7" t="s">
         <v>22</v>
       </c>
       <c r="E507" s="7" t="s">
@@ -37313,19 +37338,35 @@
       <c r="G507" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H507" s="21"/>
-      <c r="I507" s="19"/>
-      <c r="J507" s="10"/>
-      <c r="K507" s="22"/>
-      <c r="L507" s="23"/>
-      <c r="M507" s="22"/>
+      <c r="H507" s="63" t="s">
+        <v>1851</v>
+      </c>
+      <c r="I507" s="64">
+        <v>44085.0</v>
+      </c>
+      <c r="J507" s="10">
+        <v>44071.0</v>
+      </c>
+      <c r="K507" s="65" t="s">
+        <v>1852</v>
+      </c>
+      <c r="L507" s="12" t="s">
+        <v>1674</v>
+      </c>
+      <c r="M507" s="65" t="s">
+        <v>518</v>
+      </c>
       <c r="N507" s="25"/>
-      <c r="O507" s="21"/>
-      <c r="P507" s="21"/>
+      <c r="O507" s="63" t="s">
+        <v>85</v>
+      </c>
+      <c r="P507" s="63" t="s">
+        <v>1853</v>
+      </c>
       <c r="Q507" s="19"/>
       <c r="R507" s="19"/>
       <c r="S507" s="61" t="s">
-        <v>1844</v>
+        <v>1845</v>
       </c>
       <c r="T507" s="20"/>
       <c r="U507" s="18" t="str">
@@ -37334,34 +37375,64 @@
       </c>
     </row>
     <row r="508">
-      <c r="A508" s="70"/>
-      <c r="B508" s="71"/>
-      <c r="C508" s="34"/>
-      <c r="D508" s="34"/>
-      <c r="E508" s="34"/>
+      <c r="A508" s="66" t="s">
+        <v>1854</v>
+      </c>
+      <c r="B508" s="6">
+        <v>44094.0</v>
+      </c>
+      <c r="C508" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D508" s="67" t="s">
+        <v>116</v>
+      </c>
+      <c r="E508" s="7" t="s">
+        <v>205</v>
+      </c>
       <c r="F508" s="34"/>
-      <c r="G508" s="34"/>
-      <c r="H508" s="21"/>
-      <c r="I508" s="19"/>
-      <c r="J508" s="10"/>
-      <c r="K508" s="22"/>
-      <c r="L508" s="23"/>
-      <c r="M508" s="22"/>
+      <c r="G508" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H508" s="63" t="s">
+        <v>1855</v>
+      </c>
+      <c r="I508" s="64">
+        <v>44092.0</v>
+      </c>
+      <c r="J508" s="68" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K508" s="65" t="s">
+        <v>1856</v>
+      </c>
+      <c r="L508" s="68" t="s">
+        <v>363</v>
+      </c>
+      <c r="M508" s="65" t="s">
+        <v>1442</v>
+      </c>
       <c r="N508" s="25"/>
-      <c r="O508" s="21"/>
-      <c r="P508" s="21"/>
+      <c r="O508" s="63" t="s">
+        <v>85</v>
+      </c>
+      <c r="P508" s="63" t="s">
+        <v>1819</v>
+      </c>
       <c r="Q508" s="19"/>
       <c r="R508" s="19"/>
-      <c r="S508" s="20"/>
+      <c r="S508" s="61" t="s">
+        <v>1820</v>
+      </c>
       <c r="T508" s="20"/>
       <c r="U508" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#507</v>
       </c>
     </row>
     <row r="509">
-      <c r="A509" s="70"/>
-      <c r="B509" s="71"/>
+      <c r="A509" s="69"/>
+      <c r="B509" s="70"/>
       <c r="C509" s="34"/>
       <c r="D509" s="34"/>
       <c r="E509" s="34"/>
@@ -37386,8 +37457,8 @@
       </c>
     </row>
     <row r="510">
-      <c r="A510" s="70"/>
-      <c r="B510" s="71"/>
+      <c r="A510" s="69"/>
+      <c r="B510" s="70"/>
       <c r="C510" s="34"/>
       <c r="D510" s="34"/>
       <c r="E510" s="34"/>
@@ -37412,8 +37483,8 @@
       </c>
     </row>
     <row r="511">
-      <c r="A511" s="70"/>
-      <c r="B511" s="71"/>
+      <c r="A511" s="69"/>
+      <c r="B511" s="70"/>
       <c r="C511" s="34"/>
       <c r="D511" s="34"/>
       <c r="E511" s="34"/>
@@ -37438,8 +37509,8 @@
       </c>
     </row>
     <row r="512">
-      <c r="A512" s="70"/>
-      <c r="B512" s="71"/>
+      <c r="A512" s="69"/>
+      <c r="B512" s="70"/>
       <c r="C512" s="34"/>
       <c r="D512" s="34"/>
       <c r="E512" s="34"/>
@@ -37464,8 +37535,8 @@
       </c>
     </row>
     <row r="513">
-      <c r="A513" s="70"/>
-      <c r="B513" s="71"/>
+      <c r="A513" s="69"/>
+      <c r="B513" s="70"/>
       <c r="C513" s="34"/>
       <c r="D513" s="34"/>
       <c r="E513" s="34"/>
@@ -37490,8 +37561,8 @@
       </c>
     </row>
     <row r="514">
-      <c r="A514" s="70"/>
-      <c r="B514" s="71"/>
+      <c r="A514" s="69"/>
+      <c r="B514" s="70"/>
       <c r="C514" s="34"/>
       <c r="D514" s="34"/>
       <c r="E514" s="34"/>
@@ -37516,8 +37587,8 @@
       </c>
     </row>
     <row r="515">
-      <c r="A515" s="70"/>
-      <c r="B515" s="71"/>
+      <c r="A515" s="69"/>
+      <c r="B515" s="70"/>
       <c r="C515" s="34"/>
       <c r="D515" s="34"/>
       <c r="E515" s="34"/>
@@ -37542,8 +37613,8 @@
       </c>
     </row>
     <row r="516">
-      <c r="A516" s="70"/>
-      <c r="B516" s="71"/>
+      <c r="A516" s="69"/>
+      <c r="B516" s="70"/>
       <c r="C516" s="34"/>
       <c r="D516" s="34"/>
       <c r="E516" s="34"/>
@@ -37568,8 +37639,8 @@
       </c>
     </row>
     <row r="517">
-      <c r="A517" s="70"/>
-      <c r="B517" s="71"/>
+      <c r="A517" s="69"/>
+      <c r="B517" s="70"/>
       <c r="C517" s="34"/>
       <c r="D517" s="34"/>
       <c r="E517" s="34"/>
@@ -37594,8 +37665,8 @@
       </c>
     </row>
     <row r="518">
-      <c r="A518" s="70"/>
-      <c r="B518" s="71"/>
+      <c r="A518" s="69"/>
+      <c r="B518" s="70"/>
       <c r="C518" s="34"/>
       <c r="D518" s="34"/>
       <c r="E518" s="34"/>
@@ -37620,8 +37691,8 @@
       </c>
     </row>
     <row r="519">
-      <c r="A519" s="70"/>
-      <c r="B519" s="71"/>
+      <c r="A519" s="69"/>
+      <c r="B519" s="70"/>
       <c r="C519" s="34"/>
       <c r="D519" s="34"/>
       <c r="E519" s="34"/>
@@ -37646,8 +37717,8 @@
       </c>
     </row>
     <row r="520">
-      <c r="A520" s="70"/>
-      <c r="B520" s="71"/>
+      <c r="A520" s="69"/>
+      <c r="B520" s="70"/>
       <c r="C520" s="34"/>
       <c r="D520" s="34"/>
       <c r="E520" s="34"/>
@@ -37672,8 +37743,8 @@
       </c>
     </row>
     <row r="521">
-      <c r="A521" s="70"/>
-      <c r="B521" s="71"/>
+      <c r="A521" s="69"/>
+      <c r="B521" s="70"/>
       <c r="C521" s="34"/>
       <c r="D521" s="34"/>
       <c r="E521" s="34"/>
@@ -37698,8 +37769,8 @@
       </c>
     </row>
     <row r="522">
-      <c r="A522" s="70"/>
-      <c r="B522" s="71"/>
+      <c r="A522" s="69"/>
+      <c r="B522" s="70"/>
       <c r="C522" s="34"/>
       <c r="D522" s="34"/>
       <c r="E522" s="34"/>
@@ -37724,8 +37795,8 @@
       </c>
     </row>
     <row r="523">
-      <c r="A523" s="70"/>
-      <c r="B523" s="71"/>
+      <c r="A523" s="69"/>
+      <c r="B523" s="70"/>
       <c r="C523" s="34"/>
       <c r="D523" s="34"/>
       <c r="E523" s="34"/>
@@ -37750,8 +37821,8 @@
       </c>
     </row>
     <row r="524">
-      <c r="A524" s="70"/>
-      <c r="B524" s="71"/>
+      <c r="A524" s="69"/>
+      <c r="B524" s="70"/>
       <c r="C524" s="34"/>
       <c r="D524" s="34"/>
       <c r="E524" s="34"/>
@@ -37776,8 +37847,8 @@
       </c>
     </row>
     <row r="525">
-      <c r="A525" s="70"/>
-      <c r="B525" s="71"/>
+      <c r="A525" s="69"/>
+      <c r="B525" s="70"/>
       <c r="C525" s="34"/>
       <c r="D525" s="34"/>
       <c r="E525" s="34"/>
@@ -37802,8 +37873,8 @@
       </c>
     </row>
     <row r="526">
-      <c r="A526" s="70"/>
-      <c r="B526" s="71"/>
+      <c r="A526" s="69"/>
+      <c r="B526" s="70"/>
       <c r="C526" s="34"/>
       <c r="D526" s="34"/>
       <c r="E526" s="34"/>
@@ -37828,8 +37899,8 @@
       </c>
     </row>
     <row r="527">
-      <c r="A527" s="70"/>
-      <c r="B527" s="71"/>
+      <c r="A527" s="69"/>
+      <c r="B527" s="70"/>
       <c r="C527" s="34"/>
       <c r="D527" s="34"/>
       <c r="E527" s="34"/>
@@ -37854,8 +37925,8 @@
       </c>
     </row>
     <row r="528">
-      <c r="A528" s="70"/>
-      <c r="B528" s="71"/>
+      <c r="A528" s="69"/>
+      <c r="B528" s="70"/>
       <c r="C528" s="34"/>
       <c r="D528" s="34"/>
       <c r="E528" s="34"/>
@@ -37880,8 +37951,8 @@
       </c>
     </row>
     <row r="529">
-      <c r="A529" s="70"/>
-      <c r="B529" s="71"/>
+      <c r="A529" s="69"/>
+      <c r="B529" s="70"/>
       <c r="C529" s="34"/>
       <c r="D529" s="34"/>
       <c r="E529" s="34"/>
@@ -37906,8 +37977,8 @@
       </c>
     </row>
     <row r="530">
-      <c r="A530" s="70"/>
-      <c r="B530" s="71"/>
+      <c r="A530" s="69"/>
+      <c r="B530" s="70"/>
       <c r="C530" s="34"/>
       <c r="D530" s="34"/>
       <c r="E530" s="34"/>
@@ -37932,8 +38003,8 @@
       </c>
     </row>
     <row r="531">
-      <c r="A531" s="70"/>
-      <c r="B531" s="71"/>
+      <c r="A531" s="69"/>
+      <c r="B531" s="70"/>
       <c r="C531" s="34"/>
       <c r="D531" s="34"/>
       <c r="E531" s="34"/>
@@ -37958,8 +38029,8 @@
       </c>
     </row>
     <row r="532">
-      <c r="A532" s="70"/>
-      <c r="B532" s="71"/>
+      <c r="A532" s="69"/>
+      <c r="B532" s="70"/>
       <c r="C532" s="34"/>
       <c r="D532" s="34"/>
       <c r="E532" s="34"/>
@@ -37984,8 +38055,8 @@
       </c>
     </row>
     <row r="533">
-      <c r="A533" s="70"/>
-      <c r="B533" s="71"/>
+      <c r="A533" s="69"/>
+      <c r="B533" s="70"/>
       <c r="C533" s="34"/>
       <c r="D533" s="34"/>
       <c r="E533" s="34"/>
@@ -38010,8 +38081,8 @@
       </c>
     </row>
     <row r="534">
-      <c r="A534" s="70"/>
-      <c r="B534" s="71"/>
+      <c r="A534" s="69"/>
+      <c r="B534" s="70"/>
       <c r="C534" s="34"/>
       <c r="D534" s="34"/>
       <c r="E534" s="34"/>
@@ -38036,8 +38107,8 @@
       </c>
     </row>
     <row r="535">
-      <c r="A535" s="70"/>
-      <c r="B535" s="71"/>
+      <c r="A535" s="69"/>
+      <c r="B535" s="70"/>
       <c r="C535" s="34"/>
       <c r="D535" s="34"/>
       <c r="E535" s="34"/>
@@ -38062,8 +38133,8 @@
       </c>
     </row>
     <row r="536">
-      <c r="A536" s="70"/>
-      <c r="B536" s="71"/>
+      <c r="A536" s="69"/>
+      <c r="B536" s="70"/>
       <c r="C536" s="34"/>
       <c r="D536" s="34"/>
       <c r="E536" s="34"/>
@@ -38088,8 +38159,8 @@
       </c>
     </row>
     <row r="537">
-      <c r="A537" s="70"/>
-      <c r="B537" s="71"/>
+      <c r="A537" s="69"/>
+      <c r="B537" s="70"/>
       <c r="C537" s="34"/>
       <c r="D537" s="34"/>
       <c r="E537" s="34"/>
@@ -38114,8 +38185,8 @@
       </c>
     </row>
     <row r="538">
-      <c r="A538" s="70"/>
-      <c r="B538" s="71"/>
+      <c r="A538" s="69"/>
+      <c r="B538" s="70"/>
       <c r="C538" s="34"/>
       <c r="D538" s="34"/>
       <c r="E538" s="34"/>
@@ -38140,8 +38211,8 @@
       </c>
     </row>
     <row r="539">
-      <c r="A539" s="70"/>
-      <c r="B539" s="71"/>
+      <c r="A539" s="69"/>
+      <c r="B539" s="70"/>
       <c r="C539" s="34"/>
       <c r="D539" s="34"/>
       <c r="E539" s="34"/>
@@ -38166,8 +38237,8 @@
       </c>
     </row>
     <row r="540">
-      <c r="A540" s="70"/>
-      <c r="B540" s="71"/>
+      <c r="A540" s="69"/>
+      <c r="B540" s="70"/>
       <c r="C540" s="34"/>
       <c r="D540" s="34"/>
       <c r="E540" s="34"/>
@@ -38192,8 +38263,8 @@
       </c>
     </row>
     <row r="541">
-      <c r="A541" s="70"/>
-      <c r="B541" s="71"/>
+      <c r="A541" s="69"/>
+      <c r="B541" s="70"/>
       <c r="C541" s="34"/>
       <c r="D541" s="34"/>
       <c r="E541" s="34"/>
@@ -38218,8 +38289,8 @@
       </c>
     </row>
     <row r="542">
-      <c r="A542" s="70"/>
-      <c r="B542" s="71"/>
+      <c r="A542" s="69"/>
+      <c r="B542" s="70"/>
       <c r="C542" s="34"/>
       <c r="D542" s="34"/>
       <c r="E542" s="34"/>
@@ -38244,8 +38315,8 @@
       </c>
     </row>
     <row r="543">
-      <c r="A543" s="70"/>
-      <c r="B543" s="71"/>
+      <c r="A543" s="69"/>
+      <c r="B543" s="70"/>
       <c r="C543" s="34"/>
       <c r="D543" s="34"/>
       <c r="E543" s="34"/>
@@ -38270,8 +38341,8 @@
       </c>
     </row>
     <row r="544">
-      <c r="A544" s="70"/>
-      <c r="B544" s="71"/>
+      <c r="A544" s="69"/>
+      <c r="B544" s="70"/>
       <c r="C544" s="34"/>
       <c r="D544" s="34"/>
       <c r="E544" s="34"/>
@@ -38296,8 +38367,8 @@
       </c>
     </row>
     <row r="545">
-      <c r="A545" s="70"/>
-      <c r="B545" s="71"/>
+      <c r="A545" s="69"/>
+      <c r="B545" s="70"/>
       <c r="C545" s="34"/>
       <c r="D545" s="34"/>
       <c r="E545" s="34"/>
@@ -38322,8 +38393,8 @@
       </c>
     </row>
     <row r="546">
-      <c r="A546" s="70"/>
-      <c r="B546" s="71"/>
+      <c r="A546" s="69"/>
+      <c r="B546" s="70"/>
       <c r="C546" s="34"/>
       <c r="D546" s="34"/>
       <c r="E546" s="34"/>
@@ -38348,8 +38419,8 @@
       </c>
     </row>
     <row r="547">
-      <c r="A547" s="70"/>
-      <c r="B547" s="71"/>
+      <c r="A547" s="69"/>
+      <c r="B547" s="70"/>
       <c r="C547" s="34"/>
       <c r="D547" s="34"/>
       <c r="E547" s="34"/>
@@ -38374,8 +38445,8 @@
       </c>
     </row>
     <row r="548">
-      <c r="A548" s="70"/>
-      <c r="B548" s="71"/>
+      <c r="A548" s="69"/>
+      <c r="B548" s="70"/>
       <c r="C548" s="34"/>
       <c r="D548" s="34"/>
       <c r="E548" s="34"/>
@@ -38400,8 +38471,8 @@
       </c>
     </row>
     <row r="549">
-      <c r="A549" s="70"/>
-      <c r="B549" s="71"/>
+      <c r="A549" s="69"/>
+      <c r="B549" s="70"/>
       <c r="C549" s="34"/>
       <c r="D549" s="34"/>
       <c r="E549" s="34"/>
@@ -38426,8 +38497,8 @@
       </c>
     </row>
     <row r="550">
-      <c r="A550" s="70"/>
-      <c r="B550" s="71"/>
+      <c r="A550" s="69"/>
+      <c r="B550" s="70"/>
       <c r="C550" s="34"/>
       <c r="D550" s="34"/>
       <c r="E550" s="34"/>
@@ -38452,8 +38523,8 @@
       </c>
     </row>
     <row r="551">
-      <c r="A551" s="70"/>
-      <c r="B551" s="71"/>
+      <c r="A551" s="69"/>
+      <c r="B551" s="70"/>
       <c r="C551" s="34"/>
       <c r="D551" s="34"/>
       <c r="E551" s="34"/>
@@ -38872,15 +38943,16 @@
     <hyperlink r:id="rId67" ref="S505"/>
     <hyperlink r:id="rId68" ref="S506"/>
     <hyperlink r:id="rId69" ref="S507"/>
+    <hyperlink r:id="rId70" ref="S508"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId70"/>
-  <legacyDrawing r:id="rId71"/>
+  <drawing r:id="rId71"/>
+  <legacyDrawing r:id="rId72"/>
   <tableParts count="2">
-    <tablePart r:id="rId74"/>
     <tablePart r:id="rId75"/>
+    <tablePart r:id="rId76"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20200921
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -563,7 +563,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5583" uniqueCount="1857">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5584" uniqueCount="1857">
   <si>
     <t>案例</t>
   </si>
@@ -6885,7 +6885,7 @@
     <numFmt numFmtId="164" formatCode="mm&quot;月&quot;dd&quot;日 &quot;dddd"/>
     <numFmt numFmtId="165" formatCode="m/d"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="18">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -6962,7 +6962,6 @@
       <u/>
       <color rgb="FF1155CC"/>
     </font>
-    <font/>
     <font>
       <color rgb="FF000000"/>
     </font>
@@ -7011,7 +7010,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="66">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -7198,26 +7197,11 @@
     <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
@@ -35115,7 +35099,9 @@
       <c r="L467" s="12" t="s">
         <v>363</v>
       </c>
-      <c r="M467" s="22"/>
+      <c r="M467" s="62" t="s">
+        <v>1442</v>
+      </c>
       <c r="N467" s="14" t="s">
         <v>1658</v>
       </c>
@@ -35205,7 +35191,7 @@
       <c r="D469" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E469" s="62" t="s">
+      <c r="E469" s="63" t="s">
         <v>1663</v>
       </c>
       <c r="F469" s="34"/>
@@ -37248,7 +37234,7 @@
       <c r="O505" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P505" s="63" t="s">
+      <c r="P505" s="8" t="s">
         <v>1844</v>
       </c>
       <c r="Q505" s="19"/>
@@ -37304,7 +37290,7 @@
       <c r="O506" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P506" s="63" t="s">
+      <c r="P506" s="8" t="s">
         <v>1849</v>
       </c>
       <c r="Q506" s="19"/>
@@ -37338,29 +37324,29 @@
       <c r="G507" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H507" s="63" t="s">
+      <c r="H507" s="8" t="s">
         <v>1851</v>
       </c>
-      <c r="I507" s="64">
+      <c r="I507" s="9">
         <v>44085.0</v>
       </c>
       <c r="J507" s="10">
         <v>44071.0</v>
       </c>
-      <c r="K507" s="65" t="s">
+      <c r="K507" s="13" t="s">
         <v>1852</v>
       </c>
       <c r="L507" s="12" t="s">
         <v>1674</v>
       </c>
-      <c r="M507" s="65" t="s">
+      <c r="M507" s="13" t="s">
         <v>518</v>
       </c>
       <c r="N507" s="25"/>
-      <c r="O507" s="63" t="s">
+      <c r="O507" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P507" s="63" t="s">
+      <c r="P507" s="8" t="s">
         <v>1853</v>
       </c>
       <c r="Q507" s="19"/>
@@ -37375,7 +37361,7 @@
       </c>
     </row>
     <row r="508">
-      <c r="A508" s="66" t="s">
+      <c r="A508" s="16" t="s">
         <v>1854</v>
       </c>
       <c r="B508" s="6">
@@ -37384,7 +37370,7 @@
       <c r="C508" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D508" s="67" t="s">
+      <c r="D508" s="7" t="s">
         <v>116</v>
       </c>
       <c r="E508" s="7" t="s">
@@ -37394,29 +37380,29 @@
       <c r="G508" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H508" s="63" t="s">
+      <c r="H508" s="8" t="s">
         <v>1855</v>
       </c>
-      <c r="I508" s="64">
+      <c r="I508" s="9">
         <v>44092.0</v>
       </c>
-      <c r="J508" s="68" t="s">
+      <c r="J508" s="12" t="s">
         <v>1442</v>
       </c>
-      <c r="K508" s="65" t="s">
+      <c r="K508" s="13" t="s">
         <v>1856</v>
       </c>
-      <c r="L508" s="68" t="s">
+      <c r="L508" s="12" t="s">
         <v>363</v>
       </c>
-      <c r="M508" s="65" t="s">
+      <c r="M508" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N508" s="25"/>
-      <c r="O508" s="63" t="s">
+      <c r="O508" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P508" s="63" t="s">
+      <c r="P508" s="8" t="s">
         <v>1819</v>
       </c>
       <c r="Q508" s="19"/>
@@ -37431,8 +37417,8 @@
       </c>
     </row>
     <row r="509">
-      <c r="A509" s="69"/>
-      <c r="B509" s="70"/>
+      <c r="A509" s="64"/>
+      <c r="B509" s="65"/>
       <c r="C509" s="34"/>
       <c r="D509" s="34"/>
       <c r="E509" s="34"/>
@@ -37457,8 +37443,8 @@
       </c>
     </row>
     <row r="510">
-      <c r="A510" s="69"/>
-      <c r="B510" s="70"/>
+      <c r="A510" s="64"/>
+      <c r="B510" s="65"/>
       <c r="C510" s="34"/>
       <c r="D510" s="34"/>
       <c r="E510" s="34"/>
@@ -37483,8 +37469,8 @@
       </c>
     </row>
     <row r="511">
-      <c r="A511" s="69"/>
-      <c r="B511" s="70"/>
+      <c r="A511" s="64"/>
+      <c r="B511" s="65"/>
       <c r="C511" s="34"/>
       <c r="D511" s="34"/>
       <c r="E511" s="34"/>
@@ -37509,8 +37495,8 @@
       </c>
     </row>
     <row r="512">
-      <c r="A512" s="69"/>
-      <c r="B512" s="70"/>
+      <c r="A512" s="64"/>
+      <c r="B512" s="65"/>
       <c r="C512" s="34"/>
       <c r="D512" s="34"/>
       <c r="E512" s="34"/>
@@ -37535,8 +37521,8 @@
       </c>
     </row>
     <row r="513">
-      <c r="A513" s="69"/>
-      <c r="B513" s="70"/>
+      <c r="A513" s="64"/>
+      <c r="B513" s="65"/>
       <c r="C513" s="34"/>
       <c r="D513" s="34"/>
       <c r="E513" s="34"/>
@@ -37561,8 +37547,8 @@
       </c>
     </row>
     <row r="514">
-      <c r="A514" s="69"/>
-      <c r="B514" s="70"/>
+      <c r="A514" s="64"/>
+      <c r="B514" s="65"/>
       <c r="C514" s="34"/>
       <c r="D514" s="34"/>
       <c r="E514" s="34"/>
@@ -37587,8 +37573,8 @@
       </c>
     </row>
     <row r="515">
-      <c r="A515" s="69"/>
-      <c r="B515" s="70"/>
+      <c r="A515" s="64"/>
+      <c r="B515" s="65"/>
       <c r="C515" s="34"/>
       <c r="D515" s="34"/>
       <c r="E515" s="34"/>
@@ -37613,8 +37599,8 @@
       </c>
     </row>
     <row r="516">
-      <c r="A516" s="69"/>
-      <c r="B516" s="70"/>
+      <c r="A516" s="64"/>
+      <c r="B516" s="65"/>
       <c r="C516" s="34"/>
       <c r="D516" s="34"/>
       <c r="E516" s="34"/>
@@ -37639,8 +37625,8 @@
       </c>
     </row>
     <row r="517">
-      <c r="A517" s="69"/>
-      <c r="B517" s="70"/>
+      <c r="A517" s="64"/>
+      <c r="B517" s="65"/>
       <c r="C517" s="34"/>
       <c r="D517" s="34"/>
       <c r="E517" s="34"/>
@@ -37665,8 +37651,8 @@
       </c>
     </row>
     <row r="518">
-      <c r="A518" s="69"/>
-      <c r="B518" s="70"/>
+      <c r="A518" s="64"/>
+      <c r="B518" s="65"/>
       <c r="C518" s="34"/>
       <c r="D518" s="34"/>
       <c r="E518" s="34"/>
@@ -37691,8 +37677,8 @@
       </c>
     </row>
     <row r="519">
-      <c r="A519" s="69"/>
-      <c r="B519" s="70"/>
+      <c r="A519" s="64"/>
+      <c r="B519" s="65"/>
       <c r="C519" s="34"/>
       <c r="D519" s="34"/>
       <c r="E519" s="34"/>
@@ -37717,8 +37703,8 @@
       </c>
     </row>
     <row r="520">
-      <c r="A520" s="69"/>
-      <c r="B520" s="70"/>
+      <c r="A520" s="64"/>
+      <c r="B520" s="65"/>
       <c r="C520" s="34"/>
       <c r="D520" s="34"/>
       <c r="E520" s="34"/>
@@ -37743,8 +37729,8 @@
       </c>
     </row>
     <row r="521">
-      <c r="A521" s="69"/>
-      <c r="B521" s="70"/>
+      <c r="A521" s="64"/>
+      <c r="B521" s="65"/>
       <c r="C521" s="34"/>
       <c r="D521" s="34"/>
       <c r="E521" s="34"/>
@@ -37769,8 +37755,8 @@
       </c>
     </row>
     <row r="522">
-      <c r="A522" s="69"/>
-      <c r="B522" s="70"/>
+      <c r="A522" s="64"/>
+      <c r="B522" s="65"/>
       <c r="C522" s="34"/>
       <c r="D522" s="34"/>
       <c r="E522" s="34"/>
@@ -37795,8 +37781,8 @@
       </c>
     </row>
     <row r="523">
-      <c r="A523" s="69"/>
-      <c r="B523" s="70"/>
+      <c r="A523" s="64"/>
+      <c r="B523" s="65"/>
       <c r="C523" s="34"/>
       <c r="D523" s="34"/>
       <c r="E523" s="34"/>
@@ -37821,8 +37807,8 @@
       </c>
     </row>
     <row r="524">
-      <c r="A524" s="69"/>
-      <c r="B524" s="70"/>
+      <c r="A524" s="64"/>
+      <c r="B524" s="65"/>
       <c r="C524" s="34"/>
       <c r="D524" s="34"/>
       <c r="E524" s="34"/>
@@ -37847,8 +37833,8 @@
       </c>
     </row>
     <row r="525">
-      <c r="A525" s="69"/>
-      <c r="B525" s="70"/>
+      <c r="A525" s="64"/>
+      <c r="B525" s="65"/>
       <c r="C525" s="34"/>
       <c r="D525" s="34"/>
       <c r="E525" s="34"/>
@@ -37873,8 +37859,8 @@
       </c>
     </row>
     <row r="526">
-      <c r="A526" s="69"/>
-      <c r="B526" s="70"/>
+      <c r="A526" s="64"/>
+      <c r="B526" s="65"/>
       <c r="C526" s="34"/>
       <c r="D526" s="34"/>
       <c r="E526" s="34"/>
@@ -37899,8 +37885,8 @@
       </c>
     </row>
     <row r="527">
-      <c r="A527" s="69"/>
-      <c r="B527" s="70"/>
+      <c r="A527" s="64"/>
+      <c r="B527" s="65"/>
       <c r="C527" s="34"/>
       <c r="D527" s="34"/>
       <c r="E527" s="34"/>
@@ -37925,8 +37911,8 @@
       </c>
     </row>
     <row r="528">
-      <c r="A528" s="69"/>
-      <c r="B528" s="70"/>
+      <c r="A528" s="64"/>
+      <c r="B528" s="65"/>
       <c r="C528" s="34"/>
       <c r="D528" s="34"/>
       <c r="E528" s="34"/>
@@ -37951,8 +37937,8 @@
       </c>
     </row>
     <row r="529">
-      <c r="A529" s="69"/>
-      <c r="B529" s="70"/>
+      <c r="A529" s="64"/>
+      <c r="B529" s="65"/>
       <c r="C529" s="34"/>
       <c r="D529" s="34"/>
       <c r="E529" s="34"/>
@@ -37977,8 +37963,8 @@
       </c>
     </row>
     <row r="530">
-      <c r="A530" s="69"/>
-      <c r="B530" s="70"/>
+      <c r="A530" s="64"/>
+      <c r="B530" s="65"/>
       <c r="C530" s="34"/>
       <c r="D530" s="34"/>
       <c r="E530" s="34"/>
@@ -38003,8 +37989,8 @@
       </c>
     </row>
     <row r="531">
-      <c r="A531" s="69"/>
-      <c r="B531" s="70"/>
+      <c r="A531" s="64"/>
+      <c r="B531" s="65"/>
       <c r="C531" s="34"/>
       <c r="D531" s="34"/>
       <c r="E531" s="34"/>
@@ -38029,8 +38015,8 @@
       </c>
     </row>
     <row r="532">
-      <c r="A532" s="69"/>
-      <c r="B532" s="70"/>
+      <c r="A532" s="64"/>
+      <c r="B532" s="65"/>
       <c r="C532" s="34"/>
       <c r="D532" s="34"/>
       <c r="E532" s="34"/>
@@ -38055,8 +38041,8 @@
       </c>
     </row>
     <row r="533">
-      <c r="A533" s="69"/>
-      <c r="B533" s="70"/>
+      <c r="A533" s="64"/>
+      <c r="B533" s="65"/>
       <c r="C533" s="34"/>
       <c r="D533" s="34"/>
       <c r="E533" s="34"/>
@@ -38081,8 +38067,8 @@
       </c>
     </row>
     <row r="534">
-      <c r="A534" s="69"/>
-      <c r="B534" s="70"/>
+      <c r="A534" s="64"/>
+      <c r="B534" s="65"/>
       <c r="C534" s="34"/>
       <c r="D534" s="34"/>
       <c r="E534" s="34"/>
@@ -38107,8 +38093,8 @@
       </c>
     </row>
     <row r="535">
-      <c r="A535" s="69"/>
-      <c r="B535" s="70"/>
+      <c r="A535" s="64"/>
+      <c r="B535" s="65"/>
       <c r="C535" s="34"/>
       <c r="D535" s="34"/>
       <c r="E535" s="34"/>
@@ -38133,8 +38119,8 @@
       </c>
     </row>
     <row r="536">
-      <c r="A536" s="69"/>
-      <c r="B536" s="70"/>
+      <c r="A536" s="64"/>
+      <c r="B536" s="65"/>
       <c r="C536" s="34"/>
       <c r="D536" s="34"/>
       <c r="E536" s="34"/>
@@ -38159,8 +38145,8 @@
       </c>
     </row>
     <row r="537">
-      <c r="A537" s="69"/>
-      <c r="B537" s="70"/>
+      <c r="A537" s="64"/>
+      <c r="B537" s="65"/>
       <c r="C537" s="34"/>
       <c r="D537" s="34"/>
       <c r="E537" s="34"/>
@@ -38185,8 +38171,8 @@
       </c>
     </row>
     <row r="538">
-      <c r="A538" s="69"/>
-      <c r="B538" s="70"/>
+      <c r="A538" s="64"/>
+      <c r="B538" s="65"/>
       <c r="C538" s="34"/>
       <c r="D538" s="34"/>
       <c r="E538" s="34"/>
@@ -38211,8 +38197,8 @@
       </c>
     </row>
     <row r="539">
-      <c r="A539" s="69"/>
-      <c r="B539" s="70"/>
+      <c r="A539" s="64"/>
+      <c r="B539" s="65"/>
       <c r="C539" s="34"/>
       <c r="D539" s="34"/>
       <c r="E539" s="34"/>
@@ -38237,8 +38223,8 @@
       </c>
     </row>
     <row r="540">
-      <c r="A540" s="69"/>
-      <c r="B540" s="70"/>
+      <c r="A540" s="64"/>
+      <c r="B540" s="65"/>
       <c r="C540" s="34"/>
       <c r="D540" s="34"/>
       <c r="E540" s="34"/>
@@ -38263,8 +38249,8 @@
       </c>
     </row>
     <row r="541">
-      <c r="A541" s="69"/>
-      <c r="B541" s="70"/>
+      <c r="A541" s="64"/>
+      <c r="B541" s="65"/>
       <c r="C541" s="34"/>
       <c r="D541" s="34"/>
       <c r="E541" s="34"/>
@@ -38289,8 +38275,8 @@
       </c>
     </row>
     <row r="542">
-      <c r="A542" s="69"/>
-      <c r="B542" s="70"/>
+      <c r="A542" s="64"/>
+      <c r="B542" s="65"/>
       <c r="C542" s="34"/>
       <c r="D542" s="34"/>
       <c r="E542" s="34"/>
@@ -38315,8 +38301,8 @@
       </c>
     </row>
     <row r="543">
-      <c r="A543" s="69"/>
-      <c r="B543" s="70"/>
+      <c r="A543" s="64"/>
+      <c r="B543" s="65"/>
       <c r="C543" s="34"/>
       <c r="D543" s="34"/>
       <c r="E543" s="34"/>
@@ -38341,8 +38327,8 @@
       </c>
     </row>
     <row r="544">
-      <c r="A544" s="69"/>
-      <c r="B544" s="70"/>
+      <c r="A544" s="64"/>
+      <c r="B544" s="65"/>
       <c r="C544" s="34"/>
       <c r="D544" s="34"/>
       <c r="E544" s="34"/>
@@ -38367,8 +38353,8 @@
       </c>
     </row>
     <row r="545">
-      <c r="A545" s="69"/>
-      <c r="B545" s="70"/>
+      <c r="A545" s="64"/>
+      <c r="B545" s="65"/>
       <c r="C545" s="34"/>
       <c r="D545" s="34"/>
       <c r="E545" s="34"/>
@@ -38393,8 +38379,8 @@
       </c>
     </row>
     <row r="546">
-      <c r="A546" s="69"/>
-      <c r="B546" s="70"/>
+      <c r="A546" s="64"/>
+      <c r="B546" s="65"/>
       <c r="C546" s="34"/>
       <c r="D546" s="34"/>
       <c r="E546" s="34"/>
@@ -38419,8 +38405,8 @@
       </c>
     </row>
     <row r="547">
-      <c r="A547" s="69"/>
-      <c r="B547" s="70"/>
+      <c r="A547" s="64"/>
+      <c r="B547" s="65"/>
       <c r="C547" s="34"/>
       <c r="D547" s="34"/>
       <c r="E547" s="34"/>
@@ -38445,8 +38431,8 @@
       </c>
     </row>
     <row r="548">
-      <c r="A548" s="69"/>
-      <c r="B548" s="70"/>
+      <c r="A548" s="64"/>
+      <c r="B548" s="65"/>
       <c r="C548" s="34"/>
       <c r="D548" s="34"/>
       <c r="E548" s="34"/>
@@ -38471,8 +38457,8 @@
       </c>
     </row>
     <row r="549">
-      <c r="A549" s="69"/>
-      <c r="B549" s="70"/>
+      <c r="A549" s="64"/>
+      <c r="B549" s="65"/>
       <c r="C549" s="34"/>
       <c r="D549" s="34"/>
       <c r="E549" s="34"/>
@@ -38497,8 +38483,8 @@
       </c>
     </row>
     <row r="550">
-      <c r="A550" s="69"/>
-      <c r="B550" s="70"/>
+      <c r="A550" s="64"/>
+      <c r="B550" s="65"/>
       <c r="C550" s="34"/>
       <c r="D550" s="34"/>
       <c r="E550" s="34"/>
@@ -38523,8 +38509,8 @@
       </c>
     </row>
     <row r="551">
-      <c r="A551" s="69"/>
-      <c r="B551" s="70"/>
+      <c r="A551" s="64"/>
+      <c r="B551" s="65"/>
       <c r="C551" s="34"/>
       <c r="D551" s="34"/>
       <c r="E551" s="34"/>

</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20200922
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -563,7 +563,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5584" uniqueCount="1857">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5608" uniqueCount="1867">
   <si>
     <t>案例</t>
   </si>
@@ -6876,6 +6876,38 @@
     <t>9/18 採檢
 9/20 確診</t>
   </si>
+  <si>
+    <t>#508</t>
+  </si>
+  <si>
+    <t>6月-9/19 印尼</t>
+  </si>
+  <si>
+    <t>9/19 採檢
+9/21 確診</t>
+  </si>
+  <si>
+    <t>發燒 嗅覺異常</t>
+  </si>
+  <si>
+    <t>2男分赴印尼、緬甸工作，返國後確診COVID-19</t>
+  </si>
+  <si>
+    <t>#509</t>
+  </si>
+  <si>
+    <t>4月-9/17 緬甸</t>
+  </si>
+  <si>
+    <t>9/18 採檢
+9/21 確診</t>
+  </si>
+  <si>
+    <t>咳嗽 發燒 味覺異常</t>
+  </si>
+  <si>
+    <t>入境時無症狀，入境後前往防疫旅館進行居家檢疫，因為案505同班機前一排座位旅客，改列為居家隔離對象</t>
+  </si>
 </sst>
 </file>
 
@@ -6885,7 +6917,7 @@
     <numFmt numFmtId="164" formatCode="mm&quot;月&quot;dd&quot;日 &quot;dddd"/>
     <numFmt numFmtId="165" formatCode="m/d"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -6965,6 +6997,7 @@
     <font>
       <color rgb="FF000000"/>
     </font>
+    <font/>
   </fonts>
   <fills count="7">
     <fill>
@@ -7010,7 +7043,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="72">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -7202,6 +7235,24 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="18" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
@@ -7936,7 +7987,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="B1:U551" displayName="Table_1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:A551" displayName="Table_1" id="1">
+  <tableColumns count="1">
+    <tableColumn name="案例" id="1"/>
+  </tableColumns>
+  <tableStyleInfo name="臺灣武漢肺炎病例-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="B1:U551" displayName="Table_2" id="2">
   <tableColumns count="20">
     <tableColumn name="新聞稿發布日期" id="1"/>
     <tableColumn name="性別" id="2"/>
@@ -7958,15 +8018,6 @@
     <tableColumn name="疾管署新聞稿" id="18"/>
     <tableColumn name="出院新聞稿" id="19"/>
     <tableColumn name="案例" id="20"/>
-  </tableColumns>
-  <tableStyleInfo name="臺灣武漢肺炎病例-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:A551" displayName="Table_2" id="2">
-  <tableColumns count="1">
-    <tableColumn name="案例" id="1"/>
   </tableColumns>
   <tableStyleInfo name="臺灣武漢肺炎病例-style 2" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
@@ -37417,60 +37468,120 @@
       </c>
     </row>
     <row r="509">
-      <c r="A509" s="64"/>
-      <c r="B509" s="65"/>
-      <c r="C509" s="34"/>
-      <c r="D509" s="34"/>
-      <c r="E509" s="34"/>
+      <c r="A509" s="64" t="s">
+        <v>1857</v>
+      </c>
+      <c r="B509" s="6">
+        <v>44095.0</v>
+      </c>
+      <c r="C509" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D509" s="65" t="s">
+        <v>76</v>
+      </c>
+      <c r="E509" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F509" s="34"/>
-      <c r="G509" s="34"/>
-      <c r="H509" s="21"/>
-      <c r="I509" s="19"/>
-      <c r="J509" s="10"/>
-      <c r="K509" s="22"/>
-      <c r="L509" s="23"/>
-      <c r="M509" s="22"/>
+      <c r="G509" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H509" s="66" t="s">
+        <v>1858</v>
+      </c>
+      <c r="I509" s="67">
+        <v>44093.0</v>
+      </c>
+      <c r="J509" s="10">
+        <v>44091.0</v>
+      </c>
+      <c r="K509" s="62" t="s">
+        <v>1859</v>
+      </c>
+      <c r="L509" s="68" t="s">
+        <v>363</v>
+      </c>
+      <c r="M509" s="62" t="s">
+        <v>1860</v>
+      </c>
       <c r="N509" s="25"/>
-      <c r="O509" s="21"/>
-      <c r="P509" s="21"/>
+      <c r="O509" s="66" t="s">
+        <v>85</v>
+      </c>
+      <c r="P509" s="66" t="s">
+        <v>334</v>
+      </c>
       <c r="Q509" s="19"/>
       <c r="R509" s="19"/>
-      <c r="S509" s="20"/>
+      <c r="S509" s="61" t="s">
+        <v>1861</v>
+      </c>
       <c r="T509" s="20"/>
       <c r="U509" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#508</v>
       </c>
     </row>
     <row r="510">
-      <c r="A510" s="64"/>
-      <c r="B510" s="65"/>
-      <c r="C510" s="34"/>
-      <c r="D510" s="34"/>
-      <c r="E510" s="34"/>
+      <c r="A510" s="64" t="s">
+        <v>1862</v>
+      </c>
+      <c r="B510" s="6">
+        <v>44095.0</v>
+      </c>
+      <c r="C510" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D510" s="65" t="s">
+        <v>116</v>
+      </c>
+      <c r="E510" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F510" s="34"/>
-      <c r="G510" s="34"/>
-      <c r="H510" s="21"/>
-      <c r="I510" s="19"/>
-      <c r="J510" s="10"/>
-      <c r="K510" s="22"/>
-      <c r="L510" s="23"/>
-      <c r="M510" s="22"/>
+      <c r="G510" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H510" s="66" t="s">
+        <v>1863</v>
+      </c>
+      <c r="I510" s="67">
+        <v>44091.0</v>
+      </c>
+      <c r="J510" s="69">
+        <v>44091.0</v>
+      </c>
+      <c r="K510" s="62" t="s">
+        <v>1864</v>
+      </c>
+      <c r="L510" s="68" t="s">
+        <v>447</v>
+      </c>
+      <c r="M510" s="62" t="s">
+        <v>1865</v>
+      </c>
       <c r="N510" s="25"/>
-      <c r="O510" s="21"/>
-      <c r="P510" s="21"/>
+      <c r="O510" s="66" t="s">
+        <v>85</v>
+      </c>
+      <c r="P510" s="66" t="s">
+        <v>1866</v>
+      </c>
       <c r="Q510" s="19"/>
       <c r="R510" s="19"/>
-      <c r="S510" s="20"/>
+      <c r="S510" s="61" t="s">
+        <v>1861</v>
+      </c>
       <c r="T510" s="20"/>
       <c r="U510" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#509</v>
       </c>
     </row>
     <row r="511">
-      <c r="A511" s="64"/>
-      <c r="B511" s="65"/>
+      <c r="A511" s="70"/>
+      <c r="B511" s="71"/>
       <c r="C511" s="34"/>
       <c r="D511" s="34"/>
       <c r="E511" s="34"/>
@@ -37495,8 +37606,8 @@
       </c>
     </row>
     <row r="512">
-      <c r="A512" s="64"/>
-      <c r="B512" s="65"/>
+      <c r="A512" s="70"/>
+      <c r="B512" s="71"/>
       <c r="C512" s="34"/>
       <c r="D512" s="34"/>
       <c r="E512" s="34"/>
@@ -37521,8 +37632,8 @@
       </c>
     </row>
     <row r="513">
-      <c r="A513" s="64"/>
-      <c r="B513" s="65"/>
+      <c r="A513" s="70"/>
+      <c r="B513" s="71"/>
       <c r="C513" s="34"/>
       <c r="D513" s="34"/>
       <c r="E513" s="34"/>
@@ -37547,8 +37658,8 @@
       </c>
     </row>
     <row r="514">
-      <c r="A514" s="64"/>
-      <c r="B514" s="65"/>
+      <c r="A514" s="70"/>
+      <c r="B514" s="71"/>
       <c r="C514" s="34"/>
       <c r="D514" s="34"/>
       <c r="E514" s="34"/>
@@ -37573,8 +37684,8 @@
       </c>
     </row>
     <row r="515">
-      <c r="A515" s="64"/>
-      <c r="B515" s="65"/>
+      <c r="A515" s="70"/>
+      <c r="B515" s="71"/>
       <c r="C515" s="34"/>
       <c r="D515" s="34"/>
       <c r="E515" s="34"/>
@@ -37599,8 +37710,8 @@
       </c>
     </row>
     <row r="516">
-      <c r="A516" s="64"/>
-      <c r="B516" s="65"/>
+      <c r="A516" s="70"/>
+      <c r="B516" s="71"/>
       <c r="C516" s="34"/>
       <c r="D516" s="34"/>
       <c r="E516" s="34"/>
@@ -37625,8 +37736,8 @@
       </c>
     </row>
     <row r="517">
-      <c r="A517" s="64"/>
-      <c r="B517" s="65"/>
+      <c r="A517" s="70"/>
+      <c r="B517" s="71"/>
       <c r="C517" s="34"/>
       <c r="D517" s="34"/>
       <c r="E517" s="34"/>
@@ -37651,8 +37762,8 @@
       </c>
     </row>
     <row r="518">
-      <c r="A518" s="64"/>
-      <c r="B518" s="65"/>
+      <c r="A518" s="70"/>
+      <c r="B518" s="71"/>
       <c r="C518" s="34"/>
       <c r="D518" s="34"/>
       <c r="E518" s="34"/>
@@ -37677,8 +37788,8 @@
       </c>
     </row>
     <row r="519">
-      <c r="A519" s="64"/>
-      <c r="B519" s="65"/>
+      <c r="A519" s="70"/>
+      <c r="B519" s="71"/>
       <c r="C519" s="34"/>
       <c r="D519" s="34"/>
       <c r="E519" s="34"/>
@@ -37703,8 +37814,8 @@
       </c>
     </row>
     <row r="520">
-      <c r="A520" s="64"/>
-      <c r="B520" s="65"/>
+      <c r="A520" s="70"/>
+      <c r="B520" s="71"/>
       <c r="C520" s="34"/>
       <c r="D520" s="34"/>
       <c r="E520" s="34"/>
@@ -37729,8 +37840,8 @@
       </c>
     </row>
     <row r="521">
-      <c r="A521" s="64"/>
-      <c r="B521" s="65"/>
+      <c r="A521" s="70"/>
+      <c r="B521" s="71"/>
       <c r="C521" s="34"/>
       <c r="D521" s="34"/>
       <c r="E521" s="34"/>
@@ -37755,8 +37866,8 @@
       </c>
     </row>
     <row r="522">
-      <c r="A522" s="64"/>
-      <c r="B522" s="65"/>
+      <c r="A522" s="70"/>
+      <c r="B522" s="71"/>
       <c r="C522" s="34"/>
       <c r="D522" s="34"/>
       <c r="E522" s="34"/>
@@ -37781,8 +37892,8 @@
       </c>
     </row>
     <row r="523">
-      <c r="A523" s="64"/>
-      <c r="B523" s="65"/>
+      <c r="A523" s="70"/>
+      <c r="B523" s="71"/>
       <c r="C523" s="34"/>
       <c r="D523" s="34"/>
       <c r="E523" s="34"/>
@@ -37807,8 +37918,8 @@
       </c>
     </row>
     <row r="524">
-      <c r="A524" s="64"/>
-      <c r="B524" s="65"/>
+      <c r="A524" s="70"/>
+      <c r="B524" s="71"/>
       <c r="C524" s="34"/>
       <c r="D524" s="34"/>
       <c r="E524" s="34"/>
@@ -37833,8 +37944,8 @@
       </c>
     </row>
     <row r="525">
-      <c r="A525" s="64"/>
-      <c r="B525" s="65"/>
+      <c r="A525" s="70"/>
+      <c r="B525" s="71"/>
       <c r="C525" s="34"/>
       <c r="D525" s="34"/>
       <c r="E525" s="34"/>
@@ -37859,8 +37970,8 @@
       </c>
     </row>
     <row r="526">
-      <c r="A526" s="64"/>
-      <c r="B526" s="65"/>
+      <c r="A526" s="70"/>
+      <c r="B526" s="71"/>
       <c r="C526" s="34"/>
       <c r="D526" s="34"/>
       <c r="E526" s="34"/>
@@ -37885,8 +37996,8 @@
       </c>
     </row>
     <row r="527">
-      <c r="A527" s="64"/>
-      <c r="B527" s="65"/>
+      <c r="A527" s="70"/>
+      <c r="B527" s="71"/>
       <c r="C527" s="34"/>
       <c r="D527" s="34"/>
       <c r="E527" s="34"/>
@@ -37911,8 +38022,8 @@
       </c>
     </row>
     <row r="528">
-      <c r="A528" s="64"/>
-      <c r="B528" s="65"/>
+      <c r="A528" s="70"/>
+      <c r="B528" s="71"/>
       <c r="C528" s="34"/>
       <c r="D528" s="34"/>
       <c r="E528" s="34"/>
@@ -37937,8 +38048,8 @@
       </c>
     </row>
     <row r="529">
-      <c r="A529" s="64"/>
-      <c r="B529" s="65"/>
+      <c r="A529" s="70"/>
+      <c r="B529" s="71"/>
       <c r="C529" s="34"/>
       <c r="D529" s="34"/>
       <c r="E529" s="34"/>
@@ -37963,8 +38074,8 @@
       </c>
     </row>
     <row r="530">
-      <c r="A530" s="64"/>
-      <c r="B530" s="65"/>
+      <c r="A530" s="70"/>
+      <c r="B530" s="71"/>
       <c r="C530" s="34"/>
       <c r="D530" s="34"/>
       <c r="E530" s="34"/>
@@ -37989,8 +38100,8 @@
       </c>
     </row>
     <row r="531">
-      <c r="A531" s="64"/>
-      <c r="B531" s="65"/>
+      <c r="A531" s="70"/>
+      <c r="B531" s="71"/>
       <c r="C531" s="34"/>
       <c r="D531" s="34"/>
       <c r="E531" s="34"/>
@@ -38015,8 +38126,8 @@
       </c>
     </row>
     <row r="532">
-      <c r="A532" s="64"/>
-      <c r="B532" s="65"/>
+      <c r="A532" s="70"/>
+      <c r="B532" s="71"/>
       <c r="C532" s="34"/>
       <c r="D532" s="34"/>
       <c r="E532" s="34"/>
@@ -38041,8 +38152,8 @@
       </c>
     </row>
     <row r="533">
-      <c r="A533" s="64"/>
-      <c r="B533" s="65"/>
+      <c r="A533" s="70"/>
+      <c r="B533" s="71"/>
       <c r="C533" s="34"/>
       <c r="D533" s="34"/>
       <c r="E533" s="34"/>
@@ -38067,8 +38178,8 @@
       </c>
     </row>
     <row r="534">
-      <c r="A534" s="64"/>
-      <c r="B534" s="65"/>
+      <c r="A534" s="70"/>
+      <c r="B534" s="71"/>
       <c r="C534" s="34"/>
       <c r="D534" s="34"/>
       <c r="E534" s="34"/>
@@ -38093,8 +38204,8 @@
       </c>
     </row>
     <row r="535">
-      <c r="A535" s="64"/>
-      <c r="B535" s="65"/>
+      <c r="A535" s="70"/>
+      <c r="B535" s="71"/>
       <c r="C535" s="34"/>
       <c r="D535" s="34"/>
       <c r="E535" s="34"/>
@@ -38119,8 +38230,8 @@
       </c>
     </row>
     <row r="536">
-      <c r="A536" s="64"/>
-      <c r="B536" s="65"/>
+      <c r="A536" s="70"/>
+      <c r="B536" s="71"/>
       <c r="C536" s="34"/>
       <c r="D536" s="34"/>
       <c r="E536" s="34"/>
@@ -38145,8 +38256,8 @@
       </c>
     </row>
     <row r="537">
-      <c r="A537" s="64"/>
-      <c r="B537" s="65"/>
+      <c r="A537" s="70"/>
+      <c r="B537" s="71"/>
       <c r="C537" s="34"/>
       <c r="D537" s="34"/>
       <c r="E537" s="34"/>
@@ -38171,8 +38282,8 @@
       </c>
     </row>
     <row r="538">
-      <c r="A538" s="64"/>
-      <c r="B538" s="65"/>
+      <c r="A538" s="70"/>
+      <c r="B538" s="71"/>
       <c r="C538" s="34"/>
       <c r="D538" s="34"/>
       <c r="E538" s="34"/>
@@ -38197,8 +38308,8 @@
       </c>
     </row>
     <row r="539">
-      <c r="A539" s="64"/>
-      <c r="B539" s="65"/>
+      <c r="A539" s="70"/>
+      <c r="B539" s="71"/>
       <c r="C539" s="34"/>
       <c r="D539" s="34"/>
       <c r="E539" s="34"/>
@@ -38223,8 +38334,8 @@
       </c>
     </row>
     <row r="540">
-      <c r="A540" s="64"/>
-      <c r="B540" s="65"/>
+      <c r="A540" s="70"/>
+      <c r="B540" s="71"/>
       <c r="C540" s="34"/>
       <c r="D540" s="34"/>
       <c r="E540" s="34"/>
@@ -38249,8 +38360,8 @@
       </c>
     </row>
     <row r="541">
-      <c r="A541" s="64"/>
-      <c r="B541" s="65"/>
+      <c r="A541" s="70"/>
+      <c r="B541" s="71"/>
       <c r="C541" s="34"/>
       <c r="D541" s="34"/>
       <c r="E541" s="34"/>
@@ -38275,8 +38386,8 @@
       </c>
     </row>
     <row r="542">
-      <c r="A542" s="64"/>
-      <c r="B542" s="65"/>
+      <c r="A542" s="70"/>
+      <c r="B542" s="71"/>
       <c r="C542" s="34"/>
       <c r="D542" s="34"/>
       <c r="E542" s="34"/>
@@ -38301,8 +38412,8 @@
       </c>
     </row>
     <row r="543">
-      <c r="A543" s="64"/>
-      <c r="B543" s="65"/>
+      <c r="A543" s="70"/>
+      <c r="B543" s="71"/>
       <c r="C543" s="34"/>
       <c r="D543" s="34"/>
       <c r="E543" s="34"/>
@@ -38327,8 +38438,8 @@
       </c>
     </row>
     <row r="544">
-      <c r="A544" s="64"/>
-      <c r="B544" s="65"/>
+      <c r="A544" s="70"/>
+      <c r="B544" s="71"/>
       <c r="C544" s="34"/>
       <c r="D544" s="34"/>
       <c r="E544" s="34"/>
@@ -38353,8 +38464,8 @@
       </c>
     </row>
     <row r="545">
-      <c r="A545" s="64"/>
-      <c r="B545" s="65"/>
+      <c r="A545" s="70"/>
+      <c r="B545" s="71"/>
       <c r="C545" s="34"/>
       <c r="D545" s="34"/>
       <c r="E545" s="34"/>
@@ -38379,8 +38490,8 @@
       </c>
     </row>
     <row r="546">
-      <c r="A546" s="64"/>
-      <c r="B546" s="65"/>
+      <c r="A546" s="70"/>
+      <c r="B546" s="71"/>
       <c r="C546" s="34"/>
       <c r="D546" s="34"/>
       <c r="E546" s="34"/>
@@ -38405,8 +38516,8 @@
       </c>
     </row>
     <row r="547">
-      <c r="A547" s="64"/>
-      <c r="B547" s="65"/>
+      <c r="A547" s="70"/>
+      <c r="B547" s="71"/>
       <c r="C547" s="34"/>
       <c r="D547" s="34"/>
       <c r="E547" s="34"/>
@@ -38431,8 +38542,8 @@
       </c>
     </row>
     <row r="548">
-      <c r="A548" s="64"/>
-      <c r="B548" s="65"/>
+      <c r="A548" s="70"/>
+      <c r="B548" s="71"/>
       <c r="C548" s="34"/>
       <c r="D548" s="34"/>
       <c r="E548" s="34"/>
@@ -38457,8 +38568,8 @@
       </c>
     </row>
     <row r="549">
-      <c r="A549" s="64"/>
-      <c r="B549" s="65"/>
+      <c r="A549" s="70"/>
+      <c r="B549" s="71"/>
       <c r="C549" s="34"/>
       <c r="D549" s="34"/>
       <c r="E549" s="34"/>
@@ -38483,8 +38594,8 @@
       </c>
     </row>
     <row r="550">
-      <c r="A550" s="64"/>
-      <c r="B550" s="65"/>
+      <c r="A550" s="70"/>
+      <c r="B550" s="71"/>
       <c r="C550" s="34"/>
       <c r="D550" s="34"/>
       <c r="E550" s="34"/>
@@ -38509,8 +38620,8 @@
       </c>
     </row>
     <row r="551">
-      <c r="A551" s="64"/>
-      <c r="B551" s="65"/>
+      <c r="A551" s="70"/>
+      <c r="B551" s="71"/>
       <c r="C551" s="34"/>
       <c r="D551" s="34"/>
       <c r="E551" s="34"/>
@@ -38930,15 +39041,17 @@
     <hyperlink r:id="rId68" ref="S506"/>
     <hyperlink r:id="rId69" ref="S507"/>
     <hyperlink r:id="rId70" ref="S508"/>
+    <hyperlink r:id="rId71" ref="S509"/>
+    <hyperlink r:id="rId72" ref="S510"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId71"/>
-  <legacyDrawing r:id="rId72"/>
+  <drawing r:id="rId73"/>
+  <legacyDrawing r:id="rId74"/>
   <tableParts count="2">
-    <tablePart r:id="rId75"/>
-    <tablePart r:id="rId76"/>
+    <tablePart r:id="rId77"/>
+    <tablePart r:id="rId78"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20200923
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -7987,16 +7987,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:A551" displayName="Table_1" id="1">
-  <tableColumns count="1">
-    <tableColumn name="案例" id="1"/>
-  </tableColumns>
-  <tableStyleInfo name="臺灣武漢肺炎病例-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="B1:U551" displayName="Table_2" id="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="B1:U551" displayName="Table_1" id="1">
   <tableColumns count="20">
     <tableColumn name="新聞稿發布日期" id="1"/>
     <tableColumn name="性別" id="2"/>
@@ -8018,6 +8009,15 @@
     <tableColumn name="疾管署新聞稿" id="18"/>
     <tableColumn name="出院新聞稿" id="19"/>
     <tableColumn name="案例" id="20"/>
+  </tableColumns>
+  <tableStyleInfo name="臺灣武漢肺炎病例-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:A551" displayName="Table_2" id="2">
+  <tableColumns count="1">
+    <tableColumn name="案例" id="1"/>
   </tableColumns>
   <tableStyleInfo name="臺灣武漢肺炎病例-style 2" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>

</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20200924
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -7987,7 +7987,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="B1:U551" displayName="Table_1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:A551" displayName="Table_1" id="1">
+  <tableColumns count="1">
+    <tableColumn name="案例" id="1"/>
+  </tableColumns>
+  <tableStyleInfo name="臺灣武漢肺炎病例-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="B1:U551" displayName="Table_2" id="2">
   <tableColumns count="20">
     <tableColumn name="新聞稿發布日期" id="1"/>
     <tableColumn name="性別" id="2"/>
@@ -8009,15 +8018,6 @@
     <tableColumn name="疾管署新聞稿" id="18"/>
     <tableColumn name="出院新聞稿" id="19"/>
     <tableColumn name="案例" id="20"/>
-  </tableColumns>
-  <tableStyleInfo name="臺灣武漢肺炎病例-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:A551" displayName="Table_2" id="2">
-  <tableColumns count="1">
-    <tableColumn name="案例" id="1"/>
   </tableColumns>
   <tableStyleInfo name="臺灣武漢肺炎病例-style 2" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>

</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20200925
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -563,7 +563,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5608" uniqueCount="1867">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5620" uniqueCount="1871">
   <si>
     <t>案例</t>
   </si>
@@ -6907,6 +6907,21 @@
   </si>
   <si>
     <t>入境時無症狀，入境後前往防疫旅館進行居家檢疫，因為案505同班機前一排座位旅客，改列為居家隔離對象</t>
+  </si>
+  <si>
+    <t>#510</t>
+  </si>
+  <si>
+    <t>9/24 採檢
+9/25 確診</t>
+  </si>
+  <si>
+    <t>入境時無症狀，於機場採檢結果為陰性
+9月21日、22日曾出現腹瀉情形，因自認吃壞肚子故未通報
+9月24日集中檢疫期滿前進行採檢，因檢出武漢肺炎陽性於今日確診</t>
+  </si>
+  <si>
+    <t>菲籍男子來台工作，檢疫期滿前確診COVID-19</t>
   </si>
 </sst>
 </file>
@@ -37580,29 +37595,59 @@
       </c>
     </row>
     <row r="511">
-      <c r="A511" s="70"/>
-      <c r="B511" s="71"/>
-      <c r="C511" s="34"/>
-      <c r="D511" s="34"/>
-      <c r="E511" s="34"/>
+      <c r="A511" s="64" t="s">
+        <v>1867</v>
+      </c>
+      <c r="B511" s="6">
+        <v>44099.0</v>
+      </c>
+      <c r="C511" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D511" s="65" t="s">
+        <v>116</v>
+      </c>
+      <c r="E511" s="7" t="s">
+        <v>205</v>
+      </c>
       <c r="F511" s="34"/>
-      <c r="G511" s="34"/>
-      <c r="H511" s="21"/>
-      <c r="I511" s="19"/>
-      <c r="J511" s="10"/>
-      <c r="K511" s="22"/>
-      <c r="L511" s="23"/>
-      <c r="M511" s="22"/>
+      <c r="G511" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H511" s="66" t="s">
+        <v>1817</v>
+      </c>
+      <c r="I511" s="67">
+        <v>44084.0</v>
+      </c>
+      <c r="J511" s="69">
+        <v>44095.0</v>
+      </c>
+      <c r="K511" s="13" t="s">
+        <v>1868</v>
+      </c>
+      <c r="L511" s="68" t="s">
+        <v>426</v>
+      </c>
+      <c r="M511" s="62" t="s">
+        <v>470</v>
+      </c>
       <c r="N511" s="25"/>
-      <c r="O511" s="21"/>
-      <c r="P511" s="21"/>
+      <c r="O511" s="66" t="s">
+        <v>85</v>
+      </c>
+      <c r="P511" s="66" t="s">
+        <v>1869</v>
+      </c>
       <c r="Q511" s="19"/>
       <c r="R511" s="19"/>
-      <c r="S511" s="20"/>
+      <c r="S511" s="61" t="s">
+        <v>1870</v>
+      </c>
       <c r="T511" s="20"/>
       <c r="U511" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#510</v>
       </c>
     </row>
     <row r="512">
@@ -39043,15 +39088,16 @@
     <hyperlink r:id="rId70" ref="S508"/>
     <hyperlink r:id="rId71" ref="S509"/>
     <hyperlink r:id="rId72" ref="S510"/>
+    <hyperlink r:id="rId73" ref="S511"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId73"/>
-  <legacyDrawing r:id="rId74"/>
+  <drawing r:id="rId74"/>
+  <legacyDrawing r:id="rId75"/>
   <tableParts count="2">
-    <tablePart r:id="rId77"/>
     <tablePart r:id="rId78"/>
+    <tablePart r:id="rId79"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20200927
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -6932,7 +6932,7 @@
     <numFmt numFmtId="164" formatCode="mm&quot;月&quot;dd&quot;日 &quot;dddd"/>
     <numFmt numFmtId="165" formatCode="m/d"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="17">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -7009,10 +7009,6 @@
       <u/>
       <color rgb="FF1155CC"/>
     </font>
-    <font>
-      <color rgb="FF000000"/>
-    </font>
-    <font/>
   </fonts>
   <fills count="7">
     <fill>
@@ -7058,7 +7054,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="65">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -7245,29 +7241,8 @@
     <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="18" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
@@ -35165,7 +35140,7 @@
       <c r="L467" s="12" t="s">
         <v>363</v>
       </c>
-      <c r="M467" s="62" t="s">
+      <c r="M467" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N467" s="14" t="s">
@@ -35257,7 +35232,7 @@
       <c r="D469" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E469" s="63" t="s">
+      <c r="E469" s="62" t="s">
         <v>1663</v>
       </c>
       <c r="F469" s="34"/>
@@ -37483,7 +37458,7 @@
       </c>
     </row>
     <row r="509">
-      <c r="A509" s="64" t="s">
+      <c r="A509" s="16" t="s">
         <v>1857</v>
       </c>
       <c r="B509" s="6">
@@ -37492,7 +37467,7 @@
       <c r="C509" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D509" s="65" t="s">
+      <c r="D509" s="7" t="s">
         <v>76</v>
       </c>
       <c r="E509" s="7" t="s">
@@ -37502,29 +37477,29 @@
       <c r="G509" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H509" s="66" t="s">
+      <c r="H509" s="8" t="s">
         <v>1858</v>
       </c>
-      <c r="I509" s="67">
+      <c r="I509" s="9">
         <v>44093.0</v>
       </c>
       <c r="J509" s="10">
         <v>44091.0</v>
       </c>
-      <c r="K509" s="62" t="s">
+      <c r="K509" s="13" t="s">
         <v>1859</v>
       </c>
-      <c r="L509" s="68" t="s">
+      <c r="L509" s="12" t="s">
         <v>363</v>
       </c>
-      <c r="M509" s="62" t="s">
+      <c r="M509" s="13" t="s">
         <v>1860</v>
       </c>
       <c r="N509" s="25"/>
-      <c r="O509" s="66" t="s">
+      <c r="O509" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P509" s="66" t="s">
+      <c r="P509" s="8" t="s">
         <v>334</v>
       </c>
       <c r="Q509" s="19"/>
@@ -37539,7 +37514,7 @@
       </c>
     </row>
     <row r="510">
-      <c r="A510" s="64" t="s">
+      <c r="A510" s="16" t="s">
         <v>1862</v>
       </c>
       <c r="B510" s="6">
@@ -37548,7 +37523,7 @@
       <c r="C510" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D510" s="65" t="s">
+      <c r="D510" s="7" t="s">
         <v>116</v>
       </c>
       <c r="E510" s="7" t="s">
@@ -37558,29 +37533,29 @@
       <c r="G510" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H510" s="66" t="s">
+      <c r="H510" s="8" t="s">
         <v>1863</v>
       </c>
-      <c r="I510" s="67">
+      <c r="I510" s="9">
         <v>44091.0</v>
       </c>
-      <c r="J510" s="69">
+      <c r="J510" s="10">
         <v>44091.0</v>
       </c>
-      <c r="K510" s="62" t="s">
+      <c r="K510" s="13" t="s">
         <v>1864</v>
       </c>
-      <c r="L510" s="68" t="s">
+      <c r="L510" s="12" t="s">
         <v>447</v>
       </c>
-      <c r="M510" s="62" t="s">
+      <c r="M510" s="13" t="s">
         <v>1865</v>
       </c>
       <c r="N510" s="25"/>
-      <c r="O510" s="66" t="s">
+      <c r="O510" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P510" s="66" t="s">
+      <c r="P510" s="8" t="s">
         <v>1866</v>
       </c>
       <c r="Q510" s="19"/>
@@ -37595,7 +37570,7 @@
       </c>
     </row>
     <row r="511">
-      <c r="A511" s="64" t="s">
+      <c r="A511" s="16" t="s">
         <v>1867</v>
       </c>
       <c r="B511" s="6">
@@ -37604,7 +37579,7 @@
       <c r="C511" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D511" s="65" t="s">
+      <c r="D511" s="7" t="s">
         <v>116</v>
       </c>
       <c r="E511" s="7" t="s">
@@ -37614,29 +37589,29 @@
       <c r="G511" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H511" s="66" t="s">
+      <c r="H511" s="8" t="s">
         <v>1817</v>
       </c>
-      <c r="I511" s="67">
+      <c r="I511" s="9">
         <v>44084.0</v>
       </c>
-      <c r="J511" s="69">
+      <c r="J511" s="10">
         <v>44095.0</v>
       </c>
       <c r="K511" s="13" t="s">
         <v>1868</v>
       </c>
-      <c r="L511" s="68" t="s">
+      <c r="L511" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M511" s="62" t="s">
+      <c r="M511" s="13" t="s">
         <v>470</v>
       </c>
       <c r="N511" s="25"/>
-      <c r="O511" s="66" t="s">
+      <c r="O511" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P511" s="66" t="s">
+      <c r="P511" s="8" t="s">
         <v>1869</v>
       </c>
       <c r="Q511" s="19"/>
@@ -37651,8 +37626,8 @@
       </c>
     </row>
     <row r="512">
-      <c r="A512" s="70"/>
-      <c r="B512" s="71"/>
+      <c r="A512" s="63"/>
+      <c r="B512" s="64"/>
       <c r="C512" s="34"/>
       <c r="D512" s="34"/>
       <c r="E512" s="34"/>
@@ -37677,8 +37652,8 @@
       </c>
     </row>
     <row r="513">
-      <c r="A513" s="70"/>
-      <c r="B513" s="71"/>
+      <c r="A513" s="63"/>
+      <c r="B513" s="64"/>
       <c r="C513" s="34"/>
       <c r="D513" s="34"/>
       <c r="E513" s="34"/>
@@ -37703,8 +37678,8 @@
       </c>
     </row>
     <row r="514">
-      <c r="A514" s="70"/>
-      <c r="B514" s="71"/>
+      <c r="A514" s="63"/>
+      <c r="B514" s="64"/>
       <c r="C514" s="34"/>
       <c r="D514" s="34"/>
       <c r="E514" s="34"/>
@@ -37729,8 +37704,8 @@
       </c>
     </row>
     <row r="515">
-      <c r="A515" s="70"/>
-      <c r="B515" s="71"/>
+      <c r="A515" s="63"/>
+      <c r="B515" s="64"/>
       <c r="C515" s="34"/>
       <c r="D515" s="34"/>
       <c r="E515" s="34"/>
@@ -37755,8 +37730,8 @@
       </c>
     </row>
     <row r="516">
-      <c r="A516" s="70"/>
-      <c r="B516" s="71"/>
+      <c r="A516" s="63"/>
+      <c r="B516" s="64"/>
       <c r="C516" s="34"/>
       <c r="D516" s="34"/>
       <c r="E516" s="34"/>
@@ -37781,8 +37756,8 @@
       </c>
     </row>
     <row r="517">
-      <c r="A517" s="70"/>
-      <c r="B517" s="71"/>
+      <c r="A517" s="63"/>
+      <c r="B517" s="64"/>
       <c r="C517" s="34"/>
       <c r="D517" s="34"/>
       <c r="E517" s="34"/>
@@ -37807,8 +37782,8 @@
       </c>
     </row>
     <row r="518">
-      <c r="A518" s="70"/>
-      <c r="B518" s="71"/>
+      <c r="A518" s="63"/>
+      <c r="B518" s="64"/>
       <c r="C518" s="34"/>
       <c r="D518" s="34"/>
       <c r="E518" s="34"/>
@@ -37833,8 +37808,8 @@
       </c>
     </row>
     <row r="519">
-      <c r="A519" s="70"/>
-      <c r="B519" s="71"/>
+      <c r="A519" s="63"/>
+      <c r="B519" s="64"/>
       <c r="C519" s="34"/>
       <c r="D519" s="34"/>
       <c r="E519" s="34"/>
@@ -37859,8 +37834,8 @@
       </c>
     </row>
     <row r="520">
-      <c r="A520" s="70"/>
-      <c r="B520" s="71"/>
+      <c r="A520" s="63"/>
+      <c r="B520" s="64"/>
       <c r="C520" s="34"/>
       <c r="D520" s="34"/>
       <c r="E520" s="34"/>
@@ -37885,8 +37860,8 @@
       </c>
     </row>
     <row r="521">
-      <c r="A521" s="70"/>
-      <c r="B521" s="71"/>
+      <c r="A521" s="63"/>
+      <c r="B521" s="64"/>
       <c r="C521" s="34"/>
       <c r="D521" s="34"/>
       <c r="E521" s="34"/>
@@ -37911,8 +37886,8 @@
       </c>
     </row>
     <row r="522">
-      <c r="A522" s="70"/>
-      <c r="B522" s="71"/>
+      <c r="A522" s="63"/>
+      <c r="B522" s="64"/>
       <c r="C522" s="34"/>
       <c r="D522" s="34"/>
       <c r="E522" s="34"/>
@@ -37937,8 +37912,8 @@
       </c>
     </row>
     <row r="523">
-      <c r="A523" s="70"/>
-      <c r="B523" s="71"/>
+      <c r="A523" s="63"/>
+      <c r="B523" s="64"/>
       <c r="C523" s="34"/>
       <c r="D523" s="34"/>
       <c r="E523" s="34"/>
@@ -37963,8 +37938,8 @@
       </c>
     </row>
     <row r="524">
-      <c r="A524" s="70"/>
-      <c r="B524" s="71"/>
+      <c r="A524" s="63"/>
+      <c r="B524" s="64"/>
       <c r="C524" s="34"/>
       <c r="D524" s="34"/>
       <c r="E524" s="34"/>
@@ -37989,8 +37964,8 @@
       </c>
     </row>
     <row r="525">
-      <c r="A525" s="70"/>
-      <c r="B525" s="71"/>
+      <c r="A525" s="63"/>
+      <c r="B525" s="64"/>
       <c r="C525" s="34"/>
       <c r="D525" s="34"/>
       <c r="E525" s="34"/>
@@ -38015,8 +37990,8 @@
       </c>
     </row>
     <row r="526">
-      <c r="A526" s="70"/>
-      <c r="B526" s="71"/>
+      <c r="A526" s="63"/>
+      <c r="B526" s="64"/>
       <c r="C526" s="34"/>
       <c r="D526" s="34"/>
       <c r="E526" s="34"/>
@@ -38041,8 +38016,8 @@
       </c>
     </row>
     <row r="527">
-      <c r="A527" s="70"/>
-      <c r="B527" s="71"/>
+      <c r="A527" s="63"/>
+      <c r="B527" s="64"/>
       <c r="C527" s="34"/>
       <c r="D527" s="34"/>
       <c r="E527" s="34"/>
@@ -38067,8 +38042,8 @@
       </c>
     </row>
     <row r="528">
-      <c r="A528" s="70"/>
-      <c r="B528" s="71"/>
+      <c r="A528" s="63"/>
+      <c r="B528" s="64"/>
       <c r="C528" s="34"/>
       <c r="D528" s="34"/>
       <c r="E528" s="34"/>
@@ -38093,8 +38068,8 @@
       </c>
     </row>
     <row r="529">
-      <c r="A529" s="70"/>
-      <c r="B529" s="71"/>
+      <c r="A529" s="63"/>
+      <c r="B529" s="64"/>
       <c r="C529" s="34"/>
       <c r="D529" s="34"/>
       <c r="E529" s="34"/>
@@ -38119,8 +38094,8 @@
       </c>
     </row>
     <row r="530">
-      <c r="A530" s="70"/>
-      <c r="B530" s="71"/>
+      <c r="A530" s="63"/>
+      <c r="B530" s="64"/>
       <c r="C530" s="34"/>
       <c r="D530" s="34"/>
       <c r="E530" s="34"/>
@@ -38145,8 +38120,8 @@
       </c>
     </row>
     <row r="531">
-      <c r="A531" s="70"/>
-      <c r="B531" s="71"/>
+      <c r="A531" s="63"/>
+      <c r="B531" s="64"/>
       <c r="C531" s="34"/>
       <c r="D531" s="34"/>
       <c r="E531" s="34"/>
@@ -38171,8 +38146,8 @@
       </c>
     </row>
     <row r="532">
-      <c r="A532" s="70"/>
-      <c r="B532" s="71"/>
+      <c r="A532" s="63"/>
+      <c r="B532" s="64"/>
       <c r="C532" s="34"/>
       <c r="D532" s="34"/>
       <c r="E532" s="34"/>
@@ -38197,8 +38172,8 @@
       </c>
     </row>
     <row r="533">
-      <c r="A533" s="70"/>
-      <c r="B533" s="71"/>
+      <c r="A533" s="63"/>
+      <c r="B533" s="64"/>
       <c r="C533" s="34"/>
       <c r="D533" s="34"/>
       <c r="E533" s="34"/>
@@ -38223,8 +38198,8 @@
       </c>
     </row>
     <row r="534">
-      <c r="A534" s="70"/>
-      <c r="B534" s="71"/>
+      <c r="A534" s="63"/>
+      <c r="B534" s="64"/>
       <c r="C534" s="34"/>
       <c r="D534" s="34"/>
       <c r="E534" s="34"/>
@@ -38249,8 +38224,8 @@
       </c>
     </row>
     <row r="535">
-      <c r="A535" s="70"/>
-      <c r="B535" s="71"/>
+      <c r="A535" s="63"/>
+      <c r="B535" s="64"/>
       <c r="C535" s="34"/>
       <c r="D535" s="34"/>
       <c r="E535" s="34"/>
@@ -38275,8 +38250,8 @@
       </c>
     </row>
     <row r="536">
-      <c r="A536" s="70"/>
-      <c r="B536" s="71"/>
+      <c r="A536" s="63"/>
+      <c r="B536" s="64"/>
       <c r="C536" s="34"/>
       <c r="D536" s="34"/>
       <c r="E536" s="34"/>
@@ -38301,8 +38276,8 @@
       </c>
     </row>
     <row r="537">
-      <c r="A537" s="70"/>
-      <c r="B537" s="71"/>
+      <c r="A537" s="63"/>
+      <c r="B537" s="64"/>
       <c r="C537" s="34"/>
       <c r="D537" s="34"/>
       <c r="E537" s="34"/>
@@ -38327,8 +38302,8 @@
       </c>
     </row>
     <row r="538">
-      <c r="A538" s="70"/>
-      <c r="B538" s="71"/>
+      <c r="A538" s="63"/>
+      <c r="B538" s="64"/>
       <c r="C538" s="34"/>
       <c r="D538" s="34"/>
       <c r="E538" s="34"/>
@@ -38353,8 +38328,8 @@
       </c>
     </row>
     <row r="539">
-      <c r="A539" s="70"/>
-      <c r="B539" s="71"/>
+      <c r="A539" s="63"/>
+      <c r="B539" s="64"/>
       <c r="C539" s="34"/>
       <c r="D539" s="34"/>
       <c r="E539" s="34"/>
@@ -38379,8 +38354,8 @@
       </c>
     </row>
     <row r="540">
-      <c r="A540" s="70"/>
-      <c r="B540" s="71"/>
+      <c r="A540" s="63"/>
+      <c r="B540" s="64"/>
       <c r="C540" s="34"/>
       <c r="D540" s="34"/>
       <c r="E540" s="34"/>
@@ -38405,8 +38380,8 @@
       </c>
     </row>
     <row r="541">
-      <c r="A541" s="70"/>
-      <c r="B541" s="71"/>
+      <c r="A541" s="63"/>
+      <c r="B541" s="64"/>
       <c r="C541" s="34"/>
       <c r="D541" s="34"/>
       <c r="E541" s="34"/>
@@ -38431,8 +38406,8 @@
       </c>
     </row>
     <row r="542">
-      <c r="A542" s="70"/>
-      <c r="B542" s="71"/>
+      <c r="A542" s="63"/>
+      <c r="B542" s="64"/>
       <c r="C542" s="34"/>
       <c r="D542" s="34"/>
       <c r="E542" s="34"/>
@@ -38457,8 +38432,8 @@
       </c>
     </row>
     <row r="543">
-      <c r="A543" s="70"/>
-      <c r="B543" s="71"/>
+      <c r="A543" s="63"/>
+      <c r="B543" s="64"/>
       <c r="C543" s="34"/>
       <c r="D543" s="34"/>
       <c r="E543" s="34"/>
@@ -38483,8 +38458,8 @@
       </c>
     </row>
     <row r="544">
-      <c r="A544" s="70"/>
-      <c r="B544" s="71"/>
+      <c r="A544" s="63"/>
+      <c r="B544" s="64"/>
       <c r="C544" s="34"/>
       <c r="D544" s="34"/>
       <c r="E544" s="34"/>
@@ -38509,8 +38484,8 @@
       </c>
     </row>
     <row r="545">
-      <c r="A545" s="70"/>
-      <c r="B545" s="71"/>
+      <c r="A545" s="63"/>
+      <c r="B545" s="64"/>
       <c r="C545" s="34"/>
       <c r="D545" s="34"/>
       <c r="E545" s="34"/>
@@ -38535,8 +38510,8 @@
       </c>
     </row>
     <row r="546">
-      <c r="A546" s="70"/>
-      <c r="B546" s="71"/>
+      <c r="A546" s="63"/>
+      <c r="B546" s="64"/>
       <c r="C546" s="34"/>
       <c r="D546" s="34"/>
       <c r="E546" s="34"/>
@@ -38561,8 +38536,8 @@
       </c>
     </row>
     <row r="547">
-      <c r="A547" s="70"/>
-      <c r="B547" s="71"/>
+      <c r="A547" s="63"/>
+      <c r="B547" s="64"/>
       <c r="C547" s="34"/>
       <c r="D547" s="34"/>
       <c r="E547" s="34"/>
@@ -38587,8 +38562,8 @@
       </c>
     </row>
     <row r="548">
-      <c r="A548" s="70"/>
-      <c r="B548" s="71"/>
+      <c r="A548" s="63"/>
+      <c r="B548" s="64"/>
       <c r="C548" s="34"/>
       <c r="D548" s="34"/>
       <c r="E548" s="34"/>
@@ -38613,8 +38588,8 @@
       </c>
     </row>
     <row r="549">
-      <c r="A549" s="70"/>
-      <c r="B549" s="71"/>
+      <c r="A549" s="63"/>
+      <c r="B549" s="64"/>
       <c r="C549" s="34"/>
       <c r="D549" s="34"/>
       <c r="E549" s="34"/>
@@ -38639,8 +38614,8 @@
       </c>
     </row>
     <row r="550">
-      <c r="A550" s="70"/>
-      <c r="B550" s="71"/>
+      <c r="A550" s="63"/>
+      <c r="B550" s="64"/>
       <c r="C550" s="34"/>
       <c r="D550" s="34"/>
       <c r="E550" s="34"/>
@@ -38665,8 +38640,8 @@
       </c>
     </row>
     <row r="551">
-      <c r="A551" s="70"/>
-      <c r="B551" s="71"/>
+      <c r="A551" s="63"/>
+      <c r="B551" s="64"/>
       <c r="C551" s="34"/>
       <c r="D551" s="34"/>
       <c r="E551" s="34"/>

</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20200929
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -563,7 +563,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5620" uniqueCount="1871">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5658" uniqueCount="1885">
   <si>
     <t>案例</t>
   </si>
@@ -6230,7 +6230,7 @@
     <t>瓜地馬拉</t>
   </si>
   <si>
-    <t>-7/26 台灣</t>
+    <t>-7/26 瓜地馬拉→台灣</t>
   </si>
   <si>
     <t>7/30 採檢 通報
@@ -6252,7 +6252,7 @@
     <t>不明</t>
   </si>
   <si>
-    <t>1/31-5/3 台灣</t>
+    <t>1/31-5/3 比利時→台灣</t>
   </si>
   <si>
     <t>X</t>
@@ -6272,8 +6272,8 @@
     <t>#470</t>
   </si>
   <si>
-    <t>-7/18 香港
--7/30 台灣</t>
+    <t>-7/18 菲律賓→香港
+-7/30 香港→台灣</t>
   </si>
   <si>
     <t>7/20 接獲香港檢驗確診
@@ -6326,7 +6326,7 @@
     <t>#473</t>
   </si>
   <si>
-    <t>6/22-7/15 台灣</t>
+    <t>6/22-7/15 菲律賓→台灣</t>
   </si>
   <si>
     <t>7/29 採檢 通報
@@ -6353,7 +6353,7 @@
     <t>#475</t>
   </si>
   <si>
-    <t>-7/31 台灣</t>
+    <t>-7/31 菲律賓→台灣</t>
   </si>
   <si>
     <t>8/1 採檢
@@ -6567,7 +6567,7 @@
     <t>#489</t>
   </si>
   <si>
-    <t>-8/16 台灣</t>
+    <t>-8/16 印尼→台灣</t>
   </si>
   <si>
     <t>8/31 採檢
@@ -6601,7 +6601,7 @@
     <t>#491</t>
   </si>
   <si>
-    <t>-9/3 台灣</t>
+    <t>-9/3 菲律賓→台灣</t>
   </si>
   <si>
     <t>9/3 採檢
@@ -6708,7 +6708,7 @@
     <t>#497</t>
   </si>
   <si>
-    <t>-8/30 台灣</t>
+    <t>-8/30 菲律賓→台灣</t>
   </si>
   <si>
     <t>9/10 採檢
@@ -6743,7 +6743,7 @@
     <t>#499</t>
   </si>
   <si>
-    <t>-9/10 台灣</t>
+    <t>-9/10 菲律賓→台灣</t>
   </si>
   <si>
     <t>9/10 採檢
@@ -6759,7 +6759,7 @@
     <t>#500</t>
   </si>
   <si>
-    <t>-9/13 台灣</t>
+    <t>-9/13 菲律賓→台灣</t>
   </si>
   <si>
     <t>9/13 採檢
@@ -6823,7 +6823,7 @@
     <t>#504</t>
   </si>
   <si>
-    <t>-9/17 台灣</t>
+    <t>-9/17 菲律賓→台灣</t>
   </si>
   <si>
     <t>9/17 採檢
@@ -6870,7 +6870,7 @@
     <t>#507</t>
   </si>
   <si>
-    <t>-9/18 台灣</t>
+    <t>-9/18 菲律賓→台灣</t>
   </si>
   <si>
     <t>9/18 採檢
@@ -6922,6 +6922,55 @@
   </si>
   <si>
     <t>菲籍男子來台工作，檢疫期滿前確診COVID-19</t>
+  </si>
+  <si>
+    <t>#511</t>
+  </si>
+  <si>
+    <t>-9/11 菲律賓→台灣</t>
+  </si>
+  <si>
+    <t>9/11 採檢
+9/26 二採
+9/28 確診</t>
+  </si>
+  <si>
+    <t>9月11日自菲律賓搭機來台，機場檢驗結果為陰性，入境迄今無疑似症狀
+集中檢疫期滿隔日(9月26日)再次採檢，於今日確診</t>
+  </si>
+  <si>
+    <t>國內新增3例境外移入COVID-19確診，分別自菲律賓及印尼入境</t>
+  </si>
+  <si>
+    <t>#512</t>
+  </si>
+  <si>
+    <t>-9/23 菲律賓→台灣</t>
+  </si>
+  <si>
+    <t>9/23 採檢
+9/26 二採
+9/28 確診</t>
+  </si>
+  <si>
+    <t>機場採檢結果為弱陽性
+於9月26日再次採檢</t>
+  </si>
+  <si>
+    <t>#513</t>
+  </si>
+  <si>
+    <t>7月下旬-9/26 印尼</t>
+  </si>
+  <si>
+    <t>9/26 採檢
+9/28 確診</t>
+  </si>
+  <si>
+    <t>倦怠 腹瀉 腹痛</t>
+  </si>
+  <si>
+    <t>於當地就醫並診斷為胃潰瘍</t>
   </si>
 </sst>
 </file>
@@ -6932,7 +6981,7 @@
     <numFmt numFmtId="164" formatCode="mm&quot;月&quot;dd&quot;日 &quot;dddd"/>
     <numFmt numFmtId="165" formatCode="m/d"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -7009,6 +7058,7 @@
       <u/>
       <color rgb="FF1155CC"/>
     </font>
+    <font/>
   </fonts>
   <fills count="7">
     <fill>
@@ -7054,7 +7104,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -7243,6 +7293,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
@@ -35239,7 +35292,7 @@
       <c r="G469" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H469" s="8" t="s">
+      <c r="H469" s="63" t="s">
         <v>1664</v>
       </c>
       <c r="I469" s="9">
@@ -35297,7 +35350,7 @@
       <c r="G470" s="7" t="s">
         <v>1670</v>
       </c>
-      <c r="H470" s="8" t="s">
+      <c r="H470" s="63" t="s">
         <v>1671</v>
       </c>
       <c r="I470" s="9">
@@ -35353,7 +35406,7 @@
       <c r="G471" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H471" s="8" t="s">
+      <c r="H471" s="63" t="s">
         <v>1677</v>
       </c>
       <c r="I471" s="9">
@@ -35523,7 +35576,7 @@
       <c r="G474" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H474" s="8" t="s">
+      <c r="H474" s="63" t="s">
         <v>1692</v>
       </c>
       <c r="I474" s="9">
@@ -35635,7 +35688,7 @@
       <c r="G476" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H476" s="8" t="s">
+      <c r="H476" s="63" t="s">
         <v>1700</v>
       </c>
       <c r="I476" s="9">
@@ -36417,7 +36470,7 @@
       <c r="G490" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H490" s="8" t="s">
+      <c r="H490" s="63" t="s">
         <v>1765</v>
       </c>
       <c r="I490" s="9">
@@ -37626,86 +37679,176 @@
       </c>
     </row>
     <row r="512">
-      <c r="A512" s="63"/>
-      <c r="B512" s="64"/>
-      <c r="C512" s="34"/>
-      <c r="D512" s="34"/>
-      <c r="E512" s="34"/>
+      <c r="A512" s="16" t="s">
+        <v>1871</v>
+      </c>
+      <c r="B512" s="6">
+        <v>44102.0</v>
+      </c>
+      <c r="C512" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D512" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E512" s="7" t="s">
+        <v>205</v>
+      </c>
       <c r="F512" s="34"/>
-      <c r="G512" s="34"/>
-      <c r="H512" s="21"/>
-      <c r="I512" s="19"/>
-      <c r="J512" s="10"/>
-      <c r="K512" s="22"/>
-      <c r="L512" s="23"/>
-      <c r="M512" s="22"/>
+      <c r="G512" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H512" s="8" t="s">
+        <v>1872</v>
+      </c>
+      <c r="I512" s="9">
+        <v>44085.0</v>
+      </c>
+      <c r="J512" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K512" s="13" t="s">
+        <v>1873</v>
+      </c>
+      <c r="L512" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M512" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N512" s="25"/>
-      <c r="O512" s="21"/>
-      <c r="P512" s="21"/>
+      <c r="O512" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P512" s="8" t="s">
+        <v>1874</v>
+      </c>
       <c r="Q512" s="19"/>
       <c r="R512" s="19"/>
-      <c r="S512" s="20"/>
+      <c r="S512" s="61" t="s">
+        <v>1875</v>
+      </c>
       <c r="T512" s="20"/>
       <c r="U512" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#511</v>
       </c>
     </row>
     <row r="513">
-      <c r="A513" s="63"/>
-      <c r="B513" s="64"/>
-      <c r="C513" s="34"/>
-      <c r="D513" s="34"/>
-      <c r="E513" s="34"/>
+      <c r="A513" s="16" t="s">
+        <v>1876</v>
+      </c>
+      <c r="B513" s="6">
+        <v>44102.0</v>
+      </c>
+      <c r="C513" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D513" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E513" s="7" t="s">
+        <v>205</v>
+      </c>
       <c r="F513" s="34"/>
-      <c r="G513" s="34"/>
-      <c r="H513" s="21"/>
-      <c r="I513" s="19"/>
-      <c r="J513" s="10"/>
-      <c r="K513" s="22"/>
-      <c r="L513" s="23"/>
-      <c r="M513" s="22"/>
+      <c r="G513" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H513" s="8" t="s">
+        <v>1877</v>
+      </c>
+      <c r="I513" s="9">
+        <v>44097.0</v>
+      </c>
+      <c r="J513" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K513" s="13" t="s">
+        <v>1878</v>
+      </c>
+      <c r="L513" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M513" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N513" s="25"/>
-      <c r="O513" s="21"/>
-      <c r="P513" s="21"/>
+      <c r="O513" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P513" s="8" t="s">
+        <v>1879</v>
+      </c>
       <c r="Q513" s="19"/>
       <c r="R513" s="19"/>
-      <c r="S513" s="20"/>
+      <c r="S513" s="61" t="s">
+        <v>1875</v>
+      </c>
       <c r="T513" s="20"/>
       <c r="U513" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#512</v>
       </c>
     </row>
     <row r="514">
-      <c r="A514" s="63"/>
-      <c r="B514" s="64"/>
-      <c r="C514" s="34"/>
-      <c r="D514" s="34"/>
-      <c r="E514" s="34"/>
+      <c r="A514" s="16" t="s">
+        <v>1880</v>
+      </c>
+      <c r="B514" s="6">
+        <v>44102.0</v>
+      </c>
+      <c r="C514" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D514" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E514" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F514" s="34"/>
-      <c r="G514" s="34"/>
-      <c r="H514" s="21"/>
-      <c r="I514" s="19"/>
-      <c r="J514" s="10"/>
-      <c r="K514" s="22"/>
-      <c r="L514" s="23"/>
-      <c r="M514" s="22"/>
+      <c r="G514" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H514" s="8" t="s">
+        <v>1881</v>
+      </c>
+      <c r="I514" s="9">
+        <v>44100.0</v>
+      </c>
+      <c r="J514" s="10">
+        <v>44093.0</v>
+      </c>
+      <c r="K514" s="13" t="s">
+        <v>1882</v>
+      </c>
+      <c r="L514" s="12" t="s">
+        <v>363</v>
+      </c>
+      <c r="M514" s="13" t="s">
+        <v>1883</v>
+      </c>
       <c r="N514" s="25"/>
-      <c r="O514" s="21"/>
-      <c r="P514" s="21"/>
+      <c r="O514" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P514" s="8" t="s">
+        <v>1884</v>
+      </c>
       <c r="Q514" s="19"/>
       <c r="R514" s="19"/>
-      <c r="S514" s="20"/>
+      <c r="S514" s="61" t="s">
+        <v>1875</v>
+      </c>
       <c r="T514" s="20"/>
       <c r="U514" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#513</v>
       </c>
     </row>
     <row r="515">
-      <c r="A515" s="63"/>
-      <c r="B515" s="64"/>
+      <c r="A515" s="64"/>
+      <c r="B515" s="65"/>
       <c r="C515" s="34"/>
       <c r="D515" s="34"/>
       <c r="E515" s="34"/>
@@ -37730,8 +37873,8 @@
       </c>
     </row>
     <row r="516">
-      <c r="A516" s="63"/>
-      <c r="B516" s="64"/>
+      <c r="A516" s="64"/>
+      <c r="B516" s="65"/>
       <c r="C516" s="34"/>
       <c r="D516" s="34"/>
       <c r="E516" s="34"/>
@@ -37756,8 +37899,8 @@
       </c>
     </row>
     <row r="517">
-      <c r="A517" s="63"/>
-      <c r="B517" s="64"/>
+      <c r="A517" s="64"/>
+      <c r="B517" s="65"/>
       <c r="C517" s="34"/>
       <c r="D517" s="34"/>
       <c r="E517" s="34"/>
@@ -37782,8 +37925,8 @@
       </c>
     </row>
     <row r="518">
-      <c r="A518" s="63"/>
-      <c r="B518" s="64"/>
+      <c r="A518" s="64"/>
+      <c r="B518" s="65"/>
       <c r="C518" s="34"/>
       <c r="D518" s="34"/>
       <c r="E518" s="34"/>
@@ -37808,8 +37951,8 @@
       </c>
     </row>
     <row r="519">
-      <c r="A519" s="63"/>
-      <c r="B519" s="64"/>
+      <c r="A519" s="64"/>
+      <c r="B519" s="65"/>
       <c r="C519" s="34"/>
       <c r="D519" s="34"/>
       <c r="E519" s="34"/>
@@ -37834,8 +37977,8 @@
       </c>
     </row>
     <row r="520">
-      <c r="A520" s="63"/>
-      <c r="B520" s="64"/>
+      <c r="A520" s="64"/>
+      <c r="B520" s="65"/>
       <c r="C520" s="34"/>
       <c r="D520" s="34"/>
       <c r="E520" s="34"/>
@@ -37860,8 +38003,8 @@
       </c>
     </row>
     <row r="521">
-      <c r="A521" s="63"/>
-      <c r="B521" s="64"/>
+      <c r="A521" s="64"/>
+      <c r="B521" s="65"/>
       <c r="C521" s="34"/>
       <c r="D521" s="34"/>
       <c r="E521" s="34"/>
@@ -37886,8 +38029,8 @@
       </c>
     </row>
     <row r="522">
-      <c r="A522" s="63"/>
-      <c r="B522" s="64"/>
+      <c r="A522" s="64"/>
+      <c r="B522" s="65"/>
       <c r="C522" s="34"/>
       <c r="D522" s="34"/>
       <c r="E522" s="34"/>
@@ -37912,8 +38055,8 @@
       </c>
     </row>
     <row r="523">
-      <c r="A523" s="63"/>
-      <c r="B523" s="64"/>
+      <c r="A523" s="64"/>
+      <c r="B523" s="65"/>
       <c r="C523" s="34"/>
       <c r="D523" s="34"/>
       <c r="E523" s="34"/>
@@ -37938,8 +38081,8 @@
       </c>
     </row>
     <row r="524">
-      <c r="A524" s="63"/>
-      <c r="B524" s="64"/>
+      <c r="A524" s="64"/>
+      <c r="B524" s="65"/>
       <c r="C524" s="34"/>
       <c r="D524" s="34"/>
       <c r="E524" s="34"/>
@@ -37964,8 +38107,8 @@
       </c>
     </row>
     <row r="525">
-      <c r="A525" s="63"/>
-      <c r="B525" s="64"/>
+      <c r="A525" s="64"/>
+      <c r="B525" s="65"/>
       <c r="C525" s="34"/>
       <c r="D525" s="34"/>
       <c r="E525" s="34"/>
@@ -37990,8 +38133,8 @@
       </c>
     </row>
     <row r="526">
-      <c r="A526" s="63"/>
-      <c r="B526" s="64"/>
+      <c r="A526" s="64"/>
+      <c r="B526" s="65"/>
       <c r="C526" s="34"/>
       <c r="D526" s="34"/>
       <c r="E526" s="34"/>
@@ -38016,8 +38159,8 @@
       </c>
     </row>
     <row r="527">
-      <c r="A527" s="63"/>
-      <c r="B527" s="64"/>
+      <c r="A527" s="64"/>
+      <c r="B527" s="65"/>
       <c r="C527" s="34"/>
       <c r="D527" s="34"/>
       <c r="E527" s="34"/>
@@ -38042,8 +38185,8 @@
       </c>
     </row>
     <row r="528">
-      <c r="A528" s="63"/>
-      <c r="B528" s="64"/>
+      <c r="A528" s="64"/>
+      <c r="B528" s="65"/>
       <c r="C528" s="34"/>
       <c r="D528" s="34"/>
       <c r="E528" s="34"/>
@@ -38068,8 +38211,8 @@
       </c>
     </row>
     <row r="529">
-      <c r="A529" s="63"/>
-      <c r="B529" s="64"/>
+      <c r="A529" s="64"/>
+      <c r="B529" s="65"/>
       <c r="C529" s="34"/>
       <c r="D529" s="34"/>
       <c r="E529" s="34"/>
@@ -38094,8 +38237,8 @@
       </c>
     </row>
     <row r="530">
-      <c r="A530" s="63"/>
-      <c r="B530" s="64"/>
+      <c r="A530" s="64"/>
+      <c r="B530" s="65"/>
       <c r="C530" s="34"/>
       <c r="D530" s="34"/>
       <c r="E530" s="34"/>
@@ -38120,8 +38263,8 @@
       </c>
     </row>
     <row r="531">
-      <c r="A531" s="63"/>
-      <c r="B531" s="64"/>
+      <c r="A531" s="64"/>
+      <c r="B531" s="65"/>
       <c r="C531" s="34"/>
       <c r="D531" s="34"/>
       <c r="E531" s="34"/>
@@ -38146,8 +38289,8 @@
       </c>
     </row>
     <row r="532">
-      <c r="A532" s="63"/>
-      <c r="B532" s="64"/>
+      <c r="A532" s="64"/>
+      <c r="B532" s="65"/>
       <c r="C532" s="34"/>
       <c r="D532" s="34"/>
       <c r="E532" s="34"/>
@@ -38172,8 +38315,8 @@
       </c>
     </row>
     <row r="533">
-      <c r="A533" s="63"/>
-      <c r="B533" s="64"/>
+      <c r="A533" s="64"/>
+      <c r="B533" s="65"/>
       <c r="C533" s="34"/>
       <c r="D533" s="34"/>
       <c r="E533" s="34"/>
@@ -38198,8 +38341,8 @@
       </c>
     </row>
     <row r="534">
-      <c r="A534" s="63"/>
-      <c r="B534" s="64"/>
+      <c r="A534" s="64"/>
+      <c r="B534" s="65"/>
       <c r="C534" s="34"/>
       <c r="D534" s="34"/>
       <c r="E534" s="34"/>
@@ -38224,8 +38367,8 @@
       </c>
     </row>
     <row r="535">
-      <c r="A535" s="63"/>
-      <c r="B535" s="64"/>
+      <c r="A535" s="64"/>
+      <c r="B535" s="65"/>
       <c r="C535" s="34"/>
       <c r="D535" s="34"/>
       <c r="E535" s="34"/>
@@ -38250,8 +38393,8 @@
       </c>
     </row>
     <row r="536">
-      <c r="A536" s="63"/>
-      <c r="B536" s="64"/>
+      <c r="A536" s="64"/>
+      <c r="B536" s="65"/>
       <c r="C536" s="34"/>
       <c r="D536" s="34"/>
       <c r="E536" s="34"/>
@@ -38276,8 +38419,8 @@
       </c>
     </row>
     <row r="537">
-      <c r="A537" s="63"/>
-      <c r="B537" s="64"/>
+      <c r="A537" s="64"/>
+      <c r="B537" s="65"/>
       <c r="C537" s="34"/>
       <c r="D537" s="34"/>
       <c r="E537" s="34"/>
@@ -38302,8 +38445,8 @@
       </c>
     </row>
     <row r="538">
-      <c r="A538" s="63"/>
-      <c r="B538" s="64"/>
+      <c r="A538" s="64"/>
+      <c r="B538" s="65"/>
       <c r="C538" s="34"/>
       <c r="D538" s="34"/>
       <c r="E538" s="34"/>
@@ -38328,8 +38471,8 @@
       </c>
     </row>
     <row r="539">
-      <c r="A539" s="63"/>
-      <c r="B539" s="64"/>
+      <c r="A539" s="64"/>
+      <c r="B539" s="65"/>
       <c r="C539" s="34"/>
       <c r="D539" s="34"/>
       <c r="E539" s="34"/>
@@ -38354,8 +38497,8 @@
       </c>
     </row>
     <row r="540">
-      <c r="A540" s="63"/>
-      <c r="B540" s="64"/>
+      <c r="A540" s="64"/>
+      <c r="B540" s="65"/>
       <c r="C540" s="34"/>
       <c r="D540" s="34"/>
       <c r="E540" s="34"/>
@@ -38380,8 +38523,8 @@
       </c>
     </row>
     <row r="541">
-      <c r="A541" s="63"/>
-      <c r="B541" s="64"/>
+      <c r="A541" s="64"/>
+      <c r="B541" s="65"/>
       <c r="C541" s="34"/>
       <c r="D541" s="34"/>
       <c r="E541" s="34"/>
@@ -38406,8 +38549,8 @@
       </c>
     </row>
     <row r="542">
-      <c r="A542" s="63"/>
-      <c r="B542" s="64"/>
+      <c r="A542" s="64"/>
+      <c r="B542" s="65"/>
       <c r="C542" s="34"/>
       <c r="D542" s="34"/>
       <c r="E542" s="34"/>
@@ -38432,8 +38575,8 @@
       </c>
     </row>
     <row r="543">
-      <c r="A543" s="63"/>
-      <c r="B543" s="64"/>
+      <c r="A543" s="64"/>
+      <c r="B543" s="65"/>
       <c r="C543" s="34"/>
       <c r="D543" s="34"/>
       <c r="E543" s="34"/>
@@ -38458,8 +38601,8 @@
       </c>
     </row>
     <row r="544">
-      <c r="A544" s="63"/>
-      <c r="B544" s="64"/>
+      <c r="A544" s="64"/>
+      <c r="B544" s="65"/>
       <c r="C544" s="34"/>
       <c r="D544" s="34"/>
       <c r="E544" s="34"/>
@@ -38484,8 +38627,8 @@
       </c>
     </row>
     <row r="545">
-      <c r="A545" s="63"/>
-      <c r="B545" s="64"/>
+      <c r="A545" s="64"/>
+      <c r="B545" s="65"/>
       <c r="C545" s="34"/>
       <c r="D545" s="34"/>
       <c r="E545" s="34"/>
@@ -38510,8 +38653,8 @@
       </c>
     </row>
     <row r="546">
-      <c r="A546" s="63"/>
-      <c r="B546" s="64"/>
+      <c r="A546" s="64"/>
+      <c r="B546" s="65"/>
       <c r="C546" s="34"/>
       <c r="D546" s="34"/>
       <c r="E546" s="34"/>
@@ -38536,8 +38679,8 @@
       </c>
     </row>
     <row r="547">
-      <c r="A547" s="63"/>
-      <c r="B547" s="64"/>
+      <c r="A547" s="64"/>
+      <c r="B547" s="65"/>
       <c r="C547" s="34"/>
       <c r="D547" s="34"/>
       <c r="E547" s="34"/>
@@ -38562,8 +38705,8 @@
       </c>
     </row>
     <row r="548">
-      <c r="A548" s="63"/>
-      <c r="B548" s="64"/>
+      <c r="A548" s="64"/>
+      <c r="B548" s="65"/>
       <c r="C548" s="34"/>
       <c r="D548" s="34"/>
       <c r="E548" s="34"/>
@@ -38588,8 +38731,8 @@
       </c>
     </row>
     <row r="549">
-      <c r="A549" s="63"/>
-      <c r="B549" s="64"/>
+      <c r="A549" s="64"/>
+      <c r="B549" s="65"/>
       <c r="C549" s="34"/>
       <c r="D549" s="34"/>
       <c r="E549" s="34"/>
@@ -38614,8 +38757,8 @@
       </c>
     </row>
     <row r="550">
-      <c r="A550" s="63"/>
-      <c r="B550" s="64"/>
+      <c r="A550" s="64"/>
+      <c r="B550" s="65"/>
       <c r="C550" s="34"/>
       <c r="D550" s="34"/>
       <c r="E550" s="34"/>
@@ -38640,8 +38783,8 @@
       </c>
     </row>
     <row r="551">
-      <c r="A551" s="63"/>
-      <c r="B551" s="64"/>
+      <c r="A551" s="64"/>
+      <c r="B551" s="65"/>
       <c r="C551" s="34"/>
       <c r="D551" s="34"/>
       <c r="E551" s="34"/>
@@ -39064,15 +39207,18 @@
     <hyperlink r:id="rId71" ref="S509"/>
     <hyperlink r:id="rId72" ref="S510"/>
     <hyperlink r:id="rId73" ref="S511"/>
+    <hyperlink r:id="rId74" ref="S512"/>
+    <hyperlink r:id="rId75" ref="S513"/>
+    <hyperlink r:id="rId76" ref="S514"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId74"/>
-  <legacyDrawing r:id="rId75"/>
+  <drawing r:id="rId77"/>
+  <legacyDrawing r:id="rId78"/>
   <tableParts count="2">
-    <tablePart r:id="rId78"/>
-    <tablePart r:id="rId79"/>
+    <tablePart r:id="rId81"/>
+    <tablePart r:id="rId82"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201001
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -563,7 +563,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5658" uniqueCount="1885">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5671" uniqueCount="1891">
   <si>
     <t>案例</t>
   </si>
@@ -6972,6 +6972,29 @@
   <si>
     <t>於當地就醫並診斷為胃潰瘍</t>
   </si>
+  <si>
+    <t>#514</t>
+  </si>
+  <si>
+    <t>-9/11 法國→台灣</t>
+  </si>
+  <si>
+    <t>9/11 採檢
+9/28 自費檢驗
+9/30 確診</t>
+  </si>
+  <si>
+    <t>自費檢驗</t>
+  </si>
+  <si>
+    <t>持有登機前3日內檢驗陰性報告，入境迄今無疑似症狀
+於今(2020)年9月11日入境後，直接前往防疫旅館進行居家檢疫
+居家檢疫期滿後至9月26日於飯店進行自主健康管理
+9月28日由公司安排自費檢驗，於今日確診</t>
+  </si>
+  <si>
+    <t>國內新增1例境外移入COVID-19個案，為法國籍製造業技師</t>
+  </si>
 </sst>
 </file>
 
@@ -6981,7 +7004,7 @@
     <numFmt numFmtId="164" formatCode="mm&quot;月&quot;dd&quot;日 &quot;dddd"/>
     <numFmt numFmtId="165" formatCode="m/d"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -7059,6 +7082,9 @@
       <color rgb="FF1155CC"/>
     </font>
     <font/>
+    <font>
+      <color rgb="FF000000"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -7104,7 +7130,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="71">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -7295,6 +7321,21 @@
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -37847,34 +37888,64 @@
       </c>
     </row>
     <row r="515">
-      <c r="A515" s="64"/>
-      <c r="B515" s="65"/>
-      <c r="C515" s="34"/>
-      <c r="D515" s="34"/>
-      <c r="E515" s="34"/>
+      <c r="A515" s="64" t="s">
+        <v>1885</v>
+      </c>
+      <c r="B515" s="6">
+        <v>44104.0</v>
+      </c>
+      <c r="C515" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D515" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="E515" s="7" t="s">
+        <v>351</v>
+      </c>
       <c r="F515" s="34"/>
-      <c r="G515" s="34"/>
-      <c r="H515" s="21"/>
-      <c r="I515" s="19"/>
-      <c r="J515" s="10"/>
-      <c r="K515" s="22"/>
-      <c r="L515" s="23"/>
-      <c r="M515" s="22"/>
+      <c r="G515" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H515" s="63" t="s">
+        <v>1886</v>
+      </c>
+      <c r="I515" s="66">
+        <v>44085.0</v>
+      </c>
+      <c r="J515" s="67" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K515" s="68" t="s">
+        <v>1887</v>
+      </c>
+      <c r="L515" s="12" t="s">
+        <v>1888</v>
+      </c>
+      <c r="M515" s="68" t="s">
+        <v>1442</v>
+      </c>
       <c r="N515" s="25"/>
-      <c r="O515" s="21"/>
-      <c r="P515" s="21"/>
+      <c r="O515" s="63" t="s">
+        <v>85</v>
+      </c>
+      <c r="P515" s="63" t="s">
+        <v>1889</v>
+      </c>
       <c r="Q515" s="19"/>
       <c r="R515" s="19"/>
-      <c r="S515" s="20"/>
+      <c r="S515" s="61" t="s">
+        <v>1890</v>
+      </c>
       <c r="T515" s="20"/>
       <c r="U515" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#514</v>
       </c>
     </row>
     <row r="516">
-      <c r="A516" s="64"/>
-      <c r="B516" s="65"/>
+      <c r="A516" s="69"/>
+      <c r="B516" s="70"/>
       <c r="C516" s="34"/>
       <c r="D516" s="34"/>
       <c r="E516" s="34"/>
@@ -37899,8 +37970,8 @@
       </c>
     </row>
     <row r="517">
-      <c r="A517" s="64"/>
-      <c r="B517" s="65"/>
+      <c r="A517" s="69"/>
+      <c r="B517" s="70"/>
       <c r="C517" s="34"/>
       <c r="D517" s="34"/>
       <c r="E517" s="34"/>
@@ -37925,8 +37996,8 @@
       </c>
     </row>
     <row r="518">
-      <c r="A518" s="64"/>
-      <c r="B518" s="65"/>
+      <c r="A518" s="69"/>
+      <c r="B518" s="70"/>
       <c r="C518" s="34"/>
       <c r="D518" s="34"/>
       <c r="E518" s="34"/>
@@ -37951,8 +38022,8 @@
       </c>
     </row>
     <row r="519">
-      <c r="A519" s="64"/>
-      <c r="B519" s="65"/>
+      <c r="A519" s="69"/>
+      <c r="B519" s="70"/>
       <c r="C519" s="34"/>
       <c r="D519" s="34"/>
       <c r="E519" s="34"/>
@@ -37977,8 +38048,8 @@
       </c>
     </row>
     <row r="520">
-      <c r="A520" s="64"/>
-      <c r="B520" s="65"/>
+      <c r="A520" s="69"/>
+      <c r="B520" s="70"/>
       <c r="C520" s="34"/>
       <c r="D520" s="34"/>
       <c r="E520" s="34"/>
@@ -38003,8 +38074,8 @@
       </c>
     </row>
     <row r="521">
-      <c r="A521" s="64"/>
-      <c r="B521" s="65"/>
+      <c r="A521" s="69"/>
+      <c r="B521" s="70"/>
       <c r="C521" s="34"/>
       <c r="D521" s="34"/>
       <c r="E521" s="34"/>
@@ -38029,8 +38100,8 @@
       </c>
     </row>
     <row r="522">
-      <c r="A522" s="64"/>
-      <c r="B522" s="65"/>
+      <c r="A522" s="69"/>
+      <c r="B522" s="70"/>
       <c r="C522" s="34"/>
       <c r="D522" s="34"/>
       <c r="E522" s="34"/>
@@ -38055,8 +38126,8 @@
       </c>
     </row>
     <row r="523">
-      <c r="A523" s="64"/>
-      <c r="B523" s="65"/>
+      <c r="A523" s="69"/>
+      <c r="B523" s="70"/>
       <c r="C523" s="34"/>
       <c r="D523" s="34"/>
       <c r="E523" s="34"/>
@@ -38081,8 +38152,8 @@
       </c>
     </row>
     <row r="524">
-      <c r="A524" s="64"/>
-      <c r="B524" s="65"/>
+      <c r="A524" s="69"/>
+      <c r="B524" s="70"/>
       <c r="C524" s="34"/>
       <c r="D524" s="34"/>
       <c r="E524" s="34"/>
@@ -38107,8 +38178,8 @@
       </c>
     </row>
     <row r="525">
-      <c r="A525" s="64"/>
-      <c r="B525" s="65"/>
+      <c r="A525" s="69"/>
+      <c r="B525" s="70"/>
       <c r="C525" s="34"/>
       <c r="D525" s="34"/>
       <c r="E525" s="34"/>
@@ -38133,8 +38204,8 @@
       </c>
     </row>
     <row r="526">
-      <c r="A526" s="64"/>
-      <c r="B526" s="65"/>
+      <c r="A526" s="69"/>
+      <c r="B526" s="70"/>
       <c r="C526" s="34"/>
       <c r="D526" s="34"/>
       <c r="E526" s="34"/>
@@ -38159,8 +38230,8 @@
       </c>
     </row>
     <row r="527">
-      <c r="A527" s="64"/>
-      <c r="B527" s="65"/>
+      <c r="A527" s="69"/>
+      <c r="B527" s="70"/>
       <c r="C527" s="34"/>
       <c r="D527" s="34"/>
       <c r="E527" s="34"/>
@@ -38185,8 +38256,8 @@
       </c>
     </row>
     <row r="528">
-      <c r="A528" s="64"/>
-      <c r="B528" s="65"/>
+      <c r="A528" s="69"/>
+      <c r="B528" s="70"/>
       <c r="C528" s="34"/>
       <c r="D528" s="34"/>
       <c r="E528" s="34"/>
@@ -38211,8 +38282,8 @@
       </c>
     </row>
     <row r="529">
-      <c r="A529" s="64"/>
-      <c r="B529" s="65"/>
+      <c r="A529" s="69"/>
+      <c r="B529" s="70"/>
       <c r="C529" s="34"/>
       <c r="D529" s="34"/>
       <c r="E529" s="34"/>
@@ -38237,8 +38308,8 @@
       </c>
     </row>
     <row r="530">
-      <c r="A530" s="64"/>
-      <c r="B530" s="65"/>
+      <c r="A530" s="69"/>
+      <c r="B530" s="70"/>
       <c r="C530" s="34"/>
       <c r="D530" s="34"/>
       <c r="E530" s="34"/>
@@ -38263,8 +38334,8 @@
       </c>
     </row>
     <row r="531">
-      <c r="A531" s="64"/>
-      <c r="B531" s="65"/>
+      <c r="A531" s="69"/>
+      <c r="B531" s="70"/>
       <c r="C531" s="34"/>
       <c r="D531" s="34"/>
       <c r="E531" s="34"/>
@@ -38289,8 +38360,8 @@
       </c>
     </row>
     <row r="532">
-      <c r="A532" s="64"/>
-      <c r="B532" s="65"/>
+      <c r="A532" s="69"/>
+      <c r="B532" s="70"/>
       <c r="C532" s="34"/>
       <c r="D532" s="34"/>
       <c r="E532" s="34"/>
@@ -38315,8 +38386,8 @@
       </c>
     </row>
     <row r="533">
-      <c r="A533" s="64"/>
-      <c r="B533" s="65"/>
+      <c r="A533" s="69"/>
+      <c r="B533" s="70"/>
       <c r="C533" s="34"/>
       <c r="D533" s="34"/>
       <c r="E533" s="34"/>
@@ -38341,8 +38412,8 @@
       </c>
     </row>
     <row r="534">
-      <c r="A534" s="64"/>
-      <c r="B534" s="65"/>
+      <c r="A534" s="69"/>
+      <c r="B534" s="70"/>
       <c r="C534" s="34"/>
       <c r="D534" s="34"/>
       <c r="E534" s="34"/>
@@ -38367,8 +38438,8 @@
       </c>
     </row>
     <row r="535">
-      <c r="A535" s="64"/>
-      <c r="B535" s="65"/>
+      <c r="A535" s="69"/>
+      <c r="B535" s="70"/>
       <c r="C535" s="34"/>
       <c r="D535" s="34"/>
       <c r="E535" s="34"/>
@@ -38393,8 +38464,8 @@
       </c>
     </row>
     <row r="536">
-      <c r="A536" s="64"/>
-      <c r="B536" s="65"/>
+      <c r="A536" s="69"/>
+      <c r="B536" s="70"/>
       <c r="C536" s="34"/>
       <c r="D536" s="34"/>
       <c r="E536" s="34"/>
@@ -38419,8 +38490,8 @@
       </c>
     </row>
     <row r="537">
-      <c r="A537" s="64"/>
-      <c r="B537" s="65"/>
+      <c r="A537" s="69"/>
+      <c r="B537" s="70"/>
       <c r="C537" s="34"/>
       <c r="D537" s="34"/>
       <c r="E537" s="34"/>
@@ -38445,8 +38516,8 @@
       </c>
     </row>
     <row r="538">
-      <c r="A538" s="64"/>
-      <c r="B538" s="65"/>
+      <c r="A538" s="69"/>
+      <c r="B538" s="70"/>
       <c r="C538" s="34"/>
       <c r="D538" s="34"/>
       <c r="E538" s="34"/>
@@ -38471,8 +38542,8 @@
       </c>
     </row>
     <row r="539">
-      <c r="A539" s="64"/>
-      <c r="B539" s="65"/>
+      <c r="A539" s="69"/>
+      <c r="B539" s="70"/>
       <c r="C539" s="34"/>
       <c r="D539" s="34"/>
       <c r="E539" s="34"/>
@@ -38497,8 +38568,8 @@
       </c>
     </row>
     <row r="540">
-      <c r="A540" s="64"/>
-      <c r="B540" s="65"/>
+      <c r="A540" s="69"/>
+      <c r="B540" s="70"/>
       <c r="C540" s="34"/>
       <c r="D540" s="34"/>
       <c r="E540" s="34"/>
@@ -38523,8 +38594,8 @@
       </c>
     </row>
     <row r="541">
-      <c r="A541" s="64"/>
-      <c r="B541" s="65"/>
+      <c r="A541" s="69"/>
+      <c r="B541" s="70"/>
       <c r="C541" s="34"/>
       <c r="D541" s="34"/>
       <c r="E541" s="34"/>
@@ -38549,8 +38620,8 @@
       </c>
     </row>
     <row r="542">
-      <c r="A542" s="64"/>
-      <c r="B542" s="65"/>
+      <c r="A542" s="69"/>
+      <c r="B542" s="70"/>
       <c r="C542" s="34"/>
       <c r="D542" s="34"/>
       <c r="E542" s="34"/>
@@ -38575,8 +38646,8 @@
       </c>
     </row>
     <row r="543">
-      <c r="A543" s="64"/>
-      <c r="B543" s="65"/>
+      <c r="A543" s="69"/>
+      <c r="B543" s="70"/>
       <c r="C543" s="34"/>
       <c r="D543" s="34"/>
       <c r="E543" s="34"/>
@@ -38601,8 +38672,8 @@
       </c>
     </row>
     <row r="544">
-      <c r="A544" s="64"/>
-      <c r="B544" s="65"/>
+      <c r="A544" s="69"/>
+      <c r="B544" s="70"/>
       <c r="C544" s="34"/>
       <c r="D544" s="34"/>
       <c r="E544" s="34"/>
@@ -38627,8 +38698,8 @@
       </c>
     </row>
     <row r="545">
-      <c r="A545" s="64"/>
-      <c r="B545" s="65"/>
+      <c r="A545" s="69"/>
+      <c r="B545" s="70"/>
       <c r="C545" s="34"/>
       <c r="D545" s="34"/>
       <c r="E545" s="34"/>
@@ -38653,8 +38724,8 @@
       </c>
     </row>
     <row r="546">
-      <c r="A546" s="64"/>
-      <c r="B546" s="65"/>
+      <c r="A546" s="69"/>
+      <c r="B546" s="70"/>
       <c r="C546" s="34"/>
       <c r="D546" s="34"/>
       <c r="E546" s="34"/>
@@ -38679,8 +38750,8 @@
       </c>
     </row>
     <row r="547">
-      <c r="A547" s="64"/>
-      <c r="B547" s="65"/>
+      <c r="A547" s="69"/>
+      <c r="B547" s="70"/>
       <c r="C547" s="34"/>
       <c r="D547" s="34"/>
       <c r="E547" s="34"/>
@@ -38705,8 +38776,8 @@
       </c>
     </row>
     <row r="548">
-      <c r="A548" s="64"/>
-      <c r="B548" s="65"/>
+      <c r="A548" s="69"/>
+      <c r="B548" s="70"/>
       <c r="C548" s="34"/>
       <c r="D548" s="34"/>
       <c r="E548" s="34"/>
@@ -38731,8 +38802,8 @@
       </c>
     </row>
     <row r="549">
-      <c r="A549" s="64"/>
-      <c r="B549" s="65"/>
+      <c r="A549" s="69"/>
+      <c r="B549" s="70"/>
       <c r="C549" s="34"/>
       <c r="D549" s="34"/>
       <c r="E549" s="34"/>
@@ -38757,8 +38828,8 @@
       </c>
     </row>
     <row r="550">
-      <c r="A550" s="64"/>
-      <c r="B550" s="65"/>
+      <c r="A550" s="69"/>
+      <c r="B550" s="70"/>
       <c r="C550" s="34"/>
       <c r="D550" s="34"/>
       <c r="E550" s="34"/>
@@ -38783,8 +38854,8 @@
       </c>
     </row>
     <row r="551">
-      <c r="A551" s="64"/>
-      <c r="B551" s="65"/>
+      <c r="A551" s="69"/>
+      <c r="B551" s="70"/>
       <c r="C551" s="34"/>
       <c r="D551" s="34"/>
       <c r="E551" s="34"/>
@@ -39210,15 +39281,16 @@
     <hyperlink r:id="rId74" ref="S512"/>
     <hyperlink r:id="rId75" ref="S513"/>
     <hyperlink r:id="rId76" ref="S514"/>
+    <hyperlink r:id="rId77" ref="S515"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId77"/>
-  <legacyDrawing r:id="rId78"/>
+  <drawing r:id="rId78"/>
+  <legacyDrawing r:id="rId79"/>
   <tableParts count="2">
-    <tablePart r:id="rId81"/>
     <tablePart r:id="rId82"/>
+    <tablePart r:id="rId83"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201002
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -563,7 +563,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5671" uniqueCount="1891">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5683" uniqueCount="1896">
   <si>
     <t>案例</t>
   </si>
@@ -6994,6 +6994,23 @@
   </si>
   <si>
     <t>國內新增1例境外移入COVID-19個案，為法國籍製造業技師</t>
+  </si>
+  <si>
+    <t>#515</t>
+  </si>
+  <si>
+    <t>2019/6月-2020/9/29 印尼</t>
+  </si>
+  <si>
+    <t>9/29 採檢
+10/1 確診</t>
+  </si>
+  <si>
+    <t>個案與家人長期居住印尼
+登機前無不適症狀，個案因途中出現喉嚨痛及輕微咳嗽症狀，且其父親9月25日於當地確診</t>
+  </si>
+  <si>
+    <t>男子自印尼返台，返國入境採檢確診</t>
   </si>
 </sst>
 </file>
@@ -37944,29 +37961,57 @@
       </c>
     </row>
     <row r="516">
-      <c r="A516" s="69"/>
-      <c r="B516" s="70"/>
-      <c r="C516" s="34"/>
-      <c r="D516" s="34"/>
-      <c r="E516" s="34"/>
+      <c r="A516" s="64" t="s">
+        <v>1891</v>
+      </c>
+      <c r="B516" s="6">
+        <v>44105.0</v>
+      </c>
+      <c r="C516" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D516" s="65" t="s">
+        <v>59</v>
+      </c>
+      <c r="E516" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F516" s="34"/>
-      <c r="G516" s="34"/>
-      <c r="H516" s="21"/>
-      <c r="I516" s="19"/>
+      <c r="G516" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H516" s="63" t="s">
+        <v>1892</v>
+      </c>
+      <c r="I516" s="66">
+        <v>44103.0</v>
+      </c>
       <c r="J516" s="10"/>
-      <c r="K516" s="22"/>
-      <c r="L516" s="23"/>
-      <c r="M516" s="22"/>
+      <c r="K516" s="68" t="s">
+        <v>1893</v>
+      </c>
+      <c r="L516" s="67" t="s">
+        <v>363</v>
+      </c>
+      <c r="M516" s="68" t="s">
+        <v>388</v>
+      </c>
       <c r="N516" s="25"/>
-      <c r="O516" s="21"/>
-      <c r="P516" s="21"/>
+      <c r="O516" s="63" t="s">
+        <v>85</v>
+      </c>
+      <c r="P516" s="63" t="s">
+        <v>1894</v>
+      </c>
       <c r="Q516" s="19"/>
       <c r="R516" s="19"/>
-      <c r="S516" s="20"/>
+      <c r="S516" s="61" t="s">
+        <v>1895</v>
+      </c>
       <c r="T516" s="20"/>
       <c r="U516" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#515</v>
       </c>
     </row>
     <row r="517">
@@ -39282,15 +39327,16 @@
     <hyperlink r:id="rId75" ref="S513"/>
     <hyperlink r:id="rId76" ref="S514"/>
     <hyperlink r:id="rId77" ref="S515"/>
+    <hyperlink r:id="rId78" ref="S516"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId78"/>
-  <legacyDrawing r:id="rId79"/>
+  <drawing r:id="rId79"/>
+  <legacyDrawing r:id="rId80"/>
   <tableParts count="2">
-    <tablePart r:id="rId82"/>
     <tablePart r:id="rId83"/>
+    <tablePart r:id="rId84"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201003
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -563,7 +563,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5683" uniqueCount="1896">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5707" uniqueCount="1907">
   <si>
     <t>案例</t>
   </si>
@@ -7011,6 +7011,45 @@
   </si>
   <si>
     <t>男子自印尼返台，返國入境採檢確診</t>
+  </si>
+  <si>
+    <t>#516</t>
+  </si>
+  <si>
+    <t>-9/20 美國</t>
+  </si>
+  <si>
+    <t>9/20 採檢
+9/30 二採
+10/2 確診</t>
+  </si>
+  <si>
+    <t>發燒 嗅覺喪失 乾咳</t>
+  </si>
+  <si>
+    <t>長年於美國工作
+入境時無不適症狀，主動告知在美國當地曾接觸確診者，且於8月28日出現發燒、嗅覺消失及乾咳等症狀，
+由機場檢疫人員安排採檢結果為陰性後持續居家檢疫
+個案9月24日至30日出現乾咳症狀，由衛生單位協助安排送醫採檢，於今日確診</t>
+  </si>
+  <si>
+    <t>國內新增2例境外移入COVID-19確診，分別自美國及日本入境</t>
+  </si>
+  <si>
+    <t>#517</t>
+  </si>
+  <si>
+    <t>1月-9/30 日本</t>
+  </si>
+  <si>
+    <t>9/30 採檢
+10/2 確診</t>
+  </si>
+  <si>
+    <t>輕微腹瀉 肌肉 痠痛 鼻塞 發燒 咳嗽 嗅覺異常</t>
+  </si>
+  <si>
+    <t>曾於當地二次就醫，被診斷為感冒、病毒性感染，皆開立藥物返家休養</t>
   </si>
 </sst>
 </file>
@@ -38015,55 +38054,115 @@
       </c>
     </row>
     <row r="517">
-      <c r="A517" s="69"/>
-      <c r="B517" s="70"/>
-      <c r="C517" s="34"/>
-      <c r="D517" s="34"/>
-      <c r="E517" s="34"/>
+      <c r="A517" s="64" t="s">
+        <v>1896</v>
+      </c>
+      <c r="B517" s="6">
+        <v>44106.0</v>
+      </c>
+      <c r="C517" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D517" s="65" t="s">
+        <v>116</v>
+      </c>
+      <c r="E517" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F517" s="34"/>
-      <c r="G517" s="34"/>
-      <c r="H517" s="21"/>
-      <c r="I517" s="19"/>
-      <c r="J517" s="10"/>
-      <c r="K517" s="22"/>
-      <c r="L517" s="23"/>
-      <c r="M517" s="22"/>
+      <c r="G517" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H517" s="63" t="s">
+        <v>1897</v>
+      </c>
+      <c r="I517" s="66">
+        <v>44094.0</v>
+      </c>
+      <c r="J517" s="10">
+        <v>44071.0</v>
+      </c>
+      <c r="K517" s="68" t="s">
+        <v>1898</v>
+      </c>
+      <c r="L517" s="67" t="s">
+        <v>426</v>
+      </c>
+      <c r="M517" s="68" t="s">
+        <v>1899</v>
+      </c>
       <c r="N517" s="25"/>
-      <c r="O517" s="21"/>
-      <c r="P517" s="21"/>
+      <c r="O517" s="63" t="s">
+        <v>85</v>
+      </c>
+      <c r="P517" s="63" t="s">
+        <v>1900</v>
+      </c>
       <c r="Q517" s="19"/>
       <c r="R517" s="19"/>
-      <c r="S517" s="20"/>
+      <c r="S517" s="61" t="s">
+        <v>1901</v>
+      </c>
       <c r="T517" s="20"/>
       <c r="U517" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#516</v>
       </c>
     </row>
     <row r="518">
-      <c r="A518" s="69"/>
-      <c r="B518" s="70"/>
-      <c r="C518" s="34"/>
-      <c r="D518" s="34"/>
-      <c r="E518" s="34"/>
+      <c r="A518" s="64" t="s">
+        <v>1902</v>
+      </c>
+      <c r="B518" s="6">
+        <v>44106.0</v>
+      </c>
+      <c r="C518" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D518" s="65" t="s">
+        <v>59</v>
+      </c>
+      <c r="E518" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F518" s="34"/>
-      <c r="G518" s="34"/>
-      <c r="H518" s="21"/>
-      <c r="I518" s="19"/>
-      <c r="J518" s="10"/>
-      <c r="K518" s="22"/>
-      <c r="L518" s="23"/>
-      <c r="M518" s="22"/>
+      <c r="G518" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H518" s="63" t="s">
+        <v>1903</v>
+      </c>
+      <c r="I518" s="66">
+        <v>44104.0</v>
+      </c>
+      <c r="J518" s="10">
+        <v>44089.0</v>
+      </c>
+      <c r="K518" s="68" t="s">
+        <v>1904</v>
+      </c>
+      <c r="L518" s="67" t="s">
+        <v>363</v>
+      </c>
+      <c r="M518" s="68" t="s">
+        <v>1905</v>
+      </c>
       <c r="N518" s="25"/>
-      <c r="O518" s="21"/>
-      <c r="P518" s="21"/>
+      <c r="O518" s="63" t="s">
+        <v>85</v>
+      </c>
+      <c r="P518" s="63" t="s">
+        <v>1906</v>
+      </c>
       <c r="Q518" s="19"/>
       <c r="R518" s="19"/>
-      <c r="S518" s="20"/>
+      <c r="S518" s="61" t="s">
+        <v>1901</v>
+      </c>
       <c r="T518" s="20"/>
       <c r="U518" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#517</v>
       </c>
     </row>
     <row r="519">
@@ -39328,15 +39427,17 @@
     <hyperlink r:id="rId76" ref="S514"/>
     <hyperlink r:id="rId77" ref="S515"/>
     <hyperlink r:id="rId78" ref="S516"/>
+    <hyperlink r:id="rId79" ref="S517"/>
+    <hyperlink r:id="rId80" ref="S518"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId79"/>
-  <legacyDrawing r:id="rId80"/>
+  <drawing r:id="rId81"/>
+  <legacyDrawing r:id="rId82"/>
   <tableParts count="2">
-    <tablePart r:id="rId83"/>
-    <tablePart r:id="rId84"/>
+    <tablePart r:id="rId85"/>
+    <tablePart r:id="rId86"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201004
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -7060,7 +7060,7 @@
     <numFmt numFmtId="164" formatCode="mm&quot;月&quot;dd&quot;日 &quot;dddd"/>
     <numFmt numFmtId="165" formatCode="m/d"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="17">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -7137,10 +7137,6 @@
       <u/>
       <color rgb="FF1155CC"/>
     </font>
-    <font/>
-    <font>
-      <color rgb="FF000000"/>
-    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -7186,7 +7182,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="65">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -7375,24 +7371,6 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
@@ -35389,7 +35367,7 @@
       <c r="G469" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H469" s="63" t="s">
+      <c r="H469" s="8" t="s">
         <v>1664</v>
       </c>
       <c r="I469" s="9">
@@ -35447,7 +35425,7 @@
       <c r="G470" s="7" t="s">
         <v>1670</v>
       </c>
-      <c r="H470" s="63" t="s">
+      <c r="H470" s="8" t="s">
         <v>1671</v>
       </c>
       <c r="I470" s="9">
@@ -35503,7 +35481,7 @@
       <c r="G471" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H471" s="63" t="s">
+      <c r="H471" s="8" t="s">
         <v>1677</v>
       </c>
       <c r="I471" s="9">
@@ -35673,7 +35651,7 @@
       <c r="G474" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H474" s="63" t="s">
+      <c r="H474" s="8" t="s">
         <v>1692</v>
       </c>
       <c r="I474" s="9">
@@ -35785,7 +35763,7 @@
       <c r="G476" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H476" s="63" t="s">
+      <c r="H476" s="8" t="s">
         <v>1700</v>
       </c>
       <c r="I476" s="9">
@@ -36567,7 +36545,7 @@
       <c r="G490" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H490" s="63" t="s">
+      <c r="H490" s="8" t="s">
         <v>1765</v>
       </c>
       <c r="I490" s="9">
@@ -37944,7 +37922,7 @@
       </c>
     </row>
     <row r="515">
-      <c r="A515" s="64" t="s">
+      <c r="A515" s="16" t="s">
         <v>1885</v>
       </c>
       <c r="B515" s="6">
@@ -37953,7 +37931,7 @@
       <c r="C515" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D515" s="65" t="s">
+      <c r="D515" s="7" t="s">
         <v>22</v>
       </c>
       <c r="E515" s="7" t="s">
@@ -37963,29 +37941,29 @@
       <c r="G515" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H515" s="63" t="s">
+      <c r="H515" s="8" t="s">
         <v>1886</v>
       </c>
-      <c r="I515" s="66">
+      <c r="I515" s="9">
         <v>44085.0</v>
       </c>
-      <c r="J515" s="67" t="s">
+      <c r="J515" s="12" t="s">
         <v>1442</v>
       </c>
-      <c r="K515" s="68" t="s">
+      <c r="K515" s="13" t="s">
         <v>1887</v>
       </c>
       <c r="L515" s="12" t="s">
         <v>1888</v>
       </c>
-      <c r="M515" s="68" t="s">
+      <c r="M515" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N515" s="25"/>
-      <c r="O515" s="63" t="s">
+      <c r="O515" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P515" s="63" t="s">
+      <c r="P515" s="8" t="s">
         <v>1889</v>
       </c>
       <c r="Q515" s="19"/>
@@ -38000,7 +37978,7 @@
       </c>
     </row>
     <row r="516">
-      <c r="A516" s="64" t="s">
+      <c r="A516" s="16" t="s">
         <v>1891</v>
       </c>
       <c r="B516" s="6">
@@ -38009,7 +37987,7 @@
       <c r="C516" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D516" s="65" t="s">
+      <c r="D516" s="7" t="s">
         <v>59</v>
       </c>
       <c r="E516" s="7" t="s">
@@ -38019,27 +37997,27 @@
       <c r="G516" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H516" s="63" t="s">
+      <c r="H516" s="8" t="s">
         <v>1892</v>
       </c>
-      <c r="I516" s="66">
+      <c r="I516" s="9">
         <v>44103.0</v>
       </c>
       <c r="J516" s="10"/>
-      <c r="K516" s="68" t="s">
+      <c r="K516" s="13" t="s">
         <v>1893</v>
       </c>
-      <c r="L516" s="67" t="s">
+      <c r="L516" s="12" t="s">
         <v>363</v>
       </c>
-      <c r="M516" s="68" t="s">
+      <c r="M516" s="13" t="s">
         <v>388</v>
       </c>
       <c r="N516" s="25"/>
-      <c r="O516" s="63" t="s">
+      <c r="O516" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P516" s="63" t="s">
+      <c r="P516" s="8" t="s">
         <v>1894</v>
       </c>
       <c r="Q516" s="19"/>
@@ -38054,7 +38032,7 @@
       </c>
     </row>
     <row r="517">
-      <c r="A517" s="64" t="s">
+      <c r="A517" s="16" t="s">
         <v>1896</v>
       </c>
       <c r="B517" s="6">
@@ -38063,7 +38041,7 @@
       <c r="C517" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D517" s="65" t="s">
+      <c r="D517" s="7" t="s">
         <v>116</v>
       </c>
       <c r="E517" s="7" t="s">
@@ -38073,29 +38051,29 @@
       <c r="G517" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H517" s="63" t="s">
+      <c r="H517" s="8" t="s">
         <v>1897</v>
       </c>
-      <c r="I517" s="66">
+      <c r="I517" s="9">
         <v>44094.0</v>
       </c>
       <c r="J517" s="10">
         <v>44071.0</v>
       </c>
-      <c r="K517" s="68" t="s">
+      <c r="K517" s="13" t="s">
         <v>1898</v>
       </c>
-      <c r="L517" s="67" t="s">
+      <c r="L517" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M517" s="68" t="s">
+      <c r="M517" s="13" t="s">
         <v>1899</v>
       </c>
       <c r="N517" s="25"/>
-      <c r="O517" s="63" t="s">
+      <c r="O517" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P517" s="63" t="s">
+      <c r="P517" s="8" t="s">
         <v>1900</v>
       </c>
       <c r="Q517" s="19"/>
@@ -38110,7 +38088,7 @@
       </c>
     </row>
     <row r="518">
-      <c r="A518" s="64" t="s">
+      <c r="A518" s="16" t="s">
         <v>1902</v>
       </c>
       <c r="B518" s="6">
@@ -38119,7 +38097,7 @@
       <c r="C518" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D518" s="65" t="s">
+      <c r="D518" s="7" t="s">
         <v>59</v>
       </c>
       <c r="E518" s="7" t="s">
@@ -38129,29 +38107,29 @@
       <c r="G518" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H518" s="63" t="s">
+      <c r="H518" s="8" t="s">
         <v>1903</v>
       </c>
-      <c r="I518" s="66">
+      <c r="I518" s="9">
         <v>44104.0</v>
       </c>
       <c r="J518" s="10">
         <v>44089.0</v>
       </c>
-      <c r="K518" s="68" t="s">
+      <c r="K518" s="13" t="s">
         <v>1904</v>
       </c>
-      <c r="L518" s="67" t="s">
+      <c r="L518" s="12" t="s">
         <v>363</v>
       </c>
-      <c r="M518" s="68" t="s">
+      <c r="M518" s="13" t="s">
         <v>1905</v>
       </c>
       <c r="N518" s="25"/>
-      <c r="O518" s="63" t="s">
+      <c r="O518" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P518" s="63" t="s">
+      <c r="P518" s="8" t="s">
         <v>1906</v>
       </c>
       <c r="Q518" s="19"/>
@@ -38166,8 +38144,8 @@
       </c>
     </row>
     <row r="519">
-      <c r="A519" s="69"/>
-      <c r="B519" s="70"/>
+      <c r="A519" s="63"/>
+      <c r="B519" s="64"/>
       <c r="C519" s="34"/>
       <c r="D519" s="34"/>
       <c r="E519" s="34"/>
@@ -38192,8 +38170,8 @@
       </c>
     </row>
     <row r="520">
-      <c r="A520" s="69"/>
-      <c r="B520" s="70"/>
+      <c r="A520" s="63"/>
+      <c r="B520" s="64"/>
       <c r="C520" s="34"/>
       <c r="D520" s="34"/>
       <c r="E520" s="34"/>
@@ -38218,8 +38196,8 @@
       </c>
     </row>
     <row r="521">
-      <c r="A521" s="69"/>
-      <c r="B521" s="70"/>
+      <c r="A521" s="63"/>
+      <c r="B521" s="64"/>
       <c r="C521" s="34"/>
       <c r="D521" s="34"/>
       <c r="E521" s="34"/>
@@ -38244,8 +38222,8 @@
       </c>
     </row>
     <row r="522">
-      <c r="A522" s="69"/>
-      <c r="B522" s="70"/>
+      <c r="A522" s="63"/>
+      <c r="B522" s="64"/>
       <c r="C522" s="34"/>
       <c r="D522" s="34"/>
       <c r="E522" s="34"/>
@@ -38270,8 +38248,8 @@
       </c>
     </row>
     <row r="523">
-      <c r="A523" s="69"/>
-      <c r="B523" s="70"/>
+      <c r="A523" s="63"/>
+      <c r="B523" s="64"/>
       <c r="C523" s="34"/>
       <c r="D523" s="34"/>
       <c r="E523" s="34"/>
@@ -38296,8 +38274,8 @@
       </c>
     </row>
     <row r="524">
-      <c r="A524" s="69"/>
-      <c r="B524" s="70"/>
+      <c r="A524" s="63"/>
+      <c r="B524" s="64"/>
       <c r="C524" s="34"/>
       <c r="D524" s="34"/>
       <c r="E524" s="34"/>
@@ -38322,8 +38300,8 @@
       </c>
     </row>
     <row r="525">
-      <c r="A525" s="69"/>
-      <c r="B525" s="70"/>
+      <c r="A525" s="63"/>
+      <c r="B525" s="64"/>
       <c r="C525" s="34"/>
       <c r="D525" s="34"/>
       <c r="E525" s="34"/>
@@ -38348,8 +38326,8 @@
       </c>
     </row>
     <row r="526">
-      <c r="A526" s="69"/>
-      <c r="B526" s="70"/>
+      <c r="A526" s="63"/>
+      <c r="B526" s="64"/>
       <c r="C526" s="34"/>
       <c r="D526" s="34"/>
       <c r="E526" s="34"/>
@@ -38374,8 +38352,8 @@
       </c>
     </row>
     <row r="527">
-      <c r="A527" s="69"/>
-      <c r="B527" s="70"/>
+      <c r="A527" s="63"/>
+      <c r="B527" s="64"/>
       <c r="C527" s="34"/>
       <c r="D527" s="34"/>
       <c r="E527" s="34"/>
@@ -38400,8 +38378,8 @@
       </c>
     </row>
     <row r="528">
-      <c r="A528" s="69"/>
-      <c r="B528" s="70"/>
+      <c r="A528" s="63"/>
+      <c r="B528" s="64"/>
       <c r="C528" s="34"/>
       <c r="D528" s="34"/>
       <c r="E528" s="34"/>
@@ -38426,8 +38404,8 @@
       </c>
     </row>
     <row r="529">
-      <c r="A529" s="69"/>
-      <c r="B529" s="70"/>
+      <c r="A529" s="63"/>
+      <c r="B529" s="64"/>
       <c r="C529" s="34"/>
       <c r="D529" s="34"/>
       <c r="E529" s="34"/>
@@ -38452,8 +38430,8 @@
       </c>
     </row>
     <row r="530">
-      <c r="A530" s="69"/>
-      <c r="B530" s="70"/>
+      <c r="A530" s="63"/>
+      <c r="B530" s="64"/>
       <c r="C530" s="34"/>
       <c r="D530" s="34"/>
       <c r="E530" s="34"/>
@@ -38478,8 +38456,8 @@
       </c>
     </row>
     <row r="531">
-      <c r="A531" s="69"/>
-      <c r="B531" s="70"/>
+      <c r="A531" s="63"/>
+      <c r="B531" s="64"/>
       <c r="C531" s="34"/>
       <c r="D531" s="34"/>
       <c r="E531" s="34"/>
@@ -38504,8 +38482,8 @@
       </c>
     </row>
     <row r="532">
-      <c r="A532" s="69"/>
-      <c r="B532" s="70"/>
+      <c r="A532" s="63"/>
+      <c r="B532" s="64"/>
       <c r="C532" s="34"/>
       <c r="D532" s="34"/>
       <c r="E532" s="34"/>
@@ -38530,8 +38508,8 @@
       </c>
     </row>
     <row r="533">
-      <c r="A533" s="69"/>
-      <c r="B533" s="70"/>
+      <c r="A533" s="63"/>
+      <c r="B533" s="64"/>
       <c r="C533" s="34"/>
       <c r="D533" s="34"/>
       <c r="E533" s="34"/>
@@ -38556,8 +38534,8 @@
       </c>
     </row>
     <row r="534">
-      <c r="A534" s="69"/>
-      <c r="B534" s="70"/>
+      <c r="A534" s="63"/>
+      <c r="B534" s="64"/>
       <c r="C534" s="34"/>
       <c r="D534" s="34"/>
       <c r="E534" s="34"/>
@@ -38582,8 +38560,8 @@
       </c>
     </row>
     <row r="535">
-      <c r="A535" s="69"/>
-      <c r="B535" s="70"/>
+      <c r="A535" s="63"/>
+      <c r="B535" s="64"/>
       <c r="C535" s="34"/>
       <c r="D535" s="34"/>
       <c r="E535" s="34"/>
@@ -38608,8 +38586,8 @@
       </c>
     </row>
     <row r="536">
-      <c r="A536" s="69"/>
-      <c r="B536" s="70"/>
+      <c r="A536" s="63"/>
+      <c r="B536" s="64"/>
       <c r="C536" s="34"/>
       <c r="D536" s="34"/>
       <c r="E536" s="34"/>
@@ -38634,8 +38612,8 @@
       </c>
     </row>
     <row r="537">
-      <c r="A537" s="69"/>
-      <c r="B537" s="70"/>
+      <c r="A537" s="63"/>
+      <c r="B537" s="64"/>
       <c r="C537" s="34"/>
       <c r="D537" s="34"/>
       <c r="E537" s="34"/>
@@ -38660,8 +38638,8 @@
       </c>
     </row>
     <row r="538">
-      <c r="A538" s="69"/>
-      <c r="B538" s="70"/>
+      <c r="A538" s="63"/>
+      <c r="B538" s="64"/>
       <c r="C538" s="34"/>
       <c r="D538" s="34"/>
       <c r="E538" s="34"/>
@@ -38686,8 +38664,8 @@
       </c>
     </row>
     <row r="539">
-      <c r="A539" s="69"/>
-      <c r="B539" s="70"/>
+      <c r="A539" s="63"/>
+      <c r="B539" s="64"/>
       <c r="C539" s="34"/>
       <c r="D539" s="34"/>
       <c r="E539" s="34"/>
@@ -38712,8 +38690,8 @@
       </c>
     </row>
     <row r="540">
-      <c r="A540" s="69"/>
-      <c r="B540" s="70"/>
+      <c r="A540" s="63"/>
+      <c r="B540" s="64"/>
       <c r="C540" s="34"/>
       <c r="D540" s="34"/>
       <c r="E540" s="34"/>
@@ -38738,8 +38716,8 @@
       </c>
     </row>
     <row r="541">
-      <c r="A541" s="69"/>
-      <c r="B541" s="70"/>
+      <c r="A541" s="63"/>
+      <c r="B541" s="64"/>
       <c r="C541" s="34"/>
       <c r="D541" s="34"/>
       <c r="E541" s="34"/>
@@ -38764,8 +38742,8 @@
       </c>
     </row>
     <row r="542">
-      <c r="A542" s="69"/>
-      <c r="B542" s="70"/>
+      <c r="A542" s="63"/>
+      <c r="B542" s="64"/>
       <c r="C542" s="34"/>
       <c r="D542" s="34"/>
       <c r="E542" s="34"/>
@@ -38790,8 +38768,8 @@
       </c>
     </row>
     <row r="543">
-      <c r="A543" s="69"/>
-      <c r="B543" s="70"/>
+      <c r="A543" s="63"/>
+      <c r="B543" s="64"/>
       <c r="C543" s="34"/>
       <c r="D543" s="34"/>
       <c r="E543" s="34"/>
@@ -38816,8 +38794,8 @@
       </c>
     </row>
     <row r="544">
-      <c r="A544" s="69"/>
-      <c r="B544" s="70"/>
+      <c r="A544" s="63"/>
+      <c r="B544" s="64"/>
       <c r="C544" s="34"/>
       <c r="D544" s="34"/>
       <c r="E544" s="34"/>
@@ -38842,8 +38820,8 @@
       </c>
     </row>
     <row r="545">
-      <c r="A545" s="69"/>
-      <c r="B545" s="70"/>
+      <c r="A545" s="63"/>
+      <c r="B545" s="64"/>
       <c r="C545" s="34"/>
       <c r="D545" s="34"/>
       <c r="E545" s="34"/>
@@ -38868,8 +38846,8 @@
       </c>
     </row>
     <row r="546">
-      <c r="A546" s="69"/>
-      <c r="B546" s="70"/>
+      <c r="A546" s="63"/>
+      <c r="B546" s="64"/>
       <c r="C546" s="34"/>
       <c r="D546" s="34"/>
       <c r="E546" s="34"/>
@@ -38894,8 +38872,8 @@
       </c>
     </row>
     <row r="547">
-      <c r="A547" s="69"/>
-      <c r="B547" s="70"/>
+      <c r="A547" s="63"/>
+      <c r="B547" s="64"/>
       <c r="C547" s="34"/>
       <c r="D547" s="34"/>
       <c r="E547" s="34"/>
@@ -38920,8 +38898,8 @@
       </c>
     </row>
     <row r="548">
-      <c r="A548" s="69"/>
-      <c r="B548" s="70"/>
+      <c r="A548" s="63"/>
+      <c r="B548" s="64"/>
       <c r="C548" s="34"/>
       <c r="D548" s="34"/>
       <c r="E548" s="34"/>
@@ -38946,8 +38924,8 @@
       </c>
     </row>
     <row r="549">
-      <c r="A549" s="69"/>
-      <c r="B549" s="70"/>
+      <c r="A549" s="63"/>
+      <c r="B549" s="64"/>
       <c r="C549" s="34"/>
       <c r="D549" s="34"/>
       <c r="E549" s="34"/>
@@ -38972,8 +38950,8 @@
       </c>
     </row>
     <row r="550">
-      <c r="A550" s="69"/>
-      <c r="B550" s="70"/>
+      <c r="A550" s="63"/>
+      <c r="B550" s="64"/>
       <c r="C550" s="34"/>
       <c r="D550" s="34"/>
       <c r="E550" s="34"/>
@@ -38998,8 +38976,8 @@
       </c>
     </row>
     <row r="551">
-      <c r="A551" s="69"/>
-      <c r="B551" s="70"/>
+      <c r="A551" s="63"/>
+      <c r="B551" s="64"/>
       <c r="C551" s="34"/>
       <c r="D551" s="34"/>
       <c r="E551" s="34"/>

</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201005
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -563,7 +563,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5707" uniqueCount="1907">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5719" uniqueCount="1912">
   <si>
     <t>案例</t>
   </si>
@@ -6984,9 +6984,6 @@
 9/30 確診</t>
   </si>
   <si>
-    <t>自費檢驗</t>
-  </si>
-  <si>
     <t>持有登機前3日內檢驗陰性報告，入境迄今無疑似症狀
 於今(2020)年9月11日入境後，直接前往防疫旅館進行居家檢疫
 居家檢疫期滿後至9月26日於飯店進行自主健康管理
@@ -7050,6 +7047,28 @@
   </si>
   <si>
     <t>曾於當地二次就醫，被診斷為感冒、病毒性感染，皆開立藥物返家休養</t>
+  </si>
+  <si>
+    <t>#518</t>
+  </si>
+  <si>
+    <t>1月-9/18 菲律賓</t>
+  </si>
+  <si>
+    <t>9/18 採檢
+10/3 自費採檢
+10/5 確診</t>
+  </si>
+  <si>
+    <t>發燒 嗅覺喪失 腹瀉</t>
+  </si>
+  <si>
+    <t>曾於6月19日至27日間陸續出現發燒、嗅覺喪失、腹瀉等症狀，於當地就醫及檢出武漢肺炎陽性，經住院治療後症狀改善，並於7月下旬進行兩次採檢，結果皆為陰性
+個案因擔心自身健康，於10月3日檢疫期滿離開檢疫所後，前往醫院自
+費採檢，因檢出弱陽性(Ct值33)於今日確診</t>
+  </si>
+  <si>
+    <t>女赴菲律賓工作染疫，返台後確診COVID-19</t>
   </si>
 </sst>
 </file>
@@ -7060,7 +7079,7 @@
     <numFmt numFmtId="164" formatCode="mm&quot;月&quot;dd&quot;日 &quot;dddd"/>
     <numFmt numFmtId="165" formatCode="m/d"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="19">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -7137,6 +7156,10 @@
       <u/>
       <color rgb="FF1155CC"/>
     </font>
+    <font/>
+    <font>
+      <color rgb="FF000000"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -7182,7 +7205,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="70">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -7372,6 +7395,21 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -7382,7 +7420,7 @@
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
-  <dxfs count="63">
+  <dxfs count="68">
     <dxf>
       <font>
         <color rgb="FF0000FF"/>
@@ -8048,6 +8086,66 @@
       <border/>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF674EA7"/>
+          <bgColor rgb="FF674EA7"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA64D79"/>
+          <bgColor rgb="FFA64D79"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF85200C"/>
+          <bgColor rgb="FF85200C"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF990000"/>
+          <bgColor rgb="FF990000"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB45F06"/>
+          <bgColor rgb="FFB45F06"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
       <font/>
       <fill>
         <patternFill patternType="none"/>
@@ -8087,14 +8185,14 @@
   </dxfs>
   <tableStyles count="2">
     <tableStyle count="3" pivot="0" name="臺灣武漢肺炎病例-style">
-      <tableStyleElement dxfId="60" type="headerRow"/>
-      <tableStyleElement dxfId="61" type="firstRowStripe"/>
-      <tableStyleElement dxfId="62" type="secondRowStripe"/>
+      <tableStyleElement dxfId="65" type="headerRow"/>
+      <tableStyleElement dxfId="66" type="firstRowStripe"/>
+      <tableStyleElement dxfId="67" type="secondRowStripe"/>
     </tableStyle>
     <tableStyle count="3" pivot="0" name="臺灣武漢肺炎病例-style 2">
-      <tableStyleElement dxfId="60" type="headerRow"/>
-      <tableStyleElement dxfId="61" type="firstRowStripe"/>
-      <tableStyleElement dxfId="62" type="secondRowStripe"/>
+      <tableStyleElement dxfId="65" type="headerRow"/>
+      <tableStyleElement dxfId="66" type="firstRowStripe"/>
+      <tableStyleElement dxfId="67" type="secondRowStripe"/>
     </tableStyle>
   </tableStyles>
 </styleSheet>
@@ -37954,7 +38052,7 @@
         <v>1887</v>
       </c>
       <c r="L515" s="12" t="s">
-        <v>1888</v>
+        <v>1674</v>
       </c>
       <c r="M515" s="13" t="s">
         <v>1442</v>
@@ -37964,12 +38062,12 @@
         <v>85</v>
       </c>
       <c r="P515" s="8" t="s">
-        <v>1889</v>
+        <v>1888</v>
       </c>
       <c r="Q515" s="19"/>
       <c r="R515" s="19"/>
       <c r="S515" s="61" t="s">
-        <v>1890</v>
+        <v>1889</v>
       </c>
       <c r="T515" s="20"/>
       <c r="U515" s="18" t="str">
@@ -37979,7 +38077,7 @@
     </row>
     <row r="516">
       <c r="A516" s="16" t="s">
-        <v>1891</v>
+        <v>1890</v>
       </c>
       <c r="B516" s="6">
         <v>44105.0</v>
@@ -37998,14 +38096,14 @@
         <v>25</v>
       </c>
       <c r="H516" s="8" t="s">
-        <v>1892</v>
+        <v>1891</v>
       </c>
       <c r="I516" s="9">
         <v>44103.0</v>
       </c>
       <c r="J516" s="10"/>
       <c r="K516" s="13" t="s">
-        <v>1893</v>
+        <v>1892</v>
       </c>
       <c r="L516" s="12" t="s">
         <v>363</v>
@@ -38018,12 +38116,12 @@
         <v>85</v>
       </c>
       <c r="P516" s="8" t="s">
-        <v>1894</v>
+        <v>1893</v>
       </c>
       <c r="Q516" s="19"/>
       <c r="R516" s="19"/>
       <c r="S516" s="61" t="s">
-        <v>1895</v>
+        <v>1894</v>
       </c>
       <c r="T516" s="20"/>
       <c r="U516" s="18" t="str">
@@ -38033,7 +38131,7 @@
     </row>
     <row r="517">
       <c r="A517" s="16" t="s">
-        <v>1896</v>
+        <v>1895</v>
       </c>
       <c r="B517" s="6">
         <v>44106.0</v>
@@ -38052,7 +38150,7 @@
         <v>25</v>
       </c>
       <c r="H517" s="8" t="s">
-        <v>1897</v>
+        <v>1896</v>
       </c>
       <c r="I517" s="9">
         <v>44094.0</v>
@@ -38061,25 +38159,25 @@
         <v>44071.0</v>
       </c>
       <c r="K517" s="13" t="s">
-        <v>1898</v>
+        <v>1897</v>
       </c>
       <c r="L517" s="12" t="s">
         <v>426</v>
       </c>
       <c r="M517" s="13" t="s">
-        <v>1899</v>
+        <v>1898</v>
       </c>
       <c r="N517" s="25"/>
       <c r="O517" s="8" t="s">
         <v>85</v>
       </c>
       <c r="P517" s="8" t="s">
-        <v>1900</v>
+        <v>1899</v>
       </c>
       <c r="Q517" s="19"/>
       <c r="R517" s="19"/>
       <c r="S517" s="61" t="s">
-        <v>1901</v>
+        <v>1900</v>
       </c>
       <c r="T517" s="20"/>
       <c r="U517" s="18" t="str">
@@ -38089,7 +38187,7 @@
     </row>
     <row r="518">
       <c r="A518" s="16" t="s">
-        <v>1902</v>
+        <v>1901</v>
       </c>
       <c r="B518" s="6">
         <v>44106.0</v>
@@ -38108,7 +38206,7 @@
         <v>25</v>
       </c>
       <c r="H518" s="8" t="s">
-        <v>1903</v>
+        <v>1902</v>
       </c>
       <c r="I518" s="9">
         <v>44104.0</v>
@@ -38117,25 +38215,25 @@
         <v>44089.0</v>
       </c>
       <c r="K518" s="13" t="s">
-        <v>1904</v>
+        <v>1903</v>
       </c>
       <c r="L518" s="12" t="s">
         <v>363</v>
       </c>
       <c r="M518" s="13" t="s">
-        <v>1905</v>
+        <v>1904</v>
       </c>
       <c r="N518" s="25"/>
       <c r="O518" s="8" t="s">
         <v>85</v>
       </c>
       <c r="P518" s="8" t="s">
-        <v>1906</v>
+        <v>1905</v>
       </c>
       <c r="Q518" s="19"/>
       <c r="R518" s="19"/>
       <c r="S518" s="61" t="s">
-        <v>1901</v>
+        <v>1900</v>
       </c>
       <c r="T518" s="20"/>
       <c r="U518" s="18" t="str">
@@ -38144,34 +38242,64 @@
       </c>
     </row>
     <row r="519">
-      <c r="A519" s="63"/>
-      <c r="B519" s="64"/>
-      <c r="C519" s="34"/>
-      <c r="D519" s="34"/>
-      <c r="E519" s="34"/>
+      <c r="A519" s="63" t="s">
+        <v>1906</v>
+      </c>
+      <c r="B519" s="6">
+        <v>44109.0</v>
+      </c>
+      <c r="C519" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D519" s="64" t="s">
+        <v>116</v>
+      </c>
+      <c r="E519" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F519" s="34"/>
-      <c r="G519" s="34"/>
-      <c r="H519" s="21"/>
-      <c r="I519" s="19"/>
-      <c r="J519" s="10"/>
-      <c r="K519" s="22"/>
-      <c r="L519" s="23"/>
-      <c r="M519" s="22"/>
+      <c r="G519" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H519" s="65" t="s">
+        <v>1907</v>
+      </c>
+      <c r="I519" s="66">
+        <v>44092.0</v>
+      </c>
+      <c r="J519" s="10">
+        <v>44001.0</v>
+      </c>
+      <c r="K519" s="67" t="s">
+        <v>1908</v>
+      </c>
+      <c r="L519" s="12" t="s">
+        <v>1674</v>
+      </c>
+      <c r="M519" s="67" t="s">
+        <v>1909</v>
+      </c>
       <c r="N519" s="25"/>
-      <c r="O519" s="21"/>
-      <c r="P519" s="21"/>
+      <c r="O519" s="65" t="s">
+        <v>85</v>
+      </c>
+      <c r="P519" s="65" t="s">
+        <v>1910</v>
+      </c>
       <c r="Q519" s="19"/>
       <c r="R519" s="19"/>
-      <c r="S519" s="20"/>
+      <c r="S519" s="61" t="s">
+        <v>1911</v>
+      </c>
       <c r="T519" s="20"/>
       <c r="U519" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#518</v>
       </c>
     </row>
     <row r="520">
-      <c r="A520" s="63"/>
-      <c r="B520" s="64"/>
+      <c r="A520" s="68"/>
+      <c r="B520" s="69"/>
       <c r="C520" s="34"/>
       <c r="D520" s="34"/>
       <c r="E520" s="34"/>
@@ -38196,8 +38324,8 @@
       </c>
     </row>
     <row r="521">
-      <c r="A521" s="63"/>
-      <c r="B521" s="64"/>
+      <c r="A521" s="68"/>
+      <c r="B521" s="69"/>
       <c r="C521" s="34"/>
       <c r="D521" s="34"/>
       <c r="E521" s="34"/>
@@ -38222,8 +38350,8 @@
       </c>
     </row>
     <row r="522">
-      <c r="A522" s="63"/>
-      <c r="B522" s="64"/>
+      <c r="A522" s="68"/>
+      <c r="B522" s="69"/>
       <c r="C522" s="34"/>
       <c r="D522" s="34"/>
       <c r="E522" s="34"/>
@@ -38248,8 +38376,8 @@
       </c>
     </row>
     <row r="523">
-      <c r="A523" s="63"/>
-      <c r="B523" s="64"/>
+      <c r="A523" s="68"/>
+      <c r="B523" s="69"/>
       <c r="C523" s="34"/>
       <c r="D523" s="34"/>
       <c r="E523" s="34"/>
@@ -38274,8 +38402,8 @@
       </c>
     </row>
     <row r="524">
-      <c r="A524" s="63"/>
-      <c r="B524" s="64"/>
+      <c r="A524" s="68"/>
+      <c r="B524" s="69"/>
       <c r="C524" s="34"/>
       <c r="D524" s="34"/>
       <c r="E524" s="34"/>
@@ -38300,8 +38428,8 @@
       </c>
     </row>
     <row r="525">
-      <c r="A525" s="63"/>
-      <c r="B525" s="64"/>
+      <c r="A525" s="68"/>
+      <c r="B525" s="69"/>
       <c r="C525" s="34"/>
       <c r="D525" s="34"/>
       <c r="E525" s="34"/>
@@ -38326,8 +38454,8 @@
       </c>
     </row>
     <row r="526">
-      <c r="A526" s="63"/>
-      <c r="B526" s="64"/>
+      <c r="A526" s="68"/>
+      <c r="B526" s="69"/>
       <c r="C526" s="34"/>
       <c r="D526" s="34"/>
       <c r="E526" s="34"/>
@@ -38352,8 +38480,8 @@
       </c>
     </row>
     <row r="527">
-      <c r="A527" s="63"/>
-      <c r="B527" s="64"/>
+      <c r="A527" s="68"/>
+      <c r="B527" s="69"/>
       <c r="C527" s="34"/>
       <c r="D527" s="34"/>
       <c r="E527" s="34"/>
@@ -38378,8 +38506,8 @@
       </c>
     </row>
     <row r="528">
-      <c r="A528" s="63"/>
-      <c r="B528" s="64"/>
+      <c r="A528" s="68"/>
+      <c r="B528" s="69"/>
       <c r="C528" s="34"/>
       <c r="D528" s="34"/>
       <c r="E528" s="34"/>
@@ -38404,8 +38532,8 @@
       </c>
     </row>
     <row r="529">
-      <c r="A529" s="63"/>
-      <c r="B529" s="64"/>
+      <c r="A529" s="68"/>
+      <c r="B529" s="69"/>
       <c r="C529" s="34"/>
       <c r="D529" s="34"/>
       <c r="E529" s="34"/>
@@ -38430,8 +38558,8 @@
       </c>
     </row>
     <row r="530">
-      <c r="A530" s="63"/>
-      <c r="B530" s="64"/>
+      <c r="A530" s="68"/>
+      <c r="B530" s="69"/>
       <c r="C530" s="34"/>
       <c r="D530" s="34"/>
       <c r="E530" s="34"/>
@@ -38456,8 +38584,8 @@
       </c>
     </row>
     <row r="531">
-      <c r="A531" s="63"/>
-      <c r="B531" s="64"/>
+      <c r="A531" s="68"/>
+      <c r="B531" s="69"/>
       <c r="C531" s="34"/>
       <c r="D531" s="34"/>
       <c r="E531" s="34"/>
@@ -38482,8 +38610,8 @@
       </c>
     </row>
     <row r="532">
-      <c r="A532" s="63"/>
-      <c r="B532" s="64"/>
+      <c r="A532" s="68"/>
+      <c r="B532" s="69"/>
       <c r="C532" s="34"/>
       <c r="D532" s="34"/>
       <c r="E532" s="34"/>
@@ -38508,8 +38636,8 @@
       </c>
     </row>
     <row r="533">
-      <c r="A533" s="63"/>
-      <c r="B533" s="64"/>
+      <c r="A533" s="68"/>
+      <c r="B533" s="69"/>
       <c r="C533" s="34"/>
       <c r="D533" s="34"/>
       <c r="E533" s="34"/>
@@ -38534,8 +38662,8 @@
       </c>
     </row>
     <row r="534">
-      <c r="A534" s="63"/>
-      <c r="B534" s="64"/>
+      <c r="A534" s="68"/>
+      <c r="B534" s="69"/>
       <c r="C534" s="34"/>
       <c r="D534" s="34"/>
       <c r="E534" s="34"/>
@@ -38560,8 +38688,8 @@
       </c>
     </row>
     <row r="535">
-      <c r="A535" s="63"/>
-      <c r="B535" s="64"/>
+      <c r="A535" s="68"/>
+      <c r="B535" s="69"/>
       <c r="C535" s="34"/>
       <c r="D535" s="34"/>
       <c r="E535" s="34"/>
@@ -38586,8 +38714,8 @@
       </c>
     </row>
     <row r="536">
-      <c r="A536" s="63"/>
-      <c r="B536" s="64"/>
+      <c r="A536" s="68"/>
+      <c r="B536" s="69"/>
       <c r="C536" s="34"/>
       <c r="D536" s="34"/>
       <c r="E536" s="34"/>
@@ -38612,8 +38740,8 @@
       </c>
     </row>
     <row r="537">
-      <c r="A537" s="63"/>
-      <c r="B537" s="64"/>
+      <c r="A537" s="68"/>
+      <c r="B537" s="69"/>
       <c r="C537" s="34"/>
       <c r="D537" s="34"/>
       <c r="E537" s="34"/>
@@ -38638,8 +38766,8 @@
       </c>
     </row>
     <row r="538">
-      <c r="A538" s="63"/>
-      <c r="B538" s="64"/>
+      <c r="A538" s="68"/>
+      <c r="B538" s="69"/>
       <c r="C538" s="34"/>
       <c r="D538" s="34"/>
       <c r="E538" s="34"/>
@@ -38664,8 +38792,8 @@
       </c>
     </row>
     <row r="539">
-      <c r="A539" s="63"/>
-      <c r="B539" s="64"/>
+      <c r="A539" s="68"/>
+      <c r="B539" s="69"/>
       <c r="C539" s="34"/>
       <c r="D539" s="34"/>
       <c r="E539" s="34"/>
@@ -38690,8 +38818,8 @@
       </c>
     </row>
     <row r="540">
-      <c r="A540" s="63"/>
-      <c r="B540" s="64"/>
+      <c r="A540" s="68"/>
+      <c r="B540" s="69"/>
       <c r="C540" s="34"/>
       <c r="D540" s="34"/>
       <c r="E540" s="34"/>
@@ -38716,8 +38844,8 @@
       </c>
     </row>
     <row r="541">
-      <c r="A541" s="63"/>
-      <c r="B541" s="64"/>
+      <c r="A541" s="68"/>
+      <c r="B541" s="69"/>
       <c r="C541" s="34"/>
       <c r="D541" s="34"/>
       <c r="E541" s="34"/>
@@ -38742,8 +38870,8 @@
       </c>
     </row>
     <row r="542">
-      <c r="A542" s="63"/>
-      <c r="B542" s="64"/>
+      <c r="A542" s="68"/>
+      <c r="B542" s="69"/>
       <c r="C542" s="34"/>
       <c r="D542" s="34"/>
       <c r="E542" s="34"/>
@@ -38768,8 +38896,8 @@
       </c>
     </row>
     <row r="543">
-      <c r="A543" s="63"/>
-      <c r="B543" s="64"/>
+      <c r="A543" s="68"/>
+      <c r="B543" s="69"/>
       <c r="C543" s="34"/>
       <c r="D543" s="34"/>
       <c r="E543" s="34"/>
@@ -38794,8 +38922,8 @@
       </c>
     </row>
     <row r="544">
-      <c r="A544" s="63"/>
-      <c r="B544" s="64"/>
+      <c r="A544" s="68"/>
+      <c r="B544" s="69"/>
       <c r="C544" s="34"/>
       <c r="D544" s="34"/>
       <c r="E544" s="34"/>
@@ -38820,8 +38948,8 @@
       </c>
     </row>
     <row r="545">
-      <c r="A545" s="63"/>
-      <c r="B545" s="64"/>
+      <c r="A545" s="68"/>
+      <c r="B545" s="69"/>
       <c r="C545" s="34"/>
       <c r="D545" s="34"/>
       <c r="E545" s="34"/>
@@ -38846,8 +38974,8 @@
       </c>
     </row>
     <row r="546">
-      <c r="A546" s="63"/>
-      <c r="B546" s="64"/>
+      <c r="A546" s="68"/>
+      <c r="B546" s="69"/>
       <c r="C546" s="34"/>
       <c r="D546" s="34"/>
       <c r="E546" s="34"/>
@@ -38872,8 +39000,8 @@
       </c>
     </row>
     <row r="547">
-      <c r="A547" s="63"/>
-      <c r="B547" s="64"/>
+      <c r="A547" s="68"/>
+      <c r="B547" s="69"/>
       <c r="C547" s="34"/>
       <c r="D547" s="34"/>
       <c r="E547" s="34"/>
@@ -38898,8 +39026,8 @@
       </c>
     </row>
     <row r="548">
-      <c r="A548" s="63"/>
-      <c r="B548" s="64"/>
+      <c r="A548" s="68"/>
+      <c r="B548" s="69"/>
       <c r="C548" s="34"/>
       <c r="D548" s="34"/>
       <c r="E548" s="34"/>
@@ -38924,8 +39052,8 @@
       </c>
     </row>
     <row r="549">
-      <c r="A549" s="63"/>
-      <c r="B549" s="64"/>
+      <c r="A549" s="68"/>
+      <c r="B549" s="69"/>
       <c r="C549" s="34"/>
       <c r="D549" s="34"/>
       <c r="E549" s="34"/>
@@ -38950,8 +39078,8 @@
       </c>
     </row>
     <row r="550">
-      <c r="A550" s="63"/>
-      <c r="B550" s="64"/>
+      <c r="A550" s="68"/>
+      <c r="B550" s="69"/>
       <c r="C550" s="34"/>
       <c r="D550" s="34"/>
       <c r="E550" s="34"/>
@@ -38976,8 +39104,8 @@
       </c>
     </row>
     <row r="551">
-      <c r="A551" s="63"/>
-      <c r="B551" s="64"/>
+      <c r="A551" s="68"/>
+      <c r="B551" s="69"/>
       <c r="C551" s="34"/>
       <c r="D551" s="34"/>
       <c r="E551" s="34"/>
@@ -39327,6 +39455,31 @@
       <formula>NOT(ISERROR(SEARCH(("自費"),(L1))))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B357:B551">
+    <cfRule type="expression" dxfId="59" priority="66">
+      <formula>B357&lt;44115.0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B357:B551">
+    <cfRule type="expression" dxfId="60" priority="67">
+      <formula>B357&lt;44122.0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B357:B551">
+    <cfRule type="expression" dxfId="61" priority="68">
+      <formula>B357&lt;44129.0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B357:B551">
+    <cfRule type="expression" dxfId="62" priority="69">
+      <formula>B357&lt;44136.0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B357:B551">
+    <cfRule type="expression" dxfId="63" priority="70">
+      <formula>B357&lt;44143.0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink r:id="rId2" ref="S440"/>
     <hyperlink r:id="rId3" ref="S441"/>
@@ -39407,15 +39560,16 @@
     <hyperlink r:id="rId78" ref="S516"/>
     <hyperlink r:id="rId79" ref="S517"/>
     <hyperlink r:id="rId80" ref="S518"/>
+    <hyperlink r:id="rId81" ref="S519"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId81"/>
-  <legacyDrawing r:id="rId82"/>
+  <drawing r:id="rId82"/>
+  <legacyDrawing r:id="rId83"/>
   <tableParts count="2">
-    <tablePart r:id="rId85"/>
     <tablePart r:id="rId86"/>
+    <tablePart r:id="rId87"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201007
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -563,7 +563,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5719" uniqueCount="1912">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5755" uniqueCount="1925">
   <si>
     <t>案例</t>
   </si>
@@ -7069,6 +7069,46 @@
   </si>
   <si>
     <t>女赴菲律賓工作染疫，返台後確診COVID-19</t>
+  </si>
+  <si>
+    <t>#519</t>
+  </si>
+  <si>
+    <t>-10/4 美國</t>
+  </si>
+  <si>
+    <t>10/4 採檢
+10/6 確診</t>
+  </si>
+  <si>
+    <t>長期在美國工作，約2至3個月返台一次，在美國期間無不適症狀</t>
+  </si>
+  <si>
+    <t>國內新增3例境外移入COVID-19病例，分別自美國、法國返台</t>
+  </si>
+  <si>
+    <t>#520</t>
+  </si>
+  <si>
+    <t>9月中旬-10/4 法國</t>
+  </si>
+  <si>
+    <t>發燒 頭痛 流鼻水 鼻塞 嗅覺異常</t>
+  </si>
+  <si>
+    <t>今年已於法國留學畢業，9月中旬再前往法國處理私人事務</t>
+  </si>
+  <si>
+    <t>#521</t>
+  </si>
+  <si>
+    <t>5月-10/4 美國</t>
+  </si>
+  <si>
+    <t>腹瀉 喉嚨腫</t>
+  </si>
+  <si>
+    <t>長期於美國工作</t>
   </si>
 </sst>
 </file>
@@ -7205,7 +7245,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -7409,6 +7449,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
@@ -38298,86 +38341,174 @@
       </c>
     </row>
     <row r="520">
-      <c r="A520" s="68"/>
-      <c r="B520" s="69"/>
-      <c r="C520" s="34"/>
-      <c r="D520" s="34"/>
-      <c r="E520" s="34"/>
+      <c r="A520" s="63" t="s">
+        <v>1912</v>
+      </c>
+      <c r="B520" s="6">
+        <v>44110.0</v>
+      </c>
+      <c r="C520" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D520" s="64" t="s">
+        <v>116</v>
+      </c>
+      <c r="E520" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F520" s="34"/>
-      <c r="G520" s="34"/>
-      <c r="H520" s="21"/>
-      <c r="I520" s="19"/>
+      <c r="G520" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H520" s="65" t="s">
+        <v>1913</v>
+      </c>
+      <c r="I520" s="66">
+        <v>44108.0</v>
+      </c>
       <c r="J520" s="10"/>
-      <c r="K520" s="22"/>
-      <c r="L520" s="23"/>
-      <c r="M520" s="22"/>
+      <c r="K520" s="67" t="s">
+        <v>1914</v>
+      </c>
+      <c r="L520" s="68" t="s">
+        <v>363</v>
+      </c>
+      <c r="M520" s="67" t="s">
+        <v>429</v>
+      </c>
       <c r="N520" s="25"/>
-      <c r="O520" s="21"/>
-      <c r="P520" s="21"/>
+      <c r="O520" s="65" t="s">
+        <v>85</v>
+      </c>
+      <c r="P520" s="65" t="s">
+        <v>1915</v>
+      </c>
       <c r="Q520" s="19"/>
       <c r="R520" s="19"/>
-      <c r="S520" s="20"/>
+      <c r="S520" s="61" t="s">
+        <v>1916</v>
+      </c>
       <c r="T520" s="20"/>
       <c r="U520" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#519</v>
       </c>
     </row>
     <row r="521">
-      <c r="A521" s="68"/>
-      <c r="B521" s="69"/>
-      <c r="C521" s="34"/>
-      <c r="D521" s="34"/>
-      <c r="E521" s="34"/>
+      <c r="A521" s="63" t="s">
+        <v>1917</v>
+      </c>
+      <c r="B521" s="6">
+        <v>44110.0</v>
+      </c>
+      <c r="C521" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D521" s="64" t="s">
+        <v>76</v>
+      </c>
+      <c r="E521" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F521" s="34"/>
-      <c r="G521" s="34"/>
-      <c r="H521" s="21"/>
-      <c r="I521" s="19"/>
-      <c r="J521" s="10"/>
-      <c r="K521" s="22"/>
-      <c r="L521" s="23"/>
-      <c r="M521" s="22"/>
+      <c r="G521" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H521" s="65" t="s">
+        <v>1918</v>
+      </c>
+      <c r="I521" s="66">
+        <v>44108.0</v>
+      </c>
+      <c r="J521" s="10">
+        <v>44101.0</v>
+      </c>
+      <c r="K521" s="67" t="s">
+        <v>1914</v>
+      </c>
+      <c r="L521" s="68" t="s">
+        <v>363</v>
+      </c>
+      <c r="M521" s="67" t="s">
+        <v>1919</v>
+      </c>
       <c r="N521" s="25"/>
-      <c r="O521" s="21"/>
-      <c r="P521" s="21"/>
+      <c r="O521" s="65" t="s">
+        <v>85</v>
+      </c>
+      <c r="P521" s="65" t="s">
+        <v>1920</v>
+      </c>
       <c r="Q521" s="19"/>
       <c r="R521" s="19"/>
-      <c r="S521" s="20"/>
+      <c r="S521" s="61" t="s">
+        <v>1916</v>
+      </c>
       <c r="T521" s="20"/>
       <c r="U521" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#520</v>
       </c>
     </row>
     <row r="522">
-      <c r="A522" s="68"/>
-      <c r="B522" s="69"/>
-      <c r="C522" s="34"/>
-      <c r="D522" s="34"/>
-      <c r="E522" s="34"/>
+      <c r="A522" s="63" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B522" s="6">
+        <v>44110.0</v>
+      </c>
+      <c r="C522" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D522" s="64" t="s">
+        <v>116</v>
+      </c>
+      <c r="E522" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F522" s="34"/>
-      <c r="G522" s="34"/>
-      <c r="H522" s="21"/>
-      <c r="I522" s="19"/>
-      <c r="J522" s="10"/>
-      <c r="K522" s="22"/>
-      <c r="L522" s="23"/>
-      <c r="M522" s="22"/>
+      <c r="G522" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H522" s="65" t="s">
+        <v>1922</v>
+      </c>
+      <c r="I522" s="66">
+        <v>44108.0</v>
+      </c>
+      <c r="J522" s="10">
+        <v>44107.0</v>
+      </c>
+      <c r="K522" s="67" t="s">
+        <v>1914</v>
+      </c>
+      <c r="L522" s="68" t="s">
+        <v>363</v>
+      </c>
+      <c r="M522" s="67" t="s">
+        <v>1923</v>
+      </c>
       <c r="N522" s="25"/>
-      <c r="O522" s="21"/>
-      <c r="P522" s="21"/>
+      <c r="O522" s="65" t="s">
+        <v>85</v>
+      </c>
+      <c r="P522" s="65" t="s">
+        <v>1924</v>
+      </c>
       <c r="Q522" s="19"/>
       <c r="R522" s="19"/>
-      <c r="S522" s="20"/>
+      <c r="S522" s="61" t="s">
+        <v>1916</v>
+      </c>
       <c r="T522" s="20"/>
       <c r="U522" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#521</v>
       </c>
     </row>
     <row r="523">
-      <c r="A523" s="68"/>
-      <c r="B523" s="69"/>
+      <c r="A523" s="69"/>
+      <c r="B523" s="70"/>
       <c r="C523" s="34"/>
       <c r="D523" s="34"/>
       <c r="E523" s="34"/>
@@ -38402,8 +38533,8 @@
       </c>
     </row>
     <row r="524">
-      <c r="A524" s="68"/>
-      <c r="B524" s="69"/>
+      <c r="A524" s="69"/>
+      <c r="B524" s="70"/>
       <c r="C524" s="34"/>
       <c r="D524" s="34"/>
       <c r="E524" s="34"/>
@@ -38428,8 +38559,8 @@
       </c>
     </row>
     <row r="525">
-      <c r="A525" s="68"/>
-      <c r="B525" s="69"/>
+      <c r="A525" s="69"/>
+      <c r="B525" s="70"/>
       <c r="C525" s="34"/>
       <c r="D525" s="34"/>
       <c r="E525" s="34"/>
@@ -38454,8 +38585,8 @@
       </c>
     </row>
     <row r="526">
-      <c r="A526" s="68"/>
-      <c r="B526" s="69"/>
+      <c r="A526" s="69"/>
+      <c r="B526" s="70"/>
       <c r="C526" s="34"/>
       <c r="D526" s="34"/>
       <c r="E526" s="34"/>
@@ -38480,8 +38611,8 @@
       </c>
     </row>
     <row r="527">
-      <c r="A527" s="68"/>
-      <c r="B527" s="69"/>
+      <c r="A527" s="69"/>
+      <c r="B527" s="70"/>
       <c r="C527" s="34"/>
       <c r="D527" s="34"/>
       <c r="E527" s="34"/>
@@ -38506,8 +38637,8 @@
       </c>
     </row>
     <row r="528">
-      <c r="A528" s="68"/>
-      <c r="B528" s="69"/>
+      <c r="A528" s="69"/>
+      <c r="B528" s="70"/>
       <c r="C528" s="34"/>
       <c r="D528" s="34"/>
       <c r="E528" s="34"/>
@@ -38532,8 +38663,8 @@
       </c>
     </row>
     <row r="529">
-      <c r="A529" s="68"/>
-      <c r="B529" s="69"/>
+      <c r="A529" s="69"/>
+      <c r="B529" s="70"/>
       <c r="C529" s="34"/>
       <c r="D529" s="34"/>
       <c r="E529" s="34"/>
@@ -38558,8 +38689,8 @@
       </c>
     </row>
     <row r="530">
-      <c r="A530" s="68"/>
-      <c r="B530" s="69"/>
+      <c r="A530" s="69"/>
+      <c r="B530" s="70"/>
       <c r="C530" s="34"/>
       <c r="D530" s="34"/>
       <c r="E530" s="34"/>
@@ -38584,8 +38715,8 @@
       </c>
     </row>
     <row r="531">
-      <c r="A531" s="68"/>
-      <c r="B531" s="69"/>
+      <c r="A531" s="69"/>
+      <c r="B531" s="70"/>
       <c r="C531" s="34"/>
       <c r="D531" s="34"/>
       <c r="E531" s="34"/>
@@ -38610,8 +38741,8 @@
       </c>
     </row>
     <row r="532">
-      <c r="A532" s="68"/>
-      <c r="B532" s="69"/>
+      <c r="A532" s="69"/>
+      <c r="B532" s="70"/>
       <c r="C532" s="34"/>
       <c r="D532" s="34"/>
       <c r="E532" s="34"/>
@@ -38636,8 +38767,8 @@
       </c>
     </row>
     <row r="533">
-      <c r="A533" s="68"/>
-      <c r="B533" s="69"/>
+      <c r="A533" s="69"/>
+      <c r="B533" s="70"/>
       <c r="C533" s="34"/>
       <c r="D533" s="34"/>
       <c r="E533" s="34"/>
@@ -38662,8 +38793,8 @@
       </c>
     </row>
     <row r="534">
-      <c r="A534" s="68"/>
-      <c r="B534" s="69"/>
+      <c r="A534" s="69"/>
+      <c r="B534" s="70"/>
       <c r="C534" s="34"/>
       <c r="D534" s="34"/>
       <c r="E534" s="34"/>
@@ -38688,8 +38819,8 @@
       </c>
     </row>
     <row r="535">
-      <c r="A535" s="68"/>
-      <c r="B535" s="69"/>
+      <c r="A535" s="69"/>
+      <c r="B535" s="70"/>
       <c r="C535" s="34"/>
       <c r="D535" s="34"/>
       <c r="E535" s="34"/>
@@ -38714,8 +38845,8 @@
       </c>
     </row>
     <row r="536">
-      <c r="A536" s="68"/>
-      <c r="B536" s="69"/>
+      <c r="A536" s="69"/>
+      <c r="B536" s="70"/>
       <c r="C536" s="34"/>
       <c r="D536" s="34"/>
       <c r="E536" s="34"/>
@@ -38740,8 +38871,8 @@
       </c>
     </row>
     <row r="537">
-      <c r="A537" s="68"/>
-      <c r="B537" s="69"/>
+      <c r="A537" s="69"/>
+      <c r="B537" s="70"/>
       <c r="C537" s="34"/>
       <c r="D537" s="34"/>
       <c r="E537" s="34"/>
@@ -38766,8 +38897,8 @@
       </c>
     </row>
     <row r="538">
-      <c r="A538" s="68"/>
-      <c r="B538" s="69"/>
+      <c r="A538" s="69"/>
+      <c r="B538" s="70"/>
       <c r="C538" s="34"/>
       <c r="D538" s="34"/>
       <c r="E538" s="34"/>
@@ -38792,8 +38923,8 @@
       </c>
     </row>
     <row r="539">
-      <c r="A539" s="68"/>
-      <c r="B539" s="69"/>
+      <c r="A539" s="69"/>
+      <c r="B539" s="70"/>
       <c r="C539" s="34"/>
       <c r="D539" s="34"/>
       <c r="E539" s="34"/>
@@ -38818,8 +38949,8 @@
       </c>
     </row>
     <row r="540">
-      <c r="A540" s="68"/>
-      <c r="B540" s="69"/>
+      <c r="A540" s="69"/>
+      <c r="B540" s="70"/>
       <c r="C540" s="34"/>
       <c r="D540" s="34"/>
       <c r="E540" s="34"/>
@@ -38844,8 +38975,8 @@
       </c>
     </row>
     <row r="541">
-      <c r="A541" s="68"/>
-      <c r="B541" s="69"/>
+      <c r="A541" s="69"/>
+      <c r="B541" s="70"/>
       <c r="C541" s="34"/>
       <c r="D541" s="34"/>
       <c r="E541" s="34"/>
@@ -38870,8 +39001,8 @@
       </c>
     </row>
     <row r="542">
-      <c r="A542" s="68"/>
-      <c r="B542" s="69"/>
+      <c r="A542" s="69"/>
+      <c r="B542" s="70"/>
       <c r="C542" s="34"/>
       <c r="D542" s="34"/>
       <c r="E542" s="34"/>
@@ -38896,8 +39027,8 @@
       </c>
     </row>
     <row r="543">
-      <c r="A543" s="68"/>
-      <c r="B543" s="69"/>
+      <c r="A543" s="69"/>
+      <c r="B543" s="70"/>
       <c r="C543" s="34"/>
       <c r="D543" s="34"/>
       <c r="E543" s="34"/>
@@ -38922,8 +39053,8 @@
       </c>
     </row>
     <row r="544">
-      <c r="A544" s="68"/>
-      <c r="B544" s="69"/>
+      <c r="A544" s="69"/>
+      <c r="B544" s="70"/>
       <c r="C544" s="34"/>
       <c r="D544" s="34"/>
       <c r="E544" s="34"/>
@@ -38948,8 +39079,8 @@
       </c>
     </row>
     <row r="545">
-      <c r="A545" s="68"/>
-      <c r="B545" s="69"/>
+      <c r="A545" s="69"/>
+      <c r="B545" s="70"/>
       <c r="C545" s="34"/>
       <c r="D545" s="34"/>
       <c r="E545" s="34"/>
@@ -38974,8 +39105,8 @@
       </c>
     </row>
     <row r="546">
-      <c r="A546" s="68"/>
-      <c r="B546" s="69"/>
+      <c r="A546" s="69"/>
+      <c r="B546" s="70"/>
       <c r="C546" s="34"/>
       <c r="D546" s="34"/>
       <c r="E546" s="34"/>
@@ -39000,8 +39131,8 @@
       </c>
     </row>
     <row r="547">
-      <c r="A547" s="68"/>
-      <c r="B547" s="69"/>
+      <c r="A547" s="69"/>
+      <c r="B547" s="70"/>
       <c r="C547" s="34"/>
       <c r="D547" s="34"/>
       <c r="E547" s="34"/>
@@ -39026,8 +39157,8 @@
       </c>
     </row>
     <row r="548">
-      <c r="A548" s="68"/>
-      <c r="B548" s="69"/>
+      <c r="A548" s="69"/>
+      <c r="B548" s="70"/>
       <c r="C548" s="34"/>
       <c r="D548" s="34"/>
       <c r="E548" s="34"/>
@@ -39052,8 +39183,8 @@
       </c>
     </row>
     <row r="549">
-      <c r="A549" s="68"/>
-      <c r="B549" s="69"/>
+      <c r="A549" s="69"/>
+      <c r="B549" s="70"/>
       <c r="C549" s="34"/>
       <c r="D549" s="34"/>
       <c r="E549" s="34"/>
@@ -39078,8 +39209,8 @@
       </c>
     </row>
     <row r="550">
-      <c r="A550" s="68"/>
-      <c r="B550" s="69"/>
+      <c r="A550" s="69"/>
+      <c r="B550" s="70"/>
       <c r="C550" s="34"/>
       <c r="D550" s="34"/>
       <c r="E550" s="34"/>
@@ -39104,8 +39235,8 @@
       </c>
     </row>
     <row r="551">
-      <c r="A551" s="68"/>
-      <c r="B551" s="69"/>
+      <c r="A551" s="69"/>
+      <c r="B551" s="70"/>
       <c r="C551" s="34"/>
       <c r="D551" s="34"/>
       <c r="E551" s="34"/>
@@ -39561,15 +39692,18 @@
     <hyperlink r:id="rId79" ref="S517"/>
     <hyperlink r:id="rId80" ref="S518"/>
     <hyperlink r:id="rId81" ref="S519"/>
+    <hyperlink r:id="rId82" ref="S520"/>
+    <hyperlink r:id="rId83" ref="S521"/>
+    <hyperlink r:id="rId84" ref="S522"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId82"/>
-  <legacyDrawing r:id="rId83"/>
+  <drawing r:id="rId85"/>
+  <legacyDrawing r:id="rId86"/>
   <tableParts count="2">
-    <tablePart r:id="rId86"/>
-    <tablePart r:id="rId87"/>
+    <tablePart r:id="rId89"/>
+    <tablePart r:id="rId90"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201008
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -563,7 +563,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5755" uniqueCount="1925">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5780" uniqueCount="1935">
   <si>
     <t>案例</t>
   </si>
@@ -7109,6 +7109,41 @@
   </si>
   <si>
     <t>長期於美國工作</t>
+  </si>
+  <si>
+    <t>#522</t>
+  </si>
+  <si>
+    <t>2019/10月-2020/10/4 愛爾蘭</t>
+  </si>
+  <si>
+    <t>10/5 採檢
+10/7 確診</t>
+  </si>
+  <si>
+    <t>發燒 全身肌肉痠痛</t>
+  </si>
+  <si>
+    <t>國內新增2例境外移入COVID-19確診，分別自愛爾蘭及印度入境</t>
+  </si>
+  <si>
+    <t>#523</t>
+  </si>
+  <si>
+    <t>印度</t>
+  </si>
+  <si>
+    <t>-9/9 印度→台灣</t>
+  </si>
+  <si>
+    <t>9/9 採檢
+10/5 二採
+10/7 確診</t>
+  </si>
+  <si>
+    <t>因工作來台，持有登機前3日內檢驗陰性報告，入境迄今無疑似症狀
+9月9日入境後前往防疫旅館進行居家檢疫(9月9日至9月23日)
+9月24日至30日於飯店進行自主健康管理，10月5日因工作需求自費檢驗</t>
   </si>
 </sst>
 </file>
@@ -7196,10 +7231,10 @@
       <u/>
       <color rgb="FF1155CC"/>
     </font>
-    <font/>
     <font>
       <color rgb="FF000000"/>
     </font>
+    <font/>
   </fonts>
   <fills count="7">
     <fill>
@@ -7436,21 +7471,21 @@
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="18" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="17" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -38285,7 +38320,7 @@
       </c>
     </row>
     <row r="519">
-      <c r="A519" s="63" t="s">
+      <c r="A519" s="16" t="s">
         <v>1906</v>
       </c>
       <c r="B519" s="6">
@@ -38294,7 +38329,7 @@
       <c r="C519" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D519" s="64" t="s">
+      <c r="D519" s="7" t="s">
         <v>116</v>
       </c>
       <c r="E519" s="7" t="s">
@@ -38304,29 +38339,29 @@
       <c r="G519" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H519" s="65" t="s">
+      <c r="H519" s="8" t="s">
         <v>1907</v>
       </c>
-      <c r="I519" s="66">
+      <c r="I519" s="9">
         <v>44092.0</v>
       </c>
       <c r="J519" s="10">
         <v>44001.0</v>
       </c>
-      <c r="K519" s="67" t="s">
+      <c r="K519" s="13" t="s">
         <v>1908</v>
       </c>
       <c r="L519" s="12" t="s">
         <v>1674</v>
       </c>
-      <c r="M519" s="67" t="s">
+      <c r="M519" s="13" t="s">
         <v>1909</v>
       </c>
       <c r="N519" s="25"/>
-      <c r="O519" s="65" t="s">
+      <c r="O519" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P519" s="65" t="s">
+      <c r="P519" s="8" t="s">
         <v>1910</v>
       </c>
       <c r="Q519" s="19"/>
@@ -38341,7 +38376,7 @@
       </c>
     </row>
     <row r="520">
-      <c r="A520" s="63" t="s">
+      <c r="A520" s="16" t="s">
         <v>1912</v>
       </c>
       <c r="B520" s="6">
@@ -38350,7 +38385,7 @@
       <c r="C520" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D520" s="64" t="s">
+      <c r="D520" s="7" t="s">
         <v>116</v>
       </c>
       <c r="E520" s="7" t="s">
@@ -38360,27 +38395,27 @@
       <c r="G520" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H520" s="65" t="s">
+      <c r="H520" s="8" t="s">
         <v>1913</v>
       </c>
-      <c r="I520" s="66">
+      <c r="I520" s="9">
         <v>44108.0</v>
       </c>
       <c r="J520" s="10"/>
-      <c r="K520" s="67" t="s">
+      <c r="K520" s="13" t="s">
         <v>1914</v>
       </c>
-      <c r="L520" s="68" t="s">
+      <c r="L520" s="12" t="s">
         <v>363</v>
       </c>
-      <c r="M520" s="67" t="s">
+      <c r="M520" s="13" t="s">
         <v>429</v>
       </c>
       <c r="N520" s="25"/>
-      <c r="O520" s="65" t="s">
+      <c r="O520" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P520" s="65" t="s">
+      <c r="P520" s="8" t="s">
         <v>1915</v>
       </c>
       <c r="Q520" s="19"/>
@@ -38395,7 +38430,7 @@
       </c>
     </row>
     <row r="521">
-      <c r="A521" s="63" t="s">
+      <c r="A521" s="16" t="s">
         <v>1917</v>
       </c>
       <c r="B521" s="6">
@@ -38404,7 +38439,7 @@
       <c r="C521" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D521" s="64" t="s">
+      <c r="D521" s="7" t="s">
         <v>76</v>
       </c>
       <c r="E521" s="7" t="s">
@@ -38414,29 +38449,29 @@
       <c r="G521" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H521" s="65" t="s">
+      <c r="H521" s="8" t="s">
         <v>1918</v>
       </c>
-      <c r="I521" s="66">
+      <c r="I521" s="9">
         <v>44108.0</v>
       </c>
       <c r="J521" s="10">
         <v>44101.0</v>
       </c>
-      <c r="K521" s="67" t="s">
+      <c r="K521" s="13" t="s">
         <v>1914</v>
       </c>
-      <c r="L521" s="68" t="s">
+      <c r="L521" s="12" t="s">
         <v>363</v>
       </c>
-      <c r="M521" s="67" t="s">
+      <c r="M521" s="13" t="s">
         <v>1919</v>
       </c>
       <c r="N521" s="25"/>
-      <c r="O521" s="65" t="s">
+      <c r="O521" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P521" s="65" t="s">
+      <c r="P521" s="8" t="s">
         <v>1920</v>
       </c>
       <c r="Q521" s="19"/>
@@ -38451,7 +38486,7 @@
       </c>
     </row>
     <row r="522">
-      <c r="A522" s="63" t="s">
+      <c r="A522" s="16" t="s">
         <v>1921</v>
       </c>
       <c r="B522" s="6">
@@ -38460,7 +38495,7 @@
       <c r="C522" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D522" s="64" t="s">
+      <c r="D522" s="7" t="s">
         <v>116</v>
       </c>
       <c r="E522" s="7" t="s">
@@ -38470,29 +38505,29 @@
       <c r="G522" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H522" s="65" t="s">
+      <c r="H522" s="8" t="s">
         <v>1922</v>
       </c>
-      <c r="I522" s="66">
+      <c r="I522" s="9">
         <v>44108.0</v>
       </c>
       <c r="J522" s="10">
         <v>44107.0</v>
       </c>
-      <c r="K522" s="67" t="s">
+      <c r="K522" s="13" t="s">
         <v>1914</v>
       </c>
-      <c r="L522" s="68" t="s">
+      <c r="L522" s="12" t="s">
         <v>363</v>
       </c>
-      <c r="M522" s="67" t="s">
+      <c r="M522" s="63" t="s">
         <v>1923</v>
       </c>
       <c r="N522" s="25"/>
-      <c r="O522" s="65" t="s">
+      <c r="O522" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P522" s="65" t="s">
+      <c r="P522" s="8" t="s">
         <v>1924</v>
       </c>
       <c r="Q522" s="19"/>
@@ -38507,55 +38542,115 @@
       </c>
     </row>
     <row r="523">
-      <c r="A523" s="69"/>
-      <c r="B523" s="70"/>
-      <c r="C523" s="34"/>
-      <c r="D523" s="34"/>
-      <c r="E523" s="34"/>
+      <c r="A523" s="16" t="s">
+        <v>1925</v>
+      </c>
+      <c r="B523" s="6">
+        <v>44111.0</v>
+      </c>
+      <c r="C523" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D523" s="64" t="s">
+        <v>76</v>
+      </c>
+      <c r="E523" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F523" s="34"/>
-      <c r="G523" s="34"/>
-      <c r="H523" s="21"/>
-      <c r="I523" s="19"/>
-      <c r="J523" s="10"/>
-      <c r="K523" s="22"/>
-      <c r="L523" s="23"/>
-      <c r="M523" s="22"/>
+      <c r="G523" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H523" s="65" t="s">
+        <v>1926</v>
+      </c>
+      <c r="I523" s="66">
+        <v>44108.0</v>
+      </c>
+      <c r="J523" s="67">
+        <v>44109.0</v>
+      </c>
+      <c r="K523" s="63" t="s">
+        <v>1927</v>
+      </c>
+      <c r="L523" s="68" t="s">
+        <v>426</v>
+      </c>
+      <c r="M523" s="63" t="s">
+        <v>1928</v>
+      </c>
       <c r="N523" s="25"/>
-      <c r="O523" s="21"/>
-      <c r="P523" s="21"/>
+      <c r="O523" s="65" t="s">
+        <v>85</v>
+      </c>
+      <c r="P523" s="65" t="s">
+        <v>334</v>
+      </c>
       <c r="Q523" s="19"/>
       <c r="R523" s="19"/>
-      <c r="S523" s="20"/>
+      <c r="S523" s="61" t="s">
+        <v>1929</v>
+      </c>
       <c r="T523" s="20"/>
       <c r="U523" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#522</v>
       </c>
     </row>
     <row r="524">
-      <c r="A524" s="69"/>
-      <c r="B524" s="70"/>
-      <c r="C524" s="34"/>
-      <c r="D524" s="34"/>
-      <c r="E524" s="34"/>
+      <c r="A524" s="16" t="s">
+        <v>1930</v>
+      </c>
+      <c r="B524" s="6">
+        <v>44111.0</v>
+      </c>
+      <c r="C524" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D524" s="64" t="s">
+        <v>116</v>
+      </c>
+      <c r="E524" s="7" t="s">
+        <v>1931</v>
+      </c>
       <c r="F524" s="34"/>
-      <c r="G524" s="34"/>
-      <c r="H524" s="21"/>
-      <c r="I524" s="19"/>
-      <c r="J524" s="10"/>
-      <c r="K524" s="22"/>
-      <c r="L524" s="23"/>
-      <c r="M524" s="22"/>
+      <c r="G524" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H524" s="65" t="s">
+        <v>1932</v>
+      </c>
+      <c r="I524" s="66">
+        <v>44083.0</v>
+      </c>
+      <c r="J524" s="68" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K524" s="63" t="s">
+        <v>1933</v>
+      </c>
+      <c r="L524" s="12" t="s">
+        <v>1674</v>
+      </c>
+      <c r="M524" s="63" t="s">
+        <v>1442</v>
+      </c>
       <c r="N524" s="25"/>
-      <c r="O524" s="21"/>
-      <c r="P524" s="21"/>
+      <c r="O524" s="65" t="s">
+        <v>85</v>
+      </c>
+      <c r="P524" s="65" t="s">
+        <v>1934</v>
+      </c>
       <c r="Q524" s="19"/>
       <c r="R524" s="19"/>
-      <c r="S524" s="20"/>
+      <c r="S524" s="61" t="s">
+        <v>1929</v>
+      </c>
       <c r="T524" s="20"/>
       <c r="U524" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#523</v>
       </c>
     </row>
     <row r="525">
@@ -39695,15 +39790,17 @@
     <hyperlink r:id="rId82" ref="S520"/>
     <hyperlink r:id="rId83" ref="S521"/>
     <hyperlink r:id="rId84" ref="S522"/>
+    <hyperlink r:id="rId85" ref="S523"/>
+    <hyperlink r:id="rId86" ref="S524"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId85"/>
-  <legacyDrawing r:id="rId86"/>
+  <drawing r:id="rId87"/>
+  <legacyDrawing r:id="rId88"/>
   <tableParts count="2">
-    <tablePart r:id="rId89"/>
-    <tablePart r:id="rId90"/>
+    <tablePart r:id="rId91"/>
+    <tablePart r:id="rId92"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201009
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -563,7 +563,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5780" uniqueCount="1935">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5793" uniqueCount="1940">
   <si>
     <t>案例</t>
   </si>
@@ -7144,6 +7144,26 @@
     <t>因工作來台，持有登機前3日內檢驗陰性報告，入境迄今無疑似症狀
 9月9日入境後前往防疫旅館進行居家檢疫(9月9日至9月23日)
 9月24日至30日於飯店進行自主健康管理，10月5日因工作需求自費檢驗</t>
+  </si>
+  <si>
+    <t>#524</t>
+  </si>
+  <si>
+    <t>-9/15 菲律賓→台灣</t>
+  </si>
+  <si>
+    <t>9/15 採檢
+10/5 二採
+10/6 三採
+10/8 確診</t>
+  </si>
+  <si>
+    <t>9月15日入境後進行集中檢疫至9月29日
+9月30日檢疫期滿後搭乘專車至飯店
+10月5日由公司安排至醫院自費採檢，因檢驗結果呈現弱陽性，10月6日再次採檢，並於今日確診</t>
+  </si>
+  <si>
+    <t>國內新增1例境外移入COVID-19病例，為無症狀菲籍船員</t>
   </si>
 </sst>
 </file>
@@ -7280,7 +7300,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -7486,6 +7506,9 @@
       <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -38654,34 +38677,64 @@
       </c>
     </row>
     <row r="525">
-      <c r="A525" s="69"/>
-      <c r="B525" s="70"/>
-      <c r="C525" s="34"/>
-      <c r="D525" s="34"/>
-      <c r="E525" s="34"/>
+      <c r="A525" s="69" t="s">
+        <v>1935</v>
+      </c>
+      <c r="B525" s="6">
+        <v>44112.0</v>
+      </c>
+      <c r="C525" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D525" s="64" t="s">
+        <v>22</v>
+      </c>
+      <c r="E525" s="7" t="s">
+        <v>205</v>
+      </c>
       <c r="F525" s="34"/>
-      <c r="G525" s="34"/>
-      <c r="H525" s="21"/>
-      <c r="I525" s="19"/>
-      <c r="J525" s="10"/>
-      <c r="K525" s="22"/>
-      <c r="L525" s="23"/>
-      <c r="M525" s="22"/>
+      <c r="G525" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H525" s="65" t="s">
+        <v>1936</v>
+      </c>
+      <c r="I525" s="66">
+        <v>44089.0</v>
+      </c>
+      <c r="J525" s="68" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K525" s="63" t="s">
+        <v>1937</v>
+      </c>
+      <c r="L525" s="12" t="s">
+        <v>1674</v>
+      </c>
+      <c r="M525" s="63" t="s">
+        <v>1442</v>
+      </c>
       <c r="N525" s="25"/>
-      <c r="O525" s="21"/>
-      <c r="P525" s="21"/>
+      <c r="O525" s="65" t="s">
+        <v>85</v>
+      </c>
+      <c r="P525" s="65" t="s">
+        <v>1938</v>
+      </c>
       <c r="Q525" s="19"/>
       <c r="R525" s="19"/>
-      <c r="S525" s="20"/>
+      <c r="S525" s="61" t="s">
+        <v>1939</v>
+      </c>
       <c r="T525" s="20"/>
       <c r="U525" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#524</v>
       </c>
     </row>
     <row r="526">
-      <c r="A526" s="69"/>
-      <c r="B526" s="70"/>
+      <c r="A526" s="70"/>
+      <c r="B526" s="71"/>
       <c r="C526" s="34"/>
       <c r="D526" s="34"/>
       <c r="E526" s="34"/>
@@ -38706,8 +38759,8 @@
       </c>
     </row>
     <row r="527">
-      <c r="A527" s="69"/>
-      <c r="B527" s="70"/>
+      <c r="A527" s="70"/>
+      <c r="B527" s="71"/>
       <c r="C527" s="34"/>
       <c r="D527" s="34"/>
       <c r="E527" s="34"/>
@@ -38732,8 +38785,8 @@
       </c>
     </row>
     <row r="528">
-      <c r="A528" s="69"/>
-      <c r="B528" s="70"/>
+      <c r="A528" s="70"/>
+      <c r="B528" s="71"/>
       <c r="C528" s="34"/>
       <c r="D528" s="34"/>
       <c r="E528" s="34"/>
@@ -38758,8 +38811,8 @@
       </c>
     </row>
     <row r="529">
-      <c r="A529" s="69"/>
-      <c r="B529" s="70"/>
+      <c r="A529" s="70"/>
+      <c r="B529" s="71"/>
       <c r="C529" s="34"/>
       <c r="D529" s="34"/>
       <c r="E529" s="34"/>
@@ -38784,8 +38837,8 @@
       </c>
     </row>
     <row r="530">
-      <c r="A530" s="69"/>
-      <c r="B530" s="70"/>
+      <c r="A530" s="70"/>
+      <c r="B530" s="71"/>
       <c r="C530" s="34"/>
       <c r="D530" s="34"/>
       <c r="E530" s="34"/>
@@ -38810,8 +38863,8 @@
       </c>
     </row>
     <row r="531">
-      <c r="A531" s="69"/>
-      <c r="B531" s="70"/>
+      <c r="A531" s="70"/>
+      <c r="B531" s="71"/>
       <c r="C531" s="34"/>
       <c r="D531" s="34"/>
       <c r="E531" s="34"/>
@@ -38836,8 +38889,8 @@
       </c>
     </row>
     <row r="532">
-      <c r="A532" s="69"/>
-      <c r="B532" s="70"/>
+      <c r="A532" s="70"/>
+      <c r="B532" s="71"/>
       <c r="C532" s="34"/>
       <c r="D532" s="34"/>
       <c r="E532" s="34"/>
@@ -38862,8 +38915,8 @@
       </c>
     </row>
     <row r="533">
-      <c r="A533" s="69"/>
-      <c r="B533" s="70"/>
+      <c r="A533" s="70"/>
+      <c r="B533" s="71"/>
       <c r="C533" s="34"/>
       <c r="D533" s="34"/>
       <c r="E533" s="34"/>
@@ -38888,8 +38941,8 @@
       </c>
     </row>
     <row r="534">
-      <c r="A534" s="69"/>
-      <c r="B534" s="70"/>
+      <c r="A534" s="70"/>
+      <c r="B534" s="71"/>
       <c r="C534" s="34"/>
       <c r="D534" s="34"/>
       <c r="E534" s="34"/>
@@ -38914,8 +38967,8 @@
       </c>
     </row>
     <row r="535">
-      <c r="A535" s="69"/>
-      <c r="B535" s="70"/>
+      <c r="A535" s="70"/>
+      <c r="B535" s="71"/>
       <c r="C535" s="34"/>
       <c r="D535" s="34"/>
       <c r="E535" s="34"/>
@@ -38940,8 +38993,8 @@
       </c>
     </row>
     <row r="536">
-      <c r="A536" s="69"/>
-      <c r="B536" s="70"/>
+      <c r="A536" s="70"/>
+      <c r="B536" s="71"/>
       <c r="C536" s="34"/>
       <c r="D536" s="34"/>
       <c r="E536" s="34"/>
@@ -38966,8 +39019,8 @@
       </c>
     </row>
     <row r="537">
-      <c r="A537" s="69"/>
-      <c r="B537" s="70"/>
+      <c r="A537" s="70"/>
+      <c r="B537" s="71"/>
       <c r="C537" s="34"/>
       <c r="D537" s="34"/>
       <c r="E537" s="34"/>
@@ -38992,8 +39045,8 @@
       </c>
     </row>
     <row r="538">
-      <c r="A538" s="69"/>
-      <c r="B538" s="70"/>
+      <c r="A538" s="70"/>
+      <c r="B538" s="71"/>
       <c r="C538" s="34"/>
       <c r="D538" s="34"/>
       <c r="E538" s="34"/>
@@ -39018,8 +39071,8 @@
       </c>
     </row>
     <row r="539">
-      <c r="A539" s="69"/>
-      <c r="B539" s="70"/>
+      <c r="A539" s="70"/>
+      <c r="B539" s="71"/>
       <c r="C539" s="34"/>
       <c r="D539" s="34"/>
       <c r="E539" s="34"/>
@@ -39044,8 +39097,8 @@
       </c>
     </row>
     <row r="540">
-      <c r="A540" s="69"/>
-      <c r="B540" s="70"/>
+      <c r="A540" s="70"/>
+      <c r="B540" s="71"/>
       <c r="C540" s="34"/>
       <c r="D540" s="34"/>
       <c r="E540" s="34"/>
@@ -39070,8 +39123,8 @@
       </c>
     </row>
     <row r="541">
-      <c r="A541" s="69"/>
-      <c r="B541" s="70"/>
+      <c r="A541" s="70"/>
+      <c r="B541" s="71"/>
       <c r="C541" s="34"/>
       <c r="D541" s="34"/>
       <c r="E541" s="34"/>
@@ -39096,8 +39149,8 @@
       </c>
     </row>
     <row r="542">
-      <c r="A542" s="69"/>
-      <c r="B542" s="70"/>
+      <c r="A542" s="70"/>
+      <c r="B542" s="71"/>
       <c r="C542" s="34"/>
       <c r="D542" s="34"/>
       <c r="E542" s="34"/>
@@ -39122,8 +39175,8 @@
       </c>
     </row>
     <row r="543">
-      <c r="A543" s="69"/>
-      <c r="B543" s="70"/>
+      <c r="A543" s="70"/>
+      <c r="B543" s="71"/>
       <c r="C543" s="34"/>
       <c r="D543" s="34"/>
       <c r="E543" s="34"/>
@@ -39148,8 +39201,8 @@
       </c>
     </row>
     <row r="544">
-      <c r="A544" s="69"/>
-      <c r="B544" s="70"/>
+      <c r="A544" s="70"/>
+      <c r="B544" s="71"/>
       <c r="C544" s="34"/>
       <c r="D544" s="34"/>
       <c r="E544" s="34"/>
@@ -39174,8 +39227,8 @@
       </c>
     </row>
     <row r="545">
-      <c r="A545" s="69"/>
-      <c r="B545" s="70"/>
+      <c r="A545" s="70"/>
+      <c r="B545" s="71"/>
       <c r="C545" s="34"/>
       <c r="D545" s="34"/>
       <c r="E545" s="34"/>
@@ -39200,8 +39253,8 @@
       </c>
     </row>
     <row r="546">
-      <c r="A546" s="69"/>
-      <c r="B546" s="70"/>
+      <c r="A546" s="70"/>
+      <c r="B546" s="71"/>
       <c r="C546" s="34"/>
       <c r="D546" s="34"/>
       <c r="E546" s="34"/>
@@ -39226,8 +39279,8 @@
       </c>
     </row>
     <row r="547">
-      <c r="A547" s="69"/>
-      <c r="B547" s="70"/>
+      <c r="A547" s="70"/>
+      <c r="B547" s="71"/>
       <c r="C547" s="34"/>
       <c r="D547" s="34"/>
       <c r="E547" s="34"/>
@@ -39252,8 +39305,8 @@
       </c>
     </row>
     <row r="548">
-      <c r="A548" s="69"/>
-      <c r="B548" s="70"/>
+      <c r="A548" s="70"/>
+      <c r="B548" s="71"/>
       <c r="C548" s="34"/>
       <c r="D548" s="34"/>
       <c r="E548" s="34"/>
@@ -39278,8 +39331,8 @@
       </c>
     </row>
     <row r="549">
-      <c r="A549" s="69"/>
-      <c r="B549" s="70"/>
+      <c r="A549" s="70"/>
+      <c r="B549" s="71"/>
       <c r="C549" s="34"/>
       <c r="D549" s="34"/>
       <c r="E549" s="34"/>
@@ -39304,8 +39357,8 @@
       </c>
     </row>
     <row r="550">
-      <c r="A550" s="69"/>
-      <c r="B550" s="70"/>
+      <c r="A550" s="70"/>
+      <c r="B550" s="71"/>
       <c r="C550" s="34"/>
       <c r="D550" s="34"/>
       <c r="E550" s="34"/>
@@ -39330,8 +39383,8 @@
       </c>
     </row>
     <row r="551">
-      <c r="A551" s="69"/>
-      <c r="B551" s="70"/>
+      <c r="A551" s="70"/>
+      <c r="B551" s="71"/>
       <c r="C551" s="34"/>
       <c r="D551" s="34"/>
       <c r="E551" s="34"/>
@@ -39792,15 +39845,16 @@
     <hyperlink r:id="rId84" ref="S522"/>
     <hyperlink r:id="rId85" ref="S523"/>
     <hyperlink r:id="rId86" ref="S524"/>
+    <hyperlink r:id="rId87" ref="S525"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId87"/>
-  <legacyDrawing r:id="rId88"/>
+  <drawing r:id="rId88"/>
+  <legacyDrawing r:id="rId89"/>
   <tableParts count="2">
-    <tablePart r:id="rId91"/>
     <tablePart r:id="rId92"/>
+    <tablePart r:id="rId93"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201010
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -563,7 +563,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5793" uniqueCount="1940">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5830" uniqueCount="1952">
   <si>
     <t>案例</t>
   </si>
@@ -7164,6 +7164,45 @@
   </si>
   <si>
     <t>國內新增1例境外移入COVID-19病例，為無症狀菲籍船員</t>
+  </si>
+  <si>
+    <t>#525</t>
+  </si>
+  <si>
+    <t>-9/24 菲律賓→台灣</t>
+  </si>
+  <si>
+    <t>10/7 採檢
+10/9 確診</t>
+  </si>
+  <si>
+    <t>入境時無症狀，10月7日集中檢疫期滿前進行採檢</t>
+  </si>
+  <si>
+    <t>國內新增3例境外移入COVID-19病例，分別自菲律賓及烏克蘭入境</t>
+  </si>
+  <si>
+    <t>#526</t>
+  </si>
+  <si>
+    <t>10/7 採檢
+10/8 二採
+10/9 確診</t>
+  </si>
+  <si>
+    <t>入境時無症狀，10月7日集中檢疫期滿前採檢為弱陽性，10月8日再次採檢</t>
+  </si>
+  <si>
+    <t>#527</t>
+  </si>
+  <si>
+    <t>烏克蘭</t>
+  </si>
+  <si>
+    <t>-9/22 烏克蘭→台灣</t>
+  </si>
+  <si>
+    <t>於10月7日居家檢疫期滿解除後，由公司安排自費採檢</t>
   </si>
 </sst>
 </file>
@@ -7251,10 +7290,10 @@
       <u/>
       <color rgb="FF1155CC"/>
     </font>
+    <font/>
     <font>
       <color rgb="FF000000"/>
     </font>
-    <font/>
   </fonts>
   <fills count="7">
     <fill>
@@ -7300,7 +7339,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="70">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -7491,25 +7530,19 @@
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="18" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="17" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
@@ -38543,7 +38576,7 @@
       <c r="L522" s="12" t="s">
         <v>363</v>
       </c>
-      <c r="M522" s="63" t="s">
+      <c r="M522" s="13" t="s">
         <v>1923</v>
       </c>
       <c r="N522" s="25"/>
@@ -38574,7 +38607,7 @@
       <c r="C523" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D523" s="64" t="s">
+      <c r="D523" s="7" t="s">
         <v>76</v>
       </c>
       <c r="E523" s="7" t="s">
@@ -38584,29 +38617,29 @@
       <c r="G523" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H523" s="65" t="s">
+      <c r="H523" s="8" t="s">
         <v>1926</v>
       </c>
-      <c r="I523" s="66">
+      <c r="I523" s="9">
         <v>44108.0</v>
       </c>
-      <c r="J523" s="67">
+      <c r="J523" s="10">
         <v>44109.0</v>
       </c>
-      <c r="K523" s="63" t="s">
+      <c r="K523" s="13" t="s">
         <v>1927</v>
       </c>
-      <c r="L523" s="68" t="s">
+      <c r="L523" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M523" s="63" t="s">
+      <c r="M523" s="13" t="s">
         <v>1928</v>
       </c>
       <c r="N523" s="25"/>
-      <c r="O523" s="65" t="s">
+      <c r="O523" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P523" s="65" t="s">
+      <c r="P523" s="8" t="s">
         <v>334</v>
       </c>
       <c r="Q523" s="19"/>
@@ -38630,7 +38663,7 @@
       <c r="C524" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D524" s="64" t="s">
+      <c r="D524" s="7" t="s">
         <v>116</v>
       </c>
       <c r="E524" s="7" t="s">
@@ -38640,29 +38673,29 @@
       <c r="G524" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H524" s="65" t="s">
+      <c r="H524" s="8" t="s">
         <v>1932</v>
       </c>
-      <c r="I524" s="66">
+      <c r="I524" s="9">
         <v>44083.0</v>
       </c>
-      <c r="J524" s="68" t="s">
+      <c r="J524" s="12" t="s">
         <v>1442</v>
       </c>
-      <c r="K524" s="63" t="s">
+      <c r="K524" s="13" t="s">
         <v>1933</v>
       </c>
       <c r="L524" s="12" t="s">
         <v>1674</v>
       </c>
-      <c r="M524" s="63" t="s">
+      <c r="M524" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N524" s="25"/>
-      <c r="O524" s="65" t="s">
+      <c r="O524" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P524" s="65" t="s">
+      <c r="P524" s="8" t="s">
         <v>1934</v>
       </c>
       <c r="Q524" s="19"/>
@@ -38677,7 +38710,7 @@
       </c>
     </row>
     <row r="525">
-      <c r="A525" s="69" t="s">
+      <c r="A525" s="16" t="s">
         <v>1935</v>
       </c>
       <c r="B525" s="6">
@@ -38686,7 +38719,7 @@
       <c r="C525" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D525" s="64" t="s">
+      <c r="D525" s="7" t="s">
         <v>22</v>
       </c>
       <c r="E525" s="7" t="s">
@@ -38696,29 +38729,29 @@
       <c r="G525" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H525" s="65" t="s">
+      <c r="H525" s="8" t="s">
         <v>1936</v>
       </c>
-      <c r="I525" s="66">
+      <c r="I525" s="9">
         <v>44089.0</v>
       </c>
-      <c r="J525" s="68" t="s">
+      <c r="J525" s="12" t="s">
         <v>1442</v>
       </c>
-      <c r="K525" s="63" t="s">
+      <c r="K525" s="13" t="s">
         <v>1937</v>
       </c>
       <c r="L525" s="12" t="s">
         <v>1674</v>
       </c>
-      <c r="M525" s="63" t="s">
+      <c r="M525" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N525" s="25"/>
-      <c r="O525" s="65" t="s">
+      <c r="O525" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P525" s="65" t="s">
+      <c r="P525" s="8" t="s">
         <v>1938</v>
       </c>
       <c r="Q525" s="19"/>
@@ -38733,86 +38766,172 @@
       </c>
     </row>
     <row r="526">
-      <c r="A526" s="70"/>
-      <c r="B526" s="71"/>
-      <c r="C526" s="34"/>
-      <c r="D526" s="34"/>
-      <c r="E526" s="34"/>
+      <c r="A526" s="16" t="s">
+        <v>1940</v>
+      </c>
+      <c r="B526" s="6">
+        <v>44113.0</v>
+      </c>
+      <c r="C526" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D526" s="63" t="s">
+        <v>76</v>
+      </c>
+      <c r="E526" s="7" t="s">
+        <v>205</v>
+      </c>
       <c r="F526" s="34"/>
-      <c r="G526" s="34"/>
-      <c r="H526" s="21"/>
-      <c r="I526" s="19"/>
-      <c r="J526" s="10"/>
-      <c r="K526" s="22"/>
-      <c r="L526" s="23"/>
-      <c r="M526" s="22"/>
+      <c r="G526" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H526" s="64" t="s">
+        <v>1941</v>
+      </c>
+      <c r="I526" s="65">
+        <v>44098.0</v>
+      </c>
+      <c r="J526" s="66" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K526" s="13" t="s">
+        <v>1942</v>
+      </c>
+      <c r="L526" s="66" t="s">
+        <v>426</v>
+      </c>
+      <c r="M526" s="67" t="s">
+        <v>1442</v>
+      </c>
       <c r="N526" s="25"/>
-      <c r="O526" s="21"/>
-      <c r="P526" s="21"/>
+      <c r="O526" s="64" t="s">
+        <v>85</v>
+      </c>
+      <c r="P526" s="64" t="s">
+        <v>1943</v>
+      </c>
       <c r="Q526" s="19"/>
       <c r="R526" s="19"/>
-      <c r="S526" s="20"/>
+      <c r="S526" s="61" t="s">
+        <v>1944</v>
+      </c>
       <c r="T526" s="20"/>
       <c r="U526" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#525</v>
       </c>
     </row>
     <row r="527">
-      <c r="A527" s="70"/>
-      <c r="B527" s="71"/>
-      <c r="C527" s="34"/>
-      <c r="D527" s="34"/>
-      <c r="E527" s="34"/>
+      <c r="A527" s="16" t="s">
+        <v>1945</v>
+      </c>
+      <c r="B527" s="6">
+        <v>44113.0</v>
+      </c>
+      <c r="C527" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D527" s="63" t="s">
+        <v>116</v>
+      </c>
+      <c r="E527" s="7" t="s">
+        <v>205</v>
+      </c>
       <c r="F527" s="34"/>
-      <c r="G527" s="34"/>
-      <c r="H527" s="21"/>
-      <c r="I527" s="19"/>
-      <c r="J527" s="10"/>
-      <c r="K527" s="22"/>
-      <c r="L527" s="23"/>
-      <c r="M527" s="22"/>
+      <c r="G527" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H527" s="64" t="s">
+        <v>1941</v>
+      </c>
+      <c r="I527" s="65">
+        <v>44098.0</v>
+      </c>
+      <c r="J527" s="66" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K527" s="13" t="s">
+        <v>1946</v>
+      </c>
+      <c r="L527" s="66" t="s">
+        <v>426</v>
+      </c>
+      <c r="M527" s="67" t="s">
+        <v>1442</v>
+      </c>
       <c r="N527" s="25"/>
-      <c r="O527" s="21"/>
-      <c r="P527" s="21"/>
+      <c r="O527" s="64" t="s">
+        <v>85</v>
+      </c>
+      <c r="P527" s="64" t="s">
+        <v>1947</v>
+      </c>
       <c r="Q527" s="19"/>
       <c r="R527" s="19"/>
-      <c r="S527" s="20"/>
+      <c r="S527" s="61" t="s">
+        <v>1944</v>
+      </c>
       <c r="T527" s="20"/>
       <c r="U527" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#526</v>
       </c>
     </row>
     <row r="528">
-      <c r="A528" s="70"/>
-      <c r="B528" s="71"/>
-      <c r="C528" s="34"/>
-      <c r="D528" s="34"/>
-      <c r="E528" s="34"/>
+      <c r="A528" s="16" t="s">
+        <v>1948</v>
+      </c>
+      <c r="B528" s="6">
+        <v>44113.0</v>
+      </c>
+      <c r="C528" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D528" s="63" t="s">
+        <v>116</v>
+      </c>
+      <c r="E528" s="7" t="s">
+        <v>1949</v>
+      </c>
       <c r="F528" s="34"/>
-      <c r="G528" s="34"/>
-      <c r="H528" s="21"/>
-      <c r="I528" s="19"/>
-      <c r="J528" s="10"/>
-      <c r="K528" s="22"/>
-      <c r="L528" s="23"/>
-      <c r="M528" s="22"/>
+      <c r="G528" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H528" s="64" t="s">
+        <v>1950</v>
+      </c>
+      <c r="I528" s="65">
+        <v>44096.0</v>
+      </c>
+      <c r="J528" s="12"/>
+      <c r="K528" s="13" t="s">
+        <v>1942</v>
+      </c>
+      <c r="L528" s="12" t="s">
+        <v>1674</v>
+      </c>
+      <c r="M528" s="67"/>
       <c r="N528" s="25"/>
-      <c r="O528" s="21"/>
-      <c r="P528" s="21"/>
+      <c r="O528" s="64" t="s">
+        <v>85</v>
+      </c>
+      <c r="P528" s="64" t="s">
+        <v>1951</v>
+      </c>
       <c r="Q528" s="19"/>
       <c r="R528" s="19"/>
-      <c r="S528" s="20"/>
+      <c r="S528" s="61" t="s">
+        <v>1944</v>
+      </c>
       <c r="T528" s="20"/>
       <c r="U528" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#527</v>
       </c>
     </row>
     <row r="529">
-      <c r="A529" s="70"/>
-      <c r="B529" s="71"/>
+      <c r="A529" s="68"/>
+      <c r="B529" s="69"/>
       <c r="C529" s="34"/>
       <c r="D529" s="34"/>
       <c r="E529" s="34"/>
@@ -38837,8 +38956,8 @@
       </c>
     </row>
     <row r="530">
-      <c r="A530" s="70"/>
-      <c r="B530" s="71"/>
+      <c r="A530" s="68"/>
+      <c r="B530" s="69"/>
       <c r="C530" s="34"/>
       <c r="D530" s="34"/>
       <c r="E530" s="34"/>
@@ -38863,8 +38982,8 @@
       </c>
     </row>
     <row r="531">
-      <c r="A531" s="70"/>
-      <c r="B531" s="71"/>
+      <c r="A531" s="68"/>
+      <c r="B531" s="69"/>
       <c r="C531" s="34"/>
       <c r="D531" s="34"/>
       <c r="E531" s="34"/>
@@ -38889,8 +39008,8 @@
       </c>
     </row>
     <row r="532">
-      <c r="A532" s="70"/>
-      <c r="B532" s="71"/>
+      <c r="A532" s="68"/>
+      <c r="B532" s="69"/>
       <c r="C532" s="34"/>
       <c r="D532" s="34"/>
       <c r="E532" s="34"/>
@@ -38915,8 +39034,8 @@
       </c>
     </row>
     <row r="533">
-      <c r="A533" s="70"/>
-      <c r="B533" s="71"/>
+      <c r="A533" s="68"/>
+      <c r="B533" s="69"/>
       <c r="C533" s="34"/>
       <c r="D533" s="34"/>
       <c r="E533" s="34"/>
@@ -38941,8 +39060,8 @@
       </c>
     </row>
     <row r="534">
-      <c r="A534" s="70"/>
-      <c r="B534" s="71"/>
+      <c r="A534" s="68"/>
+      <c r="B534" s="69"/>
       <c r="C534" s="34"/>
       <c r="D534" s="34"/>
       <c r="E534" s="34"/>
@@ -38967,8 +39086,8 @@
       </c>
     </row>
     <row r="535">
-      <c r="A535" s="70"/>
-      <c r="B535" s="71"/>
+      <c r="A535" s="68"/>
+      <c r="B535" s="69"/>
       <c r="C535" s="34"/>
       <c r="D535" s="34"/>
       <c r="E535" s="34"/>
@@ -38993,8 +39112,8 @@
       </c>
     </row>
     <row r="536">
-      <c r="A536" s="70"/>
-      <c r="B536" s="71"/>
+      <c r="A536" s="68"/>
+      <c r="B536" s="69"/>
       <c r="C536" s="34"/>
       <c r="D536" s="34"/>
       <c r="E536" s="34"/>
@@ -39019,8 +39138,8 @@
       </c>
     </row>
     <row r="537">
-      <c r="A537" s="70"/>
-      <c r="B537" s="71"/>
+      <c r="A537" s="68"/>
+      <c r="B537" s="69"/>
       <c r="C537" s="34"/>
       <c r="D537" s="34"/>
       <c r="E537" s="34"/>
@@ -39045,8 +39164,8 @@
       </c>
     </row>
     <row r="538">
-      <c r="A538" s="70"/>
-      <c r="B538" s="71"/>
+      <c r="A538" s="68"/>
+      <c r="B538" s="69"/>
       <c r="C538" s="34"/>
       <c r="D538" s="34"/>
       <c r="E538" s="34"/>
@@ -39071,8 +39190,8 @@
       </c>
     </row>
     <row r="539">
-      <c r="A539" s="70"/>
-      <c r="B539" s="71"/>
+      <c r="A539" s="68"/>
+      <c r="B539" s="69"/>
       <c r="C539" s="34"/>
       <c r="D539" s="34"/>
       <c r="E539" s="34"/>
@@ -39097,8 +39216,8 @@
       </c>
     </row>
     <row r="540">
-      <c r="A540" s="70"/>
-      <c r="B540" s="71"/>
+      <c r="A540" s="68"/>
+      <c r="B540" s="69"/>
       <c r="C540" s="34"/>
       <c r="D540" s="34"/>
       <c r="E540" s="34"/>
@@ -39123,8 +39242,8 @@
       </c>
     </row>
     <row r="541">
-      <c r="A541" s="70"/>
-      <c r="B541" s="71"/>
+      <c r="A541" s="68"/>
+      <c r="B541" s="69"/>
       <c r="C541" s="34"/>
       <c r="D541" s="34"/>
       <c r="E541" s="34"/>
@@ -39149,8 +39268,8 @@
       </c>
     </row>
     <row r="542">
-      <c r="A542" s="70"/>
-      <c r="B542" s="71"/>
+      <c r="A542" s="68"/>
+      <c r="B542" s="69"/>
       <c r="C542" s="34"/>
       <c r="D542" s="34"/>
       <c r="E542" s="34"/>
@@ -39175,8 +39294,8 @@
       </c>
     </row>
     <row r="543">
-      <c r="A543" s="70"/>
-      <c r="B543" s="71"/>
+      <c r="A543" s="68"/>
+      <c r="B543" s="69"/>
       <c r="C543" s="34"/>
       <c r="D543" s="34"/>
       <c r="E543" s="34"/>
@@ -39201,8 +39320,8 @@
       </c>
     </row>
     <row r="544">
-      <c r="A544" s="70"/>
-      <c r="B544" s="71"/>
+      <c r="A544" s="68"/>
+      <c r="B544" s="69"/>
       <c r="C544" s="34"/>
       <c r="D544" s="34"/>
       <c r="E544" s="34"/>
@@ -39227,8 +39346,8 @@
       </c>
     </row>
     <row r="545">
-      <c r="A545" s="70"/>
-      <c r="B545" s="71"/>
+      <c r="A545" s="68"/>
+      <c r="B545" s="69"/>
       <c r="C545" s="34"/>
       <c r="D545" s="34"/>
       <c r="E545" s="34"/>
@@ -39253,8 +39372,8 @@
       </c>
     </row>
     <row r="546">
-      <c r="A546" s="70"/>
-      <c r="B546" s="71"/>
+      <c r="A546" s="68"/>
+      <c r="B546" s="69"/>
       <c r="C546" s="34"/>
       <c r="D546" s="34"/>
       <c r="E546" s="34"/>
@@ -39279,8 +39398,8 @@
       </c>
     </row>
     <row r="547">
-      <c r="A547" s="70"/>
-      <c r="B547" s="71"/>
+      <c r="A547" s="68"/>
+      <c r="B547" s="69"/>
       <c r="C547" s="34"/>
       <c r="D547" s="34"/>
       <c r="E547" s="34"/>
@@ -39305,8 +39424,8 @@
       </c>
     </row>
     <row r="548">
-      <c r="A548" s="70"/>
-      <c r="B548" s="71"/>
+      <c r="A548" s="68"/>
+      <c r="B548" s="69"/>
       <c r="C548" s="34"/>
       <c r="D548" s="34"/>
       <c r="E548" s="34"/>
@@ -39331,8 +39450,8 @@
       </c>
     </row>
     <row r="549">
-      <c r="A549" s="70"/>
-      <c r="B549" s="71"/>
+      <c r="A549" s="68"/>
+      <c r="B549" s="69"/>
       <c r="C549" s="34"/>
       <c r="D549" s="34"/>
       <c r="E549" s="34"/>
@@ -39357,8 +39476,8 @@
       </c>
     </row>
     <row r="550">
-      <c r="A550" s="70"/>
-      <c r="B550" s="71"/>
+      <c r="A550" s="68"/>
+      <c r="B550" s="69"/>
       <c r="C550" s="34"/>
       <c r="D550" s="34"/>
       <c r="E550" s="34"/>
@@ -39383,8 +39502,8 @@
       </c>
     </row>
     <row r="551">
-      <c r="A551" s="70"/>
-      <c r="B551" s="71"/>
+      <c r="A551" s="68"/>
+      <c r="B551" s="69"/>
       <c r="C551" s="34"/>
       <c r="D551" s="34"/>
       <c r="E551" s="34"/>
@@ -39846,15 +39965,18 @@
     <hyperlink r:id="rId85" ref="S523"/>
     <hyperlink r:id="rId86" ref="S524"/>
     <hyperlink r:id="rId87" ref="S525"/>
+    <hyperlink r:id="rId88" ref="S526"/>
+    <hyperlink r:id="rId89" ref="S527"/>
+    <hyperlink r:id="rId90" ref="S528"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId88"/>
-  <legacyDrawing r:id="rId89"/>
+  <drawing r:id="rId91"/>
+  <legacyDrawing r:id="rId92"/>
   <tableParts count="2">
-    <tablePart r:id="rId92"/>
-    <tablePart r:id="rId93"/>
+    <tablePart r:id="rId95"/>
+    <tablePart r:id="rId96"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201013
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -563,7 +563,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5830" uniqueCount="1952">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5854" uniqueCount="1963">
   <si>
     <t>案例</t>
   </si>
@@ -7204,6 +7204,41 @@
   <si>
     <t>於10月7日居家檢疫期滿解除後，由公司安排自費採檢</t>
   </si>
+  <si>
+    <t>#528</t>
+  </si>
+  <si>
+    <t>1月-10/4 法國</t>
+  </si>
+  <si>
+    <t>10/9 採檢
+10/12 確診</t>
+  </si>
+  <si>
+    <t>流鼻水 喉嚨癢</t>
+  </si>
+  <si>
+    <t>入境時無症狀</t>
+  </si>
+  <si>
+    <t>2女分自法國、杜拜返國，居家檢疫期間確診</t>
+  </si>
+  <si>
+    <t>#529</t>
+  </si>
+  <si>
+    <t>1月-9/30 杜拜</t>
+  </si>
+  <si>
+    <t>10/10 採檢
+10/12 確診</t>
+  </si>
+  <si>
+    <t>味覺異常</t>
+  </si>
+  <si>
+    <t>長期於杜拜及其他國家工作</t>
+  </si>
 </sst>
 </file>
 
@@ -7213,7 +7248,7 @@
     <numFmt numFmtId="164" formatCode="mm&quot;月&quot;dd&quot;日 &quot;dddd"/>
     <numFmt numFmtId="165" formatCode="m/d"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="17">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -7290,10 +7325,6 @@
       <u/>
       <color rgb="FF1155CC"/>
     </font>
-    <font/>
-    <font>
-      <color rgb="FF000000"/>
-    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -7339,7 +7370,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="65">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -7528,21 +7559,6 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
@@ -38775,7 +38791,7 @@
       <c r="C526" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D526" s="63" t="s">
+      <c r="D526" s="7" t="s">
         <v>76</v>
       </c>
       <c r="E526" s="7" t="s">
@@ -38785,29 +38801,29 @@
       <c r="G526" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H526" s="64" t="s">
+      <c r="H526" s="8" t="s">
         <v>1941</v>
       </c>
-      <c r="I526" s="65">
+      <c r="I526" s="9">
         <v>44098.0</v>
       </c>
-      <c r="J526" s="66" t="s">
+      <c r="J526" s="12" t="s">
         <v>1442</v>
       </c>
       <c r="K526" s="13" t="s">
         <v>1942</v>
       </c>
-      <c r="L526" s="66" t="s">
+      <c r="L526" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M526" s="67" t="s">
+      <c r="M526" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N526" s="25"/>
-      <c r="O526" s="64" t="s">
+      <c r="O526" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P526" s="64" t="s">
+      <c r="P526" s="8" t="s">
         <v>1943</v>
       </c>
       <c r="Q526" s="19"/>
@@ -38831,7 +38847,7 @@
       <c r="C527" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D527" s="63" t="s">
+      <c r="D527" s="7" t="s">
         <v>116</v>
       </c>
       <c r="E527" s="7" t="s">
@@ -38841,29 +38857,29 @@
       <c r="G527" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H527" s="64" t="s">
+      <c r="H527" s="8" t="s">
         <v>1941</v>
       </c>
-      <c r="I527" s="65">
+      <c r="I527" s="9">
         <v>44098.0</v>
       </c>
-      <c r="J527" s="66" t="s">
+      <c r="J527" s="12" t="s">
         <v>1442</v>
       </c>
       <c r="K527" s="13" t="s">
         <v>1946</v>
       </c>
-      <c r="L527" s="66" t="s">
+      <c r="L527" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M527" s="67" t="s">
+      <c r="M527" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N527" s="25"/>
-      <c r="O527" s="64" t="s">
+      <c r="O527" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P527" s="64" t="s">
+      <c r="P527" s="8" t="s">
         <v>1947</v>
       </c>
       <c r="Q527" s="19"/>
@@ -38887,7 +38903,7 @@
       <c r="C528" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D528" s="63" t="s">
+      <c r="D528" s="7" t="s">
         <v>116</v>
       </c>
       <c r="E528" s="7" t="s">
@@ -38897,10 +38913,10 @@
       <c r="G528" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H528" s="64" t="s">
+      <c r="H528" s="8" t="s">
         <v>1950</v>
       </c>
-      <c r="I528" s="65">
+      <c r="I528" s="9">
         <v>44096.0</v>
       </c>
       <c r="J528" s="12"/>
@@ -38910,12 +38926,12 @@
       <c r="L528" s="12" t="s">
         <v>1674</v>
       </c>
-      <c r="M528" s="67"/>
+      <c r="M528" s="13"/>
       <c r="N528" s="25"/>
-      <c r="O528" s="64" t="s">
+      <c r="O528" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P528" s="64" t="s">
+      <c r="P528" s="8" t="s">
         <v>1951</v>
       </c>
       <c r="Q528" s="19"/>
@@ -38930,60 +38946,120 @@
       </c>
     </row>
     <row r="529">
-      <c r="A529" s="68"/>
-      <c r="B529" s="69"/>
-      <c r="C529" s="34"/>
-      <c r="D529" s="34"/>
-      <c r="E529" s="34"/>
+      <c r="A529" s="16" t="s">
+        <v>1952</v>
+      </c>
+      <c r="B529" s="6">
+        <v>44116.0</v>
+      </c>
+      <c r="C529" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D529" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E529" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F529" s="34"/>
-      <c r="G529" s="34"/>
-      <c r="H529" s="21"/>
-      <c r="I529" s="19"/>
-      <c r="J529" s="10"/>
-      <c r="K529" s="22"/>
-      <c r="L529" s="23"/>
-      <c r="M529" s="22"/>
+      <c r="G529" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H529" s="8" t="s">
+        <v>1953</v>
+      </c>
+      <c r="I529" s="9">
+        <v>44108.0</v>
+      </c>
+      <c r="J529" s="10">
+        <v>44111.0</v>
+      </c>
+      <c r="K529" s="13" t="s">
+        <v>1954</v>
+      </c>
+      <c r="L529" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M529" s="13" t="s">
+        <v>1955</v>
+      </c>
       <c r="N529" s="25"/>
-      <c r="O529" s="21"/>
-      <c r="P529" s="21"/>
+      <c r="O529" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P529" s="8" t="s">
+        <v>1956</v>
+      </c>
       <c r="Q529" s="19"/>
       <c r="R529" s="19"/>
-      <c r="S529" s="20"/>
+      <c r="S529" s="61" t="s">
+        <v>1957</v>
+      </c>
       <c r="T529" s="20"/>
       <c r="U529" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#528</v>
       </c>
     </row>
     <row r="530">
-      <c r="A530" s="68"/>
-      <c r="B530" s="69"/>
-      <c r="C530" s="34"/>
-      <c r="D530" s="34"/>
-      <c r="E530" s="34"/>
+      <c r="A530" s="16" t="s">
+        <v>1958</v>
+      </c>
+      <c r="B530" s="6">
+        <v>44116.0</v>
+      </c>
+      <c r="C530" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D530" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E530" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F530" s="34"/>
-      <c r="G530" s="34"/>
-      <c r="H530" s="21"/>
-      <c r="I530" s="19"/>
-      <c r="J530" s="10"/>
-      <c r="K530" s="22"/>
-      <c r="L530" s="23"/>
-      <c r="M530" s="22"/>
+      <c r="G530" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H530" s="8" t="s">
+        <v>1959</v>
+      </c>
+      <c r="I530" s="9">
+        <v>44104.0</v>
+      </c>
+      <c r="J530" s="10">
+        <v>44114.0</v>
+      </c>
+      <c r="K530" s="13" t="s">
+        <v>1960</v>
+      </c>
+      <c r="L530" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M530" s="13" t="s">
+        <v>1961</v>
+      </c>
       <c r="N530" s="25"/>
-      <c r="O530" s="21"/>
-      <c r="P530" s="21"/>
+      <c r="O530" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P530" s="8" t="s">
+        <v>1962</v>
+      </c>
       <c r="Q530" s="19"/>
       <c r="R530" s="19"/>
-      <c r="S530" s="20"/>
+      <c r="S530" s="61" t="s">
+        <v>1957</v>
+      </c>
       <c r="T530" s="20"/>
       <c r="U530" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#529</v>
       </c>
     </row>
     <row r="531">
-      <c r="A531" s="68"/>
-      <c r="B531" s="69"/>
+      <c r="A531" s="63"/>
+      <c r="B531" s="64"/>
       <c r="C531" s="34"/>
       <c r="D531" s="34"/>
       <c r="E531" s="34"/>
@@ -39008,8 +39084,8 @@
       </c>
     </row>
     <row r="532">
-      <c r="A532" s="68"/>
-      <c r="B532" s="69"/>
+      <c r="A532" s="63"/>
+      <c r="B532" s="64"/>
       <c r="C532" s="34"/>
       <c r="D532" s="34"/>
       <c r="E532" s="34"/>
@@ -39034,8 +39110,8 @@
       </c>
     </row>
     <row r="533">
-      <c r="A533" s="68"/>
-      <c r="B533" s="69"/>
+      <c r="A533" s="63"/>
+      <c r="B533" s="64"/>
       <c r="C533" s="34"/>
       <c r="D533" s="34"/>
       <c r="E533" s="34"/>
@@ -39060,8 +39136,8 @@
       </c>
     </row>
     <row r="534">
-      <c r="A534" s="68"/>
-      <c r="B534" s="69"/>
+      <c r="A534" s="63"/>
+      <c r="B534" s="64"/>
       <c r="C534" s="34"/>
       <c r="D534" s="34"/>
       <c r="E534" s="34"/>
@@ -39086,8 +39162,8 @@
       </c>
     </row>
     <row r="535">
-      <c r="A535" s="68"/>
-      <c r="B535" s="69"/>
+      <c r="A535" s="63"/>
+      <c r="B535" s="64"/>
       <c r="C535" s="34"/>
       <c r="D535" s="34"/>
       <c r="E535" s="34"/>
@@ -39112,8 +39188,8 @@
       </c>
     </row>
     <row r="536">
-      <c r="A536" s="68"/>
-      <c r="B536" s="69"/>
+      <c r="A536" s="63"/>
+      <c r="B536" s="64"/>
       <c r="C536" s="34"/>
       <c r="D536" s="34"/>
       <c r="E536" s="34"/>
@@ -39138,8 +39214,8 @@
       </c>
     </row>
     <row r="537">
-      <c r="A537" s="68"/>
-      <c r="B537" s="69"/>
+      <c r="A537" s="63"/>
+      <c r="B537" s="64"/>
       <c r="C537" s="34"/>
       <c r="D537" s="34"/>
       <c r="E537" s="34"/>
@@ -39164,8 +39240,8 @@
       </c>
     </row>
     <row r="538">
-      <c r="A538" s="68"/>
-      <c r="B538" s="69"/>
+      <c r="A538" s="63"/>
+      <c r="B538" s="64"/>
       <c r="C538" s="34"/>
       <c r="D538" s="34"/>
       <c r="E538" s="34"/>
@@ -39190,8 +39266,8 @@
       </c>
     </row>
     <row r="539">
-      <c r="A539" s="68"/>
-      <c r="B539" s="69"/>
+      <c r="A539" s="63"/>
+      <c r="B539" s="64"/>
       <c r="C539" s="34"/>
       <c r="D539" s="34"/>
       <c r="E539" s="34"/>
@@ -39216,8 +39292,8 @@
       </c>
     </row>
     <row r="540">
-      <c r="A540" s="68"/>
-      <c r="B540" s="69"/>
+      <c r="A540" s="63"/>
+      <c r="B540" s="64"/>
       <c r="C540" s="34"/>
       <c r="D540" s="34"/>
       <c r="E540" s="34"/>
@@ -39242,8 +39318,8 @@
       </c>
     </row>
     <row r="541">
-      <c r="A541" s="68"/>
-      <c r="B541" s="69"/>
+      <c r="A541" s="63"/>
+      <c r="B541" s="64"/>
       <c r="C541" s="34"/>
       <c r="D541" s="34"/>
       <c r="E541" s="34"/>
@@ -39268,8 +39344,8 @@
       </c>
     </row>
     <row r="542">
-      <c r="A542" s="68"/>
-      <c r="B542" s="69"/>
+      <c r="A542" s="63"/>
+      <c r="B542" s="64"/>
       <c r="C542" s="34"/>
       <c r="D542" s="34"/>
       <c r="E542" s="34"/>
@@ -39294,8 +39370,8 @@
       </c>
     </row>
     <row r="543">
-      <c r="A543" s="68"/>
-      <c r="B543" s="69"/>
+      <c r="A543" s="63"/>
+      <c r="B543" s="64"/>
       <c r="C543" s="34"/>
       <c r="D543" s="34"/>
       <c r="E543" s="34"/>
@@ -39320,8 +39396,8 @@
       </c>
     </row>
     <row r="544">
-      <c r="A544" s="68"/>
-      <c r="B544" s="69"/>
+      <c r="A544" s="63"/>
+      <c r="B544" s="64"/>
       <c r="C544" s="34"/>
       <c r="D544" s="34"/>
       <c r="E544" s="34"/>
@@ -39346,8 +39422,8 @@
       </c>
     </row>
     <row r="545">
-      <c r="A545" s="68"/>
-      <c r="B545" s="69"/>
+      <c r="A545" s="63"/>
+      <c r="B545" s="64"/>
       <c r="C545" s="34"/>
       <c r="D545" s="34"/>
       <c r="E545" s="34"/>
@@ -39372,8 +39448,8 @@
       </c>
     </row>
     <row r="546">
-      <c r="A546" s="68"/>
-      <c r="B546" s="69"/>
+      <c r="A546" s="63"/>
+      <c r="B546" s="64"/>
       <c r="C546" s="34"/>
       <c r="D546" s="34"/>
       <c r="E546" s="34"/>
@@ -39398,8 +39474,8 @@
       </c>
     </row>
     <row r="547">
-      <c r="A547" s="68"/>
-      <c r="B547" s="69"/>
+      <c r="A547" s="63"/>
+      <c r="B547" s="64"/>
       <c r="C547" s="34"/>
       <c r="D547" s="34"/>
       <c r="E547" s="34"/>
@@ -39424,8 +39500,8 @@
       </c>
     </row>
     <row r="548">
-      <c r="A548" s="68"/>
-      <c r="B548" s="69"/>
+      <c r="A548" s="63"/>
+      <c r="B548" s="64"/>
       <c r="C548" s="34"/>
       <c r="D548" s="34"/>
       <c r="E548" s="34"/>
@@ -39450,8 +39526,8 @@
       </c>
     </row>
     <row r="549">
-      <c r="A549" s="68"/>
-      <c r="B549" s="69"/>
+      <c r="A549" s="63"/>
+      <c r="B549" s="64"/>
       <c r="C549" s="34"/>
       <c r="D549" s="34"/>
       <c r="E549" s="34"/>
@@ -39476,8 +39552,8 @@
       </c>
     </row>
     <row r="550">
-      <c r="A550" s="68"/>
-      <c r="B550" s="69"/>
+      <c r="A550" s="63"/>
+      <c r="B550" s="64"/>
       <c r="C550" s="34"/>
       <c r="D550" s="34"/>
       <c r="E550" s="34"/>
@@ -39502,8 +39578,8 @@
       </c>
     </row>
     <row r="551">
-      <c r="A551" s="68"/>
-      <c r="B551" s="69"/>
+      <c r="A551" s="63"/>
+      <c r="B551" s="64"/>
       <c r="C551" s="34"/>
       <c r="D551" s="34"/>
       <c r="E551" s="34"/>
@@ -39968,15 +40044,17 @@
     <hyperlink r:id="rId88" ref="S526"/>
     <hyperlink r:id="rId89" ref="S527"/>
     <hyperlink r:id="rId90" ref="S528"/>
+    <hyperlink r:id="rId91" ref="S529"/>
+    <hyperlink r:id="rId92" ref="S530"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId91"/>
-  <legacyDrawing r:id="rId92"/>
+  <drawing r:id="rId93"/>
+  <legacyDrawing r:id="rId94"/>
   <tableParts count="2">
-    <tablePart r:id="rId95"/>
-    <tablePart r:id="rId96"/>
+    <tablePart r:id="rId97"/>
+    <tablePart r:id="rId98"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201014
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -563,7 +563,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5854" uniqueCount="1963">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5866" uniqueCount="1969">
   <si>
     <t>案例</t>
   </si>
@@ -7239,6 +7239,26 @@
   <si>
     <t>長期於杜拜及其他國家工作</t>
   </si>
+  <si>
+    <t>#530</t>
+  </si>
+  <si>
+    <t>2月-10/11 中國江蘇</t>
+  </si>
+  <si>
+    <t>10/11 採檢
+10/13 確診</t>
+  </si>
+  <si>
+    <t>咳嗽 流鼻水 鼻塞 有痰</t>
+  </si>
+  <si>
+    <t>10月1日出現流鼻水及有痰等症狀，僅自行買藥服用，
+未在當地就醫</t>
+  </si>
+  <si>
+    <t>男赴中國江蘇工作，返國入境檢驗確診COVID-19</t>
+  </si>
 </sst>
 </file>
 
@@ -7248,7 +7268,7 @@
     <numFmt numFmtId="164" formatCode="mm&quot;月&quot;dd&quot;日 &quot;dddd"/>
     <numFmt numFmtId="165" formatCode="m/d"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="19">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -7325,6 +7345,10 @@
       <u/>
       <color rgb="FF1155CC"/>
     </font>
+    <font/>
+    <font>
+      <color rgb="FF000000"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -7370,7 +7394,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="71">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -7559,6 +7583,24 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
@@ -39058,34 +39100,64 @@
       </c>
     </row>
     <row r="531">
-      <c r="A531" s="63"/>
-      <c r="B531" s="64"/>
-      <c r="C531" s="34"/>
-      <c r="D531" s="34"/>
-      <c r="E531" s="34"/>
+      <c r="A531" s="63" t="s">
+        <v>1963</v>
+      </c>
+      <c r="B531" s="6">
+        <v>44117.0</v>
+      </c>
+      <c r="C531" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D531" s="64" t="s">
+        <v>59</v>
+      </c>
+      <c r="E531" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F531" s="34"/>
-      <c r="G531" s="34"/>
-      <c r="H531" s="21"/>
-      <c r="I531" s="19"/>
-      <c r="J531" s="10"/>
-      <c r="K531" s="22"/>
-      <c r="L531" s="23"/>
-      <c r="M531" s="22"/>
+      <c r="G531" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H531" s="65" t="s">
+        <v>1964</v>
+      </c>
+      <c r="I531" s="66">
+        <v>44115.0</v>
+      </c>
+      <c r="J531" s="10">
+        <v>44105.0</v>
+      </c>
+      <c r="K531" s="67" t="s">
+        <v>1965</v>
+      </c>
+      <c r="L531" s="68" t="s">
+        <v>363</v>
+      </c>
+      <c r="M531" s="67" t="s">
+        <v>1966</v>
+      </c>
       <c r="N531" s="25"/>
-      <c r="O531" s="21"/>
-      <c r="P531" s="21"/>
+      <c r="O531" s="65" t="s">
+        <v>85</v>
+      </c>
+      <c r="P531" s="65" t="s">
+        <v>1967</v>
+      </c>
       <c r="Q531" s="19"/>
       <c r="R531" s="19"/>
-      <c r="S531" s="20"/>
+      <c r="S531" s="61" t="s">
+        <v>1968</v>
+      </c>
       <c r="T531" s="20"/>
       <c r="U531" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#530</v>
       </c>
     </row>
     <row r="532">
-      <c r="A532" s="63"/>
-      <c r="B532" s="64"/>
+      <c r="A532" s="69"/>
+      <c r="B532" s="70"/>
       <c r="C532" s="34"/>
       <c r="D532" s="34"/>
       <c r="E532" s="34"/>
@@ -39110,8 +39182,8 @@
       </c>
     </row>
     <row r="533">
-      <c r="A533" s="63"/>
-      <c r="B533" s="64"/>
+      <c r="A533" s="69"/>
+      <c r="B533" s="70"/>
       <c r="C533" s="34"/>
       <c r="D533" s="34"/>
       <c r="E533" s="34"/>
@@ -39136,8 +39208,8 @@
       </c>
     </row>
     <row r="534">
-      <c r="A534" s="63"/>
-      <c r="B534" s="64"/>
+      <c r="A534" s="69"/>
+      <c r="B534" s="70"/>
       <c r="C534" s="34"/>
       <c r="D534" s="34"/>
       <c r="E534" s="34"/>
@@ -39162,8 +39234,8 @@
       </c>
     </row>
     <row r="535">
-      <c r="A535" s="63"/>
-      <c r="B535" s="64"/>
+      <c r="A535" s="69"/>
+      <c r="B535" s="70"/>
       <c r="C535" s="34"/>
       <c r="D535" s="34"/>
       <c r="E535" s="34"/>
@@ -39188,8 +39260,8 @@
       </c>
     </row>
     <row r="536">
-      <c r="A536" s="63"/>
-      <c r="B536" s="64"/>
+      <c r="A536" s="69"/>
+      <c r="B536" s="70"/>
       <c r="C536" s="34"/>
       <c r="D536" s="34"/>
       <c r="E536" s="34"/>
@@ -39214,8 +39286,8 @@
       </c>
     </row>
     <row r="537">
-      <c r="A537" s="63"/>
-      <c r="B537" s="64"/>
+      <c r="A537" s="69"/>
+      <c r="B537" s="70"/>
       <c r="C537" s="34"/>
       <c r="D537" s="34"/>
       <c r="E537" s="34"/>
@@ -39240,8 +39312,8 @@
       </c>
     </row>
     <row r="538">
-      <c r="A538" s="63"/>
-      <c r="B538" s="64"/>
+      <c r="A538" s="69"/>
+      <c r="B538" s="70"/>
       <c r="C538" s="34"/>
       <c r="D538" s="34"/>
       <c r="E538" s="34"/>
@@ -39266,8 +39338,8 @@
       </c>
     </row>
     <row r="539">
-      <c r="A539" s="63"/>
-      <c r="B539" s="64"/>
+      <c r="A539" s="69"/>
+      <c r="B539" s="70"/>
       <c r="C539" s="34"/>
       <c r="D539" s="34"/>
       <c r="E539" s="34"/>
@@ -39292,8 +39364,8 @@
       </c>
     </row>
     <row r="540">
-      <c r="A540" s="63"/>
-      <c r="B540" s="64"/>
+      <c r="A540" s="69"/>
+      <c r="B540" s="70"/>
       <c r="C540" s="34"/>
       <c r="D540" s="34"/>
       <c r="E540" s="34"/>
@@ -39318,8 +39390,8 @@
       </c>
     </row>
     <row r="541">
-      <c r="A541" s="63"/>
-      <c r="B541" s="64"/>
+      <c r="A541" s="69"/>
+      <c r="B541" s="70"/>
       <c r="C541" s="34"/>
       <c r="D541" s="34"/>
       <c r="E541" s="34"/>
@@ -39344,8 +39416,8 @@
       </c>
     </row>
     <row r="542">
-      <c r="A542" s="63"/>
-      <c r="B542" s="64"/>
+      <c r="A542" s="69"/>
+      <c r="B542" s="70"/>
       <c r="C542" s="34"/>
       <c r="D542" s="34"/>
       <c r="E542" s="34"/>
@@ -39370,8 +39442,8 @@
       </c>
     </row>
     <row r="543">
-      <c r="A543" s="63"/>
-      <c r="B543" s="64"/>
+      <c r="A543" s="69"/>
+      <c r="B543" s="70"/>
       <c r="C543" s="34"/>
       <c r="D543" s="34"/>
       <c r="E543" s="34"/>
@@ -39396,8 +39468,8 @@
       </c>
     </row>
     <row r="544">
-      <c r="A544" s="63"/>
-      <c r="B544" s="64"/>
+      <c r="A544" s="69"/>
+      <c r="B544" s="70"/>
       <c r="C544" s="34"/>
       <c r="D544" s="34"/>
       <c r="E544" s="34"/>
@@ -39422,8 +39494,8 @@
       </c>
     </row>
     <row r="545">
-      <c r="A545" s="63"/>
-      <c r="B545" s="64"/>
+      <c r="A545" s="69"/>
+      <c r="B545" s="70"/>
       <c r="C545" s="34"/>
       <c r="D545" s="34"/>
       <c r="E545" s="34"/>
@@ -39448,8 +39520,8 @@
       </c>
     </row>
     <row r="546">
-      <c r="A546" s="63"/>
-      <c r="B546" s="64"/>
+      <c r="A546" s="69"/>
+      <c r="B546" s="70"/>
       <c r="C546" s="34"/>
       <c r="D546" s="34"/>
       <c r="E546" s="34"/>
@@ -39474,8 +39546,8 @@
       </c>
     </row>
     <row r="547">
-      <c r="A547" s="63"/>
-      <c r="B547" s="64"/>
+      <c r="A547" s="69"/>
+      <c r="B547" s="70"/>
       <c r="C547" s="34"/>
       <c r="D547" s="34"/>
       <c r="E547" s="34"/>
@@ -39500,8 +39572,8 @@
       </c>
     </row>
     <row r="548">
-      <c r="A548" s="63"/>
-      <c r="B548" s="64"/>
+      <c r="A548" s="69"/>
+      <c r="B548" s="70"/>
       <c r="C548" s="34"/>
       <c r="D548" s="34"/>
       <c r="E548" s="34"/>
@@ -39526,8 +39598,8 @@
       </c>
     </row>
     <row r="549">
-      <c r="A549" s="63"/>
-      <c r="B549" s="64"/>
+      <c r="A549" s="69"/>
+      <c r="B549" s="70"/>
       <c r="C549" s="34"/>
       <c r="D549" s="34"/>
       <c r="E549" s="34"/>
@@ -39552,8 +39624,8 @@
       </c>
     </row>
     <row r="550">
-      <c r="A550" s="63"/>
-      <c r="B550" s="64"/>
+      <c r="A550" s="69"/>
+      <c r="B550" s="70"/>
       <c r="C550" s="34"/>
       <c r="D550" s="34"/>
       <c r="E550" s="34"/>
@@ -39578,8 +39650,8 @@
       </c>
     </row>
     <row r="551">
-      <c r="A551" s="63"/>
-      <c r="B551" s="64"/>
+      <c r="A551" s="69"/>
+      <c r="B551" s="70"/>
       <c r="C551" s="34"/>
       <c r="D551" s="34"/>
       <c r="E551" s="34"/>
@@ -40046,15 +40118,16 @@
     <hyperlink r:id="rId90" ref="S528"/>
     <hyperlink r:id="rId91" ref="S529"/>
     <hyperlink r:id="rId92" ref="S530"/>
+    <hyperlink r:id="rId93" ref="S531"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId93"/>
-  <legacyDrawing r:id="rId94"/>
+  <drawing r:id="rId94"/>
+  <legacyDrawing r:id="rId95"/>
   <tableParts count="2">
-    <tablePart r:id="rId97"/>
     <tablePart r:id="rId98"/>
+    <tablePart r:id="rId99"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201015
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -7268,7 +7268,7 @@
     <numFmt numFmtId="164" formatCode="mm&quot;月&quot;dd&quot;日 &quot;dddd"/>
     <numFmt numFmtId="165" formatCode="m/d"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="17">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -7345,10 +7345,6 @@
       <u/>
       <color rgb="FF1155CC"/>
     </font>
-    <font/>
-    <font>
-      <color rgb="FF000000"/>
-    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -7394,7 +7390,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="65">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -7583,24 +7579,6 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
@@ -39100,7 +39078,7 @@
       </c>
     </row>
     <row r="531">
-      <c r="A531" s="63" t="s">
+      <c r="A531" s="16" t="s">
         <v>1963</v>
       </c>
       <c r="B531" s="6">
@@ -39109,7 +39087,7 @@
       <c r="C531" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D531" s="64" t="s">
+      <c r="D531" s="7" t="s">
         <v>59</v>
       </c>
       <c r="E531" s="7" t="s">
@@ -39119,29 +39097,29 @@
       <c r="G531" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H531" s="65" t="s">
+      <c r="H531" s="8" t="s">
         <v>1964</v>
       </c>
-      <c r="I531" s="66">
+      <c r="I531" s="9">
         <v>44115.0</v>
       </c>
       <c r="J531" s="10">
         <v>44105.0</v>
       </c>
-      <c r="K531" s="67" t="s">
+      <c r="K531" s="13" t="s">
         <v>1965</v>
       </c>
-      <c r="L531" s="68" t="s">
+      <c r="L531" s="12" t="s">
         <v>363</v>
       </c>
-      <c r="M531" s="67" t="s">
+      <c r="M531" s="13" t="s">
         <v>1966</v>
       </c>
       <c r="N531" s="25"/>
-      <c r="O531" s="65" t="s">
+      <c r="O531" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P531" s="65" t="s">
+      <c r="P531" s="8" t="s">
         <v>1967</v>
       </c>
       <c r="Q531" s="19"/>
@@ -39156,8 +39134,8 @@
       </c>
     </row>
     <row r="532">
-      <c r="A532" s="69"/>
-      <c r="B532" s="70"/>
+      <c r="A532" s="63"/>
+      <c r="B532" s="64"/>
       <c r="C532" s="34"/>
       <c r="D532" s="34"/>
       <c r="E532" s="34"/>
@@ -39182,8 +39160,8 @@
       </c>
     </row>
     <row r="533">
-      <c r="A533" s="69"/>
-      <c r="B533" s="70"/>
+      <c r="A533" s="63"/>
+      <c r="B533" s="64"/>
       <c r="C533" s="34"/>
       <c r="D533" s="34"/>
       <c r="E533" s="34"/>
@@ -39208,8 +39186,8 @@
       </c>
     </row>
     <row r="534">
-      <c r="A534" s="69"/>
-      <c r="B534" s="70"/>
+      <c r="A534" s="63"/>
+      <c r="B534" s="64"/>
       <c r="C534" s="34"/>
       <c r="D534" s="34"/>
       <c r="E534" s="34"/>
@@ -39234,8 +39212,8 @@
       </c>
     </row>
     <row r="535">
-      <c r="A535" s="69"/>
-      <c r="B535" s="70"/>
+      <c r="A535" s="63"/>
+      <c r="B535" s="64"/>
       <c r="C535" s="34"/>
       <c r="D535" s="34"/>
       <c r="E535" s="34"/>
@@ -39260,8 +39238,8 @@
       </c>
     </row>
     <row r="536">
-      <c r="A536" s="69"/>
-      <c r="B536" s="70"/>
+      <c r="A536" s="63"/>
+      <c r="B536" s="64"/>
       <c r="C536" s="34"/>
       <c r="D536" s="34"/>
       <c r="E536" s="34"/>
@@ -39286,8 +39264,8 @@
       </c>
     </row>
     <row r="537">
-      <c r="A537" s="69"/>
-      <c r="B537" s="70"/>
+      <c r="A537" s="63"/>
+      <c r="B537" s="64"/>
       <c r="C537" s="34"/>
       <c r="D537" s="34"/>
       <c r="E537" s="34"/>
@@ -39312,8 +39290,8 @@
       </c>
     </row>
     <row r="538">
-      <c r="A538" s="69"/>
-      <c r="B538" s="70"/>
+      <c r="A538" s="63"/>
+      <c r="B538" s="64"/>
       <c r="C538" s="34"/>
       <c r="D538" s="34"/>
       <c r="E538" s="34"/>
@@ -39338,8 +39316,8 @@
       </c>
     </row>
     <row r="539">
-      <c r="A539" s="69"/>
-      <c r="B539" s="70"/>
+      <c r="A539" s="63"/>
+      <c r="B539" s="64"/>
       <c r="C539" s="34"/>
       <c r="D539" s="34"/>
       <c r="E539" s="34"/>
@@ -39364,8 +39342,8 @@
       </c>
     </row>
     <row r="540">
-      <c r="A540" s="69"/>
-      <c r="B540" s="70"/>
+      <c r="A540" s="63"/>
+      <c r="B540" s="64"/>
       <c r="C540" s="34"/>
       <c r="D540" s="34"/>
       <c r="E540" s="34"/>
@@ -39390,8 +39368,8 @@
       </c>
     </row>
     <row r="541">
-      <c r="A541" s="69"/>
-      <c r="B541" s="70"/>
+      <c r="A541" s="63"/>
+      <c r="B541" s="64"/>
       <c r="C541" s="34"/>
       <c r="D541" s="34"/>
       <c r="E541" s="34"/>
@@ -39416,8 +39394,8 @@
       </c>
     </row>
     <row r="542">
-      <c r="A542" s="69"/>
-      <c r="B542" s="70"/>
+      <c r="A542" s="63"/>
+      <c r="B542" s="64"/>
       <c r="C542" s="34"/>
       <c r="D542" s="34"/>
       <c r="E542" s="34"/>
@@ -39442,8 +39420,8 @@
       </c>
     </row>
     <row r="543">
-      <c r="A543" s="69"/>
-      <c r="B543" s="70"/>
+      <c r="A543" s="63"/>
+      <c r="B543" s="64"/>
       <c r="C543" s="34"/>
       <c r="D543" s="34"/>
       <c r="E543" s="34"/>
@@ -39468,8 +39446,8 @@
       </c>
     </row>
     <row r="544">
-      <c r="A544" s="69"/>
-      <c r="B544" s="70"/>
+      <c r="A544" s="63"/>
+      <c r="B544" s="64"/>
       <c r="C544" s="34"/>
       <c r="D544" s="34"/>
       <c r="E544" s="34"/>
@@ -39494,8 +39472,8 @@
       </c>
     </row>
     <row r="545">
-      <c r="A545" s="69"/>
-      <c r="B545" s="70"/>
+      <c r="A545" s="63"/>
+      <c r="B545" s="64"/>
       <c r="C545" s="34"/>
       <c r="D545" s="34"/>
       <c r="E545" s="34"/>
@@ -39520,8 +39498,8 @@
       </c>
     </row>
     <row r="546">
-      <c r="A546" s="69"/>
-      <c r="B546" s="70"/>
+      <c r="A546" s="63"/>
+      <c r="B546" s="64"/>
       <c r="C546" s="34"/>
       <c r="D546" s="34"/>
       <c r="E546" s="34"/>
@@ -39546,8 +39524,8 @@
       </c>
     </row>
     <row r="547">
-      <c r="A547" s="69"/>
-      <c r="B547" s="70"/>
+      <c r="A547" s="63"/>
+      <c r="B547" s="64"/>
       <c r="C547" s="34"/>
       <c r="D547" s="34"/>
       <c r="E547" s="34"/>
@@ -39572,8 +39550,8 @@
       </c>
     </row>
     <row r="548">
-      <c r="A548" s="69"/>
-      <c r="B548" s="70"/>
+      <c r="A548" s="63"/>
+      <c r="B548" s="64"/>
       <c r="C548" s="34"/>
       <c r="D548" s="34"/>
       <c r="E548" s="34"/>
@@ -39598,8 +39576,8 @@
       </c>
     </row>
     <row r="549">
-      <c r="A549" s="69"/>
-      <c r="B549" s="70"/>
+      <c r="A549" s="63"/>
+      <c r="B549" s="64"/>
       <c r="C549" s="34"/>
       <c r="D549" s="34"/>
       <c r="E549" s="34"/>
@@ -39624,8 +39602,8 @@
       </c>
     </row>
     <row r="550">
-      <c r="A550" s="69"/>
-      <c r="B550" s="70"/>
+      <c r="A550" s="63"/>
+      <c r="B550" s="64"/>
       <c r="C550" s="34"/>
       <c r="D550" s="34"/>
       <c r="E550" s="34"/>
@@ -39650,8 +39628,8 @@
       </c>
     </row>
     <row r="551">
-      <c r="A551" s="69"/>
-      <c r="B551" s="70"/>
+      <c r="A551" s="63"/>
+      <c r="B551" s="64"/>
       <c r="C551" s="34"/>
       <c r="D551" s="34"/>
       <c r="E551" s="34"/>

</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201016
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -563,7 +563,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5866" uniqueCount="1969">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5915" uniqueCount="1982">
   <si>
     <t>案例</t>
   </si>
@@ -7259,6 +7259,53 @@
   <si>
     <t>男赴中國江蘇工作，返國入境檢驗確診COVID-19</t>
   </si>
+  <si>
+    <t>#531</t>
+  </si>
+  <si>
+    <t>9/17 採檢
+10/1 二採
+10/12 三採
+10/13 四採
+10/15 確診</t>
+  </si>
+  <si>
+    <t>9月17日入境機場採檢以及10月1日集中檢疫期滿前採檢之結果皆為陰性
+10月2日檢疫期滿後搭乘專車至旅館自主健康管理
+10月12日由仲介安排專車至醫院自費採檢，因檢驗結果呈現弱陽性，個案同日收治住院隔離，為求慎重
+10月13日再次採驗，並於今日確診(Ct值31，血清抗體IgM陰性、IgG陽性)</t>
+  </si>
+  <si>
+    <t>國內新增1例境外移入COVID-19病例，為無症狀菲籍移工</t>
+  </si>
+  <si>
+    <t>#532</t>
+  </si>
+  <si>
+    <t>1X-2X</t>
+  </si>
+  <si>
+    <t>-9/30 印尼→台灣</t>
+  </si>
+  <si>
+    <t>10/15 採檢
+10/16 確診</t>
+  </si>
+  <si>
+    <t>4名個案入境迄今均無疑似症狀，9月30日入境後即由校方分別安排至國內4家防疫旅館居家檢疫，10月15日檢疫期滿由衛生單位安排就醫採檢，並於今日確診</t>
+  </si>
+  <si>
+    <t>4名無症狀印尼學生來台就學，檢疫期滿後採檢確診COVID-19</t>
+  </si>
+  <si>
+    <t>#533</t>
+  </si>
+  <si>
+    <t>#534</t>
+  </si>
+  <si>
+    <t>#535</t>
+  </si>
 </sst>
 </file>
 
@@ -7268,7 +7315,7 @@
     <numFmt numFmtId="164" formatCode="mm&quot;月&quot;dd&quot;日 &quot;dddd"/>
     <numFmt numFmtId="165" formatCode="m/d"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="19">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -7345,6 +7392,10 @@
       <u/>
       <color rgb="FF1155CC"/>
     </font>
+    <font/>
+    <font>
+      <color rgb="FF000000"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -7390,7 +7441,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="71">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -7580,6 +7631,24 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -7590,7 +7659,7 @@
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
-  <dxfs count="68">
+  <dxfs count="67">
     <dxf>
       <font>
         <color rgb="FF0000FF"/>
@@ -7659,19 +7728,6 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFB7E1CD"/>
           <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFD966"/>
-          <bgColor rgb="FFFFD966"/>
         </patternFill>
       </fill>
       <border/>
@@ -8355,14 +8411,14 @@
   </dxfs>
   <tableStyles count="2">
     <tableStyle count="3" pivot="0" name="臺灣武漢肺炎病例-style">
-      <tableStyleElement dxfId="65" type="headerRow"/>
-      <tableStyleElement dxfId="66" type="firstRowStripe"/>
-      <tableStyleElement dxfId="67" type="secondRowStripe"/>
+      <tableStyleElement dxfId="64" type="headerRow"/>
+      <tableStyleElement dxfId="65" type="firstRowStripe"/>
+      <tableStyleElement dxfId="66" type="secondRowStripe"/>
     </tableStyle>
     <tableStyle count="3" pivot="0" name="臺灣武漢肺炎病例-style 2">
-      <tableStyleElement dxfId="65" type="headerRow"/>
-      <tableStyleElement dxfId="66" type="firstRowStripe"/>
-      <tableStyleElement dxfId="67" type="secondRowStripe"/>
+      <tableStyleElement dxfId="64" type="headerRow"/>
+      <tableStyleElement dxfId="65" type="firstRowStripe"/>
+      <tableStyleElement dxfId="66" type="secondRowStripe"/>
     </tableStyle>
   </tableStyles>
 </styleSheet>
@@ -39134,138 +39190,298 @@
       </c>
     </row>
     <row r="532">
-      <c r="A532" s="63"/>
-      <c r="B532" s="64"/>
-      <c r="C532" s="34"/>
-      <c r="D532" s="34"/>
-      <c r="E532" s="34"/>
+      <c r="A532" s="16" t="s">
+        <v>1969</v>
+      </c>
+      <c r="B532" s="6">
+        <v>44119.0</v>
+      </c>
+      <c r="C532" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D532" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E532" s="7" t="s">
+        <v>205</v>
+      </c>
       <c r="F532" s="34"/>
-      <c r="G532" s="34"/>
-      <c r="H532" s="21"/>
-      <c r="I532" s="19"/>
-      <c r="J532" s="10"/>
-      <c r="K532" s="22"/>
-      <c r="L532" s="23"/>
-      <c r="M532" s="22"/>
+      <c r="G532" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H532" s="8" t="s">
+        <v>1841</v>
+      </c>
+      <c r="I532" s="9">
+        <v>44091.0</v>
+      </c>
+      <c r="J532" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K532" s="13" t="s">
+        <v>1970</v>
+      </c>
+      <c r="L532" s="12" t="s">
+        <v>1674</v>
+      </c>
+      <c r="M532" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N532" s="25"/>
-      <c r="O532" s="21"/>
-      <c r="P532" s="21"/>
+      <c r="O532" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P532" s="8" t="s">
+        <v>1971</v>
+      </c>
       <c r="Q532" s="19"/>
       <c r="R532" s="19"/>
-      <c r="S532" s="20"/>
+      <c r="S532" s="61" t="s">
+        <v>1972</v>
+      </c>
       <c r="T532" s="20"/>
       <c r="U532" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#531</v>
       </c>
     </row>
     <row r="533">
-      <c r="A533" s="63"/>
-      <c r="B533" s="64"/>
+      <c r="A533" s="63" t="s">
+        <v>1973</v>
+      </c>
+      <c r="B533" s="6">
+        <v>44120.0</v>
+      </c>
       <c r="C533" s="34"/>
-      <c r="D533" s="34"/>
-      <c r="E533" s="34"/>
+      <c r="D533" s="64" t="s">
+        <v>1974</v>
+      </c>
+      <c r="E533" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F533" s="34"/>
-      <c r="G533" s="34"/>
-      <c r="H533" s="21"/>
-      <c r="I533" s="19"/>
-      <c r="J533" s="10"/>
-      <c r="K533" s="22"/>
-      <c r="L533" s="23"/>
-      <c r="M533" s="22"/>
+      <c r="G533" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H533" s="65" t="s">
+        <v>1975</v>
+      </c>
+      <c r="I533" s="66">
+        <v>44104.0</v>
+      </c>
+      <c r="J533" s="67" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K533" s="68" t="s">
+        <v>1976</v>
+      </c>
+      <c r="L533" s="67" t="s">
+        <v>426</v>
+      </c>
+      <c r="M533" s="68" t="s">
+        <v>1442</v>
+      </c>
       <c r="N533" s="25"/>
-      <c r="O533" s="21"/>
-      <c r="P533" s="21"/>
+      <c r="O533" s="65" t="s">
+        <v>85</v>
+      </c>
+      <c r="P533" s="65" t="s">
+        <v>1977</v>
+      </c>
       <c r="Q533" s="19"/>
       <c r="R533" s="19"/>
-      <c r="S533" s="20"/>
+      <c r="S533" s="61" t="s">
+        <v>1978</v>
+      </c>
       <c r="T533" s="20"/>
       <c r="U533" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#532</v>
       </c>
     </row>
     <row r="534">
-      <c r="A534" s="63"/>
-      <c r="B534" s="64"/>
+      <c r="A534" s="63" t="s">
+        <v>1979</v>
+      </c>
+      <c r="B534" s="6">
+        <v>44120.0</v>
+      </c>
       <c r="C534" s="34"/>
-      <c r="D534" s="34"/>
-      <c r="E534" s="34"/>
+      <c r="D534" s="64" t="s">
+        <v>1974</v>
+      </c>
+      <c r="E534" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F534" s="34"/>
-      <c r="G534" s="34"/>
-      <c r="H534" s="21"/>
-      <c r="I534" s="19"/>
-      <c r="J534" s="10"/>
-      <c r="K534" s="22"/>
-      <c r="L534" s="23"/>
-      <c r="M534" s="22"/>
+      <c r="G534" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H534" s="21" t="str">
+        <f t="shared" ref="H534:H536" si="66">$H$533</f>
+        <v>-9/30 印尼→台灣</v>
+      </c>
+      <c r="I534" s="58">
+        <f t="shared" ref="I534:I536" si="67">$I$533</f>
+        <v>44104</v>
+      </c>
+      <c r="J534" s="67" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K534" s="22" t="str">
+        <f t="shared" ref="K534:K536" si="68">$K$533</f>
+        <v>10/15 採檢
+10/16 確診</v>
+      </c>
+      <c r="L534" s="23" t="str">
+        <f t="shared" ref="L534:L536" si="69">$L$533</f>
+        <v>居家檢疫</v>
+      </c>
+      <c r="M534" s="68" t="s">
+        <v>1442</v>
+      </c>
       <c r="N534" s="25"/>
-      <c r="O534" s="21"/>
-      <c r="P534" s="21"/>
+      <c r="O534" s="65" t="s">
+        <v>85</v>
+      </c>
+      <c r="P534" s="21" t="str">
+        <f t="shared" ref="P534:P536" si="70">$P$533</f>
+        <v>4名個案入境迄今均無疑似症狀，9月30日入境後即由校方分別安排至國內4家防疫旅館居家檢疫，10月15日檢疫期滿由衛生單位安排就醫採檢，並於今日確診</v>
+      </c>
       <c r="Q534" s="19"/>
       <c r="R534" s="19"/>
-      <c r="S534" s="20"/>
+      <c r="S534" s="61" t="s">
+        <v>1978</v>
+      </c>
       <c r="T534" s="20"/>
       <c r="U534" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#533</v>
       </c>
     </row>
     <row r="535">
-      <c r="A535" s="63"/>
-      <c r="B535" s="64"/>
+      <c r="A535" s="63" t="s">
+        <v>1980</v>
+      </c>
+      <c r="B535" s="6">
+        <v>44120.0</v>
+      </c>
       <c r="C535" s="34"/>
-      <c r="D535" s="34"/>
-      <c r="E535" s="34"/>
+      <c r="D535" s="64" t="s">
+        <v>1974</v>
+      </c>
+      <c r="E535" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F535" s="34"/>
-      <c r="G535" s="34"/>
-      <c r="H535" s="21"/>
-      <c r="I535" s="19"/>
-      <c r="J535" s="10"/>
-      <c r="K535" s="22"/>
-      <c r="L535" s="23"/>
-      <c r="M535" s="22"/>
+      <c r="G535" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H535" s="21" t="str">
+        <f t="shared" si="66"/>
+        <v>-9/30 印尼→台灣</v>
+      </c>
+      <c r="I535" s="58">
+        <f t="shared" si="67"/>
+        <v>44104</v>
+      </c>
+      <c r="J535" s="67" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K535" s="22" t="str">
+        <f t="shared" si="68"/>
+        <v>10/15 採檢
+10/16 確診</v>
+      </c>
+      <c r="L535" s="23" t="str">
+        <f t="shared" si="69"/>
+        <v>居家檢疫</v>
+      </c>
+      <c r="M535" s="68" t="s">
+        <v>1442</v>
+      </c>
       <c r="N535" s="25"/>
-      <c r="O535" s="21"/>
-      <c r="P535" s="21"/>
+      <c r="O535" s="65" t="s">
+        <v>85</v>
+      </c>
+      <c r="P535" s="21" t="str">
+        <f t="shared" si="70"/>
+        <v>4名個案入境迄今均無疑似症狀，9月30日入境後即由校方分別安排至國內4家防疫旅館居家檢疫，10月15日檢疫期滿由衛生單位安排就醫採檢，並於今日確診</v>
+      </c>
       <c r="Q535" s="19"/>
       <c r="R535" s="19"/>
-      <c r="S535" s="20"/>
+      <c r="S535" s="61" t="s">
+        <v>1978</v>
+      </c>
       <c r="T535" s="20"/>
       <c r="U535" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#534</v>
       </c>
     </row>
     <row r="536">
-      <c r="A536" s="63"/>
-      <c r="B536" s="64"/>
+      <c r="A536" s="63" t="s">
+        <v>1981</v>
+      </c>
+      <c r="B536" s="6">
+        <v>44120.0</v>
+      </c>
       <c r="C536" s="34"/>
-      <c r="D536" s="34"/>
-      <c r="E536" s="34"/>
+      <c r="D536" s="64" t="s">
+        <v>1974</v>
+      </c>
+      <c r="E536" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F536" s="34"/>
-      <c r="G536" s="34"/>
-      <c r="H536" s="21"/>
-      <c r="I536" s="19"/>
-      <c r="J536" s="10"/>
-      <c r="K536" s="22"/>
-      <c r="L536" s="23"/>
-      <c r="M536" s="22"/>
+      <c r="G536" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H536" s="21" t="str">
+        <f t="shared" si="66"/>
+        <v>-9/30 印尼→台灣</v>
+      </c>
+      <c r="I536" s="58">
+        <f t="shared" si="67"/>
+        <v>44104</v>
+      </c>
+      <c r="J536" s="67" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K536" s="22" t="str">
+        <f t="shared" si="68"/>
+        <v>10/15 採檢
+10/16 確診</v>
+      </c>
+      <c r="L536" s="23" t="str">
+        <f t="shared" si="69"/>
+        <v>居家檢疫</v>
+      </c>
+      <c r="M536" s="68" t="s">
+        <v>1442</v>
+      </c>
       <c r="N536" s="25"/>
-      <c r="O536" s="21"/>
-      <c r="P536" s="21"/>
+      <c r="O536" s="65" t="s">
+        <v>85</v>
+      </c>
+      <c r="P536" s="21" t="str">
+        <f t="shared" si="70"/>
+        <v>4名個案入境迄今均無疑似症狀，9月30日入境後即由校方分別安排至國內4家防疫旅館居家檢疫，10月15日檢疫期滿由衛生單位安排就醫採檢，並於今日確診</v>
+      </c>
       <c r="Q536" s="19"/>
       <c r="R536" s="19"/>
-      <c r="S536" s="20"/>
+      <c r="S536" s="61" t="s">
+        <v>1978</v>
+      </c>
       <c r="T536" s="20"/>
       <c r="U536" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#535</v>
       </c>
     </row>
     <row r="537">
-      <c r="A537" s="63"/>
-      <c r="B537" s="64"/>
+      <c r="A537" s="69"/>
+      <c r="B537" s="70"/>
       <c r="C537" s="34"/>
       <c r="D537" s="34"/>
       <c r="E537" s="34"/>
@@ -39290,8 +39506,8 @@
       </c>
     </row>
     <row r="538">
-      <c r="A538" s="63"/>
-      <c r="B538" s="64"/>
+      <c r="A538" s="69"/>
+      <c r="B538" s="70"/>
       <c r="C538" s="34"/>
       <c r="D538" s="34"/>
       <c r="E538" s="34"/>
@@ -39316,8 +39532,8 @@
       </c>
     </row>
     <row r="539">
-      <c r="A539" s="63"/>
-      <c r="B539" s="64"/>
+      <c r="A539" s="69"/>
+      <c r="B539" s="70"/>
       <c r="C539" s="34"/>
       <c r="D539" s="34"/>
       <c r="E539" s="34"/>
@@ -39342,8 +39558,8 @@
       </c>
     </row>
     <row r="540">
-      <c r="A540" s="63"/>
-      <c r="B540" s="64"/>
+      <c r="A540" s="69"/>
+      <c r="B540" s="70"/>
       <c r="C540" s="34"/>
       <c r="D540" s="34"/>
       <c r="E540" s="34"/>
@@ -39368,8 +39584,8 @@
       </c>
     </row>
     <row r="541">
-      <c r="A541" s="63"/>
-      <c r="B541" s="64"/>
+      <c r="A541" s="69"/>
+      <c r="B541" s="70"/>
       <c r="C541" s="34"/>
       <c r="D541" s="34"/>
       <c r="E541" s="34"/>
@@ -39394,8 +39610,8 @@
       </c>
     </row>
     <row r="542">
-      <c r="A542" s="63"/>
-      <c r="B542" s="64"/>
+      <c r="A542" s="69"/>
+      <c r="B542" s="70"/>
       <c r="C542" s="34"/>
       <c r="D542" s="34"/>
       <c r="E542" s="34"/>
@@ -39420,8 +39636,8 @@
       </c>
     </row>
     <row r="543">
-      <c r="A543" s="63"/>
-      <c r="B543" s="64"/>
+      <c r="A543" s="69"/>
+      <c r="B543" s="70"/>
       <c r="C543" s="34"/>
       <c r="D543" s="34"/>
       <c r="E543" s="34"/>
@@ -39446,8 +39662,8 @@
       </c>
     </row>
     <row r="544">
-      <c r="A544" s="63"/>
-      <c r="B544" s="64"/>
+      <c r="A544" s="69"/>
+      <c r="B544" s="70"/>
       <c r="C544" s="34"/>
       <c r="D544" s="34"/>
       <c r="E544" s="34"/>
@@ -39472,8 +39688,8 @@
       </c>
     </row>
     <row r="545">
-      <c r="A545" s="63"/>
-      <c r="B545" s="64"/>
+      <c r="A545" s="69"/>
+      <c r="B545" s="70"/>
       <c r="C545" s="34"/>
       <c r="D545" s="34"/>
       <c r="E545" s="34"/>
@@ -39498,8 +39714,8 @@
       </c>
     </row>
     <row r="546">
-      <c r="A546" s="63"/>
-      <c r="B546" s="64"/>
+      <c r="A546" s="69"/>
+      <c r="B546" s="70"/>
       <c r="C546" s="34"/>
       <c r="D546" s="34"/>
       <c r="E546" s="34"/>
@@ -39524,8 +39740,8 @@
       </c>
     </row>
     <row r="547">
-      <c r="A547" s="63"/>
-      <c r="B547" s="64"/>
+      <c r="A547" s="69"/>
+      <c r="B547" s="70"/>
       <c r="C547" s="34"/>
       <c r="D547" s="34"/>
       <c r="E547" s="34"/>
@@ -39550,8 +39766,8 @@
       </c>
     </row>
     <row r="548">
-      <c r="A548" s="63"/>
-      <c r="B548" s="64"/>
+      <c r="A548" s="69"/>
+      <c r="B548" s="70"/>
       <c r="C548" s="34"/>
       <c r="D548" s="34"/>
       <c r="E548" s="34"/>
@@ -39576,8 +39792,8 @@
       </c>
     </row>
     <row r="549">
-      <c r="A549" s="63"/>
-      <c r="B549" s="64"/>
+      <c r="A549" s="69"/>
+      <c r="B549" s="70"/>
       <c r="C549" s="34"/>
       <c r="D549" s="34"/>
       <c r="E549" s="34"/>
@@ -39602,8 +39818,8 @@
       </c>
     </row>
     <row r="550">
-      <c r="A550" s="63"/>
-      <c r="B550" s="64"/>
+      <c r="A550" s="69"/>
+      <c r="B550" s="70"/>
       <c r="C550" s="34"/>
       <c r="D550" s="34"/>
       <c r="E550" s="34"/>
@@ -39628,8 +39844,8 @@
       </c>
     </row>
     <row r="551">
-      <c r="A551" s="63"/>
-      <c r="B551" s="64"/>
+      <c r="A551" s="69"/>
+      <c r="B551" s="70"/>
       <c r="C551" s="34"/>
       <c r="D551" s="34"/>
       <c r="E551" s="34"/>
@@ -39690,317 +39906,312 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E551">
-    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="中國">
-      <formula>NOT(ISERROR(SEARCH(("中國"),(E2))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E551">
-    <cfRule type="notContainsBlanks" dxfId="7" priority="9">
+    <cfRule type="notContainsBlanks" dxfId="6" priority="8">
       <formula>LEN(TRIM(E2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B551">
-    <cfRule type="expression" dxfId="8" priority="10">
+    <cfRule type="expression" dxfId="7" priority="9">
       <formula>B1&lt;43856.0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B551">
-    <cfRule type="expression" dxfId="9" priority="11">
+    <cfRule type="expression" dxfId="8" priority="10">
       <formula>B1&lt;43863.0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B551">
-    <cfRule type="expression" dxfId="10" priority="12">
+    <cfRule type="expression" dxfId="9" priority="11">
       <formula>B1&lt;43870.0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B551">
-    <cfRule type="expression" dxfId="11" priority="13">
+    <cfRule type="expression" dxfId="10" priority="12">
       <formula>B1&lt;43877.0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B551">
-    <cfRule type="expression" dxfId="12" priority="14">
+    <cfRule type="expression" dxfId="11" priority="13">
       <formula>B1&lt;43884.0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B551">
-    <cfRule type="expression" dxfId="13" priority="15">
+    <cfRule type="expression" dxfId="12" priority="14">
       <formula>B1&lt;43891.0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B551">
-    <cfRule type="expression" dxfId="14" priority="16">
+    <cfRule type="expression" dxfId="13" priority="15">
       <formula>B1&lt;43898.0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B551">
-    <cfRule type="expression" dxfId="15" priority="17">
+    <cfRule type="expression" dxfId="14" priority="16">
       <formula>B1&lt;43905.0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B551">
-    <cfRule type="expression" dxfId="16" priority="18">
+    <cfRule type="expression" dxfId="15" priority="17">
       <formula>B1&lt;43912.0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B551">
-    <cfRule type="expression" dxfId="17" priority="19">
+    <cfRule type="expression" dxfId="16" priority="18">
       <formula>B1&lt;43919.0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B551">
-    <cfRule type="expression" dxfId="18" priority="20">
+    <cfRule type="expression" dxfId="17" priority="19">
       <formula>B1&lt;43926.0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F345 F347:F551">
-    <cfRule type="containsText" dxfId="2" priority="21" operator="containsText" text="南">
+    <cfRule type="containsText" dxfId="2" priority="20" operator="containsText" text="南">
       <formula>NOT(ISERROR(SEARCH(("南"),(F1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F345 F347:F551">
-    <cfRule type="containsText" dxfId="19" priority="22" operator="containsText" text="中">
+    <cfRule type="containsText" dxfId="18" priority="21" operator="containsText" text="中">
       <formula>NOT(ISERROR(SEARCH(("中"),(F1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F345 F347:F551">
-    <cfRule type="containsText" dxfId="20" priority="23" operator="containsText" text="北">
+    <cfRule type="containsText" dxfId="19" priority="22" operator="containsText" text="北">
       <formula>NOT(ISERROR(SEARCH(("北"),(F1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F345 F347:F551">
-    <cfRule type="containsText" dxfId="21" priority="24" operator="containsText" text="東">
+    <cfRule type="containsText" dxfId="20" priority="23" operator="containsText" text="東">
       <formula>NOT(ISERROR(SEARCH(("東"),(F1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P1:P389 P394:P551">
-    <cfRule type="containsText" dxfId="22" priority="25" operator="containsText" text="R.I.P">
+    <cfRule type="containsText" dxfId="21" priority="24" operator="containsText" text="R.I.P">
       <formula>NOT(ISERROR(SEARCH(("R.I.P"),(P1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:M551 P1:P389 P394:P551">
-    <cfRule type="containsText" dxfId="23" priority="26" operator="containsText" text="首起">
+    <cfRule type="containsText" dxfId="22" priority="25" operator="containsText" text="首起">
       <formula>NOT(ISERROR(SEARCH(("首起"),(M1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:M551 P1:P389 P394:P551">
-    <cfRule type="containsText" dxfId="23" priority="27" operator="containsText" text="首次">
+    <cfRule type="containsText" dxfId="22" priority="26" operator="containsText" text="首次">
       <formula>NOT(ISERROR(SEARCH(("首次"),(M1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:M551 P1:P389 P394:P551">
-    <cfRule type="containsText" dxfId="23" priority="28" operator="containsText" text="首例">
+    <cfRule type="containsText" dxfId="22" priority="27" operator="containsText" text="首例">
       <formula>NOT(ISERROR(SEARCH(("首例"),(M1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L551">
-    <cfRule type="containsText" dxfId="24" priority="29" operator="containsText" text="自行">
+    <cfRule type="containsText" dxfId="23" priority="28" operator="containsText" text="自行">
       <formula>NOT(ISERROR(SEARCH(("自行"),(L1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:O551">
-    <cfRule type="containsText" dxfId="25" priority="30" operator="containsText" text="未知">
+    <cfRule type="containsText" dxfId="24" priority="29" operator="containsText" text="未知">
       <formula>NOT(ISERROR(SEARCH(("未知"),(O1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L551">
-    <cfRule type="containsText" dxfId="26" priority="31" operator="containsText" text="自主">
+    <cfRule type="containsText" dxfId="25" priority="30" operator="containsText" text="自主">
       <formula>NOT(ISERROR(SEARCH(("自主"),(L1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P1:P389 P394:P551">
-    <cfRule type="containsText" dxfId="27" priority="32" operator="containsText" text="重症">
+    <cfRule type="containsText" dxfId="26" priority="31" operator="containsText" text="重症">
       <formula>NOT(ISERROR(SEARCH(("重症"),(P1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J394 J397:J466 J469:J551">
-    <cfRule type="expression" dxfId="0" priority="33">
+    <cfRule type="expression" dxfId="0" priority="32">
       <formula>(J2&lt;I2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K344 K346:K551">
-    <cfRule type="expression" dxfId="28" priority="34">
+    <cfRule type="expression" dxfId="27" priority="33">
       <formula>AND( I2&lt;&gt;"", (LEFT(K2,4) - I2 ) &gt;= 7 )</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B357:B551">
-    <cfRule type="expression" dxfId="29" priority="35">
+    <cfRule type="expression" dxfId="28" priority="34">
       <formula>B357&lt;43933.0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L551">
-    <cfRule type="containsText" dxfId="30" priority="36" operator="containsText" text="回溯">
+    <cfRule type="containsText" dxfId="29" priority="35" operator="containsText" text="回溯">
       <formula>NOT(ISERROR(SEARCH(("回溯"),(L1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B357:B551">
-    <cfRule type="expression" dxfId="31" priority="37">
+    <cfRule type="expression" dxfId="30" priority="36">
       <formula>B357&lt;43940.0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B357:B551">
-    <cfRule type="expression" dxfId="32" priority="38">
+    <cfRule type="expression" dxfId="31" priority="37">
       <formula>B357&lt;43947.0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B357:B551">
-    <cfRule type="expression" dxfId="33" priority="39">
+    <cfRule type="expression" dxfId="32" priority="38">
       <formula>B357&lt;43954.0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B357:B551">
-    <cfRule type="expression" dxfId="34" priority="40">
+    <cfRule type="expression" dxfId="33" priority="39">
       <formula>B357&lt;43961.0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B357:B551">
-    <cfRule type="expression" dxfId="35" priority="41">
+    <cfRule type="expression" dxfId="34" priority="40">
       <formula>B357&lt;43968.0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B357:B551">
-    <cfRule type="expression" dxfId="36" priority="42">
+    <cfRule type="expression" dxfId="35" priority="41">
       <formula>B357&lt;43975.0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B357:B551">
-    <cfRule type="expression" dxfId="37" priority="43">
+    <cfRule type="expression" dxfId="36" priority="42">
       <formula>B357&lt;43982.0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G551">
-    <cfRule type="containsText" dxfId="38" priority="44" operator="containsText" text="敦睦">
+    <cfRule type="containsText" dxfId="37" priority="43" operator="containsText" text="敦睦">
       <formula>NOT(ISERROR(SEARCH(("敦睦"),(G2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L551">
-    <cfRule type="containsText" dxfId="14" priority="45" operator="containsText" text="集中">
+    <cfRule type="containsText" dxfId="13" priority="44" operator="containsText" text="集中">
       <formula>NOT(ISERROR(SEARCH(("集中"),(L1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:O551">
-    <cfRule type="containsText" dxfId="39" priority="46" operator="containsText" text="軍艦">
+    <cfRule type="containsText" dxfId="38" priority="45" operator="containsText" text="軍艦">
       <formula>NOT(ISERROR(SEARCH(("軍艦"),(O1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B357:B551">
-    <cfRule type="expression" dxfId="40" priority="47">
+    <cfRule type="expression" dxfId="39" priority="46">
       <formula>B357&lt;43989.0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B357:B551">
-    <cfRule type="expression" dxfId="41" priority="48">
+    <cfRule type="expression" dxfId="40" priority="47">
       <formula>B357&lt;43996.0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B357:B551">
-    <cfRule type="expression" dxfId="42" priority="49">
+    <cfRule type="expression" dxfId="41" priority="48">
       <formula>B357&lt;44003.0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B357:B551">
-    <cfRule type="expression" dxfId="43" priority="50">
+    <cfRule type="expression" dxfId="42" priority="49">
       <formula>B357&lt;44010.0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B357:B551">
-    <cfRule type="expression" dxfId="44" priority="51">
+    <cfRule type="expression" dxfId="43" priority="50">
       <formula>B357&lt;44017.0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B357:B551">
-    <cfRule type="expression" dxfId="45" priority="52">
+    <cfRule type="expression" dxfId="44" priority="51">
       <formula>B357&lt;44024.0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B357:B551">
-    <cfRule type="expression" dxfId="46" priority="53">
+    <cfRule type="expression" dxfId="45" priority="52">
       <formula>B357&lt;44031.0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B357:B551">
-    <cfRule type="expression" dxfId="47" priority="54">
+    <cfRule type="expression" dxfId="46" priority="53">
       <formula>B357&lt;44038.0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B357:B551">
-    <cfRule type="expression" dxfId="48" priority="55">
+    <cfRule type="expression" dxfId="47" priority="54">
       <formula>B357&lt;44045.0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B357:B551">
-    <cfRule type="expression" dxfId="49" priority="56">
+    <cfRule type="expression" dxfId="48" priority="55">
       <formula>B357&lt;44052.0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B357:B551">
-    <cfRule type="expression" dxfId="50" priority="57">
+    <cfRule type="expression" dxfId="49" priority="56">
       <formula>B357&lt;44059.0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B357:B551">
-    <cfRule type="expression" dxfId="51" priority="58">
+    <cfRule type="expression" dxfId="50" priority="57">
       <formula>B357&lt;44066.0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B357:B551">
-    <cfRule type="expression" dxfId="52" priority="59">
+    <cfRule type="expression" dxfId="51" priority="58">
       <formula>B357&lt;44073.0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B357:B551">
-    <cfRule type="expression" dxfId="53" priority="60">
+    <cfRule type="expression" dxfId="52" priority="59">
       <formula>B357&lt;44080.0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B357:B551">
-    <cfRule type="expression" dxfId="54" priority="61">
+    <cfRule type="expression" dxfId="53" priority="60">
       <formula>B357&lt;44087.0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B357:B551">
-    <cfRule type="expression" dxfId="55" priority="62">
+    <cfRule type="expression" dxfId="54" priority="61">
       <formula>B357&lt;44094.0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B357:B551">
-    <cfRule type="expression" dxfId="56" priority="63">
+    <cfRule type="expression" dxfId="55" priority="62">
       <formula>B357&lt;44101.0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B357:B551">
-    <cfRule type="expression" dxfId="57" priority="64">
+    <cfRule type="expression" dxfId="56" priority="63">
       <formula>B357&lt;44108.0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L551">
-    <cfRule type="containsText" dxfId="58" priority="65" operator="containsText" text="自費">
+    <cfRule type="containsText" dxfId="57" priority="64" operator="containsText" text="自費">
       <formula>NOT(ISERROR(SEARCH(("自費"),(L1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B357:B551">
-    <cfRule type="expression" dxfId="59" priority="66">
+    <cfRule type="expression" dxfId="58" priority="65">
       <formula>B357&lt;44115.0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B357:B551">
-    <cfRule type="expression" dxfId="60" priority="67">
+    <cfRule type="expression" dxfId="59" priority="66">
       <formula>B357&lt;44122.0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B357:B551">
-    <cfRule type="expression" dxfId="61" priority="68">
+    <cfRule type="expression" dxfId="60" priority="67">
       <formula>B357&lt;44129.0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B357:B551">
-    <cfRule type="expression" dxfId="62" priority="69">
+    <cfRule type="expression" dxfId="61" priority="68">
       <formula>B357&lt;44136.0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B357:B551">
-    <cfRule type="expression" dxfId="63" priority="70">
+    <cfRule type="expression" dxfId="62" priority="69">
       <formula>B357&lt;44143.0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -40097,15 +40308,20 @@
     <hyperlink r:id="rId91" ref="S529"/>
     <hyperlink r:id="rId92" ref="S530"/>
     <hyperlink r:id="rId93" ref="S531"/>
+    <hyperlink r:id="rId94" ref="S532"/>
+    <hyperlink r:id="rId95" ref="S533"/>
+    <hyperlink r:id="rId96" ref="S534"/>
+    <hyperlink r:id="rId97" ref="S535"/>
+    <hyperlink r:id="rId98" ref="S536"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId94"/>
-  <legacyDrawing r:id="rId95"/>
+  <drawing r:id="rId99"/>
+  <legacyDrawing r:id="rId100"/>
   <tableParts count="2">
-    <tablePart r:id="rId98"/>
-    <tablePart r:id="rId99"/>
+    <tablePart r:id="rId103"/>
+    <tablePart r:id="rId104"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201017
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -7315,7 +7315,7 @@
     <numFmt numFmtId="164" formatCode="mm&quot;月&quot;dd&quot;日 &quot;dddd"/>
     <numFmt numFmtId="165" formatCode="m/d"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="17">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -7392,10 +7392,6 @@
       <u/>
       <color rgb="FF1155CC"/>
     </font>
-    <font/>
-    <font>
-      <color rgb="FF000000"/>
-    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -7441,7 +7437,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="65">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -7630,24 +7626,6 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
@@ -39246,14 +39224,14 @@
       </c>
     </row>
     <row r="533">
-      <c r="A533" s="63" t="s">
+      <c r="A533" s="16" t="s">
         <v>1973</v>
       </c>
       <c r="B533" s="6">
         <v>44120.0</v>
       </c>
       <c r="C533" s="34"/>
-      <c r="D533" s="64" t="s">
+      <c r="D533" s="7" t="s">
         <v>1974</v>
       </c>
       <c r="E533" s="7" t="s">
@@ -39263,29 +39241,29 @@
       <c r="G533" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H533" s="65" t="s">
+      <c r="H533" s="8" t="s">
         <v>1975</v>
       </c>
-      <c r="I533" s="66">
+      <c r="I533" s="9">
         <v>44104.0</v>
       </c>
-      <c r="J533" s="67" t="s">
+      <c r="J533" s="12" t="s">
         <v>1442</v>
       </c>
-      <c r="K533" s="68" t="s">
+      <c r="K533" s="13" t="s">
         <v>1976</v>
       </c>
-      <c r="L533" s="67" t="s">
+      <c r="L533" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M533" s="68" t="s">
+      <c r="M533" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N533" s="25"/>
-      <c r="O533" s="65" t="s">
+      <c r="O533" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P533" s="65" t="s">
+      <c r="P533" s="8" t="s">
         <v>1977</v>
       </c>
       <c r="Q533" s="19"/>
@@ -39300,14 +39278,14 @@
       </c>
     </row>
     <row r="534">
-      <c r="A534" s="63" t="s">
+      <c r="A534" s="16" t="s">
         <v>1979</v>
       </c>
       <c r="B534" s="6">
         <v>44120.0</v>
       </c>
       <c r="C534" s="34"/>
-      <c r="D534" s="64" t="s">
+      <c r="D534" s="7" t="s">
         <v>1974</v>
       </c>
       <c r="E534" s="7" t="s">
@@ -39325,7 +39303,7 @@
         <f t="shared" ref="I534:I536" si="67">$I$533</f>
         <v>44104</v>
       </c>
-      <c r="J534" s="67" t="s">
+      <c r="J534" s="12" t="s">
         <v>1442</v>
       </c>
       <c r="K534" s="22" t="str">
@@ -39337,11 +39315,11 @@
         <f t="shared" ref="L534:L536" si="69">$L$533</f>
         <v>居家檢疫</v>
       </c>
-      <c r="M534" s="68" t="s">
+      <c r="M534" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N534" s="25"/>
-      <c r="O534" s="65" t="s">
+      <c r="O534" s="8" t="s">
         <v>85</v>
       </c>
       <c r="P534" s="21" t="str">
@@ -39360,14 +39338,14 @@
       </c>
     </row>
     <row r="535">
-      <c r="A535" s="63" t="s">
+      <c r="A535" s="16" t="s">
         <v>1980</v>
       </c>
       <c r="B535" s="6">
         <v>44120.0</v>
       </c>
       <c r="C535" s="34"/>
-      <c r="D535" s="64" t="s">
+      <c r="D535" s="7" t="s">
         <v>1974</v>
       </c>
       <c r="E535" s="7" t="s">
@@ -39385,7 +39363,7 @@
         <f t="shared" si="67"/>
         <v>44104</v>
       </c>
-      <c r="J535" s="67" t="s">
+      <c r="J535" s="12" t="s">
         <v>1442</v>
       </c>
       <c r="K535" s="22" t="str">
@@ -39397,11 +39375,11 @@
         <f t="shared" si="69"/>
         <v>居家檢疫</v>
       </c>
-      <c r="M535" s="68" t="s">
+      <c r="M535" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N535" s="25"/>
-      <c r="O535" s="65" t="s">
+      <c r="O535" s="8" t="s">
         <v>85</v>
       </c>
       <c r="P535" s="21" t="str">
@@ -39420,14 +39398,14 @@
       </c>
     </row>
     <row r="536">
-      <c r="A536" s="63" t="s">
+      <c r="A536" s="16" t="s">
         <v>1981</v>
       </c>
       <c r="B536" s="6">
         <v>44120.0</v>
       </c>
       <c r="C536" s="34"/>
-      <c r="D536" s="64" t="s">
+      <c r="D536" s="7" t="s">
         <v>1974</v>
       </c>
       <c r="E536" s="7" t="s">
@@ -39445,7 +39423,7 @@
         <f t="shared" si="67"/>
         <v>44104</v>
       </c>
-      <c r="J536" s="67" t="s">
+      <c r="J536" s="12" t="s">
         <v>1442</v>
       </c>
       <c r="K536" s="22" t="str">
@@ -39457,11 +39435,11 @@
         <f t="shared" si="69"/>
         <v>居家檢疫</v>
       </c>
-      <c r="M536" s="68" t="s">
+      <c r="M536" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N536" s="25"/>
-      <c r="O536" s="65" t="s">
+      <c r="O536" s="8" t="s">
         <v>85</v>
       </c>
       <c r="P536" s="21" t="str">
@@ -39480,8 +39458,8 @@
       </c>
     </row>
     <row r="537">
-      <c r="A537" s="69"/>
-      <c r="B537" s="70"/>
+      <c r="A537" s="63"/>
+      <c r="B537" s="64"/>
       <c r="C537" s="34"/>
       <c r="D537" s="34"/>
       <c r="E537" s="34"/>
@@ -39506,8 +39484,8 @@
       </c>
     </row>
     <row r="538">
-      <c r="A538" s="69"/>
-      <c r="B538" s="70"/>
+      <c r="A538" s="63"/>
+      <c r="B538" s="64"/>
       <c r="C538" s="34"/>
       <c r="D538" s="34"/>
       <c r="E538" s="34"/>
@@ -39532,8 +39510,8 @@
       </c>
     </row>
     <row r="539">
-      <c r="A539" s="69"/>
-      <c r="B539" s="70"/>
+      <c r="A539" s="63"/>
+      <c r="B539" s="64"/>
       <c r="C539" s="34"/>
       <c r="D539" s="34"/>
       <c r="E539" s="34"/>
@@ -39558,8 +39536,8 @@
       </c>
     </row>
     <row r="540">
-      <c r="A540" s="69"/>
-      <c r="B540" s="70"/>
+      <c r="A540" s="63"/>
+      <c r="B540" s="64"/>
       <c r="C540" s="34"/>
       <c r="D540" s="34"/>
       <c r="E540" s="34"/>
@@ -39584,8 +39562,8 @@
       </c>
     </row>
     <row r="541">
-      <c r="A541" s="69"/>
-      <c r="B541" s="70"/>
+      <c r="A541" s="63"/>
+      <c r="B541" s="64"/>
       <c r="C541" s="34"/>
       <c r="D541" s="34"/>
       <c r="E541" s="34"/>
@@ -39610,8 +39588,8 @@
       </c>
     </row>
     <row r="542">
-      <c r="A542" s="69"/>
-      <c r="B542" s="70"/>
+      <c r="A542" s="63"/>
+      <c r="B542" s="64"/>
       <c r="C542" s="34"/>
       <c r="D542" s="34"/>
       <c r="E542" s="34"/>
@@ -39636,8 +39614,8 @@
       </c>
     </row>
     <row r="543">
-      <c r="A543" s="69"/>
-      <c r="B543" s="70"/>
+      <c r="A543" s="63"/>
+      <c r="B543" s="64"/>
       <c r="C543" s="34"/>
       <c r="D543" s="34"/>
       <c r="E543" s="34"/>
@@ -39662,8 +39640,8 @@
       </c>
     </row>
     <row r="544">
-      <c r="A544" s="69"/>
-      <c r="B544" s="70"/>
+      <c r="A544" s="63"/>
+      <c r="B544" s="64"/>
       <c r="C544" s="34"/>
       <c r="D544" s="34"/>
       <c r="E544" s="34"/>
@@ -39688,8 +39666,8 @@
       </c>
     </row>
     <row r="545">
-      <c r="A545" s="69"/>
-      <c r="B545" s="70"/>
+      <c r="A545" s="63"/>
+      <c r="B545" s="64"/>
       <c r="C545" s="34"/>
       <c r="D545" s="34"/>
       <c r="E545" s="34"/>
@@ -39714,8 +39692,8 @@
       </c>
     </row>
     <row r="546">
-      <c r="A546" s="69"/>
-      <c r="B546" s="70"/>
+      <c r="A546" s="63"/>
+      <c r="B546" s="64"/>
       <c r="C546" s="34"/>
       <c r="D546" s="34"/>
       <c r="E546" s="34"/>
@@ -39740,8 +39718,8 @@
       </c>
     </row>
     <row r="547">
-      <c r="A547" s="69"/>
-      <c r="B547" s="70"/>
+      <c r="A547" s="63"/>
+      <c r="B547" s="64"/>
       <c r="C547" s="34"/>
       <c r="D547" s="34"/>
       <c r="E547" s="34"/>
@@ -39766,8 +39744,8 @@
       </c>
     </row>
     <row r="548">
-      <c r="A548" s="69"/>
-      <c r="B548" s="70"/>
+      <c r="A548" s="63"/>
+      <c r="B548" s="64"/>
       <c r="C548" s="34"/>
       <c r="D548" s="34"/>
       <c r="E548" s="34"/>
@@ -39792,8 +39770,8 @@
       </c>
     </row>
     <row r="549">
-      <c r="A549" s="69"/>
-      <c r="B549" s="70"/>
+      <c r="A549" s="63"/>
+      <c r="B549" s="64"/>
       <c r="C549" s="34"/>
       <c r="D549" s="34"/>
       <c r="E549" s="34"/>
@@ -39818,8 +39796,8 @@
       </c>
     </row>
     <row r="550">
-      <c r="A550" s="69"/>
-      <c r="B550" s="70"/>
+      <c r="A550" s="63"/>
+      <c r="B550" s="64"/>
       <c r="C550" s="34"/>
       <c r="D550" s="34"/>
       <c r="E550" s="34"/>
@@ -39844,8 +39822,8 @@
       </c>
     </row>
     <row r="551">
-      <c r="A551" s="69"/>
-      <c r="B551" s="70"/>
+      <c r="A551" s="63"/>
+      <c r="B551" s="64"/>
       <c r="C551" s="34"/>
       <c r="D551" s="34"/>
       <c r="E551" s="34"/>

</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201020
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -563,7 +563,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5915" uniqueCount="1982">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5978" uniqueCount="2005">
   <si>
     <t>案例</t>
   </si>
@@ -7305,6 +7305,84 @@
   </si>
   <si>
     <t>#535</t>
+  </si>
+  <si>
+    <t>#536</t>
+  </si>
+  <si>
+    <t>2019/8-2020/10/11 法國</t>
+  </si>
+  <si>
+    <t>10/11 採檢
+10/16 二採
+10/19 確診</t>
+  </si>
+  <si>
+    <t>喉嚨痛 咳嗽 腹瀉 全身倦怠 呼吸困難</t>
+  </si>
+  <si>
+    <t>於機場採檢結果為陰性</t>
+  </si>
+  <si>
+    <t>新增5例境外移入COVID-19病例，分自法國、菲律賓、印尼、俄羅斯入境</t>
+  </si>
+  <si>
+    <t>#537</t>
+  </si>
+  <si>
+    <t>-10/4 菲律賓</t>
+  </si>
+  <si>
+    <t>10/17 採檢
+10/19 確診</t>
+  </si>
+  <si>
+    <t>長期於菲律賓工作，約1至2個月返台一次
+本次因休假於10月4日返台，入境迄今無症狀
+10月17日進行檢疫期滿前採檢</t>
+  </si>
+  <si>
+    <t>#538</t>
+  </si>
+  <si>
+    <t>-10/4 菲律賓→台灣</t>
+  </si>
+  <si>
+    <t>因工作於10月4日入境台灣，入境迄今無症狀，10月17日由衛生單位安排進行檢疫期滿前採檢，於今日確診</t>
+  </si>
+  <si>
+    <t>#539</t>
+  </si>
+  <si>
+    <t>-10/3 印尼→台灣</t>
+  </si>
+  <si>
+    <t>10/18 採檢
+10/19 確診</t>
+  </si>
+  <si>
+    <t>因就學於10月3日入境台灣，入境迄今無症狀，10月18日由校方安排至醫院進行檢疫期滿採檢，於今日確診</t>
+  </si>
+  <si>
+    <t>#540</t>
+  </si>
+  <si>
+    <t>俄羅斯</t>
+  </si>
+  <si>
+    <t>-10/9 俄羅斯→台灣</t>
+  </si>
+  <si>
+    <t>10/7 自費採檢
+10/17 採檢
+10/19 確診</t>
+  </si>
+  <si>
+    <t>味覺喪失</t>
+  </si>
+  <si>
+    <t>因就學於10月9日入境台灣，10月7日曾於國外自費檢驗結果為陰性。
+個案居家檢疫期間，於10月16日出現味覺喪失情形，17日由衛生單位安排採檢，於今日確診</t>
   </si>
 </sst>
 </file>
@@ -39458,133 +39536,283 @@
       </c>
     </row>
     <row r="537">
-      <c r="A537" s="63"/>
-      <c r="B537" s="64"/>
-      <c r="C537" s="34"/>
-      <c r="D537" s="34"/>
-      <c r="E537" s="34"/>
+      <c r="A537" s="16" t="s">
+        <v>1982</v>
+      </c>
+      <c r="B537" s="6">
+        <v>44123.0</v>
+      </c>
+      <c r="C537" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D537" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E537" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F537" s="34"/>
-      <c r="G537" s="34"/>
-      <c r="H537" s="21"/>
-      <c r="I537" s="19"/>
-      <c r="J537" s="10"/>
-      <c r="K537" s="22"/>
-      <c r="L537" s="23"/>
-      <c r="M537" s="22"/>
+      <c r="G537" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H537" s="8" t="s">
+        <v>1983</v>
+      </c>
+      <c r="I537" s="9">
+        <v>44115.0</v>
+      </c>
+      <c r="J537" s="10">
+        <v>44113.0</v>
+      </c>
+      <c r="K537" s="13" t="s">
+        <v>1984</v>
+      </c>
+      <c r="L537" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M537" s="13" t="s">
+        <v>1985</v>
+      </c>
       <c r="N537" s="25"/>
-      <c r="O537" s="21"/>
-      <c r="P537" s="21"/>
+      <c r="O537" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P537" s="8" t="s">
+        <v>1986</v>
+      </c>
       <c r="Q537" s="19"/>
       <c r="R537" s="19"/>
-      <c r="S537" s="20"/>
+      <c r="S537" s="61" t="s">
+        <v>1987</v>
+      </c>
       <c r="T537" s="20"/>
       <c r="U537" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#536</v>
       </c>
     </row>
     <row r="538">
-      <c r="A538" s="63"/>
-      <c r="B538" s="64"/>
-      <c r="C538" s="34"/>
-      <c r="D538" s="34"/>
-      <c r="E538" s="34"/>
+      <c r="A538" s="16" t="s">
+        <v>1988</v>
+      </c>
+      <c r="B538" s="6">
+        <v>44123.0</v>
+      </c>
+      <c r="C538" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D538" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E538" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F538" s="34"/>
-      <c r="G538" s="34"/>
-      <c r="H538" s="21"/>
-      <c r="I538" s="19"/>
-      <c r="J538" s="10"/>
-      <c r="K538" s="22"/>
-      <c r="L538" s="23"/>
-      <c r="M538" s="22"/>
+      <c r="G538" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H538" s="8" t="s">
+        <v>1989</v>
+      </c>
+      <c r="I538" s="9">
+        <v>44108.0</v>
+      </c>
+      <c r="J538" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K538" s="13" t="s">
+        <v>1990</v>
+      </c>
+      <c r="L538" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M538" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N538" s="25"/>
-      <c r="O538" s="21"/>
-      <c r="P538" s="21"/>
+      <c r="O538" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P538" s="8" t="s">
+        <v>1991</v>
+      </c>
       <c r="Q538" s="19"/>
       <c r="R538" s="19"/>
-      <c r="S538" s="20"/>
+      <c r="S538" s="61" t="s">
+        <v>1987</v>
+      </c>
       <c r="T538" s="20"/>
       <c r="U538" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#537</v>
       </c>
     </row>
     <row r="539">
-      <c r="A539" s="63"/>
-      <c r="B539" s="64"/>
-      <c r="C539" s="34"/>
-      <c r="D539" s="34"/>
-      <c r="E539" s="34"/>
+      <c r="A539" s="16" t="s">
+        <v>1992</v>
+      </c>
+      <c r="B539" s="6">
+        <v>44123.0</v>
+      </c>
+      <c r="C539" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D539" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E539" s="7" t="s">
+        <v>205</v>
+      </c>
       <c r="F539" s="34"/>
-      <c r="G539" s="34"/>
-      <c r="H539" s="21"/>
-      <c r="I539" s="19"/>
-      <c r="J539" s="10"/>
-      <c r="K539" s="22"/>
-      <c r="L539" s="23"/>
-      <c r="M539" s="22"/>
+      <c r="G539" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H539" s="8" t="s">
+        <v>1993</v>
+      </c>
+      <c r="I539" s="9">
+        <v>44108.0</v>
+      </c>
+      <c r="J539" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K539" s="13" t="s">
+        <v>1990</v>
+      </c>
+      <c r="L539" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M539" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N539" s="25"/>
-      <c r="O539" s="21"/>
-      <c r="P539" s="21"/>
+      <c r="O539" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P539" s="8" t="s">
+        <v>1994</v>
+      </c>
       <c r="Q539" s="19"/>
       <c r="R539" s="19"/>
-      <c r="S539" s="20"/>
+      <c r="S539" s="61" t="s">
+        <v>1987</v>
+      </c>
       <c r="T539" s="20"/>
       <c r="U539" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#538</v>
       </c>
     </row>
     <row r="540">
-      <c r="A540" s="63"/>
-      <c r="B540" s="64"/>
-      <c r="C540" s="34"/>
-      <c r="D540" s="34"/>
-      <c r="E540" s="34"/>
+      <c r="A540" s="16" t="s">
+        <v>1995</v>
+      </c>
+      <c r="B540" s="6">
+        <v>44123.0</v>
+      </c>
+      <c r="C540" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D540" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="E540" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F540" s="34"/>
-      <c r="G540" s="34"/>
-      <c r="H540" s="21"/>
-      <c r="I540" s="19"/>
-      <c r="J540" s="10"/>
-      <c r="K540" s="22"/>
-      <c r="L540" s="23"/>
-      <c r="M540" s="22"/>
+      <c r="G540" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H540" s="8" t="s">
+        <v>1996</v>
+      </c>
+      <c r="I540" s="9">
+        <v>44107.0</v>
+      </c>
+      <c r="J540" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K540" s="13" t="s">
+        <v>1997</v>
+      </c>
+      <c r="L540" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M540" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N540" s="25"/>
-      <c r="O540" s="21"/>
-      <c r="P540" s="21"/>
+      <c r="O540" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P540" s="8" t="s">
+        <v>1998</v>
+      </c>
       <c r="Q540" s="19"/>
       <c r="R540" s="19"/>
-      <c r="S540" s="20"/>
+      <c r="S540" s="61" t="s">
+        <v>1987</v>
+      </c>
       <c r="T540" s="20"/>
       <c r="U540" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#539</v>
       </c>
     </row>
     <row r="541">
-      <c r="A541" s="63"/>
-      <c r="B541" s="64"/>
-      <c r="C541" s="34"/>
-      <c r="D541" s="34"/>
-      <c r="E541" s="34"/>
+      <c r="A541" s="16" t="s">
+        <v>1999</v>
+      </c>
+      <c r="B541" s="6">
+        <v>44123.0</v>
+      </c>
+      <c r="C541" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D541" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="E541" s="7" t="s">
+        <v>2000</v>
+      </c>
       <c r="F541" s="34"/>
-      <c r="G541" s="34"/>
-      <c r="H541" s="21"/>
-      <c r="I541" s="19"/>
-      <c r="J541" s="10"/>
-      <c r="K541" s="22"/>
-      <c r="L541" s="23"/>
-      <c r="M541" s="22"/>
+      <c r="G541" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H541" s="8" t="s">
+        <v>2001</v>
+      </c>
+      <c r="I541" s="9">
+        <v>44113.0</v>
+      </c>
+      <c r="J541" s="10">
+        <v>44120.0</v>
+      </c>
+      <c r="K541" s="13" t="s">
+        <v>2002</v>
+      </c>
+      <c r="L541" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M541" s="13" t="s">
+        <v>2003</v>
+      </c>
       <c r="N541" s="25"/>
-      <c r="O541" s="21"/>
-      <c r="P541" s="21"/>
+      <c r="O541" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P541" s="8" t="s">
+        <v>2004</v>
+      </c>
       <c r="Q541" s="19"/>
       <c r="R541" s="19"/>
-      <c r="S541" s="20"/>
+      <c r="S541" s="61" t="s">
+        <v>1987</v>
+      </c>
       <c r="T541" s="20"/>
       <c r="U541" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#540</v>
       </c>
     </row>
     <row r="542">
@@ -40291,15 +40519,20 @@
     <hyperlink r:id="rId96" ref="S534"/>
     <hyperlink r:id="rId97" ref="S535"/>
     <hyperlink r:id="rId98" ref="S536"/>
+    <hyperlink r:id="rId99" ref="S537"/>
+    <hyperlink r:id="rId100" ref="S538"/>
+    <hyperlink r:id="rId101" ref="S539"/>
+    <hyperlink r:id="rId102" ref="S540"/>
+    <hyperlink r:id="rId103" ref="S541"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId99"/>
-  <legacyDrawing r:id="rId100"/>
+  <drawing r:id="rId104"/>
+  <legacyDrawing r:id="rId105"/>
   <tableParts count="2">
-    <tablePart r:id="rId103"/>
-    <tablePart r:id="rId104"/>
+    <tablePart r:id="rId108"/>
+    <tablePart r:id="rId109"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201021
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -563,7 +563,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5978" uniqueCount="2005">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6016" uniqueCount="2016">
   <si>
     <t>案例</t>
   </si>
@@ -7383,6 +7383,44 @@
   <si>
     <t>因就學於10月9日入境台灣，10月7日曾於國外自費檢驗結果為陰性。
 個案居家檢疫期間，於10月16日出現味覺喪失情形，17日由衛生單位安排採檢，於今日確診</t>
+  </si>
+  <si>
+    <t>#541</t>
+  </si>
+  <si>
+    <t>-10/5 菲律賓→台灣</t>
+  </si>
+  <si>
+    <t>10/18 採檢
+10/20 確診</t>
+  </si>
+  <si>
+    <t>10月5日搭乘同班機入境台灣，入境後至集中檢疫所檢疫，迄今無疑似症狀，10月18日檢疫期滿前進行採檢，於今日確診</t>
+  </si>
+  <si>
+    <t>國內新增3例境外移入COVID-19病例，均自菲律賓入境</t>
+  </si>
+  <si>
+    <t>#542</t>
+  </si>
+  <si>
+    <t>#543</t>
+  </si>
+  <si>
+    <t>1月-10/5 菲律賓→台灣</t>
+  </si>
+  <si>
+    <t>10/15 採檢
+10/18 二採
+10/20 確診</t>
+  </si>
+  <si>
+    <t>輕微發燒 肌肉痠痛 咳嗽 呼吸困難</t>
+  </si>
+  <si>
+    <t>長期於菲律賓工作(前次自台灣出境時間為今年1月)
+10月5日出現輕微發燒、肌肉痠痛、咳嗽、呼吸困難情形
+10月15日於菲律賓當地就醫診斷為肺炎，但未住院治療，僅服藥與採檢(10月19日得知檢驗結果為陽性)</t>
   </si>
 </sst>
 </file>
@@ -8485,7 +8523,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:A551" displayName="Table_1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:A601" displayName="Table_1" id="1">
   <tableColumns count="1">
     <tableColumn name="案例" id="1"/>
   </tableColumns>
@@ -8494,7 +8532,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="B1:U551" displayName="Table_2" id="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="B1:U601" displayName="Table_2" id="2">
   <tableColumns count="20">
     <tableColumn name="新聞稿發布日期" id="1"/>
     <tableColumn name="性別" id="2"/>
@@ -39816,81 +39854,171 @@
       </c>
     </row>
     <row r="542">
-      <c r="A542" s="63"/>
-      <c r="B542" s="64"/>
-      <c r="C542" s="34"/>
-      <c r="D542" s="34"/>
-      <c r="E542" s="34"/>
+      <c r="A542" s="16" t="s">
+        <v>2005</v>
+      </c>
+      <c r="B542" s="6">
+        <v>44124.0</v>
+      </c>
+      <c r="C542" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D542" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E542" s="7" t="s">
+        <v>205</v>
+      </c>
       <c r="F542" s="34"/>
-      <c r="G542" s="34"/>
-      <c r="H542" s="21"/>
-      <c r="I542" s="19"/>
-      <c r="J542" s="10"/>
-      <c r="K542" s="22"/>
-      <c r="L542" s="23"/>
-      <c r="M542" s="22"/>
+      <c r="G542" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H542" s="8" t="s">
+        <v>2006</v>
+      </c>
+      <c r="I542" s="9">
+        <v>44109.0</v>
+      </c>
+      <c r="J542" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K542" s="13" t="s">
+        <v>2007</v>
+      </c>
+      <c r="L542" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M542" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N542" s="25"/>
-      <c r="O542" s="21"/>
-      <c r="P542" s="21"/>
+      <c r="O542" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P542" s="8" t="s">
+        <v>2008</v>
+      </c>
       <c r="Q542" s="19"/>
       <c r="R542" s="19"/>
-      <c r="S542" s="20"/>
+      <c r="S542" s="61" t="s">
+        <v>2009</v>
+      </c>
       <c r="T542" s="20"/>
       <c r="U542" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#541</v>
       </c>
     </row>
     <row r="543">
-      <c r="A543" s="63"/>
-      <c r="B543" s="64"/>
-      <c r="C543" s="34"/>
-      <c r="D543" s="34"/>
-      <c r="E543" s="34"/>
+      <c r="A543" s="16" t="s">
+        <v>2010</v>
+      </c>
+      <c r="B543" s="6">
+        <v>44124.0</v>
+      </c>
+      <c r="C543" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D543" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E543" s="7" t="s">
+        <v>205</v>
+      </c>
       <c r="F543" s="34"/>
-      <c r="G543" s="34"/>
-      <c r="H543" s="21"/>
-      <c r="I543" s="19"/>
-      <c r="J543" s="10"/>
-      <c r="K543" s="22"/>
-      <c r="L543" s="23"/>
-      <c r="M543" s="22"/>
+      <c r="G543" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H543" s="8" t="s">
+        <v>2006</v>
+      </c>
+      <c r="I543" s="9">
+        <v>44109.0</v>
+      </c>
+      <c r="J543" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K543" s="13" t="s">
+        <v>2007</v>
+      </c>
+      <c r="L543" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M543" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N543" s="25"/>
-      <c r="O543" s="21"/>
-      <c r="P543" s="21"/>
+      <c r="O543" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P543" s="8" t="s">
+        <v>2008</v>
+      </c>
       <c r="Q543" s="19"/>
       <c r="R543" s="19"/>
-      <c r="S543" s="20"/>
+      <c r="S543" s="61" t="s">
+        <v>2009</v>
+      </c>
       <c r="T543" s="20"/>
       <c r="U543" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#542</v>
       </c>
     </row>
     <row r="544">
-      <c r="A544" s="63"/>
-      <c r="B544" s="64"/>
-      <c r="C544" s="34"/>
-      <c r="D544" s="34"/>
-      <c r="E544" s="34"/>
+      <c r="A544" s="16" t="s">
+        <v>2011</v>
+      </c>
+      <c r="B544" s="6">
+        <v>44124.0</v>
+      </c>
+      <c r="C544" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D544" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E544" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F544" s="34"/>
-      <c r="G544" s="34"/>
-      <c r="H544" s="21"/>
-      <c r="I544" s="19"/>
-      <c r="J544" s="10"/>
-      <c r="K544" s="22"/>
-      <c r="L544" s="23"/>
-      <c r="M544" s="22"/>
+      <c r="G544" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H544" s="8" t="s">
+        <v>2012</v>
+      </c>
+      <c r="I544" s="9">
+        <v>44109.0</v>
+      </c>
+      <c r="J544" s="10">
+        <v>44109.0</v>
+      </c>
+      <c r="K544" s="13" t="s">
+        <v>2013</v>
+      </c>
+      <c r="L544" s="12" t="s">
+        <v>363</v>
+      </c>
+      <c r="M544" s="13" t="s">
+        <v>2014</v>
+      </c>
       <c r="N544" s="25"/>
-      <c r="O544" s="21"/>
-      <c r="P544" s="21"/>
+      <c r="O544" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P544" s="8" t="s">
+        <v>2015</v>
+      </c>
       <c r="Q544" s="19"/>
       <c r="R544" s="19"/>
-      <c r="S544" s="20"/>
+      <c r="S544" s="61" t="s">
+        <v>2009</v>
+      </c>
       <c r="T544" s="20"/>
       <c r="U544" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#543</v>
       </c>
     </row>
     <row r="545">
@@ -40075,348 +40203,1498 @@
         <v/>
       </c>
     </row>
+    <row r="552">
+      <c r="A552" s="63"/>
+      <c r="B552" s="64"/>
+      <c r="C552" s="34"/>
+      <c r="D552" s="34"/>
+      <c r="E552" s="34"/>
+      <c r="F552" s="34"/>
+      <c r="G552" s="34"/>
+      <c r="H552" s="21"/>
+      <c r="I552" s="19"/>
+      <c r="J552" s="10"/>
+      <c r="K552" s="22"/>
+      <c r="L552" s="23"/>
+      <c r="M552" s="22"/>
+      <c r="N552" s="25"/>
+      <c r="O552" s="21"/>
+      <c r="P552" s="21"/>
+      <c r="Q552" s="19"/>
+      <c r="R552" s="19"/>
+      <c r="S552" s="20"/>
+      <c r="T552" s="20"/>
+      <c r="U552" s="18"/>
+    </row>
+    <row r="553">
+      <c r="A553" s="63"/>
+      <c r="B553" s="64"/>
+      <c r="C553" s="34"/>
+      <c r="D553" s="34"/>
+      <c r="E553" s="34"/>
+      <c r="F553" s="34"/>
+      <c r="G553" s="34"/>
+      <c r="H553" s="21"/>
+      <c r="I553" s="19"/>
+      <c r="J553" s="10"/>
+      <c r="K553" s="22"/>
+      <c r="L553" s="23"/>
+      <c r="M553" s="22"/>
+      <c r="N553" s="25"/>
+      <c r="O553" s="21"/>
+      <c r="P553" s="21"/>
+      <c r="Q553" s="19"/>
+      <c r="R553" s="19"/>
+      <c r="S553" s="20"/>
+      <c r="T553" s="20"/>
+      <c r="U553" s="18"/>
+    </row>
+    <row r="554">
+      <c r="A554" s="63"/>
+      <c r="B554" s="64"/>
+      <c r="C554" s="34"/>
+      <c r="D554" s="34"/>
+      <c r="E554" s="34"/>
+      <c r="F554" s="34"/>
+      <c r="G554" s="34"/>
+      <c r="H554" s="21"/>
+      <c r="I554" s="19"/>
+      <c r="J554" s="10"/>
+      <c r="K554" s="22"/>
+      <c r="L554" s="23"/>
+      <c r="M554" s="22"/>
+      <c r="N554" s="25"/>
+      <c r="O554" s="21"/>
+      <c r="P554" s="21"/>
+      <c r="Q554" s="19"/>
+      <c r="R554" s="19"/>
+      <c r="S554" s="20"/>
+      <c r="T554" s="20"/>
+      <c r="U554" s="18"/>
+    </row>
+    <row r="555">
+      <c r="A555" s="63"/>
+      <c r="B555" s="64"/>
+      <c r="C555" s="34"/>
+      <c r="D555" s="34"/>
+      <c r="E555" s="34"/>
+      <c r="F555" s="34"/>
+      <c r="G555" s="34"/>
+      <c r="H555" s="21"/>
+      <c r="I555" s="19"/>
+      <c r="J555" s="10"/>
+      <c r="K555" s="22"/>
+      <c r="L555" s="23"/>
+      <c r="M555" s="22"/>
+      <c r="N555" s="25"/>
+      <c r="O555" s="21"/>
+      <c r="P555" s="21"/>
+      <c r="Q555" s="19"/>
+      <c r="R555" s="19"/>
+      <c r="S555" s="20"/>
+      <c r="T555" s="20"/>
+      <c r="U555" s="18"/>
+    </row>
+    <row r="556">
+      <c r="A556" s="63"/>
+      <c r="B556" s="64"/>
+      <c r="C556" s="34"/>
+      <c r="D556" s="34"/>
+      <c r="E556" s="34"/>
+      <c r="F556" s="34"/>
+      <c r="G556" s="34"/>
+      <c r="H556" s="21"/>
+      <c r="I556" s="19"/>
+      <c r="J556" s="10"/>
+      <c r="K556" s="22"/>
+      <c r="L556" s="23"/>
+      <c r="M556" s="22"/>
+      <c r="N556" s="25"/>
+      <c r="O556" s="21"/>
+      <c r="P556" s="21"/>
+      <c r="Q556" s="19"/>
+      <c r="R556" s="19"/>
+      <c r="S556" s="20"/>
+      <c r="T556" s="20"/>
+      <c r="U556" s="18"/>
+    </row>
+    <row r="557">
+      <c r="A557" s="63"/>
+      <c r="B557" s="64"/>
+      <c r="C557" s="34"/>
+      <c r="D557" s="34"/>
+      <c r="E557" s="34"/>
+      <c r="F557" s="34"/>
+      <c r="G557" s="34"/>
+      <c r="H557" s="21"/>
+      <c r="I557" s="19"/>
+      <c r="J557" s="10"/>
+      <c r="K557" s="22"/>
+      <c r="L557" s="23"/>
+      <c r="M557" s="22"/>
+      <c r="N557" s="25"/>
+      <c r="O557" s="21"/>
+      <c r="P557" s="21"/>
+      <c r="Q557" s="19"/>
+      <c r="R557" s="19"/>
+      <c r="S557" s="20"/>
+      <c r="T557" s="20"/>
+      <c r="U557" s="18"/>
+    </row>
+    <row r="558">
+      <c r="A558" s="63"/>
+      <c r="B558" s="64"/>
+      <c r="C558" s="34"/>
+      <c r="D558" s="34"/>
+      <c r="E558" s="34"/>
+      <c r="F558" s="34"/>
+      <c r="G558" s="34"/>
+      <c r="H558" s="21"/>
+      <c r="I558" s="19"/>
+      <c r="J558" s="10"/>
+      <c r="K558" s="22"/>
+      <c r="L558" s="23"/>
+      <c r="M558" s="22"/>
+      <c r="N558" s="25"/>
+      <c r="O558" s="21"/>
+      <c r="P558" s="21"/>
+      <c r="Q558" s="19"/>
+      <c r="R558" s="19"/>
+      <c r="S558" s="20"/>
+      <c r="T558" s="20"/>
+      <c r="U558" s="18"/>
+    </row>
+    <row r="559">
+      <c r="A559" s="63"/>
+      <c r="B559" s="64"/>
+      <c r="C559" s="34"/>
+      <c r="D559" s="34"/>
+      <c r="E559" s="34"/>
+      <c r="F559" s="34"/>
+      <c r="G559" s="34"/>
+      <c r="H559" s="21"/>
+      <c r="I559" s="19"/>
+      <c r="J559" s="10"/>
+      <c r="K559" s="22"/>
+      <c r="L559" s="23"/>
+      <c r="M559" s="22"/>
+      <c r="N559" s="25"/>
+      <c r="O559" s="21"/>
+      <c r="P559" s="21"/>
+      <c r="Q559" s="19"/>
+      <c r="R559" s="19"/>
+      <c r="S559" s="20"/>
+      <c r="T559" s="20"/>
+      <c r="U559" s="18"/>
+    </row>
+    <row r="560">
+      <c r="A560" s="63"/>
+      <c r="B560" s="64"/>
+      <c r="C560" s="34"/>
+      <c r="D560" s="34"/>
+      <c r="E560" s="34"/>
+      <c r="F560" s="34"/>
+      <c r="G560" s="34"/>
+      <c r="H560" s="21"/>
+      <c r="I560" s="19"/>
+      <c r="J560" s="10"/>
+      <c r="K560" s="22"/>
+      <c r="L560" s="23"/>
+      <c r="M560" s="22"/>
+      <c r="N560" s="25"/>
+      <c r="O560" s="21"/>
+      <c r="P560" s="21"/>
+      <c r="Q560" s="19"/>
+      <c r="R560" s="19"/>
+      <c r="S560" s="20"/>
+      <c r="T560" s="20"/>
+      <c r="U560" s="18"/>
+    </row>
+    <row r="561">
+      <c r="A561" s="63"/>
+      <c r="B561" s="64"/>
+      <c r="C561" s="34"/>
+      <c r="D561" s="34"/>
+      <c r="E561" s="34"/>
+      <c r="F561" s="34"/>
+      <c r="G561" s="34"/>
+      <c r="H561" s="21"/>
+      <c r="I561" s="19"/>
+      <c r="J561" s="10"/>
+      <c r="K561" s="22"/>
+      <c r="L561" s="23"/>
+      <c r="M561" s="22"/>
+      <c r="N561" s="25"/>
+      <c r="O561" s="21"/>
+      <c r="P561" s="21"/>
+      <c r="Q561" s="19"/>
+      <c r="R561" s="19"/>
+      <c r="S561" s="20"/>
+      <c r="T561" s="20"/>
+      <c r="U561" s="18"/>
+    </row>
+    <row r="562">
+      <c r="A562" s="63"/>
+      <c r="B562" s="64"/>
+      <c r="C562" s="34"/>
+      <c r="D562" s="34"/>
+      <c r="E562" s="34"/>
+      <c r="F562" s="34"/>
+      <c r="G562" s="34"/>
+      <c r="H562" s="21"/>
+      <c r="I562" s="19"/>
+      <c r="J562" s="10"/>
+      <c r="K562" s="22"/>
+      <c r="L562" s="23"/>
+      <c r="M562" s="22"/>
+      <c r="N562" s="25"/>
+      <c r="O562" s="21"/>
+      <c r="P562" s="21"/>
+      <c r="Q562" s="19"/>
+      <c r="R562" s="19"/>
+      <c r="S562" s="20"/>
+      <c r="T562" s="20"/>
+      <c r="U562" s="18"/>
+    </row>
+    <row r="563">
+      <c r="A563" s="63"/>
+      <c r="B563" s="64"/>
+      <c r="C563" s="34"/>
+      <c r="D563" s="34"/>
+      <c r="E563" s="34"/>
+      <c r="F563" s="34"/>
+      <c r="G563" s="34"/>
+      <c r="H563" s="21"/>
+      <c r="I563" s="19"/>
+      <c r="J563" s="10"/>
+      <c r="K563" s="22"/>
+      <c r="L563" s="23"/>
+      <c r="M563" s="22"/>
+      <c r="N563" s="25"/>
+      <c r="O563" s="21"/>
+      <c r="P563" s="21"/>
+      <c r="Q563" s="19"/>
+      <c r="R563" s="19"/>
+      <c r="S563" s="20"/>
+      <c r="T563" s="20"/>
+      <c r="U563" s="18"/>
+    </row>
+    <row r="564">
+      <c r="A564" s="63"/>
+      <c r="B564" s="64"/>
+      <c r="C564" s="34"/>
+      <c r="D564" s="34"/>
+      <c r="E564" s="34"/>
+      <c r="F564" s="34"/>
+      <c r="G564" s="34"/>
+      <c r="H564" s="21"/>
+      <c r="I564" s="19"/>
+      <c r="J564" s="10"/>
+      <c r="K564" s="22"/>
+      <c r="L564" s="23"/>
+      <c r="M564" s="22"/>
+      <c r="N564" s="25"/>
+      <c r="O564" s="21"/>
+      <c r="P564" s="21"/>
+      <c r="Q564" s="19"/>
+      <c r="R564" s="19"/>
+      <c r="S564" s="20"/>
+      <c r="T564" s="20"/>
+      <c r="U564" s="18"/>
+    </row>
+    <row r="565">
+      <c r="A565" s="63"/>
+      <c r="B565" s="64"/>
+      <c r="C565" s="34"/>
+      <c r="D565" s="34"/>
+      <c r="E565" s="34"/>
+      <c r="F565" s="34"/>
+      <c r="G565" s="34"/>
+      <c r="H565" s="21"/>
+      <c r="I565" s="19"/>
+      <c r="J565" s="10"/>
+      <c r="K565" s="22"/>
+      <c r="L565" s="23"/>
+      <c r="M565" s="22"/>
+      <c r="N565" s="25"/>
+      <c r="O565" s="21"/>
+      <c r="P565" s="21"/>
+      <c r="Q565" s="19"/>
+      <c r="R565" s="19"/>
+      <c r="S565" s="20"/>
+      <c r="T565" s="20"/>
+      <c r="U565" s="18"/>
+    </row>
+    <row r="566">
+      <c r="A566" s="63"/>
+      <c r="B566" s="64"/>
+      <c r="C566" s="34"/>
+      <c r="D566" s="34"/>
+      <c r="E566" s="34"/>
+      <c r="F566" s="34"/>
+      <c r="G566" s="34"/>
+      <c r="H566" s="21"/>
+      <c r="I566" s="19"/>
+      <c r="J566" s="10"/>
+      <c r="K566" s="22"/>
+      <c r="L566" s="23"/>
+      <c r="M566" s="22"/>
+      <c r="N566" s="25"/>
+      <c r="O566" s="21"/>
+      <c r="P566" s="21"/>
+      <c r="Q566" s="19"/>
+      <c r="R566" s="19"/>
+      <c r="S566" s="20"/>
+      <c r="T566" s="20"/>
+      <c r="U566" s="18"/>
+    </row>
+    <row r="567">
+      <c r="A567" s="63"/>
+      <c r="B567" s="64"/>
+      <c r="C567" s="34"/>
+      <c r="D567" s="34"/>
+      <c r="E567" s="34"/>
+      <c r="F567" s="34"/>
+      <c r="G567" s="34"/>
+      <c r="H567" s="21"/>
+      <c r="I567" s="19"/>
+      <c r="J567" s="10"/>
+      <c r="K567" s="22"/>
+      <c r="L567" s="23"/>
+      <c r="M567" s="22"/>
+      <c r="N567" s="25"/>
+      <c r="O567" s="21"/>
+      <c r="P567" s="21"/>
+      <c r="Q567" s="19"/>
+      <c r="R567" s="19"/>
+      <c r="S567" s="20"/>
+      <c r="T567" s="20"/>
+      <c r="U567" s="18"/>
+    </row>
+    <row r="568">
+      <c r="A568" s="63"/>
+      <c r="B568" s="64"/>
+      <c r="C568" s="34"/>
+      <c r="D568" s="34"/>
+      <c r="E568" s="34"/>
+      <c r="F568" s="34"/>
+      <c r="G568" s="34"/>
+      <c r="H568" s="21"/>
+      <c r="I568" s="19"/>
+      <c r="J568" s="10"/>
+      <c r="K568" s="22"/>
+      <c r="L568" s="23"/>
+      <c r="M568" s="22"/>
+      <c r="N568" s="25"/>
+      <c r="O568" s="21"/>
+      <c r="P568" s="21"/>
+      <c r="Q568" s="19"/>
+      <c r="R568" s="19"/>
+      <c r="S568" s="20"/>
+      <c r="T568" s="20"/>
+      <c r="U568" s="18"/>
+    </row>
+    <row r="569">
+      <c r="A569" s="63"/>
+      <c r="B569" s="64"/>
+      <c r="C569" s="34"/>
+      <c r="D569" s="34"/>
+      <c r="E569" s="34"/>
+      <c r="F569" s="34"/>
+      <c r="G569" s="34"/>
+      <c r="H569" s="21"/>
+      <c r="I569" s="19"/>
+      <c r="J569" s="10"/>
+      <c r="K569" s="22"/>
+      <c r="L569" s="23"/>
+      <c r="M569" s="22"/>
+      <c r="N569" s="25"/>
+      <c r="O569" s="21"/>
+      <c r="P569" s="21"/>
+      <c r="Q569" s="19"/>
+      <c r="R569" s="19"/>
+      <c r="S569" s="20"/>
+      <c r="T569" s="20"/>
+      <c r="U569" s="18"/>
+    </row>
+    <row r="570">
+      <c r="A570" s="63"/>
+      <c r="B570" s="64"/>
+      <c r="C570" s="34"/>
+      <c r="D570" s="34"/>
+      <c r="E570" s="34"/>
+      <c r="F570" s="34"/>
+      <c r="G570" s="34"/>
+      <c r="H570" s="21"/>
+      <c r="I570" s="19"/>
+      <c r="J570" s="10"/>
+      <c r="K570" s="22"/>
+      <c r="L570" s="23"/>
+      <c r="M570" s="22"/>
+      <c r="N570" s="25"/>
+      <c r="O570" s="21"/>
+      <c r="P570" s="21"/>
+      <c r="Q570" s="19"/>
+      <c r="R570" s="19"/>
+      <c r="S570" s="20"/>
+      <c r="T570" s="20"/>
+      <c r="U570" s="18"/>
+    </row>
+    <row r="571">
+      <c r="A571" s="63"/>
+      <c r="B571" s="64"/>
+      <c r="C571" s="34"/>
+      <c r="D571" s="34"/>
+      <c r="E571" s="34"/>
+      <c r="F571" s="34"/>
+      <c r="G571" s="34"/>
+      <c r="H571" s="21"/>
+      <c r="I571" s="19"/>
+      <c r="J571" s="10"/>
+      <c r="K571" s="22"/>
+      <c r="L571" s="23"/>
+      <c r="M571" s="22"/>
+      <c r="N571" s="25"/>
+      <c r="O571" s="21"/>
+      <c r="P571" s="21"/>
+      <c r="Q571" s="19"/>
+      <c r="R571" s="19"/>
+      <c r="S571" s="20"/>
+      <c r="T571" s="20"/>
+      <c r="U571" s="18"/>
+    </row>
+    <row r="572">
+      <c r="A572" s="63"/>
+      <c r="B572" s="64"/>
+      <c r="C572" s="34"/>
+      <c r="D572" s="34"/>
+      <c r="E572" s="34"/>
+      <c r="F572" s="34"/>
+      <c r="G572" s="34"/>
+      <c r="H572" s="21"/>
+      <c r="I572" s="19"/>
+      <c r="J572" s="10"/>
+      <c r="K572" s="22"/>
+      <c r="L572" s="23"/>
+      <c r="M572" s="22"/>
+      <c r="N572" s="25"/>
+      <c r="O572" s="21"/>
+      <c r="P572" s="21"/>
+      <c r="Q572" s="19"/>
+      <c r="R572" s="19"/>
+      <c r="S572" s="20"/>
+      <c r="T572" s="20"/>
+      <c r="U572" s="18"/>
+    </row>
+    <row r="573">
+      <c r="A573" s="63"/>
+      <c r="B573" s="64"/>
+      <c r="C573" s="34"/>
+      <c r="D573" s="34"/>
+      <c r="E573" s="34"/>
+      <c r="F573" s="34"/>
+      <c r="G573" s="34"/>
+      <c r="H573" s="21"/>
+      <c r="I573" s="19"/>
+      <c r="J573" s="10"/>
+      <c r="K573" s="22"/>
+      <c r="L573" s="23"/>
+      <c r="M573" s="22"/>
+      <c r="N573" s="25"/>
+      <c r="O573" s="21"/>
+      <c r="P573" s="21"/>
+      <c r="Q573" s="19"/>
+      <c r="R573" s="19"/>
+      <c r="S573" s="20"/>
+      <c r="T573" s="20"/>
+      <c r="U573" s="18"/>
+    </row>
+    <row r="574">
+      <c r="A574" s="63"/>
+      <c r="B574" s="64"/>
+      <c r="C574" s="34"/>
+      <c r="D574" s="34"/>
+      <c r="E574" s="34"/>
+      <c r="F574" s="34"/>
+      <c r="G574" s="34"/>
+      <c r="H574" s="21"/>
+      <c r="I574" s="19"/>
+      <c r="J574" s="10"/>
+      <c r="K574" s="22"/>
+      <c r="L574" s="23"/>
+      <c r="M574" s="22"/>
+      <c r="N574" s="25"/>
+      <c r="O574" s="21"/>
+      <c r="P574" s="21"/>
+      <c r="Q574" s="19"/>
+      <c r="R574" s="19"/>
+      <c r="S574" s="20"/>
+      <c r="T574" s="20"/>
+      <c r="U574" s="18"/>
+    </row>
+    <row r="575">
+      <c r="A575" s="63"/>
+      <c r="B575" s="64"/>
+      <c r="C575" s="34"/>
+      <c r="D575" s="34"/>
+      <c r="E575" s="34"/>
+      <c r="F575" s="34"/>
+      <c r="G575" s="34"/>
+      <c r="H575" s="21"/>
+      <c r="I575" s="19"/>
+      <c r="J575" s="10"/>
+      <c r="K575" s="22"/>
+      <c r="L575" s="23"/>
+      <c r="M575" s="22"/>
+      <c r="N575" s="25"/>
+      <c r="O575" s="21"/>
+      <c r="P575" s="21"/>
+      <c r="Q575" s="19"/>
+      <c r="R575" s="19"/>
+      <c r="S575" s="20"/>
+      <c r="T575" s="20"/>
+      <c r="U575" s="18"/>
+    </row>
+    <row r="576">
+      <c r="A576" s="63"/>
+      <c r="B576" s="64"/>
+      <c r="C576" s="34"/>
+      <c r="D576" s="34"/>
+      <c r="E576" s="34"/>
+      <c r="F576" s="34"/>
+      <c r="G576" s="34"/>
+      <c r="H576" s="21"/>
+      <c r="I576" s="19"/>
+      <c r="J576" s="10"/>
+      <c r="K576" s="22"/>
+      <c r="L576" s="23"/>
+      <c r="M576" s="22"/>
+      <c r="N576" s="25"/>
+      <c r="O576" s="21"/>
+      <c r="P576" s="21"/>
+      <c r="Q576" s="19"/>
+      <c r="R576" s="19"/>
+      <c r="S576" s="20"/>
+      <c r="T576" s="20"/>
+      <c r="U576" s="18"/>
+    </row>
+    <row r="577">
+      <c r="A577" s="63"/>
+      <c r="B577" s="64"/>
+      <c r="C577" s="34"/>
+      <c r="D577" s="34"/>
+      <c r="E577" s="34"/>
+      <c r="F577" s="34"/>
+      <c r="G577" s="34"/>
+      <c r="H577" s="21"/>
+      <c r="I577" s="19"/>
+      <c r="J577" s="10"/>
+      <c r="K577" s="22"/>
+      <c r="L577" s="23"/>
+      <c r="M577" s="22"/>
+      <c r="N577" s="25"/>
+      <c r="O577" s="21"/>
+      <c r="P577" s="21"/>
+      <c r="Q577" s="19"/>
+      <c r="R577" s="19"/>
+      <c r="S577" s="20"/>
+      <c r="T577" s="20"/>
+      <c r="U577" s="18"/>
+    </row>
+    <row r="578">
+      <c r="A578" s="63"/>
+      <c r="B578" s="64"/>
+      <c r="C578" s="34"/>
+      <c r="D578" s="34"/>
+      <c r="E578" s="34"/>
+      <c r="F578" s="34"/>
+      <c r="G578" s="34"/>
+      <c r="H578" s="21"/>
+      <c r="I578" s="19"/>
+      <c r="J578" s="10"/>
+      <c r="K578" s="22"/>
+      <c r="L578" s="23"/>
+      <c r="M578" s="22"/>
+      <c r="N578" s="25"/>
+      <c r="O578" s="21"/>
+      <c r="P578" s="21"/>
+      <c r="Q578" s="19"/>
+      <c r="R578" s="19"/>
+      <c r="S578" s="20"/>
+      <c r="T578" s="20"/>
+      <c r="U578" s="18"/>
+    </row>
+    <row r="579">
+      <c r="A579" s="63"/>
+      <c r="B579" s="64"/>
+      <c r="C579" s="34"/>
+      <c r="D579" s="34"/>
+      <c r="E579" s="34"/>
+      <c r="F579" s="34"/>
+      <c r="G579" s="34"/>
+      <c r="H579" s="21"/>
+      <c r="I579" s="19"/>
+      <c r="J579" s="10"/>
+      <c r="K579" s="22"/>
+      <c r="L579" s="23"/>
+      <c r="M579" s="22"/>
+      <c r="N579" s="25"/>
+      <c r="O579" s="21"/>
+      <c r="P579" s="21"/>
+      <c r="Q579" s="19"/>
+      <c r="R579" s="19"/>
+      <c r="S579" s="20"/>
+      <c r="T579" s="20"/>
+      <c r="U579" s="18"/>
+    </row>
+    <row r="580">
+      <c r="A580" s="63"/>
+      <c r="B580" s="64"/>
+      <c r="C580" s="34"/>
+      <c r="D580" s="34"/>
+      <c r="E580" s="34"/>
+      <c r="F580" s="34"/>
+      <c r="G580" s="34"/>
+      <c r="H580" s="21"/>
+      <c r="I580" s="19"/>
+      <c r="J580" s="10"/>
+      <c r="K580" s="22"/>
+      <c r="L580" s="23"/>
+      <c r="M580" s="22"/>
+      <c r="N580" s="25"/>
+      <c r="O580" s="21"/>
+      <c r="P580" s="21"/>
+      <c r="Q580" s="19"/>
+      <c r="R580" s="19"/>
+      <c r="S580" s="20"/>
+      <c r="T580" s="20"/>
+      <c r="U580" s="18"/>
+    </row>
+    <row r="581">
+      <c r="A581" s="63"/>
+      <c r="B581" s="64"/>
+      <c r="C581" s="34"/>
+      <c r="D581" s="34"/>
+      <c r="E581" s="34"/>
+      <c r="F581" s="34"/>
+      <c r="G581" s="34"/>
+      <c r="H581" s="21"/>
+      <c r="I581" s="19"/>
+      <c r="J581" s="10"/>
+      <c r="K581" s="22"/>
+      <c r="L581" s="23"/>
+      <c r="M581" s="22"/>
+      <c r="N581" s="25"/>
+      <c r="O581" s="21"/>
+      <c r="P581" s="21"/>
+      <c r="Q581" s="19"/>
+      <c r="R581" s="19"/>
+      <c r="S581" s="20"/>
+      <c r="T581" s="20"/>
+      <c r="U581" s="18"/>
+    </row>
+    <row r="582">
+      <c r="A582" s="63"/>
+      <c r="B582" s="64"/>
+      <c r="C582" s="34"/>
+      <c r="D582" s="34"/>
+      <c r="E582" s="34"/>
+      <c r="F582" s="34"/>
+      <c r="G582" s="34"/>
+      <c r="H582" s="21"/>
+      <c r="I582" s="19"/>
+      <c r="J582" s="10"/>
+      <c r="K582" s="22"/>
+      <c r="L582" s="23"/>
+      <c r="M582" s="22"/>
+      <c r="N582" s="25"/>
+      <c r="O582" s="21"/>
+      <c r="P582" s="21"/>
+      <c r="Q582" s="19"/>
+      <c r="R582" s="19"/>
+      <c r="S582" s="20"/>
+      <c r="T582" s="20"/>
+      <c r="U582" s="18"/>
+    </row>
+    <row r="583">
+      <c r="A583" s="63"/>
+      <c r="B583" s="64"/>
+      <c r="C583" s="34"/>
+      <c r="D583" s="34"/>
+      <c r="E583" s="34"/>
+      <c r="F583" s="34"/>
+      <c r="G583" s="34"/>
+      <c r="H583" s="21"/>
+      <c r="I583" s="19"/>
+      <c r="J583" s="10"/>
+      <c r="K583" s="22"/>
+      <c r="L583" s="23"/>
+      <c r="M583" s="22"/>
+      <c r="N583" s="25"/>
+      <c r="O583" s="21"/>
+      <c r="P583" s="21"/>
+      <c r="Q583" s="19"/>
+      <c r="R583" s="19"/>
+      <c r="S583" s="20"/>
+      <c r="T583" s="20"/>
+      <c r="U583" s="18"/>
+    </row>
+    <row r="584">
+      <c r="A584" s="63"/>
+      <c r="B584" s="64"/>
+      <c r="C584" s="34"/>
+      <c r="D584" s="34"/>
+      <c r="E584" s="34"/>
+      <c r="F584" s="34"/>
+      <c r="G584" s="34"/>
+      <c r="H584" s="21"/>
+      <c r="I584" s="19"/>
+      <c r="J584" s="10"/>
+      <c r="K584" s="22"/>
+      <c r="L584" s="23"/>
+      <c r="M584" s="22"/>
+      <c r="N584" s="25"/>
+      <c r="O584" s="21"/>
+      <c r="P584" s="21"/>
+      <c r="Q584" s="19"/>
+      <c r="R584" s="19"/>
+      <c r="S584" s="20"/>
+      <c r="T584" s="20"/>
+      <c r="U584" s="18"/>
+    </row>
+    <row r="585">
+      <c r="A585" s="63"/>
+      <c r="B585" s="64"/>
+      <c r="C585" s="34"/>
+      <c r="D585" s="34"/>
+      <c r="E585" s="34"/>
+      <c r="F585" s="34"/>
+      <c r="G585" s="34"/>
+      <c r="H585" s="21"/>
+      <c r="I585" s="19"/>
+      <c r="J585" s="10"/>
+      <c r="K585" s="22"/>
+      <c r="L585" s="23"/>
+      <c r="M585" s="22"/>
+      <c r="N585" s="25"/>
+      <c r="O585" s="21"/>
+      <c r="P585" s="21"/>
+      <c r="Q585" s="19"/>
+      <c r="R585" s="19"/>
+      <c r="S585" s="20"/>
+      <c r="T585" s="20"/>
+      <c r="U585" s="18"/>
+    </row>
+    <row r="586">
+      <c r="A586" s="63"/>
+      <c r="B586" s="64"/>
+      <c r="C586" s="34"/>
+      <c r="D586" s="34"/>
+      <c r="E586" s="34"/>
+      <c r="F586" s="34"/>
+      <c r="G586" s="34"/>
+      <c r="H586" s="21"/>
+      <c r="I586" s="19"/>
+      <c r="J586" s="10"/>
+      <c r="K586" s="22"/>
+      <c r="L586" s="23"/>
+      <c r="M586" s="22"/>
+      <c r="N586" s="25"/>
+      <c r="O586" s="21"/>
+      <c r="P586" s="21"/>
+      <c r="Q586" s="19"/>
+      <c r="R586" s="19"/>
+      <c r="S586" s="20"/>
+      <c r="T586" s="20"/>
+      <c r="U586" s="18"/>
+    </row>
+    <row r="587">
+      <c r="A587" s="63"/>
+      <c r="B587" s="64"/>
+      <c r="C587" s="34"/>
+      <c r="D587" s="34"/>
+      <c r="E587" s="34"/>
+      <c r="F587" s="34"/>
+      <c r="G587" s="34"/>
+      <c r="H587" s="21"/>
+      <c r="I587" s="19"/>
+      <c r="J587" s="10"/>
+      <c r="K587" s="22"/>
+      <c r="L587" s="23"/>
+      <c r="M587" s="22"/>
+      <c r="N587" s="25"/>
+      <c r="O587" s="21"/>
+      <c r="P587" s="21"/>
+      <c r="Q587" s="19"/>
+      <c r="R587" s="19"/>
+      <c r="S587" s="20"/>
+      <c r="T587" s="20"/>
+      <c r="U587" s="18"/>
+    </row>
+    <row r="588">
+      <c r="A588" s="63"/>
+      <c r="B588" s="64"/>
+      <c r="C588" s="34"/>
+      <c r="D588" s="34"/>
+      <c r="E588" s="34"/>
+      <c r="F588" s="34"/>
+      <c r="G588" s="34"/>
+      <c r="H588" s="21"/>
+      <c r="I588" s="19"/>
+      <c r="J588" s="10"/>
+      <c r="K588" s="22"/>
+      <c r="L588" s="23"/>
+      <c r="M588" s="22"/>
+      <c r="N588" s="25"/>
+      <c r="O588" s="21"/>
+      <c r="P588" s="21"/>
+      <c r="Q588" s="19"/>
+      <c r="R588" s="19"/>
+      <c r="S588" s="20"/>
+      <c r="T588" s="20"/>
+      <c r="U588" s="18"/>
+    </row>
+    <row r="589">
+      <c r="A589" s="63"/>
+      <c r="B589" s="64"/>
+      <c r="C589" s="34"/>
+      <c r="D589" s="34"/>
+      <c r="E589" s="34"/>
+      <c r="F589" s="34"/>
+      <c r="G589" s="34"/>
+      <c r="H589" s="21"/>
+      <c r="I589" s="19"/>
+      <c r="J589" s="10"/>
+      <c r="K589" s="22"/>
+      <c r="L589" s="23"/>
+      <c r="M589" s="22"/>
+      <c r="N589" s="25"/>
+      <c r="O589" s="21"/>
+      <c r="P589" s="21"/>
+      <c r="Q589" s="19"/>
+      <c r="R589" s="19"/>
+      <c r="S589" s="20"/>
+      <c r="T589" s="20"/>
+      <c r="U589" s="18"/>
+    </row>
+    <row r="590">
+      <c r="A590" s="63"/>
+      <c r="B590" s="64"/>
+      <c r="C590" s="34"/>
+      <c r="D590" s="34"/>
+      <c r="E590" s="34"/>
+      <c r="F590" s="34"/>
+      <c r="G590" s="34"/>
+      <c r="H590" s="21"/>
+      <c r="I590" s="19"/>
+      <c r="J590" s="10"/>
+      <c r="K590" s="22"/>
+      <c r="L590" s="23"/>
+      <c r="M590" s="22"/>
+      <c r="N590" s="25"/>
+      <c r="O590" s="21"/>
+      <c r="P590" s="21"/>
+      <c r="Q590" s="19"/>
+      <c r="R590" s="19"/>
+      <c r="S590" s="20"/>
+      <c r="T590" s="20"/>
+      <c r="U590" s="18"/>
+    </row>
+    <row r="591">
+      <c r="A591" s="63"/>
+      <c r="B591" s="64"/>
+      <c r="C591" s="34"/>
+      <c r="D591" s="34"/>
+      <c r="E591" s="34"/>
+      <c r="F591" s="34"/>
+      <c r="G591" s="34"/>
+      <c r="H591" s="21"/>
+      <c r="I591" s="19"/>
+      <c r="J591" s="10"/>
+      <c r="K591" s="22"/>
+      <c r="L591" s="23"/>
+      <c r="M591" s="22"/>
+      <c r="N591" s="25"/>
+      <c r="O591" s="21"/>
+      <c r="P591" s="21"/>
+      <c r="Q591" s="19"/>
+      <c r="R591" s="19"/>
+      <c r="S591" s="20"/>
+      <c r="T591" s="20"/>
+      <c r="U591" s="18"/>
+    </row>
+    <row r="592">
+      <c r="A592" s="63"/>
+      <c r="B592" s="64"/>
+      <c r="C592" s="34"/>
+      <c r="D592" s="34"/>
+      <c r="E592" s="34"/>
+      <c r="F592" s="34"/>
+      <c r="G592" s="34"/>
+      <c r="H592" s="21"/>
+      <c r="I592" s="19"/>
+      <c r="J592" s="10"/>
+      <c r="K592" s="22"/>
+      <c r="L592" s="23"/>
+      <c r="M592" s="22"/>
+      <c r="N592" s="25"/>
+      <c r="O592" s="21"/>
+      <c r="P592" s="21"/>
+      <c r="Q592" s="19"/>
+      <c r="R592" s="19"/>
+      <c r="S592" s="20"/>
+      <c r="T592" s="20"/>
+      <c r="U592" s="18"/>
+    </row>
+    <row r="593">
+      <c r="A593" s="63"/>
+      <c r="B593" s="64"/>
+      <c r="C593" s="34"/>
+      <c r="D593" s="34"/>
+      <c r="E593" s="34"/>
+      <c r="F593" s="34"/>
+      <c r="G593" s="34"/>
+      <c r="H593" s="21"/>
+      <c r="I593" s="19"/>
+      <c r="J593" s="10"/>
+      <c r="K593" s="22"/>
+      <c r="L593" s="23"/>
+      <c r="M593" s="22"/>
+      <c r="N593" s="25"/>
+      <c r="O593" s="21"/>
+      <c r="P593" s="21"/>
+      <c r="Q593" s="19"/>
+      <c r="R593" s="19"/>
+      <c r="S593" s="20"/>
+      <c r="T593" s="20"/>
+      <c r="U593" s="18"/>
+    </row>
+    <row r="594">
+      <c r="A594" s="63"/>
+      <c r="B594" s="64"/>
+      <c r="C594" s="34"/>
+      <c r="D594" s="34"/>
+      <c r="E594" s="34"/>
+      <c r="F594" s="34"/>
+      <c r="G594" s="34"/>
+      <c r="H594" s="21"/>
+      <c r="I594" s="19"/>
+      <c r="J594" s="10"/>
+      <c r="K594" s="22"/>
+      <c r="L594" s="23"/>
+      <c r="M594" s="22"/>
+      <c r="N594" s="25"/>
+      <c r="O594" s="21"/>
+      <c r="P594" s="21"/>
+      <c r="Q594" s="19"/>
+      <c r="R594" s="19"/>
+      <c r="S594" s="20"/>
+      <c r="T594" s="20"/>
+      <c r="U594" s="18"/>
+    </row>
+    <row r="595">
+      <c r="A595" s="63"/>
+      <c r="B595" s="64"/>
+      <c r="C595" s="34"/>
+      <c r="D595" s="34"/>
+      <c r="E595" s="34"/>
+      <c r="F595" s="34"/>
+      <c r="G595" s="34"/>
+      <c r="H595" s="21"/>
+      <c r="I595" s="19"/>
+      <c r="J595" s="10"/>
+      <c r="K595" s="22"/>
+      <c r="L595" s="23"/>
+      <c r="M595" s="22"/>
+      <c r="N595" s="25"/>
+      <c r="O595" s="21"/>
+      <c r="P595" s="21"/>
+      <c r="Q595" s="19"/>
+      <c r="R595" s="19"/>
+      <c r="S595" s="20"/>
+      <c r="T595" s="20"/>
+      <c r="U595" s="18"/>
+    </row>
+    <row r="596">
+      <c r="A596" s="63"/>
+      <c r="B596" s="64"/>
+      <c r="C596" s="34"/>
+      <c r="D596" s="34"/>
+      <c r="E596" s="34"/>
+      <c r="F596" s="34"/>
+      <c r="G596" s="34"/>
+      <c r="H596" s="21"/>
+      <c r="I596" s="19"/>
+      <c r="J596" s="10"/>
+      <c r="K596" s="22"/>
+      <c r="L596" s="23"/>
+      <c r="M596" s="22"/>
+      <c r="N596" s="25"/>
+      <c r="O596" s="21"/>
+      <c r="P596" s="21"/>
+      <c r="Q596" s="19"/>
+      <c r="R596" s="19"/>
+      <c r="S596" s="20"/>
+      <c r="T596" s="20"/>
+      <c r="U596" s="18"/>
+    </row>
+    <row r="597">
+      <c r="A597" s="63"/>
+      <c r="B597" s="64"/>
+      <c r="C597" s="34"/>
+      <c r="D597" s="34"/>
+      <c r="E597" s="34"/>
+      <c r="F597" s="34"/>
+      <c r="G597" s="34"/>
+      <c r="H597" s="21"/>
+      <c r="I597" s="19"/>
+      <c r="J597" s="10"/>
+      <c r="K597" s="22"/>
+      <c r="L597" s="23"/>
+      <c r="M597" s="22"/>
+      <c r="N597" s="25"/>
+      <c r="O597" s="21"/>
+      <c r="P597" s="21"/>
+      <c r="Q597" s="19"/>
+      <c r="R597" s="19"/>
+      <c r="S597" s="20"/>
+      <c r="T597" s="20"/>
+      <c r="U597" s="18"/>
+    </row>
+    <row r="598">
+      <c r="A598" s="63"/>
+      <c r="B598" s="64"/>
+      <c r="C598" s="34"/>
+      <c r="D598" s="34"/>
+      <c r="E598" s="34"/>
+      <c r="F598" s="34"/>
+      <c r="G598" s="34"/>
+      <c r="H598" s="21"/>
+      <c r="I598" s="19"/>
+      <c r="J598" s="10"/>
+      <c r="K598" s="22"/>
+      <c r="L598" s="23"/>
+      <c r="M598" s="22"/>
+      <c r="N598" s="25"/>
+      <c r="O598" s="21"/>
+      <c r="P598" s="21"/>
+      <c r="Q598" s="19"/>
+      <c r="R598" s="19"/>
+      <c r="S598" s="20"/>
+      <c r="T598" s="20"/>
+      <c r="U598" s="18"/>
+    </row>
+    <row r="599">
+      <c r="A599" s="63"/>
+      <c r="B599" s="64"/>
+      <c r="C599" s="34"/>
+      <c r="D599" s="34"/>
+      <c r="E599" s="34"/>
+      <c r="F599" s="34"/>
+      <c r="G599" s="34"/>
+      <c r="H599" s="21"/>
+      <c r="I599" s="19"/>
+      <c r="J599" s="10"/>
+      <c r="K599" s="22"/>
+      <c r="L599" s="23"/>
+      <c r="M599" s="22"/>
+      <c r="N599" s="25"/>
+      <c r="O599" s="21"/>
+      <c r="P599" s="21"/>
+      <c r="Q599" s="19"/>
+      <c r="R599" s="19"/>
+      <c r="S599" s="20"/>
+      <c r="T599" s="20"/>
+      <c r="U599" s="18"/>
+    </row>
+    <row r="600">
+      <c r="A600" s="63"/>
+      <c r="B600" s="64"/>
+      <c r="C600" s="34"/>
+      <c r="D600" s="34"/>
+      <c r="E600" s="34"/>
+      <c r="F600" s="34"/>
+      <c r="G600" s="34"/>
+      <c r="H600" s="21"/>
+      <c r="I600" s="19"/>
+      <c r="J600" s="10"/>
+      <c r="K600" s="22"/>
+      <c r="L600" s="23"/>
+      <c r="M600" s="22"/>
+      <c r="N600" s="25"/>
+      <c r="O600" s="21"/>
+      <c r="P600" s="21"/>
+      <c r="Q600" s="19"/>
+      <c r="R600" s="19"/>
+      <c r="S600" s="20"/>
+      <c r="T600" s="20"/>
+      <c r="U600" s="18"/>
+    </row>
+    <row r="601">
+      <c r="A601" s="63"/>
+      <c r="B601" s="64"/>
+      <c r="C601" s="34"/>
+      <c r="D601" s="34"/>
+      <c r="E601" s="34"/>
+      <c r="F601" s="34"/>
+      <c r="G601" s="34"/>
+      <c r="H601" s="21"/>
+      <c r="I601" s="19"/>
+      <c r="J601" s="10"/>
+      <c r="K601" s="22"/>
+      <c r="L601" s="23"/>
+      <c r="M601" s="22"/>
+      <c r="N601" s="25"/>
+      <c r="O601" s="21"/>
+      <c r="P601" s="21"/>
+      <c r="Q601" s="19"/>
+      <c r="R601" s="19"/>
+      <c r="S601" s="20"/>
+      <c r="T601" s="20"/>
+      <c r="U601" s="18"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="J468">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>(J468&lt;I467)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C551">
+  <conditionalFormatting sqref="C1:C601">
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="男">
       <formula>NOT(ISERROR(SEARCH(("男"),(C1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C551">
+  <conditionalFormatting sqref="C1:C601">
     <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="女">
       <formula>NOT(ISERROR(SEARCH(("女"),(C1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G551">
+  <conditionalFormatting sqref="G2:G601">
     <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="境外">
       <formula>NOT(ISERROR(SEARCH(("境外"),(G2))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G551">
+  <conditionalFormatting sqref="G2:G601">
     <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="本土">
       <formula>NOT(ISERROR(SEARCH(("本土"),(G2))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E551">
+  <conditionalFormatting sqref="E2:E601">
     <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="臺灣">
       <formula>NOT(ISERROR(SEARCH(("臺灣"),(E2))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E551">
+  <conditionalFormatting sqref="E2:E601">
     <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="台灣">
       <formula>NOT(ISERROR(SEARCH(("台灣"),(E2))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E551">
+  <conditionalFormatting sqref="E2:E601">
     <cfRule type="notContainsBlanks" dxfId="6" priority="8">
       <formula>LEN(TRIM(E2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B551">
+  <conditionalFormatting sqref="B1:B601">
     <cfRule type="expression" dxfId="7" priority="9">
       <formula>B1&lt;43856.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B551">
+  <conditionalFormatting sqref="B1:B601">
     <cfRule type="expression" dxfId="8" priority="10">
       <formula>B1&lt;43863.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B551">
+  <conditionalFormatting sqref="B1:B601">
     <cfRule type="expression" dxfId="9" priority="11">
       <formula>B1&lt;43870.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B551">
+  <conditionalFormatting sqref="B1:B601">
     <cfRule type="expression" dxfId="10" priority="12">
       <formula>B1&lt;43877.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B551">
+  <conditionalFormatting sqref="B1:B601">
     <cfRule type="expression" dxfId="11" priority="13">
       <formula>B1&lt;43884.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B551">
+  <conditionalFormatting sqref="B1:B601">
     <cfRule type="expression" dxfId="12" priority="14">
       <formula>B1&lt;43891.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B551">
+  <conditionalFormatting sqref="B1:B601">
     <cfRule type="expression" dxfId="13" priority="15">
       <formula>B1&lt;43898.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B551">
+  <conditionalFormatting sqref="B1:B601">
     <cfRule type="expression" dxfId="14" priority="16">
       <formula>B1&lt;43905.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B551">
+  <conditionalFormatting sqref="B1:B601">
     <cfRule type="expression" dxfId="15" priority="17">
       <formula>B1&lt;43912.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B551">
+  <conditionalFormatting sqref="B1:B601">
     <cfRule type="expression" dxfId="16" priority="18">
       <formula>B1&lt;43919.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B551">
+  <conditionalFormatting sqref="B1:B601">
     <cfRule type="expression" dxfId="17" priority="19">
       <formula>B1&lt;43926.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F345 F347:F551">
+  <conditionalFormatting sqref="F1:F345 F347:F601">
     <cfRule type="containsText" dxfId="2" priority="20" operator="containsText" text="南">
       <formula>NOT(ISERROR(SEARCH(("南"),(F1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F345 F347:F551">
+  <conditionalFormatting sqref="F1:F345 F347:F601">
     <cfRule type="containsText" dxfId="18" priority="21" operator="containsText" text="中">
       <formula>NOT(ISERROR(SEARCH(("中"),(F1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F345 F347:F551">
+  <conditionalFormatting sqref="F1:F345 F347:F601">
     <cfRule type="containsText" dxfId="19" priority="22" operator="containsText" text="北">
       <formula>NOT(ISERROR(SEARCH(("北"),(F1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F345 F347:F551">
+  <conditionalFormatting sqref="F1:F345 F347:F601">
     <cfRule type="containsText" dxfId="20" priority="23" operator="containsText" text="東">
       <formula>NOT(ISERROR(SEARCH(("東"),(F1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P1:P389 P394:P551">
+  <conditionalFormatting sqref="P1:P389 P394:P601">
     <cfRule type="containsText" dxfId="21" priority="24" operator="containsText" text="R.I.P">
       <formula>NOT(ISERROR(SEARCH(("R.I.P"),(P1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M1:M551 P1:P389 P394:P551">
+  <conditionalFormatting sqref="M1:M601 P1:P389 P394:P601">
     <cfRule type="containsText" dxfId="22" priority="25" operator="containsText" text="首起">
       <formula>NOT(ISERROR(SEARCH(("首起"),(M1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M1:M551 P1:P389 P394:P551">
+  <conditionalFormatting sqref="M1:M601 P1:P389 P394:P601">
     <cfRule type="containsText" dxfId="22" priority="26" operator="containsText" text="首次">
       <formula>NOT(ISERROR(SEARCH(("首次"),(M1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M1:M551 P1:P389 P394:P551">
+  <conditionalFormatting sqref="M1:M601 P1:P389 P394:P601">
     <cfRule type="containsText" dxfId="22" priority="27" operator="containsText" text="首例">
       <formula>NOT(ISERROR(SEARCH(("首例"),(M1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L1:L551">
+  <conditionalFormatting sqref="L1:L601">
     <cfRule type="containsText" dxfId="23" priority="28" operator="containsText" text="自行">
       <formula>NOT(ISERROR(SEARCH(("自行"),(L1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O1:O551">
+  <conditionalFormatting sqref="O1:O601">
     <cfRule type="containsText" dxfId="24" priority="29" operator="containsText" text="未知">
       <formula>NOT(ISERROR(SEARCH(("未知"),(O1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L1:L551">
+  <conditionalFormatting sqref="L1:L601">
     <cfRule type="containsText" dxfId="25" priority="30" operator="containsText" text="自主">
       <formula>NOT(ISERROR(SEARCH(("自主"),(L1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P1:P389 P394:P551">
+  <conditionalFormatting sqref="P1:P389 P394:P601">
     <cfRule type="containsText" dxfId="26" priority="31" operator="containsText" text="重症">
       <formula>NOT(ISERROR(SEARCH(("重症"),(P1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J394 J397:J466 J469:J551">
+  <conditionalFormatting sqref="J2:J394 J397:J466 J469:J601">
     <cfRule type="expression" dxfId="0" priority="32">
       <formula>(J2&lt;I2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K344 K346:K551">
+  <conditionalFormatting sqref="K2:K344 K346:K601">
     <cfRule type="expression" dxfId="27" priority="33">
       <formula>AND( I2&lt;&gt;"", (LEFT(K2,4) - I2 ) &gt;= 7 )</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B551">
+  <conditionalFormatting sqref="B357:B601">
     <cfRule type="expression" dxfId="28" priority="34">
       <formula>B357&lt;43933.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L1:L551">
+  <conditionalFormatting sqref="L1:L601">
     <cfRule type="containsText" dxfId="29" priority="35" operator="containsText" text="回溯">
       <formula>NOT(ISERROR(SEARCH(("回溯"),(L1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B551">
+  <conditionalFormatting sqref="B357:B601">
     <cfRule type="expression" dxfId="30" priority="36">
       <formula>B357&lt;43940.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B551">
+  <conditionalFormatting sqref="B357:B601">
     <cfRule type="expression" dxfId="31" priority="37">
       <formula>B357&lt;43947.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B551">
+  <conditionalFormatting sqref="B357:B601">
     <cfRule type="expression" dxfId="32" priority="38">
       <formula>B357&lt;43954.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B551">
+  <conditionalFormatting sqref="B357:B601">
     <cfRule type="expression" dxfId="33" priority="39">
       <formula>B357&lt;43961.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B551">
+  <conditionalFormatting sqref="B357:B601">
     <cfRule type="expression" dxfId="34" priority="40">
       <formula>B357&lt;43968.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B551">
+  <conditionalFormatting sqref="B357:B601">
     <cfRule type="expression" dxfId="35" priority="41">
       <formula>B357&lt;43975.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B551">
+  <conditionalFormatting sqref="B357:B601">
     <cfRule type="expression" dxfId="36" priority="42">
       <formula>B357&lt;43982.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G551">
+  <conditionalFormatting sqref="G2:G601">
     <cfRule type="containsText" dxfId="37" priority="43" operator="containsText" text="敦睦">
       <formula>NOT(ISERROR(SEARCH(("敦睦"),(G2))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L1:L551">
+  <conditionalFormatting sqref="L1:L601">
     <cfRule type="containsText" dxfId="13" priority="44" operator="containsText" text="集中">
       <formula>NOT(ISERROR(SEARCH(("集中"),(L1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O1:O551">
+  <conditionalFormatting sqref="O1:O601">
     <cfRule type="containsText" dxfId="38" priority="45" operator="containsText" text="軍艦">
       <formula>NOT(ISERROR(SEARCH(("軍艦"),(O1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B551">
+  <conditionalFormatting sqref="B357:B601">
     <cfRule type="expression" dxfId="39" priority="46">
       <formula>B357&lt;43989.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B551">
+  <conditionalFormatting sqref="B357:B601">
     <cfRule type="expression" dxfId="40" priority="47">
       <formula>B357&lt;43996.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B551">
+  <conditionalFormatting sqref="B357:B601">
     <cfRule type="expression" dxfId="41" priority="48">
       <formula>B357&lt;44003.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B551">
+  <conditionalFormatting sqref="B357:B601">
     <cfRule type="expression" dxfId="42" priority="49">
       <formula>B357&lt;44010.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B551">
+  <conditionalFormatting sqref="B357:B601">
     <cfRule type="expression" dxfId="43" priority="50">
       <formula>B357&lt;44017.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B551">
+  <conditionalFormatting sqref="B357:B601">
     <cfRule type="expression" dxfId="44" priority="51">
       <formula>B357&lt;44024.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B551">
+  <conditionalFormatting sqref="B357:B601">
     <cfRule type="expression" dxfId="45" priority="52">
       <formula>B357&lt;44031.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B551">
+  <conditionalFormatting sqref="B357:B601">
     <cfRule type="expression" dxfId="46" priority="53">
       <formula>B357&lt;44038.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B551">
+  <conditionalFormatting sqref="B357:B601">
     <cfRule type="expression" dxfId="47" priority="54">
       <formula>B357&lt;44045.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B551">
+  <conditionalFormatting sqref="B357:B601">
     <cfRule type="expression" dxfId="48" priority="55">
       <formula>B357&lt;44052.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B551">
+  <conditionalFormatting sqref="B357:B601">
     <cfRule type="expression" dxfId="49" priority="56">
       <formula>B357&lt;44059.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B551">
+  <conditionalFormatting sqref="B357:B601">
     <cfRule type="expression" dxfId="50" priority="57">
       <formula>B357&lt;44066.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B551">
+  <conditionalFormatting sqref="B357:B601">
     <cfRule type="expression" dxfId="51" priority="58">
       <formula>B357&lt;44073.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B551">
+  <conditionalFormatting sqref="B357:B601">
     <cfRule type="expression" dxfId="52" priority="59">
       <formula>B357&lt;44080.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B551">
+  <conditionalFormatting sqref="B357:B601">
     <cfRule type="expression" dxfId="53" priority="60">
       <formula>B357&lt;44087.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B551">
+  <conditionalFormatting sqref="B357:B601">
     <cfRule type="expression" dxfId="54" priority="61">
       <formula>B357&lt;44094.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B551">
+  <conditionalFormatting sqref="B357:B601">
     <cfRule type="expression" dxfId="55" priority="62">
       <formula>B357&lt;44101.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B551">
+  <conditionalFormatting sqref="B357:B601">
     <cfRule type="expression" dxfId="56" priority="63">
       <formula>B357&lt;44108.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L1:L551">
+  <conditionalFormatting sqref="L1:L601">
     <cfRule type="containsText" dxfId="57" priority="64" operator="containsText" text="自費">
       <formula>NOT(ISERROR(SEARCH(("自費"),(L1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B551">
+  <conditionalFormatting sqref="B357:B601">
     <cfRule type="expression" dxfId="58" priority="65">
       <formula>B357&lt;44115.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B551">
+  <conditionalFormatting sqref="B357:B601">
     <cfRule type="expression" dxfId="59" priority="66">
       <formula>B357&lt;44122.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B551">
+  <conditionalFormatting sqref="B357:B601">
     <cfRule type="expression" dxfId="60" priority="67">
       <formula>B357&lt;44129.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B551">
+  <conditionalFormatting sqref="B357:B601">
     <cfRule type="expression" dxfId="61" priority="68">
       <formula>B357&lt;44136.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B551">
+  <conditionalFormatting sqref="B357:B601">
     <cfRule type="expression" dxfId="62" priority="69">
       <formula>B357&lt;44143.0</formula>
     </cfRule>
@@ -40524,15 +41802,18 @@
     <hyperlink r:id="rId101" ref="S539"/>
     <hyperlink r:id="rId102" ref="S540"/>
     <hyperlink r:id="rId103" ref="S541"/>
+    <hyperlink r:id="rId104" ref="S542"/>
+    <hyperlink r:id="rId105" ref="S543"/>
+    <hyperlink r:id="rId106" ref="S544"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId104"/>
-  <legacyDrawing r:id="rId105"/>
+  <drawing r:id="rId107"/>
+  <legacyDrawing r:id="rId108"/>
   <tableParts count="2">
-    <tablePart r:id="rId108"/>
-    <tablePart r:id="rId109"/>
+    <tablePart r:id="rId111"/>
+    <tablePart r:id="rId112"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201022
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -563,7 +563,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6016" uniqueCount="2016">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6028" uniqueCount="2021">
   <si>
     <t>案例</t>
   </si>
@@ -7415,12 +7415,30 @@
 10/20 確診</t>
   </si>
   <si>
-    <t>輕微發燒 肌肉痠痛 咳嗽 呼吸困難</t>
+    <t>輕微發燒 肌肉痠痛 咳嗽 呼吸困難 肺炎</t>
   </si>
   <si>
     <t>長期於菲律賓工作(前次自台灣出境時間為今年1月)
 10月5日出現輕微發燒、肌肉痠痛、咳嗽、呼吸困難情形
 10月15日於菲律賓當地就醫診斷為肺炎，但未住院治療，僅服藥與採檢(10月19日得知檢驗結果為陽性)</t>
+  </si>
+  <si>
+    <t>#544</t>
+  </si>
+  <si>
+    <t>-10/5 印尼→台灣</t>
+  </si>
+  <si>
+    <t>10/20 採檢
+10/21 確診</t>
+  </si>
+  <si>
+    <t>個案入境時無疑似症狀且檢附3日內檢驗抗體陰性報告，入境後即搭乘防疫計程車入住防疫旅館
+個案於居家檢疫期間均回覆無疑似症狀，惟後續經疫調了解，個案曾於10月8日至10月9日出現咳嗽、喉嚨痛症狀，10月10日後症狀緩解。
+個案於10月20日居家檢疫期滿，由校方安排專車至醫院自費採檢</t>
+  </si>
+  <si>
+    <t>國內新增1例境外移入COVID-19病例，為印尼籍學生來台就學</t>
   </si>
 </sst>
 </file>
@@ -40022,29 +40040,59 @@
       </c>
     </row>
     <row r="545">
-      <c r="A545" s="63"/>
-      <c r="B545" s="64"/>
-      <c r="C545" s="34"/>
-      <c r="D545" s="34"/>
-      <c r="E545" s="34"/>
+      <c r="A545" s="16" t="s">
+        <v>2016</v>
+      </c>
+      <c r="B545" s="6">
+        <v>44125.0</v>
+      </c>
+      <c r="C545" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D545" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="E545" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F545" s="34"/>
-      <c r="G545" s="34"/>
-      <c r="H545" s="21"/>
-      <c r="I545" s="19"/>
-      <c r="J545" s="10"/>
-      <c r="K545" s="22"/>
-      <c r="L545" s="23"/>
-      <c r="M545" s="22"/>
+      <c r="G545" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H545" s="8" t="s">
+        <v>2017</v>
+      </c>
+      <c r="I545" s="9">
+        <v>44109.0</v>
+      </c>
+      <c r="J545" s="10">
+        <v>44112.0</v>
+      </c>
+      <c r="K545" s="13" t="s">
+        <v>2018</v>
+      </c>
+      <c r="L545" s="12" t="s">
+        <v>1674</v>
+      </c>
+      <c r="M545" s="13" t="s">
+        <v>618</v>
+      </c>
       <c r="N545" s="25"/>
-      <c r="O545" s="21"/>
-      <c r="P545" s="21"/>
+      <c r="O545" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P545" s="8" t="s">
+        <v>2019</v>
+      </c>
       <c r="Q545" s="19"/>
       <c r="R545" s="19"/>
-      <c r="S545" s="20"/>
+      <c r="S545" s="61" t="s">
+        <v>2020</v>
+      </c>
       <c r="T545" s="20"/>
       <c r="U545" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#544</v>
       </c>
     </row>
     <row r="546">
@@ -41805,15 +41853,16 @@
     <hyperlink r:id="rId104" ref="S542"/>
     <hyperlink r:id="rId105" ref="S543"/>
     <hyperlink r:id="rId106" ref="S544"/>
+    <hyperlink r:id="rId107" ref="S545"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId107"/>
-  <legacyDrawing r:id="rId108"/>
+  <drawing r:id="rId108"/>
+  <legacyDrawing r:id="rId109"/>
   <tableParts count="2">
-    <tablePart r:id="rId111"/>
     <tablePart r:id="rId112"/>
+    <tablePart r:id="rId113"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201023
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -563,7 +563,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6028" uniqueCount="2021">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6077" uniqueCount="2040">
   <si>
     <t>案例</t>
   </si>
@@ -7439,6 +7439,67 @@
   </si>
   <si>
     <t>國內新增1例境外移入COVID-19病例，為印尼籍學生來台就學</t>
+  </si>
+  <si>
+    <t>#545</t>
+  </si>
+  <si>
+    <t>-10/14 印尼→台灣</t>
+  </si>
+  <si>
+    <t>10/20 採檢
+10/22 確診</t>
+  </si>
+  <si>
+    <t>頭暈 食慾不振 嘔吐 全身倦怠</t>
+  </si>
+  <si>
+    <t>因工作於10月14日入境臺灣，搭機前3日內檢驗陰性，入境時無症狀</t>
+  </si>
+  <si>
+    <t>國內新增4例境外移入COVID-19病例，分自印尼、菲律賓及土耳其入境</t>
+  </si>
+  <si>
+    <t>#546</t>
+  </si>
+  <si>
+    <t>2019/12-2020/10/20 菲律賓</t>
+  </si>
+  <si>
+    <t>10/20 採檢
+10/22 確診</t>
+  </si>
+  <si>
+    <t>上半身骨頭刺痛 輕微咳嗽 嗅覺異常</t>
+  </si>
+  <si>
+    <t>入境時主動告知嗅覺喪失，於機場進行採檢</t>
+  </si>
+  <si>
+    <t>#547</t>
+  </si>
+  <si>
+    <t>-10/8 印尼→台灣</t>
+  </si>
+  <si>
+    <t>10/21 採檢
+10/22 確診</t>
+  </si>
+  <si>
+    <t>檢疫期滿前採檢，因檢出陽性於今日確診</t>
+  </si>
+  <si>
+    <t>#548</t>
+  </si>
+  <si>
+    <t>-10/13 土耳其→台灣</t>
+  </si>
+  <si>
+    <t>流鼻水 倦怠 嗅味覺異常</t>
+  </si>
+  <si>
+    <t>過去2年於土耳其工作，因預定來臺工作，於10月13日入境臺灣，搭機前3日內檢驗陰性，入境時無症狀
+個案於防疫旅館居家檢疫期間，10月17日至20日因陸續出現流鼻水、倦怠及嗅味覺異常情形通報衛生單位，經安排就醫採檢</t>
   </si>
 </sst>
 </file>
@@ -40096,107 +40157,227 @@
       </c>
     </row>
     <row r="546">
-      <c r="A546" s="63"/>
-      <c r="B546" s="64"/>
-      <c r="C546" s="34"/>
-      <c r="D546" s="34"/>
-      <c r="E546" s="34"/>
+      <c r="A546" s="16" t="s">
+        <v>2021</v>
+      </c>
+      <c r="B546" s="6">
+        <v>44126.0</v>
+      </c>
+      <c r="C546" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D546" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E546" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F546" s="34"/>
-      <c r="G546" s="34"/>
-      <c r="H546" s="21"/>
-      <c r="I546" s="19"/>
-      <c r="J546" s="10"/>
-      <c r="K546" s="22"/>
-      <c r="L546" s="23"/>
-      <c r="M546" s="22"/>
+      <c r="G546" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H546" s="8" t="s">
+        <v>2022</v>
+      </c>
+      <c r="I546" s="9">
+        <v>44118.0</v>
+      </c>
+      <c r="J546" s="10">
+        <v>44121.0</v>
+      </c>
+      <c r="K546" s="13" t="s">
+        <v>2023</v>
+      </c>
+      <c r="L546" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M546" s="13" t="s">
+        <v>2024</v>
+      </c>
       <c r="N546" s="25"/>
-      <c r="O546" s="21"/>
-      <c r="P546" s="21"/>
+      <c r="O546" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P546" s="8" t="s">
+        <v>2025</v>
+      </c>
       <c r="Q546" s="19"/>
       <c r="R546" s="19"/>
-      <c r="S546" s="20"/>
+      <c r="S546" s="61" t="s">
+        <v>2026</v>
+      </c>
       <c r="T546" s="20"/>
       <c r="U546" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#545</v>
       </c>
     </row>
     <row r="547">
-      <c r="A547" s="63"/>
-      <c r="B547" s="64"/>
-      <c r="C547" s="34"/>
-      <c r="D547" s="34"/>
-      <c r="E547" s="34"/>
+      <c r="A547" s="16" t="s">
+        <v>2027</v>
+      </c>
+      <c r="B547" s="6">
+        <v>44126.0</v>
+      </c>
+      <c r="C547" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D547" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E547" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F547" s="34"/>
-      <c r="G547" s="34"/>
-      <c r="H547" s="21"/>
-      <c r="I547" s="19"/>
-      <c r="J547" s="10"/>
-      <c r="K547" s="22"/>
-      <c r="L547" s="23"/>
-      <c r="M547" s="22"/>
+      <c r="G547" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H547" s="8" t="s">
+        <v>2028</v>
+      </c>
+      <c r="I547" s="9">
+        <v>44124.0</v>
+      </c>
+      <c r="J547" s="10">
+        <v>44117.0</v>
+      </c>
+      <c r="K547" s="13" t="s">
+        <v>2029</v>
+      </c>
+      <c r="L547" s="12" t="s">
+        <v>363</v>
+      </c>
+      <c r="M547" s="13" t="s">
+        <v>2030</v>
+      </c>
       <c r="N547" s="25"/>
-      <c r="O547" s="21"/>
-      <c r="P547" s="21"/>
+      <c r="O547" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P547" s="8" t="s">
+        <v>2031</v>
+      </c>
       <c r="Q547" s="19"/>
       <c r="R547" s="19"/>
-      <c r="S547" s="20"/>
+      <c r="S547" s="61" t="s">
+        <v>2026</v>
+      </c>
       <c r="T547" s="20"/>
       <c r="U547" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#546</v>
       </c>
     </row>
     <row r="548">
-      <c r="A548" s="63"/>
-      <c r="B548" s="64"/>
-      <c r="C548" s="34"/>
-      <c r="D548" s="34"/>
-      <c r="E548" s="34"/>
+      <c r="A548" s="16" t="s">
+        <v>2032</v>
+      </c>
+      <c r="B548" s="6">
+        <v>44126.0</v>
+      </c>
+      <c r="C548" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D548" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E548" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F548" s="34"/>
-      <c r="G548" s="34"/>
-      <c r="H548" s="21"/>
-      <c r="I548" s="19"/>
-      <c r="J548" s="10"/>
-      <c r="K548" s="22"/>
-      <c r="L548" s="23"/>
-      <c r="M548" s="22"/>
+      <c r="G548" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H548" s="8" t="s">
+        <v>2033</v>
+      </c>
+      <c r="I548" s="9">
+        <v>44112.0</v>
+      </c>
+      <c r="J548" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K548" s="13" t="s">
+        <v>2034</v>
+      </c>
+      <c r="L548" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M548" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N548" s="25"/>
-      <c r="O548" s="21"/>
-      <c r="P548" s="21"/>
+      <c r="O548" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P548" s="8" t="s">
+        <v>2035</v>
+      </c>
       <c r="Q548" s="19"/>
       <c r="R548" s="19"/>
-      <c r="S548" s="20"/>
+      <c r="S548" s="61" t="s">
+        <v>2026</v>
+      </c>
       <c r="T548" s="20"/>
       <c r="U548" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#547</v>
       </c>
     </row>
     <row r="549">
-      <c r="A549" s="63"/>
-      <c r="B549" s="64"/>
-      <c r="C549" s="34"/>
-      <c r="D549" s="34"/>
-      <c r="E549" s="34"/>
+      <c r="A549" s="16" t="s">
+        <v>2036</v>
+      </c>
+      <c r="B549" s="6">
+        <v>44126.0</v>
+      </c>
+      <c r="C549" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D549" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E549" s="7" t="s">
+        <v>205</v>
+      </c>
       <c r="F549" s="34"/>
-      <c r="G549" s="34"/>
-      <c r="H549" s="21"/>
-      <c r="I549" s="19"/>
-      <c r="J549" s="10"/>
-      <c r="K549" s="22"/>
-      <c r="L549" s="23"/>
-      <c r="M549" s="22"/>
+      <c r="G549" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H549" s="8" t="s">
+        <v>2037</v>
+      </c>
+      <c r="I549" s="9">
+        <v>44117.0</v>
+      </c>
+      <c r="J549" s="10">
+        <v>44121.0</v>
+      </c>
+      <c r="K549" s="13" t="s">
+        <v>2029</v>
+      </c>
+      <c r="L549" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M549" s="13" t="s">
+        <v>2038</v>
+      </c>
       <c r="N549" s="25"/>
-      <c r="O549" s="21"/>
-      <c r="P549" s="21"/>
+      <c r="O549" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P549" s="8" t="s">
+        <v>2039</v>
+      </c>
       <c r="Q549" s="19"/>
       <c r="R549" s="19"/>
-      <c r="S549" s="20"/>
+      <c r="S549" s="61" t="s">
+        <v>2026</v>
+      </c>
       <c r="T549" s="20"/>
       <c r="U549" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#548</v>
       </c>
     </row>
     <row r="550">
@@ -41854,15 +42035,19 @@
     <hyperlink r:id="rId105" ref="S543"/>
     <hyperlink r:id="rId106" ref="S544"/>
     <hyperlink r:id="rId107" ref="S545"/>
+    <hyperlink r:id="rId108" ref="S546"/>
+    <hyperlink r:id="rId109" ref="S547"/>
+    <hyperlink r:id="rId110" ref="S548"/>
+    <hyperlink r:id="rId111" ref="S549"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId108"/>
-  <legacyDrawing r:id="rId109"/>
+  <drawing r:id="rId112"/>
+  <legacyDrawing r:id="rId113"/>
   <tableParts count="2">
-    <tablePart r:id="rId112"/>
-    <tablePart r:id="rId113"/>
+    <tablePart r:id="rId116"/>
+    <tablePart r:id="rId117"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201025
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -563,7 +563,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6077" uniqueCount="2040">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6101" uniqueCount="2049">
   <si>
     <t>案例</t>
   </si>
@@ -7500,6 +7500,38 @@
   <si>
     <t>過去2年於土耳其工作，因預定來臺工作，於10月13日入境臺灣，搭機前3日內檢驗陰性，入境時無症狀
 個案於防疫旅館居家檢疫期間，10月17日至20日因陸續出現流鼻水、倦怠及嗅味覺異常情形通報衛生單位，經安排就醫採檢</t>
+  </si>
+  <si>
+    <t>#549</t>
+  </si>
+  <si>
+    <t>-9/30 菲律賓→台灣</t>
+  </si>
+  <si>
+    <t>10/13 採檢
+10/22 二採
+10/24 確診</t>
+  </si>
+  <si>
+    <t>搭機前3日內檢驗陰性，入境時至集中檢疫期滿均無症狀
+10月13日檢疫期滿前採檢結果為陰性，檢疫期滿後由仲介安排至隔離宿舍進行自主健康管理
+並於10月22由仲介安排至醫院自費檢驗</t>
+  </si>
+  <si>
+    <t>國內新增2例境外移入COVID-19病例，分別自菲律賓及美國入境</t>
+  </si>
+  <si>
+    <t>#550</t>
+  </si>
+  <si>
+    <t>10/2-10/18 美國</t>
+  </si>
+  <si>
+    <t>10/21 採檢
+10/24 確診</t>
+  </si>
+  <si>
+    <t>發燒 咳嗽 肌肉痠痛 關節痛 全身倦怠</t>
   </si>
 </sst>
 </file>
@@ -40381,55 +40413,113 @@
       </c>
     </row>
     <row r="550">
-      <c r="A550" s="63"/>
-      <c r="B550" s="64"/>
-      <c r="C550" s="34"/>
-      <c r="D550" s="34"/>
-      <c r="E550" s="34"/>
+      <c r="A550" s="16" t="s">
+        <v>2040</v>
+      </c>
+      <c r="B550" s="6">
+        <v>44128.0</v>
+      </c>
+      <c r="C550" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D550" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E550" s="7" t="s">
+        <v>205</v>
+      </c>
       <c r="F550" s="34"/>
-      <c r="G550" s="34"/>
-      <c r="H550" s="21"/>
-      <c r="I550" s="19"/>
-      <c r="J550" s="10"/>
-      <c r="K550" s="22"/>
-      <c r="L550" s="23"/>
-      <c r="M550" s="22"/>
+      <c r="G550" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H550" s="8" t="s">
+        <v>2041</v>
+      </c>
+      <c r="I550" s="9">
+        <v>44104.0</v>
+      </c>
+      <c r="J550" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K550" s="13" t="s">
+        <v>2042</v>
+      </c>
+      <c r="L550" s="12" t="s">
+        <v>1674</v>
+      </c>
+      <c r="M550" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N550" s="25"/>
-      <c r="O550" s="21"/>
-      <c r="P550" s="21"/>
+      <c r="O550" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P550" s="8" t="s">
+        <v>2043</v>
+      </c>
       <c r="Q550" s="19"/>
       <c r="R550" s="19"/>
-      <c r="S550" s="20"/>
+      <c r="S550" s="61" t="s">
+        <v>2044</v>
+      </c>
       <c r="T550" s="20"/>
       <c r="U550" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#549</v>
       </c>
     </row>
     <row r="551">
-      <c r="A551" s="63"/>
-      <c r="B551" s="64"/>
-      <c r="C551" s="34"/>
-      <c r="D551" s="34"/>
-      <c r="E551" s="34"/>
+      <c r="A551" s="16" t="s">
+        <v>2045</v>
+      </c>
+      <c r="B551" s="6">
+        <v>44128.0</v>
+      </c>
+      <c r="C551" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D551" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E551" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F551" s="34"/>
-      <c r="G551" s="34"/>
-      <c r="H551" s="21"/>
-      <c r="I551" s="19"/>
-      <c r="J551" s="10"/>
-      <c r="K551" s="22"/>
-      <c r="L551" s="23"/>
-      <c r="M551" s="22"/>
+      <c r="G551" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H551" s="8" t="s">
+        <v>2046</v>
+      </c>
+      <c r="I551" s="9">
+        <v>44122.0</v>
+      </c>
+      <c r="J551" s="10">
+        <v>44125.0</v>
+      </c>
+      <c r="K551" s="13" t="s">
+        <v>2047</v>
+      </c>
+      <c r="L551" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M551" s="13" t="s">
+        <v>2048</v>
+      </c>
       <c r="N551" s="25"/>
-      <c r="O551" s="21"/>
+      <c r="O551" s="8" t="s">
+        <v>85</v>
+      </c>
       <c r="P551" s="21"/>
       <c r="Q551" s="19"/>
       <c r="R551" s="19"/>
-      <c r="S551" s="20"/>
+      <c r="S551" s="61" t="s">
+        <v>2044</v>
+      </c>
       <c r="T551" s="20"/>
       <c r="U551" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#550</v>
       </c>
     </row>
     <row r="552">
@@ -42039,15 +42129,17 @@
     <hyperlink r:id="rId109" ref="S547"/>
     <hyperlink r:id="rId110" ref="S548"/>
     <hyperlink r:id="rId111" ref="S549"/>
+    <hyperlink r:id="rId112" ref="S550"/>
+    <hyperlink r:id="rId113" ref="S551"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId112"/>
-  <legacyDrawing r:id="rId113"/>
+  <drawing r:id="rId114"/>
+  <legacyDrawing r:id="rId115"/>
   <tableParts count="2">
-    <tablePart r:id="rId116"/>
-    <tablePart r:id="rId117"/>
+    <tablePart r:id="rId118"/>
+    <tablePart r:id="rId119"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201029
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -563,7 +563,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6101" uniqueCount="2049">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6114" uniqueCount="2054">
   <si>
     <t>案例</t>
   </si>
@@ -7532,6 +7532,23 @@
   </si>
   <si>
     <t>發燒 咳嗽 肌肉痠痛 關節痛 全身倦怠</t>
+  </si>
+  <si>
+    <t>#551</t>
+  </si>
+  <si>
+    <t>-10/7 印尼→台灣</t>
+  </si>
+  <si>
+    <t>10/26 採檢
+10/28 確診</t>
+  </si>
+  <si>
+    <t>個案入境時無症狀且檢附三日內檢驗陰性報告，入境後由仲介安排入住防疫宿舍進行居家檢疫，檢疫期間均回報無症狀。
+個案10月22日檢疫期滿後，由仲介安排於原防疫宿舍持續進行自主健康管理，並於10月26日由仲介安排至醫院自費採檢</t>
+  </si>
+  <si>
+    <t>國內新增1例境外移入COVID-19病例，為無症狀印尼籍移工</t>
   </si>
 </sst>
 </file>
@@ -9028,7 +9045,7 @@
         <v>國內首例確診患者已痊癒將出院 向防疫及醫護人員表達感謝</v>
       </c>
       <c r="U2" s="18" t="str">
-        <f t="shared" ref="U2:U551" si="1">A2</f>
+        <f t="shared" ref="U2:U601" si="1">A2</f>
         <v>#001</v>
       </c>
     </row>
@@ -40523,27 +40540,60 @@
       </c>
     </row>
     <row r="552">
-      <c r="A552" s="63"/>
-      <c r="B552" s="64"/>
-      <c r="C552" s="34"/>
-      <c r="D552" s="34"/>
-      <c r="E552" s="34"/>
+      <c r="A552" s="16" t="s">
+        <v>2049</v>
+      </c>
+      <c r="B552" s="6">
+        <v>44132.0</v>
+      </c>
+      <c r="C552" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D552" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="E552" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F552" s="34"/>
-      <c r="G552" s="34"/>
-      <c r="H552" s="21"/>
-      <c r="I552" s="19"/>
-      <c r="J552" s="10"/>
-      <c r="K552" s="22"/>
-      <c r="L552" s="23"/>
-      <c r="M552" s="22"/>
+      <c r="G552" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H552" s="8" t="s">
+        <v>2050</v>
+      </c>
+      <c r="I552" s="9">
+        <v>44111.0</v>
+      </c>
+      <c r="J552" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K552" s="13" t="s">
+        <v>2051</v>
+      </c>
+      <c r="L552" s="12" t="s">
+        <v>1674</v>
+      </c>
+      <c r="M552" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N552" s="25"/>
-      <c r="O552" s="21"/>
-      <c r="P552" s="21"/>
+      <c r="O552" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P552" s="8" t="s">
+        <v>2052</v>
+      </c>
       <c r="Q552" s="19"/>
       <c r="R552" s="19"/>
-      <c r="S552" s="20"/>
+      <c r="S552" s="61" t="s">
+        <v>2053</v>
+      </c>
       <c r="T552" s="20"/>
-      <c r="U552" s="18"/>
+      <c r="U552" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v>#551</v>
+      </c>
     </row>
     <row r="553">
       <c r="A553" s="63"/>
@@ -40566,7 +40616,10 @@
       <c r="R553" s="19"/>
       <c r="S553" s="20"/>
       <c r="T553" s="20"/>
-      <c r="U553" s="18"/>
+      <c r="U553" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="554">
       <c r="A554" s="63"/>
@@ -40589,7 +40642,10 @@
       <c r="R554" s="19"/>
       <c r="S554" s="20"/>
       <c r="T554" s="20"/>
-      <c r="U554" s="18"/>
+      <c r="U554" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="555">
       <c r="A555" s="63"/>
@@ -40612,7 +40668,10 @@
       <c r="R555" s="19"/>
       <c r="S555" s="20"/>
       <c r="T555" s="20"/>
-      <c r="U555" s="18"/>
+      <c r="U555" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="556">
       <c r="A556" s="63"/>
@@ -40635,7 +40694,10 @@
       <c r="R556" s="19"/>
       <c r="S556" s="20"/>
       <c r="T556" s="20"/>
-      <c r="U556" s="18"/>
+      <c r="U556" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="557">
       <c r="A557" s="63"/>
@@ -40658,7 +40720,10 @@
       <c r="R557" s="19"/>
       <c r="S557" s="20"/>
       <c r="T557" s="20"/>
-      <c r="U557" s="18"/>
+      <c r="U557" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="558">
       <c r="A558" s="63"/>
@@ -40681,7 +40746,10 @@
       <c r="R558" s="19"/>
       <c r="S558" s="20"/>
       <c r="T558" s="20"/>
-      <c r="U558" s="18"/>
+      <c r="U558" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="559">
       <c r="A559" s="63"/>
@@ -40704,7 +40772,10 @@
       <c r="R559" s="19"/>
       <c r="S559" s="20"/>
       <c r="T559" s="20"/>
-      <c r="U559" s="18"/>
+      <c r="U559" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="560">
       <c r="A560" s="63"/>
@@ -40727,7 +40798,10 @@
       <c r="R560" s="19"/>
       <c r="S560" s="20"/>
       <c r="T560" s="20"/>
-      <c r="U560" s="18"/>
+      <c r="U560" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="561">
       <c r="A561" s="63"/>
@@ -40750,7 +40824,10 @@
       <c r="R561" s="19"/>
       <c r="S561" s="20"/>
       <c r="T561" s="20"/>
-      <c r="U561" s="18"/>
+      <c r="U561" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="562">
       <c r="A562" s="63"/>
@@ -40773,7 +40850,10 @@
       <c r="R562" s="19"/>
       <c r="S562" s="20"/>
       <c r="T562" s="20"/>
-      <c r="U562" s="18"/>
+      <c r="U562" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="563">
       <c r="A563" s="63"/>
@@ -40796,7 +40876,10 @@
       <c r="R563" s="19"/>
       <c r="S563" s="20"/>
       <c r="T563" s="20"/>
-      <c r="U563" s="18"/>
+      <c r="U563" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="564">
       <c r="A564" s="63"/>
@@ -40819,7 +40902,10 @@
       <c r="R564" s="19"/>
       <c r="S564" s="20"/>
       <c r="T564" s="20"/>
-      <c r="U564" s="18"/>
+      <c r="U564" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="565">
       <c r="A565" s="63"/>
@@ -40842,7 +40928,10 @@
       <c r="R565" s="19"/>
       <c r="S565" s="20"/>
       <c r="T565" s="20"/>
-      <c r="U565" s="18"/>
+      <c r="U565" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="566">
       <c r="A566" s="63"/>
@@ -40865,7 +40954,10 @@
       <c r="R566" s="19"/>
       <c r="S566" s="20"/>
       <c r="T566" s="20"/>
-      <c r="U566" s="18"/>
+      <c r="U566" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="567">
       <c r="A567" s="63"/>
@@ -40888,7 +40980,10 @@
       <c r="R567" s="19"/>
       <c r="S567" s="20"/>
       <c r="T567" s="20"/>
-      <c r="U567" s="18"/>
+      <c r="U567" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="568">
       <c r="A568" s="63"/>
@@ -40911,7 +41006,10 @@
       <c r="R568" s="19"/>
       <c r="S568" s="20"/>
       <c r="T568" s="20"/>
-      <c r="U568" s="18"/>
+      <c r="U568" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="569">
       <c r="A569" s="63"/>
@@ -40934,7 +41032,10 @@
       <c r="R569" s="19"/>
       <c r="S569" s="20"/>
       <c r="T569" s="20"/>
-      <c r="U569" s="18"/>
+      <c r="U569" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="570">
       <c r="A570" s="63"/>
@@ -40957,7 +41058,10 @@
       <c r="R570" s="19"/>
       <c r="S570" s="20"/>
       <c r="T570" s="20"/>
-      <c r="U570" s="18"/>
+      <c r="U570" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="571">
       <c r="A571" s="63"/>
@@ -40980,7 +41084,10 @@
       <c r="R571" s="19"/>
       <c r="S571" s="20"/>
       <c r="T571" s="20"/>
-      <c r="U571" s="18"/>
+      <c r="U571" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="572">
       <c r="A572" s="63"/>
@@ -41003,7 +41110,10 @@
       <c r="R572" s="19"/>
       <c r="S572" s="20"/>
       <c r="T572" s="20"/>
-      <c r="U572" s="18"/>
+      <c r="U572" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="573">
       <c r="A573" s="63"/>
@@ -41026,7 +41136,10 @@
       <c r="R573" s="19"/>
       <c r="S573" s="20"/>
       <c r="T573" s="20"/>
-      <c r="U573" s="18"/>
+      <c r="U573" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="574">
       <c r="A574" s="63"/>
@@ -41049,7 +41162,10 @@
       <c r="R574" s="19"/>
       <c r="S574" s="20"/>
       <c r="T574" s="20"/>
-      <c r="U574" s="18"/>
+      <c r="U574" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="575">
       <c r="A575" s="63"/>
@@ -41072,7 +41188,10 @@
       <c r="R575" s="19"/>
       <c r="S575" s="20"/>
       <c r="T575" s="20"/>
-      <c r="U575" s="18"/>
+      <c r="U575" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="576">
       <c r="A576" s="63"/>
@@ -41095,7 +41214,10 @@
       <c r="R576" s="19"/>
       <c r="S576" s="20"/>
       <c r="T576" s="20"/>
-      <c r="U576" s="18"/>
+      <c r="U576" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="577">
       <c r="A577" s="63"/>
@@ -41118,7 +41240,10 @@
       <c r="R577" s="19"/>
       <c r="S577" s="20"/>
       <c r="T577" s="20"/>
-      <c r="U577" s="18"/>
+      <c r="U577" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="578">
       <c r="A578" s="63"/>
@@ -41141,7 +41266,10 @@
       <c r="R578" s="19"/>
       <c r="S578" s="20"/>
       <c r="T578" s="20"/>
-      <c r="U578" s="18"/>
+      <c r="U578" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="579">
       <c r="A579" s="63"/>
@@ -41164,7 +41292,10 @@
       <c r="R579" s="19"/>
       <c r="S579" s="20"/>
       <c r="T579" s="20"/>
-      <c r="U579" s="18"/>
+      <c r="U579" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="580">
       <c r="A580" s="63"/>
@@ -41187,7 +41318,10 @@
       <c r="R580" s="19"/>
       <c r="S580" s="20"/>
       <c r="T580" s="20"/>
-      <c r="U580" s="18"/>
+      <c r="U580" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="581">
       <c r="A581" s="63"/>
@@ -41210,7 +41344,10 @@
       <c r="R581" s="19"/>
       <c r="S581" s="20"/>
       <c r="T581" s="20"/>
-      <c r="U581" s="18"/>
+      <c r="U581" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="582">
       <c r="A582" s="63"/>
@@ -41233,7 +41370,10 @@
       <c r="R582" s="19"/>
       <c r="S582" s="20"/>
       <c r="T582" s="20"/>
-      <c r="U582" s="18"/>
+      <c r="U582" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="583">
       <c r="A583" s="63"/>
@@ -41256,7 +41396,10 @@
       <c r="R583" s="19"/>
       <c r="S583" s="20"/>
       <c r="T583" s="20"/>
-      <c r="U583" s="18"/>
+      <c r="U583" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="584">
       <c r="A584" s="63"/>
@@ -41279,7 +41422,10 @@
       <c r="R584" s="19"/>
       <c r="S584" s="20"/>
       <c r="T584" s="20"/>
-      <c r="U584" s="18"/>
+      <c r="U584" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="585">
       <c r="A585" s="63"/>
@@ -41302,7 +41448,10 @@
       <c r="R585" s="19"/>
       <c r="S585" s="20"/>
       <c r="T585" s="20"/>
-      <c r="U585" s="18"/>
+      <c r="U585" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="586">
       <c r="A586" s="63"/>
@@ -41325,7 +41474,10 @@
       <c r="R586" s="19"/>
       <c r="S586" s="20"/>
       <c r="T586" s="20"/>
-      <c r="U586" s="18"/>
+      <c r="U586" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="587">
       <c r="A587" s="63"/>
@@ -41348,7 +41500,10 @@
       <c r="R587" s="19"/>
       <c r="S587" s="20"/>
       <c r="T587" s="20"/>
-      <c r="U587" s="18"/>
+      <c r="U587" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="588">
       <c r="A588" s="63"/>
@@ -41371,7 +41526,10 @@
       <c r="R588" s="19"/>
       <c r="S588" s="20"/>
       <c r="T588" s="20"/>
-      <c r="U588" s="18"/>
+      <c r="U588" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="589">
       <c r="A589" s="63"/>
@@ -41394,7 +41552,10 @@
       <c r="R589" s="19"/>
       <c r="S589" s="20"/>
       <c r="T589" s="20"/>
-      <c r="U589" s="18"/>
+      <c r="U589" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="590">
       <c r="A590" s="63"/>
@@ -41417,7 +41578,10 @@
       <c r="R590" s="19"/>
       <c r="S590" s="20"/>
       <c r="T590" s="20"/>
-      <c r="U590" s="18"/>
+      <c r="U590" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="591">
       <c r="A591" s="63"/>
@@ -41440,7 +41604,10 @@
       <c r="R591" s="19"/>
       <c r="S591" s="20"/>
       <c r="T591" s="20"/>
-      <c r="U591" s="18"/>
+      <c r="U591" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="592">
       <c r="A592" s="63"/>
@@ -41463,7 +41630,10 @@
       <c r="R592" s="19"/>
       <c r="S592" s="20"/>
       <c r="T592" s="20"/>
-      <c r="U592" s="18"/>
+      <c r="U592" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="593">
       <c r="A593" s="63"/>
@@ -41486,7 +41656,10 @@
       <c r="R593" s="19"/>
       <c r="S593" s="20"/>
       <c r="T593" s="20"/>
-      <c r="U593" s="18"/>
+      <c r="U593" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="594">
       <c r="A594" s="63"/>
@@ -41509,7 +41682,10 @@
       <c r="R594" s="19"/>
       <c r="S594" s="20"/>
       <c r="T594" s="20"/>
-      <c r="U594" s="18"/>
+      <c r="U594" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="595">
       <c r="A595" s="63"/>
@@ -41532,7 +41708,10 @@
       <c r="R595" s="19"/>
       <c r="S595" s="20"/>
       <c r="T595" s="20"/>
-      <c r="U595" s="18"/>
+      <c r="U595" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="596">
       <c r="A596" s="63"/>
@@ -41555,7 +41734,10 @@
       <c r="R596" s="19"/>
       <c r="S596" s="20"/>
       <c r="T596" s="20"/>
-      <c r="U596" s="18"/>
+      <c r="U596" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="597">
       <c r="A597" s="63"/>
@@ -41578,7 +41760,10 @@
       <c r="R597" s="19"/>
       <c r="S597" s="20"/>
       <c r="T597" s="20"/>
-      <c r="U597" s="18"/>
+      <c r="U597" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="598">
       <c r="A598" s="63"/>
@@ -41601,7 +41786,10 @@
       <c r="R598" s="19"/>
       <c r="S598" s="20"/>
       <c r="T598" s="20"/>
-      <c r="U598" s="18"/>
+      <c r="U598" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="599">
       <c r="A599" s="63"/>
@@ -41624,7 +41812,10 @@
       <c r="R599" s="19"/>
       <c r="S599" s="20"/>
       <c r="T599" s="20"/>
-      <c r="U599" s="18"/>
+      <c r="U599" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="600">
       <c r="A600" s="63"/>
@@ -41647,7 +41838,10 @@
       <c r="R600" s="19"/>
       <c r="S600" s="20"/>
       <c r="T600" s="20"/>
-      <c r="U600" s="18"/>
+      <c r="U600" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="601">
       <c r="A601" s="63"/>
@@ -41670,7 +41864,10 @@
       <c r="R601" s="19"/>
       <c r="S601" s="20"/>
       <c r="T601" s="20"/>
-      <c r="U601" s="18"/>
+      <c r="U601" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="J468">
@@ -42131,15 +42328,16 @@
     <hyperlink r:id="rId111" ref="S549"/>
     <hyperlink r:id="rId112" ref="S550"/>
     <hyperlink r:id="rId113" ref="S551"/>
+    <hyperlink r:id="rId114" ref="S552"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId114"/>
-  <legacyDrawing r:id="rId115"/>
+  <drawing r:id="rId115"/>
+  <legacyDrawing r:id="rId116"/>
   <tableParts count="2">
-    <tablePart r:id="rId118"/>
     <tablePart r:id="rId119"/>
+    <tablePart r:id="rId120"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201030
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -563,7 +563,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6114" uniqueCount="2054">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6159" uniqueCount="2072">
   <si>
     <t>案例</t>
   </si>
@@ -7549,6 +7549,68 @@
   </si>
   <si>
     <t>國內新增1例境外移入COVID-19病例，為無症狀印尼籍移工</t>
+  </si>
+  <si>
+    <t>#552</t>
+  </si>
+  <si>
+    <t>2019/12月-2020/10/25 菲律賓</t>
+  </si>
+  <si>
+    <t>10/25 採檢
+10/26 二採
+10/29 確診</t>
+  </si>
+  <si>
+    <t>咳嗽 流鼻水 喉嚨痛 腹瀉 全身痠痛 倦怠 肺炎 咳嗽伴隨胸痛</t>
+  </si>
+  <si>
+    <t>國內新增3例境外移入COVID-19病例，分自菲律賓、美國及印尼入境</t>
+  </si>
+  <si>
+    <t>#553</t>
+  </si>
+  <si>
+    <t>2019/11月-2020/10/27 美國</t>
+  </si>
+  <si>
+    <t>10/27 採檢
+10/29 確診</t>
+  </si>
+  <si>
+    <t>輕微咳嗽 流鼻水</t>
+  </si>
+  <si>
+    <t>長期居住美國10月15日與友人聚餐，但其中2名友人確診，因此個案10月20日曾於美國當地進行核酸檢驗結果為陰性</t>
+  </si>
+  <si>
+    <t>#554</t>
+  </si>
+  <si>
+    <t>-10/15 印尼→台灣</t>
+  </si>
+  <si>
+    <t>10/28 採檢
+10/29 確診</t>
+  </si>
+  <si>
+    <t>檢疫期滿前進行採檢</t>
+  </si>
+  <si>
+    <t>#555</t>
+  </si>
+  <si>
+    <t>-9/10 台灣→菲律賓
+9/10-10/15 菲律賓→台灣</t>
+  </si>
+  <si>
+    <t>9/17 採檢
+10/9 二採
+10/29 三採
+10/30 確診</t>
+  </si>
+  <si>
+    <t>咳嗽 呼吸困難</t>
   </si>
 </sst>
 </file>
@@ -40596,97 +40658,209 @@
       </c>
     </row>
     <row r="553">
-      <c r="A553" s="63"/>
-      <c r="B553" s="64"/>
-      <c r="C553" s="34"/>
-      <c r="D553" s="34"/>
-      <c r="E553" s="34"/>
+      <c r="A553" s="16" t="s">
+        <v>2054</v>
+      </c>
+      <c r="B553" s="6">
+        <v>44133.0</v>
+      </c>
+      <c r="C553" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D553" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E553" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F553" s="34"/>
-      <c r="G553" s="34"/>
-      <c r="H553" s="21"/>
-      <c r="I553" s="19"/>
-      <c r="J553" s="10"/>
-      <c r="K553" s="22"/>
-      <c r="L553" s="23"/>
-      <c r="M553" s="22"/>
+      <c r="G553" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H553" s="8" t="s">
+        <v>2055</v>
+      </c>
+      <c r="I553" s="9">
+        <v>44129.0</v>
+      </c>
+      <c r="J553" s="10">
+        <v>44118.0</v>
+      </c>
+      <c r="K553" s="13" t="s">
+        <v>2056</v>
+      </c>
+      <c r="L553" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M553" s="13" t="s">
+        <v>2057</v>
+      </c>
       <c r="N553" s="25"/>
-      <c r="O553" s="21"/>
+      <c r="O553" s="8" t="s">
+        <v>85</v>
+      </c>
       <c r="P553" s="21"/>
       <c r="Q553" s="19"/>
       <c r="R553" s="19"/>
-      <c r="S553" s="20"/>
+      <c r="S553" s="61" t="s">
+        <v>2058</v>
+      </c>
       <c r="T553" s="20"/>
       <c r="U553" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#552</v>
       </c>
     </row>
     <row r="554">
-      <c r="A554" s="63"/>
-      <c r="B554" s="64"/>
-      <c r="C554" s="34"/>
-      <c r="D554" s="34"/>
-      <c r="E554" s="34"/>
+      <c r="A554" s="16" t="s">
+        <v>2059</v>
+      </c>
+      <c r="B554" s="6">
+        <v>44133.0</v>
+      </c>
+      <c r="C554" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D554" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="E554" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F554" s="34"/>
-      <c r="G554" s="34"/>
-      <c r="H554" s="21"/>
-      <c r="I554" s="19"/>
-      <c r="J554" s="10"/>
-      <c r="K554" s="22"/>
-      <c r="L554" s="23"/>
-      <c r="M554" s="22"/>
+      <c r="G554" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H554" s="8" t="s">
+        <v>2060</v>
+      </c>
+      <c r="I554" s="9">
+        <v>44131.0</v>
+      </c>
+      <c r="J554" s="10">
+        <v>44130.0</v>
+      </c>
+      <c r="K554" s="13" t="s">
+        <v>2061</v>
+      </c>
+      <c r="L554" s="12" t="s">
+        <v>363</v>
+      </c>
+      <c r="M554" s="13" t="s">
+        <v>2062</v>
+      </c>
       <c r="N554" s="25"/>
-      <c r="O554" s="21"/>
-      <c r="P554" s="21"/>
+      <c r="O554" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P554" s="8" t="s">
+        <v>2063</v>
+      </c>
       <c r="Q554" s="19"/>
       <c r="R554" s="19"/>
-      <c r="S554" s="20"/>
+      <c r="S554" s="61" t="s">
+        <v>2058</v>
+      </c>
       <c r="T554" s="20"/>
       <c r="U554" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#553</v>
       </c>
     </row>
     <row r="555">
-      <c r="A555" s="63"/>
-      <c r="B555" s="64"/>
-      <c r="C555" s="34"/>
-      <c r="D555" s="34"/>
-      <c r="E555" s="34"/>
+      <c r="A555" s="16" t="s">
+        <v>2064</v>
+      </c>
+      <c r="B555" s="6">
+        <v>44133.0</v>
+      </c>
+      <c r="C555" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D555" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E555" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F555" s="34"/>
-      <c r="G555" s="34"/>
-      <c r="H555" s="21"/>
-      <c r="I555" s="19"/>
-      <c r="J555" s="10"/>
-      <c r="K555" s="22"/>
-      <c r="L555" s="23"/>
-      <c r="M555" s="22"/>
+      <c r="G555" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H555" s="8" t="s">
+        <v>2065</v>
+      </c>
+      <c r="I555" s="9">
+        <v>44119.0</v>
+      </c>
+      <c r="J555" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K555" s="13" t="s">
+        <v>2066</v>
+      </c>
+      <c r="L555" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M555" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N555" s="25"/>
-      <c r="O555" s="21"/>
-      <c r="P555" s="21"/>
+      <c r="O555" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P555" s="8" t="s">
+        <v>2067</v>
+      </c>
       <c r="Q555" s="19"/>
       <c r="R555" s="19"/>
-      <c r="S555" s="20"/>
+      <c r="S555" s="61" t="s">
+        <v>2058</v>
+      </c>
       <c r="T555" s="20"/>
       <c r="U555" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#554</v>
       </c>
     </row>
     <row r="556">
-      <c r="A556" s="63"/>
-      <c r="B556" s="64"/>
-      <c r="C556" s="34"/>
-      <c r="D556" s="34"/>
-      <c r="E556" s="34"/>
+      <c r="A556" s="16" t="s">
+        <v>2068</v>
+      </c>
+      <c r="B556" s="6">
+        <v>44134.0</v>
+      </c>
+      <c r="C556" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D556" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E556" s="7" t="s">
+        <v>205</v>
+      </c>
       <c r="F556" s="34"/>
-      <c r="G556" s="34"/>
-      <c r="H556" s="21"/>
-      <c r="I556" s="19"/>
-      <c r="J556" s="10"/>
-      <c r="K556" s="22"/>
-      <c r="L556" s="23"/>
-      <c r="M556" s="22"/>
+      <c r="G556" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H556" s="8" t="s">
+        <v>2069</v>
+      </c>
+      <c r="I556" s="9">
+        <v>44119.0</v>
+      </c>
+      <c r="J556" s="10">
+        <v>44094.0</v>
+      </c>
+      <c r="K556" s="13" t="s">
+        <v>2070</v>
+      </c>
+      <c r="L556" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M556" s="13" t="s">
+        <v>2071</v>
+      </c>
       <c r="N556" s="25"/>
       <c r="O556" s="21"/>
       <c r="P556" s="21"/>
@@ -40696,7 +40870,7 @@
       <c r="T556" s="20"/>
       <c r="U556" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#555</v>
       </c>
     </row>
     <row r="557">
@@ -42329,15 +42503,18 @@
     <hyperlink r:id="rId112" ref="S550"/>
     <hyperlink r:id="rId113" ref="S551"/>
     <hyperlink r:id="rId114" ref="S552"/>
+    <hyperlink r:id="rId115" ref="S553"/>
+    <hyperlink r:id="rId116" ref="S554"/>
+    <hyperlink r:id="rId117" ref="S555"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId115"/>
-  <legacyDrawing r:id="rId116"/>
+  <drawing r:id="rId118"/>
+  <legacyDrawing r:id="rId119"/>
   <tableParts count="2">
-    <tablePart r:id="rId119"/>
-    <tablePart r:id="rId120"/>
+    <tablePart r:id="rId122"/>
+    <tablePart r:id="rId123"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201031
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -563,7 +563,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6159" uniqueCount="2072">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6173" uniqueCount="2079">
   <si>
     <t>案例</t>
   </si>
@@ -7611,6 +7611,28 @@
   </si>
   <si>
     <t>咳嗽 呼吸困難</t>
+  </si>
+  <si>
+    <t>長期在臺灣工作，今(2020)年9月10日獨自返回菲律賓，13日於當地參加1名確診武漢肺炎之友人喪禮，並曾與其他14人同住，由於部分同住人員確診，個案9月17日於當地進行接觸者採檢，18日確診後進行隔離，20日因出現咳嗽、呼吸困難等症狀收治住院，10月3日出院，10月9日採檢結果為陰性。</t>
+  </si>
+  <si>
+    <t>國內新增1例境外移入COVID-19病例，菲籍男子檢疫期滿前採檢確診</t>
+  </si>
+  <si>
+    <t>#556</t>
+  </si>
+  <si>
+    <t>2月-10/28 印度</t>
+  </si>
+  <si>
+    <t>10/28 採檢
+10/30 確診</t>
+  </si>
+  <si>
+    <t>呼吸困難 咳嗽 發燒</t>
+  </si>
+  <si>
+    <t>國內新增1例自印度境外移入COVID-19個案</t>
   </si>
 </sst>
 </file>
@@ -40862,11 +40884,17 @@
         <v>2071</v>
       </c>
       <c r="N556" s="25"/>
-      <c r="O556" s="21"/>
-      <c r="P556" s="21"/>
+      <c r="O556" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P556" s="8" t="s">
+        <v>2072</v>
+      </c>
       <c r="Q556" s="19"/>
       <c r="R556" s="19"/>
-      <c r="S556" s="20"/>
+      <c r="S556" s="61" t="s">
+        <v>2073</v>
+      </c>
       <c r="T556" s="20"/>
       <c r="U556" s="18" t="str">
         <f t="shared" si="1"/>
@@ -40874,29 +40902,57 @@
       </c>
     </row>
     <row r="557">
-      <c r="A557" s="63"/>
-      <c r="B557" s="64"/>
-      <c r="C557" s="34"/>
-      <c r="D557" s="34"/>
-      <c r="E557" s="34"/>
+      <c r="A557" s="16" t="s">
+        <v>2074</v>
+      </c>
+      <c r="B557" s="6">
+        <v>44135.0</v>
+      </c>
+      <c r="C557" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D557" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="E557" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F557" s="34"/>
-      <c r="G557" s="34"/>
-      <c r="H557" s="21"/>
-      <c r="I557" s="19"/>
-      <c r="J557" s="10"/>
-      <c r="K557" s="22"/>
-      <c r="L557" s="23"/>
-      <c r="M557" s="22"/>
+      <c r="G557" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H557" s="8" t="s">
+        <v>2075</v>
+      </c>
+      <c r="I557" s="9">
+        <v>44132.0</v>
+      </c>
+      <c r="J557" s="10">
+        <v>44128.0</v>
+      </c>
+      <c r="K557" s="13" t="s">
+        <v>2076</v>
+      </c>
+      <c r="L557" s="12" t="s">
+        <v>363</v>
+      </c>
+      <c r="M557" s="13" t="s">
+        <v>2077</v>
+      </c>
       <c r="N557" s="25"/>
-      <c r="O557" s="21"/>
+      <c r="O557" s="8" t="s">
+        <v>85</v>
+      </c>
       <c r="P557" s="21"/>
       <c r="Q557" s="19"/>
       <c r="R557" s="19"/>
-      <c r="S557" s="20"/>
+      <c r="S557" s="61" t="s">
+        <v>2078</v>
+      </c>
       <c r="T557" s="20"/>
       <c r="U557" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#556</v>
       </c>
     </row>
     <row r="558">
@@ -42506,15 +42562,17 @@
     <hyperlink r:id="rId115" ref="S553"/>
     <hyperlink r:id="rId116" ref="S554"/>
     <hyperlink r:id="rId117" ref="S555"/>
+    <hyperlink r:id="rId118" ref="S556"/>
+    <hyperlink r:id="rId119" ref="S557"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId118"/>
-  <legacyDrawing r:id="rId119"/>
+  <drawing r:id="rId120"/>
+  <legacyDrawing r:id="rId121"/>
   <tableParts count="2">
-    <tablePart r:id="rId122"/>
-    <tablePart r:id="rId123"/>
+    <tablePart r:id="rId124"/>
+    <tablePart r:id="rId125"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201102
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -563,7 +563,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6173" uniqueCount="2079">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6214" uniqueCount="2097">
   <si>
     <t>案例</t>
   </si>
@@ -7633,6 +7633,65 @@
   </si>
   <si>
     <t>國內新增1例自印度境外移入COVID-19個案</t>
+  </si>
+  <si>
+    <t>#557</t>
+  </si>
+  <si>
+    <t>-10/29 印尼→台灣</t>
+  </si>
+  <si>
+    <t>10/29 採檢
+11/1 確診</t>
+  </si>
+  <si>
+    <t>因就學入境台灣
+個案10月7日曾出現嗅覺喪失症狀，未於當地就醫</t>
+  </si>
+  <si>
+    <t>國內新增3例境外移入COVID-19病例，分自印尼及美國入境</t>
+  </si>
+  <si>
+    <t>#558</t>
+  </si>
+  <si>
+    <t>-10/14 印尼→台灣</t>
+  </si>
+  <si>
+    <t>10月14日來臺工作，10月10日曾於國外自費檢驗結果為陰性
+曾於10月14日晚間出現流鼻水症狀，自行服用成藥後症狀緩解
+10月29日檢疫期滿後，與另2名移工一同由仲介開車送至醫院自費採檢</t>
+  </si>
+  <si>
+    <t>#559</t>
+  </si>
+  <si>
+    <t>2月-10/30 美國</t>
+  </si>
+  <si>
+    <t>10/30 採檢
+11/1 確診</t>
+  </si>
+  <si>
+    <t>發燒 肌肉痠痛 關節痛 咳嗽</t>
+  </si>
+  <si>
+    <t>因工作長期居住美國</t>
+  </si>
+  <si>
+    <t>#560</t>
+  </si>
+  <si>
+    <t>#561</t>
+  </si>
+  <si>
+    <t>#562</t>
+  </si>
+  <si>
+    <t>#563</t>
+  </si>
+  <si>
+    <t>#564</t>
   </si>
 </sst>
 </file>
@@ -40956,86 +41015,180 @@
       </c>
     </row>
     <row r="558">
-      <c r="A558" s="63"/>
-      <c r="B558" s="64"/>
-      <c r="C558" s="34"/>
-      <c r="D558" s="34"/>
-      <c r="E558" s="34"/>
+      <c r="A558" s="16" t="s">
+        <v>2079</v>
+      </c>
+      <c r="B558" s="6">
+        <v>44136.0</v>
+      </c>
+      <c r="C558" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D558" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="E558" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F558" s="34"/>
-      <c r="G558" s="34"/>
-      <c r="H558" s="21"/>
-      <c r="I558" s="19"/>
-      <c r="J558" s="10"/>
-      <c r="K558" s="22"/>
-      <c r="L558" s="23"/>
-      <c r="M558" s="22"/>
+      <c r="G558" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H558" s="8" t="s">
+        <v>2080</v>
+      </c>
+      <c r="I558" s="9">
+        <v>44133.0</v>
+      </c>
+      <c r="J558" s="10">
+        <v>44111.0</v>
+      </c>
+      <c r="K558" s="13" t="s">
+        <v>2081</v>
+      </c>
+      <c r="L558" s="12" t="s">
+        <v>363</v>
+      </c>
+      <c r="M558" s="13" t="s">
+        <v>1151</v>
+      </c>
       <c r="N558" s="25"/>
-      <c r="O558" s="21"/>
-      <c r="P558" s="21"/>
+      <c r="O558" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P558" s="8" t="s">
+        <v>2082</v>
+      </c>
       <c r="Q558" s="19"/>
       <c r="R558" s="19"/>
-      <c r="S558" s="20"/>
+      <c r="S558" s="61" t="s">
+        <v>2083</v>
+      </c>
       <c r="T558" s="20"/>
       <c r="U558" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#557</v>
       </c>
     </row>
     <row r="559">
-      <c r="A559" s="63"/>
-      <c r="B559" s="64"/>
-      <c r="C559" s="34"/>
-      <c r="D559" s="34"/>
-      <c r="E559" s="34"/>
+      <c r="A559" s="16" t="s">
+        <v>2084</v>
+      </c>
+      <c r="B559" s="6">
+        <v>44136.0</v>
+      </c>
+      <c r="C559" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D559" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E559" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F559" s="34"/>
-      <c r="G559" s="34"/>
-      <c r="H559" s="21"/>
-      <c r="I559" s="19"/>
-      <c r="J559" s="10"/>
-      <c r="K559" s="22"/>
-      <c r="L559" s="23"/>
-      <c r="M559" s="22"/>
+      <c r="G559" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H559" s="8" t="s">
+        <v>2085</v>
+      </c>
+      <c r="I559" s="9">
+        <v>44118.0</v>
+      </c>
+      <c r="J559" s="10">
+        <v>44118.0</v>
+      </c>
+      <c r="K559" s="13" t="s">
+        <v>2081</v>
+      </c>
+      <c r="L559" s="12" t="s">
+        <v>1674</v>
+      </c>
+      <c r="M559" s="13" t="s">
+        <v>482</v>
+      </c>
       <c r="N559" s="25"/>
-      <c r="O559" s="21"/>
-      <c r="P559" s="21"/>
+      <c r="O559" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P559" s="8" t="s">
+        <v>2086</v>
+      </c>
       <c r="Q559" s="19"/>
       <c r="R559" s="19"/>
-      <c r="S559" s="20"/>
+      <c r="S559" s="61" t="s">
+        <v>2083</v>
+      </c>
       <c r="T559" s="20"/>
       <c r="U559" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#558</v>
       </c>
     </row>
     <row r="560">
-      <c r="A560" s="63"/>
-      <c r="B560" s="64"/>
-      <c r="C560" s="34"/>
-      <c r="D560" s="34"/>
-      <c r="E560" s="34"/>
+      <c r="A560" s="16" t="s">
+        <v>2087</v>
+      </c>
+      <c r="B560" s="6">
+        <v>44136.0</v>
+      </c>
+      <c r="C560" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D560" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E560" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F560" s="34"/>
-      <c r="G560" s="34"/>
-      <c r="H560" s="21"/>
-      <c r="I560" s="19"/>
-      <c r="J560" s="10"/>
-      <c r="K560" s="22"/>
-      <c r="L560" s="23"/>
-      <c r="M560" s="22"/>
+      <c r="G560" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H560" s="8" t="s">
+        <v>2088</v>
+      </c>
+      <c r="I560" s="9">
+        <v>44134.0</v>
+      </c>
+      <c r="J560" s="10">
+        <v>44130.0</v>
+      </c>
+      <c r="K560" s="13" t="s">
+        <v>2089</v>
+      </c>
+      <c r="L560" s="12" t="s">
+        <v>363</v>
+      </c>
+      <c r="M560" s="13" t="s">
+        <v>2090</v>
+      </c>
       <c r="N560" s="25"/>
-      <c r="O560" s="21"/>
-      <c r="P560" s="21"/>
+      <c r="O560" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P560" s="8" t="s">
+        <v>2091</v>
+      </c>
       <c r="Q560" s="19"/>
       <c r="R560" s="19"/>
-      <c r="S560" s="20"/>
+      <c r="S560" s="61" t="s">
+        <v>2083</v>
+      </c>
       <c r="T560" s="20"/>
       <c r="U560" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#559</v>
       </c>
     </row>
     <row r="561">
-      <c r="A561" s="63"/>
-      <c r="B561" s="64"/>
+      <c r="A561" s="16" t="s">
+        <v>2092</v>
+      </c>
+      <c r="B561" s="6">
+        <v>44137.0</v>
+      </c>
       <c r="C561" s="34"/>
       <c r="D561" s="34"/>
       <c r="E561" s="34"/>
@@ -41056,12 +41209,16 @@
       <c r="T561" s="20"/>
       <c r="U561" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#560</v>
       </c>
     </row>
     <row r="562">
-      <c r="A562" s="63"/>
-      <c r="B562" s="64"/>
+      <c r="A562" s="16" t="s">
+        <v>2093</v>
+      </c>
+      <c r="B562" s="6">
+        <v>44137.0</v>
+      </c>
       <c r="C562" s="34"/>
       <c r="D562" s="34"/>
       <c r="E562" s="34"/>
@@ -41082,12 +41239,16 @@
       <c r="T562" s="20"/>
       <c r="U562" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#561</v>
       </c>
     </row>
     <row r="563">
-      <c r="A563" s="63"/>
-      <c r="B563" s="64"/>
+      <c r="A563" s="16" t="s">
+        <v>2094</v>
+      </c>
+      <c r="B563" s="6">
+        <v>44137.0</v>
+      </c>
       <c r="C563" s="34"/>
       <c r="D563" s="34"/>
       <c r="E563" s="34"/>
@@ -41108,12 +41269,16 @@
       <c r="T563" s="20"/>
       <c r="U563" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#562</v>
       </c>
     </row>
     <row r="564">
-      <c r="A564" s="63"/>
-      <c r="B564" s="64"/>
+      <c r="A564" s="16" t="s">
+        <v>2095</v>
+      </c>
+      <c r="B564" s="6">
+        <v>44137.0</v>
+      </c>
       <c r="C564" s="34"/>
       <c r="D564" s="34"/>
       <c r="E564" s="34"/>
@@ -41134,12 +41299,16 @@
       <c r="T564" s="20"/>
       <c r="U564" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#563</v>
       </c>
     </row>
     <row r="565">
-      <c r="A565" s="63"/>
-      <c r="B565" s="64"/>
+      <c r="A565" s="16" t="s">
+        <v>2096</v>
+      </c>
+      <c r="B565" s="6">
+        <v>44137.0</v>
+      </c>
       <c r="C565" s="34"/>
       <c r="D565" s="34"/>
       <c r="E565" s="34"/>
@@ -41160,7 +41329,7 @@
       <c r="T565" s="20"/>
       <c r="U565" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#564</v>
       </c>
     </row>
     <row r="566">
@@ -42564,15 +42733,18 @@
     <hyperlink r:id="rId117" ref="S555"/>
     <hyperlink r:id="rId118" ref="S556"/>
     <hyperlink r:id="rId119" ref="S557"/>
+    <hyperlink r:id="rId120" ref="S558"/>
+    <hyperlink r:id="rId121" ref="S559"/>
+    <hyperlink r:id="rId122" ref="S560"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId120"/>
-  <legacyDrawing r:id="rId121"/>
+  <drawing r:id="rId123"/>
+  <legacyDrawing r:id="rId124"/>
   <tableParts count="2">
-    <tablePart r:id="rId124"/>
-    <tablePart r:id="rId125"/>
+    <tablePart r:id="rId127"/>
+    <tablePart r:id="rId128"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201103
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -563,7 +563,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6214" uniqueCount="2097">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6276" uniqueCount="2114">
   <si>
     <t>案例</t>
   </si>
@@ -7682,16 +7682,83 @@
     <t>#560</t>
   </si>
   <si>
+    <t>10/12 採檢
+10/14 二採
+10/31 三採
+11/2 確診</t>
+  </si>
+  <si>
+    <t>來臺前曾於10月12日及14日採驗，結果皆為陰性，10月15日與1名同事來臺工作
+個案居家檢疫期滿後，因公司要求，10月31日自費採檢</t>
+  </si>
+  <si>
+    <t>新增5例境外移入COVID-19病例，為自印度、印尼及菲律賓來臺工作者</t>
+  </si>
+  <si>
     <t>#561</t>
   </si>
   <si>
+    <t>-10/18 印尼→台灣</t>
+  </si>
+  <si>
+    <t>10/31 採檢
+11/2 確診</t>
+  </si>
+  <si>
+    <t>檢疫期滿前採檢</t>
+  </si>
+  <si>
     <t>#562</t>
   </si>
   <si>
+    <t>-10/10 印尼→台灣</t>
+  </si>
+  <si>
+    <t>10/23 採檢
+10/30 二採
+11/2 確診</t>
+  </si>
+  <si>
+    <t>10月23日檢疫期滿前採檢結果為陰性
+因雇主要求，10月30日至醫院自費採檢</t>
+  </si>
+  <si>
     <t>#563</t>
   </si>
   <si>
+    <t>10/14 採檢
+10/30 二採
+11/2 確診</t>
+  </si>
+  <si>
+    <t>與 #558 同行
+登機前3日內檢驗為陰性
+檢疫期滿後自費採檢結果為陰性
+個案與另1名同行入境移工因入境前與案558密切接觸，故列為居家隔離
+於10月30日出現咳嗽、喉嚨痛症狀住院隔離並採檢</t>
+  </si>
+  <si>
     <t>#564</t>
+  </si>
+  <si>
+    <t>-10/19 菲律賓→台灣</t>
+  </si>
+  <si>
+    <t>11/1 採檢
+11/2 確診</t>
+  </si>
+  <si>
+    <t>登機前3日內檢驗為陰性
+11月1日進行檢疫期滿前採檢</t>
+  </si>
+  <si>
+    <t>#565</t>
+  </si>
+  <si>
+    <t>#566</t>
+  </si>
+  <si>
+    <t>#567</t>
   </si>
 </sst>
 </file>
@@ -41189,23 +41256,49 @@
       <c r="B561" s="6">
         <v>44137.0</v>
       </c>
-      <c r="C561" s="34"/>
-      <c r="D561" s="34"/>
-      <c r="E561" s="34"/>
+      <c r="C561" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D561" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E561" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F561" s="34"/>
-      <c r="G561" s="34"/>
-      <c r="H561" s="21"/>
-      <c r="I561" s="19"/>
-      <c r="J561" s="10"/>
-      <c r="K561" s="22"/>
-      <c r="L561" s="23"/>
-      <c r="M561" s="22"/>
+      <c r="G561" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H561" s="8" t="s">
+        <v>2065</v>
+      </c>
+      <c r="I561" s="9">
+        <v>44119.0</v>
+      </c>
+      <c r="J561" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K561" s="13" t="s">
+        <v>2093</v>
+      </c>
+      <c r="L561" s="12" t="s">
+        <v>1674</v>
+      </c>
+      <c r="M561" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N561" s="25"/>
-      <c r="O561" s="21"/>
-      <c r="P561" s="21"/>
+      <c r="O561" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P561" s="8" t="s">
+        <v>2094</v>
+      </c>
       <c r="Q561" s="19"/>
       <c r="R561" s="19"/>
-      <c r="S561" s="20"/>
+      <c r="S561" s="61" t="s">
+        <v>2095</v>
+      </c>
       <c r="T561" s="20"/>
       <c r="U561" s="18" t="str">
         <f t="shared" si="1"/>
@@ -41214,28 +41307,54 @@
     </row>
     <row r="562">
       <c r="A562" s="16" t="s">
-        <v>2093</v>
+        <v>2096</v>
       </c>
       <c r="B562" s="6">
         <v>44137.0</v>
       </c>
-      <c r="C562" s="34"/>
-      <c r="D562" s="34"/>
-      <c r="E562" s="34"/>
+      <c r="C562" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D562" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E562" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F562" s="34"/>
-      <c r="G562" s="34"/>
-      <c r="H562" s="21"/>
-      <c r="I562" s="19"/>
-      <c r="J562" s="10"/>
-      <c r="K562" s="22"/>
-      <c r="L562" s="23"/>
-      <c r="M562" s="22"/>
+      <c r="G562" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H562" s="8" t="s">
+        <v>2097</v>
+      </c>
+      <c r="I562" s="9">
+        <v>44122.0</v>
+      </c>
+      <c r="J562" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K562" s="13" t="s">
+        <v>2098</v>
+      </c>
+      <c r="L562" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M562" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N562" s="25"/>
-      <c r="O562" s="21"/>
-      <c r="P562" s="21"/>
+      <c r="O562" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P562" s="8" t="s">
+        <v>2099</v>
+      </c>
       <c r="Q562" s="19"/>
       <c r="R562" s="19"/>
-      <c r="S562" s="20"/>
+      <c r="S562" s="61" t="s">
+        <v>2095</v>
+      </c>
       <c r="T562" s="20"/>
       <c r="U562" s="18" t="str">
         <f t="shared" si="1"/>
@@ -41244,28 +41363,54 @@
     </row>
     <row r="563">
       <c r="A563" s="16" t="s">
-        <v>2094</v>
+        <v>2100</v>
       </c>
       <c r="B563" s="6">
         <v>44137.0</v>
       </c>
-      <c r="C563" s="34"/>
-      <c r="D563" s="34"/>
-      <c r="E563" s="34"/>
+      <c r="C563" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D563" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E563" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F563" s="34"/>
-      <c r="G563" s="34"/>
-      <c r="H563" s="21"/>
-      <c r="I563" s="19"/>
-      <c r="J563" s="10"/>
-      <c r="K563" s="22"/>
-      <c r="L563" s="23"/>
-      <c r="M563" s="22"/>
+      <c r="G563" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H563" s="8" t="s">
+        <v>2101</v>
+      </c>
+      <c r="I563" s="9">
+        <v>44114.0</v>
+      </c>
+      <c r="J563" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K563" s="13" t="s">
+        <v>2102</v>
+      </c>
+      <c r="L563" s="12" t="s">
+        <v>1674</v>
+      </c>
+      <c r="M563" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N563" s="25"/>
-      <c r="O563" s="21"/>
-      <c r="P563" s="21"/>
+      <c r="O563" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P563" s="8" t="s">
+        <v>2103</v>
+      </c>
       <c r="Q563" s="19"/>
       <c r="R563" s="19"/>
-      <c r="S563" s="20"/>
+      <c r="S563" s="61" t="s">
+        <v>2095</v>
+      </c>
       <c r="T563" s="20"/>
       <c r="U563" s="18" t="str">
         <f t="shared" si="1"/>
@@ -41274,28 +41419,54 @@
     </row>
     <row r="564">
       <c r="A564" s="16" t="s">
-        <v>2095</v>
+        <v>2104</v>
       </c>
       <c r="B564" s="6">
         <v>44137.0</v>
       </c>
-      <c r="C564" s="34"/>
-      <c r="D564" s="34"/>
-      <c r="E564" s="34"/>
+      <c r="C564" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D564" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E564" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F564" s="34"/>
-      <c r="G564" s="34"/>
-      <c r="H564" s="21"/>
-      <c r="I564" s="19"/>
-      <c r="J564" s="10"/>
-      <c r="K564" s="22"/>
-      <c r="L564" s="23"/>
-      <c r="M564" s="22"/>
+      <c r="G564" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H564" s="8" t="s">
+        <v>2022</v>
+      </c>
+      <c r="I564" s="9">
+        <v>44118.0</v>
+      </c>
+      <c r="J564" s="10">
+        <v>44134.0</v>
+      </c>
+      <c r="K564" s="13" t="s">
+        <v>2105</v>
+      </c>
+      <c r="L564" s="12" t="s">
+        <v>447</v>
+      </c>
+      <c r="M564" s="13" t="s">
+        <v>618</v>
+      </c>
       <c r="N564" s="25"/>
-      <c r="O564" s="21"/>
-      <c r="P564" s="21"/>
+      <c r="O564" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P564" s="8" t="s">
+        <v>2106</v>
+      </c>
       <c r="Q564" s="19"/>
       <c r="R564" s="19"/>
-      <c r="S564" s="20"/>
+      <c r="S564" s="61" t="s">
+        <v>2095</v>
+      </c>
       <c r="T564" s="20"/>
       <c r="U564" s="18" t="str">
         <f t="shared" si="1"/>
@@ -41304,28 +41475,54 @@
     </row>
     <row r="565">
       <c r="A565" s="16" t="s">
-        <v>2096</v>
+        <v>2107</v>
       </c>
       <c r="B565" s="6">
         <v>44137.0</v>
       </c>
-      <c r="C565" s="34"/>
-      <c r="D565" s="34"/>
-      <c r="E565" s="34"/>
+      <c r="C565" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D565" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E565" s="7" t="s">
+        <v>205</v>
+      </c>
       <c r="F565" s="34"/>
-      <c r="G565" s="34"/>
-      <c r="H565" s="21"/>
-      <c r="I565" s="19"/>
-      <c r="J565" s="10"/>
-      <c r="K565" s="22"/>
-      <c r="L565" s="23"/>
-      <c r="M565" s="22"/>
+      <c r="G565" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H565" s="8" t="s">
+        <v>2108</v>
+      </c>
+      <c r="I565" s="9">
+        <v>44123.0</v>
+      </c>
+      <c r="J565" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K565" s="13" t="s">
+        <v>2109</v>
+      </c>
+      <c r="L565" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M565" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N565" s="25"/>
-      <c r="O565" s="21"/>
-      <c r="P565" s="21"/>
+      <c r="O565" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P565" s="8" t="s">
+        <v>2110</v>
+      </c>
       <c r="Q565" s="19"/>
       <c r="R565" s="19"/>
-      <c r="S565" s="20"/>
+      <c r="S565" s="61" t="s">
+        <v>2095</v>
+      </c>
       <c r="T565" s="20"/>
       <c r="U565" s="18" t="str">
         <f t="shared" si="1"/>
@@ -41333,8 +41530,12 @@
       </c>
     </row>
     <row r="566">
-      <c r="A566" s="63"/>
-      <c r="B566" s="64"/>
+      <c r="A566" s="16" t="s">
+        <v>2111</v>
+      </c>
+      <c r="B566" s="6">
+        <v>44138.0</v>
+      </c>
       <c r="C566" s="34"/>
       <c r="D566" s="34"/>
       <c r="E566" s="34"/>
@@ -41355,12 +41556,16 @@
       <c r="T566" s="20"/>
       <c r="U566" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#565</v>
       </c>
     </row>
     <row r="567">
-      <c r="A567" s="63"/>
-      <c r="B567" s="64"/>
+      <c r="A567" s="16" t="s">
+        <v>2112</v>
+      </c>
+      <c r="B567" s="6">
+        <v>44138.0</v>
+      </c>
       <c r="C567" s="34"/>
       <c r="D567" s="34"/>
       <c r="E567" s="34"/>
@@ -41381,12 +41586,16 @@
       <c r="T567" s="20"/>
       <c r="U567" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#566</v>
       </c>
     </row>
     <row r="568">
-      <c r="A568" s="63"/>
-      <c r="B568" s="64"/>
+      <c r="A568" s="16" t="s">
+        <v>2113</v>
+      </c>
+      <c r="B568" s="6">
+        <v>44138.0</v>
+      </c>
       <c r="C568" s="34"/>
       <c r="D568" s="34"/>
       <c r="E568" s="34"/>
@@ -41407,7 +41616,7 @@
       <c r="T568" s="20"/>
       <c r="U568" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#567</v>
       </c>
     </row>
     <row r="569">
@@ -42736,15 +42945,20 @@
     <hyperlink r:id="rId120" ref="S558"/>
     <hyperlink r:id="rId121" ref="S559"/>
     <hyperlink r:id="rId122" ref="S560"/>
+    <hyperlink r:id="rId123" ref="S561"/>
+    <hyperlink r:id="rId124" ref="S562"/>
+    <hyperlink r:id="rId125" ref="S563"/>
+    <hyperlink r:id="rId126" ref="S564"/>
+    <hyperlink r:id="rId127" ref="S565"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId123"/>
-  <legacyDrawing r:id="rId124"/>
+  <drawing r:id="rId128"/>
+  <legacyDrawing r:id="rId129"/>
   <tableParts count="2">
-    <tablePart r:id="rId127"/>
-    <tablePart r:id="rId128"/>
+    <tablePart r:id="rId132"/>
+    <tablePart r:id="rId133"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201104
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -563,7 +563,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6276" uniqueCount="2114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6323" uniqueCount="2129">
   <si>
     <t>案例</t>
   </si>
@@ -7755,10 +7755,64 @@
     <t>#565</t>
   </si>
   <si>
+    <t>8月-11/1 法國</t>
+  </si>
+  <si>
+    <t>10月中旬</t>
+  </si>
+  <si>
+    <t>9/20 採檢
+10/8 二採
+10/15 三採
+10/19 四採
+11/1 五採
+11/3 確診</t>
+  </si>
+  <si>
+    <t>喉嚨痛 流鼻水 咳嗽 嗅覺異常</t>
+  </si>
+  <si>
+    <t>就學
+10月中旬出現喉嚨痛、流鼻水、咳嗽等症狀，10月30日出現嗅覺異常
+自述9月20日、10月8日、10月15日及10月19日由學校合作實驗室進行PCR檢驗結果均為陰性</t>
+  </si>
+  <si>
+    <t>國內新增4例境外移入COVID-19病例，分別自法國、英國、德國、菲律賓入境</t>
+  </si>
+  <si>
     <t>#566</t>
   </si>
   <si>
+    <t>8月-11/1 英國</t>
+  </si>
+  <si>
+    <t>11/1 採檢
+11/3 確診</t>
+  </si>
+  <si>
+    <t>鼻塞</t>
+  </si>
+  <si>
     <t>#567</t>
+  </si>
+  <si>
+    <t>10月-11/1 德國</t>
+  </si>
+  <si>
+    <t>流鼻水 肌肉痠痛 頭痛</t>
+  </si>
+  <si>
+    <t>#568</t>
+  </si>
+  <si>
+    <t>-10/20 菲律賓→台灣</t>
+  </si>
+  <si>
+    <t>11/2 採檢
+11/3 確診</t>
+  </si>
+  <si>
+    <t>10月20日來臺就學，持入境前3日內檢驗結果陰性報告，入境迄今無症狀，11月2日進行檢疫期滿前採檢</t>
   </si>
 </sst>
 </file>
@@ -41536,23 +41590,49 @@
       <c r="B566" s="6">
         <v>44138.0</v>
       </c>
-      <c r="C566" s="34"/>
-      <c r="D566" s="34"/>
-      <c r="E566" s="34"/>
+      <c r="C566" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D566" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E566" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F566" s="34"/>
-      <c r="G566" s="34"/>
-      <c r="H566" s="21"/>
-      <c r="I566" s="19"/>
-      <c r="J566" s="10"/>
-      <c r="K566" s="22"/>
-      <c r="L566" s="23"/>
-      <c r="M566" s="22"/>
+      <c r="G566" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H566" s="8" t="s">
+        <v>2112</v>
+      </c>
+      <c r="I566" s="9">
+        <v>44136.0</v>
+      </c>
+      <c r="J566" s="12" t="s">
+        <v>2113</v>
+      </c>
+      <c r="K566" s="13" t="s">
+        <v>2114</v>
+      </c>
+      <c r="L566" s="12" t="s">
+        <v>363</v>
+      </c>
+      <c r="M566" s="13" t="s">
+        <v>2115</v>
+      </c>
       <c r="N566" s="25"/>
-      <c r="O566" s="21"/>
-      <c r="P566" s="21"/>
+      <c r="O566" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P566" s="8" t="s">
+        <v>2116</v>
+      </c>
       <c r="Q566" s="19"/>
       <c r="R566" s="19"/>
-      <c r="S566" s="20"/>
+      <c r="S566" s="61" t="s">
+        <v>2117</v>
+      </c>
       <c r="T566" s="20"/>
       <c r="U566" s="18" t="str">
         <f t="shared" si="1"/>
@@ -41561,28 +41641,54 @@
     </row>
     <row r="567">
       <c r="A567" s="16" t="s">
-        <v>2112</v>
+        <v>2118</v>
       </c>
       <c r="B567" s="6">
         <v>44138.0</v>
       </c>
-      <c r="C567" s="34"/>
-      <c r="D567" s="34"/>
-      <c r="E567" s="34"/>
+      <c r="C567" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D567" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E567" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F567" s="34"/>
-      <c r="G567" s="34"/>
-      <c r="H567" s="21"/>
-      <c r="I567" s="19"/>
-      <c r="J567" s="10"/>
-      <c r="K567" s="22"/>
-      <c r="L567" s="23"/>
-      <c r="M567" s="22"/>
+      <c r="G567" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H567" s="8" t="s">
+        <v>2119</v>
+      </c>
+      <c r="I567" s="9">
+        <v>44136.0</v>
+      </c>
+      <c r="J567" s="10">
+        <v>44133.0</v>
+      </c>
+      <c r="K567" s="13" t="s">
+        <v>2120</v>
+      </c>
+      <c r="L567" s="12" t="s">
+        <v>363</v>
+      </c>
+      <c r="M567" s="13" t="s">
+        <v>2121</v>
+      </c>
       <c r="N567" s="25"/>
-      <c r="O567" s="21"/>
-      <c r="P567" s="21"/>
+      <c r="O567" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P567" s="8" t="s">
+        <v>360</v>
+      </c>
       <c r="Q567" s="19"/>
       <c r="R567" s="19"/>
-      <c r="S567" s="20"/>
+      <c r="S567" s="61" t="s">
+        <v>2117</v>
+      </c>
       <c r="T567" s="20"/>
       <c r="U567" s="18" t="str">
         <f t="shared" si="1"/>
@@ -41591,28 +41697,54 @@
     </row>
     <row r="568">
       <c r="A568" s="16" t="s">
-        <v>2113</v>
+        <v>2122</v>
       </c>
       <c r="B568" s="6">
         <v>44138.0</v>
       </c>
-      <c r="C568" s="34"/>
-      <c r="D568" s="34"/>
-      <c r="E568" s="34"/>
+      <c r="C568" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D568" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="E568" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F568" s="34"/>
-      <c r="G568" s="34"/>
-      <c r="H568" s="21"/>
-      <c r="I568" s="19"/>
-      <c r="J568" s="10"/>
-      <c r="K568" s="22"/>
-      <c r="L568" s="23"/>
-      <c r="M568" s="22"/>
+      <c r="G568" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H568" s="8" t="s">
+        <v>2123</v>
+      </c>
+      <c r="I568" s="9">
+        <v>44136.0</v>
+      </c>
+      <c r="J568" s="10">
+        <v>44135.0</v>
+      </c>
+      <c r="K568" s="13" t="s">
+        <v>2120</v>
+      </c>
+      <c r="L568" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M568" s="13" t="s">
+        <v>2124</v>
+      </c>
       <c r="N568" s="25"/>
-      <c r="O568" s="21"/>
-      <c r="P568" s="21"/>
+      <c r="O568" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P568" s="8" t="s">
+        <v>360</v>
+      </c>
       <c r="Q568" s="19"/>
       <c r="R568" s="19"/>
-      <c r="S568" s="20"/>
+      <c r="S568" s="61" t="s">
+        <v>2117</v>
+      </c>
       <c r="T568" s="20"/>
       <c r="U568" s="18" t="str">
         <f t="shared" si="1"/>
@@ -41620,29 +41752,59 @@
       </c>
     </row>
     <row r="569">
-      <c r="A569" s="63"/>
-      <c r="B569" s="64"/>
-      <c r="C569" s="34"/>
-      <c r="D569" s="34"/>
-      <c r="E569" s="34"/>
+      <c r="A569" s="16" t="s">
+        <v>2125</v>
+      </c>
+      <c r="B569" s="6">
+        <v>44138.0</v>
+      </c>
+      <c r="C569" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D569" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="E569" s="7" t="s">
+        <v>205</v>
+      </c>
       <c r="F569" s="34"/>
-      <c r="G569" s="34"/>
-      <c r="H569" s="21"/>
-      <c r="I569" s="19"/>
-      <c r="J569" s="10"/>
-      <c r="K569" s="22"/>
-      <c r="L569" s="23"/>
-      <c r="M569" s="22"/>
+      <c r="G569" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H569" s="8" t="s">
+        <v>2126</v>
+      </c>
+      <c r="I569" s="9">
+        <v>44124.0</v>
+      </c>
+      <c r="J569" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K569" s="13" t="s">
+        <v>2127</v>
+      </c>
+      <c r="L569" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M569" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N569" s="25"/>
-      <c r="O569" s="21"/>
-      <c r="P569" s="21"/>
+      <c r="O569" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P569" s="8" t="s">
+        <v>2128</v>
+      </c>
       <c r="Q569" s="19"/>
       <c r="R569" s="19"/>
-      <c r="S569" s="20"/>
+      <c r="S569" s="61" t="s">
+        <v>2117</v>
+      </c>
       <c r="T569" s="20"/>
       <c r="U569" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#568</v>
       </c>
     </row>
     <row r="570">
@@ -42950,15 +43112,19 @@
     <hyperlink r:id="rId125" ref="S563"/>
     <hyperlink r:id="rId126" ref="S564"/>
     <hyperlink r:id="rId127" ref="S565"/>
+    <hyperlink r:id="rId128" ref="S566"/>
+    <hyperlink r:id="rId129" ref="S567"/>
+    <hyperlink r:id="rId130" ref="S568"/>
+    <hyperlink r:id="rId131" ref="S569"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId128"/>
-  <legacyDrawing r:id="rId129"/>
+  <drawing r:id="rId132"/>
+  <legacyDrawing r:id="rId133"/>
   <tableParts count="2">
-    <tablePart r:id="rId132"/>
-    <tablePart r:id="rId133"/>
+    <tablePart r:id="rId136"/>
+    <tablePart r:id="rId137"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201105
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -563,7 +563,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6323" uniqueCount="2129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6335" uniqueCount="2135">
   <si>
     <t>案例</t>
   </si>
@@ -7813,6 +7813,25 @@
   </si>
   <si>
     <t>10月20日來臺就學，持入境前3日內檢驗結果陰性報告，入境迄今無症狀，11月2日進行檢疫期滿前採檢</t>
+  </si>
+  <si>
+    <t>#569</t>
+  </si>
+  <si>
+    <t>9/16-10/25 波蘭</t>
+  </si>
+  <si>
+    <t>11/2 採檢
+11/4 確診</t>
+  </si>
+  <si>
+    <t>全身倦怠 咳嗽 喉嚨痛 流鼻水 嗅覺異常 味覺異常</t>
+  </si>
+  <si>
+    <t>與2名同事至波蘭工作</t>
+  </si>
+  <si>
+    <t>女赴波蘭工作，返國後確診COVID-19</t>
   </si>
 </sst>
 </file>
@@ -41808,29 +41827,59 @@
       </c>
     </row>
     <row r="570">
-      <c r="A570" s="63"/>
-      <c r="B570" s="64"/>
-      <c r="C570" s="34"/>
-      <c r="D570" s="34"/>
-      <c r="E570" s="34"/>
+      <c r="A570" s="16" t="s">
+        <v>2129</v>
+      </c>
+      <c r="B570" s="6">
+        <v>44139.0</v>
+      </c>
+      <c r="C570" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D570" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E570" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F570" s="34"/>
-      <c r="G570" s="34"/>
-      <c r="H570" s="21"/>
-      <c r="I570" s="19"/>
-      <c r="J570" s="10"/>
-      <c r="K570" s="22"/>
-      <c r="L570" s="23"/>
-      <c r="M570" s="22"/>
+      <c r="G570" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H570" s="8" t="s">
+        <v>2130</v>
+      </c>
+      <c r="I570" s="9">
+        <v>44129.0</v>
+      </c>
+      <c r="J570" s="10">
+        <v>44134.0</v>
+      </c>
+      <c r="K570" s="13" t="s">
+        <v>2131</v>
+      </c>
+      <c r="L570" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M570" s="13" t="s">
+        <v>2132</v>
+      </c>
       <c r="N570" s="25"/>
-      <c r="O570" s="21"/>
-      <c r="P570" s="21"/>
+      <c r="O570" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P570" s="8" t="s">
+        <v>2133</v>
+      </c>
       <c r="Q570" s="19"/>
       <c r="R570" s="19"/>
-      <c r="S570" s="20"/>
+      <c r="S570" s="61" t="s">
+        <v>2134</v>
+      </c>
       <c r="T570" s="20"/>
       <c r="U570" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#569</v>
       </c>
     </row>
     <row r="571">
@@ -43116,15 +43165,16 @@
     <hyperlink r:id="rId129" ref="S567"/>
     <hyperlink r:id="rId130" ref="S568"/>
     <hyperlink r:id="rId131" ref="S569"/>
+    <hyperlink r:id="rId132" ref="S570"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId132"/>
-  <legacyDrawing r:id="rId133"/>
+  <drawing r:id="rId133"/>
+  <legacyDrawing r:id="rId134"/>
   <tableParts count="2">
-    <tablePart r:id="rId136"/>
     <tablePart r:id="rId137"/>
+    <tablePart r:id="rId138"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201106
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -563,7 +563,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6335" uniqueCount="2135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6347" uniqueCount="2141">
   <si>
     <t>案例</t>
   </si>
@@ -7832,6 +7832,27 @@
   </si>
   <si>
     <t>女赴波蘭工作，返國後確診COVID-19</t>
+  </si>
+  <si>
+    <t>#570</t>
+  </si>
+  <si>
+    <t>9月中旬-11/2 捷克
+11/2-11/2 荷蘭經曼谷</t>
+  </si>
+  <si>
+    <t>11/3 採檢
+11/5 確診</t>
+  </si>
+  <si>
+    <t>發燒 味覺異常 流鼻水 有痰</t>
+  </si>
+  <si>
+    <t>赴捷克就學，本身有過敏性鼻炎病史，10月10日在捷克曾出現發燒、味覺異常情形，未於當地就醫，約10天後症狀改善
+11月2日自荷蘭搭機經曼谷返國，入境時有流鼻水、有痰症狀</t>
+  </si>
+  <si>
+    <t>國內新增1例境外移入COVID-19病例，女自捷克返國後確診</t>
   </si>
 </sst>
 </file>
@@ -41883,29 +41904,59 @@
       </c>
     </row>
     <row r="571">
-      <c r="A571" s="63"/>
-      <c r="B571" s="64"/>
-      <c r="C571" s="34"/>
-      <c r="D571" s="34"/>
-      <c r="E571" s="34"/>
+      <c r="A571" s="16" t="s">
+        <v>2135</v>
+      </c>
+      <c r="B571" s="6">
+        <v>44140.0</v>
+      </c>
+      <c r="C571" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D571" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E571" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F571" s="34"/>
-      <c r="G571" s="34"/>
-      <c r="H571" s="21"/>
-      <c r="I571" s="19"/>
-      <c r="J571" s="10"/>
-      <c r="K571" s="22"/>
-      <c r="L571" s="23"/>
-      <c r="M571" s="22"/>
+      <c r="G571" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H571" s="8" t="s">
+        <v>2136</v>
+      </c>
+      <c r="I571" s="9">
+        <v>44137.0</v>
+      </c>
+      <c r="J571" s="10">
+        <v>44114.0</v>
+      </c>
+      <c r="K571" s="13" t="s">
+        <v>2137</v>
+      </c>
+      <c r="L571" s="12" t="s">
+        <v>363</v>
+      </c>
+      <c r="M571" s="13" t="s">
+        <v>2138</v>
+      </c>
       <c r="N571" s="25"/>
-      <c r="O571" s="21"/>
-      <c r="P571" s="21"/>
+      <c r="O571" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P571" s="8" t="s">
+        <v>2139</v>
+      </c>
       <c r="Q571" s="19"/>
       <c r="R571" s="19"/>
-      <c r="S571" s="20"/>
+      <c r="S571" s="61" t="s">
+        <v>2140</v>
+      </c>
       <c r="T571" s="20"/>
       <c r="U571" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#570</v>
       </c>
     </row>
     <row r="572">
@@ -43166,15 +43217,16 @@
     <hyperlink r:id="rId130" ref="S568"/>
     <hyperlink r:id="rId131" ref="S569"/>
     <hyperlink r:id="rId132" ref="S570"/>
+    <hyperlink r:id="rId133" ref="S571"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId133"/>
-  <legacyDrawing r:id="rId134"/>
+  <drawing r:id="rId134"/>
+  <legacyDrawing r:id="rId135"/>
   <tableParts count="2">
-    <tablePart r:id="rId137"/>
     <tablePart r:id="rId138"/>
+    <tablePart r:id="rId139"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201107
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -563,7 +563,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6347" uniqueCount="2141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6396" uniqueCount="2153">
   <si>
     <t>案例</t>
   </si>
@@ -7853,6 +7853,43 @@
   </si>
   <si>
     <t>國內新增1例境外移入COVID-19病例，女自捷克返國後確診</t>
+  </si>
+  <si>
+    <t>#571</t>
+  </si>
+  <si>
+    <t>2X-4X</t>
+  </si>
+  <si>
+    <t>-10/22 印尼→台灣</t>
+  </si>
+  <si>
+    <t>11/4 採檢
+11/6 確診</t>
+  </si>
+  <si>
+    <t>今(2020)年10月22日搭乘同一班機來臺工作，入境迄今均無症狀，11月4日檢疫期滿前進行採檢，皆檢出陽性於今日確診，目前住院隔離中。由於3名個案來臺迄今均無症狀</t>
+  </si>
+  <si>
+    <t>國內新增4例境外移入COVID-19病例，分自印尼、墨西哥入境</t>
+  </si>
+  <si>
+    <t>#572</t>
+  </si>
+  <si>
+    <t>#573</t>
+  </si>
+  <si>
+    <t>#574</t>
+  </si>
+  <si>
+    <t>2月-11/4 墨西哥</t>
+  </si>
+  <si>
+    <t>流鼻水 鼻塞 頭暈 嗅覺異常 味覺異常</t>
+  </si>
+  <si>
+    <t>今年2月至墨西哥工作，曾於當地接觸確診個案</t>
   </si>
 </sst>
 </file>
@@ -41960,107 +41997,229 @@
       </c>
     </row>
     <row r="572">
-      <c r="A572" s="63"/>
-      <c r="B572" s="64"/>
-      <c r="C572" s="34"/>
-      <c r="D572" s="34"/>
-      <c r="E572" s="34"/>
+      <c r="A572" s="16" t="s">
+        <v>2141</v>
+      </c>
+      <c r="B572" s="6">
+        <v>44141.0</v>
+      </c>
+      <c r="C572" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D572" s="7" t="s">
+        <v>2142</v>
+      </c>
+      <c r="E572" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F572" s="34"/>
-      <c r="G572" s="34"/>
-      <c r="H572" s="21"/>
-      <c r="I572" s="19"/>
-      <c r="J572" s="10"/>
-      <c r="K572" s="22"/>
-      <c r="L572" s="23"/>
-      <c r="M572" s="22"/>
+      <c r="G572" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H572" s="8" t="s">
+        <v>2143</v>
+      </c>
+      <c r="I572" s="9">
+        <v>44126.0</v>
+      </c>
+      <c r="J572" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K572" s="13" t="s">
+        <v>2144</v>
+      </c>
+      <c r="L572" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M572" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N572" s="25"/>
-      <c r="O572" s="21"/>
-      <c r="P572" s="21"/>
+      <c r="O572" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P572" s="8" t="s">
+        <v>2145</v>
+      </c>
       <c r="Q572" s="19"/>
       <c r="R572" s="19"/>
-      <c r="S572" s="20"/>
+      <c r="S572" s="61" t="s">
+        <v>2146</v>
+      </c>
       <c r="T572" s="20"/>
       <c r="U572" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#571</v>
       </c>
     </row>
     <row r="573">
-      <c r="A573" s="63"/>
-      <c r="B573" s="64"/>
-      <c r="C573" s="34"/>
-      <c r="D573" s="34"/>
-      <c r="E573" s="34"/>
+      <c r="A573" s="16" t="s">
+        <v>2147</v>
+      </c>
+      <c r="B573" s="6">
+        <v>44141.0</v>
+      </c>
+      <c r="C573" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D573" s="7" t="s">
+        <v>2142</v>
+      </c>
+      <c r="E573" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F573" s="34"/>
-      <c r="G573" s="34"/>
-      <c r="H573" s="21"/>
-      <c r="I573" s="19"/>
-      <c r="J573" s="10"/>
-      <c r="K573" s="22"/>
-      <c r="L573" s="23"/>
-      <c r="M573" s="22"/>
+      <c r="G573" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H573" s="21" t="str">
+        <f t="shared" ref="H573:H574" si="71">$H$572</f>
+        <v>-10/22 印尼→台灣</v>
+      </c>
+      <c r="I573" s="9">
+        <v>44126.0</v>
+      </c>
+      <c r="J573" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K573" s="13" t="s">
+        <v>2144</v>
+      </c>
+      <c r="L573" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M573" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N573" s="25"/>
-      <c r="O573" s="21"/>
-      <c r="P573" s="21"/>
+      <c r="O573" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P573" s="8" t="s">
+        <v>2145</v>
+      </c>
       <c r="Q573" s="19"/>
       <c r="R573" s="19"/>
-      <c r="S573" s="20"/>
+      <c r="S573" s="61" t="s">
+        <v>2146</v>
+      </c>
       <c r="T573" s="20"/>
       <c r="U573" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#572</v>
       </c>
     </row>
     <row r="574">
-      <c r="A574" s="63"/>
-      <c r="B574" s="64"/>
-      <c r="C574" s="34"/>
-      <c r="D574" s="34"/>
-      <c r="E574" s="34"/>
+      <c r="A574" s="16" t="s">
+        <v>2148</v>
+      </c>
+      <c r="B574" s="6">
+        <v>44141.0</v>
+      </c>
+      <c r="C574" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D574" s="7" t="s">
+        <v>2142</v>
+      </c>
+      <c r="E574" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F574" s="34"/>
-      <c r="G574" s="34"/>
-      <c r="H574" s="21"/>
-      <c r="I574" s="19"/>
-      <c r="J574" s="10"/>
-      <c r="K574" s="22"/>
-      <c r="L574" s="23"/>
-      <c r="M574" s="22"/>
+      <c r="G574" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H574" s="21" t="str">
+        <f t="shared" si="71"/>
+        <v>-10/22 印尼→台灣</v>
+      </c>
+      <c r="I574" s="9">
+        <v>44126.0</v>
+      </c>
+      <c r="J574" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K574" s="13" t="s">
+        <v>2144</v>
+      </c>
+      <c r="L574" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M574" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N574" s="25"/>
-      <c r="O574" s="21"/>
-      <c r="P574" s="21"/>
+      <c r="O574" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P574" s="8" t="s">
+        <v>2145</v>
+      </c>
       <c r="Q574" s="19"/>
       <c r="R574" s="19"/>
-      <c r="S574" s="20"/>
+      <c r="S574" s="61" t="s">
+        <v>2146</v>
+      </c>
       <c r="T574" s="20"/>
       <c r="U574" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#573</v>
       </c>
     </row>
     <row r="575">
-      <c r="A575" s="63"/>
-      <c r="B575" s="64"/>
-      <c r="C575" s="34"/>
-      <c r="D575" s="34"/>
-      <c r="E575" s="34"/>
+      <c r="A575" s="16" t="s">
+        <v>2149</v>
+      </c>
+      <c r="B575" s="6">
+        <v>44141.0</v>
+      </c>
+      <c r="C575" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D575" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E575" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F575" s="34"/>
-      <c r="G575" s="34"/>
-      <c r="H575" s="21"/>
-      <c r="I575" s="19"/>
-      <c r="J575" s="10"/>
-      <c r="K575" s="22"/>
-      <c r="L575" s="23"/>
-      <c r="M575" s="22"/>
+      <c r="G575" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H575" s="8" t="s">
+        <v>2150</v>
+      </c>
+      <c r="I575" s="9">
+        <v>44139.0</v>
+      </c>
+      <c r="J575" s="10">
+        <v>44134.0</v>
+      </c>
+      <c r="K575" s="13" t="s">
+        <v>2144</v>
+      </c>
+      <c r="L575" s="12" t="s">
+        <v>363</v>
+      </c>
+      <c r="M575" s="13" t="s">
+        <v>2151</v>
+      </c>
       <c r="N575" s="25"/>
-      <c r="O575" s="21"/>
-      <c r="P575" s="21"/>
+      <c r="O575" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P575" s="8" t="s">
+        <v>2152</v>
+      </c>
       <c r="Q575" s="19"/>
       <c r="R575" s="19"/>
-      <c r="S575" s="20"/>
+      <c r="S575" s="61" t="s">
+        <v>2146</v>
+      </c>
       <c r="T575" s="20"/>
       <c r="U575" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#574</v>
       </c>
     </row>
     <row r="576">
@@ -43218,15 +43377,19 @@
     <hyperlink r:id="rId131" ref="S569"/>
     <hyperlink r:id="rId132" ref="S570"/>
     <hyperlink r:id="rId133" ref="S571"/>
+    <hyperlink r:id="rId134" ref="S572"/>
+    <hyperlink r:id="rId135" ref="S573"/>
+    <hyperlink r:id="rId136" ref="S574"/>
+    <hyperlink r:id="rId137" ref="S575"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId134"/>
-  <legacyDrawing r:id="rId135"/>
+  <drawing r:id="rId138"/>
+  <legacyDrawing r:id="rId139"/>
   <tableParts count="2">
-    <tablePart r:id="rId138"/>
-    <tablePart r:id="rId139"/>
+    <tablePart r:id="rId142"/>
+    <tablePart r:id="rId143"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201109
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -563,7 +563,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6396" uniqueCount="2153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6448" uniqueCount="2168">
   <si>
     <t>案例</t>
   </si>
@@ -7890,6 +7890,56 @@
   </si>
   <si>
     <t>今年2月至墨西哥工作，曾於當地接觸確診個案</t>
+  </si>
+  <si>
+    <t>#575</t>
+  </si>
+  <si>
+    <t>3X-4X</t>
+  </si>
+  <si>
+    <t>-10/24 印尼→台灣</t>
+  </si>
+  <si>
+    <t>11/6 採檢
+11/8 確診</t>
+  </si>
+  <si>
+    <t>#575 #576 同班機
+10月24日搭乘同一班機來臺工作，11月6日檢疫期滿前進行採檢，皆檢出陽性並於今日確診</t>
+  </si>
+  <si>
+    <t>國內新增4例境外移入COVID-19病例，分別自印尼及菲律賓入境</t>
+  </si>
+  <si>
+    <t>#576</t>
+  </si>
+  <si>
+    <t>#577</t>
+  </si>
+  <si>
+    <t>-10/16 菲律賓→台灣</t>
+  </si>
+  <si>
+    <t>10/29 採檢
+11/5 二採
+11/8 確診</t>
+  </si>
+  <si>
+    <t>10月16日來臺工作，入境迄今無症狀，10月29日檢疫期滿前採檢結果為陰性。個案於10月31日檢疫期滿後，至防疫旅館進行自主健康管理，並由仲介安排於11月5日至醫院自費採檢</t>
+  </si>
+  <si>
+    <t>#578</t>
+  </si>
+  <si>
+    <t>-10/25 菲律賓→台灣</t>
+  </si>
+  <si>
+    <t>11/7 採檢
+11/8 確診</t>
+  </si>
+  <si>
+    <t>10月25日來臺就學，入境迄今無症狀，11月7日進行檢疫期滿前採檢，於今日確診，目前住院隔離中</t>
   </si>
 </sst>
 </file>
@@ -8222,7 +8272,7 @@
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
-  <dxfs count="67">
+  <dxfs count="73">
     <dxf>
       <font>
         <color rgb="FF0000FF"/>
@@ -8935,6 +8985,78 @@
       <border/>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFBF9000"/>
+          <bgColor rgb="FFBF9000"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF38761D"/>
+          <bgColor rgb="FF38761D"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF134F5C"/>
+          <bgColor rgb="FF134F5C"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF1155CC"/>
+          <bgColor rgb="FF1155CC"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF0B5394"/>
+          <bgColor rgb="FF0B5394"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF351C75"/>
+          <bgColor rgb="FF351C75"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
       <font/>
       <fill>
         <patternFill patternType="none"/>
@@ -8974,14 +9096,14 @@
   </dxfs>
   <tableStyles count="2">
     <tableStyle count="3" pivot="0" name="臺灣武漢肺炎病例-style">
-      <tableStyleElement dxfId="64" type="headerRow"/>
-      <tableStyleElement dxfId="65" type="firstRowStripe"/>
-      <tableStyleElement dxfId="66" type="secondRowStripe"/>
+      <tableStyleElement dxfId="70" type="headerRow"/>
+      <tableStyleElement dxfId="71" type="firstRowStripe"/>
+      <tableStyleElement dxfId="72" type="secondRowStripe"/>
     </tableStyle>
     <tableStyle count="3" pivot="0" name="臺灣武漢肺炎病例-style 2">
-      <tableStyleElement dxfId="64" type="headerRow"/>
-      <tableStyleElement dxfId="65" type="firstRowStripe"/>
-      <tableStyleElement dxfId="66" type="secondRowStripe"/>
+      <tableStyleElement dxfId="70" type="headerRow"/>
+      <tableStyleElement dxfId="71" type="firstRowStripe"/>
+      <tableStyleElement dxfId="72" type="secondRowStripe"/>
     </tableStyle>
   </tableStyles>
 </styleSheet>
@@ -42223,107 +42345,227 @@
       </c>
     </row>
     <row r="576">
-      <c r="A576" s="63"/>
-      <c r="B576" s="64"/>
-      <c r="C576" s="34"/>
-      <c r="D576" s="34"/>
-      <c r="E576" s="34"/>
+      <c r="A576" s="16" t="s">
+        <v>2153</v>
+      </c>
+      <c r="B576" s="6">
+        <v>44143.0</v>
+      </c>
+      <c r="C576" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D576" s="7" t="s">
+        <v>2154</v>
+      </c>
+      <c r="E576" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F576" s="34"/>
-      <c r="G576" s="34"/>
-      <c r="H576" s="21"/>
-      <c r="I576" s="19"/>
-      <c r="J576" s="10"/>
-      <c r="K576" s="22"/>
-      <c r="L576" s="23"/>
-      <c r="M576" s="22"/>
+      <c r="G576" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H576" s="8" t="s">
+        <v>2155</v>
+      </c>
+      <c r="I576" s="9">
+        <v>44128.0</v>
+      </c>
+      <c r="J576" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K576" s="13" t="s">
+        <v>2156</v>
+      </c>
+      <c r="L576" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M576" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N576" s="25"/>
-      <c r="O576" s="21"/>
-      <c r="P576" s="21"/>
+      <c r="O576" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P576" s="8" t="s">
+        <v>2157</v>
+      </c>
       <c r="Q576" s="19"/>
       <c r="R576" s="19"/>
-      <c r="S576" s="20"/>
+      <c r="S576" s="61" t="s">
+        <v>2158</v>
+      </c>
       <c r="T576" s="20"/>
       <c r="U576" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#575</v>
       </c>
     </row>
     <row r="577">
-      <c r="A577" s="63"/>
-      <c r="B577" s="64"/>
-      <c r="C577" s="34"/>
-      <c r="D577" s="34"/>
-      <c r="E577" s="34"/>
+      <c r="A577" s="16" t="s">
+        <v>2159</v>
+      </c>
+      <c r="B577" s="6">
+        <v>44143.0</v>
+      </c>
+      <c r="C577" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D577" s="7" t="s">
+        <v>2154</v>
+      </c>
+      <c r="E577" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F577" s="34"/>
-      <c r="G577" s="34"/>
-      <c r="H577" s="21"/>
-      <c r="I577" s="19"/>
-      <c r="J577" s="10"/>
-      <c r="K577" s="22"/>
-      <c r="L577" s="23"/>
-      <c r="M577" s="22"/>
+      <c r="G577" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H577" s="8" t="s">
+        <v>2155</v>
+      </c>
+      <c r="I577" s="9">
+        <v>44128.0</v>
+      </c>
+      <c r="J577" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K577" s="13" t="s">
+        <v>2156</v>
+      </c>
+      <c r="L577" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M577" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N577" s="25"/>
-      <c r="O577" s="21"/>
-      <c r="P577" s="21"/>
+      <c r="O577" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P577" s="8" t="s">
+        <v>2157</v>
+      </c>
       <c r="Q577" s="19"/>
       <c r="R577" s="19"/>
-      <c r="S577" s="20"/>
+      <c r="S577" s="61" t="s">
+        <v>2158</v>
+      </c>
       <c r="T577" s="20"/>
       <c r="U577" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#576</v>
       </c>
     </row>
     <row r="578">
-      <c r="A578" s="63"/>
-      <c r="B578" s="64"/>
-      <c r="C578" s="34"/>
-      <c r="D578" s="34"/>
-      <c r="E578" s="34"/>
+      <c r="A578" s="16" t="s">
+        <v>2160</v>
+      </c>
+      <c r="B578" s="6">
+        <v>44143.0</v>
+      </c>
+      <c r="C578" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D578" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E578" s="7" t="s">
+        <v>205</v>
+      </c>
       <c r="F578" s="34"/>
-      <c r="G578" s="34"/>
-      <c r="H578" s="21"/>
-      <c r="I578" s="19"/>
-      <c r="J578" s="10"/>
-      <c r="K578" s="22"/>
-      <c r="L578" s="23"/>
-      <c r="M578" s="22"/>
+      <c r="G578" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H578" s="8" t="s">
+        <v>2161</v>
+      </c>
+      <c r="I578" s="9">
+        <v>44120.0</v>
+      </c>
+      <c r="J578" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K578" s="13" t="s">
+        <v>2162</v>
+      </c>
+      <c r="L578" s="12" t="s">
+        <v>1674</v>
+      </c>
+      <c r="M578" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N578" s="25"/>
-      <c r="O578" s="21"/>
-      <c r="P578" s="21"/>
+      <c r="O578" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P578" s="8" t="s">
+        <v>2163</v>
+      </c>
       <c r="Q578" s="19"/>
       <c r="R578" s="19"/>
-      <c r="S578" s="20"/>
+      <c r="S578" s="61" t="s">
+        <v>2158</v>
+      </c>
       <c r="T578" s="20"/>
       <c r="U578" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#577</v>
       </c>
     </row>
     <row r="579">
-      <c r="A579" s="63"/>
-      <c r="B579" s="64"/>
-      <c r="C579" s="34"/>
-      <c r="D579" s="34"/>
-      <c r="E579" s="34"/>
+      <c r="A579" s="16" t="s">
+        <v>2164</v>
+      </c>
+      <c r="B579" s="6">
+        <v>44143.0</v>
+      </c>
+      <c r="C579" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D579" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="E579" s="7" t="s">
+        <v>205</v>
+      </c>
       <c r="F579" s="34"/>
-      <c r="G579" s="34"/>
-      <c r="H579" s="21"/>
-      <c r="I579" s="19"/>
-      <c r="J579" s="10"/>
-      <c r="K579" s="22"/>
-      <c r="L579" s="23"/>
-      <c r="M579" s="22"/>
+      <c r="G579" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H579" s="8" t="s">
+        <v>2165</v>
+      </c>
+      <c r="I579" s="9">
+        <v>44129.0</v>
+      </c>
+      <c r="J579" s="12" t="s">
+        <v>1672</v>
+      </c>
+      <c r="K579" s="13" t="s">
+        <v>2166</v>
+      </c>
+      <c r="L579" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M579" s="13" t="s">
+        <v>1672</v>
+      </c>
       <c r="N579" s="25"/>
-      <c r="O579" s="21"/>
-      <c r="P579" s="21"/>
+      <c r="O579" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P579" s="8" t="s">
+        <v>2167</v>
+      </c>
       <c r="Q579" s="19"/>
       <c r="R579" s="19"/>
-      <c r="S579" s="20"/>
+      <c r="S579" s="61" t="s">
+        <v>2158</v>
+      </c>
       <c r="T579" s="20"/>
       <c r="U579" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#578</v>
       </c>
     </row>
     <row r="580">
@@ -43244,6 +43486,41 @@
       <formula>B357&lt;44143.0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B357:B601">
+    <cfRule type="expression" dxfId="63" priority="70">
+      <formula>B357&lt;44150.0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B357:B601">
+    <cfRule type="expression" dxfId="64" priority="71">
+      <formula>B357&lt;44157.0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B357:B601">
+    <cfRule type="expression" dxfId="65" priority="72">
+      <formula>B357&lt;44164.0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B357:B601">
+    <cfRule type="expression" dxfId="66" priority="73">
+      <formula>B357&lt;44171.0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B357:B601">
+    <cfRule type="expression" dxfId="67" priority="74">
+      <formula>B357&lt;44178.0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B357:B601">
+    <cfRule type="expression" dxfId="68" priority="75">
+      <formula>B357&lt;44185.0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B357:B601">
+    <cfRule type="expression" dxfId="68" priority="76">
+      <formula>B357&lt;44192.0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink r:id="rId2" ref="S440"/>
     <hyperlink r:id="rId3" ref="S441"/>
@@ -43381,15 +43658,19 @@
     <hyperlink r:id="rId135" ref="S573"/>
     <hyperlink r:id="rId136" ref="S574"/>
     <hyperlink r:id="rId137" ref="S575"/>
+    <hyperlink r:id="rId138" ref="S576"/>
+    <hyperlink r:id="rId139" ref="S577"/>
+    <hyperlink r:id="rId140" ref="S578"/>
+    <hyperlink r:id="rId141" ref="S579"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId138"/>
-  <legacyDrawing r:id="rId139"/>
+  <drawing r:id="rId142"/>
+  <legacyDrawing r:id="rId143"/>
   <tableParts count="2">
-    <tablePart r:id="rId142"/>
-    <tablePart r:id="rId143"/>
+    <tablePart r:id="rId146"/>
+    <tablePart r:id="rId147"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201110
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -558,12 +558,20 @@
         <t xml:space="preserve">https://udn.com/news/story/120940/4748132</t>
       </text>
     </comment>
+    <comment authorId="0" ref="S531">
+      <text>
+        <t xml:space="preserve">中央流行疫情指揮中心今(13)日公布國內新增1例境外移入COVID-19(武漢肺炎)病例，為本國籍40多歲男性(案530)，今(2020)年2月至中國江蘇工作，10月11日返台。
+指揮中心表示，個案返台前，曾於10月1日出現流鼻水及有痰等症狀，僅自行買藥服用，未在當地就醫，其辦公室有另2名同事有感冒症狀，亦自行服藥未就醫。個案10月11日返台休假，因入境時有咳嗽、流鼻水及鼻塞等症狀，於機場進行採檢，並於今日確診，目前住院隔離治療。
+指揮中心指出，衛生單位已掌握個案同班機接觸者共17人，其中10人為前後二排座位旅客，列為居家隔離對象，7人為機組員，未入境。
+指揮中心統計，國內截至目前累計97,166例新型冠狀病毒肺炎相關通報(含96,055例排除)，其中530例確診，分別為438例境外移入、55例本土病例、36例敦睦艦隊及1例不明。確診個案中7人死亡、489人解除隔離、34人住院隔離中。 </t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6448" uniqueCount="2168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6451" uniqueCount="2171">
   <si>
     <t>案例</t>
   </si>
@@ -7243,18 +7251,7 @@
     <t>#530</t>
   </si>
   <si>
-    <t>2月-10/11 中國江蘇</t>
-  </si>
-  <si>
-    <t>10/11 採檢
-10/13 確診</t>
-  </si>
-  <si>
-    <t>咳嗽 流鼻水 鼻塞 有痰</t>
-  </si>
-  <si>
-    <t>10月1日出現流鼻水及有痰等症狀，僅自行買藥服用，
-未在當地就醫</t>
+    <t>*(10/28)檢體錯位，紀錄為空號</t>
   </si>
   <si>
     <t>男赴中國江蘇工作，返國入境檢驗確診COVID-19</t>
@@ -7940,6 +7937,25 @@
   </si>
   <si>
     <t>10月25日來臺就學，入境迄今無症狀，11月7日進行檢疫期滿前採檢，於今日確診，目前住院隔離中</t>
+  </si>
+  <si>
+    <t>#579</t>
+  </si>
+  <si>
+    <t>-11/3 烏克蘭→台灣</t>
+  </si>
+  <si>
+    <t>11/6 採檢
+11/9 確診</t>
+  </si>
+  <si>
+    <t>鼻塞 嗅覺異常 味覺異常</t>
+  </si>
+  <si>
+    <t>來臺工作，搭機前3日內檢驗陰性，入境時無上呼吸道症狀</t>
+  </si>
+  <si>
+    <t>國內新增1例境外移入COVID-19病例，烏克蘭籍女子來臺工作確診</t>
   </si>
 </sst>
 </file>
@@ -7950,7 +7966,7 @@
     <numFmt numFmtId="164" formatCode="mm&quot;月&quot;dd&quot;日 &quot;dddd"/>
     <numFmt numFmtId="165" formatCode="m/d"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -8027,6 +8043,10 @@
       <u/>
       <color rgb="FF1155CC"/>
     </font>
+    <font>
+      <u/>
+      <color rgb="FFFFFFFF"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -8072,7 +8092,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="75">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -8261,6 +8281,36 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
@@ -39819,64 +39869,40 @@
       </c>
     </row>
     <row r="531">
-      <c r="A531" s="16" t="s">
+      <c r="A531" s="63" t="s">
         <v>1963</v>
       </c>
-      <c r="B531" s="6">
-        <v>44117.0</v>
-      </c>
-      <c r="C531" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D531" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E531" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F531" s="34"/>
-      <c r="G531" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H531" s="8" t="s">
+      <c r="B531" s="64"/>
+      <c r="C531" s="65"/>
+      <c r="D531" s="65"/>
+      <c r="E531" s="65"/>
+      <c r="F531" s="66"/>
+      <c r="G531" s="65"/>
+      <c r="H531" s="67"/>
+      <c r="I531" s="24"/>
+      <c r="J531" s="24"/>
+      <c r="K531" s="67"/>
+      <c r="L531" s="63"/>
+      <c r="M531" s="67"/>
+      <c r="N531" s="68"/>
+      <c r="O531" s="67"/>
+      <c r="P531" s="67" t="s">
         <v>1964</v>
       </c>
-      <c r="I531" s="9">
-        <v>44115.0</v>
-      </c>
-      <c r="J531" s="10">
-        <v>44105.0</v>
-      </c>
-      <c r="K531" s="13" t="s">
+      <c r="Q531" s="69"/>
+      <c r="R531" s="69"/>
+      <c r="S531" s="70" t="s">
         <v>1965</v>
       </c>
-      <c r="L531" s="12" t="s">
-        <v>363</v>
-      </c>
-      <c r="M531" s="13" t="s">
-        <v>1966</v>
-      </c>
-      <c r="N531" s="25"/>
-      <c r="O531" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="P531" s="8" t="s">
-        <v>1967</v>
-      </c>
-      <c r="Q531" s="19"/>
-      <c r="R531" s="19"/>
-      <c r="S531" s="61" t="s">
-        <v>1968</v>
-      </c>
-      <c r="T531" s="20"/>
-      <c r="U531" s="18" t="str">
+      <c r="T531" s="71"/>
+      <c r="U531" s="72" t="str">
         <f t="shared" si="1"/>
         <v>#530</v>
       </c>
     </row>
     <row r="532">
       <c r="A532" s="16" t="s">
-        <v>1969</v>
+        <v>1966</v>
       </c>
       <c r="B532" s="6">
         <v>44119.0</v>
@@ -39904,7 +39930,7 @@
         <v>1442</v>
       </c>
       <c r="K532" s="13" t="s">
-        <v>1970</v>
+        <v>1967</v>
       </c>
       <c r="L532" s="12" t="s">
         <v>1674</v>
@@ -39917,12 +39943,12 @@
         <v>85</v>
       </c>
       <c r="P532" s="8" t="s">
-        <v>1971</v>
+        <v>1968</v>
       </c>
       <c r="Q532" s="19"/>
       <c r="R532" s="19"/>
       <c r="S532" s="61" t="s">
-        <v>1972</v>
+        <v>1969</v>
       </c>
       <c r="T532" s="20"/>
       <c r="U532" s="18" t="str">
@@ -39932,14 +39958,14 @@
     </row>
     <row r="533">
       <c r="A533" s="16" t="s">
-        <v>1973</v>
+        <v>1970</v>
       </c>
       <c r="B533" s="6">
         <v>44120.0</v>
       </c>
       <c r="C533" s="34"/>
       <c r="D533" s="7" t="s">
-        <v>1974</v>
+        <v>1971</v>
       </c>
       <c r="E533" s="7" t="s">
         <v>158</v>
@@ -39949,7 +39975,7 @@
         <v>25</v>
       </c>
       <c r="H533" s="8" t="s">
-        <v>1975</v>
+        <v>1972</v>
       </c>
       <c r="I533" s="9">
         <v>44104.0</v>
@@ -39958,7 +39984,7 @@
         <v>1442</v>
       </c>
       <c r="K533" s="13" t="s">
-        <v>1976</v>
+        <v>1973</v>
       </c>
       <c r="L533" s="12" t="s">
         <v>426</v>
@@ -39971,12 +39997,12 @@
         <v>85</v>
       </c>
       <c r="P533" s="8" t="s">
-        <v>1977</v>
+        <v>1974</v>
       </c>
       <c r="Q533" s="19"/>
       <c r="R533" s="19"/>
       <c r="S533" s="61" t="s">
-        <v>1978</v>
+        <v>1975</v>
       </c>
       <c r="T533" s="20"/>
       <c r="U533" s="18" t="str">
@@ -39986,14 +40012,14 @@
     </row>
     <row r="534">
       <c r="A534" s="16" t="s">
-        <v>1979</v>
+        <v>1976</v>
       </c>
       <c r="B534" s="6">
         <v>44120.0</v>
       </c>
       <c r="C534" s="34"/>
       <c r="D534" s="7" t="s">
-        <v>1974</v>
+        <v>1971</v>
       </c>
       <c r="E534" s="7" t="s">
         <v>158</v>
@@ -40036,7 +40062,7 @@
       <c r="Q534" s="19"/>
       <c r="R534" s="19"/>
       <c r="S534" s="61" t="s">
-        <v>1978</v>
+        <v>1975</v>
       </c>
       <c r="T534" s="20"/>
       <c r="U534" s="18" t="str">
@@ -40046,14 +40072,14 @@
     </row>
     <row r="535">
       <c r="A535" s="16" t="s">
-        <v>1980</v>
+        <v>1977</v>
       </c>
       <c r="B535" s="6">
         <v>44120.0</v>
       </c>
       <c r="C535" s="34"/>
       <c r="D535" s="7" t="s">
-        <v>1974</v>
+        <v>1971</v>
       </c>
       <c r="E535" s="7" t="s">
         <v>158</v>
@@ -40096,7 +40122,7 @@
       <c r="Q535" s="19"/>
       <c r="R535" s="19"/>
       <c r="S535" s="61" t="s">
-        <v>1978</v>
+        <v>1975</v>
       </c>
       <c r="T535" s="20"/>
       <c r="U535" s="18" t="str">
@@ -40106,14 +40132,14 @@
     </row>
     <row r="536">
       <c r="A536" s="16" t="s">
-        <v>1981</v>
+        <v>1978</v>
       </c>
       <c r="B536" s="6">
         <v>44120.0</v>
       </c>
       <c r="C536" s="34"/>
       <c r="D536" s="7" t="s">
-        <v>1974</v>
+        <v>1971</v>
       </c>
       <c r="E536" s="7" t="s">
         <v>158</v>
@@ -40156,7 +40182,7 @@
       <c r="Q536" s="19"/>
       <c r="R536" s="19"/>
       <c r="S536" s="61" t="s">
-        <v>1978</v>
+        <v>1975</v>
       </c>
       <c r="T536" s="20"/>
       <c r="U536" s="18" t="str">
@@ -40166,7 +40192,7 @@
     </row>
     <row r="537">
       <c r="A537" s="16" t="s">
-        <v>1982</v>
+        <v>1979</v>
       </c>
       <c r="B537" s="6">
         <v>44123.0</v>
@@ -40185,7 +40211,7 @@
         <v>25</v>
       </c>
       <c r="H537" s="8" t="s">
-        <v>1983</v>
+        <v>1980</v>
       </c>
       <c r="I537" s="9">
         <v>44115.0</v>
@@ -40194,25 +40220,25 @@
         <v>44113.0</v>
       </c>
       <c r="K537" s="13" t="s">
-        <v>1984</v>
+        <v>1981</v>
       </c>
       <c r="L537" s="12" t="s">
         <v>426</v>
       </c>
       <c r="M537" s="13" t="s">
-        <v>1985</v>
+        <v>1982</v>
       </c>
       <c r="N537" s="25"/>
       <c r="O537" s="8" t="s">
         <v>85</v>
       </c>
       <c r="P537" s="8" t="s">
-        <v>1986</v>
+        <v>1983</v>
       </c>
       <c r="Q537" s="19"/>
       <c r="R537" s="19"/>
       <c r="S537" s="61" t="s">
-        <v>1987</v>
+        <v>1984</v>
       </c>
       <c r="T537" s="20"/>
       <c r="U537" s="18" t="str">
@@ -40222,7 +40248,7 @@
     </row>
     <row r="538">
       <c r="A538" s="16" t="s">
-        <v>1988</v>
+        <v>1985</v>
       </c>
       <c r="B538" s="6">
         <v>44123.0</v>
@@ -40241,7 +40267,7 @@
         <v>25</v>
       </c>
       <c r="H538" s="8" t="s">
-        <v>1989</v>
+        <v>1986</v>
       </c>
       <c r="I538" s="9">
         <v>44108.0</v>
@@ -40250,7 +40276,7 @@
         <v>1442</v>
       </c>
       <c r="K538" s="13" t="s">
-        <v>1990</v>
+        <v>1987</v>
       </c>
       <c r="L538" s="12" t="s">
         <v>426</v>
@@ -40263,12 +40289,12 @@
         <v>85</v>
       </c>
       <c r="P538" s="8" t="s">
-        <v>1991</v>
+        <v>1988</v>
       </c>
       <c r="Q538" s="19"/>
       <c r="R538" s="19"/>
       <c r="S538" s="61" t="s">
-        <v>1987</v>
+        <v>1984</v>
       </c>
       <c r="T538" s="20"/>
       <c r="U538" s="18" t="str">
@@ -40278,7 +40304,7 @@
     </row>
     <row r="539">
       <c r="A539" s="16" t="s">
-        <v>1992</v>
+        <v>1989</v>
       </c>
       <c r="B539" s="6">
         <v>44123.0</v>
@@ -40297,7 +40323,7 @@
         <v>25</v>
       </c>
       <c r="H539" s="8" t="s">
-        <v>1993</v>
+        <v>1990</v>
       </c>
       <c r="I539" s="9">
         <v>44108.0</v>
@@ -40306,7 +40332,7 @@
         <v>1442</v>
       </c>
       <c r="K539" s="13" t="s">
-        <v>1990</v>
+        <v>1987</v>
       </c>
       <c r="L539" s="12" t="s">
         <v>426</v>
@@ -40319,12 +40345,12 @@
         <v>85</v>
       </c>
       <c r="P539" s="8" t="s">
-        <v>1994</v>
+        <v>1991</v>
       </c>
       <c r="Q539" s="19"/>
       <c r="R539" s="19"/>
       <c r="S539" s="61" t="s">
-        <v>1987</v>
+        <v>1984</v>
       </c>
       <c r="T539" s="20"/>
       <c r="U539" s="18" t="str">
@@ -40334,7 +40360,7 @@
     </row>
     <row r="540">
       <c r="A540" s="16" t="s">
-        <v>1995</v>
+        <v>1992</v>
       </c>
       <c r="B540" s="6">
         <v>44123.0</v>
@@ -40353,7 +40379,7 @@
         <v>25</v>
       </c>
       <c r="H540" s="8" t="s">
-        <v>1996</v>
+        <v>1993</v>
       </c>
       <c r="I540" s="9">
         <v>44107.0</v>
@@ -40362,7 +40388,7 @@
         <v>1442</v>
       </c>
       <c r="K540" s="13" t="s">
-        <v>1997</v>
+        <v>1994</v>
       </c>
       <c r="L540" s="12" t="s">
         <v>426</v>
@@ -40375,12 +40401,12 @@
         <v>85</v>
       </c>
       <c r="P540" s="8" t="s">
-        <v>1998</v>
+        <v>1995</v>
       </c>
       <c r="Q540" s="19"/>
       <c r="R540" s="19"/>
       <c r="S540" s="61" t="s">
-        <v>1987</v>
+        <v>1984</v>
       </c>
       <c r="T540" s="20"/>
       <c r="U540" s="18" t="str">
@@ -40390,7 +40416,7 @@
     </row>
     <row r="541">
       <c r="A541" s="16" t="s">
-        <v>1999</v>
+        <v>1996</v>
       </c>
       <c r="B541" s="6">
         <v>44123.0</v>
@@ -40402,14 +40428,14 @@
         <v>267</v>
       </c>
       <c r="E541" s="7" t="s">
-        <v>2000</v>
+        <v>1997</v>
       </c>
       <c r="F541" s="34"/>
       <c r="G541" s="7" t="s">
         <v>25</v>
       </c>
       <c r="H541" s="8" t="s">
-        <v>2001</v>
+        <v>1998</v>
       </c>
       <c r="I541" s="9">
         <v>44113.0</v>
@@ -40418,25 +40444,25 @@
         <v>44120.0</v>
       </c>
       <c r="K541" s="13" t="s">
-        <v>2002</v>
+        <v>1999</v>
       </c>
       <c r="L541" s="12" t="s">
         <v>426</v>
       </c>
       <c r="M541" s="13" t="s">
-        <v>2003</v>
+        <v>2000</v>
       </c>
       <c r="N541" s="25"/>
       <c r="O541" s="8" t="s">
         <v>85</v>
       </c>
       <c r="P541" s="8" t="s">
-        <v>2004</v>
+        <v>2001</v>
       </c>
       <c r="Q541" s="19"/>
       <c r="R541" s="19"/>
       <c r="S541" s="61" t="s">
-        <v>1987</v>
+        <v>1984</v>
       </c>
       <c r="T541" s="20"/>
       <c r="U541" s="18" t="str">
@@ -40446,7 +40472,7 @@
     </row>
     <row r="542">
       <c r="A542" s="16" t="s">
-        <v>2005</v>
+        <v>2002</v>
       </c>
       <c r="B542" s="6">
         <v>44124.0</v>
@@ -40465,7 +40491,7 @@
         <v>25</v>
       </c>
       <c r="H542" s="8" t="s">
-        <v>2006</v>
+        <v>2003</v>
       </c>
       <c r="I542" s="9">
         <v>44109.0</v>
@@ -40474,7 +40500,7 @@
         <v>1442</v>
       </c>
       <c r="K542" s="13" t="s">
-        <v>2007</v>
+        <v>2004</v>
       </c>
       <c r="L542" s="12" t="s">
         <v>426</v>
@@ -40487,12 +40513,12 @@
         <v>85</v>
       </c>
       <c r="P542" s="8" t="s">
-        <v>2008</v>
+        <v>2005</v>
       </c>
       <c r="Q542" s="19"/>
       <c r="R542" s="19"/>
       <c r="S542" s="61" t="s">
-        <v>2009</v>
+        <v>2006</v>
       </c>
       <c r="T542" s="20"/>
       <c r="U542" s="18" t="str">
@@ -40502,7 +40528,7 @@
     </row>
     <row r="543">
       <c r="A543" s="16" t="s">
-        <v>2010</v>
+        <v>2007</v>
       </c>
       <c r="B543" s="6">
         <v>44124.0</v>
@@ -40521,7 +40547,7 @@
         <v>25</v>
       </c>
       <c r="H543" s="8" t="s">
-        <v>2006</v>
+        <v>2003</v>
       </c>
       <c r="I543" s="9">
         <v>44109.0</v>
@@ -40530,7 +40556,7 @@
         <v>1442</v>
       </c>
       <c r="K543" s="13" t="s">
-        <v>2007</v>
+        <v>2004</v>
       </c>
       <c r="L543" s="12" t="s">
         <v>426</v>
@@ -40543,12 +40569,12 @@
         <v>85</v>
       </c>
       <c r="P543" s="8" t="s">
-        <v>2008</v>
+        <v>2005</v>
       </c>
       <c r="Q543" s="19"/>
       <c r="R543" s="19"/>
       <c r="S543" s="61" t="s">
-        <v>2009</v>
+        <v>2006</v>
       </c>
       <c r="T543" s="20"/>
       <c r="U543" s="18" t="str">
@@ -40558,7 +40584,7 @@
     </row>
     <row r="544">
       <c r="A544" s="16" t="s">
-        <v>2011</v>
+        <v>2008</v>
       </c>
       <c r="B544" s="6">
         <v>44124.0</v>
@@ -40577,7 +40603,7 @@
         <v>25</v>
       </c>
       <c r="H544" s="8" t="s">
-        <v>2012</v>
+        <v>2009</v>
       </c>
       <c r="I544" s="9">
         <v>44109.0</v>
@@ -40586,25 +40612,25 @@
         <v>44109.0</v>
       </c>
       <c r="K544" s="13" t="s">
-        <v>2013</v>
+        <v>2010</v>
       </c>
       <c r="L544" s="12" t="s">
         <v>363</v>
       </c>
       <c r="M544" s="13" t="s">
-        <v>2014</v>
+        <v>2011</v>
       </c>
       <c r="N544" s="25"/>
       <c r="O544" s="8" t="s">
         <v>85</v>
       </c>
       <c r="P544" s="8" t="s">
-        <v>2015</v>
+        <v>2012</v>
       </c>
       <c r="Q544" s="19"/>
       <c r="R544" s="19"/>
       <c r="S544" s="61" t="s">
-        <v>2009</v>
+        <v>2006</v>
       </c>
       <c r="T544" s="20"/>
       <c r="U544" s="18" t="str">
@@ -40614,7 +40640,7 @@
     </row>
     <row r="545">
       <c r="A545" s="16" t="s">
-        <v>2016</v>
+        <v>2013</v>
       </c>
       <c r="B545" s="6">
         <v>44125.0</v>
@@ -40633,7 +40659,7 @@
         <v>25</v>
       </c>
       <c r="H545" s="8" t="s">
-        <v>2017</v>
+        <v>2014</v>
       </c>
       <c r="I545" s="9">
         <v>44109.0</v>
@@ -40642,7 +40668,7 @@
         <v>44112.0</v>
       </c>
       <c r="K545" s="13" t="s">
-        <v>2018</v>
+        <v>2015</v>
       </c>
       <c r="L545" s="12" t="s">
         <v>1674</v>
@@ -40655,12 +40681,12 @@
         <v>85</v>
       </c>
       <c r="P545" s="8" t="s">
-        <v>2019</v>
+        <v>2016</v>
       </c>
       <c r="Q545" s="19"/>
       <c r="R545" s="19"/>
       <c r="S545" s="61" t="s">
-        <v>2020</v>
+        <v>2017</v>
       </c>
       <c r="T545" s="20"/>
       <c r="U545" s="18" t="str">
@@ -40670,7 +40696,7 @@
     </row>
     <row r="546">
       <c r="A546" s="16" t="s">
-        <v>2021</v>
+        <v>2018</v>
       </c>
       <c r="B546" s="6">
         <v>44126.0</v>
@@ -40689,7 +40715,7 @@
         <v>25</v>
       </c>
       <c r="H546" s="8" t="s">
-        <v>2022</v>
+        <v>2019</v>
       </c>
       <c r="I546" s="9">
         <v>44118.0</v>
@@ -40698,25 +40724,25 @@
         <v>44121.0</v>
       </c>
       <c r="K546" s="13" t="s">
-        <v>2023</v>
+        <v>2020</v>
       </c>
       <c r="L546" s="12" t="s">
         <v>426</v>
       </c>
       <c r="M546" s="13" t="s">
-        <v>2024</v>
+        <v>2021</v>
       </c>
       <c r="N546" s="25"/>
       <c r="O546" s="8" t="s">
         <v>85</v>
       </c>
       <c r="P546" s="8" t="s">
-        <v>2025</v>
+        <v>2022</v>
       </c>
       <c r="Q546" s="19"/>
       <c r="R546" s="19"/>
       <c r="S546" s="61" t="s">
-        <v>2026</v>
+        <v>2023</v>
       </c>
       <c r="T546" s="20"/>
       <c r="U546" s="18" t="str">
@@ -40726,7 +40752,7 @@
     </row>
     <row r="547">
       <c r="A547" s="16" t="s">
-        <v>2027</v>
+        <v>2024</v>
       </c>
       <c r="B547" s="6">
         <v>44126.0</v>
@@ -40745,7 +40771,7 @@
         <v>25</v>
       </c>
       <c r="H547" s="8" t="s">
-        <v>2028</v>
+        <v>2025</v>
       </c>
       <c r="I547" s="9">
         <v>44124.0</v>
@@ -40754,25 +40780,25 @@
         <v>44117.0</v>
       </c>
       <c r="K547" s="13" t="s">
-        <v>2029</v>
+        <v>2026</v>
       </c>
       <c r="L547" s="12" t="s">
         <v>363</v>
       </c>
       <c r="M547" s="13" t="s">
-        <v>2030</v>
+        <v>2027</v>
       </c>
       <c r="N547" s="25"/>
       <c r="O547" s="8" t="s">
         <v>85</v>
       </c>
       <c r="P547" s="8" t="s">
-        <v>2031</v>
+        <v>2028</v>
       </c>
       <c r="Q547" s="19"/>
       <c r="R547" s="19"/>
       <c r="S547" s="61" t="s">
-        <v>2026</v>
+        <v>2023</v>
       </c>
       <c r="T547" s="20"/>
       <c r="U547" s="18" t="str">
@@ -40782,7 +40808,7 @@
     </row>
     <row r="548">
       <c r="A548" s="16" t="s">
-        <v>2032</v>
+        <v>2029</v>
       </c>
       <c r="B548" s="6">
         <v>44126.0</v>
@@ -40801,7 +40827,7 @@
         <v>25</v>
       </c>
       <c r="H548" s="8" t="s">
-        <v>2033</v>
+        <v>2030</v>
       </c>
       <c r="I548" s="9">
         <v>44112.0</v>
@@ -40810,7 +40836,7 @@
         <v>1442</v>
       </c>
       <c r="K548" s="13" t="s">
-        <v>2034</v>
+        <v>2031</v>
       </c>
       <c r="L548" s="12" t="s">
         <v>426</v>
@@ -40823,12 +40849,12 @@
         <v>85</v>
       </c>
       <c r="P548" s="8" t="s">
-        <v>2035</v>
+        <v>2032</v>
       </c>
       <c r="Q548" s="19"/>
       <c r="R548" s="19"/>
       <c r="S548" s="61" t="s">
-        <v>2026</v>
+        <v>2023</v>
       </c>
       <c r="T548" s="20"/>
       <c r="U548" s="18" t="str">
@@ -40838,7 +40864,7 @@
     </row>
     <row r="549">
       <c r="A549" s="16" t="s">
-        <v>2036</v>
+        <v>2033</v>
       </c>
       <c r="B549" s="6">
         <v>44126.0</v>
@@ -40857,7 +40883,7 @@
         <v>25</v>
       </c>
       <c r="H549" s="8" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="I549" s="9">
         <v>44117.0</v>
@@ -40866,25 +40892,25 @@
         <v>44121.0</v>
       </c>
       <c r="K549" s="13" t="s">
-        <v>2029</v>
+        <v>2026</v>
       </c>
       <c r="L549" s="12" t="s">
         <v>426</v>
       </c>
       <c r="M549" s="13" t="s">
-        <v>2038</v>
+        <v>2035</v>
       </c>
       <c r="N549" s="25"/>
       <c r="O549" s="8" t="s">
         <v>85</v>
       </c>
       <c r="P549" s="8" t="s">
-        <v>2039</v>
+        <v>2036</v>
       </c>
       <c r="Q549" s="19"/>
       <c r="R549" s="19"/>
       <c r="S549" s="61" t="s">
-        <v>2026</v>
+        <v>2023</v>
       </c>
       <c r="T549" s="20"/>
       <c r="U549" s="18" t="str">
@@ -40894,7 +40920,7 @@
     </row>
     <row r="550">
       <c r="A550" s="16" t="s">
-        <v>2040</v>
+        <v>2037</v>
       </c>
       <c r="B550" s="6">
         <v>44128.0</v>
@@ -40913,7 +40939,7 @@
         <v>25</v>
       </c>
       <c r="H550" s="8" t="s">
-        <v>2041</v>
+        <v>2038</v>
       </c>
       <c r="I550" s="9">
         <v>44104.0</v>
@@ -40922,7 +40948,7 @@
         <v>1442</v>
       </c>
       <c r="K550" s="13" t="s">
-        <v>2042</v>
+        <v>2039</v>
       </c>
       <c r="L550" s="12" t="s">
         <v>1674</v>
@@ -40935,12 +40961,12 @@
         <v>85</v>
       </c>
       <c r="P550" s="8" t="s">
-        <v>2043</v>
+        <v>2040</v>
       </c>
       <c r="Q550" s="19"/>
       <c r="R550" s="19"/>
       <c r="S550" s="61" t="s">
-        <v>2044</v>
+        <v>2041</v>
       </c>
       <c r="T550" s="20"/>
       <c r="U550" s="18" t="str">
@@ -40950,7 +40976,7 @@
     </row>
     <row r="551">
       <c r="A551" s="16" t="s">
-        <v>2045</v>
+        <v>2042</v>
       </c>
       <c r="B551" s="6">
         <v>44128.0</v>
@@ -40969,7 +40995,7 @@
         <v>25</v>
       </c>
       <c r="H551" s="8" t="s">
-        <v>2046</v>
+        <v>2043</v>
       </c>
       <c r="I551" s="9">
         <v>44122.0</v>
@@ -40978,13 +41004,13 @@
         <v>44125.0</v>
       </c>
       <c r="K551" s="13" t="s">
-        <v>2047</v>
+        <v>2044</v>
       </c>
       <c r="L551" s="12" t="s">
         <v>426</v>
       </c>
       <c r="M551" s="13" t="s">
-        <v>2048</v>
+        <v>2045</v>
       </c>
       <c r="N551" s="25"/>
       <c r="O551" s="8" t="s">
@@ -40994,7 +41020,7 @@
       <c r="Q551" s="19"/>
       <c r="R551" s="19"/>
       <c r="S551" s="61" t="s">
-        <v>2044</v>
+        <v>2041</v>
       </c>
       <c r="T551" s="20"/>
       <c r="U551" s="18" t="str">
@@ -41004,7 +41030,7 @@
     </row>
     <row r="552">
       <c r="A552" s="16" t="s">
-        <v>2049</v>
+        <v>2046</v>
       </c>
       <c r="B552" s="6">
         <v>44132.0</v>
@@ -41023,7 +41049,7 @@
         <v>25</v>
       </c>
       <c r="H552" s="8" t="s">
-        <v>2050</v>
+        <v>2047</v>
       </c>
       <c r="I552" s="9">
         <v>44111.0</v>
@@ -41032,7 +41058,7 @@
         <v>1442</v>
       </c>
       <c r="K552" s="13" t="s">
-        <v>2051</v>
+        <v>2048</v>
       </c>
       <c r="L552" s="12" t="s">
         <v>1674</v>
@@ -41045,12 +41071,12 @@
         <v>85</v>
       </c>
       <c r="P552" s="8" t="s">
-        <v>2052</v>
+        <v>2049</v>
       </c>
       <c r="Q552" s="19"/>
       <c r="R552" s="19"/>
       <c r="S552" s="61" t="s">
-        <v>2053</v>
+        <v>2050</v>
       </c>
       <c r="T552" s="20"/>
       <c r="U552" s="18" t="str">
@@ -41060,7 +41086,7 @@
     </row>
     <row r="553">
       <c r="A553" s="16" t="s">
-        <v>2054</v>
+        <v>2051</v>
       </c>
       <c r="B553" s="6">
         <v>44133.0</v>
@@ -41079,7 +41105,7 @@
         <v>25</v>
       </c>
       <c r="H553" s="8" t="s">
-        <v>2055</v>
+        <v>2052</v>
       </c>
       <c r="I553" s="9">
         <v>44129.0</v>
@@ -41088,13 +41114,13 @@
         <v>44118.0</v>
       </c>
       <c r="K553" s="13" t="s">
-        <v>2056</v>
+        <v>2053</v>
       </c>
       <c r="L553" s="12" t="s">
         <v>426</v>
       </c>
       <c r="M553" s="13" t="s">
-        <v>2057</v>
+        <v>2054</v>
       </c>
       <c r="N553" s="25"/>
       <c r="O553" s="8" t="s">
@@ -41104,7 +41130,7 @@
       <c r="Q553" s="19"/>
       <c r="R553" s="19"/>
       <c r="S553" s="61" t="s">
-        <v>2058</v>
+        <v>2055</v>
       </c>
       <c r="T553" s="20"/>
       <c r="U553" s="18" t="str">
@@ -41114,7 +41140,7 @@
     </row>
     <row r="554">
       <c r="A554" s="16" t="s">
-        <v>2059</v>
+        <v>2056</v>
       </c>
       <c r="B554" s="6">
         <v>44133.0</v>
@@ -41133,7 +41159,7 @@
         <v>25</v>
       </c>
       <c r="H554" s="8" t="s">
-        <v>2060</v>
+        <v>2057</v>
       </c>
       <c r="I554" s="9">
         <v>44131.0</v>
@@ -41142,25 +41168,25 @@
         <v>44130.0</v>
       </c>
       <c r="K554" s="13" t="s">
-        <v>2061</v>
+        <v>2058</v>
       </c>
       <c r="L554" s="12" t="s">
         <v>363</v>
       </c>
       <c r="M554" s="13" t="s">
-        <v>2062</v>
+        <v>2059</v>
       </c>
       <c r="N554" s="25"/>
       <c r="O554" s="8" t="s">
         <v>85</v>
       </c>
       <c r="P554" s="8" t="s">
-        <v>2063</v>
+        <v>2060</v>
       </c>
       <c r="Q554" s="19"/>
       <c r="R554" s="19"/>
       <c r="S554" s="61" t="s">
-        <v>2058</v>
+        <v>2055</v>
       </c>
       <c r="T554" s="20"/>
       <c r="U554" s="18" t="str">
@@ -41170,7 +41196,7 @@
     </row>
     <row r="555">
       <c r="A555" s="16" t="s">
-        <v>2064</v>
+        <v>2061</v>
       </c>
       <c r="B555" s="6">
         <v>44133.0</v>
@@ -41189,7 +41215,7 @@
         <v>25</v>
       </c>
       <c r="H555" s="8" t="s">
-        <v>2065</v>
+        <v>2062</v>
       </c>
       <c r="I555" s="9">
         <v>44119.0</v>
@@ -41198,7 +41224,7 @@
         <v>1442</v>
       </c>
       <c r="K555" s="13" t="s">
-        <v>2066</v>
+        <v>2063</v>
       </c>
       <c r="L555" s="12" t="s">
         <v>426</v>
@@ -41211,12 +41237,12 @@
         <v>85</v>
       </c>
       <c r="P555" s="8" t="s">
-        <v>2067</v>
+        <v>2064</v>
       </c>
       <c r="Q555" s="19"/>
       <c r="R555" s="19"/>
       <c r="S555" s="61" t="s">
-        <v>2058</v>
+        <v>2055</v>
       </c>
       <c r="T555" s="20"/>
       <c r="U555" s="18" t="str">
@@ -41226,7 +41252,7 @@
     </row>
     <row r="556">
       <c r="A556" s="16" t="s">
-        <v>2068</v>
+        <v>2065</v>
       </c>
       <c r="B556" s="6">
         <v>44134.0</v>
@@ -41245,7 +41271,7 @@
         <v>25</v>
       </c>
       <c r="H556" s="8" t="s">
-        <v>2069</v>
+        <v>2066</v>
       </c>
       <c r="I556" s="9">
         <v>44119.0</v>
@@ -41254,25 +41280,25 @@
         <v>44094.0</v>
       </c>
       <c r="K556" s="13" t="s">
-        <v>2070</v>
+        <v>2067</v>
       </c>
       <c r="L556" s="12" t="s">
         <v>426</v>
       </c>
       <c r="M556" s="13" t="s">
-        <v>2071</v>
+        <v>2068</v>
       </c>
       <c r="N556" s="25"/>
       <c r="O556" s="8" t="s">
         <v>85</v>
       </c>
       <c r="P556" s="8" t="s">
-        <v>2072</v>
+        <v>2069</v>
       </c>
       <c r="Q556" s="19"/>
       <c r="R556" s="19"/>
       <c r="S556" s="61" t="s">
-        <v>2073</v>
+        <v>2070</v>
       </c>
       <c r="T556" s="20"/>
       <c r="U556" s="18" t="str">
@@ -41282,7 +41308,7 @@
     </row>
     <row r="557">
       <c r="A557" s="16" t="s">
-        <v>2074</v>
+        <v>2071</v>
       </c>
       <c r="B557" s="6">
         <v>44135.0</v>
@@ -41301,7 +41327,7 @@
         <v>25</v>
       </c>
       <c r="H557" s="8" t="s">
-        <v>2075</v>
+        <v>2072</v>
       </c>
       <c r="I557" s="9">
         <v>44132.0</v>
@@ -41310,13 +41336,13 @@
         <v>44128.0</v>
       </c>
       <c r="K557" s="13" t="s">
-        <v>2076</v>
+        <v>2073</v>
       </c>
       <c r="L557" s="12" t="s">
         <v>363</v>
       </c>
       <c r="M557" s="13" t="s">
-        <v>2077</v>
+        <v>2074</v>
       </c>
       <c r="N557" s="25"/>
       <c r="O557" s="8" t="s">
@@ -41326,7 +41352,7 @@
       <c r="Q557" s="19"/>
       <c r="R557" s="19"/>
       <c r="S557" s="61" t="s">
-        <v>2078</v>
+        <v>2075</v>
       </c>
       <c r="T557" s="20"/>
       <c r="U557" s="18" t="str">
@@ -41336,7 +41362,7 @@
     </row>
     <row r="558">
       <c r="A558" s="16" t="s">
-        <v>2079</v>
+        <v>2076</v>
       </c>
       <c r="B558" s="6">
         <v>44136.0</v>
@@ -41355,7 +41381,7 @@
         <v>25</v>
       </c>
       <c r="H558" s="8" t="s">
-        <v>2080</v>
+        <v>2077</v>
       </c>
       <c r="I558" s="9">
         <v>44133.0</v>
@@ -41364,7 +41390,7 @@
         <v>44111.0</v>
       </c>
       <c r="K558" s="13" t="s">
-        <v>2081</v>
+        <v>2078</v>
       </c>
       <c r="L558" s="12" t="s">
         <v>363</v>
@@ -41377,12 +41403,12 @@
         <v>85</v>
       </c>
       <c r="P558" s="8" t="s">
-        <v>2082</v>
+        <v>2079</v>
       </c>
       <c r="Q558" s="19"/>
       <c r="R558" s="19"/>
       <c r="S558" s="61" t="s">
-        <v>2083</v>
+        <v>2080</v>
       </c>
       <c r="T558" s="20"/>
       <c r="U558" s="18" t="str">
@@ -41392,7 +41418,7 @@
     </row>
     <row r="559">
       <c r="A559" s="16" t="s">
-        <v>2084</v>
+        <v>2081</v>
       </c>
       <c r="B559" s="6">
         <v>44136.0</v>
@@ -41411,7 +41437,7 @@
         <v>25</v>
       </c>
       <c r="H559" s="8" t="s">
-        <v>2085</v>
+        <v>2082</v>
       </c>
       <c r="I559" s="9">
         <v>44118.0</v>
@@ -41420,7 +41446,7 @@
         <v>44118.0</v>
       </c>
       <c r="K559" s="13" t="s">
-        <v>2081</v>
+        <v>2078</v>
       </c>
       <c r="L559" s="12" t="s">
         <v>1674</v>
@@ -41433,12 +41459,12 @@
         <v>85</v>
       </c>
       <c r="P559" s="8" t="s">
-        <v>2086</v>
+        <v>2083</v>
       </c>
       <c r="Q559" s="19"/>
       <c r="R559" s="19"/>
       <c r="S559" s="61" t="s">
-        <v>2083</v>
+        <v>2080</v>
       </c>
       <c r="T559" s="20"/>
       <c r="U559" s="18" t="str">
@@ -41448,7 +41474,7 @@
     </row>
     <row r="560">
       <c r="A560" s="16" t="s">
-        <v>2087</v>
+        <v>2084</v>
       </c>
       <c r="B560" s="6">
         <v>44136.0</v>
@@ -41467,7 +41493,7 @@
         <v>25</v>
       </c>
       <c r="H560" s="8" t="s">
-        <v>2088</v>
+        <v>2085</v>
       </c>
       <c r="I560" s="9">
         <v>44134.0</v>
@@ -41476,25 +41502,25 @@
         <v>44130.0</v>
       </c>
       <c r="K560" s="13" t="s">
-        <v>2089</v>
+        <v>2086</v>
       </c>
       <c r="L560" s="12" t="s">
         <v>363</v>
       </c>
       <c r="M560" s="13" t="s">
-        <v>2090</v>
+        <v>2087</v>
       </c>
       <c r="N560" s="25"/>
       <c r="O560" s="8" t="s">
         <v>85</v>
       </c>
       <c r="P560" s="8" t="s">
-        <v>2091</v>
+        <v>2088</v>
       </c>
       <c r="Q560" s="19"/>
       <c r="R560" s="19"/>
       <c r="S560" s="61" t="s">
-        <v>2083</v>
+        <v>2080</v>
       </c>
       <c r="T560" s="20"/>
       <c r="U560" s="18" t="str">
@@ -41504,7 +41530,7 @@
     </row>
     <row r="561">
       <c r="A561" s="16" t="s">
-        <v>2092</v>
+        <v>2089</v>
       </c>
       <c r="B561" s="6">
         <v>44137.0</v>
@@ -41523,7 +41549,7 @@
         <v>25</v>
       </c>
       <c r="H561" s="8" t="s">
-        <v>2065</v>
+        <v>2062</v>
       </c>
       <c r="I561" s="9">
         <v>44119.0</v>
@@ -41532,7 +41558,7 @@
         <v>1442</v>
       </c>
       <c r="K561" s="13" t="s">
-        <v>2093</v>
+        <v>2090</v>
       </c>
       <c r="L561" s="12" t="s">
         <v>1674</v>
@@ -41545,12 +41571,12 @@
         <v>85</v>
       </c>
       <c r="P561" s="8" t="s">
-        <v>2094</v>
+        <v>2091</v>
       </c>
       <c r="Q561" s="19"/>
       <c r="R561" s="19"/>
       <c r="S561" s="61" t="s">
-        <v>2095</v>
+        <v>2092</v>
       </c>
       <c r="T561" s="20"/>
       <c r="U561" s="18" t="str">
@@ -41560,7 +41586,7 @@
     </row>
     <row r="562">
       <c r="A562" s="16" t="s">
-        <v>2096</v>
+        <v>2093</v>
       </c>
       <c r="B562" s="6">
         <v>44137.0</v>
@@ -41579,7 +41605,7 @@
         <v>25</v>
       </c>
       <c r="H562" s="8" t="s">
-        <v>2097</v>
+        <v>2094</v>
       </c>
       <c r="I562" s="9">
         <v>44122.0</v>
@@ -41588,7 +41614,7 @@
         <v>1442</v>
       </c>
       <c r="K562" s="13" t="s">
-        <v>2098</v>
+        <v>2095</v>
       </c>
       <c r="L562" s="12" t="s">
         <v>426</v>
@@ -41601,12 +41627,12 @@
         <v>85</v>
       </c>
       <c r="P562" s="8" t="s">
-        <v>2099</v>
+        <v>2096</v>
       </c>
       <c r="Q562" s="19"/>
       <c r="R562" s="19"/>
       <c r="S562" s="61" t="s">
-        <v>2095</v>
+        <v>2092</v>
       </c>
       <c r="T562" s="20"/>
       <c r="U562" s="18" t="str">
@@ -41616,7 +41642,7 @@
     </row>
     <row r="563">
       <c r="A563" s="16" t="s">
-        <v>2100</v>
+        <v>2097</v>
       </c>
       <c r="B563" s="6">
         <v>44137.0</v>
@@ -41635,7 +41661,7 @@
         <v>25</v>
       </c>
       <c r="H563" s="8" t="s">
-        <v>2101</v>
+        <v>2098</v>
       </c>
       <c r="I563" s="9">
         <v>44114.0</v>
@@ -41644,7 +41670,7 @@
         <v>1442</v>
       </c>
       <c r="K563" s="13" t="s">
-        <v>2102</v>
+        <v>2099</v>
       </c>
       <c r="L563" s="12" t="s">
         <v>1674</v>
@@ -41657,12 +41683,12 @@
         <v>85</v>
       </c>
       <c r="P563" s="8" t="s">
-        <v>2103</v>
+        <v>2100</v>
       </c>
       <c r="Q563" s="19"/>
       <c r="R563" s="19"/>
       <c r="S563" s="61" t="s">
-        <v>2095</v>
+        <v>2092</v>
       </c>
       <c r="T563" s="20"/>
       <c r="U563" s="18" t="str">
@@ -41672,7 +41698,7 @@
     </row>
     <row r="564">
       <c r="A564" s="16" t="s">
-        <v>2104</v>
+        <v>2101</v>
       </c>
       <c r="B564" s="6">
         <v>44137.0</v>
@@ -41691,7 +41717,7 @@
         <v>25</v>
       </c>
       <c r="H564" s="8" t="s">
-        <v>2022</v>
+        <v>2019</v>
       </c>
       <c r="I564" s="9">
         <v>44118.0</v>
@@ -41700,7 +41726,7 @@
         <v>44134.0</v>
       </c>
       <c r="K564" s="13" t="s">
-        <v>2105</v>
+        <v>2102</v>
       </c>
       <c r="L564" s="12" t="s">
         <v>447</v>
@@ -41713,12 +41739,12 @@
         <v>85</v>
       </c>
       <c r="P564" s="8" t="s">
-        <v>2106</v>
+        <v>2103</v>
       </c>
       <c r="Q564" s="19"/>
       <c r="R564" s="19"/>
       <c r="S564" s="61" t="s">
-        <v>2095</v>
+        <v>2092</v>
       </c>
       <c r="T564" s="20"/>
       <c r="U564" s="18" t="str">
@@ -41728,7 +41754,7 @@
     </row>
     <row r="565">
       <c r="A565" s="16" t="s">
-        <v>2107</v>
+        <v>2104</v>
       </c>
       <c r="B565" s="6">
         <v>44137.0</v>
@@ -41747,7 +41773,7 @@
         <v>25</v>
       </c>
       <c r="H565" s="8" t="s">
-        <v>2108</v>
+        <v>2105</v>
       </c>
       <c r="I565" s="9">
         <v>44123.0</v>
@@ -41756,7 +41782,7 @@
         <v>1442</v>
       </c>
       <c r="K565" s="13" t="s">
-        <v>2109</v>
+        <v>2106</v>
       </c>
       <c r="L565" s="12" t="s">
         <v>426</v>
@@ -41769,12 +41795,12 @@
         <v>85</v>
       </c>
       <c r="P565" s="8" t="s">
-        <v>2110</v>
+        <v>2107</v>
       </c>
       <c r="Q565" s="19"/>
       <c r="R565" s="19"/>
       <c r="S565" s="61" t="s">
-        <v>2095</v>
+        <v>2092</v>
       </c>
       <c r="T565" s="20"/>
       <c r="U565" s="18" t="str">
@@ -41784,7 +41810,7 @@
     </row>
     <row r="566">
       <c r="A566" s="16" t="s">
-        <v>2111</v>
+        <v>2108</v>
       </c>
       <c r="B566" s="6">
         <v>44138.0</v>
@@ -41803,34 +41829,34 @@
         <v>25</v>
       </c>
       <c r="H566" s="8" t="s">
-        <v>2112</v>
+        <v>2109</v>
       </c>
       <c r="I566" s="9">
         <v>44136.0</v>
       </c>
       <c r="J566" s="12" t="s">
-        <v>2113</v>
+        <v>2110</v>
       </c>
       <c r="K566" s="13" t="s">
-        <v>2114</v>
+        <v>2111</v>
       </c>
       <c r="L566" s="12" t="s">
         <v>363</v>
       </c>
       <c r="M566" s="13" t="s">
-        <v>2115</v>
+        <v>2112</v>
       </c>
       <c r="N566" s="25"/>
       <c r="O566" s="8" t="s">
         <v>85</v>
       </c>
       <c r="P566" s="8" t="s">
-        <v>2116</v>
+        <v>2113</v>
       </c>
       <c r="Q566" s="19"/>
       <c r="R566" s="19"/>
       <c r="S566" s="61" t="s">
-        <v>2117</v>
+        <v>2114</v>
       </c>
       <c r="T566" s="20"/>
       <c r="U566" s="18" t="str">
@@ -41840,7 +41866,7 @@
     </row>
     <row r="567">
       <c r="A567" s="16" t="s">
-        <v>2118</v>
+        <v>2115</v>
       </c>
       <c r="B567" s="6">
         <v>44138.0</v>
@@ -41859,7 +41885,7 @@
         <v>25</v>
       </c>
       <c r="H567" s="8" t="s">
-        <v>2119</v>
+        <v>2116</v>
       </c>
       <c r="I567" s="9">
         <v>44136.0</v>
@@ -41868,13 +41894,13 @@
         <v>44133.0</v>
       </c>
       <c r="K567" s="13" t="s">
-        <v>2120</v>
+        <v>2117</v>
       </c>
       <c r="L567" s="12" t="s">
         <v>363</v>
       </c>
       <c r="M567" s="13" t="s">
-        <v>2121</v>
+        <v>2118</v>
       </c>
       <c r="N567" s="25"/>
       <c r="O567" s="8" t="s">
@@ -41886,7 +41912,7 @@
       <c r="Q567" s="19"/>
       <c r="R567" s="19"/>
       <c r="S567" s="61" t="s">
-        <v>2117</v>
+        <v>2114</v>
       </c>
       <c r="T567" s="20"/>
       <c r="U567" s="18" t="str">
@@ -41896,7 +41922,7 @@
     </row>
     <row r="568">
       <c r="A568" s="16" t="s">
-        <v>2122</v>
+        <v>2119</v>
       </c>
       <c r="B568" s="6">
         <v>44138.0</v>
@@ -41915,7 +41941,7 @@
         <v>25</v>
       </c>
       <c r="H568" s="8" t="s">
-        <v>2123</v>
+        <v>2120</v>
       </c>
       <c r="I568" s="9">
         <v>44136.0</v>
@@ -41924,13 +41950,13 @@
         <v>44135.0</v>
       </c>
       <c r="K568" s="13" t="s">
-        <v>2120</v>
+        <v>2117</v>
       </c>
       <c r="L568" s="12" t="s">
         <v>426</v>
       </c>
       <c r="M568" s="13" t="s">
-        <v>2124</v>
+        <v>2121</v>
       </c>
       <c r="N568" s="25"/>
       <c r="O568" s="8" t="s">
@@ -41942,7 +41968,7 @@
       <c r="Q568" s="19"/>
       <c r="R568" s="19"/>
       <c r="S568" s="61" t="s">
-        <v>2117</v>
+        <v>2114</v>
       </c>
       <c r="T568" s="20"/>
       <c r="U568" s="18" t="str">
@@ -41952,7 +41978,7 @@
     </row>
     <row r="569">
       <c r="A569" s="16" t="s">
-        <v>2125</v>
+        <v>2122</v>
       </c>
       <c r="B569" s="6">
         <v>44138.0</v>
@@ -41971,7 +41997,7 @@
         <v>25</v>
       </c>
       <c r="H569" s="8" t="s">
-        <v>2126</v>
+        <v>2123</v>
       </c>
       <c r="I569" s="9">
         <v>44124.0</v>
@@ -41980,7 +42006,7 @@
         <v>1442</v>
       </c>
       <c r="K569" s="13" t="s">
-        <v>2127</v>
+        <v>2124</v>
       </c>
       <c r="L569" s="12" t="s">
         <v>426</v>
@@ -41993,12 +42019,12 @@
         <v>85</v>
       </c>
       <c r="P569" s="8" t="s">
-        <v>2128</v>
+        <v>2125</v>
       </c>
       <c r="Q569" s="19"/>
       <c r="R569" s="19"/>
       <c r="S569" s="61" t="s">
-        <v>2117</v>
+        <v>2114</v>
       </c>
       <c r="T569" s="20"/>
       <c r="U569" s="18" t="str">
@@ -42008,7 +42034,7 @@
     </row>
     <row r="570">
       <c r="A570" s="16" t="s">
-        <v>2129</v>
+        <v>2126</v>
       </c>
       <c r="B570" s="6">
         <v>44139.0</v>
@@ -42027,7 +42053,7 @@
         <v>25</v>
       </c>
       <c r="H570" s="8" t="s">
-        <v>2130</v>
+        <v>2127</v>
       </c>
       <c r="I570" s="9">
         <v>44129.0</v>
@@ -42036,25 +42062,25 @@
         <v>44134.0</v>
       </c>
       <c r="K570" s="13" t="s">
-        <v>2131</v>
+        <v>2128</v>
       </c>
       <c r="L570" s="12" t="s">
         <v>426</v>
       </c>
       <c r="M570" s="13" t="s">
-        <v>2132</v>
+        <v>2129</v>
       </c>
       <c r="N570" s="25"/>
       <c r="O570" s="8" t="s">
         <v>85</v>
       </c>
       <c r="P570" s="8" t="s">
-        <v>2133</v>
+        <v>2130</v>
       </c>
       <c r="Q570" s="19"/>
       <c r="R570" s="19"/>
       <c r="S570" s="61" t="s">
-        <v>2134</v>
+        <v>2131</v>
       </c>
       <c r="T570" s="20"/>
       <c r="U570" s="18" t="str">
@@ -42064,7 +42090,7 @@
     </row>
     <row r="571">
       <c r="A571" s="16" t="s">
-        <v>2135</v>
+        <v>2132</v>
       </c>
       <c r="B571" s="6">
         <v>44140.0</v>
@@ -42083,7 +42109,7 @@
         <v>25</v>
       </c>
       <c r="H571" s="8" t="s">
-        <v>2136</v>
+        <v>2133</v>
       </c>
       <c r="I571" s="9">
         <v>44137.0</v>
@@ -42092,25 +42118,25 @@
         <v>44114.0</v>
       </c>
       <c r="K571" s="13" t="s">
-        <v>2137</v>
+        <v>2134</v>
       </c>
       <c r="L571" s="12" t="s">
         <v>363</v>
       </c>
       <c r="M571" s="13" t="s">
-        <v>2138</v>
+        <v>2135</v>
       </c>
       <c r="N571" s="25"/>
       <c r="O571" s="8" t="s">
         <v>85</v>
       </c>
       <c r="P571" s="8" t="s">
-        <v>2139</v>
+        <v>2136</v>
       </c>
       <c r="Q571" s="19"/>
       <c r="R571" s="19"/>
       <c r="S571" s="61" t="s">
-        <v>2140</v>
+        <v>2137</v>
       </c>
       <c r="T571" s="20"/>
       <c r="U571" s="18" t="str">
@@ -42120,7 +42146,7 @@
     </row>
     <row r="572">
       <c r="A572" s="16" t="s">
-        <v>2141</v>
+        <v>2138</v>
       </c>
       <c r="B572" s="6">
         <v>44141.0</v>
@@ -42129,7 +42155,7 @@
         <v>21</v>
       </c>
       <c r="D572" s="7" t="s">
-        <v>2142</v>
+        <v>2139</v>
       </c>
       <c r="E572" s="7" t="s">
         <v>158</v>
@@ -42139,7 +42165,7 @@
         <v>25</v>
       </c>
       <c r="H572" s="8" t="s">
-        <v>2143</v>
+        <v>2140</v>
       </c>
       <c r="I572" s="9">
         <v>44126.0</v>
@@ -42148,7 +42174,7 @@
         <v>1442</v>
       </c>
       <c r="K572" s="13" t="s">
-        <v>2144</v>
+        <v>2141</v>
       </c>
       <c r="L572" s="12" t="s">
         <v>426</v>
@@ -42161,12 +42187,12 @@
         <v>85</v>
       </c>
       <c r="P572" s="8" t="s">
-        <v>2145</v>
+        <v>2142</v>
       </c>
       <c r="Q572" s="19"/>
       <c r="R572" s="19"/>
       <c r="S572" s="61" t="s">
-        <v>2146</v>
+        <v>2143</v>
       </c>
       <c r="T572" s="20"/>
       <c r="U572" s="18" t="str">
@@ -42176,7 +42202,7 @@
     </row>
     <row r="573">
       <c r="A573" s="16" t="s">
-        <v>2147</v>
+        <v>2144</v>
       </c>
       <c r="B573" s="6">
         <v>44141.0</v>
@@ -42185,7 +42211,7 @@
         <v>21</v>
       </c>
       <c r="D573" s="7" t="s">
-        <v>2142</v>
+        <v>2139</v>
       </c>
       <c r="E573" s="7" t="s">
         <v>158</v>
@@ -42205,7 +42231,7 @@
         <v>1442</v>
       </c>
       <c r="K573" s="13" t="s">
-        <v>2144</v>
+        <v>2141</v>
       </c>
       <c r="L573" s="12" t="s">
         <v>426</v>
@@ -42218,12 +42244,12 @@
         <v>85</v>
       </c>
       <c r="P573" s="8" t="s">
-        <v>2145</v>
+        <v>2142</v>
       </c>
       <c r="Q573" s="19"/>
       <c r="R573" s="19"/>
       <c r="S573" s="61" t="s">
-        <v>2146</v>
+        <v>2143</v>
       </c>
       <c r="T573" s="20"/>
       <c r="U573" s="18" t="str">
@@ -42233,7 +42259,7 @@
     </row>
     <row r="574">
       <c r="A574" s="16" t="s">
-        <v>2148</v>
+        <v>2145</v>
       </c>
       <c r="B574" s="6">
         <v>44141.0</v>
@@ -42242,7 +42268,7 @@
         <v>21</v>
       </c>
       <c r="D574" s="7" t="s">
-        <v>2142</v>
+        <v>2139</v>
       </c>
       <c r="E574" s="7" t="s">
         <v>158</v>
@@ -42262,7 +42288,7 @@
         <v>1442</v>
       </c>
       <c r="K574" s="13" t="s">
-        <v>2144</v>
+        <v>2141</v>
       </c>
       <c r="L574" s="12" t="s">
         <v>426</v>
@@ -42275,12 +42301,12 @@
         <v>85</v>
       </c>
       <c r="P574" s="8" t="s">
-        <v>2145</v>
+        <v>2142</v>
       </c>
       <c r="Q574" s="19"/>
       <c r="R574" s="19"/>
       <c r="S574" s="61" t="s">
-        <v>2146</v>
+        <v>2143</v>
       </c>
       <c r="T574" s="20"/>
       <c r="U574" s="18" t="str">
@@ -42290,7 +42316,7 @@
     </row>
     <row r="575">
       <c r="A575" s="16" t="s">
-        <v>2149</v>
+        <v>2146</v>
       </c>
       <c r="B575" s="6">
         <v>44141.0</v>
@@ -42309,7 +42335,7 @@
         <v>25</v>
       </c>
       <c r="H575" s="8" t="s">
-        <v>2150</v>
+        <v>2147</v>
       </c>
       <c r="I575" s="9">
         <v>44139.0</v>
@@ -42318,25 +42344,25 @@
         <v>44134.0</v>
       </c>
       <c r="K575" s="13" t="s">
-        <v>2144</v>
+        <v>2141</v>
       </c>
       <c r="L575" s="12" t="s">
         <v>363</v>
       </c>
       <c r="M575" s="13" t="s">
-        <v>2151</v>
+        <v>2148</v>
       </c>
       <c r="N575" s="25"/>
       <c r="O575" s="8" t="s">
         <v>85</v>
       </c>
       <c r="P575" s="8" t="s">
-        <v>2152</v>
+        <v>2149</v>
       </c>
       <c r="Q575" s="19"/>
       <c r="R575" s="19"/>
       <c r="S575" s="61" t="s">
-        <v>2146</v>
+        <v>2143</v>
       </c>
       <c r="T575" s="20"/>
       <c r="U575" s="18" t="str">
@@ -42346,7 +42372,7 @@
     </row>
     <row r="576">
       <c r="A576" s="16" t="s">
-        <v>2153</v>
+        <v>2150</v>
       </c>
       <c r="B576" s="6">
         <v>44143.0</v>
@@ -42355,7 +42381,7 @@
         <v>21</v>
       </c>
       <c r="D576" s="7" t="s">
-        <v>2154</v>
+        <v>2151</v>
       </c>
       <c r="E576" s="7" t="s">
         <v>158</v>
@@ -42365,7 +42391,7 @@
         <v>25</v>
       </c>
       <c r="H576" s="8" t="s">
-        <v>2155</v>
+        <v>2152</v>
       </c>
       <c r="I576" s="9">
         <v>44128.0</v>
@@ -42374,7 +42400,7 @@
         <v>1442</v>
       </c>
       <c r="K576" s="13" t="s">
-        <v>2156</v>
+        <v>2153</v>
       </c>
       <c r="L576" s="12" t="s">
         <v>426</v>
@@ -42387,12 +42413,12 @@
         <v>85</v>
       </c>
       <c r="P576" s="8" t="s">
-        <v>2157</v>
+        <v>2154</v>
       </c>
       <c r="Q576" s="19"/>
       <c r="R576" s="19"/>
       <c r="S576" s="61" t="s">
-        <v>2158</v>
+        <v>2155</v>
       </c>
       <c r="T576" s="20"/>
       <c r="U576" s="18" t="str">
@@ -42402,7 +42428,7 @@
     </row>
     <row r="577">
       <c r="A577" s="16" t="s">
-        <v>2159</v>
+        <v>2156</v>
       </c>
       <c r="B577" s="6">
         <v>44143.0</v>
@@ -42411,7 +42437,7 @@
         <v>21</v>
       </c>
       <c r="D577" s="7" t="s">
-        <v>2154</v>
+        <v>2151</v>
       </c>
       <c r="E577" s="7" t="s">
         <v>158</v>
@@ -42421,7 +42447,7 @@
         <v>25</v>
       </c>
       <c r="H577" s="8" t="s">
-        <v>2155</v>
+        <v>2152</v>
       </c>
       <c r="I577" s="9">
         <v>44128.0</v>
@@ -42430,7 +42456,7 @@
         <v>1442</v>
       </c>
       <c r="K577" s="13" t="s">
-        <v>2156</v>
+        <v>2153</v>
       </c>
       <c r="L577" s="12" t="s">
         <v>426</v>
@@ -42443,12 +42469,12 @@
         <v>85</v>
       </c>
       <c r="P577" s="8" t="s">
-        <v>2157</v>
+        <v>2154</v>
       </c>
       <c r="Q577" s="19"/>
       <c r="R577" s="19"/>
       <c r="S577" s="61" t="s">
-        <v>2158</v>
+        <v>2155</v>
       </c>
       <c r="T577" s="20"/>
       <c r="U577" s="18" t="str">
@@ -42458,7 +42484,7 @@
     </row>
     <row r="578">
       <c r="A578" s="16" t="s">
-        <v>2160</v>
+        <v>2157</v>
       </c>
       <c r="B578" s="6">
         <v>44143.0</v>
@@ -42477,7 +42503,7 @@
         <v>25</v>
       </c>
       <c r="H578" s="8" t="s">
-        <v>2161</v>
+        <v>2158</v>
       </c>
       <c r="I578" s="9">
         <v>44120.0</v>
@@ -42486,7 +42512,7 @@
         <v>1442</v>
       </c>
       <c r="K578" s="13" t="s">
-        <v>2162</v>
+        <v>2159</v>
       </c>
       <c r="L578" s="12" t="s">
         <v>1674</v>
@@ -42499,12 +42525,12 @@
         <v>85</v>
       </c>
       <c r="P578" s="8" t="s">
-        <v>2163</v>
+        <v>2160</v>
       </c>
       <c r="Q578" s="19"/>
       <c r="R578" s="19"/>
       <c r="S578" s="61" t="s">
-        <v>2158</v>
+        <v>2155</v>
       </c>
       <c r="T578" s="20"/>
       <c r="U578" s="18" t="str">
@@ -42514,7 +42540,7 @@
     </row>
     <row r="579">
       <c r="A579" s="16" t="s">
-        <v>2164</v>
+        <v>2161</v>
       </c>
       <c r="B579" s="6">
         <v>44143.0</v>
@@ -42533,7 +42559,7 @@
         <v>25</v>
       </c>
       <c r="H579" s="8" t="s">
-        <v>2165</v>
+        <v>2162</v>
       </c>
       <c r="I579" s="9">
         <v>44129.0</v>
@@ -42542,25 +42568,25 @@
         <v>1672</v>
       </c>
       <c r="K579" s="13" t="s">
-        <v>2166</v>
+        <v>2163</v>
       </c>
       <c r="L579" s="12" t="s">
         <v>426</v>
       </c>
       <c r="M579" s="13" t="s">
-        <v>1672</v>
+        <v>1442</v>
       </c>
       <c r="N579" s="25"/>
       <c r="O579" s="8" t="s">
         <v>85</v>
       </c>
       <c r="P579" s="8" t="s">
-        <v>2167</v>
+        <v>2164</v>
       </c>
       <c r="Q579" s="19"/>
       <c r="R579" s="19"/>
       <c r="S579" s="61" t="s">
-        <v>2158</v>
+        <v>2155</v>
       </c>
       <c r="T579" s="20"/>
       <c r="U579" s="18" t="str">
@@ -42569,34 +42595,64 @@
       </c>
     </row>
     <row r="580">
-      <c r="A580" s="63"/>
-      <c r="B580" s="64"/>
-      <c r="C580" s="34"/>
-      <c r="D580" s="34"/>
-      <c r="E580" s="34"/>
+      <c r="A580" s="16" t="s">
+        <v>2165</v>
+      </c>
+      <c r="B580" s="6">
+        <v>44144.0</v>
+      </c>
+      <c r="C580" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D580" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E580" s="7" t="s">
+        <v>1949</v>
+      </c>
       <c r="F580" s="34"/>
-      <c r="G580" s="34"/>
-      <c r="H580" s="21"/>
-      <c r="I580" s="19"/>
-      <c r="J580" s="10"/>
-      <c r="K580" s="22"/>
-      <c r="L580" s="23"/>
-      <c r="M580" s="22"/>
+      <c r="G580" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H580" s="8" t="s">
+        <v>2166</v>
+      </c>
+      <c r="I580" s="9">
+        <v>44138.0</v>
+      </c>
+      <c r="J580" s="10">
+        <v>44141.0</v>
+      </c>
+      <c r="K580" s="13" t="s">
+        <v>2167</v>
+      </c>
+      <c r="L580" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M580" s="13" t="s">
+        <v>2168</v>
+      </c>
       <c r="N580" s="25"/>
-      <c r="O580" s="21"/>
-      <c r="P580" s="21"/>
+      <c r="O580" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P580" s="8" t="s">
+        <v>2169</v>
+      </c>
       <c r="Q580" s="19"/>
       <c r="R580" s="19"/>
-      <c r="S580" s="20"/>
+      <c r="S580" s="61" t="s">
+        <v>2170</v>
+      </c>
       <c r="T580" s="20"/>
       <c r="U580" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#579</v>
       </c>
     </row>
     <row r="581">
-      <c r="A581" s="63"/>
-      <c r="B581" s="64"/>
+      <c r="A581" s="73"/>
+      <c r="B581" s="74"/>
       <c r="C581" s="34"/>
       <c r="D581" s="34"/>
       <c r="E581" s="34"/>
@@ -42621,8 +42677,8 @@
       </c>
     </row>
     <row r="582">
-      <c r="A582" s="63"/>
-      <c r="B582" s="64"/>
+      <c r="A582" s="73"/>
+      <c r="B582" s="74"/>
       <c r="C582" s="34"/>
       <c r="D582" s="34"/>
       <c r="E582" s="34"/>
@@ -42647,8 +42703,8 @@
       </c>
     </row>
     <row r="583">
-      <c r="A583" s="63"/>
-      <c r="B583" s="64"/>
+      <c r="A583" s="73"/>
+      <c r="B583" s="74"/>
       <c r="C583" s="34"/>
       <c r="D583" s="34"/>
       <c r="E583" s="34"/>
@@ -42673,8 +42729,8 @@
       </c>
     </row>
     <row r="584">
-      <c r="A584" s="63"/>
-      <c r="B584" s="64"/>
+      <c r="A584" s="73"/>
+      <c r="B584" s="74"/>
       <c r="C584" s="34"/>
       <c r="D584" s="34"/>
       <c r="E584" s="34"/>
@@ -42699,8 +42755,8 @@
       </c>
     </row>
     <row r="585">
-      <c r="A585" s="63"/>
-      <c r="B585" s="64"/>
+      <c r="A585" s="73"/>
+      <c r="B585" s="74"/>
       <c r="C585" s="34"/>
       <c r="D585" s="34"/>
       <c r="E585" s="34"/>
@@ -42725,8 +42781,8 @@
       </c>
     </row>
     <row r="586">
-      <c r="A586" s="63"/>
-      <c r="B586" s="64"/>
+      <c r="A586" s="73"/>
+      <c r="B586" s="74"/>
       <c r="C586" s="34"/>
       <c r="D586" s="34"/>
       <c r="E586" s="34"/>
@@ -42751,8 +42807,8 @@
       </c>
     </row>
     <row r="587">
-      <c r="A587" s="63"/>
-      <c r="B587" s="64"/>
+      <c r="A587" s="73"/>
+      <c r="B587" s="74"/>
       <c r="C587" s="34"/>
       <c r="D587" s="34"/>
       <c r="E587" s="34"/>
@@ -42777,8 +42833,8 @@
       </c>
     </row>
     <row r="588">
-      <c r="A588" s="63"/>
-      <c r="B588" s="64"/>
+      <c r="A588" s="73"/>
+      <c r="B588" s="74"/>
       <c r="C588" s="34"/>
       <c r="D588" s="34"/>
       <c r="E588" s="34"/>
@@ -42803,8 +42859,8 @@
       </c>
     </row>
     <row r="589">
-      <c r="A589" s="63"/>
-      <c r="B589" s="64"/>
+      <c r="A589" s="73"/>
+      <c r="B589" s="74"/>
       <c r="C589" s="34"/>
       <c r="D589" s="34"/>
       <c r="E589" s="34"/>
@@ -42829,8 +42885,8 @@
       </c>
     </row>
     <row r="590">
-      <c r="A590" s="63"/>
-      <c r="B590" s="64"/>
+      <c r="A590" s="73"/>
+      <c r="B590" s="74"/>
       <c r="C590" s="34"/>
       <c r="D590" s="34"/>
       <c r="E590" s="34"/>
@@ -42855,8 +42911,8 @@
       </c>
     </row>
     <row r="591">
-      <c r="A591" s="63"/>
-      <c r="B591" s="64"/>
+      <c r="A591" s="73"/>
+      <c r="B591" s="74"/>
       <c r="C591" s="34"/>
       <c r="D591" s="34"/>
       <c r="E591" s="34"/>
@@ -42881,8 +42937,8 @@
       </c>
     </row>
     <row r="592">
-      <c r="A592" s="63"/>
-      <c r="B592" s="64"/>
+      <c r="A592" s="73"/>
+      <c r="B592" s="74"/>
       <c r="C592" s="34"/>
       <c r="D592" s="34"/>
       <c r="E592" s="34"/>
@@ -42907,8 +42963,8 @@
       </c>
     </row>
     <row r="593">
-      <c r="A593" s="63"/>
-      <c r="B593" s="64"/>
+      <c r="A593" s="73"/>
+      <c r="B593" s="74"/>
       <c r="C593" s="34"/>
       <c r="D593" s="34"/>
       <c r="E593" s="34"/>
@@ -42933,8 +42989,8 @@
       </c>
     </row>
     <row r="594">
-      <c r="A594" s="63"/>
-      <c r="B594" s="64"/>
+      <c r="A594" s="73"/>
+      <c r="B594" s="74"/>
       <c r="C594" s="34"/>
       <c r="D594" s="34"/>
       <c r="E594" s="34"/>
@@ -42959,8 +43015,8 @@
       </c>
     </row>
     <row r="595">
-      <c r="A595" s="63"/>
-      <c r="B595" s="64"/>
+      <c r="A595" s="73"/>
+      <c r="B595" s="74"/>
       <c r="C595" s="34"/>
       <c r="D595" s="34"/>
       <c r="E595" s="34"/>
@@ -42985,8 +43041,8 @@
       </c>
     </row>
     <row r="596">
-      <c r="A596" s="63"/>
-      <c r="B596" s="64"/>
+      <c r="A596" s="73"/>
+      <c r="B596" s="74"/>
       <c r="C596" s="34"/>
       <c r="D596" s="34"/>
       <c r="E596" s="34"/>
@@ -43011,8 +43067,8 @@
       </c>
     </row>
     <row r="597">
-      <c r="A597" s="63"/>
-      <c r="B597" s="64"/>
+      <c r="A597" s="73"/>
+      <c r="B597" s="74"/>
       <c r="C597" s="34"/>
       <c r="D597" s="34"/>
       <c r="E597" s="34"/>
@@ -43037,8 +43093,8 @@
       </c>
     </row>
     <row r="598">
-      <c r="A598" s="63"/>
-      <c r="B598" s="64"/>
+      <c r="A598" s="73"/>
+      <c r="B598" s="74"/>
       <c r="C598" s="34"/>
       <c r="D598" s="34"/>
       <c r="E598" s="34"/>
@@ -43063,8 +43119,8 @@
       </c>
     </row>
     <row r="599">
-      <c r="A599" s="63"/>
-      <c r="B599" s="64"/>
+      <c r="A599" s="73"/>
+      <c r="B599" s="74"/>
       <c r="C599" s="34"/>
       <c r="D599" s="34"/>
       <c r="E599" s="34"/>
@@ -43089,8 +43145,8 @@
       </c>
     </row>
     <row r="600">
-      <c r="A600" s="63"/>
-      <c r="B600" s="64"/>
+      <c r="A600" s="73"/>
+      <c r="B600" s="74"/>
       <c r="C600" s="34"/>
       <c r="D600" s="34"/>
       <c r="E600" s="34"/>
@@ -43115,8 +43171,8 @@
       </c>
     </row>
     <row r="601">
-      <c r="A601" s="63"/>
-      <c r="B601" s="64"/>
+      <c r="A601" s="73"/>
+      <c r="B601" s="74"/>
       <c r="C601" s="34"/>
       <c r="D601" s="34"/>
       <c r="E601" s="34"/>
@@ -43662,15 +43718,16 @@
     <hyperlink r:id="rId139" ref="S577"/>
     <hyperlink r:id="rId140" ref="S578"/>
     <hyperlink r:id="rId141" ref="S579"/>
+    <hyperlink r:id="rId142" ref="S580"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId142"/>
-  <legacyDrawing r:id="rId143"/>
+  <drawing r:id="rId143"/>
+  <legacyDrawing r:id="rId144"/>
   <tableParts count="2">
-    <tablePart r:id="rId146"/>
     <tablePart r:id="rId147"/>
+    <tablePart r:id="rId148"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201111
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -571,7 +571,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6451" uniqueCount="2171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6528" uniqueCount="2189">
   <si>
     <t>案例</t>
   </si>
@@ -7956,6 +7956,65 @@
   </si>
   <si>
     <t>國內新增1例境外移入COVID-19病例，烏克蘭籍女子來臺工作確診</t>
+  </si>
+  <si>
+    <t>#580</t>
+  </si>
+  <si>
+    <t>-10/26 印尼→台灣</t>
+  </si>
+  <si>
+    <t>11/8 採檢
+11/10 確診</t>
+  </si>
+  <si>
+    <t>來臺工作，入境迄今均無疑似症狀</t>
+  </si>
+  <si>
+    <t>2名印尼籍女性來臺工作，檢疫期滿前檢驗確診COVID-19</t>
+  </si>
+  <si>
+    <t>#581</t>
+  </si>
+  <si>
+    <t>-10/27 印尼→台灣</t>
+  </si>
+  <si>
+    <t>11/9 採檢
+11/10 確診</t>
+  </si>
+  <si>
+    <t>#582</t>
+  </si>
+  <si>
+    <t>-10/28 印尼→台灣</t>
+  </si>
+  <si>
+    <t>11/9 採檢
+11/11 確診</t>
+  </si>
+  <si>
+    <t>來臺工作</t>
+  </si>
+  <si>
+    <t>國內新增4例境外移入COVID-19病例，分別自印尼及比利時入境</t>
+  </si>
+  <si>
+    <t>#583</t>
+  </si>
+  <si>
+    <t>-10/24 比利時→荷蘭
+10/24-10/25 荷蘭→台灣</t>
+  </si>
+  <si>
+    <t>因受臺灣公司邀請來臺從事商務活動
+個案入境時無症狀，並持有登機前3日內檢驗陰性報告，居家檢疫期間，曾於10月31日出現嗅味覺異常症狀，因隔天症狀緩解，故未就醫及通報</t>
+  </si>
+  <si>
+    <t>#584</t>
+  </si>
+  <si>
+    <t>#585</t>
   </si>
 </sst>
 </file>
@@ -42651,159 +42710,339 @@
       </c>
     </row>
     <row r="581">
-      <c r="A581" s="73"/>
-      <c r="B581" s="74"/>
-      <c r="C581" s="34"/>
-      <c r="D581" s="34"/>
-      <c r="E581" s="34"/>
+      <c r="A581" s="16" t="s">
+        <v>2171</v>
+      </c>
+      <c r="B581" s="6">
+        <v>44145.0</v>
+      </c>
+      <c r="C581" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D581" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E581" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F581" s="34"/>
-      <c r="G581" s="34"/>
-      <c r="H581" s="21"/>
-      <c r="I581" s="19"/>
-      <c r="J581" s="10"/>
-      <c r="K581" s="22"/>
-      <c r="L581" s="23"/>
-      <c r="M581" s="22"/>
+      <c r="G581" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H581" s="8" t="s">
+        <v>2172</v>
+      </c>
+      <c r="I581" s="9">
+        <v>44130.0</v>
+      </c>
+      <c r="J581" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K581" s="13" t="s">
+        <v>2173</v>
+      </c>
+      <c r="L581" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M581" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N581" s="25"/>
-      <c r="O581" s="21"/>
-      <c r="P581" s="21"/>
+      <c r="O581" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P581" s="8" t="s">
+        <v>2174</v>
+      </c>
       <c r="Q581" s="19"/>
       <c r="R581" s="19"/>
-      <c r="S581" s="20"/>
+      <c r="S581" s="61" t="s">
+        <v>2175</v>
+      </c>
       <c r="T581" s="20"/>
       <c r="U581" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#580</v>
       </c>
     </row>
     <row r="582">
-      <c r="A582" s="73"/>
-      <c r="B582" s="74"/>
-      <c r="C582" s="34"/>
-      <c r="D582" s="34"/>
-      <c r="E582" s="34"/>
+      <c r="A582" s="16" t="s">
+        <v>2176</v>
+      </c>
+      <c r="B582" s="6">
+        <v>44145.0</v>
+      </c>
+      <c r="C582" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D582" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E582" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F582" s="34"/>
-      <c r="G582" s="34"/>
-      <c r="H582" s="21"/>
-      <c r="I582" s="19"/>
-      <c r="J582" s="10"/>
-      <c r="K582" s="22"/>
-      <c r="L582" s="23"/>
-      <c r="M582" s="22"/>
+      <c r="G582" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H582" s="8" t="s">
+        <v>2177</v>
+      </c>
+      <c r="I582" s="9">
+        <v>44131.0</v>
+      </c>
+      <c r="J582" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K582" s="13" t="s">
+        <v>2178</v>
+      </c>
+      <c r="L582" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M582" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N582" s="25"/>
-      <c r="O582" s="21"/>
-      <c r="P582" s="21"/>
+      <c r="O582" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P582" s="8" t="s">
+        <v>2174</v>
+      </c>
       <c r="Q582" s="19"/>
       <c r="R582" s="19"/>
-      <c r="S582" s="20"/>
+      <c r="S582" s="61" t="s">
+        <v>2175</v>
+      </c>
       <c r="T582" s="20"/>
       <c r="U582" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#581</v>
       </c>
     </row>
     <row r="583">
-      <c r="A583" s="73"/>
-      <c r="B583" s="74"/>
-      <c r="C583" s="34"/>
-      <c r="D583" s="34"/>
-      <c r="E583" s="34"/>
+      <c r="A583" s="16" t="s">
+        <v>2179</v>
+      </c>
+      <c r="B583" s="6">
+        <v>44146.0</v>
+      </c>
+      <c r="C583" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D583" s="7" t="s">
+        <v>2139</v>
+      </c>
+      <c r="E583" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F583" s="34"/>
-      <c r="G583" s="34"/>
-      <c r="H583" s="21"/>
-      <c r="I583" s="19"/>
-      <c r="J583" s="10"/>
-      <c r="K583" s="22"/>
-      <c r="L583" s="23"/>
-      <c r="M583" s="22"/>
+      <c r="G583" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H583" s="8" t="s">
+        <v>2180</v>
+      </c>
+      <c r="I583" s="9">
+        <v>44132.0</v>
+      </c>
+      <c r="J583" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K583" s="13" t="s">
+        <v>2181</v>
+      </c>
+      <c r="L583" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M583" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N583" s="25"/>
-      <c r="O583" s="21"/>
-      <c r="P583" s="21"/>
+      <c r="O583" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P583" s="8" t="s">
+        <v>2182</v>
+      </c>
       <c r="Q583" s="19"/>
       <c r="R583" s="19"/>
-      <c r="S583" s="20"/>
+      <c r="S583" s="61" t="s">
+        <v>2183</v>
+      </c>
       <c r="T583" s="20"/>
       <c r="U583" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#582</v>
       </c>
     </row>
     <row r="584">
-      <c r="A584" s="73"/>
-      <c r="B584" s="74"/>
-      <c r="C584" s="34"/>
-      <c r="D584" s="34"/>
-      <c r="E584" s="34"/>
+      <c r="A584" s="16" t="s">
+        <v>2184</v>
+      </c>
+      <c r="B584" s="6">
+        <v>44146.0</v>
+      </c>
+      <c r="C584" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D584" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E584" s="7" t="s">
+        <v>1669</v>
+      </c>
       <c r="F584" s="34"/>
-      <c r="G584" s="34"/>
-      <c r="H584" s="21"/>
-      <c r="I584" s="19"/>
-      <c r="J584" s="10"/>
-      <c r="K584" s="22"/>
-      <c r="L584" s="23"/>
-      <c r="M584" s="22"/>
+      <c r="G584" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H584" s="8" t="s">
+        <v>2185</v>
+      </c>
+      <c r="I584" s="9">
+        <v>44129.0</v>
+      </c>
+      <c r="J584" s="10">
+        <v>44135.0</v>
+      </c>
+      <c r="K584" s="13" t="s">
+        <v>2181</v>
+      </c>
+      <c r="L584" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M584" s="13" t="s">
+        <v>1418</v>
+      </c>
       <c r="N584" s="25"/>
-      <c r="O584" s="21"/>
-      <c r="P584" s="21"/>
+      <c r="O584" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P584" s="8" t="s">
+        <v>2186</v>
+      </c>
       <c r="Q584" s="19"/>
       <c r="R584" s="19"/>
-      <c r="S584" s="20"/>
+      <c r="S584" s="61" t="s">
+        <v>2183</v>
+      </c>
       <c r="T584" s="20"/>
       <c r="U584" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#583</v>
       </c>
     </row>
     <row r="585">
-      <c r="A585" s="73"/>
-      <c r="B585" s="74"/>
-      <c r="C585" s="34"/>
-      <c r="D585" s="34"/>
-      <c r="E585" s="34"/>
+      <c r="A585" s="16" t="s">
+        <v>2187</v>
+      </c>
+      <c r="B585" s="6">
+        <v>44146.0</v>
+      </c>
+      <c r="C585" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D585" s="7" t="s">
+        <v>2139</v>
+      </c>
+      <c r="E585" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F585" s="34"/>
-      <c r="G585" s="34"/>
-      <c r="H585" s="21"/>
-      <c r="I585" s="19"/>
-      <c r="J585" s="10"/>
-      <c r="K585" s="22"/>
-      <c r="L585" s="23"/>
-      <c r="M585" s="22"/>
+      <c r="G585" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H585" s="8" t="s">
+        <v>2180</v>
+      </c>
+      <c r="I585" s="9">
+        <v>44132.0</v>
+      </c>
+      <c r="J585" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K585" s="13" t="s">
+        <v>2181</v>
+      </c>
+      <c r="L585" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M585" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N585" s="25"/>
-      <c r="O585" s="21"/>
-      <c r="P585" s="21"/>
+      <c r="O585" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P585" s="8" t="s">
+        <v>2182</v>
+      </c>
       <c r="Q585" s="19"/>
       <c r="R585" s="19"/>
-      <c r="S585" s="20"/>
+      <c r="S585" s="61" t="s">
+        <v>2183</v>
+      </c>
       <c r="T585" s="20"/>
       <c r="U585" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#584</v>
       </c>
     </row>
     <row r="586">
-      <c r="A586" s="73"/>
-      <c r="B586" s="74"/>
-      <c r="C586" s="34"/>
-      <c r="D586" s="34"/>
-      <c r="E586" s="34"/>
+      <c r="A586" s="16" t="s">
+        <v>2188</v>
+      </c>
+      <c r="B586" s="6">
+        <v>44146.0</v>
+      </c>
+      <c r="C586" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D586" s="7" t="s">
+        <v>2139</v>
+      </c>
+      <c r="E586" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F586" s="34"/>
-      <c r="G586" s="34"/>
-      <c r="H586" s="21"/>
-      <c r="I586" s="19"/>
-      <c r="J586" s="10"/>
-      <c r="K586" s="22"/>
-      <c r="L586" s="23"/>
-      <c r="M586" s="22"/>
+      <c r="G586" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H586" s="8" t="s">
+        <v>2180</v>
+      </c>
+      <c r="I586" s="9">
+        <v>44132.0</v>
+      </c>
+      <c r="J586" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K586" s="13" t="s">
+        <v>2181</v>
+      </c>
+      <c r="L586" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M586" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N586" s="25"/>
-      <c r="O586" s="21"/>
-      <c r="P586" s="21"/>
+      <c r="O586" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P586" s="8" t="s">
+        <v>2182</v>
+      </c>
       <c r="Q586" s="19"/>
       <c r="R586" s="19"/>
-      <c r="S586" s="20"/>
+      <c r="S586" s="61" t="s">
+        <v>2183</v>
+      </c>
       <c r="T586" s="20"/>
       <c r="U586" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#585</v>
       </c>
     </row>
     <row r="587">
@@ -43719,15 +43958,21 @@
     <hyperlink r:id="rId140" ref="S578"/>
     <hyperlink r:id="rId141" ref="S579"/>
     <hyperlink r:id="rId142" ref="S580"/>
+    <hyperlink r:id="rId143" ref="S581"/>
+    <hyperlink r:id="rId144" ref="S582"/>
+    <hyperlink r:id="rId145" ref="S583"/>
+    <hyperlink r:id="rId146" ref="S584"/>
+    <hyperlink r:id="rId147" ref="S585"/>
+    <hyperlink r:id="rId148" ref="S586"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId143"/>
-  <legacyDrawing r:id="rId144"/>
+  <drawing r:id="rId149"/>
+  <legacyDrawing r:id="rId150"/>
   <tableParts count="2">
-    <tablePart r:id="rId147"/>
-    <tablePart r:id="rId148"/>
+    <tablePart r:id="rId153"/>
+    <tablePart r:id="rId154"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201113
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -571,7 +571,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6528" uniqueCount="2189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6597" uniqueCount="2200">
   <si>
     <t>案例</t>
   </si>
@@ -8015,6 +8015,40 @@
   </si>
   <si>
     <t>#585</t>
+  </si>
+  <si>
+    <t>#586</t>
+  </si>
+  <si>
+    <t>2X-3X</t>
+  </si>
+  <si>
+    <t>-10/28(29) 印尼→台灣</t>
+  </si>
+  <si>
+    <t>10/28(29)</t>
+  </si>
+  <si>
+    <t>11/10(11) 採檢
+11/12 確診</t>
+  </si>
+  <si>
+    <t>國內新增5例境外移入COVID-19病例，均為印尼籍移工</t>
+  </si>
+  <si>
+    <t>#587</t>
+  </si>
+  <si>
+    <t>#588</t>
+  </si>
+  <si>
+    <t>#589</t>
+  </si>
+  <si>
+    <t>#590</t>
+  </si>
+  <si>
+    <t>輕微發燒</t>
   </si>
 </sst>
 </file>
@@ -9223,7 +9257,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:A601" displayName="Table_1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:A701" displayName="Table_1" id="1">
   <tableColumns count="1">
     <tableColumn name="案例" id="1"/>
   </tableColumns>
@@ -9232,7 +9266,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="B1:U601" displayName="Table_2" id="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="B1:U701" displayName="Table_2" id="2">
   <tableColumns count="20">
     <tableColumn name="新聞稿發布日期" id="1"/>
     <tableColumn name="性別" id="2"/>
@@ -9617,7 +9651,7 @@
         <v>國內首例確診患者已痊癒將出院 向防疫及醫護人員表達感謝</v>
       </c>
       <c r="U2" s="18" t="str">
-        <f t="shared" ref="U2:U601" si="1">A2</f>
+        <f t="shared" ref="U2:U701" si="1">A2</f>
         <v>#001</v>
       </c>
     </row>
@@ -43046,133 +43080,283 @@
       </c>
     </row>
     <row r="587">
-      <c r="A587" s="73"/>
-      <c r="B587" s="74"/>
-      <c r="C587" s="34"/>
-      <c r="D587" s="34"/>
-      <c r="E587" s="34"/>
+      <c r="A587" s="16" t="s">
+        <v>2189</v>
+      </c>
+      <c r="B587" s="6">
+        <v>44147.0</v>
+      </c>
+      <c r="C587" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D587" s="7" t="s">
+        <v>2190</v>
+      </c>
+      <c r="E587" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F587" s="34"/>
-      <c r="G587" s="34"/>
-      <c r="H587" s="21"/>
-      <c r="I587" s="19"/>
-      <c r="J587" s="10"/>
-      <c r="K587" s="22"/>
-      <c r="L587" s="23"/>
-      <c r="M587" s="22"/>
+      <c r="G587" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H587" s="8" t="s">
+        <v>2191</v>
+      </c>
+      <c r="I587" s="16" t="s">
+        <v>2192</v>
+      </c>
+      <c r="J587" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K587" s="13" t="s">
+        <v>2193</v>
+      </c>
+      <c r="L587" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M587" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N587" s="25"/>
-      <c r="O587" s="21"/>
-      <c r="P587" s="21"/>
+      <c r="O587" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P587" s="8" t="s">
+        <v>1777</v>
+      </c>
       <c r="Q587" s="19"/>
       <c r="R587" s="19"/>
-      <c r="S587" s="20"/>
+      <c r="S587" s="61" t="s">
+        <v>2194</v>
+      </c>
       <c r="T587" s="20"/>
       <c r="U587" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#586</v>
       </c>
     </row>
     <row r="588">
-      <c r="A588" s="73"/>
-      <c r="B588" s="74"/>
-      <c r="C588" s="34"/>
-      <c r="D588" s="34"/>
-      <c r="E588" s="34"/>
+      <c r="A588" s="16" t="s">
+        <v>2195</v>
+      </c>
+      <c r="B588" s="6">
+        <v>44147.0</v>
+      </c>
+      <c r="C588" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D588" s="7" t="s">
+        <v>2190</v>
+      </c>
+      <c r="E588" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F588" s="34"/>
-      <c r="G588" s="34"/>
-      <c r="H588" s="21"/>
-      <c r="I588" s="19"/>
-      <c r="J588" s="10"/>
-      <c r="K588" s="22"/>
-      <c r="L588" s="23"/>
-      <c r="M588" s="22"/>
+      <c r="G588" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H588" s="8" t="s">
+        <v>2191</v>
+      </c>
+      <c r="I588" s="16" t="s">
+        <v>2192</v>
+      </c>
+      <c r="J588" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K588" s="13" t="s">
+        <v>2193</v>
+      </c>
+      <c r="L588" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M588" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N588" s="25"/>
-      <c r="O588" s="21"/>
-      <c r="P588" s="21"/>
+      <c r="O588" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P588" s="8" t="s">
+        <v>1777</v>
+      </c>
       <c r="Q588" s="19"/>
       <c r="R588" s="19"/>
-      <c r="S588" s="20"/>
+      <c r="S588" s="61" t="s">
+        <v>2194</v>
+      </c>
       <c r="T588" s="20"/>
       <c r="U588" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#587</v>
       </c>
     </row>
     <row r="589">
-      <c r="A589" s="73"/>
-      <c r="B589" s="74"/>
-      <c r="C589" s="34"/>
-      <c r="D589" s="34"/>
-      <c r="E589" s="34"/>
+      <c r="A589" s="16" t="s">
+        <v>2196</v>
+      </c>
+      <c r="B589" s="6">
+        <v>44147.0</v>
+      </c>
+      <c r="C589" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D589" s="7" t="s">
+        <v>2190</v>
+      </c>
+      <c r="E589" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F589" s="34"/>
-      <c r="G589" s="34"/>
-      <c r="H589" s="21"/>
-      <c r="I589" s="19"/>
-      <c r="J589" s="10"/>
-      <c r="K589" s="22"/>
-      <c r="L589" s="23"/>
-      <c r="M589" s="22"/>
+      <c r="G589" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H589" s="8" t="s">
+        <v>2191</v>
+      </c>
+      <c r="I589" s="16" t="s">
+        <v>2192</v>
+      </c>
+      <c r="J589" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K589" s="13" t="s">
+        <v>2193</v>
+      </c>
+      <c r="L589" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M589" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N589" s="25"/>
-      <c r="O589" s="21"/>
-      <c r="P589" s="21"/>
+      <c r="O589" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P589" s="8" t="s">
+        <v>1777</v>
+      </c>
       <c r="Q589" s="19"/>
       <c r="R589" s="19"/>
-      <c r="S589" s="20"/>
+      <c r="S589" s="61" t="s">
+        <v>2194</v>
+      </c>
       <c r="T589" s="20"/>
       <c r="U589" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#588</v>
       </c>
     </row>
     <row r="590">
-      <c r="A590" s="73"/>
-      <c r="B590" s="74"/>
-      <c r="C590" s="34"/>
-      <c r="D590" s="34"/>
-      <c r="E590" s="34"/>
+      <c r="A590" s="16" t="s">
+        <v>2197</v>
+      </c>
+      <c r="B590" s="6">
+        <v>44147.0</v>
+      </c>
+      <c r="C590" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D590" s="7" t="s">
+        <v>2190</v>
+      </c>
+      <c r="E590" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F590" s="34"/>
-      <c r="G590" s="34"/>
-      <c r="H590" s="21"/>
-      <c r="I590" s="19"/>
-      <c r="J590" s="10"/>
-      <c r="K590" s="22"/>
-      <c r="L590" s="23"/>
-      <c r="M590" s="22"/>
+      <c r="G590" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H590" s="8" t="s">
+        <v>2191</v>
+      </c>
+      <c r="I590" s="16" t="s">
+        <v>2192</v>
+      </c>
+      <c r="J590" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K590" s="13" t="s">
+        <v>2193</v>
+      </c>
+      <c r="L590" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M590" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N590" s="25"/>
-      <c r="O590" s="21"/>
-      <c r="P590" s="21"/>
+      <c r="O590" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P590" s="8" t="s">
+        <v>1777</v>
+      </c>
       <c r="Q590" s="19"/>
       <c r="R590" s="19"/>
-      <c r="S590" s="20"/>
+      <c r="S590" s="61" t="s">
+        <v>2194</v>
+      </c>
       <c r="T590" s="20"/>
       <c r="U590" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#589</v>
       </c>
     </row>
     <row r="591">
-      <c r="A591" s="73"/>
-      <c r="B591" s="74"/>
-      <c r="C591" s="34"/>
-      <c r="D591" s="34"/>
-      <c r="E591" s="34"/>
+      <c r="A591" s="16" t="s">
+        <v>2198</v>
+      </c>
+      <c r="B591" s="6">
+        <v>44147.0</v>
+      </c>
+      <c r="C591" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D591" s="7" t="s">
+        <v>2190</v>
+      </c>
+      <c r="E591" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F591" s="34"/>
-      <c r="G591" s="34"/>
-      <c r="H591" s="21"/>
-      <c r="I591" s="19"/>
-      <c r="J591" s="10"/>
-      <c r="K591" s="22"/>
-      <c r="L591" s="23"/>
-      <c r="M591" s="22"/>
+      <c r="G591" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H591" s="8" t="s">
+        <v>2191</v>
+      </c>
+      <c r="I591" s="16" t="s">
+        <v>2192</v>
+      </c>
+      <c r="J591" s="10">
+        <v>44133.0</v>
+      </c>
+      <c r="K591" s="13" t="s">
+        <v>2193</v>
+      </c>
+      <c r="L591" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M591" s="13" t="s">
+        <v>2199</v>
+      </c>
       <c r="N591" s="25"/>
-      <c r="O591" s="21"/>
-      <c r="P591" s="21"/>
+      <c r="O591" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P591" s="8" t="s">
+        <v>1777</v>
+      </c>
       <c r="Q591" s="19"/>
       <c r="R591" s="19"/>
-      <c r="S591" s="20"/>
+      <c r="S591" s="61" t="s">
+        <v>2194</v>
+      </c>
       <c r="T591" s="20"/>
       <c r="U591" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#590</v>
       </c>
     </row>
     <row r="592">
@@ -43435,383 +43619,2983 @@
         <v/>
       </c>
     </row>
+    <row r="602">
+      <c r="A602" s="73"/>
+      <c r="B602" s="74"/>
+      <c r="C602" s="34"/>
+      <c r="D602" s="34"/>
+      <c r="E602" s="34"/>
+      <c r="F602" s="34"/>
+      <c r="G602" s="34"/>
+      <c r="H602" s="21"/>
+      <c r="I602" s="19"/>
+      <c r="J602" s="10"/>
+      <c r="K602" s="22"/>
+      <c r="L602" s="23"/>
+      <c r="M602" s="22"/>
+      <c r="N602" s="25"/>
+      <c r="O602" s="21"/>
+      <c r="P602" s="21"/>
+      <c r="Q602" s="19"/>
+      <c r="R602" s="19"/>
+      <c r="S602" s="20"/>
+      <c r="T602" s="20"/>
+      <c r="U602" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" s="73"/>
+      <c r="B603" s="74"/>
+      <c r="C603" s="34"/>
+      <c r="D603" s="34"/>
+      <c r="E603" s="34"/>
+      <c r="F603" s="34"/>
+      <c r="G603" s="34"/>
+      <c r="H603" s="21"/>
+      <c r="I603" s="19"/>
+      <c r="J603" s="10"/>
+      <c r="K603" s="22"/>
+      <c r="L603" s="23"/>
+      <c r="M603" s="22"/>
+      <c r="N603" s="25"/>
+      <c r="O603" s="21"/>
+      <c r="P603" s="21"/>
+      <c r="Q603" s="19"/>
+      <c r="R603" s="19"/>
+      <c r="S603" s="20"/>
+      <c r="T603" s="20"/>
+      <c r="U603" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" s="73"/>
+      <c r="B604" s="74"/>
+      <c r="C604" s="34"/>
+      <c r="D604" s="34"/>
+      <c r="E604" s="34"/>
+      <c r="F604" s="34"/>
+      <c r="G604" s="34"/>
+      <c r="H604" s="21"/>
+      <c r="I604" s="19"/>
+      <c r="J604" s="10"/>
+      <c r="K604" s="22"/>
+      <c r="L604" s="23"/>
+      <c r="M604" s="22"/>
+      <c r="N604" s="25"/>
+      <c r="O604" s="21"/>
+      <c r="P604" s="21"/>
+      <c r="Q604" s="19"/>
+      <c r="R604" s="19"/>
+      <c r="S604" s="20"/>
+      <c r="T604" s="20"/>
+      <c r="U604" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" s="73"/>
+      <c r="B605" s="74"/>
+      <c r="C605" s="34"/>
+      <c r="D605" s="34"/>
+      <c r="E605" s="34"/>
+      <c r="F605" s="34"/>
+      <c r="G605" s="34"/>
+      <c r="H605" s="21"/>
+      <c r="I605" s="19"/>
+      <c r="J605" s="10"/>
+      <c r="K605" s="22"/>
+      <c r="L605" s="23"/>
+      <c r="M605" s="22"/>
+      <c r="N605" s="25"/>
+      <c r="O605" s="21"/>
+      <c r="P605" s="21"/>
+      <c r="Q605" s="19"/>
+      <c r="R605" s="19"/>
+      <c r="S605" s="20"/>
+      <c r="T605" s="20"/>
+      <c r="U605" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" s="73"/>
+      <c r="B606" s="74"/>
+      <c r="C606" s="34"/>
+      <c r="D606" s="34"/>
+      <c r="E606" s="34"/>
+      <c r="F606" s="34"/>
+      <c r="G606" s="34"/>
+      <c r="H606" s="21"/>
+      <c r="I606" s="19"/>
+      <c r="J606" s="10"/>
+      <c r="K606" s="22"/>
+      <c r="L606" s="23"/>
+      <c r="M606" s="22"/>
+      <c r="N606" s="25"/>
+      <c r="O606" s="21"/>
+      <c r="P606" s="21"/>
+      <c r="Q606" s="19"/>
+      <c r="R606" s="19"/>
+      <c r="S606" s="20"/>
+      <c r="T606" s="20"/>
+      <c r="U606" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" s="73"/>
+      <c r="B607" s="74"/>
+      <c r="C607" s="34"/>
+      <c r="D607" s="34"/>
+      <c r="E607" s="34"/>
+      <c r="F607" s="34"/>
+      <c r="G607" s="34"/>
+      <c r="H607" s="21"/>
+      <c r="I607" s="19"/>
+      <c r="J607" s="10"/>
+      <c r="K607" s="22"/>
+      <c r="L607" s="23"/>
+      <c r="M607" s="22"/>
+      <c r="N607" s="25"/>
+      <c r="O607" s="21"/>
+      <c r="P607" s="21"/>
+      <c r="Q607" s="19"/>
+      <c r="R607" s="19"/>
+      <c r="S607" s="20"/>
+      <c r="T607" s="20"/>
+      <c r="U607" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" s="73"/>
+      <c r="B608" s="74"/>
+      <c r="C608" s="34"/>
+      <c r="D608" s="34"/>
+      <c r="E608" s="34"/>
+      <c r="F608" s="34"/>
+      <c r="G608" s="34"/>
+      <c r="H608" s="21"/>
+      <c r="I608" s="19"/>
+      <c r="J608" s="10"/>
+      <c r="K608" s="22"/>
+      <c r="L608" s="23"/>
+      <c r="M608" s="22"/>
+      <c r="N608" s="25"/>
+      <c r="O608" s="21"/>
+      <c r="P608" s="21"/>
+      <c r="Q608" s="19"/>
+      <c r="R608" s="19"/>
+      <c r="S608" s="20"/>
+      <c r="T608" s="20"/>
+      <c r="U608" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" s="73"/>
+      <c r="B609" s="74"/>
+      <c r="C609" s="34"/>
+      <c r="D609" s="34"/>
+      <c r="E609" s="34"/>
+      <c r="F609" s="34"/>
+      <c r="G609" s="34"/>
+      <c r="H609" s="21"/>
+      <c r="I609" s="19"/>
+      <c r="J609" s="10"/>
+      <c r="K609" s="22"/>
+      <c r="L609" s="23"/>
+      <c r="M609" s="22"/>
+      <c r="N609" s="25"/>
+      <c r="O609" s="21"/>
+      <c r="P609" s="21"/>
+      <c r="Q609" s="19"/>
+      <c r="R609" s="19"/>
+      <c r="S609" s="20"/>
+      <c r="T609" s="20"/>
+      <c r="U609" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" s="73"/>
+      <c r="B610" s="74"/>
+      <c r="C610" s="34"/>
+      <c r="D610" s="34"/>
+      <c r="E610" s="34"/>
+      <c r="F610" s="34"/>
+      <c r="G610" s="34"/>
+      <c r="H610" s="21"/>
+      <c r="I610" s="19"/>
+      <c r="J610" s="10"/>
+      <c r="K610" s="22"/>
+      <c r="L610" s="23"/>
+      <c r="M610" s="22"/>
+      <c r="N610" s="25"/>
+      <c r="O610" s="21"/>
+      <c r="P610" s="21"/>
+      <c r="Q610" s="19"/>
+      <c r="R610" s="19"/>
+      <c r="S610" s="20"/>
+      <c r="T610" s="20"/>
+      <c r="U610" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" s="73"/>
+      <c r="B611" s="74"/>
+      <c r="C611" s="34"/>
+      <c r="D611" s="34"/>
+      <c r="E611" s="34"/>
+      <c r="F611" s="34"/>
+      <c r="G611" s="34"/>
+      <c r="H611" s="21"/>
+      <c r="I611" s="19"/>
+      <c r="J611" s="10"/>
+      <c r="K611" s="22"/>
+      <c r="L611" s="23"/>
+      <c r="M611" s="22"/>
+      <c r="N611" s="25"/>
+      <c r="O611" s="21"/>
+      <c r="P611" s="21"/>
+      <c r="Q611" s="19"/>
+      <c r="R611" s="19"/>
+      <c r="S611" s="20"/>
+      <c r="T611" s="20"/>
+      <c r="U611" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" s="73"/>
+      <c r="B612" s="74"/>
+      <c r="C612" s="34"/>
+      <c r="D612" s="34"/>
+      <c r="E612" s="34"/>
+      <c r="F612" s="34"/>
+      <c r="G612" s="34"/>
+      <c r="H612" s="21"/>
+      <c r="I612" s="19"/>
+      <c r="J612" s="10"/>
+      <c r="K612" s="22"/>
+      <c r="L612" s="23"/>
+      <c r="M612" s="22"/>
+      <c r="N612" s="25"/>
+      <c r="O612" s="21"/>
+      <c r="P612" s="21"/>
+      <c r="Q612" s="19"/>
+      <c r="R612" s="19"/>
+      <c r="S612" s="20"/>
+      <c r="T612" s="20"/>
+      <c r="U612" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" s="73"/>
+      <c r="B613" s="74"/>
+      <c r="C613" s="34"/>
+      <c r="D613" s="34"/>
+      <c r="E613" s="34"/>
+      <c r="F613" s="34"/>
+      <c r="G613" s="34"/>
+      <c r="H613" s="21"/>
+      <c r="I613" s="19"/>
+      <c r="J613" s="10"/>
+      <c r="K613" s="22"/>
+      <c r="L613" s="23"/>
+      <c r="M613" s="22"/>
+      <c r="N613" s="25"/>
+      <c r="O613" s="21"/>
+      <c r="P613" s="21"/>
+      <c r="Q613" s="19"/>
+      <c r="R613" s="19"/>
+      <c r="S613" s="20"/>
+      <c r="T613" s="20"/>
+      <c r="U613" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" s="73"/>
+      <c r="B614" s="74"/>
+      <c r="C614" s="34"/>
+      <c r="D614" s="34"/>
+      <c r="E614" s="34"/>
+      <c r="F614" s="34"/>
+      <c r="G614" s="34"/>
+      <c r="H614" s="21"/>
+      <c r="I614" s="19"/>
+      <c r="J614" s="10"/>
+      <c r="K614" s="22"/>
+      <c r="L614" s="23"/>
+      <c r="M614" s="22"/>
+      <c r="N614" s="25"/>
+      <c r="O614" s="21"/>
+      <c r="P614" s="21"/>
+      <c r="Q614" s="19"/>
+      <c r="R614" s="19"/>
+      <c r="S614" s="20"/>
+      <c r="T614" s="20"/>
+      <c r="U614" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" s="73"/>
+      <c r="B615" s="74"/>
+      <c r="C615" s="34"/>
+      <c r="D615" s="34"/>
+      <c r="E615" s="34"/>
+      <c r="F615" s="34"/>
+      <c r="G615" s="34"/>
+      <c r="H615" s="21"/>
+      <c r="I615" s="19"/>
+      <c r="J615" s="10"/>
+      <c r="K615" s="22"/>
+      <c r="L615" s="23"/>
+      <c r="M615" s="22"/>
+      <c r="N615" s="25"/>
+      <c r="O615" s="21"/>
+      <c r="P615" s="21"/>
+      <c r="Q615" s="19"/>
+      <c r="R615" s="19"/>
+      <c r="S615" s="20"/>
+      <c r="T615" s="20"/>
+      <c r="U615" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" s="73"/>
+      <c r="B616" s="74"/>
+      <c r="C616" s="34"/>
+      <c r="D616" s="34"/>
+      <c r="E616" s="34"/>
+      <c r="F616" s="34"/>
+      <c r="G616" s="34"/>
+      <c r="H616" s="21"/>
+      <c r="I616" s="19"/>
+      <c r="J616" s="10"/>
+      <c r="K616" s="22"/>
+      <c r="L616" s="23"/>
+      <c r="M616" s="22"/>
+      <c r="N616" s="25"/>
+      <c r="O616" s="21"/>
+      <c r="P616" s="21"/>
+      <c r="Q616" s="19"/>
+      <c r="R616" s="19"/>
+      <c r="S616" s="20"/>
+      <c r="T616" s="20"/>
+      <c r="U616" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" s="73"/>
+      <c r="B617" s="74"/>
+      <c r="C617" s="34"/>
+      <c r="D617" s="34"/>
+      <c r="E617" s="34"/>
+      <c r="F617" s="34"/>
+      <c r="G617" s="34"/>
+      <c r="H617" s="21"/>
+      <c r="I617" s="19"/>
+      <c r="J617" s="10"/>
+      <c r="K617" s="22"/>
+      <c r="L617" s="23"/>
+      <c r="M617" s="22"/>
+      <c r="N617" s="25"/>
+      <c r="O617" s="21"/>
+      <c r="P617" s="21"/>
+      <c r="Q617" s="19"/>
+      <c r="R617" s="19"/>
+      <c r="S617" s="20"/>
+      <c r="T617" s="20"/>
+      <c r="U617" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" s="73"/>
+      <c r="B618" s="74"/>
+      <c r="C618" s="34"/>
+      <c r="D618" s="34"/>
+      <c r="E618" s="34"/>
+      <c r="F618" s="34"/>
+      <c r="G618" s="34"/>
+      <c r="H618" s="21"/>
+      <c r="I618" s="19"/>
+      <c r="J618" s="10"/>
+      <c r="K618" s="22"/>
+      <c r="L618" s="23"/>
+      <c r="M618" s="22"/>
+      <c r="N618" s="25"/>
+      <c r="O618" s="21"/>
+      <c r="P618" s="21"/>
+      <c r="Q618" s="19"/>
+      <c r="R618" s="19"/>
+      <c r="S618" s="20"/>
+      <c r="T618" s="20"/>
+      <c r="U618" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" s="73"/>
+      <c r="B619" s="74"/>
+      <c r="C619" s="34"/>
+      <c r="D619" s="34"/>
+      <c r="E619" s="34"/>
+      <c r="F619" s="34"/>
+      <c r="G619" s="34"/>
+      <c r="H619" s="21"/>
+      <c r="I619" s="19"/>
+      <c r="J619" s="10"/>
+      <c r="K619" s="22"/>
+      <c r="L619" s="23"/>
+      <c r="M619" s="22"/>
+      <c r="N619" s="25"/>
+      <c r="O619" s="21"/>
+      <c r="P619" s="21"/>
+      <c r="Q619" s="19"/>
+      <c r="R619" s="19"/>
+      <c r="S619" s="20"/>
+      <c r="T619" s="20"/>
+      <c r="U619" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" s="73"/>
+      <c r="B620" s="74"/>
+      <c r="C620" s="34"/>
+      <c r="D620" s="34"/>
+      <c r="E620" s="34"/>
+      <c r="F620" s="34"/>
+      <c r="G620" s="34"/>
+      <c r="H620" s="21"/>
+      <c r="I620" s="19"/>
+      <c r="J620" s="10"/>
+      <c r="K620" s="22"/>
+      <c r="L620" s="23"/>
+      <c r="M620" s="22"/>
+      <c r="N620" s="25"/>
+      <c r="O620" s="21"/>
+      <c r="P620" s="21"/>
+      <c r="Q620" s="19"/>
+      <c r="R620" s="19"/>
+      <c r="S620" s="20"/>
+      <c r="T620" s="20"/>
+      <c r="U620" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" s="73"/>
+      <c r="B621" s="74"/>
+      <c r="C621" s="34"/>
+      <c r="D621" s="34"/>
+      <c r="E621" s="34"/>
+      <c r="F621" s="34"/>
+      <c r="G621" s="34"/>
+      <c r="H621" s="21"/>
+      <c r="I621" s="19"/>
+      <c r="J621" s="10"/>
+      <c r="K621" s="22"/>
+      <c r="L621" s="23"/>
+      <c r="M621" s="22"/>
+      <c r="N621" s="25"/>
+      <c r="O621" s="21"/>
+      <c r="P621" s="21"/>
+      <c r="Q621" s="19"/>
+      <c r="R621" s="19"/>
+      <c r="S621" s="20"/>
+      <c r="T621" s="20"/>
+      <c r="U621" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" s="73"/>
+      <c r="B622" s="74"/>
+      <c r="C622" s="34"/>
+      <c r="D622" s="34"/>
+      <c r="E622" s="34"/>
+      <c r="F622" s="34"/>
+      <c r="G622" s="34"/>
+      <c r="H622" s="21"/>
+      <c r="I622" s="19"/>
+      <c r="J622" s="10"/>
+      <c r="K622" s="22"/>
+      <c r="L622" s="23"/>
+      <c r="M622" s="22"/>
+      <c r="N622" s="25"/>
+      <c r="O622" s="21"/>
+      <c r="P622" s="21"/>
+      <c r="Q622" s="19"/>
+      <c r="R622" s="19"/>
+      <c r="S622" s="20"/>
+      <c r="T622" s="20"/>
+      <c r="U622" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" s="73"/>
+      <c r="B623" s="74"/>
+      <c r="C623" s="34"/>
+      <c r="D623" s="34"/>
+      <c r="E623" s="34"/>
+      <c r="F623" s="34"/>
+      <c r="G623" s="34"/>
+      <c r="H623" s="21"/>
+      <c r="I623" s="19"/>
+      <c r="J623" s="10"/>
+      <c r="K623" s="22"/>
+      <c r="L623" s="23"/>
+      <c r="M623" s="22"/>
+      <c r="N623" s="25"/>
+      <c r="O623" s="21"/>
+      <c r="P623" s="21"/>
+      <c r="Q623" s="19"/>
+      <c r="R623" s="19"/>
+      <c r="S623" s="20"/>
+      <c r="T623" s="20"/>
+      <c r="U623" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" s="73"/>
+      <c r="B624" s="74"/>
+      <c r="C624" s="34"/>
+      <c r="D624" s="34"/>
+      <c r="E624" s="34"/>
+      <c r="F624" s="34"/>
+      <c r="G624" s="34"/>
+      <c r="H624" s="21"/>
+      <c r="I624" s="19"/>
+      <c r="J624" s="10"/>
+      <c r="K624" s="22"/>
+      <c r="L624" s="23"/>
+      <c r="M624" s="22"/>
+      <c r="N624" s="25"/>
+      <c r="O624" s="21"/>
+      <c r="P624" s="21"/>
+      <c r="Q624" s="19"/>
+      <c r="R624" s="19"/>
+      <c r="S624" s="20"/>
+      <c r="T624" s="20"/>
+      <c r="U624" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" s="73"/>
+      <c r="B625" s="74"/>
+      <c r="C625" s="34"/>
+      <c r="D625" s="34"/>
+      <c r="E625" s="34"/>
+      <c r="F625" s="34"/>
+      <c r="G625" s="34"/>
+      <c r="H625" s="21"/>
+      <c r="I625" s="19"/>
+      <c r="J625" s="10"/>
+      <c r="K625" s="22"/>
+      <c r="L625" s="23"/>
+      <c r="M625" s="22"/>
+      <c r="N625" s="25"/>
+      <c r="O625" s="21"/>
+      <c r="P625" s="21"/>
+      <c r="Q625" s="19"/>
+      <c r="R625" s="19"/>
+      <c r="S625" s="20"/>
+      <c r="T625" s="20"/>
+      <c r="U625" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" s="73"/>
+      <c r="B626" s="74"/>
+      <c r="C626" s="34"/>
+      <c r="D626" s="34"/>
+      <c r="E626" s="34"/>
+      <c r="F626" s="34"/>
+      <c r="G626" s="34"/>
+      <c r="H626" s="21"/>
+      <c r="I626" s="19"/>
+      <c r="J626" s="10"/>
+      <c r="K626" s="22"/>
+      <c r="L626" s="23"/>
+      <c r="M626" s="22"/>
+      <c r="N626" s="25"/>
+      <c r="O626" s="21"/>
+      <c r="P626" s="21"/>
+      <c r="Q626" s="19"/>
+      <c r="R626" s="19"/>
+      <c r="S626" s="20"/>
+      <c r="T626" s="20"/>
+      <c r="U626" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" s="73"/>
+      <c r="B627" s="74"/>
+      <c r="C627" s="34"/>
+      <c r="D627" s="34"/>
+      <c r="E627" s="34"/>
+      <c r="F627" s="34"/>
+      <c r="G627" s="34"/>
+      <c r="H627" s="21"/>
+      <c r="I627" s="19"/>
+      <c r="J627" s="10"/>
+      <c r="K627" s="22"/>
+      <c r="L627" s="23"/>
+      <c r="M627" s="22"/>
+      <c r="N627" s="25"/>
+      <c r="O627" s="21"/>
+      <c r="P627" s="21"/>
+      <c r="Q627" s="19"/>
+      <c r="R627" s="19"/>
+      <c r="S627" s="20"/>
+      <c r="T627" s="20"/>
+      <c r="U627" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" s="73"/>
+      <c r="B628" s="74"/>
+      <c r="C628" s="34"/>
+      <c r="D628" s="34"/>
+      <c r="E628" s="34"/>
+      <c r="F628" s="34"/>
+      <c r="G628" s="34"/>
+      <c r="H628" s="21"/>
+      <c r="I628" s="19"/>
+      <c r="J628" s="10"/>
+      <c r="K628" s="22"/>
+      <c r="L628" s="23"/>
+      <c r="M628" s="22"/>
+      <c r="N628" s="25"/>
+      <c r="O628" s="21"/>
+      <c r="P628" s="21"/>
+      <c r="Q628" s="19"/>
+      <c r="R628" s="19"/>
+      <c r="S628" s="20"/>
+      <c r="T628" s="20"/>
+      <c r="U628" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" s="73"/>
+      <c r="B629" s="74"/>
+      <c r="C629" s="34"/>
+      <c r="D629" s="34"/>
+      <c r="E629" s="34"/>
+      <c r="F629" s="34"/>
+      <c r="G629" s="34"/>
+      <c r="H629" s="21"/>
+      <c r="I629" s="19"/>
+      <c r="J629" s="10"/>
+      <c r="K629" s="22"/>
+      <c r="L629" s="23"/>
+      <c r="M629" s="22"/>
+      <c r="N629" s="25"/>
+      <c r="O629" s="21"/>
+      <c r="P629" s="21"/>
+      <c r="Q629" s="19"/>
+      <c r="R629" s="19"/>
+      <c r="S629" s="20"/>
+      <c r="T629" s="20"/>
+      <c r="U629" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" s="73"/>
+      <c r="B630" s="74"/>
+      <c r="C630" s="34"/>
+      <c r="D630" s="34"/>
+      <c r="E630" s="34"/>
+      <c r="F630" s="34"/>
+      <c r="G630" s="34"/>
+      <c r="H630" s="21"/>
+      <c r="I630" s="19"/>
+      <c r="J630" s="10"/>
+      <c r="K630" s="22"/>
+      <c r="L630" s="23"/>
+      <c r="M630" s="22"/>
+      <c r="N630" s="25"/>
+      <c r="O630" s="21"/>
+      <c r="P630" s="21"/>
+      <c r="Q630" s="19"/>
+      <c r="R630" s="19"/>
+      <c r="S630" s="20"/>
+      <c r="T630" s="20"/>
+      <c r="U630" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" s="73"/>
+      <c r="B631" s="74"/>
+      <c r="C631" s="34"/>
+      <c r="D631" s="34"/>
+      <c r="E631" s="34"/>
+      <c r="F631" s="34"/>
+      <c r="G631" s="34"/>
+      <c r="H631" s="21"/>
+      <c r="I631" s="19"/>
+      <c r="J631" s="10"/>
+      <c r="K631" s="22"/>
+      <c r="L631" s="23"/>
+      <c r="M631" s="22"/>
+      <c r="N631" s="25"/>
+      <c r="O631" s="21"/>
+      <c r="P631" s="21"/>
+      <c r="Q631" s="19"/>
+      <c r="R631" s="19"/>
+      <c r="S631" s="20"/>
+      <c r="T631" s="20"/>
+      <c r="U631" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" s="73"/>
+      <c r="B632" s="74"/>
+      <c r="C632" s="34"/>
+      <c r="D632" s="34"/>
+      <c r="E632" s="34"/>
+      <c r="F632" s="34"/>
+      <c r="G632" s="34"/>
+      <c r="H632" s="21"/>
+      <c r="I632" s="19"/>
+      <c r="J632" s="10"/>
+      <c r="K632" s="22"/>
+      <c r="L632" s="23"/>
+      <c r="M632" s="22"/>
+      <c r="N632" s="25"/>
+      <c r="O632" s="21"/>
+      <c r="P632" s="21"/>
+      <c r="Q632" s="19"/>
+      <c r="R632" s="19"/>
+      <c r="S632" s="20"/>
+      <c r="T632" s="20"/>
+      <c r="U632" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" s="73"/>
+      <c r="B633" s="74"/>
+      <c r="C633" s="34"/>
+      <c r="D633" s="34"/>
+      <c r="E633" s="34"/>
+      <c r="F633" s="34"/>
+      <c r="G633" s="34"/>
+      <c r="H633" s="21"/>
+      <c r="I633" s="19"/>
+      <c r="J633" s="10"/>
+      <c r="K633" s="22"/>
+      <c r="L633" s="23"/>
+      <c r="M633" s="22"/>
+      <c r="N633" s="25"/>
+      <c r="O633" s="21"/>
+      <c r="P633" s="21"/>
+      <c r="Q633" s="19"/>
+      <c r="R633" s="19"/>
+      <c r="S633" s="20"/>
+      <c r="T633" s="20"/>
+      <c r="U633" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" s="73"/>
+      <c r="B634" s="74"/>
+      <c r="C634" s="34"/>
+      <c r="D634" s="34"/>
+      <c r="E634" s="34"/>
+      <c r="F634" s="34"/>
+      <c r="G634" s="34"/>
+      <c r="H634" s="21"/>
+      <c r="I634" s="19"/>
+      <c r="J634" s="10"/>
+      <c r="K634" s="22"/>
+      <c r="L634" s="23"/>
+      <c r="M634" s="22"/>
+      <c r="N634" s="25"/>
+      <c r="O634" s="21"/>
+      <c r="P634" s="21"/>
+      <c r="Q634" s="19"/>
+      <c r="R634" s="19"/>
+      <c r="S634" s="20"/>
+      <c r="T634" s="20"/>
+      <c r="U634" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" s="73"/>
+      <c r="B635" s="74"/>
+      <c r="C635" s="34"/>
+      <c r="D635" s="34"/>
+      <c r="E635" s="34"/>
+      <c r="F635" s="34"/>
+      <c r="G635" s="34"/>
+      <c r="H635" s="21"/>
+      <c r="I635" s="19"/>
+      <c r="J635" s="10"/>
+      <c r="K635" s="22"/>
+      <c r="L635" s="23"/>
+      <c r="M635" s="22"/>
+      <c r="N635" s="25"/>
+      <c r="O635" s="21"/>
+      <c r="P635" s="21"/>
+      <c r="Q635" s="19"/>
+      <c r="R635" s="19"/>
+      <c r="S635" s="20"/>
+      <c r="T635" s="20"/>
+      <c r="U635" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" s="73"/>
+      <c r="B636" s="74"/>
+      <c r="C636" s="34"/>
+      <c r="D636" s="34"/>
+      <c r="E636" s="34"/>
+      <c r="F636" s="34"/>
+      <c r="G636" s="34"/>
+      <c r="H636" s="21"/>
+      <c r="I636" s="19"/>
+      <c r="J636" s="10"/>
+      <c r="K636" s="22"/>
+      <c r="L636" s="23"/>
+      <c r="M636" s="22"/>
+      <c r="N636" s="25"/>
+      <c r="O636" s="21"/>
+      <c r="P636" s="21"/>
+      <c r="Q636" s="19"/>
+      <c r="R636" s="19"/>
+      <c r="S636" s="20"/>
+      <c r="T636" s="20"/>
+      <c r="U636" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" s="73"/>
+      <c r="B637" s="74"/>
+      <c r="C637" s="34"/>
+      <c r="D637" s="34"/>
+      <c r="E637" s="34"/>
+      <c r="F637" s="34"/>
+      <c r="G637" s="34"/>
+      <c r="H637" s="21"/>
+      <c r="I637" s="19"/>
+      <c r="J637" s="10"/>
+      <c r="K637" s="22"/>
+      <c r="L637" s="23"/>
+      <c r="M637" s="22"/>
+      <c r="N637" s="25"/>
+      <c r="O637" s="21"/>
+      <c r="P637" s="21"/>
+      <c r="Q637" s="19"/>
+      <c r="R637" s="19"/>
+      <c r="S637" s="20"/>
+      <c r="T637" s="20"/>
+      <c r="U637" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" s="73"/>
+      <c r="B638" s="74"/>
+      <c r="C638" s="34"/>
+      <c r="D638" s="34"/>
+      <c r="E638" s="34"/>
+      <c r="F638" s="34"/>
+      <c r="G638" s="34"/>
+      <c r="H638" s="21"/>
+      <c r="I638" s="19"/>
+      <c r="J638" s="10"/>
+      <c r="K638" s="22"/>
+      <c r="L638" s="23"/>
+      <c r="M638" s="22"/>
+      <c r="N638" s="25"/>
+      <c r="O638" s="21"/>
+      <c r="P638" s="21"/>
+      <c r="Q638" s="19"/>
+      <c r="R638" s="19"/>
+      <c r="S638" s="20"/>
+      <c r="T638" s="20"/>
+      <c r="U638" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" s="73"/>
+      <c r="B639" s="74"/>
+      <c r="C639" s="34"/>
+      <c r="D639" s="34"/>
+      <c r="E639" s="34"/>
+      <c r="F639" s="34"/>
+      <c r="G639" s="34"/>
+      <c r="H639" s="21"/>
+      <c r="I639" s="19"/>
+      <c r="J639" s="10"/>
+      <c r="K639" s="22"/>
+      <c r="L639" s="23"/>
+      <c r="M639" s="22"/>
+      <c r="N639" s="25"/>
+      <c r="O639" s="21"/>
+      <c r="P639" s="21"/>
+      <c r="Q639" s="19"/>
+      <c r="R639" s="19"/>
+      <c r="S639" s="20"/>
+      <c r="T639" s="20"/>
+      <c r="U639" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" s="73"/>
+      <c r="B640" s="74"/>
+      <c r="C640" s="34"/>
+      <c r="D640" s="34"/>
+      <c r="E640" s="34"/>
+      <c r="F640" s="34"/>
+      <c r="G640" s="34"/>
+      <c r="H640" s="21"/>
+      <c r="I640" s="19"/>
+      <c r="J640" s="10"/>
+      <c r="K640" s="22"/>
+      <c r="L640" s="23"/>
+      <c r="M640" s="22"/>
+      <c r="N640" s="25"/>
+      <c r="O640" s="21"/>
+      <c r="P640" s="21"/>
+      <c r="Q640" s="19"/>
+      <c r="R640" s="19"/>
+      <c r="S640" s="20"/>
+      <c r="T640" s="20"/>
+      <c r="U640" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" s="73"/>
+      <c r="B641" s="74"/>
+      <c r="C641" s="34"/>
+      <c r="D641" s="34"/>
+      <c r="E641" s="34"/>
+      <c r="F641" s="34"/>
+      <c r="G641" s="34"/>
+      <c r="H641" s="21"/>
+      <c r="I641" s="19"/>
+      <c r="J641" s="10"/>
+      <c r="K641" s="22"/>
+      <c r="L641" s="23"/>
+      <c r="M641" s="22"/>
+      <c r="N641" s="25"/>
+      <c r="O641" s="21"/>
+      <c r="P641" s="21"/>
+      <c r="Q641" s="19"/>
+      <c r="R641" s="19"/>
+      <c r="S641" s="20"/>
+      <c r="T641" s="20"/>
+      <c r="U641" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" s="73"/>
+      <c r="B642" s="74"/>
+      <c r="C642" s="34"/>
+      <c r="D642" s="34"/>
+      <c r="E642" s="34"/>
+      <c r="F642" s="34"/>
+      <c r="G642" s="34"/>
+      <c r="H642" s="21"/>
+      <c r="I642" s="19"/>
+      <c r="J642" s="10"/>
+      <c r="K642" s="22"/>
+      <c r="L642" s="23"/>
+      <c r="M642" s="22"/>
+      <c r="N642" s="25"/>
+      <c r="O642" s="21"/>
+      <c r="P642" s="21"/>
+      <c r="Q642" s="19"/>
+      <c r="R642" s="19"/>
+      <c r="S642" s="20"/>
+      <c r="T642" s="20"/>
+      <c r="U642" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" s="73"/>
+      <c r="B643" s="74"/>
+      <c r="C643" s="34"/>
+      <c r="D643" s="34"/>
+      <c r="E643" s="34"/>
+      <c r="F643" s="34"/>
+      <c r="G643" s="34"/>
+      <c r="H643" s="21"/>
+      <c r="I643" s="19"/>
+      <c r="J643" s="10"/>
+      <c r="K643" s="22"/>
+      <c r="L643" s="23"/>
+      <c r="M643" s="22"/>
+      <c r="N643" s="25"/>
+      <c r="O643" s="21"/>
+      <c r="P643" s="21"/>
+      <c r="Q643" s="19"/>
+      <c r="R643" s="19"/>
+      <c r="S643" s="20"/>
+      <c r="T643" s="20"/>
+      <c r="U643" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" s="73"/>
+      <c r="B644" s="74"/>
+      <c r="C644" s="34"/>
+      <c r="D644" s="34"/>
+      <c r="E644" s="34"/>
+      <c r="F644" s="34"/>
+      <c r="G644" s="34"/>
+      <c r="H644" s="21"/>
+      <c r="I644" s="19"/>
+      <c r="J644" s="10"/>
+      <c r="K644" s="22"/>
+      <c r="L644" s="23"/>
+      <c r="M644" s="22"/>
+      <c r="N644" s="25"/>
+      <c r="O644" s="21"/>
+      <c r="P644" s="21"/>
+      <c r="Q644" s="19"/>
+      <c r="R644" s="19"/>
+      <c r="S644" s="20"/>
+      <c r="T644" s="20"/>
+      <c r="U644" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" s="73"/>
+      <c r="B645" s="74"/>
+      <c r="C645" s="34"/>
+      <c r="D645" s="34"/>
+      <c r="E645" s="34"/>
+      <c r="F645" s="34"/>
+      <c r="G645" s="34"/>
+      <c r="H645" s="21"/>
+      <c r="I645" s="19"/>
+      <c r="J645" s="10"/>
+      <c r="K645" s="22"/>
+      <c r="L645" s="23"/>
+      <c r="M645" s="22"/>
+      <c r="N645" s="25"/>
+      <c r="O645" s="21"/>
+      <c r="P645" s="21"/>
+      <c r="Q645" s="19"/>
+      <c r="R645" s="19"/>
+      <c r="S645" s="20"/>
+      <c r="T645" s="20"/>
+      <c r="U645" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" s="73"/>
+      <c r="B646" s="74"/>
+      <c r="C646" s="34"/>
+      <c r="D646" s="34"/>
+      <c r="E646" s="34"/>
+      <c r="F646" s="34"/>
+      <c r="G646" s="34"/>
+      <c r="H646" s="21"/>
+      <c r="I646" s="19"/>
+      <c r="J646" s="10"/>
+      <c r="K646" s="22"/>
+      <c r="L646" s="23"/>
+      <c r="M646" s="22"/>
+      <c r="N646" s="25"/>
+      <c r="O646" s="21"/>
+      <c r="P646" s="21"/>
+      <c r="Q646" s="19"/>
+      <c r="R646" s="19"/>
+      <c r="S646" s="20"/>
+      <c r="T646" s="20"/>
+      <c r="U646" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" s="73"/>
+      <c r="B647" s="74"/>
+      <c r="C647" s="34"/>
+      <c r="D647" s="34"/>
+      <c r="E647" s="34"/>
+      <c r="F647" s="34"/>
+      <c r="G647" s="34"/>
+      <c r="H647" s="21"/>
+      <c r="I647" s="19"/>
+      <c r="J647" s="10"/>
+      <c r="K647" s="22"/>
+      <c r="L647" s="23"/>
+      <c r="M647" s="22"/>
+      <c r="N647" s="25"/>
+      <c r="O647" s="21"/>
+      <c r="P647" s="21"/>
+      <c r="Q647" s="19"/>
+      <c r="R647" s="19"/>
+      <c r="S647" s="20"/>
+      <c r="T647" s="20"/>
+      <c r="U647" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" s="73"/>
+      <c r="B648" s="74"/>
+      <c r="C648" s="34"/>
+      <c r="D648" s="34"/>
+      <c r="E648" s="34"/>
+      <c r="F648" s="34"/>
+      <c r="G648" s="34"/>
+      <c r="H648" s="21"/>
+      <c r="I648" s="19"/>
+      <c r="J648" s="10"/>
+      <c r="K648" s="22"/>
+      <c r="L648" s="23"/>
+      <c r="M648" s="22"/>
+      <c r="N648" s="25"/>
+      <c r="O648" s="21"/>
+      <c r="P648" s="21"/>
+      <c r="Q648" s="19"/>
+      <c r="R648" s="19"/>
+      <c r="S648" s="20"/>
+      <c r="T648" s="20"/>
+      <c r="U648" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" s="73"/>
+      <c r="B649" s="74"/>
+      <c r="C649" s="34"/>
+      <c r="D649" s="34"/>
+      <c r="E649" s="34"/>
+      <c r="F649" s="34"/>
+      <c r="G649" s="34"/>
+      <c r="H649" s="21"/>
+      <c r="I649" s="19"/>
+      <c r="J649" s="10"/>
+      <c r="K649" s="22"/>
+      <c r="L649" s="23"/>
+      <c r="M649" s="22"/>
+      <c r="N649" s="25"/>
+      <c r="O649" s="21"/>
+      <c r="P649" s="21"/>
+      <c r="Q649" s="19"/>
+      <c r="R649" s="19"/>
+      <c r="S649" s="20"/>
+      <c r="T649" s="20"/>
+      <c r="U649" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" s="73"/>
+      <c r="B650" s="74"/>
+      <c r="C650" s="34"/>
+      <c r="D650" s="34"/>
+      <c r="E650" s="34"/>
+      <c r="F650" s="34"/>
+      <c r="G650" s="34"/>
+      <c r="H650" s="21"/>
+      <c r="I650" s="19"/>
+      <c r="J650" s="10"/>
+      <c r="K650" s="22"/>
+      <c r="L650" s="23"/>
+      <c r="M650" s="22"/>
+      <c r="N650" s="25"/>
+      <c r="O650" s="21"/>
+      <c r="P650" s="21"/>
+      <c r="Q650" s="19"/>
+      <c r="R650" s="19"/>
+      <c r="S650" s="20"/>
+      <c r="T650" s="20"/>
+      <c r="U650" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" s="73"/>
+      <c r="B651" s="74"/>
+      <c r="C651" s="34"/>
+      <c r="D651" s="34"/>
+      <c r="E651" s="34"/>
+      <c r="F651" s="34"/>
+      <c r="G651" s="34"/>
+      <c r="H651" s="21"/>
+      <c r="I651" s="19"/>
+      <c r="J651" s="10"/>
+      <c r="K651" s="22"/>
+      <c r="L651" s="23"/>
+      <c r="M651" s="22"/>
+      <c r="N651" s="25"/>
+      <c r="O651" s="21"/>
+      <c r="P651" s="21"/>
+      <c r="Q651" s="19"/>
+      <c r="R651" s="19"/>
+      <c r="S651" s="20"/>
+      <c r="T651" s="20"/>
+      <c r="U651" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" s="73"/>
+      <c r="B652" s="74"/>
+      <c r="C652" s="34"/>
+      <c r="D652" s="34"/>
+      <c r="E652" s="34"/>
+      <c r="F652" s="34"/>
+      <c r="G652" s="34"/>
+      <c r="H652" s="21"/>
+      <c r="I652" s="19"/>
+      <c r="J652" s="10"/>
+      <c r="K652" s="22"/>
+      <c r="L652" s="23"/>
+      <c r="M652" s="22"/>
+      <c r="N652" s="25"/>
+      <c r="O652" s="21"/>
+      <c r="P652" s="21"/>
+      <c r="Q652" s="19"/>
+      <c r="R652" s="19"/>
+      <c r="S652" s="20"/>
+      <c r="T652" s="20"/>
+      <c r="U652" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" s="73"/>
+      <c r="B653" s="74"/>
+      <c r="C653" s="34"/>
+      <c r="D653" s="34"/>
+      <c r="E653" s="34"/>
+      <c r="F653" s="34"/>
+      <c r="G653" s="34"/>
+      <c r="H653" s="21"/>
+      <c r="I653" s="19"/>
+      <c r="J653" s="10"/>
+      <c r="K653" s="22"/>
+      <c r="L653" s="23"/>
+      <c r="M653" s="22"/>
+      <c r="N653" s="25"/>
+      <c r="O653" s="21"/>
+      <c r="P653" s="21"/>
+      <c r="Q653" s="19"/>
+      <c r="R653" s="19"/>
+      <c r="S653" s="20"/>
+      <c r="T653" s="20"/>
+      <c r="U653" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" s="73"/>
+      <c r="B654" s="74"/>
+      <c r="C654" s="34"/>
+      <c r="D654" s="34"/>
+      <c r="E654" s="34"/>
+      <c r="F654" s="34"/>
+      <c r="G654" s="34"/>
+      <c r="H654" s="21"/>
+      <c r="I654" s="19"/>
+      <c r="J654" s="10"/>
+      <c r="K654" s="22"/>
+      <c r="L654" s="23"/>
+      <c r="M654" s="22"/>
+      <c r="N654" s="25"/>
+      <c r="O654" s="21"/>
+      <c r="P654" s="21"/>
+      <c r="Q654" s="19"/>
+      <c r="R654" s="19"/>
+      <c r="S654" s="20"/>
+      <c r="T654" s="20"/>
+      <c r="U654" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" s="73"/>
+      <c r="B655" s="74"/>
+      <c r="C655" s="34"/>
+      <c r="D655" s="34"/>
+      <c r="E655" s="34"/>
+      <c r="F655" s="34"/>
+      <c r="G655" s="34"/>
+      <c r="H655" s="21"/>
+      <c r="I655" s="19"/>
+      <c r="J655" s="10"/>
+      <c r="K655" s="22"/>
+      <c r="L655" s="23"/>
+      <c r="M655" s="22"/>
+      <c r="N655" s="25"/>
+      <c r="O655" s="21"/>
+      <c r="P655" s="21"/>
+      <c r="Q655" s="19"/>
+      <c r="R655" s="19"/>
+      <c r="S655" s="20"/>
+      <c r="T655" s="20"/>
+      <c r="U655" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" s="73"/>
+      <c r="B656" s="74"/>
+      <c r="C656" s="34"/>
+      <c r="D656" s="34"/>
+      <c r="E656" s="34"/>
+      <c r="F656" s="34"/>
+      <c r="G656" s="34"/>
+      <c r="H656" s="21"/>
+      <c r="I656" s="19"/>
+      <c r="J656" s="10"/>
+      <c r="K656" s="22"/>
+      <c r="L656" s="23"/>
+      <c r="M656" s="22"/>
+      <c r="N656" s="25"/>
+      <c r="O656" s="21"/>
+      <c r="P656" s="21"/>
+      <c r="Q656" s="19"/>
+      <c r="R656" s="19"/>
+      <c r="S656" s="20"/>
+      <c r="T656" s="20"/>
+      <c r="U656" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" s="73"/>
+      <c r="B657" s="74"/>
+      <c r="C657" s="34"/>
+      <c r="D657" s="34"/>
+      <c r="E657" s="34"/>
+      <c r="F657" s="34"/>
+      <c r="G657" s="34"/>
+      <c r="H657" s="21"/>
+      <c r="I657" s="19"/>
+      <c r="J657" s="10"/>
+      <c r="K657" s="22"/>
+      <c r="L657" s="23"/>
+      <c r="M657" s="22"/>
+      <c r="N657" s="25"/>
+      <c r="O657" s="21"/>
+      <c r="P657" s="21"/>
+      <c r="Q657" s="19"/>
+      <c r="R657" s="19"/>
+      <c r="S657" s="20"/>
+      <c r="T657" s="20"/>
+      <c r="U657" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" s="73"/>
+      <c r="B658" s="74"/>
+      <c r="C658" s="34"/>
+      <c r="D658" s="34"/>
+      <c r="E658" s="34"/>
+      <c r="F658" s="34"/>
+      <c r="G658" s="34"/>
+      <c r="H658" s="21"/>
+      <c r="I658" s="19"/>
+      <c r="J658" s="10"/>
+      <c r="K658" s="22"/>
+      <c r="L658" s="23"/>
+      <c r="M658" s="22"/>
+      <c r="N658" s="25"/>
+      <c r="O658" s="21"/>
+      <c r="P658" s="21"/>
+      <c r="Q658" s="19"/>
+      <c r="R658" s="19"/>
+      <c r="S658" s="20"/>
+      <c r="T658" s="20"/>
+      <c r="U658" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" s="73"/>
+      <c r="B659" s="74"/>
+      <c r="C659" s="34"/>
+      <c r="D659" s="34"/>
+      <c r="E659" s="34"/>
+      <c r="F659" s="34"/>
+      <c r="G659" s="34"/>
+      <c r="H659" s="21"/>
+      <c r="I659" s="19"/>
+      <c r="J659" s="10"/>
+      <c r="K659" s="22"/>
+      <c r="L659" s="23"/>
+      <c r="M659" s="22"/>
+      <c r="N659" s="25"/>
+      <c r="O659" s="21"/>
+      <c r="P659" s="21"/>
+      <c r="Q659" s="19"/>
+      <c r="R659" s="19"/>
+      <c r="S659" s="20"/>
+      <c r="T659" s="20"/>
+      <c r="U659" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" s="73"/>
+      <c r="B660" s="74"/>
+      <c r="C660" s="34"/>
+      <c r="D660" s="34"/>
+      <c r="E660" s="34"/>
+      <c r="F660" s="34"/>
+      <c r="G660" s="34"/>
+      <c r="H660" s="21"/>
+      <c r="I660" s="19"/>
+      <c r="J660" s="10"/>
+      <c r="K660" s="22"/>
+      <c r="L660" s="23"/>
+      <c r="M660" s="22"/>
+      <c r="N660" s="25"/>
+      <c r="O660" s="21"/>
+      <c r="P660" s="21"/>
+      <c r="Q660" s="19"/>
+      <c r="R660" s="19"/>
+      <c r="S660" s="20"/>
+      <c r="T660" s="20"/>
+      <c r="U660" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" s="73"/>
+      <c r="B661" s="74"/>
+      <c r="C661" s="34"/>
+      <c r="D661" s="34"/>
+      <c r="E661" s="34"/>
+      <c r="F661" s="34"/>
+      <c r="G661" s="34"/>
+      <c r="H661" s="21"/>
+      <c r="I661" s="19"/>
+      <c r="J661" s="10"/>
+      <c r="K661" s="22"/>
+      <c r="L661" s="23"/>
+      <c r="M661" s="22"/>
+      <c r="N661" s="25"/>
+      <c r="O661" s="21"/>
+      <c r="P661" s="21"/>
+      <c r="Q661" s="19"/>
+      <c r="R661" s="19"/>
+      <c r="S661" s="20"/>
+      <c r="T661" s="20"/>
+      <c r="U661" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" s="73"/>
+      <c r="B662" s="74"/>
+      <c r="C662" s="34"/>
+      <c r="D662" s="34"/>
+      <c r="E662" s="34"/>
+      <c r="F662" s="34"/>
+      <c r="G662" s="34"/>
+      <c r="H662" s="21"/>
+      <c r="I662" s="19"/>
+      <c r="J662" s="10"/>
+      <c r="K662" s="22"/>
+      <c r="L662" s="23"/>
+      <c r="M662" s="22"/>
+      <c r="N662" s="25"/>
+      <c r="O662" s="21"/>
+      <c r="P662" s="21"/>
+      <c r="Q662" s="19"/>
+      <c r="R662" s="19"/>
+      <c r="S662" s="20"/>
+      <c r="T662" s="20"/>
+      <c r="U662" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" s="73"/>
+      <c r="B663" s="74"/>
+      <c r="C663" s="34"/>
+      <c r="D663" s="34"/>
+      <c r="E663" s="34"/>
+      <c r="F663" s="34"/>
+      <c r="G663" s="34"/>
+      <c r="H663" s="21"/>
+      <c r="I663" s="19"/>
+      <c r="J663" s="10"/>
+      <c r="K663" s="22"/>
+      <c r="L663" s="23"/>
+      <c r="M663" s="22"/>
+      <c r="N663" s="25"/>
+      <c r="O663" s="21"/>
+      <c r="P663" s="21"/>
+      <c r="Q663" s="19"/>
+      <c r="R663" s="19"/>
+      <c r="S663" s="20"/>
+      <c r="T663" s="20"/>
+      <c r="U663" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" s="73"/>
+      <c r="B664" s="74"/>
+      <c r="C664" s="34"/>
+      <c r="D664" s="34"/>
+      <c r="E664" s="34"/>
+      <c r="F664" s="34"/>
+      <c r="G664" s="34"/>
+      <c r="H664" s="21"/>
+      <c r="I664" s="19"/>
+      <c r="J664" s="10"/>
+      <c r="K664" s="22"/>
+      <c r="L664" s="23"/>
+      <c r="M664" s="22"/>
+      <c r="N664" s="25"/>
+      <c r="O664" s="21"/>
+      <c r="P664" s="21"/>
+      <c r="Q664" s="19"/>
+      <c r="R664" s="19"/>
+      <c r="S664" s="20"/>
+      <c r="T664" s="20"/>
+      <c r="U664" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" s="73"/>
+      <c r="B665" s="74"/>
+      <c r="C665" s="34"/>
+      <c r="D665" s="34"/>
+      <c r="E665" s="34"/>
+      <c r="F665" s="34"/>
+      <c r="G665" s="34"/>
+      <c r="H665" s="21"/>
+      <c r="I665" s="19"/>
+      <c r="J665" s="10"/>
+      <c r="K665" s="22"/>
+      <c r="L665" s="23"/>
+      <c r="M665" s="22"/>
+      <c r="N665" s="25"/>
+      <c r="O665" s="21"/>
+      <c r="P665" s="21"/>
+      <c r="Q665" s="19"/>
+      <c r="R665" s="19"/>
+      <c r="S665" s="20"/>
+      <c r="T665" s="20"/>
+      <c r="U665" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" s="73"/>
+      <c r="B666" s="74"/>
+      <c r="C666" s="34"/>
+      <c r="D666" s="34"/>
+      <c r="E666" s="34"/>
+      <c r="F666" s="34"/>
+      <c r="G666" s="34"/>
+      <c r="H666" s="21"/>
+      <c r="I666" s="19"/>
+      <c r="J666" s="10"/>
+      <c r="K666" s="22"/>
+      <c r="L666" s="23"/>
+      <c r="M666" s="22"/>
+      <c r="N666" s="25"/>
+      <c r="O666" s="21"/>
+      <c r="P666" s="21"/>
+      <c r="Q666" s="19"/>
+      <c r="R666" s="19"/>
+      <c r="S666" s="20"/>
+      <c r="T666" s="20"/>
+      <c r="U666" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" s="73"/>
+      <c r="B667" s="74"/>
+      <c r="C667" s="34"/>
+      <c r="D667" s="34"/>
+      <c r="E667" s="34"/>
+      <c r="F667" s="34"/>
+      <c r="G667" s="34"/>
+      <c r="H667" s="21"/>
+      <c r="I667" s="19"/>
+      <c r="J667" s="10"/>
+      <c r="K667" s="22"/>
+      <c r="L667" s="23"/>
+      <c r="M667" s="22"/>
+      <c r="N667" s="25"/>
+      <c r="O667" s="21"/>
+      <c r="P667" s="21"/>
+      <c r="Q667" s="19"/>
+      <c r="R667" s="19"/>
+      <c r="S667" s="20"/>
+      <c r="T667" s="20"/>
+      <c r="U667" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" s="73"/>
+      <c r="B668" s="74"/>
+      <c r="C668" s="34"/>
+      <c r="D668" s="34"/>
+      <c r="E668" s="34"/>
+      <c r="F668" s="34"/>
+      <c r="G668" s="34"/>
+      <c r="H668" s="21"/>
+      <c r="I668" s="19"/>
+      <c r="J668" s="10"/>
+      <c r="K668" s="22"/>
+      <c r="L668" s="23"/>
+      <c r="M668" s="22"/>
+      <c r="N668" s="25"/>
+      <c r="O668" s="21"/>
+      <c r="P668" s="21"/>
+      <c r="Q668" s="19"/>
+      <c r="R668" s="19"/>
+      <c r="S668" s="20"/>
+      <c r="T668" s="20"/>
+      <c r="U668" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" s="73"/>
+      <c r="B669" s="74"/>
+      <c r="C669" s="34"/>
+      <c r="D669" s="34"/>
+      <c r="E669" s="34"/>
+      <c r="F669" s="34"/>
+      <c r="G669" s="34"/>
+      <c r="H669" s="21"/>
+      <c r="I669" s="19"/>
+      <c r="J669" s="10"/>
+      <c r="K669" s="22"/>
+      <c r="L669" s="23"/>
+      <c r="M669" s="22"/>
+      <c r="N669" s="25"/>
+      <c r="O669" s="21"/>
+      <c r="P669" s="21"/>
+      <c r="Q669" s="19"/>
+      <c r="R669" s="19"/>
+      <c r="S669" s="20"/>
+      <c r="T669" s="20"/>
+      <c r="U669" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" s="73"/>
+      <c r="B670" s="74"/>
+      <c r="C670" s="34"/>
+      <c r="D670" s="34"/>
+      <c r="E670" s="34"/>
+      <c r="F670" s="34"/>
+      <c r="G670" s="34"/>
+      <c r="H670" s="21"/>
+      <c r="I670" s="19"/>
+      <c r="J670" s="10"/>
+      <c r="K670" s="22"/>
+      <c r="L670" s="23"/>
+      <c r="M670" s="22"/>
+      <c r="N670" s="25"/>
+      <c r="O670" s="21"/>
+      <c r="P670" s="21"/>
+      <c r="Q670" s="19"/>
+      <c r="R670" s="19"/>
+      <c r="S670" s="20"/>
+      <c r="T670" s="20"/>
+      <c r="U670" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" s="73"/>
+      <c r="B671" s="74"/>
+      <c r="C671" s="34"/>
+      <c r="D671" s="34"/>
+      <c r="E671" s="34"/>
+      <c r="F671" s="34"/>
+      <c r="G671" s="34"/>
+      <c r="H671" s="21"/>
+      <c r="I671" s="19"/>
+      <c r="J671" s="10"/>
+      <c r="K671" s="22"/>
+      <c r="L671" s="23"/>
+      <c r="M671" s="22"/>
+      <c r="N671" s="25"/>
+      <c r="O671" s="21"/>
+      <c r="P671" s="21"/>
+      <c r="Q671" s="19"/>
+      <c r="R671" s="19"/>
+      <c r="S671" s="20"/>
+      <c r="T671" s="20"/>
+      <c r="U671" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" s="73"/>
+      <c r="B672" s="74"/>
+      <c r="C672" s="34"/>
+      <c r="D672" s="34"/>
+      <c r="E672" s="34"/>
+      <c r="F672" s="34"/>
+      <c r="G672" s="34"/>
+      <c r="H672" s="21"/>
+      <c r="I672" s="19"/>
+      <c r="J672" s="10"/>
+      <c r="K672" s="22"/>
+      <c r="L672" s="23"/>
+      <c r="M672" s="22"/>
+      <c r="N672" s="25"/>
+      <c r="O672" s="21"/>
+      <c r="P672" s="21"/>
+      <c r="Q672" s="19"/>
+      <c r="R672" s="19"/>
+      <c r="S672" s="20"/>
+      <c r="T672" s="20"/>
+      <c r="U672" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" s="73"/>
+      <c r="B673" s="74"/>
+      <c r="C673" s="34"/>
+      <c r="D673" s="34"/>
+      <c r="E673" s="34"/>
+      <c r="F673" s="34"/>
+      <c r="G673" s="34"/>
+      <c r="H673" s="21"/>
+      <c r="I673" s="19"/>
+      <c r="J673" s="10"/>
+      <c r="K673" s="22"/>
+      <c r="L673" s="23"/>
+      <c r="M673" s="22"/>
+      <c r="N673" s="25"/>
+      <c r="O673" s="21"/>
+      <c r="P673" s="21"/>
+      <c r="Q673" s="19"/>
+      <c r="R673" s="19"/>
+      <c r="S673" s="20"/>
+      <c r="T673" s="20"/>
+      <c r="U673" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" s="73"/>
+      <c r="B674" s="74"/>
+      <c r="C674" s="34"/>
+      <c r="D674" s="34"/>
+      <c r="E674" s="34"/>
+      <c r="F674" s="34"/>
+      <c r="G674" s="34"/>
+      <c r="H674" s="21"/>
+      <c r="I674" s="19"/>
+      <c r="J674" s="10"/>
+      <c r="K674" s="22"/>
+      <c r="L674" s="23"/>
+      <c r="M674" s="22"/>
+      <c r="N674" s="25"/>
+      <c r="O674" s="21"/>
+      <c r="P674" s="21"/>
+      <c r="Q674" s="19"/>
+      <c r="R674" s="19"/>
+      <c r="S674" s="20"/>
+      <c r="T674" s="20"/>
+      <c r="U674" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" s="73"/>
+      <c r="B675" s="74"/>
+      <c r="C675" s="34"/>
+      <c r="D675" s="34"/>
+      <c r="E675" s="34"/>
+      <c r="F675" s="34"/>
+      <c r="G675" s="34"/>
+      <c r="H675" s="21"/>
+      <c r="I675" s="19"/>
+      <c r="J675" s="10"/>
+      <c r="K675" s="22"/>
+      <c r="L675" s="23"/>
+      <c r="M675" s="22"/>
+      <c r="N675" s="25"/>
+      <c r="O675" s="21"/>
+      <c r="P675" s="21"/>
+      <c r="Q675" s="19"/>
+      <c r="R675" s="19"/>
+      <c r="S675" s="20"/>
+      <c r="T675" s="20"/>
+      <c r="U675" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" s="73"/>
+      <c r="B676" s="74"/>
+      <c r="C676" s="34"/>
+      <c r="D676" s="34"/>
+      <c r="E676" s="34"/>
+      <c r="F676" s="34"/>
+      <c r="G676" s="34"/>
+      <c r="H676" s="21"/>
+      <c r="I676" s="19"/>
+      <c r="J676" s="10"/>
+      <c r="K676" s="22"/>
+      <c r="L676" s="23"/>
+      <c r="M676" s="22"/>
+      <c r="N676" s="25"/>
+      <c r="O676" s="21"/>
+      <c r="P676" s="21"/>
+      <c r="Q676" s="19"/>
+      <c r="R676" s="19"/>
+      <c r="S676" s="20"/>
+      <c r="T676" s="20"/>
+      <c r="U676" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" s="73"/>
+      <c r="B677" s="74"/>
+      <c r="C677" s="34"/>
+      <c r="D677" s="34"/>
+      <c r="E677" s="34"/>
+      <c r="F677" s="34"/>
+      <c r="G677" s="34"/>
+      <c r="H677" s="21"/>
+      <c r="I677" s="19"/>
+      <c r="J677" s="10"/>
+      <c r="K677" s="22"/>
+      <c r="L677" s="23"/>
+      <c r="M677" s="22"/>
+      <c r="N677" s="25"/>
+      <c r="O677" s="21"/>
+      <c r="P677" s="21"/>
+      <c r="Q677" s="19"/>
+      <c r="R677" s="19"/>
+      <c r="S677" s="20"/>
+      <c r="T677" s="20"/>
+      <c r="U677" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" s="73"/>
+      <c r="B678" s="74"/>
+      <c r="C678" s="34"/>
+      <c r="D678" s="34"/>
+      <c r="E678" s="34"/>
+      <c r="F678" s="34"/>
+      <c r="G678" s="34"/>
+      <c r="H678" s="21"/>
+      <c r="I678" s="19"/>
+      <c r="J678" s="10"/>
+      <c r="K678" s="22"/>
+      <c r="L678" s="23"/>
+      <c r="M678" s="22"/>
+      <c r="N678" s="25"/>
+      <c r="O678" s="21"/>
+      <c r="P678" s="21"/>
+      <c r="Q678" s="19"/>
+      <c r="R678" s="19"/>
+      <c r="S678" s="20"/>
+      <c r="T678" s="20"/>
+      <c r="U678" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" s="73"/>
+      <c r="B679" s="74"/>
+      <c r="C679" s="34"/>
+      <c r="D679" s="34"/>
+      <c r="E679" s="34"/>
+      <c r="F679" s="34"/>
+      <c r="G679" s="34"/>
+      <c r="H679" s="21"/>
+      <c r="I679" s="19"/>
+      <c r="J679" s="10"/>
+      <c r="K679" s="22"/>
+      <c r="L679" s="23"/>
+      <c r="M679" s="22"/>
+      <c r="N679" s="25"/>
+      <c r="O679" s="21"/>
+      <c r="P679" s="21"/>
+      <c r="Q679" s="19"/>
+      <c r="R679" s="19"/>
+      <c r="S679" s="20"/>
+      <c r="T679" s="20"/>
+      <c r="U679" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" s="73"/>
+      <c r="B680" s="74"/>
+      <c r="C680" s="34"/>
+      <c r="D680" s="34"/>
+      <c r="E680" s="34"/>
+      <c r="F680" s="34"/>
+      <c r="G680" s="34"/>
+      <c r="H680" s="21"/>
+      <c r="I680" s="19"/>
+      <c r="J680" s="10"/>
+      <c r="K680" s="22"/>
+      <c r="L680" s="23"/>
+      <c r="M680" s="22"/>
+      <c r="N680" s="25"/>
+      <c r="O680" s="21"/>
+      <c r="P680" s="21"/>
+      <c r="Q680" s="19"/>
+      <c r="R680" s="19"/>
+      <c r="S680" s="20"/>
+      <c r="T680" s="20"/>
+      <c r="U680" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" s="73"/>
+      <c r="B681" s="74"/>
+      <c r="C681" s="34"/>
+      <c r="D681" s="34"/>
+      <c r="E681" s="34"/>
+      <c r="F681" s="34"/>
+      <c r="G681" s="34"/>
+      <c r="H681" s="21"/>
+      <c r="I681" s="19"/>
+      <c r="J681" s="10"/>
+      <c r="K681" s="22"/>
+      <c r="L681" s="23"/>
+      <c r="M681" s="22"/>
+      <c r="N681" s="25"/>
+      <c r="O681" s="21"/>
+      <c r="P681" s="21"/>
+      <c r="Q681" s="19"/>
+      <c r="R681" s="19"/>
+      <c r="S681" s="20"/>
+      <c r="T681" s="20"/>
+      <c r="U681" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" s="73"/>
+      <c r="B682" s="74"/>
+      <c r="C682" s="34"/>
+      <c r="D682" s="34"/>
+      <c r="E682" s="34"/>
+      <c r="F682" s="34"/>
+      <c r="G682" s="34"/>
+      <c r="H682" s="21"/>
+      <c r="I682" s="19"/>
+      <c r="J682" s="10"/>
+      <c r="K682" s="22"/>
+      <c r="L682" s="23"/>
+      <c r="M682" s="22"/>
+      <c r="N682" s="25"/>
+      <c r="O682" s="21"/>
+      <c r="P682" s="21"/>
+      <c r="Q682" s="19"/>
+      <c r="R682" s="19"/>
+      <c r="S682" s="20"/>
+      <c r="T682" s="20"/>
+      <c r="U682" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" s="73"/>
+      <c r="B683" s="74"/>
+      <c r="C683" s="34"/>
+      <c r="D683" s="34"/>
+      <c r="E683" s="34"/>
+      <c r="F683" s="34"/>
+      <c r="G683" s="34"/>
+      <c r="H683" s="21"/>
+      <c r="I683" s="19"/>
+      <c r="J683" s="10"/>
+      <c r="K683" s="22"/>
+      <c r="L683" s="23"/>
+      <c r="M683" s="22"/>
+      <c r="N683" s="25"/>
+      <c r="O683" s="21"/>
+      <c r="P683" s="21"/>
+      <c r="Q683" s="19"/>
+      <c r="R683" s="19"/>
+      <c r="S683" s="20"/>
+      <c r="T683" s="20"/>
+      <c r="U683" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" s="73"/>
+      <c r="B684" s="74"/>
+      <c r="C684" s="34"/>
+      <c r="D684" s="34"/>
+      <c r="E684" s="34"/>
+      <c r="F684" s="34"/>
+      <c r="G684" s="34"/>
+      <c r="H684" s="21"/>
+      <c r="I684" s="19"/>
+      <c r="J684" s="10"/>
+      <c r="K684" s="22"/>
+      <c r="L684" s="23"/>
+      <c r="M684" s="22"/>
+      <c r="N684" s="25"/>
+      <c r="O684" s="21"/>
+      <c r="P684" s="21"/>
+      <c r="Q684" s="19"/>
+      <c r="R684" s="19"/>
+      <c r="S684" s="20"/>
+      <c r="T684" s="20"/>
+      <c r="U684" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" s="73"/>
+      <c r="B685" s="74"/>
+      <c r="C685" s="34"/>
+      <c r="D685" s="34"/>
+      <c r="E685" s="34"/>
+      <c r="F685" s="34"/>
+      <c r="G685" s="34"/>
+      <c r="H685" s="21"/>
+      <c r="I685" s="19"/>
+      <c r="J685" s="10"/>
+      <c r="K685" s="22"/>
+      <c r="L685" s="23"/>
+      <c r="M685" s="22"/>
+      <c r="N685" s="25"/>
+      <c r="O685" s="21"/>
+      <c r="P685" s="21"/>
+      <c r="Q685" s="19"/>
+      <c r="R685" s="19"/>
+      <c r="S685" s="20"/>
+      <c r="T685" s="20"/>
+      <c r="U685" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" s="73"/>
+      <c r="B686" s="74"/>
+      <c r="C686" s="34"/>
+      <c r="D686" s="34"/>
+      <c r="E686" s="34"/>
+      <c r="F686" s="34"/>
+      <c r="G686" s="34"/>
+      <c r="H686" s="21"/>
+      <c r="I686" s="19"/>
+      <c r="J686" s="10"/>
+      <c r="K686" s="22"/>
+      <c r="L686" s="23"/>
+      <c r="M686" s="22"/>
+      <c r="N686" s="25"/>
+      <c r="O686" s="21"/>
+      <c r="P686" s="21"/>
+      <c r="Q686" s="19"/>
+      <c r="R686" s="19"/>
+      <c r="S686" s="20"/>
+      <c r="T686" s="20"/>
+      <c r="U686" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" s="73"/>
+      <c r="B687" s="74"/>
+      <c r="C687" s="34"/>
+      <c r="D687" s="34"/>
+      <c r="E687" s="34"/>
+      <c r="F687" s="34"/>
+      <c r="G687" s="34"/>
+      <c r="H687" s="21"/>
+      <c r="I687" s="19"/>
+      <c r="J687" s="10"/>
+      <c r="K687" s="22"/>
+      <c r="L687" s="23"/>
+      <c r="M687" s="22"/>
+      <c r="N687" s="25"/>
+      <c r="O687" s="21"/>
+      <c r="P687" s="21"/>
+      <c r="Q687" s="19"/>
+      <c r="R687" s="19"/>
+      <c r="S687" s="20"/>
+      <c r="T687" s="20"/>
+      <c r="U687" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" s="73"/>
+      <c r="B688" s="74"/>
+      <c r="C688" s="34"/>
+      <c r="D688" s="34"/>
+      <c r="E688" s="34"/>
+      <c r="F688" s="34"/>
+      <c r="G688" s="34"/>
+      <c r="H688" s="21"/>
+      <c r="I688" s="19"/>
+      <c r="J688" s="10"/>
+      <c r="K688" s="22"/>
+      <c r="L688" s="23"/>
+      <c r="M688" s="22"/>
+      <c r="N688" s="25"/>
+      <c r="O688" s="21"/>
+      <c r="P688" s="21"/>
+      <c r="Q688" s="19"/>
+      <c r="R688" s="19"/>
+      <c r="S688" s="20"/>
+      <c r="T688" s="20"/>
+      <c r="U688" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" s="73"/>
+      <c r="B689" s="74"/>
+      <c r="C689" s="34"/>
+      <c r="D689" s="34"/>
+      <c r="E689" s="34"/>
+      <c r="F689" s="34"/>
+      <c r="G689" s="34"/>
+      <c r="H689" s="21"/>
+      <c r="I689" s="19"/>
+      <c r="J689" s="10"/>
+      <c r="K689" s="22"/>
+      <c r="L689" s="23"/>
+      <c r="M689" s="22"/>
+      <c r="N689" s="25"/>
+      <c r="O689" s="21"/>
+      <c r="P689" s="21"/>
+      <c r="Q689" s="19"/>
+      <c r="R689" s="19"/>
+      <c r="S689" s="20"/>
+      <c r="T689" s="20"/>
+      <c r="U689" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" s="73"/>
+      <c r="B690" s="74"/>
+      <c r="C690" s="34"/>
+      <c r="D690" s="34"/>
+      <c r="E690" s="34"/>
+      <c r="F690" s="34"/>
+      <c r="G690" s="34"/>
+      <c r="H690" s="21"/>
+      <c r="I690" s="19"/>
+      <c r="J690" s="10"/>
+      <c r="K690" s="22"/>
+      <c r="L690" s="23"/>
+      <c r="M690" s="22"/>
+      <c r="N690" s="25"/>
+      <c r="O690" s="21"/>
+      <c r="P690" s="21"/>
+      <c r="Q690" s="19"/>
+      <c r="R690" s="19"/>
+      <c r="S690" s="20"/>
+      <c r="T690" s="20"/>
+      <c r="U690" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" s="73"/>
+      <c r="B691" s="74"/>
+      <c r="C691" s="34"/>
+      <c r="D691" s="34"/>
+      <c r="E691" s="34"/>
+      <c r="F691" s="34"/>
+      <c r="G691" s="34"/>
+      <c r="H691" s="21"/>
+      <c r="I691" s="19"/>
+      <c r="J691" s="10"/>
+      <c r="K691" s="22"/>
+      <c r="L691" s="23"/>
+      <c r="M691" s="22"/>
+      <c r="N691" s="25"/>
+      <c r="O691" s="21"/>
+      <c r="P691" s="21"/>
+      <c r="Q691" s="19"/>
+      <c r="R691" s="19"/>
+      <c r="S691" s="20"/>
+      <c r="T691" s="20"/>
+      <c r="U691" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" s="73"/>
+      <c r="B692" s="74"/>
+      <c r="C692" s="34"/>
+      <c r="D692" s="34"/>
+      <c r="E692" s="34"/>
+      <c r="F692" s="34"/>
+      <c r="G692" s="34"/>
+      <c r="H692" s="21"/>
+      <c r="I692" s="19"/>
+      <c r="J692" s="10"/>
+      <c r="K692" s="22"/>
+      <c r="L692" s="23"/>
+      <c r="M692" s="22"/>
+      <c r="N692" s="25"/>
+      <c r="O692" s="21"/>
+      <c r="P692" s="21"/>
+      <c r="Q692" s="19"/>
+      <c r="R692" s="19"/>
+      <c r="S692" s="20"/>
+      <c r="T692" s="20"/>
+      <c r="U692" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" s="73"/>
+      <c r="B693" s="74"/>
+      <c r="C693" s="34"/>
+      <c r="D693" s="34"/>
+      <c r="E693" s="34"/>
+      <c r="F693" s="34"/>
+      <c r="G693" s="34"/>
+      <c r="H693" s="21"/>
+      <c r="I693" s="19"/>
+      <c r="J693" s="10"/>
+      <c r="K693" s="22"/>
+      <c r="L693" s="23"/>
+      <c r="M693" s="22"/>
+      <c r="N693" s="25"/>
+      <c r="O693" s="21"/>
+      <c r="P693" s="21"/>
+      <c r="Q693" s="19"/>
+      <c r="R693" s="19"/>
+      <c r="S693" s="20"/>
+      <c r="T693" s="20"/>
+      <c r="U693" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" s="73"/>
+      <c r="B694" s="74"/>
+      <c r="C694" s="34"/>
+      <c r="D694" s="34"/>
+      <c r="E694" s="34"/>
+      <c r="F694" s="34"/>
+      <c r="G694" s="34"/>
+      <c r="H694" s="21"/>
+      <c r="I694" s="19"/>
+      <c r="J694" s="10"/>
+      <c r="K694" s="22"/>
+      <c r="L694" s="23"/>
+      <c r="M694" s="22"/>
+      <c r="N694" s="25"/>
+      <c r="O694" s="21"/>
+      <c r="P694" s="21"/>
+      <c r="Q694" s="19"/>
+      <c r="R694" s="19"/>
+      <c r="S694" s="20"/>
+      <c r="T694" s="20"/>
+      <c r="U694" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" s="73"/>
+      <c r="B695" s="74"/>
+      <c r="C695" s="34"/>
+      <c r="D695" s="34"/>
+      <c r="E695" s="34"/>
+      <c r="F695" s="34"/>
+      <c r="G695" s="34"/>
+      <c r="H695" s="21"/>
+      <c r="I695" s="19"/>
+      <c r="J695" s="10"/>
+      <c r="K695" s="22"/>
+      <c r="L695" s="23"/>
+      <c r="M695" s="22"/>
+      <c r="N695" s="25"/>
+      <c r="O695" s="21"/>
+      <c r="P695" s="21"/>
+      <c r="Q695" s="19"/>
+      <c r="R695" s="19"/>
+      <c r="S695" s="20"/>
+      <c r="T695" s="20"/>
+      <c r="U695" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" s="73"/>
+      <c r="B696" s="74"/>
+      <c r="C696" s="34"/>
+      <c r="D696" s="34"/>
+      <c r="E696" s="34"/>
+      <c r="F696" s="34"/>
+      <c r="G696" s="34"/>
+      <c r="H696" s="21"/>
+      <c r="I696" s="19"/>
+      <c r="J696" s="10"/>
+      <c r="K696" s="22"/>
+      <c r="L696" s="23"/>
+      <c r="M696" s="22"/>
+      <c r="N696" s="25"/>
+      <c r="O696" s="21"/>
+      <c r="P696" s="21"/>
+      <c r="Q696" s="19"/>
+      <c r="R696" s="19"/>
+      <c r="S696" s="20"/>
+      <c r="T696" s="20"/>
+      <c r="U696" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" s="73"/>
+      <c r="B697" s="74"/>
+      <c r="C697" s="34"/>
+      <c r="D697" s="34"/>
+      <c r="E697" s="34"/>
+      <c r="F697" s="34"/>
+      <c r="G697" s="34"/>
+      <c r="H697" s="21"/>
+      <c r="I697" s="19"/>
+      <c r="J697" s="10"/>
+      <c r="K697" s="22"/>
+      <c r="L697" s="23"/>
+      <c r="M697" s="22"/>
+      <c r="N697" s="25"/>
+      <c r="O697" s="21"/>
+      <c r="P697" s="21"/>
+      <c r="Q697" s="19"/>
+      <c r="R697" s="19"/>
+      <c r="S697" s="20"/>
+      <c r="T697" s="20"/>
+      <c r="U697" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" s="73"/>
+      <c r="B698" s="74"/>
+      <c r="C698" s="34"/>
+      <c r="D698" s="34"/>
+      <c r="E698" s="34"/>
+      <c r="F698" s="34"/>
+      <c r="G698" s="34"/>
+      <c r="H698" s="21"/>
+      <c r="I698" s="19"/>
+      <c r="J698" s="10"/>
+      <c r="K698" s="22"/>
+      <c r="L698" s="23"/>
+      <c r="M698" s="22"/>
+      <c r="N698" s="25"/>
+      <c r="O698" s="21"/>
+      <c r="P698" s="21"/>
+      <c r="Q698" s="19"/>
+      <c r="R698" s="19"/>
+      <c r="S698" s="20"/>
+      <c r="T698" s="20"/>
+      <c r="U698" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" s="73"/>
+      <c r="B699" s="74"/>
+      <c r="C699" s="34"/>
+      <c r="D699" s="34"/>
+      <c r="E699" s="34"/>
+      <c r="F699" s="34"/>
+      <c r="G699" s="34"/>
+      <c r="H699" s="21"/>
+      <c r="I699" s="19"/>
+      <c r="J699" s="10"/>
+      <c r="K699" s="22"/>
+      <c r="L699" s="23"/>
+      <c r="M699" s="22"/>
+      <c r="N699" s="25"/>
+      <c r="O699" s="21"/>
+      <c r="P699" s="21"/>
+      <c r="Q699" s="19"/>
+      <c r="R699" s="19"/>
+      <c r="S699" s="20"/>
+      <c r="T699" s="20"/>
+      <c r="U699" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" s="73"/>
+      <c r="B700" s="74"/>
+      <c r="C700" s="34"/>
+      <c r="D700" s="34"/>
+      <c r="E700" s="34"/>
+      <c r="F700" s="34"/>
+      <c r="G700" s="34"/>
+      <c r="H700" s="21"/>
+      <c r="I700" s="19"/>
+      <c r="J700" s="10"/>
+      <c r="K700" s="22"/>
+      <c r="L700" s="23"/>
+      <c r="M700" s="22"/>
+      <c r="N700" s="25"/>
+      <c r="O700" s="21"/>
+      <c r="P700" s="21"/>
+      <c r="Q700" s="19"/>
+      <c r="R700" s="19"/>
+      <c r="S700" s="20"/>
+      <c r="T700" s="20"/>
+      <c r="U700" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" s="73"/>
+      <c r="B701" s="74"/>
+      <c r="C701" s="34"/>
+      <c r="D701" s="34"/>
+      <c r="E701" s="34"/>
+      <c r="F701" s="34"/>
+      <c r="G701" s="34"/>
+      <c r="H701" s="21"/>
+      <c r="I701" s="19"/>
+      <c r="J701" s="10"/>
+      <c r="K701" s="22"/>
+      <c r="L701" s="23"/>
+      <c r="M701" s="22"/>
+      <c r="N701" s="25"/>
+      <c r="O701" s="21"/>
+      <c r="P701" s="21"/>
+      <c r="Q701" s="19"/>
+      <c r="R701" s="19"/>
+      <c r="S701" s="20"/>
+      <c r="T701" s="20"/>
+      <c r="U701" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="J468">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>(J468&lt;I467)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C601">
+  <conditionalFormatting sqref="C1:C701">
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="男">
       <formula>NOT(ISERROR(SEARCH(("男"),(C1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C601">
+  <conditionalFormatting sqref="C1:C701">
     <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="女">
       <formula>NOT(ISERROR(SEARCH(("女"),(C1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G601">
+  <conditionalFormatting sqref="G2:G701">
     <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="境外">
       <formula>NOT(ISERROR(SEARCH(("境外"),(G2))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G601">
+  <conditionalFormatting sqref="G2:G701">
     <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="本土">
       <formula>NOT(ISERROR(SEARCH(("本土"),(G2))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E601">
+  <conditionalFormatting sqref="E2:E701">
     <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="臺灣">
       <formula>NOT(ISERROR(SEARCH(("臺灣"),(E2))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E601">
+  <conditionalFormatting sqref="E2:E701">
     <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="台灣">
       <formula>NOT(ISERROR(SEARCH(("台灣"),(E2))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E601">
+  <conditionalFormatting sqref="E2:E701">
     <cfRule type="notContainsBlanks" dxfId="6" priority="8">
       <formula>LEN(TRIM(E2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B601">
+  <conditionalFormatting sqref="B1:B701">
     <cfRule type="expression" dxfId="7" priority="9">
       <formula>B1&lt;43856.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B601">
+  <conditionalFormatting sqref="B1:B701">
     <cfRule type="expression" dxfId="8" priority="10">
       <formula>B1&lt;43863.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B601">
+  <conditionalFormatting sqref="B1:B701">
     <cfRule type="expression" dxfId="9" priority="11">
       <formula>B1&lt;43870.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B601">
+  <conditionalFormatting sqref="B1:B701">
     <cfRule type="expression" dxfId="10" priority="12">
       <formula>B1&lt;43877.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B601">
+  <conditionalFormatting sqref="B1:B701">
     <cfRule type="expression" dxfId="11" priority="13">
       <formula>B1&lt;43884.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B601">
+  <conditionalFormatting sqref="B1:B701">
     <cfRule type="expression" dxfId="12" priority="14">
       <formula>B1&lt;43891.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B601">
+  <conditionalFormatting sqref="B1:B701">
     <cfRule type="expression" dxfId="13" priority="15">
       <formula>B1&lt;43898.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B601">
+  <conditionalFormatting sqref="B1:B701">
     <cfRule type="expression" dxfId="14" priority="16">
       <formula>B1&lt;43905.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B601">
+  <conditionalFormatting sqref="B1:B701">
     <cfRule type="expression" dxfId="15" priority="17">
       <formula>B1&lt;43912.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B601">
+  <conditionalFormatting sqref="B1:B701">
     <cfRule type="expression" dxfId="16" priority="18">
       <formula>B1&lt;43919.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B601">
+  <conditionalFormatting sqref="B1:B701">
     <cfRule type="expression" dxfId="17" priority="19">
       <formula>B1&lt;43926.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F345 F347:F601">
+  <conditionalFormatting sqref="F1:F345 F347:F701">
     <cfRule type="containsText" dxfId="2" priority="20" operator="containsText" text="南">
       <formula>NOT(ISERROR(SEARCH(("南"),(F1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F345 F347:F601">
+  <conditionalFormatting sqref="F1:F345 F347:F701">
     <cfRule type="containsText" dxfId="18" priority="21" operator="containsText" text="中">
       <formula>NOT(ISERROR(SEARCH(("中"),(F1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F345 F347:F601">
+  <conditionalFormatting sqref="F1:F345 F347:F701">
     <cfRule type="containsText" dxfId="19" priority="22" operator="containsText" text="北">
       <formula>NOT(ISERROR(SEARCH(("北"),(F1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F345 F347:F601">
+  <conditionalFormatting sqref="F1:F345 F347:F701">
     <cfRule type="containsText" dxfId="20" priority="23" operator="containsText" text="東">
       <formula>NOT(ISERROR(SEARCH(("東"),(F1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P1:P389 P394:P601">
+  <conditionalFormatting sqref="P1:P389 P394:P701">
     <cfRule type="containsText" dxfId="21" priority="24" operator="containsText" text="R.I.P">
       <formula>NOT(ISERROR(SEARCH(("R.I.P"),(P1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M1:M601 P1:P389 P394:P601">
+  <conditionalFormatting sqref="M1:M701 P1:P389 P394:P701">
     <cfRule type="containsText" dxfId="22" priority="25" operator="containsText" text="首起">
       <formula>NOT(ISERROR(SEARCH(("首起"),(M1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M1:M601 P1:P389 P394:P601">
+  <conditionalFormatting sqref="M1:M701 P1:P389 P394:P701">
     <cfRule type="containsText" dxfId="22" priority="26" operator="containsText" text="首次">
       <formula>NOT(ISERROR(SEARCH(("首次"),(M1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M1:M601 P1:P389 P394:P601">
+  <conditionalFormatting sqref="M1:M701 P1:P389 P394:P701">
     <cfRule type="containsText" dxfId="22" priority="27" operator="containsText" text="首例">
       <formula>NOT(ISERROR(SEARCH(("首例"),(M1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L1:L601">
+  <conditionalFormatting sqref="L1:L701">
     <cfRule type="containsText" dxfId="23" priority="28" operator="containsText" text="自行">
       <formula>NOT(ISERROR(SEARCH(("自行"),(L1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O1:O601">
+  <conditionalFormatting sqref="O1:O701">
     <cfRule type="containsText" dxfId="24" priority="29" operator="containsText" text="未知">
       <formula>NOT(ISERROR(SEARCH(("未知"),(O1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L1:L601">
+  <conditionalFormatting sqref="L1:L701">
     <cfRule type="containsText" dxfId="25" priority="30" operator="containsText" text="自主">
       <formula>NOT(ISERROR(SEARCH(("自主"),(L1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P1:P389 P394:P601">
+  <conditionalFormatting sqref="P1:P389 P394:P701">
     <cfRule type="containsText" dxfId="26" priority="31" operator="containsText" text="重症">
       <formula>NOT(ISERROR(SEARCH(("重症"),(P1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J394 J397:J466 J469:J601">
+  <conditionalFormatting sqref="J2:J394 J397:J466 J469:J701">
     <cfRule type="expression" dxfId="0" priority="32">
       <formula>(J2&lt;I2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K344 K346:K601">
+  <conditionalFormatting sqref="K2:K344 K346:K701">
     <cfRule type="expression" dxfId="27" priority="33">
       <formula>AND( I2&lt;&gt;"", (LEFT(K2,4) - I2 ) &gt;= 7 )</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B601">
+  <conditionalFormatting sqref="B357:B701">
     <cfRule type="expression" dxfId="28" priority="34">
       <formula>B357&lt;43933.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L1:L601">
+  <conditionalFormatting sqref="L1:L701">
     <cfRule type="containsText" dxfId="29" priority="35" operator="containsText" text="回溯">
       <formula>NOT(ISERROR(SEARCH(("回溯"),(L1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B601">
+  <conditionalFormatting sqref="B357:B701">
     <cfRule type="expression" dxfId="30" priority="36">
       <formula>B357&lt;43940.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B601">
+  <conditionalFormatting sqref="B357:B701">
     <cfRule type="expression" dxfId="31" priority="37">
       <formula>B357&lt;43947.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B601">
+  <conditionalFormatting sqref="B357:B701">
     <cfRule type="expression" dxfId="32" priority="38">
       <formula>B357&lt;43954.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B601">
+  <conditionalFormatting sqref="B357:B701">
     <cfRule type="expression" dxfId="33" priority="39">
       <formula>B357&lt;43961.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B601">
+  <conditionalFormatting sqref="B357:B701">
     <cfRule type="expression" dxfId="34" priority="40">
       <formula>B357&lt;43968.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B601">
+  <conditionalFormatting sqref="B357:B701">
     <cfRule type="expression" dxfId="35" priority="41">
       <formula>B357&lt;43975.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B601">
+  <conditionalFormatting sqref="B357:B701">
     <cfRule type="expression" dxfId="36" priority="42">
       <formula>B357&lt;43982.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G601">
+  <conditionalFormatting sqref="G2:G701">
     <cfRule type="containsText" dxfId="37" priority="43" operator="containsText" text="敦睦">
       <formula>NOT(ISERROR(SEARCH(("敦睦"),(G2))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L1:L601">
+  <conditionalFormatting sqref="L1:L701">
     <cfRule type="containsText" dxfId="13" priority="44" operator="containsText" text="集中">
       <formula>NOT(ISERROR(SEARCH(("集中"),(L1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O1:O601">
+  <conditionalFormatting sqref="O1:O701">
     <cfRule type="containsText" dxfId="38" priority="45" operator="containsText" text="軍艦">
       <formula>NOT(ISERROR(SEARCH(("軍艦"),(O1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B601">
+  <conditionalFormatting sqref="B357:B701">
     <cfRule type="expression" dxfId="39" priority="46">
       <formula>B357&lt;43989.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B601">
+  <conditionalFormatting sqref="B357:B701">
     <cfRule type="expression" dxfId="40" priority="47">
       <formula>B357&lt;43996.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B601">
+  <conditionalFormatting sqref="B357:B701">
     <cfRule type="expression" dxfId="41" priority="48">
       <formula>B357&lt;44003.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B601">
+  <conditionalFormatting sqref="B357:B701">
     <cfRule type="expression" dxfId="42" priority="49">
       <formula>B357&lt;44010.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B601">
+  <conditionalFormatting sqref="B357:B701">
     <cfRule type="expression" dxfId="43" priority="50">
       <formula>B357&lt;44017.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B601">
+  <conditionalFormatting sqref="B357:B701">
     <cfRule type="expression" dxfId="44" priority="51">
       <formula>B357&lt;44024.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B601">
+  <conditionalFormatting sqref="B357:B701">
     <cfRule type="expression" dxfId="45" priority="52">
       <formula>B357&lt;44031.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B601">
+  <conditionalFormatting sqref="B357:B701">
     <cfRule type="expression" dxfId="46" priority="53">
       <formula>B357&lt;44038.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B601">
+  <conditionalFormatting sqref="B357:B701">
     <cfRule type="expression" dxfId="47" priority="54">
       <formula>B357&lt;44045.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B601">
+  <conditionalFormatting sqref="B357:B701">
     <cfRule type="expression" dxfId="48" priority="55">
       <formula>B357&lt;44052.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B601">
+  <conditionalFormatting sqref="B357:B701">
     <cfRule type="expression" dxfId="49" priority="56">
       <formula>B357&lt;44059.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B601">
+  <conditionalFormatting sqref="B357:B701">
     <cfRule type="expression" dxfId="50" priority="57">
       <formula>B357&lt;44066.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B601">
+  <conditionalFormatting sqref="B357:B701">
     <cfRule type="expression" dxfId="51" priority="58">
       <formula>B357&lt;44073.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B601">
+  <conditionalFormatting sqref="B357:B701">
     <cfRule type="expression" dxfId="52" priority="59">
       <formula>B357&lt;44080.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B601">
+  <conditionalFormatting sqref="B357:B701">
     <cfRule type="expression" dxfId="53" priority="60">
       <formula>B357&lt;44087.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B601">
+  <conditionalFormatting sqref="B357:B701">
     <cfRule type="expression" dxfId="54" priority="61">
       <formula>B357&lt;44094.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B601">
+  <conditionalFormatting sqref="B357:B701">
     <cfRule type="expression" dxfId="55" priority="62">
       <formula>B357&lt;44101.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B601">
+  <conditionalFormatting sqref="B357:B701">
     <cfRule type="expression" dxfId="56" priority="63">
       <formula>B357&lt;44108.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L1:L601">
+  <conditionalFormatting sqref="L1:L701">
     <cfRule type="containsText" dxfId="57" priority="64" operator="containsText" text="自費">
       <formula>NOT(ISERROR(SEARCH(("自費"),(L1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B601">
+  <conditionalFormatting sqref="B357:B701">
     <cfRule type="expression" dxfId="58" priority="65">
       <formula>B357&lt;44115.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B601">
+  <conditionalFormatting sqref="B357:B701">
     <cfRule type="expression" dxfId="59" priority="66">
       <formula>B357&lt;44122.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B601">
+  <conditionalFormatting sqref="B357:B701">
     <cfRule type="expression" dxfId="60" priority="67">
       <formula>B357&lt;44129.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B601">
+  <conditionalFormatting sqref="B357:B701">
     <cfRule type="expression" dxfId="61" priority="68">
       <formula>B357&lt;44136.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B601">
+  <conditionalFormatting sqref="B357:B701">
     <cfRule type="expression" dxfId="62" priority="69">
       <formula>B357&lt;44143.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B601">
+  <conditionalFormatting sqref="B357:B701">
     <cfRule type="expression" dxfId="63" priority="70">
       <formula>B357&lt;44150.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B601">
+  <conditionalFormatting sqref="B357:B701">
     <cfRule type="expression" dxfId="64" priority="71">
       <formula>B357&lt;44157.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B601">
+  <conditionalFormatting sqref="B357:B701">
     <cfRule type="expression" dxfId="65" priority="72">
       <formula>B357&lt;44164.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B601">
+  <conditionalFormatting sqref="B357:B701">
     <cfRule type="expression" dxfId="66" priority="73">
       <formula>B357&lt;44171.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B601">
+  <conditionalFormatting sqref="B357:B701">
     <cfRule type="expression" dxfId="67" priority="74">
       <formula>B357&lt;44178.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B601">
+  <conditionalFormatting sqref="B357:B701">
     <cfRule type="expression" dxfId="68" priority="75">
       <formula>B357&lt;44185.0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B357:B601">
+  <conditionalFormatting sqref="B357:B701">
     <cfRule type="expression" dxfId="68" priority="76">
       <formula>B357&lt;44192.0</formula>
     </cfRule>
@@ -43964,15 +46748,20 @@
     <hyperlink r:id="rId146" ref="S584"/>
     <hyperlink r:id="rId147" ref="S585"/>
     <hyperlink r:id="rId148" ref="S586"/>
+    <hyperlink r:id="rId149" ref="S587"/>
+    <hyperlink r:id="rId150" ref="S588"/>
+    <hyperlink r:id="rId151" ref="S589"/>
+    <hyperlink r:id="rId152" ref="S590"/>
+    <hyperlink r:id="rId153" ref="S591"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId149"/>
-  <legacyDrawing r:id="rId150"/>
+  <drawing r:id="rId154"/>
+  <legacyDrawing r:id="rId155"/>
   <tableParts count="2">
-    <tablePart r:id="rId153"/>
-    <tablePart r:id="rId154"/>
+    <tablePart r:id="rId158"/>
+    <tablePart r:id="rId159"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201114
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -571,7 +571,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6597" uniqueCount="2200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6703" uniqueCount="2220">
   <si>
     <t>案例</t>
   </si>
@@ -8049,6 +8049,70 @@
   </si>
   <si>
     <t>輕微發燒</t>
+  </si>
+  <si>
+    <t>#591</t>
+  </si>
+  <si>
+    <t>10/28(29) 菲律賓→台灣</t>
+  </si>
+  <si>
+    <t>11/11(12) 採檢
+11/13 確診</t>
+  </si>
+  <si>
+    <t>國內新增8例境外移入COVID-19病例，分自菲律賓、印尼及波蘭入境</t>
+  </si>
+  <si>
+    <t>#592</t>
+  </si>
+  <si>
+    <t>#593</t>
+  </si>
+  <si>
+    <t>7月中旬-10/29 菲律賓</t>
+  </si>
+  <si>
+    <t>11/11 採檢
+11/13 確診</t>
+  </si>
+  <si>
+    <t>輕微鼻塞 流鼻水</t>
+  </si>
+  <si>
+    <t>探親
+入境時無症狀，個案於集中檢疫所檢疫期間，11月3日上午雖曾回報有輕微鼻塞及流鼻水症狀，但同日下午即回報已改善無症狀，經評估後未安排就醫</t>
+  </si>
+  <si>
+    <t>#594</t>
+  </si>
+  <si>
+    <t>8月中旬-11/10 波蘭</t>
+  </si>
+  <si>
+    <t>11/10 採檢
+11/13 確診</t>
+  </si>
+  <si>
+    <t>嗅覺異常 喉嚨痛</t>
+  </si>
+  <si>
+    <t>#595</t>
+  </si>
+  <si>
+    <t>10/28(29) 印尼→台灣</t>
+  </si>
+  <si>
+    <t>#596</t>
+  </si>
+  <si>
+    <t>#597</t>
+  </si>
+  <si>
+    <t>#598</t>
+  </si>
+  <si>
+    <t>9月上旬-11/11 印尼</t>
   </si>
 </sst>
 </file>
@@ -43360,211 +43424,449 @@
       </c>
     </row>
     <row r="592">
-      <c r="A592" s="73"/>
-      <c r="B592" s="74"/>
-      <c r="C592" s="34"/>
-      <c r="D592" s="34"/>
-      <c r="E592" s="34"/>
+      <c r="A592" s="16" t="s">
+        <v>2200</v>
+      </c>
+      <c r="B592" s="6">
+        <v>44148.0</v>
+      </c>
+      <c r="C592" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D592" s="7" t="s">
+        <v>2190</v>
+      </c>
+      <c r="E592" s="7" t="s">
+        <v>205</v>
+      </c>
       <c r="F592" s="34"/>
-      <c r="G592" s="34"/>
-      <c r="H592" s="21"/>
-      <c r="I592" s="19"/>
-      <c r="J592" s="10"/>
-      <c r="K592" s="22"/>
-      <c r="L592" s="23"/>
-      <c r="M592" s="22"/>
+      <c r="G592" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H592" s="8" t="s">
+        <v>2201</v>
+      </c>
+      <c r="I592" s="16" t="s">
+        <v>2192</v>
+      </c>
+      <c r="J592" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K592" s="16" t="s">
+        <v>2202</v>
+      </c>
+      <c r="L592" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M592" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N592" s="25"/>
-      <c r="O592" s="21"/>
-      <c r="P592" s="21"/>
+      <c r="O592" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P592" s="8" t="s">
+        <v>1777</v>
+      </c>
       <c r="Q592" s="19"/>
       <c r="R592" s="19"/>
-      <c r="S592" s="20"/>
+      <c r="S592" s="61" t="s">
+        <v>2203</v>
+      </c>
       <c r="T592" s="20"/>
       <c r="U592" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#591</v>
       </c>
     </row>
     <row r="593">
-      <c r="A593" s="73"/>
-      <c r="B593" s="74"/>
-      <c r="C593" s="34"/>
-      <c r="D593" s="34"/>
-      <c r="E593" s="34"/>
+      <c r="A593" s="16" t="s">
+        <v>2204</v>
+      </c>
+      <c r="B593" s="6">
+        <v>44148.0</v>
+      </c>
+      <c r="C593" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D593" s="7" t="s">
+        <v>2190</v>
+      </c>
+      <c r="E593" s="7" t="s">
+        <v>205</v>
+      </c>
       <c r="F593" s="34"/>
-      <c r="G593" s="34"/>
-      <c r="H593" s="21"/>
-      <c r="I593" s="19"/>
-      <c r="J593" s="10"/>
-      <c r="K593" s="22"/>
-      <c r="L593" s="23"/>
-      <c r="M593" s="22"/>
+      <c r="G593" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H593" s="8" t="s">
+        <v>2201</v>
+      </c>
+      <c r="I593" s="16" t="s">
+        <v>2192</v>
+      </c>
+      <c r="J593" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K593" s="16" t="s">
+        <v>2202</v>
+      </c>
+      <c r="L593" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M593" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N593" s="25"/>
-      <c r="O593" s="21"/>
-      <c r="P593" s="21"/>
+      <c r="O593" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P593" s="8" t="s">
+        <v>1777</v>
+      </c>
       <c r="Q593" s="19"/>
       <c r="R593" s="19"/>
-      <c r="S593" s="20"/>
+      <c r="S593" s="61" t="s">
+        <v>2203</v>
+      </c>
       <c r="T593" s="20"/>
       <c r="U593" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#592</v>
       </c>
     </row>
     <row r="594">
-      <c r="A594" s="73"/>
-      <c r="B594" s="74"/>
-      <c r="C594" s="34"/>
-      <c r="D594" s="34"/>
-      <c r="E594" s="34"/>
+      <c r="A594" s="16" t="s">
+        <v>2205</v>
+      </c>
+      <c r="B594" s="6">
+        <v>44148.0</v>
+      </c>
+      <c r="C594" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D594" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E594" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F594" s="34"/>
-      <c r="G594" s="34"/>
-      <c r="H594" s="21"/>
-      <c r="I594" s="19"/>
-      <c r="J594" s="10"/>
-      <c r="K594" s="22"/>
-      <c r="L594" s="23"/>
-      <c r="M594" s="22"/>
+      <c r="G594" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H594" s="8" t="s">
+        <v>2206</v>
+      </c>
+      <c r="I594" s="9">
+        <v>44133.0</v>
+      </c>
+      <c r="J594" s="10">
+        <v>44138.0</v>
+      </c>
+      <c r="K594" s="13" t="s">
+        <v>2207</v>
+      </c>
+      <c r="L594" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M594" s="13" t="s">
+        <v>2208</v>
+      </c>
       <c r="N594" s="25"/>
-      <c r="O594" s="21"/>
-      <c r="P594" s="21"/>
+      <c r="O594" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P594" s="8" t="s">
+        <v>2209</v>
+      </c>
       <c r="Q594" s="19"/>
       <c r="R594" s="19"/>
-      <c r="S594" s="20"/>
+      <c r="S594" s="61" t="s">
+        <v>2203</v>
+      </c>
       <c r="T594" s="20"/>
       <c r="U594" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#593</v>
       </c>
     </row>
     <row r="595">
-      <c r="A595" s="73"/>
-      <c r="B595" s="74"/>
-      <c r="C595" s="34"/>
-      <c r="D595" s="34"/>
-      <c r="E595" s="34"/>
+      <c r="A595" s="16" t="s">
+        <v>2210</v>
+      </c>
+      <c r="B595" s="6">
+        <v>44148.0</v>
+      </c>
+      <c r="C595" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D595" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E595" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F595" s="34"/>
-      <c r="G595" s="34"/>
-      <c r="H595" s="21"/>
-      <c r="I595" s="19"/>
-      <c r="J595" s="10"/>
-      <c r="K595" s="22"/>
-      <c r="L595" s="23"/>
-      <c r="M595" s="22"/>
+      <c r="G595" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H595" s="8" t="s">
+        <v>2211</v>
+      </c>
+      <c r="I595" s="9">
+        <v>44145.0</v>
+      </c>
+      <c r="J595" s="10">
+        <v>44140.0</v>
+      </c>
+      <c r="K595" s="13" t="s">
+        <v>2212</v>
+      </c>
+      <c r="L595" s="12" t="s">
+        <v>363</v>
+      </c>
+      <c r="M595" s="13" t="s">
+        <v>2213</v>
+      </c>
       <c r="N595" s="25"/>
-      <c r="O595" s="21"/>
-      <c r="P595" s="21"/>
+      <c r="O595" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P595" s="8" t="s">
+        <v>360</v>
+      </c>
       <c r="Q595" s="19"/>
       <c r="R595" s="19"/>
-      <c r="S595" s="20"/>
+      <c r="S595" s="61" t="s">
+        <v>2203</v>
+      </c>
       <c r="T595" s="20"/>
       <c r="U595" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#594</v>
       </c>
     </row>
     <row r="596">
-      <c r="A596" s="73"/>
-      <c r="B596" s="74"/>
-      <c r="C596" s="34"/>
-      <c r="D596" s="34"/>
-      <c r="E596" s="34"/>
+      <c r="A596" s="16" t="s">
+        <v>2214</v>
+      </c>
+      <c r="B596" s="6">
+        <v>44148.0</v>
+      </c>
+      <c r="C596" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D596" s="7" t="s">
+        <v>2190</v>
+      </c>
+      <c r="E596" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F596" s="34"/>
-      <c r="G596" s="34"/>
-      <c r="H596" s="21"/>
-      <c r="I596" s="19"/>
-      <c r="J596" s="10"/>
-      <c r="K596" s="22"/>
-      <c r="L596" s="23"/>
-      <c r="M596" s="22"/>
+      <c r="G596" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H596" s="8" t="s">
+        <v>2215</v>
+      </c>
+      <c r="I596" s="16" t="s">
+        <v>2192</v>
+      </c>
+      <c r="J596" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K596" s="16" t="s">
+        <v>2202</v>
+      </c>
+      <c r="L596" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M596" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N596" s="25"/>
-      <c r="O596" s="21"/>
-      <c r="P596" s="21"/>
+      <c r="O596" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P596" s="8" t="s">
+        <v>1777</v>
+      </c>
       <c r="Q596" s="19"/>
       <c r="R596" s="19"/>
-      <c r="S596" s="20"/>
+      <c r="S596" s="61" t="s">
+        <v>2203</v>
+      </c>
       <c r="T596" s="20"/>
       <c r="U596" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#595</v>
       </c>
     </row>
     <row r="597">
-      <c r="A597" s="73"/>
-      <c r="B597" s="74"/>
-      <c r="C597" s="34"/>
-      <c r="D597" s="34"/>
-      <c r="E597" s="34"/>
+      <c r="A597" s="16" t="s">
+        <v>2216</v>
+      </c>
+      <c r="B597" s="6">
+        <v>44148.0</v>
+      </c>
+      <c r="C597" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D597" s="7" t="s">
+        <v>2190</v>
+      </c>
+      <c r="E597" s="7" t="s">
+        <v>205</v>
+      </c>
       <c r="F597" s="34"/>
-      <c r="G597" s="34"/>
-      <c r="H597" s="21"/>
-      <c r="I597" s="19"/>
-      <c r="J597" s="10"/>
-      <c r="K597" s="22"/>
-      <c r="L597" s="23"/>
-      <c r="M597" s="22"/>
+      <c r="G597" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H597" s="8" t="s">
+        <v>2201</v>
+      </c>
+      <c r="I597" s="16" t="s">
+        <v>2192</v>
+      </c>
+      <c r="J597" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K597" s="16" t="s">
+        <v>2202</v>
+      </c>
+      <c r="L597" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M597" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N597" s="25"/>
-      <c r="O597" s="21"/>
-      <c r="P597" s="21"/>
+      <c r="O597" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P597" s="8" t="s">
+        <v>1777</v>
+      </c>
       <c r="Q597" s="19"/>
       <c r="R597" s="19"/>
-      <c r="S597" s="20"/>
+      <c r="S597" s="61" t="s">
+        <v>2203</v>
+      </c>
       <c r="T597" s="20"/>
       <c r="U597" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#596</v>
       </c>
     </row>
     <row r="598">
-      <c r="A598" s="73"/>
-      <c r="B598" s="74"/>
-      <c r="C598" s="34"/>
-      <c r="D598" s="34"/>
-      <c r="E598" s="34"/>
+      <c r="A598" s="16" t="s">
+        <v>2217</v>
+      </c>
+      <c r="B598" s="6">
+        <v>44148.0</v>
+      </c>
+      <c r="C598" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D598" s="7" t="s">
+        <v>2190</v>
+      </c>
+      <c r="E598" s="7" t="s">
+        <v>205</v>
+      </c>
       <c r="F598" s="34"/>
-      <c r="G598" s="34"/>
-      <c r="H598" s="21"/>
-      <c r="I598" s="19"/>
-      <c r="J598" s="10"/>
-      <c r="K598" s="22"/>
-      <c r="L598" s="23"/>
-      <c r="M598" s="22"/>
+      <c r="G598" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H598" s="8" t="s">
+        <v>2201</v>
+      </c>
+      <c r="I598" s="16" t="s">
+        <v>2192</v>
+      </c>
+      <c r="J598" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K598" s="16" t="s">
+        <v>2202</v>
+      </c>
+      <c r="L598" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M598" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N598" s="25"/>
-      <c r="O598" s="21"/>
-      <c r="P598" s="21"/>
+      <c r="O598" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P598" s="8" t="s">
+        <v>1777</v>
+      </c>
       <c r="Q598" s="19"/>
       <c r="R598" s="19"/>
-      <c r="S598" s="20"/>
+      <c r="S598" s="61" t="s">
+        <v>2203</v>
+      </c>
       <c r="T598" s="20"/>
       <c r="U598" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#597</v>
       </c>
     </row>
     <row r="599">
-      <c r="A599" s="73"/>
-      <c r="B599" s="74"/>
-      <c r="C599" s="34"/>
-      <c r="D599" s="34"/>
-      <c r="E599" s="34"/>
+      <c r="A599" s="16" t="s">
+        <v>2218</v>
+      </c>
+      <c r="B599" s="6">
+        <v>44148.0</v>
+      </c>
+      <c r="C599" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D599" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E599" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F599" s="34"/>
-      <c r="G599" s="34"/>
-      <c r="H599" s="21"/>
-      <c r="I599" s="19"/>
+      <c r="G599" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H599" s="8" t="s">
+        <v>2219</v>
+      </c>
+      <c r="I599" s="9">
+        <v>44146.0</v>
+      </c>
       <c r="J599" s="10"/>
-      <c r="K599" s="22"/>
-      <c r="L599" s="23"/>
-      <c r="M599" s="22"/>
+      <c r="K599" s="13" t="s">
+        <v>2207</v>
+      </c>
+      <c r="L599" s="12" t="s">
+        <v>363</v>
+      </c>
+      <c r="M599" s="13" t="s">
+        <v>518</v>
+      </c>
       <c r="N599" s="25"/>
-      <c r="O599" s="21"/>
-      <c r="P599" s="21"/>
+      <c r="O599" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P599" s="8" t="s">
+        <v>334</v>
+      </c>
       <c r="Q599" s="19"/>
       <c r="R599" s="19"/>
-      <c r="S599" s="20"/>
+      <c r="S599" s="61" t="s">
+        <v>2203</v>
+      </c>
       <c r="T599" s="20"/>
       <c r="U599" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#598</v>
       </c>
     </row>
     <row r="600">
@@ -43574,7 +43876,7 @@
       <c r="D600" s="34"/>
       <c r="E600" s="34"/>
       <c r="F600" s="34"/>
-      <c r="G600" s="34"/>
+      <c r="G600" s="7"/>
       <c r="H600" s="21"/>
       <c r="I600" s="19"/>
       <c r="J600" s="10"/>
@@ -46380,7 +46682,7 @@
       <formula>(J2&lt;I2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K344 K346:K701">
+  <conditionalFormatting sqref="K2:K344 K346:K591 K594:K595 K599:K701">
     <cfRule type="expression" dxfId="27" priority="33">
       <formula>AND( I2&lt;&gt;"", (LEFT(K2,4) - I2 ) &gt;= 7 )</formula>
     </cfRule>
@@ -46753,15 +47055,23 @@
     <hyperlink r:id="rId151" ref="S589"/>
     <hyperlink r:id="rId152" ref="S590"/>
     <hyperlink r:id="rId153" ref="S591"/>
+    <hyperlink r:id="rId154" ref="S592"/>
+    <hyperlink r:id="rId155" ref="S593"/>
+    <hyperlink r:id="rId156" ref="S594"/>
+    <hyperlink r:id="rId157" ref="S595"/>
+    <hyperlink r:id="rId158" ref="S596"/>
+    <hyperlink r:id="rId159" ref="S597"/>
+    <hyperlink r:id="rId160" ref="S598"/>
+    <hyperlink r:id="rId161" ref="S599"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId154"/>
-  <legacyDrawing r:id="rId155"/>
+  <drawing r:id="rId162"/>
+  <legacyDrawing r:id="rId163"/>
   <tableParts count="2">
-    <tablePart r:id="rId158"/>
-    <tablePart r:id="rId159"/>
+    <tablePart r:id="rId166"/>
+    <tablePart r:id="rId167"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201115
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -571,7 +571,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6703" uniqueCount="2220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6747" uniqueCount="2238">
   <si>
     <t>案例</t>
   </si>
@@ -8114,6 +8114,65 @@
   <si>
     <t>9月上旬-11/11 印尼</t>
   </si>
+  <si>
+    <t>#599</t>
+  </si>
+  <si>
+    <t>2月上旬-10/29 菲律賓</t>
+  </si>
+  <si>
+    <t>11/11 採檢
+11/14 確診</t>
+  </si>
+  <si>
+    <t>探親
+11月11日進行檢疫期滿前採檢，檢驗結果有微弱訊號，經複驗結果為陰性；為求慎重，又逢實驗室引進新的檢驗試劑，故將個案檢體再以新試劑進行檢驗，結果呈現陽性(Ct值33)，於今日確診。個案是於檢疫期滿搭車返家途中接獲陽性通知，後續經調查個案座位旁無其他乘客，亦無與他人交談，且個案及同車人員全程皆佩戴口罩</t>
+  </si>
+  <si>
+    <t>新增3例境外移入COVID-19病例，自菲律賓、印尼及克羅埃西亞入境</t>
+  </si>
+  <si>
+    <t>#600</t>
+  </si>
+  <si>
+    <t>-11/7 印尼→台灣</t>
+  </si>
+  <si>
+    <t>11/13 採檢
+11/14 確診</t>
+  </si>
+  <si>
+    <t>輕微發燒 嗅覺異常 咳嗽 流鼻水 喉嚨痛</t>
+  </si>
+  <si>
+    <t>#601</t>
+  </si>
+  <si>
+    <t>克羅埃西亞</t>
+  </si>
+  <si>
+    <t>-10/29 克羅埃西亞→台灣</t>
+  </si>
+  <si>
+    <t>7月、11/1</t>
+  </si>
+  <si>
+    <t>11/13 採檢
+11/14 確診</t>
+  </si>
+  <si>
+    <t>鼻子過敏</t>
+  </si>
+  <si>
+    <t>今年7月曾出現症狀，並於克羅埃西亞確診武漢肺炎，隔離14天後症狀緩解，且經複驗陰性故解除隔離
+來臺工作，入境時無症狀，並持有登機前3日內陰性報告。個案居家檢疫期間，曾於11月1日出現鼻塞症狀，自認是過敏故未通報；11月13日檢疫期滿，因臺灣公司要求，同日自費採檢</t>
+  </si>
+  <si>
+    <t>#602</t>
+  </si>
+  <si>
+    <t>#603</t>
+  </si>
 </sst>
 </file>
 
@@ -8123,7 +8182,7 @@
     <numFmt numFmtId="164" formatCode="mm&quot;月&quot;dd&quot;日 &quot;dddd"/>
     <numFmt numFmtId="165" formatCode="m/d"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -8204,6 +8263,7 @@
       <u/>
       <color rgb="FFFFFFFF"/>
     </font>
+    <font/>
   </fonts>
   <fills count="7">
     <fill>
@@ -8249,7 +8309,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="77">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -8468,6 +8528,12 @@
     </xf>
     <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
@@ -9572,7 +9638,7 @@
     <col customWidth="1" min="2" max="2" width="15.14"/>
     <col customWidth="1" min="3" max="3" width="4.86"/>
     <col customWidth="1" min="4" max="4" width="6.29"/>
-    <col customWidth="1" min="5" max="5" width="8.14"/>
+    <col customWidth="1" min="5" max="5" width="10.29"/>
     <col customWidth="1" min="6" max="6" width="11.0"/>
     <col customWidth="1" min="7" max="7" width="5.14"/>
     <col customWidth="1" min="8" max="8" width="19.43"/>
@@ -43870,88 +43936,188 @@
       </c>
     </row>
     <row r="600">
-      <c r="A600" s="73"/>
-      <c r="B600" s="74"/>
-      <c r="C600" s="34"/>
-      <c r="D600" s="34"/>
-      <c r="E600" s="34"/>
+      <c r="A600" s="16" t="s">
+        <v>2220</v>
+      </c>
+      <c r="B600" s="6">
+        <v>44149.0</v>
+      </c>
+      <c r="C600" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D600" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E600" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F600" s="34"/>
-      <c r="G600" s="7"/>
-      <c r="H600" s="21"/>
-      <c r="I600" s="19"/>
-      <c r="J600" s="10"/>
-      <c r="K600" s="22"/>
-      <c r="L600" s="23"/>
-      <c r="M600" s="22"/>
+      <c r="G600" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H600" s="8" t="s">
+        <v>2221</v>
+      </c>
+      <c r="I600" s="9">
+        <v>44133.0</v>
+      </c>
+      <c r="J600" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K600" s="13" t="s">
+        <v>2222</v>
+      </c>
+      <c r="L600" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M600" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N600" s="25"/>
-      <c r="O600" s="21"/>
-      <c r="P600" s="21"/>
+      <c r="O600" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P600" s="8" t="s">
+        <v>2223</v>
+      </c>
       <c r="Q600" s="19"/>
       <c r="R600" s="19"/>
-      <c r="S600" s="20"/>
+      <c r="S600" s="61" t="s">
+        <v>2224</v>
+      </c>
       <c r="T600" s="20"/>
       <c r="U600" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#599</v>
       </c>
     </row>
     <row r="601">
-      <c r="A601" s="73"/>
-      <c r="B601" s="74"/>
-      <c r="C601" s="34"/>
-      <c r="D601" s="34"/>
-      <c r="E601" s="34"/>
+      <c r="A601" s="16" t="s">
+        <v>2225</v>
+      </c>
+      <c r="B601" s="6">
+        <v>44149.0</v>
+      </c>
+      <c r="C601" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D601" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E601" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F601" s="34"/>
-      <c r="G601" s="34"/>
-      <c r="H601" s="21"/>
-      <c r="I601" s="19"/>
-      <c r="J601" s="10"/>
-      <c r="K601" s="22"/>
-      <c r="L601" s="23"/>
-      <c r="M601" s="22"/>
+      <c r="G601" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H601" s="8" t="s">
+        <v>2226</v>
+      </c>
+      <c r="I601" s="9">
+        <v>44142.0</v>
+      </c>
+      <c r="J601" s="10">
+        <v>44144.0</v>
+      </c>
+      <c r="K601" s="13" t="s">
+        <v>2227</v>
+      </c>
+      <c r="L601" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M601" s="13" t="s">
+        <v>2228</v>
+      </c>
       <c r="N601" s="25"/>
-      <c r="O601" s="21"/>
-      <c r="P601" s="21"/>
+      <c r="O601" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P601" s="8" t="s">
+        <v>1777</v>
+      </c>
       <c r="Q601" s="19"/>
       <c r="R601" s="19"/>
-      <c r="S601" s="20"/>
+      <c r="S601" s="61" t="s">
+        <v>2224</v>
+      </c>
       <c r="T601" s="20"/>
       <c r="U601" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#600</v>
       </c>
     </row>
     <row r="602">
-      <c r="A602" s="73"/>
-      <c r="B602" s="74"/>
-      <c r="C602" s="34"/>
-      <c r="D602" s="34"/>
-      <c r="E602" s="34"/>
+      <c r="A602" s="16" t="s">
+        <v>2229</v>
+      </c>
+      <c r="B602" s="6">
+        <v>44149.0</v>
+      </c>
+      <c r="C602" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D602" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E602" s="7" t="s">
+        <v>2230</v>
+      </c>
       <c r="F602" s="34"/>
-      <c r="G602" s="34"/>
-      <c r="H602" s="21"/>
-      <c r="I602" s="19"/>
-      <c r="J602" s="10"/>
-      <c r="K602" s="22"/>
-      <c r="L602" s="23"/>
-      <c r="M602" s="22"/>
-      <c r="N602" s="25"/>
-      <c r="O602" s="21"/>
-      <c r="P602" s="21"/>
+      <c r="G602" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H602" s="8" t="s">
+        <v>2231</v>
+      </c>
+      <c r="I602" s="9">
+        <v>44133.0</v>
+      </c>
+      <c r="J602" s="12" t="s">
+        <v>2232</v>
+      </c>
+      <c r="K602" s="13" t="s">
+        <v>2233</v>
+      </c>
+      <c r="L602" s="12" t="s">
+        <v>1674</v>
+      </c>
+      <c r="M602" s="13" t="s">
+        <v>2118</v>
+      </c>
+      <c r="N602" s="14" t="s">
+        <v>2234</v>
+      </c>
+      <c r="O602" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P602" s="8" t="s">
+        <v>2235</v>
+      </c>
       <c r="Q602" s="19"/>
       <c r="R602" s="19"/>
-      <c r="S602" s="20"/>
+      <c r="S602" s="61" t="s">
+        <v>2224</v>
+      </c>
       <c r="T602" s="20"/>
       <c r="U602" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#601</v>
       </c>
     </row>
     <row r="603">
-      <c r="A603" s="73"/>
-      <c r="B603" s="74"/>
-      <c r="C603" s="34"/>
-      <c r="D603" s="34"/>
+      <c r="A603" s="73" t="s">
+        <v>2236</v>
+      </c>
+      <c r="B603" s="6">
+        <v>44150.0</v>
+      </c>
+      <c r="C603" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D603" s="74" t="s">
+        <v>59</v>
+      </c>
       <c r="E603" s="34"/>
       <c r="F603" s="34"/>
       <c r="G603" s="34"/>
@@ -43970,13 +44136,19 @@
       <c r="T603" s="20"/>
       <c r="U603" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#602</v>
       </c>
     </row>
     <row r="604">
-      <c r="A604" s="73"/>
-      <c r="B604" s="74"/>
-      <c r="C604" s="34"/>
+      <c r="A604" s="73" t="s">
+        <v>2237</v>
+      </c>
+      <c r="B604" s="6">
+        <v>44150.0</v>
+      </c>
+      <c r="C604" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="D604" s="34"/>
       <c r="E604" s="34"/>
       <c r="F604" s="34"/>
@@ -43996,12 +44168,12 @@
       <c r="T604" s="20"/>
       <c r="U604" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#603</v>
       </c>
     </row>
     <row r="605">
-      <c r="A605" s="73"/>
-      <c r="B605" s="74"/>
+      <c r="A605" s="75"/>
+      <c r="B605" s="76"/>
       <c r="C605" s="34"/>
       <c r="D605" s="34"/>
       <c r="E605" s="34"/>
@@ -44026,8 +44198,8 @@
       </c>
     </row>
     <row r="606">
-      <c r="A606" s="73"/>
-      <c r="B606" s="74"/>
+      <c r="A606" s="75"/>
+      <c r="B606" s="76"/>
       <c r="C606" s="34"/>
       <c r="D606" s="34"/>
       <c r="E606" s="34"/>
@@ -44052,8 +44224,8 @@
       </c>
     </row>
     <row r="607">
-      <c r="A607" s="73"/>
-      <c r="B607" s="74"/>
+      <c r="A607" s="75"/>
+      <c r="B607" s="76"/>
       <c r="C607" s="34"/>
       <c r="D607" s="34"/>
       <c r="E607" s="34"/>
@@ -44078,8 +44250,8 @@
       </c>
     </row>
     <row r="608">
-      <c r="A608" s="73"/>
-      <c r="B608" s="74"/>
+      <c r="A608" s="75"/>
+      <c r="B608" s="76"/>
       <c r="C608" s="34"/>
       <c r="D608" s="34"/>
       <c r="E608" s="34"/>
@@ -44104,8 +44276,8 @@
       </c>
     </row>
     <row r="609">
-      <c r="A609" s="73"/>
-      <c r="B609" s="74"/>
+      <c r="A609" s="75"/>
+      <c r="B609" s="76"/>
       <c r="C609" s="34"/>
       <c r="D609" s="34"/>
       <c r="E609" s="34"/>
@@ -44130,8 +44302,8 @@
       </c>
     </row>
     <row r="610">
-      <c r="A610" s="73"/>
-      <c r="B610" s="74"/>
+      <c r="A610" s="75"/>
+      <c r="B610" s="76"/>
       <c r="C610" s="34"/>
       <c r="D610" s="34"/>
       <c r="E610" s="34"/>
@@ -44156,8 +44328,8 @@
       </c>
     </row>
     <row r="611">
-      <c r="A611" s="73"/>
-      <c r="B611" s="74"/>
+      <c r="A611" s="75"/>
+      <c r="B611" s="76"/>
       <c r="C611" s="34"/>
       <c r="D611" s="34"/>
       <c r="E611" s="34"/>
@@ -44182,8 +44354,8 @@
       </c>
     </row>
     <row r="612">
-      <c r="A612" s="73"/>
-      <c r="B612" s="74"/>
+      <c r="A612" s="75"/>
+      <c r="B612" s="76"/>
       <c r="C612" s="34"/>
       <c r="D612" s="34"/>
       <c r="E612" s="34"/>
@@ -44208,8 +44380,8 @@
       </c>
     </row>
     <row r="613">
-      <c r="A613" s="73"/>
-      <c r="B613" s="74"/>
+      <c r="A613" s="75"/>
+      <c r="B613" s="76"/>
       <c r="C613" s="34"/>
       <c r="D613" s="34"/>
       <c r="E613" s="34"/>
@@ -44234,8 +44406,8 @@
       </c>
     </row>
     <row r="614">
-      <c r="A614" s="73"/>
-      <c r="B614" s="74"/>
+      <c r="A614" s="75"/>
+      <c r="B614" s="76"/>
       <c r="C614" s="34"/>
       <c r="D614" s="34"/>
       <c r="E614" s="34"/>
@@ -44260,8 +44432,8 @@
       </c>
     </row>
     <row r="615">
-      <c r="A615" s="73"/>
-      <c r="B615" s="74"/>
+      <c r="A615" s="75"/>
+      <c r="B615" s="76"/>
       <c r="C615" s="34"/>
       <c r="D615" s="34"/>
       <c r="E615" s="34"/>
@@ -44286,8 +44458,8 @@
       </c>
     </row>
     <row r="616">
-      <c r="A616" s="73"/>
-      <c r="B616" s="74"/>
+      <c r="A616" s="75"/>
+      <c r="B616" s="76"/>
       <c r="C616" s="34"/>
       <c r="D616" s="34"/>
       <c r="E616" s="34"/>
@@ -44312,8 +44484,8 @@
       </c>
     </row>
     <row r="617">
-      <c r="A617" s="73"/>
-      <c r="B617" s="74"/>
+      <c r="A617" s="75"/>
+      <c r="B617" s="76"/>
       <c r="C617" s="34"/>
       <c r="D617" s="34"/>
       <c r="E617" s="34"/>
@@ -44338,8 +44510,8 @@
       </c>
     </row>
     <row r="618">
-      <c r="A618" s="73"/>
-      <c r="B618" s="74"/>
+      <c r="A618" s="75"/>
+      <c r="B618" s="76"/>
       <c r="C618" s="34"/>
       <c r="D618" s="34"/>
       <c r="E618" s="34"/>
@@ -44364,8 +44536,8 @@
       </c>
     </row>
     <row r="619">
-      <c r="A619" s="73"/>
-      <c r="B619" s="74"/>
+      <c r="A619" s="75"/>
+      <c r="B619" s="76"/>
       <c r="C619" s="34"/>
       <c r="D619" s="34"/>
       <c r="E619" s="34"/>
@@ -44390,8 +44562,8 @@
       </c>
     </row>
     <row r="620">
-      <c r="A620" s="73"/>
-      <c r="B620" s="74"/>
+      <c r="A620" s="75"/>
+      <c r="B620" s="76"/>
       <c r="C620" s="34"/>
       <c r="D620" s="34"/>
       <c r="E620" s="34"/>
@@ -44416,8 +44588,8 @@
       </c>
     </row>
     <row r="621">
-      <c r="A621" s="73"/>
-      <c r="B621" s="74"/>
+      <c r="A621" s="75"/>
+      <c r="B621" s="76"/>
       <c r="C621" s="34"/>
       <c r="D621" s="34"/>
       <c r="E621" s="34"/>
@@ -44442,8 +44614,8 @@
       </c>
     </row>
     <row r="622">
-      <c r="A622" s="73"/>
-      <c r="B622" s="74"/>
+      <c r="A622" s="75"/>
+      <c r="B622" s="76"/>
       <c r="C622" s="34"/>
       <c r="D622" s="34"/>
       <c r="E622" s="34"/>
@@ -44468,8 +44640,8 @@
       </c>
     </row>
     <row r="623">
-      <c r="A623" s="73"/>
-      <c r="B623" s="74"/>
+      <c r="A623" s="75"/>
+      <c r="B623" s="76"/>
       <c r="C623" s="34"/>
       <c r="D623" s="34"/>
       <c r="E623" s="34"/>
@@ -44494,8 +44666,8 @@
       </c>
     </row>
     <row r="624">
-      <c r="A624" s="73"/>
-      <c r="B624" s="74"/>
+      <c r="A624" s="75"/>
+      <c r="B624" s="76"/>
       <c r="C624" s="34"/>
       <c r="D624" s="34"/>
       <c r="E624" s="34"/>
@@ -44520,8 +44692,8 @@
       </c>
     </row>
     <row r="625">
-      <c r="A625" s="73"/>
-      <c r="B625" s="74"/>
+      <c r="A625" s="75"/>
+      <c r="B625" s="76"/>
       <c r="C625" s="34"/>
       <c r="D625" s="34"/>
       <c r="E625" s="34"/>
@@ -44546,8 +44718,8 @@
       </c>
     </row>
     <row r="626">
-      <c r="A626" s="73"/>
-      <c r="B626" s="74"/>
+      <c r="A626" s="75"/>
+      <c r="B626" s="76"/>
       <c r="C626" s="34"/>
       <c r="D626" s="34"/>
       <c r="E626" s="34"/>
@@ -44572,8 +44744,8 @@
       </c>
     </row>
     <row r="627">
-      <c r="A627" s="73"/>
-      <c r="B627" s="74"/>
+      <c r="A627" s="75"/>
+      <c r="B627" s="76"/>
       <c r="C627" s="34"/>
       <c r="D627" s="34"/>
       <c r="E627" s="34"/>
@@ -44598,8 +44770,8 @@
       </c>
     </row>
     <row r="628">
-      <c r="A628" s="73"/>
-      <c r="B628" s="74"/>
+      <c r="A628" s="75"/>
+      <c r="B628" s="76"/>
       <c r="C628" s="34"/>
       <c r="D628" s="34"/>
       <c r="E628" s="34"/>
@@ -44624,8 +44796,8 @@
       </c>
     </row>
     <row r="629">
-      <c r="A629" s="73"/>
-      <c r="B629" s="74"/>
+      <c r="A629" s="75"/>
+      <c r="B629" s="76"/>
       <c r="C629" s="34"/>
       <c r="D629" s="34"/>
       <c r="E629" s="34"/>
@@ -44650,8 +44822,8 @@
       </c>
     </row>
     <row r="630">
-      <c r="A630" s="73"/>
-      <c r="B630" s="74"/>
+      <c r="A630" s="75"/>
+      <c r="B630" s="76"/>
       <c r="C630" s="34"/>
       <c r="D630" s="34"/>
       <c r="E630" s="34"/>
@@ -44676,8 +44848,8 @@
       </c>
     </row>
     <row r="631">
-      <c r="A631" s="73"/>
-      <c r="B631" s="74"/>
+      <c r="A631" s="75"/>
+      <c r="B631" s="76"/>
       <c r="C631" s="34"/>
       <c r="D631" s="34"/>
       <c r="E631" s="34"/>
@@ -44702,8 +44874,8 @@
       </c>
     </row>
     <row r="632">
-      <c r="A632" s="73"/>
-      <c r="B632" s="74"/>
+      <c r="A632" s="75"/>
+      <c r="B632" s="76"/>
       <c r="C632" s="34"/>
       <c r="D632" s="34"/>
       <c r="E632" s="34"/>
@@ -44728,8 +44900,8 @@
       </c>
     </row>
     <row r="633">
-      <c r="A633" s="73"/>
-      <c r="B633" s="74"/>
+      <c r="A633" s="75"/>
+      <c r="B633" s="76"/>
       <c r="C633" s="34"/>
       <c r="D633" s="34"/>
       <c r="E633" s="34"/>
@@ -44754,8 +44926,8 @@
       </c>
     </row>
     <row r="634">
-      <c r="A634" s="73"/>
-      <c r="B634" s="74"/>
+      <c r="A634" s="75"/>
+      <c r="B634" s="76"/>
       <c r="C634" s="34"/>
       <c r="D634" s="34"/>
       <c r="E634" s="34"/>
@@ -44780,8 +44952,8 @@
       </c>
     </row>
     <row r="635">
-      <c r="A635" s="73"/>
-      <c r="B635" s="74"/>
+      <c r="A635" s="75"/>
+      <c r="B635" s="76"/>
       <c r="C635" s="34"/>
       <c r="D635" s="34"/>
       <c r="E635" s="34"/>
@@ -44806,8 +44978,8 @@
       </c>
     </row>
     <row r="636">
-      <c r="A636" s="73"/>
-      <c r="B636" s="74"/>
+      <c r="A636" s="75"/>
+      <c r="B636" s="76"/>
       <c r="C636" s="34"/>
       <c r="D636" s="34"/>
       <c r="E636" s="34"/>
@@ -44832,8 +45004,8 @@
       </c>
     </row>
     <row r="637">
-      <c r="A637" s="73"/>
-      <c r="B637" s="74"/>
+      <c r="A637" s="75"/>
+      <c r="B637" s="76"/>
       <c r="C637" s="34"/>
       <c r="D637" s="34"/>
       <c r="E637" s="34"/>
@@ -44858,8 +45030,8 @@
       </c>
     </row>
     <row r="638">
-      <c r="A638" s="73"/>
-      <c r="B638" s="74"/>
+      <c r="A638" s="75"/>
+      <c r="B638" s="76"/>
       <c r="C638" s="34"/>
       <c r="D638" s="34"/>
       <c r="E638" s="34"/>
@@ -44884,8 +45056,8 @@
       </c>
     </row>
     <row r="639">
-      <c r="A639" s="73"/>
-      <c r="B639" s="74"/>
+      <c r="A639" s="75"/>
+      <c r="B639" s="76"/>
       <c r="C639" s="34"/>
       <c r="D639" s="34"/>
       <c r="E639" s="34"/>
@@ -44910,8 +45082,8 @@
       </c>
     </row>
     <row r="640">
-      <c r="A640" s="73"/>
-      <c r="B640" s="74"/>
+      <c r="A640" s="75"/>
+      <c r="B640" s="76"/>
       <c r="C640" s="34"/>
       <c r="D640" s="34"/>
       <c r="E640" s="34"/>
@@ -44936,8 +45108,8 @@
       </c>
     </row>
     <row r="641">
-      <c r="A641" s="73"/>
-      <c r="B641" s="74"/>
+      <c r="A641" s="75"/>
+      <c r="B641" s="76"/>
       <c r="C641" s="34"/>
       <c r="D641" s="34"/>
       <c r="E641" s="34"/>
@@ -44962,8 +45134,8 @@
       </c>
     </row>
     <row r="642">
-      <c r="A642" s="73"/>
-      <c r="B642" s="74"/>
+      <c r="A642" s="75"/>
+      <c r="B642" s="76"/>
       <c r="C642" s="34"/>
       <c r="D642" s="34"/>
       <c r="E642" s="34"/>
@@ -44988,8 +45160,8 @@
       </c>
     </row>
     <row r="643">
-      <c r="A643" s="73"/>
-      <c r="B643" s="74"/>
+      <c r="A643" s="75"/>
+      <c r="B643" s="76"/>
       <c r="C643" s="34"/>
       <c r="D643" s="34"/>
       <c r="E643" s="34"/>
@@ -45014,8 +45186,8 @@
       </c>
     </row>
     <row r="644">
-      <c r="A644" s="73"/>
-      <c r="B644" s="74"/>
+      <c r="A644" s="75"/>
+      <c r="B644" s="76"/>
       <c r="C644" s="34"/>
       <c r="D644" s="34"/>
       <c r="E644" s="34"/>
@@ -45040,8 +45212,8 @@
       </c>
     </row>
     <row r="645">
-      <c r="A645" s="73"/>
-      <c r="B645" s="74"/>
+      <c r="A645" s="75"/>
+      <c r="B645" s="76"/>
       <c r="C645" s="34"/>
       <c r="D645" s="34"/>
       <c r="E645" s="34"/>
@@ -45066,8 +45238,8 @@
       </c>
     </row>
     <row r="646">
-      <c r="A646" s="73"/>
-      <c r="B646" s="74"/>
+      <c r="A646" s="75"/>
+      <c r="B646" s="76"/>
       <c r="C646" s="34"/>
       <c r="D646" s="34"/>
       <c r="E646" s="34"/>
@@ -45092,8 +45264,8 @@
       </c>
     </row>
     <row r="647">
-      <c r="A647" s="73"/>
-      <c r="B647" s="74"/>
+      <c r="A647" s="75"/>
+      <c r="B647" s="76"/>
       <c r="C647" s="34"/>
       <c r="D647" s="34"/>
       <c r="E647" s="34"/>
@@ -45118,8 +45290,8 @@
       </c>
     </row>
     <row r="648">
-      <c r="A648" s="73"/>
-      <c r="B648" s="74"/>
+      <c r="A648" s="75"/>
+      <c r="B648" s="76"/>
       <c r="C648" s="34"/>
       <c r="D648" s="34"/>
       <c r="E648" s="34"/>
@@ -45144,8 +45316,8 @@
       </c>
     </row>
     <row r="649">
-      <c r="A649" s="73"/>
-      <c r="B649" s="74"/>
+      <c r="A649" s="75"/>
+      <c r="B649" s="76"/>
       <c r="C649" s="34"/>
       <c r="D649" s="34"/>
       <c r="E649" s="34"/>
@@ -45170,8 +45342,8 @@
       </c>
     </row>
     <row r="650">
-      <c r="A650" s="73"/>
-      <c r="B650" s="74"/>
+      <c r="A650" s="75"/>
+      <c r="B650" s="76"/>
       <c r="C650" s="34"/>
       <c r="D650" s="34"/>
       <c r="E650" s="34"/>
@@ -45196,8 +45368,8 @@
       </c>
     </row>
     <row r="651">
-      <c r="A651" s="73"/>
-      <c r="B651" s="74"/>
+      <c r="A651" s="75"/>
+      <c r="B651" s="76"/>
       <c r="C651" s="34"/>
       <c r="D651" s="34"/>
       <c r="E651" s="34"/>
@@ -45222,8 +45394,8 @@
       </c>
     </row>
     <row r="652">
-      <c r="A652" s="73"/>
-      <c r="B652" s="74"/>
+      <c r="A652" s="75"/>
+      <c r="B652" s="76"/>
       <c r="C652" s="34"/>
       <c r="D652" s="34"/>
       <c r="E652" s="34"/>
@@ -45248,8 +45420,8 @@
       </c>
     </row>
     <row r="653">
-      <c r="A653" s="73"/>
-      <c r="B653" s="74"/>
+      <c r="A653" s="75"/>
+      <c r="B653" s="76"/>
       <c r="C653" s="34"/>
       <c r="D653" s="34"/>
       <c r="E653" s="34"/>
@@ -45274,8 +45446,8 @@
       </c>
     </row>
     <row r="654">
-      <c r="A654" s="73"/>
-      <c r="B654" s="74"/>
+      <c r="A654" s="75"/>
+      <c r="B654" s="76"/>
       <c r="C654" s="34"/>
       <c r="D654" s="34"/>
       <c r="E654" s="34"/>
@@ -45300,8 +45472,8 @@
       </c>
     </row>
     <row r="655">
-      <c r="A655" s="73"/>
-      <c r="B655" s="74"/>
+      <c r="A655" s="75"/>
+      <c r="B655" s="76"/>
       <c r="C655" s="34"/>
       <c r="D655" s="34"/>
       <c r="E655" s="34"/>
@@ -45326,8 +45498,8 @@
       </c>
     </row>
     <row r="656">
-      <c r="A656" s="73"/>
-      <c r="B656" s="74"/>
+      <c r="A656" s="75"/>
+      <c r="B656" s="76"/>
       <c r="C656" s="34"/>
       <c r="D656" s="34"/>
       <c r="E656" s="34"/>
@@ -45352,8 +45524,8 @@
       </c>
     </row>
     <row r="657">
-      <c r="A657" s="73"/>
-      <c r="B657" s="74"/>
+      <c r="A657" s="75"/>
+      <c r="B657" s="76"/>
       <c r="C657" s="34"/>
       <c r="D657" s="34"/>
       <c r="E657" s="34"/>
@@ -45378,8 +45550,8 @@
       </c>
     </row>
     <row r="658">
-      <c r="A658" s="73"/>
-      <c r="B658" s="74"/>
+      <c r="A658" s="75"/>
+      <c r="B658" s="76"/>
       <c r="C658" s="34"/>
       <c r="D658" s="34"/>
       <c r="E658" s="34"/>
@@ -45404,8 +45576,8 @@
       </c>
     </row>
     <row r="659">
-      <c r="A659" s="73"/>
-      <c r="B659" s="74"/>
+      <c r="A659" s="75"/>
+      <c r="B659" s="76"/>
       <c r="C659" s="34"/>
       <c r="D659" s="34"/>
       <c r="E659" s="34"/>
@@ -45430,8 +45602,8 @@
       </c>
     </row>
     <row r="660">
-      <c r="A660" s="73"/>
-      <c r="B660" s="74"/>
+      <c r="A660" s="75"/>
+      <c r="B660" s="76"/>
       <c r="C660" s="34"/>
       <c r="D660" s="34"/>
       <c r="E660" s="34"/>
@@ -45456,8 +45628,8 @@
       </c>
     </row>
     <row r="661">
-      <c r="A661" s="73"/>
-      <c r="B661" s="74"/>
+      <c r="A661" s="75"/>
+      <c r="B661" s="76"/>
       <c r="C661" s="34"/>
       <c r="D661" s="34"/>
       <c r="E661" s="34"/>
@@ -45482,8 +45654,8 @@
       </c>
     </row>
     <row r="662">
-      <c r="A662" s="73"/>
-      <c r="B662" s="74"/>
+      <c r="A662" s="75"/>
+      <c r="B662" s="76"/>
       <c r="C662" s="34"/>
       <c r="D662" s="34"/>
       <c r="E662" s="34"/>
@@ -45508,8 +45680,8 @@
       </c>
     </row>
     <row r="663">
-      <c r="A663" s="73"/>
-      <c r="B663" s="74"/>
+      <c r="A663" s="75"/>
+      <c r="B663" s="76"/>
       <c r="C663" s="34"/>
       <c r="D663" s="34"/>
       <c r="E663" s="34"/>
@@ -45534,8 +45706,8 @@
       </c>
     </row>
     <row r="664">
-      <c r="A664" s="73"/>
-      <c r="B664" s="74"/>
+      <c r="A664" s="75"/>
+      <c r="B664" s="76"/>
       <c r="C664" s="34"/>
       <c r="D664" s="34"/>
       <c r="E664" s="34"/>
@@ -45560,8 +45732,8 @@
       </c>
     </row>
     <row r="665">
-      <c r="A665" s="73"/>
-      <c r="B665" s="74"/>
+      <c r="A665" s="75"/>
+      <c r="B665" s="76"/>
       <c r="C665" s="34"/>
       <c r="D665" s="34"/>
       <c r="E665" s="34"/>
@@ -45586,8 +45758,8 @@
       </c>
     </row>
     <row r="666">
-      <c r="A666" s="73"/>
-      <c r="B666" s="74"/>
+      <c r="A666" s="75"/>
+      <c r="B666" s="76"/>
       <c r="C666" s="34"/>
       <c r="D666" s="34"/>
       <c r="E666" s="34"/>
@@ -45612,8 +45784,8 @@
       </c>
     </row>
     <row r="667">
-      <c r="A667" s="73"/>
-      <c r="B667" s="74"/>
+      <c r="A667" s="75"/>
+      <c r="B667" s="76"/>
       <c r="C667" s="34"/>
       <c r="D667" s="34"/>
       <c r="E667" s="34"/>
@@ -45638,8 +45810,8 @@
       </c>
     </row>
     <row r="668">
-      <c r="A668" s="73"/>
-      <c r="B668" s="74"/>
+      <c r="A668" s="75"/>
+      <c r="B668" s="76"/>
       <c r="C668" s="34"/>
       <c r="D668" s="34"/>
       <c r="E668" s="34"/>
@@ -45664,8 +45836,8 @@
       </c>
     </row>
     <row r="669">
-      <c r="A669" s="73"/>
-      <c r="B669" s="74"/>
+      <c r="A669" s="75"/>
+      <c r="B669" s="76"/>
       <c r="C669" s="34"/>
       <c r="D669" s="34"/>
       <c r="E669" s="34"/>
@@ -45690,8 +45862,8 @@
       </c>
     </row>
     <row r="670">
-      <c r="A670" s="73"/>
-      <c r="B670" s="74"/>
+      <c r="A670" s="75"/>
+      <c r="B670" s="76"/>
       <c r="C670" s="34"/>
       <c r="D670" s="34"/>
       <c r="E670" s="34"/>
@@ -45716,8 +45888,8 @@
       </c>
     </row>
     <row r="671">
-      <c r="A671" s="73"/>
-      <c r="B671" s="74"/>
+      <c r="A671" s="75"/>
+      <c r="B671" s="76"/>
       <c r="C671" s="34"/>
       <c r="D671" s="34"/>
       <c r="E671" s="34"/>
@@ -45742,8 +45914,8 @@
       </c>
     </row>
     <row r="672">
-      <c r="A672" s="73"/>
-      <c r="B672" s="74"/>
+      <c r="A672" s="75"/>
+      <c r="B672" s="76"/>
       <c r="C672" s="34"/>
       <c r="D672" s="34"/>
       <c r="E672" s="34"/>
@@ -45768,8 +45940,8 @@
       </c>
     </row>
     <row r="673">
-      <c r="A673" s="73"/>
-      <c r="B673" s="74"/>
+      <c r="A673" s="75"/>
+      <c r="B673" s="76"/>
       <c r="C673" s="34"/>
       <c r="D673" s="34"/>
       <c r="E673" s="34"/>
@@ -45794,8 +45966,8 @@
       </c>
     </row>
     <row r="674">
-      <c r="A674" s="73"/>
-      <c r="B674" s="74"/>
+      <c r="A674" s="75"/>
+      <c r="B674" s="76"/>
       <c r="C674" s="34"/>
       <c r="D674" s="34"/>
       <c r="E674" s="34"/>
@@ -45820,8 +45992,8 @@
       </c>
     </row>
     <row r="675">
-      <c r="A675" s="73"/>
-      <c r="B675" s="74"/>
+      <c r="A675" s="75"/>
+      <c r="B675" s="76"/>
       <c r="C675" s="34"/>
       <c r="D675" s="34"/>
       <c r="E675" s="34"/>
@@ -45846,8 +46018,8 @@
       </c>
     </row>
     <row r="676">
-      <c r="A676" s="73"/>
-      <c r="B676" s="74"/>
+      <c r="A676" s="75"/>
+      <c r="B676" s="76"/>
       <c r="C676" s="34"/>
       <c r="D676" s="34"/>
       <c r="E676" s="34"/>
@@ -45872,8 +46044,8 @@
       </c>
     </row>
     <row r="677">
-      <c r="A677" s="73"/>
-      <c r="B677" s="74"/>
+      <c r="A677" s="75"/>
+      <c r="B677" s="76"/>
       <c r="C677" s="34"/>
       <c r="D677" s="34"/>
       <c r="E677" s="34"/>
@@ -45898,8 +46070,8 @@
       </c>
     </row>
     <row r="678">
-      <c r="A678" s="73"/>
-      <c r="B678" s="74"/>
+      <c r="A678" s="75"/>
+      <c r="B678" s="76"/>
       <c r="C678" s="34"/>
       <c r="D678" s="34"/>
       <c r="E678" s="34"/>
@@ -45924,8 +46096,8 @@
       </c>
     </row>
     <row r="679">
-      <c r="A679" s="73"/>
-      <c r="B679" s="74"/>
+      <c r="A679" s="75"/>
+      <c r="B679" s="76"/>
       <c r="C679" s="34"/>
       <c r="D679" s="34"/>
       <c r="E679" s="34"/>
@@ -45950,8 +46122,8 @@
       </c>
     </row>
     <row r="680">
-      <c r="A680" s="73"/>
-      <c r="B680" s="74"/>
+      <c r="A680" s="75"/>
+      <c r="B680" s="76"/>
       <c r="C680" s="34"/>
       <c r="D680" s="34"/>
       <c r="E680" s="34"/>
@@ -45976,8 +46148,8 @@
       </c>
     </row>
     <row r="681">
-      <c r="A681" s="73"/>
-      <c r="B681" s="74"/>
+      <c r="A681" s="75"/>
+      <c r="B681" s="76"/>
       <c r="C681" s="34"/>
       <c r="D681" s="34"/>
       <c r="E681" s="34"/>
@@ -46002,8 +46174,8 @@
       </c>
     </row>
     <row r="682">
-      <c r="A682" s="73"/>
-      <c r="B682" s="74"/>
+      <c r="A682" s="75"/>
+      <c r="B682" s="76"/>
       <c r="C682" s="34"/>
       <c r="D682" s="34"/>
       <c r="E682" s="34"/>
@@ -46028,8 +46200,8 @@
       </c>
     </row>
     <row r="683">
-      <c r="A683" s="73"/>
-      <c r="B683" s="74"/>
+      <c r="A683" s="75"/>
+      <c r="B683" s="76"/>
       <c r="C683" s="34"/>
       <c r="D683" s="34"/>
       <c r="E683" s="34"/>
@@ -46054,8 +46226,8 @@
       </c>
     </row>
     <row r="684">
-      <c r="A684" s="73"/>
-      <c r="B684" s="74"/>
+      <c r="A684" s="75"/>
+      <c r="B684" s="76"/>
       <c r="C684" s="34"/>
       <c r="D684" s="34"/>
       <c r="E684" s="34"/>
@@ -46080,8 +46252,8 @@
       </c>
     </row>
     <row r="685">
-      <c r="A685" s="73"/>
-      <c r="B685" s="74"/>
+      <c r="A685" s="75"/>
+      <c r="B685" s="76"/>
       <c r="C685" s="34"/>
       <c r="D685" s="34"/>
       <c r="E685" s="34"/>
@@ -46106,8 +46278,8 @@
       </c>
     </row>
     <row r="686">
-      <c r="A686" s="73"/>
-      <c r="B686" s="74"/>
+      <c r="A686" s="75"/>
+      <c r="B686" s="76"/>
       <c r="C686" s="34"/>
       <c r="D686" s="34"/>
       <c r="E686" s="34"/>
@@ -46132,8 +46304,8 @@
       </c>
     </row>
     <row r="687">
-      <c r="A687" s="73"/>
-      <c r="B687" s="74"/>
+      <c r="A687" s="75"/>
+      <c r="B687" s="76"/>
       <c r="C687" s="34"/>
       <c r="D687" s="34"/>
       <c r="E687" s="34"/>
@@ -46158,8 +46330,8 @@
       </c>
     </row>
     <row r="688">
-      <c r="A688" s="73"/>
-      <c r="B688" s="74"/>
+      <c r="A688" s="75"/>
+      <c r="B688" s="76"/>
       <c r="C688" s="34"/>
       <c r="D688" s="34"/>
       <c r="E688" s="34"/>
@@ -46184,8 +46356,8 @@
       </c>
     </row>
     <row r="689">
-      <c r="A689" s="73"/>
-      <c r="B689" s="74"/>
+      <c r="A689" s="75"/>
+      <c r="B689" s="76"/>
       <c r="C689" s="34"/>
       <c r="D689" s="34"/>
       <c r="E689" s="34"/>
@@ -46210,8 +46382,8 @@
       </c>
     </row>
     <row r="690">
-      <c r="A690" s="73"/>
-      <c r="B690" s="74"/>
+      <c r="A690" s="75"/>
+      <c r="B690" s="76"/>
       <c r="C690" s="34"/>
       <c r="D690" s="34"/>
       <c r="E690" s="34"/>
@@ -46236,8 +46408,8 @@
       </c>
     </row>
     <row r="691">
-      <c r="A691" s="73"/>
-      <c r="B691" s="74"/>
+      <c r="A691" s="75"/>
+      <c r="B691" s="76"/>
       <c r="C691" s="34"/>
       <c r="D691" s="34"/>
       <c r="E691" s="34"/>
@@ -46262,8 +46434,8 @@
       </c>
     </row>
     <row r="692">
-      <c r="A692" s="73"/>
-      <c r="B692" s="74"/>
+      <c r="A692" s="75"/>
+      <c r="B692" s="76"/>
       <c r="C692" s="34"/>
       <c r="D692" s="34"/>
       <c r="E692" s="34"/>
@@ -46288,8 +46460,8 @@
       </c>
     </row>
     <row r="693">
-      <c r="A693" s="73"/>
-      <c r="B693" s="74"/>
+      <c r="A693" s="75"/>
+      <c r="B693" s="76"/>
       <c r="C693" s="34"/>
       <c r="D693" s="34"/>
       <c r="E693" s="34"/>
@@ -46314,8 +46486,8 @@
       </c>
     </row>
     <row r="694">
-      <c r="A694" s="73"/>
-      <c r="B694" s="74"/>
+      <c r="A694" s="75"/>
+      <c r="B694" s="76"/>
       <c r="C694" s="34"/>
       <c r="D694" s="34"/>
       <c r="E694" s="34"/>
@@ -46340,8 +46512,8 @@
       </c>
     </row>
     <row r="695">
-      <c r="A695" s="73"/>
-      <c r="B695" s="74"/>
+      <c r="A695" s="75"/>
+      <c r="B695" s="76"/>
       <c r="C695" s="34"/>
       <c r="D695" s="34"/>
       <c r="E695" s="34"/>
@@ -46366,8 +46538,8 @@
       </c>
     </row>
     <row r="696">
-      <c r="A696" s="73"/>
-      <c r="B696" s="74"/>
+      <c r="A696" s="75"/>
+      <c r="B696" s="76"/>
       <c r="C696" s="34"/>
       <c r="D696" s="34"/>
       <c r="E696" s="34"/>
@@ -46392,8 +46564,8 @@
       </c>
     </row>
     <row r="697">
-      <c r="A697" s="73"/>
-      <c r="B697" s="74"/>
+      <c r="A697" s="75"/>
+      <c r="B697" s="76"/>
       <c r="C697" s="34"/>
       <c r="D697" s="34"/>
       <c r="E697" s="34"/>
@@ -46418,8 +46590,8 @@
       </c>
     </row>
     <row r="698">
-      <c r="A698" s="73"/>
-      <c r="B698" s="74"/>
+      <c r="A698" s="75"/>
+      <c r="B698" s="76"/>
       <c r="C698" s="34"/>
       <c r="D698" s="34"/>
       <c r="E698" s="34"/>
@@ -46444,8 +46616,8 @@
       </c>
     </row>
     <row r="699">
-      <c r="A699" s="73"/>
-      <c r="B699" s="74"/>
+      <c r="A699" s="75"/>
+      <c r="B699" s="76"/>
       <c r="C699" s="34"/>
       <c r="D699" s="34"/>
       <c r="E699" s="34"/>
@@ -46470,8 +46642,8 @@
       </c>
     </row>
     <row r="700">
-      <c r="A700" s="73"/>
-      <c r="B700" s="74"/>
+      <c r="A700" s="75"/>
+      <c r="B700" s="76"/>
       <c r="C700" s="34"/>
       <c r="D700" s="34"/>
       <c r="E700" s="34"/>
@@ -46496,8 +46668,8 @@
       </c>
     </row>
     <row r="701">
-      <c r="A701" s="73"/>
-      <c r="B701" s="74"/>
+      <c r="A701" s="75"/>
+      <c r="B701" s="76"/>
       <c r="C701" s="34"/>
       <c r="D701" s="34"/>
       <c r="E701" s="34"/>
@@ -47063,15 +47235,18 @@
     <hyperlink r:id="rId159" ref="S597"/>
     <hyperlink r:id="rId160" ref="S598"/>
     <hyperlink r:id="rId161" ref="S599"/>
+    <hyperlink r:id="rId162" ref="S600"/>
+    <hyperlink r:id="rId163" ref="S601"/>
+    <hyperlink r:id="rId164" ref="S602"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId162"/>
-  <legacyDrawing r:id="rId163"/>
+  <drawing r:id="rId165"/>
+  <legacyDrawing r:id="rId166"/>
   <tableParts count="2">
-    <tablePart r:id="rId166"/>
-    <tablePart r:id="rId167"/>
+    <tablePart r:id="rId169"/>
+    <tablePart r:id="rId170"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201116
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -571,7 +571,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6747" uniqueCount="2238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6767" uniqueCount="2247">
   <si>
     <t>案例</t>
   </si>
@@ -8171,7 +8171,37 @@
     <t>#602</t>
   </si>
   <si>
+    <t>2月-11/12 日本</t>
+  </si>
+  <si>
+    <t>11月初</t>
+  </si>
+  <si>
+    <t>11/12 採檢
+11/15 確診</t>
+  </si>
+  <si>
+    <t>鼻塞 頭痛 噁心 流鼻水 嗅覺異常 味覺異常</t>
+  </si>
+  <si>
+    <t>長期定居日本</t>
+  </si>
+  <si>
+    <t>新增2例境外移入COVID-19病例，自日本、美國入境</t>
+  </si>
+  <si>
     <t>#603</t>
+  </si>
+  <si>
+    <t>8月-11/13 美國</t>
+  </si>
+  <si>
+    <t>11/13 採檢
+11/15 確診</t>
+  </si>
+  <si>
+    <t>因工作長期居住美國
+入境時個案主動告知搭機時自覺出現嗅味覺異常情形，但下機後即恢復</t>
   </si>
 </sst>
 </file>
@@ -8182,7 +8212,7 @@
     <numFmt numFmtId="164" formatCode="mm&quot;月&quot;dd&quot;日 &quot;dddd"/>
     <numFmt numFmtId="165" formatCode="m/d"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="18">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -8263,7 +8293,6 @@
       <u/>
       <color rgb="FFFFFFFF"/>
     </font>
-    <font/>
   </fonts>
   <fills count="7">
     <fill>
@@ -8309,7 +8338,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="75">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -8528,12 +8557,6 @@
     </xf>
     <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
@@ -44106,7 +44129,7 @@
       </c>
     </row>
     <row r="603">
-      <c r="A603" s="73" t="s">
+      <c r="A603" s="16" t="s">
         <v>2236</v>
       </c>
       <c r="B603" s="6">
@@ -44115,24 +44138,46 @@
       <c r="C603" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D603" s="74" t="s">
+      <c r="D603" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E603" s="34"/>
+      <c r="E603" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F603" s="34"/>
-      <c r="G603" s="34"/>
-      <c r="H603" s="21"/>
-      <c r="I603" s="19"/>
-      <c r="J603" s="10"/>
-      <c r="K603" s="22"/>
-      <c r="L603" s="23"/>
-      <c r="M603" s="22"/>
+      <c r="G603" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H603" s="8" t="s">
+        <v>2237</v>
+      </c>
+      <c r="I603" s="9">
+        <v>44147.0</v>
+      </c>
+      <c r="J603" s="12" t="s">
+        <v>2238</v>
+      </c>
+      <c r="K603" s="13" t="s">
+        <v>2239</v>
+      </c>
+      <c r="L603" s="12" t="s">
+        <v>363</v>
+      </c>
+      <c r="M603" s="13" t="s">
+        <v>2240</v>
+      </c>
       <c r="N603" s="25"/>
-      <c r="O603" s="21"/>
-      <c r="P603" s="21"/>
+      <c r="O603" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P603" s="8" t="s">
+        <v>2241</v>
+      </c>
       <c r="Q603" s="19"/>
       <c r="R603" s="19"/>
-      <c r="S603" s="20"/>
+      <c r="S603" s="61" t="s">
+        <v>2242</v>
+      </c>
       <c r="T603" s="20"/>
       <c r="U603" s="18" t="str">
         <f t="shared" si="1"/>
@@ -44140,8 +44185,8 @@
       </c>
     </row>
     <row r="604">
-      <c r="A604" s="73" t="s">
-        <v>2237</v>
+      <c r="A604" s="16" t="s">
+        <v>2243</v>
       </c>
       <c r="B604" s="6">
         <v>44150.0</v>
@@ -44149,22 +44194,44 @@
       <c r="C604" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D604" s="34"/>
-      <c r="E604" s="34"/>
+      <c r="D604" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E604" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F604" s="34"/>
-      <c r="G604" s="34"/>
-      <c r="H604" s="21"/>
-      <c r="I604" s="19"/>
+      <c r="G604" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H604" s="8" t="s">
+        <v>2244</v>
+      </c>
+      <c r="I604" s="9">
+        <v>44148.0</v>
+      </c>
       <c r="J604" s="10"/>
-      <c r="K604" s="22"/>
-      <c r="L604" s="23"/>
-      <c r="M604" s="22"/>
+      <c r="K604" s="13" t="s">
+        <v>2245</v>
+      </c>
+      <c r="L604" s="12" t="s">
+        <v>363</v>
+      </c>
+      <c r="M604" s="13" t="s">
+        <v>1418</v>
+      </c>
       <c r="N604" s="25"/>
-      <c r="O604" s="21"/>
-      <c r="P604" s="21"/>
+      <c r="O604" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P604" s="8" t="s">
+        <v>2246</v>
+      </c>
       <c r="Q604" s="19"/>
       <c r="R604" s="19"/>
-      <c r="S604" s="20"/>
+      <c r="S604" s="61" t="s">
+        <v>2242</v>
+      </c>
       <c r="T604" s="20"/>
       <c r="U604" s="18" t="str">
         <f t="shared" si="1"/>
@@ -44172,8 +44239,8 @@
       </c>
     </row>
     <row r="605">
-      <c r="A605" s="75"/>
-      <c r="B605" s="76"/>
+      <c r="A605" s="73"/>
+      <c r="B605" s="74"/>
       <c r="C605" s="34"/>
       <c r="D605" s="34"/>
       <c r="E605" s="34"/>
@@ -44198,8 +44265,8 @@
       </c>
     </row>
     <row r="606">
-      <c r="A606" s="75"/>
-      <c r="B606" s="76"/>
+      <c r="A606" s="73"/>
+      <c r="B606" s="74"/>
       <c r="C606" s="34"/>
       <c r="D606" s="34"/>
       <c r="E606" s="34"/>
@@ -44224,8 +44291,8 @@
       </c>
     </row>
     <row r="607">
-      <c r="A607" s="75"/>
-      <c r="B607" s="76"/>
+      <c r="A607" s="73"/>
+      <c r="B607" s="74"/>
       <c r="C607" s="34"/>
       <c r="D607" s="34"/>
       <c r="E607" s="34"/>
@@ -44250,8 +44317,8 @@
       </c>
     </row>
     <row r="608">
-      <c r="A608" s="75"/>
-      <c r="B608" s="76"/>
+      <c r="A608" s="73"/>
+      <c r="B608" s="74"/>
       <c r="C608" s="34"/>
       <c r="D608" s="34"/>
       <c r="E608" s="34"/>
@@ -44276,8 +44343,8 @@
       </c>
     </row>
     <row r="609">
-      <c r="A609" s="75"/>
-      <c r="B609" s="76"/>
+      <c r="A609" s="73"/>
+      <c r="B609" s="74"/>
       <c r="C609" s="34"/>
       <c r="D609" s="34"/>
       <c r="E609" s="34"/>
@@ -44302,8 +44369,8 @@
       </c>
     </row>
     <row r="610">
-      <c r="A610" s="75"/>
-      <c r="B610" s="76"/>
+      <c r="A610" s="73"/>
+      <c r="B610" s="74"/>
       <c r="C610" s="34"/>
       <c r="D610" s="34"/>
       <c r="E610" s="34"/>
@@ -44328,8 +44395,8 @@
       </c>
     </row>
     <row r="611">
-      <c r="A611" s="75"/>
-      <c r="B611" s="76"/>
+      <c r="A611" s="73"/>
+      <c r="B611" s="74"/>
       <c r="C611" s="34"/>
       <c r="D611" s="34"/>
       <c r="E611" s="34"/>
@@ -44354,8 +44421,8 @@
       </c>
     </row>
     <row r="612">
-      <c r="A612" s="75"/>
-      <c r="B612" s="76"/>
+      <c r="A612" s="73"/>
+      <c r="B612" s="74"/>
       <c r="C612" s="34"/>
       <c r="D612" s="34"/>
       <c r="E612" s="34"/>
@@ -44380,8 +44447,8 @@
       </c>
     </row>
     <row r="613">
-      <c r="A613" s="75"/>
-      <c r="B613" s="76"/>
+      <c r="A613" s="73"/>
+      <c r="B613" s="74"/>
       <c r="C613" s="34"/>
       <c r="D613" s="34"/>
       <c r="E613" s="34"/>
@@ -44406,8 +44473,8 @@
       </c>
     </row>
     <row r="614">
-      <c r="A614" s="75"/>
-      <c r="B614" s="76"/>
+      <c r="A614" s="73"/>
+      <c r="B614" s="74"/>
       <c r="C614" s="34"/>
       <c r="D614" s="34"/>
       <c r="E614" s="34"/>
@@ -44432,8 +44499,8 @@
       </c>
     </row>
     <row r="615">
-      <c r="A615" s="75"/>
-      <c r="B615" s="76"/>
+      <c r="A615" s="73"/>
+      <c r="B615" s="74"/>
       <c r="C615" s="34"/>
       <c r="D615" s="34"/>
       <c r="E615" s="34"/>
@@ -44458,8 +44525,8 @@
       </c>
     </row>
     <row r="616">
-      <c r="A616" s="75"/>
-      <c r="B616" s="76"/>
+      <c r="A616" s="73"/>
+      <c r="B616" s="74"/>
       <c r="C616" s="34"/>
       <c r="D616" s="34"/>
       <c r="E616" s="34"/>
@@ -44484,8 +44551,8 @@
       </c>
     </row>
     <row r="617">
-      <c r="A617" s="75"/>
-      <c r="B617" s="76"/>
+      <c r="A617" s="73"/>
+      <c r="B617" s="74"/>
       <c r="C617" s="34"/>
       <c r="D617" s="34"/>
       <c r="E617" s="34"/>
@@ -44510,8 +44577,8 @@
       </c>
     </row>
     <row r="618">
-      <c r="A618" s="75"/>
-      <c r="B618" s="76"/>
+      <c r="A618" s="73"/>
+      <c r="B618" s="74"/>
       <c r="C618" s="34"/>
       <c r="D618" s="34"/>
       <c r="E618" s="34"/>
@@ -44536,8 +44603,8 @@
       </c>
     </row>
     <row r="619">
-      <c r="A619" s="75"/>
-      <c r="B619" s="76"/>
+      <c r="A619" s="73"/>
+      <c r="B619" s="74"/>
       <c r="C619" s="34"/>
       <c r="D619" s="34"/>
       <c r="E619" s="34"/>
@@ -44562,8 +44629,8 @@
       </c>
     </row>
     <row r="620">
-      <c r="A620" s="75"/>
-      <c r="B620" s="76"/>
+      <c r="A620" s="73"/>
+      <c r="B620" s="74"/>
       <c r="C620" s="34"/>
       <c r="D620" s="34"/>
       <c r="E620" s="34"/>
@@ -44588,8 +44655,8 @@
       </c>
     </row>
     <row r="621">
-      <c r="A621" s="75"/>
-      <c r="B621" s="76"/>
+      <c r="A621" s="73"/>
+      <c r="B621" s="74"/>
       <c r="C621" s="34"/>
       <c r="D621" s="34"/>
       <c r="E621" s="34"/>
@@ -44614,8 +44681,8 @@
       </c>
     </row>
     <row r="622">
-      <c r="A622" s="75"/>
-      <c r="B622" s="76"/>
+      <c r="A622" s="73"/>
+      <c r="B622" s="74"/>
       <c r="C622" s="34"/>
       <c r="D622" s="34"/>
       <c r="E622" s="34"/>
@@ -44640,8 +44707,8 @@
       </c>
     </row>
     <row r="623">
-      <c r="A623" s="75"/>
-      <c r="B623" s="76"/>
+      <c r="A623" s="73"/>
+      <c r="B623" s="74"/>
       <c r="C623" s="34"/>
       <c r="D623" s="34"/>
       <c r="E623" s="34"/>
@@ -44666,8 +44733,8 @@
       </c>
     </row>
     <row r="624">
-      <c r="A624" s="75"/>
-      <c r="B624" s="76"/>
+      <c r="A624" s="73"/>
+      <c r="B624" s="74"/>
       <c r="C624" s="34"/>
       <c r="D624" s="34"/>
       <c r="E624" s="34"/>
@@ -44692,8 +44759,8 @@
       </c>
     </row>
     <row r="625">
-      <c r="A625" s="75"/>
-      <c r="B625" s="76"/>
+      <c r="A625" s="73"/>
+      <c r="B625" s="74"/>
       <c r="C625" s="34"/>
       <c r="D625" s="34"/>
       <c r="E625" s="34"/>
@@ -44718,8 +44785,8 @@
       </c>
     </row>
     <row r="626">
-      <c r="A626" s="75"/>
-      <c r="B626" s="76"/>
+      <c r="A626" s="73"/>
+      <c r="B626" s="74"/>
       <c r="C626" s="34"/>
       <c r="D626" s="34"/>
       <c r="E626" s="34"/>
@@ -44744,8 +44811,8 @@
       </c>
     </row>
     <row r="627">
-      <c r="A627" s="75"/>
-      <c r="B627" s="76"/>
+      <c r="A627" s="73"/>
+      <c r="B627" s="74"/>
       <c r="C627" s="34"/>
       <c r="D627" s="34"/>
       <c r="E627" s="34"/>
@@ -44770,8 +44837,8 @@
       </c>
     </row>
     <row r="628">
-      <c r="A628" s="75"/>
-      <c r="B628" s="76"/>
+      <c r="A628" s="73"/>
+      <c r="B628" s="74"/>
       <c r="C628" s="34"/>
       <c r="D628" s="34"/>
       <c r="E628" s="34"/>
@@ -44796,8 +44863,8 @@
       </c>
     </row>
     <row r="629">
-      <c r="A629" s="75"/>
-      <c r="B629" s="76"/>
+      <c r="A629" s="73"/>
+      <c r="B629" s="74"/>
       <c r="C629" s="34"/>
       <c r="D629" s="34"/>
       <c r="E629" s="34"/>
@@ -44822,8 +44889,8 @@
       </c>
     </row>
     <row r="630">
-      <c r="A630" s="75"/>
-      <c r="B630" s="76"/>
+      <c r="A630" s="73"/>
+      <c r="B630" s="74"/>
       <c r="C630" s="34"/>
       <c r="D630" s="34"/>
       <c r="E630" s="34"/>
@@ -44848,8 +44915,8 @@
       </c>
     </row>
     <row r="631">
-      <c r="A631" s="75"/>
-      <c r="B631" s="76"/>
+      <c r="A631" s="73"/>
+      <c r="B631" s="74"/>
       <c r="C631" s="34"/>
       <c r="D631" s="34"/>
       <c r="E631" s="34"/>
@@ -44874,8 +44941,8 @@
       </c>
     </row>
     <row r="632">
-      <c r="A632" s="75"/>
-      <c r="B632" s="76"/>
+      <c r="A632" s="73"/>
+      <c r="B632" s="74"/>
       <c r="C632" s="34"/>
       <c r="D632" s="34"/>
       <c r="E632" s="34"/>
@@ -44900,8 +44967,8 @@
       </c>
     </row>
     <row r="633">
-      <c r="A633" s="75"/>
-      <c r="B633" s="76"/>
+      <c r="A633" s="73"/>
+      <c r="B633" s="74"/>
       <c r="C633" s="34"/>
       <c r="D633" s="34"/>
       <c r="E633" s="34"/>
@@ -44926,8 +44993,8 @@
       </c>
     </row>
     <row r="634">
-      <c r="A634" s="75"/>
-      <c r="B634" s="76"/>
+      <c r="A634" s="73"/>
+      <c r="B634" s="74"/>
       <c r="C634" s="34"/>
       <c r="D634" s="34"/>
       <c r="E634" s="34"/>
@@ -44952,8 +45019,8 @@
       </c>
     </row>
     <row r="635">
-      <c r="A635" s="75"/>
-      <c r="B635" s="76"/>
+      <c r="A635" s="73"/>
+      <c r="B635" s="74"/>
       <c r="C635" s="34"/>
       <c r="D635" s="34"/>
       <c r="E635" s="34"/>
@@ -44978,8 +45045,8 @@
       </c>
     </row>
     <row r="636">
-      <c r="A636" s="75"/>
-      <c r="B636" s="76"/>
+      <c r="A636" s="73"/>
+      <c r="B636" s="74"/>
       <c r="C636" s="34"/>
       <c r="D636" s="34"/>
       <c r="E636" s="34"/>
@@ -45004,8 +45071,8 @@
       </c>
     </row>
     <row r="637">
-      <c r="A637" s="75"/>
-      <c r="B637" s="76"/>
+      <c r="A637" s="73"/>
+      <c r="B637" s="74"/>
       <c r="C637" s="34"/>
       <c r="D637" s="34"/>
       <c r="E637" s="34"/>
@@ -45030,8 +45097,8 @@
       </c>
     </row>
     <row r="638">
-      <c r="A638" s="75"/>
-      <c r="B638" s="76"/>
+      <c r="A638" s="73"/>
+      <c r="B638" s="74"/>
       <c r="C638" s="34"/>
       <c r="D638" s="34"/>
       <c r="E638" s="34"/>
@@ -45056,8 +45123,8 @@
       </c>
     </row>
     <row r="639">
-      <c r="A639" s="75"/>
-      <c r="B639" s="76"/>
+      <c r="A639" s="73"/>
+      <c r="B639" s="74"/>
       <c r="C639" s="34"/>
       <c r="D639" s="34"/>
       <c r="E639" s="34"/>
@@ -45082,8 +45149,8 @@
       </c>
     </row>
     <row r="640">
-      <c r="A640" s="75"/>
-      <c r="B640" s="76"/>
+      <c r="A640" s="73"/>
+      <c r="B640" s="74"/>
       <c r="C640" s="34"/>
       <c r="D640" s="34"/>
       <c r="E640" s="34"/>
@@ -45108,8 +45175,8 @@
       </c>
     </row>
     <row r="641">
-      <c r="A641" s="75"/>
-      <c r="B641" s="76"/>
+      <c r="A641" s="73"/>
+      <c r="B641" s="74"/>
       <c r="C641" s="34"/>
       <c r="D641" s="34"/>
       <c r="E641" s="34"/>
@@ -45134,8 +45201,8 @@
       </c>
     </row>
     <row r="642">
-      <c r="A642" s="75"/>
-      <c r="B642" s="76"/>
+      <c r="A642" s="73"/>
+      <c r="B642" s="74"/>
       <c r="C642" s="34"/>
       <c r="D642" s="34"/>
       <c r="E642" s="34"/>
@@ -45160,8 +45227,8 @@
       </c>
     </row>
     <row r="643">
-      <c r="A643" s="75"/>
-      <c r="B643" s="76"/>
+      <c r="A643" s="73"/>
+      <c r="B643" s="74"/>
       <c r="C643" s="34"/>
       <c r="D643" s="34"/>
       <c r="E643" s="34"/>
@@ -45186,8 +45253,8 @@
       </c>
     </row>
     <row r="644">
-      <c r="A644" s="75"/>
-      <c r="B644" s="76"/>
+      <c r="A644" s="73"/>
+      <c r="B644" s="74"/>
       <c r="C644" s="34"/>
       <c r="D644" s="34"/>
       <c r="E644" s="34"/>
@@ -45212,8 +45279,8 @@
       </c>
     </row>
     <row r="645">
-      <c r="A645" s="75"/>
-      <c r="B645" s="76"/>
+      <c r="A645" s="73"/>
+      <c r="B645" s="74"/>
       <c r="C645" s="34"/>
       <c r="D645" s="34"/>
       <c r="E645" s="34"/>
@@ -45238,8 +45305,8 @@
       </c>
     </row>
     <row r="646">
-      <c r="A646" s="75"/>
-      <c r="B646" s="76"/>
+      <c r="A646" s="73"/>
+      <c r="B646" s="74"/>
       <c r="C646" s="34"/>
       <c r="D646" s="34"/>
       <c r="E646" s="34"/>
@@ -45264,8 +45331,8 @@
       </c>
     </row>
     <row r="647">
-      <c r="A647" s="75"/>
-      <c r="B647" s="76"/>
+      <c r="A647" s="73"/>
+      <c r="B647" s="74"/>
       <c r="C647" s="34"/>
       <c r="D647" s="34"/>
       <c r="E647" s="34"/>
@@ -45290,8 +45357,8 @@
       </c>
     </row>
     <row r="648">
-      <c r="A648" s="75"/>
-      <c r="B648" s="76"/>
+      <c r="A648" s="73"/>
+      <c r="B648" s="74"/>
       <c r="C648" s="34"/>
       <c r="D648" s="34"/>
       <c r="E648" s="34"/>
@@ -45316,8 +45383,8 @@
       </c>
     </row>
     <row r="649">
-      <c r="A649" s="75"/>
-      <c r="B649" s="76"/>
+      <c r="A649" s="73"/>
+      <c r="B649" s="74"/>
       <c r="C649" s="34"/>
       <c r="D649" s="34"/>
       <c r="E649" s="34"/>
@@ -45342,8 +45409,8 @@
       </c>
     </row>
     <row r="650">
-      <c r="A650" s="75"/>
-      <c r="B650" s="76"/>
+      <c r="A650" s="73"/>
+      <c r="B650" s="74"/>
       <c r="C650" s="34"/>
       <c r="D650" s="34"/>
       <c r="E650" s="34"/>
@@ -45368,8 +45435,8 @@
       </c>
     </row>
     <row r="651">
-      <c r="A651" s="75"/>
-      <c r="B651" s="76"/>
+      <c r="A651" s="73"/>
+      <c r="B651" s="74"/>
       <c r="C651" s="34"/>
       <c r="D651" s="34"/>
       <c r="E651" s="34"/>
@@ -45394,8 +45461,8 @@
       </c>
     </row>
     <row r="652">
-      <c r="A652" s="75"/>
-      <c r="B652" s="76"/>
+      <c r="A652" s="73"/>
+      <c r="B652" s="74"/>
       <c r="C652" s="34"/>
       <c r="D652" s="34"/>
       <c r="E652" s="34"/>
@@ -45420,8 +45487,8 @@
       </c>
     </row>
     <row r="653">
-      <c r="A653" s="75"/>
-      <c r="B653" s="76"/>
+      <c r="A653" s="73"/>
+      <c r="B653" s="74"/>
       <c r="C653" s="34"/>
       <c r="D653" s="34"/>
       <c r="E653" s="34"/>
@@ -45446,8 +45513,8 @@
       </c>
     </row>
     <row r="654">
-      <c r="A654" s="75"/>
-      <c r="B654" s="76"/>
+      <c r="A654" s="73"/>
+      <c r="B654" s="74"/>
       <c r="C654" s="34"/>
       <c r="D654" s="34"/>
       <c r="E654" s="34"/>
@@ -45472,8 +45539,8 @@
       </c>
     </row>
     <row r="655">
-      <c r="A655" s="75"/>
-      <c r="B655" s="76"/>
+      <c r="A655" s="73"/>
+      <c r="B655" s="74"/>
       <c r="C655" s="34"/>
       <c r="D655" s="34"/>
       <c r="E655" s="34"/>
@@ -45498,8 +45565,8 @@
       </c>
     </row>
     <row r="656">
-      <c r="A656" s="75"/>
-      <c r="B656" s="76"/>
+      <c r="A656" s="73"/>
+      <c r="B656" s="74"/>
       <c r="C656" s="34"/>
       <c r="D656" s="34"/>
       <c r="E656" s="34"/>
@@ -45524,8 +45591,8 @@
       </c>
     </row>
     <row r="657">
-      <c r="A657" s="75"/>
-      <c r="B657" s="76"/>
+      <c r="A657" s="73"/>
+      <c r="B657" s="74"/>
       <c r="C657" s="34"/>
       <c r="D657" s="34"/>
       <c r="E657" s="34"/>
@@ -45550,8 +45617,8 @@
       </c>
     </row>
     <row r="658">
-      <c r="A658" s="75"/>
-      <c r="B658" s="76"/>
+      <c r="A658" s="73"/>
+      <c r="B658" s="74"/>
       <c r="C658" s="34"/>
       <c r="D658" s="34"/>
       <c r="E658" s="34"/>
@@ -45576,8 +45643,8 @@
       </c>
     </row>
     <row r="659">
-      <c r="A659" s="75"/>
-      <c r="B659" s="76"/>
+      <c r="A659" s="73"/>
+      <c r="B659" s="74"/>
       <c r="C659" s="34"/>
       <c r="D659" s="34"/>
       <c r="E659" s="34"/>
@@ -45602,8 +45669,8 @@
       </c>
     </row>
     <row r="660">
-      <c r="A660" s="75"/>
-      <c r="B660" s="76"/>
+      <c r="A660" s="73"/>
+      <c r="B660" s="74"/>
       <c r="C660" s="34"/>
       <c r="D660" s="34"/>
       <c r="E660" s="34"/>
@@ -45628,8 +45695,8 @@
       </c>
     </row>
     <row r="661">
-      <c r="A661" s="75"/>
-      <c r="B661" s="76"/>
+      <c r="A661" s="73"/>
+      <c r="B661" s="74"/>
       <c r="C661" s="34"/>
       <c r="D661" s="34"/>
       <c r="E661" s="34"/>
@@ -45654,8 +45721,8 @@
       </c>
     </row>
     <row r="662">
-      <c r="A662" s="75"/>
-      <c r="B662" s="76"/>
+      <c r="A662" s="73"/>
+      <c r="B662" s="74"/>
       <c r="C662" s="34"/>
       <c r="D662" s="34"/>
       <c r="E662" s="34"/>
@@ -45680,8 +45747,8 @@
       </c>
     </row>
     <row r="663">
-      <c r="A663" s="75"/>
-      <c r="B663" s="76"/>
+      <c r="A663" s="73"/>
+      <c r="B663" s="74"/>
       <c r="C663" s="34"/>
       <c r="D663" s="34"/>
       <c r="E663" s="34"/>
@@ -45706,8 +45773,8 @@
       </c>
     </row>
     <row r="664">
-      <c r="A664" s="75"/>
-      <c r="B664" s="76"/>
+      <c r="A664" s="73"/>
+      <c r="B664" s="74"/>
       <c r="C664" s="34"/>
       <c r="D664" s="34"/>
       <c r="E664" s="34"/>
@@ -45732,8 +45799,8 @@
       </c>
     </row>
     <row r="665">
-      <c r="A665" s="75"/>
-      <c r="B665" s="76"/>
+      <c r="A665" s="73"/>
+      <c r="B665" s="74"/>
       <c r="C665" s="34"/>
       <c r="D665" s="34"/>
       <c r="E665" s="34"/>
@@ -45758,8 +45825,8 @@
       </c>
     </row>
     <row r="666">
-      <c r="A666" s="75"/>
-      <c r="B666" s="76"/>
+      <c r="A666" s="73"/>
+      <c r="B666" s="74"/>
       <c r="C666" s="34"/>
       <c r="D666" s="34"/>
       <c r="E666" s="34"/>
@@ -45784,8 +45851,8 @@
       </c>
     </row>
     <row r="667">
-      <c r="A667" s="75"/>
-      <c r="B667" s="76"/>
+      <c r="A667" s="73"/>
+      <c r="B667" s="74"/>
       <c r="C667" s="34"/>
       <c r="D667" s="34"/>
       <c r="E667" s="34"/>
@@ -45810,8 +45877,8 @@
       </c>
     </row>
     <row r="668">
-      <c r="A668" s="75"/>
-      <c r="B668" s="76"/>
+      <c r="A668" s="73"/>
+      <c r="B668" s="74"/>
       <c r="C668" s="34"/>
       <c r="D668" s="34"/>
       <c r="E668" s="34"/>
@@ -45836,8 +45903,8 @@
       </c>
     </row>
     <row r="669">
-      <c r="A669" s="75"/>
-      <c r="B669" s="76"/>
+      <c r="A669" s="73"/>
+      <c r="B669" s="74"/>
       <c r="C669" s="34"/>
       <c r="D669" s="34"/>
       <c r="E669" s="34"/>
@@ -45862,8 +45929,8 @@
       </c>
     </row>
     <row r="670">
-      <c r="A670" s="75"/>
-      <c r="B670" s="76"/>
+      <c r="A670" s="73"/>
+      <c r="B670" s="74"/>
       <c r="C670" s="34"/>
       <c r="D670" s="34"/>
       <c r="E670" s="34"/>
@@ -45888,8 +45955,8 @@
       </c>
     </row>
     <row r="671">
-      <c r="A671" s="75"/>
-      <c r="B671" s="76"/>
+      <c r="A671" s="73"/>
+      <c r="B671" s="74"/>
       <c r="C671" s="34"/>
       <c r="D671" s="34"/>
       <c r="E671" s="34"/>
@@ -45914,8 +45981,8 @@
       </c>
     </row>
     <row r="672">
-      <c r="A672" s="75"/>
-      <c r="B672" s="76"/>
+      <c r="A672" s="73"/>
+      <c r="B672" s="74"/>
       <c r="C672" s="34"/>
       <c r="D672" s="34"/>
       <c r="E672" s="34"/>
@@ -45940,8 +46007,8 @@
       </c>
     </row>
     <row r="673">
-      <c r="A673" s="75"/>
-      <c r="B673" s="76"/>
+      <c r="A673" s="73"/>
+      <c r="B673" s="74"/>
       <c r="C673" s="34"/>
       <c r="D673" s="34"/>
       <c r="E673" s="34"/>
@@ -45966,8 +46033,8 @@
       </c>
     </row>
     <row r="674">
-      <c r="A674" s="75"/>
-      <c r="B674" s="76"/>
+      <c r="A674" s="73"/>
+      <c r="B674" s="74"/>
       <c r="C674" s="34"/>
       <c r="D674" s="34"/>
       <c r="E674" s="34"/>
@@ -45992,8 +46059,8 @@
       </c>
     </row>
     <row r="675">
-      <c r="A675" s="75"/>
-      <c r="B675" s="76"/>
+      <c r="A675" s="73"/>
+      <c r="B675" s="74"/>
       <c r="C675" s="34"/>
       <c r="D675" s="34"/>
       <c r="E675" s="34"/>
@@ -46018,8 +46085,8 @@
       </c>
     </row>
     <row r="676">
-      <c r="A676" s="75"/>
-      <c r="B676" s="76"/>
+      <c r="A676" s="73"/>
+      <c r="B676" s="74"/>
       <c r="C676" s="34"/>
       <c r="D676" s="34"/>
       <c r="E676" s="34"/>
@@ -46044,8 +46111,8 @@
       </c>
     </row>
     <row r="677">
-      <c r="A677" s="75"/>
-      <c r="B677" s="76"/>
+      <c r="A677" s="73"/>
+      <c r="B677" s="74"/>
       <c r="C677" s="34"/>
       <c r="D677" s="34"/>
       <c r="E677" s="34"/>
@@ -46070,8 +46137,8 @@
       </c>
     </row>
     <row r="678">
-      <c r="A678" s="75"/>
-      <c r="B678" s="76"/>
+      <c r="A678" s="73"/>
+      <c r="B678" s="74"/>
       <c r="C678" s="34"/>
       <c r="D678" s="34"/>
       <c r="E678" s="34"/>
@@ -46096,8 +46163,8 @@
       </c>
     </row>
     <row r="679">
-      <c r="A679" s="75"/>
-      <c r="B679" s="76"/>
+      <c r="A679" s="73"/>
+      <c r="B679" s="74"/>
       <c r="C679" s="34"/>
       <c r="D679" s="34"/>
       <c r="E679" s="34"/>
@@ -46122,8 +46189,8 @@
       </c>
     </row>
     <row r="680">
-      <c r="A680" s="75"/>
-      <c r="B680" s="76"/>
+      <c r="A680" s="73"/>
+      <c r="B680" s="74"/>
       <c r="C680" s="34"/>
       <c r="D680" s="34"/>
       <c r="E680" s="34"/>
@@ -46148,8 +46215,8 @@
       </c>
     </row>
     <row r="681">
-      <c r="A681" s="75"/>
-      <c r="B681" s="76"/>
+      <c r="A681" s="73"/>
+      <c r="B681" s="74"/>
       <c r="C681" s="34"/>
       <c r="D681" s="34"/>
       <c r="E681" s="34"/>
@@ -46174,8 +46241,8 @@
       </c>
     </row>
     <row r="682">
-      <c r="A682" s="75"/>
-      <c r="B682" s="76"/>
+      <c r="A682" s="73"/>
+      <c r="B682" s="74"/>
       <c r="C682" s="34"/>
       <c r="D682" s="34"/>
       <c r="E682" s="34"/>
@@ -46200,8 +46267,8 @@
       </c>
     </row>
     <row r="683">
-      <c r="A683" s="75"/>
-      <c r="B683" s="76"/>
+      <c r="A683" s="73"/>
+      <c r="B683" s="74"/>
       <c r="C683" s="34"/>
       <c r="D683" s="34"/>
       <c r="E683" s="34"/>
@@ -46226,8 +46293,8 @@
       </c>
     </row>
     <row r="684">
-      <c r="A684" s="75"/>
-      <c r="B684" s="76"/>
+      <c r="A684" s="73"/>
+      <c r="B684" s="74"/>
       <c r="C684" s="34"/>
       <c r="D684" s="34"/>
       <c r="E684" s="34"/>
@@ -46252,8 +46319,8 @@
       </c>
     </row>
     <row r="685">
-      <c r="A685" s="75"/>
-      <c r="B685" s="76"/>
+      <c r="A685" s="73"/>
+      <c r="B685" s="74"/>
       <c r="C685" s="34"/>
       <c r="D685" s="34"/>
       <c r="E685" s="34"/>
@@ -46278,8 +46345,8 @@
       </c>
     </row>
     <row r="686">
-      <c r="A686" s="75"/>
-      <c r="B686" s="76"/>
+      <c r="A686" s="73"/>
+      <c r="B686" s="74"/>
       <c r="C686" s="34"/>
       <c r="D686" s="34"/>
       <c r="E686" s="34"/>
@@ -46304,8 +46371,8 @@
       </c>
     </row>
     <row r="687">
-      <c r="A687" s="75"/>
-      <c r="B687" s="76"/>
+      <c r="A687" s="73"/>
+      <c r="B687" s="74"/>
       <c r="C687" s="34"/>
       <c r="D687" s="34"/>
       <c r="E687" s="34"/>
@@ -46330,8 +46397,8 @@
       </c>
     </row>
     <row r="688">
-      <c r="A688" s="75"/>
-      <c r="B688" s="76"/>
+      <c r="A688" s="73"/>
+      <c r="B688" s="74"/>
       <c r="C688" s="34"/>
       <c r="D688" s="34"/>
       <c r="E688" s="34"/>
@@ -46356,8 +46423,8 @@
       </c>
     </row>
     <row r="689">
-      <c r="A689" s="75"/>
-      <c r="B689" s="76"/>
+      <c r="A689" s="73"/>
+      <c r="B689" s="74"/>
       <c r="C689" s="34"/>
       <c r="D689" s="34"/>
       <c r="E689" s="34"/>
@@ -46382,8 +46449,8 @@
       </c>
     </row>
     <row r="690">
-      <c r="A690" s="75"/>
-      <c r="B690" s="76"/>
+      <c r="A690" s="73"/>
+      <c r="B690" s="74"/>
       <c r="C690" s="34"/>
       <c r="D690" s="34"/>
       <c r="E690" s="34"/>
@@ -46408,8 +46475,8 @@
       </c>
     </row>
     <row r="691">
-      <c r="A691" s="75"/>
-      <c r="B691" s="76"/>
+      <c r="A691" s="73"/>
+      <c r="B691" s="74"/>
       <c r="C691" s="34"/>
       <c r="D691" s="34"/>
       <c r="E691" s="34"/>
@@ -46434,8 +46501,8 @@
       </c>
     </row>
     <row r="692">
-      <c r="A692" s="75"/>
-      <c r="B692" s="76"/>
+      <c r="A692" s="73"/>
+      <c r="B692" s="74"/>
       <c r="C692" s="34"/>
       <c r="D692" s="34"/>
       <c r="E692" s="34"/>
@@ -46460,8 +46527,8 @@
       </c>
     </row>
     <row r="693">
-      <c r="A693" s="75"/>
-      <c r="B693" s="76"/>
+      <c r="A693" s="73"/>
+      <c r="B693" s="74"/>
       <c r="C693" s="34"/>
       <c r="D693" s="34"/>
       <c r="E693" s="34"/>
@@ -46486,8 +46553,8 @@
       </c>
     </row>
     <row r="694">
-      <c r="A694" s="75"/>
-      <c r="B694" s="76"/>
+      <c r="A694" s="73"/>
+      <c r="B694" s="74"/>
       <c r="C694" s="34"/>
       <c r="D694" s="34"/>
       <c r="E694" s="34"/>
@@ -46512,8 +46579,8 @@
       </c>
     </row>
     <row r="695">
-      <c r="A695" s="75"/>
-      <c r="B695" s="76"/>
+      <c r="A695" s="73"/>
+      <c r="B695" s="74"/>
       <c r="C695" s="34"/>
       <c r="D695" s="34"/>
       <c r="E695" s="34"/>
@@ -46538,8 +46605,8 @@
       </c>
     </row>
     <row r="696">
-      <c r="A696" s="75"/>
-      <c r="B696" s="76"/>
+      <c r="A696" s="73"/>
+      <c r="B696" s="74"/>
       <c r="C696" s="34"/>
       <c r="D696" s="34"/>
       <c r="E696" s="34"/>
@@ -46564,8 +46631,8 @@
       </c>
     </row>
     <row r="697">
-      <c r="A697" s="75"/>
-      <c r="B697" s="76"/>
+      <c r="A697" s="73"/>
+      <c r="B697" s="74"/>
       <c r="C697" s="34"/>
       <c r="D697" s="34"/>
       <c r="E697" s="34"/>
@@ -46590,8 +46657,8 @@
       </c>
     </row>
     <row r="698">
-      <c r="A698" s="75"/>
-      <c r="B698" s="76"/>
+      <c r="A698" s="73"/>
+      <c r="B698" s="74"/>
       <c r="C698" s="34"/>
       <c r="D698" s="34"/>
       <c r="E698" s="34"/>
@@ -46616,8 +46683,8 @@
       </c>
     </row>
     <row r="699">
-      <c r="A699" s="75"/>
-      <c r="B699" s="76"/>
+      <c r="A699" s="73"/>
+      <c r="B699" s="74"/>
       <c r="C699" s="34"/>
       <c r="D699" s="34"/>
       <c r="E699" s="34"/>
@@ -46642,8 +46709,8 @@
       </c>
     </row>
     <row r="700">
-      <c r="A700" s="75"/>
-      <c r="B700" s="76"/>
+      <c r="A700" s="73"/>
+      <c r="B700" s="74"/>
       <c r="C700" s="34"/>
       <c r="D700" s="34"/>
       <c r="E700" s="34"/>
@@ -46668,8 +46735,8 @@
       </c>
     </row>
     <row r="701">
-      <c r="A701" s="75"/>
-      <c r="B701" s="76"/>
+      <c r="A701" s="73"/>
+      <c r="B701" s="74"/>
       <c r="C701" s="34"/>
       <c r="D701" s="34"/>
       <c r="E701" s="34"/>
@@ -47238,15 +47305,17 @@
     <hyperlink r:id="rId162" ref="S600"/>
     <hyperlink r:id="rId163" ref="S601"/>
     <hyperlink r:id="rId164" ref="S602"/>
+    <hyperlink r:id="rId165" ref="S603"/>
+    <hyperlink r:id="rId166" ref="S604"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId165"/>
-  <legacyDrawing r:id="rId166"/>
+  <drawing r:id="rId167"/>
+  <legacyDrawing r:id="rId168"/>
   <tableParts count="2">
-    <tablePart r:id="rId169"/>
-    <tablePart r:id="rId170"/>
+    <tablePart r:id="rId171"/>
+    <tablePart r:id="rId172"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201117
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -571,7 +571,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6767" uniqueCount="2247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6780" uniqueCount="2251">
   <si>
     <t>案例</t>
   </si>
@@ -8202,6 +8202,19 @@
   <si>
     <t>因工作長期居住美國
 入境時個案主動告知搭機時自覺出現嗅味覺異常情形，但下機後即恢復</t>
+  </si>
+  <si>
+    <t>#604</t>
+  </si>
+  <si>
+    <t>-11/1 印尼→台灣</t>
+  </si>
+  <si>
+    <t>11/14 採檢
+11/16 確診</t>
+  </si>
+  <si>
+    <t>國內新增1例境外移入COVID-19病例，為來臺工作之印尼籍女性</t>
   </si>
 </sst>
 </file>
@@ -44239,29 +44252,59 @@
       </c>
     </row>
     <row r="605">
-      <c r="A605" s="73"/>
-      <c r="B605" s="74"/>
-      <c r="C605" s="34"/>
-      <c r="D605" s="34"/>
-      <c r="E605" s="34"/>
+      <c r="A605" s="16" t="s">
+        <v>2247</v>
+      </c>
+      <c r="B605" s="6">
+        <v>44151.0</v>
+      </c>
+      <c r="C605" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D605" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E605" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F605" s="34"/>
-      <c r="G605" s="34"/>
-      <c r="H605" s="21"/>
-      <c r="I605" s="19"/>
-      <c r="J605" s="10"/>
-      <c r="K605" s="22"/>
-      <c r="L605" s="23"/>
-      <c r="M605" s="22"/>
+      <c r="G605" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H605" s="8" t="s">
+        <v>2248</v>
+      </c>
+      <c r="I605" s="9">
+        <v>44136.0</v>
+      </c>
+      <c r="J605" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K605" s="13" t="s">
+        <v>2249</v>
+      </c>
+      <c r="L605" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M605" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N605" s="25"/>
-      <c r="O605" s="21"/>
-      <c r="P605" s="21"/>
+      <c r="O605" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P605" s="8" t="s">
+        <v>2182</v>
+      </c>
       <c r="Q605" s="19"/>
       <c r="R605" s="19"/>
-      <c r="S605" s="20"/>
+      <c r="S605" s="61" t="s">
+        <v>2250</v>
+      </c>
       <c r="T605" s="20"/>
       <c r="U605" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#604</v>
       </c>
     </row>
     <row r="606">
@@ -47307,15 +47350,16 @@
     <hyperlink r:id="rId164" ref="S602"/>
     <hyperlink r:id="rId165" ref="S603"/>
     <hyperlink r:id="rId166" ref="S604"/>
+    <hyperlink r:id="rId167" ref="S605"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId167"/>
-  <legacyDrawing r:id="rId168"/>
+  <drawing r:id="rId168"/>
+  <legacyDrawing r:id="rId169"/>
   <tableParts count="2">
-    <tablePart r:id="rId171"/>
     <tablePart r:id="rId172"/>
+    <tablePart r:id="rId173"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201118
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -571,7 +571,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6780" uniqueCount="2251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6804" uniqueCount="2262">
   <si>
     <t>案例</t>
   </si>
@@ -8215,6 +8215,41 @@
   </si>
   <si>
     <t>國內新增1例境外移入COVID-19病例，為來臺工作之印尼籍女性</t>
+  </si>
+  <si>
+    <t>#605</t>
+  </si>
+  <si>
+    <t>3月-11/8 緬甸</t>
+  </si>
+  <si>
+    <t>9月下旬</t>
+  </si>
+  <si>
+    <t>11/13 採檢
+11/17 確診</t>
+  </si>
+  <si>
+    <t>嗜睡 發燒 嗅覺喪失 味覺喪失 喉嚨癢 輕微咳嗽</t>
+  </si>
+  <si>
+    <t>今(2020)年3月至緬甸工作，9月6日起陸續出現嗜睡、發燒、嗅味覺喪失等症狀，於當地就醫確診武漢肺炎，隔離期間未再採檢，因症狀緩解於9月下旬解除隔離。個案11月8日返國入境時，因主動告知曾於緬甸確診，且曾在當地接觸我國案501及案505，故由機場檢疫人員安排採檢，同日個案於檢疫所等待檢驗結果時，出現喉嚨癢及輕微咳嗽症狀，後續因機場採檢結果為陰性，轉至防疫旅館居家檢疫；個案11月13日咳嗽症狀加劇，主動回報衛生單位安排就醫採檢</t>
+  </si>
+  <si>
+    <t>我國新增2例境外移入COVID-19病例，分自緬甸、印尼入境</t>
+  </si>
+  <si>
+    <t>#606</t>
+  </si>
+  <si>
+    <t>9月-11/15 印尼</t>
+  </si>
+  <si>
+    <t>11/15 採檢
+11/17 確診</t>
+  </si>
+  <si>
+    <t>咳嗽 味覺異常 呼吸不順 發燒 腹瀉 肌肉痠痛</t>
   </si>
 </sst>
 </file>
@@ -44308,55 +44343,113 @@
       </c>
     </row>
     <row r="606">
-      <c r="A606" s="73"/>
-      <c r="B606" s="74"/>
-      <c r="C606" s="34"/>
-      <c r="D606" s="34"/>
-      <c r="E606" s="34"/>
+      <c r="A606" s="16" t="s">
+        <v>2251</v>
+      </c>
+      <c r="B606" s="6">
+        <v>44152.0</v>
+      </c>
+      <c r="C606" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D606" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E606" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F606" s="34"/>
-      <c r="G606" s="34"/>
-      <c r="H606" s="21"/>
-      <c r="I606" s="19"/>
-      <c r="J606" s="10"/>
-      <c r="K606" s="22"/>
-      <c r="L606" s="23"/>
-      <c r="M606" s="22"/>
+      <c r="G606" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H606" s="8" t="s">
+        <v>2252</v>
+      </c>
+      <c r="I606" s="9">
+        <v>44143.0</v>
+      </c>
+      <c r="J606" s="12" t="s">
+        <v>2253</v>
+      </c>
+      <c r="K606" s="13" t="s">
+        <v>2254</v>
+      </c>
+      <c r="L606" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M606" s="13" t="s">
+        <v>2255</v>
+      </c>
       <c r="N606" s="25"/>
-      <c r="O606" s="21"/>
-      <c r="P606" s="21"/>
+      <c r="O606" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P606" s="8" t="s">
+        <v>2256</v>
+      </c>
       <c r="Q606" s="19"/>
       <c r="R606" s="19"/>
-      <c r="S606" s="20"/>
+      <c r="S606" s="61" t="s">
+        <v>2257</v>
+      </c>
       <c r="T606" s="20"/>
       <c r="U606" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#605</v>
       </c>
     </row>
     <row r="607">
-      <c r="A607" s="73"/>
-      <c r="B607" s="74"/>
-      <c r="C607" s="34"/>
-      <c r="D607" s="34"/>
-      <c r="E607" s="34"/>
+      <c r="A607" s="16" t="s">
+        <v>2258</v>
+      </c>
+      <c r="B607" s="6">
+        <v>44152.0</v>
+      </c>
+      <c r="C607" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D607" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E607" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F607" s="34"/>
-      <c r="G607" s="34"/>
-      <c r="H607" s="21"/>
-      <c r="I607" s="19"/>
-      <c r="J607" s="10"/>
-      <c r="K607" s="22"/>
-      <c r="L607" s="23"/>
-      <c r="M607" s="22"/>
+      <c r="G607" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H607" s="8" t="s">
+        <v>2259</v>
+      </c>
+      <c r="I607" s="9">
+        <v>44150.0</v>
+      </c>
+      <c r="J607" s="10">
+        <v>44144.0</v>
+      </c>
+      <c r="K607" s="13" t="s">
+        <v>2260</v>
+      </c>
+      <c r="L607" s="12" t="s">
+        <v>363</v>
+      </c>
+      <c r="M607" s="13" t="s">
+        <v>2261</v>
+      </c>
       <c r="N607" s="25"/>
-      <c r="O607" s="21"/>
+      <c r="O607" s="8" t="s">
+        <v>85</v>
+      </c>
       <c r="P607" s="21"/>
       <c r="Q607" s="19"/>
       <c r="R607" s="19"/>
-      <c r="S607" s="20"/>
+      <c r="S607" s="61" t="s">
+        <v>2257</v>
+      </c>
       <c r="T607" s="20"/>
       <c r="U607" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#606</v>
       </c>
     </row>
     <row r="608">
@@ -47351,15 +47444,17 @@
     <hyperlink r:id="rId165" ref="S603"/>
     <hyperlink r:id="rId166" ref="S604"/>
     <hyperlink r:id="rId167" ref="S605"/>
+    <hyperlink r:id="rId168" ref="S606"/>
+    <hyperlink r:id="rId169" ref="S607"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId168"/>
-  <legacyDrawing r:id="rId169"/>
+  <drawing r:id="rId170"/>
+  <legacyDrawing r:id="rId171"/>
   <tableParts count="2">
-    <tablePart r:id="rId172"/>
-    <tablePart r:id="rId173"/>
+    <tablePart r:id="rId174"/>
+    <tablePart r:id="rId175"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201119
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -571,7 +571,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6804" uniqueCount="2262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6828" uniqueCount="2272">
   <si>
     <t>案例</t>
   </si>
@@ -5331,7 +5331,7 @@
     <t>軍艦</t>
   </si>
   <si>
-    <t xml:space="preserve">職業：國防大學政戰學院學生，軍艦實習生
+    <t>職業：國防大學政戰學院學生，軍艦實習生
 #396 #397 #415 #423 同艙間 12人房
 4/15 下船搭學校遊覽車到左營轉搭高鐵0136車次3車8A至烏日由家人接送返家
 4/16 清水的診所就醫
@@ -5339,8 +5339,7 @@
 首例軍艦群聚
 #396~#399,#401~#420
 政戰學院全校停課兩週，海軍官校也從20日起停課
-診所休診14天
-</t>
+診所休診14天</t>
   </si>
   <si>
     <t>#397</t>
@@ -8250,6 +8249,37 @@
   </si>
   <si>
     <t>咳嗽 味覺異常 呼吸不順 發燒 腹瀉 肌肉痠痛</t>
+  </si>
+  <si>
+    <t>#607</t>
+  </si>
+  <si>
+    <t>-11/12 印尼→台灣</t>
+  </si>
+  <si>
+    <t>11/16 採檢
+11/18 確診</t>
+  </si>
+  <si>
+    <t>喉嚨痛 全身痠痛 發燒 流鼻水</t>
+  </si>
+  <si>
+    <t>14日出現喉嚨痛及全身痠痛未通知檢疫所，16日因發燒、流鼻水及喉嚨痛經安排就醫採檢</t>
+  </si>
+  <si>
+    <t>我國新增2例境外移入COVID-19病例，分自印尼、美國入境</t>
+  </si>
+  <si>
+    <t>#608</t>
+  </si>
+  <si>
+    <t>2019/10-2020/11/11 美國</t>
+  </si>
+  <si>
+    <t>體溫偏高 肌肉痠痛 頭痛 咳嗽 流鼻水</t>
+  </si>
+  <si>
+    <t>長期居住美國</t>
   </si>
 </sst>
 </file>
@@ -44453,55 +44483,115 @@
       </c>
     </row>
     <row r="608">
-      <c r="A608" s="73"/>
-      <c r="B608" s="74"/>
-      <c r="C608" s="34"/>
-      <c r="D608" s="34"/>
-      <c r="E608" s="34"/>
+      <c r="A608" s="16" t="s">
+        <v>2262</v>
+      </c>
+      <c r="B608" s="6">
+        <v>44153.0</v>
+      </c>
+      <c r="C608" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D608" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E608" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F608" s="34"/>
-      <c r="G608" s="34"/>
-      <c r="H608" s="21"/>
-      <c r="I608" s="19"/>
-      <c r="J608" s="10"/>
-      <c r="K608" s="22"/>
-      <c r="L608" s="23"/>
-      <c r="M608" s="22"/>
+      <c r="G608" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H608" s="8" t="s">
+        <v>2263</v>
+      </c>
+      <c r="I608" s="9">
+        <v>44147.0</v>
+      </c>
+      <c r="J608" s="10">
+        <v>44149.0</v>
+      </c>
+      <c r="K608" s="13" t="s">
+        <v>2264</v>
+      </c>
+      <c r="L608" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M608" s="13" t="s">
+        <v>2265</v>
+      </c>
       <c r="N608" s="25"/>
-      <c r="O608" s="21"/>
-      <c r="P608" s="21"/>
+      <c r="O608" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P608" s="8" t="s">
+        <v>2266</v>
+      </c>
       <c r="Q608" s="19"/>
       <c r="R608" s="19"/>
-      <c r="S608" s="20"/>
+      <c r="S608" s="61" t="s">
+        <v>2267</v>
+      </c>
       <c r="T608" s="20"/>
       <c r="U608" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#607</v>
       </c>
     </row>
     <row r="609">
-      <c r="A609" s="73"/>
-      <c r="B609" s="74"/>
-      <c r="C609" s="34"/>
-      <c r="D609" s="34"/>
-      <c r="E609" s="34"/>
+      <c r="A609" s="16" t="s">
+        <v>2268</v>
+      </c>
+      <c r="B609" s="6">
+        <v>44153.0</v>
+      </c>
+      <c r="C609" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D609" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="E609" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F609" s="34"/>
-      <c r="G609" s="34"/>
-      <c r="H609" s="21"/>
-      <c r="I609" s="19"/>
-      <c r="J609" s="10"/>
-      <c r="K609" s="22"/>
-      <c r="L609" s="23"/>
-      <c r="M609" s="22"/>
+      <c r="G609" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H609" s="8" t="s">
+        <v>2269</v>
+      </c>
+      <c r="I609" s="9">
+        <v>44146.0</v>
+      </c>
+      <c r="J609" s="10">
+        <v>44147.0</v>
+      </c>
+      <c r="K609" s="13" t="s">
+        <v>2264</v>
+      </c>
+      <c r="L609" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M609" s="13" t="s">
+        <v>2270</v>
+      </c>
       <c r="N609" s="25"/>
-      <c r="O609" s="21"/>
-      <c r="P609" s="21"/>
+      <c r="O609" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P609" s="8" t="s">
+        <v>2271</v>
+      </c>
       <c r="Q609" s="19"/>
       <c r="R609" s="19"/>
-      <c r="S609" s="20"/>
+      <c r="S609" s="61" t="s">
+        <v>2267</v>
+      </c>
       <c r="T609" s="20"/>
       <c r="U609" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#608</v>
       </c>
     </row>
     <row r="610">
@@ -47446,15 +47536,17 @@
     <hyperlink r:id="rId167" ref="S605"/>
     <hyperlink r:id="rId168" ref="S606"/>
     <hyperlink r:id="rId169" ref="S607"/>
+    <hyperlink r:id="rId170" ref="S608"/>
+    <hyperlink r:id="rId171" ref="S609"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId170"/>
-  <legacyDrawing r:id="rId171"/>
+  <drawing r:id="rId172"/>
+  <legacyDrawing r:id="rId173"/>
   <tableParts count="2">
-    <tablePart r:id="rId174"/>
-    <tablePart r:id="rId175"/>
+    <tablePart r:id="rId176"/>
+    <tablePart r:id="rId177"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201120
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -571,7 +571,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6828" uniqueCount="2272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6852" uniqueCount="2284">
   <si>
     <t>案例</t>
   </si>
@@ -8280,6 +8280,45 @@
   </si>
   <si>
     <t>長期居住美國</t>
+  </si>
+  <si>
+    <t>#609</t>
+  </si>
+  <si>
+    <t>土耳其</t>
+  </si>
+  <si>
+    <t>-11/10 土耳其→台灣</t>
+  </si>
+  <si>
+    <t>11/16 採檢
+11/19 確診</t>
+  </si>
+  <si>
+    <t>肌肉痠痛 發燒</t>
+  </si>
+  <si>
+    <t>航空公司空服員
+原定11月13日搭機返回土耳其，但於11月12日出現肌肉痠痛及發燒症狀，隔日航空公司聯繫我國醫療單位至旅館協助診療，並由該醫療單位通知疾管署；個案11月16日依作業流程安排採檢通報</t>
+  </si>
+  <si>
+    <t>新增2例境外移入COVID-19病例，分自土耳其及印尼來臺</t>
+  </si>
+  <si>
+    <t>#610</t>
+  </si>
+  <si>
+    <t>-11/17 印尼→台灣</t>
+  </si>
+  <si>
+    <t>11/17 採檢
+11/19 確診</t>
+  </si>
+  <si>
+    <t>倦怠 全身痠痛 肚子不適</t>
+  </si>
+  <si>
+    <t>來臺工作，入境時因體溫異常於檢疫站攔檢</t>
   </si>
 </sst>
 </file>
@@ -44595,55 +44634,113 @@
       </c>
     </row>
     <row r="610">
-      <c r="A610" s="73"/>
-      <c r="B610" s="74"/>
-      <c r="C610" s="34"/>
-      <c r="D610" s="34"/>
-      <c r="E610" s="34"/>
+      <c r="A610" s="16" t="s">
+        <v>2272</v>
+      </c>
+      <c r="B610" s="6">
+        <v>44154.0</v>
+      </c>
+      <c r="C610" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D610" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E610" s="7" t="s">
+        <v>2273</v>
+      </c>
       <c r="F610" s="34"/>
-      <c r="G610" s="34"/>
-      <c r="H610" s="21"/>
-      <c r="I610" s="19"/>
-      <c r="J610" s="10"/>
-      <c r="K610" s="22"/>
-      <c r="L610" s="23"/>
-      <c r="M610" s="22"/>
+      <c r="G610" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H610" s="8" t="s">
+        <v>2274</v>
+      </c>
+      <c r="I610" s="9">
+        <v>44145.0</v>
+      </c>
+      <c r="J610" s="10">
+        <v>44147.0</v>
+      </c>
+      <c r="K610" s="13" t="s">
+        <v>2275</v>
+      </c>
+      <c r="L610" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M610" s="13" t="s">
+        <v>2276</v>
+      </c>
       <c r="N610" s="25"/>
-      <c r="O610" s="21"/>
-      <c r="P610" s="21"/>
+      <c r="O610" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P610" s="8" t="s">
+        <v>2277</v>
+      </c>
       <c r="Q610" s="19"/>
       <c r="R610" s="19"/>
-      <c r="S610" s="20"/>
+      <c r="S610" s="61" t="s">
+        <v>2278</v>
+      </c>
       <c r="T610" s="20"/>
       <c r="U610" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#609</v>
       </c>
     </row>
     <row r="611">
-      <c r="A611" s="73"/>
-      <c r="B611" s="74"/>
-      <c r="C611" s="34"/>
-      <c r="D611" s="34"/>
-      <c r="E611" s="34"/>
+      <c r="A611" s="16" t="s">
+        <v>2279</v>
+      </c>
+      <c r="B611" s="6">
+        <v>44154.0</v>
+      </c>
+      <c r="C611" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D611" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E611" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F611" s="34"/>
-      <c r="G611" s="34"/>
-      <c r="H611" s="21"/>
-      <c r="I611" s="19"/>
+      <c r="G611" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H611" s="8" t="s">
+        <v>2280</v>
+      </c>
+      <c r="I611" s="9">
+        <v>44152.0</v>
+      </c>
       <c r="J611" s="10"/>
-      <c r="K611" s="22"/>
-      <c r="L611" s="23"/>
-      <c r="M611" s="22"/>
+      <c r="K611" s="13" t="s">
+        <v>2281</v>
+      </c>
+      <c r="L611" s="12" t="s">
+        <v>363</v>
+      </c>
+      <c r="M611" s="13" t="s">
+        <v>2282</v>
+      </c>
       <c r="N611" s="25"/>
-      <c r="O611" s="21"/>
-      <c r="P611" s="21"/>
+      <c r="O611" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P611" s="8" t="s">
+        <v>2283</v>
+      </c>
       <c r="Q611" s="19"/>
       <c r="R611" s="19"/>
-      <c r="S611" s="20"/>
+      <c r="S611" s="61" t="s">
+        <v>2278</v>
+      </c>
       <c r="T611" s="20"/>
       <c r="U611" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#610</v>
       </c>
     </row>
     <row r="612">
@@ -47538,15 +47635,17 @@
     <hyperlink r:id="rId169" ref="S607"/>
     <hyperlink r:id="rId170" ref="S608"/>
     <hyperlink r:id="rId171" ref="S609"/>
+    <hyperlink r:id="rId172" ref="S610"/>
+    <hyperlink r:id="rId173" ref="S611"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId172"/>
-  <legacyDrawing r:id="rId173"/>
+  <drawing r:id="rId174"/>
+  <legacyDrawing r:id="rId175"/>
   <tableParts count="2">
-    <tablePart r:id="rId176"/>
-    <tablePart r:id="rId177"/>
+    <tablePart r:id="rId178"/>
+    <tablePart r:id="rId179"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201121
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -571,7 +571,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6852" uniqueCount="2284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6878" uniqueCount="2289">
   <si>
     <t>案例</t>
   </si>
@@ -8319,6 +8319,22 @@
   </si>
   <si>
     <t>來臺工作，入境時因體溫異常於檢疫站攔檢</t>
+  </si>
+  <si>
+    <t>#611</t>
+  </si>
+  <si>
+    <t>-11/5 印尼→台灣</t>
+  </si>
+  <si>
+    <t>11/18 採檢
+11/20 確診</t>
+  </si>
+  <si>
+    <t>新增2例境外移入COVID-19病例，均為無症狀印尼籍移工</t>
+  </si>
+  <si>
+    <t>#612</t>
   </si>
 </sst>
 </file>
@@ -44744,55 +44760,115 @@
       </c>
     </row>
     <row r="612">
-      <c r="A612" s="73"/>
-      <c r="B612" s="74"/>
-      <c r="C612" s="34"/>
-      <c r="D612" s="34"/>
-      <c r="E612" s="34"/>
+      <c r="A612" s="16" t="s">
+        <v>2284</v>
+      </c>
+      <c r="B612" s="6">
+        <v>44155.0</v>
+      </c>
+      <c r="C612" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D612" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E612" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F612" s="34"/>
-      <c r="G612" s="34"/>
-      <c r="H612" s="21"/>
-      <c r="I612" s="19"/>
-      <c r="J612" s="10"/>
-      <c r="K612" s="22"/>
-      <c r="L612" s="23"/>
-      <c r="M612" s="22"/>
+      <c r="G612" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H612" s="8" t="s">
+        <v>2285</v>
+      </c>
+      <c r="I612" s="9">
+        <v>44140.0</v>
+      </c>
+      <c r="J612" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K612" s="13" t="s">
+        <v>2286</v>
+      </c>
+      <c r="L612" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M612" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N612" s="25"/>
-      <c r="O612" s="21"/>
-      <c r="P612" s="21"/>
+      <c r="O612" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P612" s="8" t="s">
+        <v>2182</v>
+      </c>
       <c r="Q612" s="19"/>
       <c r="R612" s="19"/>
-      <c r="S612" s="20"/>
+      <c r="S612" s="61" t="s">
+        <v>2287</v>
+      </c>
       <c r="T612" s="20"/>
       <c r="U612" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#611</v>
       </c>
     </row>
     <row r="613">
-      <c r="A613" s="73"/>
-      <c r="B613" s="74"/>
-      <c r="C613" s="34"/>
-      <c r="D613" s="34"/>
-      <c r="E613" s="34"/>
+      <c r="A613" s="16" t="s">
+        <v>2288</v>
+      </c>
+      <c r="B613" s="6">
+        <v>44155.0</v>
+      </c>
+      <c r="C613" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D613" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E613" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F613" s="34"/>
-      <c r="G613" s="34"/>
-      <c r="H613" s="21"/>
-      <c r="I613" s="19"/>
-      <c r="J613" s="10"/>
-      <c r="K613" s="22"/>
-      <c r="L613" s="23"/>
-      <c r="M613" s="22"/>
+      <c r="G613" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H613" s="8" t="s">
+        <v>2285</v>
+      </c>
+      <c r="I613" s="9">
+        <v>44140.0</v>
+      </c>
+      <c r="J613" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K613" s="13" t="s">
+        <v>2286</v>
+      </c>
+      <c r="L613" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M613" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N613" s="25"/>
-      <c r="O613" s="21"/>
-      <c r="P613" s="21"/>
+      <c r="O613" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P613" s="8" t="s">
+        <v>2182</v>
+      </c>
       <c r="Q613" s="19"/>
       <c r="R613" s="19"/>
-      <c r="S613" s="20"/>
+      <c r="S613" s="61" t="s">
+        <v>2287</v>
+      </c>
       <c r="T613" s="20"/>
       <c r="U613" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#612</v>
       </c>
     </row>
     <row r="614">
@@ -47637,15 +47713,17 @@
     <hyperlink r:id="rId171" ref="S609"/>
     <hyperlink r:id="rId172" ref="S610"/>
     <hyperlink r:id="rId173" ref="S611"/>
+    <hyperlink r:id="rId174" ref="S612"/>
+    <hyperlink r:id="rId175" ref="S613"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId174"/>
-  <legacyDrawing r:id="rId175"/>
+  <drawing r:id="rId176"/>
+  <legacyDrawing r:id="rId177"/>
   <tableParts count="2">
-    <tablePart r:id="rId178"/>
-    <tablePart r:id="rId179"/>
+    <tablePart r:id="rId180"/>
+    <tablePart r:id="rId181"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201123
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -571,7 +571,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6878" uniqueCount="2289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6971" uniqueCount="2309">
   <si>
     <t>案例</t>
   </si>
@@ -8336,6 +8336,72 @@
   <si>
     <t>#612</t>
   </si>
+  <si>
+    <t>#613</t>
+  </si>
+  <si>
+    <t>-11/7(8) 印尼→台灣</t>
+  </si>
+  <si>
+    <t>11/7(8)</t>
+  </si>
+  <si>
+    <t>11/20(21) 採檢
+11/22 確診</t>
+  </si>
+  <si>
+    <t>國內新增6例境外移入COVID-19病例，分別自印尼、美國、菲律賓入境</t>
+  </si>
+  <si>
+    <t>#614</t>
+  </si>
+  <si>
+    <t>#615</t>
+  </si>
+  <si>
+    <t>8月中旬-11/20 美國</t>
+  </si>
+  <si>
+    <t>11/20 採檢
+11/22 確診</t>
+  </si>
+  <si>
+    <t>肌肉痠痛 咳嗽 有痰 流鼻水 頭痛 嗅覺異常</t>
+  </si>
+  <si>
+    <t>#616</t>
+  </si>
+  <si>
+    <t>-11/8 菲律賓→台灣</t>
+  </si>
+  <si>
+    <t>11/21 採檢
+11/22 確診</t>
+  </si>
+  <si>
+    <t>#617</t>
+  </si>
+  <si>
+    <t>#618</t>
+  </si>
+  <si>
+    <t>#619</t>
+  </si>
+  <si>
+    <t>2月-11/20 迦納</t>
+  </si>
+  <si>
+    <t>呼吸短促 胸悶 發燒</t>
+  </si>
+  <si>
+    <t>經商
+10月下旬曾接觸確診個案，因有返臺探親需求，11月4日於當地進行採檢，11月5日檢出陽性確診。
+個案原於自宅隔離，但後續出現呼吸短促、胸悶、發燒等情形，11月11日送至當地醫院治療，因病情加重，期間完成國際緊急醫療專機轉送國人返國就醫申請作業。
+11月20日個案搭乘國際緊急醫療專機抵臺，入境後即後送就醫</t>
+  </si>
+  <si>
+    <t>新增1例境外移入COVID-19病例，為自迦納返國者</t>
+  </si>
 </sst>
 </file>
 
@@ -8345,7 +8411,7 @@
     <numFmt numFmtId="164" formatCode="mm&quot;月&quot;dd&quot;日 &quot;dddd"/>
     <numFmt numFmtId="165" formatCode="m/d"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="20">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -8426,6 +8492,10 @@
       <u/>
       <color rgb="FFFFFFFF"/>
     </font>
+    <font/>
+    <font>
+      <color rgb="FF000000"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -8471,7 +8541,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="81">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -8690,6 +8760,24 @@
     </xf>
     <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="18" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
@@ -44872,190 +44960,398 @@
       </c>
     </row>
     <row r="614">
-      <c r="A614" s="73"/>
-      <c r="B614" s="74"/>
-      <c r="C614" s="34"/>
-      <c r="D614" s="34"/>
-      <c r="E614" s="34"/>
+      <c r="A614" s="16" t="s">
+        <v>2289</v>
+      </c>
+      <c r="B614" s="6">
+        <v>44157.0</v>
+      </c>
+      <c r="C614" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D614" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E614" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F614" s="34"/>
-      <c r="G614" s="34"/>
-      <c r="H614" s="21"/>
-      <c r="I614" s="19"/>
-      <c r="J614" s="10"/>
-      <c r="K614" s="22"/>
-      <c r="L614" s="23"/>
-      <c r="M614" s="22"/>
+      <c r="G614" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H614" s="8" t="s">
+        <v>2290</v>
+      </c>
+      <c r="I614" s="16" t="s">
+        <v>2291</v>
+      </c>
+      <c r="J614" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K614" s="13" t="s">
+        <v>2292</v>
+      </c>
+      <c r="L614" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M614" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N614" s="25"/>
-      <c r="O614" s="21"/>
-      <c r="P614" s="21"/>
+      <c r="O614" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P614" s="8" t="s">
+        <v>2182</v>
+      </c>
       <c r="Q614" s="19"/>
       <c r="R614" s="19"/>
-      <c r="S614" s="20"/>
+      <c r="S614" s="61" t="s">
+        <v>2293</v>
+      </c>
       <c r="T614" s="20"/>
       <c r="U614" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#613</v>
       </c>
     </row>
     <row r="615">
-      <c r="A615" s="73"/>
-      <c r="B615" s="74"/>
-      <c r="C615" s="34"/>
-      <c r="D615" s="34"/>
-      <c r="E615" s="34"/>
+      <c r="A615" s="16" t="s">
+        <v>2294</v>
+      </c>
+      <c r="B615" s="6">
+        <v>44157.0</v>
+      </c>
+      <c r="C615" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D615" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E615" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F615" s="34"/>
-      <c r="G615" s="34"/>
-      <c r="H615" s="21"/>
-      <c r="I615" s="19"/>
-      <c r="J615" s="10"/>
-      <c r="K615" s="22"/>
-      <c r="L615" s="23"/>
-      <c r="M615" s="22"/>
+      <c r="G615" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H615" s="8" t="s">
+        <v>2290</v>
+      </c>
+      <c r="I615" s="16" t="s">
+        <v>2291</v>
+      </c>
+      <c r="J615" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K615" s="13" t="s">
+        <v>2292</v>
+      </c>
+      <c r="L615" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M615" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N615" s="25"/>
-      <c r="O615" s="21"/>
-      <c r="P615" s="21"/>
+      <c r="O615" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P615" s="8" t="s">
+        <v>2182</v>
+      </c>
       <c r="Q615" s="19"/>
       <c r="R615" s="19"/>
-      <c r="S615" s="20"/>
+      <c r="S615" s="61" t="s">
+        <v>2293</v>
+      </c>
       <c r="T615" s="20"/>
       <c r="U615" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#614</v>
       </c>
     </row>
     <row r="616">
-      <c r="A616" s="73"/>
-      <c r="B616" s="74"/>
-      <c r="C616" s="34"/>
-      <c r="D616" s="34"/>
-      <c r="E616" s="34"/>
+      <c r="A616" s="16" t="s">
+        <v>2295</v>
+      </c>
+      <c r="B616" s="6">
+        <v>44157.0</v>
+      </c>
+      <c r="C616" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D616" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E616" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F616" s="34"/>
-      <c r="G616" s="34"/>
-      <c r="H616" s="21"/>
-      <c r="I616" s="19"/>
-      <c r="J616" s="10"/>
-      <c r="K616" s="22"/>
-      <c r="L616" s="23"/>
-      <c r="M616" s="22"/>
+      <c r="G616" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H616" s="8" t="s">
+        <v>2296</v>
+      </c>
+      <c r="I616" s="9">
+        <v>44155.0</v>
+      </c>
+      <c r="J616" s="10">
+        <v>44141.0</v>
+      </c>
+      <c r="K616" s="13" t="s">
+        <v>2297</v>
+      </c>
+      <c r="L616" s="12" t="s">
+        <v>363</v>
+      </c>
+      <c r="M616" s="13" t="s">
+        <v>2298</v>
+      </c>
       <c r="N616" s="25"/>
-      <c r="O616" s="21"/>
-      <c r="P616" s="21"/>
+      <c r="O616" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P616" s="8" t="s">
+        <v>360</v>
+      </c>
       <c r="Q616" s="19"/>
       <c r="R616" s="19"/>
-      <c r="S616" s="20"/>
+      <c r="S616" s="61" t="s">
+        <v>2293</v>
+      </c>
       <c r="T616" s="20"/>
       <c r="U616" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#615</v>
       </c>
     </row>
     <row r="617">
-      <c r="A617" s="73"/>
-      <c r="B617" s="74"/>
-      <c r="C617" s="34"/>
-      <c r="D617" s="34"/>
-      <c r="E617" s="34"/>
+      <c r="A617" s="16" t="s">
+        <v>2299</v>
+      </c>
+      <c r="B617" s="6">
+        <v>44157.0</v>
+      </c>
+      <c r="C617" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D617" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E617" s="7" t="s">
+        <v>205</v>
+      </c>
       <c r="F617" s="34"/>
-      <c r="G617" s="34"/>
-      <c r="H617" s="21"/>
-      <c r="I617" s="19"/>
-      <c r="J617" s="10"/>
-      <c r="K617" s="22"/>
-      <c r="L617" s="23"/>
-      <c r="M617" s="22"/>
+      <c r="G617" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H617" s="8" t="s">
+        <v>2300</v>
+      </c>
+      <c r="I617" s="9">
+        <v>44143.0</v>
+      </c>
+      <c r="J617" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K617" s="13" t="s">
+        <v>2301</v>
+      </c>
+      <c r="L617" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M617" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N617" s="25"/>
-      <c r="O617" s="21"/>
-      <c r="P617" s="21"/>
+      <c r="O617" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P617" s="8" t="s">
+        <v>2182</v>
+      </c>
       <c r="Q617" s="19"/>
       <c r="R617" s="19"/>
-      <c r="S617" s="20"/>
+      <c r="S617" s="61" t="s">
+        <v>2293</v>
+      </c>
       <c r="T617" s="20"/>
       <c r="U617" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#616</v>
       </c>
     </row>
     <row r="618">
-      <c r="A618" s="73"/>
-      <c r="B618" s="74"/>
-      <c r="C618" s="34"/>
-      <c r="D618" s="34"/>
-      <c r="E618" s="34"/>
+      <c r="A618" s="16" t="s">
+        <v>2302</v>
+      </c>
+      <c r="B618" s="6">
+        <v>44157.0</v>
+      </c>
+      <c r="C618" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D618" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E618" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F618" s="34"/>
-      <c r="G618" s="34"/>
-      <c r="H618" s="21"/>
-      <c r="I618" s="19"/>
-      <c r="J618" s="10"/>
-      <c r="K618" s="22"/>
-      <c r="L618" s="23"/>
-      <c r="M618" s="22"/>
+      <c r="G618" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H618" s="8" t="s">
+        <v>2290</v>
+      </c>
+      <c r="I618" s="16" t="s">
+        <v>2291</v>
+      </c>
+      <c r="J618" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K618" s="13" t="s">
+        <v>2292</v>
+      </c>
+      <c r="L618" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M618" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N618" s="25"/>
-      <c r="O618" s="21"/>
-      <c r="P618" s="21"/>
+      <c r="O618" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P618" s="8" t="s">
+        <v>2182</v>
+      </c>
       <c r="Q618" s="19"/>
       <c r="R618" s="19"/>
-      <c r="S618" s="20"/>
+      <c r="S618" s="61" t="s">
+        <v>2293</v>
+      </c>
       <c r="T618" s="20"/>
       <c r="U618" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#617</v>
       </c>
     </row>
     <row r="619">
-      <c r="A619" s="73"/>
-      <c r="B619" s="74"/>
-      <c r="C619" s="34"/>
-      <c r="D619" s="34"/>
-      <c r="E619" s="34"/>
+      <c r="A619" s="16" t="s">
+        <v>2303</v>
+      </c>
+      <c r="B619" s="6">
+        <v>44157.0</v>
+      </c>
+      <c r="C619" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D619" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E619" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F619" s="34"/>
-      <c r="G619" s="34"/>
-      <c r="H619" s="21"/>
-      <c r="I619" s="19"/>
-      <c r="J619" s="10"/>
-      <c r="K619" s="22"/>
-      <c r="L619" s="23"/>
-      <c r="M619" s="22"/>
+      <c r="G619" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H619" s="8" t="s">
+        <v>2290</v>
+      </c>
+      <c r="I619" s="16" t="s">
+        <v>2291</v>
+      </c>
+      <c r="J619" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K619" s="13" t="s">
+        <v>2292</v>
+      </c>
+      <c r="L619" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M619" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N619" s="25"/>
-      <c r="O619" s="21"/>
-      <c r="P619" s="21"/>
+      <c r="O619" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P619" s="8" t="s">
+        <v>2182</v>
+      </c>
       <c r="Q619" s="19"/>
       <c r="R619" s="19"/>
-      <c r="S619" s="20"/>
+      <c r="S619" s="61" t="s">
+        <v>2293</v>
+      </c>
       <c r="T619" s="20"/>
       <c r="U619" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#618</v>
       </c>
     </row>
     <row r="620">
-      <c r="A620" s="73"/>
-      <c r="B620" s="74"/>
-      <c r="C620" s="34"/>
-      <c r="D620" s="34"/>
-      <c r="E620" s="34"/>
+      <c r="A620" s="73" t="s">
+        <v>2304</v>
+      </c>
+      <c r="B620" s="6">
+        <v>44158.0</v>
+      </c>
+      <c r="C620" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D620" s="74" t="s">
+        <v>22</v>
+      </c>
+      <c r="E620" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F620" s="34"/>
-      <c r="G620" s="34"/>
-      <c r="H620" s="21"/>
-      <c r="I620" s="19"/>
+      <c r="G620" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H620" s="75" t="s">
+        <v>2305</v>
+      </c>
+      <c r="I620" s="76">
+        <v>44155.0</v>
+      </c>
       <c r="J620" s="10"/>
-      <c r="K620" s="22"/>
-      <c r="L620" s="23"/>
-      <c r="M620" s="22"/>
+      <c r="K620" s="77" t="s">
+        <v>2297</v>
+      </c>
+      <c r="L620" s="78" t="s">
+        <v>363</v>
+      </c>
+      <c r="M620" s="77" t="s">
+        <v>2306</v>
+      </c>
       <c r="N620" s="25"/>
-      <c r="O620" s="21"/>
-      <c r="P620" s="21"/>
+      <c r="O620" s="75" t="s">
+        <v>85</v>
+      </c>
+      <c r="P620" s="75" t="s">
+        <v>2307</v>
+      </c>
       <c r="Q620" s="19"/>
       <c r="R620" s="19"/>
-      <c r="S620" s="20"/>
+      <c r="S620" s="61" t="s">
+        <v>2308</v>
+      </c>
       <c r="T620" s="20"/>
       <c r="U620" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#619</v>
       </c>
     </row>
     <row r="621">
-      <c r="A621" s="73"/>
-      <c r="B621" s="74"/>
+      <c r="A621" s="79"/>
+      <c r="B621" s="80"/>
       <c r="C621" s="34"/>
       <c r="D621" s="34"/>
       <c r="E621" s="34"/>
@@ -45080,8 +45376,8 @@
       </c>
     </row>
     <row r="622">
-      <c r="A622" s="73"/>
-      <c r="B622" s="74"/>
+      <c r="A622" s="79"/>
+      <c r="B622" s="80"/>
       <c r="C622" s="34"/>
       <c r="D622" s="34"/>
       <c r="E622" s="34"/>
@@ -45106,8 +45402,8 @@
       </c>
     </row>
     <row r="623">
-      <c r="A623" s="73"/>
-      <c r="B623" s="74"/>
+      <c r="A623" s="79"/>
+      <c r="B623" s="80"/>
       <c r="C623" s="34"/>
       <c r="D623" s="34"/>
       <c r="E623" s="34"/>
@@ -45132,8 +45428,8 @@
       </c>
     </row>
     <row r="624">
-      <c r="A624" s="73"/>
-      <c r="B624" s="74"/>
+      <c r="A624" s="79"/>
+      <c r="B624" s="80"/>
       <c r="C624" s="34"/>
       <c r="D624" s="34"/>
       <c r="E624" s="34"/>
@@ -45158,8 +45454,8 @@
       </c>
     </row>
     <row r="625">
-      <c r="A625" s="73"/>
-      <c r="B625" s="74"/>
+      <c r="A625" s="79"/>
+      <c r="B625" s="80"/>
       <c r="C625" s="34"/>
       <c r="D625" s="34"/>
       <c r="E625" s="34"/>
@@ -45184,8 +45480,8 @@
       </c>
     </row>
     <row r="626">
-      <c r="A626" s="73"/>
-      <c r="B626" s="74"/>
+      <c r="A626" s="79"/>
+      <c r="B626" s="80"/>
       <c r="C626" s="34"/>
       <c r="D626" s="34"/>
       <c r="E626" s="34"/>
@@ -45210,8 +45506,8 @@
       </c>
     </row>
     <row r="627">
-      <c r="A627" s="73"/>
-      <c r="B627" s="74"/>
+      <c r="A627" s="79"/>
+      <c r="B627" s="80"/>
       <c r="C627" s="34"/>
       <c r="D627" s="34"/>
       <c r="E627" s="34"/>
@@ -45236,8 +45532,8 @@
       </c>
     </row>
     <row r="628">
-      <c r="A628" s="73"/>
-      <c r="B628" s="74"/>
+      <c r="A628" s="79"/>
+      <c r="B628" s="80"/>
       <c r="C628" s="34"/>
       <c r="D628" s="34"/>
       <c r="E628" s="34"/>
@@ -45262,8 +45558,8 @@
       </c>
     </row>
     <row r="629">
-      <c r="A629" s="73"/>
-      <c r="B629" s="74"/>
+      <c r="A629" s="79"/>
+      <c r="B629" s="80"/>
       <c r="C629" s="34"/>
       <c r="D629" s="34"/>
       <c r="E629" s="34"/>
@@ -45288,8 +45584,8 @@
       </c>
     </row>
     <row r="630">
-      <c r="A630" s="73"/>
-      <c r="B630" s="74"/>
+      <c r="A630" s="79"/>
+      <c r="B630" s="80"/>
       <c r="C630" s="34"/>
       <c r="D630" s="34"/>
       <c r="E630" s="34"/>
@@ -45314,8 +45610,8 @@
       </c>
     </row>
     <row r="631">
-      <c r="A631" s="73"/>
-      <c r="B631" s="74"/>
+      <c r="A631" s="79"/>
+      <c r="B631" s="80"/>
       <c r="C631" s="34"/>
       <c r="D631" s="34"/>
       <c r="E631" s="34"/>
@@ -45340,8 +45636,8 @@
       </c>
     </row>
     <row r="632">
-      <c r="A632" s="73"/>
-      <c r="B632" s="74"/>
+      <c r="A632" s="79"/>
+      <c r="B632" s="80"/>
       <c r="C632" s="34"/>
       <c r="D632" s="34"/>
       <c r="E632" s="34"/>
@@ -45366,8 +45662,8 @@
       </c>
     </row>
     <row r="633">
-      <c r="A633" s="73"/>
-      <c r="B633" s="74"/>
+      <c r="A633" s="79"/>
+      <c r="B633" s="80"/>
       <c r="C633" s="34"/>
       <c r="D633" s="34"/>
       <c r="E633" s="34"/>
@@ -45392,8 +45688,8 @@
       </c>
     </row>
     <row r="634">
-      <c r="A634" s="73"/>
-      <c r="B634" s="74"/>
+      <c r="A634" s="79"/>
+      <c r="B634" s="80"/>
       <c r="C634" s="34"/>
       <c r="D634" s="34"/>
       <c r="E634" s="34"/>
@@ -45418,8 +45714,8 @@
       </c>
     </row>
     <row r="635">
-      <c r="A635" s="73"/>
-      <c r="B635" s="74"/>
+      <c r="A635" s="79"/>
+      <c r="B635" s="80"/>
       <c r="C635" s="34"/>
       <c r="D635" s="34"/>
       <c r="E635" s="34"/>
@@ -45444,8 +45740,8 @@
       </c>
     </row>
     <row r="636">
-      <c r="A636" s="73"/>
-      <c r="B636" s="74"/>
+      <c r="A636" s="79"/>
+      <c r="B636" s="80"/>
       <c r="C636" s="34"/>
       <c r="D636" s="34"/>
       <c r="E636" s="34"/>
@@ -45470,8 +45766,8 @@
       </c>
     </row>
     <row r="637">
-      <c r="A637" s="73"/>
-      <c r="B637" s="74"/>
+      <c r="A637" s="79"/>
+      <c r="B637" s="80"/>
       <c r="C637" s="34"/>
       <c r="D637" s="34"/>
       <c r="E637" s="34"/>
@@ -45496,8 +45792,8 @@
       </c>
     </row>
     <row r="638">
-      <c r="A638" s="73"/>
-      <c r="B638" s="74"/>
+      <c r="A638" s="79"/>
+      <c r="B638" s="80"/>
       <c r="C638" s="34"/>
       <c r="D638" s="34"/>
       <c r="E638" s="34"/>
@@ -45522,8 +45818,8 @@
       </c>
     </row>
     <row r="639">
-      <c r="A639" s="73"/>
-      <c r="B639" s="74"/>
+      <c r="A639" s="79"/>
+      <c r="B639" s="80"/>
       <c r="C639" s="34"/>
       <c r="D639" s="34"/>
       <c r="E639" s="34"/>
@@ -45548,8 +45844,8 @@
       </c>
     </row>
     <row r="640">
-      <c r="A640" s="73"/>
-      <c r="B640" s="74"/>
+      <c r="A640" s="79"/>
+      <c r="B640" s="80"/>
       <c r="C640" s="34"/>
       <c r="D640" s="34"/>
       <c r="E640" s="34"/>
@@ -45574,8 +45870,8 @@
       </c>
     </row>
     <row r="641">
-      <c r="A641" s="73"/>
-      <c r="B641" s="74"/>
+      <c r="A641" s="79"/>
+      <c r="B641" s="80"/>
       <c r="C641" s="34"/>
       <c r="D641" s="34"/>
       <c r="E641" s="34"/>
@@ -45600,8 +45896,8 @@
       </c>
     </row>
     <row r="642">
-      <c r="A642" s="73"/>
-      <c r="B642" s="74"/>
+      <c r="A642" s="79"/>
+      <c r="B642" s="80"/>
       <c r="C642" s="34"/>
       <c r="D642" s="34"/>
       <c r="E642" s="34"/>
@@ -45626,8 +45922,8 @@
       </c>
     </row>
     <row r="643">
-      <c r="A643" s="73"/>
-      <c r="B643" s="74"/>
+      <c r="A643" s="79"/>
+      <c r="B643" s="80"/>
       <c r="C643" s="34"/>
       <c r="D643" s="34"/>
       <c r="E643" s="34"/>
@@ -45652,8 +45948,8 @@
       </c>
     </row>
     <row r="644">
-      <c r="A644" s="73"/>
-      <c r="B644" s="74"/>
+      <c r="A644" s="79"/>
+      <c r="B644" s="80"/>
       <c r="C644" s="34"/>
       <c r="D644" s="34"/>
       <c r="E644" s="34"/>
@@ -45678,8 +45974,8 @@
       </c>
     </row>
     <row r="645">
-      <c r="A645" s="73"/>
-      <c r="B645" s="74"/>
+      <c r="A645" s="79"/>
+      <c r="B645" s="80"/>
       <c r="C645" s="34"/>
       <c r="D645" s="34"/>
       <c r="E645" s="34"/>
@@ -45704,8 +46000,8 @@
       </c>
     </row>
     <row r="646">
-      <c r="A646" s="73"/>
-      <c r="B646" s="74"/>
+      <c r="A646" s="79"/>
+      <c r="B646" s="80"/>
       <c r="C646" s="34"/>
       <c r="D646" s="34"/>
       <c r="E646" s="34"/>
@@ -45730,8 +46026,8 @@
       </c>
     </row>
     <row r="647">
-      <c r="A647" s="73"/>
-      <c r="B647" s="74"/>
+      <c r="A647" s="79"/>
+      <c r="B647" s="80"/>
       <c r="C647" s="34"/>
       <c r="D647" s="34"/>
       <c r="E647" s="34"/>
@@ -45756,8 +46052,8 @@
       </c>
     </row>
     <row r="648">
-      <c r="A648" s="73"/>
-      <c r="B648" s="74"/>
+      <c r="A648" s="79"/>
+      <c r="B648" s="80"/>
       <c r="C648" s="34"/>
       <c r="D648" s="34"/>
       <c r="E648" s="34"/>
@@ -45782,8 +46078,8 @@
       </c>
     </row>
     <row r="649">
-      <c r="A649" s="73"/>
-      <c r="B649" s="74"/>
+      <c r="A649" s="79"/>
+      <c r="B649" s="80"/>
       <c r="C649" s="34"/>
       <c r="D649" s="34"/>
       <c r="E649" s="34"/>
@@ -45808,8 +46104,8 @@
       </c>
     </row>
     <row r="650">
-      <c r="A650" s="73"/>
-      <c r="B650" s="74"/>
+      <c r="A650" s="79"/>
+      <c r="B650" s="80"/>
       <c r="C650" s="34"/>
       <c r="D650" s="34"/>
       <c r="E650" s="34"/>
@@ -45834,8 +46130,8 @@
       </c>
     </row>
     <row r="651">
-      <c r="A651" s="73"/>
-      <c r="B651" s="74"/>
+      <c r="A651" s="79"/>
+      <c r="B651" s="80"/>
       <c r="C651" s="34"/>
       <c r="D651" s="34"/>
       <c r="E651" s="34"/>
@@ -45860,8 +46156,8 @@
       </c>
     </row>
     <row r="652">
-      <c r="A652" s="73"/>
-      <c r="B652" s="74"/>
+      <c r="A652" s="79"/>
+      <c r="B652" s="80"/>
       <c r="C652" s="34"/>
       <c r="D652" s="34"/>
       <c r="E652" s="34"/>
@@ -45886,8 +46182,8 @@
       </c>
     </row>
     <row r="653">
-      <c r="A653" s="73"/>
-      <c r="B653" s="74"/>
+      <c r="A653" s="79"/>
+      <c r="B653" s="80"/>
       <c r="C653" s="34"/>
       <c r="D653" s="34"/>
       <c r="E653" s="34"/>
@@ -45912,8 +46208,8 @@
       </c>
     </row>
     <row r="654">
-      <c r="A654" s="73"/>
-      <c r="B654" s="74"/>
+      <c r="A654" s="79"/>
+      <c r="B654" s="80"/>
       <c r="C654" s="34"/>
       <c r="D654" s="34"/>
       <c r="E654" s="34"/>
@@ -45938,8 +46234,8 @@
       </c>
     </row>
     <row r="655">
-      <c r="A655" s="73"/>
-      <c r="B655" s="74"/>
+      <c r="A655" s="79"/>
+      <c r="B655" s="80"/>
       <c r="C655" s="34"/>
       <c r="D655" s="34"/>
       <c r="E655" s="34"/>
@@ -45964,8 +46260,8 @@
       </c>
     </row>
     <row r="656">
-      <c r="A656" s="73"/>
-      <c r="B656" s="74"/>
+      <c r="A656" s="79"/>
+      <c r="B656" s="80"/>
       <c r="C656" s="34"/>
       <c r="D656" s="34"/>
       <c r="E656" s="34"/>
@@ -45990,8 +46286,8 @@
       </c>
     </row>
     <row r="657">
-      <c r="A657" s="73"/>
-      <c r="B657" s="74"/>
+      <c r="A657" s="79"/>
+      <c r="B657" s="80"/>
       <c r="C657" s="34"/>
       <c r="D657" s="34"/>
       <c r="E657" s="34"/>
@@ -46016,8 +46312,8 @@
       </c>
     </row>
     <row r="658">
-      <c r="A658" s="73"/>
-      <c r="B658" s="74"/>
+      <c r="A658" s="79"/>
+      <c r="B658" s="80"/>
       <c r="C658" s="34"/>
       <c r="D658" s="34"/>
       <c r="E658" s="34"/>
@@ -46042,8 +46338,8 @@
       </c>
     </row>
     <row r="659">
-      <c r="A659" s="73"/>
-      <c r="B659" s="74"/>
+      <c r="A659" s="79"/>
+      <c r="B659" s="80"/>
       <c r="C659" s="34"/>
       <c r="D659" s="34"/>
       <c r="E659" s="34"/>
@@ -46068,8 +46364,8 @@
       </c>
     </row>
     <row r="660">
-      <c r="A660" s="73"/>
-      <c r="B660" s="74"/>
+      <c r="A660" s="79"/>
+      <c r="B660" s="80"/>
       <c r="C660" s="34"/>
       <c r="D660" s="34"/>
       <c r="E660" s="34"/>
@@ -46094,8 +46390,8 @@
       </c>
     </row>
     <row r="661">
-      <c r="A661" s="73"/>
-      <c r="B661" s="74"/>
+      <c r="A661" s="79"/>
+      <c r="B661" s="80"/>
       <c r="C661" s="34"/>
       <c r="D661" s="34"/>
       <c r="E661" s="34"/>
@@ -46120,8 +46416,8 @@
       </c>
     </row>
     <row r="662">
-      <c r="A662" s="73"/>
-      <c r="B662" s="74"/>
+      <c r="A662" s="79"/>
+      <c r="B662" s="80"/>
       <c r="C662" s="34"/>
       <c r="D662" s="34"/>
       <c r="E662" s="34"/>
@@ -46146,8 +46442,8 @@
       </c>
     </row>
     <row r="663">
-      <c r="A663" s="73"/>
-      <c r="B663" s="74"/>
+      <c r="A663" s="79"/>
+      <c r="B663" s="80"/>
       <c r="C663" s="34"/>
       <c r="D663" s="34"/>
       <c r="E663" s="34"/>
@@ -46172,8 +46468,8 @@
       </c>
     </row>
     <row r="664">
-      <c r="A664" s="73"/>
-      <c r="B664" s="74"/>
+      <c r="A664" s="79"/>
+      <c r="B664" s="80"/>
       <c r="C664" s="34"/>
       <c r="D664" s="34"/>
       <c r="E664" s="34"/>
@@ -46198,8 +46494,8 @@
       </c>
     </row>
     <row r="665">
-      <c r="A665" s="73"/>
-      <c r="B665" s="74"/>
+      <c r="A665" s="79"/>
+      <c r="B665" s="80"/>
       <c r="C665" s="34"/>
       <c r="D665" s="34"/>
       <c r="E665" s="34"/>
@@ -46224,8 +46520,8 @@
       </c>
     </row>
     <row r="666">
-      <c r="A666" s="73"/>
-      <c r="B666" s="74"/>
+      <c r="A666" s="79"/>
+      <c r="B666" s="80"/>
       <c r="C666" s="34"/>
       <c r="D666" s="34"/>
       <c r="E666" s="34"/>
@@ -46250,8 +46546,8 @@
       </c>
     </row>
     <row r="667">
-      <c r="A667" s="73"/>
-      <c r="B667" s="74"/>
+      <c r="A667" s="79"/>
+      <c r="B667" s="80"/>
       <c r="C667" s="34"/>
       <c r="D667" s="34"/>
       <c r="E667" s="34"/>
@@ -46276,8 +46572,8 @@
       </c>
     </row>
     <row r="668">
-      <c r="A668" s="73"/>
-      <c r="B668" s="74"/>
+      <c r="A668" s="79"/>
+      <c r="B668" s="80"/>
       <c r="C668" s="34"/>
       <c r="D668" s="34"/>
       <c r="E668" s="34"/>
@@ -46302,8 +46598,8 @@
       </c>
     </row>
     <row r="669">
-      <c r="A669" s="73"/>
-      <c r="B669" s="74"/>
+      <c r="A669" s="79"/>
+      <c r="B669" s="80"/>
       <c r="C669" s="34"/>
       <c r="D669" s="34"/>
       <c r="E669" s="34"/>
@@ -46328,8 +46624,8 @@
       </c>
     </row>
     <row r="670">
-      <c r="A670" s="73"/>
-      <c r="B670" s="74"/>
+      <c r="A670" s="79"/>
+      <c r="B670" s="80"/>
       <c r="C670" s="34"/>
       <c r="D670" s="34"/>
       <c r="E670" s="34"/>
@@ -46354,8 +46650,8 @@
       </c>
     </row>
     <row r="671">
-      <c r="A671" s="73"/>
-      <c r="B671" s="74"/>
+      <c r="A671" s="79"/>
+      <c r="B671" s="80"/>
       <c r="C671" s="34"/>
       <c r="D671" s="34"/>
       <c r="E671" s="34"/>
@@ -46380,8 +46676,8 @@
       </c>
     </row>
     <row r="672">
-      <c r="A672" s="73"/>
-      <c r="B672" s="74"/>
+      <c r="A672" s="79"/>
+      <c r="B672" s="80"/>
       <c r="C672" s="34"/>
       <c r="D672" s="34"/>
       <c r="E672" s="34"/>
@@ -46406,8 +46702,8 @@
       </c>
     </row>
     <row r="673">
-      <c r="A673" s="73"/>
-      <c r="B673" s="74"/>
+      <c r="A673" s="79"/>
+      <c r="B673" s="80"/>
       <c r="C673" s="34"/>
       <c r="D673" s="34"/>
       <c r="E673" s="34"/>
@@ -46432,8 +46728,8 @@
       </c>
     </row>
     <row r="674">
-      <c r="A674" s="73"/>
-      <c r="B674" s="74"/>
+      <c r="A674" s="79"/>
+      <c r="B674" s="80"/>
       <c r="C674" s="34"/>
       <c r="D674" s="34"/>
       <c r="E674" s="34"/>
@@ -46458,8 +46754,8 @@
       </c>
     </row>
     <row r="675">
-      <c r="A675" s="73"/>
-      <c r="B675" s="74"/>
+      <c r="A675" s="79"/>
+      <c r="B675" s="80"/>
       <c r="C675" s="34"/>
       <c r="D675" s="34"/>
       <c r="E675" s="34"/>
@@ -46484,8 +46780,8 @@
       </c>
     </row>
     <row r="676">
-      <c r="A676" s="73"/>
-      <c r="B676" s="74"/>
+      <c r="A676" s="79"/>
+      <c r="B676" s="80"/>
       <c r="C676" s="34"/>
       <c r="D676" s="34"/>
       <c r="E676" s="34"/>
@@ -46510,8 +46806,8 @@
       </c>
     </row>
     <row r="677">
-      <c r="A677" s="73"/>
-      <c r="B677" s="74"/>
+      <c r="A677" s="79"/>
+      <c r="B677" s="80"/>
       <c r="C677" s="34"/>
       <c r="D677" s="34"/>
       <c r="E677" s="34"/>
@@ -46536,8 +46832,8 @@
       </c>
     </row>
     <row r="678">
-      <c r="A678" s="73"/>
-      <c r="B678" s="74"/>
+      <c r="A678" s="79"/>
+      <c r="B678" s="80"/>
       <c r="C678" s="34"/>
       <c r="D678" s="34"/>
       <c r="E678" s="34"/>
@@ -46562,8 +46858,8 @@
       </c>
     </row>
     <row r="679">
-      <c r="A679" s="73"/>
-      <c r="B679" s="74"/>
+      <c r="A679" s="79"/>
+      <c r="B679" s="80"/>
       <c r="C679" s="34"/>
       <c r="D679" s="34"/>
       <c r="E679" s="34"/>
@@ -46588,8 +46884,8 @@
       </c>
     </row>
     <row r="680">
-      <c r="A680" s="73"/>
-      <c r="B680" s="74"/>
+      <c r="A680" s="79"/>
+      <c r="B680" s="80"/>
       <c r="C680" s="34"/>
       <c r="D680" s="34"/>
       <c r="E680" s="34"/>
@@ -46614,8 +46910,8 @@
       </c>
     </row>
     <row r="681">
-      <c r="A681" s="73"/>
-      <c r="B681" s="74"/>
+      <c r="A681" s="79"/>
+      <c r="B681" s="80"/>
       <c r="C681" s="34"/>
       <c r="D681" s="34"/>
       <c r="E681" s="34"/>
@@ -46640,8 +46936,8 @@
       </c>
     </row>
     <row r="682">
-      <c r="A682" s="73"/>
-      <c r="B682" s="74"/>
+      <c r="A682" s="79"/>
+      <c r="B682" s="80"/>
       <c r="C682" s="34"/>
       <c r="D682" s="34"/>
       <c r="E682" s="34"/>
@@ -46666,8 +46962,8 @@
       </c>
     </row>
     <row r="683">
-      <c r="A683" s="73"/>
-      <c r="B683" s="74"/>
+      <c r="A683" s="79"/>
+      <c r="B683" s="80"/>
       <c r="C683" s="34"/>
       <c r="D683" s="34"/>
       <c r="E683" s="34"/>
@@ -46692,8 +46988,8 @@
       </c>
     </row>
     <row r="684">
-      <c r="A684" s="73"/>
-      <c r="B684" s="74"/>
+      <c r="A684" s="79"/>
+      <c r="B684" s="80"/>
       <c r="C684" s="34"/>
       <c r="D684" s="34"/>
       <c r="E684" s="34"/>
@@ -46718,8 +47014,8 @@
       </c>
     </row>
     <row r="685">
-      <c r="A685" s="73"/>
-      <c r="B685" s="74"/>
+      <c r="A685" s="79"/>
+      <c r="B685" s="80"/>
       <c r="C685" s="34"/>
       <c r="D685" s="34"/>
       <c r="E685" s="34"/>
@@ -46744,8 +47040,8 @@
       </c>
     </row>
     <row r="686">
-      <c r="A686" s="73"/>
-      <c r="B686" s="74"/>
+      <c r="A686" s="79"/>
+      <c r="B686" s="80"/>
       <c r="C686" s="34"/>
       <c r="D686" s="34"/>
       <c r="E686" s="34"/>
@@ -46770,8 +47066,8 @@
       </c>
     </row>
     <row r="687">
-      <c r="A687" s="73"/>
-      <c r="B687" s="74"/>
+      <c r="A687" s="79"/>
+      <c r="B687" s="80"/>
       <c r="C687" s="34"/>
       <c r="D687" s="34"/>
       <c r="E687" s="34"/>
@@ -46796,8 +47092,8 @@
       </c>
     </row>
     <row r="688">
-      <c r="A688" s="73"/>
-      <c r="B688" s="74"/>
+      <c r="A688" s="79"/>
+      <c r="B688" s="80"/>
       <c r="C688" s="34"/>
       <c r="D688" s="34"/>
       <c r="E688" s="34"/>
@@ -46822,8 +47118,8 @@
       </c>
     </row>
     <row r="689">
-      <c r="A689" s="73"/>
-      <c r="B689" s="74"/>
+      <c r="A689" s="79"/>
+      <c r="B689" s="80"/>
       <c r="C689" s="34"/>
       <c r="D689" s="34"/>
       <c r="E689" s="34"/>
@@ -46848,8 +47144,8 @@
       </c>
     </row>
     <row r="690">
-      <c r="A690" s="73"/>
-      <c r="B690" s="74"/>
+      <c r="A690" s="79"/>
+      <c r="B690" s="80"/>
       <c r="C690" s="34"/>
       <c r="D690" s="34"/>
       <c r="E690" s="34"/>
@@ -46874,8 +47170,8 @@
       </c>
     </row>
     <row r="691">
-      <c r="A691" s="73"/>
-      <c r="B691" s="74"/>
+      <c r="A691" s="79"/>
+      <c r="B691" s="80"/>
       <c r="C691" s="34"/>
       <c r="D691" s="34"/>
       <c r="E691" s="34"/>
@@ -46900,8 +47196,8 @@
       </c>
     </row>
     <row r="692">
-      <c r="A692" s="73"/>
-      <c r="B692" s="74"/>
+      <c r="A692" s="79"/>
+      <c r="B692" s="80"/>
       <c r="C692" s="34"/>
       <c r="D692" s="34"/>
       <c r="E692" s="34"/>
@@ -46926,8 +47222,8 @@
       </c>
     </row>
     <row r="693">
-      <c r="A693" s="73"/>
-      <c r="B693" s="74"/>
+      <c r="A693" s="79"/>
+      <c r="B693" s="80"/>
       <c r="C693" s="34"/>
       <c r="D693" s="34"/>
       <c r="E693" s="34"/>
@@ -46952,8 +47248,8 @@
       </c>
     </row>
     <row r="694">
-      <c r="A694" s="73"/>
-      <c r="B694" s="74"/>
+      <c r="A694" s="79"/>
+      <c r="B694" s="80"/>
       <c r="C694" s="34"/>
       <c r="D694" s="34"/>
       <c r="E694" s="34"/>
@@ -46978,8 +47274,8 @@
       </c>
     </row>
     <row r="695">
-      <c r="A695" s="73"/>
-      <c r="B695" s="74"/>
+      <c r="A695" s="79"/>
+      <c r="B695" s="80"/>
       <c r="C695" s="34"/>
       <c r="D695" s="34"/>
       <c r="E695" s="34"/>
@@ -47004,8 +47300,8 @@
       </c>
     </row>
     <row r="696">
-      <c r="A696" s="73"/>
-      <c r="B696" s="74"/>
+      <c r="A696" s="79"/>
+      <c r="B696" s="80"/>
       <c r="C696" s="34"/>
       <c r="D696" s="34"/>
       <c r="E696" s="34"/>
@@ -47030,8 +47326,8 @@
       </c>
     </row>
     <row r="697">
-      <c r="A697" s="73"/>
-      <c r="B697" s="74"/>
+      <c r="A697" s="79"/>
+      <c r="B697" s="80"/>
       <c r="C697" s="34"/>
       <c r="D697" s="34"/>
       <c r="E697" s="34"/>
@@ -47056,8 +47352,8 @@
       </c>
     </row>
     <row r="698">
-      <c r="A698" s="73"/>
-      <c r="B698" s="74"/>
+      <c r="A698" s="79"/>
+      <c r="B698" s="80"/>
       <c r="C698" s="34"/>
       <c r="D698" s="34"/>
       <c r="E698" s="34"/>
@@ -47082,8 +47378,8 @@
       </c>
     </row>
     <row r="699">
-      <c r="A699" s="73"/>
-      <c r="B699" s="74"/>
+      <c r="A699" s="79"/>
+      <c r="B699" s="80"/>
       <c r="C699" s="34"/>
       <c r="D699" s="34"/>
       <c r="E699" s="34"/>
@@ -47108,8 +47404,8 @@
       </c>
     </row>
     <row r="700">
-      <c r="A700" s="73"/>
-      <c r="B700" s="74"/>
+      <c r="A700" s="79"/>
+      <c r="B700" s="80"/>
       <c r="C700" s="34"/>
       <c r="D700" s="34"/>
       <c r="E700" s="34"/>
@@ -47134,8 +47430,8 @@
       </c>
     </row>
     <row r="701">
-      <c r="A701" s="73"/>
-      <c r="B701" s="74"/>
+      <c r="A701" s="79"/>
+      <c r="B701" s="80"/>
       <c r="C701" s="34"/>
       <c r="D701" s="34"/>
       <c r="E701" s="34"/>
@@ -47715,15 +48011,22 @@
     <hyperlink r:id="rId173" ref="S611"/>
     <hyperlink r:id="rId174" ref="S612"/>
     <hyperlink r:id="rId175" ref="S613"/>
+    <hyperlink r:id="rId176" ref="S614"/>
+    <hyperlink r:id="rId177" ref="S615"/>
+    <hyperlink r:id="rId178" ref="S616"/>
+    <hyperlink r:id="rId179" ref="S617"/>
+    <hyperlink r:id="rId180" ref="S618"/>
+    <hyperlink r:id="rId181" ref="S619"/>
+    <hyperlink r:id="rId182" ref="S620"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId176"/>
-  <legacyDrawing r:id="rId177"/>
+  <drawing r:id="rId183"/>
+  <legacyDrawing r:id="rId184"/>
   <tableParts count="2">
-    <tablePart r:id="rId180"/>
-    <tablePart r:id="rId181"/>
+    <tablePart r:id="rId187"/>
+    <tablePart r:id="rId188"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201124
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -8411,7 +8411,7 @@
     <numFmt numFmtId="164" formatCode="mm&quot;月&quot;dd&quot;日 &quot;dddd"/>
     <numFmt numFmtId="165" formatCode="m/d"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="18">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -8492,10 +8492,6 @@
       <u/>
       <color rgb="FFFFFFFF"/>
     </font>
-    <font/>
-    <font>
-      <color rgb="FF000000"/>
-    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -8541,7 +8537,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="75">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -8760,24 +8756,6 @@
     </xf>
     <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="18" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
@@ -45296,7 +45274,7 @@
       </c>
     </row>
     <row r="620">
-      <c r="A620" s="73" t="s">
+      <c r="A620" s="16" t="s">
         <v>2304</v>
       </c>
       <c r="B620" s="6">
@@ -45305,7 +45283,7 @@
       <c r="C620" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D620" s="74" t="s">
+      <c r="D620" s="7" t="s">
         <v>22</v>
       </c>
       <c r="E620" s="7" t="s">
@@ -45315,27 +45293,27 @@
       <c r="G620" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H620" s="75" t="s">
+      <c r="H620" s="8" t="s">
         <v>2305</v>
       </c>
-      <c r="I620" s="76">
+      <c r="I620" s="9">
         <v>44155.0</v>
       </c>
       <c r="J620" s="10"/>
-      <c r="K620" s="77" t="s">
+      <c r="K620" s="13" t="s">
         <v>2297</v>
       </c>
-      <c r="L620" s="78" t="s">
+      <c r="L620" s="12" t="s">
         <v>363</v>
       </c>
-      <c r="M620" s="77" t="s">
+      <c r="M620" s="13" t="s">
         <v>2306</v>
       </c>
       <c r="N620" s="25"/>
-      <c r="O620" s="75" t="s">
+      <c r="O620" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P620" s="75" t="s">
+      <c r="P620" s="8" t="s">
         <v>2307</v>
       </c>
       <c r="Q620" s="19"/>
@@ -45350,8 +45328,8 @@
       </c>
     </row>
     <row r="621">
-      <c r="A621" s="79"/>
-      <c r="B621" s="80"/>
+      <c r="A621" s="73"/>
+      <c r="B621" s="74"/>
       <c r="C621" s="34"/>
       <c r="D621" s="34"/>
       <c r="E621" s="34"/>
@@ -45376,8 +45354,8 @@
       </c>
     </row>
     <row r="622">
-      <c r="A622" s="79"/>
-      <c r="B622" s="80"/>
+      <c r="A622" s="73"/>
+      <c r="B622" s="74"/>
       <c r="C622" s="34"/>
       <c r="D622" s="34"/>
       <c r="E622" s="34"/>
@@ -45402,8 +45380,8 @@
       </c>
     </row>
     <row r="623">
-      <c r="A623" s="79"/>
-      <c r="B623" s="80"/>
+      <c r="A623" s="73"/>
+      <c r="B623" s="74"/>
       <c r="C623" s="34"/>
       <c r="D623" s="34"/>
       <c r="E623" s="34"/>
@@ -45428,8 +45406,8 @@
       </c>
     </row>
     <row r="624">
-      <c r="A624" s="79"/>
-      <c r="B624" s="80"/>
+      <c r="A624" s="73"/>
+      <c r="B624" s="74"/>
       <c r="C624" s="34"/>
       <c r="D624" s="34"/>
       <c r="E624" s="34"/>
@@ -45454,8 +45432,8 @@
       </c>
     </row>
     <row r="625">
-      <c r="A625" s="79"/>
-      <c r="B625" s="80"/>
+      <c r="A625" s="73"/>
+      <c r="B625" s="74"/>
       <c r="C625" s="34"/>
       <c r="D625" s="34"/>
       <c r="E625" s="34"/>
@@ -45480,8 +45458,8 @@
       </c>
     </row>
     <row r="626">
-      <c r="A626" s="79"/>
-      <c r="B626" s="80"/>
+      <c r="A626" s="73"/>
+      <c r="B626" s="74"/>
       <c r="C626" s="34"/>
       <c r="D626" s="34"/>
       <c r="E626" s="34"/>
@@ -45506,8 +45484,8 @@
       </c>
     </row>
     <row r="627">
-      <c r="A627" s="79"/>
-      <c r="B627" s="80"/>
+      <c r="A627" s="73"/>
+      <c r="B627" s="74"/>
       <c r="C627" s="34"/>
       <c r="D627" s="34"/>
       <c r="E627" s="34"/>
@@ -45532,8 +45510,8 @@
       </c>
     </row>
     <row r="628">
-      <c r="A628" s="79"/>
-      <c r="B628" s="80"/>
+      <c r="A628" s="73"/>
+      <c r="B628" s="74"/>
       <c r="C628" s="34"/>
       <c r="D628" s="34"/>
       <c r="E628" s="34"/>
@@ -45558,8 +45536,8 @@
       </c>
     </row>
     <row r="629">
-      <c r="A629" s="79"/>
-      <c r="B629" s="80"/>
+      <c r="A629" s="73"/>
+      <c r="B629" s="74"/>
       <c r="C629" s="34"/>
       <c r="D629" s="34"/>
       <c r="E629" s="34"/>
@@ -45584,8 +45562,8 @@
       </c>
     </row>
     <row r="630">
-      <c r="A630" s="79"/>
-      <c r="B630" s="80"/>
+      <c r="A630" s="73"/>
+      <c r="B630" s="74"/>
       <c r="C630" s="34"/>
       <c r="D630" s="34"/>
       <c r="E630" s="34"/>
@@ -45610,8 +45588,8 @@
       </c>
     </row>
     <row r="631">
-      <c r="A631" s="79"/>
-      <c r="B631" s="80"/>
+      <c r="A631" s="73"/>
+      <c r="B631" s="74"/>
       <c r="C631" s="34"/>
       <c r="D631" s="34"/>
       <c r="E631" s="34"/>
@@ -45636,8 +45614,8 @@
       </c>
     </row>
     <row r="632">
-      <c r="A632" s="79"/>
-      <c r="B632" s="80"/>
+      <c r="A632" s="73"/>
+      <c r="B632" s="74"/>
       <c r="C632" s="34"/>
       <c r="D632" s="34"/>
       <c r="E632" s="34"/>
@@ -45662,8 +45640,8 @@
       </c>
     </row>
     <row r="633">
-      <c r="A633" s="79"/>
-      <c r="B633" s="80"/>
+      <c r="A633" s="73"/>
+      <c r="B633" s="74"/>
       <c r="C633" s="34"/>
       <c r="D633" s="34"/>
       <c r="E633" s="34"/>
@@ -45688,8 +45666,8 @@
       </c>
     </row>
     <row r="634">
-      <c r="A634" s="79"/>
-      <c r="B634" s="80"/>
+      <c r="A634" s="73"/>
+      <c r="B634" s="74"/>
       <c r="C634" s="34"/>
       <c r="D634" s="34"/>
       <c r="E634" s="34"/>
@@ -45714,8 +45692,8 @@
       </c>
     </row>
     <row r="635">
-      <c r="A635" s="79"/>
-      <c r="B635" s="80"/>
+      <c r="A635" s="73"/>
+      <c r="B635" s="74"/>
       <c r="C635" s="34"/>
       <c r="D635" s="34"/>
       <c r="E635" s="34"/>
@@ -45740,8 +45718,8 @@
       </c>
     </row>
     <row r="636">
-      <c r="A636" s="79"/>
-      <c r="B636" s="80"/>
+      <c r="A636" s="73"/>
+      <c r="B636" s="74"/>
       <c r="C636" s="34"/>
       <c r="D636" s="34"/>
       <c r="E636" s="34"/>
@@ -45766,8 +45744,8 @@
       </c>
     </row>
     <row r="637">
-      <c r="A637" s="79"/>
-      <c r="B637" s="80"/>
+      <c r="A637" s="73"/>
+      <c r="B637" s="74"/>
       <c r="C637" s="34"/>
       <c r="D637" s="34"/>
       <c r="E637" s="34"/>
@@ -45792,8 +45770,8 @@
       </c>
     </row>
     <row r="638">
-      <c r="A638" s="79"/>
-      <c r="B638" s="80"/>
+      <c r="A638" s="73"/>
+      <c r="B638" s="74"/>
       <c r="C638" s="34"/>
       <c r="D638" s="34"/>
       <c r="E638" s="34"/>
@@ -45818,8 +45796,8 @@
       </c>
     </row>
     <row r="639">
-      <c r="A639" s="79"/>
-      <c r="B639" s="80"/>
+      <c r="A639" s="73"/>
+      <c r="B639" s="74"/>
       <c r="C639" s="34"/>
       <c r="D639" s="34"/>
       <c r="E639" s="34"/>
@@ -45844,8 +45822,8 @@
       </c>
     </row>
     <row r="640">
-      <c r="A640" s="79"/>
-      <c r="B640" s="80"/>
+      <c r="A640" s="73"/>
+      <c r="B640" s="74"/>
       <c r="C640" s="34"/>
       <c r="D640" s="34"/>
       <c r="E640" s="34"/>
@@ -45870,8 +45848,8 @@
       </c>
     </row>
     <row r="641">
-      <c r="A641" s="79"/>
-      <c r="B641" s="80"/>
+      <c r="A641" s="73"/>
+      <c r="B641" s="74"/>
       <c r="C641" s="34"/>
       <c r="D641" s="34"/>
       <c r="E641" s="34"/>
@@ -45896,8 +45874,8 @@
       </c>
     </row>
     <row r="642">
-      <c r="A642" s="79"/>
-      <c r="B642" s="80"/>
+      <c r="A642" s="73"/>
+      <c r="B642" s="74"/>
       <c r="C642" s="34"/>
       <c r="D642" s="34"/>
       <c r="E642" s="34"/>
@@ -45922,8 +45900,8 @@
       </c>
     </row>
     <row r="643">
-      <c r="A643" s="79"/>
-      <c r="B643" s="80"/>
+      <c r="A643" s="73"/>
+      <c r="B643" s="74"/>
       <c r="C643" s="34"/>
       <c r="D643" s="34"/>
       <c r="E643" s="34"/>
@@ -45948,8 +45926,8 @@
       </c>
     </row>
     <row r="644">
-      <c r="A644" s="79"/>
-      <c r="B644" s="80"/>
+      <c r="A644" s="73"/>
+      <c r="B644" s="74"/>
       <c r="C644" s="34"/>
       <c r="D644" s="34"/>
       <c r="E644" s="34"/>
@@ -45974,8 +45952,8 @@
       </c>
     </row>
     <row r="645">
-      <c r="A645" s="79"/>
-      <c r="B645" s="80"/>
+      <c r="A645" s="73"/>
+      <c r="B645" s="74"/>
       <c r="C645" s="34"/>
       <c r="D645" s="34"/>
       <c r="E645" s="34"/>
@@ -46000,8 +45978,8 @@
       </c>
     </row>
     <row r="646">
-      <c r="A646" s="79"/>
-      <c r="B646" s="80"/>
+      <c r="A646" s="73"/>
+      <c r="B646" s="74"/>
       <c r="C646" s="34"/>
       <c r="D646" s="34"/>
       <c r="E646" s="34"/>
@@ -46026,8 +46004,8 @@
       </c>
     </row>
     <row r="647">
-      <c r="A647" s="79"/>
-      <c r="B647" s="80"/>
+      <c r="A647" s="73"/>
+      <c r="B647" s="74"/>
       <c r="C647" s="34"/>
       <c r="D647" s="34"/>
       <c r="E647" s="34"/>
@@ -46052,8 +46030,8 @@
       </c>
     </row>
     <row r="648">
-      <c r="A648" s="79"/>
-      <c r="B648" s="80"/>
+      <c r="A648" s="73"/>
+      <c r="B648" s="74"/>
       <c r="C648" s="34"/>
       <c r="D648" s="34"/>
       <c r="E648" s="34"/>
@@ -46078,8 +46056,8 @@
       </c>
     </row>
     <row r="649">
-      <c r="A649" s="79"/>
-      <c r="B649" s="80"/>
+      <c r="A649" s="73"/>
+      <c r="B649" s="74"/>
       <c r="C649" s="34"/>
       <c r="D649" s="34"/>
       <c r="E649" s="34"/>
@@ -46104,8 +46082,8 @@
       </c>
     </row>
     <row r="650">
-      <c r="A650" s="79"/>
-      <c r="B650" s="80"/>
+      <c r="A650" s="73"/>
+      <c r="B650" s="74"/>
       <c r="C650" s="34"/>
       <c r="D650" s="34"/>
       <c r="E650" s="34"/>
@@ -46130,8 +46108,8 @@
       </c>
     </row>
     <row r="651">
-      <c r="A651" s="79"/>
-      <c r="B651" s="80"/>
+      <c r="A651" s="73"/>
+      <c r="B651" s="74"/>
       <c r="C651" s="34"/>
       <c r="D651" s="34"/>
       <c r="E651" s="34"/>
@@ -46156,8 +46134,8 @@
       </c>
     </row>
     <row r="652">
-      <c r="A652" s="79"/>
-      <c r="B652" s="80"/>
+      <c r="A652" s="73"/>
+      <c r="B652" s="74"/>
       <c r="C652" s="34"/>
       <c r="D652" s="34"/>
       <c r="E652" s="34"/>
@@ -46182,8 +46160,8 @@
       </c>
     </row>
     <row r="653">
-      <c r="A653" s="79"/>
-      <c r="B653" s="80"/>
+      <c r="A653" s="73"/>
+      <c r="B653" s="74"/>
       <c r="C653" s="34"/>
       <c r="D653" s="34"/>
       <c r="E653" s="34"/>
@@ -46208,8 +46186,8 @@
       </c>
     </row>
     <row r="654">
-      <c r="A654" s="79"/>
-      <c r="B654" s="80"/>
+      <c r="A654" s="73"/>
+      <c r="B654" s="74"/>
       <c r="C654" s="34"/>
       <c r="D654" s="34"/>
       <c r="E654" s="34"/>
@@ -46234,8 +46212,8 @@
       </c>
     </row>
     <row r="655">
-      <c r="A655" s="79"/>
-      <c r="B655" s="80"/>
+      <c r="A655" s="73"/>
+      <c r="B655" s="74"/>
       <c r="C655" s="34"/>
       <c r="D655" s="34"/>
       <c r="E655" s="34"/>
@@ -46260,8 +46238,8 @@
       </c>
     </row>
     <row r="656">
-      <c r="A656" s="79"/>
-      <c r="B656" s="80"/>
+      <c r="A656" s="73"/>
+      <c r="B656" s="74"/>
       <c r="C656" s="34"/>
       <c r="D656" s="34"/>
       <c r="E656" s="34"/>
@@ -46286,8 +46264,8 @@
       </c>
     </row>
     <row r="657">
-      <c r="A657" s="79"/>
-      <c r="B657" s="80"/>
+      <c r="A657" s="73"/>
+      <c r="B657" s="74"/>
       <c r="C657" s="34"/>
       <c r="D657" s="34"/>
       <c r="E657" s="34"/>
@@ -46312,8 +46290,8 @@
       </c>
     </row>
     <row r="658">
-      <c r="A658" s="79"/>
-      <c r="B658" s="80"/>
+      <c r="A658" s="73"/>
+      <c r="B658" s="74"/>
       <c r="C658" s="34"/>
       <c r="D658" s="34"/>
       <c r="E658" s="34"/>
@@ -46338,8 +46316,8 @@
       </c>
     </row>
     <row r="659">
-      <c r="A659" s="79"/>
-      <c r="B659" s="80"/>
+      <c r="A659" s="73"/>
+      <c r="B659" s="74"/>
       <c r="C659" s="34"/>
       <c r="D659" s="34"/>
       <c r="E659" s="34"/>
@@ -46364,8 +46342,8 @@
       </c>
     </row>
     <row r="660">
-      <c r="A660" s="79"/>
-      <c r="B660" s="80"/>
+      <c r="A660" s="73"/>
+      <c r="B660" s="74"/>
       <c r="C660" s="34"/>
       <c r="D660" s="34"/>
       <c r="E660" s="34"/>
@@ -46390,8 +46368,8 @@
       </c>
     </row>
     <row r="661">
-      <c r="A661" s="79"/>
-      <c r="B661" s="80"/>
+      <c r="A661" s="73"/>
+      <c r="B661" s="74"/>
       <c r="C661" s="34"/>
       <c r="D661" s="34"/>
       <c r="E661" s="34"/>
@@ -46416,8 +46394,8 @@
       </c>
     </row>
     <row r="662">
-      <c r="A662" s="79"/>
-      <c r="B662" s="80"/>
+      <c r="A662" s="73"/>
+      <c r="B662" s="74"/>
       <c r="C662" s="34"/>
       <c r="D662" s="34"/>
       <c r="E662" s="34"/>
@@ -46442,8 +46420,8 @@
       </c>
     </row>
     <row r="663">
-      <c r="A663" s="79"/>
-      <c r="B663" s="80"/>
+      <c r="A663" s="73"/>
+      <c r="B663" s="74"/>
       <c r="C663" s="34"/>
       <c r="D663" s="34"/>
       <c r="E663" s="34"/>
@@ -46468,8 +46446,8 @@
       </c>
     </row>
     <row r="664">
-      <c r="A664" s="79"/>
-      <c r="B664" s="80"/>
+      <c r="A664" s="73"/>
+      <c r="B664" s="74"/>
       <c r="C664" s="34"/>
       <c r="D664" s="34"/>
       <c r="E664" s="34"/>
@@ -46494,8 +46472,8 @@
       </c>
     </row>
     <row r="665">
-      <c r="A665" s="79"/>
-      <c r="B665" s="80"/>
+      <c r="A665" s="73"/>
+      <c r="B665" s="74"/>
       <c r="C665" s="34"/>
       <c r="D665" s="34"/>
       <c r="E665" s="34"/>
@@ -46520,8 +46498,8 @@
       </c>
     </row>
     <row r="666">
-      <c r="A666" s="79"/>
-      <c r="B666" s="80"/>
+      <c r="A666" s="73"/>
+      <c r="B666" s="74"/>
       <c r="C666" s="34"/>
       <c r="D666" s="34"/>
       <c r="E666" s="34"/>
@@ -46546,8 +46524,8 @@
       </c>
     </row>
     <row r="667">
-      <c r="A667" s="79"/>
-      <c r="B667" s="80"/>
+      <c r="A667" s="73"/>
+      <c r="B667" s="74"/>
       <c r="C667" s="34"/>
       <c r="D667" s="34"/>
       <c r="E667" s="34"/>
@@ -46572,8 +46550,8 @@
       </c>
     </row>
     <row r="668">
-      <c r="A668" s="79"/>
-      <c r="B668" s="80"/>
+      <c r="A668" s="73"/>
+      <c r="B668" s="74"/>
       <c r="C668" s="34"/>
       <c r="D668" s="34"/>
       <c r="E668" s="34"/>
@@ -46598,8 +46576,8 @@
       </c>
     </row>
     <row r="669">
-      <c r="A669" s="79"/>
-      <c r="B669" s="80"/>
+      <c r="A669" s="73"/>
+      <c r="B669" s="74"/>
       <c r="C669" s="34"/>
       <c r="D669" s="34"/>
       <c r="E669" s="34"/>
@@ -46624,8 +46602,8 @@
       </c>
     </row>
     <row r="670">
-      <c r="A670" s="79"/>
-      <c r="B670" s="80"/>
+      <c r="A670" s="73"/>
+      <c r="B670" s="74"/>
       <c r="C670" s="34"/>
       <c r="D670" s="34"/>
       <c r="E670" s="34"/>
@@ -46650,8 +46628,8 @@
       </c>
     </row>
     <row r="671">
-      <c r="A671" s="79"/>
-      <c r="B671" s="80"/>
+      <c r="A671" s="73"/>
+      <c r="B671" s="74"/>
       <c r="C671" s="34"/>
       <c r="D671" s="34"/>
       <c r="E671" s="34"/>
@@ -46676,8 +46654,8 @@
       </c>
     </row>
     <row r="672">
-      <c r="A672" s="79"/>
-      <c r="B672" s="80"/>
+      <c r="A672" s="73"/>
+      <c r="B672" s="74"/>
       <c r="C672" s="34"/>
       <c r="D672" s="34"/>
       <c r="E672" s="34"/>
@@ -46702,8 +46680,8 @@
       </c>
     </row>
     <row r="673">
-      <c r="A673" s="79"/>
-      <c r="B673" s="80"/>
+      <c r="A673" s="73"/>
+      <c r="B673" s="74"/>
       <c r="C673" s="34"/>
       <c r="D673" s="34"/>
       <c r="E673" s="34"/>
@@ -46728,8 +46706,8 @@
       </c>
     </row>
     <row r="674">
-      <c r="A674" s="79"/>
-      <c r="B674" s="80"/>
+      <c r="A674" s="73"/>
+      <c r="B674" s="74"/>
       <c r="C674" s="34"/>
       <c r="D674" s="34"/>
       <c r="E674" s="34"/>
@@ -46754,8 +46732,8 @@
       </c>
     </row>
     <row r="675">
-      <c r="A675" s="79"/>
-      <c r="B675" s="80"/>
+      <c r="A675" s="73"/>
+      <c r="B675" s="74"/>
       <c r="C675" s="34"/>
       <c r="D675" s="34"/>
       <c r="E675" s="34"/>
@@ -46780,8 +46758,8 @@
       </c>
     </row>
     <row r="676">
-      <c r="A676" s="79"/>
-      <c r="B676" s="80"/>
+      <c r="A676" s="73"/>
+      <c r="B676" s="74"/>
       <c r="C676" s="34"/>
       <c r="D676" s="34"/>
       <c r="E676" s="34"/>
@@ -46806,8 +46784,8 @@
       </c>
     </row>
     <row r="677">
-      <c r="A677" s="79"/>
-      <c r="B677" s="80"/>
+      <c r="A677" s="73"/>
+      <c r="B677" s="74"/>
       <c r="C677" s="34"/>
       <c r="D677" s="34"/>
       <c r="E677" s="34"/>
@@ -46832,8 +46810,8 @@
       </c>
     </row>
     <row r="678">
-      <c r="A678" s="79"/>
-      <c r="B678" s="80"/>
+      <c r="A678" s="73"/>
+      <c r="B678" s="74"/>
       <c r="C678" s="34"/>
       <c r="D678" s="34"/>
       <c r="E678" s="34"/>
@@ -46858,8 +46836,8 @@
       </c>
     </row>
     <row r="679">
-      <c r="A679" s="79"/>
-      <c r="B679" s="80"/>
+      <c r="A679" s="73"/>
+      <c r="B679" s="74"/>
       <c r="C679" s="34"/>
       <c r="D679" s="34"/>
       <c r="E679" s="34"/>
@@ -46884,8 +46862,8 @@
       </c>
     </row>
     <row r="680">
-      <c r="A680" s="79"/>
-      <c r="B680" s="80"/>
+      <c r="A680" s="73"/>
+      <c r="B680" s="74"/>
       <c r="C680" s="34"/>
       <c r="D680" s="34"/>
       <c r="E680" s="34"/>
@@ -46910,8 +46888,8 @@
       </c>
     </row>
     <row r="681">
-      <c r="A681" s="79"/>
-      <c r="B681" s="80"/>
+      <c r="A681" s="73"/>
+      <c r="B681" s="74"/>
       <c r="C681" s="34"/>
       <c r="D681" s="34"/>
       <c r="E681" s="34"/>
@@ -46936,8 +46914,8 @@
       </c>
     </row>
     <row r="682">
-      <c r="A682" s="79"/>
-      <c r="B682" s="80"/>
+      <c r="A682" s="73"/>
+      <c r="B682" s="74"/>
       <c r="C682" s="34"/>
       <c r="D682" s="34"/>
       <c r="E682" s="34"/>
@@ -46962,8 +46940,8 @@
       </c>
     </row>
     <row r="683">
-      <c r="A683" s="79"/>
-      <c r="B683" s="80"/>
+      <c r="A683" s="73"/>
+      <c r="B683" s="74"/>
       <c r="C683" s="34"/>
       <c r="D683" s="34"/>
       <c r="E683" s="34"/>
@@ -46988,8 +46966,8 @@
       </c>
     </row>
     <row r="684">
-      <c r="A684" s="79"/>
-      <c r="B684" s="80"/>
+      <c r="A684" s="73"/>
+      <c r="B684" s="74"/>
       <c r="C684" s="34"/>
       <c r="D684" s="34"/>
       <c r="E684" s="34"/>
@@ -47014,8 +46992,8 @@
       </c>
     </row>
     <row r="685">
-      <c r="A685" s="79"/>
-      <c r="B685" s="80"/>
+      <c r="A685" s="73"/>
+      <c r="B685" s="74"/>
       <c r="C685" s="34"/>
       <c r="D685" s="34"/>
       <c r="E685" s="34"/>
@@ -47040,8 +47018,8 @@
       </c>
     </row>
     <row r="686">
-      <c r="A686" s="79"/>
-      <c r="B686" s="80"/>
+      <c r="A686" s="73"/>
+      <c r="B686" s="74"/>
       <c r="C686" s="34"/>
       <c r="D686" s="34"/>
       <c r="E686" s="34"/>
@@ -47066,8 +47044,8 @@
       </c>
     </row>
     <row r="687">
-      <c r="A687" s="79"/>
-      <c r="B687" s="80"/>
+      <c r="A687" s="73"/>
+      <c r="B687" s="74"/>
       <c r="C687" s="34"/>
       <c r="D687" s="34"/>
       <c r="E687" s="34"/>
@@ -47092,8 +47070,8 @@
       </c>
     </row>
     <row r="688">
-      <c r="A688" s="79"/>
-      <c r="B688" s="80"/>
+      <c r="A688" s="73"/>
+      <c r="B688" s="74"/>
       <c r="C688" s="34"/>
       <c r="D688" s="34"/>
       <c r="E688" s="34"/>
@@ -47118,8 +47096,8 @@
       </c>
     </row>
     <row r="689">
-      <c r="A689" s="79"/>
-      <c r="B689" s="80"/>
+      <c r="A689" s="73"/>
+      <c r="B689" s="74"/>
       <c r="C689" s="34"/>
       <c r="D689" s="34"/>
       <c r="E689" s="34"/>
@@ -47144,8 +47122,8 @@
       </c>
     </row>
     <row r="690">
-      <c r="A690" s="79"/>
-      <c r="B690" s="80"/>
+      <c r="A690" s="73"/>
+      <c r="B690" s="74"/>
       <c r="C690" s="34"/>
       <c r="D690" s="34"/>
       <c r="E690" s="34"/>
@@ -47170,8 +47148,8 @@
       </c>
     </row>
     <row r="691">
-      <c r="A691" s="79"/>
-      <c r="B691" s="80"/>
+      <c r="A691" s="73"/>
+      <c r="B691" s="74"/>
       <c r="C691" s="34"/>
       <c r="D691" s="34"/>
       <c r="E691" s="34"/>
@@ -47196,8 +47174,8 @@
       </c>
     </row>
     <row r="692">
-      <c r="A692" s="79"/>
-      <c r="B692" s="80"/>
+      <c r="A692" s="73"/>
+      <c r="B692" s="74"/>
       <c r="C692" s="34"/>
       <c r="D692" s="34"/>
       <c r="E692" s="34"/>
@@ -47222,8 +47200,8 @@
       </c>
     </row>
     <row r="693">
-      <c r="A693" s="79"/>
-      <c r="B693" s="80"/>
+      <c r="A693" s="73"/>
+      <c r="B693" s="74"/>
       <c r="C693" s="34"/>
       <c r="D693" s="34"/>
       <c r="E693" s="34"/>
@@ -47248,8 +47226,8 @@
       </c>
     </row>
     <row r="694">
-      <c r="A694" s="79"/>
-      <c r="B694" s="80"/>
+      <c r="A694" s="73"/>
+      <c r="B694" s="74"/>
       <c r="C694" s="34"/>
       <c r="D694" s="34"/>
       <c r="E694" s="34"/>
@@ -47274,8 +47252,8 @@
       </c>
     </row>
     <row r="695">
-      <c r="A695" s="79"/>
-      <c r="B695" s="80"/>
+      <c r="A695" s="73"/>
+      <c r="B695" s="74"/>
       <c r="C695" s="34"/>
       <c r="D695" s="34"/>
       <c r="E695" s="34"/>
@@ -47300,8 +47278,8 @@
       </c>
     </row>
     <row r="696">
-      <c r="A696" s="79"/>
-      <c r="B696" s="80"/>
+      <c r="A696" s="73"/>
+      <c r="B696" s="74"/>
       <c r="C696" s="34"/>
       <c r="D696" s="34"/>
       <c r="E696" s="34"/>
@@ -47326,8 +47304,8 @@
       </c>
     </row>
     <row r="697">
-      <c r="A697" s="79"/>
-      <c r="B697" s="80"/>
+      <c r="A697" s="73"/>
+      <c r="B697" s="74"/>
       <c r="C697" s="34"/>
       <c r="D697" s="34"/>
       <c r="E697" s="34"/>
@@ -47352,8 +47330,8 @@
       </c>
     </row>
     <row r="698">
-      <c r="A698" s="79"/>
-      <c r="B698" s="80"/>
+      <c r="A698" s="73"/>
+      <c r="B698" s="74"/>
       <c r="C698" s="34"/>
       <c r="D698" s="34"/>
       <c r="E698" s="34"/>
@@ -47378,8 +47356,8 @@
       </c>
     </row>
     <row r="699">
-      <c r="A699" s="79"/>
-      <c r="B699" s="80"/>
+      <c r="A699" s="73"/>
+      <c r="B699" s="74"/>
       <c r="C699" s="34"/>
       <c r="D699" s="34"/>
       <c r="E699" s="34"/>
@@ -47404,8 +47382,8 @@
       </c>
     </row>
     <row r="700">
-      <c r="A700" s="79"/>
-      <c r="B700" s="80"/>
+      <c r="A700" s="73"/>
+      <c r="B700" s="74"/>
       <c r="C700" s="34"/>
       <c r="D700" s="34"/>
       <c r="E700" s="34"/>
@@ -47430,8 +47408,8 @@
       </c>
     </row>
     <row r="701">
-      <c r="A701" s="79"/>
-      <c r="B701" s="80"/>
+      <c r="A701" s="73"/>
+      <c r="B701" s="74"/>
       <c r="C701" s="34"/>
       <c r="D701" s="34"/>
       <c r="E701" s="34"/>

</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201126
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -571,7 +571,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6971" uniqueCount="2309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7031" uniqueCount="2320">
   <si>
     <t>案例</t>
   </si>
@@ -8401,6 +8401,41 @@
   </si>
   <si>
     <t>新增1例境外移入COVID-19病例，為自迦納返國者</t>
+  </si>
+  <si>
+    <t>#620</t>
+  </si>
+  <si>
+    <t>-11/10 印尼→台灣</t>
+  </si>
+  <si>
+    <t>11/23 採檢
+11/25 確診</t>
+  </si>
+  <si>
+    <t>新增5例境外移入COVID-19病例，為印尼籍與菲律賓籍移工</t>
+  </si>
+  <si>
+    <t>#621</t>
+  </si>
+  <si>
+    <t>#622</t>
+  </si>
+  <si>
+    <t>#623</t>
+  </si>
+  <si>
+    <t>-11/10 菲律賓→台灣</t>
+  </si>
+  <si>
+    <t>#624</t>
+  </si>
+  <si>
+    <t>-11/11 菲律賓→台灣</t>
+  </si>
+  <si>
+    <t>11/24 採檢
+11/25 確診</t>
   </si>
 </sst>
 </file>
@@ -45328,133 +45363,273 @@
       </c>
     </row>
     <row r="621">
-      <c r="A621" s="73"/>
-      <c r="B621" s="74"/>
-      <c r="C621" s="34"/>
-      <c r="D621" s="34"/>
-      <c r="E621" s="34"/>
+      <c r="A621" s="16" t="s">
+        <v>2309</v>
+      </c>
+      <c r="B621" s="6">
+        <v>44160.0</v>
+      </c>
+      <c r="C621" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D621" s="7" t="s">
+        <v>2151</v>
+      </c>
+      <c r="E621" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F621" s="34"/>
-      <c r="G621" s="34"/>
-      <c r="H621" s="21"/>
-      <c r="I621" s="19"/>
-      <c r="J621" s="10"/>
-      <c r="K621" s="22"/>
-      <c r="L621" s="23"/>
-      <c r="M621" s="22"/>
+      <c r="G621" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H621" s="8" t="s">
+        <v>2310</v>
+      </c>
+      <c r="I621" s="9">
+        <v>44145.0</v>
+      </c>
+      <c r="J621" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K621" s="13" t="s">
+        <v>2311</v>
+      </c>
+      <c r="L621" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M621" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N621" s="25"/>
-      <c r="O621" s="21"/>
+      <c r="O621" s="8" t="s">
+        <v>85</v>
+      </c>
       <c r="P621" s="21"/>
       <c r="Q621" s="19"/>
       <c r="R621" s="19"/>
-      <c r="S621" s="20"/>
+      <c r="S621" s="61" t="s">
+        <v>2312</v>
+      </c>
       <c r="T621" s="20"/>
       <c r="U621" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#620</v>
       </c>
     </row>
     <row r="622">
-      <c r="A622" s="73"/>
-      <c r="B622" s="74"/>
-      <c r="C622" s="34"/>
-      <c r="D622" s="34"/>
-      <c r="E622" s="34"/>
+      <c r="A622" s="16" t="s">
+        <v>2313</v>
+      </c>
+      <c r="B622" s="6">
+        <v>44160.0</v>
+      </c>
+      <c r="C622" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D622" s="7" t="s">
+        <v>2151</v>
+      </c>
+      <c r="E622" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F622" s="34"/>
-      <c r="G622" s="34"/>
-      <c r="H622" s="21"/>
-      <c r="I622" s="19"/>
-      <c r="J622" s="10"/>
-      <c r="K622" s="22"/>
-      <c r="L622" s="23"/>
-      <c r="M622" s="22"/>
+      <c r="G622" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H622" s="8" t="s">
+        <v>2310</v>
+      </c>
+      <c r="I622" s="9">
+        <v>44145.0</v>
+      </c>
+      <c r="J622" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K622" s="13" t="s">
+        <v>2311</v>
+      </c>
+      <c r="L622" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M622" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N622" s="25"/>
-      <c r="O622" s="21"/>
+      <c r="O622" s="8" t="s">
+        <v>85</v>
+      </c>
       <c r="P622" s="21"/>
       <c r="Q622" s="19"/>
       <c r="R622" s="19"/>
-      <c r="S622" s="20"/>
+      <c r="S622" s="61" t="s">
+        <v>2312</v>
+      </c>
       <c r="T622" s="20"/>
       <c r="U622" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#621</v>
       </c>
     </row>
     <row r="623">
-      <c r="A623" s="73"/>
-      <c r="B623" s="74"/>
-      <c r="C623" s="34"/>
-      <c r="D623" s="34"/>
-      <c r="E623" s="34"/>
+      <c r="A623" s="16" t="s">
+        <v>2314</v>
+      </c>
+      <c r="B623" s="6">
+        <v>44160.0</v>
+      </c>
+      <c r="C623" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D623" s="7" t="s">
+        <v>2151</v>
+      </c>
+      <c r="E623" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F623" s="34"/>
-      <c r="G623" s="34"/>
-      <c r="H623" s="21"/>
-      <c r="I623" s="19"/>
-      <c r="J623" s="10"/>
-      <c r="K623" s="22"/>
-      <c r="L623" s="23"/>
-      <c r="M623" s="22"/>
+      <c r="G623" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H623" s="8" t="s">
+        <v>2310</v>
+      </c>
+      <c r="I623" s="9">
+        <v>44145.0</v>
+      </c>
+      <c r="J623" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K623" s="13" t="s">
+        <v>2311</v>
+      </c>
+      <c r="L623" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M623" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N623" s="25"/>
-      <c r="O623" s="21"/>
+      <c r="O623" s="8" t="s">
+        <v>85</v>
+      </c>
       <c r="P623" s="21"/>
       <c r="Q623" s="19"/>
       <c r="R623" s="19"/>
-      <c r="S623" s="20"/>
+      <c r="S623" s="61" t="s">
+        <v>2312</v>
+      </c>
       <c r="T623" s="20"/>
       <c r="U623" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#622</v>
       </c>
     </row>
     <row r="624">
-      <c r="A624" s="73"/>
-      <c r="B624" s="74"/>
-      <c r="C624" s="34"/>
-      <c r="D624" s="34"/>
-      <c r="E624" s="34"/>
+      <c r="A624" s="16" t="s">
+        <v>2315</v>
+      </c>
+      <c r="B624" s="6">
+        <v>44160.0</v>
+      </c>
+      <c r="C624" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D624" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E624" s="7" t="s">
+        <v>205</v>
+      </c>
       <c r="F624" s="34"/>
-      <c r="G624" s="34"/>
-      <c r="H624" s="21"/>
-      <c r="I624" s="19"/>
-      <c r="J624" s="10"/>
-      <c r="K624" s="22"/>
-      <c r="L624" s="23"/>
-      <c r="M624" s="22"/>
+      <c r="G624" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H624" s="8" t="s">
+        <v>2316</v>
+      </c>
+      <c r="I624" s="9">
+        <v>44145.0</v>
+      </c>
+      <c r="J624" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K624" s="13" t="s">
+        <v>2311</v>
+      </c>
+      <c r="L624" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M624" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N624" s="25"/>
-      <c r="O624" s="21"/>
+      <c r="O624" s="8" t="s">
+        <v>85</v>
+      </c>
       <c r="P624" s="21"/>
       <c r="Q624" s="19"/>
       <c r="R624" s="19"/>
-      <c r="S624" s="20"/>
+      <c r="S624" s="61" t="s">
+        <v>2312</v>
+      </c>
       <c r="T624" s="20"/>
       <c r="U624" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#623</v>
       </c>
     </row>
     <row r="625">
-      <c r="A625" s="73"/>
-      <c r="B625" s="74"/>
-      <c r="C625" s="34"/>
-      <c r="D625" s="34"/>
-      <c r="E625" s="34"/>
+      <c r="A625" s="16" t="s">
+        <v>2317</v>
+      </c>
+      <c r="B625" s="6">
+        <v>44160.0</v>
+      </c>
+      <c r="C625" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D625" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E625" s="7" t="s">
+        <v>205</v>
+      </c>
       <c r="F625" s="34"/>
-      <c r="G625" s="34"/>
-      <c r="H625" s="21"/>
-      <c r="I625" s="19"/>
-      <c r="J625" s="10"/>
-      <c r="K625" s="22"/>
-      <c r="L625" s="23"/>
-      <c r="M625" s="22"/>
+      <c r="G625" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H625" s="8" t="s">
+        <v>2318</v>
+      </c>
+      <c r="I625" s="9">
+        <v>44146.0</v>
+      </c>
+      <c r="J625" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K625" s="13" t="s">
+        <v>2319</v>
+      </c>
+      <c r="L625" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M625" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N625" s="25"/>
-      <c r="O625" s="21"/>
+      <c r="O625" s="8" t="s">
+        <v>85</v>
+      </c>
       <c r="P625" s="21"/>
       <c r="Q625" s="19"/>
       <c r="R625" s="19"/>
-      <c r="S625" s="20"/>
+      <c r="S625" s="61" t="s">
+        <v>2312</v>
+      </c>
       <c r="T625" s="20"/>
       <c r="U625" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#624</v>
       </c>
     </row>
     <row r="626">
@@ -47996,15 +48171,20 @@
     <hyperlink r:id="rId180" ref="S618"/>
     <hyperlink r:id="rId181" ref="S619"/>
     <hyperlink r:id="rId182" ref="S620"/>
+    <hyperlink r:id="rId183" ref="S621"/>
+    <hyperlink r:id="rId184" ref="S622"/>
+    <hyperlink r:id="rId185" ref="S623"/>
+    <hyperlink r:id="rId186" ref="S624"/>
+    <hyperlink r:id="rId187" ref="S625"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId183"/>
-  <legacyDrawing r:id="rId184"/>
+  <drawing r:id="rId188"/>
+  <legacyDrawing r:id="rId189"/>
   <tableParts count="2">
-    <tablePart r:id="rId187"/>
-    <tablePart r:id="rId188"/>
+    <tablePart r:id="rId192"/>
+    <tablePart r:id="rId193"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201127
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -571,7 +571,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7031" uniqueCount="2320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7235" uniqueCount="2351">
   <si>
     <t>案例</t>
   </si>
@@ -8437,6 +8437,103 @@
     <t>11/24 採檢
 11/25 確診</t>
   </si>
+  <si>
+    <t>#625</t>
+  </si>
+  <si>
+    <t>8月下旬-11/24 美國</t>
+  </si>
+  <si>
+    <t>美國就學</t>
+  </si>
+  <si>
+    <t>國內新增2例境外移入COVID-19病例，分自美國、印尼入境</t>
+  </si>
+  <si>
+    <t>#626</t>
+  </si>
+  <si>
+    <t>-11/9 印尼→台灣</t>
+  </si>
+  <si>
+    <t>輕微頭痛 咳嗽 喉嚨痛 聲音沙啞</t>
+  </si>
+  <si>
+    <t>因工作不定期來臺(前次自臺灣出境時間為今年2月)，本次因處理私人事務及探訪友人，於11月9日再度來臺，入境時無症狀
+個案於防疫旅館居家檢疫期間，11月22日起陸續出現輕微頭痛、咳嗽、喉嚨痛及聲音沙啞等症狀，但自覺症狀輕微，檢疫期間均回報無症狀
+11月24日檢疫期滿後前往探訪友人，因仍有不適症狀，同日就醫採檢</t>
+  </si>
+  <si>
+    <t>#627</t>
+  </si>
+  <si>
+    <t>-11/11 印尼→台灣</t>
+  </si>
+  <si>
+    <t>11/25 採檢
+11/27 確診</t>
+  </si>
+  <si>
+    <t>新增14例境外移入COVID-19病例，自印尼及美國入境</t>
+  </si>
+  <si>
+    <t>#628</t>
+  </si>
+  <si>
+    <t>移工 與#607同班機</t>
+  </si>
+  <si>
+    <t>#629</t>
+  </si>
+  <si>
+    <t>#630</t>
+  </si>
+  <si>
+    <t>#631</t>
+  </si>
+  <si>
+    <t>#632</t>
+  </si>
+  <si>
+    <t>喉嚨不適 流鼻水 鼻塞</t>
+  </si>
+  <si>
+    <t>移工 與#607同班機
+曾於11月19日通報有喉嚨不適症狀，自認症狀輕微未就醫，11月23日出現流鼻水、鼻塞情形但未通報</t>
+  </si>
+  <si>
+    <t>#633</t>
+  </si>
+  <si>
+    <t>#634</t>
+  </si>
+  <si>
+    <t>#635</t>
+  </si>
+  <si>
+    <t>#636</t>
+  </si>
+  <si>
+    <t>#637</t>
+  </si>
+  <si>
+    <t>#638</t>
+  </si>
+  <si>
+    <t>#639</t>
+  </si>
+  <si>
+    <t>#640</t>
+  </si>
+  <si>
+    <t>2019/9月-11/20 美國</t>
+  </si>
+  <si>
+    <t>疲倦 喉嚨乾 喉嚨痛</t>
+  </si>
+  <si>
+    <t>長期在美國工作，返臺探親</t>
+  </si>
 </sst>
 </file>
 
@@ -8446,7 +8543,7 @@
     <numFmt numFmtId="164" formatCode="mm&quot;月&quot;dd&quot;日 &quot;dddd"/>
     <numFmt numFmtId="165" formatCode="m/d"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="20">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -8527,6 +8624,10 @@
       <u/>
       <color rgb="FFFFFFFF"/>
     </font>
+    <font/>
+    <font>
+      <color rgb="FF000000"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -8572,7 +8673,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="82">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -8791,6 +8892,27 @@
     </xf>
     <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="18" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="19" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
@@ -45633,424 +45755,904 @@
       </c>
     </row>
     <row r="626">
-      <c r="A626" s="73"/>
-      <c r="B626" s="74"/>
-      <c r="C626" s="34"/>
-      <c r="D626" s="34"/>
-      <c r="E626" s="34"/>
+      <c r="A626" s="16" t="s">
+        <v>2320</v>
+      </c>
+      <c r="B626" s="6">
+        <v>44161.0</v>
+      </c>
+      <c r="C626" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D626" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E626" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F626" s="34"/>
-      <c r="G626" s="34"/>
-      <c r="H626" s="21"/>
-      <c r="I626" s="19"/>
-      <c r="J626" s="10"/>
-      <c r="K626" s="22"/>
-      <c r="L626" s="23"/>
-      <c r="M626" s="22"/>
+      <c r="G626" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H626" s="8" t="s">
+        <v>2321</v>
+      </c>
+      <c r="I626" s="9">
+        <v>44159.0</v>
+      </c>
+      <c r="J626" s="10">
+        <v>44155.0</v>
+      </c>
+      <c r="K626" s="13" t="s">
+        <v>2319</v>
+      </c>
+      <c r="L626" s="12" t="s">
+        <v>363</v>
+      </c>
+      <c r="M626" s="13" t="s">
+        <v>364</v>
+      </c>
       <c r="N626" s="25"/>
-      <c r="O626" s="21"/>
-      <c r="P626" s="21"/>
+      <c r="O626" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P626" s="8" t="s">
+        <v>2322</v>
+      </c>
       <c r="Q626" s="19"/>
       <c r="R626" s="19"/>
-      <c r="S626" s="20"/>
+      <c r="S626" s="61" t="s">
+        <v>2323</v>
+      </c>
       <c r="T626" s="20"/>
       <c r="U626" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#625</v>
       </c>
     </row>
     <row r="627">
-      <c r="A627" s="73"/>
-      <c r="B627" s="74"/>
-      <c r="C627" s="34"/>
-      <c r="D627" s="34"/>
-      <c r="E627" s="34"/>
+      <c r="A627" s="16" t="s">
+        <v>2324</v>
+      </c>
+      <c r="B627" s="6">
+        <v>44161.0</v>
+      </c>
+      <c r="C627" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D627" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E627" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F627" s="34"/>
-      <c r="G627" s="34"/>
-      <c r="H627" s="21"/>
-      <c r="I627" s="19"/>
-      <c r="J627" s="10"/>
-      <c r="K627" s="22"/>
-      <c r="L627" s="23"/>
-      <c r="M627" s="22"/>
+      <c r="G627" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H627" s="8" t="s">
+        <v>2325</v>
+      </c>
+      <c r="I627" s="9">
+        <v>44144.0</v>
+      </c>
+      <c r="J627" s="10">
+        <v>44157.0</v>
+      </c>
+      <c r="K627" s="13" t="s">
+        <v>2319</v>
+      </c>
+      <c r="L627" s="12" t="s">
+        <v>438</v>
+      </c>
+      <c r="M627" s="13" t="s">
+        <v>2326</v>
+      </c>
       <c r="N627" s="25"/>
-      <c r="O627" s="21"/>
-      <c r="P627" s="21"/>
+      <c r="O627" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P627" s="8" t="s">
+        <v>2327</v>
+      </c>
       <c r="Q627" s="19"/>
       <c r="R627" s="19"/>
-      <c r="S627" s="20"/>
+      <c r="S627" s="61" t="s">
+        <v>2323</v>
+      </c>
       <c r="T627" s="20"/>
       <c r="U627" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#626</v>
       </c>
     </row>
     <row r="628">
-      <c r="A628" s="73"/>
-      <c r="B628" s="74"/>
-      <c r="C628" s="34"/>
-      <c r="D628" s="34"/>
-      <c r="E628" s="34"/>
+      <c r="A628" s="73" t="s">
+        <v>2328</v>
+      </c>
+      <c r="B628" s="6">
+        <v>44162.0</v>
+      </c>
+      <c r="C628" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D628" s="74" t="s">
+        <v>2139</v>
+      </c>
+      <c r="E628" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F628" s="34"/>
-      <c r="G628" s="34"/>
-      <c r="H628" s="21"/>
-      <c r="I628" s="19"/>
-      <c r="J628" s="10"/>
-      <c r="K628" s="22"/>
-      <c r="L628" s="23"/>
-      <c r="M628" s="22"/>
+      <c r="G628" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H628" s="75" t="s">
+        <v>2329</v>
+      </c>
+      <c r="I628" s="76">
+        <v>44146.0</v>
+      </c>
+      <c r="J628" s="77" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K628" s="78" t="s">
+        <v>2330</v>
+      </c>
+      <c r="L628" s="77" t="s">
+        <v>426</v>
+      </c>
+      <c r="M628" s="78" t="s">
+        <v>1442</v>
+      </c>
       <c r="N628" s="25"/>
-      <c r="O628" s="21"/>
-      <c r="P628" s="21"/>
+      <c r="O628" s="75" t="s">
+        <v>85</v>
+      </c>
+      <c r="P628" s="75" t="s">
+        <v>1777</v>
+      </c>
       <c r="Q628" s="19"/>
       <c r="R628" s="19"/>
-      <c r="S628" s="20"/>
+      <c r="S628" s="61" t="s">
+        <v>2331</v>
+      </c>
       <c r="T628" s="20"/>
       <c r="U628" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#627</v>
       </c>
     </row>
     <row r="629">
-      <c r="A629" s="73"/>
-      <c r="B629" s="74"/>
-      <c r="C629" s="34"/>
-      <c r="D629" s="34"/>
-      <c r="E629" s="34"/>
+      <c r="A629" s="73" t="s">
+        <v>2332</v>
+      </c>
+      <c r="B629" s="6">
+        <v>44162.0</v>
+      </c>
+      <c r="C629" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D629" s="74" t="s">
+        <v>2139</v>
+      </c>
+      <c r="E629" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F629" s="34"/>
-      <c r="G629" s="34"/>
-      <c r="H629" s="21"/>
-      <c r="I629" s="19"/>
-      <c r="J629" s="10"/>
-      <c r="K629" s="22"/>
-      <c r="L629" s="23"/>
-      <c r="M629" s="22"/>
+      <c r="G629" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H629" s="75" t="s">
+        <v>2263</v>
+      </c>
+      <c r="I629" s="76">
+        <v>44147.0</v>
+      </c>
+      <c r="J629" s="77" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K629" s="78" t="s">
+        <v>2330</v>
+      </c>
+      <c r="L629" s="77" t="s">
+        <v>426</v>
+      </c>
+      <c r="M629" s="78" t="s">
+        <v>1442</v>
+      </c>
       <c r="N629" s="25"/>
-      <c r="O629" s="21"/>
-      <c r="P629" s="21"/>
+      <c r="O629" s="75" t="s">
+        <v>85</v>
+      </c>
+      <c r="P629" s="75" t="s">
+        <v>2333</v>
+      </c>
       <c r="Q629" s="19"/>
       <c r="R629" s="19"/>
-      <c r="S629" s="20"/>
+      <c r="S629" s="61" t="s">
+        <v>2331</v>
+      </c>
       <c r="T629" s="20"/>
       <c r="U629" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#628</v>
       </c>
     </row>
     <row r="630">
-      <c r="A630" s="73"/>
-      <c r="B630" s="74"/>
-      <c r="C630" s="34"/>
-      <c r="D630" s="34"/>
-      <c r="E630" s="34"/>
+      <c r="A630" s="73" t="s">
+        <v>2334</v>
+      </c>
+      <c r="B630" s="6">
+        <v>44162.0</v>
+      </c>
+      <c r="C630" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D630" s="74" t="s">
+        <v>2139</v>
+      </c>
+      <c r="E630" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F630" s="34"/>
-      <c r="G630" s="34"/>
-      <c r="H630" s="21"/>
-      <c r="I630" s="19"/>
-      <c r="J630" s="10"/>
-      <c r="K630" s="22"/>
-      <c r="L630" s="23"/>
-      <c r="M630" s="22"/>
+      <c r="G630" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H630" s="75" t="s">
+        <v>2263</v>
+      </c>
+      <c r="I630" s="76">
+        <v>44147.0</v>
+      </c>
+      <c r="J630" s="77" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K630" s="78" t="s">
+        <v>2330</v>
+      </c>
+      <c r="L630" s="77" t="s">
+        <v>426</v>
+      </c>
+      <c r="M630" s="78" t="s">
+        <v>1442</v>
+      </c>
       <c r="N630" s="25"/>
-      <c r="O630" s="21"/>
-      <c r="P630" s="21"/>
+      <c r="O630" s="75" t="s">
+        <v>85</v>
+      </c>
+      <c r="P630" s="75" t="s">
+        <v>2333</v>
+      </c>
       <c r="Q630" s="19"/>
       <c r="R630" s="19"/>
-      <c r="S630" s="20"/>
+      <c r="S630" s="61" t="s">
+        <v>2331</v>
+      </c>
       <c r="T630" s="20"/>
       <c r="U630" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#629</v>
       </c>
     </row>
     <row r="631">
-      <c r="A631" s="73"/>
-      <c r="B631" s="74"/>
-      <c r="C631" s="34"/>
-      <c r="D631" s="34"/>
-      <c r="E631" s="34"/>
+      <c r="A631" s="73" t="s">
+        <v>2335</v>
+      </c>
+      <c r="B631" s="6">
+        <v>44162.0</v>
+      </c>
+      <c r="C631" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D631" s="74" t="s">
+        <v>2139</v>
+      </c>
+      <c r="E631" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F631" s="34"/>
-      <c r="G631" s="34"/>
-      <c r="H631" s="21"/>
-      <c r="I631" s="19"/>
-      <c r="J631" s="10"/>
-      <c r="K631" s="22"/>
-      <c r="L631" s="23"/>
-      <c r="M631" s="22"/>
+      <c r="G631" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H631" s="75" t="s">
+        <v>2263</v>
+      </c>
+      <c r="I631" s="76">
+        <v>44147.0</v>
+      </c>
+      <c r="J631" s="77" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K631" s="78" t="s">
+        <v>2330</v>
+      </c>
+      <c r="L631" s="77" t="s">
+        <v>426</v>
+      </c>
+      <c r="M631" s="78" t="s">
+        <v>1442</v>
+      </c>
       <c r="N631" s="25"/>
-      <c r="O631" s="21"/>
-      <c r="P631" s="21"/>
+      <c r="O631" s="75" t="s">
+        <v>85</v>
+      </c>
+      <c r="P631" s="75" t="s">
+        <v>2333</v>
+      </c>
       <c r="Q631" s="19"/>
       <c r="R631" s="19"/>
-      <c r="S631" s="20"/>
+      <c r="S631" s="61" t="s">
+        <v>2331</v>
+      </c>
       <c r="T631" s="20"/>
       <c r="U631" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#630</v>
       </c>
     </row>
     <row r="632">
-      <c r="A632" s="73"/>
-      <c r="B632" s="74"/>
-      <c r="C632" s="34"/>
-      <c r="D632" s="34"/>
-      <c r="E632" s="34"/>
+      <c r="A632" s="73" t="s">
+        <v>2336</v>
+      </c>
+      <c r="B632" s="6">
+        <v>44162.0</v>
+      </c>
+      <c r="C632" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D632" s="74" t="s">
+        <v>2139</v>
+      </c>
+      <c r="E632" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F632" s="34"/>
-      <c r="G632" s="34"/>
-      <c r="H632" s="21"/>
-      <c r="I632" s="19"/>
-      <c r="J632" s="10"/>
-      <c r="K632" s="22"/>
-      <c r="L632" s="23"/>
-      <c r="M632" s="22"/>
+      <c r="G632" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H632" s="75" t="s">
+        <v>2263</v>
+      </c>
+      <c r="I632" s="76">
+        <v>44147.0</v>
+      </c>
+      <c r="J632" s="77" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K632" s="78" t="s">
+        <v>2330</v>
+      </c>
+      <c r="L632" s="77" t="s">
+        <v>426</v>
+      </c>
+      <c r="M632" s="78" t="s">
+        <v>1442</v>
+      </c>
       <c r="N632" s="25"/>
-      <c r="O632" s="21"/>
-      <c r="P632" s="21"/>
+      <c r="O632" s="75" t="s">
+        <v>85</v>
+      </c>
+      <c r="P632" s="75" t="s">
+        <v>2333</v>
+      </c>
       <c r="Q632" s="19"/>
       <c r="R632" s="19"/>
-      <c r="S632" s="20"/>
+      <c r="S632" s="61" t="s">
+        <v>2331</v>
+      </c>
       <c r="T632" s="20"/>
       <c r="U632" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#631</v>
       </c>
     </row>
     <row r="633">
-      <c r="A633" s="73"/>
-      <c r="B633" s="74"/>
-      <c r="C633" s="34"/>
-      <c r="D633" s="34"/>
-      <c r="E633" s="34"/>
+      <c r="A633" s="73" t="s">
+        <v>2337</v>
+      </c>
+      <c r="B633" s="6">
+        <v>44162.0</v>
+      </c>
+      <c r="C633" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D633" s="74" t="s">
+        <v>2139</v>
+      </c>
+      <c r="E633" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F633" s="34"/>
-      <c r="G633" s="34"/>
-      <c r="H633" s="21"/>
-      <c r="I633" s="19"/>
-      <c r="J633" s="10"/>
-      <c r="K633" s="22"/>
-      <c r="L633" s="23"/>
-      <c r="M633" s="22"/>
+      <c r="G633" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H633" s="75" t="s">
+        <v>2263</v>
+      </c>
+      <c r="I633" s="76">
+        <v>44147.0</v>
+      </c>
+      <c r="J633" s="79">
+        <v>44154.0</v>
+      </c>
+      <c r="K633" s="78" t="s">
+        <v>2330</v>
+      </c>
+      <c r="L633" s="77" t="s">
+        <v>426</v>
+      </c>
+      <c r="M633" s="78" t="s">
+        <v>2338</v>
+      </c>
       <c r="N633" s="25"/>
-      <c r="O633" s="21"/>
-      <c r="P633" s="21"/>
+      <c r="O633" s="75" t="s">
+        <v>85</v>
+      </c>
+      <c r="P633" s="75" t="s">
+        <v>2339</v>
+      </c>
       <c r="Q633" s="19"/>
       <c r="R633" s="19"/>
-      <c r="S633" s="20"/>
+      <c r="S633" s="61" t="s">
+        <v>2331</v>
+      </c>
       <c r="T633" s="20"/>
       <c r="U633" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#632</v>
       </c>
     </row>
     <row r="634">
-      <c r="A634" s="73"/>
-      <c r="B634" s="74"/>
-      <c r="C634" s="34"/>
-      <c r="D634" s="34"/>
-      <c r="E634" s="34"/>
+      <c r="A634" s="73" t="s">
+        <v>2340</v>
+      </c>
+      <c r="B634" s="6">
+        <v>44162.0</v>
+      </c>
+      <c r="C634" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D634" s="74" t="s">
+        <v>2139</v>
+      </c>
+      <c r="E634" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F634" s="34"/>
-      <c r="G634" s="34"/>
-      <c r="H634" s="21"/>
-      <c r="I634" s="19"/>
-      <c r="J634" s="10"/>
-      <c r="K634" s="22"/>
-      <c r="L634" s="23"/>
-      <c r="M634" s="22"/>
+      <c r="G634" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H634" s="75" t="s">
+        <v>2263</v>
+      </c>
+      <c r="I634" s="76">
+        <v>44147.0</v>
+      </c>
+      <c r="J634" s="77" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K634" s="78" t="s">
+        <v>2330</v>
+      </c>
+      <c r="L634" s="77" t="s">
+        <v>426</v>
+      </c>
+      <c r="M634" s="78" t="s">
+        <v>1442</v>
+      </c>
       <c r="N634" s="25"/>
-      <c r="O634" s="21"/>
-      <c r="P634" s="21"/>
+      <c r="O634" s="75" t="s">
+        <v>85</v>
+      </c>
+      <c r="P634" s="75" t="s">
+        <v>2333</v>
+      </c>
       <c r="Q634" s="19"/>
       <c r="R634" s="19"/>
-      <c r="S634" s="20"/>
+      <c r="S634" s="61" t="s">
+        <v>2331</v>
+      </c>
       <c r="T634" s="20"/>
       <c r="U634" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#633</v>
       </c>
     </row>
     <row r="635">
-      <c r="A635" s="73"/>
-      <c r="B635" s="74"/>
-      <c r="C635" s="34"/>
-      <c r="D635" s="34"/>
-      <c r="E635" s="34"/>
+      <c r="A635" s="73" t="s">
+        <v>2341</v>
+      </c>
+      <c r="B635" s="6">
+        <v>44162.0</v>
+      </c>
+      <c r="C635" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D635" s="74" t="s">
+        <v>2139</v>
+      </c>
+      <c r="E635" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F635" s="34"/>
-      <c r="G635" s="34"/>
-      <c r="H635" s="21"/>
-      <c r="I635" s="19"/>
-      <c r="J635" s="10"/>
-      <c r="K635" s="22"/>
-      <c r="L635" s="23"/>
-      <c r="M635" s="22"/>
+      <c r="G635" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H635" s="75" t="s">
+        <v>2263</v>
+      </c>
+      <c r="I635" s="76">
+        <v>44147.0</v>
+      </c>
+      <c r="J635" s="77" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K635" s="78" t="s">
+        <v>2330</v>
+      </c>
+      <c r="L635" s="77" t="s">
+        <v>426</v>
+      </c>
+      <c r="M635" s="78" t="s">
+        <v>1442</v>
+      </c>
       <c r="N635" s="25"/>
-      <c r="O635" s="21"/>
-      <c r="P635" s="21"/>
+      <c r="O635" s="75" t="s">
+        <v>85</v>
+      </c>
+      <c r="P635" s="75" t="s">
+        <v>2333</v>
+      </c>
       <c r="Q635" s="19"/>
       <c r="R635" s="19"/>
-      <c r="S635" s="20"/>
+      <c r="S635" s="61" t="s">
+        <v>2331</v>
+      </c>
       <c r="T635" s="20"/>
       <c r="U635" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#634</v>
       </c>
     </row>
     <row r="636">
-      <c r="A636" s="73"/>
-      <c r="B636" s="74"/>
-      <c r="C636" s="34"/>
-      <c r="D636" s="34"/>
-      <c r="E636" s="34"/>
+      <c r="A636" s="73" t="s">
+        <v>2342</v>
+      </c>
+      <c r="B636" s="6">
+        <v>44162.0</v>
+      </c>
+      <c r="C636" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D636" s="74" t="s">
+        <v>2139</v>
+      </c>
+      <c r="E636" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F636" s="34"/>
-      <c r="G636" s="34"/>
-      <c r="H636" s="21"/>
-      <c r="I636" s="19"/>
-      <c r="J636" s="10"/>
-      <c r="K636" s="22"/>
-      <c r="L636" s="23"/>
-      <c r="M636" s="22"/>
+      <c r="G636" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H636" s="75" t="s">
+        <v>2263</v>
+      </c>
+      <c r="I636" s="76">
+        <v>44147.0</v>
+      </c>
+      <c r="J636" s="77" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K636" s="78" t="s">
+        <v>2330</v>
+      </c>
+      <c r="L636" s="77" t="s">
+        <v>426</v>
+      </c>
+      <c r="M636" s="78" t="s">
+        <v>1442</v>
+      </c>
       <c r="N636" s="25"/>
-      <c r="O636" s="21"/>
-      <c r="P636" s="21"/>
+      <c r="O636" s="75" t="s">
+        <v>85</v>
+      </c>
+      <c r="P636" s="75" t="s">
+        <v>2333</v>
+      </c>
       <c r="Q636" s="19"/>
       <c r="R636" s="19"/>
-      <c r="S636" s="20"/>
+      <c r="S636" s="61" t="s">
+        <v>2331</v>
+      </c>
       <c r="T636" s="20"/>
       <c r="U636" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#635</v>
       </c>
     </row>
     <row r="637">
-      <c r="A637" s="73"/>
-      <c r="B637" s="74"/>
-      <c r="C637" s="34"/>
-      <c r="D637" s="34"/>
-      <c r="E637" s="34"/>
+      <c r="A637" s="73" t="s">
+        <v>2343</v>
+      </c>
+      <c r="B637" s="6">
+        <v>44162.0</v>
+      </c>
+      <c r="C637" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D637" s="74" t="s">
+        <v>2139</v>
+      </c>
+      <c r="E637" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F637" s="34"/>
-      <c r="G637" s="34"/>
-      <c r="H637" s="21"/>
-      <c r="I637" s="19"/>
-      <c r="J637" s="10"/>
-      <c r="K637" s="22"/>
-      <c r="L637" s="23"/>
-      <c r="M637" s="22"/>
+      <c r="G637" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H637" s="75" t="s">
+        <v>2263</v>
+      </c>
+      <c r="I637" s="76">
+        <v>44147.0</v>
+      </c>
+      <c r="J637" s="77" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K637" s="78" t="s">
+        <v>2330</v>
+      </c>
+      <c r="L637" s="77" t="s">
+        <v>426</v>
+      </c>
+      <c r="M637" s="78" t="s">
+        <v>1442</v>
+      </c>
       <c r="N637" s="25"/>
-      <c r="O637" s="21"/>
-      <c r="P637" s="21"/>
+      <c r="O637" s="75" t="s">
+        <v>85</v>
+      </c>
+      <c r="P637" s="75" t="s">
+        <v>2333</v>
+      </c>
       <c r="Q637" s="19"/>
       <c r="R637" s="19"/>
-      <c r="S637" s="20"/>
+      <c r="S637" s="61" t="s">
+        <v>2331</v>
+      </c>
       <c r="T637" s="20"/>
       <c r="U637" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#636</v>
       </c>
     </row>
     <row r="638">
-      <c r="A638" s="73"/>
-      <c r="B638" s="74"/>
-      <c r="C638" s="34"/>
-      <c r="D638" s="34"/>
-      <c r="E638" s="34"/>
+      <c r="A638" s="73" t="s">
+        <v>2344</v>
+      </c>
+      <c r="B638" s="6">
+        <v>44162.0</v>
+      </c>
+      <c r="C638" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D638" s="74" t="s">
+        <v>2139</v>
+      </c>
+      <c r="E638" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F638" s="34"/>
-      <c r="G638" s="34"/>
-      <c r="H638" s="21"/>
-      <c r="I638" s="19"/>
-      <c r="J638" s="10"/>
-      <c r="K638" s="22"/>
-      <c r="L638" s="23"/>
-      <c r="M638" s="22"/>
+      <c r="G638" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H638" s="75" t="s">
+        <v>2263</v>
+      </c>
+      <c r="I638" s="76">
+        <v>44147.0</v>
+      </c>
+      <c r="J638" s="77" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K638" s="78" t="s">
+        <v>2330</v>
+      </c>
+      <c r="L638" s="77" t="s">
+        <v>426</v>
+      </c>
+      <c r="M638" s="78" t="s">
+        <v>1442</v>
+      </c>
       <c r="N638" s="25"/>
-      <c r="O638" s="21"/>
-      <c r="P638" s="21"/>
+      <c r="O638" s="75" t="s">
+        <v>85</v>
+      </c>
+      <c r="P638" s="75" t="s">
+        <v>2333</v>
+      </c>
       <c r="Q638" s="19"/>
       <c r="R638" s="19"/>
-      <c r="S638" s="20"/>
+      <c r="S638" s="61" t="s">
+        <v>2331</v>
+      </c>
       <c r="T638" s="20"/>
       <c r="U638" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#637</v>
       </c>
     </row>
     <row r="639">
-      <c r="A639" s="73"/>
-      <c r="B639" s="74"/>
-      <c r="C639" s="34"/>
-      <c r="D639" s="34"/>
-      <c r="E639" s="34"/>
+      <c r="A639" s="73" t="s">
+        <v>2345</v>
+      </c>
+      <c r="B639" s="6">
+        <v>44162.0</v>
+      </c>
+      <c r="C639" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D639" s="74" t="s">
+        <v>2139</v>
+      </c>
+      <c r="E639" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F639" s="34"/>
-      <c r="G639" s="34"/>
-      <c r="H639" s="21"/>
-      <c r="I639" s="19"/>
-      <c r="J639" s="10"/>
-      <c r="K639" s="22"/>
-      <c r="L639" s="23"/>
-      <c r="M639" s="22"/>
+      <c r="G639" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H639" s="75" t="s">
+        <v>2263</v>
+      </c>
+      <c r="I639" s="76">
+        <v>44147.0</v>
+      </c>
+      <c r="J639" s="77" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K639" s="78" t="s">
+        <v>2330</v>
+      </c>
+      <c r="L639" s="77" t="s">
+        <v>426</v>
+      </c>
+      <c r="M639" s="78" t="s">
+        <v>1442</v>
+      </c>
       <c r="N639" s="25"/>
-      <c r="O639" s="21"/>
-      <c r="P639" s="21"/>
+      <c r="O639" s="75" t="s">
+        <v>85</v>
+      </c>
+      <c r="P639" s="75" t="s">
+        <v>2333</v>
+      </c>
       <c r="Q639" s="19"/>
       <c r="R639" s="19"/>
-      <c r="S639" s="20"/>
+      <c r="S639" s="61" t="s">
+        <v>2331</v>
+      </c>
       <c r="T639" s="20"/>
       <c r="U639" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#638</v>
       </c>
     </row>
     <row r="640">
-      <c r="A640" s="73"/>
-      <c r="B640" s="74"/>
-      <c r="C640" s="34"/>
-      <c r="D640" s="34"/>
-      <c r="E640" s="34"/>
+      <c r="A640" s="73" t="s">
+        <v>2346</v>
+      </c>
+      <c r="B640" s="6">
+        <v>44162.0</v>
+      </c>
+      <c r="C640" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D640" s="74" t="s">
+        <v>2139</v>
+      </c>
+      <c r="E640" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F640" s="34"/>
-      <c r="G640" s="34"/>
-      <c r="H640" s="21"/>
-      <c r="I640" s="19"/>
-      <c r="J640" s="10"/>
-      <c r="K640" s="22"/>
-      <c r="L640" s="23"/>
-      <c r="M640" s="22"/>
+      <c r="G640" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H640" s="75" t="s">
+        <v>2263</v>
+      </c>
+      <c r="I640" s="76">
+        <v>44147.0</v>
+      </c>
+      <c r="J640" s="77" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K640" s="78" t="s">
+        <v>2330</v>
+      </c>
+      <c r="L640" s="77" t="s">
+        <v>426</v>
+      </c>
+      <c r="M640" s="78" t="s">
+        <v>1442</v>
+      </c>
       <c r="N640" s="25"/>
-      <c r="O640" s="21"/>
-      <c r="P640" s="21"/>
+      <c r="O640" s="75" t="s">
+        <v>85</v>
+      </c>
+      <c r="P640" s="75" t="s">
+        <v>2333</v>
+      </c>
       <c r="Q640" s="19"/>
       <c r="R640" s="19"/>
-      <c r="S640" s="20"/>
+      <c r="S640" s="61" t="s">
+        <v>2331</v>
+      </c>
       <c r="T640" s="20"/>
       <c r="U640" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#639</v>
       </c>
     </row>
     <row r="641">
-      <c r="A641" s="73"/>
-      <c r="B641" s="74"/>
-      <c r="C641" s="34"/>
-      <c r="D641" s="34"/>
-      <c r="E641" s="34"/>
+      <c r="A641" s="73" t="s">
+        <v>2347</v>
+      </c>
+      <c r="B641" s="6">
+        <v>44162.0</v>
+      </c>
+      <c r="C641" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D641" s="74" t="s">
+        <v>116</v>
+      </c>
+      <c r="E641" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F641" s="34"/>
-      <c r="G641" s="34"/>
-      <c r="H641" s="21"/>
-      <c r="I641" s="19"/>
-      <c r="J641" s="10"/>
-      <c r="K641" s="22"/>
-      <c r="L641" s="23"/>
-      <c r="M641" s="22"/>
+      <c r="G641" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H641" s="75" t="s">
+        <v>2348</v>
+      </c>
+      <c r="I641" s="76">
+        <v>44155.0</v>
+      </c>
+      <c r="J641" s="79">
+        <v>44156.0</v>
+      </c>
+      <c r="K641" s="78" t="s">
+        <v>2330</v>
+      </c>
+      <c r="L641" s="77" t="s">
+        <v>426</v>
+      </c>
+      <c r="M641" s="78" t="s">
+        <v>2349</v>
+      </c>
       <c r="N641" s="25"/>
-      <c r="O641" s="21"/>
-      <c r="P641" s="21"/>
+      <c r="O641" s="75" t="s">
+        <v>85</v>
+      </c>
+      <c r="P641" s="75" t="s">
+        <v>2350</v>
+      </c>
       <c r="Q641" s="19"/>
       <c r="R641" s="19"/>
-      <c r="S641" s="20"/>
+      <c r="S641" s="61" t="s">
+        <v>2331</v>
+      </c>
       <c r="T641" s="20"/>
       <c r="U641" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#640</v>
       </c>
     </row>
     <row r="642">
-      <c r="A642" s="73"/>
-      <c r="B642" s="74"/>
+      <c r="A642" s="80"/>
+      <c r="B642" s="81"/>
       <c r="C642" s="34"/>
       <c r="D642" s="34"/>
       <c r="E642" s="34"/>
@@ -46075,8 +46677,8 @@
       </c>
     </row>
     <row r="643">
-      <c r="A643" s="73"/>
-      <c r="B643" s="74"/>
+      <c r="A643" s="80"/>
+      <c r="B643" s="81"/>
       <c r="C643" s="34"/>
       <c r="D643" s="34"/>
       <c r="E643" s="34"/>
@@ -46101,8 +46703,8 @@
       </c>
     </row>
     <row r="644">
-      <c r="A644" s="73"/>
-      <c r="B644" s="74"/>
+      <c r="A644" s="80"/>
+      <c r="B644" s="81"/>
       <c r="C644" s="34"/>
       <c r="D644" s="34"/>
       <c r="E644" s="34"/>
@@ -46127,8 +46729,8 @@
       </c>
     </row>
     <row r="645">
-      <c r="A645" s="73"/>
-      <c r="B645" s="74"/>
+      <c r="A645" s="80"/>
+      <c r="B645" s="81"/>
       <c r="C645" s="34"/>
       <c r="D645" s="34"/>
       <c r="E645" s="34"/>
@@ -46153,8 +46755,8 @@
       </c>
     </row>
     <row r="646">
-      <c r="A646" s="73"/>
-      <c r="B646" s="74"/>
+      <c r="A646" s="80"/>
+      <c r="B646" s="81"/>
       <c r="C646" s="34"/>
       <c r="D646" s="34"/>
       <c r="E646" s="34"/>
@@ -46179,8 +46781,8 @@
       </c>
     </row>
     <row r="647">
-      <c r="A647" s="73"/>
-      <c r="B647" s="74"/>
+      <c r="A647" s="80"/>
+      <c r="B647" s="81"/>
       <c r="C647" s="34"/>
       <c r="D647" s="34"/>
       <c r="E647" s="34"/>
@@ -46205,8 +46807,8 @@
       </c>
     </row>
     <row r="648">
-      <c r="A648" s="73"/>
-      <c r="B648" s="74"/>
+      <c r="A648" s="80"/>
+      <c r="B648" s="81"/>
       <c r="C648" s="34"/>
       <c r="D648" s="34"/>
       <c r="E648" s="34"/>
@@ -46231,8 +46833,8 @@
       </c>
     </row>
     <row r="649">
-      <c r="A649" s="73"/>
-      <c r="B649" s="74"/>
+      <c r="A649" s="80"/>
+      <c r="B649" s="81"/>
       <c r="C649" s="34"/>
       <c r="D649" s="34"/>
       <c r="E649" s="34"/>
@@ -46257,8 +46859,8 @@
       </c>
     </row>
     <row r="650">
-      <c r="A650" s="73"/>
-      <c r="B650" s="74"/>
+      <c r="A650" s="80"/>
+      <c r="B650" s="81"/>
       <c r="C650" s="34"/>
       <c r="D650" s="34"/>
       <c r="E650" s="34"/>
@@ -46283,8 +46885,8 @@
       </c>
     </row>
     <row r="651">
-      <c r="A651" s="73"/>
-      <c r="B651" s="74"/>
+      <c r="A651" s="80"/>
+      <c r="B651" s="81"/>
       <c r="C651" s="34"/>
       <c r="D651" s="34"/>
       <c r="E651" s="34"/>
@@ -46309,8 +46911,8 @@
       </c>
     </row>
     <row r="652">
-      <c r="A652" s="73"/>
-      <c r="B652" s="74"/>
+      <c r="A652" s="80"/>
+      <c r="B652" s="81"/>
       <c r="C652" s="34"/>
       <c r="D652" s="34"/>
       <c r="E652" s="34"/>
@@ -46335,8 +46937,8 @@
       </c>
     </row>
     <row r="653">
-      <c r="A653" s="73"/>
-      <c r="B653" s="74"/>
+      <c r="A653" s="80"/>
+      <c r="B653" s="81"/>
       <c r="C653" s="34"/>
       <c r="D653" s="34"/>
       <c r="E653" s="34"/>
@@ -46361,8 +46963,8 @@
       </c>
     </row>
     <row r="654">
-      <c r="A654" s="73"/>
-      <c r="B654" s="74"/>
+      <c r="A654" s="80"/>
+      <c r="B654" s="81"/>
       <c r="C654" s="34"/>
       <c r="D654" s="34"/>
       <c r="E654" s="34"/>
@@ -46387,8 +46989,8 @@
       </c>
     </row>
     <row r="655">
-      <c r="A655" s="73"/>
-      <c r="B655" s="74"/>
+      <c r="A655" s="80"/>
+      <c r="B655" s="81"/>
       <c r="C655" s="34"/>
       <c r="D655" s="34"/>
       <c r="E655" s="34"/>
@@ -46413,8 +47015,8 @@
       </c>
     </row>
     <row r="656">
-      <c r="A656" s="73"/>
-      <c r="B656" s="74"/>
+      <c r="A656" s="80"/>
+      <c r="B656" s="81"/>
       <c r="C656" s="34"/>
       <c r="D656" s="34"/>
       <c r="E656" s="34"/>
@@ -46439,8 +47041,8 @@
       </c>
     </row>
     <row r="657">
-      <c r="A657" s="73"/>
-      <c r="B657" s="74"/>
+      <c r="A657" s="80"/>
+      <c r="B657" s="81"/>
       <c r="C657" s="34"/>
       <c r="D657" s="34"/>
       <c r="E657" s="34"/>
@@ -46465,8 +47067,8 @@
       </c>
     </row>
     <row r="658">
-      <c r="A658" s="73"/>
-      <c r="B658" s="74"/>
+      <c r="A658" s="80"/>
+      <c r="B658" s="81"/>
       <c r="C658" s="34"/>
       <c r="D658" s="34"/>
       <c r="E658" s="34"/>
@@ -46491,8 +47093,8 @@
       </c>
     </row>
     <row r="659">
-      <c r="A659" s="73"/>
-      <c r="B659" s="74"/>
+      <c r="A659" s="80"/>
+      <c r="B659" s="81"/>
       <c r="C659" s="34"/>
       <c r="D659" s="34"/>
       <c r="E659" s="34"/>
@@ -46517,8 +47119,8 @@
       </c>
     </row>
     <row r="660">
-      <c r="A660" s="73"/>
-      <c r="B660" s="74"/>
+      <c r="A660" s="80"/>
+      <c r="B660" s="81"/>
       <c r="C660" s="34"/>
       <c r="D660" s="34"/>
       <c r="E660" s="34"/>
@@ -46543,8 +47145,8 @@
       </c>
     </row>
     <row r="661">
-      <c r="A661" s="73"/>
-      <c r="B661" s="74"/>
+      <c r="A661" s="80"/>
+      <c r="B661" s="81"/>
       <c r="C661" s="34"/>
       <c r="D661" s="34"/>
       <c r="E661" s="34"/>
@@ -46569,8 +47171,8 @@
       </c>
     </row>
     <row r="662">
-      <c r="A662" s="73"/>
-      <c r="B662" s="74"/>
+      <c r="A662" s="80"/>
+      <c r="B662" s="81"/>
       <c r="C662" s="34"/>
       <c r="D662" s="34"/>
       <c r="E662" s="34"/>
@@ -46595,8 +47197,8 @@
       </c>
     </row>
     <row r="663">
-      <c r="A663" s="73"/>
-      <c r="B663" s="74"/>
+      <c r="A663" s="80"/>
+      <c r="B663" s="81"/>
       <c r="C663" s="34"/>
       <c r="D663" s="34"/>
       <c r="E663" s="34"/>
@@ -46621,8 +47223,8 @@
       </c>
     </row>
     <row r="664">
-      <c r="A664" s="73"/>
-      <c r="B664" s="74"/>
+      <c r="A664" s="80"/>
+      <c r="B664" s="81"/>
       <c r="C664" s="34"/>
       <c r="D664" s="34"/>
       <c r="E664" s="34"/>
@@ -46647,8 +47249,8 @@
       </c>
     </row>
     <row r="665">
-      <c r="A665" s="73"/>
-      <c r="B665" s="74"/>
+      <c r="A665" s="80"/>
+      <c r="B665" s="81"/>
       <c r="C665" s="34"/>
       <c r="D665" s="34"/>
       <c r="E665" s="34"/>
@@ -46673,8 +47275,8 @@
       </c>
     </row>
     <row r="666">
-      <c r="A666" s="73"/>
-      <c r="B666" s="74"/>
+      <c r="A666" s="80"/>
+      <c r="B666" s="81"/>
       <c r="C666" s="34"/>
       <c r="D666" s="34"/>
       <c r="E666" s="34"/>
@@ -46699,8 +47301,8 @@
       </c>
     </row>
     <row r="667">
-      <c r="A667" s="73"/>
-      <c r="B667" s="74"/>
+      <c r="A667" s="80"/>
+      <c r="B667" s="81"/>
       <c r="C667" s="34"/>
       <c r="D667" s="34"/>
       <c r="E667" s="34"/>
@@ -46725,8 +47327,8 @@
       </c>
     </row>
     <row r="668">
-      <c r="A668" s="73"/>
-      <c r="B668" s="74"/>
+      <c r="A668" s="80"/>
+      <c r="B668" s="81"/>
       <c r="C668" s="34"/>
       <c r="D668" s="34"/>
       <c r="E668" s="34"/>
@@ -46751,8 +47353,8 @@
       </c>
     </row>
     <row r="669">
-      <c r="A669" s="73"/>
-      <c r="B669" s="74"/>
+      <c r="A669" s="80"/>
+      <c r="B669" s="81"/>
       <c r="C669" s="34"/>
       <c r="D669" s="34"/>
       <c r="E669" s="34"/>
@@ -46777,8 +47379,8 @@
       </c>
     </row>
     <row r="670">
-      <c r="A670" s="73"/>
-      <c r="B670" s="74"/>
+      <c r="A670" s="80"/>
+      <c r="B670" s="81"/>
       <c r="C670" s="34"/>
       <c r="D670" s="34"/>
       <c r="E670" s="34"/>
@@ -46803,8 +47405,8 @@
       </c>
     </row>
     <row r="671">
-      <c r="A671" s="73"/>
-      <c r="B671" s="74"/>
+      <c r="A671" s="80"/>
+      <c r="B671" s="81"/>
       <c r="C671" s="34"/>
       <c r="D671" s="34"/>
       <c r="E671" s="34"/>
@@ -46829,8 +47431,8 @@
       </c>
     </row>
     <row r="672">
-      <c r="A672" s="73"/>
-      <c r="B672" s="74"/>
+      <c r="A672" s="80"/>
+      <c r="B672" s="81"/>
       <c r="C672" s="34"/>
       <c r="D672" s="34"/>
       <c r="E672" s="34"/>
@@ -46855,8 +47457,8 @@
       </c>
     </row>
     <row r="673">
-      <c r="A673" s="73"/>
-      <c r="B673" s="74"/>
+      <c r="A673" s="80"/>
+      <c r="B673" s="81"/>
       <c r="C673" s="34"/>
       <c r="D673" s="34"/>
       <c r="E673" s="34"/>
@@ -46881,8 +47483,8 @@
       </c>
     </row>
     <row r="674">
-      <c r="A674" s="73"/>
-      <c r="B674" s="74"/>
+      <c r="A674" s="80"/>
+      <c r="B674" s="81"/>
       <c r="C674" s="34"/>
       <c r="D674" s="34"/>
       <c r="E674" s="34"/>
@@ -46907,8 +47509,8 @@
       </c>
     </row>
     <row r="675">
-      <c r="A675" s="73"/>
-      <c r="B675" s="74"/>
+      <c r="A675" s="80"/>
+      <c r="B675" s="81"/>
       <c r="C675" s="34"/>
       <c r="D675" s="34"/>
       <c r="E675" s="34"/>
@@ -46933,8 +47535,8 @@
       </c>
     </row>
     <row r="676">
-      <c r="A676" s="73"/>
-      <c r="B676" s="74"/>
+      <c r="A676" s="80"/>
+      <c r="B676" s="81"/>
       <c r="C676" s="34"/>
       <c r="D676" s="34"/>
       <c r="E676" s="34"/>
@@ -46959,8 +47561,8 @@
       </c>
     </row>
     <row r="677">
-      <c r="A677" s="73"/>
-      <c r="B677" s="74"/>
+      <c r="A677" s="80"/>
+      <c r="B677" s="81"/>
       <c r="C677" s="34"/>
       <c r="D677" s="34"/>
       <c r="E677" s="34"/>
@@ -46985,8 +47587,8 @@
       </c>
     </row>
     <row r="678">
-      <c r="A678" s="73"/>
-      <c r="B678" s="74"/>
+      <c r="A678" s="80"/>
+      <c r="B678" s="81"/>
       <c r="C678" s="34"/>
       <c r="D678" s="34"/>
       <c r="E678" s="34"/>
@@ -47011,8 +47613,8 @@
       </c>
     </row>
     <row r="679">
-      <c r="A679" s="73"/>
-      <c r="B679" s="74"/>
+      <c r="A679" s="80"/>
+      <c r="B679" s="81"/>
       <c r="C679" s="34"/>
       <c r="D679" s="34"/>
       <c r="E679" s="34"/>
@@ -47037,8 +47639,8 @@
       </c>
     </row>
     <row r="680">
-      <c r="A680" s="73"/>
-      <c r="B680" s="74"/>
+      <c r="A680" s="80"/>
+      <c r="B680" s="81"/>
       <c r="C680" s="34"/>
       <c r="D680" s="34"/>
       <c r="E680" s="34"/>
@@ -47063,8 +47665,8 @@
       </c>
     </row>
     <row r="681">
-      <c r="A681" s="73"/>
-      <c r="B681" s="74"/>
+      <c r="A681" s="80"/>
+      <c r="B681" s="81"/>
       <c r="C681" s="34"/>
       <c r="D681" s="34"/>
       <c r="E681" s="34"/>
@@ -47089,8 +47691,8 @@
       </c>
     </row>
     <row r="682">
-      <c r="A682" s="73"/>
-      <c r="B682" s="74"/>
+      <c r="A682" s="80"/>
+      <c r="B682" s="81"/>
       <c r="C682" s="34"/>
       <c r="D682" s="34"/>
       <c r="E682" s="34"/>
@@ -47115,8 +47717,8 @@
       </c>
     </row>
     <row r="683">
-      <c r="A683" s="73"/>
-      <c r="B683" s="74"/>
+      <c r="A683" s="80"/>
+      <c r="B683" s="81"/>
       <c r="C683" s="34"/>
       <c r="D683" s="34"/>
       <c r="E683" s="34"/>
@@ -47141,8 +47743,8 @@
       </c>
     </row>
     <row r="684">
-      <c r="A684" s="73"/>
-      <c r="B684" s="74"/>
+      <c r="A684" s="80"/>
+      <c r="B684" s="81"/>
       <c r="C684" s="34"/>
       <c r="D684" s="34"/>
       <c r="E684" s="34"/>
@@ -47167,8 +47769,8 @@
       </c>
     </row>
     <row r="685">
-      <c r="A685" s="73"/>
-      <c r="B685" s="74"/>
+      <c r="A685" s="80"/>
+      <c r="B685" s="81"/>
       <c r="C685" s="34"/>
       <c r="D685" s="34"/>
       <c r="E685" s="34"/>
@@ -47193,8 +47795,8 @@
       </c>
     </row>
     <row r="686">
-      <c r="A686" s="73"/>
-      <c r="B686" s="74"/>
+      <c r="A686" s="80"/>
+      <c r="B686" s="81"/>
       <c r="C686" s="34"/>
       <c r="D686" s="34"/>
       <c r="E686" s="34"/>
@@ -47219,8 +47821,8 @@
       </c>
     </row>
     <row r="687">
-      <c r="A687" s="73"/>
-      <c r="B687" s="74"/>
+      <c r="A687" s="80"/>
+      <c r="B687" s="81"/>
       <c r="C687" s="34"/>
       <c r="D687" s="34"/>
       <c r="E687" s="34"/>
@@ -47245,8 +47847,8 @@
       </c>
     </row>
     <row r="688">
-      <c r="A688" s="73"/>
-      <c r="B688" s="74"/>
+      <c r="A688" s="80"/>
+      <c r="B688" s="81"/>
       <c r="C688" s="34"/>
       <c r="D688" s="34"/>
       <c r="E688" s="34"/>
@@ -47271,8 +47873,8 @@
       </c>
     </row>
     <row r="689">
-      <c r="A689" s="73"/>
-      <c r="B689" s="74"/>
+      <c r="A689" s="80"/>
+      <c r="B689" s="81"/>
       <c r="C689" s="34"/>
       <c r="D689" s="34"/>
       <c r="E689" s="34"/>
@@ -47297,8 +47899,8 @@
       </c>
     </row>
     <row r="690">
-      <c r="A690" s="73"/>
-      <c r="B690" s="74"/>
+      <c r="A690" s="80"/>
+      <c r="B690" s="81"/>
       <c r="C690" s="34"/>
       <c r="D690" s="34"/>
       <c r="E690" s="34"/>
@@ -47323,8 +47925,8 @@
       </c>
     </row>
     <row r="691">
-      <c r="A691" s="73"/>
-      <c r="B691" s="74"/>
+      <c r="A691" s="80"/>
+      <c r="B691" s="81"/>
       <c r="C691" s="34"/>
       <c r="D691" s="34"/>
       <c r="E691" s="34"/>
@@ -47349,8 +47951,8 @@
       </c>
     </row>
     <row r="692">
-      <c r="A692" s="73"/>
-      <c r="B692" s="74"/>
+      <c r="A692" s="80"/>
+      <c r="B692" s="81"/>
       <c r="C692" s="34"/>
       <c r="D692" s="34"/>
       <c r="E692" s="34"/>
@@ -47375,8 +47977,8 @@
       </c>
     </row>
     <row r="693">
-      <c r="A693" s="73"/>
-      <c r="B693" s="74"/>
+      <c r="A693" s="80"/>
+      <c r="B693" s="81"/>
       <c r="C693" s="34"/>
       <c r="D693" s="34"/>
       <c r="E693" s="34"/>
@@ -47401,8 +48003,8 @@
       </c>
     </row>
     <row r="694">
-      <c r="A694" s="73"/>
-      <c r="B694" s="74"/>
+      <c r="A694" s="80"/>
+      <c r="B694" s="81"/>
       <c r="C694" s="34"/>
       <c r="D694" s="34"/>
       <c r="E694" s="34"/>
@@ -47427,8 +48029,8 @@
       </c>
     </row>
     <row r="695">
-      <c r="A695" s="73"/>
-      <c r="B695" s="74"/>
+      <c r="A695" s="80"/>
+      <c r="B695" s="81"/>
       <c r="C695" s="34"/>
       <c r="D695" s="34"/>
       <c r="E695" s="34"/>
@@ -47453,8 +48055,8 @@
       </c>
     </row>
     <row r="696">
-      <c r="A696" s="73"/>
-      <c r="B696" s="74"/>
+      <c r="A696" s="80"/>
+      <c r="B696" s="81"/>
       <c r="C696" s="34"/>
       <c r="D696" s="34"/>
       <c r="E696" s="34"/>
@@ -47479,8 +48081,8 @@
       </c>
     </row>
     <row r="697">
-      <c r="A697" s="73"/>
-      <c r="B697" s="74"/>
+      <c r="A697" s="80"/>
+      <c r="B697" s="81"/>
       <c r="C697" s="34"/>
       <c r="D697" s="34"/>
       <c r="E697" s="34"/>
@@ -47505,8 +48107,8 @@
       </c>
     </row>
     <row r="698">
-      <c r="A698" s="73"/>
-      <c r="B698" s="74"/>
+      <c r="A698" s="80"/>
+      <c r="B698" s="81"/>
       <c r="C698" s="34"/>
       <c r="D698" s="34"/>
       <c r="E698" s="34"/>
@@ -47531,8 +48133,8 @@
       </c>
     </row>
     <row r="699">
-      <c r="A699" s="73"/>
-      <c r="B699" s="74"/>
+      <c r="A699" s="80"/>
+      <c r="B699" s="81"/>
       <c r="C699" s="34"/>
       <c r="D699" s="34"/>
       <c r="E699" s="34"/>
@@ -47557,8 +48159,8 @@
       </c>
     </row>
     <row r="700">
-      <c r="A700" s="73"/>
-      <c r="B700" s="74"/>
+      <c r="A700" s="80"/>
+      <c r="B700" s="81"/>
       <c r="C700" s="34"/>
       <c r="D700" s="34"/>
       <c r="E700" s="34"/>
@@ -47583,8 +48185,8 @@
       </c>
     </row>
     <row r="701">
-      <c r="A701" s="73"/>
-      <c r="B701" s="74"/>
+      <c r="A701" s="80"/>
+      <c r="B701" s="81"/>
       <c r="C701" s="34"/>
       <c r="D701" s="34"/>
       <c r="E701" s="34"/>
@@ -48176,15 +48778,31 @@
     <hyperlink r:id="rId185" ref="S623"/>
     <hyperlink r:id="rId186" ref="S624"/>
     <hyperlink r:id="rId187" ref="S625"/>
+    <hyperlink r:id="rId188" ref="S626"/>
+    <hyperlink r:id="rId189" ref="S627"/>
+    <hyperlink r:id="rId190" ref="S628"/>
+    <hyperlink r:id="rId191" ref="S629"/>
+    <hyperlink r:id="rId192" ref="S630"/>
+    <hyperlink r:id="rId193" ref="S631"/>
+    <hyperlink r:id="rId194" ref="S632"/>
+    <hyperlink r:id="rId195" ref="S633"/>
+    <hyperlink r:id="rId196" ref="S634"/>
+    <hyperlink r:id="rId197" ref="S635"/>
+    <hyperlink r:id="rId198" ref="S636"/>
+    <hyperlink r:id="rId199" ref="S637"/>
+    <hyperlink r:id="rId200" ref="S638"/>
+    <hyperlink r:id="rId201" ref="S639"/>
+    <hyperlink r:id="rId202" ref="S640"/>
+    <hyperlink r:id="rId203" ref="S641"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId188"/>
-  <legacyDrawing r:id="rId189"/>
+  <drawing r:id="rId204"/>
+  <legacyDrawing r:id="rId205"/>
   <tableParts count="2">
-    <tablePart r:id="rId192"/>
-    <tablePart r:id="rId193"/>
+    <tablePart r:id="rId208"/>
+    <tablePart r:id="rId209"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201128
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -571,7 +571,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7235" uniqueCount="2351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7346" uniqueCount="2374">
   <si>
     <t>案例</t>
   </si>
@@ -8533,6 +8533,82 @@
   </si>
   <si>
     <t>長期在美國工作，返臺探親</t>
+  </si>
+  <si>
+    <t>#641</t>
+  </si>
+  <si>
+    <t>-11/25 印尼→台灣</t>
+  </si>
+  <si>
+    <t>11/25 採檢
+11/28 確診</t>
+  </si>
+  <si>
+    <t>印尼籍女性移工，入境時主動告知有不適症狀
+#641 #642 #643 #644 同班機</t>
+  </si>
+  <si>
+    <t>新增9例境外移入COVID-19病例，分別自印尼及美國入境</t>
+  </si>
+  <si>
+    <t>#642</t>
+  </si>
+  <si>
+    <t>#643</t>
+  </si>
+  <si>
+    <t>#644</t>
+  </si>
+  <si>
+    <t>印尼籍女性移工，無症狀，但主動告知有服用藥物(後經釐清為維他命C)
+#641 #642 #643 #644 同班機</t>
+  </si>
+  <si>
+    <t>#645</t>
+  </si>
+  <si>
+    <t>2019/11月-11/19 美國</t>
+  </si>
+  <si>
+    <t>11/26 採檢
+11/28 確診</t>
+  </si>
+  <si>
+    <t>長期居住美國，返臺探親
+居家檢疫期間，提出外出奔喪申請，於11月26日由衛生單位安排自費採檢</t>
+  </si>
+  <si>
+    <t>#646</t>
+  </si>
+  <si>
+    <t>-11/13 印尼→台灣</t>
+  </si>
+  <si>
+    <t>印尼籍女性移工
+#646 #647 #649 同班機</t>
+  </si>
+  <si>
+    <t>#647</t>
+  </si>
+  <si>
+    <t>#648</t>
+  </si>
+  <si>
+    <t>-11/15 印尼→台灣</t>
+  </si>
+  <si>
+    <t>11/27 採檢
+11/28 確診</t>
+  </si>
+  <si>
+    <t>回溯性採檢</t>
+  </si>
+  <si>
+    <t>指揮中心自11月20日起暫緩4家印尼仲介公司之仲介移工來臺，並針對10月已入境之該4家公司仲介產業移工共30人進行回溯性採檢，共採檢27人</t>
+  </si>
+  <si>
+    <t>#649</t>
   </si>
 </sst>
 </file>
@@ -8673,7 +8749,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="81">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -8906,12 +8982,9 @@
       <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="19" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -45867,7 +45940,7 @@
       </c>
     </row>
     <row r="628">
-      <c r="A628" s="73" t="s">
+      <c r="A628" s="16" t="s">
         <v>2328</v>
       </c>
       <c r="B628" s="6">
@@ -45876,7 +45949,7 @@
       <c r="C628" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D628" s="74" t="s">
+      <c r="D628" s="7" t="s">
         <v>2139</v>
       </c>
       <c r="E628" s="7" t="s">
@@ -45886,29 +45959,29 @@
       <c r="G628" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H628" s="75" t="s">
+      <c r="H628" s="8" t="s">
         <v>2329</v>
       </c>
-      <c r="I628" s="76">
+      <c r="I628" s="9">
         <v>44146.0</v>
       </c>
-      <c r="J628" s="77" t="s">
+      <c r="J628" s="12" t="s">
         <v>1442</v>
       </c>
-      <c r="K628" s="78" t="s">
+      <c r="K628" s="13" t="s">
         <v>2330</v>
       </c>
-      <c r="L628" s="77" t="s">
+      <c r="L628" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M628" s="78" t="s">
+      <c r="M628" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N628" s="25"/>
-      <c r="O628" s="75" t="s">
-        <v>85</v>
-      </c>
-      <c r="P628" s="75" t="s">
+      <c r="O628" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P628" s="8" t="s">
         <v>1777</v>
       </c>
       <c r="Q628" s="19"/>
@@ -45923,7 +45996,7 @@
       </c>
     </row>
     <row r="629">
-      <c r="A629" s="73" t="s">
+      <c r="A629" s="16" t="s">
         <v>2332</v>
       </c>
       <c r="B629" s="6">
@@ -45932,7 +46005,7 @@
       <c r="C629" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D629" s="74" t="s">
+      <c r="D629" s="7" t="s">
         <v>2139</v>
       </c>
       <c r="E629" s="7" t="s">
@@ -45942,29 +46015,29 @@
       <c r="G629" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H629" s="75" t="s">
+      <c r="H629" s="8" t="s">
         <v>2263</v>
       </c>
-      <c r="I629" s="76">
+      <c r="I629" s="9">
         <v>44147.0</v>
       </c>
-      <c r="J629" s="77" t="s">
+      <c r="J629" s="12" t="s">
         <v>1442</v>
       </c>
-      <c r="K629" s="78" t="s">
+      <c r="K629" s="13" t="s">
         <v>2330</v>
       </c>
-      <c r="L629" s="77" t="s">
+      <c r="L629" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M629" s="78" t="s">
+      <c r="M629" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N629" s="25"/>
-      <c r="O629" s="75" t="s">
-        <v>85</v>
-      </c>
-      <c r="P629" s="75" t="s">
+      <c r="O629" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P629" s="8" t="s">
         <v>2333</v>
       </c>
       <c r="Q629" s="19"/>
@@ -45979,7 +46052,7 @@
       </c>
     </row>
     <row r="630">
-      <c r="A630" s="73" t="s">
+      <c r="A630" s="16" t="s">
         <v>2334</v>
       </c>
       <c r="B630" s="6">
@@ -45988,7 +46061,7 @@
       <c r="C630" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D630" s="74" t="s">
+      <c r="D630" s="7" t="s">
         <v>2139</v>
       </c>
       <c r="E630" s="7" t="s">
@@ -45998,29 +46071,29 @@
       <c r="G630" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H630" s="75" t="s">
+      <c r="H630" s="8" t="s">
         <v>2263</v>
       </c>
-      <c r="I630" s="76">
+      <c r="I630" s="9">
         <v>44147.0</v>
       </c>
-      <c r="J630" s="77" t="s">
+      <c r="J630" s="12" t="s">
         <v>1442</v>
       </c>
-      <c r="K630" s="78" t="s">
+      <c r="K630" s="13" t="s">
         <v>2330</v>
       </c>
-      <c r="L630" s="77" t="s">
+      <c r="L630" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M630" s="78" t="s">
+      <c r="M630" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N630" s="25"/>
-      <c r="O630" s="75" t="s">
-        <v>85</v>
-      </c>
-      <c r="P630" s="75" t="s">
+      <c r="O630" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P630" s="8" t="s">
         <v>2333</v>
       </c>
       <c r="Q630" s="19"/>
@@ -46035,7 +46108,7 @@
       </c>
     </row>
     <row r="631">
-      <c r="A631" s="73" t="s">
+      <c r="A631" s="16" t="s">
         <v>2335</v>
       </c>
       <c r="B631" s="6">
@@ -46044,7 +46117,7 @@
       <c r="C631" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D631" s="74" t="s">
+      <c r="D631" s="7" t="s">
         <v>2139</v>
       </c>
       <c r="E631" s="7" t="s">
@@ -46054,29 +46127,29 @@
       <c r="G631" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H631" s="75" t="s">
+      <c r="H631" s="8" t="s">
         <v>2263</v>
       </c>
-      <c r="I631" s="76">
+      <c r="I631" s="9">
         <v>44147.0</v>
       </c>
-      <c r="J631" s="77" t="s">
+      <c r="J631" s="12" t="s">
         <v>1442</v>
       </c>
-      <c r="K631" s="78" t="s">
+      <c r="K631" s="13" t="s">
         <v>2330</v>
       </c>
-      <c r="L631" s="77" t="s">
+      <c r="L631" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M631" s="78" t="s">
+      <c r="M631" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N631" s="25"/>
-      <c r="O631" s="75" t="s">
-        <v>85</v>
-      </c>
-      <c r="P631" s="75" t="s">
+      <c r="O631" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P631" s="8" t="s">
         <v>2333</v>
       </c>
       <c r="Q631" s="19"/>
@@ -46091,7 +46164,7 @@
       </c>
     </row>
     <row r="632">
-      <c r="A632" s="73" t="s">
+      <c r="A632" s="16" t="s">
         <v>2336</v>
       </c>
       <c r="B632" s="6">
@@ -46100,7 +46173,7 @@
       <c r="C632" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D632" s="74" t="s">
+      <c r="D632" s="7" t="s">
         <v>2139</v>
       </c>
       <c r="E632" s="7" t="s">
@@ -46110,29 +46183,29 @@
       <c r="G632" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H632" s="75" t="s">
+      <c r="H632" s="8" t="s">
         <v>2263</v>
       </c>
-      <c r="I632" s="76">
+      <c r="I632" s="9">
         <v>44147.0</v>
       </c>
-      <c r="J632" s="77" t="s">
+      <c r="J632" s="12" t="s">
         <v>1442</v>
       </c>
-      <c r="K632" s="78" t="s">
+      <c r="K632" s="13" t="s">
         <v>2330</v>
       </c>
-      <c r="L632" s="77" t="s">
+      <c r="L632" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M632" s="78" t="s">
+      <c r="M632" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N632" s="25"/>
-      <c r="O632" s="75" t="s">
-        <v>85</v>
-      </c>
-      <c r="P632" s="75" t="s">
+      <c r="O632" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P632" s="8" t="s">
         <v>2333</v>
       </c>
       <c r="Q632" s="19"/>
@@ -46147,7 +46220,7 @@
       </c>
     </row>
     <row r="633">
-      <c r="A633" s="73" t="s">
+      <c r="A633" s="16" t="s">
         <v>2337</v>
       </c>
       <c r="B633" s="6">
@@ -46156,7 +46229,7 @@
       <c r="C633" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D633" s="74" t="s">
+      <c r="D633" s="7" t="s">
         <v>2139</v>
       </c>
       <c r="E633" s="7" t="s">
@@ -46166,29 +46239,29 @@
       <c r="G633" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H633" s="75" t="s">
+      <c r="H633" s="8" t="s">
         <v>2263</v>
       </c>
-      <c r="I633" s="76">
+      <c r="I633" s="9">
         <v>44147.0</v>
       </c>
-      <c r="J633" s="79">
+      <c r="J633" s="10">
         <v>44154.0</v>
       </c>
-      <c r="K633" s="78" t="s">
+      <c r="K633" s="13" t="s">
         <v>2330</v>
       </c>
-      <c r="L633" s="77" t="s">
+      <c r="L633" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M633" s="78" t="s">
+      <c r="M633" s="13" t="s">
         <v>2338</v>
       </c>
       <c r="N633" s="25"/>
-      <c r="O633" s="75" t="s">
-        <v>85</v>
-      </c>
-      <c r="P633" s="75" t="s">
+      <c r="O633" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P633" s="8" t="s">
         <v>2339</v>
       </c>
       <c r="Q633" s="19"/>
@@ -46203,7 +46276,7 @@
       </c>
     </row>
     <row r="634">
-      <c r="A634" s="73" t="s">
+      <c r="A634" s="16" t="s">
         <v>2340</v>
       </c>
       <c r="B634" s="6">
@@ -46212,7 +46285,7 @@
       <c r="C634" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D634" s="74" t="s">
+      <c r="D634" s="7" t="s">
         <v>2139</v>
       </c>
       <c r="E634" s="7" t="s">
@@ -46222,29 +46295,29 @@
       <c r="G634" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H634" s="75" t="s">
+      <c r="H634" s="8" t="s">
         <v>2263</v>
       </c>
-      <c r="I634" s="76">
+      <c r="I634" s="9">
         <v>44147.0</v>
       </c>
-      <c r="J634" s="77" t="s">
+      <c r="J634" s="12" t="s">
         <v>1442</v>
       </c>
-      <c r="K634" s="78" t="s">
+      <c r="K634" s="13" t="s">
         <v>2330</v>
       </c>
-      <c r="L634" s="77" t="s">
+      <c r="L634" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M634" s="78" t="s">
+      <c r="M634" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N634" s="25"/>
-      <c r="O634" s="75" t="s">
-        <v>85</v>
-      </c>
-      <c r="P634" s="75" t="s">
+      <c r="O634" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P634" s="8" t="s">
         <v>2333</v>
       </c>
       <c r="Q634" s="19"/>
@@ -46259,7 +46332,7 @@
       </c>
     </row>
     <row r="635">
-      <c r="A635" s="73" t="s">
+      <c r="A635" s="16" t="s">
         <v>2341</v>
       </c>
       <c r="B635" s="6">
@@ -46268,7 +46341,7 @@
       <c r="C635" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D635" s="74" t="s">
+      <c r="D635" s="7" t="s">
         <v>2139</v>
       </c>
       <c r="E635" s="7" t="s">
@@ -46278,29 +46351,29 @@
       <c r="G635" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H635" s="75" t="s">
+      <c r="H635" s="8" t="s">
         <v>2263</v>
       </c>
-      <c r="I635" s="76">
+      <c r="I635" s="9">
         <v>44147.0</v>
       </c>
-      <c r="J635" s="77" t="s">
+      <c r="J635" s="12" t="s">
         <v>1442</v>
       </c>
-      <c r="K635" s="78" t="s">
+      <c r="K635" s="13" t="s">
         <v>2330</v>
       </c>
-      <c r="L635" s="77" t="s">
+      <c r="L635" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M635" s="78" t="s">
+      <c r="M635" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N635" s="25"/>
-      <c r="O635" s="75" t="s">
-        <v>85</v>
-      </c>
-      <c r="P635" s="75" t="s">
+      <c r="O635" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P635" s="8" t="s">
         <v>2333</v>
       </c>
       <c r="Q635" s="19"/>
@@ -46315,7 +46388,7 @@
       </c>
     </row>
     <row r="636">
-      <c r="A636" s="73" t="s">
+      <c r="A636" s="16" t="s">
         <v>2342</v>
       </c>
       <c r="B636" s="6">
@@ -46324,7 +46397,7 @@
       <c r="C636" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D636" s="74" t="s">
+      <c r="D636" s="7" t="s">
         <v>2139</v>
       </c>
       <c r="E636" s="7" t="s">
@@ -46334,29 +46407,29 @@
       <c r="G636" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H636" s="75" t="s">
+      <c r="H636" s="8" t="s">
         <v>2263</v>
       </c>
-      <c r="I636" s="76">
+      <c r="I636" s="9">
         <v>44147.0</v>
       </c>
-      <c r="J636" s="77" t="s">
+      <c r="J636" s="12" t="s">
         <v>1442</v>
       </c>
-      <c r="K636" s="78" t="s">
+      <c r="K636" s="13" t="s">
         <v>2330</v>
       </c>
-      <c r="L636" s="77" t="s">
+      <c r="L636" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M636" s="78" t="s">
+      <c r="M636" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N636" s="25"/>
-      <c r="O636" s="75" t="s">
-        <v>85</v>
-      </c>
-      <c r="P636" s="75" t="s">
+      <c r="O636" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P636" s="8" t="s">
         <v>2333</v>
       </c>
       <c r="Q636" s="19"/>
@@ -46371,7 +46444,7 @@
       </c>
     </row>
     <row r="637">
-      <c r="A637" s="73" t="s">
+      <c r="A637" s="16" t="s">
         <v>2343</v>
       </c>
       <c r="B637" s="6">
@@ -46380,7 +46453,7 @@
       <c r="C637" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D637" s="74" t="s">
+      <c r="D637" s="7" t="s">
         <v>2139</v>
       </c>
       <c r="E637" s="7" t="s">
@@ -46390,29 +46463,29 @@
       <c r="G637" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H637" s="75" t="s">
+      <c r="H637" s="8" t="s">
         <v>2263</v>
       </c>
-      <c r="I637" s="76">
+      <c r="I637" s="9">
         <v>44147.0</v>
       </c>
-      <c r="J637" s="77" t="s">
+      <c r="J637" s="12" t="s">
         <v>1442</v>
       </c>
-      <c r="K637" s="78" t="s">
+      <c r="K637" s="13" t="s">
         <v>2330</v>
       </c>
-      <c r="L637" s="77" t="s">
+      <c r="L637" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M637" s="78" t="s">
+      <c r="M637" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N637" s="25"/>
-      <c r="O637" s="75" t="s">
-        <v>85</v>
-      </c>
-      <c r="P637" s="75" t="s">
+      <c r="O637" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P637" s="8" t="s">
         <v>2333</v>
       </c>
       <c r="Q637" s="19"/>
@@ -46427,7 +46500,7 @@
       </c>
     </row>
     <row r="638">
-      <c r="A638" s="73" t="s">
+      <c r="A638" s="16" t="s">
         <v>2344</v>
       </c>
       <c r="B638" s="6">
@@ -46436,7 +46509,7 @@
       <c r="C638" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D638" s="74" t="s">
+      <c r="D638" s="7" t="s">
         <v>2139</v>
       </c>
       <c r="E638" s="7" t="s">
@@ -46446,29 +46519,29 @@
       <c r="G638" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H638" s="75" t="s">
+      <c r="H638" s="8" t="s">
         <v>2263</v>
       </c>
-      <c r="I638" s="76">
+      <c r="I638" s="9">
         <v>44147.0</v>
       </c>
-      <c r="J638" s="77" t="s">
+      <c r="J638" s="12" t="s">
         <v>1442</v>
       </c>
-      <c r="K638" s="78" t="s">
+      <c r="K638" s="13" t="s">
         <v>2330</v>
       </c>
-      <c r="L638" s="77" t="s">
+      <c r="L638" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M638" s="78" t="s">
+      <c r="M638" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N638" s="25"/>
-      <c r="O638" s="75" t="s">
-        <v>85</v>
-      </c>
-      <c r="P638" s="75" t="s">
+      <c r="O638" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P638" s="8" t="s">
         <v>2333</v>
       </c>
       <c r="Q638" s="19"/>
@@ -46483,7 +46556,7 @@
       </c>
     </row>
     <row r="639">
-      <c r="A639" s="73" t="s">
+      <c r="A639" s="16" t="s">
         <v>2345</v>
       </c>
       <c r="B639" s="6">
@@ -46492,7 +46565,7 @@
       <c r="C639" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D639" s="74" t="s">
+      <c r="D639" s="7" t="s">
         <v>2139</v>
       </c>
       <c r="E639" s="7" t="s">
@@ -46502,29 +46575,29 @@
       <c r="G639" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H639" s="75" t="s">
+      <c r="H639" s="8" t="s">
         <v>2263</v>
       </c>
-      <c r="I639" s="76">
+      <c r="I639" s="9">
         <v>44147.0</v>
       </c>
-      <c r="J639" s="77" t="s">
+      <c r="J639" s="12" t="s">
         <v>1442</v>
       </c>
-      <c r="K639" s="78" t="s">
+      <c r="K639" s="13" t="s">
         <v>2330</v>
       </c>
-      <c r="L639" s="77" t="s">
+      <c r="L639" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M639" s="78" t="s">
+      <c r="M639" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N639" s="25"/>
-      <c r="O639" s="75" t="s">
-        <v>85</v>
-      </c>
-      <c r="P639" s="75" t="s">
+      <c r="O639" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P639" s="8" t="s">
         <v>2333</v>
       </c>
       <c r="Q639" s="19"/>
@@ -46539,7 +46612,7 @@
       </c>
     </row>
     <row r="640">
-      <c r="A640" s="73" t="s">
+      <c r="A640" s="16" t="s">
         <v>2346</v>
       </c>
       <c r="B640" s="6">
@@ -46548,7 +46621,7 @@
       <c r="C640" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D640" s="74" t="s">
+      <c r="D640" s="7" t="s">
         <v>2139</v>
       </c>
       <c r="E640" s="7" t="s">
@@ -46558,29 +46631,29 @@
       <c r="G640" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H640" s="75" t="s">
+      <c r="H640" s="8" t="s">
         <v>2263</v>
       </c>
-      <c r="I640" s="76">
+      <c r="I640" s="9">
         <v>44147.0</v>
       </c>
-      <c r="J640" s="77" t="s">
+      <c r="J640" s="12" t="s">
         <v>1442</v>
       </c>
-      <c r="K640" s="78" t="s">
+      <c r="K640" s="13" t="s">
         <v>2330</v>
       </c>
-      <c r="L640" s="77" t="s">
+      <c r="L640" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M640" s="78" t="s">
+      <c r="M640" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N640" s="25"/>
-      <c r="O640" s="75" t="s">
-        <v>85</v>
-      </c>
-      <c r="P640" s="75" t="s">
+      <c r="O640" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P640" s="8" t="s">
         <v>2333</v>
       </c>
       <c r="Q640" s="19"/>
@@ -46595,7 +46668,7 @@
       </c>
     </row>
     <row r="641">
-      <c r="A641" s="73" t="s">
+      <c r="A641" s="16" t="s">
         <v>2347</v>
       </c>
       <c r="B641" s="6">
@@ -46604,7 +46677,7 @@
       <c r="C641" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D641" s="74" t="s">
+      <c r="D641" s="7" t="s">
         <v>116</v>
       </c>
       <c r="E641" s="7" t="s">
@@ -46614,29 +46687,29 @@
       <c r="G641" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H641" s="75" t="s">
+      <c r="H641" s="8" t="s">
         <v>2348</v>
       </c>
-      <c r="I641" s="76">
+      <c r="I641" s="9">
         <v>44155.0</v>
       </c>
-      <c r="J641" s="79">
+      <c r="J641" s="10">
         <v>44156.0</v>
       </c>
-      <c r="K641" s="78" t="s">
+      <c r="K641" s="13" t="s">
         <v>2330</v>
       </c>
-      <c r="L641" s="77" t="s">
+      <c r="L641" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M641" s="78" t="s">
+      <c r="M641" s="13" t="s">
         <v>2349</v>
       </c>
       <c r="N641" s="25"/>
-      <c r="O641" s="75" t="s">
-        <v>85</v>
-      </c>
-      <c r="P641" s="75" t="s">
+      <c r="O641" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P641" s="8" t="s">
         <v>2350</v>
       </c>
       <c r="Q641" s="19"/>
@@ -46651,242 +46724,500 @@
       </c>
     </row>
     <row r="642">
-      <c r="A642" s="80"/>
-      <c r="B642" s="81"/>
-      <c r="C642" s="34"/>
-      <c r="D642" s="34"/>
-      <c r="E642" s="34"/>
+      <c r="A642" s="73" t="s">
+        <v>2351</v>
+      </c>
+      <c r="B642" s="6">
+        <v>44163.0</v>
+      </c>
+      <c r="C642" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D642" s="74" t="s">
+        <v>2190</v>
+      </c>
+      <c r="E642" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F642" s="34"/>
-      <c r="G642" s="34"/>
-      <c r="H642" s="21"/>
-      <c r="I642" s="19"/>
+      <c r="G642" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H642" s="75" t="s">
+        <v>2352</v>
+      </c>
+      <c r="I642" s="76">
+        <v>44160.0</v>
+      </c>
       <c r="J642" s="10"/>
-      <c r="K642" s="22"/>
-      <c r="L642" s="23"/>
+      <c r="K642" s="77" t="s">
+        <v>2353</v>
+      </c>
+      <c r="L642" s="78" t="s">
+        <v>363</v>
+      </c>
       <c r="M642" s="22"/>
       <c r="N642" s="25"/>
-      <c r="O642" s="21"/>
-      <c r="P642" s="21"/>
+      <c r="O642" s="75" t="s">
+        <v>85</v>
+      </c>
+      <c r="P642" s="75" t="s">
+        <v>2354</v>
+      </c>
       <c r="Q642" s="19"/>
       <c r="R642" s="19"/>
-      <c r="S642" s="20"/>
+      <c r="S642" s="61" t="s">
+        <v>2355</v>
+      </c>
       <c r="T642" s="20"/>
       <c r="U642" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#641</v>
       </c>
     </row>
     <row r="643">
-      <c r="A643" s="80"/>
-      <c r="B643" s="81"/>
-      <c r="C643" s="34"/>
-      <c r="D643" s="34"/>
-      <c r="E643" s="34"/>
+      <c r="A643" s="73" t="s">
+        <v>2356</v>
+      </c>
+      <c r="B643" s="6">
+        <v>44163.0</v>
+      </c>
+      <c r="C643" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D643" s="74" t="s">
+        <v>2190</v>
+      </c>
+      <c r="E643" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F643" s="34"/>
-      <c r="G643" s="34"/>
-      <c r="H643" s="21"/>
-      <c r="I643" s="19"/>
+      <c r="G643" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H643" s="75" t="s">
+        <v>2352</v>
+      </c>
+      <c r="I643" s="76">
+        <v>44160.0</v>
+      </c>
       <c r="J643" s="10"/>
-      <c r="K643" s="22"/>
-      <c r="L643" s="23"/>
+      <c r="K643" s="77" t="s">
+        <v>2353</v>
+      </c>
+      <c r="L643" s="78" t="s">
+        <v>363</v>
+      </c>
       <c r="M643" s="22"/>
       <c r="N643" s="25"/>
-      <c r="O643" s="21"/>
-      <c r="P643" s="21"/>
+      <c r="O643" s="75" t="s">
+        <v>85</v>
+      </c>
+      <c r="P643" s="75" t="s">
+        <v>2354</v>
+      </c>
       <c r="Q643" s="19"/>
       <c r="R643" s="19"/>
-      <c r="S643" s="20"/>
+      <c r="S643" s="61" t="s">
+        <v>2355</v>
+      </c>
       <c r="T643" s="20"/>
       <c r="U643" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#642</v>
       </c>
     </row>
     <row r="644">
-      <c r="A644" s="80"/>
-      <c r="B644" s="81"/>
-      <c r="C644" s="34"/>
-      <c r="D644" s="34"/>
-      <c r="E644" s="34"/>
+      <c r="A644" s="73" t="s">
+        <v>2357</v>
+      </c>
+      <c r="B644" s="6">
+        <v>44163.0</v>
+      </c>
+      <c r="C644" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D644" s="74" t="s">
+        <v>2190</v>
+      </c>
+      <c r="E644" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F644" s="34"/>
-      <c r="G644" s="34"/>
-      <c r="H644" s="21"/>
-      <c r="I644" s="19"/>
+      <c r="G644" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H644" s="75" t="s">
+        <v>2352</v>
+      </c>
+      <c r="I644" s="76">
+        <v>44160.0</v>
+      </c>
       <c r="J644" s="10"/>
-      <c r="K644" s="22"/>
-      <c r="L644" s="23"/>
+      <c r="K644" s="77" t="s">
+        <v>2353</v>
+      </c>
+      <c r="L644" s="78" t="s">
+        <v>363</v>
+      </c>
       <c r="M644" s="22"/>
       <c r="N644" s="25"/>
-      <c r="O644" s="21"/>
-      <c r="P644" s="21"/>
+      <c r="O644" s="75" t="s">
+        <v>85</v>
+      </c>
+      <c r="P644" s="75" t="s">
+        <v>2354</v>
+      </c>
       <c r="Q644" s="19"/>
       <c r="R644" s="19"/>
-      <c r="S644" s="20"/>
+      <c r="S644" s="61" t="s">
+        <v>2355</v>
+      </c>
       <c r="T644" s="20"/>
       <c r="U644" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#643</v>
       </c>
     </row>
     <row r="645">
-      <c r="A645" s="80"/>
-      <c r="B645" s="81"/>
-      <c r="C645" s="34"/>
-      <c r="D645" s="34"/>
-      <c r="E645" s="34"/>
+      <c r="A645" s="73" t="s">
+        <v>2358</v>
+      </c>
+      <c r="B645" s="6">
+        <v>44163.0</v>
+      </c>
+      <c r="C645" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D645" s="74" t="s">
+        <v>2190</v>
+      </c>
+      <c r="E645" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F645" s="34"/>
-      <c r="G645" s="34"/>
-      <c r="H645" s="21"/>
-      <c r="I645" s="19"/>
-      <c r="J645" s="10"/>
-      <c r="K645" s="22"/>
-      <c r="L645" s="23"/>
-      <c r="M645" s="22"/>
+      <c r="G645" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H645" s="75" t="s">
+        <v>2352</v>
+      </c>
+      <c r="I645" s="76">
+        <v>44160.0</v>
+      </c>
+      <c r="J645" s="78" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K645" s="77" t="s">
+        <v>2353</v>
+      </c>
+      <c r="L645" s="78" t="s">
+        <v>363</v>
+      </c>
+      <c r="M645" s="77" t="s">
+        <v>1442</v>
+      </c>
       <c r="N645" s="25"/>
-      <c r="O645" s="21"/>
-      <c r="P645" s="21"/>
+      <c r="O645" s="75" t="s">
+        <v>85</v>
+      </c>
+      <c r="P645" s="75" t="s">
+        <v>2359</v>
+      </c>
       <c r="Q645" s="19"/>
       <c r="R645" s="19"/>
-      <c r="S645" s="20"/>
+      <c r="S645" s="61" t="s">
+        <v>2355</v>
+      </c>
       <c r="T645" s="20"/>
       <c r="U645" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#644</v>
       </c>
     </row>
     <row r="646">
-      <c r="A646" s="80"/>
-      <c r="B646" s="81"/>
-      <c r="C646" s="34"/>
-      <c r="D646" s="34"/>
-      <c r="E646" s="34"/>
+      <c r="A646" s="73" t="s">
+        <v>2360</v>
+      </c>
+      <c r="B646" s="6">
+        <v>44163.0</v>
+      </c>
+      <c r="C646" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D646" s="74" t="s">
+        <v>59</v>
+      </c>
+      <c r="E646" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F646" s="34"/>
-      <c r="G646" s="34"/>
-      <c r="H646" s="21"/>
-      <c r="I646" s="19"/>
-      <c r="J646" s="10"/>
-      <c r="K646" s="22"/>
-      <c r="L646" s="23"/>
-      <c r="M646" s="22"/>
+      <c r="G646" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H646" s="75" t="s">
+        <v>2361</v>
+      </c>
+      <c r="I646" s="76">
+        <v>44154.0</v>
+      </c>
+      <c r="J646" s="78" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K646" s="77" t="s">
+        <v>2362</v>
+      </c>
+      <c r="L646" s="78" t="s">
+        <v>426</v>
+      </c>
+      <c r="M646" s="77" t="s">
+        <v>1442</v>
+      </c>
       <c r="N646" s="25"/>
-      <c r="O646" s="21"/>
-      <c r="P646" s="21"/>
+      <c r="O646" s="75" t="s">
+        <v>85</v>
+      </c>
+      <c r="P646" s="75" t="s">
+        <v>2363</v>
+      </c>
       <c r="Q646" s="19"/>
       <c r="R646" s="19"/>
-      <c r="S646" s="20"/>
+      <c r="S646" s="61" t="s">
+        <v>2355</v>
+      </c>
       <c r="T646" s="20"/>
       <c r="U646" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#645</v>
       </c>
     </row>
     <row r="647">
-      <c r="A647" s="80"/>
-      <c r="B647" s="81"/>
-      <c r="C647" s="34"/>
-      <c r="D647" s="34"/>
-      <c r="E647" s="34"/>
+      <c r="A647" s="73" t="s">
+        <v>2364</v>
+      </c>
+      <c r="B647" s="6">
+        <v>44163.0</v>
+      </c>
+      <c r="C647" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D647" s="74" t="s">
+        <v>2139</v>
+      </c>
+      <c r="E647" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F647" s="34"/>
-      <c r="G647" s="34"/>
-      <c r="H647" s="21"/>
-      <c r="I647" s="19"/>
-      <c r="J647" s="10"/>
-      <c r="K647" s="22"/>
-      <c r="L647" s="23"/>
-      <c r="M647" s="22"/>
+      <c r="G647" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H647" s="75" t="s">
+        <v>2365</v>
+      </c>
+      <c r="I647" s="76">
+        <v>44148.0</v>
+      </c>
+      <c r="J647" s="78" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K647" s="77" t="s">
+        <v>2362</v>
+      </c>
+      <c r="L647" s="78" t="s">
+        <v>426</v>
+      </c>
+      <c r="M647" s="77" t="s">
+        <v>1442</v>
+      </c>
       <c r="N647" s="25"/>
-      <c r="O647" s="21"/>
-      <c r="P647" s="21"/>
+      <c r="O647" s="75" t="s">
+        <v>85</v>
+      </c>
+      <c r="P647" s="75" t="s">
+        <v>2366</v>
+      </c>
       <c r="Q647" s="19"/>
       <c r="R647" s="19"/>
-      <c r="S647" s="20"/>
+      <c r="S647" s="61" t="s">
+        <v>2355</v>
+      </c>
       <c r="T647" s="20"/>
       <c r="U647" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#646</v>
       </c>
     </row>
     <row r="648">
-      <c r="A648" s="80"/>
-      <c r="B648" s="81"/>
-      <c r="C648" s="34"/>
-      <c r="D648" s="34"/>
-      <c r="E648" s="34"/>
+      <c r="A648" s="73" t="s">
+        <v>2367</v>
+      </c>
+      <c r="B648" s="6">
+        <v>44163.0</v>
+      </c>
+      <c r="C648" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D648" s="74" t="s">
+        <v>2139</v>
+      </c>
+      <c r="E648" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F648" s="34"/>
-      <c r="G648" s="34"/>
-      <c r="H648" s="21"/>
-      <c r="I648" s="19"/>
-      <c r="J648" s="10"/>
-      <c r="K648" s="22"/>
-      <c r="L648" s="23"/>
-      <c r="M648" s="22"/>
+      <c r="G648" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H648" s="75" t="s">
+        <v>2365</v>
+      </c>
+      <c r="I648" s="76">
+        <v>44148.0</v>
+      </c>
+      <c r="J648" s="78" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K648" s="77" t="s">
+        <v>2362</v>
+      </c>
+      <c r="L648" s="78" t="s">
+        <v>426</v>
+      </c>
+      <c r="M648" s="77" t="s">
+        <v>1442</v>
+      </c>
       <c r="N648" s="25"/>
-      <c r="O648" s="21"/>
-      <c r="P648" s="21"/>
+      <c r="O648" s="75" t="s">
+        <v>85</v>
+      </c>
+      <c r="P648" s="75" t="s">
+        <v>2366</v>
+      </c>
       <c r="Q648" s="19"/>
       <c r="R648" s="19"/>
-      <c r="S648" s="20"/>
+      <c r="S648" s="61" t="s">
+        <v>2355</v>
+      </c>
       <c r="T648" s="20"/>
       <c r="U648" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#647</v>
       </c>
     </row>
     <row r="649">
-      <c r="A649" s="80"/>
-      <c r="B649" s="81"/>
-      <c r="C649" s="34"/>
-      <c r="D649" s="34"/>
-      <c r="E649" s="34"/>
+      <c r="A649" s="73" t="s">
+        <v>2368</v>
+      </c>
+      <c r="B649" s="6">
+        <v>44163.0</v>
+      </c>
+      <c r="C649" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D649" s="74" t="s">
+        <v>76</v>
+      </c>
+      <c r="E649" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F649" s="34"/>
-      <c r="G649" s="34"/>
-      <c r="H649" s="21"/>
-      <c r="I649" s="19"/>
-      <c r="J649" s="10"/>
-      <c r="K649" s="22"/>
-      <c r="L649" s="23"/>
-      <c r="M649" s="22"/>
+      <c r="G649" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H649" s="75" t="s">
+        <v>2369</v>
+      </c>
+      <c r="I649" s="76">
+        <v>44150.0</v>
+      </c>
+      <c r="J649" s="78" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K649" s="77" t="s">
+        <v>2370</v>
+      </c>
+      <c r="L649" s="12" t="s">
+        <v>2371</v>
+      </c>
+      <c r="M649" s="77" t="s">
+        <v>1442</v>
+      </c>
       <c r="N649" s="25"/>
-      <c r="O649" s="21"/>
-      <c r="P649" s="21"/>
+      <c r="O649" s="75" t="s">
+        <v>85</v>
+      </c>
+      <c r="P649" s="75" t="s">
+        <v>2372</v>
+      </c>
       <c r="Q649" s="19"/>
       <c r="R649" s="19"/>
-      <c r="S649" s="20"/>
+      <c r="S649" s="61" t="s">
+        <v>2355</v>
+      </c>
       <c r="T649" s="20"/>
       <c r="U649" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#648</v>
       </c>
     </row>
     <row r="650">
-      <c r="A650" s="80"/>
-      <c r="B650" s="81"/>
-      <c r="C650" s="34"/>
-      <c r="D650" s="34"/>
-      <c r="E650" s="34"/>
+      <c r="A650" s="73" t="s">
+        <v>2373</v>
+      </c>
+      <c r="B650" s="6">
+        <v>44163.0</v>
+      </c>
+      <c r="C650" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D650" s="74" t="s">
+        <v>2139</v>
+      </c>
+      <c r="E650" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F650" s="34"/>
-      <c r="G650" s="34"/>
-      <c r="H650" s="21"/>
-      <c r="I650" s="19"/>
-      <c r="J650" s="10"/>
-      <c r="K650" s="22"/>
-      <c r="L650" s="23"/>
-      <c r="M650" s="22"/>
+      <c r="G650" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H650" s="75" t="s">
+        <v>2365</v>
+      </c>
+      <c r="I650" s="76">
+        <v>44148.0</v>
+      </c>
+      <c r="J650" s="78" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K650" s="77" t="s">
+        <v>2362</v>
+      </c>
+      <c r="L650" s="78" t="s">
+        <v>426</v>
+      </c>
+      <c r="M650" s="77" t="s">
+        <v>1442</v>
+      </c>
       <c r="N650" s="25"/>
-      <c r="O650" s="21"/>
-      <c r="P650" s="21"/>
+      <c r="O650" s="75" t="s">
+        <v>85</v>
+      </c>
+      <c r="P650" s="75" t="s">
+        <v>2366</v>
+      </c>
       <c r="Q650" s="19"/>
       <c r="R650" s="19"/>
-      <c r="S650" s="20"/>
+      <c r="S650" s="61" t="s">
+        <v>2355</v>
+      </c>
       <c r="T650" s="20"/>
       <c r="U650" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#649</v>
       </c>
     </row>
     <row r="651">
-      <c r="A651" s="80"/>
-      <c r="B651" s="81"/>
+      <c r="A651" s="79"/>
+      <c r="B651" s="80"/>
       <c r="C651" s="34"/>
       <c r="D651" s="34"/>
       <c r="E651" s="34"/>
@@ -46911,8 +47242,8 @@
       </c>
     </row>
     <row r="652">
-      <c r="A652" s="80"/>
-      <c r="B652" s="81"/>
+      <c r="A652" s="79"/>
+      <c r="B652" s="80"/>
       <c r="C652" s="34"/>
       <c r="D652" s="34"/>
       <c r="E652" s="34"/>
@@ -46937,8 +47268,8 @@
       </c>
     </row>
     <row r="653">
-      <c r="A653" s="80"/>
-      <c r="B653" s="81"/>
+      <c r="A653" s="79"/>
+      <c r="B653" s="80"/>
       <c r="C653" s="34"/>
       <c r="D653" s="34"/>
       <c r="E653" s="34"/>
@@ -46963,8 +47294,8 @@
       </c>
     </row>
     <row r="654">
-      <c r="A654" s="80"/>
-      <c r="B654" s="81"/>
+      <c r="A654" s="79"/>
+      <c r="B654" s="80"/>
       <c r="C654" s="34"/>
       <c r="D654" s="34"/>
       <c r="E654" s="34"/>
@@ -46989,8 +47320,8 @@
       </c>
     </row>
     <row r="655">
-      <c r="A655" s="80"/>
-      <c r="B655" s="81"/>
+      <c r="A655" s="79"/>
+      <c r="B655" s="80"/>
       <c r="C655" s="34"/>
       <c r="D655" s="34"/>
       <c r="E655" s="34"/>
@@ -47015,8 +47346,8 @@
       </c>
     </row>
     <row r="656">
-      <c r="A656" s="80"/>
-      <c r="B656" s="81"/>
+      <c r="A656" s="79"/>
+      <c r="B656" s="80"/>
       <c r="C656" s="34"/>
       <c r="D656" s="34"/>
       <c r="E656" s="34"/>
@@ -47041,8 +47372,8 @@
       </c>
     </row>
     <row r="657">
-      <c r="A657" s="80"/>
-      <c r="B657" s="81"/>
+      <c r="A657" s="79"/>
+      <c r="B657" s="80"/>
       <c r="C657" s="34"/>
       <c r="D657" s="34"/>
       <c r="E657" s="34"/>
@@ -47067,8 +47398,8 @@
       </c>
     </row>
     <row r="658">
-      <c r="A658" s="80"/>
-      <c r="B658" s="81"/>
+      <c r="A658" s="79"/>
+      <c r="B658" s="80"/>
       <c r="C658" s="34"/>
       <c r="D658" s="34"/>
       <c r="E658" s="34"/>
@@ -47093,8 +47424,8 @@
       </c>
     </row>
     <row r="659">
-      <c r="A659" s="80"/>
-      <c r="B659" s="81"/>
+      <c r="A659" s="79"/>
+      <c r="B659" s="80"/>
       <c r="C659" s="34"/>
       <c r="D659" s="34"/>
       <c r="E659" s="34"/>
@@ -47119,8 +47450,8 @@
       </c>
     </row>
     <row r="660">
-      <c r="A660" s="80"/>
-      <c r="B660" s="81"/>
+      <c r="A660" s="79"/>
+      <c r="B660" s="80"/>
       <c r="C660" s="34"/>
       <c r="D660" s="34"/>
       <c r="E660" s="34"/>
@@ -47145,8 +47476,8 @@
       </c>
     </row>
     <row r="661">
-      <c r="A661" s="80"/>
-      <c r="B661" s="81"/>
+      <c r="A661" s="79"/>
+      <c r="B661" s="80"/>
       <c r="C661" s="34"/>
       <c r="D661" s="34"/>
       <c r="E661" s="34"/>
@@ -47171,8 +47502,8 @@
       </c>
     </row>
     <row r="662">
-      <c r="A662" s="80"/>
-      <c r="B662" s="81"/>
+      <c r="A662" s="79"/>
+      <c r="B662" s="80"/>
       <c r="C662" s="34"/>
       <c r="D662" s="34"/>
       <c r="E662" s="34"/>
@@ -47197,8 +47528,8 @@
       </c>
     </row>
     <row r="663">
-      <c r="A663" s="80"/>
-      <c r="B663" s="81"/>
+      <c r="A663" s="79"/>
+      <c r="B663" s="80"/>
       <c r="C663" s="34"/>
       <c r="D663" s="34"/>
       <c r="E663" s="34"/>
@@ -47223,8 +47554,8 @@
       </c>
     </row>
     <row r="664">
-      <c r="A664" s="80"/>
-      <c r="B664" s="81"/>
+      <c r="A664" s="79"/>
+      <c r="B664" s="80"/>
       <c r="C664" s="34"/>
       <c r="D664" s="34"/>
       <c r="E664" s="34"/>
@@ -47249,8 +47580,8 @@
       </c>
     </row>
     <row r="665">
-      <c r="A665" s="80"/>
-      <c r="B665" s="81"/>
+      <c r="A665" s="79"/>
+      <c r="B665" s="80"/>
       <c r="C665" s="34"/>
       <c r="D665" s="34"/>
       <c r="E665" s="34"/>
@@ -47275,8 +47606,8 @@
       </c>
     </row>
     <row r="666">
-      <c r="A666" s="80"/>
-      <c r="B666" s="81"/>
+      <c r="A666" s="79"/>
+      <c r="B666" s="80"/>
       <c r="C666" s="34"/>
       <c r="D666" s="34"/>
       <c r="E666" s="34"/>
@@ -47301,8 +47632,8 @@
       </c>
     </row>
     <row r="667">
-      <c r="A667" s="80"/>
-      <c r="B667" s="81"/>
+      <c r="A667" s="79"/>
+      <c r="B667" s="80"/>
       <c r="C667" s="34"/>
       <c r="D667" s="34"/>
       <c r="E667" s="34"/>
@@ -47327,8 +47658,8 @@
       </c>
     </row>
     <row r="668">
-      <c r="A668" s="80"/>
-      <c r="B668" s="81"/>
+      <c r="A668" s="79"/>
+      <c r="B668" s="80"/>
       <c r="C668" s="34"/>
       <c r="D668" s="34"/>
       <c r="E668" s="34"/>
@@ -47353,8 +47684,8 @@
       </c>
     </row>
     <row r="669">
-      <c r="A669" s="80"/>
-      <c r="B669" s="81"/>
+      <c r="A669" s="79"/>
+      <c r="B669" s="80"/>
       <c r="C669" s="34"/>
       <c r="D669" s="34"/>
       <c r="E669" s="34"/>
@@ -47379,8 +47710,8 @@
       </c>
     </row>
     <row r="670">
-      <c r="A670" s="80"/>
-      <c r="B670" s="81"/>
+      <c r="A670" s="79"/>
+      <c r="B670" s="80"/>
       <c r="C670" s="34"/>
       <c r="D670" s="34"/>
       <c r="E670" s="34"/>
@@ -47405,8 +47736,8 @@
       </c>
     </row>
     <row r="671">
-      <c r="A671" s="80"/>
-      <c r="B671" s="81"/>
+      <c r="A671" s="79"/>
+      <c r="B671" s="80"/>
       <c r="C671" s="34"/>
       <c r="D671" s="34"/>
       <c r="E671" s="34"/>
@@ -47431,8 +47762,8 @@
       </c>
     </row>
     <row r="672">
-      <c r="A672" s="80"/>
-      <c r="B672" s="81"/>
+      <c r="A672" s="79"/>
+      <c r="B672" s="80"/>
       <c r="C672" s="34"/>
       <c r="D672" s="34"/>
       <c r="E672" s="34"/>
@@ -47457,8 +47788,8 @@
       </c>
     </row>
     <row r="673">
-      <c r="A673" s="80"/>
-      <c r="B673" s="81"/>
+      <c r="A673" s="79"/>
+      <c r="B673" s="80"/>
       <c r="C673" s="34"/>
       <c r="D673" s="34"/>
       <c r="E673" s="34"/>
@@ -47483,8 +47814,8 @@
       </c>
     </row>
     <row r="674">
-      <c r="A674" s="80"/>
-      <c r="B674" s="81"/>
+      <c r="A674" s="79"/>
+      <c r="B674" s="80"/>
       <c r="C674" s="34"/>
       <c r="D674" s="34"/>
       <c r="E674" s="34"/>
@@ -47509,8 +47840,8 @@
       </c>
     </row>
     <row r="675">
-      <c r="A675" s="80"/>
-      <c r="B675" s="81"/>
+      <c r="A675" s="79"/>
+      <c r="B675" s="80"/>
       <c r="C675" s="34"/>
       <c r="D675" s="34"/>
       <c r="E675" s="34"/>
@@ -47535,8 +47866,8 @@
       </c>
     </row>
     <row r="676">
-      <c r="A676" s="80"/>
-      <c r="B676" s="81"/>
+      <c r="A676" s="79"/>
+      <c r="B676" s="80"/>
       <c r="C676" s="34"/>
       <c r="D676" s="34"/>
       <c r="E676" s="34"/>
@@ -47561,8 +47892,8 @@
       </c>
     </row>
     <row r="677">
-      <c r="A677" s="80"/>
-      <c r="B677" s="81"/>
+      <c r="A677" s="79"/>
+      <c r="B677" s="80"/>
       <c r="C677" s="34"/>
       <c r="D677" s="34"/>
       <c r="E677" s="34"/>
@@ -47587,8 +47918,8 @@
       </c>
     </row>
     <row r="678">
-      <c r="A678" s="80"/>
-      <c r="B678" s="81"/>
+      <c r="A678" s="79"/>
+      <c r="B678" s="80"/>
       <c r="C678" s="34"/>
       <c r="D678" s="34"/>
       <c r="E678" s="34"/>
@@ -47613,8 +47944,8 @@
       </c>
     </row>
     <row r="679">
-      <c r="A679" s="80"/>
-      <c r="B679" s="81"/>
+      <c r="A679" s="79"/>
+      <c r="B679" s="80"/>
       <c r="C679" s="34"/>
       <c r="D679" s="34"/>
       <c r="E679" s="34"/>
@@ -47639,8 +47970,8 @@
       </c>
     </row>
     <row r="680">
-      <c r="A680" s="80"/>
-      <c r="B680" s="81"/>
+      <c r="A680" s="79"/>
+      <c r="B680" s="80"/>
       <c r="C680" s="34"/>
       <c r="D680" s="34"/>
       <c r="E680" s="34"/>
@@ -47665,8 +47996,8 @@
       </c>
     </row>
     <row r="681">
-      <c r="A681" s="80"/>
-      <c r="B681" s="81"/>
+      <c r="A681" s="79"/>
+      <c r="B681" s="80"/>
       <c r="C681" s="34"/>
       <c r="D681" s="34"/>
       <c r="E681" s="34"/>
@@ -47691,8 +48022,8 @@
       </c>
     </row>
     <row r="682">
-      <c r="A682" s="80"/>
-      <c r="B682" s="81"/>
+      <c r="A682" s="79"/>
+      <c r="B682" s="80"/>
       <c r="C682" s="34"/>
       <c r="D682" s="34"/>
       <c r="E682" s="34"/>
@@ -47717,8 +48048,8 @@
       </c>
     </row>
     <row r="683">
-      <c r="A683" s="80"/>
-      <c r="B683" s="81"/>
+      <c r="A683" s="79"/>
+      <c r="B683" s="80"/>
       <c r="C683" s="34"/>
       <c r="D683" s="34"/>
       <c r="E683" s="34"/>
@@ -47743,8 +48074,8 @@
       </c>
     </row>
     <row r="684">
-      <c r="A684" s="80"/>
-      <c r="B684" s="81"/>
+      <c r="A684" s="79"/>
+      <c r="B684" s="80"/>
       <c r="C684" s="34"/>
       <c r="D684" s="34"/>
       <c r="E684" s="34"/>
@@ -47769,8 +48100,8 @@
       </c>
     </row>
     <row r="685">
-      <c r="A685" s="80"/>
-      <c r="B685" s="81"/>
+      <c r="A685" s="79"/>
+      <c r="B685" s="80"/>
       <c r="C685" s="34"/>
       <c r="D685" s="34"/>
       <c r="E685" s="34"/>
@@ -47795,8 +48126,8 @@
       </c>
     </row>
     <row r="686">
-      <c r="A686" s="80"/>
-      <c r="B686" s="81"/>
+      <c r="A686" s="79"/>
+      <c r="B686" s="80"/>
       <c r="C686" s="34"/>
       <c r="D686" s="34"/>
       <c r="E686" s="34"/>
@@ -47821,8 +48152,8 @@
       </c>
     </row>
     <row r="687">
-      <c r="A687" s="80"/>
-      <c r="B687" s="81"/>
+      <c r="A687" s="79"/>
+      <c r="B687" s="80"/>
       <c r="C687" s="34"/>
       <c r="D687" s="34"/>
       <c r="E687" s="34"/>
@@ -47847,8 +48178,8 @@
       </c>
     </row>
     <row r="688">
-      <c r="A688" s="80"/>
-      <c r="B688" s="81"/>
+      <c r="A688" s="79"/>
+      <c r="B688" s="80"/>
       <c r="C688" s="34"/>
       <c r="D688" s="34"/>
       <c r="E688" s="34"/>
@@ -47873,8 +48204,8 @@
       </c>
     </row>
     <row r="689">
-      <c r="A689" s="80"/>
-      <c r="B689" s="81"/>
+      <c r="A689" s="79"/>
+      <c r="B689" s="80"/>
       <c r="C689" s="34"/>
       <c r="D689" s="34"/>
       <c r="E689" s="34"/>
@@ -47899,8 +48230,8 @@
       </c>
     </row>
     <row r="690">
-      <c r="A690" s="80"/>
-      <c r="B690" s="81"/>
+      <c r="A690" s="79"/>
+      <c r="B690" s="80"/>
       <c r="C690" s="34"/>
       <c r="D690" s="34"/>
       <c r="E690" s="34"/>
@@ -47925,8 +48256,8 @@
       </c>
     </row>
     <row r="691">
-      <c r="A691" s="80"/>
-      <c r="B691" s="81"/>
+      <c r="A691" s="79"/>
+      <c r="B691" s="80"/>
       <c r="C691" s="34"/>
       <c r="D691" s="34"/>
       <c r="E691" s="34"/>
@@ -47951,8 +48282,8 @@
       </c>
     </row>
     <row r="692">
-      <c r="A692" s="80"/>
-      <c r="B692" s="81"/>
+      <c r="A692" s="79"/>
+      <c r="B692" s="80"/>
       <c r="C692" s="34"/>
       <c r="D692" s="34"/>
       <c r="E692" s="34"/>
@@ -47977,8 +48308,8 @@
       </c>
     </row>
     <row r="693">
-      <c r="A693" s="80"/>
-      <c r="B693" s="81"/>
+      <c r="A693" s="79"/>
+      <c r="B693" s="80"/>
       <c r="C693" s="34"/>
       <c r="D693" s="34"/>
       <c r="E693" s="34"/>
@@ -48003,8 +48334,8 @@
       </c>
     </row>
     <row r="694">
-      <c r="A694" s="80"/>
-      <c r="B694" s="81"/>
+      <c r="A694" s="79"/>
+      <c r="B694" s="80"/>
       <c r="C694" s="34"/>
       <c r="D694" s="34"/>
       <c r="E694" s="34"/>
@@ -48029,8 +48360,8 @@
       </c>
     </row>
     <row r="695">
-      <c r="A695" s="80"/>
-      <c r="B695" s="81"/>
+      <c r="A695" s="79"/>
+      <c r="B695" s="80"/>
       <c r="C695" s="34"/>
       <c r="D695" s="34"/>
       <c r="E695" s="34"/>
@@ -48055,8 +48386,8 @@
       </c>
     </row>
     <row r="696">
-      <c r="A696" s="80"/>
-      <c r="B696" s="81"/>
+      <c r="A696" s="79"/>
+      <c r="B696" s="80"/>
       <c r="C696" s="34"/>
       <c r="D696" s="34"/>
       <c r="E696" s="34"/>
@@ -48081,8 +48412,8 @@
       </c>
     </row>
     <row r="697">
-      <c r="A697" s="80"/>
-      <c r="B697" s="81"/>
+      <c r="A697" s="79"/>
+      <c r="B697" s="80"/>
       <c r="C697" s="34"/>
       <c r="D697" s="34"/>
       <c r="E697" s="34"/>
@@ -48107,8 +48438,8 @@
       </c>
     </row>
     <row r="698">
-      <c r="A698" s="80"/>
-      <c r="B698" s="81"/>
+      <c r="A698" s="79"/>
+      <c r="B698" s="80"/>
       <c r="C698" s="34"/>
       <c r="D698" s="34"/>
       <c r="E698" s="34"/>
@@ -48133,8 +48464,8 @@
       </c>
     </row>
     <row r="699">
-      <c r="A699" s="80"/>
-      <c r="B699" s="81"/>
+      <c r="A699" s="79"/>
+      <c r="B699" s="80"/>
       <c r="C699" s="34"/>
       <c r="D699" s="34"/>
       <c r="E699" s="34"/>
@@ -48159,8 +48490,8 @@
       </c>
     </row>
     <row r="700">
-      <c r="A700" s="80"/>
-      <c r="B700" s="81"/>
+      <c r="A700" s="79"/>
+      <c r="B700" s="80"/>
       <c r="C700" s="34"/>
       <c r="D700" s="34"/>
       <c r="E700" s="34"/>
@@ -48185,8 +48516,8 @@
       </c>
     </row>
     <row r="701">
-      <c r="A701" s="80"/>
-      <c r="B701" s="81"/>
+      <c r="A701" s="79"/>
+      <c r="B701" s="80"/>
       <c r="C701" s="34"/>
       <c r="D701" s="34"/>
       <c r="E701" s="34"/>
@@ -48794,15 +49125,24 @@
     <hyperlink r:id="rId201" ref="S639"/>
     <hyperlink r:id="rId202" ref="S640"/>
     <hyperlink r:id="rId203" ref="S641"/>
+    <hyperlink r:id="rId204" ref="S642"/>
+    <hyperlink r:id="rId205" ref="S643"/>
+    <hyperlink r:id="rId206" ref="S644"/>
+    <hyperlink r:id="rId207" ref="S645"/>
+    <hyperlink r:id="rId208" ref="S646"/>
+    <hyperlink r:id="rId209" ref="S647"/>
+    <hyperlink r:id="rId210" ref="S648"/>
+    <hyperlink r:id="rId211" ref="S649"/>
+    <hyperlink r:id="rId212" ref="S650"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId204"/>
-  <legacyDrawing r:id="rId205"/>
+  <drawing r:id="rId213"/>
+  <legacyDrawing r:id="rId214"/>
   <tableParts count="2">
-    <tablePart r:id="rId208"/>
-    <tablePart r:id="rId209"/>
+    <tablePart r:id="rId217"/>
+    <tablePart r:id="rId218"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201202
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -571,7 +571,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7684" uniqueCount="2426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7721" uniqueCount="2439">
   <si>
     <t>案例</t>
   </si>
@@ -8774,13 +8774,57 @@
     <t>#677</t>
   </si>
   <si>
+    <t>-11/16 菲律賓→台灣</t>
+  </si>
+  <si>
+    <t>11/29 採檢
+12/1 確診</t>
+  </si>
+  <si>
+    <t>新增4例境外移入COVID-19病例，自菲律賓、印尼、英國及白俄羅斯入境</t>
+  </si>
+  <si>
     <t>#678</t>
   </si>
   <si>
+    <t>-11/28 印尼→台灣</t>
+  </si>
+  <si>
+    <t>11/28 採檢
+12/1 確診</t>
+  </si>
+  <si>
+    <t>頭暈</t>
+  </si>
+  <si>
     <t>#679</t>
   </si>
   <si>
+    <t>-11/28 英國</t>
+  </si>
+  <si>
+    <t>全身倦怠 流鼻水 鼻塞 嗅覺喪失 味覺喪失</t>
+  </si>
+  <si>
+    <t>長期於英國工作</t>
+  </si>
+  <si>
     <t>#680</t>
+  </si>
+  <si>
+    <t>白俄羅斯</t>
+  </si>
+  <si>
+    <t>-10月中旬 白俄羅斯
+-11/13 白俄羅斯→台灣</t>
+  </si>
+  <si>
+    <t>11/30 採檢
+12/1 確診</t>
+  </si>
+  <si>
+    <t>10月中旬返回母國探親，11月13日再次來臺工作，入境迄今無疑似症狀
+個案檢疫期滿後，於11月30日由公司安排至醫院自費採檢</t>
   </si>
 </sst>
 </file>
@@ -8791,7 +8835,7 @@
     <numFmt numFmtId="164" formatCode="mm&quot;月&quot;dd&quot;日 &quot;dddd"/>
     <numFmt numFmtId="165" formatCode="m/d"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="19">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -8876,7 +8920,6 @@
       <u/>
       <color rgb="FF0000FF"/>
     </font>
-    <font/>
   </fonts>
   <fills count="7">
     <fill>
@@ -8922,7 +8965,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="76">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -9143,12 +9186,6 @@
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -48814,33 +48851,55 @@
       </c>
     </row>
     <row r="678">
-      <c r="A678" s="74" t="s">
+      <c r="A678" s="16" t="s">
         <v>2422</v>
       </c>
       <c r="B678" s="6">
         <v>44166.0</v>
       </c>
-      <c r="C678" s="34"/>
-      <c r="D678" s="34"/>
-      <c r="E678" s="34"/>
+      <c r="C678" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D678" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E678" s="7" t="s">
+        <v>205</v>
+      </c>
       <c r="F678" s="34"/>
       <c r="G678" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H678" s="21"/>
-      <c r="I678" s="19"/>
-      <c r="J678" s="10"/>
-      <c r="K678" s="22"/>
-      <c r="L678" s="23"/>
-      <c r="M678" s="22"/>
+      <c r="H678" s="8" t="s">
+        <v>2423</v>
+      </c>
+      <c r="I678" s="9">
+        <v>44151.0</v>
+      </c>
+      <c r="J678" s="10">
+        <v>44162.0</v>
+      </c>
+      <c r="K678" s="13" t="s">
+        <v>2424</v>
+      </c>
+      <c r="L678" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M678" s="13" t="s">
+        <v>482</v>
+      </c>
       <c r="N678" s="25"/>
-      <c r="O678" s="75" t="s">
+      <c r="O678" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P678" s="21"/>
+      <c r="P678" s="8" t="s">
+        <v>2182</v>
+      </c>
       <c r="Q678" s="19"/>
       <c r="R678" s="19"/>
-      <c r="S678" s="20"/>
+      <c r="S678" s="61" t="s">
+        <v>2425</v>
+      </c>
       <c r="T678" s="20"/>
       <c r="U678" s="18" t="str">
         <f t="shared" si="1"/>
@@ -48848,33 +48907,55 @@
       </c>
     </row>
     <row r="679">
-      <c r="A679" s="74" t="s">
-        <v>2423</v>
+      <c r="A679" s="16" t="s">
+        <v>2426</v>
       </c>
       <c r="B679" s="6">
         <v>44166.0</v>
       </c>
-      <c r="C679" s="34"/>
-      <c r="D679" s="34"/>
-      <c r="E679" s="34"/>
+      <c r="C679" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D679" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E679" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F679" s="34"/>
       <c r="G679" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H679" s="21"/>
-      <c r="I679" s="19"/>
-      <c r="J679" s="10"/>
-      <c r="K679" s="22"/>
-      <c r="L679" s="23"/>
-      <c r="M679" s="22"/>
+      <c r="H679" s="8" t="s">
+        <v>2427</v>
+      </c>
+      <c r="I679" s="9">
+        <v>44163.0</v>
+      </c>
+      <c r="J679" s="10">
+        <v>44156.0</v>
+      </c>
+      <c r="K679" s="13" t="s">
+        <v>2428</v>
+      </c>
+      <c r="L679" s="12" t="s">
+        <v>363</v>
+      </c>
+      <c r="M679" s="13" t="s">
+        <v>2429</v>
+      </c>
       <c r="N679" s="25"/>
-      <c r="O679" s="75" t="s">
+      <c r="O679" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P679" s="21"/>
+      <c r="P679" s="8" t="s">
+        <v>2182</v>
+      </c>
       <c r="Q679" s="19"/>
       <c r="R679" s="19"/>
-      <c r="S679" s="20"/>
+      <c r="S679" s="61" t="s">
+        <v>2425</v>
+      </c>
       <c r="T679" s="20"/>
       <c r="U679" s="18" t="str">
         <f t="shared" si="1"/>
@@ -48882,33 +48963,55 @@
       </c>
     </row>
     <row r="680">
-      <c r="A680" s="74" t="s">
-        <v>2424</v>
+      <c r="A680" s="16" t="s">
+        <v>2430</v>
       </c>
       <c r="B680" s="6">
         <v>44166.0</v>
       </c>
-      <c r="C680" s="34"/>
-      <c r="D680" s="34"/>
-      <c r="E680" s="34"/>
+      <c r="C680" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D680" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E680" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F680" s="34"/>
       <c r="G680" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H680" s="21"/>
-      <c r="I680" s="19"/>
-      <c r="J680" s="10"/>
-      <c r="K680" s="22"/>
-      <c r="L680" s="23"/>
-      <c r="M680" s="22"/>
+      <c r="H680" s="8" t="s">
+        <v>2431</v>
+      </c>
+      <c r="I680" s="9">
+        <v>44163.0</v>
+      </c>
+      <c r="J680" s="10">
+        <v>44130.0</v>
+      </c>
+      <c r="K680" s="13" t="s">
+        <v>2428</v>
+      </c>
+      <c r="L680" s="12" t="s">
+        <v>363</v>
+      </c>
+      <c r="M680" s="13" t="s">
+        <v>2432</v>
+      </c>
       <c r="N680" s="25"/>
-      <c r="O680" s="75" t="s">
+      <c r="O680" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P680" s="21"/>
+      <c r="P680" s="8" t="s">
+        <v>2433</v>
+      </c>
       <c r="Q680" s="19"/>
       <c r="R680" s="19"/>
-      <c r="S680" s="20"/>
+      <c r="S680" s="61" t="s">
+        <v>2425</v>
+      </c>
       <c r="T680" s="20"/>
       <c r="U680" s="18" t="str">
         <f t="shared" si="1"/>
@@ -48916,33 +49019,55 @@
       </c>
     </row>
     <row r="681">
-      <c r="A681" s="74" t="s">
-        <v>2425</v>
+      <c r="A681" s="16" t="s">
+        <v>2434</v>
       </c>
       <c r="B681" s="6">
         <v>44166.0</v>
       </c>
-      <c r="C681" s="34"/>
-      <c r="D681" s="34"/>
-      <c r="E681" s="34"/>
+      <c r="C681" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D681" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E681" s="7" t="s">
+        <v>2435</v>
+      </c>
       <c r="F681" s="34"/>
       <c r="G681" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H681" s="21"/>
-      <c r="I681" s="19"/>
-      <c r="J681" s="10"/>
-      <c r="K681" s="22"/>
-      <c r="L681" s="23"/>
-      <c r="M681" s="22"/>
+      <c r="H681" s="8" t="s">
+        <v>2436</v>
+      </c>
+      <c r="I681" s="9">
+        <v>44148.0</v>
+      </c>
+      <c r="J681" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K681" s="13" t="s">
+        <v>2437</v>
+      </c>
+      <c r="L681" s="12" t="s">
+        <v>1674</v>
+      </c>
+      <c r="M681" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N681" s="25"/>
-      <c r="O681" s="75" t="s">
+      <c r="O681" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P681" s="21"/>
+      <c r="P681" s="8" t="s">
+        <v>2438</v>
+      </c>
       <c r="Q681" s="19"/>
       <c r="R681" s="19"/>
-      <c r="S681" s="20"/>
+      <c r="S681" s="61" t="s">
+        <v>2425</v>
+      </c>
       <c r="T681" s="20"/>
       <c r="U681" s="18" t="str">
         <f t="shared" si="1"/>
@@ -48950,8 +49075,8 @@
       </c>
     </row>
     <row r="682">
-      <c r="A682" s="76"/>
-      <c r="B682" s="77"/>
+      <c r="A682" s="74"/>
+      <c r="B682" s="75"/>
       <c r="C682" s="34"/>
       <c r="D682" s="34"/>
       <c r="E682" s="34"/>
@@ -48976,8 +49101,8 @@
       </c>
     </row>
     <row r="683">
-      <c r="A683" s="76"/>
-      <c r="B683" s="77"/>
+      <c r="A683" s="74"/>
+      <c r="B683" s="75"/>
       <c r="C683" s="34"/>
       <c r="D683" s="34"/>
       <c r="E683" s="34"/>
@@ -49002,8 +49127,8 @@
       </c>
     </row>
     <row r="684">
-      <c r="A684" s="76"/>
-      <c r="B684" s="77"/>
+      <c r="A684" s="74"/>
+      <c r="B684" s="75"/>
       <c r="C684" s="34"/>
       <c r="D684" s="34"/>
       <c r="E684" s="34"/>
@@ -49028,8 +49153,8 @@
       </c>
     </row>
     <row r="685">
-      <c r="A685" s="76"/>
-      <c r="B685" s="77"/>
+      <c r="A685" s="74"/>
+      <c r="B685" s="75"/>
       <c r="C685" s="34"/>
       <c r="D685" s="34"/>
       <c r="E685" s="34"/>
@@ -49054,8 +49179,8 @@
       </c>
     </row>
     <row r="686">
-      <c r="A686" s="76"/>
-      <c r="B686" s="77"/>
+      <c r="A686" s="74"/>
+      <c r="B686" s="75"/>
       <c r="C686" s="34"/>
       <c r="D686" s="34"/>
       <c r="E686" s="34"/>
@@ -49080,8 +49205,8 @@
       </c>
     </row>
     <row r="687">
-      <c r="A687" s="76"/>
-      <c r="B687" s="77"/>
+      <c r="A687" s="74"/>
+      <c r="B687" s="75"/>
       <c r="C687" s="34"/>
       <c r="D687" s="34"/>
       <c r="E687" s="34"/>
@@ -49106,8 +49231,8 @@
       </c>
     </row>
     <row r="688">
-      <c r="A688" s="76"/>
-      <c r="B688" s="77"/>
+      <c r="A688" s="74"/>
+      <c r="B688" s="75"/>
       <c r="C688" s="34"/>
       <c r="D688" s="34"/>
       <c r="E688" s="34"/>
@@ -49132,8 +49257,8 @@
       </c>
     </row>
     <row r="689">
-      <c r="A689" s="76"/>
-      <c r="B689" s="77"/>
+      <c r="A689" s="74"/>
+      <c r="B689" s="75"/>
       <c r="C689" s="34"/>
       <c r="D689" s="34"/>
       <c r="E689" s="34"/>
@@ -49158,8 +49283,8 @@
       </c>
     </row>
     <row r="690">
-      <c r="A690" s="76"/>
-      <c r="B690" s="77"/>
+      <c r="A690" s="74"/>
+      <c r="B690" s="75"/>
       <c r="C690" s="34"/>
       <c r="D690" s="34"/>
       <c r="E690" s="34"/>
@@ -49184,8 +49309,8 @@
       </c>
     </row>
     <row r="691">
-      <c r="A691" s="76"/>
-      <c r="B691" s="77"/>
+      <c r="A691" s="74"/>
+      <c r="B691" s="75"/>
       <c r="C691" s="34"/>
       <c r="D691" s="34"/>
       <c r="E691" s="34"/>
@@ -49210,8 +49335,8 @@
       </c>
     </row>
     <row r="692">
-      <c r="A692" s="76"/>
-      <c r="B692" s="77"/>
+      <c r="A692" s="74"/>
+      <c r="B692" s="75"/>
       <c r="C692" s="34"/>
       <c r="D692" s="34"/>
       <c r="E692" s="34"/>
@@ -49236,8 +49361,8 @@
       </c>
     </row>
     <row r="693">
-      <c r="A693" s="76"/>
-      <c r="B693" s="77"/>
+      <c r="A693" s="74"/>
+      <c r="B693" s="75"/>
       <c r="C693" s="34"/>
       <c r="D693" s="34"/>
       <c r="E693" s="34"/>
@@ -49262,8 +49387,8 @@
       </c>
     </row>
     <row r="694">
-      <c r="A694" s="76"/>
-      <c r="B694" s="77"/>
+      <c r="A694" s="74"/>
+      <c r="B694" s="75"/>
       <c r="C694" s="34"/>
       <c r="D694" s="34"/>
       <c r="E694" s="34"/>
@@ -49288,8 +49413,8 @@
       </c>
     </row>
     <row r="695">
-      <c r="A695" s="76"/>
-      <c r="B695" s="77"/>
+      <c r="A695" s="74"/>
+      <c r="B695" s="75"/>
       <c r="C695" s="34"/>
       <c r="D695" s="34"/>
       <c r="E695" s="34"/>
@@ -49314,8 +49439,8 @@
       </c>
     </row>
     <row r="696">
-      <c r="A696" s="76"/>
-      <c r="B696" s="77"/>
+      <c r="A696" s="74"/>
+      <c r="B696" s="75"/>
       <c r="C696" s="34"/>
       <c r="D696" s="34"/>
       <c r="E696" s="34"/>
@@ -49340,8 +49465,8 @@
       </c>
     </row>
     <row r="697">
-      <c r="A697" s="76"/>
-      <c r="B697" s="77"/>
+      <c r="A697" s="74"/>
+      <c r="B697" s="75"/>
       <c r="C697" s="34"/>
       <c r="D697" s="34"/>
       <c r="E697" s="34"/>
@@ -49366,8 +49491,8 @@
       </c>
     </row>
     <row r="698">
-      <c r="A698" s="76"/>
-      <c r="B698" s="77"/>
+      <c r="A698" s="74"/>
+      <c r="B698" s="75"/>
       <c r="C698" s="34"/>
       <c r="D698" s="34"/>
       <c r="E698" s="34"/>
@@ -49392,8 +49517,8 @@
       </c>
     </row>
     <row r="699">
-      <c r="A699" s="76"/>
-      <c r="B699" s="77"/>
+      <c r="A699" s="74"/>
+      <c r="B699" s="75"/>
       <c r="C699" s="34"/>
       <c r="D699" s="34"/>
       <c r="E699" s="34"/>
@@ -49418,8 +49543,8 @@
       </c>
     </row>
     <row r="700">
-      <c r="A700" s="76"/>
-      <c r="B700" s="77"/>
+      <c r="A700" s="74"/>
+      <c r="B700" s="75"/>
       <c r="C700" s="34"/>
       <c r="D700" s="34"/>
       <c r="E700" s="34"/>
@@ -49444,8 +49569,8 @@
       </c>
     </row>
     <row r="701">
-      <c r="A701" s="76"/>
-      <c r="B701" s="77"/>
+      <c r="A701" s="74"/>
+      <c r="B701" s="75"/>
       <c r="C701" s="34"/>
       <c r="D701" s="34"/>
       <c r="E701" s="34"/>
@@ -49470,8 +49595,8 @@
       </c>
     </row>
     <row r="702">
-      <c r="A702" s="76"/>
-      <c r="B702" s="77"/>
+      <c r="A702" s="74"/>
+      <c r="B702" s="75"/>
       <c r="C702" s="34"/>
       <c r="D702" s="34"/>
       <c r="E702" s="34"/>
@@ -49496,8 +49621,8 @@
       </c>
     </row>
     <row r="703">
-      <c r="A703" s="76"/>
-      <c r="B703" s="77"/>
+      <c r="A703" s="74"/>
+      <c r="B703" s="75"/>
       <c r="C703" s="34"/>
       <c r="D703" s="34"/>
       <c r="E703" s="34"/>
@@ -49522,8 +49647,8 @@
       </c>
     </row>
     <row r="704">
-      <c r="A704" s="76"/>
-      <c r="B704" s="77"/>
+      <c r="A704" s="74"/>
+      <c r="B704" s="75"/>
       <c r="C704" s="34"/>
       <c r="D704" s="34"/>
       <c r="E704" s="34"/>
@@ -49548,8 +49673,8 @@
       </c>
     </row>
     <row r="705">
-      <c r="A705" s="76"/>
-      <c r="B705" s="77"/>
+      <c r="A705" s="74"/>
+      <c r="B705" s="75"/>
       <c r="C705" s="34"/>
       <c r="D705" s="34"/>
       <c r="E705" s="34"/>
@@ -49574,8 +49699,8 @@
       </c>
     </row>
     <row r="706">
-      <c r="A706" s="76"/>
-      <c r="B706" s="77"/>
+      <c r="A706" s="74"/>
+      <c r="B706" s="75"/>
       <c r="C706" s="34"/>
       <c r="D706" s="34"/>
       <c r="E706" s="34"/>
@@ -49600,8 +49725,8 @@
       </c>
     </row>
     <row r="707">
-      <c r="A707" s="76"/>
-      <c r="B707" s="77"/>
+      <c r="A707" s="74"/>
+      <c r="B707" s="75"/>
       <c r="C707" s="34"/>
       <c r="D707" s="34"/>
       <c r="E707" s="34"/>
@@ -49626,8 +49751,8 @@
       </c>
     </row>
     <row r="708">
-      <c r="A708" s="76"/>
-      <c r="B708" s="77"/>
+      <c r="A708" s="74"/>
+      <c r="B708" s="75"/>
       <c r="C708" s="34"/>
       <c r="D708" s="34"/>
       <c r="E708" s="34"/>
@@ -49652,8 +49777,8 @@
       </c>
     </row>
     <row r="709">
-      <c r="A709" s="76"/>
-      <c r="B709" s="77"/>
+      <c r="A709" s="74"/>
+      <c r="B709" s="75"/>
       <c r="C709" s="34"/>
       <c r="D709" s="34"/>
       <c r="E709" s="34"/>
@@ -49678,8 +49803,8 @@
       </c>
     </row>
     <row r="710">
-      <c r="A710" s="76"/>
-      <c r="B710" s="77"/>
+      <c r="A710" s="74"/>
+      <c r="B710" s="75"/>
       <c r="C710" s="34"/>
       <c r="D710" s="34"/>
       <c r="E710" s="34"/>
@@ -49704,8 +49829,8 @@
       </c>
     </row>
     <row r="711">
-      <c r="A711" s="76"/>
-      <c r="B711" s="77"/>
+      <c r="A711" s="74"/>
+      <c r="B711" s="75"/>
       <c r="C711" s="34"/>
       <c r="D711" s="34"/>
       <c r="E711" s="34"/>
@@ -49730,8 +49855,8 @@
       </c>
     </row>
     <row r="712">
-      <c r="A712" s="76"/>
-      <c r="B712" s="77"/>
+      <c r="A712" s="74"/>
+      <c r="B712" s="75"/>
       <c r="C712" s="34"/>
       <c r="D712" s="34"/>
       <c r="E712" s="34"/>
@@ -49756,8 +49881,8 @@
       </c>
     </row>
     <row r="713">
-      <c r="A713" s="76"/>
-      <c r="B713" s="77"/>
+      <c r="A713" s="74"/>
+      <c r="B713" s="75"/>
       <c r="C713" s="34"/>
       <c r="D713" s="34"/>
       <c r="E713" s="34"/>
@@ -49782,8 +49907,8 @@
       </c>
     </row>
     <row r="714">
-      <c r="A714" s="76"/>
-      <c r="B714" s="77"/>
+      <c r="A714" s="74"/>
+      <c r="B714" s="75"/>
       <c r="C714" s="34"/>
       <c r="D714" s="34"/>
       <c r="E714" s="34"/>
@@ -49808,8 +49933,8 @@
       </c>
     </row>
     <row r="715">
-      <c r="A715" s="76"/>
-      <c r="B715" s="77"/>
+      <c r="A715" s="74"/>
+      <c r="B715" s="75"/>
       <c r="C715" s="34"/>
       <c r="D715" s="34"/>
       <c r="E715" s="34"/>
@@ -49834,8 +49959,8 @@
       </c>
     </row>
     <row r="716">
-      <c r="A716" s="76"/>
-      <c r="B716" s="77"/>
+      <c r="A716" s="74"/>
+      <c r="B716" s="75"/>
       <c r="C716" s="34"/>
       <c r="D716" s="34"/>
       <c r="E716" s="34"/>
@@ -49860,8 +49985,8 @@
       </c>
     </row>
     <row r="717">
-      <c r="A717" s="76"/>
-      <c r="B717" s="77"/>
+      <c r="A717" s="74"/>
+      <c r="B717" s="75"/>
       <c r="C717" s="34"/>
       <c r="D717" s="34"/>
       <c r="E717" s="34"/>
@@ -49886,8 +50011,8 @@
       </c>
     </row>
     <row r="718">
-      <c r="A718" s="76"/>
-      <c r="B718" s="77"/>
+      <c r="A718" s="74"/>
+      <c r="B718" s="75"/>
       <c r="C718" s="34"/>
       <c r="D718" s="34"/>
       <c r="E718" s="34"/>
@@ -49912,8 +50037,8 @@
       </c>
     </row>
     <row r="719">
-      <c r="A719" s="76"/>
-      <c r="B719" s="77"/>
+      <c r="A719" s="74"/>
+      <c r="B719" s="75"/>
       <c r="C719" s="34"/>
       <c r="D719" s="34"/>
       <c r="E719" s="34"/>
@@ -49938,8 +50063,8 @@
       </c>
     </row>
     <row r="720">
-      <c r="A720" s="76"/>
-      <c r="B720" s="77"/>
+      <c r="A720" s="74"/>
+      <c r="B720" s="75"/>
       <c r="C720" s="34"/>
       <c r="D720" s="34"/>
       <c r="E720" s="34"/>
@@ -49964,8 +50089,8 @@
       </c>
     </row>
     <row r="721">
-      <c r="A721" s="76"/>
-      <c r="B721" s="77"/>
+      <c r="A721" s="74"/>
+      <c r="B721" s="75"/>
       <c r="C721" s="34"/>
       <c r="D721" s="34"/>
       <c r="E721" s="34"/>
@@ -49990,8 +50115,8 @@
       </c>
     </row>
     <row r="722">
-      <c r="A722" s="76"/>
-      <c r="B722" s="77"/>
+      <c r="A722" s="74"/>
+      <c r="B722" s="75"/>
       <c r="C722" s="34"/>
       <c r="D722" s="34"/>
       <c r="E722" s="34"/>
@@ -50016,8 +50141,8 @@
       </c>
     </row>
     <row r="723">
-      <c r="A723" s="76"/>
-      <c r="B723" s="77"/>
+      <c r="A723" s="74"/>
+      <c r="B723" s="75"/>
       <c r="C723" s="34"/>
       <c r="D723" s="34"/>
       <c r="E723" s="34"/>
@@ -50042,8 +50167,8 @@
       </c>
     </row>
     <row r="724">
-      <c r="A724" s="76"/>
-      <c r="B724" s="77"/>
+      <c r="A724" s="74"/>
+      <c r="B724" s="75"/>
       <c r="C724" s="34"/>
       <c r="D724" s="34"/>
       <c r="E724" s="34"/>
@@ -50068,8 +50193,8 @@
       </c>
     </row>
     <row r="725">
-      <c r="A725" s="76"/>
-      <c r="B725" s="77"/>
+      <c r="A725" s="74"/>
+      <c r="B725" s="75"/>
       <c r="C725" s="34"/>
       <c r="D725" s="34"/>
       <c r="E725" s="34"/>
@@ -50094,8 +50219,8 @@
       </c>
     </row>
     <row r="726">
-      <c r="A726" s="76"/>
-      <c r="B726" s="77"/>
+      <c r="A726" s="74"/>
+      <c r="B726" s="75"/>
       <c r="C726" s="34"/>
       <c r="D726" s="34"/>
       <c r="E726" s="34"/>
@@ -50120,8 +50245,8 @@
       </c>
     </row>
     <row r="727">
-      <c r="A727" s="76"/>
-      <c r="B727" s="77"/>
+      <c r="A727" s="74"/>
+      <c r="B727" s="75"/>
       <c r="C727" s="34"/>
       <c r="D727" s="34"/>
       <c r="E727" s="34"/>
@@ -50146,8 +50271,8 @@
       </c>
     </row>
     <row r="728">
-      <c r="A728" s="76"/>
-      <c r="B728" s="77"/>
+      <c r="A728" s="74"/>
+      <c r="B728" s="75"/>
       <c r="C728" s="34"/>
       <c r="D728" s="34"/>
       <c r="E728" s="34"/>
@@ -50172,8 +50297,8 @@
       </c>
     </row>
     <row r="729">
-      <c r="A729" s="76"/>
-      <c r="B729" s="77"/>
+      <c r="A729" s="74"/>
+      <c r="B729" s="75"/>
       <c r="C729" s="34"/>
       <c r="D729" s="34"/>
       <c r="E729" s="34"/>
@@ -50198,8 +50323,8 @@
       </c>
     </row>
     <row r="730">
-      <c r="A730" s="76"/>
-      <c r="B730" s="77"/>
+      <c r="A730" s="74"/>
+      <c r="B730" s="75"/>
       <c r="C730" s="34"/>
       <c r="D730" s="34"/>
       <c r="E730" s="34"/>
@@ -50224,8 +50349,8 @@
       </c>
     </row>
     <row r="731">
-      <c r="A731" s="76"/>
-      <c r="B731" s="77"/>
+      <c r="A731" s="74"/>
+      <c r="B731" s="75"/>
       <c r="C731" s="34"/>
       <c r="D731" s="34"/>
       <c r="E731" s="34"/>
@@ -50250,8 +50375,8 @@
       </c>
     </row>
     <row r="732">
-      <c r="A732" s="76"/>
-      <c r="B732" s="77"/>
+      <c r="A732" s="74"/>
+      <c r="B732" s="75"/>
       <c r="C732" s="34"/>
       <c r="D732" s="34"/>
       <c r="E732" s="34"/>
@@ -50276,8 +50401,8 @@
       </c>
     </row>
     <row r="733">
-      <c r="A733" s="76"/>
-      <c r="B733" s="77"/>
+      <c r="A733" s="74"/>
+      <c r="B733" s="75"/>
       <c r="C733" s="34"/>
       <c r="D733" s="34"/>
       <c r="E733" s="34"/>
@@ -50302,8 +50427,8 @@
       </c>
     </row>
     <row r="734">
-      <c r="A734" s="76"/>
-      <c r="B734" s="77"/>
+      <c r="A734" s="74"/>
+      <c r="B734" s="75"/>
       <c r="C734" s="34"/>
       <c r="D734" s="34"/>
       <c r="E734" s="34"/>
@@ -50328,8 +50453,8 @@
       </c>
     </row>
     <row r="735">
-      <c r="A735" s="76"/>
-      <c r="B735" s="77"/>
+      <c r="A735" s="74"/>
+      <c r="B735" s="75"/>
       <c r="C735" s="34"/>
       <c r="D735" s="34"/>
       <c r="E735" s="34"/>
@@ -50354,8 +50479,8 @@
       </c>
     </row>
     <row r="736">
-      <c r="A736" s="76"/>
-      <c r="B736" s="77"/>
+      <c r="A736" s="74"/>
+      <c r="B736" s="75"/>
       <c r="C736" s="34"/>
       <c r="D736" s="34"/>
       <c r="E736" s="34"/>
@@ -50380,8 +50505,8 @@
       </c>
     </row>
     <row r="737">
-      <c r="A737" s="76"/>
-      <c r="B737" s="77"/>
+      <c r="A737" s="74"/>
+      <c r="B737" s="75"/>
       <c r="C737" s="34"/>
       <c r="D737" s="34"/>
       <c r="E737" s="34"/>
@@ -50406,8 +50531,8 @@
       </c>
     </row>
     <row r="738">
-      <c r="A738" s="76"/>
-      <c r="B738" s="77"/>
+      <c r="A738" s="74"/>
+      <c r="B738" s="75"/>
       <c r="C738" s="34"/>
       <c r="D738" s="34"/>
       <c r="E738" s="34"/>
@@ -50432,8 +50557,8 @@
       </c>
     </row>
     <row r="739">
-      <c r="A739" s="76"/>
-      <c r="B739" s="77"/>
+      <c r="A739" s="74"/>
+      <c r="B739" s="75"/>
       <c r="C739" s="34"/>
       <c r="D739" s="34"/>
       <c r="E739" s="34"/>
@@ -50458,8 +50583,8 @@
       </c>
     </row>
     <row r="740">
-      <c r="A740" s="76"/>
-      <c r="B740" s="77"/>
+      <c r="A740" s="74"/>
+      <c r="B740" s="75"/>
       <c r="C740" s="34"/>
       <c r="D740" s="34"/>
       <c r="E740" s="34"/>
@@ -50484,8 +50609,8 @@
       </c>
     </row>
     <row r="741">
-      <c r="A741" s="76"/>
-      <c r="B741" s="77"/>
+      <c r="A741" s="74"/>
+      <c r="B741" s="75"/>
       <c r="C741" s="34"/>
       <c r="D741" s="34"/>
       <c r="E741" s="34"/>
@@ -50510,8 +50635,8 @@
       </c>
     </row>
     <row r="742">
-      <c r="A742" s="76"/>
-      <c r="B742" s="77"/>
+      <c r="A742" s="74"/>
+      <c r="B742" s="75"/>
       <c r="C742" s="34"/>
       <c r="D742" s="34"/>
       <c r="E742" s="34"/>
@@ -50536,8 +50661,8 @@
       </c>
     </row>
     <row r="743">
-      <c r="A743" s="76"/>
-      <c r="B743" s="77"/>
+      <c r="A743" s="74"/>
+      <c r="B743" s="75"/>
       <c r="C743" s="34"/>
       <c r="D743" s="34"/>
       <c r="E743" s="34"/>
@@ -50562,8 +50687,8 @@
       </c>
     </row>
     <row r="744">
-      <c r="A744" s="76"/>
-      <c r="B744" s="77"/>
+      <c r="A744" s="74"/>
+      <c r="B744" s="75"/>
       <c r="C744" s="34"/>
       <c r="D744" s="34"/>
       <c r="E744" s="34"/>
@@ -50588,8 +50713,8 @@
       </c>
     </row>
     <row r="745">
-      <c r="A745" s="76"/>
-      <c r="B745" s="77"/>
+      <c r="A745" s="74"/>
+      <c r="B745" s="75"/>
       <c r="C745" s="34"/>
       <c r="D745" s="34"/>
       <c r="E745" s="34"/>
@@ -50614,8 +50739,8 @@
       </c>
     </row>
     <row r="746">
-      <c r="A746" s="76"/>
-      <c r="B746" s="77"/>
+      <c r="A746" s="74"/>
+      <c r="B746" s="75"/>
       <c r="C746" s="34"/>
       <c r="D746" s="34"/>
       <c r="E746" s="34"/>
@@ -50640,8 +50765,8 @@
       </c>
     </row>
     <row r="747">
-      <c r="A747" s="76"/>
-      <c r="B747" s="77"/>
+      <c r="A747" s="74"/>
+      <c r="B747" s="75"/>
       <c r="C747" s="34"/>
       <c r="D747" s="34"/>
       <c r="E747" s="34"/>
@@ -50666,8 +50791,8 @@
       </c>
     </row>
     <row r="748">
-      <c r="A748" s="76"/>
-      <c r="B748" s="77"/>
+      <c r="A748" s="74"/>
+      <c r="B748" s="75"/>
       <c r="C748" s="34"/>
       <c r="D748" s="34"/>
       <c r="E748" s="34"/>
@@ -50692,8 +50817,8 @@
       </c>
     </row>
     <row r="749">
-      <c r="A749" s="76"/>
-      <c r="B749" s="77"/>
+      <c r="A749" s="74"/>
+      <c r="B749" s="75"/>
       <c r="C749" s="34"/>
       <c r="D749" s="34"/>
       <c r="E749" s="34"/>
@@ -50718,8 +50843,8 @@
       </c>
     </row>
     <row r="750">
-      <c r="A750" s="76"/>
-      <c r="B750" s="77"/>
+      <c r="A750" s="74"/>
+      <c r="B750" s="75"/>
       <c r="C750" s="34"/>
       <c r="D750" s="34"/>
       <c r="E750" s="34"/>
@@ -50744,8 +50869,8 @@
       </c>
     </row>
     <row r="751">
-      <c r="A751" s="76"/>
-      <c r="B751" s="77"/>
+      <c r="A751" s="74"/>
+      <c r="B751" s="75"/>
       <c r="C751" s="34"/>
       <c r="D751" s="34"/>
       <c r="E751" s="34"/>
@@ -50770,8 +50895,8 @@
       </c>
     </row>
     <row r="752">
-      <c r="A752" s="76"/>
-      <c r="B752" s="77"/>
+      <c r="A752" s="74"/>
+      <c r="B752" s="75"/>
       <c r="C752" s="34"/>
       <c r="D752" s="34"/>
       <c r="E752" s="34"/>
@@ -50796,8 +50921,8 @@
       </c>
     </row>
     <row r="753">
-      <c r="A753" s="76"/>
-      <c r="B753" s="77"/>
+      <c r="A753" s="74"/>
+      <c r="B753" s="75"/>
       <c r="C753" s="34"/>
       <c r="D753" s="34"/>
       <c r="E753" s="34"/>
@@ -50822,8 +50947,8 @@
       </c>
     </row>
     <row r="754">
-      <c r="A754" s="76"/>
-      <c r="B754" s="77"/>
+      <c r="A754" s="74"/>
+      <c r="B754" s="75"/>
       <c r="C754" s="34"/>
       <c r="D754" s="34"/>
       <c r="E754" s="34"/>
@@ -50848,8 +50973,8 @@
       </c>
     </row>
     <row r="755">
-      <c r="A755" s="76"/>
-      <c r="B755" s="77"/>
+      <c r="A755" s="74"/>
+      <c r="B755" s="75"/>
       <c r="C755" s="34"/>
       <c r="D755" s="34"/>
       <c r="E755" s="34"/>
@@ -50874,8 +50999,8 @@
       </c>
     </row>
     <row r="756">
-      <c r="A756" s="76"/>
-      <c r="B756" s="77"/>
+      <c r="A756" s="74"/>
+      <c r="B756" s="75"/>
       <c r="C756" s="34"/>
       <c r="D756" s="34"/>
       <c r="E756" s="34"/>
@@ -50900,8 +51025,8 @@
       </c>
     </row>
     <row r="757">
-      <c r="A757" s="76"/>
-      <c r="B757" s="77"/>
+      <c r="A757" s="74"/>
+      <c r="B757" s="75"/>
       <c r="C757" s="34"/>
       <c r="D757" s="34"/>
       <c r="E757" s="34"/>
@@ -50926,8 +51051,8 @@
       </c>
     </row>
     <row r="758">
-      <c r="A758" s="76"/>
-      <c r="B758" s="77"/>
+      <c r="A758" s="74"/>
+      <c r="B758" s="75"/>
       <c r="C758" s="34"/>
       <c r="D758" s="34"/>
       <c r="E758" s="34"/>
@@ -50952,8 +51077,8 @@
       </c>
     </row>
     <row r="759">
-      <c r="A759" s="76"/>
-      <c r="B759" s="77"/>
+      <c r="A759" s="74"/>
+      <c r="B759" s="75"/>
       <c r="C759" s="34"/>
       <c r="D759" s="34"/>
       <c r="E759" s="34"/>
@@ -50978,8 +51103,8 @@
       </c>
     </row>
     <row r="760">
-      <c r="A760" s="76"/>
-      <c r="B760" s="77"/>
+      <c r="A760" s="74"/>
+      <c r="B760" s="75"/>
       <c r="C760" s="34"/>
       <c r="D760" s="34"/>
       <c r="E760" s="34"/>
@@ -51004,8 +51129,8 @@
       </c>
     </row>
     <row r="761">
-      <c r="A761" s="76"/>
-      <c r="B761" s="77"/>
+      <c r="A761" s="74"/>
+      <c r="B761" s="75"/>
       <c r="C761" s="34"/>
       <c r="D761" s="34"/>
       <c r="E761" s="34"/>
@@ -51030,8 +51155,8 @@
       </c>
     </row>
     <row r="762">
-      <c r="A762" s="76"/>
-      <c r="B762" s="77"/>
+      <c r="A762" s="74"/>
+      <c r="B762" s="75"/>
       <c r="C762" s="34"/>
       <c r="D762" s="34"/>
       <c r="E762" s="34"/>
@@ -51056,8 +51181,8 @@
       </c>
     </row>
     <row r="763">
-      <c r="A763" s="76"/>
-      <c r="B763" s="77"/>
+      <c r="A763" s="74"/>
+      <c r="B763" s="75"/>
       <c r="C763" s="34"/>
       <c r="D763" s="34"/>
       <c r="E763" s="34"/>
@@ -51082,8 +51207,8 @@
       </c>
     </row>
     <row r="764">
-      <c r="A764" s="76"/>
-      <c r="B764" s="77"/>
+      <c r="A764" s="74"/>
+      <c r="B764" s="75"/>
       <c r="C764" s="34"/>
       <c r="D764" s="34"/>
       <c r="E764" s="34"/>
@@ -51108,8 +51233,8 @@
       </c>
     </row>
     <row r="765">
-      <c r="A765" s="76"/>
-      <c r="B765" s="77"/>
+      <c r="A765" s="74"/>
+      <c r="B765" s="75"/>
       <c r="C765" s="34"/>
       <c r="D765" s="34"/>
       <c r="E765" s="34"/>
@@ -51134,8 +51259,8 @@
       </c>
     </row>
     <row r="766">
-      <c r="A766" s="76"/>
-      <c r="B766" s="77"/>
+      <c r="A766" s="74"/>
+      <c r="B766" s="75"/>
       <c r="C766" s="34"/>
       <c r="D766" s="34"/>
       <c r="E766" s="34"/>
@@ -51160,8 +51285,8 @@
       </c>
     </row>
     <row r="767">
-      <c r="A767" s="76"/>
-      <c r="B767" s="77"/>
+      <c r="A767" s="74"/>
+      <c r="B767" s="75"/>
       <c r="C767" s="34"/>
       <c r="D767" s="34"/>
       <c r="E767" s="34"/>
@@ -51186,8 +51311,8 @@
       </c>
     </row>
     <row r="768">
-      <c r="A768" s="76"/>
-      <c r="B768" s="77"/>
+      <c r="A768" s="74"/>
+      <c r="B768" s="75"/>
       <c r="C768" s="34"/>
       <c r="D768" s="34"/>
       <c r="E768" s="34"/>
@@ -51212,8 +51337,8 @@
       </c>
     </row>
     <row r="769">
-      <c r="A769" s="76"/>
-      <c r="B769" s="77"/>
+      <c r="A769" s="74"/>
+      <c r="B769" s="75"/>
       <c r="C769" s="34"/>
       <c r="D769" s="34"/>
       <c r="E769" s="34"/>
@@ -51238,8 +51363,8 @@
       </c>
     </row>
     <row r="770">
-      <c r="A770" s="76"/>
-      <c r="B770" s="77"/>
+      <c r="A770" s="74"/>
+      <c r="B770" s="75"/>
       <c r="C770" s="34"/>
       <c r="D770" s="34"/>
       <c r="E770" s="34"/>
@@ -51264,8 +51389,8 @@
       </c>
     </row>
     <row r="771">
-      <c r="A771" s="76"/>
-      <c r="B771" s="77"/>
+      <c r="A771" s="74"/>
+      <c r="B771" s="75"/>
       <c r="C771" s="34"/>
       <c r="D771" s="34"/>
       <c r="E771" s="34"/>
@@ -51290,8 +51415,8 @@
       </c>
     </row>
     <row r="772">
-      <c r="A772" s="76"/>
-      <c r="B772" s="77"/>
+      <c r="A772" s="74"/>
+      <c r="B772" s="75"/>
       <c r="C772" s="34"/>
       <c r="D772" s="34"/>
       <c r="E772" s="34"/>
@@ -51316,8 +51441,8 @@
       </c>
     </row>
     <row r="773">
-      <c r="A773" s="76"/>
-      <c r="B773" s="77"/>
+      <c r="A773" s="74"/>
+      <c r="B773" s="75"/>
       <c r="C773" s="34"/>
       <c r="D773" s="34"/>
       <c r="E773" s="34"/>
@@ -51342,8 +51467,8 @@
       </c>
     </row>
     <row r="774">
-      <c r="A774" s="76"/>
-      <c r="B774" s="77"/>
+      <c r="A774" s="74"/>
+      <c r="B774" s="75"/>
       <c r="C774" s="34"/>
       <c r="D774" s="34"/>
       <c r="E774" s="34"/>
@@ -51368,8 +51493,8 @@
       </c>
     </row>
     <row r="775">
-      <c r="A775" s="76"/>
-      <c r="B775" s="77"/>
+      <c r="A775" s="74"/>
+      <c r="B775" s="75"/>
       <c r="C775" s="34"/>
       <c r="D775" s="34"/>
       <c r="E775" s="34"/>
@@ -51394,8 +51519,8 @@
       </c>
     </row>
     <row r="776">
-      <c r="A776" s="76"/>
-      <c r="B776" s="77"/>
+      <c r="A776" s="74"/>
+      <c r="B776" s="75"/>
       <c r="C776" s="34"/>
       <c r="D776" s="34"/>
       <c r="E776" s="34"/>
@@ -51420,8 +51545,8 @@
       </c>
     </row>
     <row r="777">
-      <c r="A777" s="76"/>
-      <c r="B777" s="77"/>
+      <c r="A777" s="74"/>
+      <c r="B777" s="75"/>
       <c r="C777" s="34"/>
       <c r="D777" s="34"/>
       <c r="E777" s="34"/>
@@ -51446,8 +51571,8 @@
       </c>
     </row>
     <row r="778">
-      <c r="A778" s="76"/>
-      <c r="B778" s="77"/>
+      <c r="A778" s="74"/>
+      <c r="B778" s="75"/>
       <c r="C778" s="34"/>
       <c r="D778" s="34"/>
       <c r="E778" s="34"/>
@@ -51472,8 +51597,8 @@
       </c>
     </row>
     <row r="779">
-      <c r="A779" s="76"/>
-      <c r="B779" s="77"/>
+      <c r="A779" s="74"/>
+      <c r="B779" s="75"/>
       <c r="C779" s="34"/>
       <c r="D779" s="34"/>
       <c r="E779" s="34"/>
@@ -51498,8 +51623,8 @@
       </c>
     </row>
     <row r="780">
-      <c r="A780" s="76"/>
-      <c r="B780" s="77"/>
+      <c r="A780" s="74"/>
+      <c r="B780" s="75"/>
       <c r="C780" s="34"/>
       <c r="D780" s="34"/>
       <c r="E780" s="34"/>
@@ -51524,8 +51649,8 @@
       </c>
     </row>
     <row r="781">
-      <c r="A781" s="76"/>
-      <c r="B781" s="77"/>
+      <c r="A781" s="74"/>
+      <c r="B781" s="75"/>
       <c r="C781" s="34"/>
       <c r="D781" s="34"/>
       <c r="E781" s="34"/>
@@ -51550,8 +51675,8 @@
       </c>
     </row>
     <row r="782">
-      <c r="A782" s="76"/>
-      <c r="B782" s="77"/>
+      <c r="A782" s="74"/>
+      <c r="B782" s="75"/>
       <c r="C782" s="34"/>
       <c r="D782" s="34"/>
       <c r="E782" s="34"/>
@@ -51576,8 +51701,8 @@
       </c>
     </row>
     <row r="783">
-      <c r="A783" s="76"/>
-      <c r="B783" s="77"/>
+      <c r="A783" s="74"/>
+      <c r="B783" s="75"/>
       <c r="C783" s="34"/>
       <c r="D783" s="34"/>
       <c r="E783" s="34"/>
@@ -51602,8 +51727,8 @@
       </c>
     </row>
     <row r="784">
-      <c r="A784" s="76"/>
-      <c r="B784" s="77"/>
+      <c r="A784" s="74"/>
+      <c r="B784" s="75"/>
       <c r="C784" s="34"/>
       <c r="D784" s="34"/>
       <c r="E784" s="34"/>
@@ -51628,8 +51753,8 @@
       </c>
     </row>
     <row r="785">
-      <c r="A785" s="76"/>
-      <c r="B785" s="77"/>
+      <c r="A785" s="74"/>
+      <c r="B785" s="75"/>
       <c r="C785" s="34"/>
       <c r="D785" s="34"/>
       <c r="E785" s="34"/>
@@ -51654,8 +51779,8 @@
       </c>
     </row>
     <row r="786">
-      <c r="A786" s="76"/>
-      <c r="B786" s="77"/>
+      <c r="A786" s="74"/>
+      <c r="B786" s="75"/>
       <c r="C786" s="34"/>
       <c r="D786" s="34"/>
       <c r="E786" s="34"/>
@@ -51680,8 +51805,8 @@
       </c>
     </row>
     <row r="787">
-      <c r="A787" s="76"/>
-      <c r="B787" s="77"/>
+      <c r="A787" s="74"/>
+      <c r="B787" s="75"/>
       <c r="C787" s="34"/>
       <c r="D787" s="34"/>
       <c r="E787" s="34"/>
@@ -51706,8 +51831,8 @@
       </c>
     </row>
     <row r="788">
-      <c r="A788" s="76"/>
-      <c r="B788" s="77"/>
+      <c r="A788" s="74"/>
+      <c r="B788" s="75"/>
       <c r="C788" s="34"/>
       <c r="D788" s="34"/>
       <c r="E788" s="34"/>
@@ -51732,8 +51857,8 @@
       </c>
     </row>
     <row r="789">
-      <c r="A789" s="76"/>
-      <c r="B789" s="77"/>
+      <c r="A789" s="74"/>
+      <c r="B789" s="75"/>
       <c r="C789" s="34"/>
       <c r="D789" s="34"/>
       <c r="E789" s="34"/>
@@ -51758,8 +51883,8 @@
       </c>
     </row>
     <row r="790">
-      <c r="A790" s="76"/>
-      <c r="B790" s="77"/>
+      <c r="A790" s="74"/>
+      <c r="B790" s="75"/>
       <c r="C790" s="34"/>
       <c r="D790" s="34"/>
       <c r="E790" s="34"/>
@@ -51784,8 +51909,8 @@
       </c>
     </row>
     <row r="791">
-      <c r="A791" s="76"/>
-      <c r="B791" s="77"/>
+      <c r="A791" s="74"/>
+      <c r="B791" s="75"/>
       <c r="C791" s="34"/>
       <c r="D791" s="34"/>
       <c r="E791" s="34"/>
@@ -51810,8 +51935,8 @@
       </c>
     </row>
     <row r="792">
-      <c r="A792" s="76"/>
-      <c r="B792" s="77"/>
+      <c r="A792" s="74"/>
+      <c r="B792" s="75"/>
       <c r="C792" s="34"/>
       <c r="D792" s="34"/>
       <c r="E792" s="34"/>
@@ -51836,8 +51961,8 @@
       </c>
     </row>
     <row r="793">
-      <c r="A793" s="76"/>
-      <c r="B793" s="77"/>
+      <c r="A793" s="74"/>
+      <c r="B793" s="75"/>
       <c r="C793" s="34"/>
       <c r="D793" s="34"/>
       <c r="E793" s="34"/>
@@ -51862,8 +51987,8 @@
       </c>
     </row>
     <row r="794">
-      <c r="A794" s="76"/>
-      <c r="B794" s="77"/>
+      <c r="A794" s="74"/>
+      <c r="B794" s="75"/>
       <c r="C794" s="34"/>
       <c r="D794" s="34"/>
       <c r="E794" s="34"/>
@@ -51888,8 +52013,8 @@
       </c>
     </row>
     <row r="795">
-      <c r="A795" s="76"/>
-      <c r="B795" s="77"/>
+      <c r="A795" s="74"/>
+      <c r="B795" s="75"/>
       <c r="C795" s="34"/>
       <c r="D795" s="34"/>
       <c r="E795" s="34"/>
@@ -51914,8 +52039,8 @@
       </c>
     </row>
     <row r="796">
-      <c r="A796" s="76"/>
-      <c r="B796" s="77"/>
+      <c r="A796" s="74"/>
+      <c r="B796" s="75"/>
       <c r="C796" s="34"/>
       <c r="D796" s="34"/>
       <c r="E796" s="34"/>
@@ -51940,8 +52065,8 @@
       </c>
     </row>
     <row r="797">
-      <c r="A797" s="76"/>
-      <c r="B797" s="77"/>
+      <c r="A797" s="74"/>
+      <c r="B797" s="75"/>
       <c r="C797" s="34"/>
       <c r="D797" s="34"/>
       <c r="E797" s="34"/>
@@ -51966,8 +52091,8 @@
       </c>
     </row>
     <row r="798">
-      <c r="A798" s="76"/>
-      <c r="B798" s="77"/>
+      <c r="A798" s="74"/>
+      <c r="B798" s="75"/>
       <c r="C798" s="34"/>
       <c r="D798" s="34"/>
       <c r="E798" s="34"/>
@@ -51992,8 +52117,8 @@
       </c>
     </row>
     <row r="799">
-      <c r="A799" s="76"/>
-      <c r="B799" s="77"/>
+      <c r="A799" s="74"/>
+      <c r="B799" s="75"/>
       <c r="C799" s="34"/>
       <c r="D799" s="34"/>
       <c r="E799" s="34"/>
@@ -52018,8 +52143,8 @@
       </c>
     </row>
     <row r="800">
-      <c r="A800" s="76"/>
-      <c r="B800" s="77"/>
+      <c r="A800" s="74"/>
+      <c r="B800" s="75"/>
       <c r="C800" s="34"/>
       <c r="D800" s="34"/>
       <c r="E800" s="34"/>
@@ -52044,8 +52169,8 @@
       </c>
     </row>
     <row r="801">
-      <c r="A801" s="76"/>
-      <c r="B801" s="77"/>
+      <c r="A801" s="74"/>
+      <c r="B801" s="75"/>
       <c r="C801" s="34"/>
       <c r="D801" s="34"/>
       <c r="E801" s="34"/>
@@ -52070,8 +52195,8 @@
       </c>
     </row>
     <row r="802">
-      <c r="A802" s="76"/>
-      <c r="B802" s="77"/>
+      <c r="A802" s="74"/>
+      <c r="B802" s="75"/>
       <c r="C802" s="34"/>
       <c r="D802" s="34"/>
       <c r="E802" s="34"/>
@@ -52096,8 +52221,8 @@
       </c>
     </row>
     <row r="803">
-      <c r="A803" s="76"/>
-      <c r="B803" s="77"/>
+      <c r="A803" s="74"/>
+      <c r="B803" s="75"/>
       <c r="C803" s="34"/>
       <c r="D803" s="34"/>
       <c r="E803" s="34"/>
@@ -52122,8 +52247,8 @@
       </c>
     </row>
     <row r="804">
-      <c r="A804" s="76"/>
-      <c r="B804" s="77"/>
+      <c r="A804" s="74"/>
+      <c r="B804" s="75"/>
       <c r="C804" s="34"/>
       <c r="D804" s="34"/>
       <c r="E804" s="34"/>
@@ -52148,8 +52273,8 @@
       </c>
     </row>
     <row r="805">
-      <c r="A805" s="76"/>
-      <c r="B805" s="77"/>
+      <c r="A805" s="74"/>
+      <c r="B805" s="75"/>
       <c r="C805" s="34"/>
       <c r="D805" s="34"/>
       <c r="E805" s="34"/>
@@ -52174,8 +52299,8 @@
       </c>
     </row>
     <row r="806">
-      <c r="A806" s="76"/>
-      <c r="B806" s="77"/>
+      <c r="A806" s="74"/>
+      <c r="B806" s="75"/>
       <c r="C806" s="34"/>
       <c r="D806" s="34"/>
       <c r="E806" s="34"/>
@@ -52200,8 +52325,8 @@
       </c>
     </row>
     <row r="807">
-      <c r="A807" s="76"/>
-      <c r="B807" s="77"/>
+      <c r="A807" s="74"/>
+      <c r="B807" s="75"/>
       <c r="C807" s="34"/>
       <c r="D807" s="34"/>
       <c r="E807" s="34"/>
@@ -52226,8 +52351,8 @@
       </c>
     </row>
     <row r="808">
-      <c r="A808" s="76"/>
-      <c r="B808" s="77"/>
+      <c r="A808" s="74"/>
+      <c r="B808" s="75"/>
       <c r="C808" s="34"/>
       <c r="D808" s="34"/>
       <c r="E808" s="34"/>
@@ -52252,8 +52377,8 @@
       </c>
     </row>
     <row r="809">
-      <c r="A809" s="76"/>
-      <c r="B809" s="77"/>
+      <c r="A809" s="74"/>
+      <c r="B809" s="75"/>
       <c r="C809" s="34"/>
       <c r="D809" s="34"/>
       <c r="E809" s="34"/>
@@ -52278,8 +52403,8 @@
       </c>
     </row>
     <row r="810">
-      <c r="A810" s="76"/>
-      <c r="B810" s="77"/>
+      <c r="A810" s="74"/>
+      <c r="B810" s="75"/>
       <c r="C810" s="34"/>
       <c r="D810" s="34"/>
       <c r="E810" s="34"/>
@@ -52304,8 +52429,8 @@
       </c>
     </row>
     <row r="811">
-      <c r="A811" s="76"/>
-      <c r="B811" s="77"/>
+      <c r="A811" s="74"/>
+      <c r="B811" s="75"/>
       <c r="C811" s="34"/>
       <c r="D811" s="34"/>
       <c r="E811" s="34"/>
@@ -52330,8 +52455,8 @@
       </c>
     </row>
     <row r="812">
-      <c r="A812" s="76"/>
-      <c r="B812" s="77"/>
+      <c r="A812" s="74"/>
+      <c r="B812" s="75"/>
       <c r="C812" s="34"/>
       <c r="D812" s="34"/>
       <c r="E812" s="34"/>
@@ -52356,8 +52481,8 @@
       </c>
     </row>
     <row r="813">
-      <c r="A813" s="76"/>
-      <c r="B813" s="77"/>
+      <c r="A813" s="74"/>
+      <c r="B813" s="75"/>
       <c r="C813" s="34"/>
       <c r="D813" s="34"/>
       <c r="E813" s="34"/>
@@ -52382,8 +52507,8 @@
       </c>
     </row>
     <row r="814">
-      <c r="A814" s="76"/>
-      <c r="B814" s="77"/>
+      <c r="A814" s="74"/>
+      <c r="B814" s="75"/>
       <c r="C814" s="34"/>
       <c r="D814" s="34"/>
       <c r="E814" s="34"/>
@@ -52408,8 +52533,8 @@
       </c>
     </row>
     <row r="815">
-      <c r="A815" s="76"/>
-      <c r="B815" s="77"/>
+      <c r="A815" s="74"/>
+      <c r="B815" s="75"/>
       <c r="C815" s="34"/>
       <c r="D815" s="34"/>
       <c r="E815" s="34"/>
@@ -52434,8 +52559,8 @@
       </c>
     </row>
     <row r="816">
-      <c r="A816" s="76"/>
-      <c r="B816" s="77"/>
+      <c r="A816" s="74"/>
+      <c r="B816" s="75"/>
       <c r="C816" s="34"/>
       <c r="D816" s="34"/>
       <c r="E816" s="34"/>
@@ -52460,8 +52585,8 @@
       </c>
     </row>
     <row r="817">
-      <c r="A817" s="76"/>
-      <c r="B817" s="77"/>
+      <c r="A817" s="74"/>
+      <c r="B817" s="75"/>
       <c r="C817" s="34"/>
       <c r="D817" s="34"/>
       <c r="E817" s="34"/>
@@ -52486,8 +52611,8 @@
       </c>
     </row>
     <row r="818">
-      <c r="A818" s="76"/>
-      <c r="B818" s="77"/>
+      <c r="A818" s="74"/>
+      <c r="B818" s="75"/>
       <c r="C818" s="34"/>
       <c r="D818" s="34"/>
       <c r="E818" s="34"/>
@@ -52512,8 +52637,8 @@
       </c>
     </row>
     <row r="819">
-      <c r="A819" s="76"/>
-      <c r="B819" s="77"/>
+      <c r="A819" s="74"/>
+      <c r="B819" s="75"/>
       <c r="C819" s="34"/>
       <c r="D819" s="34"/>
       <c r="E819" s="34"/>
@@ -52538,8 +52663,8 @@
       </c>
     </row>
     <row r="820">
-      <c r="A820" s="76"/>
-      <c r="B820" s="77"/>
+      <c r="A820" s="74"/>
+      <c r="B820" s="75"/>
       <c r="C820" s="34"/>
       <c r="D820" s="34"/>
       <c r="E820" s="34"/>
@@ -52564,8 +52689,8 @@
       </c>
     </row>
     <row r="821">
-      <c r="A821" s="76"/>
-      <c r="B821" s="77"/>
+      <c r="A821" s="74"/>
+      <c r="B821" s="75"/>
       <c r="C821" s="34"/>
       <c r="D821" s="34"/>
       <c r="E821" s="34"/>
@@ -52590,8 +52715,8 @@
       </c>
     </row>
     <row r="822">
-      <c r="A822" s="76"/>
-      <c r="B822" s="77"/>
+      <c r="A822" s="74"/>
+      <c r="B822" s="75"/>
       <c r="C822" s="34"/>
       <c r="D822" s="34"/>
       <c r="E822" s="34"/>
@@ -52616,8 +52741,8 @@
       </c>
     </row>
     <row r="823">
-      <c r="A823" s="76"/>
-      <c r="B823" s="77"/>
+      <c r="A823" s="74"/>
+      <c r="B823" s="75"/>
       <c r="C823" s="34"/>
       <c r="D823" s="34"/>
       <c r="E823" s="34"/>
@@ -52642,8 +52767,8 @@
       </c>
     </row>
     <row r="824">
-      <c r="A824" s="76"/>
-      <c r="B824" s="77"/>
+      <c r="A824" s="74"/>
+      <c r="B824" s="75"/>
       <c r="C824" s="34"/>
       <c r="D824" s="34"/>
       <c r="E824" s="34"/>
@@ -52668,8 +52793,8 @@
       </c>
     </row>
     <row r="825">
-      <c r="A825" s="76"/>
-      <c r="B825" s="77"/>
+      <c r="A825" s="74"/>
+      <c r="B825" s="75"/>
       <c r="C825" s="34"/>
       <c r="D825" s="34"/>
       <c r="E825" s="34"/>
@@ -52694,8 +52819,8 @@
       </c>
     </row>
     <row r="826">
-      <c r="A826" s="76"/>
-      <c r="B826" s="77"/>
+      <c r="A826" s="74"/>
+      <c r="B826" s="75"/>
       <c r="C826" s="34"/>
       <c r="D826" s="34"/>
       <c r="E826" s="34"/>
@@ -52720,8 +52845,8 @@
       </c>
     </row>
     <row r="827">
-      <c r="A827" s="76"/>
-      <c r="B827" s="77"/>
+      <c r="A827" s="74"/>
+      <c r="B827" s="75"/>
       <c r="C827" s="34"/>
       <c r="D827" s="34"/>
       <c r="E827" s="34"/>
@@ -52746,8 +52871,8 @@
       </c>
     </row>
     <row r="828">
-      <c r="A828" s="76"/>
-      <c r="B828" s="77"/>
+      <c r="A828" s="74"/>
+      <c r="B828" s="75"/>
       <c r="C828" s="34"/>
       <c r="D828" s="34"/>
       <c r="E828" s="34"/>
@@ -52772,8 +52897,8 @@
       </c>
     </row>
     <row r="829">
-      <c r="A829" s="76"/>
-      <c r="B829" s="77"/>
+      <c r="A829" s="74"/>
+      <c r="B829" s="75"/>
       <c r="C829" s="34"/>
       <c r="D829" s="34"/>
       <c r="E829" s="34"/>
@@ -52798,8 +52923,8 @@
       </c>
     </row>
     <row r="830">
-      <c r="A830" s="76"/>
-      <c r="B830" s="77"/>
+      <c r="A830" s="74"/>
+      <c r="B830" s="75"/>
       <c r="C830" s="34"/>
       <c r="D830" s="34"/>
       <c r="E830" s="34"/>
@@ -52824,8 +52949,8 @@
       </c>
     </row>
     <row r="831">
-      <c r="A831" s="76"/>
-      <c r="B831" s="77"/>
+      <c r="A831" s="74"/>
+      <c r="B831" s="75"/>
       <c r="C831" s="34"/>
       <c r="D831" s="34"/>
       <c r="E831" s="34"/>
@@ -52850,8 +52975,8 @@
       </c>
     </row>
     <row r="832">
-      <c r="A832" s="76"/>
-      <c r="B832" s="77"/>
+      <c r="A832" s="74"/>
+      <c r="B832" s="75"/>
       <c r="C832" s="34"/>
       <c r="D832" s="34"/>
       <c r="E832" s="34"/>
@@ -52876,8 +53001,8 @@
       </c>
     </row>
     <row r="833">
-      <c r="A833" s="76"/>
-      <c r="B833" s="77"/>
+      <c r="A833" s="74"/>
+      <c r="B833" s="75"/>
       <c r="C833" s="34"/>
       <c r="D833" s="34"/>
       <c r="E833" s="34"/>
@@ -52902,8 +53027,8 @@
       </c>
     </row>
     <row r="834">
-      <c r="A834" s="76"/>
-      <c r="B834" s="77"/>
+      <c r="A834" s="74"/>
+      <c r="B834" s="75"/>
       <c r="C834" s="34"/>
       <c r="D834" s="34"/>
       <c r="E834" s="34"/>
@@ -52928,8 +53053,8 @@
       </c>
     </row>
     <row r="835">
-      <c r="A835" s="76"/>
-      <c r="B835" s="77"/>
+      <c r="A835" s="74"/>
+      <c r="B835" s="75"/>
       <c r="C835" s="34"/>
       <c r="D835" s="34"/>
       <c r="E835" s="34"/>
@@ -52954,8 +53079,8 @@
       </c>
     </row>
     <row r="836">
-      <c r="A836" s="76"/>
-      <c r="B836" s="77"/>
+      <c r="A836" s="74"/>
+      <c r="B836" s="75"/>
       <c r="C836" s="34"/>
       <c r="D836" s="34"/>
       <c r="E836" s="34"/>
@@ -52980,8 +53105,8 @@
       </c>
     </row>
     <row r="837">
-      <c r="A837" s="76"/>
-      <c r="B837" s="77"/>
+      <c r="A837" s="74"/>
+      <c r="B837" s="75"/>
       <c r="C837" s="34"/>
       <c r="D837" s="34"/>
       <c r="E837" s="34"/>
@@ -53006,8 +53131,8 @@
       </c>
     </row>
     <row r="838">
-      <c r="A838" s="76"/>
-      <c r="B838" s="77"/>
+      <c r="A838" s="74"/>
+      <c r="B838" s="75"/>
       <c r="C838" s="34"/>
       <c r="D838" s="34"/>
       <c r="E838" s="34"/>
@@ -53032,8 +53157,8 @@
       </c>
     </row>
     <row r="839">
-      <c r="A839" s="76"/>
-      <c r="B839" s="77"/>
+      <c r="A839" s="74"/>
+      <c r="B839" s="75"/>
       <c r="C839" s="34"/>
       <c r="D839" s="34"/>
       <c r="E839" s="34"/>
@@ -53058,8 +53183,8 @@
       </c>
     </row>
     <row r="840">
-      <c r="A840" s="76"/>
-      <c r="B840" s="77"/>
+      <c r="A840" s="74"/>
+      <c r="B840" s="75"/>
       <c r="C840" s="34"/>
       <c r="D840" s="34"/>
       <c r="E840" s="34"/>
@@ -53084,8 +53209,8 @@
       </c>
     </row>
     <row r="841">
-      <c r="A841" s="76"/>
-      <c r="B841" s="77"/>
+      <c r="A841" s="74"/>
+      <c r="B841" s="75"/>
       <c r="C841" s="34"/>
       <c r="D841" s="34"/>
       <c r="E841" s="34"/>
@@ -53110,8 +53235,8 @@
       </c>
     </row>
     <row r="842">
-      <c r="A842" s="76"/>
-      <c r="B842" s="77"/>
+      <c r="A842" s="74"/>
+      <c r="B842" s="75"/>
       <c r="C842" s="34"/>
       <c r="D842" s="34"/>
       <c r="E842" s="34"/>
@@ -53136,8 +53261,8 @@
       </c>
     </row>
     <row r="843">
-      <c r="A843" s="76"/>
-      <c r="B843" s="77"/>
+      <c r="A843" s="74"/>
+      <c r="B843" s="75"/>
       <c r="C843" s="34"/>
       <c r="D843" s="34"/>
       <c r="E843" s="34"/>
@@ -53162,8 +53287,8 @@
       </c>
     </row>
     <row r="844">
-      <c r="A844" s="76"/>
-      <c r="B844" s="77"/>
+      <c r="A844" s="74"/>
+      <c r="B844" s="75"/>
       <c r="C844" s="34"/>
       <c r="D844" s="34"/>
       <c r="E844" s="34"/>
@@ -53188,8 +53313,8 @@
       </c>
     </row>
     <row r="845">
-      <c r="A845" s="76"/>
-      <c r="B845" s="77"/>
+      <c r="A845" s="74"/>
+      <c r="B845" s="75"/>
       <c r="C845" s="34"/>
       <c r="D845" s="34"/>
       <c r="E845" s="34"/>
@@ -53214,8 +53339,8 @@
       </c>
     </row>
     <row r="846">
-      <c r="A846" s="76"/>
-      <c r="B846" s="77"/>
+      <c r="A846" s="74"/>
+      <c r="B846" s="75"/>
       <c r="C846" s="34"/>
       <c r="D846" s="34"/>
       <c r="E846" s="34"/>
@@ -53240,8 +53365,8 @@
       </c>
     </row>
     <row r="847">
-      <c r="A847" s="76"/>
-      <c r="B847" s="77"/>
+      <c r="A847" s="74"/>
+      <c r="B847" s="75"/>
       <c r="C847" s="34"/>
       <c r="D847" s="34"/>
       <c r="E847" s="34"/>
@@ -53266,8 +53391,8 @@
       </c>
     </row>
     <row r="848">
-      <c r="A848" s="76"/>
-      <c r="B848" s="77"/>
+      <c r="A848" s="74"/>
+      <c r="B848" s="75"/>
       <c r="C848" s="34"/>
       <c r="D848" s="34"/>
       <c r="E848" s="34"/>
@@ -53292,8 +53417,8 @@
       </c>
     </row>
     <row r="849">
-      <c r="A849" s="76"/>
-      <c r="B849" s="77"/>
+      <c r="A849" s="74"/>
+      <c r="B849" s="75"/>
       <c r="C849" s="34"/>
       <c r="D849" s="34"/>
       <c r="E849" s="34"/>
@@ -53318,8 +53443,8 @@
       </c>
     </row>
     <row r="850">
-      <c r="A850" s="76"/>
-      <c r="B850" s="77"/>
+      <c r="A850" s="74"/>
+      <c r="B850" s="75"/>
       <c r="C850" s="34"/>
       <c r="D850" s="34"/>
       <c r="E850" s="34"/>
@@ -53344,8 +53469,8 @@
       </c>
     </row>
     <row r="851">
-      <c r="A851" s="76"/>
-      <c r="B851" s="77"/>
+      <c r="A851" s="74"/>
+      <c r="B851" s="75"/>
       <c r="C851" s="34"/>
       <c r="D851" s="34"/>
       <c r="E851" s="34"/>
@@ -53370,8 +53495,8 @@
       </c>
     </row>
     <row r="852">
-      <c r="A852" s="76"/>
-      <c r="B852" s="77"/>
+      <c r="A852" s="74"/>
+      <c r="B852" s="75"/>
       <c r="C852" s="34"/>
       <c r="D852" s="34"/>
       <c r="E852" s="34"/>
@@ -53396,8 +53521,8 @@
       </c>
     </row>
     <row r="853">
-      <c r="A853" s="76"/>
-      <c r="B853" s="77"/>
+      <c r="A853" s="74"/>
+      <c r="B853" s="75"/>
       <c r="C853" s="34"/>
       <c r="D853" s="34"/>
       <c r="E853" s="34"/>
@@ -53422,8 +53547,8 @@
       </c>
     </row>
     <row r="854">
-      <c r="A854" s="76"/>
-      <c r="B854" s="77"/>
+      <c r="A854" s="74"/>
+      <c r="B854" s="75"/>
       <c r="C854" s="34"/>
       <c r="D854" s="34"/>
       <c r="E854" s="34"/>
@@ -53448,8 +53573,8 @@
       </c>
     </row>
     <row r="855">
-      <c r="A855" s="76"/>
-      <c r="B855" s="77"/>
+      <c r="A855" s="74"/>
+      <c r="B855" s="75"/>
       <c r="C855" s="34"/>
       <c r="D855" s="34"/>
       <c r="E855" s="34"/>
@@ -53474,8 +53599,8 @@
       </c>
     </row>
     <row r="856">
-      <c r="A856" s="76"/>
-      <c r="B856" s="77"/>
+      <c r="A856" s="74"/>
+      <c r="B856" s="75"/>
       <c r="C856" s="34"/>
       <c r="D856" s="34"/>
       <c r="E856" s="34"/>
@@ -53500,8 +53625,8 @@
       </c>
     </row>
     <row r="857">
-      <c r="A857" s="76"/>
-      <c r="B857" s="77"/>
+      <c r="A857" s="74"/>
+      <c r="B857" s="75"/>
       <c r="C857" s="34"/>
       <c r="D857" s="34"/>
       <c r="E857" s="34"/>
@@ -53526,8 +53651,8 @@
       </c>
     </row>
     <row r="858">
-      <c r="A858" s="76"/>
-      <c r="B858" s="77"/>
+      <c r="A858" s="74"/>
+      <c r="B858" s="75"/>
       <c r="C858" s="34"/>
       <c r="D858" s="34"/>
       <c r="E858" s="34"/>
@@ -53552,8 +53677,8 @@
       </c>
     </row>
     <row r="859">
-      <c r="A859" s="76"/>
-      <c r="B859" s="77"/>
+      <c r="A859" s="74"/>
+      <c r="B859" s="75"/>
       <c r="C859" s="34"/>
       <c r="D859" s="34"/>
       <c r="E859" s="34"/>
@@ -53578,8 +53703,8 @@
       </c>
     </row>
     <row r="860">
-      <c r="A860" s="76"/>
-      <c r="B860" s="77"/>
+      <c r="A860" s="74"/>
+      <c r="B860" s="75"/>
       <c r="C860" s="34"/>
       <c r="D860" s="34"/>
       <c r="E860" s="34"/>
@@ -53604,8 +53729,8 @@
       </c>
     </row>
     <row r="861">
-      <c r="A861" s="76"/>
-      <c r="B861" s="77"/>
+      <c r="A861" s="74"/>
+      <c r="B861" s="75"/>
       <c r="C861" s="34"/>
       <c r="D861" s="34"/>
       <c r="E861" s="34"/>
@@ -53630,8 +53755,8 @@
       </c>
     </row>
     <row r="862">
-      <c r="A862" s="76"/>
-      <c r="B862" s="77"/>
+      <c r="A862" s="74"/>
+      <c r="B862" s="75"/>
       <c r="C862" s="34"/>
       <c r="D862" s="34"/>
       <c r="E862" s="34"/>
@@ -53656,8 +53781,8 @@
       </c>
     </row>
     <row r="863">
-      <c r="A863" s="76"/>
-      <c r="B863" s="77"/>
+      <c r="A863" s="74"/>
+      <c r="B863" s="75"/>
       <c r="C863" s="34"/>
       <c r="D863" s="34"/>
       <c r="E863" s="34"/>
@@ -53682,8 +53807,8 @@
       </c>
     </row>
     <row r="864">
-      <c r="A864" s="76"/>
-      <c r="B864" s="77"/>
+      <c r="A864" s="74"/>
+      <c r="B864" s="75"/>
       <c r="C864" s="34"/>
       <c r="D864" s="34"/>
       <c r="E864" s="34"/>
@@ -53708,8 +53833,8 @@
       </c>
     </row>
     <row r="865">
-      <c r="A865" s="76"/>
-      <c r="B865" s="77"/>
+      <c r="A865" s="74"/>
+      <c r="B865" s="75"/>
       <c r="C865" s="34"/>
       <c r="D865" s="34"/>
       <c r="E865" s="34"/>
@@ -53734,8 +53859,8 @@
       </c>
     </row>
     <row r="866">
-      <c r="A866" s="76"/>
-      <c r="B866" s="77"/>
+      <c r="A866" s="74"/>
+      <c r="B866" s="75"/>
       <c r="C866" s="34"/>
       <c r="D866" s="34"/>
       <c r="E866" s="34"/>
@@ -53760,8 +53885,8 @@
       </c>
     </row>
     <row r="867">
-      <c r="A867" s="76"/>
-      <c r="B867" s="77"/>
+      <c r="A867" s="74"/>
+      <c r="B867" s="75"/>
       <c r="C867" s="34"/>
       <c r="D867" s="34"/>
       <c r="E867" s="34"/>
@@ -53786,8 +53911,8 @@
       </c>
     </row>
     <row r="868">
-      <c r="A868" s="76"/>
-      <c r="B868" s="77"/>
+      <c r="A868" s="74"/>
+      <c r="B868" s="75"/>
       <c r="C868" s="34"/>
       <c r="D868" s="34"/>
       <c r="E868" s="34"/>
@@ -53812,8 +53937,8 @@
       </c>
     </row>
     <row r="869">
-      <c r="A869" s="76"/>
-      <c r="B869" s="77"/>
+      <c r="A869" s="74"/>
+      <c r="B869" s="75"/>
       <c r="C869" s="34"/>
       <c r="D869" s="34"/>
       <c r="E869" s="34"/>
@@ -53838,8 +53963,8 @@
       </c>
     </row>
     <row r="870">
-      <c r="A870" s="76"/>
-      <c r="B870" s="77"/>
+      <c r="A870" s="74"/>
+      <c r="B870" s="75"/>
       <c r="C870" s="34"/>
       <c r="D870" s="34"/>
       <c r="E870" s="34"/>
@@ -53864,8 +53989,8 @@
       </c>
     </row>
     <row r="871">
-      <c r="A871" s="76"/>
-      <c r="B871" s="77"/>
+      <c r="A871" s="74"/>
+      <c r="B871" s="75"/>
       <c r="C871" s="34"/>
       <c r="D871" s="34"/>
       <c r="E871" s="34"/>
@@ -53890,8 +54015,8 @@
       </c>
     </row>
     <row r="872">
-      <c r="A872" s="76"/>
-      <c r="B872" s="77"/>
+      <c r="A872" s="74"/>
+      <c r="B872" s="75"/>
       <c r="C872" s="34"/>
       <c r="D872" s="34"/>
       <c r="E872" s="34"/>
@@ -53916,8 +54041,8 @@
       </c>
     </row>
     <row r="873">
-      <c r="A873" s="76"/>
-      <c r="B873" s="77"/>
+      <c r="A873" s="74"/>
+      <c r="B873" s="75"/>
       <c r="C873" s="34"/>
       <c r="D873" s="34"/>
       <c r="E873" s="34"/>
@@ -53942,8 +54067,8 @@
       </c>
     </row>
     <row r="874">
-      <c r="A874" s="76"/>
-      <c r="B874" s="77"/>
+      <c r="A874" s="74"/>
+      <c r="B874" s="75"/>
       <c r="C874" s="34"/>
       <c r="D874" s="34"/>
       <c r="E874" s="34"/>
@@ -53968,8 +54093,8 @@
       </c>
     </row>
     <row r="875">
-      <c r="A875" s="76"/>
-      <c r="B875" s="77"/>
+      <c r="A875" s="74"/>
+      <c r="B875" s="75"/>
       <c r="C875" s="34"/>
       <c r="D875" s="34"/>
       <c r="E875" s="34"/>
@@ -53994,8 +54119,8 @@
       </c>
     </row>
     <row r="876">
-      <c r="A876" s="76"/>
-      <c r="B876" s="77"/>
+      <c r="A876" s="74"/>
+      <c r="B876" s="75"/>
       <c r="C876" s="34"/>
       <c r="D876" s="34"/>
       <c r="E876" s="34"/>
@@ -54020,8 +54145,8 @@
       </c>
     </row>
     <row r="877">
-      <c r="A877" s="76"/>
-      <c r="B877" s="77"/>
+      <c r="A877" s="74"/>
+      <c r="B877" s="75"/>
       <c r="C877" s="34"/>
       <c r="D877" s="34"/>
       <c r="E877" s="34"/>
@@ -54046,8 +54171,8 @@
       </c>
     </row>
     <row r="878">
-      <c r="A878" s="76"/>
-      <c r="B878" s="77"/>
+      <c r="A878" s="74"/>
+      <c r="B878" s="75"/>
       <c r="C878" s="34"/>
       <c r="D878" s="34"/>
       <c r="E878" s="34"/>
@@ -54072,8 +54197,8 @@
       </c>
     </row>
     <row r="879">
-      <c r="A879" s="76"/>
-      <c r="B879" s="77"/>
+      <c r="A879" s="74"/>
+      <c r="B879" s="75"/>
       <c r="C879" s="34"/>
       <c r="D879" s="34"/>
       <c r="E879" s="34"/>
@@ -54098,8 +54223,8 @@
       </c>
     </row>
     <row r="880">
-      <c r="A880" s="76"/>
-      <c r="B880" s="77"/>
+      <c r="A880" s="74"/>
+      <c r="B880" s="75"/>
       <c r="C880" s="34"/>
       <c r="D880" s="34"/>
       <c r="E880" s="34"/>
@@ -54124,8 +54249,8 @@
       </c>
     </row>
     <row r="881">
-      <c r="A881" s="76"/>
-      <c r="B881" s="77"/>
+      <c r="A881" s="74"/>
+      <c r="B881" s="75"/>
       <c r="C881" s="34"/>
       <c r="D881" s="34"/>
       <c r="E881" s="34"/>
@@ -54150,8 +54275,8 @@
       </c>
     </row>
     <row r="882">
-      <c r="A882" s="76"/>
-      <c r="B882" s="77"/>
+      <c r="A882" s="74"/>
+      <c r="B882" s="75"/>
       <c r="C882" s="34"/>
       <c r="D882" s="34"/>
       <c r="E882" s="34"/>
@@ -54176,8 +54301,8 @@
       </c>
     </row>
     <row r="883">
-      <c r="A883" s="76"/>
-      <c r="B883" s="77"/>
+      <c r="A883" s="74"/>
+      <c r="B883" s="75"/>
       <c r="C883" s="34"/>
       <c r="D883" s="34"/>
       <c r="E883" s="34"/>
@@ -54202,8 +54327,8 @@
       </c>
     </row>
     <row r="884">
-      <c r="A884" s="76"/>
-      <c r="B884" s="77"/>
+      <c r="A884" s="74"/>
+      <c r="B884" s="75"/>
       <c r="C884" s="34"/>
       <c r="D884" s="34"/>
       <c r="E884" s="34"/>
@@ -54228,8 +54353,8 @@
       </c>
     </row>
     <row r="885">
-      <c r="A885" s="76"/>
-      <c r="B885" s="77"/>
+      <c r="A885" s="74"/>
+      <c r="B885" s="75"/>
       <c r="C885" s="34"/>
       <c r="D885" s="34"/>
       <c r="E885" s="34"/>
@@ -54254,8 +54379,8 @@
       </c>
     </row>
     <row r="886">
-      <c r="A886" s="76"/>
-      <c r="B886" s="77"/>
+      <c r="A886" s="74"/>
+      <c r="B886" s="75"/>
       <c r="C886" s="34"/>
       <c r="D886" s="34"/>
       <c r="E886" s="34"/>
@@ -54280,8 +54405,8 @@
       </c>
     </row>
     <row r="887">
-      <c r="A887" s="76"/>
-      <c r="B887" s="77"/>
+      <c r="A887" s="74"/>
+      <c r="B887" s="75"/>
       <c r="C887" s="34"/>
       <c r="D887" s="34"/>
       <c r="E887" s="34"/>
@@ -54306,8 +54431,8 @@
       </c>
     </row>
     <row r="888">
-      <c r="A888" s="76"/>
-      <c r="B888" s="77"/>
+      <c r="A888" s="74"/>
+      <c r="B888" s="75"/>
       <c r="C888" s="34"/>
       <c r="D888" s="34"/>
       <c r="E888" s="34"/>
@@ -54332,8 +54457,8 @@
       </c>
     </row>
     <row r="889">
-      <c r="A889" s="76"/>
-      <c r="B889" s="77"/>
+      <c r="A889" s="74"/>
+      <c r="B889" s="75"/>
       <c r="C889" s="34"/>
       <c r="D889" s="34"/>
       <c r="E889" s="34"/>
@@ -54358,8 +54483,8 @@
       </c>
     </row>
     <row r="890">
-      <c r="A890" s="76"/>
-      <c r="B890" s="77"/>
+      <c r="A890" s="74"/>
+      <c r="B890" s="75"/>
       <c r="C890" s="34"/>
       <c r="D890" s="34"/>
       <c r="E890" s="34"/>
@@ -54384,8 +54509,8 @@
       </c>
     </row>
     <row r="891">
-      <c r="A891" s="76"/>
-      <c r="B891" s="77"/>
+      <c r="A891" s="74"/>
+      <c r="B891" s="75"/>
       <c r="C891" s="34"/>
       <c r="D891" s="34"/>
       <c r="E891" s="34"/>
@@ -54410,8 +54535,8 @@
       </c>
     </row>
     <row r="892">
-      <c r="A892" s="76"/>
-      <c r="B892" s="77"/>
+      <c r="A892" s="74"/>
+      <c r="B892" s="75"/>
       <c r="C892" s="34"/>
       <c r="D892" s="34"/>
       <c r="E892" s="34"/>
@@ -54436,8 +54561,8 @@
       </c>
     </row>
     <row r="893">
-      <c r="A893" s="76"/>
-      <c r="B893" s="77"/>
+      <c r="A893" s="74"/>
+      <c r="B893" s="75"/>
       <c r="C893" s="34"/>
       <c r="D893" s="34"/>
       <c r="E893" s="34"/>
@@ -54462,8 +54587,8 @@
       </c>
     </row>
     <row r="894">
-      <c r="A894" s="76"/>
-      <c r="B894" s="77"/>
+      <c r="A894" s="74"/>
+      <c r="B894" s="75"/>
       <c r="C894" s="34"/>
       <c r="D894" s="34"/>
       <c r="E894" s="34"/>
@@ -54488,8 +54613,8 @@
       </c>
     </row>
     <row r="895">
-      <c r="A895" s="76"/>
-      <c r="B895" s="77"/>
+      <c r="A895" s="74"/>
+      <c r="B895" s="75"/>
       <c r="C895" s="34"/>
       <c r="D895" s="34"/>
       <c r="E895" s="34"/>
@@ -54514,8 +54639,8 @@
       </c>
     </row>
     <row r="896">
-      <c r="A896" s="76"/>
-      <c r="B896" s="77"/>
+      <c r="A896" s="74"/>
+      <c r="B896" s="75"/>
       <c r="C896" s="34"/>
       <c r="D896" s="34"/>
       <c r="E896" s="34"/>
@@ -54540,8 +54665,8 @@
       </c>
     </row>
     <row r="897">
-      <c r="A897" s="76"/>
-      <c r="B897" s="77"/>
+      <c r="A897" s="74"/>
+      <c r="B897" s="75"/>
       <c r="C897" s="34"/>
       <c r="D897" s="34"/>
       <c r="E897" s="34"/>
@@ -54566,8 +54691,8 @@
       </c>
     </row>
     <row r="898">
-      <c r="A898" s="76"/>
-      <c r="B898" s="77"/>
+      <c r="A898" s="74"/>
+      <c r="B898" s="75"/>
       <c r="C898" s="34"/>
       <c r="D898" s="34"/>
       <c r="E898" s="34"/>
@@ -54592,8 +54717,8 @@
       </c>
     </row>
     <row r="899">
-      <c r="A899" s="76"/>
-      <c r="B899" s="77"/>
+      <c r="A899" s="74"/>
+      <c r="B899" s="75"/>
       <c r="C899" s="34"/>
       <c r="D899" s="34"/>
       <c r="E899" s="34"/>
@@ -54618,8 +54743,8 @@
       </c>
     </row>
     <row r="900">
-      <c r="A900" s="76"/>
-      <c r="B900" s="77"/>
+      <c r="A900" s="74"/>
+      <c r="B900" s="75"/>
       <c r="C900" s="34"/>
       <c r="D900" s="34"/>
       <c r="E900" s="34"/>
@@ -54644,8 +54769,8 @@
       </c>
     </row>
     <row r="901">
-      <c r="A901" s="76"/>
-      <c r="B901" s="77"/>
+      <c r="A901" s="74"/>
+      <c r="B901" s="75"/>
       <c r="C901" s="34"/>
       <c r="D901" s="34"/>
       <c r="E901" s="34"/>
@@ -54670,8 +54795,8 @@
       </c>
     </row>
     <row r="902">
-      <c r="A902" s="76"/>
-      <c r="B902" s="77"/>
+      <c r="A902" s="74"/>
+      <c r="B902" s="75"/>
       <c r="C902" s="34"/>
       <c r="D902" s="34"/>
       <c r="E902" s="34"/>
@@ -54696,8 +54821,8 @@
       </c>
     </row>
     <row r="903">
-      <c r="A903" s="76"/>
-      <c r="B903" s="77"/>
+      <c r="A903" s="74"/>
+      <c r="B903" s="75"/>
       <c r="C903" s="34"/>
       <c r="D903" s="34"/>
       <c r="E903" s="34"/>
@@ -54722,8 +54847,8 @@
       </c>
     </row>
     <row r="904">
-      <c r="A904" s="76"/>
-      <c r="B904" s="77"/>
+      <c r="A904" s="74"/>
+      <c r="B904" s="75"/>
       <c r="C904" s="34"/>
       <c r="D904" s="34"/>
       <c r="E904" s="34"/>
@@ -54748,8 +54873,8 @@
       </c>
     </row>
     <row r="905">
-      <c r="A905" s="76"/>
-      <c r="B905" s="77"/>
+      <c r="A905" s="74"/>
+      <c r="B905" s="75"/>
       <c r="C905" s="34"/>
       <c r="D905" s="34"/>
       <c r="E905" s="34"/>
@@ -54774,8 +54899,8 @@
       </c>
     </row>
     <row r="906">
-      <c r="A906" s="76"/>
-      <c r="B906" s="77"/>
+      <c r="A906" s="74"/>
+      <c r="B906" s="75"/>
       <c r="C906" s="34"/>
       <c r="D906" s="34"/>
       <c r="E906" s="34"/>
@@ -54800,8 +54925,8 @@
       </c>
     </row>
     <row r="907">
-      <c r="A907" s="76"/>
-      <c r="B907" s="77"/>
+      <c r="A907" s="74"/>
+      <c r="B907" s="75"/>
       <c r="C907" s="34"/>
       <c r="D907" s="34"/>
       <c r="E907" s="34"/>
@@ -54826,8 +54951,8 @@
       </c>
     </row>
     <row r="908">
-      <c r="A908" s="76"/>
-      <c r="B908" s="77"/>
+      <c r="A908" s="74"/>
+      <c r="B908" s="75"/>
       <c r="C908" s="34"/>
       <c r="D908" s="34"/>
       <c r="E908" s="34"/>
@@ -54852,8 +54977,8 @@
       </c>
     </row>
     <row r="909">
-      <c r="A909" s="76"/>
-      <c r="B909" s="77"/>
+      <c r="A909" s="74"/>
+      <c r="B909" s="75"/>
       <c r="C909" s="34"/>
       <c r="D909" s="34"/>
       <c r="E909" s="34"/>
@@ -54878,8 +55003,8 @@
       </c>
     </row>
     <row r="910">
-      <c r="A910" s="76"/>
-      <c r="B910" s="77"/>
+      <c r="A910" s="74"/>
+      <c r="B910" s="75"/>
       <c r="C910" s="34"/>
       <c r="D910" s="34"/>
       <c r="E910" s="34"/>
@@ -54904,8 +55029,8 @@
       </c>
     </row>
     <row r="911">
-      <c r="A911" s="76"/>
-      <c r="B911" s="77"/>
+      <c r="A911" s="74"/>
+      <c r="B911" s="75"/>
       <c r="C911" s="34"/>
       <c r="D911" s="34"/>
       <c r="E911" s="34"/>
@@ -54930,8 +55055,8 @@
       </c>
     </row>
     <row r="912">
-      <c r="A912" s="76"/>
-      <c r="B912" s="77"/>
+      <c r="A912" s="74"/>
+      <c r="B912" s="75"/>
       <c r="C912" s="34"/>
       <c r="D912" s="34"/>
       <c r="E912" s="34"/>
@@ -54956,8 +55081,8 @@
       </c>
     </row>
     <row r="913">
-      <c r="A913" s="76"/>
-      <c r="B913" s="77"/>
+      <c r="A913" s="74"/>
+      <c r="B913" s="75"/>
       <c r="C913" s="34"/>
       <c r="D913" s="34"/>
       <c r="E913" s="34"/>
@@ -54982,8 +55107,8 @@
       </c>
     </row>
     <row r="914">
-      <c r="A914" s="76"/>
-      <c r="B914" s="77"/>
+      <c r="A914" s="74"/>
+      <c r="B914" s="75"/>
       <c r="C914" s="34"/>
       <c r="D914" s="34"/>
       <c r="E914" s="34"/>
@@ -55008,8 +55133,8 @@
       </c>
     </row>
     <row r="915">
-      <c r="A915" s="76"/>
-      <c r="B915" s="77"/>
+      <c r="A915" s="74"/>
+      <c r="B915" s="75"/>
       <c r="C915" s="34"/>
       <c r="D915" s="34"/>
       <c r="E915" s="34"/>
@@ -55034,8 +55159,8 @@
       </c>
     </row>
     <row r="916">
-      <c r="A916" s="76"/>
-      <c r="B916" s="77"/>
+      <c r="A916" s="74"/>
+      <c r="B916" s="75"/>
       <c r="C916" s="34"/>
       <c r="D916" s="34"/>
       <c r="E916" s="34"/>
@@ -55060,8 +55185,8 @@
       </c>
     </row>
     <row r="917">
-      <c r="A917" s="76"/>
-      <c r="B917" s="77"/>
+      <c r="A917" s="74"/>
+      <c r="B917" s="75"/>
       <c r="C917" s="34"/>
       <c r="D917" s="34"/>
       <c r="E917" s="34"/>
@@ -55086,8 +55211,8 @@
       </c>
     </row>
     <row r="918">
-      <c r="A918" s="76"/>
-      <c r="B918" s="77"/>
+      <c r="A918" s="74"/>
+      <c r="B918" s="75"/>
       <c r="C918" s="34"/>
       <c r="D918" s="34"/>
       <c r="E918" s="34"/>
@@ -55112,8 +55237,8 @@
       </c>
     </row>
     <row r="919">
-      <c r="A919" s="76"/>
-      <c r="B919" s="77"/>
+      <c r="A919" s="74"/>
+      <c r="B919" s="75"/>
       <c r="C919" s="34"/>
       <c r="D919" s="34"/>
       <c r="E919" s="34"/>
@@ -55138,8 +55263,8 @@
       </c>
     </row>
     <row r="920">
-      <c r="A920" s="76"/>
-      <c r="B920" s="77"/>
+      <c r="A920" s="74"/>
+      <c r="B920" s="75"/>
       <c r="C920" s="34"/>
       <c r="D920" s="34"/>
       <c r="E920" s="34"/>
@@ -55164,8 +55289,8 @@
       </c>
     </row>
     <row r="921">
-      <c r="A921" s="76"/>
-      <c r="B921" s="77"/>
+      <c r="A921" s="74"/>
+      <c r="B921" s="75"/>
       <c r="C921" s="34"/>
       <c r="D921" s="34"/>
       <c r="E921" s="34"/>
@@ -55190,8 +55315,8 @@
       </c>
     </row>
     <row r="922">
-      <c r="A922" s="76"/>
-      <c r="B922" s="77"/>
+      <c r="A922" s="74"/>
+      <c r="B922" s="75"/>
       <c r="C922" s="34"/>
       <c r="D922" s="34"/>
       <c r="E922" s="34"/>
@@ -55216,8 +55341,8 @@
       </c>
     </row>
     <row r="923">
-      <c r="A923" s="76"/>
-      <c r="B923" s="77"/>
+      <c r="A923" s="74"/>
+      <c r="B923" s="75"/>
       <c r="C923" s="34"/>
       <c r="D923" s="34"/>
       <c r="E923" s="34"/>
@@ -55242,8 +55367,8 @@
       </c>
     </row>
     <row r="924">
-      <c r="A924" s="76"/>
-      <c r="B924" s="77"/>
+      <c r="A924" s="74"/>
+      <c r="B924" s="75"/>
       <c r="C924" s="34"/>
       <c r="D924" s="34"/>
       <c r="E924" s="34"/>
@@ -55268,8 +55393,8 @@
       </c>
     </row>
     <row r="925">
-      <c r="A925" s="76"/>
-      <c r="B925" s="77"/>
+      <c r="A925" s="74"/>
+      <c r="B925" s="75"/>
       <c r="C925" s="34"/>
       <c r="D925" s="34"/>
       <c r="E925" s="34"/>
@@ -55294,8 +55419,8 @@
       </c>
     </row>
     <row r="926">
-      <c r="A926" s="76"/>
-      <c r="B926" s="77"/>
+      <c r="A926" s="74"/>
+      <c r="B926" s="75"/>
       <c r="C926" s="34"/>
       <c r="D926" s="34"/>
       <c r="E926" s="34"/>
@@ -55320,8 +55445,8 @@
       </c>
     </row>
     <row r="927">
-      <c r="A927" s="76"/>
-      <c r="B927" s="77"/>
+      <c r="A927" s="74"/>
+      <c r="B927" s="75"/>
       <c r="C927" s="34"/>
       <c r="D927" s="34"/>
       <c r="E927" s="34"/>
@@ -55346,8 +55471,8 @@
       </c>
     </row>
     <row r="928">
-      <c r="A928" s="76"/>
-      <c r="B928" s="77"/>
+      <c r="A928" s="74"/>
+      <c r="B928" s="75"/>
       <c r="C928" s="34"/>
       <c r="D928" s="34"/>
       <c r="E928" s="34"/>
@@ -55372,8 +55497,8 @@
       </c>
     </row>
     <row r="929">
-      <c r="A929" s="76"/>
-      <c r="B929" s="77"/>
+      <c r="A929" s="74"/>
+      <c r="B929" s="75"/>
       <c r="C929" s="34"/>
       <c r="D929" s="34"/>
       <c r="E929" s="34"/>
@@ -55398,8 +55523,8 @@
       </c>
     </row>
     <row r="930">
-      <c r="A930" s="76"/>
-      <c r="B930" s="77"/>
+      <c r="A930" s="74"/>
+      <c r="B930" s="75"/>
       <c r="C930" s="34"/>
       <c r="D930" s="34"/>
       <c r="E930" s="34"/>
@@ -55424,8 +55549,8 @@
       </c>
     </row>
     <row r="931">
-      <c r="A931" s="76"/>
-      <c r="B931" s="77"/>
+      <c r="A931" s="74"/>
+      <c r="B931" s="75"/>
       <c r="C931" s="34"/>
       <c r="D931" s="34"/>
       <c r="E931" s="34"/>
@@ -55450,8 +55575,8 @@
       </c>
     </row>
     <row r="932">
-      <c r="A932" s="76"/>
-      <c r="B932" s="77"/>
+      <c r="A932" s="74"/>
+      <c r="B932" s="75"/>
       <c r="C932" s="34"/>
       <c r="D932" s="34"/>
       <c r="E932" s="34"/>
@@ -55476,8 +55601,8 @@
       </c>
     </row>
     <row r="933">
-      <c r="A933" s="76"/>
-      <c r="B933" s="77"/>
+      <c r="A933" s="74"/>
+      <c r="B933" s="75"/>
       <c r="C933" s="34"/>
       <c r="D933" s="34"/>
       <c r="E933" s="34"/>
@@ -55502,8 +55627,8 @@
       </c>
     </row>
     <row r="934">
-      <c r="A934" s="76"/>
-      <c r="B934" s="77"/>
+      <c r="A934" s="74"/>
+      <c r="B934" s="75"/>
       <c r="C934" s="34"/>
       <c r="D934" s="34"/>
       <c r="E934" s="34"/>
@@ -55528,8 +55653,8 @@
       </c>
     </row>
     <row r="935">
-      <c r="A935" s="76"/>
-      <c r="B935" s="77"/>
+      <c r="A935" s="74"/>
+      <c r="B935" s="75"/>
       <c r="C935" s="34"/>
       <c r="D935" s="34"/>
       <c r="E935" s="34"/>
@@ -55554,8 +55679,8 @@
       </c>
     </row>
     <row r="936">
-      <c r="A936" s="76"/>
-      <c r="B936" s="77"/>
+      <c r="A936" s="74"/>
+      <c r="B936" s="75"/>
       <c r="C936" s="34"/>
       <c r="D936" s="34"/>
       <c r="E936" s="34"/>
@@ -55580,8 +55705,8 @@
       </c>
     </row>
     <row r="937">
-      <c r="A937" s="76"/>
-      <c r="B937" s="77"/>
+      <c r="A937" s="74"/>
+      <c r="B937" s="75"/>
       <c r="C937" s="34"/>
       <c r="D937" s="34"/>
       <c r="E937" s="34"/>
@@ -55606,8 +55731,8 @@
       </c>
     </row>
     <row r="938">
-      <c r="A938" s="76"/>
-      <c r="B938" s="77"/>
+      <c r="A938" s="74"/>
+      <c r="B938" s="75"/>
       <c r="C938" s="34"/>
       <c r="D938" s="34"/>
       <c r="E938" s="34"/>
@@ -55632,8 +55757,8 @@
       </c>
     </row>
     <row r="939">
-      <c r="A939" s="76"/>
-      <c r="B939" s="77"/>
+      <c r="A939" s="74"/>
+      <c r="B939" s="75"/>
       <c r="C939" s="34"/>
       <c r="D939" s="34"/>
       <c r="E939" s="34"/>
@@ -55658,8 +55783,8 @@
       </c>
     </row>
     <row r="940">
-      <c r="A940" s="76"/>
-      <c r="B940" s="77"/>
+      <c r="A940" s="74"/>
+      <c r="B940" s="75"/>
       <c r="C940" s="34"/>
       <c r="D940" s="34"/>
       <c r="E940" s="34"/>
@@ -55684,8 +55809,8 @@
       </c>
     </row>
     <row r="941">
-      <c r="A941" s="76"/>
-      <c r="B941" s="77"/>
+      <c r="A941" s="74"/>
+      <c r="B941" s="75"/>
       <c r="C941" s="34"/>
       <c r="D941" s="34"/>
       <c r="E941" s="34"/>
@@ -55710,8 +55835,8 @@
       </c>
     </row>
     <row r="942">
-      <c r="A942" s="76"/>
-      <c r="B942" s="77"/>
+      <c r="A942" s="74"/>
+      <c r="B942" s="75"/>
       <c r="C942" s="34"/>
       <c r="D942" s="34"/>
       <c r="E942" s="34"/>
@@ -55736,8 +55861,8 @@
       </c>
     </row>
     <row r="943">
-      <c r="A943" s="76"/>
-      <c r="B943" s="77"/>
+      <c r="A943" s="74"/>
+      <c r="B943" s="75"/>
       <c r="C943" s="34"/>
       <c r="D943" s="34"/>
       <c r="E943" s="34"/>
@@ -55762,8 +55887,8 @@
       </c>
     </row>
     <row r="944">
-      <c r="A944" s="76"/>
-      <c r="B944" s="77"/>
+      <c r="A944" s="74"/>
+      <c r="B944" s="75"/>
       <c r="C944" s="34"/>
       <c r="D944" s="34"/>
       <c r="E944" s="34"/>
@@ -55788,8 +55913,8 @@
       </c>
     </row>
     <row r="945">
-      <c r="A945" s="76"/>
-      <c r="B945" s="77"/>
+      <c r="A945" s="74"/>
+      <c r="B945" s="75"/>
       <c r="C945" s="34"/>
       <c r="D945" s="34"/>
       <c r="E945" s="34"/>
@@ -55814,8 +55939,8 @@
       </c>
     </row>
     <row r="946">
-      <c r="A946" s="76"/>
-      <c r="B946" s="77"/>
+      <c r="A946" s="74"/>
+      <c r="B946" s="75"/>
       <c r="C946" s="34"/>
       <c r="D946" s="34"/>
       <c r="E946" s="34"/>
@@ -55840,8 +55965,8 @@
       </c>
     </row>
     <row r="947">
-      <c r="A947" s="76"/>
-      <c r="B947" s="77"/>
+      <c r="A947" s="74"/>
+      <c r="B947" s="75"/>
       <c r="C947" s="34"/>
       <c r="D947" s="34"/>
       <c r="E947" s="34"/>
@@ -55866,8 +55991,8 @@
       </c>
     </row>
     <row r="948">
-      <c r="A948" s="76"/>
-      <c r="B948" s="77"/>
+      <c r="A948" s="74"/>
+      <c r="B948" s="75"/>
       <c r="C948" s="34"/>
       <c r="D948" s="34"/>
       <c r="E948" s="34"/>
@@ -55892,8 +56017,8 @@
       </c>
     </row>
     <row r="949">
-      <c r="A949" s="76"/>
-      <c r="B949" s="77"/>
+      <c r="A949" s="74"/>
+      <c r="B949" s="75"/>
       <c r="C949" s="34"/>
       <c r="D949" s="34"/>
       <c r="E949" s="34"/>
@@ -55918,8 +56043,8 @@
       </c>
     </row>
     <row r="950">
-      <c r="A950" s="76"/>
-      <c r="B950" s="77"/>
+      <c r="A950" s="74"/>
+      <c r="B950" s="75"/>
       <c r="C950" s="34"/>
       <c r="D950" s="34"/>
       <c r="E950" s="34"/>
@@ -55944,8 +56069,8 @@
       </c>
     </row>
     <row r="951">
-      <c r="A951" s="76"/>
-      <c r="B951" s="77"/>
+      <c r="A951" s="74"/>
+      <c r="B951" s="75"/>
       <c r="C951" s="34"/>
       <c r="D951" s="34"/>
       <c r="E951" s="34"/>
@@ -55970,8 +56095,8 @@
       </c>
     </row>
     <row r="952">
-      <c r="A952" s="76"/>
-      <c r="B952" s="77"/>
+      <c r="A952" s="74"/>
+      <c r="B952" s="75"/>
       <c r="C952" s="34"/>
       <c r="D952" s="34"/>
       <c r="E952" s="34"/>
@@ -55996,8 +56121,8 @@
       </c>
     </row>
     <row r="953">
-      <c r="A953" s="76"/>
-      <c r="B953" s="77"/>
+      <c r="A953" s="74"/>
+      <c r="B953" s="75"/>
       <c r="C953" s="34"/>
       <c r="D953" s="34"/>
       <c r="E953" s="34"/>
@@ -56022,8 +56147,8 @@
       </c>
     </row>
     <row r="954">
-      <c r="A954" s="76"/>
-      <c r="B954" s="77"/>
+      <c r="A954" s="74"/>
+      <c r="B954" s="75"/>
       <c r="C954" s="34"/>
       <c r="D954" s="34"/>
       <c r="E954" s="34"/>
@@ -56048,8 +56173,8 @@
       </c>
     </row>
     <row r="955">
-      <c r="A955" s="76"/>
-      <c r="B955" s="77"/>
+      <c r="A955" s="74"/>
+      <c r="B955" s="75"/>
       <c r="C955" s="34"/>
       <c r="D955" s="34"/>
       <c r="E955" s="34"/>
@@ -56074,8 +56199,8 @@
       </c>
     </row>
     <row r="956">
-      <c r="A956" s="76"/>
-      <c r="B956" s="77"/>
+      <c r="A956" s="74"/>
+      <c r="B956" s="75"/>
       <c r="C956" s="34"/>
       <c r="D956" s="34"/>
       <c r="E956" s="34"/>
@@ -56100,8 +56225,8 @@
       </c>
     </row>
     <row r="957">
-      <c r="A957" s="76"/>
-      <c r="B957" s="77"/>
+      <c r="A957" s="74"/>
+      <c r="B957" s="75"/>
       <c r="C957" s="34"/>
       <c r="D957" s="34"/>
       <c r="E957" s="34"/>
@@ -56126,8 +56251,8 @@
       </c>
     </row>
     <row r="958">
-      <c r="A958" s="76"/>
-      <c r="B958" s="77"/>
+      <c r="A958" s="74"/>
+      <c r="B958" s="75"/>
       <c r="C958" s="34"/>
       <c r="D958" s="34"/>
       <c r="E958" s="34"/>
@@ -56152,8 +56277,8 @@
       </c>
     </row>
     <row r="959">
-      <c r="A959" s="76"/>
-      <c r="B959" s="77"/>
+      <c r="A959" s="74"/>
+      <c r="B959" s="75"/>
       <c r="C959" s="34"/>
       <c r="D959" s="34"/>
       <c r="E959" s="34"/>
@@ -56178,8 +56303,8 @@
       </c>
     </row>
     <row r="960">
-      <c r="A960" s="76"/>
-      <c r="B960" s="77"/>
+      <c r="A960" s="74"/>
+      <c r="B960" s="75"/>
       <c r="C960" s="34"/>
       <c r="D960" s="34"/>
       <c r="E960" s="34"/>
@@ -56204,8 +56329,8 @@
       </c>
     </row>
     <row r="961">
-      <c r="A961" s="76"/>
-      <c r="B961" s="77"/>
+      <c r="A961" s="74"/>
+      <c r="B961" s="75"/>
       <c r="C961" s="34"/>
       <c r="D961" s="34"/>
       <c r="E961" s="34"/>
@@ -56230,8 +56355,8 @@
       </c>
     </row>
     <row r="962">
-      <c r="A962" s="76"/>
-      <c r="B962" s="77"/>
+      <c r="A962" s="74"/>
+      <c r="B962" s="75"/>
       <c r="C962" s="34"/>
       <c r="D962" s="34"/>
       <c r="E962" s="34"/>
@@ -56256,8 +56381,8 @@
       </c>
     </row>
     <row r="963">
-      <c r="A963" s="76"/>
-      <c r="B963" s="77"/>
+      <c r="A963" s="74"/>
+      <c r="B963" s="75"/>
       <c r="C963" s="34"/>
       <c r="D963" s="34"/>
       <c r="E963" s="34"/>
@@ -56282,8 +56407,8 @@
       </c>
     </row>
     <row r="964">
-      <c r="A964" s="76"/>
-      <c r="B964" s="77"/>
+      <c r="A964" s="74"/>
+      <c r="B964" s="75"/>
       <c r="C964" s="34"/>
       <c r="D964" s="34"/>
       <c r="E964" s="34"/>
@@ -56308,8 +56433,8 @@
       </c>
     </row>
     <row r="965">
-      <c r="A965" s="76"/>
-      <c r="B965" s="77"/>
+      <c r="A965" s="74"/>
+      <c r="B965" s="75"/>
       <c r="C965" s="34"/>
       <c r="D965" s="34"/>
       <c r="E965" s="34"/>
@@ -56334,8 +56459,8 @@
       </c>
     </row>
     <row r="966">
-      <c r="A966" s="76"/>
-      <c r="B966" s="77"/>
+      <c r="A966" s="74"/>
+      <c r="B966" s="75"/>
       <c r="C966" s="34"/>
       <c r="D966" s="34"/>
       <c r="E966" s="34"/>
@@ -56360,8 +56485,8 @@
       </c>
     </row>
     <row r="967">
-      <c r="A967" s="76"/>
-      <c r="B967" s="77"/>
+      <c r="A967" s="74"/>
+      <c r="B967" s="75"/>
       <c r="C967" s="34"/>
       <c r="D967" s="34"/>
       <c r="E967" s="34"/>
@@ -56386,8 +56511,8 @@
       </c>
     </row>
     <row r="968">
-      <c r="A968" s="76"/>
-      <c r="B968" s="77"/>
+      <c r="A968" s="74"/>
+      <c r="B968" s="75"/>
       <c r="C968" s="34"/>
       <c r="D968" s="34"/>
       <c r="E968" s="34"/>
@@ -56412,8 +56537,8 @@
       </c>
     </row>
     <row r="969">
-      <c r="A969" s="76"/>
-      <c r="B969" s="77"/>
+      <c r="A969" s="74"/>
+      <c r="B969" s="75"/>
       <c r="C969" s="34"/>
       <c r="D969" s="34"/>
       <c r="E969" s="34"/>
@@ -56438,8 +56563,8 @@
       </c>
     </row>
     <row r="970">
-      <c r="A970" s="76"/>
-      <c r="B970" s="77"/>
+      <c r="A970" s="74"/>
+      <c r="B970" s="75"/>
       <c r="C970" s="34"/>
       <c r="D970" s="34"/>
       <c r="E970" s="34"/>
@@ -56464,8 +56589,8 @@
       </c>
     </row>
     <row r="971">
-      <c r="A971" s="76"/>
-      <c r="B971" s="77"/>
+      <c r="A971" s="74"/>
+      <c r="B971" s="75"/>
       <c r="C971" s="34"/>
       <c r="D971" s="34"/>
       <c r="E971" s="34"/>
@@ -56490,8 +56615,8 @@
       </c>
     </row>
     <row r="972">
-      <c r="A972" s="76"/>
-      <c r="B972" s="77"/>
+      <c r="A972" s="74"/>
+      <c r="B972" s="75"/>
       <c r="C972" s="34"/>
       <c r="D972" s="34"/>
       <c r="E972" s="34"/>
@@ -56516,8 +56641,8 @@
       </c>
     </row>
     <row r="973">
-      <c r="A973" s="76"/>
-      <c r="B973" s="77"/>
+      <c r="A973" s="74"/>
+      <c r="B973" s="75"/>
       <c r="C973" s="34"/>
       <c r="D973" s="34"/>
       <c r="E973" s="34"/>
@@ -56542,8 +56667,8 @@
       </c>
     </row>
     <row r="974">
-      <c r="A974" s="76"/>
-      <c r="B974" s="77"/>
+      <c r="A974" s="74"/>
+      <c r="B974" s="75"/>
       <c r="C974" s="34"/>
       <c r="D974" s="34"/>
       <c r="E974" s="34"/>
@@ -56568,8 +56693,8 @@
       </c>
     </row>
     <row r="975">
-      <c r="A975" s="76"/>
-      <c r="B975" s="77"/>
+      <c r="A975" s="74"/>
+      <c r="B975" s="75"/>
       <c r="C975" s="34"/>
       <c r="D975" s="34"/>
       <c r="E975" s="34"/>
@@ -56594,8 +56719,8 @@
       </c>
     </row>
     <row r="976">
-      <c r="A976" s="76"/>
-      <c r="B976" s="77"/>
+      <c r="A976" s="74"/>
+      <c r="B976" s="75"/>
       <c r="C976" s="34"/>
       <c r="D976" s="34"/>
       <c r="E976" s="34"/>
@@ -56620,8 +56745,8 @@
       </c>
     </row>
     <row r="977">
-      <c r="A977" s="76"/>
-      <c r="B977" s="77"/>
+      <c r="A977" s="74"/>
+      <c r="B977" s="75"/>
       <c r="C977" s="34"/>
       <c r="D977" s="34"/>
       <c r="E977" s="34"/>
@@ -56646,8 +56771,8 @@
       </c>
     </row>
     <row r="978">
-      <c r="A978" s="76"/>
-      <c r="B978" s="77"/>
+      <c r="A978" s="74"/>
+      <c r="B978" s="75"/>
       <c r="C978" s="34"/>
       <c r="D978" s="34"/>
       <c r="E978" s="34"/>
@@ -56672,8 +56797,8 @@
       </c>
     </row>
     <row r="979">
-      <c r="A979" s="76"/>
-      <c r="B979" s="77"/>
+      <c r="A979" s="74"/>
+      <c r="B979" s="75"/>
       <c r="C979" s="34"/>
       <c r="D979" s="34"/>
       <c r="E979" s="34"/>
@@ -56698,8 +56823,8 @@
       </c>
     </row>
     <row r="980">
-      <c r="A980" s="76"/>
-      <c r="B980" s="77"/>
+      <c r="A980" s="74"/>
+      <c r="B980" s="75"/>
       <c r="C980" s="34"/>
       <c r="D980" s="34"/>
       <c r="E980" s="34"/>
@@ -56724,8 +56849,8 @@
       </c>
     </row>
     <row r="981">
-      <c r="A981" s="76"/>
-      <c r="B981" s="77"/>
+      <c r="A981" s="74"/>
+      <c r="B981" s="75"/>
       <c r="C981" s="34"/>
       <c r="D981" s="34"/>
       <c r="E981" s="34"/>
@@ -56750,8 +56875,8 @@
       </c>
     </row>
     <row r="982">
-      <c r="A982" s="76"/>
-      <c r="B982" s="77"/>
+      <c r="A982" s="74"/>
+      <c r="B982" s="75"/>
       <c r="C982" s="34"/>
       <c r="D982" s="34"/>
       <c r="E982" s="34"/>
@@ -56776,8 +56901,8 @@
       </c>
     </row>
     <row r="983">
-      <c r="A983" s="76"/>
-      <c r="B983" s="77"/>
+      <c r="A983" s="74"/>
+      <c r="B983" s="75"/>
       <c r="C983" s="34"/>
       <c r="D983" s="34"/>
       <c r="E983" s="34"/>
@@ -56802,8 +56927,8 @@
       </c>
     </row>
     <row r="984">
-      <c r="A984" s="76"/>
-      <c r="B984" s="77"/>
+      <c r="A984" s="74"/>
+      <c r="B984" s="75"/>
       <c r="C984" s="34"/>
       <c r="D984" s="34"/>
       <c r="E984" s="34"/>
@@ -56828,8 +56953,8 @@
       </c>
     </row>
     <row r="985">
-      <c r="A985" s="76"/>
-      <c r="B985" s="77"/>
+      <c r="A985" s="74"/>
+      <c r="B985" s="75"/>
       <c r="C985" s="34"/>
       <c r="D985" s="34"/>
       <c r="E985" s="34"/>
@@ -56854,8 +56979,8 @@
       </c>
     </row>
     <row r="986">
-      <c r="A986" s="76"/>
-      <c r="B986" s="77"/>
+      <c r="A986" s="74"/>
+      <c r="B986" s="75"/>
       <c r="C986" s="34"/>
       <c r="D986" s="34"/>
       <c r="E986" s="34"/>
@@ -56880,8 +57005,8 @@
       </c>
     </row>
     <row r="987">
-      <c r="A987" s="76"/>
-      <c r="B987" s="77"/>
+      <c r="A987" s="74"/>
+      <c r="B987" s="75"/>
       <c r="C987" s="34"/>
       <c r="D987" s="34"/>
       <c r="E987" s="34"/>
@@ -56906,8 +57031,8 @@
       </c>
     </row>
     <row r="988">
-      <c r="A988" s="76"/>
-      <c r="B988" s="77"/>
+      <c r="A988" s="74"/>
+      <c r="B988" s="75"/>
       <c r="C988" s="34"/>
       <c r="D988" s="34"/>
       <c r="E988" s="34"/>
@@ -56932,8 +57057,8 @@
       </c>
     </row>
     <row r="989">
-      <c r="A989" s="76"/>
-      <c r="B989" s="77"/>
+      <c r="A989" s="74"/>
+      <c r="B989" s="75"/>
       <c r="C989" s="34"/>
       <c r="D989" s="34"/>
       <c r="E989" s="34"/>
@@ -56958,8 +57083,8 @@
       </c>
     </row>
     <row r="990">
-      <c r="A990" s="76"/>
-      <c r="B990" s="77"/>
+      <c r="A990" s="74"/>
+      <c r="B990" s="75"/>
       <c r="C990" s="34"/>
       <c r="D990" s="34"/>
       <c r="E990" s="34"/>
@@ -56984,8 +57109,8 @@
       </c>
     </row>
     <row r="991">
-      <c r="A991" s="76"/>
-      <c r="B991" s="77"/>
+      <c r="A991" s="74"/>
+      <c r="B991" s="75"/>
       <c r="C991" s="34"/>
       <c r="D991" s="34"/>
       <c r="E991" s="34"/>
@@ -57010,8 +57135,8 @@
       </c>
     </row>
     <row r="992">
-      <c r="A992" s="76"/>
-      <c r="B992" s="77"/>
+      <c r="A992" s="74"/>
+      <c r="B992" s="75"/>
       <c r="C992" s="34"/>
       <c r="D992" s="34"/>
       <c r="E992" s="34"/>
@@ -57036,8 +57161,8 @@
       </c>
     </row>
     <row r="993">
-      <c r="A993" s="76"/>
-      <c r="B993" s="77"/>
+      <c r="A993" s="74"/>
+      <c r="B993" s="75"/>
       <c r="C993" s="34"/>
       <c r="D993" s="34"/>
       <c r="E993" s="34"/>
@@ -57062,8 +57187,8 @@
       </c>
     </row>
     <row r="994">
-      <c r="A994" s="76"/>
-      <c r="B994" s="77"/>
+      <c r="A994" s="74"/>
+      <c r="B994" s="75"/>
       <c r="C994" s="34"/>
       <c r="D994" s="34"/>
       <c r="E994" s="34"/>
@@ -57088,8 +57213,8 @@
       </c>
     </row>
     <row r="995">
-      <c r="A995" s="76"/>
-      <c r="B995" s="77"/>
+      <c r="A995" s="74"/>
+      <c r="B995" s="75"/>
       <c r="C995" s="34"/>
       <c r="D995" s="34"/>
       <c r="E995" s="34"/>
@@ -57114,8 +57239,8 @@
       </c>
     </row>
     <row r="996">
-      <c r="A996" s="76"/>
-      <c r="B996" s="77"/>
+      <c r="A996" s="74"/>
+      <c r="B996" s="75"/>
       <c r="C996" s="34"/>
       <c r="D996" s="34"/>
       <c r="E996" s="34"/>
@@ -57140,8 +57265,8 @@
       </c>
     </row>
     <row r="997">
-      <c r="A997" s="76"/>
-      <c r="B997" s="77"/>
+      <c r="A997" s="74"/>
+      <c r="B997" s="75"/>
       <c r="C997" s="34"/>
       <c r="D997" s="34"/>
       <c r="E997" s="34"/>
@@ -57166,8 +57291,8 @@
       </c>
     </row>
     <row r="998">
-      <c r="A998" s="76"/>
-      <c r="B998" s="77"/>
+      <c r="A998" s="74"/>
+      <c r="B998" s="75"/>
       <c r="C998" s="34"/>
       <c r="D998" s="34"/>
       <c r="E998" s="34"/>
@@ -57192,8 +57317,8 @@
       </c>
     </row>
     <row r="999">
-      <c r="A999" s="76"/>
-      <c r="B999" s="77"/>
+      <c r="A999" s="74"/>
+      <c r="B999" s="75"/>
       <c r="C999" s="34"/>
       <c r="D999" s="34"/>
       <c r="E999" s="34"/>
@@ -57218,8 +57343,8 @@
       </c>
     </row>
     <row r="1000">
-      <c r="A1000" s="76"/>
-      <c r="B1000" s="77"/>
+      <c r="A1000" s="74"/>
+      <c r="B1000" s="75"/>
       <c r="C1000" s="34"/>
       <c r="D1000" s="34"/>
       <c r="E1000" s="34"/>
@@ -57244,8 +57369,8 @@
       </c>
     </row>
     <row r="1001">
-      <c r="A1001" s="76"/>
-      <c r="B1001" s="77"/>
+      <c r="A1001" s="74"/>
+      <c r="B1001" s="75"/>
       <c r="C1001" s="34"/>
       <c r="D1001" s="34"/>
       <c r="E1001" s="34"/>
@@ -57890,15 +58015,19 @@
     <hyperlink r:id="rId238" ref="S675"/>
     <hyperlink r:id="rId239" ref="S676"/>
     <hyperlink r:id="rId240" ref="S677"/>
+    <hyperlink r:id="rId241" ref="S678"/>
+    <hyperlink r:id="rId242" ref="S679"/>
+    <hyperlink r:id="rId243" ref="S680"/>
+    <hyperlink r:id="rId244" ref="S681"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId241"/>
-  <legacyDrawing r:id="rId242"/>
+  <drawing r:id="rId245"/>
+  <legacyDrawing r:id="rId246"/>
   <tableParts count="2">
-    <tablePart r:id="rId245"/>
-    <tablePart r:id="rId246"/>
+    <tablePart r:id="rId249"/>
+    <tablePart r:id="rId250"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201203
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -571,7 +571,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7721" uniqueCount="2439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7796" uniqueCount="2460">
   <si>
     <t>案例</t>
   </si>
@@ -8826,6 +8826,76 @@
     <t>10月中旬返回母國探親，11月13日再次來臺工作，入境迄今無疑似症狀
 個案檢疫期滿後，於11月30日由公司安排至醫院自費採檢</t>
   </si>
+  <si>
+    <t>#681</t>
+  </si>
+  <si>
+    <t>11/30 採檢
+12/2 確診</t>
+  </si>
+  <si>
+    <t>依11月28日因應「1127印尼專案」檢驗皆陰性，30日進行期滿前採檢</t>
+  </si>
+  <si>
+    <t>新增6例境外移入COVID-19病例，自印尼、美國及法國入境</t>
+  </si>
+  <si>
+    <t>#682</t>
+  </si>
+  <si>
+    <t>#683</t>
+  </si>
+  <si>
+    <t>11/29 採檢
+12/2 確診</t>
+  </si>
+  <si>
+    <t>11月29日檢疫期滿後搭乘專車至公司宿舍自主健康管理，同日由公司安排自費採檢</t>
+  </si>
+  <si>
+    <t>#684</t>
+  </si>
+  <si>
+    <t>-11/22 美國</t>
+  </si>
+  <si>
+    <t>11/26 採檢
+12/2 確診</t>
+  </si>
+  <si>
+    <t>長期於美國工作，11月22日返國入境後前往防疫旅館居家檢疫，同日晚間出現輕微嗅覺異常，11月23日症狀緩解，但隔天因嗅覺異常症狀加劇通報，11月26日經衛生單位安排就醫採檢</t>
+  </si>
+  <si>
+    <t>#685</t>
+  </si>
+  <si>
+    <t>賽普勒斯</t>
+  </si>
+  <si>
+    <t>-11/29 美國→台灣</t>
+  </si>
+  <si>
+    <t>11/29 採檢
+12/1 二採
+12/2 確診</t>
+  </si>
+  <si>
+    <t>發燒 食慾不振</t>
+  </si>
+  <si>
+    <t>自美國來臺洽商，持有登機前3日內核酸檢驗陰性報告，入境時因體溫異常(38.6度)，由機場檢疫人員安排至醫院採檢後前往集中檢疫所等待結果，11月30日持續有發燒症狀，12月1日因食慾不振，由衛生單位安排採檢通報</t>
+  </si>
+  <si>
+    <t>#686</t>
+  </si>
+  <si>
+    <t>-11/19 法國→土耳其
+-11/20 土耳其→台灣</t>
+  </si>
+  <si>
+    <t>因受臺灣公司邀請來臺從事商務活動，持有登機前3日內核酸檢驗陰性報告，11月19日自法國經土耳其轉機，於11月20日入境臺灣後，持前往防疫旅館居家檢疫。
+個案11月27日曾出現喉嚨痛症狀，因症狀持續，11月30日由衛生單位安排就醫採檢</t>
+  </si>
 </sst>
 </file>
 
@@ -8835,7 +8905,7 @@
     <numFmt numFmtId="164" formatCode="mm&quot;月&quot;dd&quot;日 &quot;dddd"/>
     <numFmt numFmtId="165" formatCode="m/d"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="21">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -8920,6 +8990,10 @@
       <u/>
       <color rgb="FF0000FF"/>
     </font>
+    <font/>
+    <font>
+      <color rgb="FF000000"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -8965,7 +9039,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="83">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -9187,6 +9261,27 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="19" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="20" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
@@ -49075,164 +49170,342 @@
       </c>
     </row>
     <row r="682">
-      <c r="A682" s="74"/>
-      <c r="B682" s="75"/>
-      <c r="C682" s="34"/>
-      <c r="D682" s="34"/>
-      <c r="E682" s="34"/>
+      <c r="A682" s="74" t="s">
+        <v>2439</v>
+      </c>
+      <c r="B682" s="6">
+        <v>44167.0</v>
+      </c>
+      <c r="C682" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D682" s="75" t="s">
+        <v>59</v>
+      </c>
+      <c r="E682" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F682" s="34"/>
-      <c r="G682" s="34"/>
-      <c r="H682" s="21"/>
-      <c r="I682" s="19"/>
-      <c r="J682" s="10"/>
-      <c r="K682" s="22"/>
-      <c r="L682" s="23"/>
-      <c r="M682" s="22"/>
+      <c r="G682" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H682" s="76" t="s">
+        <v>2280</v>
+      </c>
+      <c r="I682" s="77">
+        <v>44152.0</v>
+      </c>
+      <c r="J682" s="78" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K682" s="79" t="s">
+        <v>2440</v>
+      </c>
+      <c r="L682" s="78" t="s">
+        <v>426</v>
+      </c>
+      <c r="M682" s="79" t="s">
+        <v>1442</v>
+      </c>
       <c r="N682" s="25"/>
-      <c r="O682" s="21"/>
-      <c r="P682" s="21"/>
+      <c r="O682" s="76" t="s">
+        <v>85</v>
+      </c>
+      <c r="P682" s="76" t="s">
+        <v>2441</v>
+      </c>
       <c r="Q682" s="19"/>
       <c r="R682" s="19"/>
-      <c r="S682" s="20"/>
+      <c r="S682" s="61" t="s">
+        <v>2442</v>
+      </c>
       <c r="T682" s="20"/>
       <c r="U682" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#681</v>
       </c>
     </row>
     <row r="683">
-      <c r="A683" s="74"/>
-      <c r="B683" s="75"/>
-      <c r="C683" s="34"/>
-      <c r="D683" s="34"/>
-      <c r="E683" s="34"/>
+      <c r="A683" s="74" t="s">
+        <v>2443</v>
+      </c>
+      <c r="B683" s="6">
+        <v>44167.0</v>
+      </c>
+      <c r="C683" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D683" s="75" t="s">
+        <v>116</v>
+      </c>
+      <c r="E683" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F683" s="34"/>
-      <c r="G683" s="34"/>
-      <c r="H683" s="21"/>
-      <c r="I683" s="19"/>
-      <c r="J683" s="10"/>
-      <c r="K683" s="22"/>
-      <c r="L683" s="23"/>
-      <c r="M683" s="22"/>
+      <c r="G683" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H683" s="76" t="s">
+        <v>2280</v>
+      </c>
+      <c r="I683" s="77">
+        <v>44152.0</v>
+      </c>
+      <c r="J683" s="78" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K683" s="79" t="s">
+        <v>2440</v>
+      </c>
+      <c r="L683" s="78" t="s">
+        <v>426</v>
+      </c>
+      <c r="M683" s="79" t="s">
+        <v>1442</v>
+      </c>
       <c r="N683" s="25"/>
-      <c r="O683" s="21"/>
-      <c r="P683" s="21"/>
+      <c r="O683" s="76" t="s">
+        <v>85</v>
+      </c>
+      <c r="P683" s="76" t="s">
+        <v>2441</v>
+      </c>
       <c r="Q683" s="19"/>
       <c r="R683" s="19"/>
-      <c r="S683" s="20"/>
+      <c r="S683" s="61" t="s">
+        <v>2442</v>
+      </c>
       <c r="T683" s="20"/>
       <c r="U683" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#682</v>
       </c>
     </row>
     <row r="684">
-      <c r="A684" s="74"/>
-      <c r="B684" s="75"/>
-      <c r="C684" s="34"/>
-      <c r="D684" s="34"/>
-      <c r="E684" s="34"/>
+      <c r="A684" s="74" t="s">
+        <v>2444</v>
+      </c>
+      <c r="B684" s="6">
+        <v>44167.0</v>
+      </c>
+      <c r="C684" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D684" s="75" t="s">
+        <v>76</v>
+      </c>
+      <c r="E684" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F684" s="34"/>
-      <c r="G684" s="34"/>
-      <c r="H684" s="21"/>
-      <c r="I684" s="19"/>
-      <c r="J684" s="10"/>
-      <c r="K684" s="22"/>
-      <c r="L684" s="23"/>
-      <c r="M684" s="22"/>
+      <c r="G684" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H684" s="76" t="s">
+        <v>2375</v>
+      </c>
+      <c r="I684" s="77">
+        <v>44149.0</v>
+      </c>
+      <c r="J684" s="78" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K684" s="79" t="s">
+        <v>2445</v>
+      </c>
+      <c r="L684" s="12" t="s">
+        <v>1674</v>
+      </c>
+      <c r="M684" s="79" t="s">
+        <v>1442</v>
+      </c>
       <c r="N684" s="25"/>
-      <c r="O684" s="21"/>
-      <c r="P684" s="21"/>
+      <c r="O684" s="76" t="s">
+        <v>85</v>
+      </c>
+      <c r="P684" s="76" t="s">
+        <v>2446</v>
+      </c>
       <c r="Q684" s="19"/>
       <c r="R684" s="19"/>
-      <c r="S684" s="20"/>
+      <c r="S684" s="61" t="s">
+        <v>2442</v>
+      </c>
       <c r="T684" s="20"/>
       <c r="U684" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#683</v>
       </c>
     </row>
     <row r="685">
-      <c r="A685" s="74"/>
-      <c r="B685" s="75"/>
-      <c r="C685" s="34"/>
-      <c r="D685" s="34"/>
-      <c r="E685" s="34"/>
+      <c r="A685" s="74" t="s">
+        <v>2447</v>
+      </c>
+      <c r="B685" s="6">
+        <v>44167.0</v>
+      </c>
+      <c r="C685" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D685" s="75" t="s">
+        <v>116</v>
+      </c>
+      <c r="E685" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F685" s="34"/>
-      <c r="G685" s="34"/>
-      <c r="H685" s="21"/>
-      <c r="I685" s="19"/>
-      <c r="J685" s="10"/>
-      <c r="K685" s="22"/>
-      <c r="L685" s="23"/>
-      <c r="M685" s="22"/>
+      <c r="G685" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H685" s="76" t="s">
+        <v>2448</v>
+      </c>
+      <c r="I685" s="77">
+        <v>44157.0</v>
+      </c>
+      <c r="J685" s="80">
+        <v>44157.0</v>
+      </c>
+      <c r="K685" s="79" t="s">
+        <v>2449</v>
+      </c>
+      <c r="L685" s="78" t="s">
+        <v>426</v>
+      </c>
+      <c r="M685" s="79" t="s">
+        <v>1596</v>
+      </c>
       <c r="N685" s="25"/>
-      <c r="O685" s="21"/>
-      <c r="P685" s="21"/>
+      <c r="O685" s="76" t="s">
+        <v>85</v>
+      </c>
+      <c r="P685" s="76" t="s">
+        <v>2450</v>
+      </c>
       <c r="Q685" s="19"/>
       <c r="R685" s="19"/>
-      <c r="S685" s="20"/>
+      <c r="S685" s="61" t="s">
+        <v>2442</v>
+      </c>
       <c r="T685" s="20"/>
       <c r="U685" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#684</v>
       </c>
     </row>
     <row r="686">
-      <c r="A686" s="74"/>
-      <c r="B686" s="75"/>
-      <c r="C686" s="34"/>
-      <c r="D686" s="34"/>
-      <c r="E686" s="34"/>
+      <c r="A686" s="74" t="s">
+        <v>2451</v>
+      </c>
+      <c r="B686" s="6">
+        <v>44167.0</v>
+      </c>
+      <c r="C686" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D686" s="75" t="s">
+        <v>59</v>
+      </c>
+      <c r="E686" s="7" t="s">
+        <v>2452</v>
+      </c>
       <c r="F686" s="34"/>
-      <c r="G686" s="34"/>
-      <c r="H686" s="21"/>
-      <c r="I686" s="19"/>
+      <c r="G686" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H686" s="76" t="s">
+        <v>2453</v>
+      </c>
+      <c r="I686" s="77">
+        <v>44164.0</v>
+      </c>
       <c r="J686" s="10"/>
-      <c r="K686" s="22"/>
-      <c r="L686" s="23"/>
-      <c r="M686" s="22"/>
+      <c r="K686" s="79" t="s">
+        <v>2454</v>
+      </c>
+      <c r="L686" s="78" t="s">
+        <v>426</v>
+      </c>
+      <c r="M686" s="79" t="s">
+        <v>2455</v>
+      </c>
       <c r="N686" s="25"/>
-      <c r="O686" s="21"/>
-      <c r="P686" s="21"/>
+      <c r="O686" s="76" t="s">
+        <v>85</v>
+      </c>
+      <c r="P686" s="76" t="s">
+        <v>2456</v>
+      </c>
       <c r="Q686" s="19"/>
       <c r="R686" s="19"/>
-      <c r="S686" s="20"/>
+      <c r="S686" s="61" t="s">
+        <v>2442</v>
+      </c>
       <c r="T686" s="20"/>
       <c r="U686" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#685</v>
       </c>
     </row>
     <row r="687">
-      <c r="A687" s="74"/>
-      <c r="B687" s="75"/>
-      <c r="C687" s="34"/>
-      <c r="D687" s="34"/>
-      <c r="E687" s="34"/>
+      <c r="A687" s="74" t="s">
+        <v>2457</v>
+      </c>
+      <c r="B687" s="6">
+        <v>44167.0</v>
+      </c>
+      <c r="C687" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D687" s="75" t="s">
+        <v>22</v>
+      </c>
+      <c r="E687" s="7" t="s">
+        <v>351</v>
+      </c>
       <c r="F687" s="34"/>
-      <c r="G687" s="34"/>
-      <c r="H687" s="21"/>
-      <c r="I687" s="19"/>
-      <c r="J687" s="10"/>
-      <c r="K687" s="22"/>
-      <c r="L687" s="23"/>
-      <c r="M687" s="22"/>
+      <c r="G687" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H687" s="76" t="s">
+        <v>2458</v>
+      </c>
+      <c r="I687" s="77">
+        <v>44155.0</v>
+      </c>
+      <c r="J687" s="80">
+        <v>44162.0</v>
+      </c>
+      <c r="K687" s="79" t="s">
+        <v>2440</v>
+      </c>
+      <c r="L687" s="78" t="s">
+        <v>426</v>
+      </c>
+      <c r="M687" s="79" t="s">
+        <v>518</v>
+      </c>
       <c r="N687" s="25"/>
-      <c r="O687" s="21"/>
-      <c r="P687" s="21"/>
+      <c r="O687" s="76" t="s">
+        <v>85</v>
+      </c>
+      <c r="P687" s="76" t="s">
+        <v>2459</v>
+      </c>
       <c r="Q687" s="19"/>
       <c r="R687" s="19"/>
-      <c r="S687" s="20"/>
+      <c r="S687" s="61" t="s">
+        <v>2442</v>
+      </c>
       <c r="T687" s="20"/>
       <c r="U687" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#686</v>
       </c>
     </row>
     <row r="688">
-      <c r="A688" s="74"/>
-      <c r="B688" s="75"/>
+      <c r="A688" s="81"/>
+      <c r="B688" s="82"/>
       <c r="C688" s="34"/>
       <c r="D688" s="34"/>
       <c r="E688" s="34"/>
@@ -49257,8 +49530,8 @@
       </c>
     </row>
     <row r="689">
-      <c r="A689" s="74"/>
-      <c r="B689" s="75"/>
+      <c r="A689" s="81"/>
+      <c r="B689" s="82"/>
       <c r="C689" s="34"/>
       <c r="D689" s="34"/>
       <c r="E689" s="34"/>
@@ -49283,8 +49556,8 @@
       </c>
     </row>
     <row r="690">
-      <c r="A690" s="74"/>
-      <c r="B690" s="75"/>
+      <c r="A690" s="81"/>
+      <c r="B690" s="82"/>
       <c r="C690" s="34"/>
       <c r="D690" s="34"/>
       <c r="E690" s="34"/>
@@ -49309,8 +49582,8 @@
       </c>
     </row>
     <row r="691">
-      <c r="A691" s="74"/>
-      <c r="B691" s="75"/>
+      <c r="A691" s="81"/>
+      <c r="B691" s="82"/>
       <c r="C691" s="34"/>
       <c r="D691" s="34"/>
       <c r="E691" s="34"/>
@@ -49335,8 +49608,8 @@
       </c>
     </row>
     <row r="692">
-      <c r="A692" s="74"/>
-      <c r="B692" s="75"/>
+      <c r="A692" s="81"/>
+      <c r="B692" s="82"/>
       <c r="C692" s="34"/>
       <c r="D692" s="34"/>
       <c r="E692" s="34"/>
@@ -49361,8 +49634,8 @@
       </c>
     </row>
     <row r="693">
-      <c r="A693" s="74"/>
-      <c r="B693" s="75"/>
+      <c r="A693" s="81"/>
+      <c r="B693" s="82"/>
       <c r="C693" s="34"/>
       <c r="D693" s="34"/>
       <c r="E693" s="34"/>
@@ -49387,8 +49660,8 @@
       </c>
     </row>
     <row r="694">
-      <c r="A694" s="74"/>
-      <c r="B694" s="75"/>
+      <c r="A694" s="81"/>
+      <c r="B694" s="82"/>
       <c r="C694" s="34"/>
       <c r="D694" s="34"/>
       <c r="E694" s="34"/>
@@ -49413,8 +49686,8 @@
       </c>
     </row>
     <row r="695">
-      <c r="A695" s="74"/>
-      <c r="B695" s="75"/>
+      <c r="A695" s="81"/>
+      <c r="B695" s="82"/>
       <c r="C695" s="34"/>
       <c r="D695" s="34"/>
       <c r="E695" s="34"/>
@@ -49439,8 +49712,8 @@
       </c>
     </row>
     <row r="696">
-      <c r="A696" s="74"/>
-      <c r="B696" s="75"/>
+      <c r="A696" s="81"/>
+      <c r="B696" s="82"/>
       <c r="C696" s="34"/>
       <c r="D696" s="34"/>
       <c r="E696" s="34"/>
@@ -49465,8 +49738,8 @@
       </c>
     </row>
     <row r="697">
-      <c r="A697" s="74"/>
-      <c r="B697" s="75"/>
+      <c r="A697" s="81"/>
+      <c r="B697" s="82"/>
       <c r="C697" s="34"/>
       <c r="D697" s="34"/>
       <c r="E697" s="34"/>
@@ -49491,8 +49764,8 @@
       </c>
     </row>
     <row r="698">
-      <c r="A698" s="74"/>
-      <c r="B698" s="75"/>
+      <c r="A698" s="81"/>
+      <c r="B698" s="82"/>
       <c r="C698" s="34"/>
       <c r="D698" s="34"/>
       <c r="E698" s="34"/>
@@ -49517,8 +49790,8 @@
       </c>
     </row>
     <row r="699">
-      <c r="A699" s="74"/>
-      <c r="B699" s="75"/>
+      <c r="A699" s="81"/>
+      <c r="B699" s="82"/>
       <c r="C699" s="34"/>
       <c r="D699" s="34"/>
       <c r="E699" s="34"/>
@@ -49543,8 +49816,8 @@
       </c>
     </row>
     <row r="700">
-      <c r="A700" s="74"/>
-      <c r="B700" s="75"/>
+      <c r="A700" s="81"/>
+      <c r="B700" s="82"/>
       <c r="C700" s="34"/>
       <c r="D700" s="34"/>
       <c r="E700" s="34"/>
@@ -49569,8 +49842,8 @@
       </c>
     </row>
     <row r="701">
-      <c r="A701" s="74"/>
-      <c r="B701" s="75"/>
+      <c r="A701" s="81"/>
+      <c r="B701" s="82"/>
       <c r="C701" s="34"/>
       <c r="D701" s="34"/>
       <c r="E701" s="34"/>
@@ -49595,8 +49868,8 @@
       </c>
     </row>
     <row r="702">
-      <c r="A702" s="74"/>
-      <c r="B702" s="75"/>
+      <c r="A702" s="81"/>
+      <c r="B702" s="82"/>
       <c r="C702" s="34"/>
       <c r="D702" s="34"/>
       <c r="E702" s="34"/>
@@ -49621,8 +49894,8 @@
       </c>
     </row>
     <row r="703">
-      <c r="A703" s="74"/>
-      <c r="B703" s="75"/>
+      <c r="A703" s="81"/>
+      <c r="B703" s="82"/>
       <c r="C703" s="34"/>
       <c r="D703" s="34"/>
       <c r="E703" s="34"/>
@@ -49647,8 +49920,8 @@
       </c>
     </row>
     <row r="704">
-      <c r="A704" s="74"/>
-      <c r="B704" s="75"/>
+      <c r="A704" s="81"/>
+      <c r="B704" s="82"/>
       <c r="C704" s="34"/>
       <c r="D704" s="34"/>
       <c r="E704" s="34"/>
@@ -49673,8 +49946,8 @@
       </c>
     </row>
     <row r="705">
-      <c r="A705" s="74"/>
-      <c r="B705" s="75"/>
+      <c r="A705" s="81"/>
+      <c r="B705" s="82"/>
       <c r="C705" s="34"/>
       <c r="D705" s="34"/>
       <c r="E705" s="34"/>
@@ -49699,8 +49972,8 @@
       </c>
     </row>
     <row r="706">
-      <c r="A706" s="74"/>
-      <c r="B706" s="75"/>
+      <c r="A706" s="81"/>
+      <c r="B706" s="82"/>
       <c r="C706" s="34"/>
       <c r="D706" s="34"/>
       <c r="E706" s="34"/>
@@ -49725,8 +49998,8 @@
       </c>
     </row>
     <row r="707">
-      <c r="A707" s="74"/>
-      <c r="B707" s="75"/>
+      <c r="A707" s="81"/>
+      <c r="B707" s="82"/>
       <c r="C707" s="34"/>
       <c r="D707" s="34"/>
       <c r="E707" s="34"/>
@@ -49751,8 +50024,8 @@
       </c>
     </row>
     <row r="708">
-      <c r="A708" s="74"/>
-      <c r="B708" s="75"/>
+      <c r="A708" s="81"/>
+      <c r="B708" s="82"/>
       <c r="C708" s="34"/>
       <c r="D708" s="34"/>
       <c r="E708" s="34"/>
@@ -49777,8 +50050,8 @@
       </c>
     </row>
     <row r="709">
-      <c r="A709" s="74"/>
-      <c r="B709" s="75"/>
+      <c r="A709" s="81"/>
+      <c r="B709" s="82"/>
       <c r="C709" s="34"/>
       <c r="D709" s="34"/>
       <c r="E709" s="34"/>
@@ -49803,8 +50076,8 @@
       </c>
     </row>
     <row r="710">
-      <c r="A710" s="74"/>
-      <c r="B710" s="75"/>
+      <c r="A710" s="81"/>
+      <c r="B710" s="82"/>
       <c r="C710" s="34"/>
       <c r="D710" s="34"/>
       <c r="E710" s="34"/>
@@ -49829,8 +50102,8 @@
       </c>
     </row>
     <row r="711">
-      <c r="A711" s="74"/>
-      <c r="B711" s="75"/>
+      <c r="A711" s="81"/>
+      <c r="B711" s="82"/>
       <c r="C711" s="34"/>
       <c r="D711" s="34"/>
       <c r="E711" s="34"/>
@@ -49855,8 +50128,8 @@
       </c>
     </row>
     <row r="712">
-      <c r="A712" s="74"/>
-      <c r="B712" s="75"/>
+      <c r="A712" s="81"/>
+      <c r="B712" s="82"/>
       <c r="C712" s="34"/>
       <c r="D712" s="34"/>
       <c r="E712" s="34"/>
@@ -49881,8 +50154,8 @@
       </c>
     </row>
     <row r="713">
-      <c r="A713" s="74"/>
-      <c r="B713" s="75"/>
+      <c r="A713" s="81"/>
+      <c r="B713" s="82"/>
       <c r="C713" s="34"/>
       <c r="D713" s="34"/>
       <c r="E713" s="34"/>
@@ -49907,8 +50180,8 @@
       </c>
     </row>
     <row r="714">
-      <c r="A714" s="74"/>
-      <c r="B714" s="75"/>
+      <c r="A714" s="81"/>
+      <c r="B714" s="82"/>
       <c r="C714" s="34"/>
       <c r="D714" s="34"/>
       <c r="E714" s="34"/>
@@ -49933,8 +50206,8 @@
       </c>
     </row>
     <row r="715">
-      <c r="A715" s="74"/>
-      <c r="B715" s="75"/>
+      <c r="A715" s="81"/>
+      <c r="B715" s="82"/>
       <c r="C715" s="34"/>
       <c r="D715" s="34"/>
       <c r="E715" s="34"/>
@@ -49959,8 +50232,8 @@
       </c>
     </row>
     <row r="716">
-      <c r="A716" s="74"/>
-      <c r="B716" s="75"/>
+      <c r="A716" s="81"/>
+      <c r="B716" s="82"/>
       <c r="C716" s="34"/>
       <c r="D716" s="34"/>
       <c r="E716" s="34"/>
@@ -49985,8 +50258,8 @@
       </c>
     </row>
     <row r="717">
-      <c r="A717" s="74"/>
-      <c r="B717" s="75"/>
+      <c r="A717" s="81"/>
+      <c r="B717" s="82"/>
       <c r="C717" s="34"/>
       <c r="D717" s="34"/>
       <c r="E717" s="34"/>
@@ -50011,8 +50284,8 @@
       </c>
     </row>
     <row r="718">
-      <c r="A718" s="74"/>
-      <c r="B718" s="75"/>
+      <c r="A718" s="81"/>
+      <c r="B718" s="82"/>
       <c r="C718" s="34"/>
       <c r="D718" s="34"/>
       <c r="E718" s="34"/>
@@ -50037,8 +50310,8 @@
       </c>
     </row>
     <row r="719">
-      <c r="A719" s="74"/>
-      <c r="B719" s="75"/>
+      <c r="A719" s="81"/>
+      <c r="B719" s="82"/>
       <c r="C719" s="34"/>
       <c r="D719" s="34"/>
       <c r="E719" s="34"/>
@@ -50063,8 +50336,8 @@
       </c>
     </row>
     <row r="720">
-      <c r="A720" s="74"/>
-      <c r="B720" s="75"/>
+      <c r="A720" s="81"/>
+      <c r="B720" s="82"/>
       <c r="C720" s="34"/>
       <c r="D720" s="34"/>
       <c r="E720" s="34"/>
@@ -50089,8 +50362,8 @@
       </c>
     </row>
     <row r="721">
-      <c r="A721" s="74"/>
-      <c r="B721" s="75"/>
+      <c r="A721" s="81"/>
+      <c r="B721" s="82"/>
       <c r="C721" s="34"/>
       <c r="D721" s="34"/>
       <c r="E721" s="34"/>
@@ -50115,8 +50388,8 @@
       </c>
     </row>
     <row r="722">
-      <c r="A722" s="74"/>
-      <c r="B722" s="75"/>
+      <c r="A722" s="81"/>
+      <c r="B722" s="82"/>
       <c r="C722" s="34"/>
       <c r="D722" s="34"/>
       <c r="E722" s="34"/>
@@ -50141,8 +50414,8 @@
       </c>
     </row>
     <row r="723">
-      <c r="A723" s="74"/>
-      <c r="B723" s="75"/>
+      <c r="A723" s="81"/>
+      <c r="B723" s="82"/>
       <c r="C723" s="34"/>
       <c r="D723" s="34"/>
       <c r="E723" s="34"/>
@@ -50167,8 +50440,8 @@
       </c>
     </row>
     <row r="724">
-      <c r="A724" s="74"/>
-      <c r="B724" s="75"/>
+      <c r="A724" s="81"/>
+      <c r="B724" s="82"/>
       <c r="C724" s="34"/>
       <c r="D724" s="34"/>
       <c r="E724" s="34"/>
@@ -50193,8 +50466,8 @@
       </c>
     </row>
     <row r="725">
-      <c r="A725" s="74"/>
-      <c r="B725" s="75"/>
+      <c r="A725" s="81"/>
+      <c r="B725" s="82"/>
       <c r="C725" s="34"/>
       <c r="D725" s="34"/>
       <c r="E725" s="34"/>
@@ -50219,8 +50492,8 @@
       </c>
     </row>
     <row r="726">
-      <c r="A726" s="74"/>
-      <c r="B726" s="75"/>
+      <c r="A726" s="81"/>
+      <c r="B726" s="82"/>
       <c r="C726" s="34"/>
       <c r="D726" s="34"/>
       <c r="E726" s="34"/>
@@ -50245,8 +50518,8 @@
       </c>
     </row>
     <row r="727">
-      <c r="A727" s="74"/>
-      <c r="B727" s="75"/>
+      <c r="A727" s="81"/>
+      <c r="B727" s="82"/>
       <c r="C727" s="34"/>
       <c r="D727" s="34"/>
       <c r="E727" s="34"/>
@@ -50271,8 +50544,8 @@
       </c>
     </row>
     <row r="728">
-      <c r="A728" s="74"/>
-      <c r="B728" s="75"/>
+      <c r="A728" s="81"/>
+      <c r="B728" s="82"/>
       <c r="C728" s="34"/>
       <c r="D728" s="34"/>
       <c r="E728" s="34"/>
@@ -50297,8 +50570,8 @@
       </c>
     </row>
     <row r="729">
-      <c r="A729" s="74"/>
-      <c r="B729" s="75"/>
+      <c r="A729" s="81"/>
+      <c r="B729" s="82"/>
       <c r="C729" s="34"/>
       <c r="D729" s="34"/>
       <c r="E729" s="34"/>
@@ -50323,8 +50596,8 @@
       </c>
     </row>
     <row r="730">
-      <c r="A730" s="74"/>
-      <c r="B730" s="75"/>
+      <c r="A730" s="81"/>
+      <c r="B730" s="82"/>
       <c r="C730" s="34"/>
       <c r="D730" s="34"/>
       <c r="E730" s="34"/>
@@ -50349,8 +50622,8 @@
       </c>
     </row>
     <row r="731">
-      <c r="A731" s="74"/>
-      <c r="B731" s="75"/>
+      <c r="A731" s="81"/>
+      <c r="B731" s="82"/>
       <c r="C731" s="34"/>
       <c r="D731" s="34"/>
       <c r="E731" s="34"/>
@@ -50375,8 +50648,8 @@
       </c>
     </row>
     <row r="732">
-      <c r="A732" s="74"/>
-      <c r="B732" s="75"/>
+      <c r="A732" s="81"/>
+      <c r="B732" s="82"/>
       <c r="C732" s="34"/>
       <c r="D732" s="34"/>
       <c r="E732" s="34"/>
@@ -50401,8 +50674,8 @@
       </c>
     </row>
     <row r="733">
-      <c r="A733" s="74"/>
-      <c r="B733" s="75"/>
+      <c r="A733" s="81"/>
+      <c r="B733" s="82"/>
       <c r="C733" s="34"/>
       <c r="D733" s="34"/>
       <c r="E733" s="34"/>
@@ -50427,8 +50700,8 @@
       </c>
     </row>
     <row r="734">
-      <c r="A734" s="74"/>
-      <c r="B734" s="75"/>
+      <c r="A734" s="81"/>
+      <c r="B734" s="82"/>
       <c r="C734" s="34"/>
       <c r="D734" s="34"/>
       <c r="E734" s="34"/>
@@ -50453,8 +50726,8 @@
       </c>
     </row>
     <row r="735">
-      <c r="A735" s="74"/>
-      <c r="B735" s="75"/>
+      <c r="A735" s="81"/>
+      <c r="B735" s="82"/>
       <c r="C735" s="34"/>
       <c r="D735" s="34"/>
       <c r="E735" s="34"/>
@@ -50479,8 +50752,8 @@
       </c>
     </row>
     <row r="736">
-      <c r="A736" s="74"/>
-      <c r="B736" s="75"/>
+      <c r="A736" s="81"/>
+      <c r="B736" s="82"/>
       <c r="C736" s="34"/>
       <c r="D736" s="34"/>
       <c r="E736" s="34"/>
@@ -50505,8 +50778,8 @@
       </c>
     </row>
     <row r="737">
-      <c r="A737" s="74"/>
-      <c r="B737" s="75"/>
+      <c r="A737" s="81"/>
+      <c r="B737" s="82"/>
       <c r="C737" s="34"/>
       <c r="D737" s="34"/>
       <c r="E737" s="34"/>
@@ -50531,8 +50804,8 @@
       </c>
     </row>
     <row r="738">
-      <c r="A738" s="74"/>
-      <c r="B738" s="75"/>
+      <c r="A738" s="81"/>
+      <c r="B738" s="82"/>
       <c r="C738" s="34"/>
       <c r="D738" s="34"/>
       <c r="E738" s="34"/>
@@ -50557,8 +50830,8 @@
       </c>
     </row>
     <row r="739">
-      <c r="A739" s="74"/>
-      <c r="B739" s="75"/>
+      <c r="A739" s="81"/>
+      <c r="B739" s="82"/>
       <c r="C739" s="34"/>
       <c r="D739" s="34"/>
       <c r="E739" s="34"/>
@@ -50583,8 +50856,8 @@
       </c>
     </row>
     <row r="740">
-      <c r="A740" s="74"/>
-      <c r="B740" s="75"/>
+      <c r="A740" s="81"/>
+      <c r="B740" s="82"/>
       <c r="C740" s="34"/>
       <c r="D740" s="34"/>
       <c r="E740" s="34"/>
@@ -50609,8 +50882,8 @@
       </c>
     </row>
     <row r="741">
-      <c r="A741" s="74"/>
-      <c r="B741" s="75"/>
+      <c r="A741" s="81"/>
+      <c r="B741" s="82"/>
       <c r="C741" s="34"/>
       <c r="D741" s="34"/>
       <c r="E741" s="34"/>
@@ -50635,8 +50908,8 @@
       </c>
     </row>
     <row r="742">
-      <c r="A742" s="74"/>
-      <c r="B742" s="75"/>
+      <c r="A742" s="81"/>
+      <c r="B742" s="82"/>
       <c r="C742" s="34"/>
       <c r="D742" s="34"/>
       <c r="E742" s="34"/>
@@ -50661,8 +50934,8 @@
       </c>
     </row>
     <row r="743">
-      <c r="A743" s="74"/>
-      <c r="B743" s="75"/>
+      <c r="A743" s="81"/>
+      <c r="B743" s="82"/>
       <c r="C743" s="34"/>
       <c r="D743" s="34"/>
       <c r="E743" s="34"/>
@@ -50687,8 +50960,8 @@
       </c>
     </row>
     <row r="744">
-      <c r="A744" s="74"/>
-      <c r="B744" s="75"/>
+      <c r="A744" s="81"/>
+      <c r="B744" s="82"/>
       <c r="C744" s="34"/>
       <c r="D744" s="34"/>
       <c r="E744" s="34"/>
@@ -50713,8 +50986,8 @@
       </c>
     </row>
     <row r="745">
-      <c r="A745" s="74"/>
-      <c r="B745" s="75"/>
+      <c r="A745" s="81"/>
+      <c r="B745" s="82"/>
       <c r="C745" s="34"/>
       <c r="D745" s="34"/>
       <c r="E745" s="34"/>
@@ -50739,8 +51012,8 @@
       </c>
     </row>
     <row r="746">
-      <c r="A746" s="74"/>
-      <c r="B746" s="75"/>
+      <c r="A746" s="81"/>
+      <c r="B746" s="82"/>
       <c r="C746" s="34"/>
       <c r="D746" s="34"/>
       <c r="E746" s="34"/>
@@ -50765,8 +51038,8 @@
       </c>
     </row>
     <row r="747">
-      <c r="A747" s="74"/>
-      <c r="B747" s="75"/>
+      <c r="A747" s="81"/>
+      <c r="B747" s="82"/>
       <c r="C747" s="34"/>
       <c r="D747" s="34"/>
       <c r="E747" s="34"/>
@@ -50791,8 +51064,8 @@
       </c>
     </row>
     <row r="748">
-      <c r="A748" s="74"/>
-      <c r="B748" s="75"/>
+      <c r="A748" s="81"/>
+      <c r="B748" s="82"/>
       <c r="C748" s="34"/>
       <c r="D748" s="34"/>
       <c r="E748" s="34"/>
@@ -50817,8 +51090,8 @@
       </c>
     </row>
     <row r="749">
-      <c r="A749" s="74"/>
-      <c r="B749" s="75"/>
+      <c r="A749" s="81"/>
+      <c r="B749" s="82"/>
       <c r="C749" s="34"/>
       <c r="D749" s="34"/>
       <c r="E749" s="34"/>
@@ -50843,8 +51116,8 @@
       </c>
     </row>
     <row r="750">
-      <c r="A750" s="74"/>
-      <c r="B750" s="75"/>
+      <c r="A750" s="81"/>
+      <c r="B750" s="82"/>
       <c r="C750" s="34"/>
       <c r="D750" s="34"/>
       <c r="E750" s="34"/>
@@ -50869,8 +51142,8 @@
       </c>
     </row>
     <row r="751">
-      <c r="A751" s="74"/>
-      <c r="B751" s="75"/>
+      <c r="A751" s="81"/>
+      <c r="B751" s="82"/>
       <c r="C751" s="34"/>
       <c r="D751" s="34"/>
       <c r="E751" s="34"/>
@@ -50895,8 +51168,8 @@
       </c>
     </row>
     <row r="752">
-      <c r="A752" s="74"/>
-      <c r="B752" s="75"/>
+      <c r="A752" s="81"/>
+      <c r="B752" s="82"/>
       <c r="C752" s="34"/>
       <c r="D752" s="34"/>
       <c r="E752" s="34"/>
@@ -50921,8 +51194,8 @@
       </c>
     </row>
     <row r="753">
-      <c r="A753" s="74"/>
-      <c r="B753" s="75"/>
+      <c r="A753" s="81"/>
+      <c r="B753" s="82"/>
       <c r="C753" s="34"/>
       <c r="D753" s="34"/>
       <c r="E753" s="34"/>
@@ -50947,8 +51220,8 @@
       </c>
     </row>
     <row r="754">
-      <c r="A754" s="74"/>
-      <c r="B754" s="75"/>
+      <c r="A754" s="81"/>
+      <c r="B754" s="82"/>
       <c r="C754" s="34"/>
       <c r="D754" s="34"/>
       <c r="E754" s="34"/>
@@ -50973,8 +51246,8 @@
       </c>
     </row>
     <row r="755">
-      <c r="A755" s="74"/>
-      <c r="B755" s="75"/>
+      <c r="A755" s="81"/>
+      <c r="B755" s="82"/>
       <c r="C755" s="34"/>
       <c r="D755" s="34"/>
       <c r="E755" s="34"/>
@@ -50999,8 +51272,8 @@
       </c>
     </row>
     <row r="756">
-      <c r="A756" s="74"/>
-      <c r="B756" s="75"/>
+      <c r="A756" s="81"/>
+      <c r="B756" s="82"/>
       <c r="C756" s="34"/>
       <c r="D756" s="34"/>
       <c r="E756" s="34"/>
@@ -51025,8 +51298,8 @@
       </c>
     </row>
     <row r="757">
-      <c r="A757" s="74"/>
-      <c r="B757" s="75"/>
+      <c r="A757" s="81"/>
+      <c r="B757" s="82"/>
       <c r="C757" s="34"/>
       <c r="D757" s="34"/>
       <c r="E757" s="34"/>
@@ -51051,8 +51324,8 @@
       </c>
     </row>
     <row r="758">
-      <c r="A758" s="74"/>
-      <c r="B758" s="75"/>
+      <c r="A758" s="81"/>
+      <c r="B758" s="82"/>
       <c r="C758" s="34"/>
       <c r="D758" s="34"/>
       <c r="E758" s="34"/>
@@ -51077,8 +51350,8 @@
       </c>
     </row>
     <row r="759">
-      <c r="A759" s="74"/>
-      <c r="B759" s="75"/>
+      <c r="A759" s="81"/>
+      <c r="B759" s="82"/>
       <c r="C759" s="34"/>
       <c r="D759" s="34"/>
       <c r="E759" s="34"/>
@@ -51103,8 +51376,8 @@
       </c>
     </row>
     <row r="760">
-      <c r="A760" s="74"/>
-      <c r="B760" s="75"/>
+      <c r="A760" s="81"/>
+      <c r="B760" s="82"/>
       <c r="C760" s="34"/>
       <c r="D760" s="34"/>
       <c r="E760" s="34"/>
@@ -51129,8 +51402,8 @@
       </c>
     </row>
     <row r="761">
-      <c r="A761" s="74"/>
-      <c r="B761" s="75"/>
+      <c r="A761" s="81"/>
+      <c r="B761" s="82"/>
       <c r="C761" s="34"/>
       <c r="D761" s="34"/>
       <c r="E761" s="34"/>
@@ -51155,8 +51428,8 @@
       </c>
     </row>
     <row r="762">
-      <c r="A762" s="74"/>
-      <c r="B762" s="75"/>
+      <c r="A762" s="81"/>
+      <c r="B762" s="82"/>
       <c r="C762" s="34"/>
       <c r="D762" s="34"/>
       <c r="E762" s="34"/>
@@ -51181,8 +51454,8 @@
       </c>
     </row>
     <row r="763">
-      <c r="A763" s="74"/>
-      <c r="B763" s="75"/>
+      <c r="A763" s="81"/>
+      <c r="B763" s="82"/>
       <c r="C763" s="34"/>
       <c r="D763" s="34"/>
       <c r="E763" s="34"/>
@@ -51207,8 +51480,8 @@
       </c>
     </row>
     <row r="764">
-      <c r="A764" s="74"/>
-      <c r="B764" s="75"/>
+      <c r="A764" s="81"/>
+      <c r="B764" s="82"/>
       <c r="C764" s="34"/>
       <c r="D764" s="34"/>
       <c r="E764" s="34"/>
@@ -51233,8 +51506,8 @@
       </c>
     </row>
     <row r="765">
-      <c r="A765" s="74"/>
-      <c r="B765" s="75"/>
+      <c r="A765" s="81"/>
+      <c r="B765" s="82"/>
       <c r="C765" s="34"/>
       <c r="D765" s="34"/>
       <c r="E765" s="34"/>
@@ -51259,8 +51532,8 @@
       </c>
     </row>
     <row r="766">
-      <c r="A766" s="74"/>
-      <c r="B766" s="75"/>
+      <c r="A766" s="81"/>
+      <c r="B766" s="82"/>
       <c r="C766" s="34"/>
       <c r="D766" s="34"/>
       <c r="E766" s="34"/>
@@ -51285,8 +51558,8 @@
       </c>
     </row>
     <row r="767">
-      <c r="A767" s="74"/>
-      <c r="B767" s="75"/>
+      <c r="A767" s="81"/>
+      <c r="B767" s="82"/>
       <c r="C767" s="34"/>
       <c r="D767" s="34"/>
       <c r="E767" s="34"/>
@@ -51311,8 +51584,8 @@
       </c>
     </row>
     <row r="768">
-      <c r="A768" s="74"/>
-      <c r="B768" s="75"/>
+      <c r="A768" s="81"/>
+      <c r="B768" s="82"/>
       <c r="C768" s="34"/>
       <c r="D768" s="34"/>
       <c r="E768" s="34"/>
@@ -51337,8 +51610,8 @@
       </c>
     </row>
     <row r="769">
-      <c r="A769" s="74"/>
-      <c r="B769" s="75"/>
+      <c r="A769" s="81"/>
+      <c r="B769" s="82"/>
       <c r="C769" s="34"/>
       <c r="D769" s="34"/>
       <c r="E769" s="34"/>
@@ -51363,8 +51636,8 @@
       </c>
     </row>
     <row r="770">
-      <c r="A770" s="74"/>
-      <c r="B770" s="75"/>
+      <c r="A770" s="81"/>
+      <c r="B770" s="82"/>
       <c r="C770" s="34"/>
       <c r="D770" s="34"/>
       <c r="E770" s="34"/>
@@ -51389,8 +51662,8 @@
       </c>
     </row>
     <row r="771">
-      <c r="A771" s="74"/>
-      <c r="B771" s="75"/>
+      <c r="A771" s="81"/>
+      <c r="B771" s="82"/>
       <c r="C771" s="34"/>
       <c r="D771" s="34"/>
       <c r="E771" s="34"/>
@@ -51415,8 +51688,8 @@
       </c>
     </row>
     <row r="772">
-      <c r="A772" s="74"/>
-      <c r="B772" s="75"/>
+      <c r="A772" s="81"/>
+      <c r="B772" s="82"/>
       <c r="C772" s="34"/>
       <c r="D772" s="34"/>
       <c r="E772" s="34"/>
@@ -51441,8 +51714,8 @@
       </c>
     </row>
     <row r="773">
-      <c r="A773" s="74"/>
-      <c r="B773" s="75"/>
+      <c r="A773" s="81"/>
+      <c r="B773" s="82"/>
       <c r="C773" s="34"/>
       <c r="D773" s="34"/>
       <c r="E773" s="34"/>
@@ -51467,8 +51740,8 @@
       </c>
     </row>
     <row r="774">
-      <c r="A774" s="74"/>
-      <c r="B774" s="75"/>
+      <c r="A774" s="81"/>
+      <c r="B774" s="82"/>
       <c r="C774" s="34"/>
       <c r="D774" s="34"/>
       <c r="E774" s="34"/>
@@ -51493,8 +51766,8 @@
       </c>
     </row>
     <row r="775">
-      <c r="A775" s="74"/>
-      <c r="B775" s="75"/>
+      <c r="A775" s="81"/>
+      <c r="B775" s="82"/>
       <c r="C775" s="34"/>
       <c r="D775" s="34"/>
       <c r="E775" s="34"/>
@@ -51519,8 +51792,8 @@
       </c>
     </row>
     <row r="776">
-      <c r="A776" s="74"/>
-      <c r="B776" s="75"/>
+      <c r="A776" s="81"/>
+      <c r="B776" s="82"/>
       <c r="C776" s="34"/>
       <c r="D776" s="34"/>
       <c r="E776" s="34"/>
@@ -51545,8 +51818,8 @@
       </c>
     </row>
     <row r="777">
-      <c r="A777" s="74"/>
-      <c r="B777" s="75"/>
+      <c r="A777" s="81"/>
+      <c r="B777" s="82"/>
       <c r="C777" s="34"/>
       <c r="D777" s="34"/>
       <c r="E777" s="34"/>
@@ -51571,8 +51844,8 @@
       </c>
     </row>
     <row r="778">
-      <c r="A778" s="74"/>
-      <c r="B778" s="75"/>
+      <c r="A778" s="81"/>
+      <c r="B778" s="82"/>
       <c r="C778" s="34"/>
       <c r="D778" s="34"/>
       <c r="E778" s="34"/>
@@ -51597,8 +51870,8 @@
       </c>
     </row>
     <row r="779">
-      <c r="A779" s="74"/>
-      <c r="B779" s="75"/>
+      <c r="A779" s="81"/>
+      <c r="B779" s="82"/>
       <c r="C779" s="34"/>
       <c r="D779" s="34"/>
       <c r="E779" s="34"/>
@@ -51623,8 +51896,8 @@
       </c>
     </row>
     <row r="780">
-      <c r="A780" s="74"/>
-      <c r="B780" s="75"/>
+      <c r="A780" s="81"/>
+      <c r="B780" s="82"/>
       <c r="C780" s="34"/>
       <c r="D780" s="34"/>
       <c r="E780" s="34"/>
@@ -51649,8 +51922,8 @@
       </c>
     </row>
     <row r="781">
-      <c r="A781" s="74"/>
-      <c r="B781" s="75"/>
+      <c r="A781" s="81"/>
+      <c r="B781" s="82"/>
       <c r="C781" s="34"/>
       <c r="D781" s="34"/>
       <c r="E781" s="34"/>
@@ -51675,8 +51948,8 @@
       </c>
     </row>
     <row r="782">
-      <c r="A782" s="74"/>
-      <c r="B782" s="75"/>
+      <c r="A782" s="81"/>
+      <c r="B782" s="82"/>
       <c r="C782" s="34"/>
       <c r="D782" s="34"/>
       <c r="E782" s="34"/>
@@ -51701,8 +51974,8 @@
       </c>
     </row>
     <row r="783">
-      <c r="A783" s="74"/>
-      <c r="B783" s="75"/>
+      <c r="A783" s="81"/>
+      <c r="B783" s="82"/>
       <c r="C783" s="34"/>
       <c r="D783" s="34"/>
       <c r="E783" s="34"/>
@@ -51727,8 +52000,8 @@
       </c>
     </row>
     <row r="784">
-      <c r="A784" s="74"/>
-      <c r="B784" s="75"/>
+      <c r="A784" s="81"/>
+      <c r="B784" s="82"/>
       <c r="C784" s="34"/>
       <c r="D784" s="34"/>
       <c r="E784" s="34"/>
@@ -51753,8 +52026,8 @@
       </c>
     </row>
     <row r="785">
-      <c r="A785" s="74"/>
-      <c r="B785" s="75"/>
+      <c r="A785" s="81"/>
+      <c r="B785" s="82"/>
       <c r="C785" s="34"/>
       <c r="D785" s="34"/>
       <c r="E785" s="34"/>
@@ -51779,8 +52052,8 @@
       </c>
     </row>
     <row r="786">
-      <c r="A786" s="74"/>
-      <c r="B786" s="75"/>
+      <c r="A786" s="81"/>
+      <c r="B786" s="82"/>
       <c r="C786" s="34"/>
       <c r="D786" s="34"/>
       <c r="E786" s="34"/>
@@ -51805,8 +52078,8 @@
       </c>
     </row>
     <row r="787">
-      <c r="A787" s="74"/>
-      <c r="B787" s="75"/>
+      <c r="A787" s="81"/>
+      <c r="B787" s="82"/>
       <c r="C787" s="34"/>
       <c r="D787" s="34"/>
       <c r="E787" s="34"/>
@@ -51831,8 +52104,8 @@
       </c>
     </row>
     <row r="788">
-      <c r="A788" s="74"/>
-      <c r="B788" s="75"/>
+      <c r="A788" s="81"/>
+      <c r="B788" s="82"/>
       <c r="C788" s="34"/>
       <c r="D788" s="34"/>
       <c r="E788" s="34"/>
@@ -51857,8 +52130,8 @@
       </c>
     </row>
     <row r="789">
-      <c r="A789" s="74"/>
-      <c r="B789" s="75"/>
+      <c r="A789" s="81"/>
+      <c r="B789" s="82"/>
       <c r="C789" s="34"/>
       <c r="D789" s="34"/>
       <c r="E789" s="34"/>
@@ -51883,8 +52156,8 @@
       </c>
     </row>
     <row r="790">
-      <c r="A790" s="74"/>
-      <c r="B790" s="75"/>
+      <c r="A790" s="81"/>
+      <c r="B790" s="82"/>
       <c r="C790" s="34"/>
       <c r="D790" s="34"/>
       <c r="E790" s="34"/>
@@ -51909,8 +52182,8 @@
       </c>
     </row>
     <row r="791">
-      <c r="A791" s="74"/>
-      <c r="B791" s="75"/>
+      <c r="A791" s="81"/>
+      <c r="B791" s="82"/>
       <c r="C791" s="34"/>
       <c r="D791" s="34"/>
       <c r="E791" s="34"/>
@@ -51935,8 +52208,8 @@
       </c>
     </row>
     <row r="792">
-      <c r="A792" s="74"/>
-      <c r="B792" s="75"/>
+      <c r="A792" s="81"/>
+      <c r="B792" s="82"/>
       <c r="C792" s="34"/>
       <c r="D792" s="34"/>
       <c r="E792" s="34"/>
@@ -51961,8 +52234,8 @@
       </c>
     </row>
     <row r="793">
-      <c r="A793" s="74"/>
-      <c r="B793" s="75"/>
+      <c r="A793" s="81"/>
+      <c r="B793" s="82"/>
       <c r="C793" s="34"/>
       <c r="D793" s="34"/>
       <c r="E793" s="34"/>
@@ -51987,8 +52260,8 @@
       </c>
     </row>
     <row r="794">
-      <c r="A794" s="74"/>
-      <c r="B794" s="75"/>
+      <c r="A794" s="81"/>
+      <c r="B794" s="82"/>
       <c r="C794" s="34"/>
       <c r="D794" s="34"/>
       <c r="E794" s="34"/>
@@ -52013,8 +52286,8 @@
       </c>
     </row>
     <row r="795">
-      <c r="A795" s="74"/>
-      <c r="B795" s="75"/>
+      <c r="A795" s="81"/>
+      <c r="B795" s="82"/>
       <c r="C795" s="34"/>
       <c r="D795" s="34"/>
       <c r="E795" s="34"/>
@@ -52039,8 +52312,8 @@
       </c>
     </row>
     <row r="796">
-      <c r="A796" s="74"/>
-      <c r="B796" s="75"/>
+      <c r="A796" s="81"/>
+      <c r="B796" s="82"/>
       <c r="C796" s="34"/>
       <c r="D796" s="34"/>
       <c r="E796" s="34"/>
@@ -52065,8 +52338,8 @@
       </c>
     </row>
     <row r="797">
-      <c r="A797" s="74"/>
-      <c r="B797" s="75"/>
+      <c r="A797" s="81"/>
+      <c r="B797" s="82"/>
       <c r="C797" s="34"/>
       <c r="D797" s="34"/>
       <c r="E797" s="34"/>
@@ -52091,8 +52364,8 @@
       </c>
     </row>
     <row r="798">
-      <c r="A798" s="74"/>
-      <c r="B798" s="75"/>
+      <c r="A798" s="81"/>
+      <c r="B798" s="82"/>
       <c r="C798" s="34"/>
       <c r="D798" s="34"/>
       <c r="E798" s="34"/>
@@ -52117,8 +52390,8 @@
       </c>
     </row>
     <row r="799">
-      <c r="A799" s="74"/>
-      <c r="B799" s="75"/>
+      <c r="A799" s="81"/>
+      <c r="B799" s="82"/>
       <c r="C799" s="34"/>
       <c r="D799" s="34"/>
       <c r="E799" s="34"/>
@@ -52143,8 +52416,8 @@
       </c>
     </row>
     <row r="800">
-      <c r="A800" s="74"/>
-      <c r="B800" s="75"/>
+      <c r="A800" s="81"/>
+      <c r="B800" s="82"/>
       <c r="C800" s="34"/>
       <c r="D800" s="34"/>
       <c r="E800" s="34"/>
@@ -52169,8 +52442,8 @@
       </c>
     </row>
     <row r="801">
-      <c r="A801" s="74"/>
-      <c r="B801" s="75"/>
+      <c r="A801" s="81"/>
+      <c r="B801" s="82"/>
       <c r="C801" s="34"/>
       <c r="D801" s="34"/>
       <c r="E801" s="34"/>
@@ -52195,8 +52468,8 @@
       </c>
     </row>
     <row r="802">
-      <c r="A802" s="74"/>
-      <c r="B802" s="75"/>
+      <c r="A802" s="81"/>
+      <c r="B802" s="82"/>
       <c r="C802" s="34"/>
       <c r="D802" s="34"/>
       <c r="E802" s="34"/>
@@ -52221,8 +52494,8 @@
       </c>
     </row>
     <row r="803">
-      <c r="A803" s="74"/>
-      <c r="B803" s="75"/>
+      <c r="A803" s="81"/>
+      <c r="B803" s="82"/>
       <c r="C803" s="34"/>
       <c r="D803" s="34"/>
       <c r="E803" s="34"/>
@@ -52247,8 +52520,8 @@
       </c>
     </row>
     <row r="804">
-      <c r="A804" s="74"/>
-      <c r="B804" s="75"/>
+      <c r="A804" s="81"/>
+      <c r="B804" s="82"/>
       <c r="C804" s="34"/>
       <c r="D804" s="34"/>
       <c r="E804" s="34"/>
@@ -52273,8 +52546,8 @@
       </c>
     </row>
     <row r="805">
-      <c r="A805" s="74"/>
-      <c r="B805" s="75"/>
+      <c r="A805" s="81"/>
+      <c r="B805" s="82"/>
       <c r="C805" s="34"/>
       <c r="D805" s="34"/>
       <c r="E805" s="34"/>
@@ -52299,8 +52572,8 @@
       </c>
     </row>
     <row r="806">
-      <c r="A806" s="74"/>
-      <c r="B806" s="75"/>
+      <c r="A806" s="81"/>
+      <c r="B806" s="82"/>
       <c r="C806" s="34"/>
       <c r="D806" s="34"/>
       <c r="E806" s="34"/>
@@ -52325,8 +52598,8 @@
       </c>
     </row>
     <row r="807">
-      <c r="A807" s="74"/>
-      <c r="B807" s="75"/>
+      <c r="A807" s="81"/>
+      <c r="B807" s="82"/>
       <c r="C807" s="34"/>
       <c r="D807" s="34"/>
       <c r="E807" s="34"/>
@@ -52351,8 +52624,8 @@
       </c>
     </row>
     <row r="808">
-      <c r="A808" s="74"/>
-      <c r="B808" s="75"/>
+      <c r="A808" s="81"/>
+      <c r="B808" s="82"/>
       <c r="C808" s="34"/>
       <c r="D808" s="34"/>
       <c r="E808" s="34"/>
@@ -52377,8 +52650,8 @@
       </c>
     </row>
     <row r="809">
-      <c r="A809" s="74"/>
-      <c r="B809" s="75"/>
+      <c r="A809" s="81"/>
+      <c r="B809" s="82"/>
       <c r="C809" s="34"/>
       <c r="D809" s="34"/>
       <c r="E809" s="34"/>
@@ -52403,8 +52676,8 @@
       </c>
     </row>
     <row r="810">
-      <c r="A810" s="74"/>
-      <c r="B810" s="75"/>
+      <c r="A810" s="81"/>
+      <c r="B810" s="82"/>
       <c r="C810" s="34"/>
       <c r="D810" s="34"/>
       <c r="E810" s="34"/>
@@ -52429,8 +52702,8 @@
       </c>
     </row>
     <row r="811">
-      <c r="A811" s="74"/>
-      <c r="B811" s="75"/>
+      <c r="A811" s="81"/>
+      <c r="B811" s="82"/>
       <c r="C811" s="34"/>
       <c r="D811" s="34"/>
       <c r="E811" s="34"/>
@@ -52455,8 +52728,8 @@
       </c>
     </row>
     <row r="812">
-      <c r="A812" s="74"/>
-      <c r="B812" s="75"/>
+      <c r="A812" s="81"/>
+      <c r="B812" s="82"/>
       <c r="C812" s="34"/>
       <c r="D812" s="34"/>
       <c r="E812" s="34"/>
@@ -52481,8 +52754,8 @@
       </c>
     </row>
     <row r="813">
-      <c r="A813" s="74"/>
-      <c r="B813" s="75"/>
+      <c r="A813" s="81"/>
+      <c r="B813" s="82"/>
       <c r="C813" s="34"/>
       <c r="D813" s="34"/>
       <c r="E813" s="34"/>
@@ -52507,8 +52780,8 @@
       </c>
     </row>
     <row r="814">
-      <c r="A814" s="74"/>
-      <c r="B814" s="75"/>
+      <c r="A814" s="81"/>
+      <c r="B814" s="82"/>
       <c r="C814" s="34"/>
       <c r="D814" s="34"/>
       <c r="E814" s="34"/>
@@ -52533,8 +52806,8 @@
       </c>
     </row>
     <row r="815">
-      <c r="A815" s="74"/>
-      <c r="B815" s="75"/>
+      <c r="A815" s="81"/>
+      <c r="B815" s="82"/>
       <c r="C815" s="34"/>
       <c r="D815" s="34"/>
       <c r="E815" s="34"/>
@@ -52559,8 +52832,8 @@
       </c>
     </row>
     <row r="816">
-      <c r="A816" s="74"/>
-      <c r="B816" s="75"/>
+      <c r="A816" s="81"/>
+      <c r="B816" s="82"/>
       <c r="C816" s="34"/>
       <c r="D816" s="34"/>
       <c r="E816" s="34"/>
@@ -52585,8 +52858,8 @@
       </c>
     </row>
     <row r="817">
-      <c r="A817" s="74"/>
-      <c r="B817" s="75"/>
+      <c r="A817" s="81"/>
+      <c r="B817" s="82"/>
       <c r="C817" s="34"/>
       <c r="D817" s="34"/>
       <c r="E817" s="34"/>
@@ -52611,8 +52884,8 @@
       </c>
     </row>
     <row r="818">
-      <c r="A818" s="74"/>
-      <c r="B818" s="75"/>
+      <c r="A818" s="81"/>
+      <c r="B818" s="82"/>
       <c r="C818" s="34"/>
       <c r="D818" s="34"/>
       <c r="E818" s="34"/>
@@ -52637,8 +52910,8 @@
       </c>
     </row>
     <row r="819">
-      <c r="A819" s="74"/>
-      <c r="B819" s="75"/>
+      <c r="A819" s="81"/>
+      <c r="B819" s="82"/>
       <c r="C819" s="34"/>
       <c r="D819" s="34"/>
       <c r="E819" s="34"/>
@@ -52663,8 +52936,8 @@
       </c>
     </row>
     <row r="820">
-      <c r="A820" s="74"/>
-      <c r="B820" s="75"/>
+      <c r="A820" s="81"/>
+      <c r="B820" s="82"/>
       <c r="C820" s="34"/>
       <c r="D820" s="34"/>
       <c r="E820" s="34"/>
@@ -52689,8 +52962,8 @@
       </c>
     </row>
     <row r="821">
-      <c r="A821" s="74"/>
-      <c r="B821" s="75"/>
+      <c r="A821" s="81"/>
+      <c r="B821" s="82"/>
       <c r="C821" s="34"/>
       <c r="D821" s="34"/>
       <c r="E821" s="34"/>
@@ -52715,8 +52988,8 @@
       </c>
     </row>
     <row r="822">
-      <c r="A822" s="74"/>
-      <c r="B822" s="75"/>
+      <c r="A822" s="81"/>
+      <c r="B822" s="82"/>
       <c r="C822" s="34"/>
       <c r="D822" s="34"/>
       <c r="E822" s="34"/>
@@ -52741,8 +53014,8 @@
       </c>
     </row>
     <row r="823">
-      <c r="A823" s="74"/>
-      <c r="B823" s="75"/>
+      <c r="A823" s="81"/>
+      <c r="B823" s="82"/>
       <c r="C823" s="34"/>
       <c r="D823" s="34"/>
       <c r="E823" s="34"/>
@@ -52767,8 +53040,8 @@
       </c>
     </row>
     <row r="824">
-      <c r="A824" s="74"/>
-      <c r="B824" s="75"/>
+      <c r="A824" s="81"/>
+      <c r="B824" s="82"/>
       <c r="C824" s="34"/>
       <c r="D824" s="34"/>
       <c r="E824" s="34"/>
@@ -52793,8 +53066,8 @@
       </c>
     </row>
     <row r="825">
-      <c r="A825" s="74"/>
-      <c r="B825" s="75"/>
+      <c r="A825" s="81"/>
+      <c r="B825" s="82"/>
       <c r="C825" s="34"/>
       <c r="D825" s="34"/>
       <c r="E825" s="34"/>
@@ -52819,8 +53092,8 @@
       </c>
     </row>
     <row r="826">
-      <c r="A826" s="74"/>
-      <c r="B826" s="75"/>
+      <c r="A826" s="81"/>
+      <c r="B826" s="82"/>
       <c r="C826" s="34"/>
       <c r="D826" s="34"/>
       <c r="E826" s="34"/>
@@ -52845,8 +53118,8 @@
       </c>
     </row>
     <row r="827">
-      <c r="A827" s="74"/>
-      <c r="B827" s="75"/>
+      <c r="A827" s="81"/>
+      <c r="B827" s="82"/>
       <c r="C827" s="34"/>
       <c r="D827" s="34"/>
       <c r="E827" s="34"/>
@@ -52871,8 +53144,8 @@
       </c>
     </row>
     <row r="828">
-      <c r="A828" s="74"/>
-      <c r="B828" s="75"/>
+      <c r="A828" s="81"/>
+      <c r="B828" s="82"/>
       <c r="C828" s="34"/>
       <c r="D828" s="34"/>
       <c r="E828" s="34"/>
@@ -52897,8 +53170,8 @@
       </c>
     </row>
     <row r="829">
-      <c r="A829" s="74"/>
-      <c r="B829" s="75"/>
+      <c r="A829" s="81"/>
+      <c r="B829" s="82"/>
       <c r="C829" s="34"/>
       <c r="D829" s="34"/>
       <c r="E829" s="34"/>
@@ -52923,8 +53196,8 @@
       </c>
     </row>
     <row r="830">
-      <c r="A830" s="74"/>
-      <c r="B830" s="75"/>
+      <c r="A830" s="81"/>
+      <c r="B830" s="82"/>
       <c r="C830" s="34"/>
       <c r="D830" s="34"/>
       <c r="E830" s="34"/>
@@ -52949,8 +53222,8 @@
       </c>
     </row>
     <row r="831">
-      <c r="A831" s="74"/>
-      <c r="B831" s="75"/>
+      <c r="A831" s="81"/>
+      <c r="B831" s="82"/>
       <c r="C831" s="34"/>
       <c r="D831" s="34"/>
       <c r="E831" s="34"/>
@@ -52975,8 +53248,8 @@
       </c>
     </row>
     <row r="832">
-      <c r="A832" s="74"/>
-      <c r="B832" s="75"/>
+      <c r="A832" s="81"/>
+      <c r="B832" s="82"/>
       <c r="C832" s="34"/>
       <c r="D832" s="34"/>
       <c r="E832" s="34"/>
@@ -53001,8 +53274,8 @@
       </c>
     </row>
     <row r="833">
-      <c r="A833" s="74"/>
-      <c r="B833" s="75"/>
+      <c r="A833" s="81"/>
+      <c r="B833" s="82"/>
       <c r="C833" s="34"/>
       <c r="D833" s="34"/>
       <c r="E833" s="34"/>
@@ -53027,8 +53300,8 @@
       </c>
     </row>
     <row r="834">
-      <c r="A834" s="74"/>
-      <c r="B834" s="75"/>
+      <c r="A834" s="81"/>
+      <c r="B834" s="82"/>
       <c r="C834" s="34"/>
       <c r="D834" s="34"/>
       <c r="E834" s="34"/>
@@ -53053,8 +53326,8 @@
       </c>
     </row>
     <row r="835">
-      <c r="A835" s="74"/>
-      <c r="B835" s="75"/>
+      <c r="A835" s="81"/>
+      <c r="B835" s="82"/>
       <c r="C835" s="34"/>
       <c r="D835" s="34"/>
       <c r="E835" s="34"/>
@@ -53079,8 +53352,8 @@
       </c>
     </row>
     <row r="836">
-      <c r="A836" s="74"/>
-      <c r="B836" s="75"/>
+      <c r="A836" s="81"/>
+      <c r="B836" s="82"/>
       <c r="C836" s="34"/>
       <c r="D836" s="34"/>
       <c r="E836" s="34"/>
@@ -53105,8 +53378,8 @@
       </c>
     </row>
     <row r="837">
-      <c r="A837" s="74"/>
-      <c r="B837" s="75"/>
+      <c r="A837" s="81"/>
+      <c r="B837" s="82"/>
       <c r="C837" s="34"/>
       <c r="D837" s="34"/>
       <c r="E837" s="34"/>
@@ -53131,8 +53404,8 @@
       </c>
     </row>
     <row r="838">
-      <c r="A838" s="74"/>
-      <c r="B838" s="75"/>
+      <c r="A838" s="81"/>
+      <c r="B838" s="82"/>
       <c r="C838" s="34"/>
       <c r="D838" s="34"/>
       <c r="E838" s="34"/>
@@ -53157,8 +53430,8 @@
       </c>
     </row>
     <row r="839">
-      <c r="A839" s="74"/>
-      <c r="B839" s="75"/>
+      <c r="A839" s="81"/>
+      <c r="B839" s="82"/>
       <c r="C839" s="34"/>
       <c r="D839" s="34"/>
       <c r="E839" s="34"/>
@@ -53183,8 +53456,8 @@
       </c>
     </row>
     <row r="840">
-      <c r="A840" s="74"/>
-      <c r="B840" s="75"/>
+      <c r="A840" s="81"/>
+      <c r="B840" s="82"/>
       <c r="C840" s="34"/>
       <c r="D840" s="34"/>
       <c r="E840" s="34"/>
@@ -53209,8 +53482,8 @@
       </c>
     </row>
     <row r="841">
-      <c r="A841" s="74"/>
-      <c r="B841" s="75"/>
+      <c r="A841" s="81"/>
+      <c r="B841" s="82"/>
       <c r="C841" s="34"/>
       <c r="D841" s="34"/>
       <c r="E841" s="34"/>
@@ -53235,8 +53508,8 @@
       </c>
     </row>
     <row r="842">
-      <c r="A842" s="74"/>
-      <c r="B842" s="75"/>
+      <c r="A842" s="81"/>
+      <c r="B842" s="82"/>
       <c r="C842" s="34"/>
       <c r="D842" s="34"/>
       <c r="E842" s="34"/>
@@ -53261,8 +53534,8 @@
       </c>
     </row>
     <row r="843">
-      <c r="A843" s="74"/>
-      <c r="B843" s="75"/>
+      <c r="A843" s="81"/>
+      <c r="B843" s="82"/>
       <c r="C843" s="34"/>
       <c r="D843" s="34"/>
       <c r="E843" s="34"/>
@@ -53287,8 +53560,8 @@
       </c>
     </row>
     <row r="844">
-      <c r="A844" s="74"/>
-      <c r="B844" s="75"/>
+      <c r="A844" s="81"/>
+      <c r="B844" s="82"/>
       <c r="C844" s="34"/>
       <c r="D844" s="34"/>
       <c r="E844" s="34"/>
@@ -53313,8 +53586,8 @@
       </c>
     </row>
     <row r="845">
-      <c r="A845" s="74"/>
-      <c r="B845" s="75"/>
+      <c r="A845" s="81"/>
+      <c r="B845" s="82"/>
       <c r="C845" s="34"/>
       <c r="D845" s="34"/>
       <c r="E845" s="34"/>
@@ -53339,8 +53612,8 @@
       </c>
     </row>
     <row r="846">
-      <c r="A846" s="74"/>
-      <c r="B846" s="75"/>
+      <c r="A846" s="81"/>
+      <c r="B846" s="82"/>
       <c r="C846" s="34"/>
       <c r="D846" s="34"/>
       <c r="E846" s="34"/>
@@ -53365,8 +53638,8 @@
       </c>
     </row>
     <row r="847">
-      <c r="A847" s="74"/>
-      <c r="B847" s="75"/>
+      <c r="A847" s="81"/>
+      <c r="B847" s="82"/>
       <c r="C847" s="34"/>
       <c r="D847" s="34"/>
       <c r="E847" s="34"/>
@@ -53391,8 +53664,8 @@
       </c>
     </row>
     <row r="848">
-      <c r="A848" s="74"/>
-      <c r="B848" s="75"/>
+      <c r="A848" s="81"/>
+      <c r="B848" s="82"/>
       <c r="C848" s="34"/>
       <c r="D848" s="34"/>
       <c r="E848" s="34"/>
@@ -53417,8 +53690,8 @@
       </c>
     </row>
     <row r="849">
-      <c r="A849" s="74"/>
-      <c r="B849" s="75"/>
+      <c r="A849" s="81"/>
+      <c r="B849" s="82"/>
       <c r="C849" s="34"/>
       <c r="D849" s="34"/>
       <c r="E849" s="34"/>
@@ -53443,8 +53716,8 @@
       </c>
     </row>
     <row r="850">
-      <c r="A850" s="74"/>
-      <c r="B850" s="75"/>
+      <c r="A850" s="81"/>
+      <c r="B850" s="82"/>
       <c r="C850" s="34"/>
       <c r="D850" s="34"/>
       <c r="E850" s="34"/>
@@ -53469,8 +53742,8 @@
       </c>
     </row>
     <row r="851">
-      <c r="A851" s="74"/>
-      <c r="B851" s="75"/>
+      <c r="A851" s="81"/>
+      <c r="B851" s="82"/>
       <c r="C851" s="34"/>
       <c r="D851" s="34"/>
       <c r="E851" s="34"/>
@@ -53495,8 +53768,8 @@
       </c>
     </row>
     <row r="852">
-      <c r="A852" s="74"/>
-      <c r="B852" s="75"/>
+      <c r="A852" s="81"/>
+      <c r="B852" s="82"/>
       <c r="C852" s="34"/>
       <c r="D852" s="34"/>
       <c r="E852" s="34"/>
@@ -53521,8 +53794,8 @@
       </c>
     </row>
     <row r="853">
-      <c r="A853" s="74"/>
-      <c r="B853" s="75"/>
+      <c r="A853" s="81"/>
+      <c r="B853" s="82"/>
       <c r="C853" s="34"/>
       <c r="D853" s="34"/>
       <c r="E853" s="34"/>
@@ -53547,8 +53820,8 @@
       </c>
     </row>
     <row r="854">
-      <c r="A854" s="74"/>
-      <c r="B854" s="75"/>
+      <c r="A854" s="81"/>
+      <c r="B854" s="82"/>
       <c r="C854" s="34"/>
       <c r="D854" s="34"/>
       <c r="E854" s="34"/>
@@ -53573,8 +53846,8 @@
       </c>
     </row>
     <row r="855">
-      <c r="A855" s="74"/>
-      <c r="B855" s="75"/>
+      <c r="A855" s="81"/>
+      <c r="B855" s="82"/>
       <c r="C855" s="34"/>
       <c r="D855" s="34"/>
       <c r="E855" s="34"/>
@@ -53599,8 +53872,8 @@
       </c>
     </row>
     <row r="856">
-      <c r="A856" s="74"/>
-      <c r="B856" s="75"/>
+      <c r="A856" s="81"/>
+      <c r="B856" s="82"/>
       <c r="C856" s="34"/>
       <c r="D856" s="34"/>
       <c r="E856" s="34"/>
@@ -53625,8 +53898,8 @@
       </c>
     </row>
     <row r="857">
-      <c r="A857" s="74"/>
-      <c r="B857" s="75"/>
+      <c r="A857" s="81"/>
+      <c r="B857" s="82"/>
       <c r="C857" s="34"/>
       <c r="D857" s="34"/>
       <c r="E857" s="34"/>
@@ -53651,8 +53924,8 @@
       </c>
     </row>
     <row r="858">
-      <c r="A858" s="74"/>
-      <c r="B858" s="75"/>
+      <c r="A858" s="81"/>
+      <c r="B858" s="82"/>
       <c r="C858" s="34"/>
       <c r="D858" s="34"/>
       <c r="E858" s="34"/>
@@ -53677,8 +53950,8 @@
       </c>
     </row>
     <row r="859">
-      <c r="A859" s="74"/>
-      <c r="B859" s="75"/>
+      <c r="A859" s="81"/>
+      <c r="B859" s="82"/>
       <c r="C859" s="34"/>
       <c r="D859" s="34"/>
       <c r="E859" s="34"/>
@@ -53703,8 +53976,8 @@
       </c>
     </row>
     <row r="860">
-      <c r="A860" s="74"/>
-      <c r="B860" s="75"/>
+      <c r="A860" s="81"/>
+      <c r="B860" s="82"/>
       <c r="C860" s="34"/>
       <c r="D860" s="34"/>
       <c r="E860" s="34"/>
@@ -53729,8 +54002,8 @@
       </c>
     </row>
     <row r="861">
-      <c r="A861" s="74"/>
-      <c r="B861" s="75"/>
+      <c r="A861" s="81"/>
+      <c r="B861" s="82"/>
       <c r="C861" s="34"/>
       <c r="D861" s="34"/>
       <c r="E861" s="34"/>
@@ -53755,8 +54028,8 @@
       </c>
     </row>
     <row r="862">
-      <c r="A862" s="74"/>
-      <c r="B862" s="75"/>
+      <c r="A862" s="81"/>
+      <c r="B862" s="82"/>
       <c r="C862" s="34"/>
       <c r="D862" s="34"/>
       <c r="E862" s="34"/>
@@ -53781,8 +54054,8 @@
       </c>
     </row>
     <row r="863">
-      <c r="A863" s="74"/>
-      <c r="B863" s="75"/>
+      <c r="A863" s="81"/>
+      <c r="B863" s="82"/>
       <c r="C863" s="34"/>
       <c r="D863" s="34"/>
       <c r="E863" s="34"/>
@@ -53807,8 +54080,8 @@
       </c>
     </row>
     <row r="864">
-      <c r="A864" s="74"/>
-      <c r="B864" s="75"/>
+      <c r="A864" s="81"/>
+      <c r="B864" s="82"/>
       <c r="C864" s="34"/>
       <c r="D864" s="34"/>
       <c r="E864" s="34"/>
@@ -53833,8 +54106,8 @@
       </c>
     </row>
     <row r="865">
-      <c r="A865" s="74"/>
-      <c r="B865" s="75"/>
+      <c r="A865" s="81"/>
+      <c r="B865" s="82"/>
       <c r="C865" s="34"/>
       <c r="D865" s="34"/>
       <c r="E865" s="34"/>
@@ -53859,8 +54132,8 @@
       </c>
     </row>
     <row r="866">
-      <c r="A866" s="74"/>
-      <c r="B866" s="75"/>
+      <c r="A866" s="81"/>
+      <c r="B866" s="82"/>
       <c r="C866" s="34"/>
       <c r="D866" s="34"/>
       <c r="E866" s="34"/>
@@ -53885,8 +54158,8 @@
       </c>
     </row>
     <row r="867">
-      <c r="A867" s="74"/>
-      <c r="B867" s="75"/>
+      <c r="A867" s="81"/>
+      <c r="B867" s="82"/>
       <c r="C867" s="34"/>
       <c r="D867" s="34"/>
       <c r="E867" s="34"/>
@@ -53911,8 +54184,8 @@
       </c>
     </row>
     <row r="868">
-      <c r="A868" s="74"/>
-      <c r="B868" s="75"/>
+      <c r="A868" s="81"/>
+      <c r="B868" s="82"/>
       <c r="C868" s="34"/>
       <c r="D868" s="34"/>
       <c r="E868" s="34"/>
@@ -53937,8 +54210,8 @@
       </c>
     </row>
     <row r="869">
-      <c r="A869" s="74"/>
-      <c r="B869" s="75"/>
+      <c r="A869" s="81"/>
+      <c r="B869" s="82"/>
       <c r="C869" s="34"/>
       <c r="D869" s="34"/>
       <c r="E869" s="34"/>
@@ -53963,8 +54236,8 @@
       </c>
     </row>
     <row r="870">
-      <c r="A870" s="74"/>
-      <c r="B870" s="75"/>
+      <c r="A870" s="81"/>
+      <c r="B870" s="82"/>
       <c r="C870" s="34"/>
       <c r="D870" s="34"/>
       <c r="E870" s="34"/>
@@ -53989,8 +54262,8 @@
       </c>
     </row>
     <row r="871">
-      <c r="A871" s="74"/>
-      <c r="B871" s="75"/>
+      <c r="A871" s="81"/>
+      <c r="B871" s="82"/>
       <c r="C871" s="34"/>
       <c r="D871" s="34"/>
       <c r="E871" s="34"/>
@@ -54015,8 +54288,8 @@
       </c>
     </row>
     <row r="872">
-      <c r="A872" s="74"/>
-      <c r="B872" s="75"/>
+      <c r="A872" s="81"/>
+      <c r="B872" s="82"/>
       <c r="C872" s="34"/>
       <c r="D872" s="34"/>
       <c r="E872" s="34"/>
@@ -54041,8 +54314,8 @@
       </c>
     </row>
     <row r="873">
-      <c r="A873" s="74"/>
-      <c r="B873" s="75"/>
+      <c r="A873" s="81"/>
+      <c r="B873" s="82"/>
       <c r="C873" s="34"/>
       <c r="D873" s="34"/>
       <c r="E873" s="34"/>
@@ -54067,8 +54340,8 @@
       </c>
     </row>
     <row r="874">
-      <c r="A874" s="74"/>
-      <c r="B874" s="75"/>
+      <c r="A874" s="81"/>
+      <c r="B874" s="82"/>
       <c r="C874" s="34"/>
       <c r="D874" s="34"/>
       <c r="E874" s="34"/>
@@ -54093,8 +54366,8 @@
       </c>
     </row>
     <row r="875">
-      <c r="A875" s="74"/>
-      <c r="B875" s="75"/>
+      <c r="A875" s="81"/>
+      <c r="B875" s="82"/>
       <c r="C875" s="34"/>
       <c r="D875" s="34"/>
       <c r="E875" s="34"/>
@@ -54119,8 +54392,8 @@
       </c>
     </row>
     <row r="876">
-      <c r="A876" s="74"/>
-      <c r="B876" s="75"/>
+      <c r="A876" s="81"/>
+      <c r="B876" s="82"/>
       <c r="C876" s="34"/>
       <c r="D876" s="34"/>
       <c r="E876" s="34"/>
@@ -54145,8 +54418,8 @@
       </c>
     </row>
     <row r="877">
-      <c r="A877" s="74"/>
-      <c r="B877" s="75"/>
+      <c r="A877" s="81"/>
+      <c r="B877" s="82"/>
       <c r="C877" s="34"/>
       <c r="D877" s="34"/>
       <c r="E877" s="34"/>
@@ -54171,8 +54444,8 @@
       </c>
     </row>
     <row r="878">
-      <c r="A878" s="74"/>
-      <c r="B878" s="75"/>
+      <c r="A878" s="81"/>
+      <c r="B878" s="82"/>
       <c r="C878" s="34"/>
       <c r="D878" s="34"/>
       <c r="E878" s="34"/>
@@ -54197,8 +54470,8 @@
       </c>
     </row>
     <row r="879">
-      <c r="A879" s="74"/>
-      <c r="B879" s="75"/>
+      <c r="A879" s="81"/>
+      <c r="B879" s="82"/>
       <c r="C879" s="34"/>
       <c r="D879" s="34"/>
       <c r="E879" s="34"/>
@@ -54223,8 +54496,8 @@
       </c>
     </row>
     <row r="880">
-      <c r="A880" s="74"/>
-      <c r="B880" s="75"/>
+      <c r="A880" s="81"/>
+      <c r="B880" s="82"/>
       <c r="C880" s="34"/>
       <c r="D880" s="34"/>
       <c r="E880" s="34"/>
@@ -54249,8 +54522,8 @@
       </c>
     </row>
     <row r="881">
-      <c r="A881" s="74"/>
-      <c r="B881" s="75"/>
+      <c r="A881" s="81"/>
+      <c r="B881" s="82"/>
       <c r="C881" s="34"/>
       <c r="D881" s="34"/>
       <c r="E881" s="34"/>
@@ -54275,8 +54548,8 @@
       </c>
     </row>
     <row r="882">
-      <c r="A882" s="74"/>
-      <c r="B882" s="75"/>
+      <c r="A882" s="81"/>
+      <c r="B882" s="82"/>
       <c r="C882" s="34"/>
       <c r="D882" s="34"/>
       <c r="E882" s="34"/>
@@ -54301,8 +54574,8 @@
       </c>
     </row>
     <row r="883">
-      <c r="A883" s="74"/>
-      <c r="B883" s="75"/>
+      <c r="A883" s="81"/>
+      <c r="B883" s="82"/>
       <c r="C883" s="34"/>
       <c r="D883" s="34"/>
       <c r="E883" s="34"/>
@@ -54327,8 +54600,8 @@
       </c>
     </row>
     <row r="884">
-      <c r="A884" s="74"/>
-      <c r="B884" s="75"/>
+      <c r="A884" s="81"/>
+      <c r="B884" s="82"/>
       <c r="C884" s="34"/>
       <c r="D884" s="34"/>
       <c r="E884" s="34"/>
@@ -54353,8 +54626,8 @@
       </c>
     </row>
     <row r="885">
-      <c r="A885" s="74"/>
-      <c r="B885" s="75"/>
+      <c r="A885" s="81"/>
+      <c r="B885" s="82"/>
       <c r="C885" s="34"/>
       <c r="D885" s="34"/>
       <c r="E885" s="34"/>
@@ -54379,8 +54652,8 @@
       </c>
     </row>
     <row r="886">
-      <c r="A886" s="74"/>
-      <c r="B886" s="75"/>
+      <c r="A886" s="81"/>
+      <c r="B886" s="82"/>
       <c r="C886" s="34"/>
       <c r="D886" s="34"/>
       <c r="E886" s="34"/>
@@ -54405,8 +54678,8 @@
       </c>
     </row>
     <row r="887">
-      <c r="A887" s="74"/>
-      <c r="B887" s="75"/>
+      <c r="A887" s="81"/>
+      <c r="B887" s="82"/>
       <c r="C887" s="34"/>
       <c r="D887" s="34"/>
       <c r="E887" s="34"/>
@@ -54431,8 +54704,8 @@
       </c>
     </row>
     <row r="888">
-      <c r="A888" s="74"/>
-      <c r="B888" s="75"/>
+      <c r="A888" s="81"/>
+      <c r="B888" s="82"/>
       <c r="C888" s="34"/>
       <c r="D888" s="34"/>
       <c r="E888" s="34"/>
@@ -54457,8 +54730,8 @@
       </c>
     </row>
     <row r="889">
-      <c r="A889" s="74"/>
-      <c r="B889" s="75"/>
+      <c r="A889" s="81"/>
+      <c r="B889" s="82"/>
       <c r="C889" s="34"/>
       <c r="D889" s="34"/>
       <c r="E889" s="34"/>
@@ -54483,8 +54756,8 @@
       </c>
     </row>
     <row r="890">
-      <c r="A890" s="74"/>
-      <c r="B890" s="75"/>
+      <c r="A890" s="81"/>
+      <c r="B890" s="82"/>
       <c r="C890" s="34"/>
       <c r="D890" s="34"/>
       <c r="E890" s="34"/>
@@ -54509,8 +54782,8 @@
       </c>
     </row>
     <row r="891">
-      <c r="A891" s="74"/>
-      <c r="B891" s="75"/>
+      <c r="A891" s="81"/>
+      <c r="B891" s="82"/>
       <c r="C891" s="34"/>
       <c r="D891" s="34"/>
       <c r="E891" s="34"/>
@@ -54535,8 +54808,8 @@
       </c>
     </row>
     <row r="892">
-      <c r="A892" s="74"/>
-      <c r="B892" s="75"/>
+      <c r="A892" s="81"/>
+      <c r="B892" s="82"/>
       <c r="C892" s="34"/>
       <c r="D892" s="34"/>
       <c r="E892" s="34"/>
@@ -54561,8 +54834,8 @@
       </c>
     </row>
     <row r="893">
-      <c r="A893" s="74"/>
-      <c r="B893" s="75"/>
+      <c r="A893" s="81"/>
+      <c r="B893" s="82"/>
       <c r="C893" s="34"/>
       <c r="D893" s="34"/>
       <c r="E893" s="34"/>
@@ -54587,8 +54860,8 @@
       </c>
     </row>
     <row r="894">
-      <c r="A894" s="74"/>
-      <c r="B894" s="75"/>
+      <c r="A894" s="81"/>
+      <c r="B894" s="82"/>
       <c r="C894" s="34"/>
       <c r="D894" s="34"/>
       <c r="E894" s="34"/>
@@ -54613,8 +54886,8 @@
       </c>
     </row>
     <row r="895">
-      <c r="A895" s="74"/>
-      <c r="B895" s="75"/>
+      <c r="A895" s="81"/>
+      <c r="B895" s="82"/>
       <c r="C895" s="34"/>
       <c r="D895" s="34"/>
       <c r="E895" s="34"/>
@@ -54639,8 +54912,8 @@
       </c>
     </row>
     <row r="896">
-      <c r="A896" s="74"/>
-      <c r="B896" s="75"/>
+      <c r="A896" s="81"/>
+      <c r="B896" s="82"/>
       <c r="C896" s="34"/>
       <c r="D896" s="34"/>
       <c r="E896" s="34"/>
@@ -54665,8 +54938,8 @@
       </c>
     </row>
     <row r="897">
-      <c r="A897" s="74"/>
-      <c r="B897" s="75"/>
+      <c r="A897" s="81"/>
+      <c r="B897" s="82"/>
       <c r="C897" s="34"/>
       <c r="D897" s="34"/>
       <c r="E897" s="34"/>
@@ -54691,8 +54964,8 @@
       </c>
     </row>
     <row r="898">
-      <c r="A898" s="74"/>
-      <c r="B898" s="75"/>
+      <c r="A898" s="81"/>
+      <c r="B898" s="82"/>
       <c r="C898" s="34"/>
       <c r="D898" s="34"/>
       <c r="E898" s="34"/>
@@ -54717,8 +54990,8 @@
       </c>
     </row>
     <row r="899">
-      <c r="A899" s="74"/>
-      <c r="B899" s="75"/>
+      <c r="A899" s="81"/>
+      <c r="B899" s="82"/>
       <c r="C899" s="34"/>
       <c r="D899" s="34"/>
       <c r="E899" s="34"/>
@@ -54743,8 +55016,8 @@
       </c>
     </row>
     <row r="900">
-      <c r="A900" s="74"/>
-      <c r="B900" s="75"/>
+      <c r="A900" s="81"/>
+      <c r="B900" s="82"/>
       <c r="C900" s="34"/>
       <c r="D900" s="34"/>
       <c r="E900" s="34"/>
@@ -54769,8 +55042,8 @@
       </c>
     </row>
     <row r="901">
-      <c r="A901" s="74"/>
-      <c r="B901" s="75"/>
+      <c r="A901" s="81"/>
+      <c r="B901" s="82"/>
       <c r="C901" s="34"/>
       <c r="D901" s="34"/>
       <c r="E901" s="34"/>
@@ -54795,8 +55068,8 @@
       </c>
     </row>
     <row r="902">
-      <c r="A902" s="74"/>
-      <c r="B902" s="75"/>
+      <c r="A902" s="81"/>
+      <c r="B902" s="82"/>
       <c r="C902" s="34"/>
       <c r="D902" s="34"/>
       <c r="E902" s="34"/>
@@ -54821,8 +55094,8 @@
       </c>
     </row>
     <row r="903">
-      <c r="A903" s="74"/>
-      <c r="B903" s="75"/>
+      <c r="A903" s="81"/>
+      <c r="B903" s="82"/>
       <c r="C903" s="34"/>
       <c r="D903" s="34"/>
       <c r="E903" s="34"/>
@@ -54847,8 +55120,8 @@
       </c>
     </row>
     <row r="904">
-      <c r="A904" s="74"/>
-      <c r="B904" s="75"/>
+      <c r="A904" s="81"/>
+      <c r="B904" s="82"/>
       <c r="C904" s="34"/>
       <c r="D904" s="34"/>
       <c r="E904" s="34"/>
@@ -54873,8 +55146,8 @@
       </c>
     </row>
     <row r="905">
-      <c r="A905" s="74"/>
-      <c r="B905" s="75"/>
+      <c r="A905" s="81"/>
+      <c r="B905" s="82"/>
       <c r="C905" s="34"/>
       <c r="D905" s="34"/>
       <c r="E905" s="34"/>
@@ -54899,8 +55172,8 @@
       </c>
     </row>
     <row r="906">
-      <c r="A906" s="74"/>
-      <c r="B906" s="75"/>
+      <c r="A906" s="81"/>
+      <c r="B906" s="82"/>
       <c r="C906" s="34"/>
       <c r="D906" s="34"/>
       <c r="E906" s="34"/>
@@ -54925,8 +55198,8 @@
       </c>
     </row>
     <row r="907">
-      <c r="A907" s="74"/>
-      <c r="B907" s="75"/>
+      <c r="A907" s="81"/>
+      <c r="B907" s="82"/>
       <c r="C907" s="34"/>
       <c r="D907" s="34"/>
       <c r="E907" s="34"/>
@@ -54951,8 +55224,8 @@
       </c>
     </row>
     <row r="908">
-      <c r="A908" s="74"/>
-      <c r="B908" s="75"/>
+      <c r="A908" s="81"/>
+      <c r="B908" s="82"/>
       <c r="C908" s="34"/>
       <c r="D908" s="34"/>
       <c r="E908" s="34"/>
@@ -54977,8 +55250,8 @@
       </c>
     </row>
     <row r="909">
-      <c r="A909" s="74"/>
-      <c r="B909" s="75"/>
+      <c r="A909" s="81"/>
+      <c r="B909" s="82"/>
       <c r="C909" s="34"/>
       <c r="D909" s="34"/>
       <c r="E909" s="34"/>
@@ -55003,8 +55276,8 @@
       </c>
     </row>
     <row r="910">
-      <c r="A910" s="74"/>
-      <c r="B910" s="75"/>
+      <c r="A910" s="81"/>
+      <c r="B910" s="82"/>
       <c r="C910" s="34"/>
       <c r="D910" s="34"/>
       <c r="E910" s="34"/>
@@ -55029,8 +55302,8 @@
       </c>
     </row>
     <row r="911">
-      <c r="A911" s="74"/>
-      <c r="B911" s="75"/>
+      <c r="A911" s="81"/>
+      <c r="B911" s="82"/>
       <c r="C911" s="34"/>
       <c r="D911" s="34"/>
       <c r="E911" s="34"/>
@@ -55055,8 +55328,8 @@
       </c>
     </row>
     <row r="912">
-      <c r="A912" s="74"/>
-      <c r="B912" s="75"/>
+      <c r="A912" s="81"/>
+      <c r="B912" s="82"/>
       <c r="C912" s="34"/>
       <c r="D912" s="34"/>
       <c r="E912" s="34"/>
@@ -55081,8 +55354,8 @@
       </c>
     </row>
     <row r="913">
-      <c r="A913" s="74"/>
-      <c r="B913" s="75"/>
+      <c r="A913" s="81"/>
+      <c r="B913" s="82"/>
       <c r="C913" s="34"/>
       <c r="D913" s="34"/>
       <c r="E913" s="34"/>
@@ -55107,8 +55380,8 @@
       </c>
     </row>
     <row r="914">
-      <c r="A914" s="74"/>
-      <c r="B914" s="75"/>
+      <c r="A914" s="81"/>
+      <c r="B914" s="82"/>
       <c r="C914" s="34"/>
       <c r="D914" s="34"/>
       <c r="E914" s="34"/>
@@ -55133,8 +55406,8 @@
       </c>
     </row>
     <row r="915">
-      <c r="A915" s="74"/>
-      <c r="B915" s="75"/>
+      <c r="A915" s="81"/>
+      <c r="B915" s="82"/>
       <c r="C915" s="34"/>
       <c r="D915" s="34"/>
       <c r="E915" s="34"/>
@@ -55159,8 +55432,8 @@
       </c>
     </row>
     <row r="916">
-      <c r="A916" s="74"/>
-      <c r="B916" s="75"/>
+      <c r="A916" s="81"/>
+      <c r="B916" s="82"/>
       <c r="C916" s="34"/>
       <c r="D916" s="34"/>
       <c r="E916" s="34"/>
@@ -55185,8 +55458,8 @@
       </c>
     </row>
     <row r="917">
-      <c r="A917" s="74"/>
-      <c r="B917" s="75"/>
+      <c r="A917" s="81"/>
+      <c r="B917" s="82"/>
       <c r="C917" s="34"/>
       <c r="D917" s="34"/>
       <c r="E917" s="34"/>
@@ -55211,8 +55484,8 @@
       </c>
     </row>
     <row r="918">
-      <c r="A918" s="74"/>
-      <c r="B918" s="75"/>
+      <c r="A918" s="81"/>
+      <c r="B918" s="82"/>
       <c r="C918" s="34"/>
       <c r="D918" s="34"/>
       <c r="E918" s="34"/>
@@ -55237,8 +55510,8 @@
       </c>
     </row>
     <row r="919">
-      <c r="A919" s="74"/>
-      <c r="B919" s="75"/>
+      <c r="A919" s="81"/>
+      <c r="B919" s="82"/>
       <c r="C919" s="34"/>
       <c r="D919" s="34"/>
       <c r="E919" s="34"/>
@@ -55263,8 +55536,8 @@
       </c>
     </row>
     <row r="920">
-      <c r="A920" s="74"/>
-      <c r="B920" s="75"/>
+      <c r="A920" s="81"/>
+      <c r="B920" s="82"/>
       <c r="C920" s="34"/>
       <c r="D920" s="34"/>
       <c r="E920" s="34"/>
@@ -55289,8 +55562,8 @@
       </c>
     </row>
     <row r="921">
-      <c r="A921" s="74"/>
-      <c r="B921" s="75"/>
+      <c r="A921" s="81"/>
+      <c r="B921" s="82"/>
       <c r="C921" s="34"/>
       <c r="D921" s="34"/>
       <c r="E921" s="34"/>
@@ -55315,8 +55588,8 @@
       </c>
     </row>
     <row r="922">
-      <c r="A922" s="74"/>
-      <c r="B922" s="75"/>
+      <c r="A922" s="81"/>
+      <c r="B922" s="82"/>
       <c r="C922" s="34"/>
       <c r="D922" s="34"/>
       <c r="E922" s="34"/>
@@ -55341,8 +55614,8 @@
       </c>
     </row>
     <row r="923">
-      <c r="A923" s="74"/>
-      <c r="B923" s="75"/>
+      <c r="A923" s="81"/>
+      <c r="B923" s="82"/>
       <c r="C923" s="34"/>
       <c r="D923" s="34"/>
       <c r="E923" s="34"/>
@@ -55367,8 +55640,8 @@
       </c>
     </row>
     <row r="924">
-      <c r="A924" s="74"/>
-      <c r="B924" s="75"/>
+      <c r="A924" s="81"/>
+      <c r="B924" s="82"/>
       <c r="C924" s="34"/>
       <c r="D924" s="34"/>
       <c r="E924" s="34"/>
@@ -55393,8 +55666,8 @@
       </c>
     </row>
     <row r="925">
-      <c r="A925" s="74"/>
-      <c r="B925" s="75"/>
+      <c r="A925" s="81"/>
+      <c r="B925" s="82"/>
       <c r="C925" s="34"/>
       <c r="D925" s="34"/>
       <c r="E925" s="34"/>
@@ -55419,8 +55692,8 @@
       </c>
     </row>
     <row r="926">
-      <c r="A926" s="74"/>
-      <c r="B926" s="75"/>
+      <c r="A926" s="81"/>
+      <c r="B926" s="82"/>
       <c r="C926" s="34"/>
       <c r="D926" s="34"/>
       <c r="E926" s="34"/>
@@ -55445,8 +55718,8 @@
       </c>
     </row>
     <row r="927">
-      <c r="A927" s="74"/>
-      <c r="B927" s="75"/>
+      <c r="A927" s="81"/>
+      <c r="B927" s="82"/>
       <c r="C927" s="34"/>
       <c r="D927" s="34"/>
       <c r="E927" s="34"/>
@@ -55471,8 +55744,8 @@
       </c>
     </row>
     <row r="928">
-      <c r="A928" s="74"/>
-      <c r="B928" s="75"/>
+      <c r="A928" s="81"/>
+      <c r="B928" s="82"/>
       <c r="C928" s="34"/>
       <c r="D928" s="34"/>
       <c r="E928" s="34"/>
@@ -55497,8 +55770,8 @@
       </c>
     </row>
     <row r="929">
-      <c r="A929" s="74"/>
-      <c r="B929" s="75"/>
+      <c r="A929" s="81"/>
+      <c r="B929" s="82"/>
       <c r="C929" s="34"/>
       <c r="D929" s="34"/>
       <c r="E929" s="34"/>
@@ -55523,8 +55796,8 @@
       </c>
     </row>
     <row r="930">
-      <c r="A930" s="74"/>
-      <c r="B930" s="75"/>
+      <c r="A930" s="81"/>
+      <c r="B930" s="82"/>
       <c r="C930" s="34"/>
       <c r="D930" s="34"/>
       <c r="E930" s="34"/>
@@ -55549,8 +55822,8 @@
       </c>
     </row>
     <row r="931">
-      <c r="A931" s="74"/>
-      <c r="B931" s="75"/>
+      <c r="A931" s="81"/>
+      <c r="B931" s="82"/>
       <c r="C931" s="34"/>
       <c r="D931" s="34"/>
       <c r="E931" s="34"/>
@@ -55575,8 +55848,8 @@
       </c>
     </row>
     <row r="932">
-      <c r="A932" s="74"/>
-      <c r="B932" s="75"/>
+      <c r="A932" s="81"/>
+      <c r="B932" s="82"/>
       <c r="C932" s="34"/>
       <c r="D932" s="34"/>
       <c r="E932" s="34"/>
@@ -55601,8 +55874,8 @@
       </c>
     </row>
     <row r="933">
-      <c r="A933" s="74"/>
-      <c r="B933" s="75"/>
+      <c r="A933" s="81"/>
+      <c r="B933" s="82"/>
       <c r="C933" s="34"/>
       <c r="D933" s="34"/>
       <c r="E933" s="34"/>
@@ -55627,8 +55900,8 @@
       </c>
     </row>
     <row r="934">
-      <c r="A934" s="74"/>
-      <c r="B934" s="75"/>
+      <c r="A934" s="81"/>
+      <c r="B934" s="82"/>
       <c r="C934" s="34"/>
       <c r="D934" s="34"/>
       <c r="E934" s="34"/>
@@ -55653,8 +55926,8 @@
       </c>
     </row>
     <row r="935">
-      <c r="A935" s="74"/>
-      <c r="B935" s="75"/>
+      <c r="A935" s="81"/>
+      <c r="B935" s="82"/>
       <c r="C935" s="34"/>
       <c r="D935" s="34"/>
       <c r="E935" s="34"/>
@@ -55679,8 +55952,8 @@
       </c>
     </row>
     <row r="936">
-      <c r="A936" s="74"/>
-      <c r="B936" s="75"/>
+      <c r="A936" s="81"/>
+      <c r="B936" s="82"/>
       <c r="C936" s="34"/>
       <c r="D936" s="34"/>
       <c r="E936" s="34"/>
@@ -55705,8 +55978,8 @@
       </c>
     </row>
     <row r="937">
-      <c r="A937" s="74"/>
-      <c r="B937" s="75"/>
+      <c r="A937" s="81"/>
+      <c r="B937" s="82"/>
       <c r="C937" s="34"/>
       <c r="D937" s="34"/>
       <c r="E937" s="34"/>
@@ -55731,8 +56004,8 @@
       </c>
     </row>
     <row r="938">
-      <c r="A938" s="74"/>
-      <c r="B938" s="75"/>
+      <c r="A938" s="81"/>
+      <c r="B938" s="82"/>
       <c r="C938" s="34"/>
       <c r="D938" s="34"/>
       <c r="E938" s="34"/>
@@ -55757,8 +56030,8 @@
       </c>
     </row>
     <row r="939">
-      <c r="A939" s="74"/>
-      <c r="B939" s="75"/>
+      <c r="A939" s="81"/>
+      <c r="B939" s="82"/>
       <c r="C939" s="34"/>
       <c r="D939" s="34"/>
       <c r="E939" s="34"/>
@@ -55783,8 +56056,8 @@
       </c>
     </row>
     <row r="940">
-      <c r="A940" s="74"/>
-      <c r="B940" s="75"/>
+      <c r="A940" s="81"/>
+      <c r="B940" s="82"/>
       <c r="C940" s="34"/>
       <c r="D940" s="34"/>
       <c r="E940" s="34"/>
@@ -55809,8 +56082,8 @@
       </c>
     </row>
     <row r="941">
-      <c r="A941" s="74"/>
-      <c r="B941" s="75"/>
+      <c r="A941" s="81"/>
+      <c r="B941" s="82"/>
       <c r="C941" s="34"/>
       <c r="D941" s="34"/>
       <c r="E941" s="34"/>
@@ -55835,8 +56108,8 @@
       </c>
     </row>
     <row r="942">
-      <c r="A942" s="74"/>
-      <c r="B942" s="75"/>
+      <c r="A942" s="81"/>
+      <c r="B942" s="82"/>
       <c r="C942" s="34"/>
       <c r="D942" s="34"/>
       <c r="E942" s="34"/>
@@ -55861,8 +56134,8 @@
       </c>
     </row>
     <row r="943">
-      <c r="A943" s="74"/>
-      <c r="B943" s="75"/>
+      <c r="A943" s="81"/>
+      <c r="B943" s="82"/>
       <c r="C943" s="34"/>
       <c r="D943" s="34"/>
       <c r="E943" s="34"/>
@@ -55887,8 +56160,8 @@
       </c>
     </row>
     <row r="944">
-      <c r="A944" s="74"/>
-      <c r="B944" s="75"/>
+      <c r="A944" s="81"/>
+      <c r="B944" s="82"/>
       <c r="C944" s="34"/>
       <c r="D944" s="34"/>
       <c r="E944" s="34"/>
@@ -55913,8 +56186,8 @@
       </c>
     </row>
     <row r="945">
-      <c r="A945" s="74"/>
-      <c r="B945" s="75"/>
+      <c r="A945" s="81"/>
+      <c r="B945" s="82"/>
       <c r="C945" s="34"/>
       <c r="D945" s="34"/>
       <c r="E945" s="34"/>
@@ -55939,8 +56212,8 @@
       </c>
     </row>
     <row r="946">
-      <c r="A946" s="74"/>
-      <c r="B946" s="75"/>
+      <c r="A946" s="81"/>
+      <c r="B946" s="82"/>
       <c r="C946" s="34"/>
       <c r="D946" s="34"/>
       <c r="E946" s="34"/>
@@ -55965,8 +56238,8 @@
       </c>
     </row>
     <row r="947">
-      <c r="A947" s="74"/>
-      <c r="B947" s="75"/>
+      <c r="A947" s="81"/>
+      <c r="B947" s="82"/>
       <c r="C947" s="34"/>
       <c r="D947" s="34"/>
       <c r="E947" s="34"/>
@@ -55991,8 +56264,8 @@
       </c>
     </row>
     <row r="948">
-      <c r="A948" s="74"/>
-      <c r="B948" s="75"/>
+      <c r="A948" s="81"/>
+      <c r="B948" s="82"/>
       <c r="C948" s="34"/>
       <c r="D948" s="34"/>
       <c r="E948" s="34"/>
@@ -56017,8 +56290,8 @@
       </c>
     </row>
     <row r="949">
-      <c r="A949" s="74"/>
-      <c r="B949" s="75"/>
+      <c r="A949" s="81"/>
+      <c r="B949" s="82"/>
       <c r="C949" s="34"/>
       <c r="D949" s="34"/>
       <c r="E949" s="34"/>
@@ -56043,8 +56316,8 @@
       </c>
     </row>
     <row r="950">
-      <c r="A950" s="74"/>
-      <c r="B950" s="75"/>
+      <c r="A950" s="81"/>
+      <c r="B950" s="82"/>
       <c r="C950" s="34"/>
       <c r="D950" s="34"/>
       <c r="E950" s="34"/>
@@ -56069,8 +56342,8 @@
       </c>
     </row>
     <row r="951">
-      <c r="A951" s="74"/>
-      <c r="B951" s="75"/>
+      <c r="A951" s="81"/>
+      <c r="B951" s="82"/>
       <c r="C951" s="34"/>
       <c r="D951" s="34"/>
       <c r="E951" s="34"/>
@@ -56095,8 +56368,8 @@
       </c>
     </row>
     <row r="952">
-      <c r="A952" s="74"/>
-      <c r="B952" s="75"/>
+      <c r="A952" s="81"/>
+      <c r="B952" s="82"/>
       <c r="C952" s="34"/>
       <c r="D952" s="34"/>
       <c r="E952" s="34"/>
@@ -56121,8 +56394,8 @@
       </c>
     </row>
     <row r="953">
-      <c r="A953" s="74"/>
-      <c r="B953" s="75"/>
+      <c r="A953" s="81"/>
+      <c r="B953" s="82"/>
       <c r="C953" s="34"/>
       <c r="D953" s="34"/>
       <c r="E953" s="34"/>
@@ -56147,8 +56420,8 @@
       </c>
     </row>
     <row r="954">
-      <c r="A954" s="74"/>
-      <c r="B954" s="75"/>
+      <c r="A954" s="81"/>
+      <c r="B954" s="82"/>
       <c r="C954" s="34"/>
       <c r="D954" s="34"/>
       <c r="E954" s="34"/>
@@ -56173,8 +56446,8 @@
       </c>
     </row>
     <row r="955">
-      <c r="A955" s="74"/>
-      <c r="B955" s="75"/>
+      <c r="A955" s="81"/>
+      <c r="B955" s="82"/>
       <c r="C955" s="34"/>
       <c r="D955" s="34"/>
       <c r="E955" s="34"/>
@@ -56199,8 +56472,8 @@
       </c>
     </row>
     <row r="956">
-      <c r="A956" s="74"/>
-      <c r="B956" s="75"/>
+      <c r="A956" s="81"/>
+      <c r="B956" s="82"/>
       <c r="C956" s="34"/>
       <c r="D956" s="34"/>
       <c r="E956" s="34"/>
@@ -56225,8 +56498,8 @@
       </c>
     </row>
     <row r="957">
-      <c r="A957" s="74"/>
-      <c r="B957" s="75"/>
+      <c r="A957" s="81"/>
+      <c r="B957" s="82"/>
       <c r="C957" s="34"/>
       <c r="D957" s="34"/>
       <c r="E957" s="34"/>
@@ -56251,8 +56524,8 @@
       </c>
     </row>
     <row r="958">
-      <c r="A958" s="74"/>
-      <c r="B958" s="75"/>
+      <c r="A958" s="81"/>
+      <c r="B958" s="82"/>
       <c r="C958" s="34"/>
       <c r="D958" s="34"/>
       <c r="E958" s="34"/>
@@ -56277,8 +56550,8 @@
       </c>
     </row>
     <row r="959">
-      <c r="A959" s="74"/>
-      <c r="B959" s="75"/>
+      <c r="A959" s="81"/>
+      <c r="B959" s="82"/>
       <c r="C959" s="34"/>
       <c r="D959" s="34"/>
       <c r="E959" s="34"/>
@@ -56303,8 +56576,8 @@
       </c>
     </row>
     <row r="960">
-      <c r="A960" s="74"/>
-      <c r="B960" s="75"/>
+      <c r="A960" s="81"/>
+      <c r="B960" s="82"/>
       <c r="C960" s="34"/>
       <c r="D960" s="34"/>
       <c r="E960" s="34"/>
@@ -56329,8 +56602,8 @@
       </c>
     </row>
     <row r="961">
-      <c r="A961" s="74"/>
-      <c r="B961" s="75"/>
+      <c r="A961" s="81"/>
+      <c r="B961" s="82"/>
       <c r="C961" s="34"/>
       <c r="D961" s="34"/>
       <c r="E961" s="34"/>
@@ -56355,8 +56628,8 @@
       </c>
     </row>
     <row r="962">
-      <c r="A962" s="74"/>
-      <c r="B962" s="75"/>
+      <c r="A962" s="81"/>
+      <c r="B962" s="82"/>
       <c r="C962" s="34"/>
       <c r="D962" s="34"/>
       <c r="E962" s="34"/>
@@ -56381,8 +56654,8 @@
       </c>
     </row>
     <row r="963">
-      <c r="A963" s="74"/>
-      <c r="B963" s="75"/>
+      <c r="A963" s="81"/>
+      <c r="B963" s="82"/>
       <c r="C963" s="34"/>
       <c r="D963" s="34"/>
       <c r="E963" s="34"/>
@@ -56407,8 +56680,8 @@
       </c>
     </row>
     <row r="964">
-      <c r="A964" s="74"/>
-      <c r="B964" s="75"/>
+      <c r="A964" s="81"/>
+      <c r="B964" s="82"/>
       <c r="C964" s="34"/>
       <c r="D964" s="34"/>
       <c r="E964" s="34"/>
@@ -56433,8 +56706,8 @@
       </c>
     </row>
     <row r="965">
-      <c r="A965" s="74"/>
-      <c r="B965" s="75"/>
+      <c r="A965" s="81"/>
+      <c r="B965" s="82"/>
       <c r="C965" s="34"/>
       <c r="D965" s="34"/>
       <c r="E965" s="34"/>
@@ -56459,8 +56732,8 @@
       </c>
     </row>
     <row r="966">
-      <c r="A966" s="74"/>
-      <c r="B966" s="75"/>
+      <c r="A966" s="81"/>
+      <c r="B966" s="82"/>
       <c r="C966" s="34"/>
       <c r="D966" s="34"/>
       <c r="E966" s="34"/>
@@ -56485,8 +56758,8 @@
       </c>
     </row>
     <row r="967">
-      <c r="A967" s="74"/>
-      <c r="B967" s="75"/>
+      <c r="A967" s="81"/>
+      <c r="B967" s="82"/>
       <c r="C967" s="34"/>
       <c r="D967" s="34"/>
       <c r="E967" s="34"/>
@@ -56511,8 +56784,8 @@
       </c>
     </row>
     <row r="968">
-      <c r="A968" s="74"/>
-      <c r="B968" s="75"/>
+      <c r="A968" s="81"/>
+      <c r="B968" s="82"/>
       <c r="C968" s="34"/>
       <c r="D968" s="34"/>
       <c r="E968" s="34"/>
@@ -56537,8 +56810,8 @@
       </c>
     </row>
     <row r="969">
-      <c r="A969" s="74"/>
-      <c r="B969" s="75"/>
+      <c r="A969" s="81"/>
+      <c r="B969" s="82"/>
       <c r="C969" s="34"/>
       <c r="D969" s="34"/>
       <c r="E969" s="34"/>
@@ -56563,8 +56836,8 @@
       </c>
     </row>
     <row r="970">
-      <c r="A970" s="74"/>
-      <c r="B970" s="75"/>
+      <c r="A970" s="81"/>
+      <c r="B970" s="82"/>
       <c r="C970" s="34"/>
       <c r="D970" s="34"/>
       <c r="E970" s="34"/>
@@ -56589,8 +56862,8 @@
       </c>
     </row>
     <row r="971">
-      <c r="A971" s="74"/>
-      <c r="B971" s="75"/>
+      <c r="A971" s="81"/>
+      <c r="B971" s="82"/>
       <c r="C971" s="34"/>
       <c r="D971" s="34"/>
       <c r="E971" s="34"/>
@@ -56615,8 +56888,8 @@
       </c>
     </row>
     <row r="972">
-      <c r="A972" s="74"/>
-      <c r="B972" s="75"/>
+      <c r="A972" s="81"/>
+      <c r="B972" s="82"/>
       <c r="C972" s="34"/>
       <c r="D972" s="34"/>
       <c r="E972" s="34"/>
@@ -56641,8 +56914,8 @@
       </c>
     </row>
     <row r="973">
-      <c r="A973" s="74"/>
-      <c r="B973" s="75"/>
+      <c r="A973" s="81"/>
+      <c r="B973" s="82"/>
       <c r="C973" s="34"/>
       <c r="D973" s="34"/>
       <c r="E973" s="34"/>
@@ -56667,8 +56940,8 @@
       </c>
     </row>
     <row r="974">
-      <c r="A974" s="74"/>
-      <c r="B974" s="75"/>
+      <c r="A974" s="81"/>
+      <c r="B974" s="82"/>
       <c r="C974" s="34"/>
       <c r="D974" s="34"/>
       <c r="E974" s="34"/>
@@ -56693,8 +56966,8 @@
       </c>
     </row>
     <row r="975">
-      <c r="A975" s="74"/>
-      <c r="B975" s="75"/>
+      <c r="A975" s="81"/>
+      <c r="B975" s="82"/>
       <c r="C975" s="34"/>
       <c r="D975" s="34"/>
       <c r="E975" s="34"/>
@@ -56719,8 +56992,8 @@
       </c>
     </row>
     <row r="976">
-      <c r="A976" s="74"/>
-      <c r="B976" s="75"/>
+      <c r="A976" s="81"/>
+      <c r="B976" s="82"/>
       <c r="C976" s="34"/>
       <c r="D976" s="34"/>
       <c r="E976" s="34"/>
@@ -56745,8 +57018,8 @@
       </c>
     </row>
     <row r="977">
-      <c r="A977" s="74"/>
-      <c r="B977" s="75"/>
+      <c r="A977" s="81"/>
+      <c r="B977" s="82"/>
       <c r="C977" s="34"/>
       <c r="D977" s="34"/>
       <c r="E977" s="34"/>
@@ -56771,8 +57044,8 @@
       </c>
     </row>
     <row r="978">
-      <c r="A978" s="74"/>
-      <c r="B978" s="75"/>
+      <c r="A978" s="81"/>
+      <c r="B978" s="82"/>
       <c r="C978" s="34"/>
       <c r="D978" s="34"/>
       <c r="E978" s="34"/>
@@ -56797,8 +57070,8 @@
       </c>
     </row>
     <row r="979">
-      <c r="A979" s="74"/>
-      <c r="B979" s="75"/>
+      <c r="A979" s="81"/>
+      <c r="B979" s="82"/>
       <c r="C979" s="34"/>
       <c r="D979" s="34"/>
       <c r="E979" s="34"/>
@@ -56823,8 +57096,8 @@
       </c>
     </row>
     <row r="980">
-      <c r="A980" s="74"/>
-      <c r="B980" s="75"/>
+      <c r="A980" s="81"/>
+      <c r="B980" s="82"/>
       <c r="C980" s="34"/>
       <c r="D980" s="34"/>
       <c r="E980" s="34"/>
@@ -56849,8 +57122,8 @@
       </c>
     </row>
     <row r="981">
-      <c r="A981" s="74"/>
-      <c r="B981" s="75"/>
+      <c r="A981" s="81"/>
+      <c r="B981" s="82"/>
       <c r="C981" s="34"/>
       <c r="D981" s="34"/>
       <c r="E981" s="34"/>
@@ -56875,8 +57148,8 @@
       </c>
     </row>
     <row r="982">
-      <c r="A982" s="74"/>
-      <c r="B982" s="75"/>
+      <c r="A982" s="81"/>
+      <c r="B982" s="82"/>
       <c r="C982" s="34"/>
       <c r="D982" s="34"/>
       <c r="E982" s="34"/>
@@ -56901,8 +57174,8 @@
       </c>
     </row>
     <row r="983">
-      <c r="A983" s="74"/>
-      <c r="B983" s="75"/>
+      <c r="A983" s="81"/>
+      <c r="B983" s="82"/>
       <c r="C983" s="34"/>
       <c r="D983" s="34"/>
       <c r="E983" s="34"/>
@@ -56927,8 +57200,8 @@
       </c>
     </row>
     <row r="984">
-      <c r="A984" s="74"/>
-      <c r="B984" s="75"/>
+      <c r="A984" s="81"/>
+      <c r="B984" s="82"/>
       <c r="C984" s="34"/>
       <c r="D984" s="34"/>
       <c r="E984" s="34"/>
@@ -56953,8 +57226,8 @@
       </c>
     </row>
     <row r="985">
-      <c r="A985" s="74"/>
-      <c r="B985" s="75"/>
+      <c r="A985" s="81"/>
+      <c r="B985" s="82"/>
       <c r="C985" s="34"/>
       <c r="D985" s="34"/>
       <c r="E985" s="34"/>
@@ -56979,8 +57252,8 @@
       </c>
     </row>
     <row r="986">
-      <c r="A986" s="74"/>
-      <c r="B986" s="75"/>
+      <c r="A986" s="81"/>
+      <c r="B986" s="82"/>
       <c r="C986" s="34"/>
       <c r="D986" s="34"/>
       <c r="E986" s="34"/>
@@ -57005,8 +57278,8 @@
       </c>
     </row>
     <row r="987">
-      <c r="A987" s="74"/>
-      <c r="B987" s="75"/>
+      <c r="A987" s="81"/>
+      <c r="B987" s="82"/>
       <c r="C987" s="34"/>
       <c r="D987" s="34"/>
       <c r="E987" s="34"/>
@@ -57031,8 +57304,8 @@
       </c>
     </row>
     <row r="988">
-      <c r="A988" s="74"/>
-      <c r="B988" s="75"/>
+      <c r="A988" s="81"/>
+      <c r="B988" s="82"/>
       <c r="C988" s="34"/>
       <c r="D988" s="34"/>
       <c r="E988" s="34"/>
@@ -57057,8 +57330,8 @@
       </c>
     </row>
     <row r="989">
-      <c r="A989" s="74"/>
-      <c r="B989" s="75"/>
+      <c r="A989" s="81"/>
+      <c r="B989" s="82"/>
       <c r="C989" s="34"/>
       <c r="D989" s="34"/>
       <c r="E989" s="34"/>
@@ -57083,8 +57356,8 @@
       </c>
     </row>
     <row r="990">
-      <c r="A990" s="74"/>
-      <c r="B990" s="75"/>
+      <c r="A990" s="81"/>
+      <c r="B990" s="82"/>
       <c r="C990" s="34"/>
       <c r="D990" s="34"/>
       <c r="E990" s="34"/>
@@ -57109,8 +57382,8 @@
       </c>
     </row>
     <row r="991">
-      <c r="A991" s="74"/>
-      <c r="B991" s="75"/>
+      <c r="A991" s="81"/>
+      <c r="B991" s="82"/>
       <c r="C991" s="34"/>
       <c r="D991" s="34"/>
       <c r="E991" s="34"/>
@@ -57135,8 +57408,8 @@
       </c>
     </row>
     <row r="992">
-      <c r="A992" s="74"/>
-      <c r="B992" s="75"/>
+      <c r="A992" s="81"/>
+      <c r="B992" s="82"/>
       <c r="C992" s="34"/>
       <c r="D992" s="34"/>
       <c r="E992" s="34"/>
@@ -57161,8 +57434,8 @@
       </c>
     </row>
     <row r="993">
-      <c r="A993" s="74"/>
-      <c r="B993" s="75"/>
+      <c r="A993" s="81"/>
+      <c r="B993" s="82"/>
       <c r="C993" s="34"/>
       <c r="D993" s="34"/>
       <c r="E993" s="34"/>
@@ -57187,8 +57460,8 @@
       </c>
     </row>
     <row r="994">
-      <c r="A994" s="74"/>
-      <c r="B994" s="75"/>
+      <c r="A994" s="81"/>
+      <c r="B994" s="82"/>
       <c r="C994" s="34"/>
       <c r="D994" s="34"/>
       <c r="E994" s="34"/>
@@ -57213,8 +57486,8 @@
       </c>
     </row>
     <row r="995">
-      <c r="A995" s="74"/>
-      <c r="B995" s="75"/>
+      <c r="A995" s="81"/>
+      <c r="B995" s="82"/>
       <c r="C995" s="34"/>
       <c r="D995" s="34"/>
       <c r="E995" s="34"/>
@@ -57239,8 +57512,8 @@
       </c>
     </row>
     <row r="996">
-      <c r="A996" s="74"/>
-      <c r="B996" s="75"/>
+      <c r="A996" s="81"/>
+      <c r="B996" s="82"/>
       <c r="C996" s="34"/>
       <c r="D996" s="34"/>
       <c r="E996" s="34"/>
@@ -57265,8 +57538,8 @@
       </c>
     </row>
     <row r="997">
-      <c r="A997" s="74"/>
-      <c r="B997" s="75"/>
+      <c r="A997" s="81"/>
+      <c r="B997" s="82"/>
       <c r="C997" s="34"/>
       <c r="D997" s="34"/>
       <c r="E997" s="34"/>
@@ -57291,8 +57564,8 @@
       </c>
     </row>
     <row r="998">
-      <c r="A998" s="74"/>
-      <c r="B998" s="75"/>
+      <c r="A998" s="81"/>
+      <c r="B998" s="82"/>
       <c r="C998" s="34"/>
       <c r="D998" s="34"/>
       <c r="E998" s="34"/>
@@ -57317,8 +57590,8 @@
       </c>
     </row>
     <row r="999">
-      <c r="A999" s="74"/>
-      <c r="B999" s="75"/>
+      <c r="A999" s="81"/>
+      <c r="B999" s="82"/>
       <c r="C999" s="34"/>
       <c r="D999" s="34"/>
       <c r="E999" s="34"/>
@@ -57343,8 +57616,8 @@
       </c>
     </row>
     <row r="1000">
-      <c r="A1000" s="74"/>
-      <c r="B1000" s="75"/>
+      <c r="A1000" s="81"/>
+      <c r="B1000" s="82"/>
       <c r="C1000" s="34"/>
       <c r="D1000" s="34"/>
       <c r="E1000" s="34"/>
@@ -57369,8 +57642,8 @@
       </c>
     </row>
     <row r="1001">
-      <c r="A1001" s="74"/>
-      <c r="B1001" s="75"/>
+      <c r="A1001" s="81"/>
+      <c r="B1001" s="82"/>
       <c r="C1001" s="34"/>
       <c r="D1001" s="34"/>
       <c r="E1001" s="34"/>
@@ -58019,15 +58292,21 @@
     <hyperlink r:id="rId242" ref="S679"/>
     <hyperlink r:id="rId243" ref="S680"/>
     <hyperlink r:id="rId244" ref="S681"/>
+    <hyperlink r:id="rId245" ref="S682"/>
+    <hyperlink r:id="rId246" ref="S683"/>
+    <hyperlink r:id="rId247" ref="S684"/>
+    <hyperlink r:id="rId248" ref="S685"/>
+    <hyperlink r:id="rId249" ref="S686"/>
+    <hyperlink r:id="rId250" ref="S687"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId245"/>
-  <legacyDrawing r:id="rId246"/>
+  <drawing r:id="rId251"/>
+  <legacyDrawing r:id="rId252"/>
   <tableParts count="2">
-    <tablePart r:id="rId249"/>
-    <tablePart r:id="rId250"/>
+    <tablePart r:id="rId255"/>
+    <tablePart r:id="rId256"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201204
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -571,7 +571,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7796" uniqueCount="2460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7808" uniqueCount="2465">
   <si>
     <t>案例</t>
   </si>
@@ -8895,6 +8895,22 @@
   <si>
     <t>因受臺灣公司邀請來臺從事商務活動，持有登機前3日內核酸檢驗陰性報告，11月19日自法國經土耳其轉機，於11月20日入境臺灣後，持前往防疫旅館居家檢疫。
 個案11月27日曾出現喉嚨痛症狀，因症狀持續，11月30日由衛生單位安排就醫採檢</t>
+  </si>
+  <si>
+    <t>#687</t>
+  </si>
+  <si>
+    <t>-11/29 美國</t>
+  </si>
+  <si>
+    <t>11/29 採檢
+12/3 確診</t>
+  </si>
+  <si>
+    <t>國工作，11月29日返臺探親，入境後至住處居家檢疫，同日於住處出現喉嚨不適情形並主動通報，由衛生單位安排就醫採檢及收治住院</t>
+  </si>
+  <si>
+    <t>女自美返臺探親，居家檢疫期間發病確診COVID-19</t>
   </si>
 </sst>
 </file>
@@ -9039,7 +9055,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="82">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -9263,9 +9279,6 @@
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -9274,13 +9287,13 @@
     <xf borderId="0" fillId="0" fontId="19" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="20" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="20" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -49170,7 +49183,7 @@
       </c>
     </row>
     <row r="682">
-      <c r="A682" s="74" t="s">
+      <c r="A682" s="16" t="s">
         <v>2439</v>
       </c>
       <c r="B682" s="6">
@@ -49179,7 +49192,7 @@
       <c r="C682" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D682" s="75" t="s">
+      <c r="D682" s="7" t="s">
         <v>59</v>
       </c>
       <c r="E682" s="7" t="s">
@@ -49189,29 +49202,29 @@
       <c r="G682" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H682" s="76" t="s">
+      <c r="H682" s="8" t="s">
         <v>2280</v>
       </c>
-      <c r="I682" s="77">
+      <c r="I682" s="9">
         <v>44152.0</v>
       </c>
-      <c r="J682" s="78" t="s">
+      <c r="J682" s="12" t="s">
         <v>1442</v>
       </c>
-      <c r="K682" s="79" t="s">
+      <c r="K682" s="13" t="s">
         <v>2440</v>
       </c>
-      <c r="L682" s="78" t="s">
+      <c r="L682" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M682" s="79" t="s">
+      <c r="M682" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N682" s="25"/>
-      <c r="O682" s="76" t="s">
+      <c r="O682" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P682" s="76" t="s">
+      <c r="P682" s="8" t="s">
         <v>2441</v>
       </c>
       <c r="Q682" s="19"/>
@@ -49226,7 +49239,7 @@
       </c>
     </row>
     <row r="683">
-      <c r="A683" s="74" t="s">
+      <c r="A683" s="16" t="s">
         <v>2443</v>
       </c>
       <c r="B683" s="6">
@@ -49235,7 +49248,7 @@
       <c r="C683" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D683" s="75" t="s">
+      <c r="D683" s="7" t="s">
         <v>116</v>
       </c>
       <c r="E683" s="7" t="s">
@@ -49245,29 +49258,29 @@
       <c r="G683" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H683" s="76" t="s">
+      <c r="H683" s="8" t="s">
         <v>2280</v>
       </c>
-      <c r="I683" s="77">
+      <c r="I683" s="9">
         <v>44152.0</v>
       </c>
-      <c r="J683" s="78" t="s">
+      <c r="J683" s="12" t="s">
         <v>1442</v>
       </c>
-      <c r="K683" s="79" t="s">
+      <c r="K683" s="13" t="s">
         <v>2440</v>
       </c>
-      <c r="L683" s="78" t="s">
+      <c r="L683" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M683" s="79" t="s">
+      <c r="M683" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N683" s="25"/>
-      <c r="O683" s="76" t="s">
+      <c r="O683" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P683" s="76" t="s">
+      <c r="P683" s="8" t="s">
         <v>2441</v>
       </c>
       <c r="Q683" s="19"/>
@@ -49282,7 +49295,7 @@
       </c>
     </row>
     <row r="684">
-      <c r="A684" s="74" t="s">
+      <c r="A684" s="16" t="s">
         <v>2444</v>
       </c>
       <c r="B684" s="6">
@@ -49291,7 +49304,7 @@
       <c r="C684" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D684" s="75" t="s">
+      <c r="D684" s="7" t="s">
         <v>76</v>
       </c>
       <c r="E684" s="7" t="s">
@@ -49301,29 +49314,29 @@
       <c r="G684" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H684" s="76" t="s">
+      <c r="H684" s="8" t="s">
         <v>2375</v>
       </c>
-      <c r="I684" s="77">
+      <c r="I684" s="9">
         <v>44149.0</v>
       </c>
-      <c r="J684" s="78" t="s">
+      <c r="J684" s="12" t="s">
         <v>1442</v>
       </c>
-      <c r="K684" s="79" t="s">
+      <c r="K684" s="13" t="s">
         <v>2445</v>
       </c>
       <c r="L684" s="12" t="s">
         <v>1674</v>
       </c>
-      <c r="M684" s="79" t="s">
+      <c r="M684" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N684" s="25"/>
-      <c r="O684" s="76" t="s">
+      <c r="O684" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P684" s="76" t="s">
+      <c r="P684" s="8" t="s">
         <v>2446</v>
       </c>
       <c r="Q684" s="19"/>
@@ -49338,7 +49351,7 @@
       </c>
     </row>
     <row r="685">
-      <c r="A685" s="74" t="s">
+      <c r="A685" s="16" t="s">
         <v>2447</v>
       </c>
       <c r="B685" s="6">
@@ -49347,7 +49360,7 @@
       <c r="C685" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D685" s="75" t="s">
+      <c r="D685" s="7" t="s">
         <v>116</v>
       </c>
       <c r="E685" s="7" t="s">
@@ -49357,29 +49370,29 @@
       <c r="G685" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H685" s="76" t="s">
+      <c r="H685" s="8" t="s">
         <v>2448</v>
       </c>
-      <c r="I685" s="77">
+      <c r="I685" s="9">
         <v>44157.0</v>
       </c>
-      <c r="J685" s="80">
+      <c r="J685" s="10">
         <v>44157.0</v>
       </c>
-      <c r="K685" s="79" t="s">
+      <c r="K685" s="13" t="s">
         <v>2449</v>
       </c>
-      <c r="L685" s="78" t="s">
+      <c r="L685" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M685" s="79" t="s">
+      <c r="M685" s="13" t="s">
         <v>1596</v>
       </c>
       <c r="N685" s="25"/>
-      <c r="O685" s="76" t="s">
+      <c r="O685" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P685" s="76" t="s">
+      <c r="P685" s="8" t="s">
         <v>2450</v>
       </c>
       <c r="Q685" s="19"/>
@@ -49394,7 +49407,7 @@
       </c>
     </row>
     <row r="686">
-      <c r="A686" s="74" t="s">
+      <c r="A686" s="16" t="s">
         <v>2451</v>
       </c>
       <c r="B686" s="6">
@@ -49403,7 +49416,7 @@
       <c r="C686" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D686" s="75" t="s">
+      <c r="D686" s="7" t="s">
         <v>59</v>
       </c>
       <c r="E686" s="7" t="s">
@@ -49413,27 +49426,27 @@
       <c r="G686" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H686" s="76" t="s">
+      <c r="H686" s="8" t="s">
         <v>2453</v>
       </c>
-      <c r="I686" s="77">
+      <c r="I686" s="9">
         <v>44164.0</v>
       </c>
       <c r="J686" s="10"/>
-      <c r="K686" s="79" t="s">
+      <c r="K686" s="13" t="s">
         <v>2454</v>
       </c>
-      <c r="L686" s="78" t="s">
+      <c r="L686" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M686" s="79" t="s">
+      <c r="M686" s="13" t="s">
         <v>2455</v>
       </c>
       <c r="N686" s="25"/>
-      <c r="O686" s="76" t="s">
+      <c r="O686" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P686" s="76" t="s">
+      <c r="P686" s="8" t="s">
         <v>2456</v>
       </c>
       <c r="Q686" s="19"/>
@@ -49448,7 +49461,7 @@
       </c>
     </row>
     <row r="687">
-      <c r="A687" s="74" t="s">
+      <c r="A687" s="16" t="s">
         <v>2457</v>
       </c>
       <c r="B687" s="6">
@@ -49457,7 +49470,7 @@
       <c r="C687" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D687" s="75" t="s">
+      <c r="D687" s="7" t="s">
         <v>22</v>
       </c>
       <c r="E687" s="7" t="s">
@@ -49467,29 +49480,29 @@
       <c r="G687" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H687" s="76" t="s">
+      <c r="H687" s="8" t="s">
         <v>2458</v>
       </c>
-      <c r="I687" s="77">
+      <c r="I687" s="9">
         <v>44155.0</v>
       </c>
-      <c r="J687" s="80">
+      <c r="J687" s="10">
         <v>44162.0</v>
       </c>
-      <c r="K687" s="79" t="s">
+      <c r="K687" s="13" t="s">
         <v>2440</v>
       </c>
-      <c r="L687" s="78" t="s">
+      <c r="L687" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M687" s="79" t="s">
+      <c r="M687" s="13" t="s">
         <v>518</v>
       </c>
       <c r="N687" s="25"/>
-      <c r="O687" s="76" t="s">
+      <c r="O687" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P687" s="76" t="s">
+      <c r="P687" s="8" t="s">
         <v>2459</v>
       </c>
       <c r="Q687" s="19"/>
@@ -49504,34 +49517,64 @@
       </c>
     </row>
     <row r="688">
-      <c r="A688" s="81"/>
-      <c r="B688" s="82"/>
-      <c r="C688" s="34"/>
-      <c r="D688" s="34"/>
-      <c r="E688" s="34"/>
+      <c r="A688" s="16" t="s">
+        <v>2460</v>
+      </c>
+      <c r="B688" s="6">
+        <v>44168.0</v>
+      </c>
+      <c r="C688" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D688" s="74" t="s">
+        <v>116</v>
+      </c>
+      <c r="E688" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F688" s="34"/>
-      <c r="G688" s="34"/>
-      <c r="H688" s="21"/>
-      <c r="I688" s="19"/>
-      <c r="J688" s="10"/>
-      <c r="K688" s="22"/>
-      <c r="L688" s="23"/>
-      <c r="M688" s="22"/>
+      <c r="G688" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H688" s="75" t="s">
+        <v>2461</v>
+      </c>
+      <c r="I688" s="76">
+        <v>44164.0</v>
+      </c>
+      <c r="J688" s="77">
+        <v>44164.0</v>
+      </c>
+      <c r="K688" s="78" t="s">
+        <v>2462</v>
+      </c>
+      <c r="L688" s="79" t="s">
+        <v>426</v>
+      </c>
+      <c r="M688" s="78" t="s">
+        <v>149</v>
+      </c>
       <c r="N688" s="25"/>
-      <c r="O688" s="21"/>
-      <c r="P688" s="21"/>
+      <c r="O688" s="75" t="s">
+        <v>85</v>
+      </c>
+      <c r="P688" s="75" t="s">
+        <v>2463</v>
+      </c>
       <c r="Q688" s="19"/>
       <c r="R688" s="19"/>
-      <c r="S688" s="20"/>
+      <c r="S688" s="61" t="s">
+        <v>2464</v>
+      </c>
       <c r="T688" s="20"/>
       <c r="U688" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#687</v>
       </c>
     </row>
     <row r="689">
-      <c r="A689" s="81"/>
-      <c r="B689" s="82"/>
+      <c r="A689" s="80"/>
+      <c r="B689" s="81"/>
       <c r="C689" s="34"/>
       <c r="D689" s="34"/>
       <c r="E689" s="34"/>
@@ -49556,8 +49599,8 @@
       </c>
     </row>
     <row r="690">
-      <c r="A690" s="81"/>
-      <c r="B690" s="82"/>
+      <c r="A690" s="80"/>
+      <c r="B690" s="81"/>
       <c r="C690" s="34"/>
       <c r="D690" s="34"/>
       <c r="E690" s="34"/>
@@ -49582,8 +49625,8 @@
       </c>
     </row>
     <row r="691">
-      <c r="A691" s="81"/>
-      <c r="B691" s="82"/>
+      <c r="A691" s="80"/>
+      <c r="B691" s="81"/>
       <c r="C691" s="34"/>
       <c r="D691" s="34"/>
       <c r="E691" s="34"/>
@@ -49608,8 +49651,8 @@
       </c>
     </row>
     <row r="692">
-      <c r="A692" s="81"/>
-      <c r="B692" s="82"/>
+      <c r="A692" s="80"/>
+      <c r="B692" s="81"/>
       <c r="C692" s="34"/>
       <c r="D692" s="34"/>
       <c r="E692" s="34"/>
@@ -49634,8 +49677,8 @@
       </c>
     </row>
     <row r="693">
-      <c r="A693" s="81"/>
-      <c r="B693" s="82"/>
+      <c r="A693" s="80"/>
+      <c r="B693" s="81"/>
       <c r="C693" s="34"/>
       <c r="D693" s="34"/>
       <c r="E693" s="34"/>
@@ -49660,8 +49703,8 @@
       </c>
     </row>
     <row r="694">
-      <c r="A694" s="81"/>
-      <c r="B694" s="82"/>
+      <c r="A694" s="80"/>
+      <c r="B694" s="81"/>
       <c r="C694" s="34"/>
       <c r="D694" s="34"/>
       <c r="E694" s="34"/>
@@ -49686,8 +49729,8 @@
       </c>
     </row>
     <row r="695">
-      <c r="A695" s="81"/>
-      <c r="B695" s="82"/>
+      <c r="A695" s="80"/>
+      <c r="B695" s="81"/>
       <c r="C695" s="34"/>
       <c r="D695" s="34"/>
       <c r="E695" s="34"/>
@@ -49712,8 +49755,8 @@
       </c>
     </row>
     <row r="696">
-      <c r="A696" s="81"/>
-      <c r="B696" s="82"/>
+      <c r="A696" s="80"/>
+      <c r="B696" s="81"/>
       <c r="C696" s="34"/>
       <c r="D696" s="34"/>
       <c r="E696" s="34"/>
@@ -49738,8 +49781,8 @@
       </c>
     </row>
     <row r="697">
-      <c r="A697" s="81"/>
-      <c r="B697" s="82"/>
+      <c r="A697" s="80"/>
+      <c r="B697" s="81"/>
       <c r="C697" s="34"/>
       <c r="D697" s="34"/>
       <c r="E697" s="34"/>
@@ -49764,8 +49807,8 @@
       </c>
     </row>
     <row r="698">
-      <c r="A698" s="81"/>
-      <c r="B698" s="82"/>
+      <c r="A698" s="80"/>
+      <c r="B698" s="81"/>
       <c r="C698" s="34"/>
       <c r="D698" s="34"/>
       <c r="E698" s="34"/>
@@ -49790,8 +49833,8 @@
       </c>
     </row>
     <row r="699">
-      <c r="A699" s="81"/>
-      <c r="B699" s="82"/>
+      <c r="A699" s="80"/>
+      <c r="B699" s="81"/>
       <c r="C699" s="34"/>
       <c r="D699" s="34"/>
       <c r="E699" s="34"/>
@@ -49816,8 +49859,8 @@
       </c>
     </row>
     <row r="700">
-      <c r="A700" s="81"/>
-      <c r="B700" s="82"/>
+      <c r="A700" s="80"/>
+      <c r="B700" s="81"/>
       <c r="C700" s="34"/>
       <c r="D700" s="34"/>
       <c r="E700" s="34"/>
@@ -49842,8 +49885,8 @@
       </c>
     </row>
     <row r="701">
-      <c r="A701" s="81"/>
-      <c r="B701" s="82"/>
+      <c r="A701" s="80"/>
+      <c r="B701" s="81"/>
       <c r="C701" s="34"/>
       <c r="D701" s="34"/>
       <c r="E701" s="34"/>
@@ -49868,8 +49911,8 @@
       </c>
     </row>
     <row r="702">
-      <c r="A702" s="81"/>
-      <c r="B702" s="82"/>
+      <c r="A702" s="80"/>
+      <c r="B702" s="81"/>
       <c r="C702" s="34"/>
       <c r="D702" s="34"/>
       <c r="E702" s="34"/>
@@ -49894,8 +49937,8 @@
       </c>
     </row>
     <row r="703">
-      <c r="A703" s="81"/>
-      <c r="B703" s="82"/>
+      <c r="A703" s="80"/>
+      <c r="B703" s="81"/>
       <c r="C703" s="34"/>
       <c r="D703" s="34"/>
       <c r="E703" s="34"/>
@@ -49920,8 +49963,8 @@
       </c>
     </row>
     <row r="704">
-      <c r="A704" s="81"/>
-      <c r="B704" s="82"/>
+      <c r="A704" s="80"/>
+      <c r="B704" s="81"/>
       <c r="C704" s="34"/>
       <c r="D704" s="34"/>
       <c r="E704" s="34"/>
@@ -49946,8 +49989,8 @@
       </c>
     </row>
     <row r="705">
-      <c r="A705" s="81"/>
-      <c r="B705" s="82"/>
+      <c r="A705" s="80"/>
+      <c r="B705" s="81"/>
       <c r="C705" s="34"/>
       <c r="D705" s="34"/>
       <c r="E705" s="34"/>
@@ -49972,8 +50015,8 @@
       </c>
     </row>
     <row r="706">
-      <c r="A706" s="81"/>
-      <c r="B706" s="82"/>
+      <c r="A706" s="80"/>
+      <c r="B706" s="81"/>
       <c r="C706" s="34"/>
       <c r="D706" s="34"/>
       <c r="E706" s="34"/>
@@ -49998,8 +50041,8 @@
       </c>
     </row>
     <row r="707">
-      <c r="A707" s="81"/>
-      <c r="B707" s="82"/>
+      <c r="A707" s="80"/>
+      <c r="B707" s="81"/>
       <c r="C707" s="34"/>
       <c r="D707" s="34"/>
       <c r="E707" s="34"/>
@@ -50024,8 +50067,8 @@
       </c>
     </row>
     <row r="708">
-      <c r="A708" s="81"/>
-      <c r="B708" s="82"/>
+      <c r="A708" s="80"/>
+      <c r="B708" s="81"/>
       <c r="C708" s="34"/>
       <c r="D708" s="34"/>
       <c r="E708" s="34"/>
@@ -50050,8 +50093,8 @@
       </c>
     </row>
     <row r="709">
-      <c r="A709" s="81"/>
-      <c r="B709" s="82"/>
+      <c r="A709" s="80"/>
+      <c r="B709" s="81"/>
       <c r="C709" s="34"/>
       <c r="D709" s="34"/>
       <c r="E709" s="34"/>
@@ -50076,8 +50119,8 @@
       </c>
     </row>
     <row r="710">
-      <c r="A710" s="81"/>
-      <c r="B710" s="82"/>
+      <c r="A710" s="80"/>
+      <c r="B710" s="81"/>
       <c r="C710" s="34"/>
       <c r="D710" s="34"/>
       <c r="E710" s="34"/>
@@ -50102,8 +50145,8 @@
       </c>
     </row>
     <row r="711">
-      <c r="A711" s="81"/>
-      <c r="B711" s="82"/>
+      <c r="A711" s="80"/>
+      <c r="B711" s="81"/>
       <c r="C711" s="34"/>
       <c r="D711" s="34"/>
       <c r="E711" s="34"/>
@@ -50128,8 +50171,8 @@
       </c>
     </row>
     <row r="712">
-      <c r="A712" s="81"/>
-      <c r="B712" s="82"/>
+      <c r="A712" s="80"/>
+      <c r="B712" s="81"/>
       <c r="C712" s="34"/>
       <c r="D712" s="34"/>
       <c r="E712" s="34"/>
@@ -50154,8 +50197,8 @@
       </c>
     </row>
     <row r="713">
-      <c r="A713" s="81"/>
-      <c r="B713" s="82"/>
+      <c r="A713" s="80"/>
+      <c r="B713" s="81"/>
       <c r="C713" s="34"/>
       <c r="D713" s="34"/>
       <c r="E713" s="34"/>
@@ -50180,8 +50223,8 @@
       </c>
     </row>
     <row r="714">
-      <c r="A714" s="81"/>
-      <c r="B714" s="82"/>
+      <c r="A714" s="80"/>
+      <c r="B714" s="81"/>
       <c r="C714" s="34"/>
       <c r="D714" s="34"/>
       <c r="E714" s="34"/>
@@ -50206,8 +50249,8 @@
       </c>
     </row>
     <row r="715">
-      <c r="A715" s="81"/>
-      <c r="B715" s="82"/>
+      <c r="A715" s="80"/>
+      <c r="B715" s="81"/>
       <c r="C715" s="34"/>
       <c r="D715" s="34"/>
       <c r="E715" s="34"/>
@@ -50232,8 +50275,8 @@
       </c>
     </row>
     <row r="716">
-      <c r="A716" s="81"/>
-      <c r="B716" s="82"/>
+      <c r="A716" s="80"/>
+      <c r="B716" s="81"/>
       <c r="C716" s="34"/>
       <c r="D716" s="34"/>
       <c r="E716" s="34"/>
@@ -50258,8 +50301,8 @@
       </c>
     </row>
     <row r="717">
-      <c r="A717" s="81"/>
-      <c r="B717" s="82"/>
+      <c r="A717" s="80"/>
+      <c r="B717" s="81"/>
       <c r="C717" s="34"/>
       <c r="D717" s="34"/>
       <c r="E717" s="34"/>
@@ -50284,8 +50327,8 @@
       </c>
     </row>
     <row r="718">
-      <c r="A718" s="81"/>
-      <c r="B718" s="82"/>
+      <c r="A718" s="80"/>
+      <c r="B718" s="81"/>
       <c r="C718" s="34"/>
       <c r="D718" s="34"/>
       <c r="E718" s="34"/>
@@ -50310,8 +50353,8 @@
       </c>
     </row>
     <row r="719">
-      <c r="A719" s="81"/>
-      <c r="B719" s="82"/>
+      <c r="A719" s="80"/>
+      <c r="B719" s="81"/>
       <c r="C719" s="34"/>
       <c r="D719" s="34"/>
       <c r="E719" s="34"/>
@@ -50336,8 +50379,8 @@
       </c>
     </row>
     <row r="720">
-      <c r="A720" s="81"/>
-      <c r="B720" s="82"/>
+      <c r="A720" s="80"/>
+      <c r="B720" s="81"/>
       <c r="C720" s="34"/>
       <c r="D720" s="34"/>
       <c r="E720" s="34"/>
@@ -50362,8 +50405,8 @@
       </c>
     </row>
     <row r="721">
-      <c r="A721" s="81"/>
-      <c r="B721" s="82"/>
+      <c r="A721" s="80"/>
+      <c r="B721" s="81"/>
       <c r="C721" s="34"/>
       <c r="D721" s="34"/>
       <c r="E721" s="34"/>
@@ -50388,8 +50431,8 @@
       </c>
     </row>
     <row r="722">
-      <c r="A722" s="81"/>
-      <c r="B722" s="82"/>
+      <c r="A722" s="80"/>
+      <c r="B722" s="81"/>
       <c r="C722" s="34"/>
       <c r="D722" s="34"/>
       <c r="E722" s="34"/>
@@ -50414,8 +50457,8 @@
       </c>
     </row>
     <row r="723">
-      <c r="A723" s="81"/>
-      <c r="B723" s="82"/>
+      <c r="A723" s="80"/>
+      <c r="B723" s="81"/>
       <c r="C723" s="34"/>
       <c r="D723" s="34"/>
       <c r="E723" s="34"/>
@@ -50440,8 +50483,8 @@
       </c>
     </row>
     <row r="724">
-      <c r="A724" s="81"/>
-      <c r="B724" s="82"/>
+      <c r="A724" s="80"/>
+      <c r="B724" s="81"/>
       <c r="C724" s="34"/>
       <c r="D724" s="34"/>
       <c r="E724" s="34"/>
@@ -50466,8 +50509,8 @@
       </c>
     </row>
     <row r="725">
-      <c r="A725" s="81"/>
-      <c r="B725" s="82"/>
+      <c r="A725" s="80"/>
+      <c r="B725" s="81"/>
       <c r="C725" s="34"/>
       <c r="D725" s="34"/>
       <c r="E725" s="34"/>
@@ -50492,8 +50535,8 @@
       </c>
     </row>
     <row r="726">
-      <c r="A726" s="81"/>
-      <c r="B726" s="82"/>
+      <c r="A726" s="80"/>
+      <c r="B726" s="81"/>
       <c r="C726" s="34"/>
       <c r="D726" s="34"/>
       <c r="E726" s="34"/>
@@ -50518,8 +50561,8 @@
       </c>
     </row>
     <row r="727">
-      <c r="A727" s="81"/>
-      <c r="B727" s="82"/>
+      <c r="A727" s="80"/>
+      <c r="B727" s="81"/>
       <c r="C727" s="34"/>
       <c r="D727" s="34"/>
       <c r="E727" s="34"/>
@@ -50544,8 +50587,8 @@
       </c>
     </row>
     <row r="728">
-      <c r="A728" s="81"/>
-      <c r="B728" s="82"/>
+      <c r="A728" s="80"/>
+      <c r="B728" s="81"/>
       <c r="C728" s="34"/>
       <c r="D728" s="34"/>
       <c r="E728" s="34"/>
@@ -50570,8 +50613,8 @@
       </c>
     </row>
     <row r="729">
-      <c r="A729" s="81"/>
-      <c r="B729" s="82"/>
+      <c r="A729" s="80"/>
+      <c r="B729" s="81"/>
       <c r="C729" s="34"/>
       <c r="D729" s="34"/>
       <c r="E729" s="34"/>
@@ -50596,8 +50639,8 @@
       </c>
     </row>
     <row r="730">
-      <c r="A730" s="81"/>
-      <c r="B730" s="82"/>
+      <c r="A730" s="80"/>
+      <c r="B730" s="81"/>
       <c r="C730" s="34"/>
       <c r="D730" s="34"/>
       <c r="E730" s="34"/>
@@ -50622,8 +50665,8 @@
       </c>
     </row>
     <row r="731">
-      <c r="A731" s="81"/>
-      <c r="B731" s="82"/>
+      <c r="A731" s="80"/>
+      <c r="B731" s="81"/>
       <c r="C731" s="34"/>
       <c r="D731" s="34"/>
       <c r="E731" s="34"/>
@@ -50648,8 +50691,8 @@
       </c>
     </row>
     <row r="732">
-      <c r="A732" s="81"/>
-      <c r="B732" s="82"/>
+      <c r="A732" s="80"/>
+      <c r="B732" s="81"/>
       <c r="C732" s="34"/>
       <c r="D732" s="34"/>
       <c r="E732" s="34"/>
@@ -50674,8 +50717,8 @@
       </c>
     </row>
     <row r="733">
-      <c r="A733" s="81"/>
-      <c r="B733" s="82"/>
+      <c r="A733" s="80"/>
+      <c r="B733" s="81"/>
       <c r="C733" s="34"/>
       <c r="D733" s="34"/>
       <c r="E733" s="34"/>
@@ -50700,8 +50743,8 @@
       </c>
     </row>
     <row r="734">
-      <c r="A734" s="81"/>
-      <c r="B734" s="82"/>
+      <c r="A734" s="80"/>
+      <c r="B734" s="81"/>
       <c r="C734" s="34"/>
       <c r="D734" s="34"/>
       <c r="E734" s="34"/>
@@ -50726,8 +50769,8 @@
       </c>
     </row>
     <row r="735">
-      <c r="A735" s="81"/>
-      <c r="B735" s="82"/>
+      <c r="A735" s="80"/>
+      <c r="B735" s="81"/>
       <c r="C735" s="34"/>
       <c r="D735" s="34"/>
       <c r="E735" s="34"/>
@@ -50752,8 +50795,8 @@
       </c>
     </row>
     <row r="736">
-      <c r="A736" s="81"/>
-      <c r="B736" s="82"/>
+      <c r="A736" s="80"/>
+      <c r="B736" s="81"/>
       <c r="C736" s="34"/>
       <c r="D736" s="34"/>
       <c r="E736" s="34"/>
@@ -50778,8 +50821,8 @@
       </c>
     </row>
     <row r="737">
-      <c r="A737" s="81"/>
-      <c r="B737" s="82"/>
+      <c r="A737" s="80"/>
+      <c r="B737" s="81"/>
       <c r="C737" s="34"/>
       <c r="D737" s="34"/>
       <c r="E737" s="34"/>
@@ -50804,8 +50847,8 @@
       </c>
     </row>
     <row r="738">
-      <c r="A738" s="81"/>
-      <c r="B738" s="82"/>
+      <c r="A738" s="80"/>
+      <c r="B738" s="81"/>
       <c r="C738" s="34"/>
       <c r="D738" s="34"/>
       <c r="E738" s="34"/>
@@ -50830,8 +50873,8 @@
       </c>
     </row>
     <row r="739">
-      <c r="A739" s="81"/>
-      <c r="B739" s="82"/>
+      <c r="A739" s="80"/>
+      <c r="B739" s="81"/>
       <c r="C739" s="34"/>
       <c r="D739" s="34"/>
       <c r="E739" s="34"/>
@@ -50856,8 +50899,8 @@
       </c>
     </row>
     <row r="740">
-      <c r="A740" s="81"/>
-      <c r="B740" s="82"/>
+      <c r="A740" s="80"/>
+      <c r="B740" s="81"/>
       <c r="C740" s="34"/>
       <c r="D740" s="34"/>
       <c r="E740" s="34"/>
@@ -50882,8 +50925,8 @@
       </c>
     </row>
     <row r="741">
-      <c r="A741" s="81"/>
-      <c r="B741" s="82"/>
+      <c r="A741" s="80"/>
+      <c r="B741" s="81"/>
       <c r="C741" s="34"/>
       <c r="D741" s="34"/>
       <c r="E741" s="34"/>
@@ -50908,8 +50951,8 @@
       </c>
     </row>
     <row r="742">
-      <c r="A742" s="81"/>
-      <c r="B742" s="82"/>
+      <c r="A742" s="80"/>
+      <c r="B742" s="81"/>
       <c r="C742" s="34"/>
       <c r="D742" s="34"/>
       <c r="E742" s="34"/>
@@ -50934,8 +50977,8 @@
       </c>
     </row>
     <row r="743">
-      <c r="A743" s="81"/>
-      <c r="B743" s="82"/>
+      <c r="A743" s="80"/>
+      <c r="B743" s="81"/>
       <c r="C743" s="34"/>
       <c r="D743" s="34"/>
       <c r="E743" s="34"/>
@@ -50960,8 +51003,8 @@
       </c>
     </row>
     <row r="744">
-      <c r="A744" s="81"/>
-      <c r="B744" s="82"/>
+      <c r="A744" s="80"/>
+      <c r="B744" s="81"/>
       <c r="C744" s="34"/>
       <c r="D744" s="34"/>
       <c r="E744" s="34"/>
@@ -50986,8 +51029,8 @@
       </c>
     </row>
     <row r="745">
-      <c r="A745" s="81"/>
-      <c r="B745" s="82"/>
+      <c r="A745" s="80"/>
+      <c r="B745" s="81"/>
       <c r="C745" s="34"/>
       <c r="D745" s="34"/>
       <c r="E745" s="34"/>
@@ -51012,8 +51055,8 @@
       </c>
     </row>
     <row r="746">
-      <c r="A746" s="81"/>
-      <c r="B746" s="82"/>
+      <c r="A746" s="80"/>
+      <c r="B746" s="81"/>
       <c r="C746" s="34"/>
       <c r="D746" s="34"/>
       <c r="E746" s="34"/>
@@ -51038,8 +51081,8 @@
       </c>
     </row>
     <row r="747">
-      <c r="A747" s="81"/>
-      <c r="B747" s="82"/>
+      <c r="A747" s="80"/>
+      <c r="B747" s="81"/>
       <c r="C747" s="34"/>
       <c r="D747" s="34"/>
       <c r="E747" s="34"/>
@@ -51064,8 +51107,8 @@
       </c>
     </row>
     <row r="748">
-      <c r="A748" s="81"/>
-      <c r="B748" s="82"/>
+      <c r="A748" s="80"/>
+      <c r="B748" s="81"/>
       <c r="C748" s="34"/>
       <c r="D748" s="34"/>
       <c r="E748" s="34"/>
@@ -51090,8 +51133,8 @@
       </c>
     </row>
     <row r="749">
-      <c r="A749" s="81"/>
-      <c r="B749" s="82"/>
+      <c r="A749" s="80"/>
+      <c r="B749" s="81"/>
       <c r="C749" s="34"/>
       <c r="D749" s="34"/>
       <c r="E749" s="34"/>
@@ -51116,8 +51159,8 @@
       </c>
     </row>
     <row r="750">
-      <c r="A750" s="81"/>
-      <c r="B750" s="82"/>
+      <c r="A750" s="80"/>
+      <c r="B750" s="81"/>
       <c r="C750" s="34"/>
       <c r="D750" s="34"/>
       <c r="E750" s="34"/>
@@ -51142,8 +51185,8 @@
       </c>
     </row>
     <row r="751">
-      <c r="A751" s="81"/>
-      <c r="B751" s="82"/>
+      <c r="A751" s="80"/>
+      <c r="B751" s="81"/>
       <c r="C751" s="34"/>
       <c r="D751" s="34"/>
       <c r="E751" s="34"/>
@@ -51168,8 +51211,8 @@
       </c>
     </row>
     <row r="752">
-      <c r="A752" s="81"/>
-      <c r="B752" s="82"/>
+      <c r="A752" s="80"/>
+      <c r="B752" s="81"/>
       <c r="C752" s="34"/>
       <c r="D752" s="34"/>
       <c r="E752" s="34"/>
@@ -51194,8 +51237,8 @@
       </c>
     </row>
     <row r="753">
-      <c r="A753" s="81"/>
-      <c r="B753" s="82"/>
+      <c r="A753" s="80"/>
+      <c r="B753" s="81"/>
       <c r="C753" s="34"/>
       <c r="D753" s="34"/>
       <c r="E753" s="34"/>
@@ -51220,8 +51263,8 @@
       </c>
     </row>
     <row r="754">
-      <c r="A754" s="81"/>
-      <c r="B754" s="82"/>
+      <c r="A754" s="80"/>
+      <c r="B754" s="81"/>
       <c r="C754" s="34"/>
       <c r="D754" s="34"/>
       <c r="E754" s="34"/>
@@ -51246,8 +51289,8 @@
       </c>
     </row>
     <row r="755">
-      <c r="A755" s="81"/>
-      <c r="B755" s="82"/>
+      <c r="A755" s="80"/>
+      <c r="B755" s="81"/>
       <c r="C755" s="34"/>
       <c r="D755" s="34"/>
       <c r="E755" s="34"/>
@@ -51272,8 +51315,8 @@
       </c>
     </row>
     <row r="756">
-      <c r="A756" s="81"/>
-      <c r="B756" s="82"/>
+      <c r="A756" s="80"/>
+      <c r="B756" s="81"/>
       <c r="C756" s="34"/>
       <c r="D756" s="34"/>
       <c r="E756" s="34"/>
@@ -51298,8 +51341,8 @@
       </c>
     </row>
     <row r="757">
-      <c r="A757" s="81"/>
-      <c r="B757" s="82"/>
+      <c r="A757" s="80"/>
+      <c r="B757" s="81"/>
       <c r="C757" s="34"/>
       <c r="D757" s="34"/>
       <c r="E757" s="34"/>
@@ -51324,8 +51367,8 @@
       </c>
     </row>
     <row r="758">
-      <c r="A758" s="81"/>
-      <c r="B758" s="82"/>
+      <c r="A758" s="80"/>
+      <c r="B758" s="81"/>
       <c r="C758" s="34"/>
       <c r="D758" s="34"/>
       <c r="E758" s="34"/>
@@ -51350,8 +51393,8 @@
       </c>
     </row>
     <row r="759">
-      <c r="A759" s="81"/>
-      <c r="B759" s="82"/>
+      <c r="A759" s="80"/>
+      <c r="B759" s="81"/>
       <c r="C759" s="34"/>
       <c r="D759" s="34"/>
       <c r="E759" s="34"/>
@@ -51376,8 +51419,8 @@
       </c>
     </row>
     <row r="760">
-      <c r="A760" s="81"/>
-      <c r="B760" s="82"/>
+      <c r="A760" s="80"/>
+      <c r="B760" s="81"/>
       <c r="C760" s="34"/>
       <c r="D760" s="34"/>
       <c r="E760" s="34"/>
@@ -51402,8 +51445,8 @@
       </c>
     </row>
     <row r="761">
-      <c r="A761" s="81"/>
-      <c r="B761" s="82"/>
+      <c r="A761" s="80"/>
+      <c r="B761" s="81"/>
       <c r="C761" s="34"/>
       <c r="D761" s="34"/>
       <c r="E761" s="34"/>
@@ -51428,8 +51471,8 @@
       </c>
     </row>
     <row r="762">
-      <c r="A762" s="81"/>
-      <c r="B762" s="82"/>
+      <c r="A762" s="80"/>
+      <c r="B762" s="81"/>
       <c r="C762" s="34"/>
       <c r="D762" s="34"/>
       <c r="E762" s="34"/>
@@ -51454,8 +51497,8 @@
       </c>
     </row>
     <row r="763">
-      <c r="A763" s="81"/>
-      <c r="B763" s="82"/>
+      <c r="A763" s="80"/>
+      <c r="B763" s="81"/>
       <c r="C763" s="34"/>
       <c r="D763" s="34"/>
       <c r="E763" s="34"/>
@@ -51480,8 +51523,8 @@
       </c>
     </row>
     <row r="764">
-      <c r="A764" s="81"/>
-      <c r="B764" s="82"/>
+      <c r="A764" s="80"/>
+      <c r="B764" s="81"/>
       <c r="C764" s="34"/>
       <c r="D764" s="34"/>
       <c r="E764" s="34"/>
@@ -51506,8 +51549,8 @@
       </c>
     </row>
     <row r="765">
-      <c r="A765" s="81"/>
-      <c r="B765" s="82"/>
+      <c r="A765" s="80"/>
+      <c r="B765" s="81"/>
       <c r="C765" s="34"/>
       <c r="D765" s="34"/>
       <c r="E765" s="34"/>
@@ -51532,8 +51575,8 @@
       </c>
     </row>
     <row r="766">
-      <c r="A766" s="81"/>
-      <c r="B766" s="82"/>
+      <c r="A766" s="80"/>
+      <c r="B766" s="81"/>
       <c r="C766" s="34"/>
       <c r="D766" s="34"/>
       <c r="E766" s="34"/>
@@ -51558,8 +51601,8 @@
       </c>
     </row>
     <row r="767">
-      <c r="A767" s="81"/>
-      <c r="B767" s="82"/>
+      <c r="A767" s="80"/>
+      <c r="B767" s="81"/>
       <c r="C767" s="34"/>
       <c r="D767" s="34"/>
       <c r="E767" s="34"/>
@@ -51584,8 +51627,8 @@
       </c>
     </row>
     <row r="768">
-      <c r="A768" s="81"/>
-      <c r="B768" s="82"/>
+      <c r="A768" s="80"/>
+      <c r="B768" s="81"/>
       <c r="C768" s="34"/>
       <c r="D768" s="34"/>
       <c r="E768" s="34"/>
@@ -51610,8 +51653,8 @@
       </c>
     </row>
     <row r="769">
-      <c r="A769" s="81"/>
-      <c r="B769" s="82"/>
+      <c r="A769" s="80"/>
+      <c r="B769" s="81"/>
       <c r="C769" s="34"/>
       <c r="D769" s="34"/>
       <c r="E769" s="34"/>
@@ -51636,8 +51679,8 @@
       </c>
     </row>
     <row r="770">
-      <c r="A770" s="81"/>
-      <c r="B770" s="82"/>
+      <c r="A770" s="80"/>
+      <c r="B770" s="81"/>
       <c r="C770" s="34"/>
       <c r="D770" s="34"/>
       <c r="E770" s="34"/>
@@ -51662,8 +51705,8 @@
       </c>
     </row>
     <row r="771">
-      <c r="A771" s="81"/>
-      <c r="B771" s="82"/>
+      <c r="A771" s="80"/>
+      <c r="B771" s="81"/>
       <c r="C771" s="34"/>
       <c r="D771" s="34"/>
       <c r="E771" s="34"/>
@@ -51688,8 +51731,8 @@
       </c>
     </row>
     <row r="772">
-      <c r="A772" s="81"/>
-      <c r="B772" s="82"/>
+      <c r="A772" s="80"/>
+      <c r="B772" s="81"/>
       <c r="C772" s="34"/>
       <c r="D772" s="34"/>
       <c r="E772" s="34"/>
@@ -51714,8 +51757,8 @@
       </c>
     </row>
     <row r="773">
-      <c r="A773" s="81"/>
-      <c r="B773" s="82"/>
+      <c r="A773" s="80"/>
+      <c r="B773" s="81"/>
       <c r="C773" s="34"/>
       <c r="D773" s="34"/>
       <c r="E773" s="34"/>
@@ -51740,8 +51783,8 @@
       </c>
     </row>
     <row r="774">
-      <c r="A774" s="81"/>
-      <c r="B774" s="82"/>
+      <c r="A774" s="80"/>
+      <c r="B774" s="81"/>
       <c r="C774" s="34"/>
       <c r="D774" s="34"/>
       <c r="E774" s="34"/>
@@ -51766,8 +51809,8 @@
       </c>
     </row>
     <row r="775">
-      <c r="A775" s="81"/>
-      <c r="B775" s="82"/>
+      <c r="A775" s="80"/>
+      <c r="B775" s="81"/>
       <c r="C775" s="34"/>
       <c r="D775" s="34"/>
       <c r="E775" s="34"/>
@@ -51792,8 +51835,8 @@
       </c>
     </row>
     <row r="776">
-      <c r="A776" s="81"/>
-      <c r="B776" s="82"/>
+      <c r="A776" s="80"/>
+      <c r="B776" s="81"/>
       <c r="C776" s="34"/>
       <c r="D776" s="34"/>
       <c r="E776" s="34"/>
@@ -51818,8 +51861,8 @@
       </c>
     </row>
     <row r="777">
-      <c r="A777" s="81"/>
-      <c r="B777" s="82"/>
+      <c r="A777" s="80"/>
+      <c r="B777" s="81"/>
       <c r="C777" s="34"/>
       <c r="D777" s="34"/>
       <c r="E777" s="34"/>
@@ -51844,8 +51887,8 @@
       </c>
     </row>
     <row r="778">
-      <c r="A778" s="81"/>
-      <c r="B778" s="82"/>
+      <c r="A778" s="80"/>
+      <c r="B778" s="81"/>
       <c r="C778" s="34"/>
       <c r="D778" s="34"/>
       <c r="E778" s="34"/>
@@ -51870,8 +51913,8 @@
       </c>
     </row>
     <row r="779">
-      <c r="A779" s="81"/>
-      <c r="B779" s="82"/>
+      <c r="A779" s="80"/>
+      <c r="B779" s="81"/>
       <c r="C779" s="34"/>
       <c r="D779" s="34"/>
       <c r="E779" s="34"/>
@@ -51896,8 +51939,8 @@
       </c>
     </row>
     <row r="780">
-      <c r="A780" s="81"/>
-      <c r="B780" s="82"/>
+      <c r="A780" s="80"/>
+      <c r="B780" s="81"/>
       <c r="C780" s="34"/>
       <c r="D780" s="34"/>
       <c r="E780" s="34"/>
@@ -51922,8 +51965,8 @@
       </c>
     </row>
     <row r="781">
-      <c r="A781" s="81"/>
-      <c r="B781" s="82"/>
+      <c r="A781" s="80"/>
+      <c r="B781" s="81"/>
       <c r="C781" s="34"/>
       <c r="D781" s="34"/>
       <c r="E781" s="34"/>
@@ -51948,8 +51991,8 @@
       </c>
     </row>
     <row r="782">
-      <c r="A782" s="81"/>
-      <c r="B782" s="82"/>
+      <c r="A782" s="80"/>
+      <c r="B782" s="81"/>
       <c r="C782" s="34"/>
       <c r="D782" s="34"/>
       <c r="E782" s="34"/>
@@ -51974,8 +52017,8 @@
       </c>
     </row>
     <row r="783">
-      <c r="A783" s="81"/>
-      <c r="B783" s="82"/>
+      <c r="A783" s="80"/>
+      <c r="B783" s="81"/>
       <c r="C783" s="34"/>
       <c r="D783" s="34"/>
       <c r="E783" s="34"/>
@@ -52000,8 +52043,8 @@
       </c>
     </row>
     <row r="784">
-      <c r="A784" s="81"/>
-      <c r="B784" s="82"/>
+      <c r="A784" s="80"/>
+      <c r="B784" s="81"/>
       <c r="C784" s="34"/>
       <c r="D784" s="34"/>
       <c r="E784" s="34"/>
@@ -52026,8 +52069,8 @@
       </c>
     </row>
     <row r="785">
-      <c r="A785" s="81"/>
-      <c r="B785" s="82"/>
+      <c r="A785" s="80"/>
+      <c r="B785" s="81"/>
       <c r="C785" s="34"/>
       <c r="D785" s="34"/>
       <c r="E785" s="34"/>
@@ -52052,8 +52095,8 @@
       </c>
     </row>
     <row r="786">
-      <c r="A786" s="81"/>
-      <c r="B786" s="82"/>
+      <c r="A786" s="80"/>
+      <c r="B786" s="81"/>
       <c r="C786" s="34"/>
       <c r="D786" s="34"/>
       <c r="E786" s="34"/>
@@ -52078,8 +52121,8 @@
       </c>
     </row>
     <row r="787">
-      <c r="A787" s="81"/>
-      <c r="B787" s="82"/>
+      <c r="A787" s="80"/>
+      <c r="B787" s="81"/>
       <c r="C787" s="34"/>
       <c r="D787" s="34"/>
       <c r="E787" s="34"/>
@@ -52104,8 +52147,8 @@
       </c>
     </row>
     <row r="788">
-      <c r="A788" s="81"/>
-      <c r="B788" s="82"/>
+      <c r="A788" s="80"/>
+      <c r="B788" s="81"/>
       <c r="C788" s="34"/>
       <c r="D788" s="34"/>
       <c r="E788" s="34"/>
@@ -52130,8 +52173,8 @@
       </c>
     </row>
     <row r="789">
-      <c r="A789" s="81"/>
-      <c r="B789" s="82"/>
+      <c r="A789" s="80"/>
+      <c r="B789" s="81"/>
       <c r="C789" s="34"/>
       <c r="D789" s="34"/>
       <c r="E789" s="34"/>
@@ -52156,8 +52199,8 @@
       </c>
     </row>
     <row r="790">
-      <c r="A790" s="81"/>
-      <c r="B790" s="82"/>
+      <c r="A790" s="80"/>
+      <c r="B790" s="81"/>
       <c r="C790" s="34"/>
       <c r="D790" s="34"/>
       <c r="E790" s="34"/>
@@ -52182,8 +52225,8 @@
       </c>
     </row>
     <row r="791">
-      <c r="A791" s="81"/>
-      <c r="B791" s="82"/>
+      <c r="A791" s="80"/>
+      <c r="B791" s="81"/>
       <c r="C791" s="34"/>
       <c r="D791" s="34"/>
       <c r="E791" s="34"/>
@@ -52208,8 +52251,8 @@
       </c>
     </row>
     <row r="792">
-      <c r="A792" s="81"/>
-      <c r="B792" s="82"/>
+      <c r="A792" s="80"/>
+      <c r="B792" s="81"/>
       <c r="C792" s="34"/>
       <c r="D792" s="34"/>
       <c r="E792" s="34"/>
@@ -52234,8 +52277,8 @@
       </c>
     </row>
     <row r="793">
-      <c r="A793" s="81"/>
-      <c r="B793" s="82"/>
+      <c r="A793" s="80"/>
+      <c r="B793" s="81"/>
       <c r="C793" s="34"/>
       <c r="D793" s="34"/>
       <c r="E793" s="34"/>
@@ -52260,8 +52303,8 @@
       </c>
     </row>
     <row r="794">
-      <c r="A794" s="81"/>
-      <c r="B794" s="82"/>
+      <c r="A794" s="80"/>
+      <c r="B794" s="81"/>
       <c r="C794" s="34"/>
       <c r="D794" s="34"/>
       <c r="E794" s="34"/>
@@ -52286,8 +52329,8 @@
       </c>
     </row>
     <row r="795">
-      <c r="A795" s="81"/>
-      <c r="B795" s="82"/>
+      <c r="A795" s="80"/>
+      <c r="B795" s="81"/>
       <c r="C795" s="34"/>
       <c r="D795" s="34"/>
       <c r="E795" s="34"/>
@@ -52312,8 +52355,8 @@
       </c>
     </row>
     <row r="796">
-      <c r="A796" s="81"/>
-      <c r="B796" s="82"/>
+      <c r="A796" s="80"/>
+      <c r="B796" s="81"/>
       <c r="C796" s="34"/>
       <c r="D796" s="34"/>
       <c r="E796" s="34"/>
@@ -52338,8 +52381,8 @@
       </c>
     </row>
     <row r="797">
-      <c r="A797" s="81"/>
-      <c r="B797" s="82"/>
+      <c r="A797" s="80"/>
+      <c r="B797" s="81"/>
       <c r="C797" s="34"/>
       <c r="D797" s="34"/>
       <c r="E797" s="34"/>
@@ -52364,8 +52407,8 @@
       </c>
     </row>
     <row r="798">
-      <c r="A798" s="81"/>
-      <c r="B798" s="82"/>
+      <c r="A798" s="80"/>
+      <c r="B798" s="81"/>
       <c r="C798" s="34"/>
       <c r="D798" s="34"/>
       <c r="E798" s="34"/>
@@ -52390,8 +52433,8 @@
       </c>
     </row>
     <row r="799">
-      <c r="A799" s="81"/>
-      <c r="B799" s="82"/>
+      <c r="A799" s="80"/>
+      <c r="B799" s="81"/>
       <c r="C799" s="34"/>
       <c r="D799" s="34"/>
       <c r="E799" s="34"/>
@@ -52416,8 +52459,8 @@
       </c>
     </row>
     <row r="800">
-      <c r="A800" s="81"/>
-      <c r="B800" s="82"/>
+      <c r="A800" s="80"/>
+      <c r="B800" s="81"/>
       <c r="C800" s="34"/>
       <c r="D800" s="34"/>
       <c r="E800" s="34"/>
@@ -52442,8 +52485,8 @@
       </c>
     </row>
     <row r="801">
-      <c r="A801" s="81"/>
-      <c r="B801" s="82"/>
+      <c r="A801" s="80"/>
+      <c r="B801" s="81"/>
       <c r="C801" s="34"/>
       <c r="D801" s="34"/>
       <c r="E801" s="34"/>
@@ -52468,8 +52511,8 @@
       </c>
     </row>
     <row r="802">
-      <c r="A802" s="81"/>
-      <c r="B802" s="82"/>
+      <c r="A802" s="80"/>
+      <c r="B802" s="81"/>
       <c r="C802" s="34"/>
       <c r="D802" s="34"/>
       <c r="E802" s="34"/>
@@ -52494,8 +52537,8 @@
       </c>
     </row>
     <row r="803">
-      <c r="A803" s="81"/>
-      <c r="B803" s="82"/>
+      <c r="A803" s="80"/>
+      <c r="B803" s="81"/>
       <c r="C803" s="34"/>
       <c r="D803" s="34"/>
       <c r="E803" s="34"/>
@@ -52520,8 +52563,8 @@
       </c>
     </row>
     <row r="804">
-      <c r="A804" s="81"/>
-      <c r="B804" s="82"/>
+      <c r="A804" s="80"/>
+      <c r="B804" s="81"/>
       <c r="C804" s="34"/>
       <c r="D804" s="34"/>
       <c r="E804" s="34"/>
@@ -52546,8 +52589,8 @@
       </c>
     </row>
     <row r="805">
-      <c r="A805" s="81"/>
-      <c r="B805" s="82"/>
+      <c r="A805" s="80"/>
+      <c r="B805" s="81"/>
       <c r="C805" s="34"/>
       <c r="D805" s="34"/>
       <c r="E805" s="34"/>
@@ -52572,8 +52615,8 @@
       </c>
     </row>
     <row r="806">
-      <c r="A806" s="81"/>
-      <c r="B806" s="82"/>
+      <c r="A806" s="80"/>
+      <c r="B806" s="81"/>
       <c r="C806" s="34"/>
       <c r="D806" s="34"/>
       <c r="E806" s="34"/>
@@ -52598,8 +52641,8 @@
       </c>
     </row>
     <row r="807">
-      <c r="A807" s="81"/>
-      <c r="B807" s="82"/>
+      <c r="A807" s="80"/>
+      <c r="B807" s="81"/>
       <c r="C807" s="34"/>
       <c r="D807" s="34"/>
       <c r="E807" s="34"/>
@@ -52624,8 +52667,8 @@
       </c>
     </row>
     <row r="808">
-      <c r="A808" s="81"/>
-      <c r="B808" s="82"/>
+      <c r="A808" s="80"/>
+      <c r="B808" s="81"/>
       <c r="C808" s="34"/>
       <c r="D808" s="34"/>
       <c r="E808" s="34"/>
@@ -52650,8 +52693,8 @@
       </c>
     </row>
     <row r="809">
-      <c r="A809" s="81"/>
-      <c r="B809" s="82"/>
+      <c r="A809" s="80"/>
+      <c r="B809" s="81"/>
       <c r="C809" s="34"/>
       <c r="D809" s="34"/>
       <c r="E809" s="34"/>
@@ -52676,8 +52719,8 @@
       </c>
     </row>
     <row r="810">
-      <c r="A810" s="81"/>
-      <c r="B810" s="82"/>
+      <c r="A810" s="80"/>
+      <c r="B810" s="81"/>
       <c r="C810" s="34"/>
       <c r="D810" s="34"/>
       <c r="E810" s="34"/>
@@ -52702,8 +52745,8 @@
       </c>
     </row>
     <row r="811">
-      <c r="A811" s="81"/>
-      <c r="B811" s="82"/>
+      <c r="A811" s="80"/>
+      <c r="B811" s="81"/>
       <c r="C811" s="34"/>
       <c r="D811" s="34"/>
       <c r="E811" s="34"/>
@@ -52728,8 +52771,8 @@
       </c>
     </row>
     <row r="812">
-      <c r="A812" s="81"/>
-      <c r="B812" s="82"/>
+      <c r="A812" s="80"/>
+      <c r="B812" s="81"/>
       <c r="C812" s="34"/>
       <c r="D812" s="34"/>
       <c r="E812" s="34"/>
@@ -52754,8 +52797,8 @@
       </c>
     </row>
     <row r="813">
-      <c r="A813" s="81"/>
-      <c r="B813" s="82"/>
+      <c r="A813" s="80"/>
+      <c r="B813" s="81"/>
       <c r="C813" s="34"/>
       <c r="D813" s="34"/>
       <c r="E813" s="34"/>
@@ -52780,8 +52823,8 @@
       </c>
     </row>
     <row r="814">
-      <c r="A814" s="81"/>
-      <c r="B814" s="82"/>
+      <c r="A814" s="80"/>
+      <c r="B814" s="81"/>
       <c r="C814" s="34"/>
       <c r="D814" s="34"/>
       <c r="E814" s="34"/>
@@ -52806,8 +52849,8 @@
       </c>
     </row>
     <row r="815">
-      <c r="A815" s="81"/>
-      <c r="B815" s="82"/>
+      <c r="A815" s="80"/>
+      <c r="B815" s="81"/>
       <c r="C815" s="34"/>
       <c r="D815" s="34"/>
       <c r="E815" s="34"/>
@@ -52832,8 +52875,8 @@
       </c>
     </row>
     <row r="816">
-      <c r="A816" s="81"/>
-      <c r="B816" s="82"/>
+      <c r="A816" s="80"/>
+      <c r="B816" s="81"/>
       <c r="C816" s="34"/>
       <c r="D816" s="34"/>
       <c r="E816" s="34"/>
@@ -52858,8 +52901,8 @@
       </c>
     </row>
     <row r="817">
-      <c r="A817" s="81"/>
-      <c r="B817" s="82"/>
+      <c r="A817" s="80"/>
+      <c r="B817" s="81"/>
       <c r="C817" s="34"/>
       <c r="D817" s="34"/>
       <c r="E817" s="34"/>
@@ -52884,8 +52927,8 @@
       </c>
     </row>
     <row r="818">
-      <c r="A818" s="81"/>
-      <c r="B818" s="82"/>
+      <c r="A818" s="80"/>
+      <c r="B818" s="81"/>
       <c r="C818" s="34"/>
       <c r="D818" s="34"/>
       <c r="E818" s="34"/>
@@ -52910,8 +52953,8 @@
       </c>
     </row>
     <row r="819">
-      <c r="A819" s="81"/>
-      <c r="B819" s="82"/>
+      <c r="A819" s="80"/>
+      <c r="B819" s="81"/>
       <c r="C819" s="34"/>
       <c r="D819" s="34"/>
       <c r="E819" s="34"/>
@@ -52936,8 +52979,8 @@
       </c>
     </row>
     <row r="820">
-      <c r="A820" s="81"/>
-      <c r="B820" s="82"/>
+      <c r="A820" s="80"/>
+      <c r="B820" s="81"/>
       <c r="C820" s="34"/>
       <c r="D820" s="34"/>
       <c r="E820" s="34"/>
@@ -52962,8 +53005,8 @@
       </c>
     </row>
     <row r="821">
-      <c r="A821" s="81"/>
-      <c r="B821" s="82"/>
+      <c r="A821" s="80"/>
+      <c r="B821" s="81"/>
       <c r="C821" s="34"/>
       <c r="D821" s="34"/>
       <c r="E821" s="34"/>
@@ -52988,8 +53031,8 @@
       </c>
     </row>
     <row r="822">
-      <c r="A822" s="81"/>
-      <c r="B822" s="82"/>
+      <c r="A822" s="80"/>
+      <c r="B822" s="81"/>
       <c r="C822" s="34"/>
       <c r="D822" s="34"/>
       <c r="E822" s="34"/>
@@ -53014,8 +53057,8 @@
       </c>
     </row>
     <row r="823">
-      <c r="A823" s="81"/>
-      <c r="B823" s="82"/>
+      <c r="A823" s="80"/>
+      <c r="B823" s="81"/>
       <c r="C823" s="34"/>
       <c r="D823" s="34"/>
       <c r="E823" s="34"/>
@@ -53040,8 +53083,8 @@
       </c>
     </row>
     <row r="824">
-      <c r="A824" s="81"/>
-      <c r="B824" s="82"/>
+      <c r="A824" s="80"/>
+      <c r="B824" s="81"/>
       <c r="C824" s="34"/>
       <c r="D824" s="34"/>
       <c r="E824" s="34"/>
@@ -53066,8 +53109,8 @@
       </c>
     </row>
     <row r="825">
-      <c r="A825" s="81"/>
-      <c r="B825" s="82"/>
+      <c r="A825" s="80"/>
+      <c r="B825" s="81"/>
       <c r="C825" s="34"/>
       <c r="D825" s="34"/>
       <c r="E825" s="34"/>
@@ -53092,8 +53135,8 @@
       </c>
     </row>
     <row r="826">
-      <c r="A826" s="81"/>
-      <c r="B826" s="82"/>
+      <c r="A826" s="80"/>
+      <c r="B826" s="81"/>
       <c r="C826" s="34"/>
       <c r="D826" s="34"/>
       <c r="E826" s="34"/>
@@ -53118,8 +53161,8 @@
       </c>
     </row>
     <row r="827">
-      <c r="A827" s="81"/>
-      <c r="B827" s="82"/>
+      <c r="A827" s="80"/>
+      <c r="B827" s="81"/>
       <c r="C827" s="34"/>
       <c r="D827" s="34"/>
       <c r="E827" s="34"/>
@@ -53144,8 +53187,8 @@
       </c>
     </row>
     <row r="828">
-      <c r="A828" s="81"/>
-      <c r="B828" s="82"/>
+      <c r="A828" s="80"/>
+      <c r="B828" s="81"/>
       <c r="C828" s="34"/>
       <c r="D828" s="34"/>
       <c r="E828" s="34"/>
@@ -53170,8 +53213,8 @@
       </c>
     </row>
     <row r="829">
-      <c r="A829" s="81"/>
-      <c r="B829" s="82"/>
+      <c r="A829" s="80"/>
+      <c r="B829" s="81"/>
       <c r="C829" s="34"/>
       <c r="D829" s="34"/>
       <c r="E829" s="34"/>
@@ -53196,8 +53239,8 @@
       </c>
     </row>
     <row r="830">
-      <c r="A830" s="81"/>
-      <c r="B830" s="82"/>
+      <c r="A830" s="80"/>
+      <c r="B830" s="81"/>
       <c r="C830" s="34"/>
       <c r="D830" s="34"/>
       <c r="E830" s="34"/>
@@ -53222,8 +53265,8 @@
       </c>
     </row>
     <row r="831">
-      <c r="A831" s="81"/>
-      <c r="B831" s="82"/>
+      <c r="A831" s="80"/>
+      <c r="B831" s="81"/>
       <c r="C831" s="34"/>
       <c r="D831" s="34"/>
       <c r="E831" s="34"/>
@@ -53248,8 +53291,8 @@
       </c>
     </row>
     <row r="832">
-      <c r="A832" s="81"/>
-      <c r="B832" s="82"/>
+      <c r="A832" s="80"/>
+      <c r="B832" s="81"/>
       <c r="C832" s="34"/>
       <c r="D832" s="34"/>
       <c r="E832" s="34"/>
@@ -53274,8 +53317,8 @@
       </c>
     </row>
     <row r="833">
-      <c r="A833" s="81"/>
-      <c r="B833" s="82"/>
+      <c r="A833" s="80"/>
+      <c r="B833" s="81"/>
       <c r="C833" s="34"/>
       <c r="D833" s="34"/>
       <c r="E833" s="34"/>
@@ -53300,8 +53343,8 @@
       </c>
     </row>
     <row r="834">
-      <c r="A834" s="81"/>
-      <c r="B834" s="82"/>
+      <c r="A834" s="80"/>
+      <c r="B834" s="81"/>
       <c r="C834" s="34"/>
       <c r="D834" s="34"/>
       <c r="E834" s="34"/>
@@ -53326,8 +53369,8 @@
       </c>
     </row>
     <row r="835">
-      <c r="A835" s="81"/>
-      <c r="B835" s="82"/>
+      <c r="A835" s="80"/>
+      <c r="B835" s="81"/>
       <c r="C835" s="34"/>
       <c r="D835" s="34"/>
       <c r="E835" s="34"/>
@@ -53352,8 +53395,8 @@
       </c>
     </row>
     <row r="836">
-      <c r="A836" s="81"/>
-      <c r="B836" s="82"/>
+      <c r="A836" s="80"/>
+      <c r="B836" s="81"/>
       <c r="C836" s="34"/>
       <c r="D836" s="34"/>
       <c r="E836" s="34"/>
@@ -53378,8 +53421,8 @@
       </c>
     </row>
     <row r="837">
-      <c r="A837" s="81"/>
-      <c r="B837" s="82"/>
+      <c r="A837" s="80"/>
+      <c r="B837" s="81"/>
       <c r="C837" s="34"/>
       <c r="D837" s="34"/>
       <c r="E837" s="34"/>
@@ -53404,8 +53447,8 @@
       </c>
     </row>
     <row r="838">
-      <c r="A838" s="81"/>
-      <c r="B838" s="82"/>
+      <c r="A838" s="80"/>
+      <c r="B838" s="81"/>
       <c r="C838" s="34"/>
       <c r="D838" s="34"/>
       <c r="E838" s="34"/>
@@ -53430,8 +53473,8 @@
       </c>
     </row>
     <row r="839">
-      <c r="A839" s="81"/>
-      <c r="B839" s="82"/>
+      <c r="A839" s="80"/>
+      <c r="B839" s="81"/>
       <c r="C839" s="34"/>
       <c r="D839" s="34"/>
       <c r="E839" s="34"/>
@@ -53456,8 +53499,8 @@
       </c>
     </row>
     <row r="840">
-      <c r="A840" s="81"/>
-      <c r="B840" s="82"/>
+      <c r="A840" s="80"/>
+      <c r="B840" s="81"/>
       <c r="C840" s="34"/>
       <c r="D840" s="34"/>
       <c r="E840" s="34"/>
@@ -53482,8 +53525,8 @@
       </c>
     </row>
     <row r="841">
-      <c r="A841" s="81"/>
-      <c r="B841" s="82"/>
+      <c r="A841" s="80"/>
+      <c r="B841" s="81"/>
       <c r="C841" s="34"/>
       <c r="D841" s="34"/>
       <c r="E841" s="34"/>
@@ -53508,8 +53551,8 @@
       </c>
     </row>
     <row r="842">
-      <c r="A842" s="81"/>
-      <c r="B842" s="82"/>
+      <c r="A842" s="80"/>
+      <c r="B842" s="81"/>
       <c r="C842" s="34"/>
       <c r="D842" s="34"/>
       <c r="E842" s="34"/>
@@ -53534,8 +53577,8 @@
       </c>
     </row>
     <row r="843">
-      <c r="A843" s="81"/>
-      <c r="B843" s="82"/>
+      <c r="A843" s="80"/>
+      <c r="B843" s="81"/>
       <c r="C843" s="34"/>
       <c r="D843" s="34"/>
       <c r="E843" s="34"/>
@@ -53560,8 +53603,8 @@
       </c>
     </row>
     <row r="844">
-      <c r="A844" s="81"/>
-      <c r="B844" s="82"/>
+      <c r="A844" s="80"/>
+      <c r="B844" s="81"/>
       <c r="C844" s="34"/>
       <c r="D844" s="34"/>
       <c r="E844" s="34"/>
@@ -53586,8 +53629,8 @@
       </c>
     </row>
     <row r="845">
-      <c r="A845" s="81"/>
-      <c r="B845" s="82"/>
+      <c r="A845" s="80"/>
+      <c r="B845" s="81"/>
       <c r="C845" s="34"/>
       <c r="D845" s="34"/>
       <c r="E845" s="34"/>
@@ -53612,8 +53655,8 @@
       </c>
     </row>
     <row r="846">
-      <c r="A846" s="81"/>
-      <c r="B846" s="82"/>
+      <c r="A846" s="80"/>
+      <c r="B846" s="81"/>
       <c r="C846" s="34"/>
       <c r="D846" s="34"/>
       <c r="E846" s="34"/>
@@ -53638,8 +53681,8 @@
       </c>
     </row>
     <row r="847">
-      <c r="A847" s="81"/>
-      <c r="B847" s="82"/>
+      <c r="A847" s="80"/>
+      <c r="B847" s="81"/>
       <c r="C847" s="34"/>
       <c r="D847" s="34"/>
       <c r="E847" s="34"/>
@@ -53664,8 +53707,8 @@
       </c>
     </row>
     <row r="848">
-      <c r="A848" s="81"/>
-      <c r="B848" s="82"/>
+      <c r="A848" s="80"/>
+      <c r="B848" s="81"/>
       <c r="C848" s="34"/>
       <c r="D848" s="34"/>
       <c r="E848" s="34"/>
@@ -53690,8 +53733,8 @@
       </c>
     </row>
     <row r="849">
-      <c r="A849" s="81"/>
-      <c r="B849" s="82"/>
+      <c r="A849" s="80"/>
+      <c r="B849" s="81"/>
       <c r="C849" s="34"/>
       <c r="D849" s="34"/>
       <c r="E849" s="34"/>
@@ -53716,8 +53759,8 @@
       </c>
     </row>
     <row r="850">
-      <c r="A850" s="81"/>
-      <c r="B850" s="82"/>
+      <c r="A850" s="80"/>
+      <c r="B850" s="81"/>
       <c r="C850" s="34"/>
       <c r="D850" s="34"/>
       <c r="E850" s="34"/>
@@ -53742,8 +53785,8 @@
       </c>
     </row>
     <row r="851">
-      <c r="A851" s="81"/>
-      <c r="B851" s="82"/>
+      <c r="A851" s="80"/>
+      <c r="B851" s="81"/>
       <c r="C851" s="34"/>
       <c r="D851" s="34"/>
       <c r="E851" s="34"/>
@@ -53768,8 +53811,8 @@
       </c>
     </row>
     <row r="852">
-      <c r="A852" s="81"/>
-      <c r="B852" s="82"/>
+      <c r="A852" s="80"/>
+      <c r="B852" s="81"/>
       <c r="C852" s="34"/>
       <c r="D852" s="34"/>
       <c r="E852" s="34"/>
@@ -53794,8 +53837,8 @@
       </c>
     </row>
     <row r="853">
-      <c r="A853" s="81"/>
-      <c r="B853" s="82"/>
+      <c r="A853" s="80"/>
+      <c r="B853" s="81"/>
       <c r="C853" s="34"/>
       <c r="D853" s="34"/>
       <c r="E853" s="34"/>
@@ -53820,8 +53863,8 @@
       </c>
     </row>
     <row r="854">
-      <c r="A854" s="81"/>
-      <c r="B854" s="82"/>
+      <c r="A854" s="80"/>
+      <c r="B854" s="81"/>
       <c r="C854" s="34"/>
       <c r="D854" s="34"/>
       <c r="E854" s="34"/>
@@ -53846,8 +53889,8 @@
       </c>
     </row>
     <row r="855">
-      <c r="A855" s="81"/>
-      <c r="B855" s="82"/>
+      <c r="A855" s="80"/>
+      <c r="B855" s="81"/>
       <c r="C855" s="34"/>
       <c r="D855" s="34"/>
       <c r="E855" s="34"/>
@@ -53872,8 +53915,8 @@
       </c>
     </row>
     <row r="856">
-      <c r="A856" s="81"/>
-      <c r="B856" s="82"/>
+      <c r="A856" s="80"/>
+      <c r="B856" s="81"/>
       <c r="C856" s="34"/>
       <c r="D856" s="34"/>
       <c r="E856" s="34"/>
@@ -53898,8 +53941,8 @@
       </c>
     </row>
     <row r="857">
-      <c r="A857" s="81"/>
-      <c r="B857" s="82"/>
+      <c r="A857" s="80"/>
+      <c r="B857" s="81"/>
       <c r="C857" s="34"/>
       <c r="D857" s="34"/>
       <c r="E857" s="34"/>
@@ -53924,8 +53967,8 @@
       </c>
     </row>
     <row r="858">
-      <c r="A858" s="81"/>
-      <c r="B858" s="82"/>
+      <c r="A858" s="80"/>
+      <c r="B858" s="81"/>
       <c r="C858" s="34"/>
       <c r="D858" s="34"/>
       <c r="E858" s="34"/>
@@ -53950,8 +53993,8 @@
       </c>
     </row>
     <row r="859">
-      <c r="A859" s="81"/>
-      <c r="B859" s="82"/>
+      <c r="A859" s="80"/>
+      <c r="B859" s="81"/>
       <c r="C859" s="34"/>
       <c r="D859" s="34"/>
       <c r="E859" s="34"/>
@@ -53976,8 +54019,8 @@
       </c>
     </row>
     <row r="860">
-      <c r="A860" s="81"/>
-      <c r="B860" s="82"/>
+      <c r="A860" s="80"/>
+      <c r="B860" s="81"/>
       <c r="C860" s="34"/>
       <c r="D860" s="34"/>
       <c r="E860" s="34"/>
@@ -54002,8 +54045,8 @@
       </c>
     </row>
     <row r="861">
-      <c r="A861" s="81"/>
-      <c r="B861" s="82"/>
+      <c r="A861" s="80"/>
+      <c r="B861" s="81"/>
       <c r="C861" s="34"/>
       <c r="D861" s="34"/>
       <c r="E861" s="34"/>
@@ -54028,8 +54071,8 @@
       </c>
     </row>
     <row r="862">
-      <c r="A862" s="81"/>
-      <c r="B862" s="82"/>
+      <c r="A862" s="80"/>
+      <c r="B862" s="81"/>
       <c r="C862" s="34"/>
       <c r="D862" s="34"/>
       <c r="E862" s="34"/>
@@ -54054,8 +54097,8 @@
       </c>
     </row>
     <row r="863">
-      <c r="A863" s="81"/>
-      <c r="B863" s="82"/>
+      <c r="A863" s="80"/>
+      <c r="B863" s="81"/>
       <c r="C863" s="34"/>
       <c r="D863" s="34"/>
       <c r="E863" s="34"/>
@@ -54080,8 +54123,8 @@
       </c>
     </row>
     <row r="864">
-      <c r="A864" s="81"/>
-      <c r="B864" s="82"/>
+      <c r="A864" s="80"/>
+      <c r="B864" s="81"/>
       <c r="C864" s="34"/>
       <c r="D864" s="34"/>
       <c r="E864" s="34"/>
@@ -54106,8 +54149,8 @@
       </c>
     </row>
     <row r="865">
-      <c r="A865" s="81"/>
-      <c r="B865" s="82"/>
+      <c r="A865" s="80"/>
+      <c r="B865" s="81"/>
       <c r="C865" s="34"/>
       <c r="D865" s="34"/>
       <c r="E865" s="34"/>
@@ -54132,8 +54175,8 @@
       </c>
     </row>
     <row r="866">
-      <c r="A866" s="81"/>
-      <c r="B866" s="82"/>
+      <c r="A866" s="80"/>
+      <c r="B866" s="81"/>
       <c r="C866" s="34"/>
       <c r="D866" s="34"/>
       <c r="E866" s="34"/>
@@ -54158,8 +54201,8 @@
       </c>
     </row>
     <row r="867">
-      <c r="A867" s="81"/>
-      <c r="B867" s="82"/>
+      <c r="A867" s="80"/>
+      <c r="B867" s="81"/>
       <c r="C867" s="34"/>
       <c r="D867" s="34"/>
       <c r="E867" s="34"/>
@@ -54184,8 +54227,8 @@
       </c>
     </row>
     <row r="868">
-      <c r="A868" s="81"/>
-      <c r="B868" s="82"/>
+      <c r="A868" s="80"/>
+      <c r="B868" s="81"/>
       <c r="C868" s="34"/>
       <c r="D868" s="34"/>
       <c r="E868" s="34"/>
@@ -54210,8 +54253,8 @@
       </c>
     </row>
     <row r="869">
-      <c r="A869" s="81"/>
-      <c r="B869" s="82"/>
+      <c r="A869" s="80"/>
+      <c r="B869" s="81"/>
       <c r="C869" s="34"/>
       <c r="D869" s="34"/>
       <c r="E869" s="34"/>
@@ -54236,8 +54279,8 @@
       </c>
     </row>
     <row r="870">
-      <c r="A870" s="81"/>
-      <c r="B870" s="82"/>
+      <c r="A870" s="80"/>
+      <c r="B870" s="81"/>
       <c r="C870" s="34"/>
       <c r="D870" s="34"/>
       <c r="E870" s="34"/>
@@ -54262,8 +54305,8 @@
       </c>
     </row>
     <row r="871">
-      <c r="A871" s="81"/>
-      <c r="B871" s="82"/>
+      <c r="A871" s="80"/>
+      <c r="B871" s="81"/>
       <c r="C871" s="34"/>
       <c r="D871" s="34"/>
       <c r="E871" s="34"/>
@@ -54288,8 +54331,8 @@
       </c>
     </row>
     <row r="872">
-      <c r="A872" s="81"/>
-      <c r="B872" s="82"/>
+      <c r="A872" s="80"/>
+      <c r="B872" s="81"/>
       <c r="C872" s="34"/>
       <c r="D872" s="34"/>
       <c r="E872" s="34"/>
@@ -54314,8 +54357,8 @@
       </c>
     </row>
     <row r="873">
-      <c r="A873" s="81"/>
-      <c r="B873" s="82"/>
+      <c r="A873" s="80"/>
+      <c r="B873" s="81"/>
       <c r="C873" s="34"/>
       <c r="D873" s="34"/>
       <c r="E873" s="34"/>
@@ -54340,8 +54383,8 @@
       </c>
     </row>
     <row r="874">
-      <c r="A874" s="81"/>
-      <c r="B874" s="82"/>
+      <c r="A874" s="80"/>
+      <c r="B874" s="81"/>
       <c r="C874" s="34"/>
       <c r="D874" s="34"/>
       <c r="E874" s="34"/>
@@ -54366,8 +54409,8 @@
       </c>
     </row>
     <row r="875">
-      <c r="A875" s="81"/>
-      <c r="B875" s="82"/>
+      <c r="A875" s="80"/>
+      <c r="B875" s="81"/>
       <c r="C875" s="34"/>
       <c r="D875" s="34"/>
       <c r="E875" s="34"/>
@@ -54392,8 +54435,8 @@
       </c>
     </row>
     <row r="876">
-      <c r="A876" s="81"/>
-      <c r="B876" s="82"/>
+      <c r="A876" s="80"/>
+      <c r="B876" s="81"/>
       <c r="C876" s="34"/>
       <c r="D876" s="34"/>
       <c r="E876" s="34"/>
@@ -54418,8 +54461,8 @@
       </c>
     </row>
     <row r="877">
-      <c r="A877" s="81"/>
-      <c r="B877" s="82"/>
+      <c r="A877" s="80"/>
+      <c r="B877" s="81"/>
       <c r="C877" s="34"/>
       <c r="D877" s="34"/>
       <c r="E877" s="34"/>
@@ -54444,8 +54487,8 @@
       </c>
     </row>
     <row r="878">
-      <c r="A878" s="81"/>
-      <c r="B878" s="82"/>
+      <c r="A878" s="80"/>
+      <c r="B878" s="81"/>
       <c r="C878" s="34"/>
       <c r="D878" s="34"/>
       <c r="E878" s="34"/>
@@ -54470,8 +54513,8 @@
       </c>
     </row>
     <row r="879">
-      <c r="A879" s="81"/>
-      <c r="B879" s="82"/>
+      <c r="A879" s="80"/>
+      <c r="B879" s="81"/>
       <c r="C879" s="34"/>
       <c r="D879" s="34"/>
       <c r="E879" s="34"/>
@@ -54496,8 +54539,8 @@
       </c>
     </row>
     <row r="880">
-      <c r="A880" s="81"/>
-      <c r="B880" s="82"/>
+      <c r="A880" s="80"/>
+      <c r="B880" s="81"/>
       <c r="C880" s="34"/>
       <c r="D880" s="34"/>
       <c r="E880" s="34"/>
@@ -54522,8 +54565,8 @@
       </c>
     </row>
     <row r="881">
-      <c r="A881" s="81"/>
-      <c r="B881" s="82"/>
+      <c r="A881" s="80"/>
+      <c r="B881" s="81"/>
       <c r="C881" s="34"/>
       <c r="D881" s="34"/>
       <c r="E881" s="34"/>
@@ -54548,8 +54591,8 @@
       </c>
     </row>
     <row r="882">
-      <c r="A882" s="81"/>
-      <c r="B882" s="82"/>
+      <c r="A882" s="80"/>
+      <c r="B882" s="81"/>
       <c r="C882" s="34"/>
       <c r="D882" s="34"/>
       <c r="E882" s="34"/>
@@ -54574,8 +54617,8 @@
       </c>
     </row>
     <row r="883">
-      <c r="A883" s="81"/>
-      <c r="B883" s="82"/>
+      <c r="A883" s="80"/>
+      <c r="B883" s="81"/>
       <c r="C883" s="34"/>
       <c r="D883" s="34"/>
       <c r="E883" s="34"/>
@@ -54600,8 +54643,8 @@
       </c>
     </row>
     <row r="884">
-      <c r="A884" s="81"/>
-      <c r="B884" s="82"/>
+      <c r="A884" s="80"/>
+      <c r="B884" s="81"/>
       <c r="C884" s="34"/>
       <c r="D884" s="34"/>
       <c r="E884" s="34"/>
@@ -54626,8 +54669,8 @@
       </c>
     </row>
     <row r="885">
-      <c r="A885" s="81"/>
-      <c r="B885" s="82"/>
+      <c r="A885" s="80"/>
+      <c r="B885" s="81"/>
       <c r="C885" s="34"/>
       <c r="D885" s="34"/>
       <c r="E885" s="34"/>
@@ -54652,8 +54695,8 @@
       </c>
     </row>
     <row r="886">
-      <c r="A886" s="81"/>
-      <c r="B886" s="82"/>
+      <c r="A886" s="80"/>
+      <c r="B886" s="81"/>
       <c r="C886" s="34"/>
       <c r="D886" s="34"/>
       <c r="E886" s="34"/>
@@ -54678,8 +54721,8 @@
       </c>
     </row>
     <row r="887">
-      <c r="A887" s="81"/>
-      <c r="B887" s="82"/>
+      <c r="A887" s="80"/>
+      <c r="B887" s="81"/>
       <c r="C887" s="34"/>
       <c r="D887" s="34"/>
       <c r="E887" s="34"/>
@@ -54704,8 +54747,8 @@
       </c>
     </row>
     <row r="888">
-      <c r="A888" s="81"/>
-      <c r="B888" s="82"/>
+      <c r="A888" s="80"/>
+      <c r="B888" s="81"/>
       <c r="C888" s="34"/>
       <c r="D888" s="34"/>
       <c r="E888" s="34"/>
@@ -54730,8 +54773,8 @@
       </c>
     </row>
     <row r="889">
-      <c r="A889" s="81"/>
-      <c r="B889" s="82"/>
+      <c r="A889" s="80"/>
+      <c r="B889" s="81"/>
       <c r="C889" s="34"/>
       <c r="D889" s="34"/>
       <c r="E889" s="34"/>
@@ -54756,8 +54799,8 @@
       </c>
     </row>
     <row r="890">
-      <c r="A890" s="81"/>
-      <c r="B890" s="82"/>
+      <c r="A890" s="80"/>
+      <c r="B890" s="81"/>
       <c r="C890" s="34"/>
       <c r="D890" s="34"/>
       <c r="E890" s="34"/>
@@ -54782,8 +54825,8 @@
       </c>
     </row>
     <row r="891">
-      <c r="A891" s="81"/>
-      <c r="B891" s="82"/>
+      <c r="A891" s="80"/>
+      <c r="B891" s="81"/>
       <c r="C891" s="34"/>
       <c r="D891" s="34"/>
       <c r="E891" s="34"/>
@@ -54808,8 +54851,8 @@
       </c>
     </row>
     <row r="892">
-      <c r="A892" s="81"/>
-      <c r="B892" s="82"/>
+      <c r="A892" s="80"/>
+      <c r="B892" s="81"/>
       <c r="C892" s="34"/>
       <c r="D892" s="34"/>
       <c r="E892" s="34"/>
@@ -54834,8 +54877,8 @@
       </c>
     </row>
     <row r="893">
-      <c r="A893" s="81"/>
-      <c r="B893" s="82"/>
+      <c r="A893" s="80"/>
+      <c r="B893" s="81"/>
       <c r="C893" s="34"/>
       <c r="D893" s="34"/>
       <c r="E893" s="34"/>
@@ -54860,8 +54903,8 @@
       </c>
     </row>
     <row r="894">
-      <c r="A894" s="81"/>
-      <c r="B894" s="82"/>
+      <c r="A894" s="80"/>
+      <c r="B894" s="81"/>
       <c r="C894" s="34"/>
       <c r="D894" s="34"/>
       <c r="E894" s="34"/>
@@ -54886,8 +54929,8 @@
       </c>
     </row>
     <row r="895">
-      <c r="A895" s="81"/>
-      <c r="B895" s="82"/>
+      <c r="A895" s="80"/>
+      <c r="B895" s="81"/>
       <c r="C895" s="34"/>
       <c r="D895" s="34"/>
       <c r="E895" s="34"/>
@@ -54912,8 +54955,8 @@
       </c>
     </row>
     <row r="896">
-      <c r="A896" s="81"/>
-      <c r="B896" s="82"/>
+      <c r="A896" s="80"/>
+      <c r="B896" s="81"/>
       <c r="C896" s="34"/>
       <c r="D896" s="34"/>
       <c r="E896" s="34"/>
@@ -54938,8 +54981,8 @@
       </c>
     </row>
     <row r="897">
-      <c r="A897" s="81"/>
-      <c r="B897" s="82"/>
+      <c r="A897" s="80"/>
+      <c r="B897" s="81"/>
       <c r="C897" s="34"/>
       <c r="D897" s="34"/>
       <c r="E897" s="34"/>
@@ -54964,8 +55007,8 @@
       </c>
     </row>
     <row r="898">
-      <c r="A898" s="81"/>
-      <c r="B898" s="82"/>
+      <c r="A898" s="80"/>
+      <c r="B898" s="81"/>
       <c r="C898" s="34"/>
       <c r="D898" s="34"/>
       <c r="E898" s="34"/>
@@ -54990,8 +55033,8 @@
       </c>
     </row>
     <row r="899">
-      <c r="A899" s="81"/>
-      <c r="B899" s="82"/>
+      <c r="A899" s="80"/>
+      <c r="B899" s="81"/>
       <c r="C899" s="34"/>
       <c r="D899" s="34"/>
       <c r="E899" s="34"/>
@@ -55016,8 +55059,8 @@
       </c>
     </row>
     <row r="900">
-      <c r="A900" s="81"/>
-      <c r="B900" s="82"/>
+      <c r="A900" s="80"/>
+      <c r="B900" s="81"/>
       <c r="C900" s="34"/>
       <c r="D900" s="34"/>
       <c r="E900" s="34"/>
@@ -55042,8 +55085,8 @@
       </c>
     </row>
     <row r="901">
-      <c r="A901" s="81"/>
-      <c r="B901" s="82"/>
+      <c r="A901" s="80"/>
+      <c r="B901" s="81"/>
       <c r="C901" s="34"/>
       <c r="D901" s="34"/>
       <c r="E901" s="34"/>
@@ -55068,8 +55111,8 @@
       </c>
     </row>
     <row r="902">
-      <c r="A902" s="81"/>
-      <c r="B902" s="82"/>
+      <c r="A902" s="80"/>
+      <c r="B902" s="81"/>
       <c r="C902" s="34"/>
       <c r="D902" s="34"/>
       <c r="E902" s="34"/>
@@ -55094,8 +55137,8 @@
       </c>
     </row>
     <row r="903">
-      <c r="A903" s="81"/>
-      <c r="B903" s="82"/>
+      <c r="A903" s="80"/>
+      <c r="B903" s="81"/>
       <c r="C903" s="34"/>
       <c r="D903" s="34"/>
       <c r="E903" s="34"/>
@@ -55120,8 +55163,8 @@
       </c>
     </row>
     <row r="904">
-      <c r="A904" s="81"/>
-      <c r="B904" s="82"/>
+      <c r="A904" s="80"/>
+      <c r="B904" s="81"/>
       <c r="C904" s="34"/>
       <c r="D904" s="34"/>
       <c r="E904" s="34"/>
@@ -55146,8 +55189,8 @@
       </c>
     </row>
     <row r="905">
-      <c r="A905" s="81"/>
-      <c r="B905" s="82"/>
+      <c r="A905" s="80"/>
+      <c r="B905" s="81"/>
       <c r="C905" s="34"/>
       <c r="D905" s="34"/>
       <c r="E905" s="34"/>
@@ -55172,8 +55215,8 @@
       </c>
     </row>
     <row r="906">
-      <c r="A906" s="81"/>
-      <c r="B906" s="82"/>
+      <c r="A906" s="80"/>
+      <c r="B906" s="81"/>
       <c r="C906" s="34"/>
       <c r="D906" s="34"/>
       <c r="E906" s="34"/>
@@ -55198,8 +55241,8 @@
       </c>
     </row>
     <row r="907">
-      <c r="A907" s="81"/>
-      <c r="B907" s="82"/>
+      <c r="A907" s="80"/>
+      <c r="B907" s="81"/>
       <c r="C907" s="34"/>
       <c r="D907" s="34"/>
       <c r="E907" s="34"/>
@@ -55224,8 +55267,8 @@
       </c>
     </row>
     <row r="908">
-      <c r="A908" s="81"/>
-      <c r="B908" s="82"/>
+      <c r="A908" s="80"/>
+      <c r="B908" s="81"/>
       <c r="C908" s="34"/>
       <c r="D908" s="34"/>
       <c r="E908" s="34"/>
@@ -55250,8 +55293,8 @@
       </c>
     </row>
     <row r="909">
-      <c r="A909" s="81"/>
-      <c r="B909" s="82"/>
+      <c r="A909" s="80"/>
+      <c r="B909" s="81"/>
       <c r="C909" s="34"/>
       <c r="D909" s="34"/>
       <c r="E909" s="34"/>
@@ -55276,8 +55319,8 @@
       </c>
     </row>
     <row r="910">
-      <c r="A910" s="81"/>
-      <c r="B910" s="82"/>
+      <c r="A910" s="80"/>
+      <c r="B910" s="81"/>
       <c r="C910" s="34"/>
       <c r="D910" s="34"/>
       <c r="E910" s="34"/>
@@ -55302,8 +55345,8 @@
       </c>
     </row>
     <row r="911">
-      <c r="A911" s="81"/>
-      <c r="B911" s="82"/>
+      <c r="A911" s="80"/>
+      <c r="B911" s="81"/>
       <c r="C911" s="34"/>
       <c r="D911" s="34"/>
       <c r="E911" s="34"/>
@@ -55328,8 +55371,8 @@
       </c>
     </row>
     <row r="912">
-      <c r="A912" s="81"/>
-      <c r="B912" s="82"/>
+      <c r="A912" s="80"/>
+      <c r="B912" s="81"/>
       <c r="C912" s="34"/>
       <c r="D912" s="34"/>
       <c r="E912" s="34"/>
@@ -55354,8 +55397,8 @@
       </c>
     </row>
     <row r="913">
-      <c r="A913" s="81"/>
-      <c r="B913" s="82"/>
+      <c r="A913" s="80"/>
+      <c r="B913" s="81"/>
       <c r="C913" s="34"/>
       <c r="D913" s="34"/>
       <c r="E913" s="34"/>
@@ -55380,8 +55423,8 @@
       </c>
     </row>
     <row r="914">
-      <c r="A914" s="81"/>
-      <c r="B914" s="82"/>
+      <c r="A914" s="80"/>
+      <c r="B914" s="81"/>
       <c r="C914" s="34"/>
       <c r="D914" s="34"/>
       <c r="E914" s="34"/>
@@ -55406,8 +55449,8 @@
       </c>
     </row>
     <row r="915">
-      <c r="A915" s="81"/>
-      <c r="B915" s="82"/>
+      <c r="A915" s="80"/>
+      <c r="B915" s="81"/>
       <c r="C915" s="34"/>
       <c r="D915" s="34"/>
       <c r="E915" s="34"/>
@@ -55432,8 +55475,8 @@
       </c>
     </row>
     <row r="916">
-      <c r="A916" s="81"/>
-      <c r="B916" s="82"/>
+      <c r="A916" s="80"/>
+      <c r="B916" s="81"/>
       <c r="C916" s="34"/>
       <c r="D916" s="34"/>
       <c r="E916" s="34"/>
@@ -55458,8 +55501,8 @@
       </c>
     </row>
     <row r="917">
-      <c r="A917" s="81"/>
-      <c r="B917" s="82"/>
+      <c r="A917" s="80"/>
+      <c r="B917" s="81"/>
       <c r="C917" s="34"/>
       <c r="D917" s="34"/>
       <c r="E917" s="34"/>
@@ -55484,8 +55527,8 @@
       </c>
     </row>
     <row r="918">
-      <c r="A918" s="81"/>
-      <c r="B918" s="82"/>
+      <c r="A918" s="80"/>
+      <c r="B918" s="81"/>
       <c r="C918" s="34"/>
       <c r="D918" s="34"/>
       <c r="E918" s="34"/>
@@ -55510,8 +55553,8 @@
       </c>
     </row>
     <row r="919">
-      <c r="A919" s="81"/>
-      <c r="B919" s="82"/>
+      <c r="A919" s="80"/>
+      <c r="B919" s="81"/>
       <c r="C919" s="34"/>
       <c r="D919" s="34"/>
       <c r="E919" s="34"/>
@@ -55536,8 +55579,8 @@
       </c>
     </row>
     <row r="920">
-      <c r="A920" s="81"/>
-      <c r="B920" s="82"/>
+      <c r="A920" s="80"/>
+      <c r="B920" s="81"/>
       <c r="C920" s="34"/>
       <c r="D920" s="34"/>
       <c r="E920" s="34"/>
@@ -55562,8 +55605,8 @@
       </c>
     </row>
     <row r="921">
-      <c r="A921" s="81"/>
-      <c r="B921" s="82"/>
+      <c r="A921" s="80"/>
+      <c r="B921" s="81"/>
       <c r="C921" s="34"/>
       <c r="D921" s="34"/>
       <c r="E921" s="34"/>
@@ -55588,8 +55631,8 @@
       </c>
     </row>
     <row r="922">
-      <c r="A922" s="81"/>
-      <c r="B922" s="82"/>
+      <c r="A922" s="80"/>
+      <c r="B922" s="81"/>
       <c r="C922" s="34"/>
       <c r="D922" s="34"/>
       <c r="E922" s="34"/>
@@ -55614,8 +55657,8 @@
       </c>
     </row>
     <row r="923">
-      <c r="A923" s="81"/>
-      <c r="B923" s="82"/>
+      <c r="A923" s="80"/>
+      <c r="B923" s="81"/>
       <c r="C923" s="34"/>
       <c r="D923" s="34"/>
       <c r="E923" s="34"/>
@@ -55640,8 +55683,8 @@
       </c>
     </row>
     <row r="924">
-      <c r="A924" s="81"/>
-      <c r="B924" s="82"/>
+      <c r="A924" s="80"/>
+      <c r="B924" s="81"/>
       <c r="C924" s="34"/>
       <c r="D924" s="34"/>
       <c r="E924" s="34"/>
@@ -55666,8 +55709,8 @@
       </c>
     </row>
     <row r="925">
-      <c r="A925" s="81"/>
-      <c r="B925" s="82"/>
+      <c r="A925" s="80"/>
+      <c r="B925" s="81"/>
       <c r="C925" s="34"/>
       <c r="D925" s="34"/>
       <c r="E925" s="34"/>
@@ -55692,8 +55735,8 @@
       </c>
     </row>
     <row r="926">
-      <c r="A926" s="81"/>
-      <c r="B926" s="82"/>
+      <c r="A926" s="80"/>
+      <c r="B926" s="81"/>
       <c r="C926" s="34"/>
       <c r="D926" s="34"/>
       <c r="E926" s="34"/>
@@ -55718,8 +55761,8 @@
       </c>
     </row>
     <row r="927">
-      <c r="A927" s="81"/>
-      <c r="B927" s="82"/>
+      <c r="A927" s="80"/>
+      <c r="B927" s="81"/>
       <c r="C927" s="34"/>
       <c r="D927" s="34"/>
       <c r="E927" s="34"/>
@@ -55744,8 +55787,8 @@
       </c>
     </row>
     <row r="928">
-      <c r="A928" s="81"/>
-      <c r="B928" s="82"/>
+      <c r="A928" s="80"/>
+      <c r="B928" s="81"/>
       <c r="C928" s="34"/>
       <c r="D928" s="34"/>
       <c r="E928" s="34"/>
@@ -55770,8 +55813,8 @@
       </c>
     </row>
     <row r="929">
-      <c r="A929" s="81"/>
-      <c r="B929" s="82"/>
+      <c r="A929" s="80"/>
+      <c r="B929" s="81"/>
       <c r="C929" s="34"/>
       <c r="D929" s="34"/>
       <c r="E929" s="34"/>
@@ -55796,8 +55839,8 @@
       </c>
     </row>
     <row r="930">
-      <c r="A930" s="81"/>
-      <c r="B930" s="82"/>
+      <c r="A930" s="80"/>
+      <c r="B930" s="81"/>
       <c r="C930" s="34"/>
       <c r="D930" s="34"/>
       <c r="E930" s="34"/>
@@ -55822,8 +55865,8 @@
       </c>
     </row>
     <row r="931">
-      <c r="A931" s="81"/>
-      <c r="B931" s="82"/>
+      <c r="A931" s="80"/>
+      <c r="B931" s="81"/>
       <c r="C931" s="34"/>
       <c r="D931" s="34"/>
       <c r="E931" s="34"/>
@@ -55848,8 +55891,8 @@
       </c>
     </row>
     <row r="932">
-      <c r="A932" s="81"/>
-      <c r="B932" s="82"/>
+      <c r="A932" s="80"/>
+      <c r="B932" s="81"/>
       <c r="C932" s="34"/>
       <c r="D932" s="34"/>
       <c r="E932" s="34"/>
@@ -55874,8 +55917,8 @@
       </c>
     </row>
     <row r="933">
-      <c r="A933" s="81"/>
-      <c r="B933" s="82"/>
+      <c r="A933" s="80"/>
+      <c r="B933" s="81"/>
       <c r="C933" s="34"/>
       <c r="D933" s="34"/>
       <c r="E933" s="34"/>
@@ -55900,8 +55943,8 @@
       </c>
     </row>
     <row r="934">
-      <c r="A934" s="81"/>
-      <c r="B934" s="82"/>
+      <c r="A934" s="80"/>
+      <c r="B934" s="81"/>
       <c r="C934" s="34"/>
       <c r="D934" s="34"/>
       <c r="E934" s="34"/>
@@ -55926,8 +55969,8 @@
       </c>
     </row>
     <row r="935">
-      <c r="A935" s="81"/>
-      <c r="B935" s="82"/>
+      <c r="A935" s="80"/>
+      <c r="B935" s="81"/>
       <c r="C935" s="34"/>
       <c r="D935" s="34"/>
       <c r="E935" s="34"/>
@@ -55952,8 +55995,8 @@
       </c>
     </row>
     <row r="936">
-      <c r="A936" s="81"/>
-      <c r="B936" s="82"/>
+      <c r="A936" s="80"/>
+      <c r="B936" s="81"/>
       <c r="C936" s="34"/>
       <c r="D936" s="34"/>
       <c r="E936" s="34"/>
@@ -55978,8 +56021,8 @@
       </c>
     </row>
     <row r="937">
-      <c r="A937" s="81"/>
-      <c r="B937" s="82"/>
+      <c r="A937" s="80"/>
+      <c r="B937" s="81"/>
       <c r="C937" s="34"/>
       <c r="D937" s="34"/>
       <c r="E937" s="34"/>
@@ -56004,8 +56047,8 @@
       </c>
     </row>
     <row r="938">
-      <c r="A938" s="81"/>
-      <c r="B938" s="82"/>
+      <c r="A938" s="80"/>
+      <c r="B938" s="81"/>
       <c r="C938" s="34"/>
       <c r="D938" s="34"/>
       <c r="E938" s="34"/>
@@ -56030,8 +56073,8 @@
       </c>
     </row>
     <row r="939">
-      <c r="A939" s="81"/>
-      <c r="B939" s="82"/>
+      <c r="A939" s="80"/>
+      <c r="B939" s="81"/>
       <c r="C939" s="34"/>
       <c r="D939" s="34"/>
       <c r="E939" s="34"/>
@@ -56056,8 +56099,8 @@
       </c>
     </row>
     <row r="940">
-      <c r="A940" s="81"/>
-      <c r="B940" s="82"/>
+      <c r="A940" s="80"/>
+      <c r="B940" s="81"/>
       <c r="C940" s="34"/>
       <c r="D940" s="34"/>
       <c r="E940" s="34"/>
@@ -56082,8 +56125,8 @@
       </c>
     </row>
     <row r="941">
-      <c r="A941" s="81"/>
-      <c r="B941" s="82"/>
+      <c r="A941" s="80"/>
+      <c r="B941" s="81"/>
       <c r="C941" s="34"/>
       <c r="D941" s="34"/>
       <c r="E941" s="34"/>
@@ -56108,8 +56151,8 @@
       </c>
     </row>
     <row r="942">
-      <c r="A942" s="81"/>
-      <c r="B942" s="82"/>
+      <c r="A942" s="80"/>
+      <c r="B942" s="81"/>
       <c r="C942" s="34"/>
       <c r="D942" s="34"/>
       <c r="E942" s="34"/>
@@ -56134,8 +56177,8 @@
       </c>
     </row>
     <row r="943">
-      <c r="A943" s="81"/>
-      <c r="B943" s="82"/>
+      <c r="A943" s="80"/>
+      <c r="B943" s="81"/>
       <c r="C943" s="34"/>
       <c r="D943" s="34"/>
       <c r="E943" s="34"/>
@@ -56160,8 +56203,8 @@
       </c>
     </row>
     <row r="944">
-      <c r="A944" s="81"/>
-      <c r="B944" s="82"/>
+      <c r="A944" s="80"/>
+      <c r="B944" s="81"/>
       <c r="C944" s="34"/>
       <c r="D944" s="34"/>
       <c r="E944" s="34"/>
@@ -56186,8 +56229,8 @@
       </c>
     </row>
     <row r="945">
-      <c r="A945" s="81"/>
-      <c r="B945" s="82"/>
+      <c r="A945" s="80"/>
+      <c r="B945" s="81"/>
       <c r="C945" s="34"/>
       <c r="D945" s="34"/>
       <c r="E945" s="34"/>
@@ -56212,8 +56255,8 @@
       </c>
     </row>
     <row r="946">
-      <c r="A946" s="81"/>
-      <c r="B946" s="82"/>
+      <c r="A946" s="80"/>
+      <c r="B946" s="81"/>
       <c r="C946" s="34"/>
       <c r="D946" s="34"/>
       <c r="E946" s="34"/>
@@ -56238,8 +56281,8 @@
       </c>
     </row>
     <row r="947">
-      <c r="A947" s="81"/>
-      <c r="B947" s="82"/>
+      <c r="A947" s="80"/>
+      <c r="B947" s="81"/>
       <c r="C947" s="34"/>
       <c r="D947" s="34"/>
       <c r="E947" s="34"/>
@@ -56264,8 +56307,8 @@
       </c>
     </row>
     <row r="948">
-      <c r="A948" s="81"/>
-      <c r="B948" s="82"/>
+      <c r="A948" s="80"/>
+      <c r="B948" s="81"/>
       <c r="C948" s="34"/>
       <c r="D948" s="34"/>
       <c r="E948" s="34"/>
@@ -56290,8 +56333,8 @@
       </c>
     </row>
     <row r="949">
-      <c r="A949" s="81"/>
-      <c r="B949" s="82"/>
+      <c r="A949" s="80"/>
+      <c r="B949" s="81"/>
       <c r="C949" s="34"/>
       <c r="D949" s="34"/>
       <c r="E949" s="34"/>
@@ -56316,8 +56359,8 @@
       </c>
     </row>
     <row r="950">
-      <c r="A950" s="81"/>
-      <c r="B950" s="82"/>
+      <c r="A950" s="80"/>
+      <c r="B950" s="81"/>
       <c r="C950" s="34"/>
       <c r="D950" s="34"/>
       <c r="E950" s="34"/>
@@ -56342,8 +56385,8 @@
       </c>
     </row>
     <row r="951">
-      <c r="A951" s="81"/>
-      <c r="B951" s="82"/>
+      <c r="A951" s="80"/>
+      <c r="B951" s="81"/>
       <c r="C951" s="34"/>
       <c r="D951" s="34"/>
       <c r="E951" s="34"/>
@@ -56368,8 +56411,8 @@
       </c>
     </row>
     <row r="952">
-      <c r="A952" s="81"/>
-      <c r="B952" s="82"/>
+      <c r="A952" s="80"/>
+      <c r="B952" s="81"/>
       <c r="C952" s="34"/>
       <c r="D952" s="34"/>
       <c r="E952" s="34"/>
@@ -56394,8 +56437,8 @@
       </c>
     </row>
     <row r="953">
-      <c r="A953" s="81"/>
-      <c r="B953" s="82"/>
+      <c r="A953" s="80"/>
+      <c r="B953" s="81"/>
       <c r="C953" s="34"/>
       <c r="D953" s="34"/>
       <c r="E953" s="34"/>
@@ -56420,8 +56463,8 @@
       </c>
     </row>
     <row r="954">
-      <c r="A954" s="81"/>
-      <c r="B954" s="82"/>
+      <c r="A954" s="80"/>
+      <c r="B954" s="81"/>
       <c r="C954" s="34"/>
       <c r="D954" s="34"/>
       <c r="E954" s="34"/>
@@ -56446,8 +56489,8 @@
       </c>
     </row>
     <row r="955">
-      <c r="A955" s="81"/>
-      <c r="B955" s="82"/>
+      <c r="A955" s="80"/>
+      <c r="B955" s="81"/>
       <c r="C955" s="34"/>
       <c r="D955" s="34"/>
       <c r="E955" s="34"/>
@@ -56472,8 +56515,8 @@
       </c>
     </row>
     <row r="956">
-      <c r="A956" s="81"/>
-      <c r="B956" s="82"/>
+      <c r="A956" s="80"/>
+      <c r="B956" s="81"/>
       <c r="C956" s="34"/>
       <c r="D956" s="34"/>
       <c r="E956" s="34"/>
@@ -56498,8 +56541,8 @@
       </c>
     </row>
     <row r="957">
-      <c r="A957" s="81"/>
-      <c r="B957" s="82"/>
+      <c r="A957" s="80"/>
+      <c r="B957" s="81"/>
       <c r="C957" s="34"/>
       <c r="D957" s="34"/>
       <c r="E957" s="34"/>
@@ -56524,8 +56567,8 @@
       </c>
     </row>
     <row r="958">
-      <c r="A958" s="81"/>
-      <c r="B958" s="82"/>
+      <c r="A958" s="80"/>
+      <c r="B958" s="81"/>
       <c r="C958" s="34"/>
       <c r="D958" s="34"/>
       <c r="E958" s="34"/>
@@ -56550,8 +56593,8 @@
       </c>
     </row>
     <row r="959">
-      <c r="A959" s="81"/>
-      <c r="B959" s="82"/>
+      <c r="A959" s="80"/>
+      <c r="B959" s="81"/>
       <c r="C959" s="34"/>
       <c r="D959" s="34"/>
       <c r="E959" s="34"/>
@@ -56576,8 +56619,8 @@
       </c>
     </row>
     <row r="960">
-      <c r="A960" s="81"/>
-      <c r="B960" s="82"/>
+      <c r="A960" s="80"/>
+      <c r="B960" s="81"/>
       <c r="C960" s="34"/>
       <c r="D960" s="34"/>
       <c r="E960" s="34"/>
@@ -56602,8 +56645,8 @@
       </c>
     </row>
     <row r="961">
-      <c r="A961" s="81"/>
-      <c r="B961" s="82"/>
+      <c r="A961" s="80"/>
+      <c r="B961" s="81"/>
       <c r="C961" s="34"/>
       <c r="D961" s="34"/>
       <c r="E961" s="34"/>
@@ -56628,8 +56671,8 @@
       </c>
     </row>
     <row r="962">
-      <c r="A962" s="81"/>
-      <c r="B962" s="82"/>
+      <c r="A962" s="80"/>
+      <c r="B962" s="81"/>
       <c r="C962" s="34"/>
       <c r="D962" s="34"/>
       <c r="E962" s="34"/>
@@ -56654,8 +56697,8 @@
       </c>
     </row>
     <row r="963">
-      <c r="A963" s="81"/>
-      <c r="B963" s="82"/>
+      <c r="A963" s="80"/>
+      <c r="B963" s="81"/>
       <c r="C963" s="34"/>
       <c r="D963" s="34"/>
       <c r="E963" s="34"/>
@@ -56680,8 +56723,8 @@
       </c>
     </row>
     <row r="964">
-      <c r="A964" s="81"/>
-      <c r="B964" s="82"/>
+      <c r="A964" s="80"/>
+      <c r="B964" s="81"/>
       <c r="C964" s="34"/>
       <c r="D964" s="34"/>
       <c r="E964" s="34"/>
@@ -56706,8 +56749,8 @@
       </c>
     </row>
     <row r="965">
-      <c r="A965" s="81"/>
-      <c r="B965" s="82"/>
+      <c r="A965" s="80"/>
+      <c r="B965" s="81"/>
       <c r="C965" s="34"/>
       <c r="D965" s="34"/>
       <c r="E965" s="34"/>
@@ -56732,8 +56775,8 @@
       </c>
     </row>
     <row r="966">
-      <c r="A966" s="81"/>
-      <c r="B966" s="82"/>
+      <c r="A966" s="80"/>
+      <c r="B966" s="81"/>
       <c r="C966" s="34"/>
       <c r="D966" s="34"/>
       <c r="E966" s="34"/>
@@ -56758,8 +56801,8 @@
       </c>
     </row>
     <row r="967">
-      <c r="A967" s="81"/>
-      <c r="B967" s="82"/>
+      <c r="A967" s="80"/>
+      <c r="B967" s="81"/>
       <c r="C967" s="34"/>
       <c r="D967" s="34"/>
       <c r="E967" s="34"/>
@@ -56784,8 +56827,8 @@
       </c>
     </row>
     <row r="968">
-      <c r="A968" s="81"/>
-      <c r="B968" s="82"/>
+      <c r="A968" s="80"/>
+      <c r="B968" s="81"/>
       <c r="C968" s="34"/>
       <c r="D968" s="34"/>
       <c r="E968" s="34"/>
@@ -56810,8 +56853,8 @@
       </c>
     </row>
     <row r="969">
-      <c r="A969" s="81"/>
-      <c r="B969" s="82"/>
+      <c r="A969" s="80"/>
+      <c r="B969" s="81"/>
       <c r="C969" s="34"/>
       <c r="D969" s="34"/>
       <c r="E969" s="34"/>
@@ -56836,8 +56879,8 @@
       </c>
     </row>
     <row r="970">
-      <c r="A970" s="81"/>
-      <c r="B970" s="82"/>
+      <c r="A970" s="80"/>
+      <c r="B970" s="81"/>
       <c r="C970" s="34"/>
       <c r="D970" s="34"/>
       <c r="E970" s="34"/>
@@ -56862,8 +56905,8 @@
       </c>
     </row>
     <row r="971">
-      <c r="A971" s="81"/>
-      <c r="B971" s="82"/>
+      <c r="A971" s="80"/>
+      <c r="B971" s="81"/>
       <c r="C971" s="34"/>
       <c r="D971" s="34"/>
       <c r="E971" s="34"/>
@@ -56888,8 +56931,8 @@
       </c>
     </row>
     <row r="972">
-      <c r="A972" s="81"/>
-      <c r="B972" s="82"/>
+      <c r="A972" s="80"/>
+      <c r="B972" s="81"/>
       <c r="C972" s="34"/>
       <c r="D972" s="34"/>
       <c r="E972" s="34"/>
@@ -56914,8 +56957,8 @@
       </c>
     </row>
     <row r="973">
-      <c r="A973" s="81"/>
-      <c r="B973" s="82"/>
+      <c r="A973" s="80"/>
+      <c r="B973" s="81"/>
       <c r="C973" s="34"/>
       <c r="D973" s="34"/>
       <c r="E973" s="34"/>
@@ -56940,8 +56983,8 @@
       </c>
     </row>
     <row r="974">
-      <c r="A974" s="81"/>
-      <c r="B974" s="82"/>
+      <c r="A974" s="80"/>
+      <c r="B974" s="81"/>
       <c r="C974" s="34"/>
       <c r="D974" s="34"/>
       <c r="E974" s="34"/>
@@ -56966,8 +57009,8 @@
       </c>
     </row>
     <row r="975">
-      <c r="A975" s="81"/>
-      <c r="B975" s="82"/>
+      <c r="A975" s="80"/>
+      <c r="B975" s="81"/>
       <c r="C975" s="34"/>
       <c r="D975" s="34"/>
       <c r="E975" s="34"/>
@@ -56992,8 +57035,8 @@
       </c>
     </row>
     <row r="976">
-      <c r="A976" s="81"/>
-      <c r="B976" s="82"/>
+      <c r="A976" s="80"/>
+      <c r="B976" s="81"/>
       <c r="C976" s="34"/>
       <c r="D976" s="34"/>
       <c r="E976" s="34"/>
@@ -57018,8 +57061,8 @@
       </c>
     </row>
     <row r="977">
-      <c r="A977" s="81"/>
-      <c r="B977" s="82"/>
+      <c r="A977" s="80"/>
+      <c r="B977" s="81"/>
       <c r="C977" s="34"/>
       <c r="D977" s="34"/>
       <c r="E977" s="34"/>
@@ -57044,8 +57087,8 @@
       </c>
     </row>
     <row r="978">
-      <c r="A978" s="81"/>
-      <c r="B978" s="82"/>
+      <c r="A978" s="80"/>
+      <c r="B978" s="81"/>
       <c r="C978" s="34"/>
       <c r="D978" s="34"/>
       <c r="E978" s="34"/>
@@ -57070,8 +57113,8 @@
       </c>
     </row>
     <row r="979">
-      <c r="A979" s="81"/>
-      <c r="B979" s="82"/>
+      <c r="A979" s="80"/>
+      <c r="B979" s="81"/>
       <c r="C979" s="34"/>
       <c r="D979" s="34"/>
       <c r="E979" s="34"/>
@@ -57096,8 +57139,8 @@
       </c>
     </row>
     <row r="980">
-      <c r="A980" s="81"/>
-      <c r="B980" s="82"/>
+      <c r="A980" s="80"/>
+      <c r="B980" s="81"/>
       <c r="C980" s="34"/>
       <c r="D980" s="34"/>
       <c r="E980" s="34"/>
@@ -57122,8 +57165,8 @@
       </c>
     </row>
     <row r="981">
-      <c r="A981" s="81"/>
-      <c r="B981" s="82"/>
+      <c r="A981" s="80"/>
+      <c r="B981" s="81"/>
       <c r="C981" s="34"/>
       <c r="D981" s="34"/>
       <c r="E981" s="34"/>
@@ -57148,8 +57191,8 @@
       </c>
     </row>
     <row r="982">
-      <c r="A982" s="81"/>
-      <c r="B982" s="82"/>
+      <c r="A982" s="80"/>
+      <c r="B982" s="81"/>
       <c r="C982" s="34"/>
       <c r="D982" s="34"/>
       <c r="E982" s="34"/>
@@ -57174,8 +57217,8 @@
       </c>
     </row>
     <row r="983">
-      <c r="A983" s="81"/>
-      <c r="B983" s="82"/>
+      <c r="A983" s="80"/>
+      <c r="B983" s="81"/>
       <c r="C983" s="34"/>
       <c r="D983" s="34"/>
       <c r="E983" s="34"/>
@@ -57200,8 +57243,8 @@
       </c>
     </row>
     <row r="984">
-      <c r="A984" s="81"/>
-      <c r="B984" s="82"/>
+      <c r="A984" s="80"/>
+      <c r="B984" s="81"/>
       <c r="C984" s="34"/>
       <c r="D984" s="34"/>
       <c r="E984" s="34"/>
@@ -57226,8 +57269,8 @@
       </c>
     </row>
     <row r="985">
-      <c r="A985" s="81"/>
-      <c r="B985" s="82"/>
+      <c r="A985" s="80"/>
+      <c r="B985" s="81"/>
       <c r="C985" s="34"/>
       <c r="D985" s="34"/>
       <c r="E985" s="34"/>
@@ -57252,8 +57295,8 @@
       </c>
     </row>
     <row r="986">
-      <c r="A986" s="81"/>
-      <c r="B986" s="82"/>
+      <c r="A986" s="80"/>
+      <c r="B986" s="81"/>
       <c r="C986" s="34"/>
       <c r="D986" s="34"/>
       <c r="E986" s="34"/>
@@ -57278,8 +57321,8 @@
       </c>
     </row>
     <row r="987">
-      <c r="A987" s="81"/>
-      <c r="B987" s="82"/>
+      <c r="A987" s="80"/>
+      <c r="B987" s="81"/>
       <c r="C987" s="34"/>
       <c r="D987" s="34"/>
       <c r="E987" s="34"/>
@@ -57304,8 +57347,8 @@
       </c>
     </row>
     <row r="988">
-      <c r="A988" s="81"/>
-      <c r="B988" s="82"/>
+      <c r="A988" s="80"/>
+      <c r="B988" s="81"/>
       <c r="C988" s="34"/>
       <c r="D988" s="34"/>
       <c r="E988" s="34"/>
@@ -57330,8 +57373,8 @@
       </c>
     </row>
     <row r="989">
-      <c r="A989" s="81"/>
-      <c r="B989" s="82"/>
+      <c r="A989" s="80"/>
+      <c r="B989" s="81"/>
       <c r="C989" s="34"/>
       <c r="D989" s="34"/>
       <c r="E989" s="34"/>
@@ -57356,8 +57399,8 @@
       </c>
     </row>
     <row r="990">
-      <c r="A990" s="81"/>
-      <c r="B990" s="82"/>
+      <c r="A990" s="80"/>
+      <c r="B990" s="81"/>
       <c r="C990" s="34"/>
       <c r="D990" s="34"/>
       <c r="E990" s="34"/>
@@ -57382,8 +57425,8 @@
       </c>
     </row>
     <row r="991">
-      <c r="A991" s="81"/>
-      <c r="B991" s="82"/>
+      <c r="A991" s="80"/>
+      <c r="B991" s="81"/>
       <c r="C991" s="34"/>
       <c r="D991" s="34"/>
       <c r="E991" s="34"/>
@@ -57408,8 +57451,8 @@
       </c>
     </row>
     <row r="992">
-      <c r="A992" s="81"/>
-      <c r="B992" s="82"/>
+      <c r="A992" s="80"/>
+      <c r="B992" s="81"/>
       <c r="C992" s="34"/>
       <c r="D992" s="34"/>
       <c r="E992" s="34"/>
@@ -57434,8 +57477,8 @@
       </c>
     </row>
     <row r="993">
-      <c r="A993" s="81"/>
-      <c r="B993" s="82"/>
+      <c r="A993" s="80"/>
+      <c r="B993" s="81"/>
       <c r="C993" s="34"/>
       <c r="D993" s="34"/>
       <c r="E993" s="34"/>
@@ -57460,8 +57503,8 @@
       </c>
     </row>
     <row r="994">
-      <c r="A994" s="81"/>
-      <c r="B994" s="82"/>
+      <c r="A994" s="80"/>
+      <c r="B994" s="81"/>
       <c r="C994" s="34"/>
       <c r="D994" s="34"/>
       <c r="E994" s="34"/>
@@ -57486,8 +57529,8 @@
       </c>
     </row>
     <row r="995">
-      <c r="A995" s="81"/>
-      <c r="B995" s="82"/>
+      <c r="A995" s="80"/>
+      <c r="B995" s="81"/>
       <c r="C995" s="34"/>
       <c r="D995" s="34"/>
       <c r="E995" s="34"/>
@@ -57512,8 +57555,8 @@
       </c>
     </row>
     <row r="996">
-      <c r="A996" s="81"/>
-      <c r="B996" s="82"/>
+      <c r="A996" s="80"/>
+      <c r="B996" s="81"/>
       <c r="C996" s="34"/>
       <c r="D996" s="34"/>
       <c r="E996" s="34"/>
@@ -57538,8 +57581,8 @@
       </c>
     </row>
     <row r="997">
-      <c r="A997" s="81"/>
-      <c r="B997" s="82"/>
+      <c r="A997" s="80"/>
+      <c r="B997" s="81"/>
       <c r="C997" s="34"/>
       <c r="D997" s="34"/>
       <c r="E997" s="34"/>
@@ -57564,8 +57607,8 @@
       </c>
     </row>
     <row r="998">
-      <c r="A998" s="81"/>
-      <c r="B998" s="82"/>
+      <c r="A998" s="80"/>
+      <c r="B998" s="81"/>
       <c r="C998" s="34"/>
       <c r="D998" s="34"/>
       <c r="E998" s="34"/>
@@ -57590,8 +57633,8 @@
       </c>
     </row>
     <row r="999">
-      <c r="A999" s="81"/>
-      <c r="B999" s="82"/>
+      <c r="A999" s="80"/>
+      <c r="B999" s="81"/>
       <c r="C999" s="34"/>
       <c r="D999" s="34"/>
       <c r="E999" s="34"/>
@@ -57616,8 +57659,8 @@
       </c>
     </row>
     <row r="1000">
-      <c r="A1000" s="81"/>
-      <c r="B1000" s="82"/>
+      <c r="A1000" s="80"/>
+      <c r="B1000" s="81"/>
       <c r="C1000" s="34"/>
       <c r="D1000" s="34"/>
       <c r="E1000" s="34"/>
@@ -57642,8 +57685,8 @@
       </c>
     </row>
     <row r="1001">
-      <c r="A1001" s="81"/>
-      <c r="B1001" s="82"/>
+      <c r="A1001" s="80"/>
+      <c r="B1001" s="81"/>
       <c r="C1001" s="34"/>
       <c r="D1001" s="34"/>
       <c r="E1001" s="34"/>
@@ -58298,15 +58341,16 @@
     <hyperlink r:id="rId248" ref="S685"/>
     <hyperlink r:id="rId249" ref="S686"/>
     <hyperlink r:id="rId250" ref="S687"/>
+    <hyperlink r:id="rId251" ref="S688"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId251"/>
-  <legacyDrawing r:id="rId252"/>
+  <drawing r:id="rId252"/>
+  <legacyDrawing r:id="rId253"/>
   <tableParts count="2">
-    <tablePart r:id="rId255"/>
     <tablePart r:id="rId256"/>
+    <tablePart r:id="rId257"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201205
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -571,7 +571,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7808" uniqueCount="2465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7866" uniqueCount="2485">
   <si>
     <t>案例</t>
   </si>
@@ -8912,6 +8912,69 @@
   <si>
     <t>女自美返臺探親，居家檢疫期間發病確診COVID-19</t>
   </si>
+  <si>
+    <t>#688</t>
+  </si>
+  <si>
+    <t>12/1 採檢
+12/4 確診</t>
+  </si>
+  <si>
+    <t>檢疫期滿前採檢為陰性。個案11月28日檢疫期滿後，由仲介安排至宿舍自主健康管理至11月30日，因雇主要求，於12月1日由仲介安排至醫院自費採檢</t>
+  </si>
+  <si>
+    <t>新增4例境外移入COVID-19病例，自印尼及美國入境</t>
+  </si>
+  <si>
+    <t>#689</t>
+  </si>
+  <si>
+    <t>-11/23 美國
+-11/30 美國→台灣</t>
+  </si>
+  <si>
+    <t>12/2 採檢
+12/4 確診</t>
+  </si>
+  <si>
+    <t>嗅覺喪失 味覺喪失</t>
+  </si>
+  <si>
+    <t>因工作於11月23日前往美國，因被毒蜘蛛咬傷，分別於11月27日及28日至當地醫院就醫，11月30日入境臺灣後前往防疫旅館居家檢疫。個案因咬傷部位不適情形未改善，分別於11月30日及12月2日由衛生單位安排就醫，並於12月2日收治住院隔離及採檢，個案12月3日出現嗅味覺喪失</t>
+  </si>
+  <si>
+    <t>#690</t>
+  </si>
+  <si>
+    <t>8月-11/30 美國</t>
+  </si>
+  <si>
+    <t>發冷 發燒 咳嗽</t>
+  </si>
+  <si>
+    <t>#691</t>
+  </si>
+  <si>
+    <t>9X</t>
+  </si>
+  <si>
+    <t>11月上旬-11/22 美國</t>
+  </si>
+  <si>
+    <t>全身倦怠 頭暈 發燒 肺炎</t>
+  </si>
+  <si>
+    <t>不定期於美國及臺灣兩地居住</t>
+  </si>
+  <si>
+    <t>#692</t>
+  </si>
+  <si>
+    <t>#693</t>
+  </si>
+  <si>
+    <t>#694</t>
+  </si>
 </sst>
 </file>
 
@@ -8921,7 +8984,7 @@
     <numFmt numFmtId="164" formatCode="mm&quot;月&quot;dd&quot;日 &quot;dddd"/>
     <numFmt numFmtId="165" formatCode="m/d"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="19">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -9006,10 +9069,6 @@
       <u/>
       <color rgb="FF0000FF"/>
     </font>
-    <font/>
-    <font>
-      <color rgb="FF000000"/>
-    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -9055,7 +9114,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="76">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -9277,24 +9336,6 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="19" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="20" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
@@ -49526,7 +49567,7 @@
       <c r="C688" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D688" s="74" t="s">
+      <c r="D688" s="7" t="s">
         <v>116</v>
       </c>
       <c r="E688" s="7" t="s">
@@ -49536,29 +49577,29 @@
       <c r="G688" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H688" s="75" t="s">
+      <c r="H688" s="8" t="s">
         <v>2461</v>
       </c>
-      <c r="I688" s="76">
+      <c r="I688" s="9">
         <v>44164.0</v>
       </c>
-      <c r="J688" s="77">
+      <c r="J688" s="10">
         <v>44164.0</v>
       </c>
-      <c r="K688" s="78" t="s">
+      <c r="K688" s="13" t="s">
         <v>2462</v>
       </c>
-      <c r="L688" s="79" t="s">
+      <c r="L688" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M688" s="78" t="s">
+      <c r="M688" s="13" t="s">
         <v>149</v>
       </c>
       <c r="N688" s="25"/>
-      <c r="O688" s="75" t="s">
+      <c r="O688" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P688" s="75" t="s">
+      <c r="P688" s="8" t="s">
         <v>2463</v>
       </c>
       <c r="Q688" s="19"/>
@@ -49573,117 +49614,243 @@
       </c>
     </row>
     <row r="689">
-      <c r="A689" s="80"/>
-      <c r="B689" s="81"/>
-      <c r="C689" s="34"/>
-      <c r="D689" s="34"/>
-      <c r="E689" s="34"/>
+      <c r="A689" s="16" t="s">
+        <v>2465</v>
+      </c>
+      <c r="B689" s="6">
+        <v>44169.0</v>
+      </c>
+      <c r="C689" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D689" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E689" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F689" s="34"/>
-      <c r="G689" s="34"/>
-      <c r="H689" s="21"/>
-      <c r="I689" s="19"/>
-      <c r="J689" s="10"/>
-      <c r="K689" s="22"/>
-      <c r="L689" s="23"/>
-      <c r="M689" s="22"/>
+      <c r="G689" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H689" s="8" t="s">
+        <v>2365</v>
+      </c>
+      <c r="I689" s="9">
+        <v>44148.0</v>
+      </c>
+      <c r="J689" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K689" s="13" t="s">
+        <v>2466</v>
+      </c>
+      <c r="L689" s="12" t="s">
+        <v>1674</v>
+      </c>
+      <c r="M689" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N689" s="25"/>
-      <c r="O689" s="21"/>
-      <c r="P689" s="21"/>
+      <c r="O689" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P689" s="8" t="s">
+        <v>2467</v>
+      </c>
       <c r="Q689" s="19"/>
       <c r="R689" s="19"/>
-      <c r="S689" s="20"/>
+      <c r="S689" s="61" t="s">
+        <v>2468</v>
+      </c>
       <c r="T689" s="20"/>
       <c r="U689" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#688</v>
       </c>
     </row>
     <row r="690">
-      <c r="A690" s="80"/>
-      <c r="B690" s="81"/>
-      <c r="C690" s="34"/>
-      <c r="D690" s="34"/>
-      <c r="E690" s="34"/>
+      <c r="A690" s="16" t="s">
+        <v>2469</v>
+      </c>
+      <c r="B690" s="6">
+        <v>44169.0</v>
+      </c>
+      <c r="C690" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D690" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E690" s="7" t="s">
+        <v>351</v>
+      </c>
       <c r="F690" s="34"/>
-      <c r="G690" s="34"/>
-      <c r="H690" s="21"/>
-      <c r="I690" s="19"/>
-      <c r="J690" s="10"/>
-      <c r="K690" s="22"/>
-      <c r="L690" s="23"/>
-      <c r="M690" s="22"/>
+      <c r="G690" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H690" s="8" t="s">
+        <v>2470</v>
+      </c>
+      <c r="I690" s="9">
+        <v>44165.0</v>
+      </c>
+      <c r="J690" s="10">
+        <v>44168.0</v>
+      </c>
+      <c r="K690" s="13" t="s">
+        <v>2471</v>
+      </c>
+      <c r="L690" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M690" s="13" t="s">
+        <v>2472</v>
+      </c>
       <c r="N690" s="25"/>
-      <c r="O690" s="21"/>
-      <c r="P690" s="21"/>
+      <c r="O690" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P690" s="8" t="s">
+        <v>2473</v>
+      </c>
       <c r="Q690" s="19"/>
       <c r="R690" s="19"/>
-      <c r="S690" s="20"/>
+      <c r="S690" s="61" t="s">
+        <v>2468</v>
+      </c>
       <c r="T690" s="20"/>
       <c r="U690" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#689</v>
       </c>
     </row>
     <row r="691">
-      <c r="A691" s="80"/>
-      <c r="B691" s="81"/>
-      <c r="C691" s="34"/>
-      <c r="D691" s="34"/>
-      <c r="E691" s="34"/>
+      <c r="A691" s="16" t="s">
+        <v>2474</v>
+      </c>
+      <c r="B691" s="6">
+        <v>44169.0</v>
+      </c>
+      <c r="C691" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D691" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E691" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F691" s="34"/>
-      <c r="G691" s="34"/>
-      <c r="H691" s="21"/>
-      <c r="I691" s="19"/>
-      <c r="J691" s="10"/>
-      <c r="K691" s="22"/>
-      <c r="L691" s="23"/>
-      <c r="M691" s="22"/>
+      <c r="G691" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H691" s="8" t="s">
+        <v>2475</v>
+      </c>
+      <c r="I691" s="9">
+        <v>44165.0</v>
+      </c>
+      <c r="J691" s="10">
+        <v>44166.0</v>
+      </c>
+      <c r="K691" s="13" t="s">
+        <v>2471</v>
+      </c>
+      <c r="L691" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M691" s="13" t="s">
+        <v>2476</v>
+      </c>
       <c r="N691" s="25"/>
-      <c r="O691" s="21"/>
-      <c r="P691" s="21"/>
+      <c r="O691" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P691" s="8" t="s">
+        <v>360</v>
+      </c>
       <c r="Q691" s="19"/>
       <c r="R691" s="19"/>
-      <c r="S691" s="20"/>
+      <c r="S691" s="61" t="s">
+        <v>2468</v>
+      </c>
       <c r="T691" s="20"/>
       <c r="U691" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#690</v>
       </c>
     </row>
     <row r="692">
-      <c r="A692" s="80"/>
-      <c r="B692" s="81"/>
-      <c r="C692" s="34"/>
-      <c r="D692" s="34"/>
-      <c r="E692" s="34"/>
+      <c r="A692" s="16" t="s">
+        <v>2477</v>
+      </c>
+      <c r="B692" s="6">
+        <v>44169.0</v>
+      </c>
+      <c r="C692" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D692" s="7" t="s">
+        <v>2478</v>
+      </c>
+      <c r="E692" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F692" s="34"/>
-      <c r="G692" s="34"/>
-      <c r="H692" s="21"/>
-      <c r="I692" s="19"/>
-      <c r="J692" s="10"/>
-      <c r="K692" s="22"/>
-      <c r="L692" s="23"/>
-      <c r="M692" s="22"/>
+      <c r="G692" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H692" s="8" t="s">
+        <v>2479</v>
+      </c>
+      <c r="I692" s="9">
+        <v>44157.0</v>
+      </c>
+      <c r="J692" s="10">
+        <v>44167.0</v>
+      </c>
+      <c r="K692" s="13" t="s">
+        <v>2471</v>
+      </c>
+      <c r="L692" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M692" s="13" t="s">
+        <v>2480</v>
+      </c>
       <c r="N692" s="25"/>
-      <c r="O692" s="21"/>
-      <c r="P692" s="21"/>
+      <c r="O692" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P692" s="8" t="s">
+        <v>2481</v>
+      </c>
       <c r="Q692" s="19"/>
       <c r="R692" s="19"/>
-      <c r="S692" s="20"/>
+      <c r="S692" s="61" t="s">
+        <v>2468</v>
+      </c>
       <c r="T692" s="20"/>
       <c r="U692" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#691</v>
       </c>
     </row>
     <row r="693">
-      <c r="A693" s="80"/>
-      <c r="B693" s="81"/>
+      <c r="A693" s="16" t="s">
+        <v>2482</v>
+      </c>
+      <c r="B693" s="6">
+        <v>44170.0</v>
+      </c>
       <c r="C693" s="34"/>
       <c r="D693" s="34"/>
       <c r="E693" s="34"/>
       <c r="F693" s="34"/>
-      <c r="G693" s="34"/>
+      <c r="G693" s="7" t="s">
+        <v>25</v>
+      </c>
       <c r="H693" s="21"/>
       <c r="I693" s="19"/>
       <c r="J693" s="10"/>
@@ -49691,7 +49858,9 @@
       <c r="L693" s="23"/>
       <c r="M693" s="22"/>
       <c r="N693" s="25"/>
-      <c r="O693" s="21"/>
+      <c r="O693" s="8" t="s">
+        <v>85</v>
+      </c>
       <c r="P693" s="21"/>
       <c r="Q693" s="19"/>
       <c r="R693" s="19"/>
@@ -49699,17 +49868,23 @@
       <c r="T693" s="20"/>
       <c r="U693" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#692</v>
       </c>
     </row>
     <row r="694">
-      <c r="A694" s="80"/>
-      <c r="B694" s="81"/>
+      <c r="A694" s="16" t="s">
+        <v>2483</v>
+      </c>
+      <c r="B694" s="6">
+        <v>44170.0</v>
+      </c>
       <c r="C694" s="34"/>
       <c r="D694" s="34"/>
       <c r="E694" s="34"/>
       <c r="F694" s="34"/>
-      <c r="G694" s="34"/>
+      <c r="G694" s="7" t="s">
+        <v>25</v>
+      </c>
       <c r="H694" s="21"/>
       <c r="I694" s="19"/>
       <c r="J694" s="10"/>
@@ -49717,7 +49892,9 @@
       <c r="L694" s="23"/>
       <c r="M694" s="22"/>
       <c r="N694" s="25"/>
-      <c r="O694" s="21"/>
+      <c r="O694" s="8" t="s">
+        <v>85</v>
+      </c>
       <c r="P694" s="21"/>
       <c r="Q694" s="19"/>
       <c r="R694" s="19"/>
@@ -49725,17 +49902,23 @@
       <c r="T694" s="20"/>
       <c r="U694" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#693</v>
       </c>
     </row>
     <row r="695">
-      <c r="A695" s="80"/>
-      <c r="B695" s="81"/>
+      <c r="A695" s="16" t="s">
+        <v>2484</v>
+      </c>
+      <c r="B695" s="6">
+        <v>44170.0</v>
+      </c>
       <c r="C695" s="34"/>
       <c r="D695" s="34"/>
       <c r="E695" s="34"/>
       <c r="F695" s="34"/>
-      <c r="G695" s="34"/>
+      <c r="G695" s="7" t="s">
+        <v>25</v>
+      </c>
       <c r="H695" s="21"/>
       <c r="I695" s="19"/>
       <c r="J695" s="10"/>
@@ -49743,7 +49926,9 @@
       <c r="L695" s="23"/>
       <c r="M695" s="22"/>
       <c r="N695" s="25"/>
-      <c r="O695" s="21"/>
+      <c r="O695" s="8" t="s">
+        <v>85</v>
+      </c>
       <c r="P695" s="21"/>
       <c r="Q695" s="19"/>
       <c r="R695" s="19"/>
@@ -49751,12 +49936,12 @@
       <c r="T695" s="20"/>
       <c r="U695" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#694</v>
       </c>
     </row>
     <row r="696">
-      <c r="A696" s="80"/>
-      <c r="B696" s="81"/>
+      <c r="A696" s="74"/>
+      <c r="B696" s="75"/>
       <c r="C696" s="34"/>
       <c r="D696" s="34"/>
       <c r="E696" s="34"/>
@@ -49781,8 +49966,8 @@
       </c>
     </row>
     <row r="697">
-      <c r="A697" s="80"/>
-      <c r="B697" s="81"/>
+      <c r="A697" s="74"/>
+      <c r="B697" s="75"/>
       <c r="C697" s="34"/>
       <c r="D697" s="34"/>
       <c r="E697" s="34"/>
@@ -49807,8 +49992,8 @@
       </c>
     </row>
     <row r="698">
-      <c r="A698" s="80"/>
-      <c r="B698" s="81"/>
+      <c r="A698" s="74"/>
+      <c r="B698" s="75"/>
       <c r="C698" s="34"/>
       <c r="D698" s="34"/>
       <c r="E698" s="34"/>
@@ -49833,8 +50018,8 @@
       </c>
     </row>
     <row r="699">
-      <c r="A699" s="80"/>
-      <c r="B699" s="81"/>
+      <c r="A699" s="74"/>
+      <c r="B699" s="75"/>
       <c r="C699" s="34"/>
       <c r="D699" s="34"/>
       <c r="E699" s="34"/>
@@ -49859,8 +50044,8 @@
       </c>
     </row>
     <row r="700">
-      <c r="A700" s="80"/>
-      <c r="B700" s="81"/>
+      <c r="A700" s="74"/>
+      <c r="B700" s="75"/>
       <c r="C700" s="34"/>
       <c r="D700" s="34"/>
       <c r="E700" s="34"/>
@@ -49885,8 +50070,8 @@
       </c>
     </row>
     <row r="701">
-      <c r="A701" s="80"/>
-      <c r="B701" s="81"/>
+      <c r="A701" s="74"/>
+      <c r="B701" s="75"/>
       <c r="C701" s="34"/>
       <c r="D701" s="34"/>
       <c r="E701" s="34"/>
@@ -49911,8 +50096,8 @@
       </c>
     </row>
     <row r="702">
-      <c r="A702" s="80"/>
-      <c r="B702" s="81"/>
+      <c r="A702" s="74"/>
+      <c r="B702" s="75"/>
       <c r="C702" s="34"/>
       <c r="D702" s="34"/>
       <c r="E702" s="34"/>
@@ -49937,8 +50122,8 @@
       </c>
     </row>
     <row r="703">
-      <c r="A703" s="80"/>
-      <c r="B703" s="81"/>
+      <c r="A703" s="74"/>
+      <c r="B703" s="75"/>
       <c r="C703" s="34"/>
       <c r="D703" s="34"/>
       <c r="E703" s="34"/>
@@ -49963,8 +50148,8 @@
       </c>
     </row>
     <row r="704">
-      <c r="A704" s="80"/>
-      <c r="B704" s="81"/>
+      <c r="A704" s="74"/>
+      <c r="B704" s="75"/>
       <c r="C704" s="34"/>
       <c r="D704" s="34"/>
       <c r="E704" s="34"/>
@@ -49989,8 +50174,8 @@
       </c>
     </row>
     <row r="705">
-      <c r="A705" s="80"/>
-      <c r="B705" s="81"/>
+      <c r="A705" s="74"/>
+      <c r="B705" s="75"/>
       <c r="C705" s="34"/>
       <c r="D705" s="34"/>
       <c r="E705" s="34"/>
@@ -50015,8 +50200,8 @@
       </c>
     </row>
     <row r="706">
-      <c r="A706" s="80"/>
-      <c r="B706" s="81"/>
+      <c r="A706" s="74"/>
+      <c r="B706" s="75"/>
       <c r="C706" s="34"/>
       <c r="D706" s="34"/>
       <c r="E706" s="34"/>
@@ -50041,8 +50226,8 @@
       </c>
     </row>
     <row r="707">
-      <c r="A707" s="80"/>
-      <c r="B707" s="81"/>
+      <c r="A707" s="74"/>
+      <c r="B707" s="75"/>
       <c r="C707" s="34"/>
       <c r="D707" s="34"/>
       <c r="E707" s="34"/>
@@ -50067,8 +50252,8 @@
       </c>
     </row>
     <row r="708">
-      <c r="A708" s="80"/>
-      <c r="B708" s="81"/>
+      <c r="A708" s="74"/>
+      <c r="B708" s="75"/>
       <c r="C708" s="34"/>
       <c r="D708" s="34"/>
       <c r="E708" s="34"/>
@@ -50093,8 +50278,8 @@
       </c>
     </row>
     <row r="709">
-      <c r="A709" s="80"/>
-      <c r="B709" s="81"/>
+      <c r="A709" s="74"/>
+      <c r="B709" s="75"/>
       <c r="C709" s="34"/>
       <c r="D709" s="34"/>
       <c r="E709" s="34"/>
@@ -50119,8 +50304,8 @@
       </c>
     </row>
     <row r="710">
-      <c r="A710" s="80"/>
-      <c r="B710" s="81"/>
+      <c r="A710" s="74"/>
+      <c r="B710" s="75"/>
       <c r="C710" s="34"/>
       <c r="D710" s="34"/>
       <c r="E710" s="34"/>
@@ -50145,8 +50330,8 @@
       </c>
     </row>
     <row r="711">
-      <c r="A711" s="80"/>
-      <c r="B711" s="81"/>
+      <c r="A711" s="74"/>
+      <c r="B711" s="75"/>
       <c r="C711" s="34"/>
       <c r="D711" s="34"/>
       <c r="E711" s="34"/>
@@ -50171,8 +50356,8 @@
       </c>
     </row>
     <row r="712">
-      <c r="A712" s="80"/>
-      <c r="B712" s="81"/>
+      <c r="A712" s="74"/>
+      <c r="B712" s="75"/>
       <c r="C712" s="34"/>
       <c r="D712" s="34"/>
       <c r="E712" s="34"/>
@@ -50197,8 +50382,8 @@
       </c>
     </row>
     <row r="713">
-      <c r="A713" s="80"/>
-      <c r="B713" s="81"/>
+      <c r="A713" s="74"/>
+      <c r="B713" s="75"/>
       <c r="C713" s="34"/>
       <c r="D713" s="34"/>
       <c r="E713" s="34"/>
@@ -50223,8 +50408,8 @@
       </c>
     </row>
     <row r="714">
-      <c r="A714" s="80"/>
-      <c r="B714" s="81"/>
+      <c r="A714" s="74"/>
+      <c r="B714" s="75"/>
       <c r="C714" s="34"/>
       <c r="D714" s="34"/>
       <c r="E714" s="34"/>
@@ -50249,8 +50434,8 @@
       </c>
     </row>
     <row r="715">
-      <c r="A715" s="80"/>
-      <c r="B715" s="81"/>
+      <c r="A715" s="74"/>
+      <c r="B715" s="75"/>
       <c r="C715" s="34"/>
       <c r="D715" s="34"/>
       <c r="E715" s="34"/>
@@ -50275,8 +50460,8 @@
       </c>
     </row>
     <row r="716">
-      <c r="A716" s="80"/>
-      <c r="B716" s="81"/>
+      <c r="A716" s="74"/>
+      <c r="B716" s="75"/>
       <c r="C716" s="34"/>
       <c r="D716" s="34"/>
       <c r="E716" s="34"/>
@@ -50301,8 +50486,8 @@
       </c>
     </row>
     <row r="717">
-      <c r="A717" s="80"/>
-      <c r="B717" s="81"/>
+      <c r="A717" s="74"/>
+      <c r="B717" s="75"/>
       <c r="C717" s="34"/>
       <c r="D717" s="34"/>
       <c r="E717" s="34"/>
@@ -50327,8 +50512,8 @@
       </c>
     </row>
     <row r="718">
-      <c r="A718" s="80"/>
-      <c r="B718" s="81"/>
+      <c r="A718" s="74"/>
+      <c r="B718" s="75"/>
       <c r="C718" s="34"/>
       <c r="D718" s="34"/>
       <c r="E718" s="34"/>
@@ -50353,8 +50538,8 @@
       </c>
     </row>
     <row r="719">
-      <c r="A719" s="80"/>
-      <c r="B719" s="81"/>
+      <c r="A719" s="74"/>
+      <c r="B719" s="75"/>
       <c r="C719" s="34"/>
       <c r="D719" s="34"/>
       <c r="E719" s="34"/>
@@ -50379,8 +50564,8 @@
       </c>
     </row>
     <row r="720">
-      <c r="A720" s="80"/>
-      <c r="B720" s="81"/>
+      <c r="A720" s="74"/>
+      <c r="B720" s="75"/>
       <c r="C720" s="34"/>
       <c r="D720" s="34"/>
       <c r="E720" s="34"/>
@@ -50405,8 +50590,8 @@
       </c>
     </row>
     <row r="721">
-      <c r="A721" s="80"/>
-      <c r="B721" s="81"/>
+      <c r="A721" s="74"/>
+      <c r="B721" s="75"/>
       <c r="C721" s="34"/>
       <c r="D721" s="34"/>
       <c r="E721" s="34"/>
@@ -50431,8 +50616,8 @@
       </c>
     </row>
     <row r="722">
-      <c r="A722" s="80"/>
-      <c r="B722" s="81"/>
+      <c r="A722" s="74"/>
+      <c r="B722" s="75"/>
       <c r="C722" s="34"/>
       <c r="D722" s="34"/>
       <c r="E722" s="34"/>
@@ -50457,8 +50642,8 @@
       </c>
     </row>
     <row r="723">
-      <c r="A723" s="80"/>
-      <c r="B723" s="81"/>
+      <c r="A723" s="74"/>
+      <c r="B723" s="75"/>
       <c r="C723" s="34"/>
       <c r="D723" s="34"/>
       <c r="E723" s="34"/>
@@ -50483,8 +50668,8 @@
       </c>
     </row>
     <row r="724">
-      <c r="A724" s="80"/>
-      <c r="B724" s="81"/>
+      <c r="A724" s="74"/>
+      <c r="B724" s="75"/>
       <c r="C724" s="34"/>
       <c r="D724" s="34"/>
       <c r="E724" s="34"/>
@@ -50509,8 +50694,8 @@
       </c>
     </row>
     <row r="725">
-      <c r="A725" s="80"/>
-      <c r="B725" s="81"/>
+      <c r="A725" s="74"/>
+      <c r="B725" s="75"/>
       <c r="C725" s="34"/>
       <c r="D725" s="34"/>
       <c r="E725" s="34"/>
@@ -50535,8 +50720,8 @@
       </c>
     </row>
     <row r="726">
-      <c r="A726" s="80"/>
-      <c r="B726" s="81"/>
+      <c r="A726" s="74"/>
+      <c r="B726" s="75"/>
       <c r="C726" s="34"/>
       <c r="D726" s="34"/>
       <c r="E726" s="34"/>
@@ -50561,8 +50746,8 @@
       </c>
     </row>
     <row r="727">
-      <c r="A727" s="80"/>
-      <c r="B727" s="81"/>
+      <c r="A727" s="74"/>
+      <c r="B727" s="75"/>
       <c r="C727" s="34"/>
       <c r="D727" s="34"/>
       <c r="E727" s="34"/>
@@ -50587,8 +50772,8 @@
       </c>
     </row>
     <row r="728">
-      <c r="A728" s="80"/>
-      <c r="B728" s="81"/>
+      <c r="A728" s="74"/>
+      <c r="B728" s="75"/>
       <c r="C728" s="34"/>
       <c r="D728" s="34"/>
       <c r="E728" s="34"/>
@@ -50613,8 +50798,8 @@
       </c>
     </row>
     <row r="729">
-      <c r="A729" s="80"/>
-      <c r="B729" s="81"/>
+      <c r="A729" s="74"/>
+      <c r="B729" s="75"/>
       <c r="C729" s="34"/>
       <c r="D729" s="34"/>
       <c r="E729" s="34"/>
@@ -50639,8 +50824,8 @@
       </c>
     </row>
     <row r="730">
-      <c r="A730" s="80"/>
-      <c r="B730" s="81"/>
+      <c r="A730" s="74"/>
+      <c r="B730" s="75"/>
       <c r="C730" s="34"/>
       <c r="D730" s="34"/>
       <c r="E730" s="34"/>
@@ -50665,8 +50850,8 @@
       </c>
     </row>
     <row r="731">
-      <c r="A731" s="80"/>
-      <c r="B731" s="81"/>
+      <c r="A731" s="74"/>
+      <c r="B731" s="75"/>
       <c r="C731" s="34"/>
       <c r="D731" s="34"/>
       <c r="E731" s="34"/>
@@ -50691,8 +50876,8 @@
       </c>
     </row>
     <row r="732">
-      <c r="A732" s="80"/>
-      <c r="B732" s="81"/>
+      <c r="A732" s="74"/>
+      <c r="B732" s="75"/>
       <c r="C732" s="34"/>
       <c r="D732" s="34"/>
       <c r="E732" s="34"/>
@@ -50717,8 +50902,8 @@
       </c>
     </row>
     <row r="733">
-      <c r="A733" s="80"/>
-      <c r="B733" s="81"/>
+      <c r="A733" s="74"/>
+      <c r="B733" s="75"/>
       <c r="C733" s="34"/>
       <c r="D733" s="34"/>
       <c r="E733" s="34"/>
@@ -50743,8 +50928,8 @@
       </c>
     </row>
     <row r="734">
-      <c r="A734" s="80"/>
-      <c r="B734" s="81"/>
+      <c r="A734" s="74"/>
+      <c r="B734" s="75"/>
       <c r="C734" s="34"/>
       <c r="D734" s="34"/>
       <c r="E734" s="34"/>
@@ -50769,8 +50954,8 @@
       </c>
     </row>
     <row r="735">
-      <c r="A735" s="80"/>
-      <c r="B735" s="81"/>
+      <c r="A735" s="74"/>
+      <c r="B735" s="75"/>
       <c r="C735" s="34"/>
       <c r="D735" s="34"/>
       <c r="E735" s="34"/>
@@ -50795,8 +50980,8 @@
       </c>
     </row>
     <row r="736">
-      <c r="A736" s="80"/>
-      <c r="B736" s="81"/>
+      <c r="A736" s="74"/>
+      <c r="B736" s="75"/>
       <c r="C736" s="34"/>
       <c r="D736" s="34"/>
       <c r="E736" s="34"/>
@@ -50821,8 +51006,8 @@
       </c>
     </row>
     <row r="737">
-      <c r="A737" s="80"/>
-      <c r="B737" s="81"/>
+      <c r="A737" s="74"/>
+      <c r="B737" s="75"/>
       <c r="C737" s="34"/>
       <c r="D737" s="34"/>
       <c r="E737" s="34"/>
@@ -50847,8 +51032,8 @@
       </c>
     </row>
     <row r="738">
-      <c r="A738" s="80"/>
-      <c r="B738" s="81"/>
+      <c r="A738" s="74"/>
+      <c r="B738" s="75"/>
       <c r="C738" s="34"/>
       <c r="D738" s="34"/>
       <c r="E738" s="34"/>
@@ -50873,8 +51058,8 @@
       </c>
     </row>
     <row r="739">
-      <c r="A739" s="80"/>
-      <c r="B739" s="81"/>
+      <c r="A739" s="74"/>
+      <c r="B739" s="75"/>
       <c r="C739" s="34"/>
       <c r="D739" s="34"/>
       <c r="E739" s="34"/>
@@ -50899,8 +51084,8 @@
       </c>
     </row>
     <row r="740">
-      <c r="A740" s="80"/>
-      <c r="B740" s="81"/>
+      <c r="A740" s="74"/>
+      <c r="B740" s="75"/>
       <c r="C740" s="34"/>
       <c r="D740" s="34"/>
       <c r="E740" s="34"/>
@@ -50925,8 +51110,8 @@
       </c>
     </row>
     <row r="741">
-      <c r="A741" s="80"/>
-      <c r="B741" s="81"/>
+      <c r="A741" s="74"/>
+      <c r="B741" s="75"/>
       <c r="C741" s="34"/>
       <c r="D741" s="34"/>
       <c r="E741" s="34"/>
@@ -50951,8 +51136,8 @@
       </c>
     </row>
     <row r="742">
-      <c r="A742" s="80"/>
-      <c r="B742" s="81"/>
+      <c r="A742" s="74"/>
+      <c r="B742" s="75"/>
       <c r="C742" s="34"/>
       <c r="D742" s="34"/>
       <c r="E742" s="34"/>
@@ -50977,8 +51162,8 @@
       </c>
     </row>
     <row r="743">
-      <c r="A743" s="80"/>
-      <c r="B743" s="81"/>
+      <c r="A743" s="74"/>
+      <c r="B743" s="75"/>
       <c r="C743" s="34"/>
       <c r="D743" s="34"/>
       <c r="E743" s="34"/>
@@ -51003,8 +51188,8 @@
       </c>
     </row>
     <row r="744">
-      <c r="A744" s="80"/>
-      <c r="B744" s="81"/>
+      <c r="A744" s="74"/>
+      <c r="B744" s="75"/>
       <c r="C744" s="34"/>
       <c r="D744" s="34"/>
       <c r="E744" s="34"/>
@@ -51029,8 +51214,8 @@
       </c>
     </row>
     <row r="745">
-      <c r="A745" s="80"/>
-      <c r="B745" s="81"/>
+      <c r="A745" s="74"/>
+      <c r="B745" s="75"/>
       <c r="C745" s="34"/>
       <c r="D745" s="34"/>
       <c r="E745" s="34"/>
@@ -51055,8 +51240,8 @@
       </c>
     </row>
     <row r="746">
-      <c r="A746" s="80"/>
-      <c r="B746" s="81"/>
+      <c r="A746" s="74"/>
+      <c r="B746" s="75"/>
       <c r="C746" s="34"/>
       <c r="D746" s="34"/>
       <c r="E746" s="34"/>
@@ -51081,8 +51266,8 @@
       </c>
     </row>
     <row r="747">
-      <c r="A747" s="80"/>
-      <c r="B747" s="81"/>
+      <c r="A747" s="74"/>
+      <c r="B747" s="75"/>
       <c r="C747" s="34"/>
       <c r="D747" s="34"/>
       <c r="E747" s="34"/>
@@ -51107,8 +51292,8 @@
       </c>
     </row>
     <row r="748">
-      <c r="A748" s="80"/>
-      <c r="B748" s="81"/>
+      <c r="A748" s="74"/>
+      <c r="B748" s="75"/>
       <c r="C748" s="34"/>
       <c r="D748" s="34"/>
       <c r="E748" s="34"/>
@@ -51133,8 +51318,8 @@
       </c>
     </row>
     <row r="749">
-      <c r="A749" s="80"/>
-      <c r="B749" s="81"/>
+      <c r="A749" s="74"/>
+      <c r="B749" s="75"/>
       <c r="C749" s="34"/>
       <c r="D749" s="34"/>
       <c r="E749" s="34"/>
@@ -51159,8 +51344,8 @@
       </c>
     </row>
     <row r="750">
-      <c r="A750" s="80"/>
-      <c r="B750" s="81"/>
+      <c r="A750" s="74"/>
+      <c r="B750" s="75"/>
       <c r="C750" s="34"/>
       <c r="D750" s="34"/>
       <c r="E750" s="34"/>
@@ -51185,8 +51370,8 @@
       </c>
     </row>
     <row r="751">
-      <c r="A751" s="80"/>
-      <c r="B751" s="81"/>
+      <c r="A751" s="74"/>
+      <c r="B751" s="75"/>
       <c r="C751" s="34"/>
       <c r="D751" s="34"/>
       <c r="E751" s="34"/>
@@ -51211,8 +51396,8 @@
       </c>
     </row>
     <row r="752">
-      <c r="A752" s="80"/>
-      <c r="B752" s="81"/>
+      <c r="A752" s="74"/>
+      <c r="B752" s="75"/>
       <c r="C752" s="34"/>
       <c r="D752" s="34"/>
       <c r="E752" s="34"/>
@@ -51237,8 +51422,8 @@
       </c>
     </row>
     <row r="753">
-      <c r="A753" s="80"/>
-      <c r="B753" s="81"/>
+      <c r="A753" s="74"/>
+      <c r="B753" s="75"/>
       <c r="C753" s="34"/>
       <c r="D753" s="34"/>
       <c r="E753" s="34"/>
@@ -51263,8 +51448,8 @@
       </c>
     </row>
     <row r="754">
-      <c r="A754" s="80"/>
-      <c r="B754" s="81"/>
+      <c r="A754" s="74"/>
+      <c r="B754" s="75"/>
       <c r="C754" s="34"/>
       <c r="D754" s="34"/>
       <c r="E754" s="34"/>
@@ -51289,8 +51474,8 @@
       </c>
     </row>
     <row r="755">
-      <c r="A755" s="80"/>
-      <c r="B755" s="81"/>
+      <c r="A755" s="74"/>
+      <c r="B755" s="75"/>
       <c r="C755" s="34"/>
       <c r="D755" s="34"/>
       <c r="E755" s="34"/>
@@ -51315,8 +51500,8 @@
       </c>
     </row>
     <row r="756">
-      <c r="A756" s="80"/>
-      <c r="B756" s="81"/>
+      <c r="A756" s="74"/>
+      <c r="B756" s="75"/>
       <c r="C756" s="34"/>
       <c r="D756" s="34"/>
       <c r="E756" s="34"/>
@@ -51341,8 +51526,8 @@
       </c>
     </row>
     <row r="757">
-      <c r="A757" s="80"/>
-      <c r="B757" s="81"/>
+      <c r="A757" s="74"/>
+      <c r="B757" s="75"/>
       <c r="C757" s="34"/>
       <c r="D757" s="34"/>
       <c r="E757" s="34"/>
@@ -51367,8 +51552,8 @@
       </c>
     </row>
     <row r="758">
-      <c r="A758" s="80"/>
-      <c r="B758" s="81"/>
+      <c r="A758" s="74"/>
+      <c r="B758" s="75"/>
       <c r="C758" s="34"/>
       <c r="D758" s="34"/>
       <c r="E758" s="34"/>
@@ -51393,8 +51578,8 @@
       </c>
     </row>
     <row r="759">
-      <c r="A759" s="80"/>
-      <c r="B759" s="81"/>
+      <c r="A759" s="74"/>
+      <c r="B759" s="75"/>
       <c r="C759" s="34"/>
       <c r="D759" s="34"/>
       <c r="E759" s="34"/>
@@ -51419,8 +51604,8 @@
       </c>
     </row>
     <row r="760">
-      <c r="A760" s="80"/>
-      <c r="B760" s="81"/>
+      <c r="A760" s="74"/>
+      <c r="B760" s="75"/>
       <c r="C760" s="34"/>
       <c r="D760" s="34"/>
       <c r="E760" s="34"/>
@@ -51445,8 +51630,8 @@
       </c>
     </row>
     <row r="761">
-      <c r="A761" s="80"/>
-      <c r="B761" s="81"/>
+      <c r="A761" s="74"/>
+      <c r="B761" s="75"/>
       <c r="C761" s="34"/>
       <c r="D761" s="34"/>
       <c r="E761" s="34"/>
@@ -51471,8 +51656,8 @@
       </c>
     </row>
     <row r="762">
-      <c r="A762" s="80"/>
-      <c r="B762" s="81"/>
+      <c r="A762" s="74"/>
+      <c r="B762" s="75"/>
       <c r="C762" s="34"/>
       <c r="D762" s="34"/>
       <c r="E762" s="34"/>
@@ -51497,8 +51682,8 @@
       </c>
     </row>
     <row r="763">
-      <c r="A763" s="80"/>
-      <c r="B763" s="81"/>
+      <c r="A763" s="74"/>
+      <c r="B763" s="75"/>
       <c r="C763" s="34"/>
       <c r="D763" s="34"/>
       <c r="E763" s="34"/>
@@ -51523,8 +51708,8 @@
       </c>
     </row>
     <row r="764">
-      <c r="A764" s="80"/>
-      <c r="B764" s="81"/>
+      <c r="A764" s="74"/>
+      <c r="B764" s="75"/>
       <c r="C764" s="34"/>
       <c r="D764" s="34"/>
       <c r="E764" s="34"/>
@@ -51549,8 +51734,8 @@
       </c>
     </row>
     <row r="765">
-      <c r="A765" s="80"/>
-      <c r="B765" s="81"/>
+      <c r="A765" s="74"/>
+      <c r="B765" s="75"/>
       <c r="C765" s="34"/>
       <c r="D765" s="34"/>
       <c r="E765" s="34"/>
@@ -51575,8 +51760,8 @@
       </c>
     </row>
     <row r="766">
-      <c r="A766" s="80"/>
-      <c r="B766" s="81"/>
+      <c r="A766" s="74"/>
+      <c r="B766" s="75"/>
       <c r="C766" s="34"/>
       <c r="D766" s="34"/>
       <c r="E766" s="34"/>
@@ -51601,8 +51786,8 @@
       </c>
     </row>
     <row r="767">
-      <c r="A767" s="80"/>
-      <c r="B767" s="81"/>
+      <c r="A767" s="74"/>
+      <c r="B767" s="75"/>
       <c r="C767" s="34"/>
       <c r="D767" s="34"/>
       <c r="E767" s="34"/>
@@ -51627,8 +51812,8 @@
       </c>
     </row>
     <row r="768">
-      <c r="A768" s="80"/>
-      <c r="B768" s="81"/>
+      <c r="A768" s="74"/>
+      <c r="B768" s="75"/>
       <c r="C768" s="34"/>
       <c r="D768" s="34"/>
       <c r="E768" s="34"/>
@@ -51653,8 +51838,8 @@
       </c>
     </row>
     <row r="769">
-      <c r="A769" s="80"/>
-      <c r="B769" s="81"/>
+      <c r="A769" s="74"/>
+      <c r="B769" s="75"/>
       <c r="C769" s="34"/>
       <c r="D769" s="34"/>
       <c r="E769" s="34"/>
@@ -51679,8 +51864,8 @@
       </c>
     </row>
     <row r="770">
-      <c r="A770" s="80"/>
-      <c r="B770" s="81"/>
+      <c r="A770" s="74"/>
+      <c r="B770" s="75"/>
       <c r="C770" s="34"/>
       <c r="D770" s="34"/>
       <c r="E770" s="34"/>
@@ -51705,8 +51890,8 @@
       </c>
     </row>
     <row r="771">
-      <c r="A771" s="80"/>
-      <c r="B771" s="81"/>
+      <c r="A771" s="74"/>
+      <c r="B771" s="75"/>
       <c r="C771" s="34"/>
       <c r="D771" s="34"/>
       <c r="E771" s="34"/>
@@ -51731,8 +51916,8 @@
       </c>
     </row>
     <row r="772">
-      <c r="A772" s="80"/>
-      <c r="B772" s="81"/>
+      <c r="A772" s="74"/>
+      <c r="B772" s="75"/>
       <c r="C772" s="34"/>
       <c r="D772" s="34"/>
       <c r="E772" s="34"/>
@@ -51757,8 +51942,8 @@
       </c>
     </row>
     <row r="773">
-      <c r="A773" s="80"/>
-      <c r="B773" s="81"/>
+      <c r="A773" s="74"/>
+      <c r="B773" s="75"/>
       <c r="C773" s="34"/>
       <c r="D773" s="34"/>
       <c r="E773" s="34"/>
@@ -51783,8 +51968,8 @@
       </c>
     </row>
     <row r="774">
-      <c r="A774" s="80"/>
-      <c r="B774" s="81"/>
+      <c r="A774" s="74"/>
+      <c r="B774" s="75"/>
       <c r="C774" s="34"/>
       <c r="D774" s="34"/>
       <c r="E774" s="34"/>
@@ -51809,8 +51994,8 @@
       </c>
     </row>
     <row r="775">
-      <c r="A775" s="80"/>
-      <c r="B775" s="81"/>
+      <c r="A775" s="74"/>
+      <c r="B775" s="75"/>
       <c r="C775" s="34"/>
       <c r="D775" s="34"/>
       <c r="E775" s="34"/>
@@ -51835,8 +52020,8 @@
       </c>
     </row>
     <row r="776">
-      <c r="A776" s="80"/>
-      <c r="B776" s="81"/>
+      <c r="A776" s="74"/>
+      <c r="B776" s="75"/>
       <c r="C776" s="34"/>
       <c r="D776" s="34"/>
       <c r="E776" s="34"/>
@@ -51861,8 +52046,8 @@
       </c>
     </row>
     <row r="777">
-      <c r="A777" s="80"/>
-      <c r="B777" s="81"/>
+      <c r="A777" s="74"/>
+      <c r="B777" s="75"/>
       <c r="C777" s="34"/>
       <c r="D777" s="34"/>
       <c r="E777" s="34"/>
@@ -51887,8 +52072,8 @@
       </c>
     </row>
     <row r="778">
-      <c r="A778" s="80"/>
-      <c r="B778" s="81"/>
+      <c r="A778" s="74"/>
+      <c r="B778" s="75"/>
       <c r="C778" s="34"/>
       <c r="D778" s="34"/>
       <c r="E778" s="34"/>
@@ -51913,8 +52098,8 @@
       </c>
     </row>
     <row r="779">
-      <c r="A779" s="80"/>
-      <c r="B779" s="81"/>
+      <c r="A779" s="74"/>
+      <c r="B779" s="75"/>
       <c r="C779" s="34"/>
       <c r="D779" s="34"/>
       <c r="E779" s="34"/>
@@ -51939,8 +52124,8 @@
       </c>
     </row>
     <row r="780">
-      <c r="A780" s="80"/>
-      <c r="B780" s="81"/>
+      <c r="A780" s="74"/>
+      <c r="B780" s="75"/>
       <c r="C780" s="34"/>
       <c r="D780" s="34"/>
       <c r="E780" s="34"/>
@@ -51965,8 +52150,8 @@
       </c>
     </row>
     <row r="781">
-      <c r="A781" s="80"/>
-      <c r="B781" s="81"/>
+      <c r="A781" s="74"/>
+      <c r="B781" s="75"/>
       <c r="C781" s="34"/>
       <c r="D781" s="34"/>
       <c r="E781" s="34"/>
@@ -51991,8 +52176,8 @@
       </c>
     </row>
     <row r="782">
-      <c r="A782" s="80"/>
-      <c r="B782" s="81"/>
+      <c r="A782" s="74"/>
+      <c r="B782" s="75"/>
       <c r="C782" s="34"/>
       <c r="D782" s="34"/>
       <c r="E782" s="34"/>
@@ -52017,8 +52202,8 @@
       </c>
     </row>
     <row r="783">
-      <c r="A783" s="80"/>
-      <c r="B783" s="81"/>
+      <c r="A783" s="74"/>
+      <c r="B783" s="75"/>
       <c r="C783" s="34"/>
       <c r="D783" s="34"/>
       <c r="E783" s="34"/>
@@ -52043,8 +52228,8 @@
       </c>
     </row>
     <row r="784">
-      <c r="A784" s="80"/>
-      <c r="B784" s="81"/>
+      <c r="A784" s="74"/>
+      <c r="B784" s="75"/>
       <c r="C784" s="34"/>
       <c r="D784" s="34"/>
       <c r="E784" s="34"/>
@@ -52069,8 +52254,8 @@
       </c>
     </row>
     <row r="785">
-      <c r="A785" s="80"/>
-      <c r="B785" s="81"/>
+      <c r="A785" s="74"/>
+      <c r="B785" s="75"/>
       <c r="C785" s="34"/>
       <c r="D785" s="34"/>
       <c r="E785" s="34"/>
@@ -52095,8 +52280,8 @@
       </c>
     </row>
     <row r="786">
-      <c r="A786" s="80"/>
-      <c r="B786" s="81"/>
+      <c r="A786" s="74"/>
+      <c r="B786" s="75"/>
       <c r="C786" s="34"/>
       <c r="D786" s="34"/>
       <c r="E786" s="34"/>
@@ -52121,8 +52306,8 @@
       </c>
     </row>
     <row r="787">
-      <c r="A787" s="80"/>
-      <c r="B787" s="81"/>
+      <c r="A787" s="74"/>
+      <c r="B787" s="75"/>
       <c r="C787" s="34"/>
       <c r="D787" s="34"/>
       <c r="E787" s="34"/>
@@ -52147,8 +52332,8 @@
       </c>
     </row>
     <row r="788">
-      <c r="A788" s="80"/>
-      <c r="B788" s="81"/>
+      <c r="A788" s="74"/>
+      <c r="B788" s="75"/>
       <c r="C788" s="34"/>
       <c r="D788" s="34"/>
       <c r="E788" s="34"/>
@@ -52173,8 +52358,8 @@
       </c>
     </row>
     <row r="789">
-      <c r="A789" s="80"/>
-      <c r="B789" s="81"/>
+      <c r="A789" s="74"/>
+      <c r="B789" s="75"/>
       <c r="C789" s="34"/>
       <c r="D789" s="34"/>
       <c r="E789" s="34"/>
@@ -52199,8 +52384,8 @@
       </c>
     </row>
     <row r="790">
-      <c r="A790" s="80"/>
-      <c r="B790" s="81"/>
+      <c r="A790" s="74"/>
+      <c r="B790" s="75"/>
       <c r="C790" s="34"/>
       <c r="D790" s="34"/>
       <c r="E790" s="34"/>
@@ -52225,8 +52410,8 @@
       </c>
     </row>
     <row r="791">
-      <c r="A791" s="80"/>
-      <c r="B791" s="81"/>
+      <c r="A791" s="74"/>
+      <c r="B791" s="75"/>
       <c r="C791" s="34"/>
       <c r="D791" s="34"/>
       <c r="E791" s="34"/>
@@ -52251,8 +52436,8 @@
       </c>
     </row>
     <row r="792">
-      <c r="A792" s="80"/>
-      <c r="B792" s="81"/>
+      <c r="A792" s="74"/>
+      <c r="B792" s="75"/>
       <c r="C792" s="34"/>
       <c r="D792" s="34"/>
       <c r="E792" s="34"/>
@@ -52277,8 +52462,8 @@
       </c>
     </row>
     <row r="793">
-      <c r="A793" s="80"/>
-      <c r="B793" s="81"/>
+      <c r="A793" s="74"/>
+      <c r="B793" s="75"/>
       <c r="C793" s="34"/>
       <c r="D793" s="34"/>
       <c r="E793" s="34"/>
@@ -52303,8 +52488,8 @@
       </c>
     </row>
     <row r="794">
-      <c r="A794" s="80"/>
-      <c r="B794" s="81"/>
+      <c r="A794" s="74"/>
+      <c r="B794" s="75"/>
       <c r="C794" s="34"/>
       <c r="D794" s="34"/>
       <c r="E794" s="34"/>
@@ -52329,8 +52514,8 @@
       </c>
     </row>
     <row r="795">
-      <c r="A795" s="80"/>
-      <c r="B795" s="81"/>
+      <c r="A795" s="74"/>
+      <c r="B795" s="75"/>
       <c r="C795" s="34"/>
       <c r="D795" s="34"/>
       <c r="E795" s="34"/>
@@ -52355,8 +52540,8 @@
       </c>
     </row>
     <row r="796">
-      <c r="A796" s="80"/>
-      <c r="B796" s="81"/>
+      <c r="A796" s="74"/>
+      <c r="B796" s="75"/>
       <c r="C796" s="34"/>
       <c r="D796" s="34"/>
       <c r="E796" s="34"/>
@@ -52381,8 +52566,8 @@
       </c>
     </row>
     <row r="797">
-      <c r="A797" s="80"/>
-      <c r="B797" s="81"/>
+      <c r="A797" s="74"/>
+      <c r="B797" s="75"/>
       <c r="C797" s="34"/>
       <c r="D797" s="34"/>
       <c r="E797" s="34"/>
@@ -52407,8 +52592,8 @@
       </c>
     </row>
     <row r="798">
-      <c r="A798" s="80"/>
-      <c r="B798" s="81"/>
+      <c r="A798" s="74"/>
+      <c r="B798" s="75"/>
       <c r="C798" s="34"/>
       <c r="D798" s="34"/>
       <c r="E798" s="34"/>
@@ -52433,8 +52618,8 @@
       </c>
     </row>
     <row r="799">
-      <c r="A799" s="80"/>
-      <c r="B799" s="81"/>
+      <c r="A799" s="74"/>
+      <c r="B799" s="75"/>
       <c r="C799" s="34"/>
       <c r="D799" s="34"/>
       <c r="E799" s="34"/>
@@ -52459,8 +52644,8 @@
       </c>
     </row>
     <row r="800">
-      <c r="A800" s="80"/>
-      <c r="B800" s="81"/>
+      <c r="A800" s="74"/>
+      <c r="B800" s="75"/>
       <c r="C800" s="34"/>
       <c r="D800" s="34"/>
       <c r="E800" s="34"/>
@@ -52485,8 +52670,8 @@
       </c>
     </row>
     <row r="801">
-      <c r="A801" s="80"/>
-      <c r="B801" s="81"/>
+      <c r="A801" s="74"/>
+      <c r="B801" s="75"/>
       <c r="C801" s="34"/>
       <c r="D801" s="34"/>
       <c r="E801" s="34"/>
@@ -52511,8 +52696,8 @@
       </c>
     </row>
     <row r="802">
-      <c r="A802" s="80"/>
-      <c r="B802" s="81"/>
+      <c r="A802" s="74"/>
+      <c r="B802" s="75"/>
       <c r="C802" s="34"/>
       <c r="D802" s="34"/>
       <c r="E802" s="34"/>
@@ -52537,8 +52722,8 @@
       </c>
     </row>
     <row r="803">
-      <c r="A803" s="80"/>
-      <c r="B803" s="81"/>
+      <c r="A803" s="74"/>
+      <c r="B803" s="75"/>
       <c r="C803" s="34"/>
       <c r="D803" s="34"/>
       <c r="E803" s="34"/>
@@ -52563,8 +52748,8 @@
       </c>
     </row>
     <row r="804">
-      <c r="A804" s="80"/>
-      <c r="B804" s="81"/>
+      <c r="A804" s="74"/>
+      <c r="B804" s="75"/>
       <c r="C804" s="34"/>
       <c r="D804" s="34"/>
       <c r="E804" s="34"/>
@@ -52589,8 +52774,8 @@
       </c>
     </row>
     <row r="805">
-      <c r="A805" s="80"/>
-      <c r="B805" s="81"/>
+      <c r="A805" s="74"/>
+      <c r="B805" s="75"/>
       <c r="C805" s="34"/>
       <c r="D805" s="34"/>
       <c r="E805" s="34"/>
@@ -52615,8 +52800,8 @@
       </c>
     </row>
     <row r="806">
-      <c r="A806" s="80"/>
-      <c r="B806" s="81"/>
+      <c r="A806" s="74"/>
+      <c r="B806" s="75"/>
       <c r="C806" s="34"/>
       <c r="D806" s="34"/>
       <c r="E806" s="34"/>
@@ -52641,8 +52826,8 @@
       </c>
     </row>
     <row r="807">
-      <c r="A807" s="80"/>
-      <c r="B807" s="81"/>
+      <c r="A807" s="74"/>
+      <c r="B807" s="75"/>
       <c r="C807" s="34"/>
       <c r="D807" s="34"/>
       <c r="E807" s="34"/>
@@ -52667,8 +52852,8 @@
       </c>
     </row>
     <row r="808">
-      <c r="A808" s="80"/>
-      <c r="B808" s="81"/>
+      <c r="A808" s="74"/>
+      <c r="B808" s="75"/>
       <c r="C808" s="34"/>
       <c r="D808" s="34"/>
       <c r="E808" s="34"/>
@@ -52693,8 +52878,8 @@
       </c>
     </row>
     <row r="809">
-      <c r="A809" s="80"/>
-      <c r="B809" s="81"/>
+      <c r="A809" s="74"/>
+      <c r="B809" s="75"/>
       <c r="C809" s="34"/>
       <c r="D809" s="34"/>
       <c r="E809" s="34"/>
@@ -52719,8 +52904,8 @@
       </c>
     </row>
     <row r="810">
-      <c r="A810" s="80"/>
-      <c r="B810" s="81"/>
+      <c r="A810" s="74"/>
+      <c r="B810" s="75"/>
       <c r="C810" s="34"/>
       <c r="D810" s="34"/>
       <c r="E810" s="34"/>
@@ -52745,8 +52930,8 @@
       </c>
     </row>
     <row r="811">
-      <c r="A811" s="80"/>
-      <c r="B811" s="81"/>
+      <c r="A811" s="74"/>
+      <c r="B811" s="75"/>
       <c r="C811" s="34"/>
       <c r="D811" s="34"/>
       <c r="E811" s="34"/>
@@ -52771,8 +52956,8 @@
       </c>
     </row>
     <row r="812">
-      <c r="A812" s="80"/>
-      <c r="B812" s="81"/>
+      <c r="A812" s="74"/>
+      <c r="B812" s="75"/>
       <c r="C812" s="34"/>
       <c r="D812" s="34"/>
       <c r="E812" s="34"/>
@@ -52797,8 +52982,8 @@
       </c>
     </row>
     <row r="813">
-      <c r="A813" s="80"/>
-      <c r="B813" s="81"/>
+      <c r="A813" s="74"/>
+      <c r="B813" s="75"/>
       <c r="C813" s="34"/>
       <c r="D813" s="34"/>
       <c r="E813" s="34"/>
@@ -52823,8 +53008,8 @@
       </c>
     </row>
     <row r="814">
-      <c r="A814" s="80"/>
-      <c r="B814" s="81"/>
+      <c r="A814" s="74"/>
+      <c r="B814" s="75"/>
       <c r="C814" s="34"/>
       <c r="D814" s="34"/>
       <c r="E814" s="34"/>
@@ -52849,8 +53034,8 @@
       </c>
     </row>
     <row r="815">
-      <c r="A815" s="80"/>
-      <c r="B815" s="81"/>
+      <c r="A815" s="74"/>
+      <c r="B815" s="75"/>
       <c r="C815" s="34"/>
       <c r="D815" s="34"/>
       <c r="E815" s="34"/>
@@ -52875,8 +53060,8 @@
       </c>
     </row>
     <row r="816">
-      <c r="A816" s="80"/>
-      <c r="B816" s="81"/>
+      <c r="A816" s="74"/>
+      <c r="B816" s="75"/>
       <c r="C816" s="34"/>
       <c r="D816" s="34"/>
       <c r="E816" s="34"/>
@@ -52901,8 +53086,8 @@
       </c>
     </row>
     <row r="817">
-      <c r="A817" s="80"/>
-      <c r="B817" s="81"/>
+      <c r="A817" s="74"/>
+      <c r="B817" s="75"/>
       <c r="C817" s="34"/>
       <c r="D817" s="34"/>
       <c r="E817" s="34"/>
@@ -52927,8 +53112,8 @@
       </c>
     </row>
     <row r="818">
-      <c r="A818" s="80"/>
-      <c r="B818" s="81"/>
+      <c r="A818" s="74"/>
+      <c r="B818" s="75"/>
       <c r="C818" s="34"/>
       <c r="D818" s="34"/>
       <c r="E818" s="34"/>
@@ -52953,8 +53138,8 @@
       </c>
     </row>
     <row r="819">
-      <c r="A819" s="80"/>
-      <c r="B819" s="81"/>
+      <c r="A819" s="74"/>
+      <c r="B819" s="75"/>
       <c r="C819" s="34"/>
       <c r="D819" s="34"/>
       <c r="E819" s="34"/>
@@ -52979,8 +53164,8 @@
       </c>
     </row>
     <row r="820">
-      <c r="A820" s="80"/>
-      <c r="B820" s="81"/>
+      <c r="A820" s="74"/>
+      <c r="B820" s="75"/>
       <c r="C820" s="34"/>
       <c r="D820" s="34"/>
       <c r="E820" s="34"/>
@@ -53005,8 +53190,8 @@
       </c>
     </row>
     <row r="821">
-      <c r="A821" s="80"/>
-      <c r="B821" s="81"/>
+      <c r="A821" s="74"/>
+      <c r="B821" s="75"/>
       <c r="C821" s="34"/>
       <c r="D821" s="34"/>
       <c r="E821" s="34"/>
@@ -53031,8 +53216,8 @@
       </c>
     </row>
     <row r="822">
-      <c r="A822" s="80"/>
-      <c r="B822" s="81"/>
+      <c r="A822" s="74"/>
+      <c r="B822" s="75"/>
       <c r="C822" s="34"/>
       <c r="D822" s="34"/>
       <c r="E822" s="34"/>
@@ -53057,8 +53242,8 @@
       </c>
     </row>
     <row r="823">
-      <c r="A823" s="80"/>
-      <c r="B823" s="81"/>
+      <c r="A823" s="74"/>
+      <c r="B823" s="75"/>
       <c r="C823" s="34"/>
       <c r="D823" s="34"/>
       <c r="E823" s="34"/>
@@ -53083,8 +53268,8 @@
       </c>
     </row>
     <row r="824">
-      <c r="A824" s="80"/>
-      <c r="B824" s="81"/>
+      <c r="A824" s="74"/>
+      <c r="B824" s="75"/>
       <c r="C824" s="34"/>
       <c r="D824" s="34"/>
       <c r="E824" s="34"/>
@@ -53109,8 +53294,8 @@
       </c>
     </row>
     <row r="825">
-      <c r="A825" s="80"/>
-      <c r="B825" s="81"/>
+      <c r="A825" s="74"/>
+      <c r="B825" s="75"/>
       <c r="C825" s="34"/>
       <c r="D825" s="34"/>
       <c r="E825" s="34"/>
@@ -53135,8 +53320,8 @@
       </c>
     </row>
     <row r="826">
-      <c r="A826" s="80"/>
-      <c r="B826" s="81"/>
+      <c r="A826" s="74"/>
+      <c r="B826" s="75"/>
       <c r="C826" s="34"/>
       <c r="D826" s="34"/>
       <c r="E826" s="34"/>
@@ -53161,8 +53346,8 @@
       </c>
     </row>
     <row r="827">
-      <c r="A827" s="80"/>
-      <c r="B827" s="81"/>
+      <c r="A827" s="74"/>
+      <c r="B827" s="75"/>
       <c r="C827" s="34"/>
       <c r="D827" s="34"/>
       <c r="E827" s="34"/>
@@ -53187,8 +53372,8 @@
       </c>
     </row>
     <row r="828">
-      <c r="A828" s="80"/>
-      <c r="B828" s="81"/>
+      <c r="A828" s="74"/>
+      <c r="B828" s="75"/>
       <c r="C828" s="34"/>
       <c r="D828" s="34"/>
       <c r="E828" s="34"/>
@@ -53213,8 +53398,8 @@
       </c>
     </row>
     <row r="829">
-      <c r="A829" s="80"/>
-      <c r="B829" s="81"/>
+      <c r="A829" s="74"/>
+      <c r="B829" s="75"/>
       <c r="C829" s="34"/>
       <c r="D829" s="34"/>
       <c r="E829" s="34"/>
@@ -53239,8 +53424,8 @@
       </c>
     </row>
     <row r="830">
-      <c r="A830" s="80"/>
-      <c r="B830" s="81"/>
+      <c r="A830" s="74"/>
+      <c r="B830" s="75"/>
       <c r="C830" s="34"/>
       <c r="D830" s="34"/>
       <c r="E830" s="34"/>
@@ -53265,8 +53450,8 @@
       </c>
     </row>
     <row r="831">
-      <c r="A831" s="80"/>
-      <c r="B831" s="81"/>
+      <c r="A831" s="74"/>
+      <c r="B831" s="75"/>
       <c r="C831" s="34"/>
       <c r="D831" s="34"/>
       <c r="E831" s="34"/>
@@ -53291,8 +53476,8 @@
       </c>
     </row>
     <row r="832">
-      <c r="A832" s="80"/>
-      <c r="B832" s="81"/>
+      <c r="A832" s="74"/>
+      <c r="B832" s="75"/>
       <c r="C832" s="34"/>
       <c r="D832" s="34"/>
       <c r="E832" s="34"/>
@@ -53317,8 +53502,8 @@
       </c>
     </row>
     <row r="833">
-      <c r="A833" s="80"/>
-      <c r="B833" s="81"/>
+      <c r="A833" s="74"/>
+      <c r="B833" s="75"/>
       <c r="C833" s="34"/>
       <c r="D833" s="34"/>
       <c r="E833" s="34"/>
@@ -53343,8 +53528,8 @@
       </c>
     </row>
     <row r="834">
-      <c r="A834" s="80"/>
-      <c r="B834" s="81"/>
+      <c r="A834" s="74"/>
+      <c r="B834" s="75"/>
       <c r="C834" s="34"/>
       <c r="D834" s="34"/>
       <c r="E834" s="34"/>
@@ -53369,8 +53554,8 @@
       </c>
     </row>
     <row r="835">
-      <c r="A835" s="80"/>
-      <c r="B835" s="81"/>
+      <c r="A835" s="74"/>
+      <c r="B835" s="75"/>
       <c r="C835" s="34"/>
       <c r="D835" s="34"/>
       <c r="E835" s="34"/>
@@ -53395,8 +53580,8 @@
       </c>
     </row>
     <row r="836">
-      <c r="A836" s="80"/>
-      <c r="B836" s="81"/>
+      <c r="A836" s="74"/>
+      <c r="B836" s="75"/>
       <c r="C836" s="34"/>
       <c r="D836" s="34"/>
       <c r="E836" s="34"/>
@@ -53421,8 +53606,8 @@
       </c>
     </row>
     <row r="837">
-      <c r="A837" s="80"/>
-      <c r="B837" s="81"/>
+      <c r="A837" s="74"/>
+      <c r="B837" s="75"/>
       <c r="C837" s="34"/>
       <c r="D837" s="34"/>
       <c r="E837" s="34"/>
@@ -53447,8 +53632,8 @@
       </c>
     </row>
     <row r="838">
-      <c r="A838" s="80"/>
-      <c r="B838" s="81"/>
+      <c r="A838" s="74"/>
+      <c r="B838" s="75"/>
       <c r="C838" s="34"/>
       <c r="D838" s="34"/>
       <c r="E838" s="34"/>
@@ -53473,8 +53658,8 @@
       </c>
     </row>
     <row r="839">
-      <c r="A839" s="80"/>
-      <c r="B839" s="81"/>
+      <c r="A839" s="74"/>
+      <c r="B839" s="75"/>
       <c r="C839" s="34"/>
       <c r="D839" s="34"/>
       <c r="E839" s="34"/>
@@ -53499,8 +53684,8 @@
       </c>
     </row>
     <row r="840">
-      <c r="A840" s="80"/>
-      <c r="B840" s="81"/>
+      <c r="A840" s="74"/>
+      <c r="B840" s="75"/>
       <c r="C840" s="34"/>
       <c r="D840" s="34"/>
       <c r="E840" s="34"/>
@@ -53525,8 +53710,8 @@
       </c>
     </row>
     <row r="841">
-      <c r="A841" s="80"/>
-      <c r="B841" s="81"/>
+      <c r="A841" s="74"/>
+      <c r="B841" s="75"/>
       <c r="C841" s="34"/>
       <c r="D841" s="34"/>
       <c r="E841" s="34"/>
@@ -53551,8 +53736,8 @@
       </c>
     </row>
     <row r="842">
-      <c r="A842" s="80"/>
-      <c r="B842" s="81"/>
+      <c r="A842" s="74"/>
+      <c r="B842" s="75"/>
       <c r="C842" s="34"/>
       <c r="D842" s="34"/>
       <c r="E842" s="34"/>
@@ -53577,8 +53762,8 @@
       </c>
     </row>
     <row r="843">
-      <c r="A843" s="80"/>
-      <c r="B843" s="81"/>
+      <c r="A843" s="74"/>
+      <c r="B843" s="75"/>
       <c r="C843" s="34"/>
       <c r="D843" s="34"/>
       <c r="E843" s="34"/>
@@ -53603,8 +53788,8 @@
       </c>
     </row>
     <row r="844">
-      <c r="A844" s="80"/>
-      <c r="B844" s="81"/>
+      <c r="A844" s="74"/>
+      <c r="B844" s="75"/>
       <c r="C844" s="34"/>
       <c r="D844" s="34"/>
       <c r="E844" s="34"/>
@@ -53629,8 +53814,8 @@
       </c>
     </row>
     <row r="845">
-      <c r="A845" s="80"/>
-      <c r="B845" s="81"/>
+      <c r="A845" s="74"/>
+      <c r="B845" s="75"/>
       <c r="C845" s="34"/>
       <c r="D845" s="34"/>
       <c r="E845" s="34"/>
@@ -53655,8 +53840,8 @@
       </c>
     </row>
     <row r="846">
-      <c r="A846" s="80"/>
-      <c r="B846" s="81"/>
+      <c r="A846" s="74"/>
+      <c r="B846" s="75"/>
       <c r="C846" s="34"/>
       <c r="D846" s="34"/>
       <c r="E846" s="34"/>
@@ -53681,8 +53866,8 @@
       </c>
     </row>
     <row r="847">
-      <c r="A847" s="80"/>
-      <c r="B847" s="81"/>
+      <c r="A847" s="74"/>
+      <c r="B847" s="75"/>
       <c r="C847" s="34"/>
       <c r="D847" s="34"/>
       <c r="E847" s="34"/>
@@ -53707,8 +53892,8 @@
       </c>
     </row>
     <row r="848">
-      <c r="A848" s="80"/>
-      <c r="B848" s="81"/>
+      <c r="A848" s="74"/>
+      <c r="B848" s="75"/>
       <c r="C848" s="34"/>
       <c r="D848" s="34"/>
       <c r="E848" s="34"/>
@@ -53733,8 +53918,8 @@
       </c>
     </row>
     <row r="849">
-      <c r="A849" s="80"/>
-      <c r="B849" s="81"/>
+      <c r="A849" s="74"/>
+      <c r="B849" s="75"/>
       <c r="C849" s="34"/>
       <c r="D849" s="34"/>
       <c r="E849" s="34"/>
@@ -53759,8 +53944,8 @@
       </c>
     </row>
     <row r="850">
-      <c r="A850" s="80"/>
-      <c r="B850" s="81"/>
+      <c r="A850" s="74"/>
+      <c r="B850" s="75"/>
       <c r="C850" s="34"/>
       <c r="D850" s="34"/>
       <c r="E850" s="34"/>
@@ -53785,8 +53970,8 @@
       </c>
     </row>
     <row r="851">
-      <c r="A851" s="80"/>
-      <c r="B851" s="81"/>
+      <c r="A851" s="74"/>
+      <c r="B851" s="75"/>
       <c r="C851" s="34"/>
       <c r="D851" s="34"/>
       <c r="E851" s="34"/>
@@ -53811,8 +53996,8 @@
       </c>
     </row>
     <row r="852">
-      <c r="A852" s="80"/>
-      <c r="B852" s="81"/>
+      <c r="A852" s="74"/>
+      <c r="B852" s="75"/>
       <c r="C852" s="34"/>
       <c r="D852" s="34"/>
       <c r="E852" s="34"/>
@@ -53837,8 +54022,8 @@
       </c>
     </row>
     <row r="853">
-      <c r="A853" s="80"/>
-      <c r="B853" s="81"/>
+      <c r="A853" s="74"/>
+      <c r="B853" s="75"/>
       <c r="C853" s="34"/>
       <c r="D853" s="34"/>
       <c r="E853" s="34"/>
@@ -53863,8 +54048,8 @@
       </c>
     </row>
     <row r="854">
-      <c r="A854" s="80"/>
-      <c r="B854" s="81"/>
+      <c r="A854" s="74"/>
+      <c r="B854" s="75"/>
       <c r="C854" s="34"/>
       <c r="D854" s="34"/>
       <c r="E854" s="34"/>
@@ -53889,8 +54074,8 @@
       </c>
     </row>
     <row r="855">
-      <c r="A855" s="80"/>
-      <c r="B855" s="81"/>
+      <c r="A855" s="74"/>
+      <c r="B855" s="75"/>
       <c r="C855" s="34"/>
       <c r="D855" s="34"/>
       <c r="E855" s="34"/>
@@ -53915,8 +54100,8 @@
       </c>
     </row>
     <row r="856">
-      <c r="A856" s="80"/>
-      <c r="B856" s="81"/>
+      <c r="A856" s="74"/>
+      <c r="B856" s="75"/>
       <c r="C856" s="34"/>
       <c r="D856" s="34"/>
       <c r="E856" s="34"/>
@@ -53941,8 +54126,8 @@
       </c>
     </row>
     <row r="857">
-      <c r="A857" s="80"/>
-      <c r="B857" s="81"/>
+      <c r="A857" s="74"/>
+      <c r="B857" s="75"/>
       <c r="C857" s="34"/>
       <c r="D857" s="34"/>
       <c r="E857" s="34"/>
@@ -53967,8 +54152,8 @@
       </c>
     </row>
     <row r="858">
-      <c r="A858" s="80"/>
-      <c r="B858" s="81"/>
+      <c r="A858" s="74"/>
+      <c r="B858" s="75"/>
       <c r="C858" s="34"/>
       <c r="D858" s="34"/>
       <c r="E858" s="34"/>
@@ -53993,8 +54178,8 @@
       </c>
     </row>
     <row r="859">
-      <c r="A859" s="80"/>
-      <c r="B859" s="81"/>
+      <c r="A859" s="74"/>
+      <c r="B859" s="75"/>
       <c r="C859" s="34"/>
       <c r="D859" s="34"/>
       <c r="E859" s="34"/>
@@ -54019,8 +54204,8 @@
       </c>
     </row>
     <row r="860">
-      <c r="A860" s="80"/>
-      <c r="B860" s="81"/>
+      <c r="A860" s="74"/>
+      <c r="B860" s="75"/>
       <c r="C860" s="34"/>
       <c r="D860" s="34"/>
       <c r="E860" s="34"/>
@@ -54045,8 +54230,8 @@
       </c>
     </row>
     <row r="861">
-      <c r="A861" s="80"/>
-      <c r="B861" s="81"/>
+      <c r="A861" s="74"/>
+      <c r="B861" s="75"/>
       <c r="C861" s="34"/>
       <c r="D861" s="34"/>
       <c r="E861" s="34"/>
@@ -54071,8 +54256,8 @@
       </c>
     </row>
     <row r="862">
-      <c r="A862" s="80"/>
-      <c r="B862" s="81"/>
+      <c r="A862" s="74"/>
+      <c r="B862" s="75"/>
       <c r="C862" s="34"/>
       <c r="D862" s="34"/>
       <c r="E862" s="34"/>
@@ -54097,8 +54282,8 @@
       </c>
     </row>
     <row r="863">
-      <c r="A863" s="80"/>
-      <c r="B863" s="81"/>
+      <c r="A863" s="74"/>
+      <c r="B863" s="75"/>
       <c r="C863" s="34"/>
       <c r="D863" s="34"/>
       <c r="E863" s="34"/>
@@ -54123,8 +54308,8 @@
       </c>
     </row>
     <row r="864">
-      <c r="A864" s="80"/>
-      <c r="B864" s="81"/>
+      <c r="A864" s="74"/>
+      <c r="B864" s="75"/>
       <c r="C864" s="34"/>
       <c r="D864" s="34"/>
       <c r="E864" s="34"/>
@@ -54149,8 +54334,8 @@
       </c>
     </row>
     <row r="865">
-      <c r="A865" s="80"/>
-      <c r="B865" s="81"/>
+      <c r="A865" s="74"/>
+      <c r="B865" s="75"/>
       <c r="C865" s="34"/>
       <c r="D865" s="34"/>
       <c r="E865" s="34"/>
@@ -54175,8 +54360,8 @@
       </c>
     </row>
     <row r="866">
-      <c r="A866" s="80"/>
-      <c r="B866" s="81"/>
+      <c r="A866" s="74"/>
+      <c r="B866" s="75"/>
       <c r="C866" s="34"/>
       <c r="D866" s="34"/>
       <c r="E866" s="34"/>
@@ -54201,8 +54386,8 @@
       </c>
     </row>
     <row r="867">
-      <c r="A867" s="80"/>
-      <c r="B867" s="81"/>
+      <c r="A867" s="74"/>
+      <c r="B867" s="75"/>
       <c r="C867" s="34"/>
       <c r="D867" s="34"/>
       <c r="E867" s="34"/>
@@ -54227,8 +54412,8 @@
       </c>
     </row>
     <row r="868">
-      <c r="A868" s="80"/>
-      <c r="B868" s="81"/>
+      <c r="A868" s="74"/>
+      <c r="B868" s="75"/>
       <c r="C868" s="34"/>
       <c r="D868" s="34"/>
       <c r="E868" s="34"/>
@@ -54253,8 +54438,8 @@
       </c>
     </row>
     <row r="869">
-      <c r="A869" s="80"/>
-      <c r="B869" s="81"/>
+      <c r="A869" s="74"/>
+      <c r="B869" s="75"/>
       <c r="C869" s="34"/>
       <c r="D869" s="34"/>
       <c r="E869" s="34"/>
@@ -54279,8 +54464,8 @@
       </c>
     </row>
     <row r="870">
-      <c r="A870" s="80"/>
-      <c r="B870" s="81"/>
+      <c r="A870" s="74"/>
+      <c r="B870" s="75"/>
       <c r="C870" s="34"/>
       <c r="D870" s="34"/>
       <c r="E870" s="34"/>
@@ -54305,8 +54490,8 @@
       </c>
     </row>
     <row r="871">
-      <c r="A871" s="80"/>
-      <c r="B871" s="81"/>
+      <c r="A871" s="74"/>
+      <c r="B871" s="75"/>
       <c r="C871" s="34"/>
       <c r="D871" s="34"/>
       <c r="E871" s="34"/>
@@ -54331,8 +54516,8 @@
       </c>
     </row>
     <row r="872">
-      <c r="A872" s="80"/>
-      <c r="B872" s="81"/>
+      <c r="A872" s="74"/>
+      <c r="B872" s="75"/>
       <c r="C872" s="34"/>
       <c r="D872" s="34"/>
       <c r="E872" s="34"/>
@@ -54357,8 +54542,8 @@
       </c>
     </row>
     <row r="873">
-      <c r="A873" s="80"/>
-      <c r="B873" s="81"/>
+      <c r="A873" s="74"/>
+      <c r="B873" s="75"/>
       <c r="C873" s="34"/>
       <c r="D873" s="34"/>
       <c r="E873" s="34"/>
@@ -54383,8 +54568,8 @@
       </c>
     </row>
     <row r="874">
-      <c r="A874" s="80"/>
-      <c r="B874" s="81"/>
+      <c r="A874" s="74"/>
+      <c r="B874" s="75"/>
       <c r="C874" s="34"/>
       <c r="D874" s="34"/>
       <c r="E874" s="34"/>
@@ -54409,8 +54594,8 @@
       </c>
     </row>
     <row r="875">
-      <c r="A875" s="80"/>
-      <c r="B875" s="81"/>
+      <c r="A875" s="74"/>
+      <c r="B875" s="75"/>
       <c r="C875" s="34"/>
       <c r="D875" s="34"/>
       <c r="E875" s="34"/>
@@ -54435,8 +54620,8 @@
       </c>
     </row>
     <row r="876">
-      <c r="A876" s="80"/>
-      <c r="B876" s="81"/>
+      <c r="A876" s="74"/>
+      <c r="B876" s="75"/>
       <c r="C876" s="34"/>
       <c r="D876" s="34"/>
       <c r="E876" s="34"/>
@@ -54461,8 +54646,8 @@
       </c>
     </row>
     <row r="877">
-      <c r="A877" s="80"/>
-      <c r="B877" s="81"/>
+      <c r="A877" s="74"/>
+      <c r="B877" s="75"/>
       <c r="C877" s="34"/>
       <c r="D877" s="34"/>
       <c r="E877" s="34"/>
@@ -54487,8 +54672,8 @@
       </c>
     </row>
     <row r="878">
-      <c r="A878" s="80"/>
-      <c r="B878" s="81"/>
+      <c r="A878" s="74"/>
+      <c r="B878" s="75"/>
       <c r="C878" s="34"/>
       <c r="D878" s="34"/>
       <c r="E878" s="34"/>
@@ -54513,8 +54698,8 @@
       </c>
     </row>
     <row r="879">
-      <c r="A879" s="80"/>
-      <c r="B879" s="81"/>
+      <c r="A879" s="74"/>
+      <c r="B879" s="75"/>
       <c r="C879" s="34"/>
       <c r="D879" s="34"/>
       <c r="E879" s="34"/>
@@ -54539,8 +54724,8 @@
       </c>
     </row>
     <row r="880">
-      <c r="A880" s="80"/>
-      <c r="B880" s="81"/>
+      <c r="A880" s="74"/>
+      <c r="B880" s="75"/>
       <c r="C880" s="34"/>
       <c r="D880" s="34"/>
       <c r="E880" s="34"/>
@@ -54565,8 +54750,8 @@
       </c>
     </row>
     <row r="881">
-      <c r="A881" s="80"/>
-      <c r="B881" s="81"/>
+      <c r="A881" s="74"/>
+      <c r="B881" s="75"/>
       <c r="C881" s="34"/>
       <c r="D881" s="34"/>
       <c r="E881" s="34"/>
@@ -54591,8 +54776,8 @@
       </c>
     </row>
     <row r="882">
-      <c r="A882" s="80"/>
-      <c r="B882" s="81"/>
+      <c r="A882" s="74"/>
+      <c r="B882" s="75"/>
       <c r="C882" s="34"/>
       <c r="D882" s="34"/>
       <c r="E882" s="34"/>
@@ -54617,8 +54802,8 @@
       </c>
     </row>
     <row r="883">
-      <c r="A883" s="80"/>
-      <c r="B883" s="81"/>
+      <c r="A883" s="74"/>
+      <c r="B883" s="75"/>
       <c r="C883" s="34"/>
       <c r="D883" s="34"/>
       <c r="E883" s="34"/>
@@ -54643,8 +54828,8 @@
       </c>
     </row>
     <row r="884">
-      <c r="A884" s="80"/>
-      <c r="B884" s="81"/>
+      <c r="A884" s="74"/>
+      <c r="B884" s="75"/>
       <c r="C884" s="34"/>
       <c r="D884" s="34"/>
       <c r="E884" s="34"/>
@@ -54669,8 +54854,8 @@
       </c>
     </row>
     <row r="885">
-      <c r="A885" s="80"/>
-      <c r="B885" s="81"/>
+      <c r="A885" s="74"/>
+      <c r="B885" s="75"/>
       <c r="C885" s="34"/>
       <c r="D885" s="34"/>
       <c r="E885" s="34"/>
@@ -54695,8 +54880,8 @@
       </c>
     </row>
     <row r="886">
-      <c r="A886" s="80"/>
-      <c r="B886" s="81"/>
+      <c r="A886" s="74"/>
+      <c r="B886" s="75"/>
       <c r="C886" s="34"/>
       <c r="D886" s="34"/>
       <c r="E886" s="34"/>
@@ -54721,8 +54906,8 @@
       </c>
     </row>
     <row r="887">
-      <c r="A887" s="80"/>
-      <c r="B887" s="81"/>
+      <c r="A887" s="74"/>
+      <c r="B887" s="75"/>
       <c r="C887" s="34"/>
       <c r="D887" s="34"/>
       <c r="E887" s="34"/>
@@ -54747,8 +54932,8 @@
       </c>
     </row>
     <row r="888">
-      <c r="A888" s="80"/>
-      <c r="B888" s="81"/>
+      <c r="A888" s="74"/>
+      <c r="B888" s="75"/>
       <c r="C888" s="34"/>
       <c r="D888" s="34"/>
       <c r="E888" s="34"/>
@@ -54773,8 +54958,8 @@
       </c>
     </row>
     <row r="889">
-      <c r="A889" s="80"/>
-      <c r="B889" s="81"/>
+      <c r="A889" s="74"/>
+      <c r="B889" s="75"/>
       <c r="C889" s="34"/>
       <c r="D889" s="34"/>
       <c r="E889" s="34"/>
@@ -54799,8 +54984,8 @@
       </c>
     </row>
     <row r="890">
-      <c r="A890" s="80"/>
-      <c r="B890" s="81"/>
+      <c r="A890" s="74"/>
+      <c r="B890" s="75"/>
       <c r="C890" s="34"/>
       <c r="D890" s="34"/>
       <c r="E890" s="34"/>
@@ -54825,8 +55010,8 @@
       </c>
     </row>
     <row r="891">
-      <c r="A891" s="80"/>
-      <c r="B891" s="81"/>
+      <c r="A891" s="74"/>
+      <c r="B891" s="75"/>
       <c r="C891" s="34"/>
       <c r="D891" s="34"/>
       <c r="E891" s="34"/>
@@ -54851,8 +55036,8 @@
       </c>
     </row>
     <row r="892">
-      <c r="A892" s="80"/>
-      <c r="B892" s="81"/>
+      <c r="A892" s="74"/>
+      <c r="B892" s="75"/>
       <c r="C892" s="34"/>
       <c r="D892" s="34"/>
       <c r="E892" s="34"/>
@@ -54877,8 +55062,8 @@
       </c>
     </row>
     <row r="893">
-      <c r="A893" s="80"/>
-      <c r="B893" s="81"/>
+      <c r="A893" s="74"/>
+      <c r="B893" s="75"/>
       <c r="C893" s="34"/>
       <c r="D893" s="34"/>
       <c r="E893" s="34"/>
@@ -54903,8 +55088,8 @@
       </c>
     </row>
     <row r="894">
-      <c r="A894" s="80"/>
-      <c r="B894" s="81"/>
+      <c r="A894" s="74"/>
+      <c r="B894" s="75"/>
       <c r="C894" s="34"/>
       <c r="D894" s="34"/>
       <c r="E894" s="34"/>
@@ -54929,8 +55114,8 @@
       </c>
     </row>
     <row r="895">
-      <c r="A895" s="80"/>
-      <c r="B895" s="81"/>
+      <c r="A895" s="74"/>
+      <c r="B895" s="75"/>
       <c r="C895" s="34"/>
       <c r="D895" s="34"/>
       <c r="E895" s="34"/>
@@ -54955,8 +55140,8 @@
       </c>
     </row>
     <row r="896">
-      <c r="A896" s="80"/>
-      <c r="B896" s="81"/>
+      <c r="A896" s="74"/>
+      <c r="B896" s="75"/>
       <c r="C896" s="34"/>
       <c r="D896" s="34"/>
       <c r="E896" s="34"/>
@@ -54981,8 +55166,8 @@
       </c>
     </row>
     <row r="897">
-      <c r="A897" s="80"/>
-      <c r="B897" s="81"/>
+      <c r="A897" s="74"/>
+      <c r="B897" s="75"/>
       <c r="C897" s="34"/>
       <c r="D897" s="34"/>
       <c r="E897" s="34"/>
@@ -55007,8 +55192,8 @@
       </c>
     </row>
     <row r="898">
-      <c r="A898" s="80"/>
-      <c r="B898" s="81"/>
+      <c r="A898" s="74"/>
+      <c r="B898" s="75"/>
       <c r="C898" s="34"/>
       <c r="D898" s="34"/>
       <c r="E898" s="34"/>
@@ -55033,8 +55218,8 @@
       </c>
     </row>
     <row r="899">
-      <c r="A899" s="80"/>
-      <c r="B899" s="81"/>
+      <c r="A899" s="74"/>
+      <c r="B899" s="75"/>
       <c r="C899" s="34"/>
       <c r="D899" s="34"/>
       <c r="E899" s="34"/>
@@ -55059,8 +55244,8 @@
       </c>
     </row>
     <row r="900">
-      <c r="A900" s="80"/>
-      <c r="B900" s="81"/>
+      <c r="A900" s="74"/>
+      <c r="B900" s="75"/>
       <c r="C900" s="34"/>
       <c r="D900" s="34"/>
       <c r="E900" s="34"/>
@@ -55085,8 +55270,8 @@
       </c>
     </row>
     <row r="901">
-      <c r="A901" s="80"/>
-      <c r="B901" s="81"/>
+      <c r="A901" s="74"/>
+      <c r="B901" s="75"/>
       <c r="C901" s="34"/>
       <c r="D901" s="34"/>
       <c r="E901" s="34"/>
@@ -55111,8 +55296,8 @@
       </c>
     </row>
     <row r="902">
-      <c r="A902" s="80"/>
-      <c r="B902" s="81"/>
+      <c r="A902" s="74"/>
+      <c r="B902" s="75"/>
       <c r="C902" s="34"/>
       <c r="D902" s="34"/>
       <c r="E902" s="34"/>
@@ -55137,8 +55322,8 @@
       </c>
     </row>
     <row r="903">
-      <c r="A903" s="80"/>
-      <c r="B903" s="81"/>
+      <c r="A903" s="74"/>
+      <c r="B903" s="75"/>
       <c r="C903" s="34"/>
       <c r="D903" s="34"/>
       <c r="E903" s="34"/>
@@ -55163,8 +55348,8 @@
       </c>
     </row>
     <row r="904">
-      <c r="A904" s="80"/>
-      <c r="B904" s="81"/>
+      <c r="A904" s="74"/>
+      <c r="B904" s="75"/>
       <c r="C904" s="34"/>
       <c r="D904" s="34"/>
       <c r="E904" s="34"/>
@@ -55189,8 +55374,8 @@
       </c>
     </row>
     <row r="905">
-      <c r="A905" s="80"/>
-      <c r="B905" s="81"/>
+      <c r="A905" s="74"/>
+      <c r="B905" s="75"/>
       <c r="C905" s="34"/>
       <c r="D905" s="34"/>
       <c r="E905" s="34"/>
@@ -55215,8 +55400,8 @@
       </c>
     </row>
     <row r="906">
-      <c r="A906" s="80"/>
-      <c r="B906" s="81"/>
+      <c r="A906" s="74"/>
+      <c r="B906" s="75"/>
       <c r="C906" s="34"/>
       <c r="D906" s="34"/>
       <c r="E906" s="34"/>
@@ -55241,8 +55426,8 @@
       </c>
     </row>
     <row r="907">
-      <c r="A907" s="80"/>
-      <c r="B907" s="81"/>
+      <c r="A907" s="74"/>
+      <c r="B907" s="75"/>
       <c r="C907" s="34"/>
       <c r="D907" s="34"/>
       <c r="E907" s="34"/>
@@ -55267,8 +55452,8 @@
       </c>
     </row>
     <row r="908">
-      <c r="A908" s="80"/>
-      <c r="B908" s="81"/>
+      <c r="A908" s="74"/>
+      <c r="B908" s="75"/>
       <c r="C908" s="34"/>
       <c r="D908" s="34"/>
       <c r="E908" s="34"/>
@@ -55293,8 +55478,8 @@
       </c>
     </row>
     <row r="909">
-      <c r="A909" s="80"/>
-      <c r="B909" s="81"/>
+      <c r="A909" s="74"/>
+      <c r="B909" s="75"/>
       <c r="C909" s="34"/>
       <c r="D909" s="34"/>
       <c r="E909" s="34"/>
@@ -55319,8 +55504,8 @@
       </c>
     </row>
     <row r="910">
-      <c r="A910" s="80"/>
-      <c r="B910" s="81"/>
+      <c r="A910" s="74"/>
+      <c r="B910" s="75"/>
       <c r="C910" s="34"/>
       <c r="D910" s="34"/>
       <c r="E910" s="34"/>
@@ -55345,8 +55530,8 @@
       </c>
     </row>
     <row r="911">
-      <c r="A911" s="80"/>
-      <c r="B911" s="81"/>
+      <c r="A911" s="74"/>
+      <c r="B911" s="75"/>
       <c r="C911" s="34"/>
       <c r="D911" s="34"/>
       <c r="E911" s="34"/>
@@ -55371,8 +55556,8 @@
       </c>
     </row>
     <row r="912">
-      <c r="A912" s="80"/>
-      <c r="B912" s="81"/>
+      <c r="A912" s="74"/>
+      <c r="B912" s="75"/>
       <c r="C912" s="34"/>
       <c r="D912" s="34"/>
       <c r="E912" s="34"/>
@@ -55397,8 +55582,8 @@
       </c>
     </row>
     <row r="913">
-      <c r="A913" s="80"/>
-      <c r="B913" s="81"/>
+      <c r="A913" s="74"/>
+      <c r="B913" s="75"/>
       <c r="C913" s="34"/>
       <c r="D913" s="34"/>
       <c r="E913" s="34"/>
@@ -55423,8 +55608,8 @@
       </c>
     </row>
     <row r="914">
-      <c r="A914" s="80"/>
-      <c r="B914" s="81"/>
+      <c r="A914" s="74"/>
+      <c r="B914" s="75"/>
       <c r="C914" s="34"/>
       <c r="D914" s="34"/>
       <c r="E914" s="34"/>
@@ -55449,8 +55634,8 @@
       </c>
     </row>
     <row r="915">
-      <c r="A915" s="80"/>
-      <c r="B915" s="81"/>
+      <c r="A915" s="74"/>
+      <c r="B915" s="75"/>
       <c r="C915" s="34"/>
       <c r="D915" s="34"/>
       <c r="E915" s="34"/>
@@ -55475,8 +55660,8 @@
       </c>
     </row>
     <row r="916">
-      <c r="A916" s="80"/>
-      <c r="B916" s="81"/>
+      <c r="A916" s="74"/>
+      <c r="B916" s="75"/>
       <c r="C916" s="34"/>
       <c r="D916" s="34"/>
       <c r="E916" s="34"/>
@@ -55501,8 +55686,8 @@
       </c>
     </row>
     <row r="917">
-      <c r="A917" s="80"/>
-      <c r="B917" s="81"/>
+      <c r="A917" s="74"/>
+      <c r="B917" s="75"/>
       <c r="C917" s="34"/>
       <c r="D917" s="34"/>
       <c r="E917" s="34"/>
@@ -55527,8 +55712,8 @@
       </c>
     </row>
     <row r="918">
-      <c r="A918" s="80"/>
-      <c r="B918" s="81"/>
+      <c r="A918" s="74"/>
+      <c r="B918" s="75"/>
       <c r="C918" s="34"/>
       <c r="D918" s="34"/>
       <c r="E918" s="34"/>
@@ -55553,8 +55738,8 @@
       </c>
     </row>
     <row r="919">
-      <c r="A919" s="80"/>
-      <c r="B919" s="81"/>
+      <c r="A919" s="74"/>
+      <c r="B919" s="75"/>
       <c r="C919" s="34"/>
       <c r="D919" s="34"/>
       <c r="E919" s="34"/>
@@ -55579,8 +55764,8 @@
       </c>
     </row>
     <row r="920">
-      <c r="A920" s="80"/>
-      <c r="B920" s="81"/>
+      <c r="A920" s="74"/>
+      <c r="B920" s="75"/>
       <c r="C920" s="34"/>
       <c r="D920" s="34"/>
       <c r="E920" s="34"/>
@@ -55605,8 +55790,8 @@
       </c>
     </row>
     <row r="921">
-      <c r="A921" s="80"/>
-      <c r="B921" s="81"/>
+      <c r="A921" s="74"/>
+      <c r="B921" s="75"/>
       <c r="C921" s="34"/>
       <c r="D921" s="34"/>
       <c r="E921" s="34"/>
@@ -55631,8 +55816,8 @@
       </c>
     </row>
     <row r="922">
-      <c r="A922" s="80"/>
-      <c r="B922" s="81"/>
+      <c r="A922" s="74"/>
+      <c r="B922" s="75"/>
       <c r="C922" s="34"/>
       <c r="D922" s="34"/>
       <c r="E922" s="34"/>
@@ -55657,8 +55842,8 @@
       </c>
     </row>
     <row r="923">
-      <c r="A923" s="80"/>
-      <c r="B923" s="81"/>
+      <c r="A923" s="74"/>
+      <c r="B923" s="75"/>
       <c r="C923" s="34"/>
       <c r="D923" s="34"/>
       <c r="E923" s="34"/>
@@ -55683,8 +55868,8 @@
       </c>
     </row>
     <row r="924">
-      <c r="A924" s="80"/>
-      <c r="B924" s="81"/>
+      <c r="A924" s="74"/>
+      <c r="B924" s="75"/>
       <c r="C924" s="34"/>
       <c r="D924" s="34"/>
       <c r="E924" s="34"/>
@@ -55709,8 +55894,8 @@
       </c>
     </row>
     <row r="925">
-      <c r="A925" s="80"/>
-      <c r="B925" s="81"/>
+      <c r="A925" s="74"/>
+      <c r="B925" s="75"/>
       <c r="C925" s="34"/>
       <c r="D925" s="34"/>
       <c r="E925" s="34"/>
@@ -55735,8 +55920,8 @@
       </c>
     </row>
     <row r="926">
-      <c r="A926" s="80"/>
-      <c r="B926" s="81"/>
+      <c r="A926" s="74"/>
+      <c r="B926" s="75"/>
       <c r="C926" s="34"/>
       <c r="D926" s="34"/>
       <c r="E926" s="34"/>
@@ -55761,8 +55946,8 @@
       </c>
     </row>
     <row r="927">
-      <c r="A927" s="80"/>
-      <c r="B927" s="81"/>
+      <c r="A927" s="74"/>
+      <c r="B927" s="75"/>
       <c r="C927" s="34"/>
       <c r="D927" s="34"/>
       <c r="E927" s="34"/>
@@ -55787,8 +55972,8 @@
       </c>
     </row>
     <row r="928">
-      <c r="A928" s="80"/>
-      <c r="B928" s="81"/>
+      <c r="A928" s="74"/>
+      <c r="B928" s="75"/>
       <c r="C928" s="34"/>
       <c r="D928" s="34"/>
       <c r="E928" s="34"/>
@@ -55813,8 +55998,8 @@
       </c>
     </row>
     <row r="929">
-      <c r="A929" s="80"/>
-      <c r="B929" s="81"/>
+      <c r="A929" s="74"/>
+      <c r="B929" s="75"/>
       <c r="C929" s="34"/>
       <c r="D929" s="34"/>
       <c r="E929" s="34"/>
@@ -55839,8 +56024,8 @@
       </c>
     </row>
     <row r="930">
-      <c r="A930" s="80"/>
-      <c r="B930" s="81"/>
+      <c r="A930" s="74"/>
+      <c r="B930" s="75"/>
       <c r="C930" s="34"/>
       <c r="D930" s="34"/>
       <c r="E930" s="34"/>
@@ -55865,8 +56050,8 @@
       </c>
     </row>
     <row r="931">
-      <c r="A931" s="80"/>
-      <c r="B931" s="81"/>
+      <c r="A931" s="74"/>
+      <c r="B931" s="75"/>
       <c r="C931" s="34"/>
       <c r="D931" s="34"/>
       <c r="E931" s="34"/>
@@ -55891,8 +56076,8 @@
       </c>
     </row>
     <row r="932">
-      <c r="A932" s="80"/>
-      <c r="B932" s="81"/>
+      <c r="A932" s="74"/>
+      <c r="B932" s="75"/>
       <c r="C932" s="34"/>
       <c r="D932" s="34"/>
       <c r="E932" s="34"/>
@@ -55917,8 +56102,8 @@
       </c>
     </row>
     <row r="933">
-      <c r="A933" s="80"/>
-      <c r="B933" s="81"/>
+      <c r="A933" s="74"/>
+      <c r="B933" s="75"/>
       <c r="C933" s="34"/>
       <c r="D933" s="34"/>
       <c r="E933" s="34"/>
@@ -55943,8 +56128,8 @@
       </c>
     </row>
     <row r="934">
-      <c r="A934" s="80"/>
-      <c r="B934" s="81"/>
+      <c r="A934" s="74"/>
+      <c r="B934" s="75"/>
       <c r="C934" s="34"/>
       <c r="D934" s="34"/>
       <c r="E934" s="34"/>
@@ -55969,8 +56154,8 @@
       </c>
     </row>
     <row r="935">
-      <c r="A935" s="80"/>
-      <c r="B935" s="81"/>
+      <c r="A935" s="74"/>
+      <c r="B935" s="75"/>
       <c r="C935" s="34"/>
       <c r="D935" s="34"/>
       <c r="E935" s="34"/>
@@ -55995,8 +56180,8 @@
       </c>
     </row>
     <row r="936">
-      <c r="A936" s="80"/>
-      <c r="B936" s="81"/>
+      <c r="A936" s="74"/>
+      <c r="B936" s="75"/>
       <c r="C936" s="34"/>
       <c r="D936" s="34"/>
       <c r="E936" s="34"/>
@@ -56021,8 +56206,8 @@
       </c>
     </row>
     <row r="937">
-      <c r="A937" s="80"/>
-      <c r="B937" s="81"/>
+      <c r="A937" s="74"/>
+      <c r="B937" s="75"/>
       <c r="C937" s="34"/>
       <c r="D937" s="34"/>
       <c r="E937" s="34"/>
@@ -56047,8 +56232,8 @@
       </c>
     </row>
     <row r="938">
-      <c r="A938" s="80"/>
-      <c r="B938" s="81"/>
+      <c r="A938" s="74"/>
+      <c r="B938" s="75"/>
       <c r="C938" s="34"/>
       <c r="D938" s="34"/>
       <c r="E938" s="34"/>
@@ -56073,8 +56258,8 @@
       </c>
     </row>
     <row r="939">
-      <c r="A939" s="80"/>
-      <c r="B939" s="81"/>
+      <c r="A939" s="74"/>
+      <c r="B939" s="75"/>
       <c r="C939" s="34"/>
       <c r="D939" s="34"/>
       <c r="E939" s="34"/>
@@ -56099,8 +56284,8 @@
       </c>
     </row>
     <row r="940">
-      <c r="A940" s="80"/>
-      <c r="B940" s="81"/>
+      <c r="A940" s="74"/>
+      <c r="B940" s="75"/>
       <c r="C940" s="34"/>
       <c r="D940" s="34"/>
       <c r="E940" s="34"/>
@@ -56125,8 +56310,8 @@
       </c>
     </row>
     <row r="941">
-      <c r="A941" s="80"/>
-      <c r="B941" s="81"/>
+      <c r="A941" s="74"/>
+      <c r="B941" s="75"/>
       <c r="C941" s="34"/>
       <c r="D941" s="34"/>
       <c r="E941" s="34"/>
@@ -56151,8 +56336,8 @@
       </c>
     </row>
     <row r="942">
-      <c r="A942" s="80"/>
-      <c r="B942" s="81"/>
+      <c r="A942" s="74"/>
+      <c r="B942" s="75"/>
       <c r="C942" s="34"/>
       <c r="D942" s="34"/>
       <c r="E942" s="34"/>
@@ -56177,8 +56362,8 @@
       </c>
     </row>
     <row r="943">
-      <c r="A943" s="80"/>
-      <c r="B943" s="81"/>
+      <c r="A943" s="74"/>
+      <c r="B943" s="75"/>
       <c r="C943" s="34"/>
       <c r="D943" s="34"/>
       <c r="E943" s="34"/>
@@ -56203,8 +56388,8 @@
       </c>
     </row>
     <row r="944">
-      <c r="A944" s="80"/>
-      <c r="B944" s="81"/>
+      <c r="A944" s="74"/>
+      <c r="B944" s="75"/>
       <c r="C944" s="34"/>
       <c r="D944" s="34"/>
       <c r="E944" s="34"/>
@@ -56229,8 +56414,8 @@
       </c>
     </row>
     <row r="945">
-      <c r="A945" s="80"/>
-      <c r="B945" s="81"/>
+      <c r="A945" s="74"/>
+      <c r="B945" s="75"/>
       <c r="C945" s="34"/>
       <c r="D945" s="34"/>
       <c r="E945" s="34"/>
@@ -56255,8 +56440,8 @@
       </c>
     </row>
     <row r="946">
-      <c r="A946" s="80"/>
-      <c r="B946" s="81"/>
+      <c r="A946" s="74"/>
+      <c r="B946" s="75"/>
       <c r="C946" s="34"/>
       <c r="D946" s="34"/>
       <c r="E946" s="34"/>
@@ -56281,8 +56466,8 @@
       </c>
     </row>
     <row r="947">
-      <c r="A947" s="80"/>
-      <c r="B947" s="81"/>
+      <c r="A947" s="74"/>
+      <c r="B947" s="75"/>
       <c r="C947" s="34"/>
       <c r="D947" s="34"/>
       <c r="E947" s="34"/>
@@ -56307,8 +56492,8 @@
       </c>
     </row>
     <row r="948">
-      <c r="A948" s="80"/>
-      <c r="B948" s="81"/>
+      <c r="A948" s="74"/>
+      <c r="B948" s="75"/>
       <c r="C948" s="34"/>
       <c r="D948" s="34"/>
       <c r="E948" s="34"/>
@@ -56333,8 +56518,8 @@
       </c>
     </row>
     <row r="949">
-      <c r="A949" s="80"/>
-      <c r="B949" s="81"/>
+      <c r="A949" s="74"/>
+      <c r="B949" s="75"/>
       <c r="C949" s="34"/>
       <c r="D949" s="34"/>
       <c r="E949" s="34"/>
@@ -56359,8 +56544,8 @@
       </c>
     </row>
     <row r="950">
-      <c r="A950" s="80"/>
-      <c r="B950" s="81"/>
+      <c r="A950" s="74"/>
+      <c r="B950" s="75"/>
       <c r="C950" s="34"/>
       <c r="D950" s="34"/>
       <c r="E950" s="34"/>
@@ -56385,8 +56570,8 @@
       </c>
     </row>
     <row r="951">
-      <c r="A951" s="80"/>
-      <c r="B951" s="81"/>
+      <c r="A951" s="74"/>
+      <c r="B951" s="75"/>
       <c r="C951" s="34"/>
       <c r="D951" s="34"/>
       <c r="E951" s="34"/>
@@ -56411,8 +56596,8 @@
       </c>
     </row>
     <row r="952">
-      <c r="A952" s="80"/>
-      <c r="B952" s="81"/>
+      <c r="A952" s="74"/>
+      <c r="B952" s="75"/>
       <c r="C952" s="34"/>
       <c r="D952" s="34"/>
       <c r="E952" s="34"/>
@@ -56437,8 +56622,8 @@
       </c>
     </row>
     <row r="953">
-      <c r="A953" s="80"/>
-      <c r="B953" s="81"/>
+      <c r="A953" s="74"/>
+      <c r="B953" s="75"/>
       <c r="C953" s="34"/>
       <c r="D953" s="34"/>
       <c r="E953" s="34"/>
@@ -56463,8 +56648,8 @@
       </c>
     </row>
     <row r="954">
-      <c r="A954" s="80"/>
-      <c r="B954" s="81"/>
+      <c r="A954" s="74"/>
+      <c r="B954" s="75"/>
       <c r="C954" s="34"/>
       <c r="D954" s="34"/>
       <c r="E954" s="34"/>
@@ -56489,8 +56674,8 @@
       </c>
     </row>
     <row r="955">
-      <c r="A955" s="80"/>
-      <c r="B955" s="81"/>
+      <c r="A955" s="74"/>
+      <c r="B955" s="75"/>
       <c r="C955" s="34"/>
       <c r="D955" s="34"/>
       <c r="E955" s="34"/>
@@ -56515,8 +56700,8 @@
       </c>
     </row>
     <row r="956">
-      <c r="A956" s="80"/>
-      <c r="B956" s="81"/>
+      <c r="A956" s="74"/>
+      <c r="B956" s="75"/>
       <c r="C956" s="34"/>
       <c r="D956" s="34"/>
       <c r="E956" s="34"/>
@@ -56541,8 +56726,8 @@
       </c>
     </row>
     <row r="957">
-      <c r="A957" s="80"/>
-      <c r="B957" s="81"/>
+      <c r="A957" s="74"/>
+      <c r="B957" s="75"/>
       <c r="C957" s="34"/>
       <c r="D957" s="34"/>
       <c r="E957" s="34"/>
@@ -56567,8 +56752,8 @@
       </c>
     </row>
     <row r="958">
-      <c r="A958" s="80"/>
-      <c r="B958" s="81"/>
+      <c r="A958" s="74"/>
+      <c r="B958" s="75"/>
       <c r="C958" s="34"/>
       <c r="D958" s="34"/>
       <c r="E958" s="34"/>
@@ -56593,8 +56778,8 @@
       </c>
     </row>
     <row r="959">
-      <c r="A959" s="80"/>
-      <c r="B959" s="81"/>
+      <c r="A959" s="74"/>
+      <c r="B959" s="75"/>
       <c r="C959" s="34"/>
       <c r="D959" s="34"/>
       <c r="E959" s="34"/>
@@ -56619,8 +56804,8 @@
       </c>
     </row>
     <row r="960">
-      <c r="A960" s="80"/>
-      <c r="B960" s="81"/>
+      <c r="A960" s="74"/>
+      <c r="B960" s="75"/>
       <c r="C960" s="34"/>
       <c r="D960" s="34"/>
       <c r="E960" s="34"/>
@@ -56645,8 +56830,8 @@
       </c>
     </row>
     <row r="961">
-      <c r="A961" s="80"/>
-      <c r="B961" s="81"/>
+      <c r="A961" s="74"/>
+      <c r="B961" s="75"/>
       <c r="C961" s="34"/>
       <c r="D961" s="34"/>
       <c r="E961" s="34"/>
@@ -56671,8 +56856,8 @@
       </c>
     </row>
     <row r="962">
-      <c r="A962" s="80"/>
-      <c r="B962" s="81"/>
+      <c r="A962" s="74"/>
+      <c r="B962" s="75"/>
       <c r="C962" s="34"/>
       <c r="D962" s="34"/>
       <c r="E962" s="34"/>
@@ -56697,8 +56882,8 @@
       </c>
     </row>
     <row r="963">
-      <c r="A963" s="80"/>
-      <c r="B963" s="81"/>
+      <c r="A963" s="74"/>
+      <c r="B963" s="75"/>
       <c r="C963" s="34"/>
       <c r="D963" s="34"/>
       <c r="E963" s="34"/>
@@ -56723,8 +56908,8 @@
       </c>
     </row>
     <row r="964">
-      <c r="A964" s="80"/>
-      <c r="B964" s="81"/>
+      <c r="A964" s="74"/>
+      <c r="B964" s="75"/>
       <c r="C964" s="34"/>
       <c r="D964" s="34"/>
       <c r="E964" s="34"/>
@@ -56749,8 +56934,8 @@
       </c>
     </row>
     <row r="965">
-      <c r="A965" s="80"/>
-      <c r="B965" s="81"/>
+      <c r="A965" s="74"/>
+      <c r="B965" s="75"/>
       <c r="C965" s="34"/>
       <c r="D965" s="34"/>
       <c r="E965" s="34"/>
@@ -56775,8 +56960,8 @@
       </c>
     </row>
     <row r="966">
-      <c r="A966" s="80"/>
-      <c r="B966" s="81"/>
+      <c r="A966" s="74"/>
+      <c r="B966" s="75"/>
       <c r="C966" s="34"/>
       <c r="D966" s="34"/>
       <c r="E966" s="34"/>
@@ -56801,8 +56986,8 @@
       </c>
     </row>
     <row r="967">
-      <c r="A967" s="80"/>
-      <c r="B967" s="81"/>
+      <c r="A967" s="74"/>
+      <c r="B967" s="75"/>
       <c r="C967" s="34"/>
       <c r="D967" s="34"/>
       <c r="E967" s="34"/>
@@ -56827,8 +57012,8 @@
       </c>
     </row>
     <row r="968">
-      <c r="A968" s="80"/>
-      <c r="B968" s="81"/>
+      <c r="A968" s="74"/>
+      <c r="B968" s="75"/>
       <c r="C968" s="34"/>
       <c r="D968" s="34"/>
       <c r="E968" s="34"/>
@@ -56853,8 +57038,8 @@
       </c>
     </row>
     <row r="969">
-      <c r="A969" s="80"/>
-      <c r="B969" s="81"/>
+      <c r="A969" s="74"/>
+      <c r="B969" s="75"/>
       <c r="C969" s="34"/>
       <c r="D969" s="34"/>
       <c r="E969" s="34"/>
@@ -56879,8 +57064,8 @@
       </c>
     </row>
     <row r="970">
-      <c r="A970" s="80"/>
-      <c r="B970" s="81"/>
+      <c r="A970" s="74"/>
+      <c r="B970" s="75"/>
       <c r="C970" s="34"/>
       <c r="D970" s="34"/>
       <c r="E970" s="34"/>
@@ -56905,8 +57090,8 @@
       </c>
     </row>
     <row r="971">
-      <c r="A971" s="80"/>
-      <c r="B971" s="81"/>
+      <c r="A971" s="74"/>
+      <c r="B971" s="75"/>
       <c r="C971" s="34"/>
       <c r="D971" s="34"/>
       <c r="E971" s="34"/>
@@ -56931,8 +57116,8 @@
       </c>
     </row>
     <row r="972">
-      <c r="A972" s="80"/>
-      <c r="B972" s="81"/>
+      <c r="A972" s="74"/>
+      <c r="B972" s="75"/>
       <c r="C972" s="34"/>
       <c r="D972" s="34"/>
       <c r="E972" s="34"/>
@@ -56957,8 +57142,8 @@
       </c>
     </row>
     <row r="973">
-      <c r="A973" s="80"/>
-      <c r="B973" s="81"/>
+      <c r="A973" s="74"/>
+      <c r="B973" s="75"/>
       <c r="C973" s="34"/>
       <c r="D973" s="34"/>
       <c r="E973" s="34"/>
@@ -56983,8 +57168,8 @@
       </c>
     </row>
     <row r="974">
-      <c r="A974" s="80"/>
-      <c r="B974" s="81"/>
+      <c r="A974" s="74"/>
+      <c r="B974" s="75"/>
       <c r="C974" s="34"/>
       <c r="D974" s="34"/>
       <c r="E974" s="34"/>
@@ -57009,8 +57194,8 @@
       </c>
     </row>
     <row r="975">
-      <c r="A975" s="80"/>
-      <c r="B975" s="81"/>
+      <c r="A975" s="74"/>
+      <c r="B975" s="75"/>
       <c r="C975" s="34"/>
       <c r="D975" s="34"/>
       <c r="E975" s="34"/>
@@ -57035,8 +57220,8 @@
       </c>
     </row>
     <row r="976">
-      <c r="A976" s="80"/>
-      <c r="B976" s="81"/>
+      <c r="A976" s="74"/>
+      <c r="B976" s="75"/>
       <c r="C976" s="34"/>
       <c r="D976" s="34"/>
       <c r="E976" s="34"/>
@@ -57061,8 +57246,8 @@
       </c>
     </row>
     <row r="977">
-      <c r="A977" s="80"/>
-      <c r="B977" s="81"/>
+      <c r="A977" s="74"/>
+      <c r="B977" s="75"/>
       <c r="C977" s="34"/>
       <c r="D977" s="34"/>
       <c r="E977" s="34"/>
@@ -57087,8 +57272,8 @@
       </c>
     </row>
     <row r="978">
-      <c r="A978" s="80"/>
-      <c r="B978" s="81"/>
+      <c r="A978" s="74"/>
+      <c r="B978" s="75"/>
       <c r="C978" s="34"/>
       <c r="D978" s="34"/>
       <c r="E978" s="34"/>
@@ -57113,8 +57298,8 @@
       </c>
     </row>
     <row r="979">
-      <c r="A979" s="80"/>
-      <c r="B979" s="81"/>
+      <c r="A979" s="74"/>
+      <c r="B979" s="75"/>
       <c r="C979" s="34"/>
       <c r="D979" s="34"/>
       <c r="E979" s="34"/>
@@ -57139,8 +57324,8 @@
       </c>
     </row>
     <row r="980">
-      <c r="A980" s="80"/>
-      <c r="B980" s="81"/>
+      <c r="A980" s="74"/>
+      <c r="B980" s="75"/>
       <c r="C980" s="34"/>
       <c r="D980" s="34"/>
       <c r="E980" s="34"/>
@@ -57165,8 +57350,8 @@
       </c>
     </row>
     <row r="981">
-      <c r="A981" s="80"/>
-      <c r="B981" s="81"/>
+      <c r="A981" s="74"/>
+      <c r="B981" s="75"/>
       <c r="C981" s="34"/>
       <c r="D981" s="34"/>
       <c r="E981" s="34"/>
@@ -57191,8 +57376,8 @@
       </c>
     </row>
     <row r="982">
-      <c r="A982" s="80"/>
-      <c r="B982" s="81"/>
+      <c r="A982" s="74"/>
+      <c r="B982" s="75"/>
       <c r="C982" s="34"/>
       <c r="D982" s="34"/>
       <c r="E982" s="34"/>
@@ -57217,8 +57402,8 @@
       </c>
     </row>
     <row r="983">
-      <c r="A983" s="80"/>
-      <c r="B983" s="81"/>
+      <c r="A983" s="74"/>
+      <c r="B983" s="75"/>
       <c r="C983" s="34"/>
       <c r="D983" s="34"/>
       <c r="E983" s="34"/>
@@ -57243,8 +57428,8 @@
       </c>
     </row>
     <row r="984">
-      <c r="A984" s="80"/>
-      <c r="B984" s="81"/>
+      <c r="A984" s="74"/>
+      <c r="B984" s="75"/>
       <c r="C984" s="34"/>
       <c r="D984" s="34"/>
       <c r="E984" s="34"/>
@@ -57269,8 +57454,8 @@
       </c>
     </row>
     <row r="985">
-      <c r="A985" s="80"/>
-      <c r="B985" s="81"/>
+      <c r="A985" s="74"/>
+      <c r="B985" s="75"/>
       <c r="C985" s="34"/>
       <c r="D985" s="34"/>
       <c r="E985" s="34"/>
@@ -57295,8 +57480,8 @@
       </c>
     </row>
     <row r="986">
-      <c r="A986" s="80"/>
-      <c r="B986" s="81"/>
+      <c r="A986" s="74"/>
+      <c r="B986" s="75"/>
       <c r="C986" s="34"/>
       <c r="D986" s="34"/>
       <c r="E986" s="34"/>
@@ -57321,8 +57506,8 @@
       </c>
     </row>
     <row r="987">
-      <c r="A987" s="80"/>
-      <c r="B987" s="81"/>
+      <c r="A987" s="74"/>
+      <c r="B987" s="75"/>
       <c r="C987" s="34"/>
       <c r="D987" s="34"/>
       <c r="E987" s="34"/>
@@ -57347,8 +57532,8 @@
       </c>
     </row>
     <row r="988">
-      <c r="A988" s="80"/>
-      <c r="B988" s="81"/>
+      <c r="A988" s="74"/>
+      <c r="B988" s="75"/>
       <c r="C988" s="34"/>
       <c r="D988" s="34"/>
       <c r="E988" s="34"/>
@@ -57373,8 +57558,8 @@
       </c>
     </row>
     <row r="989">
-      <c r="A989" s="80"/>
-      <c r="B989" s="81"/>
+      <c r="A989" s="74"/>
+      <c r="B989" s="75"/>
       <c r="C989" s="34"/>
       <c r="D989" s="34"/>
       <c r="E989" s="34"/>
@@ -57399,8 +57584,8 @@
       </c>
     </row>
     <row r="990">
-      <c r="A990" s="80"/>
-      <c r="B990" s="81"/>
+      <c r="A990" s="74"/>
+      <c r="B990" s="75"/>
       <c r="C990" s="34"/>
       <c r="D990" s="34"/>
       <c r="E990" s="34"/>
@@ -57425,8 +57610,8 @@
       </c>
     </row>
     <row r="991">
-      <c r="A991" s="80"/>
-      <c r="B991" s="81"/>
+      <c r="A991" s="74"/>
+      <c r="B991" s="75"/>
       <c r="C991" s="34"/>
       <c r="D991" s="34"/>
       <c r="E991" s="34"/>
@@ -57451,8 +57636,8 @@
       </c>
     </row>
     <row r="992">
-      <c r="A992" s="80"/>
-      <c r="B992" s="81"/>
+      <c r="A992" s="74"/>
+      <c r="B992" s="75"/>
       <c r="C992" s="34"/>
       <c r="D992" s="34"/>
       <c r="E992" s="34"/>
@@ -57477,8 +57662,8 @@
       </c>
     </row>
     <row r="993">
-      <c r="A993" s="80"/>
-      <c r="B993" s="81"/>
+      <c r="A993" s="74"/>
+      <c r="B993" s="75"/>
       <c r="C993" s="34"/>
       <c r="D993" s="34"/>
       <c r="E993" s="34"/>
@@ -57503,8 +57688,8 @@
       </c>
     </row>
     <row r="994">
-      <c r="A994" s="80"/>
-      <c r="B994" s="81"/>
+      <c r="A994" s="74"/>
+      <c r="B994" s="75"/>
       <c r="C994" s="34"/>
       <c r="D994" s="34"/>
       <c r="E994" s="34"/>
@@ -57529,8 +57714,8 @@
       </c>
     </row>
     <row r="995">
-      <c r="A995" s="80"/>
-      <c r="B995" s="81"/>
+      <c r="A995" s="74"/>
+      <c r="B995" s="75"/>
       <c r="C995" s="34"/>
       <c r="D995" s="34"/>
       <c r="E995" s="34"/>
@@ -57555,8 +57740,8 @@
       </c>
     </row>
     <row r="996">
-      <c r="A996" s="80"/>
-      <c r="B996" s="81"/>
+      <c r="A996" s="74"/>
+      <c r="B996" s="75"/>
       <c r="C996" s="34"/>
       <c r="D996" s="34"/>
       <c r="E996" s="34"/>
@@ -57581,8 +57766,8 @@
       </c>
     </row>
     <row r="997">
-      <c r="A997" s="80"/>
-      <c r="B997" s="81"/>
+      <c r="A997" s="74"/>
+      <c r="B997" s="75"/>
       <c r="C997" s="34"/>
       <c r="D997" s="34"/>
       <c r="E997" s="34"/>
@@ -57607,8 +57792,8 @@
       </c>
     </row>
     <row r="998">
-      <c r="A998" s="80"/>
-      <c r="B998" s="81"/>
+      <c r="A998" s="74"/>
+      <c r="B998" s="75"/>
       <c r="C998" s="34"/>
       <c r="D998" s="34"/>
       <c r="E998" s="34"/>
@@ -57633,8 +57818,8 @@
       </c>
     </row>
     <row r="999">
-      <c r="A999" s="80"/>
-      <c r="B999" s="81"/>
+      <c r="A999" s="74"/>
+      <c r="B999" s="75"/>
       <c r="C999" s="34"/>
       <c r="D999" s="34"/>
       <c r="E999" s="34"/>
@@ -57659,8 +57844,8 @@
       </c>
     </row>
     <row r="1000">
-      <c r="A1000" s="80"/>
-      <c r="B1000" s="81"/>
+      <c r="A1000" s="74"/>
+      <c r="B1000" s="75"/>
       <c r="C1000" s="34"/>
       <c r="D1000" s="34"/>
       <c r="E1000" s="34"/>
@@ -57685,8 +57870,8 @@
       </c>
     </row>
     <row r="1001">
-      <c r="A1001" s="80"/>
-      <c r="B1001" s="81"/>
+      <c r="A1001" s="74"/>
+      <c r="B1001" s="75"/>
       <c r="C1001" s="34"/>
       <c r="D1001" s="34"/>
       <c r="E1001" s="34"/>
@@ -58342,15 +58527,19 @@
     <hyperlink r:id="rId249" ref="S686"/>
     <hyperlink r:id="rId250" ref="S687"/>
     <hyperlink r:id="rId251" ref="S688"/>
+    <hyperlink r:id="rId252" ref="S689"/>
+    <hyperlink r:id="rId253" ref="S690"/>
+    <hyperlink r:id="rId254" ref="S691"/>
+    <hyperlink r:id="rId255" ref="S692"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId252"/>
-  <legacyDrawing r:id="rId253"/>
+  <drawing r:id="rId256"/>
+  <legacyDrawing r:id="rId257"/>
   <tableParts count="2">
-    <tablePart r:id="rId256"/>
-    <tablePart r:id="rId257"/>
+    <tablePart r:id="rId260"/>
+    <tablePart r:id="rId261"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201207
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -9158,7 +9158,7 @@
     <numFmt numFmtId="164" formatCode="mm&quot;月&quot;dd&quot;日 &quot;dddd"/>
     <numFmt numFmtId="165" formatCode="m/d"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="19">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -9243,10 +9243,6 @@
       <u/>
       <color rgb="FF0000FF"/>
     </font>
-    <font/>
-    <font>
-      <color rgb="FF000000"/>
-    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -9292,7 +9288,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="78">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -9515,26 +9511,8 @@
     <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="19" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -50225,29 +50203,29 @@
       <c r="G696" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H696" s="74" t="s">
+      <c r="H696" s="8" t="s">
         <v>2375</v>
       </c>
-      <c r="I696" s="75">
+      <c r="I696" s="9">
         <v>44149.0</v>
       </c>
-      <c r="J696" s="76" t="s">
+      <c r="J696" s="12" t="s">
         <v>1442</v>
       </c>
       <c r="K696" s="13" t="s">
         <v>2499</v>
       </c>
-      <c r="L696" s="76" t="s">
+      <c r="L696" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M696" s="77" t="s">
+      <c r="M696" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N696" s="25"/>
-      <c r="O696" s="74" t="s">
+      <c r="O696" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P696" s="78" t="s">
+      <c r="P696" s="74" t="s">
         <v>2500</v>
       </c>
       <c r="Q696" s="19"/>
@@ -50262,14 +50240,14 @@
       </c>
     </row>
     <row r="697">
-      <c r="A697" s="79" t="s">
+      <c r="A697" s="16" t="s">
         <v>2502</v>
       </c>
       <c r="B697" s="6">
         <v>44171.0</v>
       </c>
       <c r="C697" s="34"/>
-      <c r="D697" s="80" t="s">
+      <c r="D697" s="7" t="s">
         <v>2139</v>
       </c>
       <c r="E697" s="7" t="s">
@@ -50279,29 +50257,29 @@
       <c r="G697" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H697" s="74" t="s">
+      <c r="H697" s="8" t="s">
         <v>2503</v>
       </c>
-      <c r="I697" s="79" t="s">
+      <c r="I697" s="16" t="s">
         <v>2504</v>
       </c>
-      <c r="J697" s="76" t="s">
+      <c r="J697" s="12" t="s">
         <v>1442</v>
       </c>
-      <c r="K697" s="77" t="s">
+      <c r="K697" s="13" t="s">
         <v>2505</v>
       </c>
-      <c r="L697" s="76" t="s">
+      <c r="L697" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M697" s="77" t="s">
+      <c r="M697" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N697" s="25"/>
-      <c r="O697" s="74" t="s">
+      <c r="O697" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P697" s="74" t="s">
+      <c r="P697" s="8" t="s">
         <v>2506</v>
       </c>
       <c r="Q697" s="19"/>
@@ -50316,14 +50294,14 @@
       </c>
     </row>
     <row r="698">
-      <c r="A698" s="79" t="s">
+      <c r="A698" s="16" t="s">
         <v>2508</v>
       </c>
       <c r="B698" s="6">
         <v>44171.0</v>
       </c>
       <c r="C698" s="34"/>
-      <c r="D698" s="80" t="s">
+      <c r="D698" s="7" t="s">
         <v>2139</v>
       </c>
       <c r="E698" s="7" t="s">
@@ -50333,29 +50311,29 @@
       <c r="G698" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H698" s="74" t="s">
+      <c r="H698" s="8" t="s">
         <v>2503</v>
       </c>
-      <c r="I698" s="79" t="s">
+      <c r="I698" s="16" t="s">
         <v>2504</v>
       </c>
-      <c r="J698" s="76" t="s">
+      <c r="J698" s="12" t="s">
         <v>1442</v>
       </c>
-      <c r="K698" s="77" t="s">
+      <c r="K698" s="13" t="s">
         <v>2505</v>
       </c>
-      <c r="L698" s="76" t="s">
+      <c r="L698" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M698" s="77" t="s">
+      <c r="M698" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N698" s="25"/>
-      <c r="O698" s="74" t="s">
+      <c r="O698" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P698" s="74" t="s">
+      <c r="P698" s="8" t="s">
         <v>2506</v>
       </c>
       <c r="Q698" s="19"/>
@@ -50370,14 +50348,14 @@
       </c>
     </row>
     <row r="699">
-      <c r="A699" s="79" t="s">
+      <c r="A699" s="16" t="s">
         <v>2509</v>
       </c>
       <c r="B699" s="6">
         <v>44171.0</v>
       </c>
       <c r="C699" s="34"/>
-      <c r="D699" s="80" t="s">
+      <c r="D699" s="7" t="s">
         <v>2139</v>
       </c>
       <c r="E699" s="7" t="s">
@@ -50387,29 +50365,29 @@
       <c r="G699" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H699" s="74" t="s">
+      <c r="H699" s="8" t="s">
         <v>2503</v>
       </c>
-      <c r="I699" s="79" t="s">
+      <c r="I699" s="16" t="s">
         <v>2504</v>
       </c>
-      <c r="J699" s="76" t="s">
+      <c r="J699" s="12" t="s">
         <v>1442</v>
       </c>
-      <c r="K699" s="77" t="s">
+      <c r="K699" s="13" t="s">
         <v>2505</v>
       </c>
-      <c r="L699" s="76" t="s">
+      <c r="L699" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M699" s="77" t="s">
+      <c r="M699" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N699" s="25"/>
-      <c r="O699" s="74" t="s">
+      <c r="O699" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P699" s="74" t="s">
+      <c r="P699" s="8" t="s">
         <v>2506</v>
       </c>
       <c r="Q699" s="19"/>
@@ -50424,14 +50402,14 @@
       </c>
     </row>
     <row r="700">
-      <c r="A700" s="79" t="s">
+      <c r="A700" s="16" t="s">
         <v>2510</v>
       </c>
       <c r="B700" s="6">
         <v>44171.0</v>
       </c>
       <c r="C700" s="34"/>
-      <c r="D700" s="80" t="s">
+      <c r="D700" s="7" t="s">
         <v>2139</v>
       </c>
       <c r="E700" s="7" t="s">
@@ -50441,29 +50419,29 @@
       <c r="G700" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H700" s="74" t="s">
+      <c r="H700" s="8" t="s">
         <v>2503</v>
       </c>
-      <c r="I700" s="79" t="s">
+      <c r="I700" s="16" t="s">
         <v>2504</v>
       </c>
       <c r="J700" s="10">
         <v>44166.0</v>
       </c>
-      <c r="K700" s="77" t="s">
+      <c r="K700" s="13" t="s">
         <v>2505</v>
       </c>
-      <c r="L700" s="76" t="s">
+      <c r="L700" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M700" s="81" t="s">
+      <c r="M700" s="75" t="s">
         <v>2511</v>
       </c>
       <c r="N700" s="25"/>
-      <c r="O700" s="74" t="s">
+      <c r="O700" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P700" s="74" t="s">
+      <c r="P700" s="8" t="s">
         <v>2506</v>
       </c>
       <c r="Q700" s="19"/>
@@ -50478,14 +50456,14 @@
       </c>
     </row>
     <row r="701">
-      <c r="A701" s="79" t="s">
+      <c r="A701" s="16" t="s">
         <v>2512</v>
       </c>
       <c r="B701" s="6">
         <v>44171.0</v>
       </c>
       <c r="C701" s="34"/>
-      <c r="D701" s="80" t="s">
+      <c r="D701" s="7" t="s">
         <v>2139</v>
       </c>
       <c r="E701" s="7" t="s">
@@ -50495,29 +50473,29 @@
       <c r="G701" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H701" s="74" t="s">
+      <c r="H701" s="8" t="s">
         <v>2503</v>
       </c>
-      <c r="I701" s="79" t="s">
+      <c r="I701" s="16" t="s">
         <v>2504</v>
       </c>
-      <c r="J701" s="76" t="s">
+      <c r="J701" s="12" t="s">
         <v>1442</v>
       </c>
-      <c r="K701" s="77" t="s">
+      <c r="K701" s="13" t="s">
         <v>2505</v>
       </c>
-      <c r="L701" s="76" t="s">
+      <c r="L701" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M701" s="77" t="s">
+      <c r="M701" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N701" s="25"/>
-      <c r="O701" s="74" t="s">
+      <c r="O701" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P701" s="74" t="s">
+      <c r="P701" s="8" t="s">
         <v>2506</v>
       </c>
       <c r="Q701" s="19"/>
@@ -50532,14 +50510,14 @@
       </c>
     </row>
     <row r="702">
-      <c r="A702" s="79" t="s">
+      <c r="A702" s="16" t="s">
         <v>2513</v>
       </c>
       <c r="B702" s="6">
         <v>44171.0</v>
       </c>
       <c r="C702" s="34"/>
-      <c r="D702" s="80" t="s">
+      <c r="D702" s="7" t="s">
         <v>2139</v>
       </c>
       <c r="E702" s="7" t="s">
@@ -50549,29 +50527,29 @@
       <c r="G702" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H702" s="74" t="s">
+      <c r="H702" s="8" t="s">
         <v>2503</v>
       </c>
-      <c r="I702" s="79" t="s">
+      <c r="I702" s="16" t="s">
         <v>2504</v>
       </c>
       <c r="J702" s="10">
         <v>44166.0</v>
       </c>
-      <c r="K702" s="77" t="s">
+      <c r="K702" s="13" t="s">
         <v>2505</v>
       </c>
-      <c r="L702" s="76" t="s">
+      <c r="L702" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M702" s="77" t="s">
+      <c r="M702" s="13" t="s">
         <v>2514</v>
       </c>
       <c r="N702" s="25"/>
-      <c r="O702" s="74" t="s">
+      <c r="O702" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P702" s="74" t="s">
+      <c r="P702" s="8" t="s">
         <v>2506</v>
       </c>
       <c r="Q702" s="19"/>
@@ -50586,14 +50564,14 @@
       </c>
     </row>
     <row r="703">
-      <c r="A703" s="79" t="s">
+      <c r="A703" s="16" t="s">
         <v>2515</v>
       </c>
       <c r="B703" s="6">
         <v>44171.0</v>
       </c>
       <c r="C703" s="34"/>
-      <c r="D703" s="80" t="s">
+      <c r="D703" s="7" t="s">
         <v>2139</v>
       </c>
       <c r="E703" s="7" t="s">
@@ -50603,29 +50581,29 @@
       <c r="G703" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H703" s="74" t="s">
+      <c r="H703" s="8" t="s">
         <v>2503</v>
       </c>
-      <c r="I703" s="79" t="s">
+      <c r="I703" s="16" t="s">
         <v>2504</v>
       </c>
-      <c r="J703" s="76" t="s">
+      <c r="J703" s="12" t="s">
         <v>1442</v>
       </c>
-      <c r="K703" s="77" t="s">
+      <c r="K703" s="13" t="s">
         <v>2505</v>
       </c>
-      <c r="L703" s="76" t="s">
+      <c r="L703" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M703" s="77" t="s">
+      <c r="M703" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N703" s="25"/>
-      <c r="O703" s="74" t="s">
+      <c r="O703" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P703" s="74" t="s">
+      <c r="P703" s="8" t="s">
         <v>2506</v>
       </c>
       <c r="Q703" s="19"/>
@@ -50640,14 +50618,14 @@
       </c>
     </row>
     <row r="704">
-      <c r="A704" s="79" t="s">
+      <c r="A704" s="16" t="s">
         <v>2516</v>
       </c>
       <c r="B704" s="6">
         <v>44171.0</v>
       </c>
       <c r="C704" s="34"/>
-      <c r="D704" s="80" t="s">
+      <c r="D704" s="7" t="s">
         <v>2139</v>
       </c>
       <c r="E704" s="7" t="s">
@@ -50657,29 +50635,29 @@
       <c r="G704" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H704" s="74" t="s">
+      <c r="H704" s="8" t="s">
         <v>2503</v>
       </c>
-      <c r="I704" s="79" t="s">
+      <c r="I704" s="16" t="s">
         <v>2504</v>
       </c>
-      <c r="J704" s="76" t="s">
+      <c r="J704" s="12" t="s">
         <v>1442</v>
       </c>
-      <c r="K704" s="77" t="s">
+      <c r="K704" s="13" t="s">
         <v>2505</v>
       </c>
-      <c r="L704" s="76" t="s">
+      <c r="L704" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M704" s="77" t="s">
+      <c r="M704" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N704" s="25"/>
-      <c r="O704" s="74" t="s">
+      <c r="O704" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P704" s="74" t="s">
+      <c r="P704" s="8" t="s">
         <v>2506</v>
       </c>
       <c r="Q704" s="19"/>
@@ -50694,14 +50672,14 @@
       </c>
     </row>
     <row r="705">
-      <c r="A705" s="79" t="s">
+      <c r="A705" s="16" t="s">
         <v>2517</v>
       </c>
       <c r="B705" s="6">
         <v>44171.0</v>
       </c>
       <c r="C705" s="34"/>
-      <c r="D705" s="80" t="s">
+      <c r="D705" s="7" t="s">
         <v>2139</v>
       </c>
       <c r="E705" s="7" t="s">
@@ -50711,29 +50689,29 @@
       <c r="G705" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H705" s="74" t="s">
+      <c r="H705" s="8" t="s">
         <v>2503</v>
       </c>
-      <c r="I705" s="79" t="s">
+      <c r="I705" s="16" t="s">
         <v>2504</v>
       </c>
-      <c r="J705" s="76" t="s">
+      <c r="J705" s="12" t="s">
         <v>1442</v>
       </c>
-      <c r="K705" s="77" t="s">
+      <c r="K705" s="13" t="s">
         <v>2505</v>
       </c>
-      <c r="L705" s="76" t="s">
+      <c r="L705" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M705" s="77" t="s">
+      <c r="M705" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N705" s="25"/>
-      <c r="O705" s="74" t="s">
+      <c r="O705" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P705" s="74" t="s">
+      <c r="P705" s="8" t="s">
         <v>2506</v>
       </c>
       <c r="Q705" s="19"/>
@@ -50748,14 +50726,14 @@
       </c>
     </row>
     <row r="706">
-      <c r="A706" s="79" t="s">
+      <c r="A706" s="16" t="s">
         <v>2518</v>
       </c>
       <c r="B706" s="6">
         <v>44171.0</v>
       </c>
       <c r="C706" s="34"/>
-      <c r="D706" s="80" t="s">
+      <c r="D706" s="7" t="s">
         <v>2139</v>
       </c>
       <c r="E706" s="7" t="s">
@@ -50765,29 +50743,29 @@
       <c r="G706" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H706" s="74" t="s">
+      <c r="H706" s="8" t="s">
         <v>2503</v>
       </c>
-      <c r="I706" s="79" t="s">
+      <c r="I706" s="16" t="s">
         <v>2504</v>
       </c>
-      <c r="J706" s="76" t="s">
+      <c r="J706" s="12" t="s">
         <v>1442</v>
       </c>
-      <c r="K706" s="77" t="s">
+      <c r="K706" s="13" t="s">
         <v>2505</v>
       </c>
-      <c r="L706" s="76" t="s">
+      <c r="L706" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M706" s="77" t="s">
+      <c r="M706" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N706" s="25"/>
-      <c r="O706" s="74" t="s">
+      <c r="O706" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P706" s="74" t="s">
+      <c r="P706" s="8" t="s">
         <v>2506</v>
       </c>
       <c r="Q706" s="19"/>
@@ -50802,14 +50780,14 @@
       </c>
     </row>
     <row r="707">
-      <c r="A707" s="79" t="s">
+      <c r="A707" s="16" t="s">
         <v>2519</v>
       </c>
       <c r="B707" s="6">
         <v>44171.0</v>
       </c>
       <c r="C707" s="34"/>
-      <c r="D707" s="80" t="s">
+      <c r="D707" s="7" t="s">
         <v>2139</v>
       </c>
       <c r="E707" s="7" t="s">
@@ -50819,29 +50797,29 @@
       <c r="G707" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H707" s="74" t="s">
+      <c r="H707" s="8" t="s">
         <v>2503</v>
       </c>
-      <c r="I707" s="79" t="s">
+      <c r="I707" s="16" t="s">
         <v>2504</v>
       </c>
-      <c r="J707" s="76" t="s">
+      <c r="J707" s="12" t="s">
         <v>1442</v>
       </c>
-      <c r="K707" s="77" t="s">
+      <c r="K707" s="13" t="s">
         <v>2505</v>
       </c>
-      <c r="L707" s="76" t="s">
+      <c r="L707" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M707" s="77" t="s">
+      <c r="M707" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N707" s="25"/>
-      <c r="O707" s="74" t="s">
+      <c r="O707" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P707" s="74" t="s">
+      <c r="P707" s="8" t="s">
         <v>2506</v>
       </c>
       <c r="Q707" s="19"/>
@@ -50856,14 +50834,14 @@
       </c>
     </row>
     <row r="708">
-      <c r="A708" s="79" t="s">
+      <c r="A708" s="16" t="s">
         <v>2520</v>
       </c>
       <c r="B708" s="6">
         <v>44171.0</v>
       </c>
       <c r="C708" s="34"/>
-      <c r="D708" s="80" t="s">
+      <c r="D708" s="7" t="s">
         <v>2139</v>
       </c>
       <c r="E708" s="7" t="s">
@@ -50873,29 +50851,29 @@
       <c r="G708" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H708" s="74" t="s">
+      <c r="H708" s="8" t="s">
         <v>2503</v>
       </c>
-      <c r="I708" s="79" t="s">
+      <c r="I708" s="16" t="s">
         <v>2504</v>
       </c>
-      <c r="J708" s="76" t="s">
+      <c r="J708" s="12" t="s">
         <v>1442</v>
       </c>
-      <c r="K708" s="77" t="s">
+      <c r="K708" s="13" t="s">
         <v>2505</v>
       </c>
-      <c r="L708" s="76" t="s">
+      <c r="L708" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M708" s="77" t="s">
+      <c r="M708" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N708" s="25"/>
-      <c r="O708" s="74" t="s">
+      <c r="O708" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P708" s="74" t="s">
+      <c r="P708" s="8" t="s">
         <v>2506</v>
       </c>
       <c r="Q708" s="19"/>
@@ -50910,14 +50888,14 @@
       </c>
     </row>
     <row r="709">
-      <c r="A709" s="79" t="s">
+      <c r="A709" s="16" t="s">
         <v>2521</v>
       </c>
       <c r="B709" s="6">
         <v>44171.0</v>
       </c>
       <c r="C709" s="34"/>
-      <c r="D709" s="80" t="s">
+      <c r="D709" s="7" t="s">
         <v>2139</v>
       </c>
       <c r="E709" s="7" t="s">
@@ -50927,29 +50905,29 @@
       <c r="G709" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H709" s="74" t="s">
+      <c r="H709" s="8" t="s">
         <v>2503</v>
       </c>
-      <c r="I709" s="79" t="s">
+      <c r="I709" s="16" t="s">
         <v>2504</v>
       </c>
-      <c r="J709" s="76" t="s">
+      <c r="J709" s="12" t="s">
         <v>1442</v>
       </c>
-      <c r="K709" s="77" t="s">
+      <c r="K709" s="13" t="s">
         <v>2505</v>
       </c>
-      <c r="L709" s="76" t="s">
+      <c r="L709" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M709" s="77" t="s">
+      <c r="M709" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N709" s="25"/>
-      <c r="O709" s="74" t="s">
+      <c r="O709" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P709" s="74" t="s">
+      <c r="P709" s="8" t="s">
         <v>2506</v>
       </c>
       <c r="Q709" s="19"/>
@@ -50964,14 +50942,14 @@
       </c>
     </row>
     <row r="710">
-      <c r="A710" s="79" t="s">
+      <c r="A710" s="16" t="s">
         <v>2522</v>
       </c>
       <c r="B710" s="6">
         <v>44171.0</v>
       </c>
       <c r="C710" s="34"/>
-      <c r="D710" s="80" t="s">
+      <c r="D710" s="7" t="s">
         <v>2139</v>
       </c>
       <c r="E710" s="7" t="s">
@@ -50981,29 +50959,29 @@
       <c r="G710" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H710" s="74" t="s">
+      <c r="H710" s="8" t="s">
         <v>2503</v>
       </c>
-      <c r="I710" s="79" t="s">
+      <c r="I710" s="16" t="s">
         <v>2504</v>
       </c>
-      <c r="J710" s="76" t="s">
+      <c r="J710" s="12" t="s">
         <v>1442</v>
       </c>
-      <c r="K710" s="77" t="s">
+      <c r="K710" s="13" t="s">
         <v>2505</v>
       </c>
-      <c r="L710" s="76" t="s">
+      <c r="L710" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M710" s="77" t="s">
+      <c r="M710" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N710" s="25"/>
-      <c r="O710" s="74" t="s">
+      <c r="O710" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P710" s="74" t="s">
+      <c r="P710" s="8" t="s">
         <v>2506</v>
       </c>
       <c r="Q710" s="19"/>
@@ -51018,14 +50996,14 @@
       </c>
     </row>
     <row r="711">
-      <c r="A711" s="79" t="s">
+      <c r="A711" s="16" t="s">
         <v>2523</v>
       </c>
       <c r="B711" s="6">
         <v>44171.0</v>
       </c>
       <c r="C711" s="34"/>
-      <c r="D711" s="80" t="s">
+      <c r="D711" s="7" t="s">
         <v>2139</v>
       </c>
       <c r="E711" s="7" t="s">
@@ -51035,29 +51013,29 @@
       <c r="G711" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H711" s="74" t="s">
+      <c r="H711" s="8" t="s">
         <v>2503</v>
       </c>
-      <c r="I711" s="79" t="s">
+      <c r="I711" s="16" t="s">
         <v>2504</v>
       </c>
-      <c r="J711" s="76" t="s">
+      <c r="J711" s="12" t="s">
         <v>1442</v>
       </c>
-      <c r="K711" s="77" t="s">
+      <c r="K711" s="13" t="s">
         <v>2505</v>
       </c>
-      <c r="L711" s="76" t="s">
+      <c r="L711" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M711" s="77" t="s">
+      <c r="M711" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N711" s="25"/>
-      <c r="O711" s="74" t="s">
+      <c r="O711" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P711" s="74" t="s">
+      <c r="P711" s="8" t="s">
         <v>2506</v>
       </c>
       <c r="Q711" s="19"/>
@@ -51072,14 +51050,14 @@
       </c>
     </row>
     <row r="712">
-      <c r="A712" s="79" t="s">
+      <c r="A712" s="16" t="s">
         <v>2524</v>
       </c>
       <c r="B712" s="6">
         <v>44171.0</v>
       </c>
       <c r="C712" s="34"/>
-      <c r="D712" s="80" t="s">
+      <c r="D712" s="7" t="s">
         <v>2139</v>
       </c>
       <c r="E712" s="7" t="s">
@@ -51089,29 +51067,29 @@
       <c r="G712" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H712" s="74" t="s">
+      <c r="H712" s="8" t="s">
         <v>2503</v>
       </c>
-      <c r="I712" s="79" t="s">
+      <c r="I712" s="16" t="s">
         <v>2504</v>
       </c>
-      <c r="J712" s="76" t="s">
+      <c r="J712" s="12" t="s">
         <v>1442</v>
       </c>
-      <c r="K712" s="77" t="s">
+      <c r="K712" s="13" t="s">
         <v>2505</v>
       </c>
-      <c r="L712" s="76" t="s">
+      <c r="L712" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M712" s="77" t="s">
+      <c r="M712" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N712" s="25"/>
-      <c r="O712" s="74" t="s">
+      <c r="O712" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P712" s="74" t="s">
+      <c r="P712" s="8" t="s">
         <v>2506</v>
       </c>
       <c r="Q712" s="19"/>
@@ -51126,14 +51104,14 @@
       </c>
     </row>
     <row r="713">
-      <c r="A713" s="79" t="s">
+      <c r="A713" s="16" t="s">
         <v>2525</v>
       </c>
       <c r="B713" s="6">
         <v>44171.0</v>
       </c>
       <c r="C713" s="34"/>
-      <c r="D713" s="80" t="s">
+      <c r="D713" s="7" t="s">
         <v>2139</v>
       </c>
       <c r="E713" s="7" t="s">
@@ -51143,29 +51121,29 @@
       <c r="G713" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H713" s="74" t="s">
+      <c r="H713" s="8" t="s">
         <v>2503</v>
       </c>
-      <c r="I713" s="79" t="s">
+      <c r="I713" s="16" t="s">
         <v>2504</v>
       </c>
-      <c r="J713" s="76" t="s">
+      <c r="J713" s="12" t="s">
         <v>1442</v>
       </c>
-      <c r="K713" s="77" t="s">
+      <c r="K713" s="13" t="s">
         <v>2505</v>
       </c>
-      <c r="L713" s="76" t="s">
+      <c r="L713" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M713" s="77" t="s">
+      <c r="M713" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N713" s="25"/>
-      <c r="O713" s="74" t="s">
+      <c r="O713" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P713" s="74" t="s">
+      <c r="P713" s="8" t="s">
         <v>2506</v>
       </c>
       <c r="Q713" s="19"/>
@@ -51180,7 +51158,7 @@
       </c>
     </row>
     <row r="714">
-      <c r="A714" s="79" t="s">
+      <c r="A714" s="16" t="s">
         <v>2526</v>
       </c>
       <c r="B714" s="6">
@@ -51189,7 +51167,7 @@
       <c r="C714" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D714" s="80" t="s">
+      <c r="D714" s="7" t="s">
         <v>116</v>
       </c>
       <c r="E714" s="7" t="s">
@@ -51199,13 +51177,13 @@
       <c r="G714" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H714" s="74" t="s">
+      <c r="H714" s="8" t="s">
         <v>2527</v>
       </c>
-      <c r="I714" s="75">
+      <c r="I714" s="9">
         <v>44154.0</v>
       </c>
-      <c r="J714" s="76" t="s">
+      <c r="J714" s="12" t="s">
         <v>1442</v>
       </c>
       <c r="K714" s="13" t="s">
@@ -51214,14 +51192,14 @@
       <c r="L714" s="12" t="s">
         <v>1674</v>
       </c>
-      <c r="M714" s="77" t="s">
+      <c r="M714" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N714" s="25"/>
-      <c r="O714" s="74" t="s">
+      <c r="O714" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P714" s="74" t="s">
+      <c r="P714" s="8" t="s">
         <v>2528</v>
       </c>
       <c r="Q714" s="19"/>
@@ -51236,7 +51214,7 @@
       </c>
     </row>
     <row r="715">
-      <c r="A715" s="79" t="s">
+      <c r="A715" s="16" t="s">
         <v>2529</v>
       </c>
       <c r="B715" s="6">
@@ -51245,7 +51223,7 @@
       <c r="C715" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D715" s="80" t="s">
+      <c r="D715" s="7" t="s">
         <v>116</v>
       </c>
       <c r="E715" s="7" t="s">
@@ -51255,13 +51233,13 @@
       <c r="G715" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H715" s="74" t="s">
+      <c r="H715" s="8" t="s">
         <v>2263</v>
       </c>
-      <c r="I715" s="75">
+      <c r="I715" s="9">
         <v>44147.0</v>
       </c>
-      <c r="J715" s="76" t="s">
+      <c r="J715" s="12" t="s">
         <v>1442</v>
       </c>
       <c r="K715" s="13" t="s">
@@ -51270,14 +51248,14 @@
       <c r="L715" s="12" t="s">
         <v>1674</v>
       </c>
-      <c r="M715" s="77" t="s">
+      <c r="M715" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N715" s="25"/>
-      <c r="O715" s="74" t="s">
+      <c r="O715" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P715" s="74" t="s">
+      <c r="P715" s="8" t="s">
         <v>2530</v>
       </c>
       <c r="Q715" s="19"/>
@@ -51292,7 +51270,7 @@
       </c>
     </row>
     <row r="716">
-      <c r="A716" s="79" t="s">
+      <c r="A716" s="16" t="s">
         <v>2531</v>
       </c>
       <c r="B716" s="6">
@@ -51301,7 +51279,7 @@
       <c r="C716" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D716" s="80" t="s">
+      <c r="D716" s="7" t="s">
         <v>76</v>
       </c>
       <c r="E716" s="7" t="s">
@@ -51311,13 +51289,13 @@
       <c r="G716" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H716" s="74" t="s">
+      <c r="H716" s="8" t="s">
         <v>2318</v>
       </c>
-      <c r="I716" s="75">
+      <c r="I716" s="9">
         <v>44146.0</v>
       </c>
-      <c r="J716" s="76" t="s">
+      <c r="J716" s="12" t="s">
         <v>1442</v>
       </c>
       <c r="K716" s="13" t="s">
@@ -51326,14 +51304,14 @@
       <c r="L716" s="12" t="s">
         <v>1674</v>
       </c>
-      <c r="M716" s="77" t="s">
+      <c r="M716" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N716" s="25"/>
-      <c r="O716" s="74" t="s">
+      <c r="O716" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P716" s="74" t="s">
+      <c r="P716" s="8" t="s">
         <v>2532</v>
       </c>
       <c r="Q716" s="19"/>
@@ -51348,7 +51326,7 @@
       </c>
     </row>
     <row r="717">
-      <c r="A717" s="79" t="s">
+      <c r="A717" s="16" t="s">
         <v>2533</v>
       </c>
       <c r="B717" s="6">
@@ -51357,7 +51335,7 @@
       <c r="C717" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D717" s="80" t="s">
+      <c r="D717" s="7" t="s">
         <v>76</v>
       </c>
       <c r="E717" s="7" t="s">
@@ -51367,29 +51345,29 @@
       <c r="G717" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H717" s="74" t="s">
+      <c r="H717" s="8" t="s">
         <v>2534</v>
       </c>
-      <c r="I717" s="75">
+      <c r="I717" s="9">
         <v>44157.0</v>
       </c>
-      <c r="J717" s="76" t="s">
+      <c r="J717" s="12" t="s">
         <v>1442</v>
       </c>
       <c r="K717" s="13" t="s">
         <v>2535</v>
       </c>
-      <c r="L717" s="76" t="s">
+      <c r="L717" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M717" s="77" t="s">
+      <c r="M717" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N717" s="25"/>
-      <c r="O717" s="74" t="s">
+      <c r="O717" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P717" s="74" t="s">
+      <c r="P717" s="8" t="s">
         <v>2182</v>
       </c>
       <c r="Q717" s="19"/>
@@ -51404,7 +51382,7 @@
       </c>
     </row>
     <row r="718">
-      <c r="A718" s="79" t="s">
+      <c r="A718" s="16" t="s">
         <v>2536</v>
       </c>
       <c r="B718" s="6">
@@ -51413,7 +51391,7 @@
       <c r="C718" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D718" s="80" t="s">
+      <c r="D718" s="7" t="s">
         <v>59</v>
       </c>
       <c r="E718" s="7" t="s">
@@ -51423,13 +51401,13 @@
       <c r="G718" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H718" s="74" t="s">
+      <c r="H718" s="8" t="s">
         <v>2537</v>
       </c>
-      <c r="I718" s="75">
+      <c r="I718" s="9">
         <v>44155.0</v>
       </c>
-      <c r="J718" s="76" t="s">
+      <c r="J718" s="12" t="s">
         <v>1442</v>
       </c>
       <c r="K718" s="13" t="s">
@@ -51438,14 +51416,14 @@
       <c r="L718" s="12" t="s">
         <v>1674</v>
       </c>
-      <c r="M718" s="77" t="s">
+      <c r="M718" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N718" s="25"/>
-      <c r="O718" s="74" t="s">
+      <c r="O718" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P718" s="74" t="s">
+      <c r="P718" s="8" t="s">
         <v>2538</v>
       </c>
       <c r="Q718" s="19"/>
@@ -51460,8 +51438,8 @@
       </c>
     </row>
     <row r="719">
-      <c r="A719" s="82"/>
-      <c r="B719" s="83"/>
+      <c r="A719" s="76"/>
+      <c r="B719" s="77"/>
       <c r="C719" s="34"/>
       <c r="D719" s="34"/>
       <c r="E719" s="34"/>
@@ -51486,8 +51464,8 @@
       </c>
     </row>
     <row r="720">
-      <c r="A720" s="82"/>
-      <c r="B720" s="83"/>
+      <c r="A720" s="76"/>
+      <c r="B720" s="77"/>
       <c r="C720" s="34"/>
       <c r="D720" s="34"/>
       <c r="E720" s="34"/>
@@ -51512,8 +51490,8 @@
       </c>
     </row>
     <row r="721">
-      <c r="A721" s="82"/>
-      <c r="B721" s="83"/>
+      <c r="A721" s="76"/>
+      <c r="B721" s="77"/>
       <c r="C721" s="34"/>
       <c r="D721" s="34"/>
       <c r="E721" s="34"/>
@@ -51538,8 +51516,8 @@
       </c>
     </row>
     <row r="722">
-      <c r="A722" s="82"/>
-      <c r="B722" s="83"/>
+      <c r="A722" s="76"/>
+      <c r="B722" s="77"/>
       <c r="C722" s="34"/>
       <c r="D722" s="34"/>
       <c r="E722" s="34"/>
@@ -51564,8 +51542,8 @@
       </c>
     </row>
     <row r="723">
-      <c r="A723" s="82"/>
-      <c r="B723" s="83"/>
+      <c r="A723" s="76"/>
+      <c r="B723" s="77"/>
       <c r="C723" s="34"/>
       <c r="D723" s="34"/>
       <c r="E723" s="34"/>
@@ -51590,8 +51568,8 @@
       </c>
     </row>
     <row r="724">
-      <c r="A724" s="82"/>
-      <c r="B724" s="83"/>
+      <c r="A724" s="76"/>
+      <c r="B724" s="77"/>
       <c r="C724" s="34"/>
       <c r="D724" s="34"/>
       <c r="E724" s="34"/>
@@ -51616,8 +51594,8 @@
       </c>
     </row>
     <row r="725">
-      <c r="A725" s="82"/>
-      <c r="B725" s="83"/>
+      <c r="A725" s="76"/>
+      <c r="B725" s="77"/>
       <c r="C725" s="34"/>
       <c r="D725" s="34"/>
       <c r="E725" s="34"/>
@@ -51642,8 +51620,8 @@
       </c>
     </row>
     <row r="726">
-      <c r="A726" s="82"/>
-      <c r="B726" s="83"/>
+      <c r="A726" s="76"/>
+      <c r="B726" s="77"/>
       <c r="C726" s="34"/>
       <c r="D726" s="34"/>
       <c r="E726" s="34"/>
@@ -51668,8 +51646,8 @@
       </c>
     </row>
     <row r="727">
-      <c r="A727" s="82"/>
-      <c r="B727" s="83"/>
+      <c r="A727" s="76"/>
+      <c r="B727" s="77"/>
       <c r="C727" s="34"/>
       <c r="D727" s="34"/>
       <c r="E727" s="34"/>
@@ -51694,8 +51672,8 @@
       </c>
     </row>
     <row r="728">
-      <c r="A728" s="82"/>
-      <c r="B728" s="83"/>
+      <c r="A728" s="76"/>
+      <c r="B728" s="77"/>
       <c r="C728" s="34"/>
       <c r="D728" s="34"/>
       <c r="E728" s="34"/>
@@ -51720,8 +51698,8 @@
       </c>
     </row>
     <row r="729">
-      <c r="A729" s="82"/>
-      <c r="B729" s="83"/>
+      <c r="A729" s="76"/>
+      <c r="B729" s="77"/>
       <c r="C729" s="34"/>
       <c r="D729" s="34"/>
       <c r="E729" s="34"/>
@@ -51746,8 +51724,8 @@
       </c>
     </row>
     <row r="730">
-      <c r="A730" s="82"/>
-      <c r="B730" s="83"/>
+      <c r="A730" s="76"/>
+      <c r="B730" s="77"/>
       <c r="C730" s="34"/>
       <c r="D730" s="34"/>
       <c r="E730" s="34"/>
@@ -51772,8 +51750,8 @@
       </c>
     </row>
     <row r="731">
-      <c r="A731" s="82"/>
-      <c r="B731" s="83"/>
+      <c r="A731" s="76"/>
+      <c r="B731" s="77"/>
       <c r="C731" s="34"/>
       <c r="D731" s="34"/>
       <c r="E731" s="34"/>
@@ -51798,8 +51776,8 @@
       </c>
     </row>
     <row r="732">
-      <c r="A732" s="82"/>
-      <c r="B732" s="83"/>
+      <c r="A732" s="76"/>
+      <c r="B732" s="77"/>
       <c r="C732" s="34"/>
       <c r="D732" s="34"/>
       <c r="E732" s="34"/>
@@ -51824,8 +51802,8 @@
       </c>
     </row>
     <row r="733">
-      <c r="A733" s="82"/>
-      <c r="B733" s="83"/>
+      <c r="A733" s="76"/>
+      <c r="B733" s="77"/>
       <c r="C733" s="34"/>
       <c r="D733" s="34"/>
       <c r="E733" s="34"/>
@@ -51850,8 +51828,8 @@
       </c>
     </row>
     <row r="734">
-      <c r="A734" s="82"/>
-      <c r="B734" s="83"/>
+      <c r="A734" s="76"/>
+      <c r="B734" s="77"/>
       <c r="C734" s="34"/>
       <c r="D734" s="34"/>
       <c r="E734" s="34"/>
@@ -51876,8 +51854,8 @@
       </c>
     </row>
     <row r="735">
-      <c r="A735" s="82"/>
-      <c r="B735" s="83"/>
+      <c r="A735" s="76"/>
+      <c r="B735" s="77"/>
       <c r="C735" s="34"/>
       <c r="D735" s="34"/>
       <c r="E735" s="34"/>
@@ -51902,8 +51880,8 @@
       </c>
     </row>
     <row r="736">
-      <c r="A736" s="82"/>
-      <c r="B736" s="83"/>
+      <c r="A736" s="76"/>
+      <c r="B736" s="77"/>
       <c r="C736" s="34"/>
       <c r="D736" s="34"/>
       <c r="E736" s="34"/>
@@ -51928,8 +51906,8 @@
       </c>
     </row>
     <row r="737">
-      <c r="A737" s="82"/>
-      <c r="B737" s="83"/>
+      <c r="A737" s="76"/>
+      <c r="B737" s="77"/>
       <c r="C737" s="34"/>
       <c r="D737" s="34"/>
       <c r="E737" s="34"/>
@@ -51954,8 +51932,8 @@
       </c>
     </row>
     <row r="738">
-      <c r="A738" s="82"/>
-      <c r="B738" s="83"/>
+      <c r="A738" s="76"/>
+      <c r="B738" s="77"/>
       <c r="C738" s="34"/>
       <c r="D738" s="34"/>
       <c r="E738" s="34"/>
@@ -51980,8 +51958,8 @@
       </c>
     </row>
     <row r="739">
-      <c r="A739" s="82"/>
-      <c r="B739" s="83"/>
+      <c r="A739" s="76"/>
+      <c r="B739" s="77"/>
       <c r="C739" s="34"/>
       <c r="D739" s="34"/>
       <c r="E739" s="34"/>
@@ -52006,8 +51984,8 @@
       </c>
     </row>
     <row r="740">
-      <c r="A740" s="82"/>
-      <c r="B740" s="83"/>
+      <c r="A740" s="76"/>
+      <c r="B740" s="77"/>
       <c r="C740" s="34"/>
       <c r="D740" s="34"/>
       <c r="E740" s="34"/>
@@ -52032,8 +52010,8 @@
       </c>
     </row>
     <row r="741">
-      <c r="A741" s="82"/>
-      <c r="B741" s="83"/>
+      <c r="A741" s="76"/>
+      <c r="B741" s="77"/>
       <c r="C741" s="34"/>
       <c r="D741" s="34"/>
       <c r="E741" s="34"/>
@@ -52058,8 +52036,8 @@
       </c>
     </row>
     <row r="742">
-      <c r="A742" s="82"/>
-      <c r="B742" s="83"/>
+      <c r="A742" s="76"/>
+      <c r="B742" s="77"/>
       <c r="C742" s="34"/>
       <c r="D742" s="34"/>
       <c r="E742" s="34"/>
@@ -52084,8 +52062,8 @@
       </c>
     </row>
     <row r="743">
-      <c r="A743" s="82"/>
-      <c r="B743" s="83"/>
+      <c r="A743" s="76"/>
+      <c r="B743" s="77"/>
       <c r="C743" s="34"/>
       <c r="D743" s="34"/>
       <c r="E743" s="34"/>
@@ -52110,8 +52088,8 @@
       </c>
     </row>
     <row r="744">
-      <c r="A744" s="82"/>
-      <c r="B744" s="83"/>
+      <c r="A744" s="76"/>
+      <c r="B744" s="77"/>
       <c r="C744" s="34"/>
       <c r="D744" s="34"/>
       <c r="E744" s="34"/>
@@ -52136,8 +52114,8 @@
       </c>
     </row>
     <row r="745">
-      <c r="A745" s="82"/>
-      <c r="B745" s="83"/>
+      <c r="A745" s="76"/>
+      <c r="B745" s="77"/>
       <c r="C745" s="34"/>
       <c r="D745" s="34"/>
       <c r="E745" s="34"/>
@@ -52162,8 +52140,8 @@
       </c>
     </row>
     <row r="746">
-      <c r="A746" s="82"/>
-      <c r="B746" s="83"/>
+      <c r="A746" s="76"/>
+      <c r="B746" s="77"/>
       <c r="C746" s="34"/>
       <c r="D746" s="34"/>
       <c r="E746" s="34"/>
@@ -52188,8 +52166,8 @@
       </c>
     </row>
     <row r="747">
-      <c r="A747" s="82"/>
-      <c r="B747" s="83"/>
+      <c r="A747" s="76"/>
+      <c r="B747" s="77"/>
       <c r="C747" s="34"/>
       <c r="D747" s="34"/>
       <c r="E747" s="34"/>
@@ -52214,8 +52192,8 @@
       </c>
     </row>
     <row r="748">
-      <c r="A748" s="82"/>
-      <c r="B748" s="83"/>
+      <c r="A748" s="76"/>
+      <c r="B748" s="77"/>
       <c r="C748" s="34"/>
       <c r="D748" s="34"/>
       <c r="E748" s="34"/>
@@ -52240,8 +52218,8 @@
       </c>
     </row>
     <row r="749">
-      <c r="A749" s="82"/>
-      <c r="B749" s="83"/>
+      <c r="A749" s="76"/>
+      <c r="B749" s="77"/>
       <c r="C749" s="34"/>
       <c r="D749" s="34"/>
       <c r="E749" s="34"/>
@@ -52266,8 +52244,8 @@
       </c>
     </row>
     <row r="750">
-      <c r="A750" s="82"/>
-      <c r="B750" s="83"/>
+      <c r="A750" s="76"/>
+      <c r="B750" s="77"/>
       <c r="C750" s="34"/>
       <c r="D750" s="34"/>
       <c r="E750" s="34"/>
@@ -52292,8 +52270,8 @@
       </c>
     </row>
     <row r="751">
-      <c r="A751" s="82"/>
-      <c r="B751" s="83"/>
+      <c r="A751" s="76"/>
+      <c r="B751" s="77"/>
       <c r="C751" s="34"/>
       <c r="D751" s="34"/>
       <c r="E751" s="34"/>
@@ -52318,8 +52296,8 @@
       </c>
     </row>
     <row r="752">
-      <c r="A752" s="82"/>
-      <c r="B752" s="83"/>
+      <c r="A752" s="76"/>
+      <c r="B752" s="77"/>
       <c r="C752" s="34"/>
       <c r="D752" s="34"/>
       <c r="E752" s="34"/>
@@ -52344,8 +52322,8 @@
       </c>
     </row>
     <row r="753">
-      <c r="A753" s="82"/>
-      <c r="B753" s="83"/>
+      <c r="A753" s="76"/>
+      <c r="B753" s="77"/>
       <c r="C753" s="34"/>
       <c r="D753" s="34"/>
       <c r="E753" s="34"/>
@@ -52370,8 +52348,8 @@
       </c>
     </row>
     <row r="754">
-      <c r="A754" s="82"/>
-      <c r="B754" s="83"/>
+      <c r="A754" s="76"/>
+      <c r="B754" s="77"/>
       <c r="C754" s="34"/>
       <c r="D754" s="34"/>
       <c r="E754" s="34"/>
@@ -52396,8 +52374,8 @@
       </c>
     </row>
     <row r="755">
-      <c r="A755" s="82"/>
-      <c r="B755" s="83"/>
+      <c r="A755" s="76"/>
+      <c r="B755" s="77"/>
       <c r="C755" s="34"/>
       <c r="D755" s="34"/>
       <c r="E755" s="34"/>
@@ -52422,8 +52400,8 @@
       </c>
     </row>
     <row r="756">
-      <c r="A756" s="82"/>
-      <c r="B756" s="83"/>
+      <c r="A756" s="76"/>
+      <c r="B756" s="77"/>
       <c r="C756" s="34"/>
       <c r="D756" s="34"/>
       <c r="E756" s="34"/>
@@ -52448,8 +52426,8 @@
       </c>
     </row>
     <row r="757">
-      <c r="A757" s="82"/>
-      <c r="B757" s="83"/>
+      <c r="A757" s="76"/>
+      <c r="B757" s="77"/>
       <c r="C757" s="34"/>
       <c r="D757" s="34"/>
       <c r="E757" s="34"/>
@@ -52474,8 +52452,8 @@
       </c>
     </row>
     <row r="758">
-      <c r="A758" s="82"/>
-      <c r="B758" s="83"/>
+      <c r="A758" s="76"/>
+      <c r="B758" s="77"/>
       <c r="C758" s="34"/>
       <c r="D758" s="34"/>
       <c r="E758" s="34"/>
@@ -52500,8 +52478,8 @@
       </c>
     </row>
     <row r="759">
-      <c r="A759" s="82"/>
-      <c r="B759" s="83"/>
+      <c r="A759" s="76"/>
+      <c r="B759" s="77"/>
       <c r="C759" s="34"/>
       <c r="D759" s="34"/>
       <c r="E759" s="34"/>
@@ -52526,8 +52504,8 @@
       </c>
     </row>
     <row r="760">
-      <c r="A760" s="82"/>
-      <c r="B760" s="83"/>
+      <c r="A760" s="76"/>
+      <c r="B760" s="77"/>
       <c r="C760" s="34"/>
       <c r="D760" s="34"/>
       <c r="E760" s="34"/>
@@ -52552,8 +52530,8 @@
       </c>
     </row>
     <row r="761">
-      <c r="A761" s="82"/>
-      <c r="B761" s="83"/>
+      <c r="A761" s="76"/>
+      <c r="B761" s="77"/>
       <c r="C761" s="34"/>
       <c r="D761" s="34"/>
       <c r="E761" s="34"/>
@@ -52578,8 +52556,8 @@
       </c>
     </row>
     <row r="762">
-      <c r="A762" s="82"/>
-      <c r="B762" s="83"/>
+      <c r="A762" s="76"/>
+      <c r="B762" s="77"/>
       <c r="C762" s="34"/>
       <c r="D762" s="34"/>
       <c r="E762" s="34"/>
@@ -52604,8 +52582,8 @@
       </c>
     </row>
     <row r="763">
-      <c r="A763" s="82"/>
-      <c r="B763" s="83"/>
+      <c r="A763" s="76"/>
+      <c r="B763" s="77"/>
       <c r="C763" s="34"/>
       <c r="D763" s="34"/>
       <c r="E763" s="34"/>
@@ -52630,8 +52608,8 @@
       </c>
     </row>
     <row r="764">
-      <c r="A764" s="82"/>
-      <c r="B764" s="83"/>
+      <c r="A764" s="76"/>
+      <c r="B764" s="77"/>
       <c r="C764" s="34"/>
       <c r="D764" s="34"/>
       <c r="E764" s="34"/>
@@ -52656,8 +52634,8 @@
       </c>
     </row>
     <row r="765">
-      <c r="A765" s="82"/>
-      <c r="B765" s="83"/>
+      <c r="A765" s="76"/>
+      <c r="B765" s="77"/>
       <c r="C765" s="34"/>
       <c r="D765" s="34"/>
       <c r="E765" s="34"/>
@@ -52682,8 +52660,8 @@
       </c>
     </row>
     <row r="766">
-      <c r="A766" s="82"/>
-      <c r="B766" s="83"/>
+      <c r="A766" s="76"/>
+      <c r="B766" s="77"/>
       <c r="C766" s="34"/>
       <c r="D766" s="34"/>
       <c r="E766" s="34"/>
@@ -52708,8 +52686,8 @@
       </c>
     </row>
     <row r="767">
-      <c r="A767" s="82"/>
-      <c r="B767" s="83"/>
+      <c r="A767" s="76"/>
+      <c r="B767" s="77"/>
       <c r="C767" s="34"/>
       <c r="D767" s="34"/>
       <c r="E767" s="34"/>
@@ -52734,8 +52712,8 @@
       </c>
     </row>
     <row r="768">
-      <c r="A768" s="82"/>
-      <c r="B768" s="83"/>
+      <c r="A768" s="76"/>
+      <c r="B768" s="77"/>
       <c r="C768" s="34"/>
       <c r="D768" s="34"/>
       <c r="E768" s="34"/>
@@ -52760,8 +52738,8 @@
       </c>
     </row>
     <row r="769">
-      <c r="A769" s="82"/>
-      <c r="B769" s="83"/>
+      <c r="A769" s="76"/>
+      <c r="B769" s="77"/>
       <c r="C769" s="34"/>
       <c r="D769" s="34"/>
       <c r="E769" s="34"/>
@@ -52786,8 +52764,8 @@
       </c>
     </row>
     <row r="770">
-      <c r="A770" s="82"/>
-      <c r="B770" s="83"/>
+      <c r="A770" s="76"/>
+      <c r="B770" s="77"/>
       <c r="C770" s="34"/>
       <c r="D770" s="34"/>
       <c r="E770" s="34"/>
@@ -52812,8 +52790,8 @@
       </c>
     </row>
     <row r="771">
-      <c r="A771" s="82"/>
-      <c r="B771" s="83"/>
+      <c r="A771" s="76"/>
+      <c r="B771" s="77"/>
       <c r="C771" s="34"/>
       <c r="D771" s="34"/>
       <c r="E771" s="34"/>
@@ -52838,8 +52816,8 @@
       </c>
     </row>
     <row r="772">
-      <c r="A772" s="82"/>
-      <c r="B772" s="83"/>
+      <c r="A772" s="76"/>
+      <c r="B772" s="77"/>
       <c r="C772" s="34"/>
       <c r="D772" s="34"/>
       <c r="E772" s="34"/>
@@ -52864,8 +52842,8 @@
       </c>
     </row>
     <row r="773">
-      <c r="A773" s="82"/>
-      <c r="B773" s="83"/>
+      <c r="A773" s="76"/>
+      <c r="B773" s="77"/>
       <c r="C773" s="34"/>
       <c r="D773" s="34"/>
       <c r="E773" s="34"/>
@@ -52890,8 +52868,8 @@
       </c>
     </row>
     <row r="774">
-      <c r="A774" s="82"/>
-      <c r="B774" s="83"/>
+      <c r="A774" s="76"/>
+      <c r="B774" s="77"/>
       <c r="C774" s="34"/>
       <c r="D774" s="34"/>
       <c r="E774" s="34"/>
@@ -52916,8 +52894,8 @@
       </c>
     </row>
     <row r="775">
-      <c r="A775" s="82"/>
-      <c r="B775" s="83"/>
+      <c r="A775" s="76"/>
+      <c r="B775" s="77"/>
       <c r="C775" s="34"/>
       <c r="D775" s="34"/>
       <c r="E775" s="34"/>
@@ -52942,8 +52920,8 @@
       </c>
     </row>
     <row r="776">
-      <c r="A776" s="82"/>
-      <c r="B776" s="83"/>
+      <c r="A776" s="76"/>
+      <c r="B776" s="77"/>
       <c r="C776" s="34"/>
       <c r="D776" s="34"/>
       <c r="E776" s="34"/>
@@ -52968,8 +52946,8 @@
       </c>
     </row>
     <row r="777">
-      <c r="A777" s="82"/>
-      <c r="B777" s="83"/>
+      <c r="A777" s="76"/>
+      <c r="B777" s="77"/>
       <c r="C777" s="34"/>
       <c r="D777" s="34"/>
       <c r="E777" s="34"/>
@@ -52994,8 +52972,8 @@
       </c>
     </row>
     <row r="778">
-      <c r="A778" s="82"/>
-      <c r="B778" s="83"/>
+      <c r="A778" s="76"/>
+      <c r="B778" s="77"/>
       <c r="C778" s="34"/>
       <c r="D778" s="34"/>
       <c r="E778" s="34"/>
@@ -53020,8 +52998,8 @@
       </c>
     </row>
     <row r="779">
-      <c r="A779" s="82"/>
-      <c r="B779" s="83"/>
+      <c r="A779" s="76"/>
+      <c r="B779" s="77"/>
       <c r="C779" s="34"/>
       <c r="D779" s="34"/>
       <c r="E779" s="34"/>
@@ -53046,8 +53024,8 @@
       </c>
     </row>
     <row r="780">
-      <c r="A780" s="82"/>
-      <c r="B780" s="83"/>
+      <c r="A780" s="76"/>
+      <c r="B780" s="77"/>
       <c r="C780" s="34"/>
       <c r="D780" s="34"/>
       <c r="E780" s="34"/>
@@ -53072,8 +53050,8 @@
       </c>
     </row>
     <row r="781">
-      <c r="A781" s="82"/>
-      <c r="B781" s="83"/>
+      <c r="A781" s="76"/>
+      <c r="B781" s="77"/>
       <c r="C781" s="34"/>
       <c r="D781" s="34"/>
       <c r="E781" s="34"/>
@@ -53098,8 +53076,8 @@
       </c>
     </row>
     <row r="782">
-      <c r="A782" s="82"/>
-      <c r="B782" s="83"/>
+      <c r="A782" s="76"/>
+      <c r="B782" s="77"/>
       <c r="C782" s="34"/>
       <c r="D782" s="34"/>
       <c r="E782" s="34"/>
@@ -53124,8 +53102,8 @@
       </c>
     </row>
     <row r="783">
-      <c r="A783" s="82"/>
-      <c r="B783" s="83"/>
+      <c r="A783" s="76"/>
+      <c r="B783" s="77"/>
       <c r="C783" s="34"/>
       <c r="D783" s="34"/>
       <c r="E783" s="34"/>
@@ -53150,8 +53128,8 @@
       </c>
     </row>
     <row r="784">
-      <c r="A784" s="82"/>
-      <c r="B784" s="83"/>
+      <c r="A784" s="76"/>
+      <c r="B784" s="77"/>
       <c r="C784" s="34"/>
       <c r="D784" s="34"/>
       <c r="E784" s="34"/>
@@ -53176,8 +53154,8 @@
       </c>
     </row>
     <row r="785">
-      <c r="A785" s="82"/>
-      <c r="B785" s="83"/>
+      <c r="A785" s="76"/>
+      <c r="B785" s="77"/>
       <c r="C785" s="34"/>
       <c r="D785" s="34"/>
       <c r="E785" s="34"/>
@@ -53202,8 +53180,8 @@
       </c>
     </row>
     <row r="786">
-      <c r="A786" s="82"/>
-      <c r="B786" s="83"/>
+      <c r="A786" s="76"/>
+      <c r="B786" s="77"/>
       <c r="C786" s="34"/>
       <c r="D786" s="34"/>
       <c r="E786" s="34"/>
@@ -53228,8 +53206,8 @@
       </c>
     </row>
     <row r="787">
-      <c r="A787" s="82"/>
-      <c r="B787" s="83"/>
+      <c r="A787" s="76"/>
+      <c r="B787" s="77"/>
       <c r="C787" s="34"/>
       <c r="D787" s="34"/>
       <c r="E787" s="34"/>
@@ -53254,8 +53232,8 @@
       </c>
     </row>
     <row r="788">
-      <c r="A788" s="82"/>
-      <c r="B788" s="83"/>
+      <c r="A788" s="76"/>
+      <c r="B788" s="77"/>
       <c r="C788" s="34"/>
       <c r="D788" s="34"/>
       <c r="E788" s="34"/>
@@ -53280,8 +53258,8 @@
       </c>
     </row>
     <row r="789">
-      <c r="A789" s="82"/>
-      <c r="B789" s="83"/>
+      <c r="A789" s="76"/>
+      <c r="B789" s="77"/>
       <c r="C789" s="34"/>
       <c r="D789" s="34"/>
       <c r="E789" s="34"/>
@@ -53306,8 +53284,8 @@
       </c>
     </row>
     <row r="790">
-      <c r="A790" s="82"/>
-      <c r="B790" s="83"/>
+      <c r="A790" s="76"/>
+      <c r="B790" s="77"/>
       <c r="C790" s="34"/>
       <c r="D790" s="34"/>
       <c r="E790" s="34"/>
@@ -53332,8 +53310,8 @@
       </c>
     </row>
     <row r="791">
-      <c r="A791" s="82"/>
-      <c r="B791" s="83"/>
+      <c r="A791" s="76"/>
+      <c r="B791" s="77"/>
       <c r="C791" s="34"/>
       <c r="D791" s="34"/>
       <c r="E791" s="34"/>
@@ -53358,8 +53336,8 @@
       </c>
     </row>
     <row r="792">
-      <c r="A792" s="82"/>
-      <c r="B792" s="83"/>
+      <c r="A792" s="76"/>
+      <c r="B792" s="77"/>
       <c r="C792" s="34"/>
       <c r="D792" s="34"/>
       <c r="E792" s="34"/>
@@ -53384,8 +53362,8 @@
       </c>
     </row>
     <row r="793">
-      <c r="A793" s="82"/>
-      <c r="B793" s="83"/>
+      <c r="A793" s="76"/>
+      <c r="B793" s="77"/>
       <c r="C793" s="34"/>
       <c r="D793" s="34"/>
       <c r="E793" s="34"/>
@@ -53410,8 +53388,8 @@
       </c>
     </row>
     <row r="794">
-      <c r="A794" s="82"/>
-      <c r="B794" s="83"/>
+      <c r="A794" s="76"/>
+      <c r="B794" s="77"/>
       <c r="C794" s="34"/>
       <c r="D794" s="34"/>
       <c r="E794" s="34"/>
@@ -53436,8 +53414,8 @@
       </c>
     </row>
     <row r="795">
-      <c r="A795" s="82"/>
-      <c r="B795" s="83"/>
+      <c r="A795" s="76"/>
+      <c r="B795" s="77"/>
       <c r="C795" s="34"/>
       <c r="D795" s="34"/>
       <c r="E795" s="34"/>
@@ -53462,8 +53440,8 @@
       </c>
     </row>
     <row r="796">
-      <c r="A796" s="82"/>
-      <c r="B796" s="83"/>
+      <c r="A796" s="76"/>
+      <c r="B796" s="77"/>
       <c r="C796" s="34"/>
       <c r="D796" s="34"/>
       <c r="E796" s="34"/>
@@ -53488,8 +53466,8 @@
       </c>
     </row>
     <row r="797">
-      <c r="A797" s="82"/>
-      <c r="B797" s="83"/>
+      <c r="A797" s="76"/>
+      <c r="B797" s="77"/>
       <c r="C797" s="34"/>
       <c r="D797" s="34"/>
       <c r="E797" s="34"/>
@@ -53514,8 +53492,8 @@
       </c>
     </row>
     <row r="798">
-      <c r="A798" s="82"/>
-      <c r="B798" s="83"/>
+      <c r="A798" s="76"/>
+      <c r="B798" s="77"/>
       <c r="C798" s="34"/>
       <c r="D798" s="34"/>
       <c r="E798" s="34"/>
@@ -53540,8 +53518,8 @@
       </c>
     </row>
     <row r="799">
-      <c r="A799" s="82"/>
-      <c r="B799" s="83"/>
+      <c r="A799" s="76"/>
+      <c r="B799" s="77"/>
       <c r="C799" s="34"/>
       <c r="D799" s="34"/>
       <c r="E799" s="34"/>
@@ -53566,8 +53544,8 @@
       </c>
     </row>
     <row r="800">
-      <c r="A800" s="82"/>
-      <c r="B800" s="83"/>
+      <c r="A800" s="76"/>
+      <c r="B800" s="77"/>
       <c r="C800" s="34"/>
       <c r="D800" s="34"/>
       <c r="E800" s="34"/>
@@ -53592,8 +53570,8 @@
       </c>
     </row>
     <row r="801">
-      <c r="A801" s="82"/>
-      <c r="B801" s="83"/>
+      <c r="A801" s="76"/>
+      <c r="B801" s="77"/>
       <c r="C801" s="34"/>
       <c r="D801" s="34"/>
       <c r="E801" s="34"/>
@@ -53618,8 +53596,8 @@
       </c>
     </row>
     <row r="802">
-      <c r="A802" s="82"/>
-      <c r="B802" s="83"/>
+      <c r="A802" s="76"/>
+      <c r="B802" s="77"/>
       <c r="C802" s="34"/>
       <c r="D802" s="34"/>
       <c r="E802" s="34"/>
@@ -53644,8 +53622,8 @@
       </c>
     </row>
     <row r="803">
-      <c r="A803" s="82"/>
-      <c r="B803" s="83"/>
+      <c r="A803" s="76"/>
+      <c r="B803" s="77"/>
       <c r="C803" s="34"/>
       <c r="D803" s="34"/>
       <c r="E803" s="34"/>
@@ -53670,8 +53648,8 @@
       </c>
     </row>
     <row r="804">
-      <c r="A804" s="82"/>
-      <c r="B804" s="83"/>
+      <c r="A804" s="76"/>
+      <c r="B804" s="77"/>
       <c r="C804" s="34"/>
       <c r="D804" s="34"/>
       <c r="E804" s="34"/>
@@ -53696,8 +53674,8 @@
       </c>
     </row>
     <row r="805">
-      <c r="A805" s="82"/>
-      <c r="B805" s="83"/>
+      <c r="A805" s="76"/>
+      <c r="B805" s="77"/>
       <c r="C805" s="34"/>
       <c r="D805" s="34"/>
       <c r="E805" s="34"/>
@@ -53722,8 +53700,8 @@
       </c>
     </row>
     <row r="806">
-      <c r="A806" s="82"/>
-      <c r="B806" s="83"/>
+      <c r="A806" s="76"/>
+      <c r="B806" s="77"/>
       <c r="C806" s="34"/>
       <c r="D806" s="34"/>
       <c r="E806" s="34"/>
@@ -53748,8 +53726,8 @@
       </c>
     </row>
     <row r="807">
-      <c r="A807" s="82"/>
-      <c r="B807" s="83"/>
+      <c r="A807" s="76"/>
+      <c r="B807" s="77"/>
       <c r="C807" s="34"/>
       <c r="D807" s="34"/>
       <c r="E807" s="34"/>
@@ -53774,8 +53752,8 @@
       </c>
     </row>
     <row r="808">
-      <c r="A808" s="82"/>
-      <c r="B808" s="83"/>
+      <c r="A808" s="76"/>
+      <c r="B808" s="77"/>
       <c r="C808" s="34"/>
       <c r="D808" s="34"/>
       <c r="E808" s="34"/>
@@ -53800,8 +53778,8 @@
       </c>
     </row>
     <row r="809">
-      <c r="A809" s="82"/>
-      <c r="B809" s="83"/>
+      <c r="A809" s="76"/>
+      <c r="B809" s="77"/>
       <c r="C809" s="34"/>
       <c r="D809" s="34"/>
       <c r="E809" s="34"/>
@@ -53826,8 +53804,8 @@
       </c>
     </row>
     <row r="810">
-      <c r="A810" s="82"/>
-      <c r="B810" s="83"/>
+      <c r="A810" s="76"/>
+      <c r="B810" s="77"/>
       <c r="C810" s="34"/>
       <c r="D810" s="34"/>
       <c r="E810" s="34"/>
@@ -53852,8 +53830,8 @@
       </c>
     </row>
     <row r="811">
-      <c r="A811" s="82"/>
-      <c r="B811" s="83"/>
+      <c r="A811" s="76"/>
+      <c r="B811" s="77"/>
       <c r="C811" s="34"/>
       <c r="D811" s="34"/>
       <c r="E811" s="34"/>
@@ -53878,8 +53856,8 @@
       </c>
     </row>
     <row r="812">
-      <c r="A812" s="82"/>
-      <c r="B812" s="83"/>
+      <c r="A812" s="76"/>
+      <c r="B812" s="77"/>
       <c r="C812" s="34"/>
       <c r="D812" s="34"/>
       <c r="E812" s="34"/>
@@ -53904,8 +53882,8 @@
       </c>
     </row>
     <row r="813">
-      <c r="A813" s="82"/>
-      <c r="B813" s="83"/>
+      <c r="A813" s="76"/>
+      <c r="B813" s="77"/>
       <c r="C813" s="34"/>
       <c r="D813" s="34"/>
       <c r="E813" s="34"/>
@@ -53930,8 +53908,8 @@
       </c>
     </row>
     <row r="814">
-      <c r="A814" s="82"/>
-      <c r="B814" s="83"/>
+      <c r="A814" s="76"/>
+      <c r="B814" s="77"/>
       <c r="C814" s="34"/>
       <c r="D814" s="34"/>
       <c r="E814" s="34"/>
@@ -53956,8 +53934,8 @@
       </c>
     </row>
     <row r="815">
-      <c r="A815" s="82"/>
-      <c r="B815" s="83"/>
+      <c r="A815" s="76"/>
+      <c r="B815" s="77"/>
       <c r="C815" s="34"/>
       <c r="D815" s="34"/>
       <c r="E815" s="34"/>
@@ -53982,8 +53960,8 @@
       </c>
     </row>
     <row r="816">
-      <c r="A816" s="82"/>
-      <c r="B816" s="83"/>
+      <c r="A816" s="76"/>
+      <c r="B816" s="77"/>
       <c r="C816" s="34"/>
       <c r="D816" s="34"/>
       <c r="E816" s="34"/>
@@ -54008,8 +53986,8 @@
       </c>
     </row>
     <row r="817">
-      <c r="A817" s="82"/>
-      <c r="B817" s="83"/>
+      <c r="A817" s="76"/>
+      <c r="B817" s="77"/>
       <c r="C817" s="34"/>
       <c r="D817" s="34"/>
       <c r="E817" s="34"/>
@@ -54034,8 +54012,8 @@
       </c>
     </row>
     <row r="818">
-      <c r="A818" s="82"/>
-      <c r="B818" s="83"/>
+      <c r="A818" s="76"/>
+      <c r="B818" s="77"/>
       <c r="C818" s="34"/>
       <c r="D818" s="34"/>
       <c r="E818" s="34"/>
@@ -54060,8 +54038,8 @@
       </c>
     </row>
     <row r="819">
-      <c r="A819" s="82"/>
-      <c r="B819" s="83"/>
+      <c r="A819" s="76"/>
+      <c r="B819" s="77"/>
       <c r="C819" s="34"/>
       <c r="D819" s="34"/>
       <c r="E819" s="34"/>
@@ -54086,8 +54064,8 @@
       </c>
     </row>
     <row r="820">
-      <c r="A820" s="82"/>
-      <c r="B820" s="83"/>
+      <c r="A820" s="76"/>
+      <c r="B820" s="77"/>
       <c r="C820" s="34"/>
       <c r="D820" s="34"/>
       <c r="E820" s="34"/>
@@ -54112,8 +54090,8 @@
       </c>
     </row>
     <row r="821">
-      <c r="A821" s="82"/>
-      <c r="B821" s="83"/>
+      <c r="A821" s="76"/>
+      <c r="B821" s="77"/>
       <c r="C821" s="34"/>
       <c r="D821" s="34"/>
       <c r="E821" s="34"/>
@@ -54138,8 +54116,8 @@
       </c>
     </row>
     <row r="822">
-      <c r="A822" s="82"/>
-      <c r="B822" s="83"/>
+      <c r="A822" s="76"/>
+      <c r="B822" s="77"/>
       <c r="C822" s="34"/>
       <c r="D822" s="34"/>
       <c r="E822" s="34"/>
@@ -54164,8 +54142,8 @@
       </c>
     </row>
     <row r="823">
-      <c r="A823" s="82"/>
-      <c r="B823" s="83"/>
+      <c r="A823" s="76"/>
+      <c r="B823" s="77"/>
       <c r="C823" s="34"/>
       <c r="D823" s="34"/>
       <c r="E823" s="34"/>
@@ -54190,8 +54168,8 @@
       </c>
     </row>
     <row r="824">
-      <c r="A824" s="82"/>
-      <c r="B824" s="83"/>
+      <c r="A824" s="76"/>
+      <c r="B824" s="77"/>
       <c r="C824" s="34"/>
       <c r="D824" s="34"/>
       <c r="E824" s="34"/>
@@ -54216,8 +54194,8 @@
       </c>
     </row>
     <row r="825">
-      <c r="A825" s="82"/>
-      <c r="B825" s="83"/>
+      <c r="A825" s="76"/>
+      <c r="B825" s="77"/>
       <c r="C825" s="34"/>
       <c r="D825" s="34"/>
       <c r="E825" s="34"/>
@@ -54242,8 +54220,8 @@
       </c>
     </row>
     <row r="826">
-      <c r="A826" s="82"/>
-      <c r="B826" s="83"/>
+      <c r="A826" s="76"/>
+      <c r="B826" s="77"/>
       <c r="C826" s="34"/>
       <c r="D826" s="34"/>
       <c r="E826" s="34"/>
@@ -54268,8 +54246,8 @@
       </c>
     </row>
     <row r="827">
-      <c r="A827" s="82"/>
-      <c r="B827" s="83"/>
+      <c r="A827" s="76"/>
+      <c r="B827" s="77"/>
       <c r="C827" s="34"/>
       <c r="D827" s="34"/>
       <c r="E827" s="34"/>
@@ -54294,8 +54272,8 @@
       </c>
     </row>
     <row r="828">
-      <c r="A828" s="82"/>
-      <c r="B828" s="83"/>
+      <c r="A828" s="76"/>
+      <c r="B828" s="77"/>
       <c r="C828" s="34"/>
       <c r="D828" s="34"/>
       <c r="E828" s="34"/>
@@ -54320,8 +54298,8 @@
       </c>
     </row>
     <row r="829">
-      <c r="A829" s="82"/>
-      <c r="B829" s="83"/>
+      <c r="A829" s="76"/>
+      <c r="B829" s="77"/>
       <c r="C829" s="34"/>
       <c r="D829" s="34"/>
       <c r="E829" s="34"/>
@@ -54346,8 +54324,8 @@
       </c>
     </row>
     <row r="830">
-      <c r="A830" s="82"/>
-      <c r="B830" s="83"/>
+      <c r="A830" s="76"/>
+      <c r="B830" s="77"/>
       <c r="C830" s="34"/>
       <c r="D830" s="34"/>
       <c r="E830" s="34"/>
@@ -54372,8 +54350,8 @@
       </c>
     </row>
     <row r="831">
-      <c r="A831" s="82"/>
-      <c r="B831" s="83"/>
+      <c r="A831" s="76"/>
+      <c r="B831" s="77"/>
       <c r="C831" s="34"/>
       <c r="D831" s="34"/>
       <c r="E831" s="34"/>
@@ -54398,8 +54376,8 @@
       </c>
     </row>
     <row r="832">
-      <c r="A832" s="82"/>
-      <c r="B832" s="83"/>
+      <c r="A832" s="76"/>
+      <c r="B832" s="77"/>
       <c r="C832" s="34"/>
       <c r="D832" s="34"/>
       <c r="E832" s="34"/>
@@ -54424,8 +54402,8 @@
       </c>
     </row>
     <row r="833">
-      <c r="A833" s="82"/>
-      <c r="B833" s="83"/>
+      <c r="A833" s="76"/>
+      <c r="B833" s="77"/>
       <c r="C833" s="34"/>
       <c r="D833" s="34"/>
       <c r="E833" s="34"/>
@@ -54450,8 +54428,8 @@
       </c>
     </row>
     <row r="834">
-      <c r="A834" s="82"/>
-      <c r="B834" s="83"/>
+      <c r="A834" s="76"/>
+      <c r="B834" s="77"/>
       <c r="C834" s="34"/>
       <c r="D834" s="34"/>
       <c r="E834" s="34"/>
@@ -54476,8 +54454,8 @@
       </c>
     </row>
     <row r="835">
-      <c r="A835" s="82"/>
-      <c r="B835" s="83"/>
+      <c r="A835" s="76"/>
+      <c r="B835" s="77"/>
       <c r="C835" s="34"/>
       <c r="D835" s="34"/>
       <c r="E835" s="34"/>
@@ -54502,8 +54480,8 @@
       </c>
     </row>
     <row r="836">
-      <c r="A836" s="82"/>
-      <c r="B836" s="83"/>
+      <c r="A836" s="76"/>
+      <c r="B836" s="77"/>
       <c r="C836" s="34"/>
       <c r="D836" s="34"/>
       <c r="E836" s="34"/>
@@ -54528,8 +54506,8 @@
       </c>
     </row>
     <row r="837">
-      <c r="A837" s="82"/>
-      <c r="B837" s="83"/>
+      <c r="A837" s="76"/>
+      <c r="B837" s="77"/>
       <c r="C837" s="34"/>
       <c r="D837" s="34"/>
       <c r="E837" s="34"/>
@@ -54554,8 +54532,8 @@
       </c>
     </row>
     <row r="838">
-      <c r="A838" s="82"/>
-      <c r="B838" s="83"/>
+      <c r="A838" s="76"/>
+      <c r="B838" s="77"/>
       <c r="C838" s="34"/>
       <c r="D838" s="34"/>
       <c r="E838" s="34"/>
@@ -54580,8 +54558,8 @@
       </c>
     </row>
     <row r="839">
-      <c r="A839" s="82"/>
-      <c r="B839" s="83"/>
+      <c r="A839" s="76"/>
+      <c r="B839" s="77"/>
       <c r="C839" s="34"/>
       <c r="D839" s="34"/>
       <c r="E839" s="34"/>
@@ -54606,8 +54584,8 @@
       </c>
     </row>
     <row r="840">
-      <c r="A840" s="82"/>
-      <c r="B840" s="83"/>
+      <c r="A840" s="76"/>
+      <c r="B840" s="77"/>
       <c r="C840" s="34"/>
       <c r="D840" s="34"/>
       <c r="E840" s="34"/>
@@ -54632,8 +54610,8 @@
       </c>
     </row>
     <row r="841">
-      <c r="A841" s="82"/>
-      <c r="B841" s="83"/>
+      <c r="A841" s="76"/>
+      <c r="B841" s="77"/>
       <c r="C841" s="34"/>
       <c r="D841" s="34"/>
       <c r="E841" s="34"/>
@@ -54658,8 +54636,8 @@
       </c>
     </row>
     <row r="842">
-      <c r="A842" s="82"/>
-      <c r="B842" s="83"/>
+      <c r="A842" s="76"/>
+      <c r="B842" s="77"/>
       <c r="C842" s="34"/>
       <c r="D842" s="34"/>
       <c r="E842" s="34"/>
@@ -54684,8 +54662,8 @@
       </c>
     </row>
     <row r="843">
-      <c r="A843" s="82"/>
-      <c r="B843" s="83"/>
+      <c r="A843" s="76"/>
+      <c r="B843" s="77"/>
       <c r="C843" s="34"/>
       <c r="D843" s="34"/>
       <c r="E843" s="34"/>
@@ -54710,8 +54688,8 @@
       </c>
     </row>
     <row r="844">
-      <c r="A844" s="82"/>
-      <c r="B844" s="83"/>
+      <c r="A844" s="76"/>
+      <c r="B844" s="77"/>
       <c r="C844" s="34"/>
       <c r="D844" s="34"/>
       <c r="E844" s="34"/>
@@ -54736,8 +54714,8 @@
       </c>
     </row>
     <row r="845">
-      <c r="A845" s="82"/>
-      <c r="B845" s="83"/>
+      <c r="A845" s="76"/>
+      <c r="B845" s="77"/>
       <c r="C845" s="34"/>
       <c r="D845" s="34"/>
       <c r="E845" s="34"/>
@@ -54762,8 +54740,8 @@
       </c>
     </row>
     <row r="846">
-      <c r="A846" s="82"/>
-      <c r="B846" s="83"/>
+      <c r="A846" s="76"/>
+      <c r="B846" s="77"/>
       <c r="C846" s="34"/>
       <c r="D846" s="34"/>
       <c r="E846" s="34"/>
@@ -54788,8 +54766,8 @@
       </c>
     </row>
     <row r="847">
-      <c r="A847" s="82"/>
-      <c r="B847" s="83"/>
+      <c r="A847" s="76"/>
+      <c r="B847" s="77"/>
       <c r="C847" s="34"/>
       <c r="D847" s="34"/>
       <c r="E847" s="34"/>
@@ -54814,8 +54792,8 @@
       </c>
     </row>
     <row r="848">
-      <c r="A848" s="82"/>
-      <c r="B848" s="83"/>
+      <c r="A848" s="76"/>
+      <c r="B848" s="77"/>
       <c r="C848" s="34"/>
       <c r="D848" s="34"/>
       <c r="E848" s="34"/>
@@ -54840,8 +54818,8 @@
       </c>
     </row>
     <row r="849">
-      <c r="A849" s="82"/>
-      <c r="B849" s="83"/>
+      <c r="A849" s="76"/>
+      <c r="B849" s="77"/>
       <c r="C849" s="34"/>
       <c r="D849" s="34"/>
       <c r="E849" s="34"/>
@@ -54866,8 +54844,8 @@
       </c>
     </row>
     <row r="850">
-      <c r="A850" s="82"/>
-      <c r="B850" s="83"/>
+      <c r="A850" s="76"/>
+      <c r="B850" s="77"/>
       <c r="C850" s="34"/>
       <c r="D850" s="34"/>
       <c r="E850" s="34"/>
@@ -54892,8 +54870,8 @@
       </c>
     </row>
     <row r="851">
-      <c r="A851" s="82"/>
-      <c r="B851" s="83"/>
+      <c r="A851" s="76"/>
+      <c r="B851" s="77"/>
       <c r="C851" s="34"/>
       <c r="D851" s="34"/>
       <c r="E851" s="34"/>
@@ -54918,8 +54896,8 @@
       </c>
     </row>
     <row r="852">
-      <c r="A852" s="82"/>
-      <c r="B852" s="83"/>
+      <c r="A852" s="76"/>
+      <c r="B852" s="77"/>
       <c r="C852" s="34"/>
       <c r="D852" s="34"/>
       <c r="E852" s="34"/>
@@ -54944,8 +54922,8 @@
       </c>
     </row>
     <row r="853">
-      <c r="A853" s="82"/>
-      <c r="B853" s="83"/>
+      <c r="A853" s="76"/>
+      <c r="B853" s="77"/>
       <c r="C853" s="34"/>
       <c r="D853" s="34"/>
       <c r="E853" s="34"/>
@@ -54970,8 +54948,8 @@
       </c>
     </row>
     <row r="854">
-      <c r="A854" s="82"/>
-      <c r="B854" s="83"/>
+      <c r="A854" s="76"/>
+      <c r="B854" s="77"/>
       <c r="C854" s="34"/>
       <c r="D854" s="34"/>
       <c r="E854" s="34"/>
@@ -54996,8 +54974,8 @@
       </c>
     </row>
     <row r="855">
-      <c r="A855" s="82"/>
-      <c r="B855" s="83"/>
+      <c r="A855" s="76"/>
+      <c r="B855" s="77"/>
       <c r="C855" s="34"/>
       <c r="D855" s="34"/>
       <c r="E855" s="34"/>
@@ -55022,8 +55000,8 @@
       </c>
     </row>
     <row r="856">
-      <c r="A856" s="82"/>
-      <c r="B856" s="83"/>
+      <c r="A856" s="76"/>
+      <c r="B856" s="77"/>
       <c r="C856" s="34"/>
       <c r="D856" s="34"/>
       <c r="E856" s="34"/>
@@ -55048,8 +55026,8 @@
       </c>
     </row>
     <row r="857">
-      <c r="A857" s="82"/>
-      <c r="B857" s="83"/>
+      <c r="A857" s="76"/>
+      <c r="B857" s="77"/>
       <c r="C857" s="34"/>
       <c r="D857" s="34"/>
       <c r="E857" s="34"/>
@@ -55074,8 +55052,8 @@
       </c>
     </row>
     <row r="858">
-      <c r="A858" s="82"/>
-      <c r="B858" s="83"/>
+      <c r="A858" s="76"/>
+      <c r="B858" s="77"/>
       <c r="C858" s="34"/>
       <c r="D858" s="34"/>
       <c r="E858" s="34"/>
@@ -55100,8 +55078,8 @@
       </c>
     </row>
     <row r="859">
-      <c r="A859" s="82"/>
-      <c r="B859" s="83"/>
+      <c r="A859" s="76"/>
+      <c r="B859" s="77"/>
       <c r="C859" s="34"/>
       <c r="D859" s="34"/>
       <c r="E859" s="34"/>
@@ -55126,8 +55104,8 @@
       </c>
     </row>
     <row r="860">
-      <c r="A860" s="82"/>
-      <c r="B860" s="83"/>
+      <c r="A860" s="76"/>
+      <c r="B860" s="77"/>
       <c r="C860" s="34"/>
       <c r="D860" s="34"/>
       <c r="E860" s="34"/>
@@ -55152,8 +55130,8 @@
       </c>
     </row>
     <row r="861">
-      <c r="A861" s="82"/>
-      <c r="B861" s="83"/>
+      <c r="A861" s="76"/>
+      <c r="B861" s="77"/>
       <c r="C861" s="34"/>
       <c r="D861" s="34"/>
       <c r="E861" s="34"/>
@@ -55178,8 +55156,8 @@
       </c>
     </row>
     <row r="862">
-      <c r="A862" s="82"/>
-      <c r="B862" s="83"/>
+      <c r="A862" s="76"/>
+      <c r="B862" s="77"/>
       <c r="C862" s="34"/>
       <c r="D862" s="34"/>
       <c r="E862" s="34"/>
@@ -55204,8 +55182,8 @@
       </c>
     </row>
     <row r="863">
-      <c r="A863" s="82"/>
-      <c r="B863" s="83"/>
+      <c r="A863" s="76"/>
+      <c r="B863" s="77"/>
       <c r="C863" s="34"/>
       <c r="D863" s="34"/>
       <c r="E863" s="34"/>
@@ -55230,8 +55208,8 @@
       </c>
     </row>
     <row r="864">
-      <c r="A864" s="82"/>
-      <c r="B864" s="83"/>
+      <c r="A864" s="76"/>
+      <c r="B864" s="77"/>
       <c r="C864" s="34"/>
       <c r="D864" s="34"/>
       <c r="E864" s="34"/>
@@ -55256,8 +55234,8 @@
       </c>
     </row>
     <row r="865">
-      <c r="A865" s="82"/>
-      <c r="B865" s="83"/>
+      <c r="A865" s="76"/>
+      <c r="B865" s="77"/>
       <c r="C865" s="34"/>
       <c r="D865" s="34"/>
       <c r="E865" s="34"/>
@@ -55282,8 +55260,8 @@
       </c>
     </row>
     <row r="866">
-      <c r="A866" s="82"/>
-      <c r="B866" s="83"/>
+      <c r="A866" s="76"/>
+      <c r="B866" s="77"/>
       <c r="C866" s="34"/>
       <c r="D866" s="34"/>
       <c r="E866" s="34"/>
@@ -55308,8 +55286,8 @@
       </c>
     </row>
     <row r="867">
-      <c r="A867" s="82"/>
-      <c r="B867" s="83"/>
+      <c r="A867" s="76"/>
+      <c r="B867" s="77"/>
       <c r="C867" s="34"/>
       <c r="D867" s="34"/>
       <c r="E867" s="34"/>
@@ -55334,8 +55312,8 @@
       </c>
     </row>
     <row r="868">
-      <c r="A868" s="82"/>
-      <c r="B868" s="83"/>
+      <c r="A868" s="76"/>
+      <c r="B868" s="77"/>
       <c r="C868" s="34"/>
       <c r="D868" s="34"/>
       <c r="E868" s="34"/>
@@ -55360,8 +55338,8 @@
       </c>
     </row>
     <row r="869">
-      <c r="A869" s="82"/>
-      <c r="B869" s="83"/>
+      <c r="A869" s="76"/>
+      <c r="B869" s="77"/>
       <c r="C869" s="34"/>
       <c r="D869" s="34"/>
       <c r="E869" s="34"/>
@@ -55386,8 +55364,8 @@
       </c>
     </row>
     <row r="870">
-      <c r="A870" s="82"/>
-      <c r="B870" s="83"/>
+      <c r="A870" s="76"/>
+      <c r="B870" s="77"/>
       <c r="C870" s="34"/>
       <c r="D870" s="34"/>
       <c r="E870" s="34"/>
@@ -55412,8 +55390,8 @@
       </c>
     </row>
     <row r="871">
-      <c r="A871" s="82"/>
-      <c r="B871" s="83"/>
+      <c r="A871" s="76"/>
+      <c r="B871" s="77"/>
       <c r="C871" s="34"/>
       <c r="D871" s="34"/>
       <c r="E871" s="34"/>
@@ -55438,8 +55416,8 @@
       </c>
     </row>
     <row r="872">
-      <c r="A872" s="82"/>
-      <c r="B872" s="83"/>
+      <c r="A872" s="76"/>
+      <c r="B872" s="77"/>
       <c r="C872" s="34"/>
       <c r="D872" s="34"/>
       <c r="E872" s="34"/>
@@ -55464,8 +55442,8 @@
       </c>
     </row>
     <row r="873">
-      <c r="A873" s="82"/>
-      <c r="B873" s="83"/>
+      <c r="A873" s="76"/>
+      <c r="B873" s="77"/>
       <c r="C873" s="34"/>
       <c r="D873" s="34"/>
       <c r="E873" s="34"/>
@@ -55490,8 +55468,8 @@
       </c>
     </row>
     <row r="874">
-      <c r="A874" s="82"/>
-      <c r="B874" s="83"/>
+      <c r="A874" s="76"/>
+      <c r="B874" s="77"/>
       <c r="C874" s="34"/>
       <c r="D874" s="34"/>
       <c r="E874" s="34"/>
@@ -55516,8 +55494,8 @@
       </c>
     </row>
     <row r="875">
-      <c r="A875" s="82"/>
-      <c r="B875" s="83"/>
+      <c r="A875" s="76"/>
+      <c r="B875" s="77"/>
       <c r="C875" s="34"/>
       <c r="D875" s="34"/>
       <c r="E875" s="34"/>
@@ -55542,8 +55520,8 @@
       </c>
     </row>
     <row r="876">
-      <c r="A876" s="82"/>
-      <c r="B876" s="83"/>
+      <c r="A876" s="76"/>
+      <c r="B876" s="77"/>
       <c r="C876" s="34"/>
       <c r="D876" s="34"/>
       <c r="E876" s="34"/>
@@ -55568,8 +55546,8 @@
       </c>
     </row>
     <row r="877">
-      <c r="A877" s="82"/>
-      <c r="B877" s="83"/>
+      <c r="A877" s="76"/>
+      <c r="B877" s="77"/>
       <c r="C877" s="34"/>
       <c r="D877" s="34"/>
       <c r="E877" s="34"/>
@@ -55594,8 +55572,8 @@
       </c>
     </row>
     <row r="878">
-      <c r="A878" s="82"/>
-      <c r="B878" s="83"/>
+      <c r="A878" s="76"/>
+      <c r="B878" s="77"/>
       <c r="C878" s="34"/>
       <c r="D878" s="34"/>
       <c r="E878" s="34"/>
@@ -55620,8 +55598,8 @@
       </c>
     </row>
     <row r="879">
-      <c r="A879" s="82"/>
-      <c r="B879" s="83"/>
+      <c r="A879" s="76"/>
+      <c r="B879" s="77"/>
       <c r="C879" s="34"/>
       <c r="D879" s="34"/>
       <c r="E879" s="34"/>
@@ -55646,8 +55624,8 @@
       </c>
     </row>
     <row r="880">
-      <c r="A880" s="82"/>
-      <c r="B880" s="83"/>
+      <c r="A880" s="76"/>
+      <c r="B880" s="77"/>
       <c r="C880" s="34"/>
       <c r="D880" s="34"/>
       <c r="E880" s="34"/>
@@ -55672,8 +55650,8 @@
       </c>
     </row>
     <row r="881">
-      <c r="A881" s="82"/>
-      <c r="B881" s="83"/>
+      <c r="A881" s="76"/>
+      <c r="B881" s="77"/>
       <c r="C881" s="34"/>
       <c r="D881" s="34"/>
       <c r="E881" s="34"/>
@@ -55698,8 +55676,8 @@
       </c>
     </row>
     <row r="882">
-      <c r="A882" s="82"/>
-      <c r="B882" s="83"/>
+      <c r="A882" s="76"/>
+      <c r="B882" s="77"/>
       <c r="C882" s="34"/>
       <c r="D882" s="34"/>
       <c r="E882" s="34"/>
@@ -55724,8 +55702,8 @@
       </c>
     </row>
     <row r="883">
-      <c r="A883" s="82"/>
-      <c r="B883" s="83"/>
+      <c r="A883" s="76"/>
+      <c r="B883" s="77"/>
       <c r="C883" s="34"/>
       <c r="D883" s="34"/>
       <c r="E883" s="34"/>
@@ -55750,8 +55728,8 @@
       </c>
     </row>
     <row r="884">
-      <c r="A884" s="82"/>
-      <c r="B884" s="83"/>
+      <c r="A884" s="76"/>
+      <c r="B884" s="77"/>
       <c r="C884" s="34"/>
       <c r="D884" s="34"/>
       <c r="E884" s="34"/>
@@ -55776,8 +55754,8 @@
       </c>
     </row>
     <row r="885">
-      <c r="A885" s="82"/>
-      <c r="B885" s="83"/>
+      <c r="A885" s="76"/>
+      <c r="B885" s="77"/>
       <c r="C885" s="34"/>
       <c r="D885" s="34"/>
       <c r="E885" s="34"/>
@@ -55802,8 +55780,8 @@
       </c>
     </row>
     <row r="886">
-      <c r="A886" s="82"/>
-      <c r="B886" s="83"/>
+      <c r="A886" s="76"/>
+      <c r="B886" s="77"/>
       <c r="C886" s="34"/>
       <c r="D886" s="34"/>
       <c r="E886" s="34"/>
@@ -55828,8 +55806,8 @@
       </c>
     </row>
     <row r="887">
-      <c r="A887" s="82"/>
-      <c r="B887" s="83"/>
+      <c r="A887" s="76"/>
+      <c r="B887" s="77"/>
       <c r="C887" s="34"/>
       <c r="D887" s="34"/>
       <c r="E887" s="34"/>
@@ -55854,8 +55832,8 @@
       </c>
     </row>
     <row r="888">
-      <c r="A888" s="82"/>
-      <c r="B888" s="83"/>
+      <c r="A888" s="76"/>
+      <c r="B888" s="77"/>
       <c r="C888" s="34"/>
       <c r="D888" s="34"/>
       <c r="E888" s="34"/>
@@ -55880,8 +55858,8 @@
       </c>
     </row>
     <row r="889">
-      <c r="A889" s="82"/>
-      <c r="B889" s="83"/>
+      <c r="A889" s="76"/>
+      <c r="B889" s="77"/>
       <c r="C889" s="34"/>
       <c r="D889" s="34"/>
       <c r="E889" s="34"/>
@@ -55906,8 +55884,8 @@
       </c>
     </row>
     <row r="890">
-      <c r="A890" s="82"/>
-      <c r="B890" s="83"/>
+      <c r="A890" s="76"/>
+      <c r="B890" s="77"/>
       <c r="C890" s="34"/>
       <c r="D890" s="34"/>
       <c r="E890" s="34"/>
@@ -55932,8 +55910,8 @@
       </c>
     </row>
     <row r="891">
-      <c r="A891" s="82"/>
-      <c r="B891" s="83"/>
+      <c r="A891" s="76"/>
+      <c r="B891" s="77"/>
       <c r="C891" s="34"/>
       <c r="D891" s="34"/>
       <c r="E891" s="34"/>
@@ -55958,8 +55936,8 @@
       </c>
     </row>
     <row r="892">
-      <c r="A892" s="82"/>
-      <c r="B892" s="83"/>
+      <c r="A892" s="76"/>
+      <c r="B892" s="77"/>
       <c r="C892" s="34"/>
       <c r="D892" s="34"/>
       <c r="E892" s="34"/>
@@ -55984,8 +55962,8 @@
       </c>
     </row>
     <row r="893">
-      <c r="A893" s="82"/>
-      <c r="B893" s="83"/>
+      <c r="A893" s="76"/>
+      <c r="B893" s="77"/>
       <c r="C893" s="34"/>
       <c r="D893" s="34"/>
       <c r="E893" s="34"/>
@@ -56010,8 +55988,8 @@
       </c>
     </row>
     <row r="894">
-      <c r="A894" s="82"/>
-      <c r="B894" s="83"/>
+      <c r="A894" s="76"/>
+      <c r="B894" s="77"/>
       <c r="C894" s="34"/>
       <c r="D894" s="34"/>
       <c r="E894" s="34"/>
@@ -56036,8 +56014,8 @@
       </c>
     </row>
     <row r="895">
-      <c r="A895" s="82"/>
-      <c r="B895" s="83"/>
+      <c r="A895" s="76"/>
+      <c r="B895" s="77"/>
       <c r="C895" s="34"/>
       <c r="D895" s="34"/>
       <c r="E895" s="34"/>
@@ -56062,8 +56040,8 @@
       </c>
     </row>
     <row r="896">
-      <c r="A896" s="82"/>
-      <c r="B896" s="83"/>
+      <c r="A896" s="76"/>
+      <c r="B896" s="77"/>
       <c r="C896" s="34"/>
       <c r="D896" s="34"/>
       <c r="E896" s="34"/>
@@ -56088,8 +56066,8 @@
       </c>
     </row>
     <row r="897">
-      <c r="A897" s="82"/>
-      <c r="B897" s="83"/>
+      <c r="A897" s="76"/>
+      <c r="B897" s="77"/>
       <c r="C897" s="34"/>
       <c r="D897" s="34"/>
       <c r="E897" s="34"/>
@@ -56114,8 +56092,8 @@
       </c>
     </row>
     <row r="898">
-      <c r="A898" s="82"/>
-      <c r="B898" s="83"/>
+      <c r="A898" s="76"/>
+      <c r="B898" s="77"/>
       <c r="C898" s="34"/>
       <c r="D898" s="34"/>
       <c r="E898" s="34"/>
@@ -56140,8 +56118,8 @@
       </c>
     </row>
     <row r="899">
-      <c r="A899" s="82"/>
-      <c r="B899" s="83"/>
+      <c r="A899" s="76"/>
+      <c r="B899" s="77"/>
       <c r="C899" s="34"/>
       <c r="D899" s="34"/>
       <c r="E899" s="34"/>
@@ -56166,8 +56144,8 @@
       </c>
     </row>
     <row r="900">
-      <c r="A900" s="82"/>
-      <c r="B900" s="83"/>
+      <c r="A900" s="76"/>
+      <c r="B900" s="77"/>
       <c r="C900" s="34"/>
       <c r="D900" s="34"/>
       <c r="E900" s="34"/>
@@ -56192,8 +56170,8 @@
       </c>
     </row>
     <row r="901">
-      <c r="A901" s="82"/>
-      <c r="B901" s="83"/>
+      <c r="A901" s="76"/>
+      <c r="B901" s="77"/>
       <c r="C901" s="34"/>
       <c r="D901" s="34"/>
       <c r="E901" s="34"/>
@@ -56218,8 +56196,8 @@
       </c>
     </row>
     <row r="902">
-      <c r="A902" s="82"/>
-      <c r="B902" s="83"/>
+      <c r="A902" s="76"/>
+      <c r="B902" s="77"/>
       <c r="C902" s="34"/>
       <c r="D902" s="34"/>
       <c r="E902" s="34"/>
@@ -56244,8 +56222,8 @@
       </c>
     </row>
     <row r="903">
-      <c r="A903" s="82"/>
-      <c r="B903" s="83"/>
+      <c r="A903" s="76"/>
+      <c r="B903" s="77"/>
       <c r="C903" s="34"/>
       <c r="D903" s="34"/>
       <c r="E903" s="34"/>
@@ -56270,8 +56248,8 @@
       </c>
     </row>
     <row r="904">
-      <c r="A904" s="82"/>
-      <c r="B904" s="83"/>
+      <c r="A904" s="76"/>
+      <c r="B904" s="77"/>
       <c r="C904" s="34"/>
       <c r="D904" s="34"/>
       <c r="E904" s="34"/>
@@ -56296,8 +56274,8 @@
       </c>
     </row>
     <row r="905">
-      <c r="A905" s="82"/>
-      <c r="B905" s="83"/>
+      <c r="A905" s="76"/>
+      <c r="B905" s="77"/>
       <c r="C905" s="34"/>
       <c r="D905" s="34"/>
       <c r="E905" s="34"/>
@@ -56322,8 +56300,8 @@
       </c>
     </row>
     <row r="906">
-      <c r="A906" s="82"/>
-      <c r="B906" s="83"/>
+      <c r="A906" s="76"/>
+      <c r="B906" s="77"/>
       <c r="C906" s="34"/>
       <c r="D906" s="34"/>
       <c r="E906" s="34"/>
@@ -56348,8 +56326,8 @@
       </c>
     </row>
     <row r="907">
-      <c r="A907" s="82"/>
-      <c r="B907" s="83"/>
+      <c r="A907" s="76"/>
+      <c r="B907" s="77"/>
       <c r="C907" s="34"/>
       <c r="D907" s="34"/>
       <c r="E907" s="34"/>
@@ -56374,8 +56352,8 @@
       </c>
     </row>
     <row r="908">
-      <c r="A908" s="82"/>
-      <c r="B908" s="83"/>
+      <c r="A908" s="76"/>
+      <c r="B908" s="77"/>
       <c r="C908" s="34"/>
       <c r="D908" s="34"/>
       <c r="E908" s="34"/>
@@ -56400,8 +56378,8 @@
       </c>
     </row>
     <row r="909">
-      <c r="A909" s="82"/>
-      <c r="B909" s="83"/>
+      <c r="A909" s="76"/>
+      <c r="B909" s="77"/>
       <c r="C909" s="34"/>
       <c r="D909" s="34"/>
       <c r="E909" s="34"/>
@@ -56426,8 +56404,8 @@
       </c>
     </row>
     <row r="910">
-      <c r="A910" s="82"/>
-      <c r="B910" s="83"/>
+      <c r="A910" s="76"/>
+      <c r="B910" s="77"/>
       <c r="C910" s="34"/>
       <c r="D910" s="34"/>
       <c r="E910" s="34"/>
@@ -56452,8 +56430,8 @@
       </c>
     </row>
     <row r="911">
-      <c r="A911" s="82"/>
-      <c r="B911" s="83"/>
+      <c r="A911" s="76"/>
+      <c r="B911" s="77"/>
       <c r="C911" s="34"/>
       <c r="D911" s="34"/>
       <c r="E911" s="34"/>
@@ -56478,8 +56456,8 @@
       </c>
     </row>
     <row r="912">
-      <c r="A912" s="82"/>
-      <c r="B912" s="83"/>
+      <c r="A912" s="76"/>
+      <c r="B912" s="77"/>
       <c r="C912" s="34"/>
       <c r="D912" s="34"/>
       <c r="E912" s="34"/>
@@ -56504,8 +56482,8 @@
       </c>
     </row>
     <row r="913">
-      <c r="A913" s="82"/>
-      <c r="B913" s="83"/>
+      <c r="A913" s="76"/>
+      <c r="B913" s="77"/>
       <c r="C913" s="34"/>
       <c r="D913" s="34"/>
       <c r="E913" s="34"/>
@@ -56530,8 +56508,8 @@
       </c>
     </row>
     <row r="914">
-      <c r="A914" s="82"/>
-      <c r="B914" s="83"/>
+      <c r="A914" s="76"/>
+      <c r="B914" s="77"/>
       <c r="C914" s="34"/>
       <c r="D914" s="34"/>
       <c r="E914" s="34"/>
@@ -56556,8 +56534,8 @@
       </c>
     </row>
     <row r="915">
-      <c r="A915" s="82"/>
-      <c r="B915" s="83"/>
+      <c r="A915" s="76"/>
+      <c r="B915" s="77"/>
       <c r="C915" s="34"/>
       <c r="D915" s="34"/>
       <c r="E915" s="34"/>
@@ -56582,8 +56560,8 @@
       </c>
     </row>
     <row r="916">
-      <c r="A916" s="82"/>
-      <c r="B916" s="83"/>
+      <c r="A916" s="76"/>
+      <c r="B916" s="77"/>
       <c r="C916" s="34"/>
       <c r="D916" s="34"/>
       <c r="E916" s="34"/>
@@ -56608,8 +56586,8 @@
       </c>
     </row>
     <row r="917">
-      <c r="A917" s="82"/>
-      <c r="B917" s="83"/>
+      <c r="A917" s="76"/>
+      <c r="B917" s="77"/>
       <c r="C917" s="34"/>
       <c r="D917" s="34"/>
       <c r="E917" s="34"/>
@@ -56634,8 +56612,8 @@
       </c>
     </row>
     <row r="918">
-      <c r="A918" s="82"/>
-      <c r="B918" s="83"/>
+      <c r="A918" s="76"/>
+      <c r="B918" s="77"/>
       <c r="C918" s="34"/>
       <c r="D918" s="34"/>
       <c r="E918" s="34"/>
@@ -56660,8 +56638,8 @@
       </c>
     </row>
     <row r="919">
-      <c r="A919" s="82"/>
-      <c r="B919" s="83"/>
+      <c r="A919" s="76"/>
+      <c r="B919" s="77"/>
       <c r="C919" s="34"/>
       <c r="D919" s="34"/>
       <c r="E919" s="34"/>
@@ -56686,8 +56664,8 @@
       </c>
     </row>
     <row r="920">
-      <c r="A920" s="82"/>
-      <c r="B920" s="83"/>
+      <c r="A920" s="76"/>
+      <c r="B920" s="77"/>
       <c r="C920" s="34"/>
       <c r="D920" s="34"/>
       <c r="E920" s="34"/>
@@ -56712,8 +56690,8 @@
       </c>
     </row>
     <row r="921">
-      <c r="A921" s="82"/>
-      <c r="B921" s="83"/>
+      <c r="A921" s="76"/>
+      <c r="B921" s="77"/>
       <c r="C921" s="34"/>
       <c r="D921" s="34"/>
       <c r="E921" s="34"/>
@@ -56738,8 +56716,8 @@
       </c>
     </row>
     <row r="922">
-      <c r="A922" s="82"/>
-      <c r="B922" s="83"/>
+      <c r="A922" s="76"/>
+      <c r="B922" s="77"/>
       <c r="C922" s="34"/>
       <c r="D922" s="34"/>
       <c r="E922" s="34"/>
@@ -56764,8 +56742,8 @@
       </c>
     </row>
     <row r="923">
-      <c r="A923" s="82"/>
-      <c r="B923" s="83"/>
+      <c r="A923" s="76"/>
+      <c r="B923" s="77"/>
       <c r="C923" s="34"/>
       <c r="D923" s="34"/>
       <c r="E923" s="34"/>
@@ -56790,8 +56768,8 @@
       </c>
     </row>
     <row r="924">
-      <c r="A924" s="82"/>
-      <c r="B924" s="83"/>
+      <c r="A924" s="76"/>
+      <c r="B924" s="77"/>
       <c r="C924" s="34"/>
       <c r="D924" s="34"/>
       <c r="E924" s="34"/>
@@ -56816,8 +56794,8 @@
       </c>
     </row>
     <row r="925">
-      <c r="A925" s="82"/>
-      <c r="B925" s="83"/>
+      <c r="A925" s="76"/>
+      <c r="B925" s="77"/>
       <c r="C925" s="34"/>
       <c r="D925" s="34"/>
       <c r="E925" s="34"/>
@@ -56842,8 +56820,8 @@
       </c>
     </row>
     <row r="926">
-      <c r="A926" s="82"/>
-      <c r="B926" s="83"/>
+      <c r="A926" s="76"/>
+      <c r="B926" s="77"/>
       <c r="C926" s="34"/>
       <c r="D926" s="34"/>
       <c r="E926" s="34"/>
@@ -56868,8 +56846,8 @@
       </c>
     </row>
     <row r="927">
-      <c r="A927" s="82"/>
-      <c r="B927" s="83"/>
+      <c r="A927" s="76"/>
+      <c r="B927" s="77"/>
       <c r="C927" s="34"/>
       <c r="D927" s="34"/>
       <c r="E927" s="34"/>
@@ -56894,8 +56872,8 @@
       </c>
     </row>
     <row r="928">
-      <c r="A928" s="82"/>
-      <c r="B928" s="83"/>
+      <c r="A928" s="76"/>
+      <c r="B928" s="77"/>
       <c r="C928" s="34"/>
       <c r="D928" s="34"/>
       <c r="E928" s="34"/>
@@ -56920,8 +56898,8 @@
       </c>
     </row>
     <row r="929">
-      <c r="A929" s="82"/>
-      <c r="B929" s="83"/>
+      <c r="A929" s="76"/>
+      <c r="B929" s="77"/>
       <c r="C929" s="34"/>
       <c r="D929" s="34"/>
       <c r="E929" s="34"/>
@@ -56946,8 +56924,8 @@
       </c>
     </row>
     <row r="930">
-      <c r="A930" s="82"/>
-      <c r="B930" s="83"/>
+      <c r="A930" s="76"/>
+      <c r="B930" s="77"/>
       <c r="C930" s="34"/>
       <c r="D930" s="34"/>
       <c r="E930" s="34"/>
@@ -56972,8 +56950,8 @@
       </c>
     </row>
     <row r="931">
-      <c r="A931" s="82"/>
-      <c r="B931" s="83"/>
+      <c r="A931" s="76"/>
+      <c r="B931" s="77"/>
       <c r="C931" s="34"/>
       <c r="D931" s="34"/>
       <c r="E931" s="34"/>
@@ -56998,8 +56976,8 @@
       </c>
     </row>
     <row r="932">
-      <c r="A932" s="82"/>
-      <c r="B932" s="83"/>
+      <c r="A932" s="76"/>
+      <c r="B932" s="77"/>
       <c r="C932" s="34"/>
       <c r="D932" s="34"/>
       <c r="E932" s="34"/>
@@ -57024,8 +57002,8 @@
       </c>
     </row>
     <row r="933">
-      <c r="A933" s="82"/>
-      <c r="B933" s="83"/>
+      <c r="A933" s="76"/>
+      <c r="B933" s="77"/>
       <c r="C933" s="34"/>
       <c r="D933" s="34"/>
       <c r="E933" s="34"/>
@@ -57050,8 +57028,8 @@
       </c>
     </row>
     <row r="934">
-      <c r="A934" s="82"/>
-      <c r="B934" s="83"/>
+      <c r="A934" s="76"/>
+      <c r="B934" s="77"/>
       <c r="C934" s="34"/>
       <c r="D934" s="34"/>
       <c r="E934" s="34"/>
@@ -57076,8 +57054,8 @@
       </c>
     </row>
     <row r="935">
-      <c r="A935" s="82"/>
-      <c r="B935" s="83"/>
+      <c r="A935" s="76"/>
+      <c r="B935" s="77"/>
       <c r="C935" s="34"/>
       <c r="D935" s="34"/>
       <c r="E935" s="34"/>
@@ -57102,8 +57080,8 @@
       </c>
     </row>
     <row r="936">
-      <c r="A936" s="82"/>
-      <c r="B936" s="83"/>
+      <c r="A936" s="76"/>
+      <c r="B936" s="77"/>
       <c r="C936" s="34"/>
       <c r="D936" s="34"/>
       <c r="E936" s="34"/>
@@ -57128,8 +57106,8 @@
       </c>
     </row>
     <row r="937">
-      <c r="A937" s="82"/>
-      <c r="B937" s="83"/>
+      <c r="A937" s="76"/>
+      <c r="B937" s="77"/>
       <c r="C937" s="34"/>
       <c r="D937" s="34"/>
       <c r="E937" s="34"/>
@@ -57154,8 +57132,8 @@
       </c>
     </row>
     <row r="938">
-      <c r="A938" s="82"/>
-      <c r="B938" s="83"/>
+      <c r="A938" s="76"/>
+      <c r="B938" s="77"/>
       <c r="C938" s="34"/>
       <c r="D938" s="34"/>
       <c r="E938" s="34"/>
@@ -57180,8 +57158,8 @@
       </c>
     </row>
     <row r="939">
-      <c r="A939" s="82"/>
-      <c r="B939" s="83"/>
+      <c r="A939" s="76"/>
+      <c r="B939" s="77"/>
       <c r="C939" s="34"/>
       <c r="D939" s="34"/>
       <c r="E939" s="34"/>
@@ -57206,8 +57184,8 @@
       </c>
     </row>
     <row r="940">
-      <c r="A940" s="82"/>
-      <c r="B940" s="83"/>
+      <c r="A940" s="76"/>
+      <c r="B940" s="77"/>
       <c r="C940" s="34"/>
       <c r="D940" s="34"/>
       <c r="E940" s="34"/>
@@ -57232,8 +57210,8 @@
       </c>
     </row>
     <row r="941">
-      <c r="A941" s="82"/>
-      <c r="B941" s="83"/>
+      <c r="A941" s="76"/>
+      <c r="B941" s="77"/>
       <c r="C941" s="34"/>
       <c r="D941" s="34"/>
       <c r="E941" s="34"/>
@@ -57258,8 +57236,8 @@
       </c>
     </row>
     <row r="942">
-      <c r="A942" s="82"/>
-      <c r="B942" s="83"/>
+      <c r="A942" s="76"/>
+      <c r="B942" s="77"/>
       <c r="C942" s="34"/>
       <c r="D942" s="34"/>
       <c r="E942" s="34"/>
@@ -57284,8 +57262,8 @@
       </c>
     </row>
     <row r="943">
-      <c r="A943" s="82"/>
-      <c r="B943" s="83"/>
+      <c r="A943" s="76"/>
+      <c r="B943" s="77"/>
       <c r="C943" s="34"/>
       <c r="D943" s="34"/>
       <c r="E943" s="34"/>
@@ -57310,8 +57288,8 @@
       </c>
     </row>
     <row r="944">
-      <c r="A944" s="82"/>
-      <c r="B944" s="83"/>
+      <c r="A944" s="76"/>
+      <c r="B944" s="77"/>
       <c r="C944" s="34"/>
       <c r="D944" s="34"/>
       <c r="E944" s="34"/>
@@ -57336,8 +57314,8 @@
       </c>
     </row>
     <row r="945">
-      <c r="A945" s="82"/>
-      <c r="B945" s="83"/>
+      <c r="A945" s="76"/>
+      <c r="B945" s="77"/>
       <c r="C945" s="34"/>
       <c r="D945" s="34"/>
       <c r="E945" s="34"/>
@@ -57362,8 +57340,8 @@
       </c>
     </row>
     <row r="946">
-      <c r="A946" s="82"/>
-      <c r="B946" s="83"/>
+      <c r="A946" s="76"/>
+      <c r="B946" s="77"/>
       <c r="C946" s="34"/>
       <c r="D946" s="34"/>
       <c r="E946" s="34"/>
@@ -57388,8 +57366,8 @@
       </c>
     </row>
     <row r="947">
-      <c r="A947" s="82"/>
-      <c r="B947" s="83"/>
+      <c r="A947" s="76"/>
+      <c r="B947" s="77"/>
       <c r="C947" s="34"/>
       <c r="D947" s="34"/>
       <c r="E947" s="34"/>
@@ -57414,8 +57392,8 @@
       </c>
     </row>
     <row r="948">
-      <c r="A948" s="82"/>
-      <c r="B948" s="83"/>
+      <c r="A948" s="76"/>
+      <c r="B948" s="77"/>
       <c r="C948" s="34"/>
       <c r="D948" s="34"/>
       <c r="E948" s="34"/>
@@ -57440,8 +57418,8 @@
       </c>
     </row>
     <row r="949">
-      <c r="A949" s="82"/>
-      <c r="B949" s="83"/>
+      <c r="A949" s="76"/>
+      <c r="B949" s="77"/>
       <c r="C949" s="34"/>
       <c r="D949" s="34"/>
       <c r="E949" s="34"/>
@@ -57466,8 +57444,8 @@
       </c>
     </row>
     <row r="950">
-      <c r="A950" s="82"/>
-      <c r="B950" s="83"/>
+      <c r="A950" s="76"/>
+      <c r="B950" s="77"/>
       <c r="C950" s="34"/>
       <c r="D950" s="34"/>
       <c r="E950" s="34"/>
@@ -57492,8 +57470,8 @@
       </c>
     </row>
     <row r="951">
-      <c r="A951" s="82"/>
-      <c r="B951" s="83"/>
+      <c r="A951" s="76"/>
+      <c r="B951" s="77"/>
       <c r="C951" s="34"/>
       <c r="D951" s="34"/>
       <c r="E951" s="34"/>
@@ -57518,8 +57496,8 @@
       </c>
     </row>
     <row r="952">
-      <c r="A952" s="82"/>
-      <c r="B952" s="83"/>
+      <c r="A952" s="76"/>
+      <c r="B952" s="77"/>
       <c r="C952" s="34"/>
       <c r="D952" s="34"/>
       <c r="E952" s="34"/>
@@ -57544,8 +57522,8 @@
       </c>
     </row>
     <row r="953">
-      <c r="A953" s="82"/>
-      <c r="B953" s="83"/>
+      <c r="A953" s="76"/>
+      <c r="B953" s="77"/>
       <c r="C953" s="34"/>
       <c r="D953" s="34"/>
       <c r="E953" s="34"/>
@@ -57570,8 +57548,8 @@
       </c>
     </row>
     <row r="954">
-      <c r="A954" s="82"/>
-      <c r="B954" s="83"/>
+      <c r="A954" s="76"/>
+      <c r="B954" s="77"/>
       <c r="C954" s="34"/>
       <c r="D954" s="34"/>
       <c r="E954" s="34"/>
@@ -57596,8 +57574,8 @@
       </c>
     </row>
     <row r="955">
-      <c r="A955" s="82"/>
-      <c r="B955" s="83"/>
+      <c r="A955" s="76"/>
+      <c r="B955" s="77"/>
       <c r="C955" s="34"/>
       <c r="D955" s="34"/>
       <c r="E955" s="34"/>
@@ -57622,8 +57600,8 @@
       </c>
     </row>
     <row r="956">
-      <c r="A956" s="82"/>
-      <c r="B956" s="83"/>
+      <c r="A956" s="76"/>
+      <c r="B956" s="77"/>
       <c r="C956" s="34"/>
       <c r="D956" s="34"/>
       <c r="E956" s="34"/>
@@ -57648,8 +57626,8 @@
       </c>
     </row>
     <row r="957">
-      <c r="A957" s="82"/>
-      <c r="B957" s="83"/>
+      <c r="A957" s="76"/>
+      <c r="B957" s="77"/>
       <c r="C957" s="34"/>
       <c r="D957" s="34"/>
       <c r="E957" s="34"/>
@@ -57674,8 +57652,8 @@
       </c>
     </row>
     <row r="958">
-      <c r="A958" s="82"/>
-      <c r="B958" s="83"/>
+      <c r="A958" s="76"/>
+      <c r="B958" s="77"/>
       <c r="C958" s="34"/>
       <c r="D958" s="34"/>
       <c r="E958" s="34"/>
@@ -57700,8 +57678,8 @@
       </c>
     </row>
     <row r="959">
-      <c r="A959" s="82"/>
-      <c r="B959" s="83"/>
+      <c r="A959" s="76"/>
+      <c r="B959" s="77"/>
       <c r="C959" s="34"/>
       <c r="D959" s="34"/>
       <c r="E959" s="34"/>
@@ -57726,8 +57704,8 @@
       </c>
     </row>
     <row r="960">
-      <c r="A960" s="82"/>
-      <c r="B960" s="83"/>
+      <c r="A960" s="76"/>
+      <c r="B960" s="77"/>
       <c r="C960" s="34"/>
       <c r="D960" s="34"/>
       <c r="E960" s="34"/>
@@ -57752,8 +57730,8 @@
       </c>
     </row>
     <row r="961">
-      <c r="A961" s="82"/>
-      <c r="B961" s="83"/>
+      <c r="A961" s="76"/>
+      <c r="B961" s="77"/>
       <c r="C961" s="34"/>
       <c r="D961" s="34"/>
       <c r="E961" s="34"/>
@@ -57778,8 +57756,8 @@
       </c>
     </row>
     <row r="962">
-      <c r="A962" s="82"/>
-      <c r="B962" s="83"/>
+      <c r="A962" s="76"/>
+      <c r="B962" s="77"/>
       <c r="C962" s="34"/>
       <c r="D962" s="34"/>
       <c r="E962" s="34"/>
@@ -57804,8 +57782,8 @@
       </c>
     </row>
     <row r="963">
-      <c r="A963" s="82"/>
-      <c r="B963" s="83"/>
+      <c r="A963" s="76"/>
+      <c r="B963" s="77"/>
       <c r="C963" s="34"/>
       <c r="D963" s="34"/>
       <c r="E963" s="34"/>
@@ -57830,8 +57808,8 @@
       </c>
     </row>
     <row r="964">
-      <c r="A964" s="82"/>
-      <c r="B964" s="83"/>
+      <c r="A964" s="76"/>
+      <c r="B964" s="77"/>
       <c r="C964" s="34"/>
       <c r="D964" s="34"/>
       <c r="E964" s="34"/>
@@ -57856,8 +57834,8 @@
       </c>
     </row>
     <row r="965">
-      <c r="A965" s="82"/>
-      <c r="B965" s="83"/>
+      <c r="A965" s="76"/>
+      <c r="B965" s="77"/>
       <c r="C965" s="34"/>
       <c r="D965" s="34"/>
       <c r="E965" s="34"/>
@@ -57882,8 +57860,8 @@
       </c>
     </row>
     <row r="966">
-      <c r="A966" s="82"/>
-      <c r="B966" s="83"/>
+      <c r="A966" s="76"/>
+      <c r="B966" s="77"/>
       <c r="C966" s="34"/>
       <c r="D966" s="34"/>
       <c r="E966" s="34"/>
@@ -57908,8 +57886,8 @@
       </c>
     </row>
     <row r="967">
-      <c r="A967" s="82"/>
-      <c r="B967" s="83"/>
+      <c r="A967" s="76"/>
+      <c r="B967" s="77"/>
       <c r="C967" s="34"/>
       <c r="D967" s="34"/>
       <c r="E967" s="34"/>
@@ -57934,8 +57912,8 @@
       </c>
     </row>
     <row r="968">
-      <c r="A968" s="82"/>
-      <c r="B968" s="83"/>
+      <c r="A968" s="76"/>
+      <c r="B968" s="77"/>
       <c r="C968" s="34"/>
       <c r="D968" s="34"/>
       <c r="E968" s="34"/>
@@ -57960,8 +57938,8 @@
       </c>
     </row>
     <row r="969">
-      <c r="A969" s="82"/>
-      <c r="B969" s="83"/>
+      <c r="A969" s="76"/>
+      <c r="B969" s="77"/>
       <c r="C969" s="34"/>
       <c r="D969" s="34"/>
       <c r="E969" s="34"/>
@@ -57986,8 +57964,8 @@
       </c>
     </row>
     <row r="970">
-      <c r="A970" s="82"/>
-      <c r="B970" s="83"/>
+      <c r="A970" s="76"/>
+      <c r="B970" s="77"/>
       <c r="C970" s="34"/>
       <c r="D970" s="34"/>
       <c r="E970" s="34"/>
@@ -58012,8 +57990,8 @@
       </c>
     </row>
     <row r="971">
-      <c r="A971" s="82"/>
-      <c r="B971" s="83"/>
+      <c r="A971" s="76"/>
+      <c r="B971" s="77"/>
       <c r="C971" s="34"/>
       <c r="D971" s="34"/>
       <c r="E971" s="34"/>
@@ -58038,8 +58016,8 @@
       </c>
     </row>
     <row r="972">
-      <c r="A972" s="82"/>
-      <c r="B972" s="83"/>
+      <c r="A972" s="76"/>
+      <c r="B972" s="77"/>
       <c r="C972" s="34"/>
       <c r="D972" s="34"/>
       <c r="E972" s="34"/>
@@ -58064,8 +58042,8 @@
       </c>
     </row>
     <row r="973">
-      <c r="A973" s="82"/>
-      <c r="B973" s="83"/>
+      <c r="A973" s="76"/>
+      <c r="B973" s="77"/>
       <c r="C973" s="34"/>
       <c r="D973" s="34"/>
       <c r="E973" s="34"/>
@@ -58090,8 +58068,8 @@
       </c>
     </row>
     <row r="974">
-      <c r="A974" s="82"/>
-      <c r="B974" s="83"/>
+      <c r="A974" s="76"/>
+      <c r="B974" s="77"/>
       <c r="C974" s="34"/>
       <c r="D974" s="34"/>
       <c r="E974" s="34"/>
@@ -58116,8 +58094,8 @@
       </c>
     </row>
     <row r="975">
-      <c r="A975" s="82"/>
-      <c r="B975" s="83"/>
+      <c r="A975" s="76"/>
+      <c r="B975" s="77"/>
       <c r="C975" s="34"/>
       <c r="D975" s="34"/>
       <c r="E975" s="34"/>
@@ -58142,8 +58120,8 @@
       </c>
     </row>
     <row r="976">
-      <c r="A976" s="82"/>
-      <c r="B976" s="83"/>
+      <c r="A976" s="76"/>
+      <c r="B976" s="77"/>
       <c r="C976" s="34"/>
       <c r="D976" s="34"/>
       <c r="E976" s="34"/>
@@ -58168,8 +58146,8 @@
       </c>
     </row>
     <row r="977">
-      <c r="A977" s="82"/>
-      <c r="B977" s="83"/>
+      <c r="A977" s="76"/>
+      <c r="B977" s="77"/>
       <c r="C977" s="34"/>
       <c r="D977" s="34"/>
       <c r="E977" s="34"/>
@@ -58194,8 +58172,8 @@
       </c>
     </row>
     <row r="978">
-      <c r="A978" s="82"/>
-      <c r="B978" s="83"/>
+      <c r="A978" s="76"/>
+      <c r="B978" s="77"/>
       <c r="C978" s="34"/>
       <c r="D978" s="34"/>
       <c r="E978" s="34"/>
@@ -58220,8 +58198,8 @@
       </c>
     </row>
     <row r="979">
-      <c r="A979" s="82"/>
-      <c r="B979" s="83"/>
+      <c r="A979" s="76"/>
+      <c r="B979" s="77"/>
       <c r="C979" s="34"/>
       <c r="D979" s="34"/>
       <c r="E979" s="34"/>
@@ -58246,8 +58224,8 @@
       </c>
     </row>
     <row r="980">
-      <c r="A980" s="82"/>
-      <c r="B980" s="83"/>
+      <c r="A980" s="76"/>
+      <c r="B980" s="77"/>
       <c r="C980" s="34"/>
       <c r="D980" s="34"/>
       <c r="E980" s="34"/>
@@ -58272,8 +58250,8 @@
       </c>
     </row>
     <row r="981">
-      <c r="A981" s="82"/>
-      <c r="B981" s="83"/>
+      <c r="A981" s="76"/>
+      <c r="B981" s="77"/>
       <c r="C981" s="34"/>
       <c r="D981" s="34"/>
       <c r="E981" s="34"/>
@@ -58298,8 +58276,8 @@
       </c>
     </row>
     <row r="982">
-      <c r="A982" s="82"/>
-      <c r="B982" s="83"/>
+      <c r="A982" s="76"/>
+      <c r="B982" s="77"/>
       <c r="C982" s="34"/>
       <c r="D982" s="34"/>
       <c r="E982" s="34"/>
@@ -58324,8 +58302,8 @@
       </c>
     </row>
     <row r="983">
-      <c r="A983" s="82"/>
-      <c r="B983" s="83"/>
+      <c r="A983" s="76"/>
+      <c r="B983" s="77"/>
       <c r="C983" s="34"/>
       <c r="D983" s="34"/>
       <c r="E983" s="34"/>
@@ -58350,8 +58328,8 @@
       </c>
     </row>
     <row r="984">
-      <c r="A984" s="82"/>
-      <c r="B984" s="83"/>
+      <c r="A984" s="76"/>
+      <c r="B984" s="77"/>
       <c r="C984" s="34"/>
       <c r="D984" s="34"/>
       <c r="E984" s="34"/>
@@ -58376,8 +58354,8 @@
       </c>
     </row>
     <row r="985">
-      <c r="A985" s="82"/>
-      <c r="B985" s="83"/>
+      <c r="A985" s="76"/>
+      <c r="B985" s="77"/>
       <c r="C985" s="34"/>
       <c r="D985" s="34"/>
       <c r="E985" s="34"/>
@@ -58402,8 +58380,8 @@
       </c>
     </row>
     <row r="986">
-      <c r="A986" s="82"/>
-      <c r="B986" s="83"/>
+      <c r="A986" s="76"/>
+      <c r="B986" s="77"/>
       <c r="C986" s="34"/>
       <c r="D986" s="34"/>
       <c r="E986" s="34"/>
@@ -58428,8 +58406,8 @@
       </c>
     </row>
     <row r="987">
-      <c r="A987" s="82"/>
-      <c r="B987" s="83"/>
+      <c r="A987" s="76"/>
+      <c r="B987" s="77"/>
       <c r="C987" s="34"/>
       <c r="D987" s="34"/>
       <c r="E987" s="34"/>
@@ -58454,8 +58432,8 @@
       </c>
     </row>
     <row r="988">
-      <c r="A988" s="82"/>
-      <c r="B988" s="83"/>
+      <c r="A988" s="76"/>
+      <c r="B988" s="77"/>
       <c r="C988" s="34"/>
       <c r="D988" s="34"/>
       <c r="E988" s="34"/>
@@ -58480,8 +58458,8 @@
       </c>
     </row>
     <row r="989">
-      <c r="A989" s="82"/>
-      <c r="B989" s="83"/>
+      <c r="A989" s="76"/>
+      <c r="B989" s="77"/>
       <c r="C989" s="34"/>
       <c r="D989" s="34"/>
       <c r="E989" s="34"/>
@@ -58506,8 +58484,8 @@
       </c>
     </row>
     <row r="990">
-      <c r="A990" s="82"/>
-      <c r="B990" s="83"/>
+      <c r="A990" s="76"/>
+      <c r="B990" s="77"/>
       <c r="C990" s="34"/>
       <c r="D990" s="34"/>
       <c r="E990" s="34"/>
@@ -58532,8 +58510,8 @@
       </c>
     </row>
     <row r="991">
-      <c r="A991" s="82"/>
-      <c r="B991" s="83"/>
+      <c r="A991" s="76"/>
+      <c r="B991" s="77"/>
       <c r="C991" s="34"/>
       <c r="D991" s="34"/>
       <c r="E991" s="34"/>
@@ -58558,8 +58536,8 @@
       </c>
     </row>
     <row r="992">
-      <c r="A992" s="82"/>
-      <c r="B992" s="83"/>
+      <c r="A992" s="76"/>
+      <c r="B992" s="77"/>
       <c r="C992" s="34"/>
       <c r="D992" s="34"/>
       <c r="E992" s="34"/>
@@ -58584,8 +58562,8 @@
       </c>
     </row>
     <row r="993">
-      <c r="A993" s="82"/>
-      <c r="B993" s="83"/>
+      <c r="A993" s="76"/>
+      <c r="B993" s="77"/>
       <c r="C993" s="34"/>
       <c r="D993" s="34"/>
       <c r="E993" s="34"/>
@@ -58610,8 +58588,8 @@
       </c>
     </row>
     <row r="994">
-      <c r="A994" s="82"/>
-      <c r="B994" s="83"/>
+      <c r="A994" s="76"/>
+      <c r="B994" s="77"/>
       <c r="C994" s="34"/>
       <c r="D994" s="34"/>
       <c r="E994" s="34"/>
@@ -58636,8 +58614,8 @@
       </c>
     </row>
     <row r="995">
-      <c r="A995" s="82"/>
-      <c r="B995" s="83"/>
+      <c r="A995" s="76"/>
+      <c r="B995" s="77"/>
       <c r="C995" s="34"/>
       <c r="D995" s="34"/>
       <c r="E995" s="34"/>
@@ -58662,8 +58640,8 @@
       </c>
     </row>
     <row r="996">
-      <c r="A996" s="82"/>
-      <c r="B996" s="83"/>
+      <c r="A996" s="76"/>
+      <c r="B996" s="77"/>
       <c r="C996" s="34"/>
       <c r="D996" s="34"/>
       <c r="E996" s="34"/>
@@ -58688,8 +58666,8 @@
       </c>
     </row>
     <row r="997">
-      <c r="A997" s="82"/>
-      <c r="B997" s="83"/>
+      <c r="A997" s="76"/>
+      <c r="B997" s="77"/>
       <c r="C997" s="34"/>
       <c r="D997" s="34"/>
       <c r="E997" s="34"/>
@@ -58714,8 +58692,8 @@
       </c>
     </row>
     <row r="998">
-      <c r="A998" s="82"/>
-      <c r="B998" s="83"/>
+      <c r="A998" s="76"/>
+      <c r="B998" s="77"/>
       <c r="C998" s="34"/>
       <c r="D998" s="34"/>
       <c r="E998" s="34"/>
@@ -58740,8 +58718,8 @@
       </c>
     </row>
     <row r="999">
-      <c r="A999" s="82"/>
-      <c r="B999" s="83"/>
+      <c r="A999" s="76"/>
+      <c r="B999" s="77"/>
       <c r="C999" s="34"/>
       <c r="D999" s="34"/>
       <c r="E999" s="34"/>
@@ -58766,8 +58744,8 @@
       </c>
     </row>
     <row r="1000">
-      <c r="A1000" s="82"/>
-      <c r="B1000" s="83"/>
+      <c r="A1000" s="76"/>
+      <c r="B1000" s="77"/>
       <c r="C1000" s="34"/>
       <c r="D1000" s="34"/>
       <c r="E1000" s="34"/>
@@ -58792,8 +58770,8 @@
       </c>
     </row>
     <row r="1001">
-      <c r="A1001" s="82"/>
-      <c r="B1001" s="83"/>
+      <c r="A1001" s="76"/>
+      <c r="B1001" s="77"/>
       <c r="C1001" s="34"/>
       <c r="D1001" s="34"/>
       <c r="E1001" s="34"/>

</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201209
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -577,7 +577,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8190" uniqueCount="2539">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8215" uniqueCount="2548">
   <si>
     <t>案例</t>
   </si>
@@ -9149,6 +9149,36 @@
   <si>
     <t>來臺工作，入境後至檢疫旅館進行居家檢疫，迄今無症狀，12月5日檢疫期滿後由仲介公司安排自費採檢</t>
   </si>
+  <si>
+    <t>#718</t>
+  </si>
+  <si>
+    <t>-11/23 印尼→台灣</t>
+  </si>
+  <si>
+    <t>12/7 採檢
+12/8 確診</t>
+  </si>
+  <si>
+    <t>新增2例境外移入COVID-19病例，自印尼及中國入境</t>
+  </si>
+  <si>
+    <t>#719</t>
+  </si>
+  <si>
+    <t>9月中旬-11/22 中國浙江</t>
+  </si>
+  <si>
+    <t>12/5 採檢
+12/8 確診</t>
+  </si>
+  <si>
+    <t>發冷 發燒</t>
+  </si>
+  <si>
+    <t>處理公事
+Ct值15</t>
+  </si>
 </sst>
 </file>
 
@@ -9158,7 +9188,7 @@
     <numFmt numFmtId="164" formatCode="mm&quot;月&quot;dd&quot;日 &quot;dddd"/>
     <numFmt numFmtId="165" formatCode="m/d"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="21">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -9243,6 +9273,10 @@
       <u/>
       <color rgb="FF0000FF"/>
     </font>
+    <font/>
+    <font>
+      <color rgb="FF000000"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -9288,7 +9322,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="85">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -9516,6 +9550,27 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="19" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="20" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
@@ -51438,60 +51493,120 @@
       </c>
     </row>
     <row r="719">
-      <c r="A719" s="76"/>
-      <c r="B719" s="77"/>
-      <c r="C719" s="34"/>
-      <c r="D719" s="34"/>
-      <c r="E719" s="34"/>
+      <c r="A719" s="76" t="s">
+        <v>2539</v>
+      </c>
+      <c r="B719" s="6">
+        <v>44173.0</v>
+      </c>
+      <c r="C719" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D719" s="77" t="s">
+        <v>76</v>
+      </c>
+      <c r="E719" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F719" s="34"/>
-      <c r="G719" s="34"/>
-      <c r="H719" s="21"/>
-      <c r="I719" s="19"/>
-      <c r="J719" s="10"/>
-      <c r="K719" s="22"/>
-      <c r="L719" s="23"/>
-      <c r="M719" s="22"/>
+      <c r="G719" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H719" s="78" t="s">
+        <v>2540</v>
+      </c>
+      <c r="I719" s="79">
+        <v>44158.0</v>
+      </c>
+      <c r="J719" s="80" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K719" s="13" t="s">
+        <v>2541</v>
+      </c>
+      <c r="L719" s="80" t="s">
+        <v>426</v>
+      </c>
+      <c r="M719" s="81" t="s">
+        <v>1442</v>
+      </c>
       <c r="N719" s="25"/>
-      <c r="O719" s="21"/>
-      <c r="P719" s="21"/>
+      <c r="O719" s="78" t="s">
+        <v>85</v>
+      </c>
+      <c r="P719" s="78" t="s">
+        <v>2096</v>
+      </c>
       <c r="Q719" s="19"/>
       <c r="R719" s="19"/>
-      <c r="S719" s="20"/>
+      <c r="S719" s="61" t="s">
+        <v>2542</v>
+      </c>
       <c r="T719" s="20"/>
       <c r="U719" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#718</v>
       </c>
     </row>
     <row r="720">
-      <c r="A720" s="76"/>
-      <c r="B720" s="77"/>
-      <c r="C720" s="34"/>
-      <c r="D720" s="34"/>
-      <c r="E720" s="34"/>
+      <c r="A720" s="76" t="s">
+        <v>2543</v>
+      </c>
+      <c r="B720" s="6">
+        <v>44173.0</v>
+      </c>
+      <c r="C720" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D720" s="77" t="s">
+        <v>22</v>
+      </c>
+      <c r="E720" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F720" s="34"/>
-      <c r="G720" s="34"/>
-      <c r="H720" s="21"/>
-      <c r="I720" s="19"/>
-      <c r="J720" s="10"/>
-      <c r="K720" s="22"/>
-      <c r="L720" s="23"/>
-      <c r="M720" s="22"/>
+      <c r="G720" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H720" s="78" t="s">
+        <v>2544</v>
+      </c>
+      <c r="I720" s="79">
+        <v>44157.0</v>
+      </c>
+      <c r="J720" s="82">
+        <v>44169.0</v>
+      </c>
+      <c r="K720" s="13" t="s">
+        <v>2545</v>
+      </c>
+      <c r="L720" s="80" t="s">
+        <v>426</v>
+      </c>
+      <c r="M720" s="81" t="s">
+        <v>2546</v>
+      </c>
       <c r="N720" s="25"/>
-      <c r="O720" s="21"/>
-      <c r="P720" s="21"/>
+      <c r="O720" s="78" t="s">
+        <v>85</v>
+      </c>
+      <c r="P720" s="78" t="s">
+        <v>2547</v>
+      </c>
       <c r="Q720" s="19"/>
       <c r="R720" s="19"/>
-      <c r="S720" s="20"/>
+      <c r="S720" s="61" t="s">
+        <v>2542</v>
+      </c>
       <c r="T720" s="20"/>
       <c r="U720" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#719</v>
       </c>
     </row>
     <row r="721">
-      <c r="A721" s="76"/>
-      <c r="B721" s="77"/>
+      <c r="A721" s="83"/>
+      <c r="B721" s="84"/>
       <c r="C721" s="34"/>
       <c r="D721" s="34"/>
       <c r="E721" s="34"/>
@@ -51516,8 +51631,8 @@
       </c>
     </row>
     <row r="722">
-      <c r="A722" s="76"/>
-      <c r="B722" s="77"/>
+      <c r="A722" s="83"/>
+      <c r="B722" s="84"/>
       <c r="C722" s="34"/>
       <c r="D722" s="34"/>
       <c r="E722" s="34"/>
@@ -51542,8 +51657,8 @@
       </c>
     </row>
     <row r="723">
-      <c r="A723" s="76"/>
-      <c r="B723" s="77"/>
+      <c r="A723" s="83"/>
+      <c r="B723" s="84"/>
       <c r="C723" s="34"/>
       <c r="D723" s="34"/>
       <c r="E723" s="34"/>
@@ -51568,8 +51683,8 @@
       </c>
     </row>
     <row r="724">
-      <c r="A724" s="76"/>
-      <c r="B724" s="77"/>
+      <c r="A724" s="83"/>
+      <c r="B724" s="84"/>
       <c r="C724" s="34"/>
       <c r="D724" s="34"/>
       <c r="E724" s="34"/>
@@ -51594,8 +51709,8 @@
       </c>
     </row>
     <row r="725">
-      <c r="A725" s="76"/>
-      <c r="B725" s="77"/>
+      <c r="A725" s="83"/>
+      <c r="B725" s="84"/>
       <c r="C725" s="34"/>
       <c r="D725" s="34"/>
       <c r="E725" s="34"/>
@@ -51620,8 +51735,8 @@
       </c>
     </row>
     <row r="726">
-      <c r="A726" s="76"/>
-      <c r="B726" s="77"/>
+      <c r="A726" s="83"/>
+      <c r="B726" s="84"/>
       <c r="C726" s="34"/>
       <c r="D726" s="34"/>
       <c r="E726" s="34"/>
@@ -51646,8 +51761,8 @@
       </c>
     </row>
     <row r="727">
-      <c r="A727" s="76"/>
-      <c r="B727" s="77"/>
+      <c r="A727" s="83"/>
+      <c r="B727" s="84"/>
       <c r="C727" s="34"/>
       <c r="D727" s="34"/>
       <c r="E727" s="34"/>
@@ -51672,8 +51787,8 @@
       </c>
     </row>
     <row r="728">
-      <c r="A728" s="76"/>
-      <c r="B728" s="77"/>
+      <c r="A728" s="83"/>
+      <c r="B728" s="84"/>
       <c r="C728" s="34"/>
       <c r="D728" s="34"/>
       <c r="E728" s="34"/>
@@ -51698,8 +51813,8 @@
       </c>
     </row>
     <row r="729">
-      <c r="A729" s="76"/>
-      <c r="B729" s="77"/>
+      <c r="A729" s="83"/>
+      <c r="B729" s="84"/>
       <c r="C729" s="34"/>
       <c r="D729" s="34"/>
       <c r="E729" s="34"/>
@@ -51724,8 +51839,8 @@
       </c>
     </row>
     <row r="730">
-      <c r="A730" s="76"/>
-      <c r="B730" s="77"/>
+      <c r="A730" s="83"/>
+      <c r="B730" s="84"/>
       <c r="C730" s="34"/>
       <c r="D730" s="34"/>
       <c r="E730" s="34"/>
@@ -51750,8 +51865,8 @@
       </c>
     </row>
     <row r="731">
-      <c r="A731" s="76"/>
-      <c r="B731" s="77"/>
+      <c r="A731" s="83"/>
+      <c r="B731" s="84"/>
       <c r="C731" s="34"/>
       <c r="D731" s="34"/>
       <c r="E731" s="34"/>
@@ -51776,8 +51891,8 @@
       </c>
     </row>
     <row r="732">
-      <c r="A732" s="76"/>
-      <c r="B732" s="77"/>
+      <c r="A732" s="83"/>
+      <c r="B732" s="84"/>
       <c r="C732" s="34"/>
       <c r="D732" s="34"/>
       <c r="E732" s="34"/>
@@ -51802,8 +51917,8 @@
       </c>
     </row>
     <row r="733">
-      <c r="A733" s="76"/>
-      <c r="B733" s="77"/>
+      <c r="A733" s="83"/>
+      <c r="B733" s="84"/>
       <c r="C733" s="34"/>
       <c r="D733" s="34"/>
       <c r="E733" s="34"/>
@@ -51828,8 +51943,8 @@
       </c>
     </row>
     <row r="734">
-      <c r="A734" s="76"/>
-      <c r="B734" s="77"/>
+      <c r="A734" s="83"/>
+      <c r="B734" s="84"/>
       <c r="C734" s="34"/>
       <c r="D734" s="34"/>
       <c r="E734" s="34"/>
@@ -51854,8 +51969,8 @@
       </c>
     </row>
     <row r="735">
-      <c r="A735" s="76"/>
-      <c r="B735" s="77"/>
+      <c r="A735" s="83"/>
+      <c r="B735" s="84"/>
       <c r="C735" s="34"/>
       <c r="D735" s="34"/>
       <c r="E735" s="34"/>
@@ -51880,8 +51995,8 @@
       </c>
     </row>
     <row r="736">
-      <c r="A736" s="76"/>
-      <c r="B736" s="77"/>
+      <c r="A736" s="83"/>
+      <c r="B736" s="84"/>
       <c r="C736" s="34"/>
       <c r="D736" s="34"/>
       <c r="E736" s="34"/>
@@ -51906,8 +52021,8 @@
       </c>
     </row>
     <row r="737">
-      <c r="A737" s="76"/>
-      <c r="B737" s="77"/>
+      <c r="A737" s="83"/>
+      <c r="B737" s="84"/>
       <c r="C737" s="34"/>
       <c r="D737" s="34"/>
       <c r="E737" s="34"/>
@@ -51932,8 +52047,8 @@
       </c>
     </row>
     <row r="738">
-      <c r="A738" s="76"/>
-      <c r="B738" s="77"/>
+      <c r="A738" s="83"/>
+      <c r="B738" s="84"/>
       <c r="C738" s="34"/>
       <c r="D738" s="34"/>
       <c r="E738" s="34"/>
@@ -51958,8 +52073,8 @@
       </c>
     </row>
     <row r="739">
-      <c r="A739" s="76"/>
-      <c r="B739" s="77"/>
+      <c r="A739" s="83"/>
+      <c r="B739" s="84"/>
       <c r="C739" s="34"/>
       <c r="D739" s="34"/>
       <c r="E739" s="34"/>
@@ -51984,8 +52099,8 @@
       </c>
     </row>
     <row r="740">
-      <c r="A740" s="76"/>
-      <c r="B740" s="77"/>
+      <c r="A740" s="83"/>
+      <c r="B740" s="84"/>
       <c r="C740" s="34"/>
       <c r="D740" s="34"/>
       <c r="E740" s="34"/>
@@ -52010,8 +52125,8 @@
       </c>
     </row>
     <row r="741">
-      <c r="A741" s="76"/>
-      <c r="B741" s="77"/>
+      <c r="A741" s="83"/>
+      <c r="B741" s="84"/>
       <c r="C741" s="34"/>
       <c r="D741" s="34"/>
       <c r="E741" s="34"/>
@@ -52036,8 +52151,8 @@
       </c>
     </row>
     <row r="742">
-      <c r="A742" s="76"/>
-      <c r="B742" s="77"/>
+      <c r="A742" s="83"/>
+      <c r="B742" s="84"/>
       <c r="C742" s="34"/>
       <c r="D742" s="34"/>
       <c r="E742" s="34"/>
@@ -52062,8 +52177,8 @@
       </c>
     </row>
     <row r="743">
-      <c r="A743" s="76"/>
-      <c r="B743" s="77"/>
+      <c r="A743" s="83"/>
+      <c r="B743" s="84"/>
       <c r="C743" s="34"/>
       <c r="D743" s="34"/>
       <c r="E743" s="34"/>
@@ -52088,8 +52203,8 @@
       </c>
     </row>
     <row r="744">
-      <c r="A744" s="76"/>
-      <c r="B744" s="77"/>
+      <c r="A744" s="83"/>
+      <c r="B744" s="84"/>
       <c r="C744" s="34"/>
       <c r="D744" s="34"/>
       <c r="E744" s="34"/>
@@ -52114,8 +52229,8 @@
       </c>
     </row>
     <row r="745">
-      <c r="A745" s="76"/>
-      <c r="B745" s="77"/>
+      <c r="A745" s="83"/>
+      <c r="B745" s="84"/>
       <c r="C745" s="34"/>
       <c r="D745" s="34"/>
       <c r="E745" s="34"/>
@@ -52140,8 +52255,8 @@
       </c>
     </row>
     <row r="746">
-      <c r="A746" s="76"/>
-      <c r="B746" s="77"/>
+      <c r="A746" s="83"/>
+      <c r="B746" s="84"/>
       <c r="C746" s="34"/>
       <c r="D746" s="34"/>
       <c r="E746" s="34"/>
@@ -52166,8 +52281,8 @@
       </c>
     </row>
     <row r="747">
-      <c r="A747" s="76"/>
-      <c r="B747" s="77"/>
+      <c r="A747" s="83"/>
+      <c r="B747" s="84"/>
       <c r="C747" s="34"/>
       <c r="D747" s="34"/>
       <c r="E747" s="34"/>
@@ -52192,8 +52307,8 @@
       </c>
     </row>
     <row r="748">
-      <c r="A748" s="76"/>
-      <c r="B748" s="77"/>
+      <c r="A748" s="83"/>
+      <c r="B748" s="84"/>
       <c r="C748" s="34"/>
       <c r="D748" s="34"/>
       <c r="E748" s="34"/>
@@ -52218,8 +52333,8 @@
       </c>
     </row>
     <row r="749">
-      <c r="A749" s="76"/>
-      <c r="B749" s="77"/>
+      <c r="A749" s="83"/>
+      <c r="B749" s="84"/>
       <c r="C749" s="34"/>
       <c r="D749" s="34"/>
       <c r="E749" s="34"/>
@@ -52244,8 +52359,8 @@
       </c>
     </row>
     <row r="750">
-      <c r="A750" s="76"/>
-      <c r="B750" s="77"/>
+      <c r="A750" s="83"/>
+      <c r="B750" s="84"/>
       <c r="C750" s="34"/>
       <c r="D750" s="34"/>
       <c r="E750" s="34"/>
@@ -52270,8 +52385,8 @@
       </c>
     </row>
     <row r="751">
-      <c r="A751" s="76"/>
-      <c r="B751" s="77"/>
+      <c r="A751" s="83"/>
+      <c r="B751" s="84"/>
       <c r="C751" s="34"/>
       <c r="D751" s="34"/>
       <c r="E751" s="34"/>
@@ -52296,8 +52411,8 @@
       </c>
     </row>
     <row r="752">
-      <c r="A752" s="76"/>
-      <c r="B752" s="77"/>
+      <c r="A752" s="83"/>
+      <c r="B752" s="84"/>
       <c r="C752" s="34"/>
       <c r="D752" s="34"/>
       <c r="E752" s="34"/>
@@ -52322,8 +52437,8 @@
       </c>
     </row>
     <row r="753">
-      <c r="A753" s="76"/>
-      <c r="B753" s="77"/>
+      <c r="A753" s="83"/>
+      <c r="B753" s="84"/>
       <c r="C753" s="34"/>
       <c r="D753" s="34"/>
       <c r="E753" s="34"/>
@@ -52348,8 +52463,8 @@
       </c>
     </row>
     <row r="754">
-      <c r="A754" s="76"/>
-      <c r="B754" s="77"/>
+      <c r="A754" s="83"/>
+      <c r="B754" s="84"/>
       <c r="C754" s="34"/>
       <c r="D754" s="34"/>
       <c r="E754" s="34"/>
@@ -52374,8 +52489,8 @@
       </c>
     </row>
     <row r="755">
-      <c r="A755" s="76"/>
-      <c r="B755" s="77"/>
+      <c r="A755" s="83"/>
+      <c r="B755" s="84"/>
       <c r="C755" s="34"/>
       <c r="D755" s="34"/>
       <c r="E755" s="34"/>
@@ -52400,8 +52515,8 @@
       </c>
     </row>
     <row r="756">
-      <c r="A756" s="76"/>
-      <c r="B756" s="77"/>
+      <c r="A756" s="83"/>
+      <c r="B756" s="84"/>
       <c r="C756" s="34"/>
       <c r="D756" s="34"/>
       <c r="E756" s="34"/>
@@ -52426,8 +52541,8 @@
       </c>
     </row>
     <row r="757">
-      <c r="A757" s="76"/>
-      <c r="B757" s="77"/>
+      <c r="A757" s="83"/>
+      <c r="B757" s="84"/>
       <c r="C757" s="34"/>
       <c r="D757" s="34"/>
       <c r="E757" s="34"/>
@@ -52452,8 +52567,8 @@
       </c>
     </row>
     <row r="758">
-      <c r="A758" s="76"/>
-      <c r="B758" s="77"/>
+      <c r="A758" s="83"/>
+      <c r="B758" s="84"/>
       <c r="C758" s="34"/>
       <c r="D758" s="34"/>
       <c r="E758" s="34"/>
@@ -52478,8 +52593,8 @@
       </c>
     </row>
     <row r="759">
-      <c r="A759" s="76"/>
-      <c r="B759" s="77"/>
+      <c r="A759" s="83"/>
+      <c r="B759" s="84"/>
       <c r="C759" s="34"/>
       <c r="D759" s="34"/>
       <c r="E759" s="34"/>
@@ -52504,8 +52619,8 @@
       </c>
     </row>
     <row r="760">
-      <c r="A760" s="76"/>
-      <c r="B760" s="77"/>
+      <c r="A760" s="83"/>
+      <c r="B760" s="84"/>
       <c r="C760" s="34"/>
       <c r="D760" s="34"/>
       <c r="E760" s="34"/>
@@ -52530,8 +52645,8 @@
       </c>
     </row>
     <row r="761">
-      <c r="A761" s="76"/>
-      <c r="B761" s="77"/>
+      <c r="A761" s="83"/>
+      <c r="B761" s="84"/>
       <c r="C761" s="34"/>
       <c r="D761" s="34"/>
       <c r="E761" s="34"/>
@@ -52556,8 +52671,8 @@
       </c>
     </row>
     <row r="762">
-      <c r="A762" s="76"/>
-      <c r="B762" s="77"/>
+      <c r="A762" s="83"/>
+      <c r="B762" s="84"/>
       <c r="C762" s="34"/>
       <c r="D762" s="34"/>
       <c r="E762" s="34"/>
@@ -52582,8 +52697,8 @@
       </c>
     </row>
     <row r="763">
-      <c r="A763" s="76"/>
-      <c r="B763" s="77"/>
+      <c r="A763" s="83"/>
+      <c r="B763" s="84"/>
       <c r="C763" s="34"/>
       <c r="D763" s="34"/>
       <c r="E763" s="34"/>
@@ -52608,8 +52723,8 @@
       </c>
     </row>
     <row r="764">
-      <c r="A764" s="76"/>
-      <c r="B764" s="77"/>
+      <c r="A764" s="83"/>
+      <c r="B764" s="84"/>
       <c r="C764" s="34"/>
       <c r="D764" s="34"/>
       <c r="E764" s="34"/>
@@ -52634,8 +52749,8 @@
       </c>
     </row>
     <row r="765">
-      <c r="A765" s="76"/>
-      <c r="B765" s="77"/>
+      <c r="A765" s="83"/>
+      <c r="B765" s="84"/>
       <c r="C765" s="34"/>
       <c r="D765" s="34"/>
       <c r="E765" s="34"/>
@@ -52660,8 +52775,8 @@
       </c>
     </row>
     <row r="766">
-      <c r="A766" s="76"/>
-      <c r="B766" s="77"/>
+      <c r="A766" s="83"/>
+      <c r="B766" s="84"/>
       <c r="C766" s="34"/>
       <c r="D766" s="34"/>
       <c r="E766" s="34"/>
@@ -52686,8 +52801,8 @@
       </c>
     </row>
     <row r="767">
-      <c r="A767" s="76"/>
-      <c r="B767" s="77"/>
+      <c r="A767" s="83"/>
+      <c r="B767" s="84"/>
       <c r="C767" s="34"/>
       <c r="D767" s="34"/>
       <c r="E767" s="34"/>
@@ -52712,8 +52827,8 @@
       </c>
     </row>
     <row r="768">
-      <c r="A768" s="76"/>
-      <c r="B768" s="77"/>
+      <c r="A768" s="83"/>
+      <c r="B768" s="84"/>
       <c r="C768" s="34"/>
       <c r="D768" s="34"/>
       <c r="E768" s="34"/>
@@ -52738,8 +52853,8 @@
       </c>
     </row>
     <row r="769">
-      <c r="A769" s="76"/>
-      <c r="B769" s="77"/>
+      <c r="A769" s="83"/>
+      <c r="B769" s="84"/>
       <c r="C769" s="34"/>
       <c r="D769" s="34"/>
       <c r="E769" s="34"/>
@@ -52764,8 +52879,8 @@
       </c>
     </row>
     <row r="770">
-      <c r="A770" s="76"/>
-      <c r="B770" s="77"/>
+      <c r="A770" s="83"/>
+      <c r="B770" s="84"/>
       <c r="C770" s="34"/>
       <c r="D770" s="34"/>
       <c r="E770" s="34"/>
@@ -52790,8 +52905,8 @@
       </c>
     </row>
     <row r="771">
-      <c r="A771" s="76"/>
-      <c r="B771" s="77"/>
+      <c r="A771" s="83"/>
+      <c r="B771" s="84"/>
       <c r="C771" s="34"/>
       <c r="D771" s="34"/>
       <c r="E771" s="34"/>
@@ -52816,8 +52931,8 @@
       </c>
     </row>
     <row r="772">
-      <c r="A772" s="76"/>
-      <c r="B772" s="77"/>
+      <c r="A772" s="83"/>
+      <c r="B772" s="84"/>
       <c r="C772" s="34"/>
       <c r="D772" s="34"/>
       <c r="E772" s="34"/>
@@ -52842,8 +52957,8 @@
       </c>
     </row>
     <row r="773">
-      <c r="A773" s="76"/>
-      <c r="B773" s="77"/>
+      <c r="A773" s="83"/>
+      <c r="B773" s="84"/>
       <c r="C773" s="34"/>
       <c r="D773" s="34"/>
       <c r="E773" s="34"/>
@@ -52868,8 +52983,8 @@
       </c>
     </row>
     <row r="774">
-      <c r="A774" s="76"/>
-      <c r="B774" s="77"/>
+      <c r="A774" s="83"/>
+      <c r="B774" s="84"/>
       <c r="C774" s="34"/>
       <c r="D774" s="34"/>
       <c r="E774" s="34"/>
@@ -52894,8 +53009,8 @@
       </c>
     </row>
     <row r="775">
-      <c r="A775" s="76"/>
-      <c r="B775" s="77"/>
+      <c r="A775" s="83"/>
+      <c r="B775" s="84"/>
       <c r="C775" s="34"/>
       <c r="D775" s="34"/>
       <c r="E775" s="34"/>
@@ -52920,8 +53035,8 @@
       </c>
     </row>
     <row r="776">
-      <c r="A776" s="76"/>
-      <c r="B776" s="77"/>
+      <c r="A776" s="83"/>
+      <c r="B776" s="84"/>
       <c r="C776" s="34"/>
       <c r="D776" s="34"/>
       <c r="E776" s="34"/>
@@ -52946,8 +53061,8 @@
       </c>
     </row>
     <row r="777">
-      <c r="A777" s="76"/>
-      <c r="B777" s="77"/>
+      <c r="A777" s="83"/>
+      <c r="B777" s="84"/>
       <c r="C777" s="34"/>
       <c r="D777" s="34"/>
       <c r="E777" s="34"/>
@@ -52972,8 +53087,8 @@
       </c>
     </row>
     <row r="778">
-      <c r="A778" s="76"/>
-      <c r="B778" s="77"/>
+      <c r="A778" s="83"/>
+      <c r="B778" s="84"/>
       <c r="C778" s="34"/>
       <c r="D778" s="34"/>
       <c r="E778" s="34"/>
@@ -52998,8 +53113,8 @@
       </c>
     </row>
     <row r="779">
-      <c r="A779" s="76"/>
-      <c r="B779" s="77"/>
+      <c r="A779" s="83"/>
+      <c r="B779" s="84"/>
       <c r="C779" s="34"/>
       <c r="D779" s="34"/>
       <c r="E779" s="34"/>
@@ -53024,8 +53139,8 @@
       </c>
     </row>
     <row r="780">
-      <c r="A780" s="76"/>
-      <c r="B780" s="77"/>
+      <c r="A780" s="83"/>
+      <c r="B780" s="84"/>
       <c r="C780" s="34"/>
       <c r="D780" s="34"/>
       <c r="E780" s="34"/>
@@ -53050,8 +53165,8 @@
       </c>
     </row>
     <row r="781">
-      <c r="A781" s="76"/>
-      <c r="B781" s="77"/>
+      <c r="A781" s="83"/>
+      <c r="B781" s="84"/>
       <c r="C781" s="34"/>
       <c r="D781" s="34"/>
       <c r="E781" s="34"/>
@@ -53076,8 +53191,8 @@
       </c>
     </row>
     <row r="782">
-      <c r="A782" s="76"/>
-      <c r="B782" s="77"/>
+      <c r="A782" s="83"/>
+      <c r="B782" s="84"/>
       <c r="C782" s="34"/>
       <c r="D782" s="34"/>
       <c r="E782" s="34"/>
@@ -53102,8 +53217,8 @@
       </c>
     </row>
     <row r="783">
-      <c r="A783" s="76"/>
-      <c r="B783" s="77"/>
+      <c r="A783" s="83"/>
+      <c r="B783" s="84"/>
       <c r="C783" s="34"/>
       <c r="D783" s="34"/>
       <c r="E783" s="34"/>
@@ -53128,8 +53243,8 @@
       </c>
     </row>
     <row r="784">
-      <c r="A784" s="76"/>
-      <c r="B784" s="77"/>
+      <c r="A784" s="83"/>
+      <c r="B784" s="84"/>
       <c r="C784" s="34"/>
       <c r="D784" s="34"/>
       <c r="E784" s="34"/>
@@ -53154,8 +53269,8 @@
       </c>
     </row>
     <row r="785">
-      <c r="A785" s="76"/>
-      <c r="B785" s="77"/>
+      <c r="A785" s="83"/>
+      <c r="B785" s="84"/>
       <c r="C785" s="34"/>
       <c r="D785" s="34"/>
       <c r="E785" s="34"/>
@@ -53180,8 +53295,8 @@
       </c>
     </row>
     <row r="786">
-      <c r="A786" s="76"/>
-      <c r="B786" s="77"/>
+      <c r="A786" s="83"/>
+      <c r="B786" s="84"/>
       <c r="C786" s="34"/>
       <c r="D786" s="34"/>
       <c r="E786" s="34"/>
@@ -53206,8 +53321,8 @@
       </c>
     </row>
     <row r="787">
-      <c r="A787" s="76"/>
-      <c r="B787" s="77"/>
+      <c r="A787" s="83"/>
+      <c r="B787" s="84"/>
       <c r="C787" s="34"/>
       <c r="D787" s="34"/>
       <c r="E787" s="34"/>
@@ -53232,8 +53347,8 @@
       </c>
     </row>
     <row r="788">
-      <c r="A788" s="76"/>
-      <c r="B788" s="77"/>
+      <c r="A788" s="83"/>
+      <c r="B788" s="84"/>
       <c r="C788" s="34"/>
       <c r="D788" s="34"/>
       <c r="E788" s="34"/>
@@ -53258,8 +53373,8 @@
       </c>
     </row>
     <row r="789">
-      <c r="A789" s="76"/>
-      <c r="B789" s="77"/>
+      <c r="A789" s="83"/>
+      <c r="B789" s="84"/>
       <c r="C789" s="34"/>
       <c r="D789" s="34"/>
       <c r="E789" s="34"/>
@@ -53284,8 +53399,8 @@
       </c>
     </row>
     <row r="790">
-      <c r="A790" s="76"/>
-      <c r="B790" s="77"/>
+      <c r="A790" s="83"/>
+      <c r="B790" s="84"/>
       <c r="C790" s="34"/>
       <c r="D790" s="34"/>
       <c r="E790" s="34"/>
@@ -53310,8 +53425,8 @@
       </c>
     </row>
     <row r="791">
-      <c r="A791" s="76"/>
-      <c r="B791" s="77"/>
+      <c r="A791" s="83"/>
+      <c r="B791" s="84"/>
       <c r="C791" s="34"/>
       <c r="D791" s="34"/>
       <c r="E791" s="34"/>
@@ -53336,8 +53451,8 @@
       </c>
     </row>
     <row r="792">
-      <c r="A792" s="76"/>
-      <c r="B792" s="77"/>
+      <c r="A792" s="83"/>
+      <c r="B792" s="84"/>
       <c r="C792" s="34"/>
       <c r="D792" s="34"/>
       <c r="E792" s="34"/>
@@ -53362,8 +53477,8 @@
       </c>
     </row>
     <row r="793">
-      <c r="A793" s="76"/>
-      <c r="B793" s="77"/>
+      <c r="A793" s="83"/>
+      <c r="B793" s="84"/>
       <c r="C793" s="34"/>
       <c r="D793" s="34"/>
       <c r="E793" s="34"/>
@@ -53388,8 +53503,8 @@
       </c>
     </row>
     <row r="794">
-      <c r="A794" s="76"/>
-      <c r="B794" s="77"/>
+      <c r="A794" s="83"/>
+      <c r="B794" s="84"/>
       <c r="C794" s="34"/>
       <c r="D794" s="34"/>
       <c r="E794" s="34"/>
@@ -53414,8 +53529,8 @@
       </c>
     </row>
     <row r="795">
-      <c r="A795" s="76"/>
-      <c r="B795" s="77"/>
+      <c r="A795" s="83"/>
+      <c r="B795" s="84"/>
       <c r="C795" s="34"/>
       <c r="D795" s="34"/>
       <c r="E795" s="34"/>
@@ -53440,8 +53555,8 @@
       </c>
     </row>
     <row r="796">
-      <c r="A796" s="76"/>
-      <c r="B796" s="77"/>
+      <c r="A796" s="83"/>
+      <c r="B796" s="84"/>
       <c r="C796" s="34"/>
       <c r="D796" s="34"/>
       <c r="E796" s="34"/>
@@ -53466,8 +53581,8 @@
       </c>
     </row>
     <row r="797">
-      <c r="A797" s="76"/>
-      <c r="B797" s="77"/>
+      <c r="A797" s="83"/>
+      <c r="B797" s="84"/>
       <c r="C797" s="34"/>
       <c r="D797" s="34"/>
       <c r="E797" s="34"/>
@@ -53492,8 +53607,8 @@
       </c>
     </row>
     <row r="798">
-      <c r="A798" s="76"/>
-      <c r="B798" s="77"/>
+      <c r="A798" s="83"/>
+      <c r="B798" s="84"/>
       <c r="C798" s="34"/>
       <c r="D798" s="34"/>
       <c r="E798" s="34"/>
@@ -53518,8 +53633,8 @@
       </c>
     </row>
     <row r="799">
-      <c r="A799" s="76"/>
-      <c r="B799" s="77"/>
+      <c r="A799" s="83"/>
+      <c r="B799" s="84"/>
       <c r="C799" s="34"/>
       <c r="D799" s="34"/>
       <c r="E799" s="34"/>
@@ -53544,8 +53659,8 @@
       </c>
     </row>
     <row r="800">
-      <c r="A800" s="76"/>
-      <c r="B800" s="77"/>
+      <c r="A800" s="83"/>
+      <c r="B800" s="84"/>
       <c r="C800" s="34"/>
       <c r="D800" s="34"/>
       <c r="E800" s="34"/>
@@ -53570,8 +53685,8 @@
       </c>
     </row>
     <row r="801">
-      <c r="A801" s="76"/>
-      <c r="B801" s="77"/>
+      <c r="A801" s="83"/>
+      <c r="B801" s="84"/>
       <c r="C801" s="34"/>
       <c r="D801" s="34"/>
       <c r="E801" s="34"/>
@@ -53596,8 +53711,8 @@
       </c>
     </row>
     <row r="802">
-      <c r="A802" s="76"/>
-      <c r="B802" s="77"/>
+      <c r="A802" s="83"/>
+      <c r="B802" s="84"/>
       <c r="C802" s="34"/>
       <c r="D802" s="34"/>
       <c r="E802" s="34"/>
@@ -53622,8 +53737,8 @@
       </c>
     </row>
     <row r="803">
-      <c r="A803" s="76"/>
-      <c r="B803" s="77"/>
+      <c r="A803" s="83"/>
+      <c r="B803" s="84"/>
       <c r="C803" s="34"/>
       <c r="D803" s="34"/>
       <c r="E803" s="34"/>
@@ -53648,8 +53763,8 @@
       </c>
     </row>
     <row r="804">
-      <c r="A804" s="76"/>
-      <c r="B804" s="77"/>
+      <c r="A804" s="83"/>
+      <c r="B804" s="84"/>
       <c r="C804" s="34"/>
       <c r="D804" s="34"/>
       <c r="E804" s="34"/>
@@ -53674,8 +53789,8 @@
       </c>
     </row>
     <row r="805">
-      <c r="A805" s="76"/>
-      <c r="B805" s="77"/>
+      <c r="A805" s="83"/>
+      <c r="B805" s="84"/>
       <c r="C805" s="34"/>
       <c r="D805" s="34"/>
       <c r="E805" s="34"/>
@@ -53700,8 +53815,8 @@
       </c>
     </row>
     <row r="806">
-      <c r="A806" s="76"/>
-      <c r="B806" s="77"/>
+      <c r="A806" s="83"/>
+      <c r="B806" s="84"/>
       <c r="C806" s="34"/>
       <c r="D806" s="34"/>
       <c r="E806" s="34"/>
@@ -53726,8 +53841,8 @@
       </c>
     </row>
     <row r="807">
-      <c r="A807" s="76"/>
-      <c r="B807" s="77"/>
+      <c r="A807" s="83"/>
+      <c r="B807" s="84"/>
       <c r="C807" s="34"/>
       <c r="D807" s="34"/>
       <c r="E807" s="34"/>
@@ -53752,8 +53867,8 @@
       </c>
     </row>
     <row r="808">
-      <c r="A808" s="76"/>
-      <c r="B808" s="77"/>
+      <c r="A808" s="83"/>
+      <c r="B808" s="84"/>
       <c r="C808" s="34"/>
       <c r="D808" s="34"/>
       <c r="E808" s="34"/>
@@ -53778,8 +53893,8 @@
       </c>
     </row>
     <row r="809">
-      <c r="A809" s="76"/>
-      <c r="B809" s="77"/>
+      <c r="A809" s="83"/>
+      <c r="B809" s="84"/>
       <c r="C809" s="34"/>
       <c r="D809" s="34"/>
       <c r="E809" s="34"/>
@@ -53804,8 +53919,8 @@
       </c>
     </row>
     <row r="810">
-      <c r="A810" s="76"/>
-      <c r="B810" s="77"/>
+      <c r="A810" s="83"/>
+      <c r="B810" s="84"/>
       <c r="C810" s="34"/>
       <c r="D810" s="34"/>
       <c r="E810" s="34"/>
@@ -53830,8 +53945,8 @@
       </c>
     </row>
     <row r="811">
-      <c r="A811" s="76"/>
-      <c r="B811" s="77"/>
+      <c r="A811" s="83"/>
+      <c r="B811" s="84"/>
       <c r="C811" s="34"/>
       <c r="D811" s="34"/>
       <c r="E811" s="34"/>
@@ -53856,8 +53971,8 @@
       </c>
     </row>
     <row r="812">
-      <c r="A812" s="76"/>
-      <c r="B812" s="77"/>
+      <c r="A812" s="83"/>
+      <c r="B812" s="84"/>
       <c r="C812" s="34"/>
       <c r="D812" s="34"/>
       <c r="E812" s="34"/>
@@ -53882,8 +53997,8 @@
       </c>
     </row>
     <row r="813">
-      <c r="A813" s="76"/>
-      <c r="B813" s="77"/>
+      <c r="A813" s="83"/>
+      <c r="B813" s="84"/>
       <c r="C813" s="34"/>
       <c r="D813" s="34"/>
       <c r="E813" s="34"/>
@@ -53908,8 +54023,8 @@
       </c>
     </row>
     <row r="814">
-      <c r="A814" s="76"/>
-      <c r="B814" s="77"/>
+      <c r="A814" s="83"/>
+      <c r="B814" s="84"/>
       <c r="C814" s="34"/>
       <c r="D814" s="34"/>
       <c r="E814" s="34"/>
@@ -53934,8 +54049,8 @@
       </c>
     </row>
     <row r="815">
-      <c r="A815" s="76"/>
-      <c r="B815" s="77"/>
+      <c r="A815" s="83"/>
+      <c r="B815" s="84"/>
       <c r="C815" s="34"/>
       <c r="D815" s="34"/>
       <c r="E815" s="34"/>
@@ -53960,8 +54075,8 @@
       </c>
     </row>
     <row r="816">
-      <c r="A816" s="76"/>
-      <c r="B816" s="77"/>
+      <c r="A816" s="83"/>
+      <c r="B816" s="84"/>
       <c r="C816" s="34"/>
       <c r="D816" s="34"/>
       <c r="E816" s="34"/>
@@ -53986,8 +54101,8 @@
       </c>
     </row>
     <row r="817">
-      <c r="A817" s="76"/>
-      <c r="B817" s="77"/>
+      <c r="A817" s="83"/>
+      <c r="B817" s="84"/>
       <c r="C817" s="34"/>
       <c r="D817" s="34"/>
       <c r="E817" s="34"/>
@@ -54012,8 +54127,8 @@
       </c>
     </row>
     <row r="818">
-      <c r="A818" s="76"/>
-      <c r="B818" s="77"/>
+      <c r="A818" s="83"/>
+      <c r="B818" s="84"/>
       <c r="C818" s="34"/>
       <c r="D818" s="34"/>
       <c r="E818" s="34"/>
@@ -54038,8 +54153,8 @@
       </c>
     </row>
     <row r="819">
-      <c r="A819" s="76"/>
-      <c r="B819" s="77"/>
+      <c r="A819" s="83"/>
+      <c r="B819" s="84"/>
       <c r="C819" s="34"/>
       <c r="D819" s="34"/>
       <c r="E819" s="34"/>
@@ -54064,8 +54179,8 @@
       </c>
     </row>
     <row r="820">
-      <c r="A820" s="76"/>
-      <c r="B820" s="77"/>
+      <c r="A820" s="83"/>
+      <c r="B820" s="84"/>
       <c r="C820" s="34"/>
       <c r="D820" s="34"/>
       <c r="E820" s="34"/>
@@ -54090,8 +54205,8 @@
       </c>
     </row>
     <row r="821">
-      <c r="A821" s="76"/>
-      <c r="B821" s="77"/>
+      <c r="A821" s="83"/>
+      <c r="B821" s="84"/>
       <c r="C821" s="34"/>
       <c r="D821" s="34"/>
       <c r="E821" s="34"/>
@@ -54116,8 +54231,8 @@
       </c>
     </row>
     <row r="822">
-      <c r="A822" s="76"/>
-      <c r="B822" s="77"/>
+      <c r="A822" s="83"/>
+      <c r="B822" s="84"/>
       <c r="C822" s="34"/>
       <c r="D822" s="34"/>
       <c r="E822" s="34"/>
@@ -54142,8 +54257,8 @@
       </c>
     </row>
     <row r="823">
-      <c r="A823" s="76"/>
-      <c r="B823" s="77"/>
+      <c r="A823" s="83"/>
+      <c r="B823" s="84"/>
       <c r="C823" s="34"/>
       <c r="D823" s="34"/>
       <c r="E823" s="34"/>
@@ -54168,8 +54283,8 @@
       </c>
     </row>
     <row r="824">
-      <c r="A824" s="76"/>
-      <c r="B824" s="77"/>
+      <c r="A824" s="83"/>
+      <c r="B824" s="84"/>
       <c r="C824" s="34"/>
       <c r="D824" s="34"/>
       <c r="E824" s="34"/>
@@ -54194,8 +54309,8 @@
       </c>
     </row>
     <row r="825">
-      <c r="A825" s="76"/>
-      <c r="B825" s="77"/>
+      <c r="A825" s="83"/>
+      <c r="B825" s="84"/>
       <c r="C825" s="34"/>
       <c r="D825" s="34"/>
       <c r="E825" s="34"/>
@@ -54220,8 +54335,8 @@
       </c>
     </row>
     <row r="826">
-      <c r="A826" s="76"/>
-      <c r="B826" s="77"/>
+      <c r="A826" s="83"/>
+      <c r="B826" s="84"/>
       <c r="C826" s="34"/>
       <c r="D826" s="34"/>
       <c r="E826" s="34"/>
@@ -54246,8 +54361,8 @@
       </c>
     </row>
     <row r="827">
-      <c r="A827" s="76"/>
-      <c r="B827" s="77"/>
+      <c r="A827" s="83"/>
+      <c r="B827" s="84"/>
       <c r="C827" s="34"/>
       <c r="D827" s="34"/>
       <c r="E827" s="34"/>
@@ -54272,8 +54387,8 @@
       </c>
     </row>
     <row r="828">
-      <c r="A828" s="76"/>
-      <c r="B828" s="77"/>
+      <c r="A828" s="83"/>
+      <c r="B828" s="84"/>
       <c r="C828" s="34"/>
       <c r="D828" s="34"/>
       <c r="E828" s="34"/>
@@ -54298,8 +54413,8 @@
       </c>
     </row>
     <row r="829">
-      <c r="A829" s="76"/>
-      <c r="B829" s="77"/>
+      <c r="A829" s="83"/>
+      <c r="B829" s="84"/>
       <c r="C829" s="34"/>
       <c r="D829" s="34"/>
       <c r="E829" s="34"/>
@@ -54324,8 +54439,8 @@
       </c>
     </row>
     <row r="830">
-      <c r="A830" s="76"/>
-      <c r="B830" s="77"/>
+      <c r="A830" s="83"/>
+      <c r="B830" s="84"/>
       <c r="C830" s="34"/>
       <c r="D830" s="34"/>
       <c r="E830" s="34"/>
@@ -54350,8 +54465,8 @@
       </c>
     </row>
     <row r="831">
-      <c r="A831" s="76"/>
-      <c r="B831" s="77"/>
+      <c r="A831" s="83"/>
+      <c r="B831" s="84"/>
       <c r="C831" s="34"/>
       <c r="D831" s="34"/>
       <c r="E831" s="34"/>
@@ -54376,8 +54491,8 @@
       </c>
     </row>
     <row r="832">
-      <c r="A832" s="76"/>
-      <c r="B832" s="77"/>
+      <c r="A832" s="83"/>
+      <c r="B832" s="84"/>
       <c r="C832" s="34"/>
       <c r="D832" s="34"/>
       <c r="E832" s="34"/>
@@ -54402,8 +54517,8 @@
       </c>
     </row>
     <row r="833">
-      <c r="A833" s="76"/>
-      <c r="B833" s="77"/>
+      <c r="A833" s="83"/>
+      <c r="B833" s="84"/>
       <c r="C833" s="34"/>
       <c r="D833" s="34"/>
       <c r="E833" s="34"/>
@@ -54428,8 +54543,8 @@
       </c>
     </row>
     <row r="834">
-      <c r="A834" s="76"/>
-      <c r="B834" s="77"/>
+      <c r="A834" s="83"/>
+      <c r="B834" s="84"/>
       <c r="C834" s="34"/>
       <c r="D834" s="34"/>
       <c r="E834" s="34"/>
@@ -54454,8 +54569,8 @@
       </c>
     </row>
     <row r="835">
-      <c r="A835" s="76"/>
-      <c r="B835" s="77"/>
+      <c r="A835" s="83"/>
+      <c r="B835" s="84"/>
       <c r="C835" s="34"/>
       <c r="D835" s="34"/>
       <c r="E835" s="34"/>
@@ -54480,8 +54595,8 @@
       </c>
     </row>
     <row r="836">
-      <c r="A836" s="76"/>
-      <c r="B836" s="77"/>
+      <c r="A836" s="83"/>
+      <c r="B836" s="84"/>
       <c r="C836" s="34"/>
       <c r="D836" s="34"/>
       <c r="E836" s="34"/>
@@ -54506,8 +54621,8 @@
       </c>
     </row>
     <row r="837">
-      <c r="A837" s="76"/>
-      <c r="B837" s="77"/>
+      <c r="A837" s="83"/>
+      <c r="B837" s="84"/>
       <c r="C837" s="34"/>
       <c r="D837" s="34"/>
       <c r="E837" s="34"/>
@@ -54532,8 +54647,8 @@
       </c>
     </row>
     <row r="838">
-      <c r="A838" s="76"/>
-      <c r="B838" s="77"/>
+      <c r="A838" s="83"/>
+      <c r="B838" s="84"/>
       <c r="C838" s="34"/>
       <c r="D838" s="34"/>
       <c r="E838" s="34"/>
@@ -54558,8 +54673,8 @@
       </c>
     </row>
     <row r="839">
-      <c r="A839" s="76"/>
-      <c r="B839" s="77"/>
+      <c r="A839" s="83"/>
+      <c r="B839" s="84"/>
       <c r="C839" s="34"/>
       <c r="D839" s="34"/>
       <c r="E839" s="34"/>
@@ -54584,8 +54699,8 @@
       </c>
     </row>
     <row r="840">
-      <c r="A840" s="76"/>
-      <c r="B840" s="77"/>
+      <c r="A840" s="83"/>
+      <c r="B840" s="84"/>
       <c r="C840" s="34"/>
       <c r="D840" s="34"/>
       <c r="E840" s="34"/>
@@ -54610,8 +54725,8 @@
       </c>
     </row>
     <row r="841">
-      <c r="A841" s="76"/>
-      <c r="B841" s="77"/>
+      <c r="A841" s="83"/>
+      <c r="B841" s="84"/>
       <c r="C841" s="34"/>
       <c r="D841" s="34"/>
       <c r="E841" s="34"/>
@@ -54636,8 +54751,8 @@
       </c>
     </row>
     <row r="842">
-      <c r="A842" s="76"/>
-      <c r="B842" s="77"/>
+      <c r="A842" s="83"/>
+      <c r="B842" s="84"/>
       <c r="C842" s="34"/>
       <c r="D842" s="34"/>
       <c r="E842" s="34"/>
@@ -54662,8 +54777,8 @@
       </c>
     </row>
     <row r="843">
-      <c r="A843" s="76"/>
-      <c r="B843" s="77"/>
+      <c r="A843" s="83"/>
+      <c r="B843" s="84"/>
       <c r="C843" s="34"/>
       <c r="D843" s="34"/>
       <c r="E843" s="34"/>
@@ -54688,8 +54803,8 @@
       </c>
     </row>
     <row r="844">
-      <c r="A844" s="76"/>
-      <c r="B844" s="77"/>
+      <c r="A844" s="83"/>
+      <c r="B844" s="84"/>
       <c r="C844" s="34"/>
       <c r="D844" s="34"/>
       <c r="E844" s="34"/>
@@ -54714,8 +54829,8 @@
       </c>
     </row>
     <row r="845">
-      <c r="A845" s="76"/>
-      <c r="B845" s="77"/>
+      <c r="A845" s="83"/>
+      <c r="B845" s="84"/>
       <c r="C845" s="34"/>
       <c r="D845" s="34"/>
       <c r="E845" s="34"/>
@@ -54740,8 +54855,8 @@
       </c>
     </row>
     <row r="846">
-      <c r="A846" s="76"/>
-      <c r="B846" s="77"/>
+      <c r="A846" s="83"/>
+      <c r="B846" s="84"/>
       <c r="C846" s="34"/>
       <c r="D846" s="34"/>
       <c r="E846" s="34"/>
@@ -54766,8 +54881,8 @@
       </c>
     </row>
     <row r="847">
-      <c r="A847" s="76"/>
-      <c r="B847" s="77"/>
+      <c r="A847" s="83"/>
+      <c r="B847" s="84"/>
       <c r="C847" s="34"/>
       <c r="D847" s="34"/>
       <c r="E847" s="34"/>
@@ -54792,8 +54907,8 @@
       </c>
     </row>
     <row r="848">
-      <c r="A848" s="76"/>
-      <c r="B848" s="77"/>
+      <c r="A848" s="83"/>
+      <c r="B848" s="84"/>
       <c r="C848" s="34"/>
       <c r="D848" s="34"/>
       <c r="E848" s="34"/>
@@ -54818,8 +54933,8 @@
       </c>
     </row>
     <row r="849">
-      <c r="A849" s="76"/>
-      <c r="B849" s="77"/>
+      <c r="A849" s="83"/>
+      <c r="B849" s="84"/>
       <c r="C849" s="34"/>
       <c r="D849" s="34"/>
       <c r="E849" s="34"/>
@@ -54844,8 +54959,8 @@
       </c>
     </row>
     <row r="850">
-      <c r="A850" s="76"/>
-      <c r="B850" s="77"/>
+      <c r="A850" s="83"/>
+      <c r="B850" s="84"/>
       <c r="C850" s="34"/>
       <c r="D850" s="34"/>
       <c r="E850" s="34"/>
@@ -54870,8 +54985,8 @@
       </c>
     </row>
     <row r="851">
-      <c r="A851" s="76"/>
-      <c r="B851" s="77"/>
+      <c r="A851" s="83"/>
+      <c r="B851" s="84"/>
       <c r="C851" s="34"/>
       <c r="D851" s="34"/>
       <c r="E851" s="34"/>
@@ -54896,8 +55011,8 @@
       </c>
     </row>
     <row r="852">
-      <c r="A852" s="76"/>
-      <c r="B852" s="77"/>
+      <c r="A852" s="83"/>
+      <c r="B852" s="84"/>
       <c r="C852" s="34"/>
       <c r="D852" s="34"/>
       <c r="E852" s="34"/>
@@ -54922,8 +55037,8 @@
       </c>
     </row>
     <row r="853">
-      <c r="A853" s="76"/>
-      <c r="B853" s="77"/>
+      <c r="A853" s="83"/>
+      <c r="B853" s="84"/>
       <c r="C853" s="34"/>
       <c r="D853" s="34"/>
       <c r="E853" s="34"/>
@@ -54948,8 +55063,8 @@
       </c>
     </row>
     <row r="854">
-      <c r="A854" s="76"/>
-      <c r="B854" s="77"/>
+      <c r="A854" s="83"/>
+      <c r="B854" s="84"/>
       <c r="C854" s="34"/>
       <c r="D854" s="34"/>
       <c r="E854" s="34"/>
@@ -54974,8 +55089,8 @@
       </c>
     </row>
     <row r="855">
-      <c r="A855" s="76"/>
-      <c r="B855" s="77"/>
+      <c r="A855" s="83"/>
+      <c r="B855" s="84"/>
       <c r="C855" s="34"/>
       <c r="D855" s="34"/>
       <c r="E855" s="34"/>
@@ -55000,8 +55115,8 @@
       </c>
     </row>
     <row r="856">
-      <c r="A856" s="76"/>
-      <c r="B856" s="77"/>
+      <c r="A856" s="83"/>
+      <c r="B856" s="84"/>
       <c r="C856" s="34"/>
       <c r="D856" s="34"/>
       <c r="E856" s="34"/>
@@ -55026,8 +55141,8 @@
       </c>
     </row>
     <row r="857">
-      <c r="A857" s="76"/>
-      <c r="B857" s="77"/>
+      <c r="A857" s="83"/>
+      <c r="B857" s="84"/>
       <c r="C857" s="34"/>
       <c r="D857" s="34"/>
       <c r="E857" s="34"/>
@@ -55052,8 +55167,8 @@
       </c>
     </row>
     <row r="858">
-      <c r="A858" s="76"/>
-      <c r="B858" s="77"/>
+      <c r="A858" s="83"/>
+      <c r="B858" s="84"/>
       <c r="C858" s="34"/>
       <c r="D858" s="34"/>
       <c r="E858" s="34"/>
@@ -55078,8 +55193,8 @@
       </c>
     </row>
     <row r="859">
-      <c r="A859" s="76"/>
-      <c r="B859" s="77"/>
+      <c r="A859" s="83"/>
+      <c r="B859" s="84"/>
       <c r="C859" s="34"/>
       <c r="D859" s="34"/>
       <c r="E859" s="34"/>
@@ -55104,8 +55219,8 @@
       </c>
     </row>
     <row r="860">
-      <c r="A860" s="76"/>
-      <c r="B860" s="77"/>
+      <c r="A860" s="83"/>
+      <c r="B860" s="84"/>
       <c r="C860" s="34"/>
       <c r="D860" s="34"/>
       <c r="E860" s="34"/>
@@ -55130,8 +55245,8 @@
       </c>
     </row>
     <row r="861">
-      <c r="A861" s="76"/>
-      <c r="B861" s="77"/>
+      <c r="A861" s="83"/>
+      <c r="B861" s="84"/>
       <c r="C861" s="34"/>
       <c r="D861" s="34"/>
       <c r="E861" s="34"/>
@@ -55156,8 +55271,8 @@
       </c>
     </row>
     <row r="862">
-      <c r="A862" s="76"/>
-      <c r="B862" s="77"/>
+      <c r="A862" s="83"/>
+      <c r="B862" s="84"/>
       <c r="C862" s="34"/>
       <c r="D862" s="34"/>
       <c r="E862" s="34"/>
@@ -55182,8 +55297,8 @@
       </c>
     </row>
     <row r="863">
-      <c r="A863" s="76"/>
-      <c r="B863" s="77"/>
+      <c r="A863" s="83"/>
+      <c r="B863" s="84"/>
       <c r="C863" s="34"/>
       <c r="D863" s="34"/>
       <c r="E863" s="34"/>
@@ -55208,8 +55323,8 @@
       </c>
     </row>
     <row r="864">
-      <c r="A864" s="76"/>
-      <c r="B864" s="77"/>
+      <c r="A864" s="83"/>
+      <c r="B864" s="84"/>
       <c r="C864" s="34"/>
       <c r="D864" s="34"/>
       <c r="E864" s="34"/>
@@ -55234,8 +55349,8 @@
       </c>
     </row>
     <row r="865">
-      <c r="A865" s="76"/>
-      <c r="B865" s="77"/>
+      <c r="A865" s="83"/>
+      <c r="B865" s="84"/>
       <c r="C865" s="34"/>
       <c r="D865" s="34"/>
       <c r="E865" s="34"/>
@@ -55260,8 +55375,8 @@
       </c>
     </row>
     <row r="866">
-      <c r="A866" s="76"/>
-      <c r="B866" s="77"/>
+      <c r="A866" s="83"/>
+      <c r="B866" s="84"/>
       <c r="C866" s="34"/>
       <c r="D866" s="34"/>
       <c r="E866" s="34"/>
@@ -55286,8 +55401,8 @@
       </c>
     </row>
     <row r="867">
-      <c r="A867" s="76"/>
-      <c r="B867" s="77"/>
+      <c r="A867" s="83"/>
+      <c r="B867" s="84"/>
       <c r="C867" s="34"/>
       <c r="D867" s="34"/>
       <c r="E867" s="34"/>
@@ -55312,8 +55427,8 @@
       </c>
     </row>
     <row r="868">
-      <c r="A868" s="76"/>
-      <c r="B868" s="77"/>
+      <c r="A868" s="83"/>
+      <c r="B868" s="84"/>
       <c r="C868" s="34"/>
       <c r="D868" s="34"/>
       <c r="E868" s="34"/>
@@ -55338,8 +55453,8 @@
       </c>
     </row>
     <row r="869">
-      <c r="A869" s="76"/>
-      <c r="B869" s="77"/>
+      <c r="A869" s="83"/>
+      <c r="B869" s="84"/>
       <c r="C869" s="34"/>
       <c r="D869" s="34"/>
       <c r="E869" s="34"/>
@@ -55364,8 +55479,8 @@
       </c>
     </row>
     <row r="870">
-      <c r="A870" s="76"/>
-      <c r="B870" s="77"/>
+      <c r="A870" s="83"/>
+      <c r="B870" s="84"/>
       <c r="C870" s="34"/>
       <c r="D870" s="34"/>
       <c r="E870" s="34"/>
@@ -55390,8 +55505,8 @@
       </c>
     </row>
     <row r="871">
-      <c r="A871" s="76"/>
-      <c r="B871" s="77"/>
+      <c r="A871" s="83"/>
+      <c r="B871" s="84"/>
       <c r="C871" s="34"/>
       <c r="D871" s="34"/>
       <c r="E871" s="34"/>
@@ -55416,8 +55531,8 @@
       </c>
     </row>
     <row r="872">
-      <c r="A872" s="76"/>
-      <c r="B872" s="77"/>
+      <c r="A872" s="83"/>
+      <c r="B872" s="84"/>
       <c r="C872" s="34"/>
       <c r="D872" s="34"/>
       <c r="E872" s="34"/>
@@ -55442,8 +55557,8 @@
       </c>
     </row>
     <row r="873">
-      <c r="A873" s="76"/>
-      <c r="B873" s="77"/>
+      <c r="A873" s="83"/>
+      <c r="B873" s="84"/>
       <c r="C873" s="34"/>
       <c r="D873" s="34"/>
       <c r="E873" s="34"/>
@@ -55468,8 +55583,8 @@
       </c>
     </row>
     <row r="874">
-      <c r="A874" s="76"/>
-      <c r="B874" s="77"/>
+      <c r="A874" s="83"/>
+      <c r="B874" s="84"/>
       <c r="C874" s="34"/>
       <c r="D874" s="34"/>
       <c r="E874" s="34"/>
@@ -55494,8 +55609,8 @@
       </c>
     </row>
     <row r="875">
-      <c r="A875" s="76"/>
-      <c r="B875" s="77"/>
+      <c r="A875" s="83"/>
+      <c r="B875" s="84"/>
       <c r="C875" s="34"/>
       <c r="D875" s="34"/>
       <c r="E875" s="34"/>
@@ -55520,8 +55635,8 @@
       </c>
     </row>
     <row r="876">
-      <c r="A876" s="76"/>
-      <c r="B876" s="77"/>
+      <c r="A876" s="83"/>
+      <c r="B876" s="84"/>
       <c r="C876" s="34"/>
       <c r="D876" s="34"/>
       <c r="E876" s="34"/>
@@ -55546,8 +55661,8 @@
       </c>
     </row>
     <row r="877">
-      <c r="A877" s="76"/>
-      <c r="B877" s="77"/>
+      <c r="A877" s="83"/>
+      <c r="B877" s="84"/>
       <c r="C877" s="34"/>
       <c r="D877" s="34"/>
       <c r="E877" s="34"/>
@@ -55572,8 +55687,8 @@
       </c>
     </row>
     <row r="878">
-      <c r="A878" s="76"/>
-      <c r="B878" s="77"/>
+      <c r="A878" s="83"/>
+      <c r="B878" s="84"/>
       <c r="C878" s="34"/>
       <c r="D878" s="34"/>
       <c r="E878" s="34"/>
@@ -55598,8 +55713,8 @@
       </c>
     </row>
     <row r="879">
-      <c r="A879" s="76"/>
-      <c r="B879" s="77"/>
+      <c r="A879" s="83"/>
+      <c r="B879" s="84"/>
       <c r="C879" s="34"/>
       <c r="D879" s="34"/>
       <c r="E879" s="34"/>
@@ -55624,8 +55739,8 @@
       </c>
     </row>
     <row r="880">
-      <c r="A880" s="76"/>
-      <c r="B880" s="77"/>
+      <c r="A880" s="83"/>
+      <c r="B880" s="84"/>
       <c r="C880" s="34"/>
       <c r="D880" s="34"/>
       <c r="E880" s="34"/>
@@ -55650,8 +55765,8 @@
       </c>
     </row>
     <row r="881">
-      <c r="A881" s="76"/>
-      <c r="B881" s="77"/>
+      <c r="A881" s="83"/>
+      <c r="B881" s="84"/>
       <c r="C881" s="34"/>
       <c r="D881" s="34"/>
       <c r="E881" s="34"/>
@@ -55676,8 +55791,8 @@
       </c>
     </row>
     <row r="882">
-      <c r="A882" s="76"/>
-      <c r="B882" s="77"/>
+      <c r="A882" s="83"/>
+      <c r="B882" s="84"/>
       <c r="C882" s="34"/>
       <c r="D882" s="34"/>
       <c r="E882" s="34"/>
@@ -55702,8 +55817,8 @@
       </c>
     </row>
     <row r="883">
-      <c r="A883" s="76"/>
-      <c r="B883" s="77"/>
+      <c r="A883" s="83"/>
+      <c r="B883" s="84"/>
       <c r="C883" s="34"/>
       <c r="D883" s="34"/>
       <c r="E883" s="34"/>
@@ -55728,8 +55843,8 @@
       </c>
     </row>
     <row r="884">
-      <c r="A884" s="76"/>
-      <c r="B884" s="77"/>
+      <c r="A884" s="83"/>
+      <c r="B884" s="84"/>
       <c r="C884" s="34"/>
       <c r="D884" s="34"/>
       <c r="E884" s="34"/>
@@ -55754,8 +55869,8 @@
       </c>
     </row>
     <row r="885">
-      <c r="A885" s="76"/>
-      <c r="B885" s="77"/>
+      <c r="A885" s="83"/>
+      <c r="B885" s="84"/>
       <c r="C885" s="34"/>
       <c r="D885" s="34"/>
       <c r="E885" s="34"/>
@@ -55780,8 +55895,8 @@
       </c>
     </row>
     <row r="886">
-      <c r="A886" s="76"/>
-      <c r="B886" s="77"/>
+      <c r="A886" s="83"/>
+      <c r="B886" s="84"/>
       <c r="C886" s="34"/>
       <c r="D886" s="34"/>
       <c r="E886" s="34"/>
@@ -55806,8 +55921,8 @@
       </c>
     </row>
     <row r="887">
-      <c r="A887" s="76"/>
-      <c r="B887" s="77"/>
+      <c r="A887" s="83"/>
+      <c r="B887" s="84"/>
       <c r="C887" s="34"/>
       <c r="D887" s="34"/>
       <c r="E887" s="34"/>
@@ -55832,8 +55947,8 @@
       </c>
     </row>
     <row r="888">
-      <c r="A888" s="76"/>
-      <c r="B888" s="77"/>
+      <c r="A888" s="83"/>
+      <c r="B888" s="84"/>
       <c r="C888" s="34"/>
       <c r="D888" s="34"/>
       <c r="E888" s="34"/>
@@ -55858,8 +55973,8 @@
       </c>
     </row>
     <row r="889">
-      <c r="A889" s="76"/>
-      <c r="B889" s="77"/>
+      <c r="A889" s="83"/>
+      <c r="B889" s="84"/>
       <c r="C889" s="34"/>
       <c r="D889" s="34"/>
       <c r="E889" s="34"/>
@@ -55884,8 +55999,8 @@
       </c>
     </row>
     <row r="890">
-      <c r="A890" s="76"/>
-      <c r="B890" s="77"/>
+      <c r="A890" s="83"/>
+      <c r="B890" s="84"/>
       <c r="C890" s="34"/>
       <c r="D890" s="34"/>
       <c r="E890" s="34"/>
@@ -55910,8 +56025,8 @@
       </c>
     </row>
     <row r="891">
-      <c r="A891" s="76"/>
-      <c r="B891" s="77"/>
+      <c r="A891" s="83"/>
+      <c r="B891" s="84"/>
       <c r="C891" s="34"/>
       <c r="D891" s="34"/>
       <c r="E891" s="34"/>
@@ -55936,8 +56051,8 @@
       </c>
     </row>
     <row r="892">
-      <c r="A892" s="76"/>
-      <c r="B892" s="77"/>
+      <c r="A892" s="83"/>
+      <c r="B892" s="84"/>
       <c r="C892" s="34"/>
       <c r="D892" s="34"/>
       <c r="E892" s="34"/>
@@ -55962,8 +56077,8 @@
       </c>
     </row>
     <row r="893">
-      <c r="A893" s="76"/>
-      <c r="B893" s="77"/>
+      <c r="A893" s="83"/>
+      <c r="B893" s="84"/>
       <c r="C893" s="34"/>
       <c r="D893" s="34"/>
       <c r="E893" s="34"/>
@@ -55988,8 +56103,8 @@
       </c>
     </row>
     <row r="894">
-      <c r="A894" s="76"/>
-      <c r="B894" s="77"/>
+      <c r="A894" s="83"/>
+      <c r="B894" s="84"/>
       <c r="C894" s="34"/>
       <c r="D894" s="34"/>
       <c r="E894" s="34"/>
@@ -56014,8 +56129,8 @@
       </c>
     </row>
     <row r="895">
-      <c r="A895" s="76"/>
-      <c r="B895" s="77"/>
+      <c r="A895" s="83"/>
+      <c r="B895" s="84"/>
       <c r="C895" s="34"/>
       <c r="D895" s="34"/>
       <c r="E895" s="34"/>
@@ -56040,8 +56155,8 @@
       </c>
     </row>
     <row r="896">
-      <c r="A896" s="76"/>
-      <c r="B896" s="77"/>
+      <c r="A896" s="83"/>
+      <c r="B896" s="84"/>
       <c r="C896" s="34"/>
       <c r="D896" s="34"/>
       <c r="E896" s="34"/>
@@ -56066,8 +56181,8 @@
       </c>
     </row>
     <row r="897">
-      <c r="A897" s="76"/>
-      <c r="B897" s="77"/>
+      <c r="A897" s="83"/>
+      <c r="B897" s="84"/>
       <c r="C897" s="34"/>
       <c r="D897" s="34"/>
       <c r="E897" s="34"/>
@@ -56092,8 +56207,8 @@
       </c>
     </row>
     <row r="898">
-      <c r="A898" s="76"/>
-      <c r="B898" s="77"/>
+      <c r="A898" s="83"/>
+      <c r="B898" s="84"/>
       <c r="C898" s="34"/>
       <c r="D898" s="34"/>
       <c r="E898" s="34"/>
@@ -56118,8 +56233,8 @@
       </c>
     </row>
     <row r="899">
-      <c r="A899" s="76"/>
-      <c r="B899" s="77"/>
+      <c r="A899" s="83"/>
+      <c r="B899" s="84"/>
       <c r="C899" s="34"/>
       <c r="D899" s="34"/>
       <c r="E899" s="34"/>
@@ -56144,8 +56259,8 @@
       </c>
     </row>
     <row r="900">
-      <c r="A900" s="76"/>
-      <c r="B900" s="77"/>
+      <c r="A900" s="83"/>
+      <c r="B900" s="84"/>
       <c r="C900" s="34"/>
       <c r="D900" s="34"/>
       <c r="E900" s="34"/>
@@ -56170,8 +56285,8 @@
       </c>
     </row>
     <row r="901">
-      <c r="A901" s="76"/>
-      <c r="B901" s="77"/>
+      <c r="A901" s="83"/>
+      <c r="B901" s="84"/>
       <c r="C901" s="34"/>
       <c r="D901" s="34"/>
       <c r="E901" s="34"/>
@@ -56196,8 +56311,8 @@
       </c>
     </row>
     <row r="902">
-      <c r="A902" s="76"/>
-      <c r="B902" s="77"/>
+      <c r="A902" s="83"/>
+      <c r="B902" s="84"/>
       <c r="C902" s="34"/>
       <c r="D902" s="34"/>
       <c r="E902" s="34"/>
@@ -56222,8 +56337,8 @@
       </c>
     </row>
     <row r="903">
-      <c r="A903" s="76"/>
-      <c r="B903" s="77"/>
+      <c r="A903" s="83"/>
+      <c r="B903" s="84"/>
       <c r="C903" s="34"/>
       <c r="D903" s="34"/>
       <c r="E903" s="34"/>
@@ -56248,8 +56363,8 @@
       </c>
     </row>
     <row r="904">
-      <c r="A904" s="76"/>
-      <c r="B904" s="77"/>
+      <c r="A904" s="83"/>
+      <c r="B904" s="84"/>
       <c r="C904" s="34"/>
       <c r="D904" s="34"/>
       <c r="E904" s="34"/>
@@ -56274,8 +56389,8 @@
       </c>
     </row>
     <row r="905">
-      <c r="A905" s="76"/>
-      <c r="B905" s="77"/>
+      <c r="A905" s="83"/>
+      <c r="B905" s="84"/>
       <c r="C905" s="34"/>
       <c r="D905" s="34"/>
       <c r="E905" s="34"/>
@@ -56300,8 +56415,8 @@
       </c>
     </row>
     <row r="906">
-      <c r="A906" s="76"/>
-      <c r="B906" s="77"/>
+      <c r="A906" s="83"/>
+      <c r="B906" s="84"/>
       <c r="C906" s="34"/>
       <c r="D906" s="34"/>
       <c r="E906" s="34"/>
@@ -56326,8 +56441,8 @@
       </c>
     </row>
     <row r="907">
-      <c r="A907" s="76"/>
-      <c r="B907" s="77"/>
+      <c r="A907" s="83"/>
+      <c r="B907" s="84"/>
       <c r="C907" s="34"/>
       <c r="D907" s="34"/>
       <c r="E907" s="34"/>
@@ -56352,8 +56467,8 @@
       </c>
     </row>
     <row r="908">
-      <c r="A908" s="76"/>
-      <c r="B908" s="77"/>
+      <c r="A908" s="83"/>
+      <c r="B908" s="84"/>
       <c r="C908" s="34"/>
       <c r="D908" s="34"/>
       <c r="E908" s="34"/>
@@ -56378,8 +56493,8 @@
       </c>
     </row>
     <row r="909">
-      <c r="A909" s="76"/>
-      <c r="B909" s="77"/>
+      <c r="A909" s="83"/>
+      <c r="B909" s="84"/>
       <c r="C909" s="34"/>
       <c r="D909" s="34"/>
       <c r="E909" s="34"/>
@@ -56404,8 +56519,8 @@
       </c>
     </row>
     <row r="910">
-      <c r="A910" s="76"/>
-      <c r="B910" s="77"/>
+      <c r="A910" s="83"/>
+      <c r="B910" s="84"/>
       <c r="C910" s="34"/>
       <c r="D910" s="34"/>
       <c r="E910" s="34"/>
@@ -56430,8 +56545,8 @@
       </c>
     </row>
     <row r="911">
-      <c r="A911" s="76"/>
-      <c r="B911" s="77"/>
+      <c r="A911" s="83"/>
+      <c r="B911" s="84"/>
       <c r="C911" s="34"/>
       <c r="D911" s="34"/>
       <c r="E911" s="34"/>
@@ -56456,8 +56571,8 @@
       </c>
     </row>
     <row r="912">
-      <c r="A912" s="76"/>
-      <c r="B912" s="77"/>
+      <c r="A912" s="83"/>
+      <c r="B912" s="84"/>
       <c r="C912" s="34"/>
       <c r="D912" s="34"/>
       <c r="E912" s="34"/>
@@ -56482,8 +56597,8 @@
       </c>
     </row>
     <row r="913">
-      <c r="A913" s="76"/>
-      <c r="B913" s="77"/>
+      <c r="A913" s="83"/>
+      <c r="B913" s="84"/>
       <c r="C913" s="34"/>
       <c r="D913" s="34"/>
       <c r="E913" s="34"/>
@@ -56508,8 +56623,8 @@
       </c>
     </row>
     <row r="914">
-      <c r="A914" s="76"/>
-      <c r="B914" s="77"/>
+      <c r="A914" s="83"/>
+      <c r="B914" s="84"/>
       <c r="C914" s="34"/>
       <c r="D914" s="34"/>
       <c r="E914" s="34"/>
@@ -56534,8 +56649,8 @@
       </c>
     </row>
     <row r="915">
-      <c r="A915" s="76"/>
-      <c r="B915" s="77"/>
+      <c r="A915" s="83"/>
+      <c r="B915" s="84"/>
       <c r="C915" s="34"/>
       <c r="D915" s="34"/>
       <c r="E915" s="34"/>
@@ -56560,8 +56675,8 @@
       </c>
     </row>
     <row r="916">
-      <c r="A916" s="76"/>
-      <c r="B916" s="77"/>
+      <c r="A916" s="83"/>
+      <c r="B916" s="84"/>
       <c r="C916" s="34"/>
       <c r="D916" s="34"/>
       <c r="E916" s="34"/>
@@ -56586,8 +56701,8 @@
       </c>
     </row>
     <row r="917">
-      <c r="A917" s="76"/>
-      <c r="B917" s="77"/>
+      <c r="A917" s="83"/>
+      <c r="B917" s="84"/>
       <c r="C917" s="34"/>
       <c r="D917" s="34"/>
       <c r="E917" s="34"/>
@@ -56612,8 +56727,8 @@
       </c>
     </row>
     <row r="918">
-      <c r="A918" s="76"/>
-      <c r="B918" s="77"/>
+      <c r="A918" s="83"/>
+      <c r="B918" s="84"/>
       <c r="C918" s="34"/>
       <c r="D918" s="34"/>
       <c r="E918" s="34"/>
@@ -56638,8 +56753,8 @@
       </c>
     </row>
     <row r="919">
-      <c r="A919" s="76"/>
-      <c r="B919" s="77"/>
+      <c r="A919" s="83"/>
+      <c r="B919" s="84"/>
       <c r="C919" s="34"/>
       <c r="D919" s="34"/>
       <c r="E919" s="34"/>
@@ -56664,8 +56779,8 @@
       </c>
     </row>
     <row r="920">
-      <c r="A920" s="76"/>
-      <c r="B920" s="77"/>
+      <c r="A920" s="83"/>
+      <c r="B920" s="84"/>
       <c r="C920" s="34"/>
       <c r="D920" s="34"/>
       <c r="E920" s="34"/>
@@ -56690,8 +56805,8 @@
       </c>
     </row>
     <row r="921">
-      <c r="A921" s="76"/>
-      <c r="B921" s="77"/>
+      <c r="A921" s="83"/>
+      <c r="B921" s="84"/>
       <c r="C921" s="34"/>
       <c r="D921" s="34"/>
       <c r="E921" s="34"/>
@@ -56716,8 +56831,8 @@
       </c>
     </row>
     <row r="922">
-      <c r="A922" s="76"/>
-      <c r="B922" s="77"/>
+      <c r="A922" s="83"/>
+      <c r="B922" s="84"/>
       <c r="C922" s="34"/>
       <c r="D922" s="34"/>
       <c r="E922" s="34"/>
@@ -56742,8 +56857,8 @@
       </c>
     </row>
     <row r="923">
-      <c r="A923" s="76"/>
-      <c r="B923" s="77"/>
+      <c r="A923" s="83"/>
+      <c r="B923" s="84"/>
       <c r="C923" s="34"/>
       <c r="D923" s="34"/>
       <c r="E923" s="34"/>
@@ -56768,8 +56883,8 @@
       </c>
     </row>
     <row r="924">
-      <c r="A924" s="76"/>
-      <c r="B924" s="77"/>
+      <c r="A924" s="83"/>
+      <c r="B924" s="84"/>
       <c r="C924" s="34"/>
       <c r="D924" s="34"/>
       <c r="E924" s="34"/>
@@ -56794,8 +56909,8 @@
       </c>
     </row>
     <row r="925">
-      <c r="A925" s="76"/>
-      <c r="B925" s="77"/>
+      <c r="A925" s="83"/>
+      <c r="B925" s="84"/>
       <c r="C925" s="34"/>
       <c r="D925" s="34"/>
       <c r="E925" s="34"/>
@@ -56820,8 +56935,8 @@
       </c>
     </row>
     <row r="926">
-      <c r="A926" s="76"/>
-      <c r="B926" s="77"/>
+      <c r="A926" s="83"/>
+      <c r="B926" s="84"/>
       <c r="C926" s="34"/>
       <c r="D926" s="34"/>
       <c r="E926" s="34"/>
@@ -56846,8 +56961,8 @@
       </c>
     </row>
     <row r="927">
-      <c r="A927" s="76"/>
-      <c r="B927" s="77"/>
+      <c r="A927" s="83"/>
+      <c r="B927" s="84"/>
       <c r="C927" s="34"/>
       <c r="D927" s="34"/>
       <c r="E927" s="34"/>
@@ -56872,8 +56987,8 @@
       </c>
     </row>
     <row r="928">
-      <c r="A928" s="76"/>
-      <c r="B928" s="77"/>
+      <c r="A928" s="83"/>
+      <c r="B928" s="84"/>
       <c r="C928" s="34"/>
       <c r="D928" s="34"/>
       <c r="E928" s="34"/>
@@ -56898,8 +57013,8 @@
       </c>
     </row>
     <row r="929">
-      <c r="A929" s="76"/>
-      <c r="B929" s="77"/>
+      <c r="A929" s="83"/>
+      <c r="B929" s="84"/>
       <c r="C929" s="34"/>
       <c r="D929" s="34"/>
       <c r="E929" s="34"/>
@@ -56924,8 +57039,8 @@
       </c>
     </row>
     <row r="930">
-      <c r="A930" s="76"/>
-      <c r="B930" s="77"/>
+      <c r="A930" s="83"/>
+      <c r="B930" s="84"/>
       <c r="C930" s="34"/>
       <c r="D930" s="34"/>
       <c r="E930" s="34"/>
@@ -56950,8 +57065,8 @@
       </c>
     </row>
     <row r="931">
-      <c r="A931" s="76"/>
-      <c r="B931" s="77"/>
+      <c r="A931" s="83"/>
+      <c r="B931" s="84"/>
       <c r="C931" s="34"/>
       <c r="D931" s="34"/>
       <c r="E931" s="34"/>
@@ -56976,8 +57091,8 @@
       </c>
     </row>
     <row r="932">
-      <c r="A932" s="76"/>
-      <c r="B932" s="77"/>
+      <c r="A932" s="83"/>
+      <c r="B932" s="84"/>
       <c r="C932" s="34"/>
       <c r="D932" s="34"/>
       <c r="E932" s="34"/>
@@ -57002,8 +57117,8 @@
       </c>
     </row>
     <row r="933">
-      <c r="A933" s="76"/>
-      <c r="B933" s="77"/>
+      <c r="A933" s="83"/>
+      <c r="B933" s="84"/>
       <c r="C933" s="34"/>
       <c r="D933" s="34"/>
       <c r="E933" s="34"/>
@@ -57028,8 +57143,8 @@
       </c>
     </row>
     <row r="934">
-      <c r="A934" s="76"/>
-      <c r="B934" s="77"/>
+      <c r="A934" s="83"/>
+      <c r="B934" s="84"/>
       <c r="C934" s="34"/>
       <c r="D934" s="34"/>
       <c r="E934" s="34"/>
@@ -57054,8 +57169,8 @@
       </c>
     </row>
     <row r="935">
-      <c r="A935" s="76"/>
-      <c r="B935" s="77"/>
+      <c r="A935" s="83"/>
+      <c r="B935" s="84"/>
       <c r="C935" s="34"/>
       <c r="D935" s="34"/>
       <c r="E935" s="34"/>
@@ -57080,8 +57195,8 @@
       </c>
     </row>
     <row r="936">
-      <c r="A936" s="76"/>
-      <c r="B936" s="77"/>
+      <c r="A936" s="83"/>
+      <c r="B936" s="84"/>
       <c r="C936" s="34"/>
       <c r="D936" s="34"/>
       <c r="E936" s="34"/>
@@ -57106,8 +57221,8 @@
       </c>
     </row>
     <row r="937">
-      <c r="A937" s="76"/>
-      <c r="B937" s="77"/>
+      <c r="A937" s="83"/>
+      <c r="B937" s="84"/>
       <c r="C937" s="34"/>
       <c r="D937" s="34"/>
       <c r="E937" s="34"/>
@@ -57132,8 +57247,8 @@
       </c>
     </row>
     <row r="938">
-      <c r="A938" s="76"/>
-      <c r="B938" s="77"/>
+      <c r="A938" s="83"/>
+      <c r="B938" s="84"/>
       <c r="C938" s="34"/>
       <c r="D938" s="34"/>
       <c r="E938" s="34"/>
@@ -57158,8 +57273,8 @@
       </c>
     </row>
     <row r="939">
-      <c r="A939" s="76"/>
-      <c r="B939" s="77"/>
+      <c r="A939" s="83"/>
+      <c r="B939" s="84"/>
       <c r="C939" s="34"/>
       <c r="D939" s="34"/>
       <c r="E939" s="34"/>
@@ -57184,8 +57299,8 @@
       </c>
     </row>
     <row r="940">
-      <c r="A940" s="76"/>
-      <c r="B940" s="77"/>
+      <c r="A940" s="83"/>
+      <c r="B940" s="84"/>
       <c r="C940" s="34"/>
       <c r="D940" s="34"/>
       <c r="E940" s="34"/>
@@ -57210,8 +57325,8 @@
       </c>
     </row>
     <row r="941">
-      <c r="A941" s="76"/>
-      <c r="B941" s="77"/>
+      <c r="A941" s="83"/>
+      <c r="B941" s="84"/>
       <c r="C941" s="34"/>
       <c r="D941" s="34"/>
       <c r="E941" s="34"/>
@@ -57236,8 +57351,8 @@
       </c>
     </row>
     <row r="942">
-      <c r="A942" s="76"/>
-      <c r="B942" s="77"/>
+      <c r="A942" s="83"/>
+      <c r="B942" s="84"/>
       <c r="C942" s="34"/>
       <c r="D942" s="34"/>
       <c r="E942" s="34"/>
@@ -57262,8 +57377,8 @@
       </c>
     </row>
     <row r="943">
-      <c r="A943" s="76"/>
-      <c r="B943" s="77"/>
+      <c r="A943" s="83"/>
+      <c r="B943" s="84"/>
       <c r="C943" s="34"/>
       <c r="D943" s="34"/>
       <c r="E943" s="34"/>
@@ -57288,8 +57403,8 @@
       </c>
     </row>
     <row r="944">
-      <c r="A944" s="76"/>
-      <c r="B944" s="77"/>
+      <c r="A944" s="83"/>
+      <c r="B944" s="84"/>
       <c r="C944" s="34"/>
       <c r="D944" s="34"/>
       <c r="E944" s="34"/>
@@ -57314,8 +57429,8 @@
       </c>
     </row>
     <row r="945">
-      <c r="A945" s="76"/>
-      <c r="B945" s="77"/>
+      <c r="A945" s="83"/>
+      <c r="B945" s="84"/>
       <c r="C945" s="34"/>
       <c r="D945" s="34"/>
       <c r="E945" s="34"/>
@@ -57340,8 +57455,8 @@
       </c>
     </row>
     <row r="946">
-      <c r="A946" s="76"/>
-      <c r="B946" s="77"/>
+      <c r="A946" s="83"/>
+      <c r="B946" s="84"/>
       <c r="C946" s="34"/>
       <c r="D946" s="34"/>
       <c r="E946" s="34"/>
@@ -57366,8 +57481,8 @@
       </c>
     </row>
     <row r="947">
-      <c r="A947" s="76"/>
-      <c r="B947" s="77"/>
+      <c r="A947" s="83"/>
+      <c r="B947" s="84"/>
       <c r="C947" s="34"/>
       <c r="D947" s="34"/>
       <c r="E947" s="34"/>
@@ -57392,8 +57507,8 @@
       </c>
     </row>
     <row r="948">
-      <c r="A948" s="76"/>
-      <c r="B948" s="77"/>
+      <c r="A948" s="83"/>
+      <c r="B948" s="84"/>
       <c r="C948" s="34"/>
       <c r="D948" s="34"/>
       <c r="E948" s="34"/>
@@ -57418,8 +57533,8 @@
       </c>
     </row>
     <row r="949">
-      <c r="A949" s="76"/>
-      <c r="B949" s="77"/>
+      <c r="A949" s="83"/>
+      <c r="B949" s="84"/>
       <c r="C949" s="34"/>
       <c r="D949" s="34"/>
       <c r="E949" s="34"/>
@@ -57444,8 +57559,8 @@
       </c>
     </row>
     <row r="950">
-      <c r="A950" s="76"/>
-      <c r="B950" s="77"/>
+      <c r="A950" s="83"/>
+      <c r="B950" s="84"/>
       <c r="C950" s="34"/>
       <c r="D950" s="34"/>
       <c r="E950" s="34"/>
@@ -57470,8 +57585,8 @@
       </c>
     </row>
     <row r="951">
-      <c r="A951" s="76"/>
-      <c r="B951" s="77"/>
+      <c r="A951" s="83"/>
+      <c r="B951" s="84"/>
       <c r="C951" s="34"/>
       <c r="D951" s="34"/>
       <c r="E951" s="34"/>
@@ -57496,8 +57611,8 @@
       </c>
     </row>
     <row r="952">
-      <c r="A952" s="76"/>
-      <c r="B952" s="77"/>
+      <c r="A952" s="83"/>
+      <c r="B952" s="84"/>
       <c r="C952" s="34"/>
       <c r="D952" s="34"/>
       <c r="E952" s="34"/>
@@ -57522,8 +57637,8 @@
       </c>
     </row>
     <row r="953">
-      <c r="A953" s="76"/>
-      <c r="B953" s="77"/>
+      <c r="A953" s="83"/>
+      <c r="B953" s="84"/>
       <c r="C953" s="34"/>
       <c r="D953" s="34"/>
       <c r="E953" s="34"/>
@@ -57548,8 +57663,8 @@
       </c>
     </row>
     <row r="954">
-      <c r="A954" s="76"/>
-      <c r="B954" s="77"/>
+      <c r="A954" s="83"/>
+      <c r="B954" s="84"/>
       <c r="C954" s="34"/>
       <c r="D954" s="34"/>
       <c r="E954" s="34"/>
@@ -57574,8 +57689,8 @@
       </c>
     </row>
     <row r="955">
-      <c r="A955" s="76"/>
-      <c r="B955" s="77"/>
+      <c r="A955" s="83"/>
+      <c r="B955" s="84"/>
       <c r="C955" s="34"/>
       <c r="D955" s="34"/>
       <c r="E955" s="34"/>
@@ -57600,8 +57715,8 @@
       </c>
     </row>
     <row r="956">
-      <c r="A956" s="76"/>
-      <c r="B956" s="77"/>
+      <c r="A956" s="83"/>
+      <c r="B956" s="84"/>
       <c r="C956" s="34"/>
       <c r="D956" s="34"/>
       <c r="E956" s="34"/>
@@ -57626,8 +57741,8 @@
       </c>
     </row>
     <row r="957">
-      <c r="A957" s="76"/>
-      <c r="B957" s="77"/>
+      <c r="A957" s="83"/>
+      <c r="B957" s="84"/>
       <c r="C957" s="34"/>
       <c r="D957" s="34"/>
       <c r="E957" s="34"/>
@@ -57652,8 +57767,8 @@
       </c>
     </row>
     <row r="958">
-      <c r="A958" s="76"/>
-      <c r="B958" s="77"/>
+      <c r="A958" s="83"/>
+      <c r="B958" s="84"/>
       <c r="C958" s="34"/>
       <c r="D958" s="34"/>
       <c r="E958" s="34"/>
@@ -57678,8 +57793,8 @@
       </c>
     </row>
     <row r="959">
-      <c r="A959" s="76"/>
-      <c r="B959" s="77"/>
+      <c r="A959" s="83"/>
+      <c r="B959" s="84"/>
       <c r="C959" s="34"/>
       <c r="D959" s="34"/>
       <c r="E959" s="34"/>
@@ -57704,8 +57819,8 @@
       </c>
     </row>
     <row r="960">
-      <c r="A960" s="76"/>
-      <c r="B960" s="77"/>
+      <c r="A960" s="83"/>
+      <c r="B960" s="84"/>
       <c r="C960" s="34"/>
       <c r="D960" s="34"/>
       <c r="E960" s="34"/>
@@ -57730,8 +57845,8 @@
       </c>
     </row>
     <row r="961">
-      <c r="A961" s="76"/>
-      <c r="B961" s="77"/>
+      <c r="A961" s="83"/>
+      <c r="B961" s="84"/>
       <c r="C961" s="34"/>
       <c r="D961" s="34"/>
       <c r="E961" s="34"/>
@@ -57756,8 +57871,8 @@
       </c>
     </row>
     <row r="962">
-      <c r="A962" s="76"/>
-      <c r="B962" s="77"/>
+      <c r="A962" s="83"/>
+      <c r="B962" s="84"/>
       <c r="C962" s="34"/>
       <c r="D962" s="34"/>
       <c r="E962" s="34"/>
@@ -57782,8 +57897,8 @@
       </c>
     </row>
     <row r="963">
-      <c r="A963" s="76"/>
-      <c r="B963" s="77"/>
+      <c r="A963" s="83"/>
+      <c r="B963" s="84"/>
       <c r="C963" s="34"/>
       <c r="D963" s="34"/>
       <c r="E963" s="34"/>
@@ -57808,8 +57923,8 @@
       </c>
     </row>
     <row r="964">
-      <c r="A964" s="76"/>
-      <c r="B964" s="77"/>
+      <c r="A964" s="83"/>
+      <c r="B964" s="84"/>
       <c r="C964" s="34"/>
       <c r="D964" s="34"/>
       <c r="E964" s="34"/>
@@ -57834,8 +57949,8 @@
       </c>
     </row>
     <row r="965">
-      <c r="A965" s="76"/>
-      <c r="B965" s="77"/>
+      <c r="A965" s="83"/>
+      <c r="B965" s="84"/>
       <c r="C965" s="34"/>
       <c r="D965" s="34"/>
       <c r="E965" s="34"/>
@@ -57860,8 +57975,8 @@
       </c>
     </row>
     <row r="966">
-      <c r="A966" s="76"/>
-      <c r="B966" s="77"/>
+      <c r="A966" s="83"/>
+      <c r="B966" s="84"/>
       <c r="C966" s="34"/>
       <c r="D966" s="34"/>
       <c r="E966" s="34"/>
@@ -57886,8 +58001,8 @@
       </c>
     </row>
     <row r="967">
-      <c r="A967" s="76"/>
-      <c r="B967" s="77"/>
+      <c r="A967" s="83"/>
+      <c r="B967" s="84"/>
       <c r="C967" s="34"/>
       <c r="D967" s="34"/>
       <c r="E967" s="34"/>
@@ -57912,8 +58027,8 @@
       </c>
     </row>
     <row r="968">
-      <c r="A968" s="76"/>
-      <c r="B968" s="77"/>
+      <c r="A968" s="83"/>
+      <c r="B968" s="84"/>
       <c r="C968" s="34"/>
       <c r="D968" s="34"/>
       <c r="E968" s="34"/>
@@ -57938,8 +58053,8 @@
       </c>
     </row>
     <row r="969">
-      <c r="A969" s="76"/>
-      <c r="B969" s="77"/>
+      <c r="A969" s="83"/>
+      <c r="B969" s="84"/>
       <c r="C969" s="34"/>
       <c r="D969" s="34"/>
       <c r="E969" s="34"/>
@@ -57964,8 +58079,8 @@
       </c>
     </row>
     <row r="970">
-      <c r="A970" s="76"/>
-      <c r="B970" s="77"/>
+      <c r="A970" s="83"/>
+      <c r="B970" s="84"/>
       <c r="C970" s="34"/>
       <c r="D970" s="34"/>
       <c r="E970" s="34"/>
@@ -57990,8 +58105,8 @@
       </c>
     </row>
     <row r="971">
-      <c r="A971" s="76"/>
-      <c r="B971" s="77"/>
+      <c r="A971" s="83"/>
+      <c r="B971" s="84"/>
       <c r="C971" s="34"/>
       <c r="D971" s="34"/>
       <c r="E971" s="34"/>
@@ -58016,8 +58131,8 @@
       </c>
     </row>
     <row r="972">
-      <c r="A972" s="76"/>
-      <c r="B972" s="77"/>
+      <c r="A972" s="83"/>
+      <c r="B972" s="84"/>
       <c r="C972" s="34"/>
       <c r="D972" s="34"/>
       <c r="E972" s="34"/>
@@ -58042,8 +58157,8 @@
       </c>
     </row>
     <row r="973">
-      <c r="A973" s="76"/>
-      <c r="B973" s="77"/>
+      <c r="A973" s="83"/>
+      <c r="B973" s="84"/>
       <c r="C973" s="34"/>
       <c r="D973" s="34"/>
       <c r="E973" s="34"/>
@@ -58068,8 +58183,8 @@
       </c>
     </row>
     <row r="974">
-      <c r="A974" s="76"/>
-      <c r="B974" s="77"/>
+      <c r="A974" s="83"/>
+      <c r="B974" s="84"/>
       <c r="C974" s="34"/>
       <c r="D974" s="34"/>
       <c r="E974" s="34"/>
@@ -58094,8 +58209,8 @@
       </c>
     </row>
     <row r="975">
-      <c r="A975" s="76"/>
-      <c r="B975" s="77"/>
+      <c r="A975" s="83"/>
+      <c r="B975" s="84"/>
       <c r="C975" s="34"/>
       <c r="D975" s="34"/>
       <c r="E975" s="34"/>
@@ -58120,8 +58235,8 @@
       </c>
     </row>
     <row r="976">
-      <c r="A976" s="76"/>
-      <c r="B976" s="77"/>
+      <c r="A976" s="83"/>
+      <c r="B976" s="84"/>
       <c r="C976" s="34"/>
       <c r="D976" s="34"/>
       <c r="E976" s="34"/>
@@ -58146,8 +58261,8 @@
       </c>
     </row>
     <row r="977">
-      <c r="A977" s="76"/>
-      <c r="B977" s="77"/>
+      <c r="A977" s="83"/>
+      <c r="B977" s="84"/>
       <c r="C977" s="34"/>
       <c r="D977" s="34"/>
       <c r="E977" s="34"/>
@@ -58172,8 +58287,8 @@
       </c>
     </row>
     <row r="978">
-      <c r="A978" s="76"/>
-      <c r="B978" s="77"/>
+      <c r="A978" s="83"/>
+      <c r="B978" s="84"/>
       <c r="C978" s="34"/>
       <c r="D978" s="34"/>
       <c r="E978" s="34"/>
@@ -58198,8 +58313,8 @@
       </c>
     </row>
     <row r="979">
-      <c r="A979" s="76"/>
-      <c r="B979" s="77"/>
+      <c r="A979" s="83"/>
+      <c r="B979" s="84"/>
       <c r="C979" s="34"/>
       <c r="D979" s="34"/>
       <c r="E979" s="34"/>
@@ -58224,8 +58339,8 @@
       </c>
     </row>
     <row r="980">
-      <c r="A980" s="76"/>
-      <c r="B980" s="77"/>
+      <c r="A980" s="83"/>
+      <c r="B980" s="84"/>
       <c r="C980" s="34"/>
       <c r="D980" s="34"/>
       <c r="E980" s="34"/>
@@ -58250,8 +58365,8 @@
       </c>
     </row>
     <row r="981">
-      <c r="A981" s="76"/>
-      <c r="B981" s="77"/>
+      <c r="A981" s="83"/>
+      <c r="B981" s="84"/>
       <c r="C981" s="34"/>
       <c r="D981" s="34"/>
       <c r="E981" s="34"/>
@@ -58276,8 +58391,8 @@
       </c>
     </row>
     <row r="982">
-      <c r="A982" s="76"/>
-      <c r="B982" s="77"/>
+      <c r="A982" s="83"/>
+      <c r="B982" s="84"/>
       <c r="C982" s="34"/>
       <c r="D982" s="34"/>
       <c r="E982" s="34"/>
@@ -58302,8 +58417,8 @@
       </c>
     </row>
     <row r="983">
-      <c r="A983" s="76"/>
-      <c r="B983" s="77"/>
+      <c r="A983" s="83"/>
+      <c r="B983" s="84"/>
       <c r="C983" s="34"/>
       <c r="D983" s="34"/>
       <c r="E983" s="34"/>
@@ -58328,8 +58443,8 @@
       </c>
     </row>
     <row r="984">
-      <c r="A984" s="76"/>
-      <c r="B984" s="77"/>
+      <c r="A984" s="83"/>
+      <c r="B984" s="84"/>
       <c r="C984" s="34"/>
       <c r="D984" s="34"/>
       <c r="E984" s="34"/>
@@ -58354,8 +58469,8 @@
       </c>
     </row>
     <row r="985">
-      <c r="A985" s="76"/>
-      <c r="B985" s="77"/>
+      <c r="A985" s="83"/>
+      <c r="B985" s="84"/>
       <c r="C985" s="34"/>
       <c r="D985" s="34"/>
       <c r="E985" s="34"/>
@@ -58380,8 +58495,8 @@
       </c>
     </row>
     <row r="986">
-      <c r="A986" s="76"/>
-      <c r="B986" s="77"/>
+      <c r="A986" s="83"/>
+      <c r="B986" s="84"/>
       <c r="C986" s="34"/>
       <c r="D986" s="34"/>
       <c r="E986" s="34"/>
@@ -58406,8 +58521,8 @@
       </c>
     </row>
     <row r="987">
-      <c r="A987" s="76"/>
-      <c r="B987" s="77"/>
+      <c r="A987" s="83"/>
+      <c r="B987" s="84"/>
       <c r="C987" s="34"/>
       <c r="D987" s="34"/>
       <c r="E987" s="34"/>
@@ -58432,8 +58547,8 @@
       </c>
     </row>
     <row r="988">
-      <c r="A988" s="76"/>
-      <c r="B988" s="77"/>
+      <c r="A988" s="83"/>
+      <c r="B988" s="84"/>
       <c r="C988" s="34"/>
       <c r="D988" s="34"/>
       <c r="E988" s="34"/>
@@ -58458,8 +58573,8 @@
       </c>
     </row>
     <row r="989">
-      <c r="A989" s="76"/>
-      <c r="B989" s="77"/>
+      <c r="A989" s="83"/>
+      <c r="B989" s="84"/>
       <c r="C989" s="34"/>
       <c r="D989" s="34"/>
       <c r="E989" s="34"/>
@@ -58484,8 +58599,8 @@
       </c>
     </row>
     <row r="990">
-      <c r="A990" s="76"/>
-      <c r="B990" s="77"/>
+      <c r="A990" s="83"/>
+      <c r="B990" s="84"/>
       <c r="C990" s="34"/>
       <c r="D990" s="34"/>
       <c r="E990" s="34"/>
@@ -58510,8 +58625,8 @@
       </c>
     </row>
     <row r="991">
-      <c r="A991" s="76"/>
-      <c r="B991" s="77"/>
+      <c r="A991" s="83"/>
+      <c r="B991" s="84"/>
       <c r="C991" s="34"/>
       <c r="D991" s="34"/>
       <c r="E991" s="34"/>
@@ -58536,8 +58651,8 @@
       </c>
     </row>
     <row r="992">
-      <c r="A992" s="76"/>
-      <c r="B992" s="77"/>
+      <c r="A992" s="83"/>
+      <c r="B992" s="84"/>
       <c r="C992" s="34"/>
       <c r="D992" s="34"/>
       <c r="E992" s="34"/>
@@ -58562,8 +58677,8 @@
       </c>
     </row>
     <row r="993">
-      <c r="A993" s="76"/>
-      <c r="B993" s="77"/>
+      <c r="A993" s="83"/>
+      <c r="B993" s="84"/>
       <c r="C993" s="34"/>
       <c r="D993" s="34"/>
       <c r="E993" s="34"/>
@@ -58588,8 +58703,8 @@
       </c>
     </row>
     <row r="994">
-      <c r="A994" s="76"/>
-      <c r="B994" s="77"/>
+      <c r="A994" s="83"/>
+      <c r="B994" s="84"/>
       <c r="C994" s="34"/>
       <c r="D994" s="34"/>
       <c r="E994" s="34"/>
@@ -58614,8 +58729,8 @@
       </c>
     </row>
     <row r="995">
-      <c r="A995" s="76"/>
-      <c r="B995" s="77"/>
+      <c r="A995" s="83"/>
+      <c r="B995" s="84"/>
       <c r="C995" s="34"/>
       <c r="D995" s="34"/>
       <c r="E995" s="34"/>
@@ -58640,8 +58755,8 @@
       </c>
     </row>
     <row r="996">
-      <c r="A996" s="76"/>
-      <c r="B996" s="77"/>
+      <c r="A996" s="83"/>
+      <c r="B996" s="84"/>
       <c r="C996" s="34"/>
       <c r="D996" s="34"/>
       <c r="E996" s="34"/>
@@ -58666,8 +58781,8 @@
       </c>
     </row>
     <row r="997">
-      <c r="A997" s="76"/>
-      <c r="B997" s="77"/>
+      <c r="A997" s="83"/>
+      <c r="B997" s="84"/>
       <c r="C997" s="34"/>
       <c r="D997" s="34"/>
       <c r="E997" s="34"/>
@@ -58692,8 +58807,8 @@
       </c>
     </row>
     <row r="998">
-      <c r="A998" s="76"/>
-      <c r="B998" s="77"/>
+      <c r="A998" s="83"/>
+      <c r="B998" s="84"/>
       <c r="C998" s="34"/>
       <c r="D998" s="34"/>
       <c r="E998" s="34"/>
@@ -58718,8 +58833,8 @@
       </c>
     </row>
     <row r="999">
-      <c r="A999" s="76"/>
-      <c r="B999" s="77"/>
+      <c r="A999" s="83"/>
+      <c r="B999" s="84"/>
       <c r="C999" s="34"/>
       <c r="D999" s="34"/>
       <c r="E999" s="34"/>
@@ -58744,8 +58859,8 @@
       </c>
     </row>
     <row r="1000">
-      <c r="A1000" s="76"/>
-      <c r="B1000" s="77"/>
+      <c r="A1000" s="83"/>
+      <c r="B1000" s="84"/>
       <c r="C1000" s="34"/>
       <c r="D1000" s="34"/>
       <c r="E1000" s="34"/>
@@ -58770,8 +58885,8 @@
       </c>
     </row>
     <row r="1001">
-      <c r="A1001" s="76"/>
-      <c r="B1001" s="77"/>
+      <c r="A1001" s="83"/>
+      <c r="B1001" s="84"/>
       <c r="C1001" s="34"/>
       <c r="D1001" s="34"/>
       <c r="E1001" s="34"/>
@@ -59462,15 +59577,17 @@
     <hyperlink r:id="rId279" ref="S716"/>
     <hyperlink r:id="rId280" ref="S717"/>
     <hyperlink r:id="rId281" ref="S718"/>
+    <hyperlink r:id="rId282" ref="S719"/>
+    <hyperlink r:id="rId283" ref="S720"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId282"/>
-  <legacyDrawing r:id="rId283"/>
+  <drawing r:id="rId284"/>
+  <legacyDrawing r:id="rId285"/>
   <tableParts count="2">
-    <tablePart r:id="rId286"/>
-    <tablePart r:id="rId287"/>
+    <tablePart r:id="rId288"/>
+    <tablePart r:id="rId289"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201210
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -577,7 +577,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8215" uniqueCount="2548">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8241" uniqueCount="2557">
   <si>
     <t>案例</t>
   </si>
@@ -9179,6 +9179,34 @@
     <t>處理公事
 Ct值15</t>
   </si>
+  <si>
+    <t>#720</t>
+  </si>
+  <si>
+    <t>緬甸</t>
+  </si>
+  <si>
+    <t>-11/22 緬甸→台灣</t>
+  </si>
+  <si>
+    <t>12/7 採檢
+12/9 確診</t>
+  </si>
+  <si>
+    <t>由仲介安排自費採檢</t>
+  </si>
+  <si>
+    <t>新增2例境外移入COVID-19病例，自緬甸及印尼入境</t>
+  </si>
+  <si>
+    <t>#721</t>
+  </si>
+  <si>
+    <t>-11/21 印尼→台灣</t>
+  </si>
+  <si>
+    <t>由公司安排自費採檢</t>
+  </si>
 </sst>
 </file>
 
@@ -9188,7 +9216,7 @@
     <numFmt numFmtId="164" formatCode="mm&quot;月&quot;dd&quot;日 &quot;dddd"/>
     <numFmt numFmtId="165" formatCode="m/d"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="19">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -9273,10 +9301,6 @@
       <u/>
       <color rgb="FF0000FF"/>
     </font>
-    <font/>
-    <font>
-      <color rgb="FF000000"/>
-    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -9322,7 +9346,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="78">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -9550,27 +9574,6 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="19" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="20" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
@@ -51493,7 +51496,7 @@
       </c>
     </row>
     <row r="719">
-      <c r="A719" s="76" t="s">
+      <c r="A719" s="16" t="s">
         <v>2539</v>
       </c>
       <c r="B719" s="6">
@@ -51502,7 +51505,7 @@
       <c r="C719" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D719" s="77" t="s">
+      <c r="D719" s="7" t="s">
         <v>76</v>
       </c>
       <c r="E719" s="7" t="s">
@@ -51512,29 +51515,29 @@
       <c r="G719" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H719" s="78" t="s">
+      <c r="H719" s="8" t="s">
         <v>2540</v>
       </c>
-      <c r="I719" s="79">
+      <c r="I719" s="9">
         <v>44158.0</v>
       </c>
-      <c r="J719" s="80" t="s">
+      <c r="J719" s="12" t="s">
         <v>1442</v>
       </c>
       <c r="K719" s="13" t="s">
         <v>2541</v>
       </c>
-      <c r="L719" s="80" t="s">
+      <c r="L719" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M719" s="81" t="s">
+      <c r="M719" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N719" s="25"/>
-      <c r="O719" s="78" t="s">
+      <c r="O719" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P719" s="78" t="s">
+      <c r="P719" s="8" t="s">
         <v>2096</v>
       </c>
       <c r="Q719" s="19"/>
@@ -51549,7 +51552,7 @@
       </c>
     </row>
     <row r="720">
-      <c r="A720" s="76" t="s">
+      <c r="A720" s="16" t="s">
         <v>2543</v>
       </c>
       <c r="B720" s="6">
@@ -51558,7 +51561,7 @@
       <c r="C720" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D720" s="77" t="s">
+      <c r="D720" s="7" t="s">
         <v>22</v>
       </c>
       <c r="E720" s="7" t="s">
@@ -51568,29 +51571,29 @@
       <c r="G720" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H720" s="78" t="s">
+      <c r="H720" s="8" t="s">
         <v>2544</v>
       </c>
-      <c r="I720" s="79">
+      <c r="I720" s="9">
         <v>44157.0</v>
       </c>
-      <c r="J720" s="82">
+      <c r="J720" s="10">
         <v>44169.0</v>
       </c>
       <c r="K720" s="13" t="s">
         <v>2545</v>
       </c>
-      <c r="L720" s="80" t="s">
+      <c r="L720" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M720" s="81" t="s">
+      <c r="M720" s="13" t="s">
         <v>2546</v>
       </c>
       <c r="N720" s="25"/>
-      <c r="O720" s="78" t="s">
+      <c r="O720" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="P720" s="78" t="s">
+      <c r="P720" s="8" t="s">
         <v>2547</v>
       </c>
       <c r="Q720" s="19"/>
@@ -51605,60 +51608,120 @@
       </c>
     </row>
     <row r="721">
-      <c r="A721" s="83"/>
-      <c r="B721" s="84"/>
-      <c r="C721" s="34"/>
-      <c r="D721" s="34"/>
-      <c r="E721" s="34"/>
+      <c r="A721" s="16" t="s">
+        <v>2548</v>
+      </c>
+      <c r="B721" s="6">
+        <v>44174.0</v>
+      </c>
+      <c r="C721" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D721" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E721" s="7" t="s">
+        <v>2549</v>
+      </c>
       <c r="F721" s="34"/>
-      <c r="G721" s="34"/>
-      <c r="H721" s="21"/>
-      <c r="I721" s="19"/>
-      <c r="J721" s="10"/>
-      <c r="K721" s="22"/>
-      <c r="L721" s="23"/>
-      <c r="M721" s="22"/>
+      <c r="G721" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H721" s="8" t="s">
+        <v>2550</v>
+      </c>
+      <c r="I721" s="9">
+        <v>44157.0</v>
+      </c>
+      <c r="J721" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K721" s="13" t="s">
+        <v>2551</v>
+      </c>
+      <c r="L721" s="12" t="s">
+        <v>1674</v>
+      </c>
+      <c r="M721" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N721" s="25"/>
-      <c r="O721" s="21"/>
-      <c r="P721" s="21"/>
+      <c r="O721" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P721" s="8" t="s">
+        <v>2552</v>
+      </c>
       <c r="Q721" s="19"/>
       <c r="R721" s="19"/>
-      <c r="S721" s="20"/>
+      <c r="S721" s="61" t="s">
+        <v>2553</v>
+      </c>
       <c r="T721" s="20"/>
       <c r="U721" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#720</v>
       </c>
     </row>
     <row r="722">
-      <c r="A722" s="83"/>
-      <c r="B722" s="84"/>
-      <c r="C722" s="34"/>
-      <c r="D722" s="34"/>
-      <c r="E722" s="34"/>
+      <c r="A722" s="16" t="s">
+        <v>2554</v>
+      </c>
+      <c r="B722" s="6">
+        <v>44174.0</v>
+      </c>
+      <c r="C722" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D722" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E722" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F722" s="34"/>
-      <c r="G722" s="34"/>
-      <c r="H722" s="21"/>
-      <c r="I722" s="19"/>
-      <c r="J722" s="10"/>
-      <c r="K722" s="22"/>
-      <c r="L722" s="23"/>
-      <c r="M722" s="22"/>
+      <c r="G722" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H722" s="8" t="s">
+        <v>2555</v>
+      </c>
+      <c r="I722" s="9">
+        <v>44156.0</v>
+      </c>
+      <c r="J722" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K722" s="13" t="s">
+        <v>2551</v>
+      </c>
+      <c r="L722" s="12" t="s">
+        <v>1674</v>
+      </c>
+      <c r="M722" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N722" s="25"/>
-      <c r="O722" s="21"/>
-      <c r="P722" s="21"/>
+      <c r="O722" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P722" s="8" t="s">
+        <v>2556</v>
+      </c>
       <c r="Q722" s="19"/>
       <c r="R722" s="19"/>
-      <c r="S722" s="20"/>
+      <c r="S722" s="61" t="s">
+        <v>2553</v>
+      </c>
       <c r="T722" s="20"/>
       <c r="U722" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#721</v>
       </c>
     </row>
     <row r="723">
-      <c r="A723" s="83"/>
-      <c r="B723" s="84"/>
+      <c r="A723" s="76"/>
+      <c r="B723" s="77"/>
       <c r="C723" s="34"/>
       <c r="D723" s="34"/>
       <c r="E723" s="34"/>
@@ -51683,8 +51746,8 @@
       </c>
     </row>
     <row r="724">
-      <c r="A724" s="83"/>
-      <c r="B724" s="84"/>
+      <c r="A724" s="76"/>
+      <c r="B724" s="77"/>
       <c r="C724" s="34"/>
       <c r="D724" s="34"/>
       <c r="E724" s="34"/>
@@ -51709,8 +51772,8 @@
       </c>
     </row>
     <row r="725">
-      <c r="A725" s="83"/>
-      <c r="B725" s="84"/>
+      <c r="A725" s="76"/>
+      <c r="B725" s="77"/>
       <c r="C725" s="34"/>
       <c r="D725" s="34"/>
       <c r="E725" s="34"/>
@@ -51735,8 +51798,8 @@
       </c>
     </row>
     <row r="726">
-      <c r="A726" s="83"/>
-      <c r="B726" s="84"/>
+      <c r="A726" s="76"/>
+      <c r="B726" s="77"/>
       <c r="C726" s="34"/>
       <c r="D726" s="34"/>
       <c r="E726" s="34"/>
@@ -51761,8 +51824,8 @@
       </c>
     </row>
     <row r="727">
-      <c r="A727" s="83"/>
-      <c r="B727" s="84"/>
+      <c r="A727" s="76"/>
+      <c r="B727" s="77"/>
       <c r="C727" s="34"/>
       <c r="D727" s="34"/>
       <c r="E727" s="34"/>
@@ -51787,8 +51850,8 @@
       </c>
     </row>
     <row r="728">
-      <c r="A728" s="83"/>
-      <c r="B728" s="84"/>
+      <c r="A728" s="76"/>
+      <c r="B728" s="77"/>
       <c r="C728" s="34"/>
       <c r="D728" s="34"/>
       <c r="E728" s="34"/>
@@ -51813,8 +51876,8 @@
       </c>
     </row>
     <row r="729">
-      <c r="A729" s="83"/>
-      <c r="B729" s="84"/>
+      <c r="A729" s="76"/>
+      <c r="B729" s="77"/>
       <c r="C729" s="34"/>
       <c r="D729" s="34"/>
       <c r="E729" s="34"/>
@@ -51839,8 +51902,8 @@
       </c>
     </row>
     <row r="730">
-      <c r="A730" s="83"/>
-      <c r="B730" s="84"/>
+      <c r="A730" s="76"/>
+      <c r="B730" s="77"/>
       <c r="C730" s="34"/>
       <c r="D730" s="34"/>
       <c r="E730" s="34"/>
@@ -51865,8 +51928,8 @@
       </c>
     </row>
     <row r="731">
-      <c r="A731" s="83"/>
-      <c r="B731" s="84"/>
+      <c r="A731" s="76"/>
+      <c r="B731" s="77"/>
       <c r="C731" s="34"/>
       <c r="D731" s="34"/>
       <c r="E731" s="34"/>
@@ -51891,8 +51954,8 @@
       </c>
     </row>
     <row r="732">
-      <c r="A732" s="83"/>
-      <c r="B732" s="84"/>
+      <c r="A732" s="76"/>
+      <c r="B732" s="77"/>
       <c r="C732" s="34"/>
       <c r="D732" s="34"/>
       <c r="E732" s="34"/>
@@ -51917,8 +51980,8 @@
       </c>
     </row>
     <row r="733">
-      <c r="A733" s="83"/>
-      <c r="B733" s="84"/>
+      <c r="A733" s="76"/>
+      <c r="B733" s="77"/>
       <c r="C733" s="34"/>
       <c r="D733" s="34"/>
       <c r="E733" s="34"/>
@@ -51943,8 +52006,8 @@
       </c>
     </row>
     <row r="734">
-      <c r="A734" s="83"/>
-      <c r="B734" s="84"/>
+      <c r="A734" s="76"/>
+      <c r="B734" s="77"/>
       <c r="C734" s="34"/>
       <c r="D734" s="34"/>
       <c r="E734" s="34"/>
@@ -51969,8 +52032,8 @@
       </c>
     </row>
     <row r="735">
-      <c r="A735" s="83"/>
-      <c r="B735" s="84"/>
+      <c r="A735" s="76"/>
+      <c r="B735" s="77"/>
       <c r="C735" s="34"/>
       <c r="D735" s="34"/>
       <c r="E735" s="34"/>
@@ -51995,8 +52058,8 @@
       </c>
     </row>
     <row r="736">
-      <c r="A736" s="83"/>
-      <c r="B736" s="84"/>
+      <c r="A736" s="76"/>
+      <c r="B736" s="77"/>
       <c r="C736" s="34"/>
       <c r="D736" s="34"/>
       <c r="E736" s="34"/>
@@ -52021,8 +52084,8 @@
       </c>
     </row>
     <row r="737">
-      <c r="A737" s="83"/>
-      <c r="B737" s="84"/>
+      <c r="A737" s="76"/>
+      <c r="B737" s="77"/>
       <c r="C737" s="34"/>
       <c r="D737" s="34"/>
       <c r="E737" s="34"/>
@@ -52047,8 +52110,8 @@
       </c>
     </row>
     <row r="738">
-      <c r="A738" s="83"/>
-      <c r="B738" s="84"/>
+      <c r="A738" s="76"/>
+      <c r="B738" s="77"/>
       <c r="C738" s="34"/>
       <c r="D738" s="34"/>
       <c r="E738" s="34"/>
@@ -52073,8 +52136,8 @@
       </c>
     </row>
     <row r="739">
-      <c r="A739" s="83"/>
-      <c r="B739" s="84"/>
+      <c r="A739" s="76"/>
+      <c r="B739" s="77"/>
       <c r="C739" s="34"/>
       <c r="D739" s="34"/>
       <c r="E739" s="34"/>
@@ -52099,8 +52162,8 @@
       </c>
     </row>
     <row r="740">
-      <c r="A740" s="83"/>
-      <c r="B740" s="84"/>
+      <c r="A740" s="76"/>
+      <c r="B740" s="77"/>
       <c r="C740" s="34"/>
       <c r="D740" s="34"/>
       <c r="E740" s="34"/>
@@ -52125,8 +52188,8 @@
       </c>
     </row>
     <row r="741">
-      <c r="A741" s="83"/>
-      <c r="B741" s="84"/>
+      <c r="A741" s="76"/>
+      <c r="B741" s="77"/>
       <c r="C741" s="34"/>
       <c r="D741" s="34"/>
       <c r="E741" s="34"/>
@@ -52151,8 +52214,8 @@
       </c>
     </row>
     <row r="742">
-      <c r="A742" s="83"/>
-      <c r="B742" s="84"/>
+      <c r="A742" s="76"/>
+      <c r="B742" s="77"/>
       <c r="C742" s="34"/>
       <c r="D742" s="34"/>
       <c r="E742" s="34"/>
@@ -52177,8 +52240,8 @@
       </c>
     </row>
     <row r="743">
-      <c r="A743" s="83"/>
-      <c r="B743" s="84"/>
+      <c r="A743" s="76"/>
+      <c r="B743" s="77"/>
       <c r="C743" s="34"/>
       <c r="D743" s="34"/>
       <c r="E743" s="34"/>
@@ -52203,8 +52266,8 @@
       </c>
     </row>
     <row r="744">
-      <c r="A744" s="83"/>
-      <c r="B744" s="84"/>
+      <c r="A744" s="76"/>
+      <c r="B744" s="77"/>
       <c r="C744" s="34"/>
       <c r="D744" s="34"/>
       <c r="E744" s="34"/>
@@ -52229,8 +52292,8 @@
       </c>
     </row>
     <row r="745">
-      <c r="A745" s="83"/>
-      <c r="B745" s="84"/>
+      <c r="A745" s="76"/>
+      <c r="B745" s="77"/>
       <c r="C745" s="34"/>
       <c r="D745" s="34"/>
       <c r="E745" s="34"/>
@@ -52255,8 +52318,8 @@
       </c>
     </row>
     <row r="746">
-      <c r="A746" s="83"/>
-      <c r="B746" s="84"/>
+      <c r="A746" s="76"/>
+      <c r="B746" s="77"/>
       <c r="C746" s="34"/>
       <c r="D746" s="34"/>
       <c r="E746" s="34"/>
@@ -52281,8 +52344,8 @@
       </c>
     </row>
     <row r="747">
-      <c r="A747" s="83"/>
-      <c r="B747" s="84"/>
+      <c r="A747" s="76"/>
+      <c r="B747" s="77"/>
       <c r="C747" s="34"/>
       <c r="D747" s="34"/>
       <c r="E747" s="34"/>
@@ -52307,8 +52370,8 @@
       </c>
     </row>
     <row r="748">
-      <c r="A748" s="83"/>
-      <c r="B748" s="84"/>
+      <c r="A748" s="76"/>
+      <c r="B748" s="77"/>
       <c r="C748" s="34"/>
       <c r="D748" s="34"/>
       <c r="E748" s="34"/>
@@ -52333,8 +52396,8 @@
       </c>
     </row>
     <row r="749">
-      <c r="A749" s="83"/>
-      <c r="B749" s="84"/>
+      <c r="A749" s="76"/>
+      <c r="B749" s="77"/>
       <c r="C749" s="34"/>
       <c r="D749" s="34"/>
       <c r="E749" s="34"/>
@@ -52359,8 +52422,8 @@
       </c>
     </row>
     <row r="750">
-      <c r="A750" s="83"/>
-      <c r="B750" s="84"/>
+      <c r="A750" s="76"/>
+      <c r="B750" s="77"/>
       <c r="C750" s="34"/>
       <c r="D750" s="34"/>
       <c r="E750" s="34"/>
@@ -52385,8 +52448,8 @@
       </c>
     </row>
     <row r="751">
-      <c r="A751" s="83"/>
-      <c r="B751" s="84"/>
+      <c r="A751" s="76"/>
+      <c r="B751" s="77"/>
       <c r="C751" s="34"/>
       <c r="D751" s="34"/>
       <c r="E751" s="34"/>
@@ -52411,8 +52474,8 @@
       </c>
     </row>
     <row r="752">
-      <c r="A752" s="83"/>
-      <c r="B752" s="84"/>
+      <c r="A752" s="76"/>
+      <c r="B752" s="77"/>
       <c r="C752" s="34"/>
       <c r="D752" s="34"/>
       <c r="E752" s="34"/>
@@ -52437,8 +52500,8 @@
       </c>
     </row>
     <row r="753">
-      <c r="A753" s="83"/>
-      <c r="B753" s="84"/>
+      <c r="A753" s="76"/>
+      <c r="B753" s="77"/>
       <c r="C753" s="34"/>
       <c r="D753" s="34"/>
       <c r="E753" s="34"/>
@@ -52463,8 +52526,8 @@
       </c>
     </row>
     <row r="754">
-      <c r="A754" s="83"/>
-      <c r="B754" s="84"/>
+      <c r="A754" s="76"/>
+      <c r="B754" s="77"/>
       <c r="C754" s="34"/>
       <c r="D754" s="34"/>
       <c r="E754" s="34"/>
@@ -52489,8 +52552,8 @@
       </c>
     </row>
     <row r="755">
-      <c r="A755" s="83"/>
-      <c r="B755" s="84"/>
+      <c r="A755" s="76"/>
+      <c r="B755" s="77"/>
       <c r="C755" s="34"/>
       <c r="D755" s="34"/>
       <c r="E755" s="34"/>
@@ -52515,8 +52578,8 @@
       </c>
     </row>
     <row r="756">
-      <c r="A756" s="83"/>
-      <c r="B756" s="84"/>
+      <c r="A756" s="76"/>
+      <c r="B756" s="77"/>
       <c r="C756" s="34"/>
       <c r="D756" s="34"/>
       <c r="E756" s="34"/>
@@ -52541,8 +52604,8 @@
       </c>
     </row>
     <row r="757">
-      <c r="A757" s="83"/>
-      <c r="B757" s="84"/>
+      <c r="A757" s="76"/>
+      <c r="B757" s="77"/>
       <c r="C757" s="34"/>
       <c r="D757" s="34"/>
       <c r="E757" s="34"/>
@@ -52567,8 +52630,8 @@
       </c>
     </row>
     <row r="758">
-      <c r="A758" s="83"/>
-      <c r="B758" s="84"/>
+      <c r="A758" s="76"/>
+      <c r="B758" s="77"/>
       <c r="C758" s="34"/>
       <c r="D758" s="34"/>
       <c r="E758" s="34"/>
@@ -52593,8 +52656,8 @@
       </c>
     </row>
     <row r="759">
-      <c r="A759" s="83"/>
-      <c r="B759" s="84"/>
+      <c r="A759" s="76"/>
+      <c r="B759" s="77"/>
       <c r="C759" s="34"/>
       <c r="D759" s="34"/>
       <c r="E759" s="34"/>
@@ -52619,8 +52682,8 @@
       </c>
     </row>
     <row r="760">
-      <c r="A760" s="83"/>
-      <c r="B760" s="84"/>
+      <c r="A760" s="76"/>
+      <c r="B760" s="77"/>
       <c r="C760" s="34"/>
       <c r="D760" s="34"/>
       <c r="E760" s="34"/>
@@ -52645,8 +52708,8 @@
       </c>
     </row>
     <row r="761">
-      <c r="A761" s="83"/>
-      <c r="B761" s="84"/>
+      <c r="A761" s="76"/>
+      <c r="B761" s="77"/>
       <c r="C761" s="34"/>
       <c r="D761" s="34"/>
       <c r="E761" s="34"/>
@@ -52671,8 +52734,8 @@
       </c>
     </row>
     <row r="762">
-      <c r="A762" s="83"/>
-      <c r="B762" s="84"/>
+      <c r="A762" s="76"/>
+      <c r="B762" s="77"/>
       <c r="C762" s="34"/>
       <c r="D762" s="34"/>
       <c r="E762" s="34"/>
@@ -52697,8 +52760,8 @@
       </c>
     </row>
     <row r="763">
-      <c r="A763" s="83"/>
-      <c r="B763" s="84"/>
+      <c r="A763" s="76"/>
+      <c r="B763" s="77"/>
       <c r="C763" s="34"/>
       <c r="D763" s="34"/>
       <c r="E763" s="34"/>
@@ -52723,8 +52786,8 @@
       </c>
     </row>
     <row r="764">
-      <c r="A764" s="83"/>
-      <c r="B764" s="84"/>
+      <c r="A764" s="76"/>
+      <c r="B764" s="77"/>
       <c r="C764" s="34"/>
       <c r="D764" s="34"/>
       <c r="E764" s="34"/>
@@ -52749,8 +52812,8 @@
       </c>
     </row>
     <row r="765">
-      <c r="A765" s="83"/>
-      <c r="B765" s="84"/>
+      <c r="A765" s="76"/>
+      <c r="B765" s="77"/>
       <c r="C765" s="34"/>
       <c r="D765" s="34"/>
       <c r="E765" s="34"/>
@@ -52775,8 +52838,8 @@
       </c>
     </row>
     <row r="766">
-      <c r="A766" s="83"/>
-      <c r="B766" s="84"/>
+      <c r="A766" s="76"/>
+      <c r="B766" s="77"/>
       <c r="C766" s="34"/>
       <c r="D766" s="34"/>
       <c r="E766" s="34"/>
@@ -52801,8 +52864,8 @@
       </c>
     </row>
     <row r="767">
-      <c r="A767" s="83"/>
-      <c r="B767" s="84"/>
+      <c r="A767" s="76"/>
+      <c r="B767" s="77"/>
       <c r="C767" s="34"/>
       <c r="D767" s="34"/>
       <c r="E767" s="34"/>
@@ -52827,8 +52890,8 @@
       </c>
     </row>
     <row r="768">
-      <c r="A768" s="83"/>
-      <c r="B768" s="84"/>
+      <c r="A768" s="76"/>
+      <c r="B768" s="77"/>
       <c r="C768" s="34"/>
       <c r="D768" s="34"/>
       <c r="E768" s="34"/>
@@ -52853,8 +52916,8 @@
       </c>
     </row>
     <row r="769">
-      <c r="A769" s="83"/>
-      <c r="B769" s="84"/>
+      <c r="A769" s="76"/>
+      <c r="B769" s="77"/>
       <c r="C769" s="34"/>
       <c r="D769" s="34"/>
       <c r="E769" s="34"/>
@@ -52879,8 +52942,8 @@
       </c>
     </row>
     <row r="770">
-      <c r="A770" s="83"/>
-      <c r="B770" s="84"/>
+      <c r="A770" s="76"/>
+      <c r="B770" s="77"/>
       <c r="C770" s="34"/>
       <c r="D770" s="34"/>
       <c r="E770" s="34"/>
@@ -52905,8 +52968,8 @@
       </c>
     </row>
     <row r="771">
-      <c r="A771" s="83"/>
-      <c r="B771" s="84"/>
+      <c r="A771" s="76"/>
+      <c r="B771" s="77"/>
       <c r="C771" s="34"/>
       <c r="D771" s="34"/>
       <c r="E771" s="34"/>
@@ -52931,8 +52994,8 @@
       </c>
     </row>
     <row r="772">
-      <c r="A772" s="83"/>
-      <c r="B772" s="84"/>
+      <c r="A772" s="76"/>
+      <c r="B772" s="77"/>
       <c r="C772" s="34"/>
       <c r="D772" s="34"/>
       <c r="E772" s="34"/>
@@ -52957,8 +53020,8 @@
       </c>
     </row>
     <row r="773">
-      <c r="A773" s="83"/>
-      <c r="B773" s="84"/>
+      <c r="A773" s="76"/>
+      <c r="B773" s="77"/>
       <c r="C773" s="34"/>
       <c r="D773" s="34"/>
       <c r="E773" s="34"/>
@@ -52983,8 +53046,8 @@
       </c>
     </row>
     <row r="774">
-      <c r="A774" s="83"/>
-      <c r="B774" s="84"/>
+      <c r="A774" s="76"/>
+      <c r="B774" s="77"/>
       <c r="C774" s="34"/>
       <c r="D774" s="34"/>
       <c r="E774" s="34"/>
@@ -53009,8 +53072,8 @@
       </c>
     </row>
     <row r="775">
-      <c r="A775" s="83"/>
-      <c r="B775" s="84"/>
+      <c r="A775" s="76"/>
+      <c r="B775" s="77"/>
       <c r="C775" s="34"/>
       <c r="D775" s="34"/>
       <c r="E775" s="34"/>
@@ -53035,8 +53098,8 @@
       </c>
     </row>
     <row r="776">
-      <c r="A776" s="83"/>
-      <c r="B776" s="84"/>
+      <c r="A776" s="76"/>
+      <c r="B776" s="77"/>
       <c r="C776" s="34"/>
       <c r="D776" s="34"/>
       <c r="E776" s="34"/>
@@ -53061,8 +53124,8 @@
       </c>
     </row>
     <row r="777">
-      <c r="A777" s="83"/>
-      <c r="B777" s="84"/>
+      <c r="A777" s="76"/>
+      <c r="B777" s="77"/>
       <c r="C777" s="34"/>
       <c r="D777" s="34"/>
       <c r="E777" s="34"/>
@@ -53087,8 +53150,8 @@
       </c>
     </row>
     <row r="778">
-      <c r="A778" s="83"/>
-      <c r="B778" s="84"/>
+      <c r="A778" s="76"/>
+      <c r="B778" s="77"/>
       <c r="C778" s="34"/>
       <c r="D778" s="34"/>
       <c r="E778" s="34"/>
@@ -53113,8 +53176,8 @@
       </c>
     </row>
     <row r="779">
-      <c r="A779" s="83"/>
-      <c r="B779" s="84"/>
+      <c r="A779" s="76"/>
+      <c r="B779" s="77"/>
       <c r="C779" s="34"/>
       <c r="D779" s="34"/>
       <c r="E779" s="34"/>
@@ -53139,8 +53202,8 @@
       </c>
     </row>
     <row r="780">
-      <c r="A780" s="83"/>
-      <c r="B780" s="84"/>
+      <c r="A780" s="76"/>
+      <c r="B780" s="77"/>
       <c r="C780" s="34"/>
       <c r="D780" s="34"/>
       <c r="E780" s="34"/>
@@ -53165,8 +53228,8 @@
       </c>
     </row>
     <row r="781">
-      <c r="A781" s="83"/>
-      <c r="B781" s="84"/>
+      <c r="A781" s="76"/>
+      <c r="B781" s="77"/>
       <c r="C781" s="34"/>
       <c r="D781" s="34"/>
       <c r="E781" s="34"/>
@@ -53191,8 +53254,8 @@
       </c>
     </row>
     <row r="782">
-      <c r="A782" s="83"/>
-      <c r="B782" s="84"/>
+      <c r="A782" s="76"/>
+      <c r="B782" s="77"/>
       <c r="C782" s="34"/>
       <c r="D782" s="34"/>
       <c r="E782" s="34"/>
@@ -53217,8 +53280,8 @@
       </c>
     </row>
     <row r="783">
-      <c r="A783" s="83"/>
-      <c r="B783" s="84"/>
+      <c r="A783" s="76"/>
+      <c r="B783" s="77"/>
       <c r="C783" s="34"/>
       <c r="D783" s="34"/>
       <c r="E783" s="34"/>
@@ -53243,8 +53306,8 @@
       </c>
     </row>
     <row r="784">
-      <c r="A784" s="83"/>
-      <c r="B784" s="84"/>
+      <c r="A784" s="76"/>
+      <c r="B784" s="77"/>
       <c r="C784" s="34"/>
       <c r="D784" s="34"/>
       <c r="E784" s="34"/>
@@ -53269,8 +53332,8 @@
       </c>
     </row>
     <row r="785">
-      <c r="A785" s="83"/>
-      <c r="B785" s="84"/>
+      <c r="A785" s="76"/>
+      <c r="B785" s="77"/>
       <c r="C785" s="34"/>
       <c r="D785" s="34"/>
       <c r="E785" s="34"/>
@@ -53295,8 +53358,8 @@
       </c>
     </row>
     <row r="786">
-      <c r="A786" s="83"/>
-      <c r="B786" s="84"/>
+      <c r="A786" s="76"/>
+      <c r="B786" s="77"/>
       <c r="C786" s="34"/>
       <c r="D786" s="34"/>
       <c r="E786" s="34"/>
@@ -53321,8 +53384,8 @@
       </c>
     </row>
     <row r="787">
-      <c r="A787" s="83"/>
-      <c r="B787" s="84"/>
+      <c r="A787" s="76"/>
+      <c r="B787" s="77"/>
       <c r="C787" s="34"/>
       <c r="D787" s="34"/>
       <c r="E787" s="34"/>
@@ -53347,8 +53410,8 @@
       </c>
     </row>
     <row r="788">
-      <c r="A788" s="83"/>
-      <c r="B788" s="84"/>
+      <c r="A788" s="76"/>
+      <c r="B788" s="77"/>
       <c r="C788" s="34"/>
       <c r="D788" s="34"/>
       <c r="E788" s="34"/>
@@ -53373,8 +53436,8 @@
       </c>
     </row>
     <row r="789">
-      <c r="A789" s="83"/>
-      <c r="B789" s="84"/>
+      <c r="A789" s="76"/>
+      <c r="B789" s="77"/>
       <c r="C789" s="34"/>
       <c r="D789" s="34"/>
       <c r="E789" s="34"/>
@@ -53399,8 +53462,8 @@
       </c>
     </row>
     <row r="790">
-      <c r="A790" s="83"/>
-      <c r="B790" s="84"/>
+      <c r="A790" s="76"/>
+      <c r="B790" s="77"/>
       <c r="C790" s="34"/>
       <c r="D790" s="34"/>
       <c r="E790" s="34"/>
@@ -53425,8 +53488,8 @@
       </c>
     </row>
     <row r="791">
-      <c r="A791" s="83"/>
-      <c r="B791" s="84"/>
+      <c r="A791" s="76"/>
+      <c r="B791" s="77"/>
       <c r="C791" s="34"/>
       <c r="D791" s="34"/>
       <c r="E791" s="34"/>
@@ -53451,8 +53514,8 @@
       </c>
     </row>
     <row r="792">
-      <c r="A792" s="83"/>
-      <c r="B792" s="84"/>
+      <c r="A792" s="76"/>
+      <c r="B792" s="77"/>
       <c r="C792" s="34"/>
       <c r="D792" s="34"/>
       <c r="E792" s="34"/>
@@ -53477,8 +53540,8 @@
       </c>
     </row>
     <row r="793">
-      <c r="A793" s="83"/>
-      <c r="B793" s="84"/>
+      <c r="A793" s="76"/>
+      <c r="B793" s="77"/>
       <c r="C793" s="34"/>
       <c r="D793" s="34"/>
       <c r="E793" s="34"/>
@@ -53503,8 +53566,8 @@
       </c>
     </row>
     <row r="794">
-      <c r="A794" s="83"/>
-      <c r="B794" s="84"/>
+      <c r="A794" s="76"/>
+      <c r="B794" s="77"/>
       <c r="C794" s="34"/>
       <c r="D794" s="34"/>
       <c r="E794" s="34"/>
@@ -53529,8 +53592,8 @@
       </c>
     </row>
     <row r="795">
-      <c r="A795" s="83"/>
-      <c r="B795" s="84"/>
+      <c r="A795" s="76"/>
+      <c r="B795" s="77"/>
       <c r="C795" s="34"/>
       <c r="D795" s="34"/>
       <c r="E795" s="34"/>
@@ -53555,8 +53618,8 @@
       </c>
     </row>
     <row r="796">
-      <c r="A796" s="83"/>
-      <c r="B796" s="84"/>
+      <c r="A796" s="76"/>
+      <c r="B796" s="77"/>
       <c r="C796" s="34"/>
       <c r="D796" s="34"/>
       <c r="E796" s="34"/>
@@ -53581,8 +53644,8 @@
       </c>
     </row>
     <row r="797">
-      <c r="A797" s="83"/>
-      <c r="B797" s="84"/>
+      <c r="A797" s="76"/>
+      <c r="B797" s="77"/>
       <c r="C797" s="34"/>
       <c r="D797" s="34"/>
       <c r="E797" s="34"/>
@@ -53607,8 +53670,8 @@
       </c>
     </row>
     <row r="798">
-      <c r="A798" s="83"/>
-      <c r="B798" s="84"/>
+      <c r="A798" s="76"/>
+      <c r="B798" s="77"/>
       <c r="C798" s="34"/>
       <c r="D798" s="34"/>
       <c r="E798" s="34"/>
@@ -53633,8 +53696,8 @@
       </c>
     </row>
     <row r="799">
-      <c r="A799" s="83"/>
-      <c r="B799" s="84"/>
+      <c r="A799" s="76"/>
+      <c r="B799" s="77"/>
       <c r="C799" s="34"/>
       <c r="D799" s="34"/>
       <c r="E799" s="34"/>
@@ -53659,8 +53722,8 @@
       </c>
     </row>
     <row r="800">
-      <c r="A800" s="83"/>
-      <c r="B800" s="84"/>
+      <c r="A800" s="76"/>
+      <c r="B800" s="77"/>
       <c r="C800" s="34"/>
       <c r="D800" s="34"/>
       <c r="E800" s="34"/>
@@ -53685,8 +53748,8 @@
       </c>
     </row>
     <row r="801">
-      <c r="A801" s="83"/>
-      <c r="B801" s="84"/>
+      <c r="A801" s="76"/>
+      <c r="B801" s="77"/>
       <c r="C801" s="34"/>
       <c r="D801" s="34"/>
       <c r="E801" s="34"/>
@@ -53711,8 +53774,8 @@
       </c>
     </row>
     <row r="802">
-      <c r="A802" s="83"/>
-      <c r="B802" s="84"/>
+      <c r="A802" s="76"/>
+      <c r="B802" s="77"/>
       <c r="C802" s="34"/>
       <c r="D802" s="34"/>
       <c r="E802" s="34"/>
@@ -53737,8 +53800,8 @@
       </c>
     </row>
     <row r="803">
-      <c r="A803" s="83"/>
-      <c r="B803" s="84"/>
+      <c r="A803" s="76"/>
+      <c r="B803" s="77"/>
       <c r="C803" s="34"/>
       <c r="D803" s="34"/>
       <c r="E803" s="34"/>
@@ -53763,8 +53826,8 @@
       </c>
     </row>
     <row r="804">
-      <c r="A804" s="83"/>
-      <c r="B804" s="84"/>
+      <c r="A804" s="76"/>
+      <c r="B804" s="77"/>
       <c r="C804" s="34"/>
       <c r="D804" s="34"/>
       <c r="E804" s="34"/>
@@ -53789,8 +53852,8 @@
       </c>
     </row>
     <row r="805">
-      <c r="A805" s="83"/>
-      <c r="B805" s="84"/>
+      <c r="A805" s="76"/>
+      <c r="B805" s="77"/>
       <c r="C805" s="34"/>
       <c r="D805" s="34"/>
       <c r="E805" s="34"/>
@@ -53815,8 +53878,8 @@
       </c>
     </row>
     <row r="806">
-      <c r="A806" s="83"/>
-      <c r="B806" s="84"/>
+      <c r="A806" s="76"/>
+      <c r="B806" s="77"/>
       <c r="C806" s="34"/>
       <c r="D806" s="34"/>
       <c r="E806" s="34"/>
@@ -53841,8 +53904,8 @@
       </c>
     </row>
     <row r="807">
-      <c r="A807" s="83"/>
-      <c r="B807" s="84"/>
+      <c r="A807" s="76"/>
+      <c r="B807" s="77"/>
       <c r="C807" s="34"/>
       <c r="D807" s="34"/>
       <c r="E807" s="34"/>
@@ -53867,8 +53930,8 @@
       </c>
     </row>
     <row r="808">
-      <c r="A808" s="83"/>
-      <c r="B808" s="84"/>
+      <c r="A808" s="76"/>
+      <c r="B808" s="77"/>
       <c r="C808" s="34"/>
       <c r="D808" s="34"/>
       <c r="E808" s="34"/>
@@ -53893,8 +53956,8 @@
       </c>
     </row>
     <row r="809">
-      <c r="A809" s="83"/>
-      <c r="B809" s="84"/>
+      <c r="A809" s="76"/>
+      <c r="B809" s="77"/>
       <c r="C809" s="34"/>
       <c r="D809" s="34"/>
       <c r="E809" s="34"/>
@@ -53919,8 +53982,8 @@
       </c>
     </row>
     <row r="810">
-      <c r="A810" s="83"/>
-      <c r="B810" s="84"/>
+      <c r="A810" s="76"/>
+      <c r="B810" s="77"/>
       <c r="C810" s="34"/>
       <c r="D810" s="34"/>
       <c r="E810" s="34"/>
@@ -53945,8 +54008,8 @@
       </c>
     </row>
     <row r="811">
-      <c r="A811" s="83"/>
-      <c r="B811" s="84"/>
+      <c r="A811" s="76"/>
+      <c r="B811" s="77"/>
       <c r="C811" s="34"/>
       <c r="D811" s="34"/>
       <c r="E811" s="34"/>
@@ -53971,8 +54034,8 @@
       </c>
     </row>
     <row r="812">
-      <c r="A812" s="83"/>
-      <c r="B812" s="84"/>
+      <c r="A812" s="76"/>
+      <c r="B812" s="77"/>
       <c r="C812" s="34"/>
       <c r="D812" s="34"/>
       <c r="E812" s="34"/>
@@ -53997,8 +54060,8 @@
       </c>
     </row>
     <row r="813">
-      <c r="A813" s="83"/>
-      <c r="B813" s="84"/>
+      <c r="A813" s="76"/>
+      <c r="B813" s="77"/>
       <c r="C813" s="34"/>
       <c r="D813" s="34"/>
       <c r="E813" s="34"/>
@@ -54023,8 +54086,8 @@
       </c>
     </row>
     <row r="814">
-      <c r="A814" s="83"/>
-      <c r="B814" s="84"/>
+      <c r="A814" s="76"/>
+      <c r="B814" s="77"/>
       <c r="C814" s="34"/>
       <c r="D814" s="34"/>
       <c r="E814" s="34"/>
@@ -54049,8 +54112,8 @@
       </c>
     </row>
     <row r="815">
-      <c r="A815" s="83"/>
-      <c r="B815" s="84"/>
+      <c r="A815" s="76"/>
+      <c r="B815" s="77"/>
       <c r="C815" s="34"/>
       <c r="D815" s="34"/>
       <c r="E815" s="34"/>
@@ -54075,8 +54138,8 @@
       </c>
     </row>
     <row r="816">
-      <c r="A816" s="83"/>
-      <c r="B816" s="84"/>
+      <c r="A816" s="76"/>
+      <c r="B816" s="77"/>
       <c r="C816" s="34"/>
       <c r="D816" s="34"/>
       <c r="E816" s="34"/>
@@ -54101,8 +54164,8 @@
       </c>
     </row>
     <row r="817">
-      <c r="A817" s="83"/>
-      <c r="B817" s="84"/>
+      <c r="A817" s="76"/>
+      <c r="B817" s="77"/>
       <c r="C817" s="34"/>
       <c r="D817" s="34"/>
       <c r="E817" s="34"/>
@@ -54127,8 +54190,8 @@
       </c>
     </row>
     <row r="818">
-      <c r="A818" s="83"/>
-      <c r="B818" s="84"/>
+      <c r="A818" s="76"/>
+      <c r="B818" s="77"/>
       <c r="C818" s="34"/>
       <c r="D818" s="34"/>
       <c r="E818" s="34"/>
@@ -54153,8 +54216,8 @@
       </c>
     </row>
     <row r="819">
-      <c r="A819" s="83"/>
-      <c r="B819" s="84"/>
+      <c r="A819" s="76"/>
+      <c r="B819" s="77"/>
       <c r="C819" s="34"/>
       <c r="D819" s="34"/>
       <c r="E819" s="34"/>
@@ -54179,8 +54242,8 @@
       </c>
     </row>
     <row r="820">
-      <c r="A820" s="83"/>
-      <c r="B820" s="84"/>
+      <c r="A820" s="76"/>
+      <c r="B820" s="77"/>
       <c r="C820" s="34"/>
       <c r="D820" s="34"/>
       <c r="E820" s="34"/>
@@ -54205,8 +54268,8 @@
       </c>
     </row>
     <row r="821">
-      <c r="A821" s="83"/>
-      <c r="B821" s="84"/>
+      <c r="A821" s="76"/>
+      <c r="B821" s="77"/>
       <c r="C821" s="34"/>
       <c r="D821" s="34"/>
       <c r="E821" s="34"/>
@@ -54231,8 +54294,8 @@
       </c>
     </row>
     <row r="822">
-      <c r="A822" s="83"/>
-      <c r="B822" s="84"/>
+      <c r="A822" s="76"/>
+      <c r="B822" s="77"/>
       <c r="C822" s="34"/>
       <c r="D822" s="34"/>
       <c r="E822" s="34"/>
@@ -54257,8 +54320,8 @@
       </c>
     </row>
     <row r="823">
-      <c r="A823" s="83"/>
-      <c r="B823" s="84"/>
+      <c r="A823" s="76"/>
+      <c r="B823" s="77"/>
       <c r="C823" s="34"/>
       <c r="D823" s="34"/>
       <c r="E823" s="34"/>
@@ -54283,8 +54346,8 @@
       </c>
     </row>
     <row r="824">
-      <c r="A824" s="83"/>
-      <c r="B824" s="84"/>
+      <c r="A824" s="76"/>
+      <c r="B824" s="77"/>
       <c r="C824" s="34"/>
       <c r="D824" s="34"/>
       <c r="E824" s="34"/>
@@ -54309,8 +54372,8 @@
       </c>
     </row>
     <row r="825">
-      <c r="A825" s="83"/>
-      <c r="B825" s="84"/>
+      <c r="A825" s="76"/>
+      <c r="B825" s="77"/>
       <c r="C825" s="34"/>
       <c r="D825" s="34"/>
       <c r="E825" s="34"/>
@@ -54335,8 +54398,8 @@
       </c>
     </row>
     <row r="826">
-      <c r="A826" s="83"/>
-      <c r="B826" s="84"/>
+      <c r="A826" s="76"/>
+      <c r="B826" s="77"/>
       <c r="C826" s="34"/>
       <c r="D826" s="34"/>
       <c r="E826" s="34"/>
@@ -54361,8 +54424,8 @@
       </c>
     </row>
     <row r="827">
-      <c r="A827" s="83"/>
-      <c r="B827" s="84"/>
+      <c r="A827" s="76"/>
+      <c r="B827" s="77"/>
       <c r="C827" s="34"/>
       <c r="D827" s="34"/>
       <c r="E827" s="34"/>
@@ -54387,8 +54450,8 @@
       </c>
     </row>
     <row r="828">
-      <c r="A828" s="83"/>
-      <c r="B828" s="84"/>
+      <c r="A828" s="76"/>
+      <c r="B828" s="77"/>
       <c r="C828" s="34"/>
       <c r="D828" s="34"/>
       <c r="E828" s="34"/>
@@ -54413,8 +54476,8 @@
       </c>
     </row>
     <row r="829">
-      <c r="A829" s="83"/>
-      <c r="B829" s="84"/>
+      <c r="A829" s="76"/>
+      <c r="B829" s="77"/>
       <c r="C829" s="34"/>
       <c r="D829" s="34"/>
       <c r="E829" s="34"/>
@@ -54439,8 +54502,8 @@
       </c>
     </row>
     <row r="830">
-      <c r="A830" s="83"/>
-      <c r="B830" s="84"/>
+      <c r="A830" s="76"/>
+      <c r="B830" s="77"/>
       <c r="C830" s="34"/>
       <c r="D830" s="34"/>
       <c r="E830" s="34"/>
@@ -54465,8 +54528,8 @@
       </c>
     </row>
     <row r="831">
-      <c r="A831" s="83"/>
-      <c r="B831" s="84"/>
+      <c r="A831" s="76"/>
+      <c r="B831" s="77"/>
       <c r="C831" s="34"/>
       <c r="D831" s="34"/>
       <c r="E831" s="34"/>
@@ -54491,8 +54554,8 @@
       </c>
     </row>
     <row r="832">
-      <c r="A832" s="83"/>
-      <c r="B832" s="84"/>
+      <c r="A832" s="76"/>
+      <c r="B832" s="77"/>
       <c r="C832" s="34"/>
       <c r="D832" s="34"/>
       <c r="E832" s="34"/>
@@ -54517,8 +54580,8 @@
       </c>
     </row>
     <row r="833">
-      <c r="A833" s="83"/>
-      <c r="B833" s="84"/>
+      <c r="A833" s="76"/>
+      <c r="B833" s="77"/>
       <c r="C833" s="34"/>
       <c r="D833" s="34"/>
       <c r="E833" s="34"/>
@@ -54543,8 +54606,8 @@
       </c>
     </row>
     <row r="834">
-      <c r="A834" s="83"/>
-      <c r="B834" s="84"/>
+      <c r="A834" s="76"/>
+      <c r="B834" s="77"/>
       <c r="C834" s="34"/>
       <c r="D834" s="34"/>
       <c r="E834" s="34"/>
@@ -54569,8 +54632,8 @@
       </c>
     </row>
     <row r="835">
-      <c r="A835" s="83"/>
-      <c r="B835" s="84"/>
+      <c r="A835" s="76"/>
+      <c r="B835" s="77"/>
       <c r="C835" s="34"/>
       <c r="D835" s="34"/>
       <c r="E835" s="34"/>
@@ -54595,8 +54658,8 @@
       </c>
     </row>
     <row r="836">
-      <c r="A836" s="83"/>
-      <c r="B836" s="84"/>
+      <c r="A836" s="76"/>
+      <c r="B836" s="77"/>
       <c r="C836" s="34"/>
       <c r="D836" s="34"/>
       <c r="E836" s="34"/>
@@ -54621,8 +54684,8 @@
       </c>
     </row>
     <row r="837">
-      <c r="A837" s="83"/>
-      <c r="B837" s="84"/>
+      <c r="A837" s="76"/>
+      <c r="B837" s="77"/>
       <c r="C837" s="34"/>
       <c r="D837" s="34"/>
       <c r="E837" s="34"/>
@@ -54647,8 +54710,8 @@
       </c>
     </row>
     <row r="838">
-      <c r="A838" s="83"/>
-      <c r="B838" s="84"/>
+      <c r="A838" s="76"/>
+      <c r="B838" s="77"/>
       <c r="C838" s="34"/>
       <c r="D838" s="34"/>
       <c r="E838" s="34"/>
@@ -54673,8 +54736,8 @@
       </c>
     </row>
     <row r="839">
-      <c r="A839" s="83"/>
-      <c r="B839" s="84"/>
+      <c r="A839" s="76"/>
+      <c r="B839" s="77"/>
       <c r="C839" s="34"/>
       <c r="D839" s="34"/>
       <c r="E839" s="34"/>
@@ -54699,8 +54762,8 @@
       </c>
     </row>
     <row r="840">
-      <c r="A840" s="83"/>
-      <c r="B840" s="84"/>
+      <c r="A840" s="76"/>
+      <c r="B840" s="77"/>
       <c r="C840" s="34"/>
       <c r="D840" s="34"/>
       <c r="E840" s="34"/>
@@ -54725,8 +54788,8 @@
       </c>
     </row>
     <row r="841">
-      <c r="A841" s="83"/>
-      <c r="B841" s="84"/>
+      <c r="A841" s="76"/>
+      <c r="B841" s="77"/>
       <c r="C841" s="34"/>
       <c r="D841" s="34"/>
       <c r="E841" s="34"/>
@@ -54751,8 +54814,8 @@
       </c>
     </row>
     <row r="842">
-      <c r="A842" s="83"/>
-      <c r="B842" s="84"/>
+      <c r="A842" s="76"/>
+      <c r="B842" s="77"/>
       <c r="C842" s="34"/>
       <c r="D842" s="34"/>
       <c r="E842" s="34"/>
@@ -54777,8 +54840,8 @@
       </c>
     </row>
     <row r="843">
-      <c r="A843" s="83"/>
-      <c r="B843" s="84"/>
+      <c r="A843" s="76"/>
+      <c r="B843" s="77"/>
       <c r="C843" s="34"/>
       <c r="D843" s="34"/>
       <c r="E843" s="34"/>
@@ -54803,8 +54866,8 @@
       </c>
     </row>
     <row r="844">
-      <c r="A844" s="83"/>
-      <c r="B844" s="84"/>
+      <c r="A844" s="76"/>
+      <c r="B844" s="77"/>
       <c r="C844" s="34"/>
       <c r="D844" s="34"/>
       <c r="E844" s="34"/>
@@ -54829,8 +54892,8 @@
       </c>
     </row>
     <row r="845">
-      <c r="A845" s="83"/>
-      <c r="B845" s="84"/>
+      <c r="A845" s="76"/>
+      <c r="B845" s="77"/>
       <c r="C845" s="34"/>
       <c r="D845" s="34"/>
       <c r="E845" s="34"/>
@@ -54855,8 +54918,8 @@
       </c>
     </row>
     <row r="846">
-      <c r="A846" s="83"/>
-      <c r="B846" s="84"/>
+      <c r="A846" s="76"/>
+      <c r="B846" s="77"/>
       <c r="C846" s="34"/>
       <c r="D846" s="34"/>
       <c r="E846" s="34"/>
@@ -54881,8 +54944,8 @@
       </c>
     </row>
     <row r="847">
-      <c r="A847" s="83"/>
-      <c r="B847" s="84"/>
+      <c r="A847" s="76"/>
+      <c r="B847" s="77"/>
       <c r="C847" s="34"/>
       <c r="D847" s="34"/>
       <c r="E847" s="34"/>
@@ -54907,8 +54970,8 @@
       </c>
     </row>
     <row r="848">
-      <c r="A848" s="83"/>
-      <c r="B848" s="84"/>
+      <c r="A848" s="76"/>
+      <c r="B848" s="77"/>
       <c r="C848" s="34"/>
       <c r="D848" s="34"/>
       <c r="E848" s="34"/>
@@ -54933,8 +54996,8 @@
       </c>
     </row>
     <row r="849">
-      <c r="A849" s="83"/>
-      <c r="B849" s="84"/>
+      <c r="A849" s="76"/>
+      <c r="B849" s="77"/>
       <c r="C849" s="34"/>
       <c r="D849" s="34"/>
       <c r="E849" s="34"/>
@@ -54959,8 +55022,8 @@
       </c>
     </row>
     <row r="850">
-      <c r="A850" s="83"/>
-      <c r="B850" s="84"/>
+      <c r="A850" s="76"/>
+      <c r="B850" s="77"/>
       <c r="C850" s="34"/>
       <c r="D850" s="34"/>
       <c r="E850" s="34"/>
@@ -54985,8 +55048,8 @@
       </c>
     </row>
     <row r="851">
-      <c r="A851" s="83"/>
-      <c r="B851" s="84"/>
+      <c r="A851" s="76"/>
+      <c r="B851" s="77"/>
       <c r="C851" s="34"/>
       <c r="D851" s="34"/>
       <c r="E851" s="34"/>
@@ -55011,8 +55074,8 @@
       </c>
     </row>
     <row r="852">
-      <c r="A852" s="83"/>
-      <c r="B852" s="84"/>
+      <c r="A852" s="76"/>
+      <c r="B852" s="77"/>
       <c r="C852" s="34"/>
       <c r="D852" s="34"/>
       <c r="E852" s="34"/>
@@ -55037,8 +55100,8 @@
       </c>
     </row>
     <row r="853">
-      <c r="A853" s="83"/>
-      <c r="B853" s="84"/>
+      <c r="A853" s="76"/>
+      <c r="B853" s="77"/>
       <c r="C853" s="34"/>
       <c r="D853" s="34"/>
       <c r="E853" s="34"/>
@@ -55063,8 +55126,8 @@
       </c>
     </row>
     <row r="854">
-      <c r="A854" s="83"/>
-      <c r="B854" s="84"/>
+      <c r="A854" s="76"/>
+      <c r="B854" s="77"/>
       <c r="C854" s="34"/>
       <c r="D854" s="34"/>
       <c r="E854" s="34"/>
@@ -55089,8 +55152,8 @@
       </c>
     </row>
     <row r="855">
-      <c r="A855" s="83"/>
-      <c r="B855" s="84"/>
+      <c r="A855" s="76"/>
+      <c r="B855" s="77"/>
       <c r="C855" s="34"/>
       <c r="D855" s="34"/>
       <c r="E855" s="34"/>
@@ -55115,8 +55178,8 @@
       </c>
     </row>
     <row r="856">
-      <c r="A856" s="83"/>
-      <c r="B856" s="84"/>
+      <c r="A856" s="76"/>
+      <c r="B856" s="77"/>
       <c r="C856" s="34"/>
       <c r="D856" s="34"/>
       <c r="E856" s="34"/>
@@ -55141,8 +55204,8 @@
       </c>
     </row>
     <row r="857">
-      <c r="A857" s="83"/>
-      <c r="B857" s="84"/>
+      <c r="A857" s="76"/>
+      <c r="B857" s="77"/>
       <c r="C857" s="34"/>
       <c r="D857" s="34"/>
       <c r="E857" s="34"/>
@@ -55167,8 +55230,8 @@
       </c>
     </row>
     <row r="858">
-      <c r="A858" s="83"/>
-      <c r="B858" s="84"/>
+      <c r="A858" s="76"/>
+      <c r="B858" s="77"/>
       <c r="C858" s="34"/>
       <c r="D858" s="34"/>
       <c r="E858" s="34"/>
@@ -55193,8 +55256,8 @@
       </c>
     </row>
     <row r="859">
-      <c r="A859" s="83"/>
-      <c r="B859" s="84"/>
+      <c r="A859" s="76"/>
+      <c r="B859" s="77"/>
       <c r="C859" s="34"/>
       <c r="D859" s="34"/>
       <c r="E859" s="34"/>
@@ -55219,8 +55282,8 @@
       </c>
     </row>
     <row r="860">
-      <c r="A860" s="83"/>
-      <c r="B860" s="84"/>
+      <c r="A860" s="76"/>
+      <c r="B860" s="77"/>
       <c r="C860" s="34"/>
       <c r="D860" s="34"/>
       <c r="E860" s="34"/>
@@ -55245,8 +55308,8 @@
       </c>
     </row>
     <row r="861">
-      <c r="A861" s="83"/>
-      <c r="B861" s="84"/>
+      <c r="A861" s="76"/>
+      <c r="B861" s="77"/>
       <c r="C861" s="34"/>
       <c r="D861" s="34"/>
       <c r="E861" s="34"/>
@@ -55271,8 +55334,8 @@
       </c>
     </row>
     <row r="862">
-      <c r="A862" s="83"/>
-      <c r="B862" s="84"/>
+      <c r="A862" s="76"/>
+      <c r="B862" s="77"/>
       <c r="C862" s="34"/>
       <c r="D862" s="34"/>
       <c r="E862" s="34"/>
@@ -55297,8 +55360,8 @@
       </c>
     </row>
     <row r="863">
-      <c r="A863" s="83"/>
-      <c r="B863" s="84"/>
+      <c r="A863" s="76"/>
+      <c r="B863" s="77"/>
       <c r="C863" s="34"/>
       <c r="D863" s="34"/>
       <c r="E863" s="34"/>
@@ -55323,8 +55386,8 @@
       </c>
     </row>
     <row r="864">
-      <c r="A864" s="83"/>
-      <c r="B864" s="84"/>
+      <c r="A864" s="76"/>
+      <c r="B864" s="77"/>
       <c r="C864" s="34"/>
       <c r="D864" s="34"/>
       <c r="E864" s="34"/>
@@ -55349,8 +55412,8 @@
       </c>
     </row>
     <row r="865">
-      <c r="A865" s="83"/>
-      <c r="B865" s="84"/>
+      <c r="A865" s="76"/>
+      <c r="B865" s="77"/>
       <c r="C865" s="34"/>
       <c r="D865" s="34"/>
       <c r="E865" s="34"/>
@@ -55375,8 +55438,8 @@
       </c>
     </row>
     <row r="866">
-      <c r="A866" s="83"/>
-      <c r="B866" s="84"/>
+      <c r="A866" s="76"/>
+      <c r="B866" s="77"/>
       <c r="C866" s="34"/>
       <c r="D866" s="34"/>
       <c r="E866" s="34"/>
@@ -55401,8 +55464,8 @@
       </c>
     </row>
     <row r="867">
-      <c r="A867" s="83"/>
-      <c r="B867" s="84"/>
+      <c r="A867" s="76"/>
+      <c r="B867" s="77"/>
       <c r="C867" s="34"/>
       <c r="D867" s="34"/>
       <c r="E867" s="34"/>
@@ -55427,8 +55490,8 @@
       </c>
     </row>
     <row r="868">
-      <c r="A868" s="83"/>
-      <c r="B868" s="84"/>
+      <c r="A868" s="76"/>
+      <c r="B868" s="77"/>
       <c r="C868" s="34"/>
       <c r="D868" s="34"/>
       <c r="E868" s="34"/>
@@ -55453,8 +55516,8 @@
       </c>
     </row>
     <row r="869">
-      <c r="A869" s="83"/>
-      <c r="B869" s="84"/>
+      <c r="A869" s="76"/>
+      <c r="B869" s="77"/>
       <c r="C869" s="34"/>
       <c r="D869" s="34"/>
       <c r="E869" s="34"/>
@@ -55479,8 +55542,8 @@
       </c>
     </row>
     <row r="870">
-      <c r="A870" s="83"/>
-      <c r="B870" s="84"/>
+      <c r="A870" s="76"/>
+      <c r="B870" s="77"/>
       <c r="C870" s="34"/>
       <c r="D870" s="34"/>
       <c r="E870" s="34"/>
@@ -55505,8 +55568,8 @@
       </c>
     </row>
     <row r="871">
-      <c r="A871" s="83"/>
-      <c r="B871" s="84"/>
+      <c r="A871" s="76"/>
+      <c r="B871" s="77"/>
       <c r="C871" s="34"/>
       <c r="D871" s="34"/>
       <c r="E871" s="34"/>
@@ -55531,8 +55594,8 @@
       </c>
     </row>
     <row r="872">
-      <c r="A872" s="83"/>
-      <c r="B872" s="84"/>
+      <c r="A872" s="76"/>
+      <c r="B872" s="77"/>
       <c r="C872" s="34"/>
       <c r="D872" s="34"/>
       <c r="E872" s="34"/>
@@ -55557,8 +55620,8 @@
       </c>
     </row>
     <row r="873">
-      <c r="A873" s="83"/>
-      <c r="B873" s="84"/>
+      <c r="A873" s="76"/>
+      <c r="B873" s="77"/>
       <c r="C873" s="34"/>
       <c r="D873" s="34"/>
       <c r="E873" s="34"/>
@@ -55583,8 +55646,8 @@
       </c>
     </row>
     <row r="874">
-      <c r="A874" s="83"/>
-      <c r="B874" s="84"/>
+      <c r="A874" s="76"/>
+      <c r="B874" s="77"/>
       <c r="C874" s="34"/>
       <c r="D874" s="34"/>
       <c r="E874" s="34"/>
@@ -55609,8 +55672,8 @@
       </c>
     </row>
     <row r="875">
-      <c r="A875" s="83"/>
-      <c r="B875" s="84"/>
+      <c r="A875" s="76"/>
+      <c r="B875" s="77"/>
       <c r="C875" s="34"/>
       <c r="D875" s="34"/>
       <c r="E875" s="34"/>
@@ -55635,8 +55698,8 @@
       </c>
     </row>
     <row r="876">
-      <c r="A876" s="83"/>
-      <c r="B876" s="84"/>
+      <c r="A876" s="76"/>
+      <c r="B876" s="77"/>
       <c r="C876" s="34"/>
       <c r="D876" s="34"/>
       <c r="E876" s="34"/>
@@ -55661,8 +55724,8 @@
       </c>
     </row>
     <row r="877">
-      <c r="A877" s="83"/>
-      <c r="B877" s="84"/>
+      <c r="A877" s="76"/>
+      <c r="B877" s="77"/>
       <c r="C877" s="34"/>
       <c r="D877" s="34"/>
       <c r="E877" s="34"/>
@@ -55687,8 +55750,8 @@
       </c>
     </row>
     <row r="878">
-      <c r="A878" s="83"/>
-      <c r="B878" s="84"/>
+      <c r="A878" s="76"/>
+      <c r="B878" s="77"/>
       <c r="C878" s="34"/>
       <c r="D878" s="34"/>
       <c r="E878" s="34"/>
@@ -55713,8 +55776,8 @@
       </c>
     </row>
     <row r="879">
-      <c r="A879" s="83"/>
-      <c r="B879" s="84"/>
+      <c r="A879" s="76"/>
+      <c r="B879" s="77"/>
       <c r="C879" s="34"/>
       <c r="D879" s="34"/>
       <c r="E879" s="34"/>
@@ -55739,8 +55802,8 @@
       </c>
     </row>
     <row r="880">
-      <c r="A880" s="83"/>
-      <c r="B880" s="84"/>
+      <c r="A880" s="76"/>
+      <c r="B880" s="77"/>
       <c r="C880" s="34"/>
       <c r="D880" s="34"/>
       <c r="E880" s="34"/>
@@ -55765,8 +55828,8 @@
       </c>
     </row>
     <row r="881">
-      <c r="A881" s="83"/>
-      <c r="B881" s="84"/>
+      <c r="A881" s="76"/>
+      <c r="B881" s="77"/>
       <c r="C881" s="34"/>
       <c r="D881" s="34"/>
       <c r="E881" s="34"/>
@@ -55791,8 +55854,8 @@
       </c>
     </row>
     <row r="882">
-      <c r="A882" s="83"/>
-      <c r="B882" s="84"/>
+      <c r="A882" s="76"/>
+      <c r="B882" s="77"/>
       <c r="C882" s="34"/>
       <c r="D882" s="34"/>
       <c r="E882" s="34"/>
@@ -55817,8 +55880,8 @@
       </c>
     </row>
     <row r="883">
-      <c r="A883" s="83"/>
-      <c r="B883" s="84"/>
+      <c r="A883" s="76"/>
+      <c r="B883" s="77"/>
       <c r="C883" s="34"/>
       <c r="D883" s="34"/>
       <c r="E883" s="34"/>
@@ -55843,8 +55906,8 @@
       </c>
     </row>
     <row r="884">
-      <c r="A884" s="83"/>
-      <c r="B884" s="84"/>
+      <c r="A884" s="76"/>
+      <c r="B884" s="77"/>
       <c r="C884" s="34"/>
       <c r="D884" s="34"/>
       <c r="E884" s="34"/>
@@ -55869,8 +55932,8 @@
       </c>
     </row>
     <row r="885">
-      <c r="A885" s="83"/>
-      <c r="B885" s="84"/>
+      <c r="A885" s="76"/>
+      <c r="B885" s="77"/>
       <c r="C885" s="34"/>
       <c r="D885" s="34"/>
       <c r="E885" s="34"/>
@@ -55895,8 +55958,8 @@
       </c>
     </row>
     <row r="886">
-      <c r="A886" s="83"/>
-      <c r="B886" s="84"/>
+      <c r="A886" s="76"/>
+      <c r="B886" s="77"/>
       <c r="C886" s="34"/>
       <c r="D886" s="34"/>
       <c r="E886" s="34"/>
@@ -55921,8 +55984,8 @@
       </c>
     </row>
     <row r="887">
-      <c r="A887" s="83"/>
-      <c r="B887" s="84"/>
+      <c r="A887" s="76"/>
+      <c r="B887" s="77"/>
       <c r="C887" s="34"/>
       <c r="D887" s="34"/>
       <c r="E887" s="34"/>
@@ -55947,8 +56010,8 @@
       </c>
     </row>
     <row r="888">
-      <c r="A888" s="83"/>
-      <c r="B888" s="84"/>
+      <c r="A888" s="76"/>
+      <c r="B888" s="77"/>
       <c r="C888" s="34"/>
       <c r="D888" s="34"/>
       <c r="E888" s="34"/>
@@ -55973,8 +56036,8 @@
       </c>
     </row>
     <row r="889">
-      <c r="A889" s="83"/>
-      <c r="B889" s="84"/>
+      <c r="A889" s="76"/>
+      <c r="B889" s="77"/>
       <c r="C889" s="34"/>
       <c r="D889" s="34"/>
       <c r="E889" s="34"/>
@@ -55999,8 +56062,8 @@
       </c>
     </row>
     <row r="890">
-      <c r="A890" s="83"/>
-      <c r="B890" s="84"/>
+      <c r="A890" s="76"/>
+      <c r="B890" s="77"/>
       <c r="C890" s="34"/>
       <c r="D890" s="34"/>
       <c r="E890" s="34"/>
@@ -56025,8 +56088,8 @@
       </c>
     </row>
     <row r="891">
-      <c r="A891" s="83"/>
-      <c r="B891" s="84"/>
+      <c r="A891" s="76"/>
+      <c r="B891" s="77"/>
       <c r="C891" s="34"/>
       <c r="D891" s="34"/>
       <c r="E891" s="34"/>
@@ -56051,8 +56114,8 @@
       </c>
     </row>
     <row r="892">
-      <c r="A892" s="83"/>
-      <c r="B892" s="84"/>
+      <c r="A892" s="76"/>
+      <c r="B892" s="77"/>
       <c r="C892" s="34"/>
       <c r="D892" s="34"/>
       <c r="E892" s="34"/>
@@ -56077,8 +56140,8 @@
       </c>
     </row>
     <row r="893">
-      <c r="A893" s="83"/>
-      <c r="B893" s="84"/>
+      <c r="A893" s="76"/>
+      <c r="B893" s="77"/>
       <c r="C893" s="34"/>
       <c r="D893" s="34"/>
       <c r="E893" s="34"/>
@@ -56103,8 +56166,8 @@
       </c>
     </row>
     <row r="894">
-      <c r="A894" s="83"/>
-      <c r="B894" s="84"/>
+      <c r="A894" s="76"/>
+      <c r="B894" s="77"/>
       <c r="C894" s="34"/>
       <c r="D894" s="34"/>
       <c r="E894" s="34"/>
@@ -56129,8 +56192,8 @@
       </c>
     </row>
     <row r="895">
-      <c r="A895" s="83"/>
-      <c r="B895" s="84"/>
+      <c r="A895" s="76"/>
+      <c r="B895" s="77"/>
       <c r="C895" s="34"/>
       <c r="D895" s="34"/>
       <c r="E895" s="34"/>
@@ -56155,8 +56218,8 @@
       </c>
     </row>
     <row r="896">
-      <c r="A896" s="83"/>
-      <c r="B896" s="84"/>
+      <c r="A896" s="76"/>
+      <c r="B896" s="77"/>
       <c r="C896" s="34"/>
       <c r="D896" s="34"/>
       <c r="E896" s="34"/>
@@ -56181,8 +56244,8 @@
       </c>
     </row>
     <row r="897">
-      <c r="A897" s="83"/>
-      <c r="B897" s="84"/>
+      <c r="A897" s="76"/>
+      <c r="B897" s="77"/>
       <c r="C897" s="34"/>
       <c r="D897" s="34"/>
       <c r="E897" s="34"/>
@@ -56207,8 +56270,8 @@
       </c>
     </row>
     <row r="898">
-      <c r="A898" s="83"/>
-      <c r="B898" s="84"/>
+      <c r="A898" s="76"/>
+      <c r="B898" s="77"/>
       <c r="C898" s="34"/>
       <c r="D898" s="34"/>
       <c r="E898" s="34"/>
@@ -56233,8 +56296,8 @@
       </c>
     </row>
     <row r="899">
-      <c r="A899" s="83"/>
-      <c r="B899" s="84"/>
+      <c r="A899" s="76"/>
+      <c r="B899" s="77"/>
       <c r="C899" s="34"/>
       <c r="D899" s="34"/>
       <c r="E899" s="34"/>
@@ -56259,8 +56322,8 @@
       </c>
     </row>
     <row r="900">
-      <c r="A900" s="83"/>
-      <c r="B900" s="84"/>
+      <c r="A900" s="76"/>
+      <c r="B900" s="77"/>
       <c r="C900" s="34"/>
       <c r="D900" s="34"/>
       <c r="E900" s="34"/>
@@ -56285,8 +56348,8 @@
       </c>
     </row>
     <row r="901">
-      <c r="A901" s="83"/>
-      <c r="B901" s="84"/>
+      <c r="A901" s="76"/>
+      <c r="B901" s="77"/>
       <c r="C901" s="34"/>
       <c r="D901" s="34"/>
       <c r="E901" s="34"/>
@@ -56311,8 +56374,8 @@
       </c>
     </row>
     <row r="902">
-      <c r="A902" s="83"/>
-      <c r="B902" s="84"/>
+      <c r="A902" s="76"/>
+      <c r="B902" s="77"/>
       <c r="C902" s="34"/>
       <c r="D902" s="34"/>
       <c r="E902" s="34"/>
@@ -56337,8 +56400,8 @@
       </c>
     </row>
     <row r="903">
-      <c r="A903" s="83"/>
-      <c r="B903" s="84"/>
+      <c r="A903" s="76"/>
+      <c r="B903" s="77"/>
       <c r="C903" s="34"/>
       <c r="D903" s="34"/>
       <c r="E903" s="34"/>
@@ -56363,8 +56426,8 @@
       </c>
     </row>
     <row r="904">
-      <c r="A904" s="83"/>
-      <c r="B904" s="84"/>
+      <c r="A904" s="76"/>
+      <c r="B904" s="77"/>
       <c r="C904" s="34"/>
       <c r="D904" s="34"/>
       <c r="E904" s="34"/>
@@ -56389,8 +56452,8 @@
       </c>
     </row>
     <row r="905">
-      <c r="A905" s="83"/>
-      <c r="B905" s="84"/>
+      <c r="A905" s="76"/>
+      <c r="B905" s="77"/>
       <c r="C905" s="34"/>
       <c r="D905" s="34"/>
       <c r="E905" s="34"/>
@@ -56415,8 +56478,8 @@
       </c>
     </row>
     <row r="906">
-      <c r="A906" s="83"/>
-      <c r="B906" s="84"/>
+      <c r="A906" s="76"/>
+      <c r="B906" s="77"/>
       <c r="C906" s="34"/>
       <c r="D906" s="34"/>
       <c r="E906" s="34"/>
@@ -56441,8 +56504,8 @@
       </c>
     </row>
     <row r="907">
-      <c r="A907" s="83"/>
-      <c r="B907" s="84"/>
+      <c r="A907" s="76"/>
+      <c r="B907" s="77"/>
       <c r="C907" s="34"/>
       <c r="D907" s="34"/>
       <c r="E907" s="34"/>
@@ -56467,8 +56530,8 @@
       </c>
     </row>
     <row r="908">
-      <c r="A908" s="83"/>
-      <c r="B908" s="84"/>
+      <c r="A908" s="76"/>
+      <c r="B908" s="77"/>
       <c r="C908" s="34"/>
       <c r="D908" s="34"/>
       <c r="E908" s="34"/>
@@ -56493,8 +56556,8 @@
       </c>
     </row>
     <row r="909">
-      <c r="A909" s="83"/>
-      <c r="B909" s="84"/>
+      <c r="A909" s="76"/>
+      <c r="B909" s="77"/>
       <c r="C909" s="34"/>
       <c r="D909" s="34"/>
       <c r="E909" s="34"/>
@@ -56519,8 +56582,8 @@
       </c>
     </row>
     <row r="910">
-      <c r="A910" s="83"/>
-      <c r="B910" s="84"/>
+      <c r="A910" s="76"/>
+      <c r="B910" s="77"/>
       <c r="C910" s="34"/>
       <c r="D910" s="34"/>
       <c r="E910" s="34"/>
@@ -56545,8 +56608,8 @@
       </c>
     </row>
     <row r="911">
-      <c r="A911" s="83"/>
-      <c r="B911" s="84"/>
+      <c r="A911" s="76"/>
+      <c r="B911" s="77"/>
       <c r="C911" s="34"/>
       <c r="D911" s="34"/>
       <c r="E911" s="34"/>
@@ -56571,8 +56634,8 @@
       </c>
     </row>
     <row r="912">
-      <c r="A912" s="83"/>
-      <c r="B912" s="84"/>
+      <c r="A912" s="76"/>
+      <c r="B912" s="77"/>
       <c r="C912" s="34"/>
       <c r="D912" s="34"/>
       <c r="E912" s="34"/>
@@ -56597,8 +56660,8 @@
       </c>
     </row>
     <row r="913">
-      <c r="A913" s="83"/>
-      <c r="B913" s="84"/>
+      <c r="A913" s="76"/>
+      <c r="B913" s="77"/>
       <c r="C913" s="34"/>
       <c r="D913" s="34"/>
       <c r="E913" s="34"/>
@@ -56623,8 +56686,8 @@
       </c>
     </row>
     <row r="914">
-      <c r="A914" s="83"/>
-      <c r="B914" s="84"/>
+      <c r="A914" s="76"/>
+      <c r="B914" s="77"/>
       <c r="C914" s="34"/>
       <c r="D914" s="34"/>
       <c r="E914" s="34"/>
@@ -56649,8 +56712,8 @@
       </c>
     </row>
     <row r="915">
-      <c r="A915" s="83"/>
-      <c r="B915" s="84"/>
+      <c r="A915" s="76"/>
+      <c r="B915" s="77"/>
       <c r="C915" s="34"/>
       <c r="D915" s="34"/>
       <c r="E915" s="34"/>
@@ -56675,8 +56738,8 @@
       </c>
     </row>
     <row r="916">
-      <c r="A916" s="83"/>
-      <c r="B916" s="84"/>
+      <c r="A916" s="76"/>
+      <c r="B916" s="77"/>
       <c r="C916" s="34"/>
       <c r="D916" s="34"/>
       <c r="E916" s="34"/>
@@ -56701,8 +56764,8 @@
       </c>
     </row>
     <row r="917">
-      <c r="A917" s="83"/>
-      <c r="B917" s="84"/>
+      <c r="A917" s="76"/>
+      <c r="B917" s="77"/>
       <c r="C917" s="34"/>
       <c r="D917" s="34"/>
       <c r="E917" s="34"/>
@@ -56727,8 +56790,8 @@
       </c>
     </row>
     <row r="918">
-      <c r="A918" s="83"/>
-      <c r="B918" s="84"/>
+      <c r="A918" s="76"/>
+      <c r="B918" s="77"/>
       <c r="C918" s="34"/>
       <c r="D918" s="34"/>
       <c r="E918" s="34"/>
@@ -56753,8 +56816,8 @@
       </c>
     </row>
     <row r="919">
-      <c r="A919" s="83"/>
-      <c r="B919" s="84"/>
+      <c r="A919" s="76"/>
+      <c r="B919" s="77"/>
       <c r="C919" s="34"/>
       <c r="D919" s="34"/>
       <c r="E919" s="34"/>
@@ -56779,8 +56842,8 @@
       </c>
     </row>
     <row r="920">
-      <c r="A920" s="83"/>
-      <c r="B920" s="84"/>
+      <c r="A920" s="76"/>
+      <c r="B920" s="77"/>
       <c r="C920" s="34"/>
       <c r="D920" s="34"/>
       <c r="E920" s="34"/>
@@ -56805,8 +56868,8 @@
       </c>
     </row>
     <row r="921">
-      <c r="A921" s="83"/>
-      <c r="B921" s="84"/>
+      <c r="A921" s="76"/>
+      <c r="B921" s="77"/>
       <c r="C921" s="34"/>
       <c r="D921" s="34"/>
       <c r="E921" s="34"/>
@@ -56831,8 +56894,8 @@
       </c>
     </row>
     <row r="922">
-      <c r="A922" s="83"/>
-      <c r="B922" s="84"/>
+      <c r="A922" s="76"/>
+      <c r="B922" s="77"/>
       <c r="C922" s="34"/>
       <c r="D922" s="34"/>
       <c r="E922" s="34"/>
@@ -56857,8 +56920,8 @@
       </c>
     </row>
     <row r="923">
-      <c r="A923" s="83"/>
-      <c r="B923" s="84"/>
+      <c r="A923" s="76"/>
+      <c r="B923" s="77"/>
       <c r="C923" s="34"/>
       <c r="D923" s="34"/>
       <c r="E923" s="34"/>
@@ -56883,8 +56946,8 @@
       </c>
     </row>
     <row r="924">
-      <c r="A924" s="83"/>
-      <c r="B924" s="84"/>
+      <c r="A924" s="76"/>
+      <c r="B924" s="77"/>
       <c r="C924" s="34"/>
       <c r="D924" s="34"/>
       <c r="E924" s="34"/>
@@ -56909,8 +56972,8 @@
       </c>
     </row>
     <row r="925">
-      <c r="A925" s="83"/>
-      <c r="B925" s="84"/>
+      <c r="A925" s="76"/>
+      <c r="B925" s="77"/>
       <c r="C925" s="34"/>
       <c r="D925" s="34"/>
       <c r="E925" s="34"/>
@@ -56935,8 +56998,8 @@
       </c>
     </row>
     <row r="926">
-      <c r="A926" s="83"/>
-      <c r="B926" s="84"/>
+      <c r="A926" s="76"/>
+      <c r="B926" s="77"/>
       <c r="C926" s="34"/>
       <c r="D926" s="34"/>
       <c r="E926" s="34"/>
@@ -56961,8 +57024,8 @@
       </c>
     </row>
     <row r="927">
-      <c r="A927" s="83"/>
-      <c r="B927" s="84"/>
+      <c r="A927" s="76"/>
+      <c r="B927" s="77"/>
       <c r="C927" s="34"/>
       <c r="D927" s="34"/>
       <c r="E927" s="34"/>
@@ -56987,8 +57050,8 @@
       </c>
     </row>
     <row r="928">
-      <c r="A928" s="83"/>
-      <c r="B928" s="84"/>
+      <c r="A928" s="76"/>
+      <c r="B928" s="77"/>
       <c r="C928" s="34"/>
       <c r="D928" s="34"/>
       <c r="E928" s="34"/>
@@ -57013,8 +57076,8 @@
       </c>
     </row>
     <row r="929">
-      <c r="A929" s="83"/>
-      <c r="B929" s="84"/>
+      <c r="A929" s="76"/>
+      <c r="B929" s="77"/>
       <c r="C929" s="34"/>
       <c r="D929" s="34"/>
       <c r="E929" s="34"/>
@@ -57039,8 +57102,8 @@
       </c>
     </row>
     <row r="930">
-      <c r="A930" s="83"/>
-      <c r="B930" s="84"/>
+      <c r="A930" s="76"/>
+      <c r="B930" s="77"/>
       <c r="C930" s="34"/>
       <c r="D930" s="34"/>
       <c r="E930" s="34"/>
@@ -57065,8 +57128,8 @@
       </c>
     </row>
     <row r="931">
-      <c r="A931" s="83"/>
-      <c r="B931" s="84"/>
+      <c r="A931" s="76"/>
+      <c r="B931" s="77"/>
       <c r="C931" s="34"/>
       <c r="D931" s="34"/>
       <c r="E931" s="34"/>
@@ -57091,8 +57154,8 @@
       </c>
     </row>
     <row r="932">
-      <c r="A932" s="83"/>
-      <c r="B932" s="84"/>
+      <c r="A932" s="76"/>
+      <c r="B932" s="77"/>
       <c r="C932" s="34"/>
       <c r="D932" s="34"/>
       <c r="E932" s="34"/>
@@ -57117,8 +57180,8 @@
       </c>
     </row>
     <row r="933">
-      <c r="A933" s="83"/>
-      <c r="B933" s="84"/>
+      <c r="A933" s="76"/>
+      <c r="B933" s="77"/>
       <c r="C933" s="34"/>
       <c r="D933" s="34"/>
       <c r="E933" s="34"/>
@@ -57143,8 +57206,8 @@
       </c>
     </row>
     <row r="934">
-      <c r="A934" s="83"/>
-      <c r="B934" s="84"/>
+      <c r="A934" s="76"/>
+      <c r="B934" s="77"/>
       <c r="C934" s="34"/>
       <c r="D934" s="34"/>
       <c r="E934" s="34"/>
@@ -57169,8 +57232,8 @@
       </c>
     </row>
     <row r="935">
-      <c r="A935" s="83"/>
-      <c r="B935" s="84"/>
+      <c r="A935" s="76"/>
+      <c r="B935" s="77"/>
       <c r="C935" s="34"/>
       <c r="D935" s="34"/>
       <c r="E935" s="34"/>
@@ -57195,8 +57258,8 @@
       </c>
     </row>
     <row r="936">
-      <c r="A936" s="83"/>
-      <c r="B936" s="84"/>
+      <c r="A936" s="76"/>
+      <c r="B936" s="77"/>
       <c r="C936" s="34"/>
       <c r="D936" s="34"/>
       <c r="E936" s="34"/>
@@ -57221,8 +57284,8 @@
       </c>
     </row>
     <row r="937">
-      <c r="A937" s="83"/>
-      <c r="B937" s="84"/>
+      <c r="A937" s="76"/>
+      <c r="B937" s="77"/>
       <c r="C937" s="34"/>
       <c r="D937" s="34"/>
       <c r="E937" s="34"/>
@@ -57247,8 +57310,8 @@
       </c>
     </row>
     <row r="938">
-      <c r="A938" s="83"/>
-      <c r="B938" s="84"/>
+      <c r="A938" s="76"/>
+      <c r="B938" s="77"/>
       <c r="C938" s="34"/>
       <c r="D938" s="34"/>
       <c r="E938" s="34"/>
@@ -57273,8 +57336,8 @@
       </c>
     </row>
     <row r="939">
-      <c r="A939" s="83"/>
-      <c r="B939" s="84"/>
+      <c r="A939" s="76"/>
+      <c r="B939" s="77"/>
       <c r="C939" s="34"/>
       <c r="D939" s="34"/>
       <c r="E939" s="34"/>
@@ -57299,8 +57362,8 @@
       </c>
     </row>
     <row r="940">
-      <c r="A940" s="83"/>
-      <c r="B940" s="84"/>
+      <c r="A940" s="76"/>
+      <c r="B940" s="77"/>
       <c r="C940" s="34"/>
       <c r="D940" s="34"/>
       <c r="E940" s="34"/>
@@ -57325,8 +57388,8 @@
       </c>
     </row>
     <row r="941">
-      <c r="A941" s="83"/>
-      <c r="B941" s="84"/>
+      <c r="A941" s="76"/>
+      <c r="B941" s="77"/>
       <c r="C941" s="34"/>
       <c r="D941" s="34"/>
       <c r="E941" s="34"/>
@@ -57351,8 +57414,8 @@
       </c>
     </row>
     <row r="942">
-      <c r="A942" s="83"/>
-      <c r="B942" s="84"/>
+      <c r="A942" s="76"/>
+      <c r="B942" s="77"/>
       <c r="C942" s="34"/>
       <c r="D942" s="34"/>
       <c r="E942" s="34"/>
@@ -57377,8 +57440,8 @@
       </c>
     </row>
     <row r="943">
-      <c r="A943" s="83"/>
-      <c r="B943" s="84"/>
+      <c r="A943" s="76"/>
+      <c r="B943" s="77"/>
       <c r="C943" s="34"/>
       <c r="D943" s="34"/>
       <c r="E943" s="34"/>
@@ -57403,8 +57466,8 @@
       </c>
     </row>
     <row r="944">
-      <c r="A944" s="83"/>
-      <c r="B944" s="84"/>
+      <c r="A944" s="76"/>
+      <c r="B944" s="77"/>
       <c r="C944" s="34"/>
       <c r="D944" s="34"/>
       <c r="E944" s="34"/>
@@ -57429,8 +57492,8 @@
       </c>
     </row>
     <row r="945">
-      <c r="A945" s="83"/>
-      <c r="B945" s="84"/>
+      <c r="A945" s="76"/>
+      <c r="B945" s="77"/>
       <c r="C945" s="34"/>
       <c r="D945" s="34"/>
       <c r="E945" s="34"/>
@@ -57455,8 +57518,8 @@
       </c>
     </row>
     <row r="946">
-      <c r="A946" s="83"/>
-      <c r="B946" s="84"/>
+      <c r="A946" s="76"/>
+      <c r="B946" s="77"/>
       <c r="C946" s="34"/>
       <c r="D946" s="34"/>
       <c r="E946" s="34"/>
@@ -57481,8 +57544,8 @@
       </c>
     </row>
     <row r="947">
-      <c r="A947" s="83"/>
-      <c r="B947" s="84"/>
+      <c r="A947" s="76"/>
+      <c r="B947" s="77"/>
       <c r="C947" s="34"/>
       <c r="D947" s="34"/>
       <c r="E947" s="34"/>
@@ -57507,8 +57570,8 @@
       </c>
     </row>
     <row r="948">
-      <c r="A948" s="83"/>
-      <c r="B948" s="84"/>
+      <c r="A948" s="76"/>
+      <c r="B948" s="77"/>
       <c r="C948" s="34"/>
       <c r="D948" s="34"/>
       <c r="E948" s="34"/>
@@ -57533,8 +57596,8 @@
       </c>
     </row>
     <row r="949">
-      <c r="A949" s="83"/>
-      <c r="B949" s="84"/>
+      <c r="A949" s="76"/>
+      <c r="B949" s="77"/>
       <c r="C949" s="34"/>
       <c r="D949" s="34"/>
       <c r="E949" s="34"/>
@@ -57559,8 +57622,8 @@
       </c>
     </row>
     <row r="950">
-      <c r="A950" s="83"/>
-      <c r="B950" s="84"/>
+      <c r="A950" s="76"/>
+      <c r="B950" s="77"/>
       <c r="C950" s="34"/>
       <c r="D950" s="34"/>
       <c r="E950" s="34"/>
@@ -57585,8 +57648,8 @@
       </c>
     </row>
     <row r="951">
-      <c r="A951" s="83"/>
-      <c r="B951" s="84"/>
+      <c r="A951" s="76"/>
+      <c r="B951" s="77"/>
       <c r="C951" s="34"/>
       <c r="D951" s="34"/>
       <c r="E951" s="34"/>
@@ -57611,8 +57674,8 @@
       </c>
     </row>
     <row r="952">
-      <c r="A952" s="83"/>
-      <c r="B952" s="84"/>
+      <c r="A952" s="76"/>
+      <c r="B952" s="77"/>
       <c r="C952" s="34"/>
       <c r="D952" s="34"/>
       <c r="E952" s="34"/>
@@ -57637,8 +57700,8 @@
       </c>
     </row>
     <row r="953">
-      <c r="A953" s="83"/>
-      <c r="B953" s="84"/>
+      <c r="A953" s="76"/>
+      <c r="B953" s="77"/>
       <c r="C953" s="34"/>
       <c r="D953" s="34"/>
       <c r="E953" s="34"/>
@@ -57663,8 +57726,8 @@
       </c>
     </row>
     <row r="954">
-      <c r="A954" s="83"/>
-      <c r="B954" s="84"/>
+      <c r="A954" s="76"/>
+      <c r="B954" s="77"/>
       <c r="C954" s="34"/>
       <c r="D954" s="34"/>
       <c r="E954" s="34"/>
@@ -57689,8 +57752,8 @@
       </c>
     </row>
     <row r="955">
-      <c r="A955" s="83"/>
-      <c r="B955" s="84"/>
+      <c r="A955" s="76"/>
+      <c r="B955" s="77"/>
       <c r="C955" s="34"/>
       <c r="D955" s="34"/>
       <c r="E955" s="34"/>
@@ -57715,8 +57778,8 @@
       </c>
     </row>
     <row r="956">
-      <c r="A956" s="83"/>
-      <c r="B956" s="84"/>
+      <c r="A956" s="76"/>
+      <c r="B956" s="77"/>
       <c r="C956" s="34"/>
       <c r="D956" s="34"/>
       <c r="E956" s="34"/>
@@ -57741,8 +57804,8 @@
       </c>
     </row>
     <row r="957">
-      <c r="A957" s="83"/>
-      <c r="B957" s="84"/>
+      <c r="A957" s="76"/>
+      <c r="B957" s="77"/>
       <c r="C957" s="34"/>
       <c r="D957" s="34"/>
       <c r="E957" s="34"/>
@@ -57767,8 +57830,8 @@
       </c>
     </row>
     <row r="958">
-      <c r="A958" s="83"/>
-      <c r="B958" s="84"/>
+      <c r="A958" s="76"/>
+      <c r="B958" s="77"/>
       <c r="C958" s="34"/>
       <c r="D958" s="34"/>
       <c r="E958" s="34"/>
@@ -57793,8 +57856,8 @@
       </c>
     </row>
     <row r="959">
-      <c r="A959" s="83"/>
-      <c r="B959" s="84"/>
+      <c r="A959" s="76"/>
+      <c r="B959" s="77"/>
       <c r="C959" s="34"/>
       <c r="D959" s="34"/>
       <c r="E959" s="34"/>
@@ -57819,8 +57882,8 @@
       </c>
     </row>
     <row r="960">
-      <c r="A960" s="83"/>
-      <c r="B960" s="84"/>
+      <c r="A960" s="76"/>
+      <c r="B960" s="77"/>
       <c r="C960" s="34"/>
       <c r="D960" s="34"/>
       <c r="E960" s="34"/>
@@ -57845,8 +57908,8 @@
       </c>
     </row>
     <row r="961">
-      <c r="A961" s="83"/>
-      <c r="B961" s="84"/>
+      <c r="A961" s="76"/>
+      <c r="B961" s="77"/>
       <c r="C961" s="34"/>
       <c r="D961" s="34"/>
       <c r="E961" s="34"/>
@@ -57871,8 +57934,8 @@
       </c>
     </row>
     <row r="962">
-      <c r="A962" s="83"/>
-      <c r="B962" s="84"/>
+      <c r="A962" s="76"/>
+      <c r="B962" s="77"/>
       <c r="C962" s="34"/>
       <c r="D962" s="34"/>
       <c r="E962" s="34"/>
@@ -57897,8 +57960,8 @@
       </c>
     </row>
     <row r="963">
-      <c r="A963" s="83"/>
-      <c r="B963" s="84"/>
+      <c r="A963" s="76"/>
+      <c r="B963" s="77"/>
       <c r="C963" s="34"/>
       <c r="D963" s="34"/>
       <c r="E963" s="34"/>
@@ -57923,8 +57986,8 @@
       </c>
     </row>
     <row r="964">
-      <c r="A964" s="83"/>
-      <c r="B964" s="84"/>
+      <c r="A964" s="76"/>
+      <c r="B964" s="77"/>
       <c r="C964" s="34"/>
       <c r="D964" s="34"/>
       <c r="E964" s="34"/>
@@ -57949,8 +58012,8 @@
       </c>
     </row>
     <row r="965">
-      <c r="A965" s="83"/>
-      <c r="B965" s="84"/>
+      <c r="A965" s="76"/>
+      <c r="B965" s="77"/>
       <c r="C965" s="34"/>
       <c r="D965" s="34"/>
       <c r="E965" s="34"/>
@@ -57975,8 +58038,8 @@
       </c>
     </row>
     <row r="966">
-      <c r="A966" s="83"/>
-      <c r="B966" s="84"/>
+      <c r="A966" s="76"/>
+      <c r="B966" s="77"/>
       <c r="C966" s="34"/>
       <c r="D966" s="34"/>
       <c r="E966" s="34"/>
@@ -58001,8 +58064,8 @@
       </c>
     </row>
     <row r="967">
-      <c r="A967" s="83"/>
-      <c r="B967" s="84"/>
+      <c r="A967" s="76"/>
+      <c r="B967" s="77"/>
       <c r="C967" s="34"/>
       <c r="D967" s="34"/>
       <c r="E967" s="34"/>
@@ -58027,8 +58090,8 @@
       </c>
     </row>
     <row r="968">
-      <c r="A968" s="83"/>
-      <c r="B968" s="84"/>
+      <c r="A968" s="76"/>
+      <c r="B968" s="77"/>
       <c r="C968" s="34"/>
       <c r="D968" s="34"/>
       <c r="E968" s="34"/>
@@ -58053,8 +58116,8 @@
       </c>
     </row>
     <row r="969">
-      <c r="A969" s="83"/>
-      <c r="B969" s="84"/>
+      <c r="A969" s="76"/>
+      <c r="B969" s="77"/>
       <c r="C969" s="34"/>
       <c r="D969" s="34"/>
       <c r="E969" s="34"/>
@@ -58079,8 +58142,8 @@
       </c>
     </row>
     <row r="970">
-      <c r="A970" s="83"/>
-      <c r="B970" s="84"/>
+      <c r="A970" s="76"/>
+      <c r="B970" s="77"/>
       <c r="C970" s="34"/>
       <c r="D970" s="34"/>
       <c r="E970" s="34"/>
@@ -58105,8 +58168,8 @@
       </c>
     </row>
     <row r="971">
-      <c r="A971" s="83"/>
-      <c r="B971" s="84"/>
+      <c r="A971" s="76"/>
+      <c r="B971" s="77"/>
       <c r="C971" s="34"/>
       <c r="D971" s="34"/>
       <c r="E971" s="34"/>
@@ -58131,8 +58194,8 @@
       </c>
     </row>
     <row r="972">
-      <c r="A972" s="83"/>
-      <c r="B972" s="84"/>
+      <c r="A972" s="76"/>
+      <c r="B972" s="77"/>
       <c r="C972" s="34"/>
       <c r="D972" s="34"/>
       <c r="E972" s="34"/>
@@ -58157,8 +58220,8 @@
       </c>
     </row>
     <row r="973">
-      <c r="A973" s="83"/>
-      <c r="B973" s="84"/>
+      <c r="A973" s="76"/>
+      <c r="B973" s="77"/>
       <c r="C973" s="34"/>
       <c r="D973" s="34"/>
       <c r="E973" s="34"/>
@@ -58183,8 +58246,8 @@
       </c>
     </row>
     <row r="974">
-      <c r="A974" s="83"/>
-      <c r="B974" s="84"/>
+      <c r="A974" s="76"/>
+      <c r="B974" s="77"/>
       <c r="C974" s="34"/>
       <c r="D974" s="34"/>
       <c r="E974" s="34"/>
@@ -58209,8 +58272,8 @@
       </c>
     </row>
     <row r="975">
-      <c r="A975" s="83"/>
-      <c r="B975" s="84"/>
+      <c r="A975" s="76"/>
+      <c r="B975" s="77"/>
       <c r="C975" s="34"/>
       <c r="D975" s="34"/>
       <c r="E975" s="34"/>
@@ -58235,8 +58298,8 @@
       </c>
     </row>
     <row r="976">
-      <c r="A976" s="83"/>
-      <c r="B976" s="84"/>
+      <c r="A976" s="76"/>
+      <c r="B976" s="77"/>
       <c r="C976" s="34"/>
       <c r="D976" s="34"/>
       <c r="E976" s="34"/>
@@ -58261,8 +58324,8 @@
       </c>
     </row>
     <row r="977">
-      <c r="A977" s="83"/>
-      <c r="B977" s="84"/>
+      <c r="A977" s="76"/>
+      <c r="B977" s="77"/>
       <c r="C977" s="34"/>
       <c r="D977" s="34"/>
       <c r="E977" s="34"/>
@@ -58287,8 +58350,8 @@
       </c>
     </row>
     <row r="978">
-      <c r="A978" s="83"/>
-      <c r="B978" s="84"/>
+      <c r="A978" s="76"/>
+      <c r="B978" s="77"/>
       <c r="C978" s="34"/>
       <c r="D978" s="34"/>
       <c r="E978" s="34"/>
@@ -58313,8 +58376,8 @@
       </c>
     </row>
     <row r="979">
-      <c r="A979" s="83"/>
-      <c r="B979" s="84"/>
+      <c r="A979" s="76"/>
+      <c r="B979" s="77"/>
       <c r="C979" s="34"/>
       <c r="D979" s="34"/>
       <c r="E979" s="34"/>
@@ -58339,8 +58402,8 @@
       </c>
     </row>
     <row r="980">
-      <c r="A980" s="83"/>
-      <c r="B980" s="84"/>
+      <c r="A980" s="76"/>
+      <c r="B980" s="77"/>
       <c r="C980" s="34"/>
       <c r="D980" s="34"/>
       <c r="E980" s="34"/>
@@ -58365,8 +58428,8 @@
       </c>
     </row>
     <row r="981">
-      <c r="A981" s="83"/>
-      <c r="B981" s="84"/>
+      <c r="A981" s="76"/>
+      <c r="B981" s="77"/>
       <c r="C981" s="34"/>
       <c r="D981" s="34"/>
       <c r="E981" s="34"/>
@@ -58391,8 +58454,8 @@
       </c>
     </row>
     <row r="982">
-      <c r="A982" s="83"/>
-      <c r="B982" s="84"/>
+      <c r="A982" s="76"/>
+      <c r="B982" s="77"/>
       <c r="C982" s="34"/>
       <c r="D982" s="34"/>
       <c r="E982" s="34"/>
@@ -58417,8 +58480,8 @@
       </c>
     </row>
     <row r="983">
-      <c r="A983" s="83"/>
-      <c r="B983" s="84"/>
+      <c r="A983" s="76"/>
+      <c r="B983" s="77"/>
       <c r="C983" s="34"/>
       <c r="D983" s="34"/>
       <c r="E983" s="34"/>
@@ -58443,8 +58506,8 @@
       </c>
     </row>
     <row r="984">
-      <c r="A984" s="83"/>
-      <c r="B984" s="84"/>
+      <c r="A984" s="76"/>
+      <c r="B984" s="77"/>
       <c r="C984" s="34"/>
       <c r="D984" s="34"/>
       <c r="E984" s="34"/>
@@ -58469,8 +58532,8 @@
       </c>
     </row>
     <row r="985">
-      <c r="A985" s="83"/>
-      <c r="B985" s="84"/>
+      <c r="A985" s="76"/>
+      <c r="B985" s="77"/>
       <c r="C985" s="34"/>
       <c r="D985" s="34"/>
       <c r="E985" s="34"/>
@@ -58495,8 +58558,8 @@
       </c>
     </row>
     <row r="986">
-      <c r="A986" s="83"/>
-      <c r="B986" s="84"/>
+      <c r="A986" s="76"/>
+      <c r="B986" s="77"/>
       <c r="C986" s="34"/>
       <c r="D986" s="34"/>
       <c r="E986" s="34"/>
@@ -58521,8 +58584,8 @@
       </c>
     </row>
     <row r="987">
-      <c r="A987" s="83"/>
-      <c r="B987" s="84"/>
+      <c r="A987" s="76"/>
+      <c r="B987" s="77"/>
       <c r="C987" s="34"/>
       <c r="D987" s="34"/>
       <c r="E987" s="34"/>
@@ -58547,8 +58610,8 @@
       </c>
     </row>
     <row r="988">
-      <c r="A988" s="83"/>
-      <c r="B988" s="84"/>
+      <c r="A988" s="76"/>
+      <c r="B988" s="77"/>
       <c r="C988" s="34"/>
       <c r="D988" s="34"/>
       <c r="E988" s="34"/>
@@ -58573,8 +58636,8 @@
       </c>
     </row>
     <row r="989">
-      <c r="A989" s="83"/>
-      <c r="B989" s="84"/>
+      <c r="A989" s="76"/>
+      <c r="B989" s="77"/>
       <c r="C989" s="34"/>
       <c r="D989" s="34"/>
       <c r="E989" s="34"/>
@@ -58599,8 +58662,8 @@
       </c>
     </row>
     <row r="990">
-      <c r="A990" s="83"/>
-      <c r="B990" s="84"/>
+      <c r="A990" s="76"/>
+      <c r="B990" s="77"/>
       <c r="C990" s="34"/>
       <c r="D990" s="34"/>
       <c r="E990" s="34"/>
@@ -58625,8 +58688,8 @@
       </c>
     </row>
     <row r="991">
-      <c r="A991" s="83"/>
-      <c r="B991" s="84"/>
+      <c r="A991" s="76"/>
+      <c r="B991" s="77"/>
       <c r="C991" s="34"/>
       <c r="D991" s="34"/>
       <c r="E991" s="34"/>
@@ -58651,8 +58714,8 @@
       </c>
     </row>
     <row r="992">
-      <c r="A992" s="83"/>
-      <c r="B992" s="84"/>
+      <c r="A992" s="76"/>
+      <c r="B992" s="77"/>
       <c r="C992" s="34"/>
       <c r="D992" s="34"/>
       <c r="E992" s="34"/>
@@ -58677,8 +58740,8 @@
       </c>
     </row>
     <row r="993">
-      <c r="A993" s="83"/>
-      <c r="B993" s="84"/>
+      <c r="A993" s="76"/>
+      <c r="B993" s="77"/>
       <c r="C993" s="34"/>
       <c r="D993" s="34"/>
       <c r="E993" s="34"/>
@@ -58703,8 +58766,8 @@
       </c>
     </row>
     <row r="994">
-      <c r="A994" s="83"/>
-      <c r="B994" s="84"/>
+      <c r="A994" s="76"/>
+      <c r="B994" s="77"/>
       <c r="C994" s="34"/>
       <c r="D994" s="34"/>
       <c r="E994" s="34"/>
@@ -58729,8 +58792,8 @@
       </c>
     </row>
     <row r="995">
-      <c r="A995" s="83"/>
-      <c r="B995" s="84"/>
+      <c r="A995" s="76"/>
+      <c r="B995" s="77"/>
       <c r="C995" s="34"/>
       <c r="D995" s="34"/>
       <c r="E995" s="34"/>
@@ -58755,8 +58818,8 @@
       </c>
     </row>
     <row r="996">
-      <c r="A996" s="83"/>
-      <c r="B996" s="84"/>
+      <c r="A996" s="76"/>
+      <c r="B996" s="77"/>
       <c r="C996" s="34"/>
       <c r="D996" s="34"/>
       <c r="E996" s="34"/>
@@ -58781,8 +58844,8 @@
       </c>
     </row>
     <row r="997">
-      <c r="A997" s="83"/>
-      <c r="B997" s="84"/>
+      <c r="A997" s="76"/>
+      <c r="B997" s="77"/>
       <c r="C997" s="34"/>
       <c r="D997" s="34"/>
       <c r="E997" s="34"/>
@@ -58807,8 +58870,8 @@
       </c>
     </row>
     <row r="998">
-      <c r="A998" s="83"/>
-      <c r="B998" s="84"/>
+      <c r="A998" s="76"/>
+      <c r="B998" s="77"/>
       <c r="C998" s="34"/>
       <c r="D998" s="34"/>
       <c r="E998" s="34"/>
@@ -58833,8 +58896,8 @@
       </c>
     </row>
     <row r="999">
-      <c r="A999" s="83"/>
-      <c r="B999" s="84"/>
+      <c r="A999" s="76"/>
+      <c r="B999" s="77"/>
       <c r="C999" s="34"/>
       <c r="D999" s="34"/>
       <c r="E999" s="34"/>
@@ -58859,8 +58922,8 @@
       </c>
     </row>
     <row r="1000">
-      <c r="A1000" s="83"/>
-      <c r="B1000" s="84"/>
+      <c r="A1000" s="76"/>
+      <c r="B1000" s="77"/>
       <c r="C1000" s="34"/>
       <c r="D1000" s="34"/>
       <c r="E1000" s="34"/>
@@ -58885,8 +58948,8 @@
       </c>
     </row>
     <row r="1001">
-      <c r="A1001" s="83"/>
-      <c r="B1001" s="84"/>
+      <c r="A1001" s="76"/>
+      <c r="B1001" s="77"/>
       <c r="C1001" s="34"/>
       <c r="D1001" s="34"/>
       <c r="E1001" s="34"/>
@@ -59579,15 +59642,17 @@
     <hyperlink r:id="rId281" ref="S718"/>
     <hyperlink r:id="rId282" ref="S719"/>
     <hyperlink r:id="rId283" ref="S720"/>
+    <hyperlink r:id="rId284" ref="S721"/>
+    <hyperlink r:id="rId285" ref="S722"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId284"/>
-  <legacyDrawing r:id="rId285"/>
+  <drawing r:id="rId286"/>
+  <legacyDrawing r:id="rId287"/>
   <tableParts count="2">
-    <tablePart r:id="rId288"/>
-    <tablePart r:id="rId289"/>
+    <tablePart r:id="rId290"/>
+    <tablePart r:id="rId291"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201211
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -577,7 +577,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8241" uniqueCount="2557">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8292" uniqueCount="2568">
   <si>
     <t>案例</t>
   </si>
@@ -9206,6 +9206,41 @@
   </si>
   <si>
     <t>由公司安排自費採檢</t>
+  </si>
+  <si>
+    <t>#722</t>
+  </si>
+  <si>
+    <t>12/8 採檢
+12/10 確診</t>
+  </si>
+  <si>
+    <t>移工，持有登機前3日內血清抗體檢驗陰性報告，11月29日曾進行「1127印尼專案」採檢，結果為陰性</t>
+  </si>
+  <si>
+    <t>新增4例境外移入COVID-19病例，自印尼及菲律賓入境</t>
+  </si>
+  <si>
+    <t>#723</t>
+  </si>
+  <si>
+    <t>-11/26 菲律賓→台灣</t>
+  </si>
+  <si>
+    <t>12/9 採檢
+12/10 確診</t>
+  </si>
+  <si>
+    <t>移工，於採檢後短暫出現流鼻水情形</t>
+  </si>
+  <si>
+    <t>#724</t>
+  </si>
+  <si>
+    <t>移工，持有10月29日採檢之核酸檢驗陰性報告</t>
+  </si>
+  <si>
+    <t>#725</t>
   </si>
 </sst>
 </file>
@@ -51720,107 +51755,227 @@
       </c>
     </row>
     <row r="723">
-      <c r="A723" s="76"/>
-      <c r="B723" s="77"/>
-      <c r="C723" s="34"/>
-      <c r="D723" s="34"/>
-      <c r="E723" s="34"/>
+      <c r="A723" s="16" t="s">
+        <v>2557</v>
+      </c>
+      <c r="B723" s="6">
+        <v>44175.0</v>
+      </c>
+      <c r="C723" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D723" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E723" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F723" s="34"/>
-      <c r="G723" s="34"/>
-      <c r="H723" s="21"/>
-      <c r="I723" s="19"/>
-      <c r="J723" s="10"/>
-      <c r="K723" s="22"/>
-      <c r="L723" s="23"/>
-      <c r="M723" s="22"/>
+      <c r="G723" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H723" s="8" t="s">
+        <v>2352</v>
+      </c>
+      <c r="I723" s="9">
+        <v>44160.0</v>
+      </c>
+      <c r="J723" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K723" s="13" t="s">
+        <v>2558</v>
+      </c>
+      <c r="L723" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M723" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N723" s="25"/>
-      <c r="O723" s="21"/>
-      <c r="P723" s="21"/>
+      <c r="O723" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P723" s="8" t="s">
+        <v>2559</v>
+      </c>
       <c r="Q723" s="19"/>
       <c r="R723" s="19"/>
-      <c r="S723" s="20"/>
+      <c r="S723" s="61" t="s">
+        <v>2560</v>
+      </c>
       <c r="T723" s="20"/>
       <c r="U723" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#722</v>
       </c>
     </row>
     <row r="724">
-      <c r="A724" s="76"/>
-      <c r="B724" s="77"/>
-      <c r="C724" s="34"/>
-      <c r="D724" s="34"/>
-      <c r="E724" s="34"/>
+      <c r="A724" s="16" t="s">
+        <v>2561</v>
+      </c>
+      <c r="B724" s="6">
+        <v>44175.0</v>
+      </c>
+      <c r="C724" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D724" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E724" s="7" t="s">
+        <v>205</v>
+      </c>
       <c r="F724" s="34"/>
-      <c r="G724" s="34"/>
-      <c r="H724" s="21"/>
-      <c r="I724" s="19"/>
-      <c r="J724" s="10"/>
-      <c r="K724" s="22"/>
-      <c r="L724" s="23"/>
-      <c r="M724" s="22"/>
+      <c r="G724" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H724" s="8" t="s">
+        <v>2562</v>
+      </c>
+      <c r="I724" s="9">
+        <v>44161.0</v>
+      </c>
+      <c r="J724" s="10">
+        <v>44174.0</v>
+      </c>
+      <c r="K724" s="13" t="s">
+        <v>2563</v>
+      </c>
+      <c r="L724" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M724" s="13" t="s">
+        <v>482</v>
+      </c>
       <c r="N724" s="25"/>
-      <c r="O724" s="21"/>
-      <c r="P724" s="21"/>
+      <c r="O724" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P724" s="8" t="s">
+        <v>2564</v>
+      </c>
       <c r="Q724" s="19"/>
       <c r="R724" s="19"/>
-      <c r="S724" s="20"/>
+      <c r="S724" s="61" t="s">
+        <v>2560</v>
+      </c>
       <c r="T724" s="20"/>
       <c r="U724" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#723</v>
       </c>
     </row>
     <row r="725">
-      <c r="A725" s="76"/>
-      <c r="B725" s="77"/>
-      <c r="C725" s="34"/>
-      <c r="D725" s="34"/>
-      <c r="E725" s="34"/>
+      <c r="A725" s="16" t="s">
+        <v>2565</v>
+      </c>
+      <c r="B725" s="6">
+        <v>44175.0</v>
+      </c>
+      <c r="C725" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D725" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E725" s="7" t="s">
+        <v>205</v>
+      </c>
       <c r="F725" s="34"/>
-      <c r="G725" s="34"/>
-      <c r="H725" s="21"/>
-      <c r="I725" s="19"/>
-      <c r="J725" s="10"/>
-      <c r="K725" s="22"/>
-      <c r="L725" s="23"/>
-      <c r="M725" s="22"/>
+      <c r="G725" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H725" s="8" t="s">
+        <v>2562</v>
+      </c>
+      <c r="I725" s="9">
+        <v>44161.0</v>
+      </c>
+      <c r="J725" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K725" s="13" t="s">
+        <v>2563</v>
+      </c>
+      <c r="L725" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M725" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N725" s="25"/>
-      <c r="O725" s="21"/>
-      <c r="P725" s="21"/>
+      <c r="O725" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P725" s="8" t="s">
+        <v>2566</v>
+      </c>
       <c r="Q725" s="19"/>
       <c r="R725" s="19"/>
-      <c r="S725" s="20"/>
+      <c r="S725" s="61" t="s">
+        <v>2560</v>
+      </c>
       <c r="T725" s="20"/>
       <c r="U725" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#724</v>
       </c>
     </row>
     <row r="726">
-      <c r="A726" s="76"/>
-      <c r="B726" s="77"/>
-      <c r="C726" s="34"/>
-      <c r="D726" s="34"/>
-      <c r="E726" s="34"/>
+      <c r="A726" s="16" t="s">
+        <v>2567</v>
+      </c>
+      <c r="B726" s="6">
+        <v>44175.0</v>
+      </c>
+      <c r="C726" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D726" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E726" s="7" t="s">
+        <v>205</v>
+      </c>
       <c r="F726" s="34"/>
-      <c r="G726" s="34"/>
-      <c r="H726" s="21"/>
-      <c r="I726" s="19"/>
-      <c r="J726" s="10"/>
-      <c r="K726" s="22"/>
-      <c r="L726" s="23"/>
-      <c r="M726" s="22"/>
+      <c r="G726" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H726" s="8" t="s">
+        <v>2562</v>
+      </c>
+      <c r="I726" s="9">
+        <v>44161.0</v>
+      </c>
+      <c r="J726" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K726" s="13" t="s">
+        <v>2563</v>
+      </c>
+      <c r="L726" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M726" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N726" s="25"/>
-      <c r="O726" s="21"/>
-      <c r="P726" s="21"/>
+      <c r="O726" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P726" s="8" t="s">
+        <v>1777</v>
+      </c>
       <c r="Q726" s="19"/>
       <c r="R726" s="19"/>
-      <c r="S726" s="20"/>
+      <c r="S726" s="61" t="s">
+        <v>2560</v>
+      </c>
       <c r="T726" s="20"/>
       <c r="U726" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#725</v>
       </c>
     </row>
     <row r="727">
@@ -51842,7 +51997,7 @@
       <c r="P727" s="21"/>
       <c r="Q727" s="19"/>
       <c r="R727" s="19"/>
-      <c r="S727" s="20"/>
+      <c r="S727" s="47"/>
       <c r="T727" s="20"/>
       <c r="U727" s="18" t="str">
         <f t="shared" si="1"/>
@@ -51868,7 +52023,7 @@
       <c r="P728" s="21"/>
       <c r="Q728" s="19"/>
       <c r="R728" s="19"/>
-      <c r="S728" s="20"/>
+      <c r="S728" s="47"/>
       <c r="T728" s="20"/>
       <c r="U728" s="18" t="str">
         <f t="shared" si="1"/>
@@ -51894,7 +52049,7 @@
       <c r="P729" s="21"/>
       <c r="Q729" s="19"/>
       <c r="R729" s="19"/>
-      <c r="S729" s="20"/>
+      <c r="S729" s="47"/>
       <c r="T729" s="20"/>
       <c r="U729" s="18" t="str">
         <f t="shared" si="1"/>
@@ -59644,15 +59799,19 @@
     <hyperlink r:id="rId283" ref="S720"/>
     <hyperlink r:id="rId284" ref="S721"/>
     <hyperlink r:id="rId285" ref="S722"/>
+    <hyperlink r:id="rId286" ref="S723"/>
+    <hyperlink r:id="rId287" ref="S724"/>
+    <hyperlink r:id="rId288" ref="S725"/>
+    <hyperlink r:id="rId289" ref="S726"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId286"/>
-  <legacyDrawing r:id="rId287"/>
+  <drawing r:id="rId290"/>
+  <legacyDrawing r:id="rId291"/>
   <tableParts count="2">
-    <tablePart r:id="rId290"/>
-    <tablePart r:id="rId291"/>
+    <tablePart r:id="rId294"/>
+    <tablePart r:id="rId295"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201212
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -577,7 +577,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8292" uniqueCount="2568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8304" uniqueCount="2573">
   <si>
     <t>案例</t>
   </si>
@@ -9241,6 +9241,22 @@
   </si>
   <si>
     <t>#725</t>
+  </si>
+  <si>
+    <t>#726</t>
+  </si>
+  <si>
+    <t>2019/9-11/30 美國</t>
+  </si>
+  <si>
+    <t>12/9 採檢
+12/11 確診</t>
+  </si>
+  <si>
+    <t>嗅覺異常 流鼻水</t>
+  </si>
+  <si>
+    <t>新增1例境外移入COVID-19病例，為自美返臺探親者</t>
   </si>
 </sst>
 </file>
@@ -51979,29 +51995,59 @@
       </c>
     </row>
     <row r="727">
-      <c r="A727" s="76"/>
-      <c r="B727" s="77"/>
-      <c r="C727" s="34"/>
-      <c r="D727" s="34"/>
-      <c r="E727" s="34"/>
+      <c r="A727" s="16" t="s">
+        <v>2568</v>
+      </c>
+      <c r="B727" s="6">
+        <v>44176.0</v>
+      </c>
+      <c r="C727" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D727" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E727" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F727" s="34"/>
-      <c r="G727" s="34"/>
-      <c r="H727" s="21"/>
-      <c r="I727" s="19"/>
-      <c r="J727" s="10"/>
-      <c r="K727" s="22"/>
-      <c r="L727" s="23"/>
-      <c r="M727" s="22"/>
+      <c r="G727" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H727" s="8" t="s">
+        <v>2569</v>
+      </c>
+      <c r="I727" s="9">
+        <v>44165.0</v>
+      </c>
+      <c r="J727" s="10">
+        <v>44172.0</v>
+      </c>
+      <c r="K727" s="13" t="s">
+        <v>2570</v>
+      </c>
+      <c r="L727" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M727" s="13" t="s">
+        <v>2571</v>
+      </c>
       <c r="N727" s="25"/>
-      <c r="O727" s="21"/>
-      <c r="P727" s="21"/>
+      <c r="O727" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P727" s="8" t="s">
+        <v>2271</v>
+      </c>
       <c r="Q727" s="19"/>
       <c r="R727" s="19"/>
-      <c r="S727" s="47"/>
+      <c r="S727" s="61" t="s">
+        <v>2572</v>
+      </c>
       <c r="T727" s="20"/>
       <c r="U727" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#726</v>
       </c>
     </row>
     <row r="728">
@@ -59803,15 +59849,16 @@
     <hyperlink r:id="rId287" ref="S724"/>
     <hyperlink r:id="rId288" ref="S725"/>
     <hyperlink r:id="rId289" ref="S726"/>
+    <hyperlink r:id="rId290" ref="S727"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId290"/>
-  <legacyDrawing r:id="rId291"/>
+  <drawing r:id="rId291"/>
+  <legacyDrawing r:id="rId292"/>
   <tableParts count="2">
-    <tablePart r:id="rId294"/>
     <tablePart r:id="rId295"/>
+    <tablePart r:id="rId296"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201213
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -572,12 +572,17 @@
 12/5 晚間臨時記者會</t>
       </text>
     </comment>
+    <comment authorId="0" ref="D735">
+      <text>
+        <t xml:space="preserve">https://www.cna.com.tw/news/firstnews/202012120024.aspx</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8304" uniqueCount="2573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8403" uniqueCount="2600">
   <si>
     <t>案例</t>
   </si>
@@ -9257,6 +9262,95 @@
   </si>
   <si>
     <t>新增1例境外移入COVID-19病例，為自美返臺探親者</t>
+  </si>
+  <si>
+    <t>#727</t>
+  </si>
+  <si>
+    <t>-11/27 印尼→台灣</t>
+  </si>
+  <si>
+    <t>11/28 採檢
+12/10 二採
+12/12 確診</t>
+  </si>
+  <si>
+    <t>移工，持有登機前3日內血清抗體檢驗陰性報告</t>
+  </si>
+  <si>
+    <t>新增8例境外移入COVID-19病例，分別自印尼、美國及英國入境</t>
+  </si>
+  <si>
+    <t>#728</t>
+  </si>
+  <si>
+    <t>7月-11/27 英國</t>
+  </si>
+  <si>
+    <t>12/6 採檢
+12/9 二採
+12/12 確診</t>
+  </si>
+  <si>
+    <t>全身倦怠 肌肉關節痠痛 頭暈 發燒</t>
+  </si>
+  <si>
+    <t>今年7月至英國工作，11月27日與2名家人一同返國；個案居家檢疫期間，於12月4日出現全身倦怠、肌肉關節痠痛、頭暈等症狀，12月6日發燒並由衛生單位安排就醫採檢，檢驗結果為陰性，因症狀未改善，12月9日再次就醫採檢並收治住院</t>
+  </si>
+  <si>
+    <t>#729</t>
+  </si>
+  <si>
+    <t>2019/8-11/30 美國</t>
+  </si>
+  <si>
+    <t>12/9 採檢
+12/12 確診</t>
+  </si>
+  <si>
+    <t>喉嚨痛 鼻塞 流鼻水 嗅覺異常 味覺異常</t>
+  </si>
+  <si>
+    <t>至美國就學，今年11月30日自美國搭機，12月2日入境臺灣後返回住處居家檢疫。個案12月5日曾有喉嚨痛症狀但未回報，12月8日起陸續出現鼻塞、流鼻水及嗅味覺異常症狀，12月9日通報衛生單位後安排就醫採檢</t>
+  </si>
+  <si>
+    <t>#730</t>
+  </si>
+  <si>
+    <t>移工，持有登機前3日內核酸檢驗陰性報告</t>
+  </si>
+  <si>
+    <t>#731</t>
+  </si>
+  <si>
+    <t>12/10 採檢
+12/12 確診</t>
+  </si>
+  <si>
+    <t>商務人士 檢疫期滿後至醫院自費採檢，於今日確診(Ct值34)</t>
+  </si>
+  <si>
+    <t>#732</t>
+  </si>
+  <si>
+    <t>#733</t>
+  </si>
+  <si>
+    <t>2019/3-12/6 美國</t>
+  </si>
+  <si>
+    <t>12/11 採檢
+12/12 確診</t>
+  </si>
+  <si>
+    <t>打噴嚏 喉嚨癢 嗅覺異常</t>
+  </si>
+  <si>
+    <t>#733 #734 家人
+長期居住美國</t>
+  </si>
+  <si>
+    <t>#734</t>
   </si>
 </sst>
 </file>
@@ -9397,7 +9491,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="79">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -9624,6 +9718,9 @@
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -52051,216 +52148,456 @@
       </c>
     </row>
     <row r="728">
-      <c r="A728" s="76"/>
-      <c r="B728" s="77"/>
-      <c r="C728" s="34"/>
-      <c r="D728" s="34"/>
-      <c r="E728" s="34"/>
+      <c r="A728" s="16" t="s">
+        <v>2573</v>
+      </c>
+      <c r="B728" s="6">
+        <v>44177.0</v>
+      </c>
+      <c r="C728" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D728" s="7" t="s">
+        <v>2190</v>
+      </c>
+      <c r="E728" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F728" s="34"/>
-      <c r="G728" s="34"/>
-      <c r="H728" s="21"/>
-      <c r="I728" s="19"/>
-      <c r="J728" s="10"/>
-      <c r="K728" s="22"/>
-      <c r="L728" s="23"/>
-      <c r="M728" s="22"/>
+      <c r="G728" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H728" s="8" t="s">
+        <v>2574</v>
+      </c>
+      <c r="I728" s="9">
+        <v>44162.0</v>
+      </c>
+      <c r="J728" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K728" s="13" t="s">
+        <v>2575</v>
+      </c>
+      <c r="L728" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M728" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N728" s="25"/>
-      <c r="O728" s="21"/>
-      <c r="P728" s="21"/>
+      <c r="O728" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P728" s="8" t="s">
+        <v>2576</v>
+      </c>
       <c r="Q728" s="19"/>
       <c r="R728" s="19"/>
-      <c r="S728" s="47"/>
+      <c r="S728" s="61" t="s">
+        <v>2577</v>
+      </c>
       <c r="T728" s="20"/>
       <c r="U728" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#727</v>
       </c>
     </row>
     <row r="729">
-      <c r="A729" s="76"/>
-      <c r="B729" s="77"/>
-      <c r="C729" s="34"/>
-      <c r="D729" s="34"/>
-      <c r="E729" s="34"/>
+      <c r="A729" s="16" t="s">
+        <v>2578</v>
+      </c>
+      <c r="B729" s="6">
+        <v>44177.0</v>
+      </c>
+      <c r="C729" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D729" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E729" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F729" s="34"/>
-      <c r="G729" s="34"/>
-      <c r="H729" s="21"/>
-      <c r="I729" s="19"/>
-      <c r="J729" s="10"/>
-      <c r="K729" s="22"/>
-      <c r="L729" s="23"/>
-      <c r="M729" s="22"/>
+      <c r="G729" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H729" s="8" t="s">
+        <v>2579</v>
+      </c>
+      <c r="I729" s="9">
+        <v>44162.0</v>
+      </c>
+      <c r="J729" s="10">
+        <v>44169.0</v>
+      </c>
+      <c r="K729" s="13" t="s">
+        <v>2580</v>
+      </c>
+      <c r="L729" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M729" s="13" t="s">
+        <v>2581</v>
+      </c>
       <c r="N729" s="25"/>
-      <c r="O729" s="21"/>
-      <c r="P729" s="21"/>
+      <c r="O729" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P729" s="8" t="s">
+        <v>2582</v>
+      </c>
       <c r="Q729" s="19"/>
       <c r="R729" s="19"/>
-      <c r="S729" s="47"/>
+      <c r="S729" s="61" t="s">
+        <v>2577</v>
+      </c>
       <c r="T729" s="20"/>
       <c r="U729" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#728</v>
       </c>
     </row>
     <row r="730">
-      <c r="A730" s="76"/>
-      <c r="B730" s="77"/>
-      <c r="C730" s="34"/>
-      <c r="D730" s="34"/>
-      <c r="E730" s="34"/>
+      <c r="A730" s="16" t="s">
+        <v>2583</v>
+      </c>
+      <c r="B730" s="6">
+        <v>44177.0</v>
+      </c>
+      <c r="C730" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D730" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E730" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F730" s="34"/>
-      <c r="G730" s="34"/>
-      <c r="H730" s="21"/>
-      <c r="I730" s="19"/>
-      <c r="J730" s="10"/>
-      <c r="K730" s="22"/>
-      <c r="L730" s="23"/>
-      <c r="M730" s="22"/>
+      <c r="G730" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H730" s="8" t="s">
+        <v>2584</v>
+      </c>
+      <c r="I730" s="9">
+        <v>44167.0</v>
+      </c>
+      <c r="J730" s="10">
+        <v>44170.0</v>
+      </c>
+      <c r="K730" s="13" t="s">
+        <v>2585</v>
+      </c>
+      <c r="L730" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M730" s="13" t="s">
+        <v>2586</v>
+      </c>
       <c r="N730" s="25"/>
-      <c r="O730" s="21"/>
-      <c r="P730" s="21"/>
+      <c r="O730" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P730" s="8" t="s">
+        <v>2587</v>
+      </c>
       <c r="Q730" s="19"/>
       <c r="R730" s="19"/>
-      <c r="S730" s="20"/>
+      <c r="S730" s="61" t="s">
+        <v>2577</v>
+      </c>
       <c r="T730" s="20"/>
       <c r="U730" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#729</v>
       </c>
     </row>
     <row r="731">
-      <c r="A731" s="76"/>
-      <c r="B731" s="77"/>
-      <c r="C731" s="34"/>
-      <c r="D731" s="34"/>
-      <c r="E731" s="34"/>
+      <c r="A731" s="16" t="s">
+        <v>2588</v>
+      </c>
+      <c r="B731" s="6">
+        <v>44177.0</v>
+      </c>
+      <c r="C731" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D731" s="7" t="s">
+        <v>2190</v>
+      </c>
+      <c r="E731" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F731" s="34"/>
-      <c r="G731" s="34"/>
-      <c r="H731" s="21"/>
-      <c r="I731" s="19"/>
-      <c r="J731" s="10"/>
-      <c r="K731" s="22"/>
-      <c r="L731" s="23"/>
-      <c r="M731" s="22"/>
+      <c r="G731" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H731" s="8" t="s">
+        <v>2574</v>
+      </c>
+      <c r="I731" s="9">
+        <v>44162.0</v>
+      </c>
+      <c r="J731" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K731" s="13" t="s">
+        <v>2575</v>
+      </c>
+      <c r="L731" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M731" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N731" s="25"/>
-      <c r="O731" s="21"/>
-      <c r="P731" s="21"/>
+      <c r="O731" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P731" s="8" t="s">
+        <v>2589</v>
+      </c>
       <c r="Q731" s="19"/>
       <c r="R731" s="19"/>
-      <c r="S731" s="20"/>
+      <c r="S731" s="61" t="s">
+        <v>2577</v>
+      </c>
       <c r="T731" s="20"/>
       <c r="U731" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#730</v>
       </c>
     </row>
     <row r="732">
-      <c r="A732" s="76"/>
-      <c r="B732" s="77"/>
-      <c r="C732" s="34"/>
-      <c r="D732" s="34"/>
-      <c r="E732" s="34"/>
+      <c r="A732" s="16" t="s">
+        <v>2590</v>
+      </c>
+      <c r="B732" s="6">
+        <v>44177.0</v>
+      </c>
+      <c r="C732" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D732" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E732" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F732" s="34"/>
-      <c r="G732" s="34"/>
-      <c r="H732" s="21"/>
-      <c r="I732" s="19"/>
-      <c r="J732" s="10"/>
-      <c r="K732" s="22"/>
-      <c r="L732" s="23"/>
-      <c r="M732" s="22"/>
+      <c r="G732" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H732" s="8" t="s">
+        <v>2352</v>
+      </c>
+      <c r="I732" s="9">
+        <v>44160.0</v>
+      </c>
+      <c r="J732" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K732" s="13" t="s">
+        <v>2591</v>
+      </c>
+      <c r="L732" s="12" t="s">
+        <v>1674</v>
+      </c>
+      <c r="M732" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N732" s="25"/>
-      <c r="O732" s="21"/>
-      <c r="P732" s="21"/>
+      <c r="O732" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P732" s="8" t="s">
+        <v>2592</v>
+      </c>
       <c r="Q732" s="19"/>
       <c r="R732" s="19"/>
-      <c r="S732" s="20"/>
+      <c r="S732" s="61" t="s">
+        <v>2577</v>
+      </c>
       <c r="T732" s="20"/>
       <c r="U732" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#731</v>
       </c>
     </row>
     <row r="733">
-      <c r="A733" s="76"/>
-      <c r="B733" s="77"/>
-      <c r="C733" s="34"/>
-      <c r="D733" s="34"/>
-      <c r="E733" s="34"/>
+      <c r="A733" s="16" t="s">
+        <v>2593</v>
+      </c>
+      <c r="B733" s="6">
+        <v>44177.0</v>
+      </c>
+      <c r="C733" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D733" s="7" t="s">
+        <v>2190</v>
+      </c>
+      <c r="E733" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F733" s="34"/>
-      <c r="G733" s="34"/>
-      <c r="H733" s="21"/>
-      <c r="I733" s="19"/>
-      <c r="J733" s="10"/>
-      <c r="K733" s="22"/>
-      <c r="L733" s="23"/>
-      <c r="M733" s="22"/>
+      <c r="G733" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H733" s="8" t="s">
+        <v>2574</v>
+      </c>
+      <c r="I733" s="9">
+        <v>44162.0</v>
+      </c>
+      <c r="J733" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K733" s="13" t="s">
+        <v>2575</v>
+      </c>
+      <c r="L733" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M733" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N733" s="25"/>
-      <c r="O733" s="21"/>
-      <c r="P733" s="21"/>
+      <c r="O733" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P733" s="76" t="s">
+        <v>2589</v>
+      </c>
       <c r="Q733" s="19"/>
       <c r="R733" s="19"/>
-      <c r="S733" s="20"/>
+      <c r="S733" s="61" t="s">
+        <v>2577</v>
+      </c>
       <c r="T733" s="20"/>
       <c r="U733" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#732</v>
       </c>
     </row>
     <row r="734">
-      <c r="A734" s="76"/>
-      <c r="B734" s="77"/>
-      <c r="C734" s="34"/>
-      <c r="D734" s="34"/>
-      <c r="E734" s="34"/>
+      <c r="A734" s="16" t="s">
+        <v>2594</v>
+      </c>
+      <c r="B734" s="6">
+        <v>44177.0</v>
+      </c>
+      <c r="C734" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D734" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E734" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F734" s="34"/>
-      <c r="G734" s="34"/>
-      <c r="H734" s="21"/>
-      <c r="I734" s="19"/>
-      <c r="J734" s="10"/>
-      <c r="K734" s="22"/>
-      <c r="L734" s="23"/>
-      <c r="M734" s="22"/>
+      <c r="G734" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H734" s="8" t="s">
+        <v>2595</v>
+      </c>
+      <c r="I734" s="9">
+        <v>44171.0</v>
+      </c>
+      <c r="J734" s="10">
+        <v>44174.0</v>
+      </c>
+      <c r="K734" s="13" t="s">
+        <v>2596</v>
+      </c>
+      <c r="L734" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M734" s="13" t="s">
+        <v>2597</v>
+      </c>
       <c r="N734" s="25"/>
-      <c r="O734" s="21"/>
-      <c r="P734" s="21"/>
+      <c r="O734" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P734" s="8" t="s">
+        <v>2598</v>
+      </c>
       <c r="Q734" s="19"/>
       <c r="R734" s="19"/>
-      <c r="S734" s="20"/>
+      <c r="S734" s="61" t="s">
+        <v>2577</v>
+      </c>
       <c r="T734" s="20"/>
       <c r="U734" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#733</v>
       </c>
     </row>
     <row r="735">
-      <c r="A735" s="76"/>
-      <c r="B735" s="77"/>
-      <c r="C735" s="34"/>
-      <c r="D735" s="34"/>
-      <c r="E735" s="34"/>
+      <c r="A735" s="16" t="s">
+        <v>2599</v>
+      </c>
+      <c r="B735" s="6">
+        <v>44177.0</v>
+      </c>
+      <c r="C735" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D735" s="7">
+        <v>3.0</v>
+      </c>
+      <c r="E735" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="F735" s="34"/>
-      <c r="G735" s="34"/>
-      <c r="H735" s="21"/>
-      <c r="I735" s="19"/>
-      <c r="J735" s="10"/>
-      <c r="K735" s="22"/>
-      <c r="L735" s="23"/>
-      <c r="M735" s="22"/>
+      <c r="G735" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H735" s="8" t="s">
+        <v>2595</v>
+      </c>
+      <c r="I735" s="9">
+        <v>44171.0</v>
+      </c>
+      <c r="J735" s="10">
+        <v>44176.0</v>
+      </c>
+      <c r="K735" s="13" t="s">
+        <v>2596</v>
+      </c>
+      <c r="L735" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M735" s="13" t="s">
+        <v>34</v>
+      </c>
       <c r="N735" s="25"/>
-      <c r="O735" s="21"/>
-      <c r="P735" s="21"/>
+      <c r="O735" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P735" s="8" t="s">
+        <v>2598</v>
+      </c>
       <c r="Q735" s="19"/>
       <c r="R735" s="19"/>
-      <c r="S735" s="20"/>
+      <c r="S735" s="61" t="s">
+        <v>2577</v>
+      </c>
       <c r="T735" s="20"/>
       <c r="U735" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#734</v>
       </c>
     </row>
     <row r="736">
-      <c r="A736" s="76"/>
-      <c r="B736" s="77"/>
+      <c r="A736" s="77"/>
+      <c r="B736" s="78"/>
       <c r="C736" s="34"/>
       <c r="D736" s="34"/>
       <c r="E736" s="34"/>
@@ -52285,8 +52622,8 @@
       </c>
     </row>
     <row r="737">
-      <c r="A737" s="76"/>
-      <c r="B737" s="77"/>
+      <c r="A737" s="77"/>
+      <c r="B737" s="78"/>
       <c r="C737" s="34"/>
       <c r="D737" s="34"/>
       <c r="E737" s="34"/>
@@ -52311,8 +52648,8 @@
       </c>
     </row>
     <row r="738">
-      <c r="A738" s="76"/>
-      <c r="B738" s="77"/>
+      <c r="A738" s="77"/>
+      <c r="B738" s="78"/>
       <c r="C738" s="34"/>
       <c r="D738" s="34"/>
       <c r="E738" s="34"/>
@@ -52337,8 +52674,8 @@
       </c>
     </row>
     <row r="739">
-      <c r="A739" s="76"/>
-      <c r="B739" s="77"/>
+      <c r="A739" s="77"/>
+      <c r="B739" s="78"/>
       <c r="C739" s="34"/>
       <c r="D739" s="34"/>
       <c r="E739" s="34"/>
@@ -52363,8 +52700,8 @@
       </c>
     </row>
     <row r="740">
-      <c r="A740" s="76"/>
-      <c r="B740" s="77"/>
+      <c r="A740" s="77"/>
+      <c r="B740" s="78"/>
       <c r="C740" s="34"/>
       <c r="D740" s="34"/>
       <c r="E740" s="34"/>
@@ -52389,8 +52726,8 @@
       </c>
     </row>
     <row r="741">
-      <c r="A741" s="76"/>
-      <c r="B741" s="77"/>
+      <c r="A741" s="77"/>
+      <c r="B741" s="78"/>
       <c r="C741" s="34"/>
       <c r="D741" s="34"/>
       <c r="E741" s="34"/>
@@ -52415,8 +52752,8 @@
       </c>
     </row>
     <row r="742">
-      <c r="A742" s="76"/>
-      <c r="B742" s="77"/>
+      <c r="A742" s="77"/>
+      <c r="B742" s="78"/>
       <c r="C742" s="34"/>
       <c r="D742" s="34"/>
       <c r="E742" s="34"/>
@@ -52441,8 +52778,8 @@
       </c>
     </row>
     <row r="743">
-      <c r="A743" s="76"/>
-      <c r="B743" s="77"/>
+      <c r="A743" s="77"/>
+      <c r="B743" s="78"/>
       <c r="C743" s="34"/>
       <c r="D743" s="34"/>
       <c r="E743" s="34"/>
@@ -52467,8 +52804,8 @@
       </c>
     </row>
     <row r="744">
-      <c r="A744" s="76"/>
-      <c r="B744" s="77"/>
+      <c r="A744" s="77"/>
+      <c r="B744" s="78"/>
       <c r="C744" s="34"/>
       <c r="D744" s="34"/>
       <c r="E744" s="34"/>
@@ -52493,8 +52830,8 @@
       </c>
     </row>
     <row r="745">
-      <c r="A745" s="76"/>
-      <c r="B745" s="77"/>
+      <c r="A745" s="77"/>
+      <c r="B745" s="78"/>
       <c r="C745" s="34"/>
       <c r="D745" s="34"/>
       <c r="E745" s="34"/>
@@ -52519,8 +52856,8 @@
       </c>
     </row>
     <row r="746">
-      <c r="A746" s="76"/>
-      <c r="B746" s="77"/>
+      <c r="A746" s="77"/>
+      <c r="B746" s="78"/>
       <c r="C746" s="34"/>
       <c r="D746" s="34"/>
       <c r="E746" s="34"/>
@@ -52545,8 +52882,8 @@
       </c>
     </row>
     <row r="747">
-      <c r="A747" s="76"/>
-      <c r="B747" s="77"/>
+      <c r="A747" s="77"/>
+      <c r="B747" s="78"/>
       <c r="C747" s="34"/>
       <c r="D747" s="34"/>
       <c r="E747" s="34"/>
@@ -52571,8 +52908,8 @@
       </c>
     </row>
     <row r="748">
-      <c r="A748" s="76"/>
-      <c r="B748" s="77"/>
+      <c r="A748" s="77"/>
+      <c r="B748" s="78"/>
       <c r="C748" s="34"/>
       <c r="D748" s="34"/>
       <c r="E748" s="34"/>
@@ -52597,8 +52934,8 @@
       </c>
     </row>
     <row r="749">
-      <c r="A749" s="76"/>
-      <c r="B749" s="77"/>
+      <c r="A749" s="77"/>
+      <c r="B749" s="78"/>
       <c r="C749" s="34"/>
       <c r="D749" s="34"/>
       <c r="E749" s="34"/>
@@ -52623,8 +52960,8 @@
       </c>
     </row>
     <row r="750">
-      <c r="A750" s="76"/>
-      <c r="B750" s="77"/>
+      <c r="A750" s="77"/>
+      <c r="B750" s="78"/>
       <c r="C750" s="34"/>
       <c r="D750" s="34"/>
       <c r="E750" s="34"/>
@@ -52649,8 +52986,8 @@
       </c>
     </row>
     <row r="751">
-      <c r="A751" s="76"/>
-      <c r="B751" s="77"/>
+      <c r="A751" s="77"/>
+      <c r="B751" s="78"/>
       <c r="C751" s="34"/>
       <c r="D751" s="34"/>
       <c r="E751" s="34"/>
@@ -52675,8 +53012,8 @@
       </c>
     </row>
     <row r="752">
-      <c r="A752" s="76"/>
-      <c r="B752" s="77"/>
+      <c r="A752" s="77"/>
+      <c r="B752" s="78"/>
       <c r="C752" s="34"/>
       <c r="D752" s="34"/>
       <c r="E752" s="34"/>
@@ -52701,8 +53038,8 @@
       </c>
     </row>
     <row r="753">
-      <c r="A753" s="76"/>
-      <c r="B753" s="77"/>
+      <c r="A753" s="77"/>
+      <c r="B753" s="78"/>
       <c r="C753" s="34"/>
       <c r="D753" s="34"/>
       <c r="E753" s="34"/>
@@ -52727,8 +53064,8 @@
       </c>
     </row>
     <row r="754">
-      <c r="A754" s="76"/>
-      <c r="B754" s="77"/>
+      <c r="A754" s="77"/>
+      <c r="B754" s="78"/>
       <c r="C754" s="34"/>
       <c r="D754" s="34"/>
       <c r="E754" s="34"/>
@@ -52753,8 +53090,8 @@
       </c>
     </row>
     <row r="755">
-      <c r="A755" s="76"/>
-      <c r="B755" s="77"/>
+      <c r="A755" s="77"/>
+      <c r="B755" s="78"/>
       <c r="C755" s="34"/>
       <c r="D755" s="34"/>
       <c r="E755" s="34"/>
@@ -52779,8 +53116,8 @@
       </c>
     </row>
     <row r="756">
-      <c r="A756" s="76"/>
-      <c r="B756" s="77"/>
+      <c r="A756" s="77"/>
+      <c r="B756" s="78"/>
       <c r="C756" s="34"/>
       <c r="D756" s="34"/>
       <c r="E756" s="34"/>
@@ -52805,8 +53142,8 @@
       </c>
     </row>
     <row r="757">
-      <c r="A757" s="76"/>
-      <c r="B757" s="77"/>
+      <c r="A757" s="77"/>
+      <c r="B757" s="78"/>
       <c r="C757" s="34"/>
       <c r="D757" s="34"/>
       <c r="E757" s="34"/>
@@ -52831,8 +53168,8 @@
       </c>
     </row>
     <row r="758">
-      <c r="A758" s="76"/>
-      <c r="B758" s="77"/>
+      <c r="A758" s="77"/>
+      <c r="B758" s="78"/>
       <c r="C758" s="34"/>
       <c r="D758" s="34"/>
       <c r="E758" s="34"/>
@@ -52857,8 +53194,8 @@
       </c>
     </row>
     <row r="759">
-      <c r="A759" s="76"/>
-      <c r="B759" s="77"/>
+      <c r="A759" s="77"/>
+      <c r="B759" s="78"/>
       <c r="C759" s="34"/>
       <c r="D759" s="34"/>
       <c r="E759" s="34"/>
@@ -52883,8 +53220,8 @@
       </c>
     </row>
     <row r="760">
-      <c r="A760" s="76"/>
-      <c r="B760" s="77"/>
+      <c r="A760" s="77"/>
+      <c r="B760" s="78"/>
       <c r="C760" s="34"/>
       <c r="D760" s="34"/>
       <c r="E760" s="34"/>
@@ -52909,8 +53246,8 @@
       </c>
     </row>
     <row r="761">
-      <c r="A761" s="76"/>
-      <c r="B761" s="77"/>
+      <c r="A761" s="77"/>
+      <c r="B761" s="78"/>
       <c r="C761" s="34"/>
       <c r="D761" s="34"/>
       <c r="E761" s="34"/>
@@ -52935,8 +53272,8 @@
       </c>
     </row>
     <row r="762">
-      <c r="A762" s="76"/>
-      <c r="B762" s="77"/>
+      <c r="A762" s="77"/>
+      <c r="B762" s="78"/>
       <c r="C762" s="34"/>
       <c r="D762" s="34"/>
       <c r="E762" s="34"/>
@@ -52961,8 +53298,8 @@
       </c>
     </row>
     <row r="763">
-      <c r="A763" s="76"/>
-      <c r="B763" s="77"/>
+      <c r="A763" s="77"/>
+      <c r="B763" s="78"/>
       <c r="C763" s="34"/>
       <c r="D763" s="34"/>
       <c r="E763" s="34"/>
@@ -52987,8 +53324,8 @@
       </c>
     </row>
     <row r="764">
-      <c r="A764" s="76"/>
-      <c r="B764" s="77"/>
+      <c r="A764" s="77"/>
+      <c r="B764" s="78"/>
       <c r="C764" s="34"/>
       <c r="D764" s="34"/>
       <c r="E764" s="34"/>
@@ -53013,8 +53350,8 @@
       </c>
     </row>
     <row r="765">
-      <c r="A765" s="76"/>
-      <c r="B765" s="77"/>
+      <c r="A765" s="77"/>
+      <c r="B765" s="78"/>
       <c r="C765" s="34"/>
       <c r="D765" s="34"/>
       <c r="E765" s="34"/>
@@ -53039,8 +53376,8 @@
       </c>
     </row>
     <row r="766">
-      <c r="A766" s="76"/>
-      <c r="B766" s="77"/>
+      <c r="A766" s="77"/>
+      <c r="B766" s="78"/>
       <c r="C766" s="34"/>
       <c r="D766" s="34"/>
       <c r="E766" s="34"/>
@@ -53065,8 +53402,8 @@
       </c>
     </row>
     <row r="767">
-      <c r="A767" s="76"/>
-      <c r="B767" s="77"/>
+      <c r="A767" s="77"/>
+      <c r="B767" s="78"/>
       <c r="C767" s="34"/>
       <c r="D767" s="34"/>
       <c r="E767" s="34"/>
@@ -53091,8 +53428,8 @@
       </c>
     </row>
     <row r="768">
-      <c r="A768" s="76"/>
-      <c r="B768" s="77"/>
+      <c r="A768" s="77"/>
+      <c r="B768" s="78"/>
       <c r="C768" s="34"/>
       <c r="D768" s="34"/>
       <c r="E768" s="34"/>
@@ -53117,8 +53454,8 @@
       </c>
     </row>
     <row r="769">
-      <c r="A769" s="76"/>
-      <c r="B769" s="77"/>
+      <c r="A769" s="77"/>
+      <c r="B769" s="78"/>
       <c r="C769" s="34"/>
       <c r="D769" s="34"/>
       <c r="E769" s="34"/>
@@ -53143,8 +53480,8 @@
       </c>
     </row>
     <row r="770">
-      <c r="A770" s="76"/>
-      <c r="B770" s="77"/>
+      <c r="A770" s="77"/>
+      <c r="B770" s="78"/>
       <c r="C770" s="34"/>
       <c r="D770" s="34"/>
       <c r="E770" s="34"/>
@@ -53169,8 +53506,8 @@
       </c>
     </row>
     <row r="771">
-      <c r="A771" s="76"/>
-      <c r="B771" s="77"/>
+      <c r="A771" s="77"/>
+      <c r="B771" s="78"/>
       <c r="C771" s="34"/>
       <c r="D771" s="34"/>
       <c r="E771" s="34"/>
@@ -53195,8 +53532,8 @@
       </c>
     </row>
     <row r="772">
-      <c r="A772" s="76"/>
-      <c r="B772" s="77"/>
+      <c r="A772" s="77"/>
+      <c r="B772" s="78"/>
       <c r="C772" s="34"/>
       <c r="D772" s="34"/>
       <c r="E772" s="34"/>
@@ -53221,8 +53558,8 @@
       </c>
     </row>
     <row r="773">
-      <c r="A773" s="76"/>
-      <c r="B773" s="77"/>
+      <c r="A773" s="77"/>
+      <c r="B773" s="78"/>
       <c r="C773" s="34"/>
       <c r="D773" s="34"/>
       <c r="E773" s="34"/>
@@ -53247,8 +53584,8 @@
       </c>
     </row>
     <row r="774">
-      <c r="A774" s="76"/>
-      <c r="B774" s="77"/>
+      <c r="A774" s="77"/>
+      <c r="B774" s="78"/>
       <c r="C774" s="34"/>
       <c r="D774" s="34"/>
       <c r="E774" s="34"/>
@@ -53273,8 +53610,8 @@
       </c>
     </row>
     <row r="775">
-      <c r="A775" s="76"/>
-      <c r="B775" s="77"/>
+      <c r="A775" s="77"/>
+      <c r="B775" s="78"/>
       <c r="C775" s="34"/>
       <c r="D775" s="34"/>
       <c r="E775" s="34"/>
@@ -53299,8 +53636,8 @@
       </c>
     </row>
     <row r="776">
-      <c r="A776" s="76"/>
-      <c r="B776" s="77"/>
+      <c r="A776" s="77"/>
+      <c r="B776" s="78"/>
       <c r="C776" s="34"/>
       <c r="D776" s="34"/>
       <c r="E776" s="34"/>
@@ -53325,8 +53662,8 @@
       </c>
     </row>
     <row r="777">
-      <c r="A777" s="76"/>
-      <c r="B777" s="77"/>
+      <c r="A777" s="77"/>
+      <c r="B777" s="78"/>
       <c r="C777" s="34"/>
       <c r="D777" s="34"/>
       <c r="E777" s="34"/>
@@ -53351,8 +53688,8 @@
       </c>
     </row>
     <row r="778">
-      <c r="A778" s="76"/>
-      <c r="B778" s="77"/>
+      <c r="A778" s="77"/>
+      <c r="B778" s="78"/>
       <c r="C778" s="34"/>
       <c r="D778" s="34"/>
       <c r="E778" s="34"/>
@@ -53377,8 +53714,8 @@
       </c>
     </row>
     <row r="779">
-      <c r="A779" s="76"/>
-      <c r="B779" s="77"/>
+      <c r="A779" s="77"/>
+      <c r="B779" s="78"/>
       <c r="C779" s="34"/>
       <c r="D779" s="34"/>
       <c r="E779" s="34"/>
@@ -53403,8 +53740,8 @@
       </c>
     </row>
     <row r="780">
-      <c r="A780" s="76"/>
-      <c r="B780" s="77"/>
+      <c r="A780" s="77"/>
+      <c r="B780" s="78"/>
       <c r="C780" s="34"/>
       <c r="D780" s="34"/>
       <c r="E780" s="34"/>
@@ -53429,8 +53766,8 @@
       </c>
     </row>
     <row r="781">
-      <c r="A781" s="76"/>
-      <c r="B781" s="77"/>
+      <c r="A781" s="77"/>
+      <c r="B781" s="78"/>
       <c r="C781" s="34"/>
       <c r="D781" s="34"/>
       <c r="E781" s="34"/>
@@ -53455,8 +53792,8 @@
       </c>
     </row>
     <row r="782">
-      <c r="A782" s="76"/>
-      <c r="B782" s="77"/>
+      <c r="A782" s="77"/>
+      <c r="B782" s="78"/>
       <c r="C782" s="34"/>
       <c r="D782" s="34"/>
       <c r="E782" s="34"/>
@@ -53481,8 +53818,8 @@
       </c>
     </row>
     <row r="783">
-      <c r="A783" s="76"/>
-      <c r="B783" s="77"/>
+      <c r="A783" s="77"/>
+      <c r="B783" s="78"/>
       <c r="C783" s="34"/>
       <c r="D783" s="34"/>
       <c r="E783" s="34"/>
@@ -53507,8 +53844,8 @@
       </c>
     </row>
     <row r="784">
-      <c r="A784" s="76"/>
-      <c r="B784" s="77"/>
+      <c r="A784" s="77"/>
+      <c r="B784" s="78"/>
       <c r="C784" s="34"/>
       <c r="D784" s="34"/>
       <c r="E784" s="34"/>
@@ -53533,8 +53870,8 @@
       </c>
     </row>
     <row r="785">
-      <c r="A785" s="76"/>
-      <c r="B785" s="77"/>
+      <c r="A785" s="77"/>
+      <c r="B785" s="78"/>
       <c r="C785" s="34"/>
       <c r="D785" s="34"/>
       <c r="E785" s="34"/>
@@ -53559,8 +53896,8 @@
       </c>
     </row>
     <row r="786">
-      <c r="A786" s="76"/>
-      <c r="B786" s="77"/>
+      <c r="A786" s="77"/>
+      <c r="B786" s="78"/>
       <c r="C786" s="34"/>
       <c r="D786" s="34"/>
       <c r="E786" s="34"/>
@@ -53585,8 +53922,8 @@
       </c>
     </row>
     <row r="787">
-      <c r="A787" s="76"/>
-      <c r="B787" s="77"/>
+      <c r="A787" s="77"/>
+      <c r="B787" s="78"/>
       <c r="C787" s="34"/>
       <c r="D787" s="34"/>
       <c r="E787" s="34"/>
@@ -53611,8 +53948,8 @@
       </c>
     </row>
     <row r="788">
-      <c r="A788" s="76"/>
-      <c r="B788" s="77"/>
+      <c r="A788" s="77"/>
+      <c r="B788" s="78"/>
       <c r="C788" s="34"/>
       <c r="D788" s="34"/>
       <c r="E788" s="34"/>
@@ -53637,8 +53974,8 @@
       </c>
     </row>
     <row r="789">
-      <c r="A789" s="76"/>
-      <c r="B789" s="77"/>
+      <c r="A789" s="77"/>
+      <c r="B789" s="78"/>
       <c r="C789" s="34"/>
       <c r="D789" s="34"/>
       <c r="E789" s="34"/>
@@ -53663,8 +54000,8 @@
       </c>
     </row>
     <row r="790">
-      <c r="A790" s="76"/>
-      <c r="B790" s="77"/>
+      <c r="A790" s="77"/>
+      <c r="B790" s="78"/>
       <c r="C790" s="34"/>
       <c r="D790" s="34"/>
       <c r="E790" s="34"/>
@@ -53689,8 +54026,8 @@
       </c>
     </row>
     <row r="791">
-      <c r="A791" s="76"/>
-      <c r="B791" s="77"/>
+      <c r="A791" s="77"/>
+      <c r="B791" s="78"/>
       <c r="C791" s="34"/>
       <c r="D791" s="34"/>
       <c r="E791" s="34"/>
@@ -53715,8 +54052,8 @@
       </c>
     </row>
     <row r="792">
-      <c r="A792" s="76"/>
-      <c r="B792" s="77"/>
+      <c r="A792" s="77"/>
+      <c r="B792" s="78"/>
       <c r="C792" s="34"/>
       <c r="D792" s="34"/>
       <c r="E792" s="34"/>
@@ -53741,8 +54078,8 @@
       </c>
     </row>
     <row r="793">
-      <c r="A793" s="76"/>
-      <c r="B793" s="77"/>
+      <c r="A793" s="77"/>
+      <c r="B793" s="78"/>
       <c r="C793" s="34"/>
       <c r="D793" s="34"/>
       <c r="E793" s="34"/>
@@ -53767,8 +54104,8 @@
       </c>
     </row>
     <row r="794">
-      <c r="A794" s="76"/>
-      <c r="B794" s="77"/>
+      <c r="A794" s="77"/>
+      <c r="B794" s="78"/>
       <c r="C794" s="34"/>
       <c r="D794" s="34"/>
       <c r="E794" s="34"/>
@@ -53793,8 +54130,8 @@
       </c>
     </row>
     <row r="795">
-      <c r="A795" s="76"/>
-      <c r="B795" s="77"/>
+      <c r="A795" s="77"/>
+      <c r="B795" s="78"/>
       <c r="C795" s="34"/>
       <c r="D795" s="34"/>
       <c r="E795" s="34"/>
@@ -53819,8 +54156,8 @@
       </c>
     </row>
     <row r="796">
-      <c r="A796" s="76"/>
-      <c r="B796" s="77"/>
+      <c r="A796" s="77"/>
+      <c r="B796" s="78"/>
       <c r="C796" s="34"/>
       <c r="D796" s="34"/>
       <c r="E796" s="34"/>
@@ -53845,8 +54182,8 @@
       </c>
     </row>
     <row r="797">
-      <c r="A797" s="76"/>
-      <c r="B797" s="77"/>
+      <c r="A797" s="77"/>
+      <c r="B797" s="78"/>
       <c r="C797" s="34"/>
       <c r="D797" s="34"/>
       <c r="E797" s="34"/>
@@ -53871,8 +54208,8 @@
       </c>
     </row>
     <row r="798">
-      <c r="A798" s="76"/>
-      <c r="B798" s="77"/>
+      <c r="A798" s="77"/>
+      <c r="B798" s="78"/>
       <c r="C798" s="34"/>
       <c r="D798" s="34"/>
       <c r="E798" s="34"/>
@@ -53897,8 +54234,8 @@
       </c>
     </row>
     <row r="799">
-      <c r="A799" s="76"/>
-      <c r="B799" s="77"/>
+      <c r="A799" s="77"/>
+      <c r="B799" s="78"/>
       <c r="C799" s="34"/>
       <c r="D799" s="34"/>
       <c r="E799" s="34"/>
@@ -53923,8 +54260,8 @@
       </c>
     </row>
     <row r="800">
-      <c r="A800" s="76"/>
-      <c r="B800" s="77"/>
+      <c r="A800" s="77"/>
+      <c r="B800" s="78"/>
       <c r="C800" s="34"/>
       <c r="D800" s="34"/>
       <c r="E800" s="34"/>
@@ -53949,8 +54286,8 @@
       </c>
     </row>
     <row r="801">
-      <c r="A801" s="76"/>
-      <c r="B801" s="77"/>
+      <c r="A801" s="77"/>
+      <c r="B801" s="78"/>
       <c r="C801" s="34"/>
       <c r="D801" s="34"/>
       <c r="E801" s="34"/>
@@ -53975,8 +54312,8 @@
       </c>
     </row>
     <row r="802">
-      <c r="A802" s="76"/>
-      <c r="B802" s="77"/>
+      <c r="A802" s="77"/>
+      <c r="B802" s="78"/>
       <c r="C802" s="34"/>
       <c r="D802" s="34"/>
       <c r="E802" s="34"/>
@@ -54001,8 +54338,8 @@
       </c>
     </row>
     <row r="803">
-      <c r="A803" s="76"/>
-      <c r="B803" s="77"/>
+      <c r="A803" s="77"/>
+      <c r="B803" s="78"/>
       <c r="C803" s="34"/>
       <c r="D803" s="34"/>
       <c r="E803" s="34"/>
@@ -54027,8 +54364,8 @@
       </c>
     </row>
     <row r="804">
-      <c r="A804" s="76"/>
-      <c r="B804" s="77"/>
+      <c r="A804" s="77"/>
+      <c r="B804" s="78"/>
       <c r="C804" s="34"/>
       <c r="D804" s="34"/>
       <c r="E804" s="34"/>
@@ -54053,8 +54390,8 @@
       </c>
     </row>
     <row r="805">
-      <c r="A805" s="76"/>
-      <c r="B805" s="77"/>
+      <c r="A805" s="77"/>
+      <c r="B805" s="78"/>
       <c r="C805" s="34"/>
       <c r="D805" s="34"/>
       <c r="E805" s="34"/>
@@ -54079,8 +54416,8 @@
       </c>
     </row>
     <row r="806">
-      <c r="A806" s="76"/>
-      <c r="B806" s="77"/>
+      <c r="A806" s="77"/>
+      <c r="B806" s="78"/>
       <c r="C806" s="34"/>
       <c r="D806" s="34"/>
       <c r="E806" s="34"/>
@@ -54105,8 +54442,8 @@
       </c>
     </row>
     <row r="807">
-      <c r="A807" s="76"/>
-      <c r="B807" s="77"/>
+      <c r="A807" s="77"/>
+      <c r="B807" s="78"/>
       <c r="C807" s="34"/>
       <c r="D807" s="34"/>
       <c r="E807" s="34"/>
@@ -54131,8 +54468,8 @@
       </c>
     </row>
     <row r="808">
-      <c r="A808" s="76"/>
-      <c r="B808" s="77"/>
+      <c r="A808" s="77"/>
+      <c r="B808" s="78"/>
       <c r="C808" s="34"/>
       <c r="D808" s="34"/>
       <c r="E808" s="34"/>
@@ -54157,8 +54494,8 @@
       </c>
     </row>
     <row r="809">
-      <c r="A809" s="76"/>
-      <c r="B809" s="77"/>
+      <c r="A809" s="77"/>
+      <c r="B809" s="78"/>
       <c r="C809" s="34"/>
       <c r="D809" s="34"/>
       <c r="E809" s="34"/>
@@ -54183,8 +54520,8 @@
       </c>
     </row>
     <row r="810">
-      <c r="A810" s="76"/>
-      <c r="B810" s="77"/>
+      <c r="A810" s="77"/>
+      <c r="B810" s="78"/>
       <c r="C810" s="34"/>
       <c r="D810" s="34"/>
       <c r="E810" s="34"/>
@@ -54209,8 +54546,8 @@
       </c>
     </row>
     <row r="811">
-      <c r="A811" s="76"/>
-      <c r="B811" s="77"/>
+      <c r="A811" s="77"/>
+      <c r="B811" s="78"/>
       <c r="C811" s="34"/>
       <c r="D811" s="34"/>
       <c r="E811" s="34"/>
@@ -54235,8 +54572,8 @@
       </c>
     </row>
     <row r="812">
-      <c r="A812" s="76"/>
-      <c r="B812" s="77"/>
+      <c r="A812" s="77"/>
+      <c r="B812" s="78"/>
       <c r="C812" s="34"/>
       <c r="D812" s="34"/>
       <c r="E812" s="34"/>
@@ -54261,8 +54598,8 @@
       </c>
     </row>
     <row r="813">
-      <c r="A813" s="76"/>
-      <c r="B813" s="77"/>
+      <c r="A813" s="77"/>
+      <c r="B813" s="78"/>
       <c r="C813" s="34"/>
       <c r="D813" s="34"/>
       <c r="E813" s="34"/>
@@ -54287,8 +54624,8 @@
       </c>
     </row>
     <row r="814">
-      <c r="A814" s="76"/>
-      <c r="B814" s="77"/>
+      <c r="A814" s="77"/>
+      <c r="B814" s="78"/>
       <c r="C814" s="34"/>
       <c r="D814" s="34"/>
       <c r="E814" s="34"/>
@@ -54313,8 +54650,8 @@
       </c>
     </row>
     <row r="815">
-      <c r="A815" s="76"/>
-      <c r="B815" s="77"/>
+      <c r="A815" s="77"/>
+      <c r="B815" s="78"/>
       <c r="C815" s="34"/>
       <c r="D815" s="34"/>
       <c r="E815" s="34"/>
@@ -54339,8 +54676,8 @@
       </c>
     </row>
     <row r="816">
-      <c r="A816" s="76"/>
-      <c r="B816" s="77"/>
+      <c r="A816" s="77"/>
+      <c r="B816" s="78"/>
       <c r="C816" s="34"/>
       <c r="D816" s="34"/>
       <c r="E816" s="34"/>
@@ -54365,8 +54702,8 @@
       </c>
     </row>
     <row r="817">
-      <c r="A817" s="76"/>
-      <c r="B817" s="77"/>
+      <c r="A817" s="77"/>
+      <c r="B817" s="78"/>
       <c r="C817" s="34"/>
       <c r="D817" s="34"/>
       <c r="E817" s="34"/>
@@ -54391,8 +54728,8 @@
       </c>
     </row>
     <row r="818">
-      <c r="A818" s="76"/>
-      <c r="B818" s="77"/>
+      <c r="A818" s="77"/>
+      <c r="B818" s="78"/>
       <c r="C818" s="34"/>
       <c r="D818" s="34"/>
       <c r="E818" s="34"/>
@@ -54417,8 +54754,8 @@
       </c>
     </row>
     <row r="819">
-      <c r="A819" s="76"/>
-      <c r="B819" s="77"/>
+      <c r="A819" s="77"/>
+      <c r="B819" s="78"/>
       <c r="C819" s="34"/>
       <c r="D819" s="34"/>
       <c r="E819" s="34"/>
@@ -54443,8 +54780,8 @@
       </c>
     </row>
     <row r="820">
-      <c r="A820" s="76"/>
-      <c r="B820" s="77"/>
+      <c r="A820" s="77"/>
+      <c r="B820" s="78"/>
       <c r="C820" s="34"/>
       <c r="D820" s="34"/>
       <c r="E820" s="34"/>
@@ -54469,8 +54806,8 @@
       </c>
     </row>
     <row r="821">
-      <c r="A821" s="76"/>
-      <c r="B821" s="77"/>
+      <c r="A821" s="77"/>
+      <c r="B821" s="78"/>
       <c r="C821" s="34"/>
       <c r="D821" s="34"/>
       <c r="E821" s="34"/>
@@ -54495,8 +54832,8 @@
       </c>
     </row>
     <row r="822">
-      <c r="A822" s="76"/>
-      <c r="B822" s="77"/>
+      <c r="A822" s="77"/>
+      <c r="B822" s="78"/>
       <c r="C822" s="34"/>
       <c r="D822" s="34"/>
       <c r="E822" s="34"/>
@@ -54521,8 +54858,8 @@
       </c>
     </row>
     <row r="823">
-      <c r="A823" s="76"/>
-      <c r="B823" s="77"/>
+      <c r="A823" s="77"/>
+      <c r="B823" s="78"/>
       <c r="C823" s="34"/>
       <c r="D823" s="34"/>
       <c r="E823" s="34"/>
@@ -54547,8 +54884,8 @@
       </c>
     </row>
     <row r="824">
-      <c r="A824" s="76"/>
-      <c r="B824" s="77"/>
+      <c r="A824" s="77"/>
+      <c r="B824" s="78"/>
       <c r="C824" s="34"/>
       <c r="D824" s="34"/>
       <c r="E824" s="34"/>
@@ -54573,8 +54910,8 @@
       </c>
     </row>
     <row r="825">
-      <c r="A825" s="76"/>
-      <c r="B825" s="77"/>
+      <c r="A825" s="77"/>
+      <c r="B825" s="78"/>
       <c r="C825" s="34"/>
       <c r="D825" s="34"/>
       <c r="E825" s="34"/>
@@ -54599,8 +54936,8 @@
       </c>
     </row>
     <row r="826">
-      <c r="A826" s="76"/>
-      <c r="B826" s="77"/>
+      <c r="A826" s="77"/>
+      <c r="B826" s="78"/>
       <c r="C826" s="34"/>
       <c r="D826" s="34"/>
       <c r="E826" s="34"/>
@@ -54625,8 +54962,8 @@
       </c>
     </row>
     <row r="827">
-      <c r="A827" s="76"/>
-      <c r="B827" s="77"/>
+      <c r="A827" s="77"/>
+      <c r="B827" s="78"/>
       <c r="C827" s="34"/>
       <c r="D827" s="34"/>
       <c r="E827" s="34"/>
@@ -54651,8 +54988,8 @@
       </c>
     </row>
     <row r="828">
-      <c r="A828" s="76"/>
-      <c r="B828" s="77"/>
+      <c r="A828" s="77"/>
+      <c r="B828" s="78"/>
       <c r="C828" s="34"/>
       <c r="D828" s="34"/>
       <c r="E828" s="34"/>
@@ -54677,8 +55014,8 @@
       </c>
     </row>
     <row r="829">
-      <c r="A829" s="76"/>
-      <c r="B829" s="77"/>
+      <c r="A829" s="77"/>
+      <c r="B829" s="78"/>
       <c r="C829" s="34"/>
       <c r="D829" s="34"/>
       <c r="E829" s="34"/>
@@ -54703,8 +55040,8 @@
       </c>
     </row>
     <row r="830">
-      <c r="A830" s="76"/>
-      <c r="B830" s="77"/>
+      <c r="A830" s="77"/>
+      <c r="B830" s="78"/>
       <c r="C830" s="34"/>
       <c r="D830" s="34"/>
       <c r="E830" s="34"/>
@@ -54729,8 +55066,8 @@
       </c>
     </row>
     <row r="831">
-      <c r="A831" s="76"/>
-      <c r="B831" s="77"/>
+      <c r="A831" s="77"/>
+      <c r="B831" s="78"/>
       <c r="C831" s="34"/>
       <c r="D831" s="34"/>
       <c r="E831" s="34"/>
@@ -54755,8 +55092,8 @@
       </c>
     </row>
     <row r="832">
-      <c r="A832" s="76"/>
-      <c r="B832" s="77"/>
+      <c r="A832" s="77"/>
+      <c r="B832" s="78"/>
       <c r="C832" s="34"/>
       <c r="D832" s="34"/>
       <c r="E832" s="34"/>
@@ -54781,8 +55118,8 @@
       </c>
     </row>
     <row r="833">
-      <c r="A833" s="76"/>
-      <c r="B833" s="77"/>
+      <c r="A833" s="77"/>
+      <c r="B833" s="78"/>
       <c r="C833" s="34"/>
       <c r="D833" s="34"/>
       <c r="E833" s="34"/>
@@ -54807,8 +55144,8 @@
       </c>
     </row>
     <row r="834">
-      <c r="A834" s="76"/>
-      <c r="B834" s="77"/>
+      <c r="A834" s="77"/>
+      <c r="B834" s="78"/>
       <c r="C834" s="34"/>
       <c r="D834" s="34"/>
       <c r="E834" s="34"/>
@@ -54833,8 +55170,8 @@
       </c>
     </row>
     <row r="835">
-      <c r="A835" s="76"/>
-      <c r="B835" s="77"/>
+      <c r="A835" s="77"/>
+      <c r="B835" s="78"/>
       <c r="C835" s="34"/>
       <c r="D835" s="34"/>
       <c r="E835" s="34"/>
@@ -54859,8 +55196,8 @@
       </c>
     </row>
     <row r="836">
-      <c r="A836" s="76"/>
-      <c r="B836" s="77"/>
+      <c r="A836" s="77"/>
+      <c r="B836" s="78"/>
       <c r="C836" s="34"/>
       <c r="D836" s="34"/>
       <c r="E836" s="34"/>
@@ -54885,8 +55222,8 @@
       </c>
     </row>
     <row r="837">
-      <c r="A837" s="76"/>
-      <c r="B837" s="77"/>
+      <c r="A837" s="77"/>
+      <c r="B837" s="78"/>
       <c r="C837" s="34"/>
       <c r="D837" s="34"/>
       <c r="E837" s="34"/>
@@ -54911,8 +55248,8 @@
       </c>
     </row>
     <row r="838">
-      <c r="A838" s="76"/>
-      <c r="B838" s="77"/>
+      <c r="A838" s="77"/>
+      <c r="B838" s="78"/>
       <c r="C838" s="34"/>
       <c r="D838" s="34"/>
       <c r="E838" s="34"/>
@@ -54937,8 +55274,8 @@
       </c>
     </row>
     <row r="839">
-      <c r="A839" s="76"/>
-      <c r="B839" s="77"/>
+      <c r="A839" s="77"/>
+      <c r="B839" s="78"/>
       <c r="C839" s="34"/>
       <c r="D839" s="34"/>
       <c r="E839" s="34"/>
@@ -54963,8 +55300,8 @@
       </c>
     </row>
     <row r="840">
-      <c r="A840" s="76"/>
-      <c r="B840" s="77"/>
+      <c r="A840" s="77"/>
+      <c r="B840" s="78"/>
       <c r="C840" s="34"/>
       <c r="D840" s="34"/>
       <c r="E840" s="34"/>
@@ -54989,8 +55326,8 @@
       </c>
     </row>
     <row r="841">
-      <c r="A841" s="76"/>
-      <c r="B841" s="77"/>
+      <c r="A841" s="77"/>
+      <c r="B841" s="78"/>
       <c r="C841" s="34"/>
       <c r="D841" s="34"/>
       <c r="E841" s="34"/>
@@ -55015,8 +55352,8 @@
       </c>
     </row>
     <row r="842">
-      <c r="A842" s="76"/>
-      <c r="B842" s="77"/>
+      <c r="A842" s="77"/>
+      <c r="B842" s="78"/>
       <c r="C842" s="34"/>
       <c r="D842" s="34"/>
       <c r="E842" s="34"/>
@@ -55041,8 +55378,8 @@
       </c>
     </row>
     <row r="843">
-      <c r="A843" s="76"/>
-      <c r="B843" s="77"/>
+      <c r="A843" s="77"/>
+      <c r="B843" s="78"/>
       <c r="C843" s="34"/>
       <c r="D843" s="34"/>
       <c r="E843" s="34"/>
@@ -55067,8 +55404,8 @@
       </c>
     </row>
     <row r="844">
-      <c r="A844" s="76"/>
-      <c r="B844" s="77"/>
+      <c r="A844" s="77"/>
+      <c r="B844" s="78"/>
       <c r="C844" s="34"/>
       <c r="D844" s="34"/>
       <c r="E844" s="34"/>
@@ -55093,8 +55430,8 @@
       </c>
     </row>
     <row r="845">
-      <c r="A845" s="76"/>
-      <c r="B845" s="77"/>
+      <c r="A845" s="77"/>
+      <c r="B845" s="78"/>
       <c r="C845" s="34"/>
       <c r="D845" s="34"/>
       <c r="E845" s="34"/>
@@ -55119,8 +55456,8 @@
       </c>
     </row>
     <row r="846">
-      <c r="A846" s="76"/>
-      <c r="B846" s="77"/>
+      <c r="A846" s="77"/>
+      <c r="B846" s="78"/>
       <c r="C846" s="34"/>
       <c r="D846" s="34"/>
       <c r="E846" s="34"/>
@@ -55145,8 +55482,8 @@
       </c>
     </row>
     <row r="847">
-      <c r="A847" s="76"/>
-      <c r="B847" s="77"/>
+      <c r="A847" s="77"/>
+      <c r="B847" s="78"/>
       <c r="C847" s="34"/>
       <c r="D847" s="34"/>
       <c r="E847" s="34"/>
@@ -55171,8 +55508,8 @@
       </c>
     </row>
     <row r="848">
-      <c r="A848" s="76"/>
-      <c r="B848" s="77"/>
+      <c r="A848" s="77"/>
+      <c r="B848" s="78"/>
       <c r="C848" s="34"/>
       <c r="D848" s="34"/>
       <c r="E848" s="34"/>
@@ -55197,8 +55534,8 @@
       </c>
     </row>
     <row r="849">
-      <c r="A849" s="76"/>
-      <c r="B849" s="77"/>
+      <c r="A849" s="77"/>
+      <c r="B849" s="78"/>
       <c r="C849" s="34"/>
       <c r="D849" s="34"/>
       <c r="E849" s="34"/>
@@ -55223,8 +55560,8 @@
       </c>
     </row>
     <row r="850">
-      <c r="A850" s="76"/>
-      <c r="B850" s="77"/>
+      <c r="A850" s="77"/>
+      <c r="B850" s="78"/>
       <c r="C850" s="34"/>
       <c r="D850" s="34"/>
       <c r="E850" s="34"/>
@@ -55249,8 +55586,8 @@
       </c>
     </row>
     <row r="851">
-      <c r="A851" s="76"/>
-      <c r="B851" s="77"/>
+      <c r="A851" s="77"/>
+      <c r="B851" s="78"/>
       <c r="C851" s="34"/>
       <c r="D851" s="34"/>
       <c r="E851" s="34"/>
@@ -55275,8 +55612,8 @@
       </c>
     </row>
     <row r="852">
-      <c r="A852" s="76"/>
-      <c r="B852" s="77"/>
+      <c r="A852" s="77"/>
+      <c r="B852" s="78"/>
       <c r="C852" s="34"/>
       <c r="D852" s="34"/>
       <c r="E852" s="34"/>
@@ -55301,8 +55638,8 @@
       </c>
     </row>
     <row r="853">
-      <c r="A853" s="76"/>
-      <c r="B853" s="77"/>
+      <c r="A853" s="77"/>
+      <c r="B853" s="78"/>
       <c r="C853" s="34"/>
       <c r="D853" s="34"/>
       <c r="E853" s="34"/>
@@ -55327,8 +55664,8 @@
       </c>
     </row>
     <row r="854">
-      <c r="A854" s="76"/>
-      <c r="B854" s="77"/>
+      <c r="A854" s="77"/>
+      <c r="B854" s="78"/>
       <c r="C854" s="34"/>
       <c r="D854" s="34"/>
       <c r="E854" s="34"/>
@@ -55353,8 +55690,8 @@
       </c>
     </row>
     <row r="855">
-      <c r="A855" s="76"/>
-      <c r="B855" s="77"/>
+      <c r="A855" s="77"/>
+      <c r="B855" s="78"/>
       <c r="C855" s="34"/>
       <c r="D855" s="34"/>
       <c r="E855" s="34"/>
@@ -55379,8 +55716,8 @@
       </c>
     </row>
     <row r="856">
-      <c r="A856" s="76"/>
-      <c r="B856" s="77"/>
+      <c r="A856" s="77"/>
+      <c r="B856" s="78"/>
       <c r="C856" s="34"/>
       <c r="D856" s="34"/>
       <c r="E856" s="34"/>
@@ -55405,8 +55742,8 @@
       </c>
     </row>
     <row r="857">
-      <c r="A857" s="76"/>
-      <c r="B857" s="77"/>
+      <c r="A857" s="77"/>
+      <c r="B857" s="78"/>
       <c r="C857" s="34"/>
       <c r="D857" s="34"/>
       <c r="E857" s="34"/>
@@ -55431,8 +55768,8 @@
       </c>
     </row>
     <row r="858">
-      <c r="A858" s="76"/>
-      <c r="B858" s="77"/>
+      <c r="A858" s="77"/>
+      <c r="B858" s="78"/>
       <c r="C858" s="34"/>
       <c r="D858" s="34"/>
       <c r="E858" s="34"/>
@@ -55457,8 +55794,8 @@
       </c>
     </row>
     <row r="859">
-      <c r="A859" s="76"/>
-      <c r="B859" s="77"/>
+      <c r="A859" s="77"/>
+      <c r="B859" s="78"/>
       <c r="C859" s="34"/>
       <c r="D859" s="34"/>
       <c r="E859" s="34"/>
@@ -55483,8 +55820,8 @@
       </c>
     </row>
     <row r="860">
-      <c r="A860" s="76"/>
-      <c r="B860" s="77"/>
+      <c r="A860" s="77"/>
+      <c r="B860" s="78"/>
       <c r="C860" s="34"/>
       <c r="D860" s="34"/>
       <c r="E860" s="34"/>
@@ -55509,8 +55846,8 @@
       </c>
     </row>
     <row r="861">
-      <c r="A861" s="76"/>
-      <c r="B861" s="77"/>
+      <c r="A861" s="77"/>
+      <c r="B861" s="78"/>
       <c r="C861" s="34"/>
       <c r="D861" s="34"/>
       <c r="E861" s="34"/>
@@ -55535,8 +55872,8 @@
       </c>
     </row>
     <row r="862">
-      <c r="A862" s="76"/>
-      <c r="B862" s="77"/>
+      <c r="A862" s="77"/>
+      <c r="B862" s="78"/>
       <c r="C862" s="34"/>
       <c r="D862" s="34"/>
       <c r="E862" s="34"/>
@@ -55561,8 +55898,8 @@
       </c>
     </row>
     <row r="863">
-      <c r="A863" s="76"/>
-      <c r="B863" s="77"/>
+      <c r="A863" s="77"/>
+      <c r="B863" s="78"/>
       <c r="C863" s="34"/>
       <c r="D863" s="34"/>
       <c r="E863" s="34"/>
@@ -55587,8 +55924,8 @@
       </c>
     </row>
     <row r="864">
-      <c r="A864" s="76"/>
-      <c r="B864" s="77"/>
+      <c r="A864" s="77"/>
+      <c r="B864" s="78"/>
       <c r="C864" s="34"/>
       <c r="D864" s="34"/>
       <c r="E864" s="34"/>
@@ -55613,8 +55950,8 @@
       </c>
     </row>
     <row r="865">
-      <c r="A865" s="76"/>
-      <c r="B865" s="77"/>
+      <c r="A865" s="77"/>
+      <c r="B865" s="78"/>
       <c r="C865" s="34"/>
       <c r="D865" s="34"/>
       <c r="E865" s="34"/>
@@ -55639,8 +55976,8 @@
       </c>
     </row>
     <row r="866">
-      <c r="A866" s="76"/>
-      <c r="B866" s="77"/>
+      <c r="A866" s="77"/>
+      <c r="B866" s="78"/>
       <c r="C866" s="34"/>
       <c r="D866" s="34"/>
       <c r="E866" s="34"/>
@@ -55665,8 +56002,8 @@
       </c>
     </row>
     <row r="867">
-      <c r="A867" s="76"/>
-      <c r="B867" s="77"/>
+      <c r="A867" s="77"/>
+      <c r="B867" s="78"/>
       <c r="C867" s="34"/>
       <c r="D867" s="34"/>
       <c r="E867" s="34"/>
@@ -55691,8 +56028,8 @@
       </c>
     </row>
     <row r="868">
-      <c r="A868" s="76"/>
-      <c r="B868" s="77"/>
+      <c r="A868" s="77"/>
+      <c r="B868" s="78"/>
       <c r="C868" s="34"/>
       <c r="D868" s="34"/>
       <c r="E868" s="34"/>
@@ -55717,8 +56054,8 @@
       </c>
     </row>
     <row r="869">
-      <c r="A869" s="76"/>
-      <c r="B869" s="77"/>
+      <c r="A869" s="77"/>
+      <c r="B869" s="78"/>
       <c r="C869" s="34"/>
       <c r="D869" s="34"/>
       <c r="E869" s="34"/>
@@ -55743,8 +56080,8 @@
       </c>
     </row>
     <row r="870">
-      <c r="A870" s="76"/>
-      <c r="B870" s="77"/>
+      <c r="A870" s="77"/>
+      <c r="B870" s="78"/>
       <c r="C870" s="34"/>
       <c r="D870" s="34"/>
       <c r="E870" s="34"/>
@@ -55769,8 +56106,8 @@
       </c>
     </row>
     <row r="871">
-      <c r="A871" s="76"/>
-      <c r="B871" s="77"/>
+      <c r="A871" s="77"/>
+      <c r="B871" s="78"/>
       <c r="C871" s="34"/>
       <c r="D871" s="34"/>
       <c r="E871" s="34"/>
@@ -55795,8 +56132,8 @@
       </c>
     </row>
     <row r="872">
-      <c r="A872" s="76"/>
-      <c r="B872" s="77"/>
+      <c r="A872" s="77"/>
+      <c r="B872" s="78"/>
       <c r="C872" s="34"/>
       <c r="D872" s="34"/>
       <c r="E872" s="34"/>
@@ -55821,8 +56158,8 @@
       </c>
     </row>
     <row r="873">
-      <c r="A873" s="76"/>
-      <c r="B873" s="77"/>
+      <c r="A873" s="77"/>
+      <c r="B873" s="78"/>
       <c r="C873" s="34"/>
       <c r="D873" s="34"/>
       <c r="E873" s="34"/>
@@ -55847,8 +56184,8 @@
       </c>
     </row>
     <row r="874">
-      <c r="A874" s="76"/>
-      <c r="B874" s="77"/>
+      <c r="A874" s="77"/>
+      <c r="B874" s="78"/>
       <c r="C874" s="34"/>
       <c r="D874" s="34"/>
       <c r="E874" s="34"/>
@@ -55873,8 +56210,8 @@
       </c>
     </row>
     <row r="875">
-      <c r="A875" s="76"/>
-      <c r="B875" s="77"/>
+      <c r="A875" s="77"/>
+      <c r="B875" s="78"/>
       <c r="C875" s="34"/>
       <c r="D875" s="34"/>
       <c r="E875" s="34"/>
@@ -55899,8 +56236,8 @@
       </c>
     </row>
     <row r="876">
-      <c r="A876" s="76"/>
-      <c r="B876" s="77"/>
+      <c r="A876" s="77"/>
+      <c r="B876" s="78"/>
       <c r="C876" s="34"/>
       <c r="D876" s="34"/>
       <c r="E876" s="34"/>
@@ -55925,8 +56262,8 @@
       </c>
     </row>
     <row r="877">
-      <c r="A877" s="76"/>
-      <c r="B877" s="77"/>
+      <c r="A877" s="77"/>
+      <c r="B877" s="78"/>
       <c r="C877" s="34"/>
       <c r="D877" s="34"/>
       <c r="E877" s="34"/>
@@ -55951,8 +56288,8 @@
       </c>
     </row>
     <row r="878">
-      <c r="A878" s="76"/>
-      <c r="B878" s="77"/>
+      <c r="A878" s="77"/>
+      <c r="B878" s="78"/>
       <c r="C878" s="34"/>
       <c r="D878" s="34"/>
       <c r="E878" s="34"/>
@@ -55977,8 +56314,8 @@
       </c>
     </row>
     <row r="879">
-      <c r="A879" s="76"/>
-      <c r="B879" s="77"/>
+      <c r="A879" s="77"/>
+      <c r="B879" s="78"/>
       <c r="C879" s="34"/>
       <c r="D879" s="34"/>
       <c r="E879" s="34"/>
@@ -56003,8 +56340,8 @@
       </c>
     </row>
     <row r="880">
-      <c r="A880" s="76"/>
-      <c r="B880" s="77"/>
+      <c r="A880" s="77"/>
+      <c r="B880" s="78"/>
       <c r="C880" s="34"/>
       <c r="D880" s="34"/>
       <c r="E880" s="34"/>
@@ -56029,8 +56366,8 @@
       </c>
     </row>
     <row r="881">
-      <c r="A881" s="76"/>
-      <c r="B881" s="77"/>
+      <c r="A881" s="77"/>
+      <c r="B881" s="78"/>
       <c r="C881" s="34"/>
       <c r="D881" s="34"/>
       <c r="E881" s="34"/>
@@ -56055,8 +56392,8 @@
       </c>
     </row>
     <row r="882">
-      <c r="A882" s="76"/>
-      <c r="B882" s="77"/>
+      <c r="A882" s="77"/>
+      <c r="B882" s="78"/>
       <c r="C882" s="34"/>
       <c r="D882" s="34"/>
       <c r="E882" s="34"/>
@@ -56081,8 +56418,8 @@
       </c>
     </row>
     <row r="883">
-      <c r="A883" s="76"/>
-      <c r="B883" s="77"/>
+      <c r="A883" s="77"/>
+      <c r="B883" s="78"/>
       <c r="C883" s="34"/>
       <c r="D883" s="34"/>
       <c r="E883" s="34"/>
@@ -56107,8 +56444,8 @@
       </c>
     </row>
     <row r="884">
-      <c r="A884" s="76"/>
-      <c r="B884" s="77"/>
+      <c r="A884" s="77"/>
+      <c r="B884" s="78"/>
       <c r="C884" s="34"/>
       <c r="D884" s="34"/>
       <c r="E884" s="34"/>
@@ -56133,8 +56470,8 @@
       </c>
     </row>
     <row r="885">
-      <c r="A885" s="76"/>
-      <c r="B885" s="77"/>
+      <c r="A885" s="77"/>
+      <c r="B885" s="78"/>
       <c r="C885" s="34"/>
       <c r="D885" s="34"/>
       <c r="E885" s="34"/>
@@ -56159,8 +56496,8 @@
       </c>
     </row>
     <row r="886">
-      <c r="A886" s="76"/>
-      <c r="B886" s="77"/>
+      <c r="A886" s="77"/>
+      <c r="B886" s="78"/>
       <c r="C886" s="34"/>
       <c r="D886" s="34"/>
       <c r="E886" s="34"/>
@@ -56185,8 +56522,8 @@
       </c>
     </row>
     <row r="887">
-      <c r="A887" s="76"/>
-      <c r="B887" s="77"/>
+      <c r="A887" s="77"/>
+      <c r="B887" s="78"/>
       <c r="C887" s="34"/>
       <c r="D887" s="34"/>
       <c r="E887" s="34"/>
@@ -56211,8 +56548,8 @@
       </c>
     </row>
     <row r="888">
-      <c r="A888" s="76"/>
-      <c r="B888" s="77"/>
+      <c r="A888" s="77"/>
+      <c r="B888" s="78"/>
       <c r="C888" s="34"/>
       <c r="D888" s="34"/>
       <c r="E888" s="34"/>
@@ -56237,8 +56574,8 @@
       </c>
     </row>
     <row r="889">
-      <c r="A889" s="76"/>
-      <c r="B889" s="77"/>
+      <c r="A889" s="77"/>
+      <c r="B889" s="78"/>
       <c r="C889" s="34"/>
       <c r="D889" s="34"/>
       <c r="E889" s="34"/>
@@ -56263,8 +56600,8 @@
       </c>
     </row>
     <row r="890">
-      <c r="A890" s="76"/>
-      <c r="B890" s="77"/>
+      <c r="A890" s="77"/>
+      <c r="B890" s="78"/>
       <c r="C890" s="34"/>
       <c r="D890" s="34"/>
       <c r="E890" s="34"/>
@@ -56289,8 +56626,8 @@
       </c>
     </row>
     <row r="891">
-      <c r="A891" s="76"/>
-      <c r="B891" s="77"/>
+      <c r="A891" s="77"/>
+      <c r="B891" s="78"/>
       <c r="C891" s="34"/>
       <c r="D891" s="34"/>
       <c r="E891" s="34"/>
@@ -56315,8 +56652,8 @@
       </c>
     </row>
     <row r="892">
-      <c r="A892" s="76"/>
-      <c r="B892" s="77"/>
+      <c r="A892" s="77"/>
+      <c r="B892" s="78"/>
       <c r="C892" s="34"/>
       <c r="D892" s="34"/>
       <c r="E892" s="34"/>
@@ -56341,8 +56678,8 @@
       </c>
     </row>
     <row r="893">
-      <c r="A893" s="76"/>
-      <c r="B893" s="77"/>
+      <c r="A893" s="77"/>
+      <c r="B893" s="78"/>
       <c r="C893" s="34"/>
       <c r="D893" s="34"/>
       <c r="E893" s="34"/>
@@ -56367,8 +56704,8 @@
       </c>
     </row>
     <row r="894">
-      <c r="A894" s="76"/>
-      <c r="B894" s="77"/>
+      <c r="A894" s="77"/>
+      <c r="B894" s="78"/>
       <c r="C894" s="34"/>
       <c r="D894" s="34"/>
       <c r="E894" s="34"/>
@@ -56393,8 +56730,8 @@
       </c>
     </row>
     <row r="895">
-      <c r="A895" s="76"/>
-      <c r="B895" s="77"/>
+      <c r="A895" s="77"/>
+      <c r="B895" s="78"/>
       <c r="C895" s="34"/>
       <c r="D895" s="34"/>
       <c r="E895" s="34"/>
@@ -56419,8 +56756,8 @@
       </c>
     </row>
     <row r="896">
-      <c r="A896" s="76"/>
-      <c r="B896" s="77"/>
+      <c r="A896" s="77"/>
+      <c r="B896" s="78"/>
       <c r="C896" s="34"/>
       <c r="D896" s="34"/>
       <c r="E896" s="34"/>
@@ -56445,8 +56782,8 @@
       </c>
     </row>
     <row r="897">
-      <c r="A897" s="76"/>
-      <c r="B897" s="77"/>
+      <c r="A897" s="77"/>
+      <c r="B897" s="78"/>
       <c r="C897" s="34"/>
       <c r="D897" s="34"/>
       <c r="E897" s="34"/>
@@ -56471,8 +56808,8 @@
       </c>
     </row>
     <row r="898">
-      <c r="A898" s="76"/>
-      <c r="B898" s="77"/>
+      <c r="A898" s="77"/>
+      <c r="B898" s="78"/>
       <c r="C898" s="34"/>
       <c r="D898" s="34"/>
       <c r="E898" s="34"/>
@@ -56497,8 +56834,8 @@
       </c>
     </row>
     <row r="899">
-      <c r="A899" s="76"/>
-      <c r="B899" s="77"/>
+      <c r="A899" s="77"/>
+      <c r="B899" s="78"/>
       <c r="C899" s="34"/>
       <c r="D899" s="34"/>
       <c r="E899" s="34"/>
@@ -56523,8 +56860,8 @@
       </c>
     </row>
     <row r="900">
-      <c r="A900" s="76"/>
-      <c r="B900" s="77"/>
+      <c r="A900" s="77"/>
+      <c r="B900" s="78"/>
       <c r="C900" s="34"/>
       <c r="D900" s="34"/>
       <c r="E900" s="34"/>
@@ -56549,8 +56886,8 @@
       </c>
     </row>
     <row r="901">
-      <c r="A901" s="76"/>
-      <c r="B901" s="77"/>
+      <c r="A901" s="77"/>
+      <c r="B901" s="78"/>
       <c r="C901" s="34"/>
       <c r="D901" s="34"/>
       <c r="E901" s="34"/>
@@ -56575,8 +56912,8 @@
       </c>
     </row>
     <row r="902">
-      <c r="A902" s="76"/>
-      <c r="B902" s="77"/>
+      <c r="A902" s="77"/>
+      <c r="B902" s="78"/>
       <c r="C902" s="34"/>
       <c r="D902" s="34"/>
       <c r="E902" s="34"/>
@@ -56601,8 +56938,8 @@
       </c>
     </row>
     <row r="903">
-      <c r="A903" s="76"/>
-      <c r="B903" s="77"/>
+      <c r="A903" s="77"/>
+      <c r="B903" s="78"/>
       <c r="C903" s="34"/>
       <c r="D903" s="34"/>
       <c r="E903" s="34"/>
@@ -56627,8 +56964,8 @@
       </c>
     </row>
     <row r="904">
-      <c r="A904" s="76"/>
-      <c r="B904" s="77"/>
+      <c r="A904" s="77"/>
+      <c r="B904" s="78"/>
       <c r="C904" s="34"/>
       <c r="D904" s="34"/>
       <c r="E904" s="34"/>
@@ -56653,8 +56990,8 @@
       </c>
     </row>
     <row r="905">
-      <c r="A905" s="76"/>
-      <c r="B905" s="77"/>
+      <c r="A905" s="77"/>
+      <c r="B905" s="78"/>
       <c r="C905" s="34"/>
       <c r="D905" s="34"/>
       <c r="E905" s="34"/>
@@ -56679,8 +57016,8 @@
       </c>
     </row>
     <row r="906">
-      <c r="A906" s="76"/>
-      <c r="B906" s="77"/>
+      <c r="A906" s="77"/>
+      <c r="B906" s="78"/>
       <c r="C906" s="34"/>
       <c r="D906" s="34"/>
       <c r="E906" s="34"/>
@@ -56705,8 +57042,8 @@
       </c>
     </row>
     <row r="907">
-      <c r="A907" s="76"/>
-      <c r="B907" s="77"/>
+      <c r="A907" s="77"/>
+      <c r="B907" s="78"/>
       <c r="C907" s="34"/>
       <c r="D907" s="34"/>
       <c r="E907" s="34"/>
@@ -56731,8 +57068,8 @@
       </c>
     </row>
     <row r="908">
-      <c r="A908" s="76"/>
-      <c r="B908" s="77"/>
+      <c r="A908" s="77"/>
+      <c r="B908" s="78"/>
       <c r="C908" s="34"/>
       <c r="D908" s="34"/>
       <c r="E908" s="34"/>
@@ -56757,8 +57094,8 @@
       </c>
     </row>
     <row r="909">
-      <c r="A909" s="76"/>
-      <c r="B909" s="77"/>
+      <c r="A909" s="77"/>
+      <c r="B909" s="78"/>
       <c r="C909" s="34"/>
       <c r="D909" s="34"/>
       <c r="E909" s="34"/>
@@ -56783,8 +57120,8 @@
       </c>
     </row>
     <row r="910">
-      <c r="A910" s="76"/>
-      <c r="B910" s="77"/>
+      <c r="A910" s="77"/>
+      <c r="B910" s="78"/>
       <c r="C910" s="34"/>
       <c r="D910" s="34"/>
       <c r="E910" s="34"/>
@@ -56809,8 +57146,8 @@
       </c>
     </row>
     <row r="911">
-      <c r="A911" s="76"/>
-      <c r="B911" s="77"/>
+      <c r="A911" s="77"/>
+      <c r="B911" s="78"/>
       <c r="C911" s="34"/>
       <c r="D911" s="34"/>
       <c r="E911" s="34"/>
@@ -56835,8 +57172,8 @@
       </c>
     </row>
     <row r="912">
-      <c r="A912" s="76"/>
-      <c r="B912" s="77"/>
+      <c r="A912" s="77"/>
+      <c r="B912" s="78"/>
       <c r="C912" s="34"/>
       <c r="D912" s="34"/>
       <c r="E912" s="34"/>
@@ -56861,8 +57198,8 @@
       </c>
     </row>
     <row r="913">
-      <c r="A913" s="76"/>
-      <c r="B913" s="77"/>
+      <c r="A913" s="77"/>
+      <c r="B913" s="78"/>
       <c r="C913" s="34"/>
       <c r="D913" s="34"/>
       <c r="E913" s="34"/>
@@ -56887,8 +57224,8 @@
       </c>
     </row>
     <row r="914">
-      <c r="A914" s="76"/>
-      <c r="B914" s="77"/>
+      <c r="A914" s="77"/>
+      <c r="B914" s="78"/>
       <c r="C914" s="34"/>
       <c r="D914" s="34"/>
       <c r="E914" s="34"/>
@@ -56913,8 +57250,8 @@
       </c>
     </row>
     <row r="915">
-      <c r="A915" s="76"/>
-      <c r="B915" s="77"/>
+      <c r="A915" s="77"/>
+      <c r="B915" s="78"/>
       <c r="C915" s="34"/>
       <c r="D915" s="34"/>
       <c r="E915" s="34"/>
@@ -56939,8 +57276,8 @@
       </c>
     </row>
     <row r="916">
-      <c r="A916" s="76"/>
-      <c r="B916" s="77"/>
+      <c r="A916" s="77"/>
+      <c r="B916" s="78"/>
       <c r="C916" s="34"/>
       <c r="D916" s="34"/>
       <c r="E916" s="34"/>
@@ -56965,8 +57302,8 @@
       </c>
     </row>
     <row r="917">
-      <c r="A917" s="76"/>
-      <c r="B917" s="77"/>
+      <c r="A917" s="77"/>
+      <c r="B917" s="78"/>
       <c r="C917" s="34"/>
       <c r="D917" s="34"/>
       <c r="E917" s="34"/>
@@ -56991,8 +57328,8 @@
       </c>
     </row>
     <row r="918">
-      <c r="A918" s="76"/>
-      <c r="B918" s="77"/>
+      <c r="A918" s="77"/>
+      <c r="B918" s="78"/>
       <c r="C918" s="34"/>
       <c r="D918" s="34"/>
       <c r="E918" s="34"/>
@@ -57017,8 +57354,8 @@
       </c>
     </row>
     <row r="919">
-      <c r="A919" s="76"/>
-      <c r="B919" s="77"/>
+      <c r="A919" s="77"/>
+      <c r="B919" s="78"/>
       <c r="C919" s="34"/>
       <c r="D919" s="34"/>
       <c r="E919" s="34"/>
@@ -57043,8 +57380,8 @@
       </c>
     </row>
     <row r="920">
-      <c r="A920" s="76"/>
-      <c r="B920" s="77"/>
+      <c r="A920" s="77"/>
+      <c r="B920" s="78"/>
       <c r="C920" s="34"/>
       <c r="D920" s="34"/>
       <c r="E920" s="34"/>
@@ -57069,8 +57406,8 @@
       </c>
     </row>
     <row r="921">
-      <c r="A921" s="76"/>
-      <c r="B921" s="77"/>
+      <c r="A921" s="77"/>
+      <c r="B921" s="78"/>
       <c r="C921" s="34"/>
       <c r="D921" s="34"/>
       <c r="E921" s="34"/>
@@ -57095,8 +57432,8 @@
       </c>
     </row>
     <row r="922">
-      <c r="A922" s="76"/>
-      <c r="B922" s="77"/>
+      <c r="A922" s="77"/>
+      <c r="B922" s="78"/>
       <c r="C922" s="34"/>
       <c r="D922" s="34"/>
       <c r="E922" s="34"/>
@@ -57121,8 +57458,8 @@
       </c>
     </row>
     <row r="923">
-      <c r="A923" s="76"/>
-      <c r="B923" s="77"/>
+      <c r="A923" s="77"/>
+      <c r="B923" s="78"/>
       <c r="C923" s="34"/>
       <c r="D923" s="34"/>
       <c r="E923" s="34"/>
@@ -57147,8 +57484,8 @@
       </c>
     </row>
     <row r="924">
-      <c r="A924" s="76"/>
-      <c r="B924" s="77"/>
+      <c r="A924" s="77"/>
+      <c r="B924" s="78"/>
       <c r="C924" s="34"/>
       <c r="D924" s="34"/>
       <c r="E924" s="34"/>
@@ -57173,8 +57510,8 @@
       </c>
     </row>
     <row r="925">
-      <c r="A925" s="76"/>
-      <c r="B925" s="77"/>
+      <c r="A925" s="77"/>
+      <c r="B925" s="78"/>
       <c r="C925" s="34"/>
       <c r="D925" s="34"/>
       <c r="E925" s="34"/>
@@ -57199,8 +57536,8 @@
       </c>
     </row>
     <row r="926">
-      <c r="A926" s="76"/>
-      <c r="B926" s="77"/>
+      <c r="A926" s="77"/>
+      <c r="B926" s="78"/>
       <c r="C926" s="34"/>
       <c r="D926" s="34"/>
       <c r="E926" s="34"/>
@@ -57225,8 +57562,8 @@
       </c>
     </row>
     <row r="927">
-      <c r="A927" s="76"/>
-      <c r="B927" s="77"/>
+      <c r="A927" s="77"/>
+      <c r="B927" s="78"/>
       <c r="C927" s="34"/>
       <c r="D927" s="34"/>
       <c r="E927" s="34"/>
@@ -57251,8 +57588,8 @@
       </c>
     </row>
     <row r="928">
-      <c r="A928" s="76"/>
-      <c r="B928" s="77"/>
+      <c r="A928" s="77"/>
+      <c r="B928" s="78"/>
       <c r="C928" s="34"/>
       <c r="D928" s="34"/>
       <c r="E928" s="34"/>
@@ -57277,8 +57614,8 @@
       </c>
     </row>
     <row r="929">
-      <c r="A929" s="76"/>
-      <c r="B929" s="77"/>
+      <c r="A929" s="77"/>
+      <c r="B929" s="78"/>
       <c r="C929" s="34"/>
       <c r="D929" s="34"/>
       <c r="E929" s="34"/>
@@ -57303,8 +57640,8 @@
       </c>
     </row>
     <row r="930">
-      <c r="A930" s="76"/>
-      <c r="B930" s="77"/>
+      <c r="A930" s="77"/>
+      <c r="B930" s="78"/>
       <c r="C930" s="34"/>
       <c r="D930" s="34"/>
       <c r="E930" s="34"/>
@@ -57329,8 +57666,8 @@
       </c>
     </row>
     <row r="931">
-      <c r="A931" s="76"/>
-      <c r="B931" s="77"/>
+      <c r="A931" s="77"/>
+      <c r="B931" s="78"/>
       <c r="C931" s="34"/>
       <c r="D931" s="34"/>
       <c r="E931" s="34"/>
@@ -57355,8 +57692,8 @@
       </c>
     </row>
     <row r="932">
-      <c r="A932" s="76"/>
-      <c r="B932" s="77"/>
+      <c r="A932" s="77"/>
+      <c r="B932" s="78"/>
       <c r="C932" s="34"/>
       <c r="D932" s="34"/>
       <c r="E932" s="34"/>
@@ -57381,8 +57718,8 @@
       </c>
     </row>
     <row r="933">
-      <c r="A933" s="76"/>
-      <c r="B933" s="77"/>
+      <c r="A933" s="77"/>
+      <c r="B933" s="78"/>
       <c r="C933" s="34"/>
       <c r="D933" s="34"/>
       <c r="E933" s="34"/>
@@ -57407,8 +57744,8 @@
       </c>
     </row>
     <row r="934">
-      <c r="A934" s="76"/>
-      <c r="B934" s="77"/>
+      <c r="A934" s="77"/>
+      <c r="B934" s="78"/>
       <c r="C934" s="34"/>
       <c r="D934" s="34"/>
       <c r="E934" s="34"/>
@@ -57433,8 +57770,8 @@
       </c>
     </row>
     <row r="935">
-      <c r="A935" s="76"/>
-      <c r="B935" s="77"/>
+      <c r="A935" s="77"/>
+      <c r="B935" s="78"/>
       <c r="C935" s="34"/>
       <c r="D935" s="34"/>
       <c r="E935" s="34"/>
@@ -57459,8 +57796,8 @@
       </c>
     </row>
     <row r="936">
-      <c r="A936" s="76"/>
-      <c r="B936" s="77"/>
+      <c r="A936" s="77"/>
+      <c r="B936" s="78"/>
       <c r="C936" s="34"/>
       <c r="D936" s="34"/>
       <c r="E936" s="34"/>
@@ -57485,8 +57822,8 @@
       </c>
     </row>
     <row r="937">
-      <c r="A937" s="76"/>
-      <c r="B937" s="77"/>
+      <c r="A937" s="77"/>
+      <c r="B937" s="78"/>
       <c r="C937" s="34"/>
       <c r="D937" s="34"/>
       <c r="E937" s="34"/>
@@ -57511,8 +57848,8 @@
       </c>
     </row>
     <row r="938">
-      <c r="A938" s="76"/>
-      <c r="B938" s="77"/>
+      <c r="A938" s="77"/>
+      <c r="B938" s="78"/>
       <c r="C938" s="34"/>
       <c r="D938" s="34"/>
       <c r="E938" s="34"/>
@@ -57537,8 +57874,8 @@
       </c>
     </row>
     <row r="939">
-      <c r="A939" s="76"/>
-      <c r="B939" s="77"/>
+      <c r="A939" s="77"/>
+      <c r="B939" s="78"/>
       <c r="C939" s="34"/>
       <c r="D939" s="34"/>
       <c r="E939" s="34"/>
@@ -57563,8 +57900,8 @@
       </c>
     </row>
     <row r="940">
-      <c r="A940" s="76"/>
-      <c r="B940" s="77"/>
+      <c r="A940" s="77"/>
+      <c r="B940" s="78"/>
       <c r="C940" s="34"/>
       <c r="D940" s="34"/>
       <c r="E940" s="34"/>
@@ -57589,8 +57926,8 @@
       </c>
     </row>
     <row r="941">
-      <c r="A941" s="76"/>
-      <c r="B941" s="77"/>
+      <c r="A941" s="77"/>
+      <c r="B941" s="78"/>
       <c r="C941" s="34"/>
       <c r="D941" s="34"/>
       <c r="E941" s="34"/>
@@ -57615,8 +57952,8 @@
       </c>
     </row>
     <row r="942">
-      <c r="A942" s="76"/>
-      <c r="B942" s="77"/>
+      <c r="A942" s="77"/>
+      <c r="B942" s="78"/>
       <c r="C942" s="34"/>
       <c r="D942" s="34"/>
       <c r="E942" s="34"/>
@@ -57641,8 +57978,8 @@
       </c>
     </row>
     <row r="943">
-      <c r="A943" s="76"/>
-      <c r="B943" s="77"/>
+      <c r="A943" s="77"/>
+      <c r="B943" s="78"/>
       <c r="C943" s="34"/>
       <c r="D943" s="34"/>
       <c r="E943" s="34"/>
@@ -57667,8 +58004,8 @@
       </c>
     </row>
     <row r="944">
-      <c r="A944" s="76"/>
-      <c r="B944" s="77"/>
+      <c r="A944" s="77"/>
+      <c r="B944" s="78"/>
       <c r="C944" s="34"/>
       <c r="D944" s="34"/>
       <c r="E944" s="34"/>
@@ -57693,8 +58030,8 @@
       </c>
     </row>
     <row r="945">
-      <c r="A945" s="76"/>
-      <c r="B945" s="77"/>
+      <c r="A945" s="77"/>
+      <c r="B945" s="78"/>
       <c r="C945" s="34"/>
       <c r="D945" s="34"/>
       <c r="E945" s="34"/>
@@ -57719,8 +58056,8 @@
       </c>
     </row>
     <row r="946">
-      <c r="A946" s="76"/>
-      <c r="B946" s="77"/>
+      <c r="A946" s="77"/>
+      <c r="B946" s="78"/>
       <c r="C946" s="34"/>
       <c r="D946" s="34"/>
       <c r="E946" s="34"/>
@@ -57745,8 +58082,8 @@
       </c>
     </row>
     <row r="947">
-      <c r="A947" s="76"/>
-      <c r="B947" s="77"/>
+      <c r="A947" s="77"/>
+      <c r="B947" s="78"/>
       <c r="C947" s="34"/>
       <c r="D947" s="34"/>
       <c r="E947" s="34"/>
@@ -57771,8 +58108,8 @@
       </c>
     </row>
     <row r="948">
-      <c r="A948" s="76"/>
-      <c r="B948" s="77"/>
+      <c r="A948" s="77"/>
+      <c r="B948" s="78"/>
       <c r="C948" s="34"/>
       <c r="D948" s="34"/>
       <c r="E948" s="34"/>
@@ -57797,8 +58134,8 @@
       </c>
     </row>
     <row r="949">
-      <c r="A949" s="76"/>
-      <c r="B949" s="77"/>
+      <c r="A949" s="77"/>
+      <c r="B949" s="78"/>
       <c r="C949" s="34"/>
       <c r="D949" s="34"/>
       <c r="E949" s="34"/>
@@ -57823,8 +58160,8 @@
       </c>
     </row>
     <row r="950">
-      <c r="A950" s="76"/>
-      <c r="B950" s="77"/>
+      <c r="A950" s="77"/>
+      <c r="B950" s="78"/>
       <c r="C950" s="34"/>
       <c r="D950" s="34"/>
       <c r="E950" s="34"/>
@@ -57849,8 +58186,8 @@
       </c>
     </row>
     <row r="951">
-      <c r="A951" s="76"/>
-      <c r="B951" s="77"/>
+      <c r="A951" s="77"/>
+      <c r="B951" s="78"/>
       <c r="C951" s="34"/>
       <c r="D951" s="34"/>
       <c r="E951" s="34"/>
@@ -57875,8 +58212,8 @@
       </c>
     </row>
     <row r="952">
-      <c r="A952" s="76"/>
-      <c r="B952" s="77"/>
+      <c r="A952" s="77"/>
+      <c r="B952" s="78"/>
       <c r="C952" s="34"/>
       <c r="D952" s="34"/>
       <c r="E952" s="34"/>
@@ -57901,8 +58238,8 @@
       </c>
     </row>
     <row r="953">
-      <c r="A953" s="76"/>
-      <c r="B953" s="77"/>
+      <c r="A953" s="77"/>
+      <c r="B953" s="78"/>
       <c r="C953" s="34"/>
       <c r="D953" s="34"/>
       <c r="E953" s="34"/>
@@ -57927,8 +58264,8 @@
       </c>
     </row>
     <row r="954">
-      <c r="A954" s="76"/>
-      <c r="B954" s="77"/>
+      <c r="A954" s="77"/>
+      <c r="B954" s="78"/>
       <c r="C954" s="34"/>
       <c r="D954" s="34"/>
       <c r="E954" s="34"/>
@@ -57953,8 +58290,8 @@
       </c>
     </row>
     <row r="955">
-      <c r="A955" s="76"/>
-      <c r="B955" s="77"/>
+      <c r="A955" s="77"/>
+      <c r="B955" s="78"/>
       <c r="C955" s="34"/>
       <c r="D955" s="34"/>
       <c r="E955" s="34"/>
@@ -57979,8 +58316,8 @@
       </c>
     </row>
     <row r="956">
-      <c r="A956" s="76"/>
-      <c r="B956" s="77"/>
+      <c r="A956" s="77"/>
+      <c r="B956" s="78"/>
       <c r="C956" s="34"/>
       <c r="D956" s="34"/>
       <c r="E956" s="34"/>
@@ -58005,8 +58342,8 @@
       </c>
     </row>
     <row r="957">
-      <c r="A957" s="76"/>
-      <c r="B957" s="77"/>
+      <c r="A957" s="77"/>
+      <c r="B957" s="78"/>
       <c r="C957" s="34"/>
       <c r="D957" s="34"/>
       <c r="E957" s="34"/>
@@ -58031,8 +58368,8 @@
       </c>
     </row>
     <row r="958">
-      <c r="A958" s="76"/>
-      <c r="B958" s="77"/>
+      <c r="A958" s="77"/>
+      <c r="B958" s="78"/>
       <c r="C958" s="34"/>
       <c r="D958" s="34"/>
       <c r="E958" s="34"/>
@@ -58057,8 +58394,8 @@
       </c>
     </row>
     <row r="959">
-      <c r="A959" s="76"/>
-      <c r="B959" s="77"/>
+      <c r="A959" s="77"/>
+      <c r="B959" s="78"/>
       <c r="C959" s="34"/>
       <c r="D959" s="34"/>
       <c r="E959" s="34"/>
@@ -58083,8 +58420,8 @@
       </c>
     </row>
     <row r="960">
-      <c r="A960" s="76"/>
-      <c r="B960" s="77"/>
+      <c r="A960" s="77"/>
+      <c r="B960" s="78"/>
       <c r="C960" s="34"/>
       <c r="D960" s="34"/>
       <c r="E960" s="34"/>
@@ -58109,8 +58446,8 @@
       </c>
     </row>
     <row r="961">
-      <c r="A961" s="76"/>
-      <c r="B961" s="77"/>
+      <c r="A961" s="77"/>
+      <c r="B961" s="78"/>
       <c r="C961" s="34"/>
       <c r="D961" s="34"/>
       <c r="E961" s="34"/>
@@ -58135,8 +58472,8 @@
       </c>
     </row>
     <row r="962">
-      <c r="A962" s="76"/>
-      <c r="B962" s="77"/>
+      <c r="A962" s="77"/>
+      <c r="B962" s="78"/>
       <c r="C962" s="34"/>
       <c r="D962" s="34"/>
       <c r="E962" s="34"/>
@@ -58161,8 +58498,8 @@
       </c>
     </row>
     <row r="963">
-      <c r="A963" s="76"/>
-      <c r="B963" s="77"/>
+      <c r="A963" s="77"/>
+      <c r="B963" s="78"/>
       <c r="C963" s="34"/>
       <c r="D963" s="34"/>
       <c r="E963" s="34"/>
@@ -58187,8 +58524,8 @@
       </c>
     </row>
     <row r="964">
-      <c r="A964" s="76"/>
-      <c r="B964" s="77"/>
+      <c r="A964" s="77"/>
+      <c r="B964" s="78"/>
       <c r="C964" s="34"/>
       <c r="D964" s="34"/>
       <c r="E964" s="34"/>
@@ -58213,8 +58550,8 @@
       </c>
     </row>
     <row r="965">
-      <c r="A965" s="76"/>
-      <c r="B965" s="77"/>
+      <c r="A965" s="77"/>
+      <c r="B965" s="78"/>
       <c r="C965" s="34"/>
       <c r="D965" s="34"/>
       <c r="E965" s="34"/>
@@ -58239,8 +58576,8 @@
       </c>
     </row>
     <row r="966">
-      <c r="A966" s="76"/>
-      <c r="B966" s="77"/>
+      <c r="A966" s="77"/>
+      <c r="B966" s="78"/>
       <c r="C966" s="34"/>
       <c r="D966" s="34"/>
       <c r="E966" s="34"/>
@@ -58265,8 +58602,8 @@
       </c>
     </row>
     <row r="967">
-      <c r="A967" s="76"/>
-      <c r="B967" s="77"/>
+      <c r="A967" s="77"/>
+      <c r="B967" s="78"/>
       <c r="C967" s="34"/>
       <c r="D967" s="34"/>
       <c r="E967" s="34"/>
@@ -58291,8 +58628,8 @@
       </c>
     </row>
     <row r="968">
-      <c r="A968" s="76"/>
-      <c r="B968" s="77"/>
+      <c r="A968" s="77"/>
+      <c r="B968" s="78"/>
       <c r="C968" s="34"/>
       <c r="D968" s="34"/>
       <c r="E968" s="34"/>
@@ -58317,8 +58654,8 @@
       </c>
     </row>
     <row r="969">
-      <c r="A969" s="76"/>
-      <c r="B969" s="77"/>
+      <c r="A969" s="77"/>
+      <c r="B969" s="78"/>
       <c r="C969" s="34"/>
       <c r="D969" s="34"/>
       <c r="E969" s="34"/>
@@ -58343,8 +58680,8 @@
       </c>
     </row>
     <row r="970">
-      <c r="A970" s="76"/>
-      <c r="B970" s="77"/>
+      <c r="A970" s="77"/>
+      <c r="B970" s="78"/>
       <c r="C970" s="34"/>
       <c r="D970" s="34"/>
       <c r="E970" s="34"/>
@@ -58369,8 +58706,8 @@
       </c>
     </row>
     <row r="971">
-      <c r="A971" s="76"/>
-      <c r="B971" s="77"/>
+      <c r="A971" s="77"/>
+      <c r="B971" s="78"/>
       <c r="C971" s="34"/>
       <c r="D971" s="34"/>
       <c r="E971" s="34"/>
@@ -58395,8 +58732,8 @@
       </c>
     </row>
     <row r="972">
-      <c r="A972" s="76"/>
-      <c r="B972" s="77"/>
+      <c r="A972" s="77"/>
+      <c r="B972" s="78"/>
       <c r="C972" s="34"/>
       <c r="D972" s="34"/>
       <c r="E972" s="34"/>
@@ -58421,8 +58758,8 @@
       </c>
     </row>
     <row r="973">
-      <c r="A973" s="76"/>
-      <c r="B973" s="77"/>
+      <c r="A973" s="77"/>
+      <c r="B973" s="78"/>
       <c r="C973" s="34"/>
       <c r="D973" s="34"/>
       <c r="E973" s="34"/>
@@ -58447,8 +58784,8 @@
       </c>
     </row>
     <row r="974">
-      <c r="A974" s="76"/>
-      <c r="B974" s="77"/>
+      <c r="A974" s="77"/>
+      <c r="B974" s="78"/>
       <c r="C974" s="34"/>
       <c r="D974" s="34"/>
       <c r="E974" s="34"/>
@@ -58473,8 +58810,8 @@
       </c>
     </row>
     <row r="975">
-      <c r="A975" s="76"/>
-      <c r="B975" s="77"/>
+      <c r="A975" s="77"/>
+      <c r="B975" s="78"/>
       <c r="C975" s="34"/>
       <c r="D975" s="34"/>
       <c r="E975" s="34"/>
@@ -58499,8 +58836,8 @@
       </c>
     </row>
     <row r="976">
-      <c r="A976" s="76"/>
-      <c r="B976" s="77"/>
+      <c r="A976" s="77"/>
+      <c r="B976" s="78"/>
       <c r="C976" s="34"/>
       <c r="D976" s="34"/>
       <c r="E976" s="34"/>
@@ -58525,8 +58862,8 @@
       </c>
     </row>
     <row r="977">
-      <c r="A977" s="76"/>
-      <c r="B977" s="77"/>
+      <c r="A977" s="77"/>
+      <c r="B977" s="78"/>
       <c r="C977" s="34"/>
       <c r="D977" s="34"/>
       <c r="E977" s="34"/>
@@ -58551,8 +58888,8 @@
       </c>
     </row>
     <row r="978">
-      <c r="A978" s="76"/>
-      <c r="B978" s="77"/>
+      <c r="A978" s="77"/>
+      <c r="B978" s="78"/>
       <c r="C978" s="34"/>
       <c r="D978" s="34"/>
       <c r="E978" s="34"/>
@@ -58577,8 +58914,8 @@
       </c>
     </row>
     <row r="979">
-      <c r="A979" s="76"/>
-      <c r="B979" s="77"/>
+      <c r="A979" s="77"/>
+      <c r="B979" s="78"/>
       <c r="C979" s="34"/>
       <c r="D979" s="34"/>
       <c r="E979" s="34"/>
@@ -58603,8 +58940,8 @@
       </c>
     </row>
     <row r="980">
-      <c r="A980" s="76"/>
-      <c r="B980" s="77"/>
+      <c r="A980" s="77"/>
+      <c r="B980" s="78"/>
       <c r="C980" s="34"/>
       <c r="D980" s="34"/>
       <c r="E980" s="34"/>
@@ -58629,8 +58966,8 @@
       </c>
     </row>
     <row r="981">
-      <c r="A981" s="76"/>
-      <c r="B981" s="77"/>
+      <c r="A981" s="77"/>
+      <c r="B981" s="78"/>
       <c r="C981" s="34"/>
       <c r="D981" s="34"/>
       <c r="E981" s="34"/>
@@ -58655,8 +58992,8 @@
       </c>
     </row>
     <row r="982">
-      <c r="A982" s="76"/>
-      <c r="B982" s="77"/>
+      <c r="A982" s="77"/>
+      <c r="B982" s="78"/>
       <c r="C982" s="34"/>
       <c r="D982" s="34"/>
       <c r="E982" s="34"/>
@@ -58681,8 +59018,8 @@
       </c>
     </row>
     <row r="983">
-      <c r="A983" s="76"/>
-      <c r="B983" s="77"/>
+      <c r="A983" s="77"/>
+      <c r="B983" s="78"/>
       <c r="C983" s="34"/>
       <c r="D983" s="34"/>
       <c r="E983" s="34"/>
@@ -58707,8 +59044,8 @@
       </c>
     </row>
     <row r="984">
-      <c r="A984" s="76"/>
-      <c r="B984" s="77"/>
+      <c r="A984" s="77"/>
+      <c r="B984" s="78"/>
       <c r="C984" s="34"/>
       <c r="D984" s="34"/>
       <c r="E984" s="34"/>
@@ -58733,8 +59070,8 @@
       </c>
     </row>
     <row r="985">
-      <c r="A985" s="76"/>
-      <c r="B985" s="77"/>
+      <c r="A985" s="77"/>
+      <c r="B985" s="78"/>
       <c r="C985" s="34"/>
       <c r="D985" s="34"/>
       <c r="E985" s="34"/>
@@ -58759,8 +59096,8 @@
       </c>
     </row>
     <row r="986">
-      <c r="A986" s="76"/>
-      <c r="B986" s="77"/>
+      <c r="A986" s="77"/>
+      <c r="B986" s="78"/>
       <c r="C986" s="34"/>
       <c r="D986" s="34"/>
       <c r="E986" s="34"/>
@@ -58785,8 +59122,8 @@
       </c>
     </row>
     <row r="987">
-      <c r="A987" s="76"/>
-      <c r="B987" s="77"/>
+      <c r="A987" s="77"/>
+      <c r="B987" s="78"/>
       <c r="C987" s="34"/>
       <c r="D987" s="34"/>
       <c r="E987" s="34"/>
@@ -58811,8 +59148,8 @@
       </c>
     </row>
     <row r="988">
-      <c r="A988" s="76"/>
-      <c r="B988" s="77"/>
+      <c r="A988" s="77"/>
+      <c r="B988" s="78"/>
       <c r="C988" s="34"/>
       <c r="D988" s="34"/>
       <c r="E988" s="34"/>
@@ -58837,8 +59174,8 @@
       </c>
     </row>
     <row r="989">
-      <c r="A989" s="76"/>
-      <c r="B989" s="77"/>
+      <c r="A989" s="77"/>
+      <c r="B989" s="78"/>
       <c r="C989" s="34"/>
       <c r="D989" s="34"/>
       <c r="E989" s="34"/>
@@ -58863,8 +59200,8 @@
       </c>
     </row>
     <row r="990">
-      <c r="A990" s="76"/>
-      <c r="B990" s="77"/>
+      <c r="A990" s="77"/>
+      <c r="B990" s="78"/>
       <c r="C990" s="34"/>
       <c r="D990" s="34"/>
       <c r="E990" s="34"/>
@@ -58889,8 +59226,8 @@
       </c>
     </row>
     <row r="991">
-      <c r="A991" s="76"/>
-      <c r="B991" s="77"/>
+      <c r="A991" s="77"/>
+      <c r="B991" s="78"/>
       <c r="C991" s="34"/>
       <c r="D991" s="34"/>
       <c r="E991" s="34"/>
@@ -58915,8 +59252,8 @@
       </c>
     </row>
     <row r="992">
-      <c r="A992" s="76"/>
-      <c r="B992" s="77"/>
+      <c r="A992" s="77"/>
+      <c r="B992" s="78"/>
       <c r="C992" s="34"/>
       <c r="D992" s="34"/>
       <c r="E992" s="34"/>
@@ -58941,8 +59278,8 @@
       </c>
     </row>
     <row r="993">
-      <c r="A993" s="76"/>
-      <c r="B993" s="77"/>
+      <c r="A993" s="77"/>
+      <c r="B993" s="78"/>
       <c r="C993" s="34"/>
       <c r="D993" s="34"/>
       <c r="E993" s="34"/>
@@ -58967,8 +59304,8 @@
       </c>
     </row>
     <row r="994">
-      <c r="A994" s="76"/>
-      <c r="B994" s="77"/>
+      <c r="A994" s="77"/>
+      <c r="B994" s="78"/>
       <c r="C994" s="34"/>
       <c r="D994" s="34"/>
       <c r="E994" s="34"/>
@@ -58993,8 +59330,8 @@
       </c>
     </row>
     <row r="995">
-      <c r="A995" s="76"/>
-      <c r="B995" s="77"/>
+      <c r="A995" s="77"/>
+      <c r="B995" s="78"/>
       <c r="C995" s="34"/>
       <c r="D995" s="34"/>
       <c r="E995" s="34"/>
@@ -59019,8 +59356,8 @@
       </c>
     </row>
     <row r="996">
-      <c r="A996" s="76"/>
-      <c r="B996" s="77"/>
+      <c r="A996" s="77"/>
+      <c r="B996" s="78"/>
       <c r="C996" s="34"/>
       <c r="D996" s="34"/>
       <c r="E996" s="34"/>
@@ -59045,8 +59382,8 @@
       </c>
     </row>
     <row r="997">
-      <c r="A997" s="76"/>
-      <c r="B997" s="77"/>
+      <c r="A997" s="77"/>
+      <c r="B997" s="78"/>
       <c r="C997" s="34"/>
       <c r="D997" s="34"/>
       <c r="E997" s="34"/>
@@ -59071,8 +59408,8 @@
       </c>
     </row>
     <row r="998">
-      <c r="A998" s="76"/>
-      <c r="B998" s="77"/>
+      <c r="A998" s="77"/>
+      <c r="B998" s="78"/>
       <c r="C998" s="34"/>
       <c r="D998" s="34"/>
       <c r="E998" s="34"/>
@@ -59097,8 +59434,8 @@
       </c>
     </row>
     <row r="999">
-      <c r="A999" s="76"/>
-      <c r="B999" s="77"/>
+      <c r="A999" s="77"/>
+      <c r="B999" s="78"/>
       <c r="C999" s="34"/>
       <c r="D999" s="34"/>
       <c r="E999" s="34"/>
@@ -59123,8 +59460,8 @@
       </c>
     </row>
     <row r="1000">
-      <c r="A1000" s="76"/>
-      <c r="B1000" s="77"/>
+      <c r="A1000" s="77"/>
+      <c r="B1000" s="78"/>
       <c r="C1000" s="34"/>
       <c r="D1000" s="34"/>
       <c r="E1000" s="34"/>
@@ -59149,8 +59486,8 @@
       </c>
     </row>
     <row r="1001">
-      <c r="A1001" s="76"/>
-      <c r="B1001" s="77"/>
+      <c r="A1001" s="77"/>
+      <c r="B1001" s="78"/>
       <c r="C1001" s="34"/>
       <c r="D1001" s="34"/>
       <c r="E1001" s="34"/>
@@ -59850,15 +60187,23 @@
     <hyperlink r:id="rId288" ref="S725"/>
     <hyperlink r:id="rId289" ref="S726"/>
     <hyperlink r:id="rId290" ref="S727"/>
+    <hyperlink r:id="rId291" ref="S728"/>
+    <hyperlink r:id="rId292" ref="S729"/>
+    <hyperlink r:id="rId293" ref="S730"/>
+    <hyperlink r:id="rId294" ref="S731"/>
+    <hyperlink r:id="rId295" ref="S732"/>
+    <hyperlink r:id="rId296" ref="S733"/>
+    <hyperlink r:id="rId297" ref="S734"/>
+    <hyperlink r:id="rId298" ref="S735"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId291"/>
-  <legacyDrawing r:id="rId292"/>
+  <drawing r:id="rId299"/>
+  <legacyDrawing r:id="rId300"/>
   <tableParts count="2">
-    <tablePart r:id="rId295"/>
-    <tablePart r:id="rId296"/>
+    <tablePart r:id="rId303"/>
+    <tablePart r:id="rId304"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201214
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -582,7 +582,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8403" uniqueCount="2600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8441" uniqueCount="2611">
   <si>
     <t>案例</t>
   </si>
@@ -9351,6 +9351,44 @@
   </si>
   <si>
     <t>#734</t>
+  </si>
+  <si>
+    <t>#735</t>
+  </si>
+  <si>
+    <t>-11/24 印尼→台灣</t>
+  </si>
+  <si>
+    <t>12/10 採檢
+12/13 確診</t>
+  </si>
+  <si>
+    <t>船員，由公司安排自費採檢，於今日確診(Ct值30)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">新增3例境外移入COVID-19病例，皆自印尼入境 </t>
+  </si>
+  <si>
+    <t>#736</t>
+  </si>
+  <si>
+    <t>12/11 採檢
+12/13 確診</t>
+  </si>
+  <si>
+    <t>腹脹 嘔吐</t>
+  </si>
+  <si>
+    <t>#737</t>
+  </si>
+  <si>
+    <t>11/28 採檢
+12/8 二採
+12/10 三採
+12/13 確診</t>
+  </si>
+  <si>
+    <t>移工，由仲介安排自費採檢，於今日確診(Ct值36)</t>
   </si>
 </sst>
 </file>
@@ -52596,81 +52634,171 @@
       </c>
     </row>
     <row r="736">
-      <c r="A736" s="77"/>
-      <c r="B736" s="78"/>
-      <c r="C736" s="34"/>
-      <c r="D736" s="34"/>
-      <c r="E736" s="34"/>
+      <c r="A736" s="16" t="s">
+        <v>2600</v>
+      </c>
+      <c r="B736" s="6">
+        <v>44178.0</v>
+      </c>
+      <c r="C736" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D736" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E736" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F736" s="34"/>
-      <c r="G736" s="34"/>
-      <c r="H736" s="21"/>
-      <c r="I736" s="19"/>
-      <c r="J736" s="10"/>
-      <c r="K736" s="22"/>
-      <c r="L736" s="23"/>
-      <c r="M736" s="22"/>
+      <c r="G736" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H736" s="8" t="s">
+        <v>2601</v>
+      </c>
+      <c r="I736" s="9">
+        <v>44159.0</v>
+      </c>
+      <c r="J736" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K736" s="13" t="s">
+        <v>2602</v>
+      </c>
+      <c r="L736" s="12" t="s">
+        <v>1674</v>
+      </c>
+      <c r="M736" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N736" s="25"/>
-      <c r="O736" s="21"/>
-      <c r="P736" s="21"/>
+      <c r="O736" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P736" s="8" t="s">
+        <v>2603</v>
+      </c>
       <c r="Q736" s="19"/>
       <c r="R736" s="19"/>
-      <c r="S736" s="20"/>
+      <c r="S736" s="61" t="s">
+        <v>2604</v>
+      </c>
       <c r="T736" s="20"/>
       <c r="U736" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#735</v>
       </c>
     </row>
     <row r="737">
-      <c r="A737" s="77"/>
-      <c r="B737" s="78"/>
-      <c r="C737" s="34"/>
-      <c r="D737" s="34"/>
-      <c r="E737" s="34"/>
+      <c r="A737" s="16" t="s">
+        <v>2605</v>
+      </c>
+      <c r="B737" s="6">
+        <v>44178.0</v>
+      </c>
+      <c r="C737" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D737" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E737" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F737" s="34"/>
-      <c r="G737" s="34"/>
-      <c r="H737" s="21"/>
-      <c r="I737" s="19"/>
-      <c r="J737" s="10"/>
-      <c r="K737" s="22"/>
-      <c r="L737" s="23"/>
-      <c r="M737" s="22"/>
+      <c r="G737" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H737" s="8" t="s">
+        <v>2427</v>
+      </c>
+      <c r="I737" s="9">
+        <v>44163.0</v>
+      </c>
+      <c r="J737" s="10">
+        <v>44175.0</v>
+      </c>
+      <c r="K737" s="13" t="s">
+        <v>2606</v>
+      </c>
+      <c r="L737" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M737" s="13" t="s">
+        <v>2607</v>
+      </c>
       <c r="N737" s="25"/>
-      <c r="O737" s="21"/>
-      <c r="P737" s="21"/>
+      <c r="O737" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P737" s="8" t="s">
+        <v>1777</v>
+      </c>
       <c r="Q737" s="19"/>
       <c r="R737" s="19"/>
-      <c r="S737" s="20"/>
+      <c r="S737" s="61" t="s">
+        <v>2604</v>
+      </c>
       <c r="T737" s="20"/>
       <c r="U737" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#736</v>
       </c>
     </row>
     <row r="738">
-      <c r="A738" s="77"/>
-      <c r="B738" s="78"/>
-      <c r="C738" s="34"/>
-      <c r="D738" s="34"/>
-      <c r="E738" s="34"/>
+      <c r="A738" s="16" t="s">
+        <v>2608</v>
+      </c>
+      <c r="B738" s="6">
+        <v>44178.0</v>
+      </c>
+      <c r="C738" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D738" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E738" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F738" s="34"/>
-      <c r="G738" s="34"/>
-      <c r="H738" s="21"/>
-      <c r="I738" s="19"/>
-      <c r="J738" s="10"/>
-      <c r="K738" s="22"/>
-      <c r="L738" s="23"/>
-      <c r="M738" s="22"/>
+      <c r="G738" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H738" s="8" t="s">
+        <v>2352</v>
+      </c>
+      <c r="I738" s="9">
+        <v>44160.0</v>
+      </c>
+      <c r="J738" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K738" s="13" t="s">
+        <v>2609</v>
+      </c>
+      <c r="L738" s="12" t="s">
+        <v>1674</v>
+      </c>
+      <c r="M738" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N738" s="25"/>
-      <c r="O738" s="21"/>
-      <c r="P738" s="21"/>
+      <c r="O738" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P738" s="8" t="s">
+        <v>2610</v>
+      </c>
       <c r="Q738" s="19"/>
       <c r="R738" s="19"/>
-      <c r="S738" s="20"/>
+      <c r="S738" s="61" t="s">
+        <v>2604</v>
+      </c>
       <c r="T738" s="20"/>
       <c r="U738" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#737</v>
       </c>
     </row>
     <row r="739">
@@ -52692,7 +52820,7 @@
       <c r="P739" s="21"/>
       <c r="Q739" s="19"/>
       <c r="R739" s="19"/>
-      <c r="S739" s="20"/>
+      <c r="S739" s="47"/>
       <c r="T739" s="20"/>
       <c r="U739" s="18" t="str">
         <f t="shared" si="1"/>
@@ -52718,7 +52846,7 @@
       <c r="P740" s="21"/>
       <c r="Q740" s="19"/>
       <c r="R740" s="19"/>
-      <c r="S740" s="20"/>
+      <c r="S740" s="47"/>
       <c r="T740" s="20"/>
       <c r="U740" s="18" t="str">
         <f t="shared" si="1"/>
@@ -52744,7 +52872,7 @@
       <c r="P741" s="21"/>
       <c r="Q741" s="19"/>
       <c r="R741" s="19"/>
-      <c r="S741" s="20"/>
+      <c r="S741" s="47"/>
       <c r="T741" s="20"/>
       <c r="U741" s="18" t="str">
         <f t="shared" si="1"/>
@@ -52770,7 +52898,7 @@
       <c r="P742" s="21"/>
       <c r="Q742" s="19"/>
       <c r="R742" s="19"/>
-      <c r="S742" s="20"/>
+      <c r="S742" s="47"/>
       <c r="T742" s="20"/>
       <c r="U742" s="18" t="str">
         <f t="shared" si="1"/>
@@ -60195,15 +60323,18 @@
     <hyperlink r:id="rId296" ref="S733"/>
     <hyperlink r:id="rId297" ref="S734"/>
     <hyperlink r:id="rId298" ref="S735"/>
+    <hyperlink r:id="rId299" ref="S736"/>
+    <hyperlink r:id="rId300" ref="S737"/>
+    <hyperlink r:id="rId301" ref="S738"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId299"/>
-  <legacyDrawing r:id="rId300"/>
+  <drawing r:id="rId302"/>
+  <legacyDrawing r:id="rId303"/>
   <tableParts count="2">
-    <tablePart r:id="rId303"/>
-    <tablePart r:id="rId304"/>
+    <tablePart r:id="rId306"/>
+    <tablePart r:id="rId307"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201215
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -582,7 +582,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8441" uniqueCount="2611">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8519" uniqueCount="2633">
   <si>
     <t>案例</t>
   </si>
@@ -9390,6 +9390,80 @@
   <si>
     <t>移工，由仲介安排自費採檢，於今日確診(Ct值36)</t>
   </si>
+  <si>
+    <t>#738</t>
+  </si>
+  <si>
+    <t>-11/26 菲律賓→台灣</t>
+  </si>
+  <si>
+    <t>12/12 採檢
+12/14 確診</t>
+  </si>
+  <si>
+    <t>非移工</t>
+  </si>
+  <si>
+    <t>新增4例境外移入COVID-19病例，分別自菲律賓及印尼入境</t>
+  </si>
+  <si>
+    <t>#739</t>
+  </si>
+  <si>
+    <t>-11/20 菲律賓→台灣</t>
+  </si>
+  <si>
+    <t>仲介安排就醫採檢(Ct值31)</t>
+  </si>
+  <si>
+    <t>#740</t>
+  </si>
+  <si>
+    <t>-11/26 印尼→台灣</t>
+  </si>
+  <si>
+    <t>12/11 採檢
+12/14 確診</t>
+  </si>
+  <si>
+    <t>由仲介安排專車就醫採檢(Ct值31)</t>
+  </si>
+  <si>
+    <t>#741</t>
+  </si>
+  <si>
+    <t>11/28 採檢
+12/2 二採
+12/11 三採
+12/14 確診</t>
+  </si>
+  <si>
+    <t>因雇主要求至醫院採檢，於今日確診(Ct值32)</t>
+  </si>
+  <si>
+    <t>#742</t>
+  </si>
+  <si>
+    <t>-11/30 菲律賓→台灣</t>
+  </si>
+  <si>
+    <t>12/13 採檢
+12/15 確診</t>
+  </si>
+  <si>
+    <t>新增2例境外移入COVID-19病例，為菲律賓籍與印尼籍無症狀移工</t>
+  </si>
+  <si>
+    <t>#743</t>
+  </si>
+  <si>
+    <t>-11/30 印尼→台灣</t>
+  </si>
+  <si>
+    <t>12/4 採檢
+12/13 二採
+12/15 確診</t>
+  </si>
 </sst>
 </file>
 
@@ -9399,7 +9473,7 @@
     <numFmt numFmtId="164" formatCode="mm&quot;月&quot;dd&quot;日 &quot;dddd"/>
     <numFmt numFmtId="165" formatCode="m/d"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="21">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -9484,6 +9558,10 @@
       <u/>
       <color rgb="FF0000FF"/>
     </font>
+    <font/>
+    <font>
+      <color rgb="FF000000"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -9529,7 +9607,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="85">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -9760,6 +9838,24 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="19" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
@@ -52802,164 +52898,344 @@
       </c>
     </row>
     <row r="739">
-      <c r="A739" s="77"/>
-      <c r="B739" s="78"/>
-      <c r="C739" s="34"/>
-      <c r="D739" s="34"/>
-      <c r="E739" s="34"/>
+      <c r="A739" s="16" t="s">
+        <v>2611</v>
+      </c>
+      <c r="B739" s="6">
+        <v>44179.0</v>
+      </c>
+      <c r="C739" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D739" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E739" s="7" t="s">
+        <v>205</v>
+      </c>
       <c r="F739" s="34"/>
-      <c r="G739" s="34"/>
-      <c r="H739" s="21"/>
-      <c r="I739" s="19"/>
-      <c r="J739" s="10"/>
-      <c r="K739" s="22"/>
-      <c r="L739" s="23"/>
-      <c r="M739" s="22"/>
+      <c r="G739" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H739" s="8" t="s">
+        <v>2612</v>
+      </c>
+      <c r="I739" s="9">
+        <v>44161.0</v>
+      </c>
+      <c r="J739" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K739" s="13" t="s">
+        <v>2613</v>
+      </c>
+      <c r="L739" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M739" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N739" s="25"/>
-      <c r="O739" s="21"/>
-      <c r="P739" s="21"/>
+      <c r="O739" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P739" s="8" t="s">
+        <v>2614</v>
+      </c>
       <c r="Q739" s="19"/>
       <c r="R739" s="19"/>
-      <c r="S739" s="47"/>
+      <c r="S739" s="61" t="s">
+        <v>2615</v>
+      </c>
       <c r="T739" s="20"/>
       <c r="U739" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#738</v>
       </c>
     </row>
     <row r="740">
-      <c r="A740" s="77"/>
-      <c r="B740" s="78"/>
-      <c r="C740" s="34"/>
-      <c r="D740" s="34"/>
-      <c r="E740" s="34"/>
+      <c r="A740" s="16" t="s">
+        <v>2616</v>
+      </c>
+      <c r="B740" s="6">
+        <v>44179.0</v>
+      </c>
+      <c r="C740" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D740" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E740" s="7" t="s">
+        <v>205</v>
+      </c>
       <c r="F740" s="34"/>
-      <c r="G740" s="34"/>
-      <c r="H740" s="21"/>
-      <c r="I740" s="19"/>
-      <c r="J740" s="10"/>
-      <c r="K740" s="22"/>
-      <c r="L740" s="23"/>
-      <c r="M740" s="22"/>
+      <c r="G740" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H740" s="8" t="s">
+        <v>2617</v>
+      </c>
+      <c r="I740" s="9">
+        <v>44155.0</v>
+      </c>
+      <c r="J740" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K740" s="13" t="s">
+        <v>2613</v>
+      </c>
+      <c r="L740" s="12" t="s">
+        <v>1674</v>
+      </c>
+      <c r="M740" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N740" s="25"/>
-      <c r="O740" s="21"/>
-      <c r="P740" s="21"/>
+      <c r="O740" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P740" s="8" t="s">
+        <v>2618</v>
+      </c>
       <c r="Q740" s="19"/>
       <c r="R740" s="19"/>
-      <c r="S740" s="47"/>
+      <c r="S740" s="61" t="s">
+        <v>2615</v>
+      </c>
       <c r="T740" s="20"/>
       <c r="U740" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#739</v>
       </c>
     </row>
     <row r="741">
-      <c r="A741" s="77"/>
-      <c r="B741" s="78"/>
-      <c r="C741" s="34"/>
-      <c r="D741" s="34"/>
-      <c r="E741" s="34"/>
+      <c r="A741" s="16" t="s">
+        <v>2619</v>
+      </c>
+      <c r="B741" s="6">
+        <v>44179.0</v>
+      </c>
+      <c r="C741" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D741" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E741" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F741" s="34"/>
-      <c r="G741" s="34"/>
-      <c r="H741" s="21"/>
-      <c r="I741" s="19"/>
-      <c r="J741" s="10"/>
-      <c r="K741" s="22"/>
-      <c r="L741" s="23"/>
-      <c r="M741" s="22"/>
+      <c r="G741" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H741" s="8" t="s">
+        <v>2620</v>
+      </c>
+      <c r="I741" s="9">
+        <v>44161.0</v>
+      </c>
+      <c r="J741" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K741" s="13" t="s">
+        <v>2621</v>
+      </c>
+      <c r="L741" s="12" t="s">
+        <v>1674</v>
+      </c>
+      <c r="M741" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N741" s="25"/>
-      <c r="O741" s="21"/>
-      <c r="P741" s="21"/>
+      <c r="O741" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P741" s="8" t="s">
+        <v>2622</v>
+      </c>
       <c r="Q741" s="19"/>
       <c r="R741" s="19"/>
-      <c r="S741" s="47"/>
+      <c r="S741" s="61" t="s">
+        <v>2615</v>
+      </c>
       <c r="T741" s="20"/>
       <c r="U741" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#740</v>
       </c>
     </row>
     <row r="742">
-      <c r="A742" s="77"/>
-      <c r="B742" s="78"/>
-      <c r="C742" s="34"/>
-      <c r="D742" s="34"/>
-      <c r="E742" s="34"/>
+      <c r="A742" s="16" t="s">
+        <v>2623</v>
+      </c>
+      <c r="B742" s="6">
+        <v>44179.0</v>
+      </c>
+      <c r="C742" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D742" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E742" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F742" s="34"/>
-      <c r="G742" s="34"/>
-      <c r="H742" s="21"/>
-      <c r="I742" s="19"/>
-      <c r="J742" s="10"/>
-      <c r="K742" s="22"/>
-      <c r="L742" s="23"/>
-      <c r="M742" s="22"/>
+      <c r="G742" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H742" s="8" t="s">
+        <v>2527</v>
+      </c>
+      <c r="I742" s="9">
+        <v>44154.0</v>
+      </c>
+      <c r="J742" s="12" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K742" s="13" t="s">
+        <v>2624</v>
+      </c>
+      <c r="L742" s="12" t="s">
+        <v>1674</v>
+      </c>
+      <c r="M742" s="13" t="s">
+        <v>1442</v>
+      </c>
       <c r="N742" s="25"/>
-      <c r="O742" s="21"/>
-      <c r="P742" s="21"/>
+      <c r="O742" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P742" s="8" t="s">
+        <v>2625</v>
+      </c>
       <c r="Q742" s="19"/>
       <c r="R742" s="19"/>
-      <c r="S742" s="47"/>
+      <c r="S742" s="61" t="s">
+        <v>2615</v>
+      </c>
       <c r="T742" s="20"/>
       <c r="U742" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#741</v>
       </c>
     </row>
     <row r="743">
-      <c r="A743" s="77"/>
-      <c r="B743" s="78"/>
-      <c r="C743" s="34"/>
-      <c r="D743" s="34"/>
-      <c r="E743" s="34"/>
+      <c r="A743" s="77" t="s">
+        <v>2626</v>
+      </c>
+      <c r="B743" s="6">
+        <v>44180.0</v>
+      </c>
+      <c r="C743" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D743" s="78" t="s">
+        <v>116</v>
+      </c>
+      <c r="E743" s="7" t="s">
+        <v>205</v>
+      </c>
       <c r="F743" s="34"/>
-      <c r="G743" s="34"/>
-      <c r="H743" s="21"/>
-      <c r="I743" s="19"/>
-      <c r="J743" s="10"/>
-      <c r="K743" s="22"/>
-      <c r="L743" s="23"/>
-      <c r="M743" s="22"/>
+      <c r="G743" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H743" s="79" t="s">
+        <v>2627</v>
+      </c>
+      <c r="I743" s="80">
+        <v>44165.0</v>
+      </c>
+      <c r="J743" s="81" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K743" s="82" t="s">
+        <v>2628</v>
+      </c>
+      <c r="L743" s="81" t="s">
+        <v>426</v>
+      </c>
+      <c r="M743" s="82" t="s">
+        <v>1442</v>
+      </c>
       <c r="N743" s="25"/>
-      <c r="O743" s="21"/>
-      <c r="P743" s="21"/>
+      <c r="O743" s="79" t="s">
+        <v>85</v>
+      </c>
+      <c r="P743" s="79" t="s">
+        <v>1777</v>
+      </c>
       <c r="Q743" s="19"/>
       <c r="R743" s="19"/>
-      <c r="S743" s="20"/>
+      <c r="S743" s="61" t="s">
+        <v>2629</v>
+      </c>
       <c r="T743" s="20"/>
       <c r="U743" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#742</v>
       </c>
     </row>
     <row r="744">
-      <c r="A744" s="77"/>
-      <c r="B744" s="78"/>
-      <c r="C744" s="34"/>
-      <c r="D744" s="34"/>
-      <c r="E744" s="34"/>
+      <c r="A744" s="77" t="s">
+        <v>2630</v>
+      </c>
+      <c r="B744" s="6">
+        <v>44180.0</v>
+      </c>
+      <c r="C744" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D744" s="78" t="s">
+        <v>116</v>
+      </c>
+      <c r="E744" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="F744" s="34"/>
-      <c r="G744" s="34"/>
-      <c r="H744" s="21"/>
-      <c r="I744" s="19"/>
-      <c r="J744" s="10"/>
-      <c r="K744" s="22"/>
-      <c r="L744" s="23"/>
-      <c r="M744" s="22"/>
+      <c r="G744" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H744" s="79" t="s">
+        <v>2631</v>
+      </c>
+      <c r="I744" s="80">
+        <v>44165.0</v>
+      </c>
+      <c r="J744" s="81" t="s">
+        <v>1442</v>
+      </c>
+      <c r="K744" s="82" t="s">
+        <v>2632</v>
+      </c>
+      <c r="L744" s="81" t="s">
+        <v>426</v>
+      </c>
+      <c r="M744" s="82" t="s">
+        <v>1442</v>
+      </c>
       <c r="N744" s="25"/>
-      <c r="O744" s="21"/>
-      <c r="P744" s="21"/>
+      <c r="O744" s="79" t="s">
+        <v>85</v>
+      </c>
+      <c r="P744" s="79" t="s">
+        <v>1777</v>
+      </c>
       <c r="Q744" s="19"/>
       <c r="R744" s="19"/>
-      <c r="S744" s="20"/>
+      <c r="S744" s="61" t="s">
+        <v>2629</v>
+      </c>
       <c r="T744" s="20"/>
       <c r="U744" s="18" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>#743</v>
       </c>
     </row>
     <row r="745">
-      <c r="A745" s="77"/>
-      <c r="B745" s="78"/>
+      <c r="A745" s="83"/>
+      <c r="B745" s="84"/>
       <c r="C745" s="34"/>
       <c r="D745" s="34"/>
       <c r="E745" s="34"/>
@@ -52984,8 +53260,8 @@
       </c>
     </row>
     <row r="746">
-      <c r="A746" s="77"/>
-      <c r="B746" s="78"/>
+      <c r="A746" s="83"/>
+      <c r="B746" s="84"/>
       <c r="C746" s="34"/>
       <c r="D746" s="34"/>
       <c r="E746" s="34"/>
@@ -53010,8 +53286,8 @@
       </c>
     </row>
     <row r="747">
-      <c r="A747" s="77"/>
-      <c r="B747" s="78"/>
+      <c r="A747" s="83"/>
+      <c r="B747" s="84"/>
       <c r="C747" s="34"/>
       <c r="D747" s="34"/>
       <c r="E747" s="34"/>
@@ -53036,8 +53312,8 @@
       </c>
     </row>
     <row r="748">
-      <c r="A748" s="77"/>
-      <c r="B748" s="78"/>
+      <c r="A748" s="83"/>
+      <c r="B748" s="84"/>
       <c r="C748" s="34"/>
       <c r="D748" s="34"/>
       <c r="E748" s="34"/>
@@ -53062,8 +53338,8 @@
       </c>
     </row>
     <row r="749">
-      <c r="A749" s="77"/>
-      <c r="B749" s="78"/>
+      <c r="A749" s="83"/>
+      <c r="B749" s="84"/>
       <c r="C749" s="34"/>
       <c r="D749" s="34"/>
       <c r="E749" s="34"/>
@@ -53088,8 +53364,8 @@
       </c>
     </row>
     <row r="750">
-      <c r="A750" s="77"/>
-      <c r="B750" s="78"/>
+      <c r="A750" s="83"/>
+      <c r="B750" s="84"/>
       <c r="C750" s="34"/>
       <c r="D750" s="34"/>
       <c r="E750" s="34"/>
@@ -53114,8 +53390,8 @@
       </c>
     </row>
     <row r="751">
-      <c r="A751" s="77"/>
-      <c r="B751" s="78"/>
+      <c r="A751" s="83"/>
+      <c r="B751" s="84"/>
       <c r="C751" s="34"/>
       <c r="D751" s="34"/>
       <c r="E751" s="34"/>
@@ -53140,8 +53416,8 @@
       </c>
     </row>
     <row r="752">
-      <c r="A752" s="77"/>
-      <c r="B752" s="78"/>
+      <c r="A752" s="83"/>
+      <c r="B752" s="84"/>
       <c r="C752" s="34"/>
       <c r="D752" s="34"/>
       <c r="E752" s="34"/>
@@ -53166,8 +53442,8 @@
       </c>
     </row>
     <row r="753">
-      <c r="A753" s="77"/>
-      <c r="B753" s="78"/>
+      <c r="A753" s="83"/>
+      <c r="B753" s="84"/>
       <c r="C753" s="34"/>
       <c r="D753" s="34"/>
       <c r="E753" s="34"/>
@@ -53192,8 +53468,8 @@
       </c>
     </row>
     <row r="754">
-      <c r="A754" s="77"/>
-      <c r="B754" s="78"/>
+      <c r="A754" s="83"/>
+      <c r="B754" s="84"/>
       <c r="C754" s="34"/>
       <c r="D754" s="34"/>
       <c r="E754" s="34"/>
@@ -53218,8 +53494,8 @@
       </c>
     </row>
     <row r="755">
-      <c r="A755" s="77"/>
-      <c r="B755" s="78"/>
+      <c r="A755" s="83"/>
+      <c r="B755" s="84"/>
       <c r="C755" s="34"/>
       <c r="D755" s="34"/>
       <c r="E755" s="34"/>
@@ -53244,8 +53520,8 @@
       </c>
     </row>
     <row r="756">
-      <c r="A756" s="77"/>
-      <c r="B756" s="78"/>
+      <c r="A756" s="83"/>
+      <c r="B756" s="84"/>
       <c r="C756" s="34"/>
       <c r="D756" s="34"/>
       <c r="E756" s="34"/>
@@ -53270,8 +53546,8 @@
       </c>
     </row>
     <row r="757">
-      <c r="A757" s="77"/>
-      <c r="B757" s="78"/>
+      <c r="A757" s="83"/>
+      <c r="B757" s="84"/>
       <c r="C757" s="34"/>
       <c r="D757" s="34"/>
       <c r="E757" s="34"/>
@@ -53296,8 +53572,8 @@
       </c>
     </row>
     <row r="758">
-      <c r="A758" s="77"/>
-      <c r="B758" s="78"/>
+      <c r="A758" s="83"/>
+      <c r="B758" s="84"/>
       <c r="C758" s="34"/>
       <c r="D758" s="34"/>
       <c r="E758" s="34"/>
@@ -53322,8 +53598,8 @@
       </c>
     </row>
     <row r="759">
-      <c r="A759" s="77"/>
-      <c r="B759" s="78"/>
+      <c r="A759" s="83"/>
+      <c r="B759" s="84"/>
       <c r="C759" s="34"/>
       <c r="D759" s="34"/>
       <c r="E759" s="34"/>
@@ -53348,8 +53624,8 @@
       </c>
     </row>
     <row r="760">
-      <c r="A760" s="77"/>
-      <c r="B760" s="78"/>
+      <c r="A760" s="83"/>
+      <c r="B760" s="84"/>
       <c r="C760" s="34"/>
       <c r="D760" s="34"/>
       <c r="E760" s="34"/>
@@ -53374,8 +53650,8 @@
       </c>
     </row>
     <row r="761">
-      <c r="A761" s="77"/>
-      <c r="B761" s="78"/>
+      <c r="A761" s="83"/>
+      <c r="B761" s="84"/>
       <c r="C761" s="34"/>
       <c r="D761" s="34"/>
       <c r="E761" s="34"/>
@@ -53400,8 +53676,8 @@
       </c>
     </row>
     <row r="762">
-      <c r="A762" s="77"/>
-      <c r="B762" s="78"/>
+      <c r="A762" s="83"/>
+      <c r="B762" s="84"/>
       <c r="C762" s="34"/>
       <c r="D762" s="34"/>
       <c r="E762" s="34"/>
@@ -53426,8 +53702,8 @@
       </c>
     </row>
     <row r="763">
-      <c r="A763" s="77"/>
-      <c r="B763" s="78"/>
+      <c r="A763" s="83"/>
+      <c r="B763" s="84"/>
       <c r="C763" s="34"/>
       <c r="D763" s="34"/>
       <c r="E763" s="34"/>
@@ -53452,8 +53728,8 @@
       </c>
     </row>
     <row r="764">
-      <c r="A764" s="77"/>
-      <c r="B764" s="78"/>
+      <c r="A764" s="83"/>
+      <c r="B764" s="84"/>
       <c r="C764" s="34"/>
       <c r="D764" s="34"/>
       <c r="E764" s="34"/>
@@ -53478,8 +53754,8 @@
       </c>
     </row>
     <row r="765">
-      <c r="A765" s="77"/>
-      <c r="B765" s="78"/>
+      <c r="A765" s="83"/>
+      <c r="B765" s="84"/>
       <c r="C765" s="34"/>
       <c r="D765" s="34"/>
       <c r="E765" s="34"/>
@@ -53504,8 +53780,8 @@
       </c>
     </row>
     <row r="766">
-      <c r="A766" s="77"/>
-      <c r="B766" s="78"/>
+      <c r="A766" s="83"/>
+      <c r="B766" s="84"/>
       <c r="C766" s="34"/>
       <c r="D766" s="34"/>
       <c r="E766" s="34"/>
@@ -53530,8 +53806,8 @@
       </c>
     </row>
     <row r="767">
-      <c r="A767" s="77"/>
-      <c r="B767" s="78"/>
+      <c r="A767" s="83"/>
+      <c r="B767" s="84"/>
       <c r="C767" s="34"/>
       <c r="D767" s="34"/>
       <c r="E767" s="34"/>
@@ -53556,8 +53832,8 @@
       </c>
     </row>
     <row r="768">
-      <c r="A768" s="77"/>
-      <c r="B768" s="78"/>
+      <c r="A768" s="83"/>
+      <c r="B768" s="84"/>
       <c r="C768" s="34"/>
       <c r="D768" s="34"/>
       <c r="E768" s="34"/>
@@ -53582,8 +53858,8 @@
       </c>
     </row>
     <row r="769">
-      <c r="A769" s="77"/>
-      <c r="B769" s="78"/>
+      <c r="A769" s="83"/>
+      <c r="B769" s="84"/>
       <c r="C769" s="34"/>
       <c r="D769" s="34"/>
       <c r="E769" s="34"/>
@@ -53608,8 +53884,8 @@
       </c>
     </row>
     <row r="770">
-      <c r="A770" s="77"/>
-      <c r="B770" s="78"/>
+      <c r="A770" s="83"/>
+      <c r="B770" s="84"/>
       <c r="C770" s="34"/>
       <c r="D770" s="34"/>
       <c r="E770" s="34"/>
@@ -53634,8 +53910,8 @@
       </c>
     </row>
     <row r="771">
-      <c r="A771" s="77"/>
-      <c r="B771" s="78"/>
+      <c r="A771" s="83"/>
+      <c r="B771" s="84"/>
       <c r="C771" s="34"/>
       <c r="D771" s="34"/>
       <c r="E771" s="34"/>
@@ -53660,8 +53936,8 @@
       </c>
     </row>
     <row r="772">
-      <c r="A772" s="77"/>
-      <c r="B772" s="78"/>
+      <c r="A772" s="83"/>
+      <c r="B772" s="84"/>
       <c r="C772" s="34"/>
       <c r="D772" s="34"/>
       <c r="E772" s="34"/>
@@ -53686,8 +53962,8 @@
       </c>
     </row>
     <row r="773">
-      <c r="A773" s="77"/>
-      <c r="B773" s="78"/>
+      <c r="A773" s="83"/>
+      <c r="B773" s="84"/>
       <c r="C773" s="34"/>
       <c r="D773" s="34"/>
       <c r="E773" s="34"/>
@@ -53712,8 +53988,8 @@
       </c>
     </row>
     <row r="774">
-      <c r="A774" s="77"/>
-      <c r="B774" s="78"/>
+      <c r="A774" s="83"/>
+      <c r="B774" s="84"/>
       <c r="C774" s="34"/>
       <c r="D774" s="34"/>
       <c r="E774" s="34"/>
@@ -53738,8 +54014,8 @@
       </c>
     </row>
     <row r="775">
-      <c r="A775" s="77"/>
-      <c r="B775" s="78"/>
+      <c r="A775" s="83"/>
+      <c r="B775" s="84"/>
       <c r="C775" s="34"/>
       <c r="D775" s="34"/>
       <c r="E775" s="34"/>
@@ -53764,8 +54040,8 @@
       </c>
     </row>
     <row r="776">
-      <c r="A776" s="77"/>
-      <c r="B776" s="78"/>
+      <c r="A776" s="83"/>
+      <c r="B776" s="84"/>
       <c r="C776" s="34"/>
       <c r="D776" s="34"/>
       <c r="E776" s="34"/>
@@ -53790,8 +54066,8 @@
       </c>
     </row>
     <row r="777">
-      <c r="A777" s="77"/>
-      <c r="B777" s="78"/>
+      <c r="A777" s="83"/>
+      <c r="B777" s="84"/>
       <c r="C777" s="34"/>
       <c r="D777" s="34"/>
       <c r="E777" s="34"/>
@@ -53816,8 +54092,8 @@
       </c>
     </row>
     <row r="778">
-      <c r="A778" s="77"/>
-      <c r="B778" s="78"/>
+      <c r="A778" s="83"/>
+      <c r="B778" s="84"/>
       <c r="C778" s="34"/>
       <c r="D778" s="34"/>
       <c r="E778" s="34"/>
@@ -53842,8 +54118,8 @@
       </c>
     </row>
     <row r="779">
-      <c r="A779" s="77"/>
-      <c r="B779" s="78"/>
+      <c r="A779" s="83"/>
+      <c r="B779" s="84"/>
       <c r="C779" s="34"/>
       <c r="D779" s="34"/>
       <c r="E779" s="34"/>
@@ -53868,8 +54144,8 @@
       </c>
     </row>
     <row r="780">
-      <c r="A780" s="77"/>
-      <c r="B780" s="78"/>
+      <c r="A780" s="83"/>
+      <c r="B780" s="84"/>
       <c r="C780" s="34"/>
       <c r="D780" s="34"/>
       <c r="E780" s="34"/>
@@ -53894,8 +54170,8 @@
       </c>
     </row>
     <row r="781">
-      <c r="A781" s="77"/>
-      <c r="B781" s="78"/>
+      <c r="A781" s="83"/>
+      <c r="B781" s="84"/>
       <c r="C781" s="34"/>
       <c r="D781" s="34"/>
       <c r="E781" s="34"/>
@@ -53920,8 +54196,8 @@
       </c>
     </row>
     <row r="782">
-      <c r="A782" s="77"/>
-      <c r="B782" s="78"/>
+      <c r="A782" s="83"/>
+      <c r="B782" s="84"/>
       <c r="C782" s="34"/>
       <c r="D782" s="34"/>
       <c r="E782" s="34"/>
@@ -53946,8 +54222,8 @@
       </c>
     </row>
     <row r="783">
-      <c r="A783" s="77"/>
-      <c r="B783" s="78"/>
+      <c r="A783" s="83"/>
+      <c r="B783" s="84"/>
       <c r="C783" s="34"/>
       <c r="D783" s="34"/>
       <c r="E783" s="34"/>
@@ -53972,8 +54248,8 @@
       </c>
     </row>
     <row r="784">
-      <c r="A784" s="77"/>
-      <c r="B784" s="78"/>
+      <c r="A784" s="83"/>
+      <c r="B784" s="84"/>
       <c r="C784" s="34"/>
       <c r="D784" s="34"/>
       <c r="E784" s="34"/>
@@ -53998,8 +54274,8 @@
       </c>
     </row>
     <row r="785">
-      <c r="A785" s="77"/>
-      <c r="B785" s="78"/>
+      <c r="A785" s="83"/>
+      <c r="B785" s="84"/>
       <c r="C785" s="34"/>
       <c r="D785" s="34"/>
       <c r="E785" s="34"/>
@@ -54024,8 +54300,8 @@
       </c>
     </row>
     <row r="786">
-      <c r="A786" s="77"/>
-      <c r="B786" s="78"/>
+      <c r="A786" s="83"/>
+      <c r="B786" s="84"/>
       <c r="C786" s="34"/>
       <c r="D786" s="34"/>
       <c r="E786" s="34"/>
@@ -54050,8 +54326,8 @@
       </c>
     </row>
     <row r="787">
-      <c r="A787" s="77"/>
-      <c r="B787" s="78"/>
+      <c r="A787" s="83"/>
+      <c r="B787" s="84"/>
       <c r="C787" s="34"/>
       <c r="D787" s="34"/>
       <c r="E787" s="34"/>
@@ -54076,8 +54352,8 @@
       </c>
     </row>
     <row r="788">
-      <c r="A788" s="77"/>
-      <c r="B788" s="78"/>
+      <c r="A788" s="83"/>
+      <c r="B788" s="84"/>
       <c r="C788" s="34"/>
       <c r="D788" s="34"/>
       <c r="E788" s="34"/>
@@ -54102,8 +54378,8 @@
       </c>
     </row>
     <row r="789">
-      <c r="A789" s="77"/>
-      <c r="B789" s="78"/>
+      <c r="A789" s="83"/>
+      <c r="B789" s="84"/>
       <c r="C789" s="34"/>
       <c r="D789" s="34"/>
       <c r="E789" s="34"/>
@@ -54128,8 +54404,8 @@
       </c>
     </row>
     <row r="790">
-      <c r="A790" s="77"/>
-      <c r="B790" s="78"/>
+      <c r="A790" s="83"/>
+      <c r="B790" s="84"/>
       <c r="C790" s="34"/>
       <c r="D790" s="34"/>
       <c r="E790" s="34"/>
@@ -54154,8 +54430,8 @@
       </c>
     </row>
     <row r="791">
-      <c r="A791" s="77"/>
-      <c r="B791" s="78"/>
+      <c r="A791" s="83"/>
+      <c r="B791" s="84"/>
       <c r="C791" s="34"/>
       <c r="D791" s="34"/>
       <c r="E791" s="34"/>
@@ -54180,8 +54456,8 @@
       </c>
     </row>
     <row r="792">
-      <c r="A792" s="77"/>
-      <c r="B792" s="78"/>
+      <c r="A792" s="83"/>
+      <c r="B792" s="84"/>
       <c r="C792" s="34"/>
       <c r="D792" s="34"/>
       <c r="E792" s="34"/>
@@ -54206,8 +54482,8 @@
       </c>
     </row>
     <row r="793">
-      <c r="A793" s="77"/>
-      <c r="B793" s="78"/>
+      <c r="A793" s="83"/>
+      <c r="B793" s="84"/>
       <c r="C793" s="34"/>
       <c r="D793" s="34"/>
       <c r="E793" s="34"/>
@@ -54232,8 +54508,8 @@
       </c>
     </row>
     <row r="794">
-      <c r="A794" s="77"/>
-      <c r="B794" s="78"/>
+      <c r="A794" s="83"/>
+      <c r="B794" s="84"/>
       <c r="C794" s="34"/>
       <c r="D794" s="34"/>
       <c r="E794" s="34"/>
@@ -54258,8 +54534,8 @@
       </c>
     </row>
     <row r="795">
-      <c r="A795" s="77"/>
-      <c r="B795" s="78"/>
+      <c r="A795" s="83"/>
+      <c r="B795" s="84"/>
       <c r="C795" s="34"/>
       <c r="D795" s="34"/>
       <c r="E795" s="34"/>
@@ -54284,8 +54560,8 @@
       </c>
     </row>
     <row r="796">
-      <c r="A796" s="77"/>
-      <c r="B796" s="78"/>
+      <c r="A796" s="83"/>
+      <c r="B796" s="84"/>
       <c r="C796" s="34"/>
       <c r="D796" s="34"/>
       <c r="E796" s="34"/>
@@ -54310,8 +54586,8 @@
       </c>
     </row>
     <row r="797">
-      <c r="A797" s="77"/>
-      <c r="B797" s="78"/>
+      <c r="A797" s="83"/>
+      <c r="B797" s="84"/>
       <c r="C797" s="34"/>
       <c r="D797" s="34"/>
       <c r="E797" s="34"/>
@@ -54336,8 +54612,8 @@
       </c>
     </row>
     <row r="798">
-      <c r="A798" s="77"/>
-      <c r="B798" s="78"/>
+      <c r="A798" s="83"/>
+      <c r="B798" s="84"/>
       <c r="C798" s="34"/>
       <c r="D798" s="34"/>
       <c r="E798" s="34"/>
@@ -54362,8 +54638,8 @@
       </c>
     </row>
     <row r="799">
-      <c r="A799" s="77"/>
-      <c r="B799" s="78"/>
+      <c r="A799" s="83"/>
+      <c r="B799" s="84"/>
       <c r="C799" s="34"/>
       <c r="D799" s="34"/>
       <c r="E799" s="34"/>
@@ -54388,8 +54664,8 @@
       </c>
     </row>
     <row r="800">
-      <c r="A800" s="77"/>
-      <c r="B800" s="78"/>
+      <c r="A800" s="83"/>
+      <c r="B800" s="84"/>
       <c r="C800" s="34"/>
       <c r="D800" s="34"/>
       <c r="E800" s="34"/>
@@ -54414,8 +54690,8 @@
       </c>
     </row>
     <row r="801">
-      <c r="A801" s="77"/>
-      <c r="B801" s="78"/>
+      <c r="A801" s="83"/>
+      <c r="B801" s="84"/>
       <c r="C801" s="34"/>
       <c r="D801" s="34"/>
       <c r="E801" s="34"/>
@@ -54440,8 +54716,8 @@
       </c>
     </row>
     <row r="802">
-      <c r="A802" s="77"/>
-      <c r="B802" s="78"/>
+      <c r="A802" s="83"/>
+      <c r="B802" s="84"/>
       <c r="C802" s="34"/>
       <c r="D802" s="34"/>
       <c r="E802" s="34"/>
@@ -54466,8 +54742,8 @@
       </c>
     </row>
     <row r="803">
-      <c r="A803" s="77"/>
-      <c r="B803" s="78"/>
+      <c r="A803" s="83"/>
+      <c r="B803" s="84"/>
       <c r="C803" s="34"/>
       <c r="D803" s="34"/>
       <c r="E803" s="34"/>
@@ -54492,8 +54768,8 @@
       </c>
     </row>
     <row r="804">
-      <c r="A804" s="77"/>
-      <c r="B804" s="78"/>
+      <c r="A804" s="83"/>
+      <c r="B804" s="84"/>
       <c r="C804" s="34"/>
       <c r="D804" s="34"/>
       <c r="E804" s="34"/>
@@ -54518,8 +54794,8 @@
       </c>
     </row>
     <row r="805">
-      <c r="A805" s="77"/>
-      <c r="B805" s="78"/>
+      <c r="A805" s="83"/>
+      <c r="B805" s="84"/>
       <c r="C805" s="34"/>
       <c r="D805" s="34"/>
       <c r="E805" s="34"/>
@@ -54544,8 +54820,8 @@
       </c>
     </row>
     <row r="806">
-      <c r="A806" s="77"/>
-      <c r="B806" s="78"/>
+      <c r="A806" s="83"/>
+      <c r="B806" s="84"/>
       <c r="C806" s="34"/>
       <c r="D806" s="34"/>
       <c r="E806" s="34"/>
@@ -54570,8 +54846,8 @@
       </c>
     </row>
     <row r="807">
-      <c r="A807" s="77"/>
-      <c r="B807" s="78"/>
+      <c r="A807" s="83"/>
+      <c r="B807" s="84"/>
       <c r="C807" s="34"/>
       <c r="D807" s="34"/>
       <c r="E807" s="34"/>
@@ -54596,8 +54872,8 @@
       </c>
     </row>
     <row r="808">
-      <c r="A808" s="77"/>
-      <c r="B808" s="78"/>
+      <c r="A808" s="83"/>
+      <c r="B808" s="84"/>
       <c r="C808" s="34"/>
       <c r="D808" s="34"/>
       <c r="E808" s="34"/>
@@ -54622,8 +54898,8 @@
       </c>
     </row>
     <row r="809">
-      <c r="A809" s="77"/>
-      <c r="B809" s="78"/>
+      <c r="A809" s="83"/>
+      <c r="B809" s="84"/>
       <c r="C809" s="34"/>
       <c r="D809" s="34"/>
       <c r="E809" s="34"/>
@@ -54648,8 +54924,8 @@
       </c>
     </row>
     <row r="810">
-      <c r="A810" s="77"/>
-      <c r="B810" s="78"/>
+      <c r="A810" s="83"/>
+      <c r="B810" s="84"/>
       <c r="C810" s="34"/>
       <c r="D810" s="34"/>
       <c r="E810" s="34"/>
@@ -54674,8 +54950,8 @@
       </c>
     </row>
     <row r="811">
-      <c r="A811" s="77"/>
-      <c r="B811" s="78"/>
+      <c r="A811" s="83"/>
+      <c r="B811" s="84"/>
       <c r="C811" s="34"/>
       <c r="D811" s="34"/>
       <c r="E811" s="34"/>
@@ -54700,8 +54976,8 @@
       </c>
     </row>
     <row r="812">
-      <c r="A812" s="77"/>
-      <c r="B812" s="78"/>
+      <c r="A812" s="83"/>
+      <c r="B812" s="84"/>
       <c r="C812" s="34"/>
       <c r="D812" s="34"/>
       <c r="E812" s="34"/>
@@ -54726,8 +55002,8 @@
       </c>
     </row>
     <row r="813">
-      <c r="A813" s="77"/>
-      <c r="B813" s="78"/>
+      <c r="A813" s="83"/>
+      <c r="B813" s="84"/>
       <c r="C813" s="34"/>
       <c r="D813" s="34"/>
       <c r="E813" s="34"/>
@@ -54752,8 +55028,8 @@
       </c>
     </row>
     <row r="814">
-      <c r="A814" s="77"/>
-      <c r="B814" s="78"/>
+      <c r="A814" s="83"/>
+      <c r="B814" s="84"/>
       <c r="C814" s="34"/>
       <c r="D814" s="34"/>
       <c r="E814" s="34"/>
@@ -54778,8 +55054,8 @@
       </c>
     </row>
     <row r="815">
-      <c r="A815" s="77"/>
-      <c r="B815" s="78"/>
+      <c r="A815" s="83"/>
+      <c r="B815" s="84"/>
       <c r="C815" s="34"/>
       <c r="D815" s="34"/>
       <c r="E815" s="34"/>
@@ -54804,8 +55080,8 @@
       </c>
     </row>
     <row r="816">
-      <c r="A816" s="77"/>
-      <c r="B816" s="78"/>
+      <c r="A816" s="83"/>
+      <c r="B816" s="84"/>
       <c r="C816" s="34"/>
       <c r="D816" s="34"/>
       <c r="E816" s="34"/>
@@ -54830,8 +55106,8 @@
       </c>
     </row>
     <row r="817">
-      <c r="A817" s="77"/>
-      <c r="B817" s="78"/>
+      <c r="A817" s="83"/>
+      <c r="B817" s="84"/>
       <c r="C817" s="34"/>
       <c r="D817" s="34"/>
       <c r="E817" s="34"/>
@@ -54856,8 +55132,8 @@
       </c>
     </row>
     <row r="818">
-      <c r="A818" s="77"/>
-      <c r="B818" s="78"/>
+      <c r="A818" s="83"/>
+      <c r="B818" s="84"/>
       <c r="C818" s="34"/>
       <c r="D818" s="34"/>
       <c r="E818" s="34"/>
@@ -54882,8 +55158,8 @@
       </c>
     </row>
     <row r="819">
-      <c r="A819" s="77"/>
-      <c r="B819" s="78"/>
+      <c r="A819" s="83"/>
+      <c r="B819" s="84"/>
       <c r="C819" s="34"/>
       <c r="D819" s="34"/>
       <c r="E819" s="34"/>
@@ -54908,8 +55184,8 @@
       </c>
     </row>
     <row r="820">
-      <c r="A820" s="77"/>
-      <c r="B820" s="78"/>
+      <c r="A820" s="83"/>
+      <c r="B820" s="84"/>
       <c r="C820" s="34"/>
       <c r="D820" s="34"/>
       <c r="E820" s="34"/>
@@ -54934,8 +55210,8 @@
       </c>
     </row>
     <row r="821">
-      <c r="A821" s="77"/>
-      <c r="B821" s="78"/>
+      <c r="A821" s="83"/>
+      <c r="B821" s="84"/>
       <c r="C821" s="34"/>
       <c r="D821" s="34"/>
       <c r="E821" s="34"/>
@@ -54960,8 +55236,8 @@
       </c>
     </row>
     <row r="822">
-      <c r="A822" s="77"/>
-      <c r="B822" s="78"/>
+      <c r="A822" s="83"/>
+      <c r="B822" s="84"/>
       <c r="C822" s="34"/>
       <c r="D822" s="34"/>
       <c r="E822" s="34"/>
@@ -54986,8 +55262,8 @@
       </c>
     </row>
     <row r="823">
-      <c r="A823" s="77"/>
-      <c r="B823" s="78"/>
+      <c r="A823" s="83"/>
+      <c r="B823" s="84"/>
       <c r="C823" s="34"/>
       <c r="D823" s="34"/>
       <c r="E823" s="34"/>
@@ -55012,8 +55288,8 @@
       </c>
     </row>
     <row r="824">
-      <c r="A824" s="77"/>
-      <c r="B824" s="78"/>
+      <c r="A824" s="83"/>
+      <c r="B824" s="84"/>
       <c r="C824" s="34"/>
       <c r="D824" s="34"/>
       <c r="E824" s="34"/>
@@ -55038,8 +55314,8 @@
       </c>
     </row>
     <row r="825">
-      <c r="A825" s="77"/>
-      <c r="B825" s="78"/>
+      <c r="A825" s="83"/>
+      <c r="B825" s="84"/>
       <c r="C825" s="34"/>
       <c r="D825" s="34"/>
       <c r="E825" s="34"/>
@@ -55064,8 +55340,8 @@
       </c>
     </row>
     <row r="826">
-      <c r="A826" s="77"/>
-      <c r="B826" s="78"/>
+      <c r="A826" s="83"/>
+      <c r="B826" s="84"/>
       <c r="C826" s="34"/>
       <c r="D826" s="34"/>
       <c r="E826" s="34"/>
@@ -55090,8 +55366,8 @@
       </c>
     </row>
     <row r="827">
-      <c r="A827" s="77"/>
-      <c r="B827" s="78"/>
+      <c r="A827" s="83"/>
+      <c r="B827" s="84"/>
       <c r="C827" s="34"/>
       <c r="D827" s="34"/>
       <c r="E827" s="34"/>
@@ -55116,8 +55392,8 @@
       </c>
     </row>
     <row r="828">
-      <c r="A828" s="77"/>
-      <c r="B828" s="78"/>
+      <c r="A828" s="83"/>
+      <c r="B828" s="84"/>
       <c r="C828" s="34"/>
       <c r="D828" s="34"/>
       <c r="E828" s="34"/>
@@ -55142,8 +55418,8 @@
       </c>
     </row>
     <row r="829">
-      <c r="A829" s="77"/>
-      <c r="B829" s="78"/>
+      <c r="A829" s="83"/>
+      <c r="B829" s="84"/>
       <c r="C829" s="34"/>
       <c r="D829" s="34"/>
       <c r="E829" s="34"/>
@@ -55168,8 +55444,8 @@
       </c>
     </row>
     <row r="830">
-      <c r="A830" s="77"/>
-      <c r="B830" s="78"/>
+      <c r="A830" s="83"/>
+      <c r="B830" s="84"/>
       <c r="C830" s="34"/>
       <c r="D830" s="34"/>
       <c r="E830" s="34"/>
@@ -55194,8 +55470,8 @@
       </c>
     </row>
     <row r="831">
-      <c r="A831" s="77"/>
-      <c r="B831" s="78"/>
+      <c r="A831" s="83"/>
+      <c r="B831" s="84"/>
       <c r="C831" s="34"/>
       <c r="D831" s="34"/>
       <c r="E831" s="34"/>
@@ -55220,8 +55496,8 @@
       </c>
     </row>
     <row r="832">
-      <c r="A832" s="77"/>
-      <c r="B832" s="78"/>
+      <c r="A832" s="83"/>
+      <c r="B832" s="84"/>
       <c r="C832" s="34"/>
       <c r="D832" s="34"/>
       <c r="E832" s="34"/>
@@ -55246,8 +55522,8 @@
       </c>
     </row>
     <row r="833">
-      <c r="A833" s="77"/>
-      <c r="B833" s="78"/>
+      <c r="A833" s="83"/>
+      <c r="B833" s="84"/>
       <c r="C833" s="34"/>
       <c r="D833" s="34"/>
       <c r="E833" s="34"/>
@@ -55272,8 +55548,8 @@
       </c>
     </row>
     <row r="834">
-      <c r="A834" s="77"/>
-      <c r="B834" s="78"/>
+      <c r="A834" s="83"/>
+      <c r="B834" s="84"/>
       <c r="C834" s="34"/>
       <c r="D834" s="34"/>
       <c r="E834" s="34"/>
@@ -55298,8 +55574,8 @@
       </c>
     </row>
     <row r="835">
-      <c r="A835" s="77"/>
-      <c r="B835" s="78"/>
+      <c r="A835" s="83"/>
+      <c r="B835" s="84"/>
       <c r="C835" s="34"/>
       <c r="D835" s="34"/>
       <c r="E835" s="34"/>
@@ -55324,8 +55600,8 @@
       </c>
     </row>
     <row r="836">
-      <c r="A836" s="77"/>
-      <c r="B836" s="78"/>
+      <c r="A836" s="83"/>
+      <c r="B836" s="84"/>
       <c r="C836" s="34"/>
       <c r="D836" s="34"/>
       <c r="E836" s="34"/>
@@ -55350,8 +55626,8 @@
       </c>
     </row>
     <row r="837">
-      <c r="A837" s="77"/>
-      <c r="B837" s="78"/>
+      <c r="A837" s="83"/>
+      <c r="B837" s="84"/>
       <c r="C837" s="34"/>
       <c r="D837" s="34"/>
       <c r="E837" s="34"/>
@@ -55376,8 +55652,8 @@
       </c>
     </row>
     <row r="838">
-      <c r="A838" s="77"/>
-      <c r="B838" s="78"/>
+      <c r="A838" s="83"/>
+      <c r="B838" s="84"/>
       <c r="C838" s="34"/>
       <c r="D838" s="34"/>
       <c r="E838" s="34"/>
@@ -55402,8 +55678,8 @@
       </c>
     </row>
     <row r="839">
-      <c r="A839" s="77"/>
-      <c r="B839" s="78"/>
+      <c r="A839" s="83"/>
+      <c r="B839" s="84"/>
       <c r="C839" s="34"/>
       <c r="D839" s="34"/>
       <c r="E839" s="34"/>
@@ -55428,8 +55704,8 @@
       </c>
     </row>
     <row r="840">
-      <c r="A840" s="77"/>
-      <c r="B840" s="78"/>
+      <c r="A840" s="83"/>
+      <c r="B840" s="84"/>
       <c r="C840" s="34"/>
       <c r="D840" s="34"/>
       <c r="E840" s="34"/>
@@ -55454,8 +55730,8 @@
       </c>
     </row>
     <row r="841">
-      <c r="A841" s="77"/>
-      <c r="B841" s="78"/>
+      <c r="A841" s="83"/>
+      <c r="B841" s="84"/>
       <c r="C841" s="34"/>
       <c r="D841" s="34"/>
       <c r="E841" s="34"/>
@@ -55480,8 +55756,8 @@
       </c>
     </row>
     <row r="842">
-      <c r="A842" s="77"/>
-      <c r="B842" s="78"/>
+      <c r="A842" s="83"/>
+      <c r="B842" s="84"/>
       <c r="C842" s="34"/>
       <c r="D842" s="34"/>
       <c r="E842" s="34"/>
@@ -55506,8 +55782,8 @@
       </c>
     </row>
     <row r="843">
-      <c r="A843" s="77"/>
-      <c r="B843" s="78"/>
+      <c r="A843" s="83"/>
+      <c r="B843" s="84"/>
       <c r="C843" s="34"/>
       <c r="D843" s="34"/>
       <c r="E843" s="34"/>
@@ -55532,8 +55808,8 @@
       </c>
     </row>
     <row r="844">
-      <c r="A844" s="77"/>
-      <c r="B844" s="78"/>
+      <c r="A844" s="83"/>
+      <c r="B844" s="84"/>
       <c r="C844" s="34"/>
       <c r="D844" s="34"/>
       <c r="E844" s="34"/>
@@ -55558,8 +55834,8 @@
       </c>
     </row>
     <row r="845">
-      <c r="A845" s="77"/>
-      <c r="B845" s="78"/>
+      <c r="A845" s="83"/>
+      <c r="B845" s="84"/>
       <c r="C845" s="34"/>
       <c r="D845" s="34"/>
       <c r="E845" s="34"/>
@@ -55584,8 +55860,8 @@
       </c>
     </row>
     <row r="846">
-      <c r="A846" s="77"/>
-      <c r="B846" s="78"/>
+      <c r="A846" s="83"/>
+      <c r="B846" s="84"/>
       <c r="C846" s="34"/>
       <c r="D846" s="34"/>
       <c r="E846" s="34"/>
@@ -55610,8 +55886,8 @@
       </c>
     </row>
     <row r="847">
-      <c r="A847" s="77"/>
-      <c r="B847" s="78"/>
+      <c r="A847" s="83"/>
+      <c r="B847" s="84"/>
       <c r="C847" s="34"/>
       <c r="D847" s="34"/>
       <c r="E847" s="34"/>
@@ -55636,8 +55912,8 @@
       </c>
     </row>
     <row r="848">
-      <c r="A848" s="77"/>
-      <c r="B848" s="78"/>
+      <c r="A848" s="83"/>
+      <c r="B848" s="84"/>
       <c r="C848" s="34"/>
       <c r="D848" s="34"/>
       <c r="E848" s="34"/>
@@ -55662,8 +55938,8 @@
       </c>
     </row>
     <row r="849">
-      <c r="A849" s="77"/>
-      <c r="B849" s="78"/>
+      <c r="A849" s="83"/>
+      <c r="B849" s="84"/>
       <c r="C849" s="34"/>
       <c r="D849" s="34"/>
       <c r="E849" s="34"/>
@@ -55688,8 +55964,8 @@
       </c>
     </row>
     <row r="850">
-      <c r="A850" s="77"/>
-      <c r="B850" s="78"/>
+      <c r="A850" s="83"/>
+      <c r="B850" s="84"/>
       <c r="C850" s="34"/>
       <c r="D850" s="34"/>
       <c r="E850" s="34"/>
@@ -55714,8 +55990,8 @@
       </c>
     </row>
     <row r="851">
-      <c r="A851" s="77"/>
-      <c r="B851" s="78"/>
+      <c r="A851" s="83"/>
+      <c r="B851" s="84"/>
       <c r="C851" s="34"/>
       <c r="D851" s="34"/>
       <c r="E851" s="34"/>
@@ -55740,8 +56016,8 @@
       </c>
     </row>
     <row r="852">
-      <c r="A852" s="77"/>
-      <c r="B852" s="78"/>
+      <c r="A852" s="83"/>
+      <c r="B852" s="84"/>
       <c r="C852" s="34"/>
       <c r="D852" s="34"/>
       <c r="E852" s="34"/>
@@ -55766,8 +56042,8 @@
       </c>
     </row>
     <row r="853">
-      <c r="A853" s="77"/>
-      <c r="B853" s="78"/>
+      <c r="A853" s="83"/>
+      <c r="B853" s="84"/>
       <c r="C853" s="34"/>
       <c r="D853" s="34"/>
       <c r="E853" s="34"/>
@@ -55792,8 +56068,8 @@
       </c>
     </row>
     <row r="854">
-      <c r="A854" s="77"/>
-      <c r="B854" s="78"/>
+      <c r="A854" s="83"/>
+      <c r="B854" s="84"/>
       <c r="C854" s="34"/>
       <c r="D854" s="34"/>
       <c r="E854" s="34"/>
@@ -55818,8 +56094,8 @@
       </c>
     </row>
     <row r="855">
-      <c r="A855" s="77"/>
-      <c r="B855" s="78"/>
+      <c r="A855" s="83"/>
+      <c r="B855" s="84"/>
       <c r="C855" s="34"/>
       <c r="D855" s="34"/>
       <c r="E855" s="34"/>
@@ -55844,8 +56120,8 @@
       </c>
     </row>
     <row r="856">
-      <c r="A856" s="77"/>
-      <c r="B856" s="78"/>
+      <c r="A856" s="83"/>
+      <c r="B856" s="84"/>
       <c r="C856" s="34"/>
       <c r="D856" s="34"/>
       <c r="E856" s="34"/>
@@ -55870,8 +56146,8 @@
       </c>
     </row>
     <row r="857">
-      <c r="A857" s="77"/>
-      <c r="B857" s="78"/>
+      <c r="A857" s="83"/>
+      <c r="B857" s="84"/>
       <c r="C857" s="34"/>
       <c r="D857" s="34"/>
       <c r="E857" s="34"/>
@@ -55896,8 +56172,8 @@
       </c>
     </row>
     <row r="858">
-      <c r="A858" s="77"/>
-      <c r="B858" s="78"/>
+      <c r="A858" s="83"/>
+      <c r="B858" s="84"/>
       <c r="C858" s="34"/>
       <c r="D858" s="34"/>
       <c r="E858" s="34"/>
@@ -55922,8 +56198,8 @@
       </c>
     </row>
     <row r="859">
-      <c r="A859" s="77"/>
-      <c r="B859" s="78"/>
+      <c r="A859" s="83"/>
+      <c r="B859" s="84"/>
       <c r="C859" s="34"/>
       <c r="D859" s="34"/>
       <c r="E859" s="34"/>
@@ -55948,8 +56224,8 @@
       </c>
     </row>
     <row r="860">
-      <c r="A860" s="77"/>
-      <c r="B860" s="78"/>
+      <c r="A860" s="83"/>
+      <c r="B860" s="84"/>
       <c r="C860" s="34"/>
       <c r="D860" s="34"/>
       <c r="E860" s="34"/>
@@ -55974,8 +56250,8 @@
       </c>
     </row>
     <row r="861">
-      <c r="A861" s="77"/>
-      <c r="B861" s="78"/>
+      <c r="A861" s="83"/>
+      <c r="B861" s="84"/>
       <c r="C861" s="34"/>
       <c r="D861" s="34"/>
       <c r="E861" s="34"/>
@@ -56000,8 +56276,8 @@
       </c>
     </row>
     <row r="862">
-      <c r="A862" s="77"/>
-      <c r="B862" s="78"/>
+      <c r="A862" s="83"/>
+      <c r="B862" s="84"/>
       <c r="C862" s="34"/>
       <c r="D862" s="34"/>
       <c r="E862" s="34"/>
@@ -56026,8 +56302,8 @@
       </c>
     </row>
     <row r="863">
-      <c r="A863" s="77"/>
-      <c r="B863" s="78"/>
+      <c r="A863" s="83"/>
+      <c r="B863" s="84"/>
       <c r="C863" s="34"/>
       <c r="D863" s="34"/>
       <c r="E863" s="34"/>
@@ -56052,8 +56328,8 @@
       </c>
     </row>
     <row r="864">
-      <c r="A864" s="77"/>
-      <c r="B864" s="78"/>
+      <c r="A864" s="83"/>
+      <c r="B864" s="84"/>
       <c r="C864" s="34"/>
       <c r="D864" s="34"/>
       <c r="E864" s="34"/>
@@ -56078,8 +56354,8 @@
       </c>
     </row>
     <row r="865">
-      <c r="A865" s="77"/>
-      <c r="B865" s="78"/>
+      <c r="A865" s="83"/>
+      <c r="B865" s="84"/>
       <c r="C865" s="34"/>
       <c r="D865" s="34"/>
       <c r="E865" s="34"/>
@@ -56104,8 +56380,8 @@
       </c>
     </row>
     <row r="866">
-      <c r="A866" s="77"/>
-      <c r="B866" s="78"/>
+      <c r="A866" s="83"/>
+      <c r="B866" s="84"/>
       <c r="C866" s="34"/>
       <c r="D866" s="34"/>
       <c r="E866" s="34"/>
@@ -56130,8 +56406,8 @@
       </c>
     </row>
     <row r="867">
-      <c r="A867" s="77"/>
-      <c r="B867" s="78"/>
+      <c r="A867" s="83"/>
+      <c r="B867" s="84"/>
       <c r="C867" s="34"/>
       <c r="D867" s="34"/>
       <c r="E867" s="34"/>
@@ -56156,8 +56432,8 @@
       </c>
     </row>
     <row r="868">
-      <c r="A868" s="77"/>
-      <c r="B868" s="78"/>
+      <c r="A868" s="83"/>
+      <c r="B868" s="84"/>
       <c r="C868" s="34"/>
       <c r="D868" s="34"/>
       <c r="E868" s="34"/>
@@ -56182,8 +56458,8 @@
       </c>
     </row>
     <row r="869">
-      <c r="A869" s="77"/>
-      <c r="B869" s="78"/>
+      <c r="A869" s="83"/>
+      <c r="B869" s="84"/>
       <c r="C869" s="34"/>
       <c r="D869" s="34"/>
       <c r="E869" s="34"/>
@@ -56208,8 +56484,8 @@
       </c>
     </row>
     <row r="870">
-      <c r="A870" s="77"/>
-      <c r="B870" s="78"/>
+      <c r="A870" s="83"/>
+      <c r="B870" s="84"/>
       <c r="C870" s="34"/>
       <c r="D870" s="34"/>
       <c r="E870" s="34"/>
@@ -56234,8 +56510,8 @@
       </c>
     </row>
     <row r="871">
-      <c r="A871" s="77"/>
-      <c r="B871" s="78"/>
+      <c r="A871" s="83"/>
+      <c r="B871" s="84"/>
       <c r="C871" s="34"/>
       <c r="D871" s="34"/>
       <c r="E871" s="34"/>
@@ -56260,8 +56536,8 @@
       </c>
     </row>
     <row r="872">
-      <c r="A872" s="77"/>
-      <c r="B872" s="78"/>
+      <c r="A872" s="83"/>
+      <c r="B872" s="84"/>
       <c r="C872" s="34"/>
       <c r="D872" s="34"/>
       <c r="E872" s="34"/>
@@ -56286,8 +56562,8 @@
       </c>
     </row>
     <row r="873">
-      <c r="A873" s="77"/>
-      <c r="B873" s="78"/>
+      <c r="A873" s="83"/>
+      <c r="B873" s="84"/>
       <c r="C873" s="34"/>
       <c r="D873" s="34"/>
       <c r="E873" s="34"/>
@@ -56312,8 +56588,8 @@
       </c>
     </row>
     <row r="874">
-      <c r="A874" s="77"/>
-      <c r="B874" s="78"/>
+      <c r="A874" s="83"/>
+      <c r="B874" s="84"/>
       <c r="C874" s="34"/>
       <c r="D874" s="34"/>
       <c r="E874" s="34"/>
@@ -56338,8 +56614,8 @@
       </c>
     </row>
     <row r="875">
-      <c r="A875" s="77"/>
-      <c r="B875" s="78"/>
+      <c r="A875" s="83"/>
+      <c r="B875" s="84"/>
       <c r="C875" s="34"/>
       <c r="D875" s="34"/>
       <c r="E875" s="34"/>
@@ -56364,8 +56640,8 @@
       </c>
     </row>
     <row r="876">
-      <c r="A876" s="77"/>
-      <c r="B876" s="78"/>
+      <c r="A876" s="83"/>
+      <c r="B876" s="84"/>
       <c r="C876" s="34"/>
       <c r="D876" s="34"/>
       <c r="E876" s="34"/>
@@ -56390,8 +56666,8 @@
       </c>
     </row>
     <row r="877">
-      <c r="A877" s="77"/>
-      <c r="B877" s="78"/>
+      <c r="A877" s="83"/>
+      <c r="B877" s="84"/>
       <c r="C877" s="34"/>
       <c r="D877" s="34"/>
       <c r="E877" s="34"/>
@@ -56416,8 +56692,8 @@
       </c>
     </row>
     <row r="878">
-      <c r="A878" s="77"/>
-      <c r="B878" s="78"/>
+      <c r="A878" s="83"/>
+      <c r="B878" s="84"/>
       <c r="C878" s="34"/>
       <c r="D878" s="34"/>
       <c r="E878" s="34"/>
@@ -56442,8 +56718,8 @@
       </c>
     </row>
     <row r="879">
-      <c r="A879" s="77"/>
-      <c r="B879" s="78"/>
+      <c r="A879" s="83"/>
+      <c r="B879" s="84"/>
       <c r="C879" s="34"/>
       <c r="D879" s="34"/>
       <c r="E879" s="34"/>
@@ -56468,8 +56744,8 @@
       </c>
     </row>
     <row r="880">
-      <c r="A880" s="77"/>
-      <c r="B880" s="78"/>
+      <c r="A880" s="83"/>
+      <c r="B880" s="84"/>
       <c r="C880" s="34"/>
       <c r="D880" s="34"/>
       <c r="E880" s="34"/>
@@ -56494,8 +56770,8 @@
       </c>
     </row>
     <row r="881">
-      <c r="A881" s="77"/>
-      <c r="B881" s="78"/>
+      <c r="A881" s="83"/>
+      <c r="B881" s="84"/>
       <c r="C881" s="34"/>
       <c r="D881" s="34"/>
       <c r="E881" s="34"/>
@@ -56520,8 +56796,8 @@
       </c>
     </row>
     <row r="882">
-      <c r="A882" s="77"/>
-      <c r="B882" s="78"/>
+      <c r="A882" s="83"/>
+      <c r="B882" s="84"/>
       <c r="C882" s="34"/>
       <c r="D882" s="34"/>
       <c r="E882" s="34"/>
@@ -56546,8 +56822,8 @@
       </c>
     </row>
     <row r="883">
-      <c r="A883" s="77"/>
-      <c r="B883" s="78"/>
+      <c r="A883" s="83"/>
+      <c r="B883" s="84"/>
       <c r="C883" s="34"/>
       <c r="D883" s="34"/>
       <c r="E883" s="34"/>
@@ -56572,8 +56848,8 @@
       </c>
     </row>
     <row r="884">
-      <c r="A884" s="77"/>
-      <c r="B884" s="78"/>
+      <c r="A884" s="83"/>
+      <c r="B884" s="84"/>
       <c r="C884" s="34"/>
       <c r="D884" s="34"/>
       <c r="E884" s="34"/>
@@ -56598,8 +56874,8 @@
       </c>
     </row>
     <row r="885">
-      <c r="A885" s="77"/>
-      <c r="B885" s="78"/>
+      <c r="A885" s="83"/>
+      <c r="B885" s="84"/>
       <c r="C885" s="34"/>
       <c r="D885" s="34"/>
       <c r="E885" s="34"/>
@@ -56624,8 +56900,8 @@
       </c>
     </row>
     <row r="886">
-      <c r="A886" s="77"/>
-      <c r="B886" s="78"/>
+      <c r="A886" s="83"/>
+      <c r="B886" s="84"/>
       <c r="C886" s="34"/>
       <c r="D886" s="34"/>
       <c r="E886" s="34"/>
@@ -56650,8 +56926,8 @@
       </c>
     </row>
     <row r="887">
-      <c r="A887" s="77"/>
-      <c r="B887" s="78"/>
+      <c r="A887" s="83"/>
+      <c r="B887" s="84"/>
       <c r="C887" s="34"/>
       <c r="D887" s="34"/>
       <c r="E887" s="34"/>
@@ -56676,8 +56952,8 @@
       </c>
     </row>
     <row r="888">
-      <c r="A888" s="77"/>
-      <c r="B888" s="78"/>
+      <c r="A888" s="83"/>
+      <c r="B888" s="84"/>
       <c r="C888" s="34"/>
       <c r="D888" s="34"/>
       <c r="E888" s="34"/>
@@ -56702,8 +56978,8 @@
       </c>
     </row>
     <row r="889">
-      <c r="A889" s="77"/>
-      <c r="B889" s="78"/>
+      <c r="A889" s="83"/>
+      <c r="B889" s="84"/>
       <c r="C889" s="34"/>
       <c r="D889" s="34"/>
       <c r="E889" s="34"/>
@@ -56728,8 +57004,8 @@
       </c>
     </row>
     <row r="890">
-      <c r="A890" s="77"/>
-      <c r="B890" s="78"/>
+      <c r="A890" s="83"/>
+      <c r="B890" s="84"/>
       <c r="C890" s="34"/>
       <c r="D890" s="34"/>
       <c r="E890" s="34"/>
@@ -56754,8 +57030,8 @@
       </c>
     </row>
     <row r="891">
-      <c r="A891" s="77"/>
-      <c r="B891" s="78"/>
+      <c r="A891" s="83"/>
+      <c r="B891" s="84"/>
       <c r="C891" s="34"/>
       <c r="D891" s="34"/>
       <c r="E891" s="34"/>
@@ -56780,8 +57056,8 @@
       </c>
     </row>
     <row r="892">
-      <c r="A892" s="77"/>
-      <c r="B892" s="78"/>
+      <c r="A892" s="83"/>
+      <c r="B892" s="84"/>
       <c r="C892" s="34"/>
       <c r="D892" s="34"/>
       <c r="E892" s="34"/>
@@ -56806,8 +57082,8 @@
       </c>
     </row>
     <row r="893">
-      <c r="A893" s="77"/>
-      <c r="B893" s="78"/>
+      <c r="A893" s="83"/>
+      <c r="B893" s="84"/>
       <c r="C893" s="34"/>
       <c r="D893" s="34"/>
       <c r="E893" s="34"/>
@@ -56832,8 +57108,8 @@
       </c>
     </row>
     <row r="894">
-      <c r="A894" s="77"/>
-      <c r="B894" s="78"/>
+      <c r="A894" s="83"/>
+      <c r="B894" s="84"/>
       <c r="C894" s="34"/>
       <c r="D894" s="34"/>
       <c r="E894" s="34"/>
@@ -56858,8 +57134,8 @@
       </c>
     </row>
     <row r="895">
-      <c r="A895" s="77"/>
-      <c r="B895" s="78"/>
+      <c r="A895" s="83"/>
+      <c r="B895" s="84"/>
       <c r="C895" s="34"/>
       <c r="D895" s="34"/>
       <c r="E895" s="34"/>
@@ -56884,8 +57160,8 @@
       </c>
     </row>
     <row r="896">
-      <c r="A896" s="77"/>
-      <c r="B896" s="78"/>
+      <c r="A896" s="83"/>
+      <c r="B896" s="84"/>
       <c r="C896" s="34"/>
       <c r="D896" s="34"/>
       <c r="E896" s="34"/>
@@ -56910,8 +57186,8 @@
       </c>
     </row>
     <row r="897">
-      <c r="A897" s="77"/>
-      <c r="B897" s="78"/>
+      <c r="A897" s="83"/>
+      <c r="B897" s="84"/>
       <c r="C897" s="34"/>
       <c r="D897" s="34"/>
       <c r="E897" s="34"/>
@@ -56936,8 +57212,8 @@
       </c>
     </row>
     <row r="898">
-      <c r="A898" s="77"/>
-      <c r="B898" s="78"/>
+      <c r="A898" s="83"/>
+      <c r="B898" s="84"/>
       <c r="C898" s="34"/>
       <c r="D898" s="34"/>
       <c r="E898" s="34"/>
@@ -56962,8 +57238,8 @@
       </c>
     </row>
     <row r="899">
-      <c r="A899" s="77"/>
-      <c r="B899" s="78"/>
+      <c r="A899" s="83"/>
+      <c r="B899" s="84"/>
       <c r="C899" s="34"/>
       <c r="D899" s="34"/>
       <c r="E899" s="34"/>
@@ -56988,8 +57264,8 @@
       </c>
     </row>
     <row r="900">
-      <c r="A900" s="77"/>
-      <c r="B900" s="78"/>
+      <c r="A900" s="83"/>
+      <c r="B900" s="84"/>
       <c r="C900" s="34"/>
       <c r="D900" s="34"/>
       <c r="E900" s="34"/>
@@ -57014,8 +57290,8 @@
       </c>
     </row>
     <row r="901">
-      <c r="A901" s="77"/>
-      <c r="B901" s="78"/>
+      <c r="A901" s="83"/>
+      <c r="B901" s="84"/>
       <c r="C901" s="34"/>
       <c r="D901" s="34"/>
       <c r="E901" s="34"/>
@@ -57040,8 +57316,8 @@
       </c>
     </row>
     <row r="902">
-      <c r="A902" s="77"/>
-      <c r="B902" s="78"/>
+      <c r="A902" s="83"/>
+      <c r="B902" s="84"/>
       <c r="C902" s="34"/>
       <c r="D902" s="34"/>
       <c r="E902" s="34"/>
@@ -57066,8 +57342,8 @@
       </c>
     </row>
     <row r="903">
-      <c r="A903" s="77"/>
-      <c r="B903" s="78"/>
+      <c r="A903" s="83"/>
+      <c r="B903" s="84"/>
       <c r="C903" s="34"/>
       <c r="D903" s="34"/>
       <c r="E903" s="34"/>
@@ -57092,8 +57368,8 @@
       </c>
     </row>
     <row r="904">
-      <c r="A904" s="77"/>
-      <c r="B904" s="78"/>
+      <c r="A904" s="83"/>
+      <c r="B904" s="84"/>
       <c r="C904" s="34"/>
       <c r="D904" s="34"/>
       <c r="E904" s="34"/>
@@ -57118,8 +57394,8 @@
       </c>
     </row>
     <row r="905">
-      <c r="A905" s="77"/>
-      <c r="B905" s="78"/>
+      <c r="A905" s="83"/>
+      <c r="B905" s="84"/>
       <c r="C905" s="34"/>
       <c r="D905" s="34"/>
       <c r="E905" s="34"/>
@@ -57144,8 +57420,8 @@
       </c>
     </row>
     <row r="906">
-      <c r="A906" s="77"/>
-      <c r="B906" s="78"/>
+      <c r="A906" s="83"/>
+      <c r="B906" s="84"/>
       <c r="C906" s="34"/>
       <c r="D906" s="34"/>
       <c r="E906" s="34"/>
@@ -57170,8 +57446,8 @@
       </c>
     </row>
     <row r="907">
-      <c r="A907" s="77"/>
-      <c r="B907" s="78"/>
+      <c r="A907" s="83"/>
+      <c r="B907" s="84"/>
       <c r="C907" s="34"/>
       <c r="D907" s="34"/>
       <c r="E907" s="34"/>
@@ -57196,8 +57472,8 @@
       </c>
     </row>
     <row r="908">
-      <c r="A908" s="77"/>
-      <c r="B908" s="78"/>
+      <c r="A908" s="83"/>
+      <c r="B908" s="84"/>
       <c r="C908" s="34"/>
       <c r="D908" s="34"/>
       <c r="E908" s="34"/>
@@ -57222,8 +57498,8 @@
       </c>
     </row>
     <row r="909">
-      <c r="A909" s="77"/>
-      <c r="B909" s="78"/>
+      <c r="A909" s="83"/>
+      <c r="B909" s="84"/>
       <c r="C909" s="34"/>
       <c r="D909" s="34"/>
       <c r="E909" s="34"/>
@@ -57248,8 +57524,8 @@
       </c>
     </row>
     <row r="910">
-      <c r="A910" s="77"/>
-      <c r="B910" s="78"/>
+      <c r="A910" s="83"/>
+      <c r="B910" s="84"/>
       <c r="C910" s="34"/>
       <c r="D910" s="34"/>
       <c r="E910" s="34"/>
@@ -57274,8 +57550,8 @@
       </c>
     </row>
     <row r="911">
-      <c r="A911" s="77"/>
-      <c r="B911" s="78"/>
+      <c r="A911" s="83"/>
+      <c r="B911" s="84"/>
       <c r="C911" s="34"/>
       <c r="D911" s="34"/>
       <c r="E911" s="34"/>
@@ -57300,8 +57576,8 @@
       </c>
     </row>
     <row r="912">
-      <c r="A912" s="77"/>
-      <c r="B912" s="78"/>
+      <c r="A912" s="83"/>
+      <c r="B912" s="84"/>
       <c r="C912" s="34"/>
       <c r="D912" s="34"/>
       <c r="E912" s="34"/>
@@ -57326,8 +57602,8 @@
       </c>
     </row>
     <row r="913">
-      <c r="A913" s="77"/>
-      <c r="B913" s="78"/>
+      <c r="A913" s="83"/>
+      <c r="B913" s="84"/>
       <c r="C913" s="34"/>
       <c r="D913" s="34"/>
       <c r="E913" s="34"/>
@@ -57352,8 +57628,8 @@
       </c>
     </row>
     <row r="914">
-      <c r="A914" s="77"/>
-      <c r="B914" s="78"/>
+      <c r="A914" s="83"/>
+      <c r="B914" s="84"/>
       <c r="C914" s="34"/>
       <c r="D914" s="34"/>
       <c r="E914" s="34"/>
@@ -57378,8 +57654,8 @@
       </c>
     </row>
     <row r="915">
-      <c r="A915" s="77"/>
-      <c r="B915" s="78"/>
+      <c r="A915" s="83"/>
+      <c r="B915" s="84"/>
       <c r="C915" s="34"/>
       <c r="D915" s="34"/>
       <c r="E915" s="34"/>
@@ -57404,8 +57680,8 @@
       </c>
     </row>
     <row r="916">
-      <c r="A916" s="77"/>
-      <c r="B916" s="78"/>
+      <c r="A916" s="83"/>
+      <c r="B916" s="84"/>
       <c r="C916" s="34"/>
       <c r="D916" s="34"/>
       <c r="E916" s="34"/>
@@ -57430,8 +57706,8 @@
       </c>
     </row>
     <row r="917">
-      <c r="A917" s="77"/>
-      <c r="B917" s="78"/>
+      <c r="A917" s="83"/>
+      <c r="B917" s="84"/>
       <c r="C917" s="34"/>
       <c r="D917" s="34"/>
       <c r="E917" s="34"/>
@@ -57456,8 +57732,8 @@
       </c>
     </row>
     <row r="918">
-      <c r="A918" s="77"/>
-      <c r="B918" s="78"/>
+      <c r="A918" s="83"/>
+      <c r="B918" s="84"/>
       <c r="C918" s="34"/>
       <c r="D918" s="34"/>
       <c r="E918" s="34"/>
@@ -57482,8 +57758,8 @@
       </c>
     </row>
     <row r="919">
-      <c r="A919" s="77"/>
-      <c r="B919" s="78"/>
+      <c r="A919" s="83"/>
+      <c r="B919" s="84"/>
       <c r="C919" s="34"/>
       <c r="D919" s="34"/>
       <c r="E919" s="34"/>
@@ -57508,8 +57784,8 @@
       </c>
     </row>
     <row r="920">
-      <c r="A920" s="77"/>
-      <c r="B920" s="78"/>
+      <c r="A920" s="83"/>
+      <c r="B920" s="84"/>
       <c r="C920" s="34"/>
       <c r="D920" s="34"/>
       <c r="E920" s="34"/>
@@ -57534,8 +57810,8 @@
       </c>
     </row>
     <row r="921">
-      <c r="A921" s="77"/>
-      <c r="B921" s="78"/>
+      <c r="A921" s="83"/>
+      <c r="B921" s="84"/>
       <c r="C921" s="34"/>
       <c r="D921" s="34"/>
       <c r="E921" s="34"/>
@@ -57560,8 +57836,8 @@
       </c>
     </row>
     <row r="922">
-      <c r="A922" s="77"/>
-      <c r="B922" s="78"/>
+      <c r="A922" s="83"/>
+      <c r="B922" s="84"/>
       <c r="C922" s="34"/>
       <c r="D922" s="34"/>
       <c r="E922" s="34"/>
@@ -57586,8 +57862,8 @@
       </c>
     </row>
     <row r="923">
-      <c r="A923" s="77"/>
-      <c r="B923" s="78"/>
+      <c r="A923" s="83"/>
+      <c r="B923" s="84"/>
       <c r="C923" s="34"/>
       <c r="D923" s="34"/>
       <c r="E923" s="34"/>
@@ -57612,8 +57888,8 @@
       </c>
     </row>
     <row r="924">
-      <c r="A924" s="77"/>
-      <c r="B924" s="78"/>
+      <c r="A924" s="83"/>
+      <c r="B924" s="84"/>
       <c r="C924" s="34"/>
       <c r="D924" s="34"/>
       <c r="E924" s="34"/>
@@ -57638,8 +57914,8 @@
       </c>
     </row>
     <row r="925">
-      <c r="A925" s="77"/>
-      <c r="B925" s="78"/>
+      <c r="A925" s="83"/>
+      <c r="B925" s="84"/>
       <c r="C925" s="34"/>
       <c r="D925" s="34"/>
       <c r="E925" s="34"/>
@@ -57664,8 +57940,8 @@
       </c>
     </row>
     <row r="926">
-      <c r="A926" s="77"/>
-      <c r="B926" s="78"/>
+      <c r="A926" s="83"/>
+      <c r="B926" s="84"/>
       <c r="C926" s="34"/>
       <c r="D926" s="34"/>
       <c r="E926" s="34"/>
@@ -57690,8 +57966,8 @@
       </c>
     </row>
     <row r="927">
-      <c r="A927" s="77"/>
-      <c r="B927" s="78"/>
+      <c r="A927" s="83"/>
+      <c r="B927" s="84"/>
       <c r="C927" s="34"/>
       <c r="D927" s="34"/>
       <c r="E927" s="34"/>
@@ -57716,8 +57992,8 @@
       </c>
     </row>
     <row r="928">
-      <c r="A928" s="77"/>
-      <c r="B928" s="78"/>
+      <c r="A928" s="83"/>
+      <c r="B928" s="84"/>
       <c r="C928" s="34"/>
       <c r="D928" s="34"/>
       <c r="E928" s="34"/>
@@ -57742,8 +58018,8 @@
       </c>
     </row>
     <row r="929">
-      <c r="A929" s="77"/>
-      <c r="B929" s="78"/>
+      <c r="A929" s="83"/>
+      <c r="B929" s="84"/>
       <c r="C929" s="34"/>
       <c r="D929" s="34"/>
       <c r="E929" s="34"/>
@@ -57768,8 +58044,8 @@
       </c>
     </row>
     <row r="930">
-      <c r="A930" s="77"/>
-      <c r="B930" s="78"/>
+      <c r="A930" s="83"/>
+      <c r="B930" s="84"/>
       <c r="C930" s="34"/>
       <c r="D930" s="34"/>
       <c r="E930" s="34"/>
@@ -57794,8 +58070,8 @@
       </c>
     </row>
     <row r="931">
-      <c r="A931" s="77"/>
-      <c r="B931" s="78"/>
+      <c r="A931" s="83"/>
+      <c r="B931" s="84"/>
       <c r="C931" s="34"/>
       <c r="D931" s="34"/>
       <c r="E931" s="34"/>
@@ -57820,8 +58096,8 @@
       </c>
     </row>
     <row r="932">
-      <c r="A932" s="77"/>
-      <c r="B932" s="78"/>
+      <c r="A932" s="83"/>
+      <c r="B932" s="84"/>
       <c r="C932" s="34"/>
       <c r="D932" s="34"/>
       <c r="E932" s="34"/>
@@ -57846,8 +58122,8 @@
       </c>
     </row>
     <row r="933">
-      <c r="A933" s="77"/>
-      <c r="B933" s="78"/>
+      <c r="A933" s="83"/>
+      <c r="B933" s="84"/>
       <c r="C933" s="34"/>
       <c r="D933" s="34"/>
       <c r="E933" s="34"/>
@@ -57872,8 +58148,8 @@
       </c>
     </row>
     <row r="934">
-      <c r="A934" s="77"/>
-      <c r="B934" s="78"/>
+      <c r="A934" s="83"/>
+      <c r="B934" s="84"/>
       <c r="C934" s="34"/>
       <c r="D934" s="34"/>
       <c r="E934" s="34"/>
@@ -57898,8 +58174,8 @@
       </c>
     </row>
     <row r="935">
-      <c r="A935" s="77"/>
-      <c r="B935" s="78"/>
+      <c r="A935" s="83"/>
+      <c r="B935" s="84"/>
       <c r="C935" s="34"/>
       <c r="D935" s="34"/>
       <c r="E935" s="34"/>
@@ -57924,8 +58200,8 @@
       </c>
     </row>
     <row r="936">
-      <c r="A936" s="77"/>
-      <c r="B936" s="78"/>
+      <c r="A936" s="83"/>
+      <c r="B936" s="84"/>
       <c r="C936" s="34"/>
       <c r="D936" s="34"/>
       <c r="E936" s="34"/>
@@ -57950,8 +58226,8 @@
       </c>
     </row>
     <row r="937">
-      <c r="A937" s="77"/>
-      <c r="B937" s="78"/>
+      <c r="A937" s="83"/>
+      <c r="B937" s="84"/>
       <c r="C937" s="34"/>
       <c r="D937" s="34"/>
       <c r="E937" s="34"/>
@@ -57976,8 +58252,8 @@
       </c>
     </row>
     <row r="938">
-      <c r="A938" s="77"/>
-      <c r="B938" s="78"/>
+      <c r="A938" s="83"/>
+      <c r="B938" s="84"/>
       <c r="C938" s="34"/>
       <c r="D938" s="34"/>
       <c r="E938" s="34"/>
@@ -58002,8 +58278,8 @@
       </c>
     </row>
     <row r="939">
-      <c r="A939" s="77"/>
-      <c r="B939" s="78"/>
+      <c r="A939" s="83"/>
+      <c r="B939" s="84"/>
       <c r="C939" s="34"/>
       <c r="D939" s="34"/>
       <c r="E939" s="34"/>
@@ -58028,8 +58304,8 @@
       </c>
     </row>
     <row r="940">
-      <c r="A940" s="77"/>
-      <c r="B940" s="78"/>
+      <c r="A940" s="83"/>
+      <c r="B940" s="84"/>
       <c r="C940" s="34"/>
       <c r="D940" s="34"/>
       <c r="E940" s="34"/>
@@ -58054,8 +58330,8 @@
       </c>
     </row>
     <row r="941">
-      <c r="A941" s="77"/>
-      <c r="B941" s="78"/>
+      <c r="A941" s="83"/>
+      <c r="B941" s="84"/>
       <c r="C941" s="34"/>
       <c r="D941" s="34"/>
       <c r="E941" s="34"/>
@@ -58080,8 +58356,8 @@
       </c>
     </row>
     <row r="942">
-      <c r="A942" s="77"/>
-      <c r="B942" s="78"/>
+      <c r="A942" s="83"/>
+      <c r="B942" s="84"/>
       <c r="C942" s="34"/>
       <c r="D942" s="34"/>
       <c r="E942" s="34"/>
@@ -58106,8 +58382,8 @@
       </c>
     </row>
     <row r="943">
-      <c r="A943" s="77"/>
-      <c r="B943" s="78"/>
+      <c r="A943" s="83"/>
+      <c r="B943" s="84"/>
       <c r="C943" s="34"/>
       <c r="D943" s="34"/>
       <c r="E943" s="34"/>
@@ -58132,8 +58408,8 @@
       </c>
     </row>
     <row r="944">
-      <c r="A944" s="77"/>
-      <c r="B944" s="78"/>
+      <c r="A944" s="83"/>
+      <c r="B944" s="84"/>
       <c r="C944" s="34"/>
       <c r="D944" s="34"/>
       <c r="E944" s="34"/>
@@ -58158,8 +58434,8 @@
       </c>
     </row>
     <row r="945">
-      <c r="A945" s="77"/>
-      <c r="B945" s="78"/>
+      <c r="A945" s="83"/>
+      <c r="B945" s="84"/>
       <c r="C945" s="34"/>
       <c r="D945" s="34"/>
       <c r="E945" s="34"/>
@@ -58184,8 +58460,8 @@
       </c>
     </row>
     <row r="946">
-      <c r="A946" s="77"/>
-      <c r="B946" s="78"/>
+      <c r="A946" s="83"/>
+      <c r="B946" s="84"/>
       <c r="C946" s="34"/>
       <c r="D946" s="34"/>
       <c r="E946" s="34"/>
@@ -58210,8 +58486,8 @@
       </c>
     </row>
     <row r="947">
-      <c r="A947" s="77"/>
-      <c r="B947" s="78"/>
+      <c r="A947" s="83"/>
+      <c r="B947" s="84"/>
       <c r="C947" s="34"/>
       <c r="D947" s="34"/>
       <c r="E947" s="34"/>
@@ -58236,8 +58512,8 @@
       </c>
     </row>
     <row r="948">
-      <c r="A948" s="77"/>
-      <c r="B948" s="78"/>
+      <c r="A948" s="83"/>
+      <c r="B948" s="84"/>
       <c r="C948" s="34"/>
       <c r="D948" s="34"/>
       <c r="E948" s="34"/>
@@ -58262,8 +58538,8 @@
       </c>
     </row>
     <row r="949">
-      <c r="A949" s="77"/>
-      <c r="B949" s="78"/>
+      <c r="A949" s="83"/>
+      <c r="B949" s="84"/>
       <c r="C949" s="34"/>
       <c r="D949" s="34"/>
       <c r="E949" s="34"/>
@@ -58288,8 +58564,8 @@
       </c>
     </row>
     <row r="950">
-      <c r="A950" s="77"/>
-      <c r="B950" s="78"/>
+      <c r="A950" s="83"/>
+      <c r="B950" s="84"/>
       <c r="C950" s="34"/>
       <c r="D950" s="34"/>
       <c r="E950" s="34"/>
@@ -58314,8 +58590,8 @@
       </c>
     </row>
     <row r="951">
-      <c r="A951" s="77"/>
-      <c r="B951" s="78"/>
+      <c r="A951" s="83"/>
+      <c r="B951" s="84"/>
       <c r="C951" s="34"/>
       <c r="D951" s="34"/>
       <c r="E951" s="34"/>
@@ -58340,8 +58616,8 @@
       </c>
     </row>
     <row r="952">
-      <c r="A952" s="77"/>
-      <c r="B952" s="78"/>
+      <c r="A952" s="83"/>
+      <c r="B952" s="84"/>
       <c r="C952" s="34"/>
       <c r="D952" s="34"/>
       <c r="E952" s="34"/>
@@ -58366,8 +58642,8 @@
       </c>
     </row>
     <row r="953">
-      <c r="A953" s="77"/>
-      <c r="B953" s="78"/>
+      <c r="A953" s="83"/>
+      <c r="B953" s="84"/>
       <c r="C953" s="34"/>
       <c r="D953" s="34"/>
       <c r="E953" s="34"/>
@@ -58392,8 +58668,8 @@
       </c>
     </row>
     <row r="954">
-      <c r="A954" s="77"/>
-      <c r="B954" s="78"/>
+      <c r="A954" s="83"/>
+      <c r="B954" s="84"/>
       <c r="C954" s="34"/>
       <c r="D954" s="34"/>
       <c r="E954" s="34"/>
@@ -58418,8 +58694,8 @@
       </c>
     </row>
     <row r="955">
-      <c r="A955" s="77"/>
-      <c r="B955" s="78"/>
+      <c r="A955" s="83"/>
+      <c r="B955" s="84"/>
       <c r="C955" s="34"/>
       <c r="D955" s="34"/>
       <c r="E955" s="34"/>
@@ -58444,8 +58720,8 @@
       </c>
     </row>
     <row r="956">
-      <c r="A956" s="77"/>
-      <c r="B956" s="78"/>
+      <c r="A956" s="83"/>
+      <c r="B956" s="84"/>
       <c r="C956" s="34"/>
       <c r="D956" s="34"/>
       <c r="E956" s="34"/>
@@ -58470,8 +58746,8 @@
       </c>
     </row>
     <row r="957">
-      <c r="A957" s="77"/>
-      <c r="B957" s="78"/>
+      <c r="A957" s="83"/>
+      <c r="B957" s="84"/>
       <c r="C957" s="34"/>
       <c r="D957" s="34"/>
       <c r="E957" s="34"/>
@@ -58496,8 +58772,8 @@
       </c>
     </row>
     <row r="958">
-      <c r="A958" s="77"/>
-      <c r="B958" s="78"/>
+      <c r="A958" s="83"/>
+      <c r="B958" s="84"/>
       <c r="C958" s="34"/>
       <c r="D958" s="34"/>
       <c r="E958" s="34"/>
@@ -58522,8 +58798,8 @@
       </c>
     </row>
     <row r="959">
-      <c r="A959" s="77"/>
-      <c r="B959" s="78"/>
+      <c r="A959" s="83"/>
+      <c r="B959" s="84"/>
       <c r="C959" s="34"/>
       <c r="D959" s="34"/>
       <c r="E959" s="34"/>
@@ -58548,8 +58824,8 @@
       </c>
     </row>
     <row r="960">
-      <c r="A960" s="77"/>
-      <c r="B960" s="78"/>
+      <c r="A960" s="83"/>
+      <c r="B960" s="84"/>
       <c r="C960" s="34"/>
       <c r="D960" s="34"/>
       <c r="E960" s="34"/>
@@ -58574,8 +58850,8 @@
       </c>
     </row>
     <row r="961">
-      <c r="A961" s="77"/>
-      <c r="B961" s="78"/>
+      <c r="A961" s="83"/>
+      <c r="B961" s="84"/>
       <c r="C961" s="34"/>
       <c r="D961" s="34"/>
       <c r="E961" s="34"/>
@@ -58600,8 +58876,8 @@
       </c>
     </row>
     <row r="962">
-      <c r="A962" s="77"/>
-      <c r="B962" s="78"/>
+      <c r="A962" s="83"/>
+      <c r="B962" s="84"/>
       <c r="C962" s="34"/>
       <c r="D962" s="34"/>
       <c r="E962" s="34"/>
@@ -58626,8 +58902,8 @@
       </c>
     </row>
     <row r="963">
-      <c r="A963" s="77"/>
-      <c r="B963" s="78"/>
+      <c r="A963" s="83"/>
+      <c r="B963" s="84"/>
       <c r="C963" s="34"/>
       <c r="D963" s="34"/>
       <c r="E963" s="34"/>
@@ -58652,8 +58928,8 @@
       </c>
     </row>
     <row r="964">
-      <c r="A964" s="77"/>
-      <c r="B964" s="78"/>
+      <c r="A964" s="83"/>
+      <c r="B964" s="84"/>
       <c r="C964" s="34"/>
       <c r="D964" s="34"/>
       <c r="E964" s="34"/>
@@ -58678,8 +58954,8 @@
       </c>
     </row>
     <row r="965">
-      <c r="A965" s="77"/>
-      <c r="B965" s="78"/>
+      <c r="A965" s="83"/>
+      <c r="B965" s="84"/>
       <c r="C965" s="34"/>
       <c r="D965" s="34"/>
       <c r="E965" s="34"/>
@@ -58704,8 +58980,8 @@
       </c>
     </row>
     <row r="966">
-      <c r="A966" s="77"/>
-      <c r="B966" s="78"/>
+      <c r="A966" s="83"/>
+      <c r="B966" s="84"/>
       <c r="C966" s="34"/>
       <c r="D966" s="34"/>
       <c r="E966" s="34"/>
@@ -58730,8 +59006,8 @@
       </c>
     </row>
     <row r="967">
-      <c r="A967" s="77"/>
-      <c r="B967" s="78"/>
+      <c r="A967" s="83"/>
+      <c r="B967" s="84"/>
       <c r="C967" s="34"/>
       <c r="D967" s="34"/>
       <c r="E967" s="34"/>
@@ -58756,8 +59032,8 @@
       </c>
     </row>
     <row r="968">
-      <c r="A968" s="77"/>
-      <c r="B968" s="78"/>
+      <c r="A968" s="83"/>
+      <c r="B968" s="84"/>
       <c r="C968" s="34"/>
       <c r="D968" s="34"/>
       <c r="E968" s="34"/>
@@ -58782,8 +59058,8 @@
       </c>
     </row>
     <row r="969">
-      <c r="A969" s="77"/>
-      <c r="B969" s="78"/>
+      <c r="A969" s="83"/>
+      <c r="B969" s="84"/>
       <c r="C969" s="34"/>
       <c r="D969" s="34"/>
       <c r="E969" s="34"/>
@@ -58808,8 +59084,8 @@
       </c>
     </row>
     <row r="970">
-      <c r="A970" s="77"/>
-      <c r="B970" s="78"/>
+      <c r="A970" s="83"/>
+      <c r="B970" s="84"/>
       <c r="C970" s="34"/>
       <c r="D970" s="34"/>
       <c r="E970" s="34"/>
@@ -58834,8 +59110,8 @@
       </c>
     </row>
     <row r="971">
-      <c r="A971" s="77"/>
-      <c r="B971" s="78"/>
+      <c r="A971" s="83"/>
+      <c r="B971" s="84"/>
       <c r="C971" s="34"/>
       <c r="D971" s="34"/>
       <c r="E971" s="34"/>
@@ -58860,8 +59136,8 @@
       </c>
     </row>
     <row r="972">
-      <c r="A972" s="77"/>
-      <c r="B972" s="78"/>
+      <c r="A972" s="83"/>
+      <c r="B972" s="84"/>
       <c r="C972" s="34"/>
       <c r="D972" s="34"/>
       <c r="E972" s="34"/>
@@ -58886,8 +59162,8 @@
       </c>
     </row>
     <row r="973">
-      <c r="A973" s="77"/>
-      <c r="B973" s="78"/>
+      <c r="A973" s="83"/>
+      <c r="B973" s="84"/>
       <c r="C973" s="34"/>
       <c r="D973" s="34"/>
       <c r="E973" s="34"/>
@@ -58912,8 +59188,8 @@
       </c>
     </row>
     <row r="974">
-      <c r="A974" s="77"/>
-      <c r="B974" s="78"/>
+      <c r="A974" s="83"/>
+      <c r="B974" s="84"/>
       <c r="C974" s="34"/>
       <c r="D974" s="34"/>
       <c r="E974" s="34"/>
@@ -58938,8 +59214,8 @@
       </c>
     </row>
     <row r="975">
-      <c r="A975" s="77"/>
-      <c r="B975" s="78"/>
+      <c r="A975" s="83"/>
+      <c r="B975" s="84"/>
       <c r="C975" s="34"/>
       <c r="D975" s="34"/>
       <c r="E975" s="34"/>
@@ -58964,8 +59240,8 @@
       </c>
     </row>
     <row r="976">
-      <c r="A976" s="77"/>
-      <c r="B976" s="78"/>
+      <c r="A976" s="83"/>
+      <c r="B976" s="84"/>
       <c r="C976" s="34"/>
       <c r="D976" s="34"/>
       <c r="E976" s="34"/>
@@ -58990,8 +59266,8 @@
       </c>
     </row>
     <row r="977">
-      <c r="A977" s="77"/>
-      <c r="B977" s="78"/>
+      <c r="A977" s="83"/>
+      <c r="B977" s="84"/>
       <c r="C977" s="34"/>
       <c r="D977" s="34"/>
       <c r="E977" s="34"/>
@@ -59016,8 +59292,8 @@
       </c>
     </row>
     <row r="978">
-      <c r="A978" s="77"/>
-      <c r="B978" s="78"/>
+      <c r="A978" s="83"/>
+      <c r="B978" s="84"/>
       <c r="C978" s="34"/>
       <c r="D978" s="34"/>
       <c r="E978" s="34"/>
@@ -59042,8 +59318,8 @@
       </c>
     </row>
     <row r="979">
-      <c r="A979" s="77"/>
-      <c r="B979" s="78"/>
+      <c r="A979" s="83"/>
+      <c r="B979" s="84"/>
       <c r="C979" s="34"/>
       <c r="D979" s="34"/>
       <c r="E979" s="34"/>
@@ -59068,8 +59344,8 @@
       </c>
     </row>
     <row r="980">
-      <c r="A980" s="77"/>
-      <c r="B980" s="78"/>
+      <c r="A980" s="83"/>
+      <c r="B980" s="84"/>
       <c r="C980" s="34"/>
       <c r="D980" s="34"/>
       <c r="E980" s="34"/>
@@ -59094,8 +59370,8 @@
       </c>
     </row>
     <row r="981">
-      <c r="A981" s="77"/>
-      <c r="B981" s="78"/>
+      <c r="A981" s="83"/>
+      <c r="B981" s="84"/>
       <c r="C981" s="34"/>
       <c r="D981" s="34"/>
       <c r="E981" s="34"/>
@@ -59120,8 +59396,8 @@
       </c>
     </row>
     <row r="982">
-      <c r="A982" s="77"/>
-      <c r="B982" s="78"/>
+      <c r="A982" s="83"/>
+      <c r="B982" s="84"/>
       <c r="C982" s="34"/>
       <c r="D982" s="34"/>
       <c r="E982" s="34"/>
@@ -59146,8 +59422,8 @@
       </c>
     </row>
     <row r="983">
-      <c r="A983" s="77"/>
-      <c r="B983" s="78"/>
+      <c r="A983" s="83"/>
+      <c r="B983" s="84"/>
       <c r="C983" s="34"/>
       <c r="D983" s="34"/>
       <c r="E983" s="34"/>
@@ -59172,8 +59448,8 @@
       </c>
     </row>
     <row r="984">
-      <c r="A984" s="77"/>
-      <c r="B984" s="78"/>
+      <c r="A984" s="83"/>
+      <c r="B984" s="84"/>
       <c r="C984" s="34"/>
       <c r="D984" s="34"/>
       <c r="E984" s="34"/>
@@ -59198,8 +59474,8 @@
       </c>
     </row>
     <row r="985">
-      <c r="A985" s="77"/>
-      <c r="B985" s="78"/>
+      <c r="A985" s="83"/>
+      <c r="B985" s="84"/>
       <c r="C985" s="34"/>
       <c r="D985" s="34"/>
       <c r="E985" s="34"/>
@@ -59224,8 +59500,8 @@
       </c>
     </row>
     <row r="986">
-      <c r="A986" s="77"/>
-      <c r="B986" s="78"/>
+      <c r="A986" s="83"/>
+      <c r="B986" s="84"/>
       <c r="C986" s="34"/>
       <c r="D986" s="34"/>
       <c r="E986" s="34"/>
@@ -59250,8 +59526,8 @@
       </c>
     </row>
     <row r="987">
-      <c r="A987" s="77"/>
-      <c r="B987" s="78"/>
+      <c r="A987" s="83"/>
+      <c r="B987" s="84"/>
       <c r="C987" s="34"/>
       <c r="D987" s="34"/>
       <c r="E987" s="34"/>
@@ -59276,8 +59552,8 @@
       </c>
     </row>
     <row r="988">
-      <c r="A988" s="77"/>
-      <c r="B988" s="78"/>
+      <c r="A988" s="83"/>
+      <c r="B988" s="84"/>
       <c r="C988" s="34"/>
       <c r="D988" s="34"/>
       <c r="E988" s="34"/>
@@ -59302,8 +59578,8 @@
       </c>
     </row>
     <row r="989">
-      <c r="A989" s="77"/>
-      <c r="B989" s="78"/>
+      <c r="A989" s="83"/>
+      <c r="B989" s="84"/>
       <c r="C989" s="34"/>
       <c r="D989" s="34"/>
       <c r="E989" s="34"/>
@@ -59328,8 +59604,8 @@
       </c>
     </row>
     <row r="990">
-      <c r="A990" s="77"/>
-      <c r="B990" s="78"/>
+      <c r="A990" s="83"/>
+      <c r="B990" s="84"/>
       <c r="C990" s="34"/>
       <c r="D990" s="34"/>
       <c r="E990" s="34"/>
@@ -59354,8 +59630,8 @@
       </c>
     </row>
     <row r="991">
-      <c r="A991" s="77"/>
-      <c r="B991" s="78"/>
+      <c r="A991" s="83"/>
+      <c r="B991" s="84"/>
       <c r="C991" s="34"/>
       <c r="D991" s="34"/>
       <c r="E991" s="34"/>
@@ -59380,8 +59656,8 @@
       </c>
     </row>
     <row r="992">
-      <c r="A992" s="77"/>
-      <c r="B992" s="78"/>
+      <c r="A992" s="83"/>
+      <c r="B992" s="84"/>
       <c r="C992" s="34"/>
       <c r="D992" s="34"/>
       <c r="E992" s="34"/>
@@ -59406,8 +59682,8 @@
       </c>
     </row>
     <row r="993">
-      <c r="A993" s="77"/>
-      <c r="B993" s="78"/>
+      <c r="A993" s="83"/>
+      <c r="B993" s="84"/>
       <c r="C993" s="34"/>
       <c r="D993" s="34"/>
       <c r="E993" s="34"/>
@@ -59432,8 +59708,8 @@
       </c>
     </row>
     <row r="994">
-      <c r="A994" s="77"/>
-      <c r="B994" s="78"/>
+      <c r="A994" s="83"/>
+      <c r="B994" s="84"/>
       <c r="C994" s="34"/>
       <c r="D994" s="34"/>
       <c r="E994" s="34"/>
@@ -59458,8 +59734,8 @@
       </c>
     </row>
     <row r="995">
-      <c r="A995" s="77"/>
-      <c r="B995" s="78"/>
+      <c r="A995" s="83"/>
+      <c r="B995" s="84"/>
       <c r="C995" s="34"/>
       <c r="D995" s="34"/>
       <c r="E995" s="34"/>
@@ -59484,8 +59760,8 @@
       </c>
     </row>
     <row r="996">
-      <c r="A996" s="77"/>
-      <c r="B996" s="78"/>
+      <c r="A996" s="83"/>
+      <c r="B996" s="84"/>
       <c r="C996" s="34"/>
       <c r="D996" s="34"/>
       <c r="E996" s="34"/>
@@ -59510,8 +59786,8 @@
       </c>
     </row>
     <row r="997">
-      <c r="A997" s="77"/>
-      <c r="B997" s="78"/>
+      <c r="A997" s="83"/>
+      <c r="B997" s="84"/>
       <c r="C997" s="34"/>
       <c r="D997" s="34"/>
       <c r="E997" s="34"/>
@@ -59536,8 +59812,8 @@
       </c>
     </row>
     <row r="998">
-      <c r="A998" s="77"/>
-      <c r="B998" s="78"/>
+      <c r="A998" s="83"/>
+      <c r="B998" s="84"/>
       <c r="C998" s="34"/>
       <c r="D998" s="34"/>
       <c r="E998" s="34"/>
@@ -59562,8 +59838,8 @@
       </c>
     </row>
     <row r="999">
-      <c r="A999" s="77"/>
-      <c r="B999" s="78"/>
+      <c r="A999" s="83"/>
+      <c r="B999" s="84"/>
       <c r="C999" s="34"/>
       <c r="D999" s="34"/>
       <c r="E999" s="34"/>
@@ -59588,8 +59864,8 @@
       </c>
     </row>
     <row r="1000">
-      <c r="A1000" s="77"/>
-      <c r="B1000" s="78"/>
+      <c r="A1000" s="83"/>
+      <c r="B1000" s="84"/>
       <c r="C1000" s="34"/>
       <c r="D1000" s="34"/>
       <c r="E1000" s="34"/>
@@ -59614,8 +59890,8 @@
       </c>
     </row>
     <row r="1001">
-      <c r="A1001" s="77"/>
-      <c r="B1001" s="78"/>
+      <c r="A1001" s="83"/>
+      <c r="B1001" s="84"/>
       <c r="C1001" s="34"/>
       <c r="D1001" s="34"/>
       <c r="E1001" s="34"/>
@@ -60326,15 +60602,21 @@
     <hyperlink r:id="rId299" ref="S736"/>
     <hyperlink r:id="rId300" ref="S737"/>
     <hyperlink r:id="rId301" ref="S738"/>
+    <hyperlink r:id="rId302" ref="S739"/>
+    <hyperlink r:id="rId303" ref="S740"/>
+    <hyperlink r:id="rId304" ref="S741"/>
+    <hyperlink r:id="rId305" ref="S742"/>
+    <hyperlink r:id="rId306" ref="S743"/>
+    <hyperlink r:id="rId307" ref="S744"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId302"/>
-  <legacyDrawing r:id="rId303"/>
+  <drawing r:id="rId308"/>
+  <legacyDrawing r:id="rId309"/>
   <tableParts count="2">
-    <tablePart r:id="rId306"/>
-    <tablePart r:id="rId307"/>
+    <tablePart r:id="rId312"/>
+    <tablePart r:id="rId313"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20201217
</commit_message>
<xml_diff>
--- a/Data/COVID-19_TW.xlsx
+++ b/Data/COVID-19_TW.xlsx
@@ -582,7 +582,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8519" uniqueCount="2633">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8605" uniqueCount="2650">
   <si>
     <t>案例</t>
   </si>
@@ -9464,6 +9464,61 @@
 12/13 二採
 12/15 確診</t>
   </si>
+  <si>
+    <t>#744</t>
+  </si>
+  <si>
+    <t>-12/1 菲律賓→台灣</t>
+  </si>
+  <si>
+    <t>12/14 採檢
+12/16 確診</t>
+  </si>
+  <si>
+    <t>新增7例境外移入COVID-19病例，分別自菲律賓、俄羅斯及美國入境</t>
+  </si>
+  <si>
+    <t>#745</t>
+  </si>
+  <si>
+    <t>-11/29 俄羅斯→台灣</t>
+  </si>
+  <si>
+    <t>俄羅斯籍藝文表演團體成員
+莫斯科古典芭蕾舞團，由邀請單位安排採檢</t>
+  </si>
+  <si>
+    <t>#746</t>
+  </si>
+  <si>
+    <t>#747</t>
+  </si>
+  <si>
+    <t>#748</t>
+  </si>
+  <si>
+    <t>#749</t>
+  </si>
+  <si>
+    <t>-11/29 菲律賓→台灣</t>
+  </si>
+  <si>
+    <t>漁工
+由仲介安排自費採檢</t>
+  </si>
+  <si>
+    <t>#750</t>
+  </si>
+  <si>
+    <t>3月-12/8 美國</t>
+  </si>
+  <si>
+    <t>12/13 採檢
+12/16 確診</t>
+  </si>
+  <si>
+    <t>畏寒 發燒 嗅覺異常 味覺異常</t>
+  </si>
 </sst>
 </file>
 
@@ -9473,7 +9528,7 @@
     <numFmt numFmtId="164" formatCode="mm&quot;月&quot;dd&quot;日 &quot;dddd"/>
     <numFmt numFmtId="165" formatCode="m/d"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -9559,9 +9614,6 @@
       <color rgb="FF0000FF"/>
     </font>
     <font/>
-    <font>
-      <color rgb="FF000000"/>
-    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -9607,7 +9659,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="80">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -9840,21 +9892,6 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="19" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -53122,7 +53159,7 @@
       </c>
     </row>
     <row r="743">
-      <c r="A743" s="77" t="s">
+      <c r="A743" s="16" t="s">
         <v>2626</v>
       </c>
       <c r="B743" s="6">
@@ -53131,7 +53168,7 @@
       <c r="C743" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D743" s="78" t="s">
+      <c r="D743" s="7" t="s">
         <v>116</v>
       </c>
       <c r="E743" s="7" t="s">
@@ -53141,29 +53178,29 @@
       <c r="G743" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H743" s="79" t="s">
+      <c r="H743" s="8" t="s">
         <v>2627</v>
       </c>
-      <c r="I743" s="80">
+      <c r="I743" s="9">
         <v>44165.0</v>
       </c>
-      <c r="J743" s="81" t="s">
+      <c r="J743" s="12" t="s">
         <v>1442</v>
       </c>
-      <c r="K743" s="82" t="s">
+      <c r="K743" s="13" t="s">
         <v>2628</v>
       </c>
-      <c r="L743" s="81" t="s">
+      <c r="L743" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="M743" s="82" t="s">
+      <c r="M743" s="13" t="s">
         <v>1442</v>
       </c>
       <c r="N743" s="25"/>
-      <c r="O743" s="79" t="s">
-        <v>85</v>
-      </c>
-      <c r="P